<commit_message>
Resource generator tools added
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="94">
   <si>
     <t>Key</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Öffnen</t>
   </si>
   <si>
-    <t>View Name</t>
-  </si>
-  <si>
     <t>General</t>
   </si>
   <si>
@@ -138,42 +135,18 @@
     <t>New Objective</t>
   </si>
   <si>
-    <t>New Objective NL</t>
-  </si>
-  <si>
-    <t>New Objective DE</t>
-  </si>
-  <si>
     <t>CreateObjective</t>
   </si>
   <si>
     <t>Objective title</t>
   </si>
   <si>
-    <t>Objective title NL</t>
-  </si>
-  <si>
-    <t>Objective title DE</t>
-  </si>
-  <si>
     <t>Objective title...</t>
   </si>
   <si>
-    <t>Objective title… NL</t>
-  </si>
-  <si>
-    <t>Objective title… DE</t>
-  </si>
-  <si>
     <t>Thumbnail</t>
   </si>
   <si>
-    <t>Thumbnail NL</t>
-  </si>
-  <si>
-    <t>Thumbnail DE</t>
-  </si>
-  <si>
     <t>CreateExperience</t>
   </si>
   <si>
@@ -201,30 +174,6 @@
     <t>Objectives in experience</t>
   </si>
   <si>
-    <t>New Experience NL</t>
-  </si>
-  <si>
-    <t>New Experience DE</t>
-  </si>
-  <si>
-    <t>Experience title NL</t>
-  </si>
-  <si>
-    <t>Experience title… NL</t>
-  </si>
-  <si>
-    <t>Objectives in experience NL</t>
-  </si>
-  <si>
-    <t>Experience title DE</t>
-  </si>
-  <si>
-    <t>Experience title… DE</t>
-  </si>
-  <si>
-    <t>Objectives in experience DE</t>
-  </si>
-  <si>
     <t>Objective</t>
   </si>
   <si>
@@ -234,12 +183,6 @@
     <t>Please, provide title for objective</t>
   </si>
   <si>
-    <t>Please, provide title for objective NL</t>
-  </si>
-  <si>
-    <t>Please, provide title for objective DE</t>
-  </si>
-  <si>
     <t>Question</t>
   </si>
   <si>
@@ -279,54 +222,12 @@
     <t>Explanations</t>
   </si>
   <si>
-    <t>Previous NL</t>
-  </si>
-  <si>
-    <t>Next NL</t>
-  </si>
-  <si>
-    <t>The answer options list is empty NL</t>
-  </si>
-  <si>
-    <t>Answer options NL</t>
-  </si>
-  <si>
-    <t>The explanations list is empty NL</t>
-  </si>
-  <si>
-    <t>Explanations NL</t>
-  </si>
-  <si>
-    <t>Explanations DE</t>
-  </si>
-  <si>
-    <t>Previous DE</t>
-  </si>
-  <si>
-    <t>Next DE</t>
-  </si>
-  <si>
-    <t>The answer options list is empty DE</t>
-  </si>
-  <si>
-    <t>Answer options DE</t>
-  </si>
-  <si>
-    <t>The explanations list is empty DE</t>
-  </si>
-  <si>
     <t>language</t>
   </si>
   <si>
     <t>Language</t>
   </si>
   <si>
-    <t>Language NL</t>
-  </si>
-  <si>
-    <t>Language DE</t>
-  </si>
-  <si>
     <t>backTo</t>
   </si>
   <si>
@@ -348,12 +249,6 @@
     <t>Related questions</t>
   </si>
   <si>
-    <t>Edit NL</t>
-  </si>
-  <si>
-    <t>Edit DE</t>
-  </si>
-  <si>
     <t>Leerdoelen</t>
   </si>
   <si>
@@ -400,6 +295,9 @@
   </si>
   <si>
     <t>Ähnliche Fragen</t>
+  </si>
+  <si>
+    <t>Page</t>
   </si>
 </sst>
 </file>
@@ -424,18 +322,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -453,7 +345,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,7 +650,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,7 +664,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>93</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -789,7 +681,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -826,10 +718,10 @@
         <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>117</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -840,10 +732,10 @@
         <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>118</v>
+        <v>83</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -896,10 +788,10 @@
         <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>121</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -910,43 +802,45 @@
         <v>25</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>122</v>
+        <v>87</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>123</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>124</v>
+        <v>89</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>125</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>102</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>5</v>
@@ -955,28 +849,36 @@
         <v>4</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>113</v>
-      </c>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>69</v>
-      </c>
-      <c r="B16" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E16" t="s">
-        <v>73</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -989,246 +891,210 @@
         <v>7</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>115</v>
-      </c>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" t="s">
-        <v>44</v>
-      </c>
-      <c r="E21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" t="s">
-        <v>51</v>
-      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" t="s">
-        <v>61</v>
-      </c>
-      <c r="E25" t="s">
-        <v>62</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" t="s">
-        <v>63</v>
-      </c>
-      <c r="E26" t="s">
-        <v>66</v>
-      </c>
+      <c r="B26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" t="s">
-        <v>64</v>
-      </c>
-      <c r="E27" t="s">
-        <v>67</v>
-      </c>
+      <c r="B27" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" t="s">
-        <v>65</v>
-      </c>
-      <c r="E28" t="s">
-        <v>68</v>
-      </c>
+      <c r="B28" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>74</v>
-      </c>
-      <c r="B30" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" t="s">
-        <v>87</v>
-      </c>
-      <c r="E30" t="s">
-        <v>94</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>76</v>
-      </c>
-      <c r="C31" t="s">
-        <v>82</v>
-      </c>
-      <c r="D31" t="s">
-        <v>88</v>
-      </c>
-      <c r="E31" t="s">
-        <v>95</v>
-      </c>
+      <c r="B31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>77</v>
-      </c>
-      <c r="C32" t="s">
-        <v>83</v>
-      </c>
-      <c r="D32" t="s">
-        <v>89</v>
-      </c>
-      <c r="E32" t="s">
-        <v>96</v>
-      </c>
+      <c r="B32" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>78</v>
-      </c>
-      <c r="C33" t="s">
-        <v>84</v>
-      </c>
-      <c r="D33" t="s">
-        <v>90</v>
-      </c>
-      <c r="E33" t="s">
-        <v>97</v>
-      </c>
+      <c r="B33" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>79</v>
-      </c>
-      <c r="C34" t="s">
-        <v>85</v>
-      </c>
-      <c r="D34" t="s">
-        <v>91</v>
-      </c>
-      <c r="E34" t="s">
-        <v>98</v>
-      </c>
+      <c r="B34" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>80</v>
-      </c>
-      <c r="C35" t="s">
-        <v>86</v>
-      </c>
-      <c r="D35" t="s">
-        <v>92</v>
-      </c>
-      <c r="E35" t="s">
-        <v>93</v>
-      </c>
+      <c r="B35" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>105</v>
-      </c>
-      <c r="B37" t="s">
-        <v>106</v>
-      </c>
-      <c r="C37" t="s">
-        <v>108</v>
-      </c>
-      <c r="D37" t="s">
-        <v>110</v>
-      </c>
-      <c r="E37" t="s">
-        <v>111</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>127</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
complete Answer Options Add/Edit/Delete
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="111">
   <si>
     <t>Key</t>
   </si>
@@ -343,6 +343,12 @@
   </si>
   <si>
     <t>Erfahrung</t>
+  </si>
+  <si>
+    <t>addAnswerOption</t>
+  </si>
+  <si>
+    <t>Click to add answer option</t>
   </si>
 </sst>
 </file>
@@ -692,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20:E20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,39 +1156,49 @@
       <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
+      <c r="B38" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>72</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="2" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EGD-22154 - Add/Delete Explanation
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="117">
   <si>
     <t>Key</t>
   </si>
@@ -349,6 +349,24 @@
   </si>
   <si>
     <t>Click to add answer option</t>
+  </si>
+  <si>
+    <t>clickToAddNewExplanation</t>
+  </si>
+  <si>
+    <t>Click here to add explanation…</t>
+  </si>
+  <si>
+    <t>remove</t>
+  </si>
+  <si>
+    <t>Remove</t>
+  </si>
+  <si>
+    <t>Wissen</t>
+  </si>
+  <si>
+    <t>Entfernen</t>
   </si>
 </sst>
 </file>
@@ -698,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,318 +906,334 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>54</v>
-      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-    </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>38</v>
-      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
       <c r="B23" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+      <c r="B26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>48</v>
-      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
       <c r="B28" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
+      <c r="B31" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
-        <v>109</v>
+        <v>61</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
+      <c r="B39" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>72</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="2" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bugs in EGD-22212 - Add/Edit/Delete Answer Option
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -345,12 +345,6 @@
     <t>Erfahrung</t>
   </si>
   <si>
-    <t>addAnswerOption</t>
-  </si>
-  <si>
-    <t>Click to add answer option</t>
-  </si>
-  <si>
     <t>clickToAddNewExplanation</t>
   </si>
   <si>
@@ -367,6 +361,12 @@
   </si>
   <si>
     <t>Entfernen</t>
+  </si>
+  <si>
+    <t>clickToAddNewAnswerOption</t>
+  </si>
+  <si>
+    <t>Click here to add answer option</t>
   </si>
 </sst>
 </file>
@@ -719,7 +719,7 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,16 +907,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13" t="s">
         <v>113</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
         <v>114</v>
-      </c>
-      <c r="D13" t="s">
-        <v>115</v>
-      </c>
-      <c r="E13" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1183,10 +1183,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -1230,10 +1230,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EGB-22153 - Display Question - added tooltips on expand-collapse btns
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="141">
   <si>
     <t>Key</t>
   </si>
@@ -415,6 +415,30 @@
   </si>
   <si>
     <t>Lernzieleigenschaften</t>
+  </si>
+  <si>
+    <t>expand</t>
+  </si>
+  <si>
+    <t>Expand</t>
+  </si>
+  <si>
+    <t>Uitklappen</t>
+  </si>
+  <si>
+    <t>Maximieren</t>
+  </si>
+  <si>
+    <t>collapse</t>
+  </si>
+  <si>
+    <t>Collapse</t>
+  </si>
+  <si>
+    <t>Inklappen</t>
+  </si>
+  <si>
+    <t>Minimieren</t>
   </si>
 </sst>
 </file>
@@ -764,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,55 +991,64 @@
         <v>109</v>
       </c>
     </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B15" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
@@ -1025,296 +1058,315 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-    </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
       <c r="B25" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
+      <c r="B27" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>43</v>
-      </c>
       <c r="B28" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>49</v>
-      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
       <c r="B30" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
+      <c r="B32" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="B33" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" t="s">
-        <v>61</v>
-      </c>
-      <c r="D34" t="s">
-        <v>95</v>
-      </c>
-      <c r="E34" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>112</v>
-      </c>
-      <c r="C35" t="s">
-        <v>113</v>
-      </c>
-      <c r="D35" t="s">
-        <v>114</v>
-      </c>
-      <c r="E35" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D36" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="E36" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>59</v>
+        <v>112</v>
       </c>
       <c r="C37" t="s">
-        <v>63</v>
+        <v>113</v>
       </c>
       <c r="D37" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E37" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>120</v>
+        <v>58</v>
       </c>
       <c r="C38" t="s">
-        <v>121</v>
+        <v>62</v>
       </c>
       <c r="D38" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E38" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>105</v>
+        <v>59</v>
       </c>
       <c r="C39" t="s">
-        <v>124</v>
+        <v>63</v>
       </c>
       <c r="D39" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E39" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40" t="s">
+        <v>121</v>
+      </c>
+      <c r="D40" t="s">
+        <v>122</v>
+      </c>
+      <c r="E40" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>105</v>
+      </c>
+      <c r="C41" t="s">
+        <v>124</v>
+      </c>
+      <c r="D41" t="s">
+        <v>125</v>
+      </c>
+      <c r="E41" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
         <v>110</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C42" t="s">
         <v>111</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D42" t="s">
         <v>127</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E42" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>68</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="2" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="E45" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="2" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D46" t="s">
         <v>131</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E46" t="s">
         <v>132</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EWD-22203 - Add tooltips
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="171">
   <si>
     <t>Key</t>
   </si>
@@ -439,6 +439,96 @@
   </si>
   <si>
     <t>Minimieren</t>
+  </si>
+  <si>
+    <t>correctAnswer</t>
+  </si>
+  <si>
+    <t>Correct answer</t>
+  </si>
+  <si>
+    <t>Juist antwoord</t>
+  </si>
+  <si>
+    <t>Korrekte Antwort</t>
+  </si>
+  <si>
+    <t>lastSaving</t>
+  </si>
+  <si>
+    <t>Last saving</t>
+  </si>
+  <si>
+    <t>addNewQuestion</t>
+  </si>
+  <si>
+    <t>Add new question</t>
+  </si>
+  <si>
+    <t>Nieuwe vraag toevoegen</t>
+  </si>
+  <si>
+    <t>Neue Fragen hinzufügen</t>
+  </si>
+  <si>
+    <t>numberOfRelatedQuestions</t>
+  </si>
+  <si>
+    <t>Number of related questions</t>
+  </si>
+  <si>
+    <t>Aantal gerelateerde vragen</t>
+  </si>
+  <si>
+    <t>Anzahl der zugehörigen Fragen</t>
+  </si>
+  <si>
+    <t>addNewObjective</t>
+  </si>
+  <si>
+    <t>Add new learning objective</t>
+  </si>
+  <si>
+    <t>Nieuw leerdoel toevoegen</t>
+  </si>
+  <si>
+    <t>Neues Lernziel hinzufügen</t>
+  </si>
+  <si>
+    <t>sortByTitle</t>
+  </si>
+  <si>
+    <t>Sort by title</t>
+  </si>
+  <si>
+    <t>Sorteren op titel</t>
+  </si>
+  <si>
+    <t>Nach Titel sortieren</t>
+  </si>
+  <si>
+    <t>ascending</t>
+  </si>
+  <si>
+    <t>Ascending</t>
+  </si>
+  <si>
+    <t>Oplopend</t>
+  </si>
+  <si>
+    <t>Aufsteigend</t>
+  </si>
+  <si>
+    <t>descending</t>
+  </si>
+  <si>
+    <t>Descending</t>
+  </si>
+  <si>
+    <t>Aflopend</t>
+  </si>
+  <si>
+    <t>Absteigend</t>
   </si>
 </sst>
 </file>
@@ -788,10 +878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,91 +1109,105 @@
         <v>140</v>
       </c>
     </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>33</v>
-      </c>
       <c r="B17" s="2" t="s">
-        <v>5</v>
+        <v>163</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>4</v>
+        <v>164</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>73</v>
+        <v>165</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>74</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>90</v>
+        <v>167</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>91</v>
+        <v>168</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>101</v>
+        <v>169</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+        <v>170</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="B21" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>7</v>
-      </c>
       <c r="B22" s="2" t="s">
-        <v>6</v>
+        <v>151</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>7</v>
+        <v>152</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>75</v>
+        <v>153</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>76</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>92</v>
+        <v>155</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>93</v>
+        <v>156</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>103</v>
+        <v>157</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>104</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1114,46 +1218,53 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
       <c r="B27" s="2" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
+        <v>93</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
@@ -1163,43 +1274,43 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1212,162 +1323,247 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>57</v>
-      </c>
-      <c r="C36" t="s">
-        <v>61</v>
-      </c>
-      <c r="D36" t="s">
-        <v>95</v>
-      </c>
-      <c r="E36" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>112</v>
-      </c>
-      <c r="C37" t="s">
-        <v>113</v>
-      </c>
-      <c r="D37" t="s">
-        <v>114</v>
-      </c>
-      <c r="E37" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>58</v>
-      </c>
-      <c r="C38" t="s">
-        <v>62</v>
-      </c>
-      <c r="D38" t="s">
-        <v>116</v>
-      </c>
-      <c r="E38" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>59</v>
-      </c>
-      <c r="C39" t="s">
-        <v>63</v>
-      </c>
-      <c r="D39" t="s">
-        <v>118</v>
-      </c>
-      <c r="E39" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>120</v>
-      </c>
-      <c r="C40" t="s">
-        <v>121</v>
-      </c>
-      <c r="D40" t="s">
-        <v>122</v>
-      </c>
-      <c r="E40" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>105</v>
+        <v>57</v>
       </c>
       <c r="C41" t="s">
-        <v>124</v>
+        <v>61</v>
       </c>
       <c r="D41" t="s">
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="E41" t="s">
-        <v>126</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
+        <v>112</v>
+      </c>
+      <c r="C42" t="s">
+        <v>113</v>
+      </c>
+      <c r="D42" t="s">
+        <v>114</v>
+      </c>
+      <c r="E42" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" t="s">
+        <v>62</v>
+      </c>
+      <c r="D43" t="s">
+        <v>116</v>
+      </c>
+      <c r="E43" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" t="s">
+        <v>118</v>
+      </c>
+      <c r="E44" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>120</v>
+      </c>
+      <c r="C45" t="s">
+        <v>121</v>
+      </c>
+      <c r="D45" t="s">
+        <v>122</v>
+      </c>
+      <c r="E45" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" t="s">
+        <v>124</v>
+      </c>
+      <c r="D46" t="s">
+        <v>125</v>
+      </c>
+      <c r="E46" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>110</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C47" t="s">
         <v>111</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D47" t="s">
         <v>127</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E47" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>68</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="2" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="E50" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="2" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D51" t="s">
         <v>131</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E51" t="s">
         <v>132</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>141</v>
+      </c>
+      <c r="C52" t="s">
+        <v>142</v>
+      </c>
+      <c r="D52" t="s">
+        <v>143</v>
+      </c>
+      <c r="E52" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>145</v>
+      </c>
+      <c r="C53" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>147</v>
+      </c>
+      <c r="C54" t="s">
+        <v>148</v>
+      </c>
+      <c r="D54" t="s">
+        <v>149</v>
+      </c>
+      <c r="E54" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EWD-22219 - Build Experience: Build/Download Experience MarkUp
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -552,9 +552,6 @@
     <t>experienceBuildingStatus</t>
   </si>
   <si>
-    <t>building…</t>
-  </si>
-  <si>
     <t>Samenstellen…</t>
   </si>
   <si>
@@ -564,25 +561,28 @@
     <t>experienceFailedStatus</t>
   </si>
   <si>
-    <t>failed</t>
-  </si>
-  <si>
-    <t>mislukt</t>
-  </si>
-  <si>
-    <t>fehlgeschlagen</t>
-  </si>
-  <si>
     <t>experienceCompleteStatus</t>
   </si>
   <si>
-    <t>complete</t>
-  </si>
-  <si>
-    <t>voltooid</t>
-  </si>
-  <si>
-    <t>vollständig</t>
+    <t>Building…</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Mislukt</t>
+  </si>
+  <si>
+    <t>Fehlgeschlagen</t>
+  </si>
+  <si>
+    <t>Vollständig</t>
+  </si>
+  <si>
+    <t>Voltooid</t>
+  </si>
+  <si>
+    <t>Complete</t>
   </si>
 </sst>
 </file>
@@ -942,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1361,41 +1361,41 @@
         <v>177</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>187</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Merged revision(s) 665-686 from branches/y.savchuk/CudQuestion: EWD-22323 - Create/update/delete question on questions list page functionality - update question title ........ EWD-22323 - Create/update/delete question on questions list page functionality ........ EWD-22323 - Create/update/delete question on questions list page functionality ........ EWD-22323 - Create/update/delete question on questions list page functionality ........
Former-commit-id: 8b4bfa6c2f5e97c9f474bb2b767231efb88309a8
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="11955"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId3"/>
-    <sheet sheetId="2" name="Sheet2" state="visible" r:id="rId4"/>
-    <sheet sheetId="3" name="Sheet3" state="visible" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="333">
   <si>
     <t>Page</t>
   </si>
@@ -819,7 +822,7 @@
     <t>Marked/highlighted text</t>
   </si>
   <si>
-    <t>Gemarkeerde/gehighlighte tekst </t>
+    <t>Gemarkeerde/gehighlighte tekst</t>
   </si>
   <si>
     <t>Markierter/hervorgehobener Text</t>
@@ -1006,147 +1009,95 @@
   </si>
   <si>
     <t>Normale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clickToAddNewQuestion   </t>
+  </si>
+  <si>
+    <t>Click here to add question</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="15">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11.0"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1154,9 +1105,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1241,1887 +1190,2195 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf fillId="2" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="1" applyFill="1"/>
-    <xf fillId="3" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="2" applyFill="1"/>
-    <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="3"/>
-    <xf fillId="4" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="4" applyFill="1"/>
-    <xf fillId="5" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="5" applyFill="1"/>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="6">
-      <alignment vertical="bottom" horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="6" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf fillId="7" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="7" applyFill="1"/>
-    <xf applyAlignment="1" fillId="8" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="8" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf fillId="9" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="9" applyFill="1"/>
-    <xf fillId="10" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="10" applyFill="1"/>
-    <xf applyAlignment="1" fillId="11" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="12" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="11" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf fillId="13" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="12" applyFill="1"/>
-    <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="13"/>
-    <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="14"/>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E114"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane topLeftCell="A2" ySplit="1.0" activePane="bottomLeft" state="frozen"/>
-      <selection sqref="A2" activeCell="A2" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="9.86" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" customWidth="1" max="1" width="26.14"/>
-    <col min="2" customWidth="1" max="2" width="33.0"/>
-    <col min="3" customWidth="1" max="3" width="28.71"/>
-    <col min="4" customWidth="1" max="4" width="42.14"/>
-    <col min="5" customWidth="1" max="5" width="39.43"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="33" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
+    <col min="4" max="4" width="42.140625" customWidth="1"/>
+    <col min="5" max="5" width="39.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row s="3" customFormat="1" r="1">
-      <c t="s" s="4" r="A1">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c t="s" s="4" r="B1">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c t="s" s="4" r="C1">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="4" r="D1">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c t="s" s="3" r="E1">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c t="s" s="10" r="A2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-      <c t="s" s="5" r="B2">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c t="s" s="5" r="C2">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="5" r="D2">
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
-      <c t="s" s="5" r="E2">
+      <c r="E2" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3">
-      <c s="10" r="A3"/>
-      <c t="s" s="5" r="B3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
-      <c t="s" s="5" r="C3">
+      <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
-      <c t="s" s="5" r="D3">
+      <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c t="s" s="5" r="E3">
+      <c r="E3" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4">
-      <c s="10" r="A4"/>
-      <c t="s" s="5" r="B4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="5" t="s">
         <v>14</v>
       </c>
-      <c t="s" s="5" r="C4">
+      <c r="C4" s="5" t="s">
         <v>15</v>
       </c>
-      <c t="s" s="5" r="D4">
+      <c r="D4" s="5" t="s">
         <v>16</v>
       </c>
-      <c t="s" s="5" r="E4">
+      <c r="E4" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5">
-      <c s="10" r="A5"/>
-      <c t="s" s="5" r="B5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
-      <c t="s" s="5" r="C5">
+      <c r="C5" s="5" t="s">
         <v>19</v>
       </c>
-      <c t="s" s="5" r="D5">
+      <c r="D5" s="5" t="s">
         <v>20</v>
       </c>
-      <c t="s" s="5" r="E5">
+      <c r="E5" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6">
-      <c s="10" r="A6"/>
-      <c t="s" s="5" r="B6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
-      <c t="s" s="5" r="C6">
+      <c r="C6" s="5" t="s">
         <v>23</v>
       </c>
-      <c t="s" s="5" r="D6">
+      <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
-      <c t="s" s="5" r="E6">
+      <c r="E6" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7">
-      <c s="10" r="A7"/>
-      <c t="s" s="5" r="B7">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="5" t="s">
         <v>24</v>
       </c>
-      <c t="s" s="5" r="C7">
+      <c r="C7" s="5" t="s">
         <v>25</v>
       </c>
-      <c t="s" s="5" r="D7">
+      <c r="D7" s="5" t="s">
         <v>25</v>
       </c>
-      <c t="s" s="5" r="E7">
+      <c r="E7" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8">
-      <c s="10" r="A8"/>
-      <c t="s" s="5" r="B8">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="5" t="s">
         <v>26</v>
       </c>
-      <c t="s" s="5" r="C8">
+      <c r="C8" s="5" t="s">
         <v>27</v>
       </c>
-      <c t="s" s="5" r="D8">
+      <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
-      <c t="s" s="5" r="E8">
+      <c r="E8" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9">
-      <c s="10" r="A9"/>
-      <c t="s" s="5" r="B9">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="5" t="s">
         <v>30</v>
       </c>
-      <c t="s" s="5" r="C9">
+      <c r="C9" s="5" t="s">
         <v>31</v>
       </c>
-      <c t="s" s="5" r="D9">
+      <c r="D9" s="5" t="s">
         <v>32</v>
       </c>
-      <c t="s" s="5" r="E9">
+      <c r="E9" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10">
-      <c s="10" r="A10"/>
-      <c t="s" s="5" r="B10">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="5" t="s">
         <v>34</v>
       </c>
-      <c t="s" s="5" r="C10">
+      <c r="C10" s="5" t="s">
         <v>35</v>
       </c>
-      <c t="s" s="5" r="D10">
+      <c r="D10" s="5" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="5" r="E10">
+      <c r="E10" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11">
-      <c s="10" r="A11"/>
-      <c t="s" s="5" r="B11">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="5" t="s">
         <v>38</v>
       </c>
-      <c t="s" s="5" r="C11">
+      <c r="C11" s="5" t="s">
         <v>39</v>
       </c>
-      <c t="s" s="5" r="D11">
+      <c r="D11" s="5" t="s">
         <v>40</v>
       </c>
-      <c t="s" s="5" r="E11">
+      <c r="E11" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12">
-      <c s="10" r="A12"/>
-      <c t="s" s="5" r="B12">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="5" t="s">
         <v>42</v>
       </c>
-      <c t="s" s="5" r="C12">
+      <c r="C12" s="5" t="s">
         <v>43</v>
       </c>
-      <c t="s" s="5" r="D12">
+      <c r="D12" s="5" t="s">
         <v>44</v>
       </c>
-      <c t="s" s="5" r="E12">
+      <c r="E12" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13">
-      <c s="15" r="A13"/>
-      <c t="s" s="5" r="B13">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="5" t="s">
         <v>46</v>
       </c>
-      <c t="s" s="5" r="C13">
+      <c r="C13" s="5" t="s">
         <v>47</v>
       </c>
-      <c t="s" s="5" r="D13">
+      <c r="D13" s="5" t="s">
         <v>48</v>
       </c>
-      <c t="s" s="5" r="E13">
+      <c r="E13" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14">
-      <c s="15" r="A14"/>
-      <c t="s" s="5" r="B14">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="5" t="s">
         <v>50</v>
       </c>
-      <c t="s" s="5" r="C14">
+      <c r="C14" s="5" t="s">
         <v>51</v>
       </c>
-      <c t="s" s="5" r="D14">
+      <c r="D14" s="5" t="s">
         <v>52</v>
       </c>
-      <c t="s" s="5" r="E14">
+      <c r="E14" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15">
-      <c s="15" r="A15"/>
-      <c t="s" s="5" r="B15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="5" t="s">
         <v>54</v>
       </c>
-      <c t="s" s="5" r="C15">
+      <c r="C15" s="5" t="s">
         <v>55</v>
       </c>
-      <c t="s" s="5" r="D15">
+      <c r="D15" s="5" t="s">
         <v>56</v>
       </c>
-      <c t="s" s="5" r="E15">
+      <c r="E15" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="16">
-      <c s="15" r="A16"/>
-      <c t="s" s="5" r="B16">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="5" t="s">
         <v>58</v>
       </c>
-      <c t="s" s="5" r="C16">
+      <c r="C16" s="5" t="s">
         <v>59</v>
       </c>
-      <c t="s" s="5" r="D16">
+      <c r="D16" s="5" t="s">
         <v>60</v>
       </c>
-      <c t="s" s="5" r="E16">
+      <c r="E16" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17">
-      <c s="15" r="A17"/>
-      <c t="s" s="5" r="B17">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="5" t="s">
         <v>62</v>
       </c>
-      <c t="s" s="5" r="C17">
+      <c r="C17" s="5" t="s">
         <v>63</v>
       </c>
-      <c t="s" s="5" r="D17">
+      <c r="D17" s="5" t="s">
         <v>64</v>
       </c>
-      <c t="s" s="5" r="E17">
+      <c r="E17" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18">
-      <c s="15" r="A18"/>
-      <c t="s" s="5" r="B18">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="5" t="s">
         <v>66</v>
       </c>
-      <c t="s" s="5" r="C18">
+      <c r="C18" s="5" t="s">
         <v>67</v>
       </c>
-      <c t="s" s="5" r="D18">
+      <c r="D18" s="5" t="s">
         <v>68</v>
       </c>
-      <c t="s" s="5" r="E18">
+      <c r="E18" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19">
-      <c s="10" r="A19"/>
-      <c s="10" r="B19"/>
-      <c s="10" r="C19"/>
-      <c s="10" r="D19"/>
-      <c s="10" r="E19"/>
-    </row>
-    <row r="20">
-      <c t="s" s="10" r="A20">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
         <v>70</v>
       </c>
-      <c t="s" s="5" r="B20">
+      <c r="B20" s="5" t="s">
         <v>71</v>
       </c>
-      <c t="s" s="5" r="C20">
+      <c r="C20" s="5" t="s">
         <v>72</v>
       </c>
-      <c t="s" s="5" r="D20">
+      <c r="D20" s="5" t="s">
         <v>73</v>
       </c>
-      <c t="s" s="5" r="E20">
+      <c r="E20" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="21">
-      <c s="10" r="A21"/>
-      <c t="s" s="5" r="B21">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="5" t="s">
         <v>75</v>
       </c>
-      <c t="s" s="5" r="C21">
+      <c r="C21" s="5" t="s">
         <v>76</v>
       </c>
-      <c t="s" s="5" r="D21">
+      <c r="D21" s="5" t="s">
         <v>77</v>
       </c>
-      <c t="s" s="5" r="E21">
+      <c r="E21" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="22">
-      <c s="10" r="A22"/>
-      <c t="s" s="5" r="B22">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="5" t="s">
         <v>79</v>
       </c>
-      <c t="s" s="5" r="C22">
+      <c r="C22" s="5" t="s">
         <v>80</v>
       </c>
-      <c t="s" s="5" r="D22">
+      <c r="D22" s="5" t="s">
         <v>81</v>
       </c>
-      <c t="s" s="5" r="E22">
+      <c r="E22" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="23">
-      <c s="10" r="A23"/>
-      <c t="s" s="5" r="B23">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="5" t="s">
         <v>83</v>
       </c>
-      <c t="s" s="5" r="C23">
+      <c r="C23" s="5" t="s">
         <v>84</v>
       </c>
-      <c t="s" s="5" r="D23">
+      <c r="D23" s="5" t="s">
         <v>85</v>
       </c>
-      <c t="s" s="5" r="E23">
+      <c r="E23" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="24">
-      <c s="10" r="A24"/>
-      <c s="10" r="B24"/>
-      <c s="10" r="C24"/>
-      <c s="10" r="D24"/>
-      <c s="15" r="E24"/>
-    </row>
-    <row r="25">
-      <c t="s" s="10" r="A25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="14"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
         <v>87</v>
       </c>
-      <c t="s" s="1" r="B25">
+      <c r="B25" s="1" t="s">
         <v>88</v>
       </c>
-      <c t="s" s="1" r="C25">
+      <c r="C25" s="1" t="s">
         <v>89</v>
       </c>
-      <c s="1" r="D25"/>
-      <c s="1" r="E25"/>
-    </row>
-    <row r="26">
-      <c s="10" r="A26"/>
-      <c s="10" r="B26"/>
-      <c s="10" r="C26"/>
-      <c s="10" r="D26"/>
-      <c s="15" r="E26"/>
-    </row>
-    <row r="27">
-      <c t="s" s="15" r="A27">
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="14"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
         <v>90</v>
       </c>
-      <c t="s" s="5" r="B27">
+      <c r="B27" s="5" t="s">
         <v>91</v>
       </c>
-      <c t="s" s="5" r="C27">
+      <c r="C27" s="5" t="s">
         <v>90</v>
       </c>
-      <c t="s" s="5" r="D27">
+      <c r="D27" s="5" t="s">
         <v>92</v>
       </c>
-      <c t="s" s="5" r="E27">
+      <c r="E27" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="28">
-      <c s="15" r="A28"/>
-      <c t="s" s="5" r="B28">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+      <c r="B28" s="5" t="s">
         <v>94</v>
       </c>
-      <c t="s" s="5" r="C28">
+      <c r="C28" s="5" t="s">
         <v>95</v>
       </c>
-      <c t="s" s="5" r="D28">
+      <c r="D28" s="5" t="s">
         <v>96</v>
       </c>
-      <c t="s" s="5" r="E28">
+      <c r="E28" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="29">
-      <c s="15" r="A29"/>
-      <c t="s" s="5" r="B29">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
+      <c r="B29" s="5" t="s">
         <v>98</v>
       </c>
-      <c t="s" s="5" r="C29">
+      <c r="C29" s="5" t="s">
         <v>99</v>
       </c>
-      <c t="s" s="5" r="D29">
+      <c r="D29" s="5" t="s">
         <v>100</v>
       </c>
-      <c t="s" s="5" r="E29">
+      <c r="E29" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="30">
-      <c s="15" r="A30"/>
-      <c t="s" s="5" r="B30">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
+      <c r="B30" s="5" t="s">
         <v>101</v>
       </c>
-      <c t="s" s="5" r="C30">
+      <c r="C30" s="5" t="s">
         <v>102</v>
       </c>
-      <c t="s" s="5" r="D30">
+      <c r="D30" s="5" t="s">
         <v>103</v>
       </c>
-      <c t="s" s="5" r="E30">
+      <c r="E30" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31">
-      <c s="15" r="A31"/>
-      <c t="s" s="5" r="B31">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="B31" s="5" t="s">
         <v>104</v>
       </c>
-      <c t="s" s="5" r="C31">
+      <c r="C31" s="5" t="s">
         <v>105</v>
       </c>
-      <c t="s" s="5" r="D31">
+      <c r="D31" s="5" t="s">
         <v>106</v>
       </c>
-      <c t="s" s="5" r="E31">
+      <c r="E31" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="32">
-      <c s="15" r="A32"/>
-      <c t="s" s="5" r="B32">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
+      <c r="B32" s="5" t="s">
         <v>108</v>
       </c>
-      <c t="s" s="5" r="C32">
+      <c r="C32" s="5" t="s">
         <v>109</v>
       </c>
-      <c t="s" s="5" r="D32">
+      <c r="D32" s="5" t="s">
         <v>110</v>
       </c>
-      <c t="s" s="5" r="E32">
+      <c r="E32" s="5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="33">
-      <c s="15" r="A33"/>
-      <c t="s" s="5" r="B33">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
+      <c r="B33" s="5" t="s">
         <v>112</v>
       </c>
-      <c t="s" s="5" r="C33">
+      <c r="C33" s="5" t="s">
         <v>113</v>
       </c>
-      <c t="s" s="5" r="D33">
+      <c r="D33" s="5" t="s">
         <v>114</v>
       </c>
-      <c t="s" s="5" r="E33">
+      <c r="E33" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="34">
-      <c s="15" r="A34"/>
-      <c s="15" r="B34"/>
-      <c s="15" r="C34"/>
-      <c s="15" r="D34"/>
-      <c s="15" r="E34"/>
-    </row>
-    <row r="35">
-      <c t="s" s="15" r="A35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
         <v>116</v>
       </c>
-      <c t="s" s="11" r="B35">
+      <c r="B35" s="10" t="s">
         <v>117</v>
       </c>
-      <c t="s" s="11" r="C35">
+      <c r="C35" s="10" t="s">
         <v>118</v>
       </c>
-      <c s="11" r="D35"/>
-      <c s="11" r="E35"/>
-    </row>
-    <row r="36">
-      <c s="15" r="A36"/>
-      <c t="s" s="11" r="B36">
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
+      <c r="B36" s="10" t="s">
         <v>119</v>
       </c>
-      <c t="s" s="11" r="C36">
+      <c r="C36" s="10" t="s">
         <v>120</v>
       </c>
-      <c s="11" r="D36"/>
-      <c s="11" r="E36"/>
-    </row>
-    <row r="37">
-      <c s="15" r="A37"/>
-      <c t="s" s="11" r="B37">
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="10" t="s">
         <v>121</v>
       </c>
-      <c t="s" s="11" r="C37">
+      <c r="C37" s="10" t="s">
         <v>122</v>
       </c>
-      <c s="11" r="D37"/>
-      <c s="11" r="E37"/>
-    </row>
-    <row r="38">
-      <c s="15" r="A38"/>
-      <c t="s" s="11" r="B38">
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="14"/>
+      <c r="B38" s="10" t="s">
         <v>123</v>
       </c>
-      <c t="s" s="11" r="C38">
+      <c r="C38" s="10" t="s">
         <v>124</v>
       </c>
-      <c s="11" r="D38"/>
-      <c s="11" r="E38"/>
-    </row>
-    <row r="39">
-      <c s="15" r="A39"/>
-      <c s="11" r="B39"/>
-      <c s="11" r="C39"/>
-      <c s="11" r="D39"/>
-      <c s="11" r="E39"/>
-    </row>
-    <row r="40">
-      <c t="s" s="15" r="A40">
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="14"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
         <v>125</v>
       </c>
-      <c t="s" s="11" r="B40">
+      <c r="B40" s="10" t="s">
         <v>126</v>
       </c>
-      <c t="s" s="11" r="C40">
+      <c r="C40" s="10" t="s">
         <v>127</v>
       </c>
-      <c s="11" r="D40"/>
-      <c s="11" r="E40"/>
-    </row>
-    <row r="41">
-      <c s="15" r="A41"/>
-      <c t="s" s="11" r="B41">
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="14"/>
+      <c r="B41" s="10" t="s">
         <v>128</v>
       </c>
-      <c t="s" s="11" r="C41">
+      <c r="C41" s="10" t="s">
         <v>129</v>
       </c>
-      <c s="11" r="D41"/>
-      <c s="11" r="E41"/>
-    </row>
-    <row r="42">
-      <c s="15" r="A42"/>
-      <c t="s" s="11" r="B42">
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="14"/>
+      <c r="B42" s="10" t="s">
         <v>130</v>
       </c>
-      <c t="s" s="11" r="C42">
+      <c r="C42" s="10" t="s">
         <v>131</v>
       </c>
-      <c s="11" r="D42"/>
-      <c s="11" r="E42"/>
-    </row>
-    <row r="43">
-      <c s="15" r="A43"/>
-      <c t="s" s="11" r="B43">
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="14"/>
+      <c r="B43" s="10" t="s">
         <v>132</v>
       </c>
-      <c t="s" s="11" r="C43">
+      <c r="C43" s="10" t="s">
         <v>133</v>
       </c>
-      <c s="11" r="D43"/>
-      <c s="11" r="E43"/>
-    </row>
-    <row r="44">
-      <c s="15" r="A44"/>
-      <c s="15" r="B44"/>
-      <c s="15" r="C44"/>
-      <c s="15" r="D44"/>
-      <c s="15" r="E44"/>
-    </row>
-    <row r="45">
-      <c t="s" s="15" r="A45">
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="14"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="14" t="s">
         <v>134</v>
       </c>
-      <c t="s" s="5" r="B45">
+      <c r="B45" s="5" t="s">
         <v>135</v>
       </c>
-      <c t="s" s="5" r="C45">
+      <c r="C45" s="5" t="s">
         <v>136</v>
       </c>
-      <c t="s" s="5" r="D45">
+      <c r="D45" s="5" t="s">
         <v>137</v>
       </c>
-      <c t="s" s="5" r="E45">
+      <c r="E45" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="46">
-      <c s="15" r="A46"/>
-      <c t="s" s="5" r="B46">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="14"/>
+      <c r="B46" s="5" t="s">
         <v>138</v>
       </c>
-      <c t="s" s="5" r="C46">
+      <c r="C46" s="5" t="s">
         <v>139</v>
       </c>
-      <c t="s" s="5" r="D46">
+      <c r="D46" s="5" t="s">
         <v>140</v>
       </c>
-      <c t="s" s="5" r="E46">
+      <c r="E46" s="5" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="47">
-      <c s="15" r="A47"/>
-      <c t="s" s="5" r="B47">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="14"/>
+      <c r="B47" s="5" t="s">
         <v>142</v>
       </c>
-      <c t="s" s="5" r="C47">
+      <c r="C47" s="5" t="s">
         <v>143</v>
       </c>
-      <c t="s" s="5" r="D47">
+      <c r="D47" s="5" t="s">
         <v>144</v>
       </c>
-      <c t="s" s="5" r="E47">
+      <c r="E47" s="5" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="48">
-      <c s="15" r="A48"/>
-      <c t="s" s="5" r="B48">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="14"/>
+      <c r="B48" s="5" t="s">
         <v>146</v>
       </c>
-      <c t="s" s="5" r="C48">
+      <c r="C48" s="5" t="s">
         <v>147</v>
       </c>
-      <c t="s" s="5" r="D48">
+      <c r="D48" s="5" t="s">
         <v>148</v>
       </c>
-      <c t="s" s="5" r="E48">
+      <c r="E48" s="5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="49">
-      <c s="15" r="A49"/>
-      <c t="s" s="5" r="B49">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="14"/>
+      <c r="B49" s="5" t="s">
         <v>150</v>
       </c>
-      <c t="s" s="5" r="C49">
+      <c r="C49" s="5" t="s">
         <v>151</v>
       </c>
-      <c t="s" s="5" r="D49">
+      <c r="D49" s="5" t="s">
         <v>152</v>
       </c>
-      <c t="s" s="5" r="E49">
+      <c r="E49" s="5" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="50">
-      <c s="15" r="A50"/>
-      <c t="s" s="5" r="B50">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="14"/>
+      <c r="B50" s="5" t="s">
         <v>154</v>
       </c>
-      <c t="s" s="5" r="C50">
+      <c r="C50" s="5" t="s">
         <v>155</v>
       </c>
-      <c t="s" s="5" r="D50">
+      <c r="D50" s="5" t="s">
         <v>156</v>
       </c>
-      <c t="s" s="5" r="E50">
+      <c r="E50" s="5" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="51">
-      <c s="15" r="A51"/>
-      <c t="s" s="5" r="B51">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="14"/>
+      <c r="B51" s="5" t="s">
         <v>158</v>
       </c>
-      <c t="s" s="5" r="C51">
+      <c r="C51" s="5" t="s">
         <v>159</v>
       </c>
-      <c t="s" s="5" r="D51">
+      <c r="D51" s="5" t="s">
         <v>160</v>
       </c>
-      <c t="s" s="5" r="E51">
+      <c r="E51" s="5" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="52">
-      <c s="15" r="A52"/>
-      <c t="s" s="5" r="B52">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="14"/>
+      <c r="B52" s="5" t="s">
         <v>162</v>
       </c>
-      <c t="s" s="5" r="C52">
+      <c r="C52" s="5" t="s">
         <v>163</v>
       </c>
-      <c t="s" s="5" r="D52">
+      <c r="D52" s="5" t="s">
         <v>164</v>
       </c>
-      <c t="s" s="5" r="E52">
+      <c r="E52" s="5" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="53">
-      <c s="15" r="A53"/>
-      <c t="s" s="8" r="B53">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="14"/>
+      <c r="B53" s="7" t="s">
         <v>166</v>
       </c>
-      <c t="s" s="8" r="C53">
+      <c r="C53" s="7" t="s">
         <v>167</v>
       </c>
-      <c s="8" r="D53"/>
-      <c s="8" r="E53"/>
-    </row>
-    <row r="54">
-      <c s="15" r="A54"/>
-      <c s="15" r="B54"/>
-      <c s="15" r="C54"/>
-      <c s="15" r="D54"/>
-      <c s="15" r="E54"/>
-    </row>
-    <row r="55">
-      <c t="s" s="15" r="A55">
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="14"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="14" t="s">
         <v>168</v>
       </c>
-      <c t="s" s="5" r="B55">
+      <c r="B55" s="5" t="s">
         <v>169</v>
       </c>
-      <c t="s" s="5" r="C55">
+      <c r="C55" s="5" t="s">
         <v>170</v>
       </c>
-      <c t="s" s="5" r="D55">
+      <c r="D55" s="5" t="s">
         <v>171</v>
       </c>
-      <c t="s" s="5" r="E55">
+      <c r="E55" s="5" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="56">
-      <c s="15" r="A56"/>
-      <c t="s" s="5" r="B56">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="14"/>
+      <c r="B56" s="5" t="s">
         <v>173</v>
       </c>
-      <c t="s" s="5" r="C56">
+      <c r="C56" s="5" t="s">
         <v>174</v>
       </c>
-      <c t="s" s="5" r="D56">
+      <c r="D56" s="5" t="s">
         <v>175</v>
       </c>
-      <c t="s" s="5" r="E56">
+      <c r="E56" s="5" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="57">
-      <c s="16" r="A57"/>
-      <c t="s" s="5" r="B57">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="15"/>
+      <c r="B57" s="5" t="s">
         <v>177</v>
       </c>
-      <c t="s" s="5" r="C57">
+      <c r="C57" s="5" t="s">
         <v>178</v>
       </c>
-      <c t="s" s="5" r="D57">
+      <c r="D57" s="5" t="s">
         <v>179</v>
       </c>
-      <c t="s" s="5" r="E57">
+      <c r="E57" s="5" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="58">
-      <c s="16" r="A58"/>
-      <c t="s" s="5" r="B58">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="15"/>
+      <c r="B58" s="5" t="s">
         <v>181</v>
       </c>
-      <c t="s" s="5" r="C58">
+      <c r="C58" s="5" t="s">
         <v>182</v>
       </c>
-      <c t="s" s="5" r="D58">
+      <c r="D58" s="5" t="s">
         <v>183</v>
       </c>
-      <c t="s" s="5" r="E58">
+      <c r="E58" s="5" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="59">
-      <c s="16" r="A59"/>
-      <c t="s" s="8" r="B59">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="15"/>
+      <c r="B59" s="7" t="s">
         <v>185</v>
       </c>
-      <c t="s" s="8" r="C59">
+      <c r="C59" s="7" t="s">
         <v>186</v>
       </c>
-      <c s="8" r="D59"/>
-      <c s="8" r="E59"/>
-    </row>
-    <row r="60">
-      <c s="16" r="A60"/>
-      <c t="s" s="2" r="B60">
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="15"/>
+      <c r="B60" s="2" t="s">
         <v>187</v>
       </c>
-      <c t="s" s="2" r="C60">
+      <c r="C60" s="2" t="s">
         <v>188</v>
       </c>
-      <c s="2" r="D60"/>
-      <c s="2" r="E60"/>
-    </row>
-    <row r="61">
-      <c s="16" r="A61"/>
-      <c t="s" s="5" r="B61">
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="15"/>
+      <c r="B61" s="5" t="s">
         <v>189</v>
       </c>
-      <c t="s" s="5" r="C61">
+      <c r="C61" s="5" t="s">
         <v>190</v>
       </c>
-      <c t="s" s="5" r="D61">
+      <c r="D61" s="5" t="s">
         <v>191</v>
       </c>
-      <c t="s" s="5" r="E61">
+      <c r="E61" s="5" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="62">
-      <c s="16" r="A62"/>
-      <c s="15" r="B62"/>
-      <c s="15" r="C62"/>
-      <c s="15" r="D62"/>
-      <c s="15" r="E62"/>
-    </row>
-    <row r="63">
-      <c t="s" s="16" r="A63">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="15"/>
+      <c r="B62" s="16" t="s">
+        <v>331</v>
+      </c>
+      <c r="C62" s="16" t="s">
+        <v>332</v>
+      </c>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="15"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="15" t="s">
         <v>193</v>
       </c>
-      <c t="s" s="5" r="B63">
+      <c r="B64" s="5" t="s">
         <v>194</v>
       </c>
-      <c t="s" s="5" r="C63">
+      <c r="C64" s="5" t="s">
         <v>195</v>
       </c>
-      <c t="s" s="5" r="D63">
+      <c r="D64" s="5" t="s">
         <v>196</v>
       </c>
-      <c t="s" s="5" r="E63">
+      <c r="E64" s="5" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="64">
-      <c s="16" r="A64"/>
-      <c t="s" s="5" r="B64">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="15"/>
+      <c r="B65" s="5" t="s">
         <v>198</v>
       </c>
-      <c t="s" s="5" r="C64">
+      <c r="C65" s="5" t="s">
         <v>199</v>
       </c>
-      <c t="s" s="5" r="D64">
+      <c r="D65" s="5" t="s">
         <v>200</v>
       </c>
-      <c t="s" s="5" r="E64">
+      <c r="E65" s="5" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="65">
-      <c s="16" r="A65"/>
-      <c t="s" s="5" r="B65">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="15"/>
+      <c r="B66" s="5" t="s">
         <v>202</v>
       </c>
-      <c t="s" s="5" r="C65">
+      <c r="C66" s="5" t="s">
         <v>203</v>
       </c>
-      <c t="s" s="5" r="D65">
+      <c r="D66" s="5" t="s">
         <v>204</v>
       </c>
-      <c t="s" s="5" r="E65">
+      <c r="E66" s="5" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="66">
-      <c s="16" r="A66"/>
-      <c t="s" s="5" r="B66">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="15"/>
+      <c r="B67" s="5" t="s">
         <v>206</v>
       </c>
-      <c t="s" s="5" r="C66">
+      <c r="C67" s="5" t="s">
         <v>207</v>
       </c>
-      <c t="s" s="5" r="D66">
+      <c r="D67" s="5" t="s">
         <v>208</v>
       </c>
-      <c t="s" s="5" r="E66">
+      <c r="E67" s="5" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="67">
-      <c s="16" r="A67"/>
-      <c t="s" s="5" r="B67">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="15"/>
+      <c r="B68" s="5" t="s">
         <v>210</v>
       </c>
-      <c t="s" s="5" r="C67">
+      <c r="C68" s="5" t="s">
         <v>211</v>
       </c>
-      <c t="s" s="5" r="D67">
+      <c r="D68" s="5" t="s">
         <v>212</v>
       </c>
-      <c t="s" s="5" r="E67">
+      <c r="E68" s="5" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="68">
-      <c s="16" r="A68"/>
-      <c t="s" s="5" r="B68">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="15"/>
+      <c r="B69" s="5" t="s">
         <v>214</v>
       </c>
-      <c t="s" s="5" r="C68">
+      <c r="C69" s="5" t="s">
         <v>215</v>
       </c>
-      <c t="s" s="5" r="D68">
+      <c r="D69" s="5" t="s">
         <v>216</v>
       </c>
-      <c t="s" s="5" r="E68">
+      <c r="E69" s="5" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="69">
-      <c s="16" r="A69"/>
-      <c t="s" s="5" r="B69">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="15"/>
+      <c r="B70" s="5" t="s">
         <v>217</v>
       </c>
-      <c t="s" s="5" r="C69">
+      <c r="C70" s="5" t="s">
         <v>218</v>
       </c>
-      <c t="s" s="5" r="D69">
+      <c r="D70" s="5" t="s">
         <v>219</v>
       </c>
-      <c t="s" s="5" r="E69">
+      <c r="E70" s="5" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="70">
-      <c s="16" r="A70"/>
-      <c t="s" s="5" r="B70">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="15"/>
+      <c r="B71" s="5" t="s">
         <v>221</v>
       </c>
-      <c t="s" s="5" r="C70">
+      <c r="C71" s="5" t="s">
         <v>222</v>
       </c>
-      <c t="s" s="5" r="D70">
+      <c r="D71" s="5" t="s">
         <v>223</v>
       </c>
-      <c t="s" s="5" r="E70">
+      <c r="E71" s="5" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="71">
-      <c s="16" r="A71"/>
-      <c t="s" s="5" r="B71">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="15"/>
+      <c r="B72" s="5" t="s">
         <v>225</v>
       </c>
-      <c t="s" s="5" r="C71">
+      <c r="C72" s="5" t="s">
         <v>226</v>
       </c>
-      <c t="s" s="5" r="D71">
+      <c r="D72" s="5" t="s">
         <v>227</v>
       </c>
-      <c t="s" s="5" r="E71">
+      <c r="E72" s="5" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="72">
-      <c s="16" r="A72"/>
-      <c t="s" s="5" r="B72">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="15"/>
+      <c r="B73" s="5" t="s">
         <v>229</v>
       </c>
-      <c t="s" s="5" r="C72">
+      <c r="C73" s="5" t="s">
         <v>230</v>
       </c>
-      <c t="s" s="5" r="D72">
+      <c r="D73" s="5" t="s">
         <v>231</v>
       </c>
-      <c t="s" s="5" r="E72">
+      <c r="E73" s="5" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="73">
-      <c s="16" r="A73"/>
-      <c t="s" s="5" r="B73">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="15"/>
+      <c r="B74" s="5" t="s">
         <v>233</v>
       </c>
-      <c t="s" s="5" r="C73">
+      <c r="C74" s="5" t="s">
         <v>234</v>
       </c>
-      <c t="s" s="5" r="D73">
+      <c r="D74" s="5" t="s">
         <v>235</v>
       </c>
-      <c t="s" s="5" r="E73">
+      <c r="E74" s="5" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="74">
-      <c s="16" r="A74"/>
-      <c t="s" s="5" r="B74">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="15"/>
+      <c r="B75" s="5" t="s">
         <v>237</v>
       </c>
-      <c t="s" s="5" r="C74">
+      <c r="C75" s="5" t="s">
         <v>238</v>
       </c>
-      <c t="s" s="5" r="D74">
+      <c r="D75" s="5" t="s">
         <v>238</v>
       </c>
-      <c t="s" s="5" r="E74">
+      <c r="E75" s="5" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="75">
-      <c s="16" r="A75"/>
-      <c t="s" s="5" r="B75">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="15"/>
+      <c r="B76" s="5" t="s">
         <v>240</v>
       </c>
-      <c t="s" s="5" r="C75">
+      <c r="C76" s="5" t="s">
         <v>241</v>
       </c>
-      <c t="s" s="5" r="D75">
+      <c r="D76" s="5" t="s">
         <v>241</v>
       </c>
-      <c t="s" s="5" r="E75">
+      <c r="E76" s="5" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="76">
-      <c s="16" r="A76"/>
-      <c t="s" s="5" r="B76">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="15"/>
+      <c r="B77" s="5" t="s">
         <v>243</v>
       </c>
-      <c t="s" s="5" r="C76">
+      <c r="C77" s="5" t="s">
         <v>244</v>
       </c>
-      <c t="s" s="5" r="D76">
+      <c r="D77" s="5" t="s">
         <v>245</v>
       </c>
-      <c t="s" s="5" r="E76">
+      <c r="E77" s="5" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="77">
-      <c s="16" r="A77"/>
-      <c t="s" s="7" r="B77">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="15"/>
+      <c r="B78" s="6" t="s">
         <v>247</v>
       </c>
-      <c t="s" s="5" r="C77">
+      <c r="C78" s="5" t="s">
         <v>248</v>
       </c>
-      <c t="s" s="5" r="D77">
+      <c r="D78" s="5" t="s">
         <v>249</v>
       </c>
-      <c t="s" s="5" r="E77">
+      <c r="E78" s="5" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="78">
-      <c s="16" r="A78"/>
-      <c t="s" s="5" r="B78">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="15"/>
+      <c r="B79" s="5" t="s">
         <v>250</v>
       </c>
-      <c t="s" s="5" r="C78">
+      <c r="C79" s="5" t="s">
         <v>251</v>
       </c>
-      <c t="s" s="5" r="D78">
+      <c r="D79" s="5" t="s">
         <v>252</v>
       </c>
-      <c t="s" s="5" r="E78">
+      <c r="E79" s="5" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="79">
-      <c s="16" r="A79"/>
-      <c t="s" s="5" r="B79">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="15"/>
+      <c r="B80" s="5" t="s">
         <v>254</v>
       </c>
-      <c t="s" s="5" r="C79">
+      <c r="C80" s="5" t="s">
         <v>255</v>
       </c>
-      <c t="s" s="5" r="D79">
+      <c r="D80" s="5" t="s">
         <v>256</v>
       </c>
-      <c t="s" s="5" r="E79">
+      <c r="E80" s="5" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="80">
-      <c s="16" r="A80"/>
-      <c t="s" s="5" r="B80">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="15"/>
+      <c r="B81" s="5" t="s">
         <v>258</v>
       </c>
-      <c t="s" s="5" r="C80">
+      <c r="C81" s="5" t="s">
         <v>259</v>
       </c>
-      <c t="s" s="5" r="D80">
+      <c r="D81" s="5" t="s">
         <v>260</v>
       </c>
-      <c t="s" s="5" r="E80">
+      <c r="E81" s="5" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="81">
-      <c s="16" r="A81"/>
-      <c t="s" s="5" r="B81">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="15"/>
+      <c r="B82" s="5" t="s">
         <v>262</v>
       </c>
-      <c t="s" s="5" r="C81">
+      <c r="C82" s="5" t="s">
         <v>263</v>
       </c>
-      <c t="s" s="5" r="D81">
+      <c r="D82" s="5" t="s">
         <v>264</v>
       </c>
-      <c t="s" s="5" r="E81">
+      <c r="E82" s="5" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="82">
-      <c s="16" r="A82"/>
-      <c t="s" s="5" r="B82">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="15"/>
+      <c r="B83" s="5" t="s">
         <v>266</v>
       </c>
-      <c t="s" s="5" r="C82">
+      <c r="C83" s="5" t="s">
         <v>267</v>
       </c>
-      <c t="s" s="5" r="D82">
+      <c r="D83" s="5" t="s">
         <v>268</v>
       </c>
-      <c t="s" s="5" r="E82">
+      <c r="E83" s="5" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="83">
-      <c s="16" r="A83"/>
-      <c t="s" s="5" r="B83">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="15"/>
+      <c r="B84" s="5" t="s">
         <v>270</v>
       </c>
-      <c t="s" s="5" r="C83">
+      <c r="C84" s="5" t="s">
         <v>271</v>
       </c>
-      <c t="s" s="5" r="D83">
+      <c r="D84" s="5" t="s">
         <v>272</v>
       </c>
-      <c t="s" s="5" r="E83">
+      <c r="E84" s="5" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="84">
-      <c s="16" r="A84"/>
-      <c t="s" s="5" r="B84">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="15"/>
+      <c r="B85" s="5" t="s">
         <v>274</v>
       </c>
-      <c t="s" s="5" r="C84">
+      <c r="C85" s="5" t="s">
         <v>275</v>
       </c>
-      <c t="s" s="5" r="D84">
+      <c r="D85" s="5" t="s">
         <v>276</v>
       </c>
-      <c t="s" s="5" r="E84">
+      <c r="E85" s="5" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="85">
-      <c s="16" r="A85"/>
-      <c t="s" s="5" r="B85">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="15"/>
+      <c r="B86" s="5" t="s">
         <v>278</v>
       </c>
-      <c t="s" s="5" r="C85">
+      <c r="C86" s="5" t="s">
         <v>279</v>
       </c>
-      <c t="s" s="5" r="D85">
+      <c r="D86" s="5" t="s">
         <v>280</v>
       </c>
-      <c t="s" s="5" r="E85">
+      <c r="E86" s="5" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="86">
-      <c s="16" r="A86"/>
-      <c t="s" s="5" r="B86">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="15"/>
+      <c r="B87" s="5" t="s">
         <v>282</v>
       </c>
-      <c t="s" s="5" r="C86">
+      <c r="C87" s="5" t="s">
         <v>283</v>
       </c>
-      <c t="s" s="5" r="D86">
+      <c r="D87" s="5" t="s">
         <v>284</v>
       </c>
-      <c t="s" s="5" r="E86">
+      <c r="E87" s="5" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="87">
-      <c s="16" r="A87"/>
-      <c t="s" s="5" r="B87">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="15"/>
+      <c r="B88" s="5" t="s">
         <v>286</v>
       </c>
-      <c t="s" s="5" r="C87">
+      <c r="C88" s="5" t="s">
         <v>287</v>
       </c>
-      <c t="s" s="5" r="D87">
+      <c r="D88" s="5" t="s">
         <v>288</v>
       </c>
-      <c t="s" s="5" r="E87">
+      <c r="E88" s="5" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="88">
-      <c s="16" r="A88"/>
-      <c t="s" s="5" r="B88">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="15"/>
+      <c r="B89" s="5" t="s">
         <v>290</v>
       </c>
-      <c t="s" s="5" r="C88">
+      <c r="C89" s="5" t="s">
         <v>291</v>
       </c>
-      <c t="s" s="5" r="D88">
+      <c r="D89" s="5" t="s">
         <v>292</v>
       </c>
-      <c t="s" s="5" r="E88">
+      <c r="E89" s="5" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="89">
-      <c s="16" r="A89"/>
-      <c t="s" s="5" r="B89">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="15"/>
+      <c r="B90" s="5" t="s">
         <v>294</v>
       </c>
-      <c t="s" s="5" r="C89">
+      <c r="C90" s="5" t="s">
         <v>295</v>
       </c>
-      <c t="s" s="5" r="D89">
+      <c r="D90" s="5" t="s">
         <v>296</v>
       </c>
-      <c t="s" s="5" r="E89">
+      <c r="E90" s="5" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="90">
-      <c s="16" r="A90"/>
-      <c t="s" s="5" r="B90">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="15"/>
+      <c r="B91" s="5" t="s">
         <v>298</v>
       </c>
-      <c t="s" s="5" r="C90">
+      <c r="C91" s="5" t="s">
         <v>299</v>
       </c>
-      <c t="s" s="5" r="D90">
+      <c r="D91" s="5" t="s">
         <v>300</v>
       </c>
-      <c t="s" s="5" r="E90">
+      <c r="E91" s="5" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="91">
-      <c s="16" r="A91"/>
-      <c t="s" s="5" r="B91">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="15"/>
+      <c r="B92" s="5" t="s">
         <v>302</v>
       </c>
-      <c t="s" s="5" r="C91">
+      <c r="C92" s="5" t="s">
         <v>303</v>
       </c>
-      <c t="s" s="5" r="D91">
+      <c r="D92" s="5" t="s">
         <v>304</v>
       </c>
-      <c t="s" s="5" r="E91">
+      <c r="E92" s="5" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="92">
-      <c s="16" r="A92"/>
-      <c t="s" s="5" r="B92">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="15"/>
+      <c r="B93" s="5" t="s">
         <v>306</v>
       </c>
-      <c t="s" s="5" r="C92">
+      <c r="C93" s="5" t="s">
         <v>307</v>
       </c>
-      <c t="s" s="5" r="D92">
+      <c r="D93" s="5" t="s">
         <v>308</v>
       </c>
-      <c t="s" s="5" r="E92">
+      <c r="E93" s="5" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="93">
-      <c s="16" r="A93"/>
-      <c t="s" s="5" r="B93">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="15"/>
+      <c r="B94" s="5" t="s">
         <v>310</v>
       </c>
-      <c t="s" s="7" r="C93">
+      <c r="C94" s="6" t="s">
         <v>311</v>
       </c>
-      <c t="s" s="5" r="D93">
+      <c r="D94" s="5" t="s">
         <v>312</v>
       </c>
-      <c t="s" s="5" r="E93">
+      <c r="E94" s="5" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="94">
-      <c s="16" r="A94"/>
-      <c t="s" s="7" r="B94">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="15"/>
+      <c r="B95" s="6" t="s">
         <v>314</v>
       </c>
-      <c t="s" s="7" r="C94">
+      <c r="C95" s="6" t="s">
         <v>315</v>
       </c>
-      <c t="s" s="5" r="D94">
+      <c r="D95" s="5" t="s">
         <v>316</v>
       </c>
-      <c t="s" s="5" r="E94">
+      <c r="E95" s="5" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="95">
-      <c s="16" r="A95"/>
-      <c t="s" s="5" r="B95">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="15"/>
+      <c r="B96" s="5" t="s">
         <v>318</v>
       </c>
-      <c t="s" s="7" r="C95">
+      <c r="C96" s="6" t="s">
         <v>315</v>
       </c>
-      <c t="s" s="5" r="D95">
+      <c r="D96" s="5" t="s">
         <v>316</v>
       </c>
-      <c t="s" s="5" r="E95">
+      <c r="E96" s="5" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="96">
-      <c s="16" r="A96"/>
-      <c t="s" s="5" r="B96">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="15"/>
+      <c r="B97" s="5" t="s">
         <v>319</v>
       </c>
-      <c t="s" s="9" r="C96">
+      <c r="C97" s="8" t="s">
         <v>320</v>
       </c>
-      <c t="s" s="5" r="D96">
+      <c r="D97" s="5" t="s">
         <v>321</v>
       </c>
-      <c t="s" s="5" r="E96">
+      <c r="E97" s="5" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="97">
-      <c s="16" r="A97"/>
-      <c t="s" s="5" r="B97">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="15"/>
+      <c r="B98" s="5" t="s">
         <v>323</v>
       </c>
-      <c t="s" s="9" r="C97">
+      <c r="C98" s="8" t="s">
         <v>324</v>
       </c>
-      <c t="s" s="5" r="D97">
+      <c r="D98" s="5" t="s">
         <v>325</v>
       </c>
-      <c t="s" s="5" r="E97">
+      <c r="E98" s="5" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="98">
-      <c s="16" r="A98"/>
-      <c t="s" s="8" r="B98">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="15"/>
+      <c r="B99" s="7" t="s">
         <v>327</v>
       </c>
-      <c t="s" s="13" r="C98">
+      <c r="C99" s="12" t="s">
         <v>328</v>
       </c>
-      <c t="s" s="8" r="D98">
+      <c r="D99" s="7" t="s">
         <v>329</v>
       </c>
-      <c t="s" s="13" r="E98">
+      <c r="E99" s="12" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="99">
-      <c s="16" r="A99"/>
-      <c s="14" r="B99"/>
-      <c s="12" r="C99"/>
-      <c s="14" r="D99"/>
-      <c s="14" r="E99"/>
-    </row>
-    <row r="100">
-      <c s="16" r="A100"/>
-      <c s="14" r="B100"/>
-      <c s="12" r="C100"/>
-      <c s="14" r="D100"/>
-      <c s="14" r="E100"/>
-    </row>
-    <row r="101">
-      <c s="16" r="A101"/>
-      <c s="14" r="B101"/>
-      <c s="12" r="C101"/>
-      <c s="14" r="D101"/>
-      <c s="14" r="E101"/>
-    </row>
-    <row r="102">
-      <c s="16" r="A102"/>
-      <c s="14" r="B102"/>
-      <c s="12" r="C102"/>
-      <c s="14" r="D102"/>
-      <c s="14" r="E102"/>
-    </row>
-    <row r="103">
-      <c s="16" r="A103"/>
-      <c s="14" r="B103"/>
-      <c s="12" r="C103"/>
-      <c s="14" r="D103"/>
-      <c s="14" r="E103"/>
-    </row>
-    <row r="104">
-      <c s="16" r="A104"/>
-      <c s="14" r="B104"/>
-      <c s="12" r="C104"/>
-      <c s="14" r="D104"/>
-      <c s="14" r="E104"/>
-    </row>
-    <row r="105">
-      <c s="16" r="A105"/>
-      <c s="14" r="B105"/>
-      <c s="12" r="C105"/>
-      <c s="14" r="D105"/>
-      <c s="14" r="E105"/>
-    </row>
-    <row r="106">
-      <c s="16" r="A106"/>
-      <c s="14" r="B106"/>
-      <c s="12" r="C106"/>
-      <c s="14" r="D106"/>
-      <c s="14" r="E106"/>
-    </row>
-    <row r="107">
-      <c s="16" r="A107"/>
-      <c s="14" r="B107"/>
-      <c s="12" r="C107"/>
-      <c s="14" r="D107"/>
-      <c s="14" r="E107"/>
-    </row>
-    <row r="108">
-      <c s="16" r="A108"/>
-      <c s="14" r="B108"/>
-      <c s="12" r="C108"/>
-      <c s="14" r="D108"/>
-      <c s="14" r="E108"/>
-    </row>
-    <row r="109">
-      <c s="16" r="A109"/>
-      <c s="14" r="B109"/>
-      <c s="12" r="C109"/>
-      <c s="14" r="D109"/>
-      <c s="14" r="E109"/>
-    </row>
-    <row r="110">
-      <c s="16" r="A110"/>
-      <c s="14" r="B110"/>
-      <c s="12" r="C110"/>
-      <c s="14" r="D110"/>
-      <c s="14" r="E110"/>
-    </row>
-    <row r="111">
-      <c s="16" r="A111"/>
-      <c s="14" r="B111"/>
-      <c s="12" r="C111"/>
-      <c s="14" r="D111"/>
-      <c s="14" r="E111"/>
-    </row>
-    <row r="112">
-      <c s="16" r="A112"/>
-      <c s="14" r="B112"/>
-      <c s="12" r="C112"/>
-      <c s="14" r="D112"/>
-      <c s="14" r="E112"/>
-    </row>
-    <row r="113">
-      <c s="16" r="A113"/>
-      <c s="14" r="B113"/>
-      <c s="12" r="C113"/>
-      <c s="14" r="D113"/>
-      <c s="14" r="E113"/>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="15"/>
+      <c r="B100" s="13"/>
+      <c r="C100" s="11"/>
+      <c r="D100" s="13"/>
+      <c r="E100" s="13"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="15"/>
+      <c r="B101" s="13"/>
+      <c r="C101" s="11"/>
+      <c r="D101" s="13"/>
+      <c r="E101" s="13"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="15"/>
+      <c r="B102" s="13"/>
+      <c r="C102" s="11"/>
+      <c r="D102" s="13"/>
+      <c r="E102" s="13"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="15"/>
+      <c r="B103" s="13"/>
+      <c r="C103" s="11"/>
+      <c r="D103" s="13"/>
+      <c r="E103" s="13"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="15"/>
+      <c r="B104" s="13"/>
+      <c r="C104" s="11"/>
+      <c r="D104" s="13"/>
+      <c r="E104" s="13"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="15"/>
+      <c r="B105" s="13"/>
+      <c r="C105" s="11"/>
+      <c r="D105" s="13"/>
+      <c r="E105" s="13"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="15"/>
+      <c r="B106" s="13"/>
+      <c r="C106" s="11"/>
+      <c r="D106" s="13"/>
+      <c r="E106" s="13"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="15"/>
+      <c r="B107" s="13"/>
+      <c r="C107" s="11"/>
+      <c r="D107" s="13"/>
+      <c r="E107" s="13"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="15"/>
+      <c r="B108" s="13"/>
+      <c r="C108" s="11"/>
+      <c r="D108" s="13"/>
+      <c r="E108" s="13"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="15"/>
+      <c r="B109" s="13"/>
+      <c r="C109" s="11"/>
+      <c r="D109" s="13"/>
+      <c r="E109" s="13"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="15"/>
+      <c r="B110" s="13"/>
+      <c r="C110" s="11"/>
+      <c r="D110" s="13"/>
+      <c r="E110" s="13"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="15"/>
+      <c r="B111" s="13"/>
+      <c r="C111" s="11"/>
+      <c r="D111" s="13"/>
+      <c r="E111" s="13"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="15"/>
+      <c r="B112" s="13"/>
+      <c r="C112" s="11"/>
+      <c r="D112" s="13"/>
+      <c r="E112" s="13"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="15"/>
+      <c r="B113" s="13"/>
+      <c r="C113" s="11"/>
+      <c r="D113" s="13"/>
+      <c r="E113" s="13"/>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="15"/>
+      <c r="B114" s="13"/>
+      <c r="C114" s="11"/>
+      <c r="D114" s="13"/>
+      <c r="E114" s="13"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="9.86" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c s="15" r="A1"/>
-      <c s="15" r="B1"/>
-      <c s="15" r="C1"/>
-      <c s="15" r="D1"/>
-      <c s="15" r="E1"/>
-      <c s="15" r="F1"/>
-    </row>
-    <row r="2">
-      <c s="15" r="A2"/>
-      <c s="15" r="B2"/>
-      <c s="15" r="C2"/>
-      <c s="15" r="D2"/>
-      <c s="15" r="E2"/>
-      <c s="15" r="F2"/>
-    </row>
-    <row r="3">
-      <c s="15" r="A3"/>
-      <c s="15" r="B3"/>
-      <c s="15" r="C3"/>
-      <c s="15" r="D3"/>
-      <c s="15" r="E3"/>
-      <c s="15" r="F3"/>
-    </row>
-    <row r="4">
-      <c s="15" r="A4"/>
-      <c s="15" r="B4"/>
-      <c s="15" r="C4"/>
-      <c s="15" r="D4"/>
-      <c s="15" r="E4"/>
-      <c s="15" r="F4"/>
-    </row>
-    <row r="5">
-      <c s="15" r="A5"/>
-      <c s="15" r="B5"/>
-      <c s="15" r="C5"/>
-      <c s="15" r="D5"/>
-      <c s="15" r="E5"/>
-      <c s="15" r="F5"/>
-    </row>
-    <row r="6">
-      <c s="15" r="A6"/>
-      <c s="15" r="B6"/>
-      <c s="15" r="C6"/>
-      <c s="15" r="D6"/>
-      <c s="15" r="E6"/>
-      <c s="15" r="F6"/>
-    </row>
-    <row r="7">
-      <c s="15" r="A7"/>
-      <c s="15" r="B7"/>
-      <c s="15" r="C7"/>
-      <c s="15" r="D7"/>
-      <c s="15" r="E7"/>
-      <c s="15" r="F7"/>
-    </row>
-    <row r="8">
-      <c s="15" r="A8"/>
-      <c s="15" r="B8"/>
-      <c s="15" r="C8"/>
-      <c s="15" r="D8"/>
-      <c s="15" r="E8"/>
-      <c s="15" r="F8"/>
-    </row>
-    <row r="9">
-      <c s="15" r="A9"/>
-      <c s="15" r="B9"/>
-      <c s="15" r="C9"/>
-      <c s="15" r="D9"/>
-      <c s="15" r="E9"/>
-      <c s="15" r="F9"/>
-    </row>
-    <row r="10">
-      <c s="15" r="A10"/>
-      <c s="15" r="B10"/>
-      <c s="15" r="C10"/>
-      <c s="15" r="D10"/>
-      <c s="15" r="E10"/>
-      <c s="15" r="F10"/>
-    </row>
-    <row r="11">
-      <c s="15" r="A11"/>
-      <c s="15" r="B11"/>
-      <c s="15" r="C11"/>
-      <c s="15" r="D11"/>
-      <c s="15" r="E11"/>
-      <c s="15" r="F11"/>
-    </row>
-    <row r="12">
-      <c s="15" r="A12"/>
-      <c s="15" r="B12"/>
-      <c s="15" r="C12"/>
-      <c s="15" r="D12"/>
-      <c s="15" r="E12"/>
-      <c s="15" r="F12"/>
-    </row>
-    <row r="13">
-      <c s="15" r="A13"/>
-      <c s="15" r="B13"/>
-      <c s="15" r="C13"/>
-      <c s="15" r="D13"/>
-      <c s="15" r="E13"/>
-      <c s="15" r="F13"/>
-    </row>
-    <row r="14">
-      <c s="15" r="A14"/>
-      <c s="15" r="B14"/>
-      <c s="15" r="C14"/>
-      <c s="15" r="D14"/>
-      <c s="15" r="E14"/>
-      <c s="15" r="F14"/>
-    </row>
-    <row r="15">
-      <c s="15" r="A15"/>
-      <c s="15" r="B15"/>
-      <c s="15" r="C15"/>
-      <c s="15" r="D15"/>
-      <c s="15" r="E15"/>
-      <c s="15" r="F15"/>
-    </row>
-    <row r="16">
-      <c s="15" r="A16"/>
-      <c s="15" r="B16"/>
-      <c s="15" r="C16"/>
-      <c s="15" r="D16"/>
-      <c s="15" r="E16"/>
-      <c s="15" r="F16"/>
-    </row>
-    <row r="17">
-      <c s="15" r="A17"/>
-      <c s="15" r="B17"/>
-      <c s="15" r="C17"/>
-      <c s="15" r="D17"/>
-      <c s="15" r="E17"/>
-      <c s="15" r="F17"/>
-    </row>
-    <row r="18">
-      <c s="15" r="A18"/>
-      <c s="15" r="B18"/>
-      <c s="15" r="C18"/>
-      <c s="15" r="D18"/>
-      <c s="15" r="E18"/>
-      <c s="15" r="F18"/>
-    </row>
-    <row r="19">
-      <c s="15" r="A19"/>
-      <c s="15" r="B19"/>
-      <c s="15" r="C19"/>
-      <c s="15" r="D19"/>
-      <c s="15" r="E19"/>
-      <c s="15" r="F19"/>
-    </row>
-    <row r="20">
-      <c s="15" r="A20"/>
-      <c s="15" r="B20"/>
-      <c s="15" r="C20"/>
-      <c s="15" r="D20"/>
-      <c s="15" r="E20"/>
-      <c s="15" r="F20"/>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="9.86" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c s="15" r="A1"/>
-      <c s="15" r="B1"/>
-      <c s="15" r="C1"/>
-      <c s="15" r="D1"/>
-      <c s="15" r="E1"/>
-      <c s="15" r="F1"/>
-    </row>
-    <row r="2">
-      <c s="15" r="A2"/>
-      <c s="15" r="B2"/>
-      <c s="15" r="C2"/>
-      <c s="15" r="D2"/>
-      <c s="15" r="E2"/>
-      <c s="15" r="F2"/>
-    </row>
-    <row r="3">
-      <c s="15" r="A3"/>
-      <c s="15" r="B3"/>
-      <c s="15" r="C3"/>
-      <c s="15" r="D3"/>
-      <c s="15" r="E3"/>
-      <c s="15" r="F3"/>
-    </row>
-    <row r="4">
-      <c s="15" r="A4"/>
-      <c s="15" r="B4"/>
-      <c s="15" r="C4"/>
-      <c s="15" r="D4"/>
-      <c s="15" r="E4"/>
-      <c s="15" r="F4"/>
-    </row>
-    <row r="5">
-      <c s="15" r="A5"/>
-      <c s="15" r="B5"/>
-      <c s="15" r="C5"/>
-      <c s="15" r="D5"/>
-      <c s="15" r="E5"/>
-      <c s="15" r="F5"/>
-    </row>
-    <row r="6">
-      <c s="15" r="A6"/>
-      <c s="15" r="B6"/>
-      <c s="15" r="C6"/>
-      <c s="15" r="D6"/>
-      <c s="15" r="E6"/>
-      <c s="15" r="F6"/>
-    </row>
-    <row r="7">
-      <c s="15" r="A7"/>
-      <c s="15" r="B7"/>
-      <c s="15" r="C7"/>
-      <c s="15" r="D7"/>
-      <c s="15" r="E7"/>
-      <c s="15" r="F7"/>
-    </row>
-    <row r="8">
-      <c s="15" r="A8"/>
-      <c s="15" r="B8"/>
-      <c s="15" r="C8"/>
-      <c s="15" r="D8"/>
-      <c s="15" r="E8"/>
-      <c s="15" r="F8"/>
-    </row>
-    <row r="9">
-      <c s="15" r="A9"/>
-      <c s="15" r="B9"/>
-      <c s="15" r="C9"/>
-      <c s="15" r="D9"/>
-      <c s="15" r="E9"/>
-      <c s="15" r="F9"/>
-    </row>
-    <row r="10">
-      <c s="15" r="A10"/>
-      <c s="15" r="B10"/>
-      <c s="15" r="C10"/>
-      <c s="15" r="D10"/>
-      <c s="15" r="E10"/>
-      <c s="15" r="F10"/>
-    </row>
-    <row r="11">
-      <c s="15" r="A11"/>
-      <c s="15" r="B11"/>
-      <c s="15" r="C11"/>
-      <c s="15" r="D11"/>
-      <c s="15" r="E11"/>
-      <c s="15" r="F11"/>
-    </row>
-    <row r="12">
-      <c s="15" r="A12"/>
-      <c s="15" r="B12"/>
-      <c s="15" r="C12"/>
-      <c s="15" r="D12"/>
-      <c s="15" r="E12"/>
-      <c s="15" r="F12"/>
-    </row>
-    <row r="13">
-      <c s="15" r="A13"/>
-      <c s="15" r="B13"/>
-      <c s="15" r="C13"/>
-      <c s="15" r="D13"/>
-      <c s="15" r="E13"/>
-      <c s="15" r="F13"/>
-    </row>
-    <row r="14">
-      <c s="15" r="A14"/>
-      <c s="15" r="B14"/>
-      <c s="15" r="C14"/>
-      <c s="15" r="D14"/>
-      <c s="15" r="E14"/>
-      <c s="15" r="F14"/>
-    </row>
-    <row r="15">
-      <c s="15" r="A15"/>
-      <c s="15" r="B15"/>
-      <c s="15" r="C15"/>
-      <c s="15" r="D15"/>
-      <c s="15" r="E15"/>
-      <c s="15" r="F15"/>
-    </row>
-    <row r="16">
-      <c s="15" r="A16"/>
-      <c s="15" r="B16"/>
-      <c s="15" r="C16"/>
-      <c s="15" r="D16"/>
-      <c s="15" r="E16"/>
-      <c s="15" r="F16"/>
-    </row>
-    <row r="17">
-      <c s="15" r="A17"/>
-      <c s="15" r="B17"/>
-      <c s="15" r="C17"/>
-      <c s="15" r="D17"/>
-      <c s="15" r="E17"/>
-      <c s="15" r="F17"/>
-    </row>
-    <row r="18">
-      <c s="15" r="A18"/>
-      <c s="15" r="B18"/>
-      <c s="15" r="C18"/>
-      <c s="15" r="D18"/>
-      <c s="15" r="E18"/>
-      <c s="15" r="F18"/>
-    </row>
-    <row r="19">
-      <c s="15" r="A19"/>
-      <c s="15" r="B19"/>
-      <c s="15" r="C19"/>
-      <c s="15" r="D19"/>
-      <c s="15" r="E19"/>
-      <c s="15" r="F19"/>
-    </row>
-    <row r="20">
-      <c s="15" r="A20"/>
-      <c s="15" r="B20"/>
-      <c s="15" r="C20"/>
-      <c s="15" r="D20"/>
-      <c s="15" r="E20"/>
-      <c s="15" r="F20"/>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
EGB-22307 - Display Experience (localization)
Former-commit-id: 4ee8be309306294eae8ab59b67a3013406a9b767
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="338">
   <si>
     <t>Page</t>
   </si>
@@ -1015,13 +1015,28 @@
   </si>
   <si>
     <t>Click here to add question</t>
+  </si>
+  <si>
+    <t>DisplayExperience</t>
+  </si>
+  <si>
+    <t>relatedLearningObjectives</t>
+  </si>
+  <si>
+    <t>Related learning objectives</t>
+  </si>
+  <si>
+    <t>Gerelateerde leerdoelen</t>
+  </si>
+  <si>
+    <t>Verwandte Lernziele</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1073,11 +1088,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1213,13 +1223,11 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1521,11 +1529,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E114"/>
+  <dimension ref="A1:E116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
+      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G98" sqref="G98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1722,7 +1730,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="5" t="s">
         <v>46</v>
       </c>
@@ -1737,7 +1745,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="5" t="s">
         <v>50</v>
       </c>
@@ -1752,7 +1760,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="5" t="s">
         <v>54</v>
       </c>
@@ -1767,7 +1775,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="5" t="s">
         <v>58</v>
       </c>
@@ -1782,7 +1790,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="5" t="s">
         <v>62</v>
       </c>
@@ -1797,7 +1805,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="5" t="s">
         <v>66</v>
       </c>
@@ -1885,7 +1893,7 @@
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
-      <c r="E24" s="14"/>
+      <c r="E24" s="13"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
@@ -1905,10 +1913,10 @@
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
-      <c r="E26" s="14"/>
+      <c r="E26" s="13"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="13" t="s">
         <v>90</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -1925,7 +1933,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
+      <c r="A28" s="13"/>
       <c r="B28" s="5" t="s">
         <v>94</v>
       </c>
@@ -1940,7 +1948,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
+      <c r="A29" s="13"/>
       <c r="B29" s="5" t="s">
         <v>98</v>
       </c>
@@ -1955,7 +1963,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
+      <c r="A30" s="13"/>
       <c r="B30" s="5" t="s">
         <v>101</v>
       </c>
@@ -1970,7 +1978,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
+      <c r="A31" s="13"/>
       <c r="B31" s="5" t="s">
         <v>104</v>
       </c>
@@ -1985,7 +1993,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
+      <c r="A32" s="13"/>
       <c r="B32" s="5" t="s">
         <v>108</v>
       </c>
@@ -2000,7 +2008,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
+      <c r="A33" s="13"/>
       <c r="B33" s="5" t="s">
         <v>112</v>
       </c>
@@ -2015,1021 +2023,1045 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="16" t="s">
+        <v>333</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B37" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C37" s="10" t="s">
         <v>118</v>
-      </c>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>122</v>
       </c>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
+      <c r="A38" s="13"/>
       <c r="B38" s="10" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>122</v>
+      </c>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="14" t="s">
-        <v>125</v>
-      </c>
+      <c r="A40" s="13"/>
       <c r="B40" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
-      <c r="B41" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>129</v>
-      </c>
+      <c r="A41" s="13"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
+      <c r="A42" s="13" t="s">
+        <v>125</v>
+      </c>
       <c r="B42" s="10" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
+      <c r="A43" s="13"/>
       <c r="B43" s="10" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
+      <c r="A44" s="13"/>
+      <c r="B44" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="14" t="s">
+      <c r="A45" s="13"/>
+      <c r="B45" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="13"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B47" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C47" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D47" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="E47" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
-      <c r="B46" s="5" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="13"/>
+      <c r="B48" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C48" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D48" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E48" s="5" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
-      <c r="B47" s="5" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="13"/>
+      <c r="B49" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C49" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D49" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="E49" s="5" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
-      <c r="B48" s="5" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="13"/>
+      <c r="B50" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C50" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D50" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="E50" s="5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
-      <c r="B49" s="5" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="13"/>
+      <c r="B51" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C51" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D51" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="E51" s="5" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
-      <c r="B50" s="5" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="13"/>
+      <c r="B52" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C52" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D52" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="E50" s="5" t="s">
+      <c r="E52" s="5" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="14"/>
-      <c r="B51" s="5" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="13"/>
+      <c r="B53" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C53" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D53" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="E51" s="5" t="s">
+      <c r="E53" s="5" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="14"/>
-      <c r="B52" s="5" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="13"/>
+      <c r="B54" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C54" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="D54" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="E52" s="5" t="s">
+      <c r="E54" s="5" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="14"/>
-      <c r="B53" s="7" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="13"/>
+      <c r="B55" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C55" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="14"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="14" t="s">
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="13"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B57" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C57" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D57" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="E55" s="5" t="s">
+      <c r="E57" s="5" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="14"/>
-      <c r="B56" s="5" t="s">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="13"/>
+      <c r="B58" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C58" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="D58" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="E56" s="5" t="s">
+      <c r="E58" s="5" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="15"/>
-      <c r="B57" s="5" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="14"/>
+      <c r="B59" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C59" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="D59" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="E57" s="5" t="s">
+      <c r="E59" s="5" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="15"/>
-      <c r="B58" s="5" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="14"/>
+      <c r="B60" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="C60" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="D60" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="E58" s="5" t="s">
+      <c r="E60" s="5" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="15"/>
-      <c r="B59" s="7" t="s">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="14"/>
+      <c r="B61" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C61" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="D59" s="7"/>
-      <c r="E59" s="7"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="15"/>
-      <c r="B60" s="2" t="s">
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="14"/>
+      <c r="B62" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="15"/>
-      <c r="B61" s="5" t="s">
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="14"/>
+      <c r="B63" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C63" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="D63" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="E61" s="5" t="s">
+      <c r="E63" s="5" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="15"/>
-      <c r="B62" s="16" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="14"/>
+      <c r="B64" s="15" t="s">
         <v>331</v>
       </c>
-      <c r="C62" s="16" t="s">
+      <c r="C64" s="15" t="s">
         <v>332</v>
       </c>
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="15"/>
-      <c r="B63" s="14"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="14"/>
-      <c r="E63" s="14"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="15" t="s">
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="14"/>
+      <c r="B65" s="13"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="13"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B66" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C66" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="D66" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="E64" s="5" t="s">
+      <c r="E66" s="5" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="15"/>
-      <c r="B65" s="5" t="s">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="14"/>
+      <c r="B67" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C67" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="D67" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="E65" s="5" t="s">
+      <c r="E67" s="5" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="15"/>
-      <c r="B66" s="5" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="14"/>
+      <c r="B68" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C68" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="D68" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="E66" s="5" t="s">
+      <c r="E68" s="5" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="15"/>
-      <c r="B67" s="5" t="s">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="14"/>
+      <c r="B69" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="C69" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="D67" s="5" t="s">
+      <c r="D69" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="E67" s="5" t="s">
+      <c r="E69" s="5" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="15"/>
-      <c r="B68" s="5" t="s">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="14"/>
+      <c r="B70" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C70" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="D68" s="5" t="s">
+      <c r="D70" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="E68" s="5" t="s">
+      <c r="E70" s="5" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="15"/>
-      <c r="B69" s="5" t="s">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="14"/>
+      <c r="B71" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C71" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="D71" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="E69" s="5" t="s">
+      <c r="E71" s="5" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="15"/>
-      <c r="B70" s="5" t="s">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="14"/>
+      <c r="B72" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C72" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="D70" s="5" t="s">
+      <c r="D72" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E70" s="5" t="s">
+      <c r="E72" s="5" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="15"/>
-      <c r="B71" s="5" t="s">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="14"/>
+      <c r="B73" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="C71" s="5" t="s">
+      <c r="C73" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="D71" s="5" t="s">
+      <c r="D73" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="E71" s="5" t="s">
+      <c r="E73" s="5" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="15"/>
-      <c r="B72" s="5" t="s">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="14"/>
+      <c r="B74" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="C72" s="5" t="s">
+      <c r="C74" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="D72" s="5" t="s">
+      <c r="D74" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="E72" s="5" t="s">
+      <c r="E74" s="5" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="15"/>
-      <c r="B73" s="5" t="s">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="14"/>
+      <c r="B75" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="C75" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="D73" s="5" t="s">
+      <c r="D75" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="E73" s="5" t="s">
+      <c r="E75" s="5" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="15"/>
-      <c r="B74" s="5" t="s">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="14"/>
+      <c r="B76" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C76" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="D76" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="E74" s="5" t="s">
+      <c r="E76" s="5" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="15"/>
-      <c r="B75" s="5" t="s">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="14"/>
+      <c r="B77" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="C75" s="5" t="s">
+      <c r="C77" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="D77" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="E75" s="5" t="s">
+      <c r="E77" s="5" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="15"/>
-      <c r="B76" s="5" t="s">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="14"/>
+      <c r="B78" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="C78" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="D78" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="E76" s="5" t="s">
+      <c r="E78" s="5" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="15"/>
-      <c r="B77" s="5" t="s">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="14"/>
+      <c r="B79" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C79" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="D77" s="5" t="s">
+      <c r="D79" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="E77" s="5" t="s">
+      <c r="E79" s="5" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="15"/>
-      <c r="B78" s="6" t="s">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="14"/>
+      <c r="B80" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="C78" s="5" t="s">
+      <c r="C80" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="D78" s="5" t="s">
+      <c r="D80" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="E78" s="5" t="s">
+      <c r="E80" s="5" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="15"/>
-      <c r="B79" s="5" t="s">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="14"/>
+      <c r="B81" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="C79" s="5" t="s">
+      <c r="C81" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="D79" s="5" t="s">
+      <c r="D81" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="E79" s="5" t="s">
+      <c r="E81" s="5" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="15"/>
-      <c r="B80" s="5" t="s">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="14"/>
+      <c r="B82" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="C80" s="5" t="s">
+      <c r="C82" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="D80" s="5" t="s">
+      <c r="D82" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="E80" s="5" t="s">
+      <c r="E82" s="5" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="15"/>
-      <c r="B81" s="5" t="s">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="14"/>
+      <c r="B83" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="C81" s="5" t="s">
+      <c r="C83" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="D81" s="5" t="s">
+      <c r="D83" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="E81" s="5" t="s">
+      <c r="E83" s="5" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="15"/>
-      <c r="B82" s="5" t="s">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="14"/>
+      <c r="B84" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="C82" s="5" t="s">
+      <c r="C84" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="D82" s="5" t="s">
+      <c r="D84" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="E82" s="5" t="s">
+      <c r="E84" s="5" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="15"/>
-      <c r="B83" s="5" t="s">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="14"/>
+      <c r="B85" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="C83" s="5" t="s">
+      <c r="C85" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="D83" s="5" t="s">
+      <c r="D85" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="E83" s="5" t="s">
+      <c r="E85" s="5" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="15"/>
-      <c r="B84" s="5" t="s">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="14"/>
+      <c r="B86" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="C84" s="5" t="s">
+      <c r="C86" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="D84" s="5" t="s">
+      <c r="D86" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="E84" s="5" t="s">
+      <c r="E86" s="5" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="15"/>
-      <c r="B85" s="5" t="s">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="14"/>
+      <c r="B87" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="C85" s="5" t="s">
+      <c r="C87" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="D85" s="5" t="s">
+      <c r="D87" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="E85" s="5" t="s">
+      <c r="E87" s="5" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="15"/>
-      <c r="B86" s="5" t="s">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="14"/>
+      <c r="B88" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="C86" s="5" t="s">
+      <c r="C88" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="D86" s="5" t="s">
+      <c r="D88" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="E86" s="5" t="s">
+      <c r="E88" s="5" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="15"/>
-      <c r="B87" s="5" t="s">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="14"/>
+      <c r="B89" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="C87" s="5" t="s">
+      <c r="C89" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="D87" s="5" t="s">
+      <c r="D89" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="E87" s="5" t="s">
+      <c r="E89" s="5" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="15"/>
-      <c r="B88" s="5" t="s">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="14"/>
+      <c r="B90" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="C88" s="5" t="s">
+      <c r="C90" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="D88" s="5" t="s">
+      <c r="D90" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="E88" s="5" t="s">
+      <c r="E90" s="5" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="15"/>
-      <c r="B89" s="5" t="s">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="14"/>
+      <c r="B91" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="C89" s="5" t="s">
+      <c r="C91" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="D89" s="5" t="s">
+      <c r="D91" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="E89" s="5" t="s">
+      <c r="E91" s="5" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="15"/>
-      <c r="B90" s="5" t="s">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="14"/>
+      <c r="B92" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="C90" s="5" t="s">
+      <c r="C92" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="D90" s="5" t="s">
+      <c r="D92" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="E90" s="5" t="s">
+      <c r="E92" s="5" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="15"/>
-      <c r="B91" s="5" t="s">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="14"/>
+      <c r="B93" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="C91" s="5" t="s">
+      <c r="C93" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="D91" s="5" t="s">
+      <c r="D93" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="E91" s="5" t="s">
+      <c r="E93" s="5" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="15"/>
-      <c r="B92" s="5" t="s">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="14"/>
+      <c r="B94" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="C92" s="5" t="s">
+      <c r="C94" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="D92" s="5" t="s">
+      <c r="D94" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="E92" s="5" t="s">
+      <c r="E94" s="5" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="15"/>
-      <c r="B93" s="5" t="s">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="14"/>
+      <c r="B95" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="C93" s="5" t="s">
+      <c r="C95" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="D93" s="5" t="s">
+      <c r="D95" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="E93" s="5" t="s">
+      <c r="E95" s="5" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="15"/>
-      <c r="B94" s="5" t="s">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="14"/>
+      <c r="B96" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="C94" s="6" t="s">
+      <c r="C96" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="D94" s="5" t="s">
+      <c r="D96" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="E94" s="5" t="s">
+      <c r="E96" s="5" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="15"/>
-      <c r="B95" s="6" t="s">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="14"/>
+      <c r="B97" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="C95" s="6" t="s">
+      <c r="C97" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="D95" s="5" t="s">
+      <c r="D97" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="E95" s="5" t="s">
+      <c r="E97" s="5" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="15"/>
-      <c r="B96" s="5" t="s">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="14"/>
+      <c r="B98" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="C96" s="6" t="s">
+      <c r="C98" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="D96" s="5" t="s">
+      <c r="D98" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="E96" s="5" t="s">
+      <c r="E98" s="5" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="15"/>
-      <c r="B97" s="5" t="s">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="14"/>
+      <c r="B99" s="5" t="s">
         <v>319</v>
       </c>
-      <c r="C97" s="8" t="s">
+      <c r="C99" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="D97" s="5" t="s">
+      <c r="D99" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="E97" s="5" t="s">
+      <c r="E99" s="5" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="15"/>
-      <c r="B98" s="5" t="s">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="14"/>
+      <c r="B100" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="C98" s="8" t="s">
+      <c r="C100" s="8" t="s">
         <v>324</v>
       </c>
-      <c r="D98" s="5" t="s">
+      <c r="D100" s="5" t="s">
         <v>325</v>
       </c>
-      <c r="E98" s="5" t="s">
+      <c r="E100" s="5" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="15"/>
-      <c r="B99" s="7" t="s">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="14"/>
+      <c r="B101" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="C99" s="12" t="s">
+      <c r="C101" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="D99" s="7" t="s">
+      <c r="D101" s="5" t="s">
         <v>329</v>
       </c>
-      <c r="E99" s="12" t="s">
+      <c r="E101" s="5" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="15"/>
-      <c r="B100" s="13"/>
-      <c r="C100" s="11"/>
-      <c r="D100" s="13"/>
-      <c r="E100" s="13"/>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="15"/>
-      <c r="B101" s="13"/>
-      <c r="C101" s="11"/>
-      <c r="D101" s="13"/>
-      <c r="E101" s="13"/>
-    </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="15"/>
-      <c r="B102" s="13"/>
+      <c r="A102" s="14"/>
+      <c r="B102" s="12"/>
       <c r="C102" s="11"/>
-      <c r="D102" s="13"/>
-      <c r="E102" s="13"/>
+      <c r="D102" s="12"/>
+      <c r="E102" s="12"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="15"/>
-      <c r="B103" s="13"/>
+      <c r="A103" s="14"/>
+      <c r="B103" s="12"/>
       <c r="C103" s="11"/>
-      <c r="D103" s="13"/>
-      <c r="E103" s="13"/>
+      <c r="D103" s="12"/>
+      <c r="E103" s="12"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="15"/>
-      <c r="B104" s="13"/>
+      <c r="A104" s="14"/>
+      <c r="B104" s="12"/>
       <c r="C104" s="11"/>
-      <c r="D104" s="13"/>
-      <c r="E104" s="13"/>
+      <c r="D104" s="12"/>
+      <c r="E104" s="12"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="15"/>
-      <c r="B105" s="13"/>
+      <c r="A105" s="14"/>
+      <c r="B105" s="12"/>
       <c r="C105" s="11"/>
-      <c r="D105" s="13"/>
-      <c r="E105" s="13"/>
+      <c r="D105" s="12"/>
+      <c r="E105" s="12"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="15"/>
-      <c r="B106" s="13"/>
+      <c r="A106" s="14"/>
+      <c r="B106" s="12"/>
       <c r="C106" s="11"/>
-      <c r="D106" s="13"/>
-      <c r="E106" s="13"/>
+      <c r="D106" s="12"/>
+      <c r="E106" s="12"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="15"/>
-      <c r="B107" s="13"/>
+      <c r="A107" s="14"/>
+      <c r="B107" s="12"/>
       <c r="C107" s="11"/>
-      <c r="D107" s="13"/>
-      <c r="E107" s="13"/>
+      <c r="D107" s="12"/>
+      <c r="E107" s="12"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="15"/>
-      <c r="B108" s="13"/>
+      <c r="A108" s="14"/>
+      <c r="B108" s="12"/>
       <c r="C108" s="11"/>
-      <c r="D108" s="13"/>
-      <c r="E108" s="13"/>
+      <c r="D108" s="12"/>
+      <c r="E108" s="12"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="15"/>
-      <c r="B109" s="13"/>
+      <c r="A109" s="14"/>
+      <c r="B109" s="12"/>
       <c r="C109" s="11"/>
-      <c r="D109" s="13"/>
-      <c r="E109" s="13"/>
+      <c r="D109" s="12"/>
+      <c r="E109" s="12"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="15"/>
-      <c r="B110" s="13"/>
+      <c r="A110" s="14"/>
+      <c r="B110" s="12"/>
       <c r="C110" s="11"/>
-      <c r="D110" s="13"/>
-      <c r="E110" s="13"/>
+      <c r="D110" s="12"/>
+      <c r="E110" s="12"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="15"/>
-      <c r="B111" s="13"/>
+      <c r="A111" s="14"/>
+      <c r="B111" s="12"/>
       <c r="C111" s="11"/>
-      <c r="D111" s="13"/>
-      <c r="E111" s="13"/>
+      <c r="D111" s="12"/>
+      <c r="E111" s="12"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" s="15"/>
-      <c r="B112" s="13"/>
+      <c r="A112" s="14"/>
+      <c r="B112" s="12"/>
       <c r="C112" s="11"/>
-      <c r="D112" s="13"/>
-      <c r="E112" s="13"/>
+      <c r="D112" s="12"/>
+      <c r="E112" s="12"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="15"/>
-      <c r="B113" s="13"/>
+      <c r="A113" s="14"/>
+      <c r="B113" s="12"/>
       <c r="C113" s="11"/>
-      <c r="D113" s="13"/>
-      <c r="E113" s="13"/>
+      <c r="D113" s="12"/>
+      <c r="E113" s="12"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="15"/>
-      <c r="B114" s="13"/>
+      <c r="A114" s="14"/>
+      <c r="B114" s="12"/>
       <c r="C114" s="11"/>
-      <c r="D114" s="13"/>
-      <c r="E114" s="13"/>
+      <c r="D114" s="12"/>
+      <c r="E114" s="12"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="14"/>
+      <c r="B115" s="12"/>
+      <c r="C115" s="11"/>
+      <c r="D115" s="12"/>
+      <c r="E115" s="12"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="14"/>
+      <c r="B116" s="12"/>
+      <c r="C116" s="11"/>
+      <c r="D116" s="12"/>
+      <c r="E116" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3046,164 +3078,164 @@
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="A1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3219,164 +3251,164 @@
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="A1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add localization de EWD-22142 - Build Experience
Former-commit-id: e4f31c18d52e95d8e13a2f1996c67fa6923fe6f5
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="11955"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId3"/>
-    <sheet sheetId="2" name="Sheet2" state="visible" r:id="rId4"/>
-    <sheet sheetId="3" name="Sheet3" state="visible" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="363">
   <si>
     <t>Page</t>
   </si>
@@ -612,8 +615,7 @@
     <t>Neue Fragen hinzufügen</t>
   </si>
   <si>
-    <t>clickToAddNewQuestion        
-</t>
+    <t>clickToAddNewQuestion</t>
   </si>
   <si>
     <t>Click here to add question</t>
@@ -850,7 +852,7 @@
     <t>Marked/highlighted text</t>
   </si>
   <si>
-    <t>Gemarkeerde/gehighlighte tekst </t>
+    <t>Gemarkeerde/gehighlighte tekst</t>
   </si>
   <si>
     <t>Markierter/hervorgehobener Text</t>
@@ -1097,138 +1099,91 @@
   </si>
   <si>
     <t>userProperties</t>
+  </si>
+  <si>
+    <t>Erstellen</t>
+  </si>
+  <si>
+    <t>Herunterladen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="14">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11.0"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="15">
@@ -1236,9 +1191,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1319,7 +1272,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1327,1974 +1280,2304 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+  <cellXfs count="19">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf fillId="3" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="1" applyFill="1"/>
-    <xf fillId="4" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="2" applyFill="1"/>
-    <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="3"/>
-    <xf fillId="5" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="4" applyFill="1"/>
-    <xf fillId="6" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="5" applyFill="1"/>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="6">
-      <alignment vertical="bottom" horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="7" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf fillId="8" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="7" applyFill="1"/>
-    <xf applyAlignment="1" fillId="9" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="8" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf fillId="10" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="9" applyFill="1"/>
-    <xf fillId="11" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="10" applyFill="1"/>
-    <xf applyAlignment="1" fillId="12" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="13" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" readingOrder="1"/>
     </xf>
-    <xf fillId="14" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="11" applyFill="1"/>
-    <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="12"/>
-    <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="13"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane topLeftCell="A2" ySplit="1.0" activePane="bottomLeft" state="frozen"/>
-      <selection sqref="A2" activeCell="A2" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29:E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="9.86" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" customWidth="1" max="1" width="26.14"/>
-    <col min="2" customWidth="1" max="2" width="33.0"/>
-    <col min="3" customWidth="1" max="3" width="28.71"/>
-    <col min="4" customWidth="1" max="4" width="42.14"/>
-    <col min="5" customWidth="1" max="5" width="39.43"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="33" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
+    <col min="4" max="4" width="42.140625" customWidth="1"/>
+    <col min="5" max="5" width="39.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row s="4" customFormat="1" r="1">
-      <c t="s" s="5" r="A1">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c t="s" s="5" r="B1">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c t="s" s="5" r="C1">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="5" r="D1">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c t="s" s="4" r="E1">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c t="s" s="11" r="A2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
-      <c t="s" s="6" r="B2">
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-      <c t="s" s="6" r="C2">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="6" r="D2">
+      <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
-      <c t="s" s="6" r="E2">
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3">
-      <c s="11" r="A3"/>
-      <c t="s" s="6" r="B3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="6" t="s">
         <v>10</v>
       </c>
-      <c t="s" s="6" r="C3">
+      <c r="C3" s="6" t="s">
         <v>11</v>
       </c>
-      <c t="s" s="6" r="D3">
+      <c r="D3" s="6" t="s">
         <v>12</v>
       </c>
-      <c t="s" s="6" r="E3">
+      <c r="E3" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4">
-      <c s="11" r="A4"/>
-      <c t="s" s="6" r="B4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="6" t="s">
         <v>14</v>
       </c>
-      <c t="s" s="6" r="C4">
+      <c r="C4" s="6" t="s">
         <v>15</v>
       </c>
-      <c t="s" s="6" r="D4">
+      <c r="D4" s="6" t="s">
         <v>16</v>
       </c>
-      <c t="s" s="6" r="E4">
+      <c r="E4" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5">
-      <c s="11" r="A5"/>
-      <c t="s" s="6" r="B5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="6" t="s">
         <v>18</v>
       </c>
-      <c t="s" s="6" r="C5">
+      <c r="C5" s="6" t="s">
         <v>19</v>
       </c>
-      <c t="s" s="6" r="D5">
+      <c r="D5" s="6" t="s">
         <v>20</v>
       </c>
-      <c t="s" s="6" r="E5">
+      <c r="E5" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6">
-      <c s="11" r="A6"/>
-      <c t="s" s="6" r="B6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="6" t="s">
         <v>22</v>
       </c>
-      <c t="s" s="6" r="C6">
+      <c r="C6" s="6" t="s">
         <v>23</v>
       </c>
-      <c t="s" s="6" r="D6">
+      <c r="D6" s="6" t="s">
         <v>23</v>
       </c>
-      <c t="s" s="6" r="E6">
+      <c r="E6" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7">
-      <c s="11" r="A7"/>
-      <c t="s" s="6" r="B7">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="6" t="s">
         <v>24</v>
       </c>
-      <c t="s" s="6" r="C7">
+      <c r="C7" s="6" t="s">
         <v>25</v>
       </c>
-      <c t="s" s="6" r="D7">
+      <c r="D7" s="6" t="s">
         <v>25</v>
       </c>
-      <c t="s" s="6" r="E7">
+      <c r="E7" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8">
-      <c s="11" r="A8"/>
-      <c t="s" s="6" r="B8">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="6" t="s">
         <v>26</v>
       </c>
-      <c t="s" s="6" r="C8">
+      <c r="C8" s="6" t="s">
         <v>27</v>
       </c>
-      <c t="s" s="6" r="D8">
+      <c r="D8" s="6" t="s">
         <v>28</v>
       </c>
-      <c t="s" s="6" r="E8">
+      <c r="E8" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9">
-      <c s="11" r="A9"/>
-      <c t="s" s="6" r="B9">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="6" t="s">
         <v>30</v>
       </c>
-      <c t="s" s="6" r="C9">
+      <c r="C9" s="6" t="s">
         <v>31</v>
       </c>
-      <c t="s" s="6" r="D9">
+      <c r="D9" s="6" t="s">
         <v>32</v>
       </c>
-      <c t="s" s="6" r="E9">
+      <c r="E9" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10">
-      <c s="11" r="A10"/>
-      <c t="s" s="6" r="B10">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="6" t="s">
         <v>34</v>
       </c>
-      <c t="s" s="6" r="C10">
+      <c r="C10" s="6" t="s">
         <v>35</v>
       </c>
-      <c t="s" s="6" r="D10">
+      <c r="D10" s="6" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="6" r="E10">
+      <c r="E10" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11">
-      <c s="11" r="A11"/>
-      <c t="s" s="6" r="B11">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="6" t="s">
         <v>38</v>
       </c>
-      <c t="s" s="6" r="C11">
+      <c r="C11" s="6" t="s">
         <v>39</v>
       </c>
-      <c t="s" s="6" r="D11">
+      <c r="D11" s="6" t="s">
         <v>40</v>
       </c>
-      <c t="s" s="6" r="E11">
+      <c r="E11" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12">
-      <c s="11" r="A12"/>
-      <c t="s" s="6" r="B12">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="6" t="s">
         <v>42</v>
       </c>
-      <c t="s" s="6" r="C12">
+      <c r="C12" s="6" t="s">
         <v>43</v>
       </c>
-      <c t="s" s="6" r="D12">
+      <c r="D12" s="6" t="s">
         <v>44</v>
       </c>
-      <c t="s" s="6" r="E12">
+      <c r="E12" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13">
-      <c s="16" r="A13"/>
-      <c t="s" s="6" r="B13">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="6" t="s">
         <v>46</v>
       </c>
-      <c t="s" s="6" r="C13">
+      <c r="C13" s="6" t="s">
         <v>47</v>
       </c>
-      <c t="s" s="6" r="D13">
+      <c r="D13" s="6" t="s">
         <v>48</v>
       </c>
-      <c t="s" s="6" r="E13">
+      <c r="E13" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14">
-      <c s="16" r="A14"/>
-      <c t="s" s="6" r="B14">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="6" t="s">
         <v>50</v>
       </c>
-      <c t="s" s="6" r="C14">
+      <c r="C14" s="6" t="s">
         <v>51</v>
       </c>
-      <c t="s" s="6" r="D14">
+      <c r="D14" s="6" t="s">
         <v>52</v>
       </c>
-      <c t="s" s="6" r="E14">
+      <c r="E14" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15">
-      <c s="16" r="A15"/>
-      <c t="s" s="6" r="B15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="B15" s="6" t="s">
         <v>54</v>
       </c>
-      <c t="s" s="6" r="C15">
+      <c r="C15" s="6" t="s">
         <v>55</v>
       </c>
-      <c t="s" s="6" r="D15">
+      <c r="D15" s="6" t="s">
         <v>56</v>
       </c>
-      <c t="s" s="6" r="E15">
+      <c r="E15" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="16">
-      <c s="16" r="A16"/>
-      <c t="s" s="6" r="B16">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="B16" s="6" t="s">
         <v>58</v>
       </c>
-      <c t="s" s="6" r="C16">
+      <c r="C16" s="6" t="s">
         <v>59</v>
       </c>
-      <c t="s" s="6" r="D16">
+      <c r="D16" s="6" t="s">
         <v>60</v>
       </c>
-      <c t="s" s="6" r="E16">
+      <c r="E16" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17">
-      <c s="16" r="A17"/>
-      <c t="s" s="6" r="B17">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="6" t="s">
         <v>62</v>
       </c>
-      <c t="s" s="6" r="C17">
+      <c r="C17" s="6" t="s">
         <v>63</v>
       </c>
-      <c t="s" s="6" r="D17">
+      <c r="D17" s="6" t="s">
         <v>64</v>
       </c>
-      <c t="s" s="6" r="E17">
+      <c r="E17" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18">
-      <c s="16" r="A18"/>
-      <c t="s" s="6" r="B18">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="6" t="s">
         <v>66</v>
       </c>
-      <c t="s" s="6" r="C18">
+      <c r="C18" s="6" t="s">
         <v>67</v>
       </c>
-      <c t="s" s="6" r="D18">
+      <c r="D18" s="6" t="s">
         <v>68</v>
       </c>
-      <c t="s" s="6" r="E18">
+      <c r="E18" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19">
-      <c s="11" r="A19"/>
-      <c s="11" r="B19"/>
-      <c s="11" r="C19"/>
-      <c s="11" r="D19"/>
-      <c s="11" r="E19"/>
-    </row>
-    <row r="20">
-      <c t="s" s="11" r="A20">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
         <v>70</v>
       </c>
-      <c t="s" s="6" r="B20">
+      <c r="B20" s="6" t="s">
         <v>71</v>
       </c>
-      <c t="s" s="6" r="C20">
+      <c r="C20" s="6" t="s">
         <v>72</v>
       </c>
-      <c t="s" s="6" r="D20">
+      <c r="D20" s="6" t="s">
         <v>73</v>
       </c>
-      <c t="s" s="6" r="E20">
+      <c r="E20" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="21">
-      <c s="11" r="A21"/>
-      <c t="s" s="6" r="B21">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="6" t="s">
         <v>75</v>
       </c>
-      <c t="s" s="6" r="C21">
+      <c r="C21" s="6" t="s">
         <v>76</v>
       </c>
-      <c t="s" s="6" r="D21">
+      <c r="D21" s="6" t="s">
         <v>77</v>
       </c>
-      <c t="s" s="6" r="E21">
+      <c r="E21" s="6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="22">
-      <c s="11" r="A22"/>
-      <c t="s" s="6" r="B22">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="6" t="s">
         <v>79</v>
       </c>
-      <c t="s" s="6" r="C22">
+      <c r="C22" s="6" t="s">
         <v>80</v>
       </c>
-      <c t="s" s="6" r="D22">
+      <c r="D22" s="6" t="s">
         <v>81</v>
       </c>
-      <c t="s" s="6" r="E22">
+      <c r="E22" s="6" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="23">
-      <c s="11" r="A23"/>
-      <c t="s" s="6" r="B23">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="6" t="s">
         <v>83</v>
       </c>
-      <c t="s" s="6" r="C23">
+      <c r="C23" s="6" t="s">
         <v>84</v>
       </c>
-      <c t="s" s="6" r="D23">
+      <c r="D23" s="6" t="s">
         <v>85</v>
       </c>
-      <c t="s" s="6" r="E23">
+      <c r="E23" s="6" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="24">
-      <c s="11" r="A24"/>
-      <c s="11" r="B24"/>
-      <c s="11" r="C24"/>
-      <c s="11" r="D24"/>
-      <c s="16" r="E24"/>
-    </row>
-    <row r="25">
-      <c t="s" s="11" r="A25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
         <v>87</v>
       </c>
-      <c t="s" s="2" r="B25">
+      <c r="B25" s="2" t="s">
         <v>88</v>
       </c>
-      <c t="s" s="2" r="C25">
+      <c r="C25" s="2" t="s">
         <v>89</v>
       </c>
-      <c s="2" r="D25"/>
-      <c s="2" r="E25"/>
-    </row>
-    <row r="26">
-      <c s="11" r="A26"/>
-      <c s="11" r="B26"/>
-      <c s="11" r="C26"/>
-      <c s="11" r="D26"/>
-      <c s="16" r="E26"/>
-    </row>
-    <row r="27">
-      <c t="s" s="16" r="A27">
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="15"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
         <v>90</v>
       </c>
-      <c t="s" s="6" r="B27">
+      <c r="B27" s="6" t="s">
         <v>91</v>
       </c>
-      <c t="s" s="6" r="C27">
+      <c r="C27" s="6" t="s">
         <v>90</v>
       </c>
-      <c t="s" s="6" r="D27">
+      <c r="D27" s="6" t="s">
         <v>92</v>
       </c>
-      <c t="s" s="6" r="E27">
+      <c r="E27" s="6" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="28">
-      <c s="16" r="A28"/>
-      <c t="s" s="6" r="B28">
+    <row r="28" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="15"/>
+      <c r="B28" s="6" t="s">
         <v>94</v>
       </c>
-      <c t="s" s="6" r="C28">
+      <c r="C28" s="6" t="s">
         <v>95</v>
       </c>
-      <c t="s" s="6" r="D28">
+      <c r="D28" s="6" t="s">
         <v>96</v>
       </c>
-      <c t="s" s="6" r="E28">
+      <c r="E28" s="6" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="29">
-      <c s="16" r="A29"/>
-      <c t="s" s="6" r="B29">
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="15"/>
+      <c r="B29" s="6" t="s">
         <v>98</v>
       </c>
-      <c t="s" s="6" r="C29">
+      <c r="C29" s="6" t="s">
         <v>99</v>
       </c>
-      <c t="s" s="6" r="D29">
+      <c r="D29" s="6" t="s">
         <v>100</v>
       </c>
-      <c t="s" s="6" r="E29">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="30">
-      <c s="16" r="A30"/>
-      <c t="s" s="6" r="B30">
+      <c r="E29" s="17" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="15"/>
+      <c r="B30" s="6" t="s">
         <v>101</v>
       </c>
-      <c t="s" s="6" r="C30">
+      <c r="C30" s="6" t="s">
         <v>102</v>
       </c>
-      <c t="s" s="6" r="D30">
+      <c r="D30" s="6" t="s">
         <v>103</v>
       </c>
-      <c t="s" s="6" r="E30">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="31">
-      <c s="16" r="A31"/>
-      <c t="s" s="6" r="B31">
+      <c r="E30" s="18" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="15"/>
+      <c r="B31" s="6" t="s">
         <v>104</v>
       </c>
-      <c t="s" s="6" r="C31">
+      <c r="C31" s="6" t="s">
         <v>105</v>
       </c>
-      <c t="s" s="6" r="D31">
+      <c r="D31" s="6" t="s">
         <v>106</v>
       </c>
-      <c t="s" s="6" r="E31">
+      <c r="E31" s="6" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="32">
-      <c s="16" r="A32"/>
-      <c t="s" s="6" r="B32">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="15"/>
+      <c r="B32" s="6" t="s">
         <v>108</v>
       </c>
-      <c t="s" s="6" r="C32">
+      <c r="C32" s="6" t="s">
         <v>109</v>
       </c>
-      <c t="s" s="6" r="D32">
+      <c r="D32" s="6" t="s">
         <v>110</v>
       </c>
-      <c t="s" s="6" r="E32">
+      <c r="E32" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="33">
-      <c s="16" r="A33"/>
-      <c t="s" s="6" r="B33">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="15"/>
+      <c r="B33" s="6" t="s">
         <v>112</v>
       </c>
-      <c t="s" s="6" r="C33">
+      <c r="C33" s="6" t="s">
         <v>113</v>
       </c>
-      <c t="s" s="6" r="D33">
+      <c r="D33" s="6" t="s">
         <v>114</v>
       </c>
-      <c t="s" s="6" r="E33">
+      <c r="E33" s="6" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="34">
-      <c s="16" r="A34"/>
-      <c s="16" r="B34"/>
-      <c s="16" r="C34"/>
-      <c s="16" r="D34"/>
-      <c s="16" r="E34"/>
-    </row>
-    <row r="35">
-      <c t="s" s="16" r="A35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
         <v>116</v>
       </c>
-      <c t="s" s="12" r="B35">
+      <c r="B35" s="11" t="s">
         <v>117</v>
       </c>
-      <c t="s" s="12" r="C35">
+      <c r="C35" s="11" t="s">
         <v>118</v>
       </c>
-      <c s="12" r="D35"/>
-      <c s="12" r="E35"/>
-    </row>
-    <row r="36">
-      <c s="16" r="A36"/>
-      <c t="s" s="12" r="B36">
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="15"/>
+      <c r="B36" s="11" t="s">
         <v>119</v>
       </c>
-      <c t="s" s="12" r="C36">
+      <c r="C36" s="11" t="s">
         <v>120</v>
       </c>
-      <c s="12" r="D36"/>
-      <c s="12" r="E36"/>
-    </row>
-    <row r="37">
-      <c s="16" r="A37"/>
-      <c t="s" s="12" r="B37">
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="15"/>
+      <c r="B37" s="11" t="s">
         <v>121</v>
       </c>
-      <c t="s" s="12" r="C37">
+      <c r="C37" s="11" t="s">
         <v>122</v>
       </c>
-      <c s="12" r="D37"/>
-      <c s="12" r="E37"/>
-    </row>
-    <row r="38">
-      <c s="16" r="A38"/>
-      <c t="s" s="12" r="B38">
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="15"/>
+      <c r="B38" s="11" t="s">
         <v>123</v>
       </c>
-      <c t="s" s="12" r="C38">
+      <c r="C38" s="11" t="s">
         <v>124</v>
       </c>
-      <c s="12" r="D38"/>
-      <c s="12" r="E38"/>
-    </row>
-    <row r="39">
-      <c s="16" r="A39"/>
-      <c s="12" r="B39"/>
-      <c s="12" r="C39"/>
-      <c s="12" r="D39"/>
-      <c s="12" r="E39"/>
-    </row>
-    <row r="40">
-      <c t="s" s="16" r="A40">
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="15"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="15" t="s">
         <v>125</v>
       </c>
-      <c t="s" s="12" r="B40">
+      <c r="B40" s="11" t="s">
         <v>126</v>
       </c>
-      <c t="s" s="12" r="C40">
+      <c r="C40" s="11" t="s">
         <v>127</v>
       </c>
-      <c s="12" r="D40"/>
-      <c s="12" r="E40"/>
-    </row>
-    <row r="41">
-      <c s="16" r="A41"/>
-      <c t="s" s="12" r="B41">
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="15"/>
+      <c r="B41" s="11" t="s">
         <v>128</v>
       </c>
-      <c t="s" s="12" r="C41">
+      <c r="C41" s="11" t="s">
         <v>129</v>
       </c>
-      <c s="12" r="D41"/>
-      <c s="12" r="E41"/>
-    </row>
-    <row r="42">
-      <c s="16" r="A42"/>
-      <c t="s" s="12" r="B42">
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="15"/>
+      <c r="B42" s="11" t="s">
         <v>130</v>
       </c>
-      <c t="s" s="12" r="C42">
+      <c r="C42" s="11" t="s">
         <v>131</v>
       </c>
-      <c s="12" r="D42"/>
-      <c s="12" r="E42"/>
-    </row>
-    <row r="43">
-      <c s="16" r="A43"/>
-      <c t="s" s="12" r="B43">
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="15"/>
+      <c r="B43" s="11" t="s">
         <v>132</v>
       </c>
-      <c t="s" s="12" r="C43">
+      <c r="C43" s="11" t="s">
         <v>133</v>
       </c>
-      <c s="12" r="D43"/>
-      <c s="12" r="E43"/>
-    </row>
-    <row r="44">
-      <c s="16" r="A44"/>
-      <c s="16" r="B44"/>
-      <c s="16" r="C44"/>
-      <c s="16" r="D44"/>
-      <c s="16" r="E44"/>
-    </row>
-    <row r="45">
-      <c t="s" s="16" r="A45">
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="15"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="15" t="s">
         <v>134</v>
       </c>
-      <c t="s" s="6" r="B45">
+      <c r="B45" s="6" t="s">
         <v>135</v>
       </c>
-      <c t="s" s="6" r="C45">
+      <c r="C45" s="6" t="s">
         <v>136</v>
       </c>
-      <c t="s" s="6" r="D45">
+      <c r="D45" s="6" t="s">
         <v>137</v>
       </c>
-      <c t="s" s="6" r="E45">
+      <c r="E45" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="46">
-      <c s="16" r="A46"/>
-      <c t="s" s="6" r="B46">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="15"/>
+      <c r="B46" s="6" t="s">
         <v>138</v>
       </c>
-      <c t="s" s="6" r="C46">
+      <c r="C46" s="6" t="s">
         <v>139</v>
       </c>
-      <c t="s" s="6" r="D46">
+      <c r="D46" s="6" t="s">
         <v>140</v>
       </c>
-      <c t="s" s="6" r="E46">
+      <c r="E46" s="6" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="47">
-      <c s="16" r="A47"/>
-      <c t="s" s="6" r="B47">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="15"/>
+      <c r="B47" s="6" t="s">
         <v>142</v>
       </c>
-      <c t="s" s="6" r="C47">
+      <c r="C47" s="6" t="s">
         <v>143</v>
       </c>
-      <c t="s" s="6" r="D47">
+      <c r="D47" s="6" t="s">
         <v>144</v>
       </c>
-      <c t="s" s="6" r="E47">
+      <c r="E47" s="6" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="48">
-      <c s="16" r="A48"/>
-      <c t="s" s="6" r="B48">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="15"/>
+      <c r="B48" s="6" t="s">
         <v>146</v>
       </c>
-      <c t="s" s="6" r="C48">
+      <c r="C48" s="6" t="s">
         <v>147</v>
       </c>
-      <c t="s" s="6" r="D48">
+      <c r="D48" s="6" t="s">
         <v>148</v>
       </c>
-      <c t="s" s="6" r="E48">
+      <c r="E48" s="6" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="49">
-      <c s="16" r="A49"/>
-      <c t="s" s="6" r="B49">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="15"/>
+      <c r="B49" s="6" t="s">
         <v>150</v>
       </c>
-      <c t="s" s="6" r="C49">
+      <c r="C49" s="6" t="s">
         <v>151</v>
       </c>
-      <c t="s" s="6" r="D49">
+      <c r="D49" s="6" t="s">
         <v>152</v>
       </c>
-      <c t="s" s="6" r="E49">
+      <c r="E49" s="6" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="50">
-      <c s="16" r="A50"/>
-      <c t="s" s="6" r="B50">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="15"/>
+      <c r="B50" s="6" t="s">
         <v>154</v>
       </c>
-      <c t="s" s="6" r="C50">
+      <c r="C50" s="6" t="s">
         <v>155</v>
       </c>
-      <c t="s" s="6" r="D50">
+      <c r="D50" s="6" t="s">
         <v>156</v>
       </c>
-      <c t="s" s="6" r="E50">
+      <c r="E50" s="6" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="51">
-      <c s="16" r="A51"/>
-      <c t="s" s="6" r="B51">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="15"/>
+      <c r="B51" s="6" t="s">
         <v>158</v>
       </c>
-      <c t="s" s="6" r="C51">
+      <c r="C51" s="6" t="s">
         <v>159</v>
       </c>
-      <c t="s" s="6" r="D51">
+      <c r="D51" s="6" t="s">
         <v>160</v>
       </c>
-      <c t="s" s="6" r="E51">
+      <c r="E51" s="6" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="52">
-      <c s="16" r="A52"/>
-      <c t="s" s="6" r="B52">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="15"/>
+      <c r="B52" s="6" t="s">
         <v>162</v>
       </c>
-      <c t="s" s="6" r="C52">
+      <c r="C52" s="6" t="s">
         <v>163</v>
       </c>
-      <c t="s" s="6" r="D52">
+      <c r="D52" s="6" t="s">
         <v>164</v>
       </c>
-      <c t="s" s="6" r="E52">
+      <c r="E52" s="6" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="53">
-      <c s="16" r="A53"/>
-      <c t="s" s="6" r="B53">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="15"/>
+      <c r="B53" s="6" t="s">
         <v>166</v>
       </c>
-      <c t="s" s="6" r="C53">
+      <c r="C53" s="6" t="s">
         <v>167</v>
       </c>
-      <c t="s" s="6" r="D53">
+      <c r="D53" s="6" t="s">
         <v>168</v>
       </c>
-      <c t="s" s="6" r="E53">
+      <c r="E53" s="6" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="54">
-      <c s="16" r="A54"/>
-      <c s="16" r="B54"/>
-      <c s="16" r="C54"/>
-      <c s="16" r="D54"/>
-      <c s="16" r="E54"/>
-    </row>
-    <row r="55">
-      <c t="s" s="16" r="A55">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="15"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="15" t="s">
         <v>170</v>
       </c>
-      <c t="s" s="6" r="B55">
+      <c r="B55" s="6" t="s">
         <v>171</v>
       </c>
-      <c t="s" s="6" r="C55">
+      <c r="C55" s="6" t="s">
         <v>172</v>
       </c>
-      <c t="s" s="6" r="D55">
+      <c r="D55" s="6" t="s">
         <v>173</v>
       </c>
-      <c t="s" s="6" r="E55">
+      <c r="E55" s="6" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="56">
-      <c s="16" r="A56"/>
-      <c t="s" s="6" r="B56">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="15"/>
+      <c r="B56" s="6" t="s">
         <v>175</v>
       </c>
-      <c t="s" s="6" r="C56">
+      <c r="C56" s="6" t="s">
         <v>176</v>
       </c>
-      <c t="s" s="6" r="D56">
+      <c r="D56" s="6" t="s">
         <v>177</v>
       </c>
-      <c t="s" s="6" r="E56">
+      <c r="E56" s="6" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="57">
-      <c s="17" r="A57"/>
-      <c t="s" s="6" r="B57">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="16"/>
+      <c r="B57" s="6" t="s">
         <v>179</v>
       </c>
-      <c t="s" s="6" r="C57">
+      <c r="C57" s="6" t="s">
         <v>180</v>
       </c>
-      <c t="s" s="6" r="D57">
+      <c r="D57" s="6" t="s">
         <v>181</v>
       </c>
-      <c t="s" s="6" r="E57">
+      <c r="E57" s="6" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="58">
-      <c s="17" r="A58"/>
-      <c t="s" s="6" r="B58">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="16"/>
+      <c r="B58" s="6" t="s">
         <v>183</v>
       </c>
-      <c t="s" s="6" r="C58">
+      <c r="C58" s="6" t="s">
         <v>184</v>
       </c>
-      <c t="s" s="6" r="D58">
+      <c r="D58" s="6" t="s">
         <v>185</v>
       </c>
-      <c t="s" s="6" r="E58">
+      <c r="E58" s="6" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="59">
-      <c s="17" r="A59"/>
-      <c t="s" s="6" r="B59">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="16"/>
+      <c r="B59" s="6" t="s">
         <v>187</v>
       </c>
-      <c t="s" s="6" r="C59">
+      <c r="C59" s="6" t="s">
         <v>188</v>
       </c>
-      <c t="s" s="6" r="D59">
+      <c r="D59" s="6" t="s">
         <v>189</v>
       </c>
-      <c t="s" s="6" r="E59">
+      <c r="E59" s="6" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="60">
-      <c s="17" r="A60"/>
-      <c t="s" s="6" r="B60">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="16"/>
+      <c r="B60" s="6" t="s">
         <v>191</v>
       </c>
-      <c t="s" s="6" r="C60">
+      <c r="C60" s="6" t="s">
         <v>192</v>
       </c>
-      <c t="s" s="6" r="D60">
+      <c r="D60" s="6" t="s">
         <v>193</v>
       </c>
-      <c t="s" s="6" r="E60">
+      <c r="E60" s="6" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="61">
-      <c s="17" r="A61"/>
-      <c t="s" s="6" r="B61">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="16"/>
+      <c r="B61" s="6" t="s">
         <v>195</v>
       </c>
-      <c t="s" s="6" r="C61">
+      <c r="C61" s="6" t="s">
         <v>196</v>
       </c>
-      <c t="s" s="6" r="D61">
+      <c r="D61" s="6" t="s">
         <v>197</v>
       </c>
-      <c t="s" s="6" r="E61">
+      <c r="E61" s="6" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="62">
-      <c s="17" r="A62"/>
-      <c t="s" s="6" r="B62">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="16"/>
+      <c r="B62" s="6" t="s">
         <v>199</v>
       </c>
-      <c t="s" s="6" r="C62">
+      <c r="C62" s="6" t="s">
         <v>200</v>
       </c>
-      <c t="s" s="6" r="D62">
+      <c r="D62" s="6" t="s">
         <v>201</v>
       </c>
-      <c t="s" s="6" r="E62">
+      <c r="E62" s="6" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="63">
-      <c s="17" r="A63"/>
-      <c s="16" r="B63"/>
-      <c s="16" r="C63"/>
-      <c s="16" r="D63"/>
-      <c s="16" r="E63"/>
-    </row>
-    <row r="64">
-      <c t="s" s="17" r="A64">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="16"/>
+      <c r="B63" s="15"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="16" t="s">
         <v>203</v>
       </c>
-      <c t="s" s="6" r="B64">
+      <c r="B64" s="6" t="s">
         <v>204</v>
       </c>
-      <c t="s" s="6" r="C64">
+      <c r="C64" s="6" t="s">
         <v>205</v>
       </c>
-      <c t="s" s="6" r="D64">
+      <c r="D64" s="6" t="s">
         <v>206</v>
       </c>
-      <c t="s" s="6" r="E64">
+      <c r="E64" s="6" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="65">
-      <c s="17" r="A65"/>
-      <c t="s" s="6" r="B65">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="16"/>
+      <c r="B65" s="6" t="s">
         <v>208</v>
       </c>
-      <c t="s" s="6" r="C65">
+      <c r="C65" s="6" t="s">
         <v>209</v>
       </c>
-      <c t="s" s="6" r="D65">
+      <c r="D65" s="6" t="s">
         <v>210</v>
       </c>
-      <c t="s" s="6" r="E65">
+      <c r="E65" s="6" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="66">
-      <c s="17" r="A66"/>
-      <c t="s" s="6" r="B66">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="16"/>
+      <c r="B66" s="6" t="s">
         <v>212</v>
       </c>
-      <c t="s" s="6" r="C66">
+      <c r="C66" s="6" t="s">
         <v>213</v>
       </c>
-      <c t="s" s="6" r="D66">
+      <c r="D66" s="6" t="s">
         <v>214</v>
       </c>
-      <c t="s" s="6" r="E66">
+      <c r="E66" s="6" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="67">
-      <c s="17" r="A67"/>
-      <c t="s" s="6" r="B67">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="16"/>
+      <c r="B67" s="6" t="s">
         <v>216</v>
       </c>
-      <c t="s" s="6" r="C67">
+      <c r="C67" s="6" t="s">
         <v>217</v>
       </c>
-      <c t="s" s="6" r="D67">
+      <c r="D67" s="6" t="s">
         <v>218</v>
       </c>
-      <c t="s" s="6" r="E67">
+      <c r="E67" s="6" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="68">
-      <c s="17" r="A68"/>
-      <c t="s" s="6" r="B68">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="16"/>
+      <c r="B68" s="6" t="s">
         <v>220</v>
       </c>
-      <c t="s" s="6" r="C68">
+      <c r="C68" s="6" t="s">
         <v>221</v>
       </c>
-      <c t="s" s="6" r="D68">
+      <c r="D68" s="6" t="s">
         <v>222</v>
       </c>
-      <c t="s" s="6" r="E68">
+      <c r="E68" s="6" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="69">
-      <c s="17" r="A69"/>
-      <c t="s" s="6" r="B69">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="16"/>
+      <c r="B69" s="6" t="s">
         <v>224</v>
       </c>
-      <c t="s" s="6" r="C69">
+      <c r="C69" s="6" t="s">
         <v>225</v>
       </c>
-      <c t="s" s="6" r="D69">
+      <c r="D69" s="6" t="s">
         <v>226</v>
       </c>
-      <c t="s" s="6" r="E69">
+      <c r="E69" s="6" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="70">
-      <c s="17" r="A70"/>
-      <c t="s" s="6" r="B70">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="16"/>
+      <c r="B70" s="6" t="s">
         <v>227</v>
       </c>
-      <c t="s" s="6" r="C70">
+      <c r="C70" s="6" t="s">
         <v>228</v>
       </c>
-      <c t="s" s="6" r="D70">
+      <c r="D70" s="6" t="s">
         <v>229</v>
       </c>
-      <c t="s" s="6" r="E70">
+      <c r="E70" s="6" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="71">
-      <c s="17" r="A71"/>
-      <c t="s" s="6" r="B71">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="16"/>
+      <c r="B71" s="6" t="s">
         <v>231</v>
       </c>
-      <c t="s" s="6" r="C71">
+      <c r="C71" s="6" t="s">
         <v>232</v>
       </c>
-      <c t="s" s="6" r="D71">
+      <c r="D71" s="6" t="s">
         <v>233</v>
       </c>
-      <c t="s" s="6" r="E71">
+      <c r="E71" s="6" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="72">
-      <c s="17" r="A72"/>
-      <c t="s" s="6" r="B72">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="16"/>
+      <c r="B72" s="6" t="s">
         <v>235</v>
       </c>
-      <c t="s" s="6" r="C72">
+      <c r="C72" s="6" t="s">
         <v>236</v>
       </c>
-      <c t="s" s="6" r="D72">
+      <c r="D72" s="6" t="s">
         <v>237</v>
       </c>
-      <c t="s" s="6" r="E72">
+      <c r="E72" s="6" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="73">
-      <c s="17" r="A73"/>
-      <c t="s" s="6" r="B73">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="16"/>
+      <c r="B73" s="6" t="s">
         <v>239</v>
       </c>
-      <c t="s" s="6" r="C73">
+      <c r="C73" s="6" t="s">
         <v>240</v>
       </c>
-      <c t="s" s="6" r="D73">
+      <c r="D73" s="6" t="s">
         <v>241</v>
       </c>
-      <c t="s" s="6" r="E73">
+      <c r="E73" s="6" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="74">
-      <c s="17" r="A74"/>
-      <c t="s" s="6" r="B74">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="16"/>
+      <c r="B74" s="6" t="s">
         <v>243</v>
       </c>
-      <c t="s" s="6" r="C74">
+      <c r="C74" s="6" t="s">
         <v>244</v>
       </c>
-      <c t="s" s="6" r="D74">
+      <c r="D74" s="6" t="s">
         <v>245</v>
       </c>
-      <c t="s" s="6" r="E74">
+      <c r="E74" s="6" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="75">
-      <c s="17" r="A75"/>
-      <c t="s" s="6" r="B75">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="16"/>
+      <c r="B75" s="6" t="s">
         <v>247</v>
       </c>
-      <c t="s" s="6" r="C75">
+      <c r="C75" s="6" t="s">
         <v>248</v>
       </c>
-      <c t="s" s="6" r="D75">
+      <c r="D75" s="6" t="s">
         <v>248</v>
       </c>
-      <c t="s" s="6" r="E75">
+      <c r="E75" s="6" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="76">
-      <c s="17" r="A76"/>
-      <c t="s" s="6" r="B76">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="16"/>
+      <c r="B76" s="6" t="s">
         <v>250</v>
       </c>
-      <c t="s" s="6" r="C76">
+      <c r="C76" s="6" t="s">
         <v>251</v>
       </c>
-      <c t="s" s="6" r="D76">
+      <c r="D76" s="6" t="s">
         <v>251</v>
       </c>
-      <c t="s" s="6" r="E76">
+      <c r="E76" s="6" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="77">
-      <c s="17" r="A77"/>
-      <c t="s" s="6" r="B77">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="16"/>
+      <c r="B77" s="6" t="s">
         <v>253</v>
       </c>
-      <c t="s" s="6" r="C77">
+      <c r="C77" s="6" t="s">
         <v>254</v>
       </c>
-      <c t="s" s="6" r="D77">
+      <c r="D77" s="6" t="s">
         <v>255</v>
       </c>
-      <c t="s" s="6" r="E77">
+      <c r="E77" s="6" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="78">
-      <c s="17" r="A78"/>
-      <c t="s" s="8" r="B78">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="16"/>
+      <c r="B78" s="7" t="s">
         <v>257</v>
       </c>
-      <c t="s" s="6" r="C78">
+      <c r="C78" s="6" t="s">
         <v>258</v>
       </c>
-      <c t="s" s="6" r="D78">
+      <c r="D78" s="6" t="s">
         <v>259</v>
       </c>
-      <c t="s" s="6" r="E78">
+      <c r="E78" s="6" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="79">
-      <c s="17" r="A79"/>
-      <c t="s" s="6" r="B79">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="16"/>
+      <c r="B79" s="6" t="s">
         <v>260</v>
       </c>
-      <c t="s" s="6" r="C79">
+      <c r="C79" s="6" t="s">
         <v>261</v>
       </c>
-      <c t="s" s="6" r="D79">
+      <c r="D79" s="6" t="s">
         <v>262</v>
       </c>
-      <c t="s" s="6" r="E79">
+      <c r="E79" s="6" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="80">
-      <c s="17" r="A80"/>
-      <c t="s" s="6" r="B80">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="16"/>
+      <c r="B80" s="6" t="s">
         <v>264</v>
       </c>
-      <c t="s" s="6" r="C80">
+      <c r="C80" s="6" t="s">
         <v>265</v>
       </c>
-      <c t="s" s="6" r="D80">
+      <c r="D80" s="6" t="s">
         <v>266</v>
       </c>
-      <c t="s" s="6" r="E80">
+      <c r="E80" s="6" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="81">
-      <c s="17" r="A81"/>
-      <c t="s" s="6" r="B81">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="16"/>
+      <c r="B81" s="6" t="s">
         <v>268</v>
       </c>
-      <c t="s" s="6" r="C81">
+      <c r="C81" s="6" t="s">
         <v>269</v>
       </c>
-      <c t="s" s="6" r="D81">
+      <c r="D81" s="6" t="s">
         <v>270</v>
       </c>
-      <c t="s" s="6" r="E81">
+      <c r="E81" s="6" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="82">
-      <c s="17" r="A82"/>
-      <c t="s" s="6" r="B82">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="16"/>
+      <c r="B82" s="6" t="s">
         <v>272</v>
       </c>
-      <c t="s" s="6" r="C82">
+      <c r="C82" s="6" t="s">
         <v>273</v>
       </c>
-      <c t="s" s="6" r="D82">
+      <c r="D82" s="6" t="s">
         <v>274</v>
       </c>
-      <c t="s" s="6" r="E82">
+      <c r="E82" s="6" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="83">
-      <c s="17" r="A83"/>
-      <c t="s" s="6" r="B83">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="16"/>
+      <c r="B83" s="6" t="s">
         <v>276</v>
       </c>
-      <c t="s" s="6" r="C83">
+      <c r="C83" s="6" t="s">
         <v>277</v>
       </c>
-      <c t="s" s="6" r="D83">
+      <c r="D83" s="6" t="s">
         <v>278</v>
       </c>
-      <c t="s" s="6" r="E83">
+      <c r="E83" s="6" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="84">
-      <c s="17" r="A84"/>
-      <c t="s" s="6" r="B84">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="16"/>
+      <c r="B84" s="6" t="s">
         <v>280</v>
       </c>
-      <c t="s" s="6" r="C84">
+      <c r="C84" s="6" t="s">
         <v>281</v>
       </c>
-      <c t="s" s="6" r="D84">
+      <c r="D84" s="6" t="s">
         <v>282</v>
       </c>
-      <c t="s" s="6" r="E84">
+      <c r="E84" s="6" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="85">
-      <c s="17" r="A85"/>
-      <c t="s" s="6" r="B85">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="16"/>
+      <c r="B85" s="6" t="s">
         <v>284</v>
       </c>
-      <c t="s" s="6" r="C85">
+      <c r="C85" s="6" t="s">
         <v>285</v>
       </c>
-      <c t="s" s="6" r="D85">
+      <c r="D85" s="6" t="s">
         <v>286</v>
       </c>
-      <c t="s" s="6" r="E85">
+      <c r="E85" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="86">
-      <c s="17" r="A86"/>
-      <c t="s" s="6" r="B86">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="16"/>
+      <c r="B86" s="6" t="s">
         <v>288</v>
       </c>
-      <c t="s" s="6" r="C86">
+      <c r="C86" s="6" t="s">
         <v>289</v>
       </c>
-      <c t="s" s="6" r="D86">
+      <c r="D86" s="6" t="s">
         <v>290</v>
       </c>
-      <c t="s" s="6" r="E86">
+      <c r="E86" s="6" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="87">
-      <c s="17" r="A87"/>
-      <c t="s" s="6" r="B87">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="16"/>
+      <c r="B87" s="6" t="s">
         <v>292</v>
       </c>
-      <c t="s" s="6" r="C87">
+      <c r="C87" s="6" t="s">
         <v>293</v>
       </c>
-      <c t="s" s="6" r="D87">
+      <c r="D87" s="6" t="s">
         <v>294</v>
       </c>
-      <c t="s" s="6" r="E87">
+      <c r="E87" s="6" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="88">
-      <c s="17" r="A88"/>
-      <c t="s" s="6" r="B88">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="16"/>
+      <c r="B88" s="6" t="s">
         <v>296</v>
       </c>
-      <c t="s" s="6" r="C88">
+      <c r="C88" s="6" t="s">
         <v>297</v>
       </c>
-      <c t="s" s="6" r="D88">
+      <c r="D88" s="6" t="s">
         <v>298</v>
       </c>
-      <c t="s" s="6" r="E88">
+      <c r="E88" s="6" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="89">
-      <c s="17" r="A89"/>
-      <c t="s" s="6" r="B89">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="16"/>
+      <c r="B89" s="6" t="s">
         <v>300</v>
       </c>
-      <c t="s" s="6" r="C89">
+      <c r="C89" s="6" t="s">
         <v>301</v>
       </c>
-      <c t="s" s="6" r="D89">
+      <c r="D89" s="6" t="s">
         <v>302</v>
       </c>
-      <c t="s" s="6" r="E89">
+      <c r="E89" s="6" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="90">
-      <c s="17" r="A90"/>
-      <c t="s" s="6" r="B90">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="16"/>
+      <c r="B90" s="6" t="s">
         <v>304</v>
       </c>
-      <c t="s" s="6" r="C90">
+      <c r="C90" s="6" t="s">
         <v>305</v>
       </c>
-      <c t="s" s="6" r="D90">
+      <c r="D90" s="6" t="s">
         <v>306</v>
       </c>
-      <c t="s" s="6" r="E90">
+      <c r="E90" s="6" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="91">
-      <c s="17" r="A91"/>
-      <c t="s" s="6" r="B91">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="16"/>
+      <c r="B91" s="6" t="s">
         <v>308</v>
       </c>
-      <c t="s" s="6" r="C91">
+      <c r="C91" s="6" t="s">
         <v>309</v>
       </c>
-      <c t="s" s="6" r="D91">
+      <c r="D91" s="6" t="s">
         <v>310</v>
       </c>
-      <c t="s" s="6" r="E91">
+      <c r="E91" s="6" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="92">
-      <c s="17" r="A92"/>
-      <c t="s" s="6" r="B92">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="16"/>
+      <c r="B92" s="6" t="s">
         <v>312</v>
       </c>
-      <c t="s" s="6" r="C92">
+      <c r="C92" s="6" t="s">
         <v>313</v>
       </c>
-      <c t="s" s="6" r="D92">
+      <c r="D92" s="6" t="s">
         <v>314</v>
       </c>
-      <c t="s" s="6" r="E92">
+      <c r="E92" s="6" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="93">
-      <c s="17" r="A93"/>
-      <c t="s" s="6" r="B93">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="16"/>
+      <c r="B93" s="6" t="s">
         <v>316</v>
       </c>
-      <c t="s" s="6" r="C93">
+      <c r="C93" s="6" t="s">
         <v>317</v>
       </c>
-      <c t="s" s="6" r="D93">
+      <c r="D93" s="6" t="s">
         <v>318</v>
       </c>
-      <c t="s" s="6" r="E93">
+      <c r="E93" s="6" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="94">
-      <c s="17" r="A94"/>
-      <c t="s" s="6" r="B94">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="16"/>
+      <c r="B94" s="6" t="s">
         <v>320</v>
       </c>
-      <c t="s" s="8" r="C94">
+      <c r="C94" s="7" t="s">
         <v>321</v>
       </c>
-      <c t="s" s="6" r="D94">
+      <c r="D94" s="6" t="s">
         <v>322</v>
       </c>
-      <c t="s" s="6" r="E94">
+      <c r="E94" s="6" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="95">
-      <c s="17" r="A95"/>
-      <c t="s" s="8" r="B95">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="16"/>
+      <c r="B95" s="7" t="s">
         <v>324</v>
       </c>
-      <c t="s" s="8" r="C95">
+      <c r="C95" s="7" t="s">
         <v>325</v>
       </c>
-      <c t="s" s="6" r="D95">
+      <c r="D95" s="6" t="s">
         <v>326</v>
       </c>
-      <c t="s" s="6" r="E95">
+      <c r="E95" s="6" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="96">
-      <c s="17" r="A96"/>
-      <c t="s" s="6" r="B96">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="16"/>
+      <c r="B96" s="6" t="s">
         <v>328</v>
       </c>
-      <c t="s" s="8" r="C96">
+      <c r="C96" s="7" t="s">
         <v>325</v>
       </c>
-      <c t="s" s="6" r="D96">
+      <c r="D96" s="6" t="s">
         <v>326</v>
       </c>
-      <c t="s" s="6" r="E96">
+      <c r="E96" s="6" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="97">
-      <c s="17" r="A97"/>
-      <c t="s" s="6" r="B97">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="16"/>
+      <c r="B97" s="6" t="s">
         <v>329</v>
       </c>
-      <c t="s" s="10" r="C97">
+      <c r="C97" s="9" t="s">
         <v>330</v>
       </c>
-      <c t="s" s="6" r="D97">
+      <c r="D97" s="6" t="s">
         <v>331</v>
       </c>
-      <c t="s" s="6" r="E97">
+      <c r="E97" s="6" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="98">
-      <c s="17" r="A98"/>
-      <c t="s" s="6" r="B98">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="16"/>
+      <c r="B98" s="6" t="s">
         <v>333</v>
       </c>
-      <c t="s" s="10" r="C98">
+      <c r="C98" s="9" t="s">
         <v>334</v>
       </c>
-      <c t="s" s="6" r="D98">
+      <c r="D98" s="6" t="s">
         <v>335</v>
       </c>
-      <c t="s" s="6" r="E98">
+      <c r="E98" s="6" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="99">
-      <c s="17" r="A99"/>
-      <c t="s" s="6" r="B99">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="16"/>
+      <c r="B99" s="6" t="s">
         <v>337</v>
       </c>
-      <c t="s" s="10" r="C99">
+      <c r="C99" s="9" t="s">
         <v>338</v>
       </c>
-      <c t="s" s="6" r="D99">
+      <c r="D99" s="6" t="s">
         <v>339</v>
       </c>
-      <c t="s" s="10" r="E99">
+      <c r="E99" s="9" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="100">
-      <c s="17" r="A100"/>
-      <c s="15" r="B100"/>
-      <c s="13" r="C100"/>
-      <c s="15" r="D100"/>
-      <c s="15" r="E100"/>
-    </row>
-    <row r="101">
-      <c t="s" s="17" r="A101">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="16"/>
+      <c r="B100" s="14"/>
+      <c r="C100" s="12"/>
+      <c r="D100" s="14"/>
+      <c r="E100" s="14"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="16" t="s">
         <v>341</v>
       </c>
-      <c t="s" s="6" r="B101">
+      <c r="B101" s="6" t="s">
         <v>342</v>
       </c>
-      <c t="s" s="8" r="C101">
+      <c r="C101" s="7" t="s">
         <v>343</v>
       </c>
-      <c t="s" s="6" r="D101">
+      <c r="D101" s="6" t="s">
         <v>344</v>
       </c>
-      <c t="s" s="6" r="E101">
+      <c r="E101" s="6" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="102">
-      <c s="17" r="A102"/>
-      <c t="s" s="9" r="B102">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="16"/>
+      <c r="B102" s="8" t="s">
         <v>346</v>
       </c>
-      <c t="s" s="14" r="C102">
+      <c r="C102" s="13" t="s">
         <v>347</v>
       </c>
-      <c s="9" r="D102"/>
-      <c s="9" r="E102"/>
-    </row>
-    <row r="103">
-      <c s="17" r="A103"/>
-      <c s="16" r="B103"/>
-      <c s="16" r="D103"/>
-      <c s="16" r="E103"/>
-    </row>
-    <row r="104">
-      <c t="s" s="17" r="A104">
+      <c r="D102" s="8"/>
+      <c r="E102" s="8"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="16"/>
+      <c r="B103" s="15"/>
+      <c r="D103" s="15"/>
+      <c r="E103" s="15"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="16" t="s">
         <v>348</v>
       </c>
-      <c t="s" s="3" r="B104">
+      <c r="B104" s="3" t="s">
         <v>349</v>
       </c>
-      <c t="s" s="1" r="C104">
+      <c r="C104" s="1" t="s">
         <v>350</v>
       </c>
-      <c s="3" r="D104"/>
-      <c s="3" r="E104"/>
-    </row>
-    <row r="105">
-      <c s="17" r="A105"/>
-      <c t="s" s="3" r="B105">
+      <c r="D104" s="3"/>
+      <c r="E104" s="3"/>
+    </row>
+    <row r="105" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A105" s="16"/>
+      <c r="B105" s="3" t="s">
         <v>351</v>
       </c>
-      <c t="s" s="1" r="C105">
+      <c r="C105" s="1" t="s">
         <v>352</v>
       </c>
-      <c s="3" r="D105"/>
-      <c s="3" r="E105"/>
-    </row>
-    <row r="106">
-      <c s="17" r="A106"/>
-      <c t="s" s="3" r="B106">
+      <c r="D105" s="3"/>
+      <c r="E105" s="3"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="16"/>
+      <c r="B106" s="3" t="s">
         <v>353</v>
       </c>
-      <c t="s" s="1" r="C106">
+      <c r="C106" s="1" t="s">
         <v>354</v>
       </c>
-      <c s="3" r="D106"/>
-      <c s="3" r="E106"/>
-    </row>
-    <row r="107">
-      <c s="17" r="A107"/>
-      <c t="s" s="3" r="B107">
+      <c r="D106" s="3"/>
+      <c r="E106" s="3"/>
+    </row>
+    <row r="107" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A107" s="16"/>
+      <c r="B107" s="3" t="s">
         <v>355</v>
       </c>
-      <c t="s" s="1" r="C107">
+      <c r="C107" s="1" t="s">
         <v>356</v>
       </c>
-      <c s="3" r="D107"/>
-      <c s="3" r="E107"/>
-    </row>
-    <row r="108">
-      <c s="17" r="A108"/>
-      <c t="s" s="3" r="B108">
+      <c r="D107" s="3"/>
+      <c r="E107" s="3"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="16"/>
+      <c r="B108" s="3" t="s">
         <v>357</v>
       </c>
-      <c t="s" s="1" r="C108">
+      <c r="C108" s="1" t="s">
         <v>358</v>
       </c>
-      <c s="3" r="D108"/>
-      <c s="3" r="E108"/>
-    </row>
-    <row r="109">
-      <c s="17" r="A109"/>
-      <c s="3" r="B109"/>
-      <c s="1" r="C109"/>
-      <c s="3" r="D109"/>
-      <c s="3" r="E109"/>
-    </row>
-    <row r="110">
-      <c t="s" s="17" r="A110">
+      <c r="D108" s="3"/>
+      <c r="E108" s="3"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="16"/>
+      <c r="B109" s="3"/>
+      <c r="C109" s="1"/>
+      <c r="D109" s="3"/>
+      <c r="E109" s="3"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="16" t="s">
         <v>359</v>
       </c>
-      <c t="s" s="3" r="B110">
+      <c r="B110" s="3" t="s">
         <v>360</v>
       </c>
-      <c t="s" s="1" r="C110">
+      <c r="C110" s="1" t="s">
         <v>359</v>
       </c>
-      <c s="3" r="D110"/>
-      <c s="3" r="E110"/>
-    </row>
-    <row r="111">
-      <c s="17" r="A111"/>
-      <c s="15" r="B111"/>
-      <c s="13" r="C111"/>
-      <c s="15" r="D111"/>
-      <c s="15" r="E111"/>
-    </row>
-    <row r="112">
-      <c s="17" r="A112"/>
-      <c s="15" r="B112"/>
-      <c s="13" r="C112"/>
-      <c s="15" r="D112"/>
-      <c s="15" r="E112"/>
-    </row>
-    <row r="113">
-      <c s="17" r="A113"/>
-      <c s="15" r="B113"/>
-      <c s="13" r="C113"/>
-      <c s="15" r="D113"/>
-      <c s="15" r="E113"/>
-    </row>
-    <row r="114">
-      <c s="17" r="A114"/>
-      <c s="15" r="B114"/>
-      <c s="13" r="C114"/>
-      <c s="15" r="D114"/>
-      <c s="15" r="E114"/>
-    </row>
-    <row r="115">
-      <c s="17" r="A115"/>
-      <c s="15" r="B115"/>
-      <c s="13" r="C115"/>
-      <c s="15" r="D115"/>
-      <c s="15" r="E115"/>
-    </row>
-    <row r="116">
-      <c s="17" r="A116"/>
-      <c s="15" r="B116"/>
-      <c s="13" r="C116"/>
-      <c s="15" r="D116"/>
-      <c s="15" r="E116"/>
+      <c r="D110" s="3"/>
+      <c r="E110" s="3"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="16"/>
+      <c r="B111" s="14"/>
+      <c r="C111" s="12"/>
+      <c r="D111" s="14"/>
+      <c r="E111" s="14"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="16"/>
+      <c r="B112" s="14"/>
+      <c r="C112" s="12"/>
+      <c r="D112" s="14"/>
+      <c r="E112" s="14"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="16"/>
+      <c r="B113" s="14"/>
+      <c r="C113" s="12"/>
+      <c r="D113" s="14"/>
+      <c r="E113" s="14"/>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="16"/>
+      <c r="B114" s="14"/>
+      <c r="C114" s="12"/>
+      <c r="D114" s="14"/>
+      <c r="E114" s="14"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="16"/>
+      <c r="B115" s="14"/>
+      <c r="C115" s="12"/>
+      <c r="D115" s="14"/>
+      <c r="E115" s="14"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="16"/>
+      <c r="B116" s="14"/>
+      <c r="C116" s="12"/>
+      <c r="D116" s="14"/>
+      <c r="E116" s="14"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="9.86" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c s="16" r="A1"/>
-      <c s="16" r="B1"/>
-      <c s="16" r="C1"/>
-      <c s="16" r="D1"/>
-      <c s="16" r="E1"/>
-      <c s="16" r="F1"/>
-    </row>
-    <row r="2">
-      <c s="16" r="A2"/>
-      <c s="16" r="B2"/>
-      <c s="16" r="C2"/>
-      <c s="16" r="D2"/>
-      <c s="16" r="E2"/>
-      <c s="16" r="F2"/>
-    </row>
-    <row r="3">
-      <c s="16" r="A3"/>
-      <c s="16" r="B3"/>
-      <c s="16" r="C3"/>
-      <c s="16" r="D3"/>
-      <c s="16" r="E3"/>
-      <c s="16" r="F3"/>
-    </row>
-    <row r="4">
-      <c s="16" r="A4"/>
-      <c s="16" r="B4"/>
-      <c s="16" r="C4"/>
-      <c s="16" r="D4"/>
-      <c s="16" r="E4"/>
-      <c s="16" r="F4"/>
-    </row>
-    <row r="5">
-      <c s="16" r="A5"/>
-      <c s="16" r="B5"/>
-      <c s="16" r="C5"/>
-      <c s="16" r="D5"/>
-      <c s="16" r="E5"/>
-      <c s="16" r="F5"/>
-    </row>
-    <row r="6">
-      <c s="16" r="A6"/>
-      <c s="16" r="B6"/>
-      <c s="16" r="C6"/>
-      <c s="16" r="D6"/>
-      <c s="16" r="E6"/>
-      <c s="16" r="F6"/>
-    </row>
-    <row r="7">
-      <c s="16" r="A7"/>
-      <c s="16" r="B7"/>
-      <c s="16" r="C7"/>
-      <c s="16" r="D7"/>
-      <c s="16" r="E7"/>
-      <c s="16" r="F7"/>
-    </row>
-    <row r="8">
-      <c s="16" r="A8"/>
-      <c s="16" r="B8"/>
-      <c s="16" r="C8"/>
-      <c s="16" r="D8"/>
-      <c s="16" r="E8"/>
-      <c s="16" r="F8"/>
-    </row>
-    <row r="9">
-      <c s="16" r="A9"/>
-      <c s="16" r="B9"/>
-      <c s="16" r="C9"/>
-      <c s="16" r="D9"/>
-      <c s="16" r="E9"/>
-      <c s="16" r="F9"/>
-    </row>
-    <row r="10">
-      <c s="16" r="A10"/>
-      <c s="16" r="B10"/>
-      <c s="16" r="C10"/>
-      <c s="16" r="D10"/>
-      <c s="16" r="E10"/>
-      <c s="16" r="F10"/>
-    </row>
-    <row r="11">
-      <c s="16" r="A11"/>
-      <c s="16" r="B11"/>
-      <c s="16" r="C11"/>
-      <c s="16" r="D11"/>
-      <c s="16" r="E11"/>
-      <c s="16" r="F11"/>
-    </row>
-    <row r="12">
-      <c s="16" r="A12"/>
-      <c s="16" r="B12"/>
-      <c s="16" r="C12"/>
-      <c s="16" r="D12"/>
-      <c s="16" r="E12"/>
-      <c s="16" r="F12"/>
-    </row>
-    <row r="13">
-      <c s="16" r="A13"/>
-      <c s="16" r="B13"/>
-      <c s="16" r="C13"/>
-      <c s="16" r="D13"/>
-      <c s="16" r="E13"/>
-      <c s="16" r="F13"/>
-    </row>
-    <row r="14">
-      <c s="16" r="A14"/>
-      <c s="16" r="B14"/>
-      <c s="16" r="C14"/>
-      <c s="16" r="D14"/>
-      <c s="16" r="E14"/>
-      <c s="16" r="F14"/>
-    </row>
-    <row r="15">
-      <c s="16" r="A15"/>
-      <c s="16" r="B15"/>
-      <c s="16" r="C15"/>
-      <c s="16" r="D15"/>
-      <c s="16" r="E15"/>
-      <c s="16" r="F15"/>
-    </row>
-    <row r="16">
-      <c s="16" r="A16"/>
-      <c s="16" r="B16"/>
-      <c s="16" r="C16"/>
-      <c s="16" r="D16"/>
-      <c s="16" r="E16"/>
-      <c s="16" r="F16"/>
-    </row>
-    <row r="17">
-      <c s="16" r="A17"/>
-      <c s="16" r="B17"/>
-      <c s="16" r="C17"/>
-      <c s="16" r="D17"/>
-      <c s="16" r="E17"/>
-      <c s="16" r="F17"/>
-    </row>
-    <row r="18">
-      <c s="16" r="A18"/>
-      <c s="16" r="B18"/>
-      <c s="16" r="C18"/>
-      <c s="16" r="D18"/>
-      <c s="16" r="E18"/>
-      <c s="16" r="F18"/>
-    </row>
-    <row r="19">
-      <c s="16" r="A19"/>
-      <c s="16" r="B19"/>
-      <c s="16" r="C19"/>
-      <c s="16" r="D19"/>
-      <c s="16" r="E19"/>
-      <c s="16" r="F19"/>
-    </row>
-    <row r="20">
-      <c s="16" r="A20"/>
-      <c s="16" r="B20"/>
-      <c s="16" r="C20"/>
-      <c s="16" r="D20"/>
-      <c s="16" r="E20"/>
-      <c s="16" r="F20"/>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="15"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="9.86" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c s="16" r="A1"/>
-      <c s="16" r="B1"/>
-      <c s="16" r="C1"/>
-      <c s="16" r="D1"/>
-      <c s="16" r="E1"/>
-      <c s="16" r="F1"/>
-    </row>
-    <row r="2">
-      <c s="16" r="A2"/>
-      <c s="16" r="B2"/>
-      <c s="16" r="C2"/>
-      <c s="16" r="D2"/>
-      <c s="16" r="E2"/>
-      <c s="16" r="F2"/>
-    </row>
-    <row r="3">
-      <c s="16" r="A3"/>
-      <c s="16" r="B3"/>
-      <c s="16" r="C3"/>
-      <c s="16" r="D3"/>
-      <c s="16" r="E3"/>
-      <c s="16" r="F3"/>
-    </row>
-    <row r="4">
-      <c s="16" r="A4"/>
-      <c s="16" r="B4"/>
-      <c s="16" r="C4"/>
-      <c s="16" r="D4"/>
-      <c s="16" r="E4"/>
-      <c s="16" r="F4"/>
-    </row>
-    <row r="5">
-      <c s="16" r="A5"/>
-      <c s="16" r="B5"/>
-      <c s="16" r="C5"/>
-      <c s="16" r="D5"/>
-      <c s="16" r="E5"/>
-      <c s="16" r="F5"/>
-    </row>
-    <row r="6">
-      <c s="16" r="A6"/>
-      <c s="16" r="B6"/>
-      <c s="16" r="C6"/>
-      <c s="16" r="D6"/>
-      <c s="16" r="E6"/>
-      <c s="16" r="F6"/>
-    </row>
-    <row r="7">
-      <c s="16" r="A7"/>
-      <c s="16" r="B7"/>
-      <c s="16" r="C7"/>
-      <c s="16" r="D7"/>
-      <c s="16" r="E7"/>
-      <c s="16" r="F7"/>
-    </row>
-    <row r="8">
-      <c s="16" r="A8"/>
-      <c s="16" r="B8"/>
-      <c s="16" r="C8"/>
-      <c s="16" r="D8"/>
-      <c s="16" r="E8"/>
-      <c s="16" r="F8"/>
-    </row>
-    <row r="9">
-      <c s="16" r="A9"/>
-      <c s="16" r="B9"/>
-      <c s="16" r="C9"/>
-      <c s="16" r="D9"/>
-      <c s="16" r="E9"/>
-      <c s="16" r="F9"/>
-    </row>
-    <row r="10">
-      <c s="16" r="A10"/>
-      <c s="16" r="B10"/>
-      <c s="16" r="C10"/>
-      <c s="16" r="D10"/>
-      <c s="16" r="E10"/>
-      <c s="16" r="F10"/>
-    </row>
-    <row r="11">
-      <c s="16" r="A11"/>
-      <c s="16" r="B11"/>
-      <c s="16" r="C11"/>
-      <c s="16" r="D11"/>
-      <c s="16" r="E11"/>
-      <c s="16" r="F11"/>
-    </row>
-    <row r="12">
-      <c s="16" r="A12"/>
-      <c s="16" r="B12"/>
-      <c s="16" r="C12"/>
-      <c s="16" r="D12"/>
-      <c s="16" r="E12"/>
-      <c s="16" r="F12"/>
-    </row>
-    <row r="13">
-      <c s="16" r="A13"/>
-      <c s="16" r="B13"/>
-      <c s="16" r="C13"/>
-      <c s="16" r="D13"/>
-      <c s="16" r="E13"/>
-      <c s="16" r="F13"/>
-    </row>
-    <row r="14">
-      <c s="16" r="A14"/>
-      <c s="16" r="B14"/>
-      <c s="16" r="C14"/>
-      <c s="16" r="D14"/>
-      <c s="16" r="E14"/>
-      <c s="16" r="F14"/>
-    </row>
-    <row r="15">
-      <c s="16" r="A15"/>
-      <c s="16" r="B15"/>
-      <c s="16" r="C15"/>
-      <c s="16" r="D15"/>
-      <c s="16" r="E15"/>
-      <c s="16" r="F15"/>
-    </row>
-    <row r="16">
-      <c s="16" r="A16"/>
-      <c s="16" r="B16"/>
-      <c s="16" r="C16"/>
-      <c s="16" r="D16"/>
-      <c s="16" r="E16"/>
-      <c s="16" r="F16"/>
-    </row>
-    <row r="17">
-      <c s="16" r="A17"/>
-      <c s="16" r="B17"/>
-      <c s="16" r="C17"/>
-      <c s="16" r="D17"/>
-      <c s="16" r="E17"/>
-      <c s="16" r="F17"/>
-    </row>
-    <row r="18">
-      <c s="16" r="A18"/>
-      <c s="16" r="B18"/>
-      <c s="16" r="C18"/>
-      <c s="16" r="D18"/>
-      <c s="16" r="E18"/>
-      <c s="16" r="F18"/>
-    </row>
-    <row r="19">
-      <c s="16" r="A19"/>
-      <c s="16" r="B19"/>
-      <c s="16" r="C19"/>
-      <c s="16" r="D19"/>
-      <c s="16" r="E19"/>
-      <c s="16" r="F19"/>
-    </row>
-    <row r="20">
-      <c s="16" r="A20"/>
-      <c s="16" r="B20"/>
-      <c s="16" r="C20"/>
-      <c s="16" r="D20"/>
-      <c s="16" r="E20"/>
-      <c s="16" r="F20"/>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="15"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
EWD-22362 - Add tooltips in Experiences list
Former-commit-id: 6374e3a7f62f2781e663ef912e8a10c4c494755b
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="386">
   <si>
     <t>Page</t>
   </si>
@@ -367,6 +367,24 @@
   </si>
   <si>
     <t>vollständig</t>
+  </si>
+  <si>
+    <t>experienceRebuildAction</t>
+  </si>
+  <si>
+    <t>Rebuild</t>
+  </si>
+  <si>
+    <t>addNewExperience</t>
+  </si>
+  <si>
+    <t>Add new experience</t>
+  </si>
+  <si>
+    <t>numberOfRelatedObjectives</t>
+  </si>
+  <si>
+    <t>Number of related objectives</t>
   </si>
   <si>
     <t>CreateObjective</t>
@@ -2085,48 +2103,48 @@
     </row>
     <row r="34">
       <c s="27" r="A34"/>
-      <c s="27" r="B34"/>
-      <c s="27" r="C34"/>
-      <c s="8" r="D34"/>
-      <c s="8" r="E34"/>
+      <c t="s" s="23" r="B34">
+        <v>118</v>
+      </c>
+      <c t="s" s="23" r="C34">
+        <v>119</v>
+      </c>
+      <c s="17" r="D34"/>
+      <c s="17" r="E34"/>
     </row>
     <row r="35">
-      <c t="s" s="27" r="A35">
-        <v>118</v>
-      </c>
-      <c t="s" s="25" r="B35">
-        <v>119</v>
-      </c>
-      <c t="s" s="25" r="C35">
+      <c s="27" r="A35"/>
+      <c t="s" s="23" r="B35">
         <v>120</v>
       </c>
-      <c s="22" r="D35"/>
-      <c s="22" r="E35"/>
+      <c t="s" s="23" r="C35">
+        <v>121</v>
+      </c>
+      <c s="17" r="D35"/>
+      <c s="17" r="E35"/>
     </row>
     <row r="36">
       <c s="27" r="A36"/>
-      <c t="s" s="25" r="B36">
-        <v>121</v>
-      </c>
-      <c t="s" s="25" r="C36">
+      <c t="s" s="23" r="B36">
         <v>122</v>
       </c>
-      <c s="22" r="D36"/>
-      <c s="22" r="E36"/>
+      <c t="s" s="23" r="C36">
+        <v>123</v>
+      </c>
+      <c s="17" r="D36"/>
+      <c s="17" r="E36"/>
     </row>
     <row r="37">
       <c s="27" r="A37"/>
-      <c t="s" s="25" r="B37">
-        <v>123</v>
-      </c>
-      <c t="s" s="25" r="C37">
+      <c s="27" r="B37"/>
+      <c s="27" r="C37"/>
+      <c s="8" r="D37"/>
+      <c s="8" r="E37"/>
+    </row>
+    <row r="38">
+      <c t="s" s="27" r="A38">
         <v>124</v>
       </c>
-      <c s="22" r="D37"/>
-      <c s="22" r="E37"/>
-    </row>
-    <row r="38">
-      <c s="27" r="A38"/>
       <c t="s" s="25" r="B38">
         <v>125</v>
       </c>
@@ -2138,20 +2156,22 @@
     </row>
     <row r="39">
       <c s="27" r="A39"/>
-      <c s="25" r="B39"/>
-      <c s="25" r="C39"/>
+      <c t="s" s="25" r="B39">
+        <v>127</v>
+      </c>
+      <c t="s" s="25" r="C39">
+        <v>128</v>
+      </c>
       <c s="22" r="D39"/>
       <c s="22" r="E39"/>
     </row>
     <row r="40">
-      <c t="s" s="27" r="A40">
-        <v>127</v>
-      </c>
+      <c s="27" r="A40"/>
       <c t="s" s="25" r="B40">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c t="s" s="25" r="C40">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c s="22" r="D40"/>
       <c s="22" r="E40"/>
@@ -2159,27 +2179,25 @@
     <row r="41">
       <c s="27" r="A41"/>
       <c t="s" s="25" r="B41">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c t="s" s="25" r="C41">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c s="22" r="D41"/>
       <c s="22" r="E41"/>
     </row>
     <row r="42">
       <c s="27" r="A42"/>
-      <c t="s" s="25" r="B42">
-        <v>132</v>
-      </c>
-      <c t="s" s="25" r="C42">
-        <v>133</v>
-      </c>
+      <c s="25" r="B42"/>
+      <c s="25" r="C42"/>
       <c s="22" r="D42"/>
       <c s="22" r="E42"/>
     </row>
     <row r="43">
-      <c s="27" r="A43"/>
+      <c t="s" s="27" r="A43">
+        <v>133</v>
+      </c>
       <c t="s" s="25" r="B43">
         <v>134</v>
       </c>
@@ -2191,999 +2209,1001 @@
     </row>
     <row r="44">
       <c s="27" r="A44"/>
-      <c s="27" r="B44"/>
-      <c s="27" r="C44"/>
-      <c s="8" r="D44"/>
-      <c s="8" r="E44"/>
+      <c t="s" s="25" r="B44">
+        <v>136</v>
+      </c>
+      <c t="s" s="25" r="C44">
+        <v>137</v>
+      </c>
+      <c s="22" r="D44"/>
+      <c s="22" r="E44"/>
     </row>
     <row r="45">
-      <c t="s" s="27" r="A45">
-        <v>136</v>
-      </c>
-      <c t="s" s="18" r="B45">
-        <v>137</v>
-      </c>
-      <c t="s" s="18" r="C45">
+      <c s="27" r="A45"/>
+      <c t="s" s="25" r="B45">
         <v>138</v>
       </c>
-      <c t="s" s="7" r="D45">
+      <c t="s" s="25" r="C45">
         <v>139</v>
       </c>
-      <c t="s" s="7" r="E45">
-        <v>17</v>
-      </c>
+      <c s="22" r="D45"/>
+      <c s="22" r="E45"/>
     </row>
     <row r="46">
       <c s="27" r="A46"/>
-      <c t="s" s="18" r="B46">
+      <c t="s" s="25" r="B46">
         <v>140</v>
       </c>
-      <c t="s" s="18" r="C46">
+      <c t="s" s="25" r="C46">
         <v>141</v>
       </c>
-      <c t="s" s="7" r="D46">
-        <v>142</v>
-      </c>
-      <c t="s" s="7" r="E46">
-        <v>143</v>
-      </c>
+      <c s="22" r="D46"/>
+      <c s="22" r="E46"/>
     </row>
     <row r="47">
       <c s="27" r="A47"/>
-      <c t="s" s="18" r="B47">
+      <c s="27" r="B47"/>
+      <c s="27" r="C47"/>
+      <c s="8" r="D47"/>
+      <c s="8" r="E47"/>
+    </row>
+    <row r="48">
+      <c t="s" s="27" r="A48">
+        <v>142</v>
+      </c>
+      <c t="s" s="18" r="B48">
+        <v>143</v>
+      </c>
+      <c t="s" s="18" r="C48">
         <v>144</v>
       </c>
-      <c t="s" s="18" r="C47">
+      <c t="s" s="7" r="D48">
         <v>145</v>
       </c>
-      <c t="s" s="7" r="D47">
-        <v>146</v>
-      </c>
-      <c t="s" s="7" r="E47">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="48">
-      <c s="27" r="A48"/>
-      <c t="s" s="18" r="B48">
-        <v>148</v>
-      </c>
-      <c t="s" s="18" r="C48">
-        <v>149</v>
-      </c>
-      <c t="s" s="7" r="D48">
-        <v>150</v>
-      </c>
       <c t="s" s="7" r="E48">
-        <v>151</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49">
       <c s="27" r="A49"/>
       <c t="s" s="18" r="B49">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c t="s" s="18" r="C49">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c t="s" s="7" r="D49">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c t="s" s="7" r="E49">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="50">
       <c s="27" r="A50"/>
       <c t="s" s="18" r="B50">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c t="s" s="18" r="C50">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c t="s" s="7" r="D50">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c t="s" s="7" r="E50">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="51">
       <c s="27" r="A51"/>
       <c t="s" s="18" r="B51">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c t="s" s="18" r="C51">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c t="s" s="7" r="D51">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c t="s" s="7" r="E51">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="52">
       <c s="27" r="A52"/>
       <c t="s" s="18" r="B52">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c t="s" s="18" r="C52">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c t="s" s="7" r="D52">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c t="s" s="7" r="E52">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="53">
       <c s="27" r="A53"/>
       <c t="s" s="18" r="B53">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c t="s" s="18" r="C53">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c t="s" s="7" r="D53">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c t="s" s="7" r="E53">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="54">
       <c s="27" r="A54"/>
-      <c s="27" r="B54"/>
-      <c s="27" r="C54"/>
-      <c s="8" r="D54"/>
-      <c s="8" r="E54"/>
+      <c t="s" s="18" r="B54">
+        <v>166</v>
+      </c>
+      <c t="s" s="18" r="C54">
+        <v>167</v>
+      </c>
+      <c t="s" s="7" r="D54">
+        <v>168</v>
+      </c>
+      <c t="s" s="7" r="E54">
+        <v>169</v>
+      </c>
     </row>
     <row r="55">
-      <c t="s" s="27" r="A55">
+      <c s="27" r="A55"/>
+      <c t="s" s="18" r="B55">
+        <v>170</v>
+      </c>
+      <c t="s" s="18" r="C55">
+        <v>171</v>
+      </c>
+      <c t="s" s="7" r="D55">
         <v>172</v>
       </c>
-      <c t="s" s="18" r="B55">
+      <c t="s" s="7" r="E55">
         <v>173</v>
-      </c>
-      <c t="s" s="18" r="C55">
-        <v>174</v>
-      </c>
-      <c t="s" s="7" r="D55">
-        <v>175</v>
-      </c>
-      <c t="s" s="7" r="E55">
-        <v>176</v>
       </c>
     </row>
     <row r="56">
       <c s="27" r="A56"/>
       <c t="s" s="18" r="B56">
+        <v>174</v>
+      </c>
+      <c t="s" s="18" r="C56">
+        <v>175</v>
+      </c>
+      <c t="s" s="7" r="D56">
+        <v>176</v>
+      </c>
+      <c t="s" s="7" r="E56">
         <v>177</v>
       </c>
-      <c t="s" s="18" r="C56">
+    </row>
+    <row r="57">
+      <c s="27" r="A57"/>
+      <c s="27" r="B57"/>
+      <c s="27" r="C57"/>
+      <c s="8" r="D57"/>
+      <c s="8" r="E57"/>
+    </row>
+    <row r="58">
+      <c t="s" s="27" r="A58">
         <v>178</v>
       </c>
-      <c t="s" s="7" r="D56">
+      <c t="s" s="18" r="B58">
         <v>179</v>
       </c>
-      <c t="s" s="7" r="E56">
+      <c t="s" s="18" r="C58">
         <v>180</v>
       </c>
-    </row>
-    <row r="57">
-      <c s="14" r="A57"/>
-      <c t="s" s="18" r="B57">
+      <c t="s" s="7" r="D58">
         <v>181</v>
       </c>
-      <c t="s" s="18" r="C57">
+      <c t="s" s="7" r="E58">
         <v>182</v>
       </c>
-      <c t="s" s="7" r="D57">
+    </row>
+    <row r="59">
+      <c s="27" r="A59"/>
+      <c t="s" s="18" r="B59">
         <v>183</v>
       </c>
-      <c t="s" s="7" r="E57">
+      <c t="s" s="18" r="C59">
         <v>184</v>
       </c>
-    </row>
-    <row r="58">
-      <c s="14" r="A58"/>
-      <c t="s" s="18" r="B58">
+      <c t="s" s="7" r="D59">
         <v>185</v>
       </c>
-      <c t="s" s="18" r="C58">
+      <c t="s" s="7" r="E59">
         <v>186</v>
-      </c>
-      <c t="s" s="7" r="D58">
-        <v>187</v>
-      </c>
-      <c t="s" s="7" r="E58">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="59">
-      <c s="14" r="A59"/>
-      <c t="s" s="18" r="B59">
-        <v>189</v>
-      </c>
-      <c t="s" s="18" r="C59">
-        <v>190</v>
-      </c>
-      <c t="s" s="7" r="D59">
-        <v>191</v>
-      </c>
-      <c t="s" s="7" r="E59">
-        <v>192</v>
       </c>
     </row>
     <row r="60">
       <c s="14" r="A60"/>
       <c t="s" s="18" r="B60">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c t="s" s="18" r="C60">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c t="s" s="7" r="D60">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c t="s" s="7" r="E60">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="61">
       <c s="14" r="A61"/>
       <c t="s" s="18" r="B61">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c t="s" s="18" r="C61">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c t="s" s="7" r="D61">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c t="s" s="7" r="E61">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="62">
       <c s="14" r="A62"/>
       <c t="s" s="18" r="B62">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c t="s" s="18" r="C62">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c t="s" s="7" r="D62">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c t="s" s="7" r="E62">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="63">
       <c s="14" r="A63"/>
-      <c s="27" r="B63"/>
-      <c s="27" r="C63"/>
-      <c s="8" r="D63"/>
-      <c s="8" r="E63"/>
+      <c t="s" s="18" r="B63">
+        <v>199</v>
+      </c>
+      <c t="s" s="18" r="C63">
+        <v>200</v>
+      </c>
+      <c t="s" s="7" r="D63">
+        <v>201</v>
+      </c>
+      <c t="s" s="7" r="E63">
+        <v>202</v>
+      </c>
     </row>
     <row r="64">
-      <c t="s" s="14" r="A64">
+      <c s="14" r="A64"/>
+      <c t="s" s="18" r="B64">
+        <v>203</v>
+      </c>
+      <c t="s" s="18" r="C64">
+        <v>204</v>
+      </c>
+      <c t="s" s="7" r="D64">
         <v>205</v>
       </c>
-      <c t="s" s="18" r="B64">
+      <c t="s" s="7" r="E64">
         <v>206</v>
-      </c>
-      <c t="s" s="18" r="C64">
-        <v>207</v>
-      </c>
-      <c t="s" s="7" r="D64">
-        <v>208</v>
-      </c>
-      <c t="s" s="7" r="E64">
-        <v>209</v>
       </c>
     </row>
     <row r="65">
       <c s="14" r="A65"/>
       <c t="s" s="18" r="B65">
+        <v>207</v>
+      </c>
+      <c t="s" s="18" r="C65">
+        <v>208</v>
+      </c>
+      <c t="s" s="7" r="D65">
+        <v>209</v>
+      </c>
+      <c t="s" s="7" r="E65">
         <v>210</v>
-      </c>
-      <c t="s" s="18" r="C65">
-        <v>211</v>
-      </c>
-      <c t="s" s="7" r="D65">
-        <v>212</v>
-      </c>
-      <c t="s" s="7" r="E65">
-        <v>213</v>
       </c>
     </row>
     <row r="66">
       <c s="14" r="A66"/>
-      <c t="s" s="18" r="B66">
+      <c s="27" r="B66"/>
+      <c s="27" r="C66"/>
+      <c s="8" r="D66"/>
+      <c s="8" r="E66"/>
+    </row>
+    <row r="67">
+      <c t="s" s="14" r="A67">
+        <v>211</v>
+      </c>
+      <c t="s" s="18" r="B67">
+        <v>212</v>
+      </c>
+      <c t="s" s="18" r="C67">
+        <v>213</v>
+      </c>
+      <c t="s" s="7" r="D67">
         <v>214</v>
       </c>
-      <c t="s" s="18" r="C66">
+      <c t="s" s="7" r="E67">
         <v>215</v>
-      </c>
-      <c t="s" s="7" r="D66">
-        <v>216</v>
-      </c>
-      <c t="s" s="7" r="E66">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="67">
-      <c s="14" r="A67"/>
-      <c t="s" s="18" r="B67">
-        <v>218</v>
-      </c>
-      <c t="s" s="18" r="C67">
-        <v>219</v>
-      </c>
-      <c t="s" s="7" r="D67">
-        <v>220</v>
-      </c>
-      <c t="s" s="7" r="E67">
-        <v>221</v>
       </c>
     </row>
     <row r="68">
       <c s="14" r="A68"/>
       <c t="s" s="18" r="B68">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c t="s" s="18" r="C68">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c t="s" s="7" r="D68">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c t="s" s="7" r="E68">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="69">
       <c s="14" r="A69"/>
       <c t="s" s="18" r="B69">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c t="s" s="18" r="C69">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c t="s" s="7" r="D69">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c t="s" s="7" r="E69">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="70">
       <c s="14" r="A70"/>
       <c t="s" s="18" r="B70">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c t="s" s="18" r="C70">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c t="s" s="7" r="D70">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c t="s" s="7" r="E70">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="71">
       <c s="14" r="A71"/>
       <c t="s" s="18" r="B71">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c t="s" s="18" r="C71">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c t="s" s="7" r="D71">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c t="s" s="7" r="E71">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="72">
       <c s="14" r="A72"/>
       <c t="s" s="18" r="B72">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c t="s" s="18" r="C72">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c t="s" s="7" r="D72">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c t="s" s="7" r="E72">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="73">
       <c s="14" r="A73"/>
       <c t="s" s="18" r="B73">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c t="s" s="18" r="C73">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c t="s" s="7" r="D73">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c t="s" s="7" r="E73">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="74">
       <c s="14" r="A74"/>
       <c t="s" s="18" r="B74">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c t="s" s="18" r="C74">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c t="s" s="7" r="D74">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c t="s" s="7" r="E74">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="75">
       <c s="14" r="A75"/>
       <c t="s" s="18" r="B75">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c t="s" s="18" r="C75">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c t="s" s="7" r="D75">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c t="s" s="7" r="E75">
-        <v>251</v>
+        <v>246</v>
       </c>
     </row>
     <row r="76">
       <c s="14" r="A76"/>
       <c t="s" s="18" r="B76">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c t="s" s="18" r="C76">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c t="s" s="7" r="D76">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c t="s" s="7" r="E76">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="77">
       <c s="14" r="A77"/>
       <c t="s" s="18" r="B77">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c t="s" s="18" r="C77">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c t="s" s="7" r="D77">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c t="s" s="7" r="E77">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="78">
       <c s="14" r="A78"/>
-      <c t="s" s="20" r="B78">
-        <v>259</v>
+      <c t="s" s="18" r="B78">
+        <v>255</v>
       </c>
       <c t="s" s="18" r="C78">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c t="s" s="7" r="D78">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c t="s" s="7" r="E78">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="79">
       <c s="14" r="A79"/>
       <c t="s" s="18" r="B79">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c t="s" s="18" r="C79">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c t="s" s="7" r="D79">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c t="s" s="7" r="E79">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="80">
       <c s="14" r="A80"/>
       <c t="s" s="18" r="B80">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c t="s" s="18" r="C80">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c t="s" s="7" r="D80">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c t="s" s="7" r="E80">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="81">
       <c s="14" r="A81"/>
-      <c t="s" s="18" r="B81">
-        <v>270</v>
+      <c t="s" s="20" r="B81">
+        <v>265</v>
       </c>
       <c t="s" s="18" r="C81">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c t="s" s="7" r="D81">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c t="s" s="7" r="E81">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="82">
       <c s="14" r="A82"/>
       <c t="s" s="18" r="B82">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c t="s" s="18" r="C82">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c t="s" s="7" r="D82">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c t="s" s="7" r="E82">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="83">
       <c s="14" r="A83"/>
       <c t="s" s="18" r="B83">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c t="s" s="18" r="C83">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c t="s" s="7" r="D83">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c t="s" s="7" r="E83">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="84">
       <c s="14" r="A84"/>
       <c t="s" s="18" r="B84">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c t="s" s="18" r="C84">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c t="s" s="7" r="D84">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c t="s" s="7" r="E84">
-        <v>285</v>
+        <v>279</v>
       </c>
     </row>
     <row r="85">
       <c s="14" r="A85"/>
       <c t="s" s="18" r="B85">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c t="s" s="18" r="C85">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c t="s" s="7" r="D85">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c t="s" s="7" r="E85">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="86">
       <c s="14" r="A86"/>
       <c t="s" s="18" r="B86">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c t="s" s="18" r="C86">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c t="s" s="7" r="D86">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c t="s" s="7" r="E86">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
     <row r="87">
       <c s="14" r="A87"/>
       <c t="s" s="18" r="B87">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c t="s" s="18" r="C87">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c t="s" s="7" r="D87">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c t="s" s="7" r="E87">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="88">
       <c s="14" r="A88"/>
       <c t="s" s="18" r="B88">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c t="s" s="18" r="C88">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c t="s" s="7" r="D88">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c t="s" s="7" r="E88">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="89">
       <c s="14" r="A89"/>
       <c t="s" s="18" r="B89">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c t="s" s="18" r="C89">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c t="s" s="7" r="D89">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c t="s" s="7" r="E89">
-        <v>305</v>
+        <v>299</v>
       </c>
     </row>
     <row r="90">
       <c s="14" r="A90"/>
       <c t="s" s="18" r="B90">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c t="s" s="18" r="C90">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c t="s" s="7" r="D90">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c t="s" s="7" r="E90">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="91">
       <c s="14" r="A91"/>
       <c t="s" s="18" r="B91">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c t="s" s="18" r="C91">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c t="s" s="7" r="D91">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c t="s" s="7" r="E91">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="92">
       <c s="14" r="A92"/>
       <c t="s" s="18" r="B92">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c t="s" s="18" r="C92">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c t="s" s="7" r="D92">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c t="s" s="7" r="E92">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="93">
       <c s="14" r="A93"/>
       <c t="s" s="18" r="B93">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c t="s" s="18" r="C93">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c t="s" s="7" r="D93">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c t="s" s="7" r="E93">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="94">
       <c s="14" r="A94"/>
       <c t="s" s="18" r="B94">
-        <v>322</v>
-      </c>
-      <c t="s" s="20" r="C94">
-        <v>323</v>
+        <v>316</v>
+      </c>
+      <c t="s" s="18" r="C94">
+        <v>317</v>
       </c>
       <c t="s" s="7" r="D94">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c t="s" s="7" r="E94">
-        <v>325</v>
+        <v>319</v>
       </c>
     </row>
     <row r="95">
       <c s="14" r="A95"/>
-      <c t="s" s="20" r="B95">
-        <v>326</v>
-      </c>
-      <c t="s" s="20" r="C95">
-        <v>327</v>
+      <c t="s" s="18" r="B95">
+        <v>320</v>
+      </c>
+      <c t="s" s="18" r="C95">
+        <v>321</v>
       </c>
       <c t="s" s="7" r="D95">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c t="s" s="7" r="E95">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="96">
       <c s="14" r="A96"/>
       <c t="s" s="18" r="B96">
-        <v>330</v>
-      </c>
-      <c t="s" s="20" r="C96">
+        <v>324</v>
+      </c>
+      <c t="s" s="18" r="C96">
+        <v>325</v>
+      </c>
+      <c t="s" s="7" r="D96">
+        <v>326</v>
+      </c>
+      <c t="s" s="7" r="E96">
         <v>327</v>
-      </c>
-      <c t="s" s="7" r="D96">
-        <v>328</v>
-      </c>
-      <c t="s" s="7" r="E96">
-        <v>329</v>
       </c>
     </row>
     <row r="97">
       <c s="14" r="A97"/>
       <c t="s" s="18" r="B97">
+        <v>328</v>
+      </c>
+      <c t="s" s="20" r="C97">
+        <v>329</v>
+      </c>
+      <c t="s" s="7" r="D97">
+        <v>330</v>
+      </c>
+      <c t="s" s="7" r="E97">
         <v>331</v>
-      </c>
-      <c t="s" s="10" r="C97">
-        <v>332</v>
-      </c>
-      <c t="s" s="7" r="D97">
-        <v>333</v>
-      </c>
-      <c t="s" s="7" r="E97">
-        <v>334</v>
       </c>
     </row>
     <row r="98">
       <c s="14" r="A98"/>
-      <c t="s" s="18" r="B98">
+      <c t="s" s="20" r="B98">
+        <v>332</v>
+      </c>
+      <c t="s" s="20" r="C98">
+        <v>333</v>
+      </c>
+      <c t="s" s="7" r="D98">
+        <v>334</v>
+      </c>
+      <c t="s" s="7" r="E98">
         <v>335</v>
-      </c>
-      <c t="s" s="10" r="C98">
-        <v>336</v>
-      </c>
-      <c t="s" s="7" r="D98">
-        <v>337</v>
-      </c>
-      <c t="s" s="7" r="E98">
-        <v>338</v>
       </c>
     </row>
     <row r="99">
       <c s="14" r="A99"/>
       <c t="s" s="18" r="B99">
-        <v>339</v>
-      </c>
-      <c t="s" s="10" r="C99">
-        <v>340</v>
+        <v>336</v>
+      </c>
+      <c t="s" s="20" r="C99">
+        <v>333</v>
       </c>
       <c t="s" s="7" r="D99">
-        <v>341</v>
-      </c>
-      <c t="s" s="3" r="E99">
-        <v>342</v>
+        <v>334</v>
+      </c>
+      <c t="s" s="7" r="E99">
+        <v>335</v>
       </c>
     </row>
     <row r="100">
       <c s="14" r="A100"/>
-      <c s="13" r="B100"/>
-      <c s="12" r="C100"/>
-      <c s="11" r="D100"/>
-      <c s="11" r="E100"/>
+      <c t="s" s="18" r="B100">
+        <v>337</v>
+      </c>
+      <c t="s" s="10" r="C100">
+        <v>338</v>
+      </c>
+      <c t="s" s="7" r="D100">
+        <v>339</v>
+      </c>
+      <c t="s" s="7" r="E100">
+        <v>340</v>
+      </c>
     </row>
     <row r="101">
-      <c t="s" s="14" r="A101">
+      <c s="14" r="A101"/>
+      <c t="s" s="18" r="B101">
+        <v>341</v>
+      </c>
+      <c t="s" s="10" r="C101">
+        <v>342</v>
+      </c>
+      <c t="s" s="7" r="D101">
         <v>343</v>
       </c>
-      <c t="s" s="18" r="B101">
+      <c t="s" s="7" r="E101">
         <v>344</v>
-      </c>
-      <c t="s" s="20" r="C101">
-        <v>345</v>
-      </c>
-      <c t="s" s="7" r="D101">
-        <v>346</v>
-      </c>
-      <c t="s" s="7" r="E101">
-        <v>347</v>
       </c>
     </row>
     <row r="102">
       <c s="14" r="A102"/>
       <c t="s" s="18" r="B102">
+        <v>345</v>
+      </c>
+      <c t="s" s="10" r="C102">
+        <v>346</v>
+      </c>
+      <c t="s" s="7" r="D102">
+        <v>347</v>
+      </c>
+      <c t="s" s="3" r="E102">
         <v>348</v>
-      </c>
-      <c t="s" s="20" r="C102">
-        <v>349</v>
-      </c>
-      <c t="s" s="7" r="D102">
-        <v>350</v>
-      </c>
-      <c t="s" s="7" r="E102">
-        <v>351</v>
       </c>
     </row>
     <row r="103">
       <c s="14" r="A103"/>
-      <c s="18" r="B103"/>
-      <c s="20" r="C103"/>
-      <c s="7" r="D103"/>
-      <c s="7" r="E103"/>
+      <c s="13" r="B103"/>
+      <c s="12" r="C103"/>
+      <c s="11" r="D103"/>
+      <c s="11" r="E103"/>
     </row>
     <row r="104">
       <c t="s" s="14" r="A104">
+        <v>349</v>
+      </c>
+      <c t="s" s="18" r="B104">
+        <v>350</v>
+      </c>
+      <c t="s" s="20" r="C104">
+        <v>351</v>
+      </c>
+      <c t="s" s="7" r="D104">
         <v>352</v>
       </c>
-      <c t="s" s="18" r="B104">
+      <c t="s" s="7" r="E104">
         <v>353</v>
-      </c>
-      <c t="s" s="20" r="C104">
-        <v>354</v>
-      </c>
-      <c t="s" s="7" r="D104">
-        <v>355</v>
-      </c>
-      <c t="s" s="7" r="E104">
-        <v>356</v>
       </c>
     </row>
     <row r="105">
       <c s="14" r="A105"/>
       <c t="s" s="18" r="B105">
+        <v>354</v>
+      </c>
+      <c t="s" s="20" r="C105">
+        <v>355</v>
+      </c>
+      <c t="s" s="7" r="D105">
+        <v>356</v>
+      </c>
+      <c t="s" s="7" r="E105">
         <v>357</v>
-      </c>
-      <c t="s" s="20" r="C105">
-        <v>358</v>
-      </c>
-      <c t="s" s="7" r="D105">
-        <v>359</v>
-      </c>
-      <c t="s" s="7" r="E105">
-        <v>360</v>
       </c>
     </row>
     <row r="106">
       <c s="14" r="A106"/>
-      <c t="s" s="18" r="B106">
+      <c s="18" r="B106"/>
+      <c s="20" r="C106"/>
+      <c s="7" r="D106"/>
+      <c s="7" r="E106"/>
+    </row>
+    <row r="107">
+      <c t="s" s="14" r="A107">
+        <v>358</v>
+      </c>
+      <c t="s" s="18" r="B107">
+        <v>359</v>
+      </c>
+      <c t="s" s="20" r="C107">
+        <v>360</v>
+      </c>
+      <c t="s" s="7" r="D107">
         <v>361</v>
       </c>
-      <c t="s" s="20" r="C106">
+      <c t="s" s="7" r="E107">
         <v>362</v>
-      </c>
-      <c t="s" s="7" r="D106">
-        <v>363</v>
-      </c>
-      <c t="s" s="7" r="E106">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="107">
-      <c s="14" r="A107"/>
-      <c t="s" s="18" r="B107">
-        <v>365</v>
-      </c>
-      <c t="s" s="20" r="C107">
-        <v>366</v>
-      </c>
-      <c t="s" s="7" r="D107">
-        <v>367</v>
-      </c>
-      <c t="s" s="7" r="E107">
-        <v>368</v>
       </c>
     </row>
     <row r="108">
       <c s="14" r="A108"/>
       <c t="s" s="18" r="B108">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c t="s" s="20" r="C108">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c t="s" s="7" r="D108">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c t="s" s="7" r="E108">
-        <v>372</v>
+        <v>366</v>
       </c>
     </row>
     <row r="109">
       <c s="14" r="A109"/>
-      <c s="24" r="B109"/>
-      <c s="4" r="C109"/>
-      <c s="15" r="D109"/>
-      <c s="15" r="E109"/>
+      <c t="s" s="18" r="B109">
+        <v>367</v>
+      </c>
+      <c t="s" s="20" r="C109">
+        <v>368</v>
+      </c>
+      <c t="s" s="7" r="D109">
+        <v>369</v>
+      </c>
+      <c t="s" s="7" r="E109">
+        <v>370</v>
+      </c>
     </row>
     <row r="110">
-      <c t="s" s="14" r="A110">
+      <c s="14" r="A110"/>
+      <c t="s" s="18" r="B110">
+        <v>371</v>
+      </c>
+      <c t="s" s="20" r="C110">
+        <v>372</v>
+      </c>
+      <c t="s" s="7" r="D110">
         <v>373</v>
       </c>
-      <c t="s" s="25" r="B110">
+      <c t="s" s="7" r="E110">
         <v>374</v>
       </c>
-      <c t="s" s="2" r="C110">
-        <v>373</v>
-      </c>
-      <c s="22" r="D110"/>
-      <c s="22" r="E110"/>
     </row>
     <row r="111">
       <c s="14" r="A111"/>
-      <c s="13" r="B111"/>
-      <c s="12" r="C111"/>
-      <c s="11" r="D111"/>
-      <c s="11" r="E111"/>
+      <c t="s" s="18" r="B111">
+        <v>375</v>
+      </c>
+      <c t="s" s="20" r="C111">
+        <v>376</v>
+      </c>
+      <c t="s" s="7" r="D111">
+        <v>377</v>
+      </c>
+      <c t="s" s="7" r="E111">
+        <v>378</v>
+      </c>
     </row>
     <row r="112">
-      <c t="s" s="14" r="A112">
-        <v>375</v>
-      </c>
-      <c t="s" s="23" r="B112">
-        <v>376</v>
-      </c>
-      <c t="s" s="26" r="C112">
-        <v>377</v>
-      </c>
-      <c s="17" r="D112"/>
-      <c s="17" r="E112"/>
+      <c s="14" r="A112"/>
+      <c s="24" r="B112"/>
+      <c s="4" r="C112"/>
+      <c s="15" r="D112"/>
+      <c s="15" r="E112"/>
     </row>
     <row r="113">
-      <c s="14" r="A113"/>
-      <c t="s" s="23" r="B113">
-        <v>378</v>
-      </c>
-      <c t="s" s="26" r="C113">
+      <c t="s" s="14" r="A113">
         <v>379</v>
       </c>
-      <c s="17" r="D113"/>
-      <c s="17" r="E113"/>
+      <c t="s" s="25" r="B113">
+        <v>380</v>
+      </c>
+      <c t="s" s="2" r="C113">
+        <v>379</v>
+      </c>
+      <c s="22" r="D113"/>
+      <c s="22" r="E113"/>
     </row>
     <row r="114">
       <c s="14" r="A114"/>
@@ -3193,18 +3213,49 @@
       <c s="11" r="E114"/>
     </row>
     <row r="115">
-      <c s="14" r="A115"/>
-      <c s="13" r="B115"/>
-      <c s="12" r="C115"/>
-      <c s="11" r="D115"/>
-      <c s="11" r="E115"/>
+      <c t="s" s="14" r="A115">
+        <v>381</v>
+      </c>
+      <c t="s" s="23" r="B115">
+        <v>382</v>
+      </c>
+      <c t="s" s="26" r="C115">
+        <v>383</v>
+      </c>
+      <c s="17" r="D115"/>
+      <c s="17" r="E115"/>
     </row>
     <row r="116">
       <c s="14" r="A116"/>
-      <c s="13" r="B116"/>
-      <c s="12" r="C116"/>
-      <c s="11" r="D116"/>
-      <c s="11" r="E116"/>
+      <c t="s" s="23" r="B116">
+        <v>384</v>
+      </c>
+      <c t="s" s="26" r="C116">
+        <v>385</v>
+      </c>
+      <c s="17" r="D116"/>
+      <c s="17" r="E116"/>
+    </row>
+    <row r="117">
+      <c s="14" r="A117"/>
+      <c s="13" r="B117"/>
+      <c s="12" r="C117"/>
+      <c s="11" r="D117"/>
+      <c s="11" r="E117"/>
+    </row>
+    <row r="118">
+      <c s="14" r="A118"/>
+      <c s="13" r="B118"/>
+      <c s="12" r="C118"/>
+      <c s="11" r="D118"/>
+      <c s="11" r="E118"/>
+    </row>
+    <row r="119">
+      <c s="14" r="A119"/>
+      <c s="13" r="B119"/>
+      <c s="12" r="C119"/>
+      <c s="11" r="D119"/>
+      <c s="11" r="E119"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
EWD-22324 - Create question page functionality
Former-commit-id: bc363c148269635ac2c3d87454fc15a5dcca37b6
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="390">
   <si>
     <t>Page</t>
   </si>
@@ -647,6 +647,18 @@
   </si>
   <si>
     <t>Hier klicken, um eine Frage hinzuzufügen</t>
+  </si>
+  <si>
+    <t>createAndEdit</t>
+  </si>
+  <si>
+    <t>Create and edit</t>
+  </si>
+  <si>
+    <t>createAndNew</t>
+  </si>
+  <si>
+    <t>Create and new</t>
   </si>
   <si>
     <t>customLocalizationPlugin</t>
@@ -2515,497 +2527,489 @@
     </row>
     <row r="66">
       <c s="14" r="A66"/>
-      <c s="27" r="B66"/>
-      <c s="27" r="C66"/>
-      <c s="8" r="D66"/>
-      <c s="8" r="E66"/>
+      <c t="s" s="23" r="B66">
+        <v>211</v>
+      </c>
+      <c t="s" s="23" r="C66">
+        <v>212</v>
+      </c>
+      <c s="17" r="D66"/>
+      <c s="17" r="E66"/>
     </row>
     <row r="67">
-      <c t="s" s="14" r="A67">
-        <v>211</v>
-      </c>
-      <c t="s" s="18" r="B67">
-        <v>212</v>
-      </c>
-      <c t="s" s="18" r="C67">
+      <c s="14" r="A67"/>
+      <c t="s" s="23" r="B67">
         <v>213</v>
       </c>
-      <c t="s" s="7" r="D67">
+      <c t="s" s="23" r="C67">
         <v>214</v>
       </c>
-      <c t="s" s="7" r="E67">
-        <v>215</v>
-      </c>
+      <c s="17" r="D67"/>
+      <c s="17" r="E67"/>
     </row>
     <row r="68">
       <c s="14" r="A68"/>
-      <c t="s" s="18" r="B68">
+      <c s="27" r="B68"/>
+      <c s="27" r="C68"/>
+      <c s="8" r="D68"/>
+      <c s="8" r="E68"/>
+    </row>
+    <row r="69">
+      <c t="s" s="14" r="A69">
+        <v>215</v>
+      </c>
+      <c t="s" s="18" r="B69">
         <v>216</v>
       </c>
-      <c t="s" s="18" r="C68">
+      <c t="s" s="18" r="C69">
         <v>217</v>
       </c>
-      <c t="s" s="7" r="D68">
+      <c t="s" s="7" r="D69">
         <v>218</v>
       </c>
-      <c t="s" s="7" r="E68">
+      <c t="s" s="7" r="E69">
         <v>219</v>
-      </c>
-    </row>
-    <row r="69">
-      <c s="14" r="A69"/>
-      <c t="s" s="18" r="B69">
-        <v>220</v>
-      </c>
-      <c t="s" s="18" r="C69">
-        <v>221</v>
-      </c>
-      <c t="s" s="7" r="D69">
-        <v>222</v>
-      </c>
-      <c t="s" s="7" r="E69">
-        <v>223</v>
       </c>
     </row>
     <row r="70">
       <c s="14" r="A70"/>
       <c t="s" s="18" r="B70">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c t="s" s="18" r="C70">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c t="s" s="7" r="D70">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c t="s" s="7" r="E70">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="71">
       <c s="14" r="A71"/>
       <c t="s" s="18" r="B71">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c t="s" s="18" r="C71">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c t="s" s="7" r="D71">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c t="s" s="7" r="E71">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="72">
       <c s="14" r="A72"/>
       <c t="s" s="18" r="B72">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c t="s" s="18" r="C72">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c t="s" s="7" r="D72">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c t="s" s="7" r="E72">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="73">
       <c s="14" r="A73"/>
       <c t="s" s="18" r="B73">
+        <v>232</v>
+      </c>
+      <c t="s" s="18" r="C73">
+        <v>233</v>
+      </c>
+      <c t="s" s="7" r="D73">
+        <v>234</v>
+      </c>
+      <c t="s" s="7" r="E73">
         <v>235</v>
-      </c>
-      <c t="s" s="18" r="C73">
-        <v>236</v>
-      </c>
-      <c t="s" s="7" r="D73">
-        <v>237</v>
-      </c>
-      <c t="s" s="7" r="E73">
-        <v>238</v>
       </c>
     </row>
     <row r="74">
       <c s="14" r="A74"/>
       <c t="s" s="18" r="B74">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c t="s" s="18" r="C74">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c t="s" s="7" r="D74">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c t="s" s="7" r="E74">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="75">
       <c s="14" r="A75"/>
       <c t="s" s="18" r="B75">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c t="s" s="18" r="C75">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c t="s" s="7" r="D75">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c t="s" s="7" r="E75">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="76">
       <c s="14" r="A76"/>
       <c t="s" s="18" r="B76">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c t="s" s="18" r="C76">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c t="s" s="7" r="D76">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c t="s" s="7" r="E76">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="77">
       <c s="14" r="A77"/>
       <c t="s" s="18" r="B77">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c t="s" s="18" r="C77">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c t="s" s="7" r="D77">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c t="s" s="7" r="E77">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="78">
       <c s="14" r="A78"/>
       <c t="s" s="18" r="B78">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c t="s" s="18" r="C78">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c t="s" s="7" r="D78">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c t="s" s="7" r="E78">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="79">
       <c s="14" r="A79"/>
       <c t="s" s="18" r="B79">
+        <v>255</v>
+      </c>
+      <c t="s" s="18" r="C79">
+        <v>256</v>
+      </c>
+      <c t="s" s="7" r="D79">
+        <v>257</v>
+      </c>
+      <c t="s" s="7" r="E79">
         <v>258</v>
-      </c>
-      <c t="s" s="18" r="C79">
-        <v>259</v>
-      </c>
-      <c t="s" s="7" r="D79">
-        <v>259</v>
-      </c>
-      <c t="s" s="7" r="E79">
-        <v>260</v>
       </c>
     </row>
     <row r="80">
       <c s="14" r="A80"/>
       <c t="s" s="18" r="B80">
+        <v>259</v>
+      </c>
+      <c t="s" s="18" r="C80">
+        <v>260</v>
+      </c>
+      <c t="s" s="7" r="D80">
+        <v>260</v>
+      </c>
+      <c t="s" s="7" r="E80">
         <v>261</v>
-      </c>
-      <c t="s" s="18" r="C80">
-        <v>262</v>
-      </c>
-      <c t="s" s="7" r="D80">
-        <v>263</v>
-      </c>
-      <c t="s" s="7" r="E80">
-        <v>264</v>
       </c>
     </row>
     <row r="81">
       <c s="14" r="A81"/>
-      <c t="s" s="20" r="B81">
-        <v>265</v>
+      <c t="s" s="18" r="B81">
+        <v>262</v>
       </c>
       <c t="s" s="18" r="C81">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c t="s" s="7" r="D81">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c t="s" s="7" r="E81">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="82">
       <c s="14" r="A82"/>
       <c t="s" s="18" r="B82">
+        <v>265</v>
+      </c>
+      <c t="s" s="18" r="C82">
+        <v>266</v>
+      </c>
+      <c t="s" s="7" r="D82">
+        <v>267</v>
+      </c>
+      <c t="s" s="7" r="E82">
         <v>268</v>
-      </c>
-      <c t="s" s="18" r="C82">
-        <v>269</v>
-      </c>
-      <c t="s" s="7" r="D82">
-        <v>270</v>
-      </c>
-      <c t="s" s="7" r="E82">
-        <v>271</v>
       </c>
     </row>
     <row r="83">
       <c s="14" r="A83"/>
-      <c t="s" s="18" r="B83">
-        <v>272</v>
+      <c t="s" s="20" r="B83">
+        <v>269</v>
       </c>
       <c t="s" s="18" r="C83">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c t="s" s="7" r="D83">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c t="s" s="7" r="E83">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="84">
       <c s="14" r="A84"/>
       <c t="s" s="18" r="B84">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c t="s" s="18" r="C84">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c t="s" s="7" r="D84">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c t="s" s="7" r="E84">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="85">
       <c s="14" r="A85"/>
       <c t="s" s="18" r="B85">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c t="s" s="18" r="C85">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c t="s" s="7" r="D85">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c t="s" s="7" r="E85">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="86">
       <c s="14" r="A86"/>
       <c t="s" s="18" r="B86">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c t="s" s="18" r="C86">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c t="s" s="7" r="D86">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c t="s" s="7" r="E86">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="87">
       <c s="14" r="A87"/>
       <c t="s" s="18" r="B87">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c t="s" s="18" r="C87">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c t="s" s="7" r="D87">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c t="s" s="7" r="E87">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="88">
       <c s="14" r="A88"/>
       <c t="s" s="18" r="B88">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c t="s" s="18" r="C88">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c t="s" s="7" r="D88">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c t="s" s="7" r="E88">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="89">
       <c s="14" r="A89"/>
       <c t="s" s="18" r="B89">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c t="s" s="18" r="C89">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c t="s" s="7" r="D89">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c t="s" s="7" r="E89">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="90">
       <c s="14" r="A90"/>
       <c t="s" s="18" r="B90">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c t="s" s="18" r="C90">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c t="s" s="7" r="D90">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c t="s" s="7" r="E90">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="91">
       <c s="14" r="A91"/>
       <c t="s" s="18" r="B91">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c t="s" s="18" r="C91">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c t="s" s="7" r="D91">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c t="s" s="7" r="E91">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="92">
       <c s="14" r="A92"/>
       <c t="s" s="18" r="B92">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c t="s" s="18" r="C92">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c t="s" s="7" r="D92">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c t="s" s="7" r="E92">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="93">
       <c s="14" r="A93"/>
       <c t="s" s="18" r="B93">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c t="s" s="18" r="C93">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c t="s" s="7" r="D93">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c t="s" s="7" r="E93">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="94">
       <c s="14" r="A94"/>
       <c t="s" s="18" r="B94">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c t="s" s="18" r="C94">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c t="s" s="7" r="D94">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c t="s" s="7" r="E94">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="95">
       <c s="14" r="A95"/>
       <c t="s" s="18" r="B95">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c t="s" s="18" r="C95">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c t="s" s="7" r="D95">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c t="s" s="7" r="E95">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="96">
       <c s="14" r="A96"/>
       <c t="s" s="18" r="B96">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c t="s" s="18" r="C96">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c t="s" s="7" r="D96">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c t="s" s="7" r="E96">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="97">
       <c s="14" r="A97"/>
       <c t="s" s="18" r="B97">
-        <v>328</v>
-      </c>
-      <c t="s" s="20" r="C97">
-        <v>329</v>
+        <v>324</v>
+      </c>
+      <c t="s" s="18" r="C97">
+        <v>325</v>
       </c>
       <c t="s" s="7" r="D97">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c t="s" s="7" r="E97">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="98">
       <c s="14" r="A98"/>
-      <c t="s" s="20" r="B98">
-        <v>332</v>
-      </c>
-      <c t="s" s="20" r="C98">
-        <v>333</v>
+      <c t="s" s="18" r="B98">
+        <v>328</v>
+      </c>
+      <c t="s" s="18" r="C98">
+        <v>329</v>
       </c>
       <c t="s" s="7" r="D98">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c t="s" s="7" r="E98">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="99">
       <c s="14" r="A99"/>
       <c t="s" s="18" r="B99">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c t="s" s="20" r="C99">
         <v>333</v>
@@ -3019,236 +3023,252 @@
     </row>
     <row r="100">
       <c s="14" r="A100"/>
-      <c t="s" s="18" r="B100">
+      <c t="s" s="20" r="B100">
+        <v>336</v>
+      </c>
+      <c t="s" s="20" r="C100">
         <v>337</v>
       </c>
-      <c t="s" s="10" r="C100">
+      <c t="s" s="7" r="D100">
         <v>338</v>
       </c>
-      <c t="s" s="7" r="D100">
+      <c t="s" s="7" r="E100">
         <v>339</v>
-      </c>
-      <c t="s" s="7" r="E100">
-        <v>340</v>
       </c>
     </row>
     <row r="101">
       <c s="14" r="A101"/>
       <c t="s" s="18" r="B101">
-        <v>341</v>
-      </c>
-      <c t="s" s="10" r="C101">
-        <v>342</v>
+        <v>340</v>
+      </c>
+      <c t="s" s="20" r="C101">
+        <v>337</v>
       </c>
       <c t="s" s="7" r="D101">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c t="s" s="7" r="E101">
-        <v>344</v>
+        <v>339</v>
       </c>
     </row>
     <row r="102">
       <c s="14" r="A102"/>
       <c t="s" s="18" r="B102">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c t="s" s="10" r="C102">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c t="s" s="7" r="D102">
-        <v>347</v>
-      </c>
-      <c t="s" s="3" r="E102">
-        <v>348</v>
+        <v>343</v>
+      </c>
+      <c t="s" s="7" r="E102">
+        <v>344</v>
       </c>
     </row>
     <row r="103">
       <c s="14" r="A103"/>
-      <c s="13" r="B103"/>
-      <c s="12" r="C103"/>
-      <c s="11" r="D103"/>
-      <c s="11" r="E103"/>
+      <c t="s" s="18" r="B103">
+        <v>345</v>
+      </c>
+      <c t="s" s="10" r="C103">
+        <v>346</v>
+      </c>
+      <c t="s" s="7" r="D103">
+        <v>347</v>
+      </c>
+      <c t="s" s="7" r="E103">
+        <v>348</v>
+      </c>
     </row>
     <row r="104">
-      <c t="s" s="14" r="A104">
+      <c s="14" r="A104"/>
+      <c t="s" s="18" r="B104">
         <v>349</v>
       </c>
-      <c t="s" s="18" r="B104">
+      <c t="s" s="10" r="C104">
         <v>350</v>
       </c>
-      <c t="s" s="20" r="C104">
+      <c t="s" s="7" r="D104">
         <v>351</v>
       </c>
-      <c t="s" s="7" r="D104">
+      <c t="s" s="3" r="E104">
         <v>352</v>
-      </c>
-      <c t="s" s="7" r="E104">
-        <v>353</v>
       </c>
     </row>
     <row r="105">
       <c s="14" r="A105"/>
-      <c t="s" s="18" r="B105">
+      <c s="13" r="B105"/>
+      <c s="12" r="C105"/>
+      <c s="11" r="D105"/>
+      <c s="11" r="E105"/>
+    </row>
+    <row r="106">
+      <c t="s" s="14" r="A106">
+        <v>353</v>
+      </c>
+      <c t="s" s="18" r="B106">
         <v>354</v>
       </c>
-      <c t="s" s="20" r="C105">
+      <c t="s" s="20" r="C106">
         <v>355</v>
       </c>
-      <c t="s" s="7" r="D105">
+      <c t="s" s="7" r="D106">
         <v>356</v>
       </c>
-      <c t="s" s="7" r="E105">
+      <c t="s" s="7" r="E106">
         <v>357</v>
       </c>
     </row>
-    <row r="106">
-      <c s="14" r="A106"/>
-      <c s="18" r="B106"/>
-      <c s="20" r="C106"/>
-      <c s="7" r="D106"/>
-      <c s="7" r="E106"/>
-    </row>
     <row r="107">
-      <c t="s" s="14" r="A107">
+      <c s="14" r="A107"/>
+      <c t="s" s="18" r="B107">
         <v>358</v>
       </c>
-      <c t="s" s="18" r="B107">
+      <c t="s" s="20" r="C107">
         <v>359</v>
       </c>
-      <c t="s" s="20" r="C107">
+      <c t="s" s="7" r="D107">
         <v>360</v>
       </c>
-      <c t="s" s="7" r="D107">
+      <c t="s" s="7" r="E107">
         <v>361</v>
-      </c>
-      <c t="s" s="7" r="E107">
-        <v>362</v>
       </c>
     </row>
     <row r="108">
       <c s="14" r="A108"/>
-      <c t="s" s="18" r="B108">
+      <c s="18" r="B108"/>
+      <c s="20" r="C108"/>
+      <c s="7" r="D108"/>
+      <c s="7" r="E108"/>
+    </row>
+    <row r="109">
+      <c t="s" s="14" r="A109">
+        <v>362</v>
+      </c>
+      <c t="s" s="18" r="B109">
         <v>363</v>
       </c>
-      <c t="s" s="20" r="C108">
+      <c t="s" s="20" r="C109">
         <v>364</v>
       </c>
-      <c t="s" s="7" r="D108">
+      <c t="s" s="7" r="D109">
         <v>365</v>
       </c>
-      <c t="s" s="7" r="E108">
+      <c t="s" s="7" r="E109">
         <v>366</v>
-      </c>
-    </row>
-    <row r="109">
-      <c s="14" r="A109"/>
-      <c t="s" s="18" r="B109">
-        <v>367</v>
-      </c>
-      <c t="s" s="20" r="C109">
-        <v>368</v>
-      </c>
-      <c t="s" s="7" r="D109">
-        <v>369</v>
-      </c>
-      <c t="s" s="7" r="E109">
-        <v>370</v>
       </c>
     </row>
     <row r="110">
       <c s="14" r="A110"/>
       <c t="s" s="18" r="B110">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c t="s" s="20" r="C110">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c t="s" s="7" r="D110">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c t="s" s="7" r="E110">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="111">
       <c s="14" r="A111"/>
       <c t="s" s="18" r="B111">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c t="s" s="20" r="C111">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c t="s" s="7" r="D111">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c t="s" s="7" r="E111">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="112">
       <c s="14" r="A112"/>
-      <c s="24" r="B112"/>
-      <c s="4" r="C112"/>
-      <c s="15" r="D112"/>
-      <c s="15" r="E112"/>
+      <c t="s" s="18" r="B112">
+        <v>375</v>
+      </c>
+      <c t="s" s="20" r="C112">
+        <v>376</v>
+      </c>
+      <c t="s" s="7" r="D112">
+        <v>377</v>
+      </c>
+      <c t="s" s="7" r="E112">
+        <v>378</v>
+      </c>
     </row>
     <row r="113">
-      <c t="s" s="14" r="A113">
+      <c s="14" r="A113"/>
+      <c t="s" s="18" r="B113">
         <v>379</v>
       </c>
-      <c t="s" s="25" r="B113">
+      <c t="s" s="20" r="C113">
         <v>380</v>
       </c>
-      <c t="s" s="2" r="C113">
-        <v>379</v>
-      </c>
-      <c s="22" r="D113"/>
-      <c s="22" r="E113"/>
+      <c t="s" s="7" r="D113">
+        <v>381</v>
+      </c>
+      <c t="s" s="7" r="E113">
+        <v>382</v>
+      </c>
     </row>
     <row r="114">
       <c s="14" r="A114"/>
-      <c s="13" r="B114"/>
-      <c s="12" r="C114"/>
-      <c s="11" r="D114"/>
-      <c s="11" r="E114"/>
+      <c s="24" r="B114"/>
+      <c s="4" r="C114"/>
+      <c s="15" r="D114"/>
+      <c s="15" r="E114"/>
     </row>
     <row r="115">
       <c t="s" s="14" r="A115">
-        <v>381</v>
-      </c>
-      <c t="s" s="23" r="B115">
-        <v>382</v>
-      </c>
-      <c t="s" s="26" r="C115">
         <v>383</v>
       </c>
-      <c s="17" r="D115"/>
-      <c s="17" r="E115"/>
+      <c t="s" s="25" r="B115">
+        <v>384</v>
+      </c>
+      <c t="s" s="2" r="C115">
+        <v>383</v>
+      </c>
+      <c s="22" r="D115"/>
+      <c s="22" r="E115"/>
     </row>
     <row r="116">
       <c s="14" r="A116"/>
-      <c t="s" s="23" r="B116">
-        <v>384</v>
-      </c>
-      <c t="s" s="26" r="C116">
+      <c s="13" r="B116"/>
+      <c s="12" r="C116"/>
+      <c s="11" r="D116"/>
+      <c s="11" r="E116"/>
+    </row>
+    <row r="117">
+      <c t="s" s="14" r="A117">
         <v>385</v>
       </c>
-      <c s="17" r="D116"/>
-      <c s="17" r="E116"/>
-    </row>
-    <row r="117">
-      <c s="14" r="A117"/>
-      <c s="13" r="B117"/>
-      <c s="12" r="C117"/>
-      <c s="11" r="D117"/>
-      <c s="11" r="E117"/>
+      <c t="s" s="23" r="B117">
+        <v>386</v>
+      </c>
+      <c t="s" s="26" r="C117">
+        <v>387</v>
+      </c>
+      <c s="17" r="D117"/>
+      <c s="17" r="E117"/>
     </row>
     <row r="118">
       <c s="14" r="A118"/>
-      <c s="13" r="B118"/>
-      <c s="12" r="C118"/>
-      <c s="11" r="D118"/>
-      <c s="11" r="E118"/>
+      <c t="s" s="23" r="B118">
+        <v>388</v>
+      </c>
+      <c t="s" s="26" r="C118">
+        <v>389</v>
+      </c>
+      <c s="17" r="D118"/>
+      <c s="17" r="E118"/>
     </row>
     <row r="119">
       <c s="14" r="A119"/>
@@ -3256,6 +3276,20 @@
       <c s="12" r="C119"/>
       <c s="11" r="D119"/>
       <c s="11" r="E119"/>
+    </row>
+    <row r="120">
+      <c s="14" r="A120"/>
+      <c s="13" r="B120"/>
+      <c s="12" r="C120"/>
+      <c s="11" r="D120"/>
+      <c s="11" r="E120"/>
+    </row>
+    <row r="121">
+      <c s="14" r="A121"/>
+      <c s="13" r="B121"/>
+      <c s="12" r="C121"/>
+      <c s="11" r="D121"/>
+      <c s="11" r="E121"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
EWD-22340 - Experience Re-Build
Former-commit-id: 1d9fcc01c2d604a8f447bdb30ef72bead080eeda
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="410">
   <si>
     <t>Page</t>
   </si>
@@ -225,6 +225,18 @@
     <t>Absteigend</t>
   </si>
   <si>
+    <t>createdOn</t>
+  </si>
+  <si>
+    <t>Created on</t>
+  </si>
+  <si>
+    <t>modifiedOn</t>
+  </si>
+  <si>
+    <t>Modified on</t>
+  </si>
+  <si>
     <t>Objectives</t>
   </si>
   <si>
@@ -375,16 +387,34 @@
     <t>Rebuild</t>
   </si>
   <si>
+    <t>Opnieuw maken</t>
+  </si>
+  <si>
+    <t>Neu aufbauen</t>
+  </si>
+  <si>
     <t>addNewExperience</t>
   </si>
   <si>
     <t>Add new experience</t>
   </si>
   <si>
+    <t>Nieuwe ervaring toevoegen</t>
+  </si>
+  <si>
+    <t>Neue Umgebung hinzufügen</t>
+  </si>
+  <si>
     <t>numberOfRelatedObjectives</t>
   </si>
   <si>
     <t>Number of related objectives</t>
+  </si>
+  <si>
+    <t>Aantal aanverwante doelstellingen</t>
+  </si>
+  <si>
+    <t>Anzahl der verwandten Ziele</t>
   </si>
   <si>
     <t>CreateObjective</t>
@@ -655,16 +685,34 @@
     <t>Create and edit</t>
   </si>
   <si>
+    <t>Maken en bewerken</t>
+  </si>
+  <si>
+    <t>Erstellen und bearbeiten</t>
+  </si>
+  <si>
     <t>createAndNew</t>
   </si>
   <si>
     <t>Create and new</t>
   </si>
   <si>
+    <t>Maken en nieuw</t>
+  </si>
+  <si>
+    <t>Erstellen und neu</t>
+  </si>
+  <si>
     <t>typeQuestionTitleHere</t>
   </si>
   <si>
     <t>Type question title here</t>
+  </si>
+  <si>
+    <t>Type titel van vraag hier</t>
+  </si>
+  <si>
+    <t>Titel der Frage hier eingeben</t>
   </si>
   <si>
     <t>relatedQuestion</t>
@@ -1987,93 +2035,95 @@
       </c>
     </row>
     <row r="19">
-      <c s="5" r="A19"/>
-      <c s="5" r="B19"/>
-      <c s="5" r="C19"/>
-      <c s="15" r="D19"/>
-      <c s="15" r="E19"/>
+      <c s="27" r="A19"/>
+      <c t="s" s="14" r="B19">
+        <v>70</v>
+      </c>
+      <c t="s" s="14" r="C19">
+        <v>71</v>
+      </c>
+      <c s="17" r="D19"/>
+      <c s="17" r="E19"/>
     </row>
     <row r="20">
-      <c t="s" s="5" r="A20">
-        <v>70</v>
-      </c>
-      <c t="s" s="11" r="B20">
-        <v>71</v>
-      </c>
-      <c t="s" s="11" r="C20">
+      <c s="27" r="A20"/>
+      <c t="s" s="14" r="B20">
         <v>72</v>
       </c>
-      <c t="s" s="3" r="D20">
+      <c t="s" s="14" r="C20">
         <v>73</v>
       </c>
-      <c t="s" s="3" r="E20">
-        <v>74</v>
-      </c>
+      <c s="17" r="D20"/>
+      <c s="17" r="E20"/>
     </row>
     <row r="21">
       <c s="5" r="A21"/>
-      <c t="s" s="11" r="B21">
+      <c s="5" r="B21"/>
+      <c s="5" r="C21"/>
+      <c s="15" r="D21"/>
+      <c s="15" r="E21"/>
+    </row>
+    <row r="22">
+      <c t="s" s="5" r="A22">
+        <v>74</v>
+      </c>
+      <c t="s" s="11" r="B22">
         <v>75</v>
       </c>
-      <c t="s" s="11" r="C21">
+      <c t="s" s="11" r="C22">
         <v>76</v>
       </c>
-      <c t="s" s="3" r="D21">
+      <c t="s" s="3" r="D22">
         <v>77</v>
       </c>
-      <c t="s" s="3" r="E21">
+      <c t="s" s="3" r="E22">
         <v>78</v>
-      </c>
-    </row>
-    <row r="22">
-      <c s="5" r="A22"/>
-      <c t="s" s="11" r="B22">
-        <v>79</v>
-      </c>
-      <c t="s" s="11" r="C22">
-        <v>80</v>
-      </c>
-      <c t="s" s="3" r="D22">
-        <v>81</v>
-      </c>
-      <c t="s" s="3" r="E22">
-        <v>82</v>
       </c>
     </row>
     <row r="23">
       <c s="5" r="A23"/>
       <c t="s" s="11" r="B23">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c t="s" s="11" r="C23">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c t="s" s="3" r="D23">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c t="s" s="3" r="E23">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24">
       <c s="5" r="A24"/>
-      <c s="5" r="B24"/>
-      <c s="5" r="C24"/>
-      <c s="15" r="D24"/>
-      <c s="7" r="E24"/>
+      <c t="s" s="11" r="B24">
+        <v>83</v>
+      </c>
+      <c t="s" s="11" r="C24">
+        <v>84</v>
+      </c>
+      <c t="s" s="3" r="D24">
+        <v>85</v>
+      </c>
+      <c t="s" s="3" r="E24">
+        <v>86</v>
+      </c>
     </row>
     <row r="25">
-      <c t="s" s="5" r="A25">
+      <c s="5" r="A25"/>
+      <c t="s" s="11" r="B25">
         <v>87</v>
       </c>
-      <c t="s" s="19" r="B25">
+      <c t="s" s="11" r="C25">
         <v>88</v>
       </c>
-      <c t="s" s="19" r="C25">
+      <c t="s" s="3" r="D25">
         <v>89</v>
       </c>
-      <c s="9" r="D25"/>
-      <c s="9" r="E25"/>
+      <c t="s" s="3" r="E25">
+        <v>90</v>
+      </c>
     </row>
     <row r="26">
       <c s="5" r="A26"/>
@@ -2083,183 +2133,193 @@
       <c s="7" r="E26"/>
     </row>
     <row r="27">
-      <c t="s" s="27" r="A27">
-        <v>90</v>
-      </c>
-      <c t="s" s="11" r="B27">
+      <c t="s" s="5" r="A27">
         <v>91</v>
       </c>
-      <c t="s" s="11" r="C27">
-        <v>90</v>
-      </c>
-      <c t="s" s="3" r="D27">
+      <c t="s" s="19" r="B27">
         <v>92</v>
       </c>
-      <c t="s" s="3" r="E27">
+      <c t="s" s="19" r="C27">
         <v>93</v>
       </c>
+      <c s="9" r="D27"/>
+      <c s="9" r="E27"/>
     </row>
     <row r="28">
-      <c s="27" r="A28"/>
-      <c t="s" s="11" r="B28">
+      <c s="5" r="A28"/>
+      <c s="5" r="B28"/>
+      <c s="5" r="C28"/>
+      <c s="15" r="D28"/>
+      <c s="7" r="E28"/>
+    </row>
+    <row r="29">
+      <c t="s" s="27" r="A29">
         <v>94</v>
       </c>
-      <c t="s" s="11" r="C28">
+      <c t="s" s="11" r="B29">
         <v>95</v>
       </c>
-      <c t="s" s="3" r="D28">
+      <c t="s" s="11" r="C29">
+        <v>94</v>
+      </c>
+      <c t="s" s="3" r="D29">
         <v>96</v>
       </c>
-      <c t="s" s="3" r="E28">
+      <c t="s" s="3" r="E29">
         <v>97</v>
-      </c>
-    </row>
-    <row r="29">
-      <c s="27" r="A29"/>
-      <c t="s" s="11" r="B29">
-        <v>98</v>
-      </c>
-      <c t="s" s="11" r="C29">
-        <v>99</v>
-      </c>
-      <c t="s" s="3" r="D29">
-        <v>100</v>
-      </c>
-      <c t="s" s="3" r="E29">
-        <v>101</v>
       </c>
     </row>
     <row r="30">
       <c s="27" r="A30"/>
       <c t="s" s="11" r="B30">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c t="s" s="11" r="C30">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c t="s" s="3" r="D30">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c t="s" s="3" r="E30">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31">
       <c s="27" r="A31"/>
       <c t="s" s="11" r="B31">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c t="s" s="11" r="C31">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c t="s" s="3" r="D31">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c t="s" s="3" r="E31">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32">
       <c s="27" r="A32"/>
       <c t="s" s="11" r="B32">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c t="s" s="11" r="C32">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c t="s" s="3" r="D32">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c t="s" s="3" r="E32">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33">
       <c s="27" r="A33"/>
       <c t="s" s="11" r="B33">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c t="s" s="11" r="C33">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c t="s" s="3" r="D33">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c t="s" s="3" r="E33">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34">
       <c s="27" r="A34"/>
-      <c t="s" s="14" r="B34">
-        <v>118</v>
-      </c>
-      <c t="s" s="14" r="C34">
-        <v>119</v>
-      </c>
-      <c s="17" r="D34"/>
-      <c s="17" r="E34"/>
+      <c t="s" s="11" r="B34">
+        <v>114</v>
+      </c>
+      <c t="s" s="11" r="C34">
+        <v>115</v>
+      </c>
+      <c t="s" s="3" r="D34">
+        <v>116</v>
+      </c>
+      <c t="s" s="3" r="E34">
+        <v>117</v>
+      </c>
     </row>
     <row r="35">
       <c s="27" r="A35"/>
-      <c t="s" s="14" r="B35">
+      <c t="s" s="11" r="B35">
+        <v>118</v>
+      </c>
+      <c t="s" s="11" r="C35">
+        <v>119</v>
+      </c>
+      <c t="s" s="3" r="D35">
         <v>120</v>
       </c>
-      <c t="s" s="14" r="C35">
+      <c t="s" s="3" r="E35">
         <v>121</v>
       </c>
-      <c s="17" r="D35"/>
-      <c s="17" r="E35"/>
     </row>
     <row r="36">
       <c s="27" r="A36"/>
-      <c t="s" s="14" r="B36">
+      <c t="s" s="11" r="B36">
         <v>122</v>
       </c>
-      <c t="s" s="14" r="C36">
+      <c t="s" s="11" r="C36">
         <v>123</v>
       </c>
-      <c s="17" r="D36"/>
-      <c s="17" r="E36"/>
+      <c t="s" s="3" r="D36">
+        <v>124</v>
+      </c>
+      <c t="s" s="3" r="E36">
+        <v>125</v>
+      </c>
     </row>
     <row r="37">
       <c s="27" r="A37"/>
-      <c s="27" r="B37"/>
-      <c s="27" r="C37"/>
-      <c s="7" r="D37"/>
-      <c s="7" r="E37"/>
+      <c t="s" s="11" r="B37">
+        <v>126</v>
+      </c>
+      <c t="s" s="11" r="C37">
+        <v>127</v>
+      </c>
+      <c t="s" s="3" r="D37">
+        <v>128</v>
+      </c>
+      <c t="s" s="3" r="E37">
+        <v>129</v>
+      </c>
     </row>
     <row r="38">
-      <c t="s" s="27" r="A38">
-        <v>124</v>
-      </c>
-      <c t="s" s="28" r="B38">
-        <v>125</v>
-      </c>
-      <c t="s" s="28" r="C38">
-        <v>126</v>
-      </c>
-      <c s="24" r="D38"/>
-      <c s="24" r="E38"/>
+      <c s="27" r="A38"/>
+      <c t="s" s="11" r="B38">
+        <v>130</v>
+      </c>
+      <c t="s" s="11" r="C38">
+        <v>131</v>
+      </c>
+      <c t="s" s="3" r="D38">
+        <v>132</v>
+      </c>
+      <c t="s" s="3" r="E38">
+        <v>133</v>
+      </c>
     </row>
     <row r="39">
       <c s="27" r="A39"/>
-      <c t="s" s="28" r="B39">
-        <v>127</v>
-      </c>
-      <c t="s" s="28" r="C39">
-        <v>128</v>
-      </c>
-      <c s="24" r="D39"/>
-      <c s="24" r="E39"/>
+      <c s="27" r="B39"/>
+      <c s="27" r="C39"/>
+      <c s="7" r="D39"/>
+      <c s="7" r="E39"/>
     </row>
     <row r="40">
-      <c s="27" r="A40"/>
+      <c t="s" s="27" r="A40">
+        <v>134</v>
+      </c>
       <c t="s" s="28" r="B40">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c t="s" s="28" r="C40">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c s="24" r="D40"/>
       <c s="24" r="E40"/>
@@ -2267,52 +2327,52 @@
     <row r="41">
       <c s="27" r="A41"/>
       <c t="s" s="28" r="B41">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c t="s" s="28" r="C41">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c s="24" r="D41"/>
       <c s="24" r="E41"/>
     </row>
     <row r="42">
       <c s="27" r="A42"/>
-      <c s="28" r="B42"/>
-      <c s="28" r="C42"/>
+      <c t="s" s="28" r="B42">
+        <v>139</v>
+      </c>
+      <c t="s" s="28" r="C42">
+        <v>140</v>
+      </c>
       <c s="24" r="D42"/>
       <c s="24" r="E42"/>
     </row>
     <row r="43">
-      <c t="s" s="27" r="A43">
-        <v>133</v>
-      </c>
+      <c s="27" r="A43"/>
       <c t="s" s="28" r="B43">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c t="s" s="28" r="C43">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c s="24" r="D43"/>
       <c s="24" r="E43"/>
     </row>
     <row r="44">
       <c s="27" r="A44"/>
-      <c t="s" s="28" r="B44">
-        <v>136</v>
-      </c>
-      <c t="s" s="28" r="C44">
-        <v>137</v>
-      </c>
+      <c s="28" r="B44"/>
+      <c s="28" r="C44"/>
       <c s="24" r="D44"/>
       <c s="24" r="E44"/>
     </row>
     <row r="45">
-      <c s="27" r="A45"/>
+      <c t="s" s="27" r="A45">
+        <v>143</v>
+      </c>
       <c t="s" s="28" r="B45">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c t="s" s="28" r="C45">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c s="24" r="D45"/>
       <c s="24" r="E45"/>
@@ -2320,1067 +2380,1087 @@
     <row r="46">
       <c s="27" r="A46"/>
       <c t="s" s="28" r="B46">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c t="s" s="28" r="C46">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c s="24" r="D46"/>
       <c s="24" r="E46"/>
     </row>
     <row r="47">
       <c s="27" r="A47"/>
-      <c s="27" r="B47"/>
-      <c s="27" r="C47"/>
-      <c s="7" r="D47"/>
-      <c s="7" r="E47"/>
+      <c t="s" s="28" r="B47">
+        <v>148</v>
+      </c>
+      <c t="s" s="28" r="C47">
+        <v>149</v>
+      </c>
+      <c s="24" r="D47"/>
+      <c s="24" r="E47"/>
     </row>
     <row r="48">
-      <c t="s" s="27" r="A48">
-        <v>142</v>
-      </c>
-      <c t="s" s="11" r="B48">
-        <v>143</v>
-      </c>
-      <c t="s" s="11" r="C48">
-        <v>144</v>
-      </c>
-      <c t="s" s="3" r="D48">
-        <v>145</v>
-      </c>
-      <c t="s" s="3" r="E48">
-        <v>17</v>
-      </c>
+      <c s="27" r="A48"/>
+      <c t="s" s="28" r="B48">
+        <v>150</v>
+      </c>
+      <c t="s" s="28" r="C48">
+        <v>151</v>
+      </c>
+      <c s="24" r="D48"/>
+      <c s="24" r="E48"/>
     </row>
     <row r="49">
       <c s="27" r="A49"/>
-      <c t="s" s="11" r="B49">
-        <v>146</v>
-      </c>
-      <c t="s" s="11" r="C49">
-        <v>147</v>
-      </c>
-      <c t="s" s="3" r="D49">
-        <v>148</v>
-      </c>
-      <c t="s" s="3" r="E49">
-        <v>149</v>
-      </c>
+      <c s="27" r="B49"/>
+      <c s="27" r="C49"/>
+      <c s="7" r="D49"/>
+      <c s="7" r="E49"/>
     </row>
     <row r="50">
-      <c s="27" r="A50"/>
+      <c t="s" s="27" r="A50">
+        <v>152</v>
+      </c>
       <c t="s" s="11" r="B50">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c t="s" s="11" r="C50">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c t="s" s="3" r="D50">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c t="s" s="3" r="E50">
-        <v>153</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51">
       <c s="27" r="A51"/>
       <c t="s" s="11" r="B51">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c t="s" s="11" r="C51">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c t="s" s="3" r="D51">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c t="s" s="3" r="E51">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="52">
       <c s="27" r="A52"/>
       <c t="s" s="11" r="B52">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c t="s" s="11" r="C52">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c t="s" s="3" r="D52">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c t="s" s="3" r="E52">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="53">
       <c s="27" r="A53"/>
       <c t="s" s="11" r="B53">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c t="s" s="11" r="C53">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c t="s" s="3" r="D53">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c t="s" s="3" r="E53">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="54">
       <c s="27" r="A54"/>
       <c t="s" s="11" r="B54">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c t="s" s="11" r="C54">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c t="s" s="3" r="D54">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c t="s" s="3" r="E54">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="55">
       <c s="27" r="A55"/>
       <c t="s" s="11" r="B55">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c t="s" s="11" r="C55">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c t="s" s="3" r="D55">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c t="s" s="3" r="E55">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="56">
       <c s="27" r="A56"/>
       <c t="s" s="11" r="B56">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c t="s" s="11" r="C56">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c t="s" s="3" r="D56">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c t="s" s="3" r="E56">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="57">
       <c s="27" r="A57"/>
-      <c s="27" r="B57"/>
-      <c s="27" r="C57"/>
-      <c s="7" r="D57"/>
-      <c s="7" r="E57"/>
+      <c t="s" s="11" r="B57">
+        <v>180</v>
+      </c>
+      <c t="s" s="11" r="C57">
+        <v>181</v>
+      </c>
+      <c t="s" s="3" r="D57">
+        <v>182</v>
+      </c>
+      <c t="s" s="3" r="E57">
+        <v>183</v>
+      </c>
     </row>
     <row r="58">
-      <c t="s" s="27" r="A58">
-        <v>178</v>
-      </c>
+      <c s="27" r="A58"/>
       <c t="s" s="11" r="B58">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c t="s" s="11" r="C58">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c t="s" s="3" r="D58">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c t="s" s="3" r="E58">
-        <v>182</v>
+        <v>187</v>
       </c>
     </row>
     <row r="59">
       <c s="27" r="A59"/>
-      <c t="s" s="11" r="B59">
-        <v>183</v>
-      </c>
-      <c t="s" s="11" r="C59">
-        <v>184</v>
-      </c>
-      <c t="s" s="3" r="D59">
-        <v>185</v>
-      </c>
-      <c t="s" s="3" r="E59">
-        <v>186</v>
-      </c>
+      <c s="27" r="B59"/>
+      <c s="27" r="C59"/>
+      <c s="7" r="D59"/>
+      <c s="7" r="E59"/>
     </row>
     <row r="60">
-      <c s="13" r="A60"/>
+      <c t="s" s="27" r="A60">
+        <v>188</v>
+      </c>
       <c t="s" s="11" r="B60">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c t="s" s="11" r="C60">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c t="s" s="3" r="D60">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c t="s" s="3" r="E60">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="61">
-      <c s="13" r="A61"/>
+      <c s="27" r="A61"/>
       <c t="s" s="11" r="B61">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c t="s" s="11" r="C61">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c t="s" s="3" r="D61">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c t="s" s="3" r="E61">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="62">
       <c s="13" r="A62"/>
       <c t="s" s="11" r="B62">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c t="s" s="11" r="C62">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c t="s" s="3" r="D62">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c t="s" s="3" r="E62">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="63">
       <c s="13" r="A63"/>
       <c t="s" s="11" r="B63">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c t="s" s="11" r="C63">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c t="s" s="3" r="D63">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c t="s" s="3" r="E63">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="64">
       <c s="13" r="A64"/>
       <c t="s" s="11" r="B64">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c t="s" s="11" r="C64">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c t="s" s="3" r="D64">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c t="s" s="3" r="E64">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="65">
       <c s="13" r="A65"/>
       <c t="s" s="11" r="B65">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c t="s" s="11" r="C65">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c t="s" s="3" r="D65">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c t="s" s="3" r="E65">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="66">
       <c s="13" r="A66"/>
-      <c t="s" s="14" r="B66">
-        <v>211</v>
-      </c>
-      <c t="s" s="14" r="C66">
-        <v>212</v>
-      </c>
-      <c s="17" r="D66"/>
-      <c s="17" r="E66"/>
+      <c t="s" s="11" r="B66">
+        <v>213</v>
+      </c>
+      <c t="s" s="11" r="C66">
+        <v>214</v>
+      </c>
+      <c t="s" s="3" r="D66">
+        <v>215</v>
+      </c>
+      <c t="s" s="3" r="E66">
+        <v>216</v>
+      </c>
     </row>
     <row r="67">
       <c s="13" r="A67"/>
-      <c t="s" s="14" r="B67">
-        <v>213</v>
-      </c>
-      <c t="s" s="14" r="C67">
-        <v>214</v>
-      </c>
-      <c s="17" r="D67"/>
-      <c s="17" r="E67"/>
+      <c t="s" s="11" r="B67">
+        <v>217</v>
+      </c>
+      <c t="s" s="11" r="C67">
+        <v>218</v>
+      </c>
+      <c t="s" s="3" r="D67">
+        <v>219</v>
+      </c>
+      <c t="s" s="3" r="E67">
+        <v>220</v>
+      </c>
     </row>
     <row r="68">
       <c s="13" r="A68"/>
-      <c t="s" s="14" r="B68">
-        <v>215</v>
-      </c>
-      <c t="s" s="14" r="C68">
-        <v>216</v>
-      </c>
-      <c s="17" r="D68"/>
-      <c s="17" r="E68"/>
+      <c t="s" s="11" r="B68">
+        <v>221</v>
+      </c>
+      <c t="s" s="11" r="C68">
+        <v>222</v>
+      </c>
+      <c t="s" s="3" r="D68">
+        <v>223</v>
+      </c>
+      <c t="s" s="3" r="E68">
+        <v>224</v>
+      </c>
     </row>
     <row r="69">
       <c s="13" r="A69"/>
-      <c t="s" s="14" r="B69">
-        <v>217</v>
-      </c>
-      <c t="s" s="14" r="C69">
-        <v>218</v>
-      </c>
-      <c s="17" r="D69"/>
-      <c s="17" r="E69"/>
+      <c t="s" s="11" r="B69">
+        <v>225</v>
+      </c>
+      <c t="s" s="11" r="C69">
+        <v>226</v>
+      </c>
+      <c t="s" s="3" r="D69">
+        <v>227</v>
+      </c>
+      <c t="s" s="3" r="E69">
+        <v>228</v>
+      </c>
     </row>
     <row r="70">
       <c s="13" r="A70"/>
-      <c s="27" r="B70"/>
-      <c s="27" r="C70"/>
-      <c s="7" r="D70"/>
-      <c s="7" r="E70"/>
+      <c t="s" s="11" r="B70">
+        <v>229</v>
+      </c>
+      <c t="s" s="11" r="C70">
+        <v>230</v>
+      </c>
+      <c t="s" s="3" r="D70">
+        <v>231</v>
+      </c>
+      <c t="s" s="3" r="E70">
+        <v>232</v>
+      </c>
     </row>
     <row r="71">
-      <c t="s" s="13" r="A71">
-        <v>219</v>
-      </c>
-      <c t="s" s="11" r="B71">
-        <v>220</v>
-      </c>
-      <c t="s" s="11" r="C71">
-        <v>221</v>
-      </c>
-      <c t="s" s="3" r="D71">
-        <v>222</v>
-      </c>
-      <c t="s" s="3" r="E71">
-        <v>223</v>
-      </c>
+      <c s="13" r="A71"/>
+      <c t="s" s="14" r="B71">
+        <v>233</v>
+      </c>
+      <c t="s" s="14" r="C71">
+        <v>234</v>
+      </c>
+      <c s="17" r="D71"/>
+      <c s="17" r="E71"/>
     </row>
     <row r="72">
       <c s="13" r="A72"/>
-      <c t="s" s="11" r="B72">
-        <v>224</v>
-      </c>
-      <c t="s" s="11" r="C72">
-        <v>225</v>
-      </c>
-      <c t="s" s="3" r="D72">
-        <v>226</v>
-      </c>
-      <c t="s" s="3" r="E72">
-        <v>227</v>
-      </c>
+      <c s="27" r="B72"/>
+      <c s="27" r="C72"/>
+      <c s="7" r="D72"/>
+      <c s="7" r="E72"/>
     </row>
     <row r="73">
-      <c s="13" r="A73"/>
+      <c t="s" s="13" r="A73">
+        <v>235</v>
+      </c>
       <c t="s" s="11" r="B73">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c t="s" s="11" r="C73">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c t="s" s="3" r="D73">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c t="s" s="3" r="E73">
-        <v>231</v>
+        <v>239</v>
       </c>
     </row>
     <row r="74">
       <c s="13" r="A74"/>
       <c t="s" s="11" r="B74">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c t="s" s="11" r="C74">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c t="s" s="3" r="D74">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c t="s" s="3" r="E74">
-        <v>235</v>
+        <v>243</v>
       </c>
     </row>
     <row r="75">
       <c s="13" r="A75"/>
       <c t="s" s="11" r="B75">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c t="s" s="11" r="C75">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c t="s" s="3" r="D75">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c t="s" s="3" r="E75">
-        <v>239</v>
+        <v>247</v>
       </c>
     </row>
     <row r="76">
       <c s="13" r="A76"/>
       <c t="s" s="11" r="B76">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c t="s" s="11" r="C76">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c t="s" s="3" r="D76">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c t="s" s="3" r="E76">
-        <v>241</v>
+        <v>251</v>
       </c>
     </row>
     <row r="77">
       <c s="13" r="A77"/>
       <c t="s" s="11" r="B77">
-        <v>243</v>
+        <v>252</v>
       </c>
       <c t="s" s="11" r="C77">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c t="s" s="3" r="D77">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c t="s" s="3" r="E77">
-        <v>246</v>
+        <v>255</v>
       </c>
     </row>
     <row r="78">
       <c s="13" r="A78"/>
       <c t="s" s="11" r="B78">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c t="s" s="11" r="C78">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c t="s" s="3" r="D78">
-        <v>249</v>
+        <v>258</v>
       </c>
       <c t="s" s="3" r="E78">
-        <v>250</v>
+        <v>257</v>
       </c>
     </row>
     <row r="79">
       <c s="13" r="A79"/>
       <c t="s" s="11" r="B79">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c t="s" s="11" r="C79">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c t="s" s="3" r="D79">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c t="s" s="3" r="E79">
-        <v>254</v>
+        <v>262</v>
       </c>
     </row>
     <row r="80">
       <c s="13" r="A80"/>
       <c t="s" s="11" r="B80">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c t="s" s="11" r="C80">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c t="s" s="3" r="D80">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c t="s" s="3" r="E80">
-        <v>258</v>
+        <v>266</v>
       </c>
     </row>
     <row r="81">
       <c s="13" r="A81"/>
       <c t="s" s="11" r="B81">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c t="s" s="11" r="C81">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c t="s" s="3" r="D81">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c t="s" s="3" r="E81">
-        <v>262</v>
+        <v>270</v>
       </c>
     </row>
     <row r="82">
       <c s="13" r="A82"/>
       <c t="s" s="11" r="B82">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c t="s" s="11" r="C82">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c t="s" s="3" r="D82">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c t="s" s="3" r="E82">
-        <v>265</v>
+        <v>274</v>
       </c>
     </row>
     <row r="83">
       <c s="13" r="A83"/>
       <c t="s" s="11" r="B83">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c t="s" s="11" r="C83">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c t="s" s="3" r="D83">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c t="s" s="3" r="E83">
-        <v>268</v>
+        <v>278</v>
       </c>
     </row>
     <row r="84">
       <c s="13" r="A84"/>
       <c t="s" s="11" r="B84">
-        <v>269</v>
+        <v>279</v>
       </c>
       <c t="s" s="11" r="C84">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c t="s" s="3" r="D84">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c t="s" s="3" r="E84">
-        <v>272</v>
+        <v>281</v>
       </c>
     </row>
     <row r="85">
       <c s="13" r="A85"/>
-      <c t="s" s="8" r="B85">
-        <v>273</v>
+      <c t="s" s="11" r="B85">
+        <v>282</v>
       </c>
       <c t="s" s="11" r="C85">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c t="s" s="3" r="D85">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c t="s" s="3" r="E85">
-        <v>275</v>
+        <v>284</v>
       </c>
     </row>
     <row r="86">
       <c s="13" r="A86"/>
       <c t="s" s="11" r="B86">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c t="s" s="11" r="C86">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c t="s" s="3" r="D86">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c t="s" s="3" r="E86">
-        <v>279</v>
+        <v>288</v>
       </c>
     </row>
     <row r="87">
       <c s="13" r="A87"/>
-      <c t="s" s="11" r="B87">
-        <v>280</v>
+      <c t="s" s="8" r="B87">
+        <v>289</v>
       </c>
       <c t="s" s="11" r="C87">
-        <v>281</v>
+        <v>290</v>
       </c>
       <c t="s" s="3" r="D87">
-        <v>282</v>
+        <v>291</v>
       </c>
       <c t="s" s="3" r="E87">
-        <v>283</v>
+        <v>291</v>
       </c>
     </row>
     <row r="88">
       <c s="13" r="A88"/>
       <c t="s" s="11" r="B88">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c t="s" s="11" r="C88">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c t="s" s="3" r="D88">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c t="s" s="3" r="E88">
-        <v>287</v>
+        <v>295</v>
       </c>
     </row>
     <row r="89">
       <c s="13" r="A89"/>
       <c t="s" s="11" r="B89">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c t="s" s="11" r="C89">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c t="s" s="3" r="D89">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c t="s" s="3" r="E89">
-        <v>291</v>
+        <v>299</v>
       </c>
     </row>
     <row r="90">
       <c s="13" r="A90"/>
       <c t="s" s="11" r="B90">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c t="s" s="11" r="C90">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c t="s" s="3" r="D90">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c t="s" s="3" r="E90">
-        <v>295</v>
+        <v>303</v>
       </c>
     </row>
     <row r="91">
       <c s="13" r="A91"/>
       <c t="s" s="11" r="B91">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c t="s" s="11" r="C91">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c t="s" s="3" r="D91">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c t="s" s="3" r="E91">
-        <v>299</v>
+        <v>307</v>
       </c>
     </row>
     <row r="92">
       <c s="13" r="A92"/>
       <c t="s" s="11" r="B92">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c t="s" s="11" r="C92">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c t="s" s="3" r="D92">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c t="s" s="3" r="E92">
-        <v>303</v>
+        <v>311</v>
       </c>
     </row>
     <row r="93">
       <c s="13" r="A93"/>
       <c t="s" s="11" r="B93">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c t="s" s="11" r="C93">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c t="s" s="3" r="D93">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c t="s" s="3" r="E93">
-        <v>307</v>
+        <v>315</v>
       </c>
     </row>
     <row r="94">
       <c s="13" r="A94"/>
       <c t="s" s="11" r="B94">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c t="s" s="11" r="C94">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c t="s" s="3" r="D94">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c t="s" s="3" r="E94">
-        <v>311</v>
+        <v>319</v>
       </c>
     </row>
     <row r="95">
       <c s="13" r="A95"/>
       <c t="s" s="11" r="B95">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c t="s" s="11" r="C95">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c t="s" s="3" r="D95">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c t="s" s="3" r="E95">
-        <v>315</v>
+        <v>323</v>
       </c>
     </row>
     <row r="96">
       <c s="13" r="A96"/>
       <c t="s" s="11" r="B96">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c t="s" s="11" r="C96">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c t="s" s="3" r="D96">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c t="s" s="3" r="E96">
-        <v>319</v>
+        <v>327</v>
       </c>
     </row>
     <row r="97">
       <c s="13" r="A97"/>
       <c t="s" s="11" r="B97">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c t="s" s="11" r="C97">
-        <v>321</v>
+        <v>329</v>
       </c>
       <c t="s" s="3" r="D97">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c t="s" s="3" r="E97">
-        <v>323</v>
+        <v>331</v>
       </c>
     </row>
     <row r="98">
       <c s="13" r="A98"/>
       <c t="s" s="11" r="B98">
-        <v>324</v>
+        <v>332</v>
       </c>
       <c t="s" s="11" r="C98">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c t="s" s="3" r="D98">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c t="s" s="3" r="E98">
-        <v>327</v>
+        <v>335</v>
       </c>
     </row>
     <row r="99">
       <c s="13" r="A99"/>
       <c t="s" s="11" r="B99">
-        <v>328</v>
+        <v>336</v>
       </c>
       <c t="s" s="11" r="C99">
-        <v>329</v>
+        <v>337</v>
       </c>
       <c t="s" s="3" r="D99">
-        <v>330</v>
+        <v>338</v>
       </c>
       <c t="s" s="3" r="E99">
-        <v>331</v>
+        <v>339</v>
       </c>
     </row>
     <row r="100">
       <c s="13" r="A100"/>
       <c t="s" s="11" r="B100">
-        <v>332</v>
+        <v>340</v>
       </c>
       <c t="s" s="11" r="C100">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c t="s" s="3" r="D100">
-        <v>334</v>
+        <v>342</v>
       </c>
       <c t="s" s="3" r="E100">
-        <v>335</v>
+        <v>343</v>
       </c>
     </row>
     <row r="101">
       <c s="13" r="A101"/>
       <c t="s" s="11" r="B101">
-        <v>336</v>
-      </c>
-      <c t="s" s="8" r="C101">
-        <v>337</v>
+        <v>344</v>
+      </c>
+      <c t="s" s="11" r="C101">
+        <v>345</v>
       </c>
       <c t="s" s="3" r="D101">
-        <v>338</v>
+        <v>346</v>
       </c>
       <c t="s" s="3" r="E101">
-        <v>339</v>
+        <v>347</v>
       </c>
     </row>
     <row r="102">
       <c s="13" r="A102"/>
-      <c t="s" s="8" r="B102">
-        <v>340</v>
-      </c>
-      <c t="s" s="8" r="C102">
-        <v>341</v>
+      <c t="s" s="11" r="B102">
+        <v>348</v>
+      </c>
+      <c t="s" s="11" r="C102">
+        <v>349</v>
       </c>
       <c t="s" s="3" r="D102">
-        <v>342</v>
+        <v>350</v>
       </c>
       <c t="s" s="3" r="E102">
-        <v>343</v>
+        <v>351</v>
       </c>
     </row>
     <row r="103">
       <c s="13" r="A103"/>
       <c t="s" s="11" r="B103">
-        <v>344</v>
+        <v>352</v>
       </c>
       <c t="s" s="8" r="C103">
-        <v>341</v>
+        <v>353</v>
       </c>
       <c t="s" s="3" r="D103">
-        <v>342</v>
+        <v>354</v>
       </c>
       <c t="s" s="3" r="E103">
-        <v>343</v>
+        <v>355</v>
       </c>
     </row>
     <row r="104">
       <c s="13" r="A104"/>
-      <c t="s" s="11" r="B104">
-        <v>345</v>
-      </c>
-      <c t="s" s="1" r="C104">
-        <v>346</v>
+      <c t="s" s="8" r="B104">
+        <v>356</v>
+      </c>
+      <c t="s" s="8" r="C104">
+        <v>357</v>
       </c>
       <c t="s" s="3" r="D104">
-        <v>347</v>
+        <v>358</v>
       </c>
       <c t="s" s="3" r="E104">
-        <v>348</v>
+        <v>359</v>
       </c>
     </row>
     <row r="105">
       <c s="13" r="A105"/>
       <c t="s" s="11" r="B105">
-        <v>349</v>
-      </c>
-      <c t="s" s="1" r="C105">
-        <v>350</v>
+        <v>360</v>
+      </c>
+      <c t="s" s="8" r="C105">
+        <v>357</v>
       </c>
       <c t="s" s="3" r="D105">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c t="s" s="3" r="E105">
-        <v>352</v>
+        <v>359</v>
       </c>
     </row>
     <row r="106">
       <c s="13" r="A106"/>
       <c t="s" s="11" r="B106">
-        <v>353</v>
+        <v>361</v>
       </c>
       <c t="s" s="1" r="C106">
-        <v>354</v>
+        <v>362</v>
       </c>
       <c t="s" s="3" r="D106">
-        <v>355</v>
-      </c>
-      <c t="s" s="1" r="E106">
-        <v>356</v>
+        <v>363</v>
+      </c>
+      <c t="s" s="3" r="E106">
+        <v>364</v>
       </c>
     </row>
     <row r="107">
       <c s="13" r="A107"/>
-      <c s="12" r="B107"/>
-      <c s="6" r="C107"/>
-      <c s="10" r="D107"/>
-      <c s="10" r="E107"/>
+      <c t="s" s="11" r="B107">
+        <v>365</v>
+      </c>
+      <c t="s" s="1" r="C107">
+        <v>366</v>
+      </c>
+      <c t="s" s="3" r="D107">
+        <v>367</v>
+      </c>
+      <c t="s" s="3" r="E107">
+        <v>368</v>
+      </c>
     </row>
     <row r="108">
-      <c t="s" s="13" r="A108">
-        <v>357</v>
-      </c>
+      <c s="13" r="A108"/>
       <c t="s" s="11" r="B108">
-        <v>358</v>
-      </c>
-      <c t="s" s="8" r="C108">
-        <v>359</v>
+        <v>369</v>
+      </c>
+      <c t="s" s="1" r="C108">
+        <v>370</v>
       </c>
       <c t="s" s="3" r="D108">
-        <v>360</v>
-      </c>
-      <c t="s" s="3" r="E108">
-        <v>361</v>
+        <v>371</v>
+      </c>
+      <c t="s" s="1" r="E108">
+        <v>372</v>
       </c>
     </row>
     <row r="109">
       <c s="13" r="A109"/>
-      <c t="s" s="11" r="B109">
-        <v>362</v>
-      </c>
-      <c t="s" s="8" r="C109">
-        <v>363</v>
-      </c>
-      <c t="s" s="3" r="D109">
-        <v>364</v>
-      </c>
-      <c t="s" s="3" r="E109">
-        <v>365</v>
-      </c>
+      <c s="12" r="B109"/>
+      <c s="6" r="C109"/>
+      <c s="10" r="D109"/>
+      <c s="10" r="E109"/>
     </row>
     <row r="110">
-      <c s="20" r="A110"/>
-      <c s="5" r="B110"/>
-      <c s="25" r="C110"/>
-      <c s="15" r="D110"/>
-      <c s="15" r="E110"/>
+      <c t="s" s="13" r="A110">
+        <v>373</v>
+      </c>
+      <c t="s" s="11" r="B110">
+        <v>374</v>
+      </c>
+      <c t="s" s="8" r="C110">
+        <v>375</v>
+      </c>
+      <c t="s" s="3" r="D110">
+        <v>376</v>
+      </c>
+      <c t="s" s="3" r="E110">
+        <v>377</v>
+      </c>
     </row>
     <row r="111">
-      <c t="s" s="13" r="A111">
-        <v>366</v>
-      </c>
+      <c s="13" r="A111"/>
       <c t="s" s="11" r="B111">
-        <v>367</v>
+        <v>378</v>
       </c>
       <c t="s" s="8" r="C111">
-        <v>368</v>
+        <v>379</v>
       </c>
       <c t="s" s="3" r="D111">
-        <v>369</v>
+        <v>380</v>
       </c>
       <c t="s" s="3" r="E111">
-        <v>370</v>
+        <v>381</v>
       </c>
     </row>
     <row r="112">
-      <c s="13" r="A112"/>
-      <c t="s" s="11" r="B112">
-        <v>371</v>
-      </c>
-      <c t="s" s="8" r="C112">
-        <v>372</v>
-      </c>
-      <c t="s" s="3" r="D112">
-        <v>373</v>
-      </c>
-      <c t="s" s="3" r="E112">
-        <v>374</v>
-      </c>
+      <c s="20" r="A112"/>
+      <c s="5" r="B112"/>
+      <c s="25" r="C112"/>
+      <c s="15" r="D112"/>
+      <c s="15" r="E112"/>
     </row>
     <row r="113">
-      <c s="13" r="A113"/>
+      <c t="s" s="13" r="A113">
+        <v>382</v>
+      </c>
       <c t="s" s="11" r="B113">
-        <v>375</v>
+        <v>383</v>
       </c>
       <c t="s" s="8" r="C113">
-        <v>376</v>
+        <v>384</v>
       </c>
       <c t="s" s="3" r="D113">
-        <v>377</v>
+        <v>385</v>
       </c>
       <c t="s" s="3" r="E113">
-        <v>378</v>
+        <v>386</v>
       </c>
     </row>
     <row r="114">
       <c s="13" r="A114"/>
       <c t="s" s="11" r="B114">
-        <v>379</v>
+        <v>387</v>
       </c>
       <c t="s" s="8" r="C114">
-        <v>380</v>
+        <v>388</v>
       </c>
       <c t="s" s="3" r="D114">
-        <v>381</v>
+        <v>389</v>
       </c>
       <c t="s" s="3" r="E114">
-        <v>382</v>
+        <v>390</v>
       </c>
     </row>
     <row r="115">
       <c s="13" r="A115"/>
       <c t="s" s="11" r="B115">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c t="s" s="8" r="C115">
-        <v>384</v>
+        <v>392</v>
       </c>
       <c t="s" s="3" r="D115">
-        <v>385</v>
+        <v>393</v>
       </c>
       <c t="s" s="3" r="E115">
-        <v>386</v>
+        <v>394</v>
       </c>
     </row>
     <row r="116">
       <c s="13" r="A116"/>
-      <c s="5" r="B116"/>
-      <c s="25" r="C116"/>
-      <c s="15" r="D116"/>
-      <c s="15" r="E116"/>
+      <c t="s" s="11" r="B116">
+        <v>395</v>
+      </c>
+      <c t="s" s="8" r="C116">
+        <v>396</v>
+      </c>
+      <c t="s" s="3" r="D116">
+        <v>397</v>
+      </c>
+      <c t="s" s="3" r="E116">
+        <v>398</v>
+      </c>
     </row>
     <row r="117">
-      <c t="s" s="13" r="A117">
-        <v>387</v>
-      </c>
-      <c t="s" s="28" r="B117">
-        <v>388</v>
-      </c>
-      <c t="s" s="16" r="C117">
-        <v>387</v>
-      </c>
-      <c s="24" r="D117"/>
-      <c s="24" r="E117"/>
+      <c s="13" r="A117"/>
+      <c t="s" s="11" r="B117">
+        <v>399</v>
+      </c>
+      <c t="s" s="8" r="C117">
+        <v>400</v>
+      </c>
+      <c t="s" s="3" r="D117">
+        <v>401</v>
+      </c>
+      <c t="s" s="3" r="E117">
+        <v>402</v>
+      </c>
     </row>
     <row r="118">
       <c s="13" r="A118"/>
-      <c s="12" r="B118"/>
-      <c s="6" r="C118"/>
-      <c s="10" r="D118"/>
-      <c s="10" r="E118"/>
+      <c s="5" r="B118"/>
+      <c s="25" r="C118"/>
+      <c s="15" r="D118"/>
+      <c s="15" r="E118"/>
     </row>
     <row r="119">
       <c t="s" s="13" r="A119">
-        <v>389</v>
-      </c>
-      <c t="s" s="22" r="B119">
-        <v>390</v>
-      </c>
-      <c t="s" s="26" r="C119">
-        <v>391</v>
-      </c>
-      <c s="30" r="D119"/>
-      <c s="30" r="E119"/>
+        <v>403</v>
+      </c>
+      <c t="s" s="28" r="B119">
+        <v>404</v>
+      </c>
+      <c t="s" s="16" r="C119">
+        <v>403</v>
+      </c>
+      <c s="24" r="D119"/>
+      <c s="24" r="E119"/>
     </row>
     <row r="120">
       <c s="13" r="A120"/>
-      <c t="s" s="22" r="B120">
-        <v>392</v>
-      </c>
-      <c t="s" s="26" r="C120">
-        <v>393</v>
-      </c>
-      <c s="30" r="D120"/>
-      <c s="30" r="E120"/>
+      <c s="12" r="B120"/>
+      <c s="6" r="C120"/>
+      <c s="10" r="D120"/>
+      <c s="10" r="E120"/>
     </row>
     <row r="121">
-      <c s="13" r="A121"/>
-      <c s="12" r="B121"/>
-      <c s="6" r="C121"/>
-      <c s="10" r="D121"/>
-      <c s="10" r="E121"/>
+      <c t="s" s="13" r="A121">
+        <v>405</v>
+      </c>
+      <c t="s" s="22" r="B121">
+        <v>406</v>
+      </c>
+      <c t="s" s="26" r="C121">
+        <v>407</v>
+      </c>
+      <c s="30" r="D121"/>
+      <c s="30" r="E121"/>
     </row>
     <row r="122">
       <c s="13" r="A122"/>
-      <c s="12" r="B122"/>
-      <c s="6" r="C122"/>
-      <c s="10" r="D122"/>
-      <c s="10" r="E122"/>
+      <c t="s" s="22" r="B122">
+        <v>408</v>
+      </c>
+      <c t="s" s="26" r="C122">
+        <v>409</v>
+      </c>
+      <c s="30" r="D122"/>
+      <c s="30" r="E122"/>
     </row>
     <row r="123">
       <c s="13" r="A123"/>
@@ -3388,6 +3468,20 @@
       <c s="6" r="C123"/>
       <c s="10" r="D123"/>
       <c s="10" r="E123"/>
+    </row>
+    <row r="124">
+      <c s="13" r="A124"/>
+      <c s="12" r="B124"/>
+      <c s="6" r="C124"/>
+      <c s="10" r="D124"/>
+      <c s="10" r="E124"/>
+    </row>
+    <row r="125">
+      <c s="13" r="A125"/>
+      <c s="12" r="B125"/>
+      <c s="6" r="C125"/>
+      <c s="10" r="D125"/>
+      <c s="10" r="E125"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
EWD-22149 - Create/Update/Delete Question - empty question list
Former-commit-id: 40dac660a2d0057fb46e2cf985f9088a4d6a46fa
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="412">
   <si>
     <t>Page</t>
   </si>
@@ -713,6 +713,12 @@
   </si>
   <si>
     <t>Titel der Frage hier eingeben</t>
+  </si>
+  <si>
+    <t>questionListIsEmpty</t>
+  </si>
+  <si>
+    <t>Question list is empty</t>
   </si>
   <si>
     <t>relatedQuestion</t>
@@ -2741,98 +2747,94 @@
     </row>
     <row r="72">
       <c s="13" r="A72"/>
-      <c s="27" r="B72"/>
-      <c s="27" r="C72"/>
-      <c s="7" r="D72"/>
-      <c s="7" r="E72"/>
+      <c t="s" s="14" r="B72">
+        <v>235</v>
+      </c>
+      <c t="s" s="14" r="C72">
+        <v>236</v>
+      </c>
+      <c s="17" r="D72"/>
+      <c s="17" r="E72"/>
     </row>
     <row r="73">
-      <c t="s" s="13" r="A73">
-        <v>235</v>
-      </c>
-      <c t="s" s="11" r="B73">
-        <v>236</v>
-      </c>
-      <c t="s" s="11" r="C73">
+      <c s="13" r="A73"/>
+      <c s="27" r="B73"/>
+      <c s="27" r="C73"/>
+      <c s="7" r="D73"/>
+      <c s="7" r="E73"/>
+    </row>
+    <row r="74">
+      <c t="s" s="13" r="A74">
         <v>237</v>
       </c>
-      <c t="s" s="3" r="D73">
+      <c t="s" s="11" r="B74">
         <v>238</v>
       </c>
-      <c t="s" s="3" r="E73">
+      <c t="s" s="11" r="C74">
         <v>239</v>
       </c>
-    </row>
-    <row r="74">
-      <c s="13" r="A74"/>
-      <c t="s" s="11" r="B74">
+      <c t="s" s="3" r="D74">
         <v>240</v>
       </c>
-      <c t="s" s="11" r="C74">
+      <c t="s" s="3" r="E74">
         <v>241</v>
-      </c>
-      <c t="s" s="3" r="D74">
-        <v>242</v>
-      </c>
-      <c t="s" s="3" r="E74">
-        <v>243</v>
       </c>
     </row>
     <row r="75">
       <c s="13" r="A75"/>
       <c t="s" s="11" r="B75">
+        <v>242</v>
+      </c>
+      <c t="s" s="11" r="C75">
+        <v>243</v>
+      </c>
+      <c t="s" s="3" r="D75">
         <v>244</v>
       </c>
-      <c t="s" s="11" r="C75">
+      <c t="s" s="3" r="E75">
         <v>245</v>
-      </c>
-      <c t="s" s="3" r="D75">
-        <v>246</v>
-      </c>
-      <c t="s" s="3" r="E75">
-        <v>247</v>
       </c>
     </row>
     <row r="76">
       <c s="13" r="A76"/>
       <c t="s" s="11" r="B76">
+        <v>246</v>
+      </c>
+      <c t="s" s="11" r="C76">
+        <v>247</v>
+      </c>
+      <c t="s" s="3" r="D76">
         <v>248</v>
       </c>
-      <c t="s" s="11" r="C76">
+      <c t="s" s="3" r="E76">
         <v>249</v>
-      </c>
-      <c t="s" s="3" r="D76">
-        <v>250</v>
-      </c>
-      <c t="s" s="3" r="E76">
-        <v>251</v>
       </c>
     </row>
     <row r="77">
       <c s="13" r="A77"/>
       <c t="s" s="11" r="B77">
+        <v>250</v>
+      </c>
+      <c t="s" s="11" r="C77">
+        <v>251</v>
+      </c>
+      <c t="s" s="3" r="D77">
         <v>252</v>
       </c>
-      <c t="s" s="11" r="C77">
+      <c t="s" s="3" r="E77">
         <v>253</v>
-      </c>
-      <c t="s" s="3" r="D77">
-        <v>254</v>
-      </c>
-      <c t="s" s="3" r="E77">
-        <v>255</v>
       </c>
     </row>
     <row r="78">
       <c s="13" r="A78"/>
       <c t="s" s="11" r="B78">
+        <v>254</v>
+      </c>
+      <c t="s" s="11" r="C78">
+        <v>255</v>
+      </c>
+      <c t="s" s="3" r="D78">
         <v>256</v>
-      </c>
-      <c t="s" s="11" r="C78">
-        <v>257</v>
-      </c>
-      <c t="s" s="3" r="D78">
-        <v>258</v>
       </c>
       <c t="s" s="3" r="E78">
         <v>257</v>
@@ -2841,618 +2843,622 @@
     <row r="79">
       <c s="13" r="A79"/>
       <c t="s" s="11" r="B79">
+        <v>258</v>
+      </c>
+      <c t="s" s="11" r="C79">
         <v>259</v>
       </c>
-      <c t="s" s="11" r="C79">
+      <c t="s" s="3" r="D79">
         <v>260</v>
       </c>
-      <c t="s" s="3" r="D79">
-        <v>261</v>
-      </c>
       <c t="s" s="3" r="E79">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="80">
       <c s="13" r="A80"/>
       <c t="s" s="11" r="B80">
+        <v>261</v>
+      </c>
+      <c t="s" s="11" r="C80">
+        <v>262</v>
+      </c>
+      <c t="s" s="3" r="D80">
         <v>263</v>
       </c>
-      <c t="s" s="11" r="C80">
+      <c t="s" s="3" r="E80">
         <v>264</v>
-      </c>
-      <c t="s" s="3" r="D80">
-        <v>265</v>
-      </c>
-      <c t="s" s="3" r="E80">
-        <v>266</v>
       </c>
     </row>
     <row r="81">
       <c s="13" r="A81"/>
       <c t="s" s="11" r="B81">
+        <v>265</v>
+      </c>
+      <c t="s" s="11" r="C81">
+        <v>266</v>
+      </c>
+      <c t="s" s="3" r="D81">
         <v>267</v>
       </c>
-      <c t="s" s="11" r="C81">
+      <c t="s" s="3" r="E81">
         <v>268</v>
-      </c>
-      <c t="s" s="3" r="D81">
-        <v>269</v>
-      </c>
-      <c t="s" s="3" r="E81">
-        <v>270</v>
       </c>
     </row>
     <row r="82">
       <c s="13" r="A82"/>
       <c t="s" s="11" r="B82">
+        <v>269</v>
+      </c>
+      <c t="s" s="11" r="C82">
+        <v>270</v>
+      </c>
+      <c t="s" s="3" r="D82">
         <v>271</v>
       </c>
-      <c t="s" s="11" r="C82">
+      <c t="s" s="3" r="E82">
         <v>272</v>
-      </c>
-      <c t="s" s="3" r="D82">
-        <v>273</v>
-      </c>
-      <c t="s" s="3" r="E82">
-        <v>274</v>
       </c>
     </row>
     <row r="83">
       <c s="13" r="A83"/>
       <c t="s" s="11" r="B83">
+        <v>273</v>
+      </c>
+      <c t="s" s="11" r="C83">
+        <v>274</v>
+      </c>
+      <c t="s" s="3" r="D83">
         <v>275</v>
       </c>
-      <c t="s" s="11" r="C83">
+      <c t="s" s="3" r="E83">
         <v>276</v>
-      </c>
-      <c t="s" s="3" r="D83">
-        <v>277</v>
-      </c>
-      <c t="s" s="3" r="E83">
-        <v>278</v>
       </c>
     </row>
     <row r="84">
       <c s="13" r="A84"/>
       <c t="s" s="11" r="B84">
+        <v>277</v>
+      </c>
+      <c t="s" s="11" r="C84">
+        <v>278</v>
+      </c>
+      <c t="s" s="3" r="D84">
         <v>279</v>
       </c>
-      <c t="s" s="11" r="C84">
+      <c t="s" s="3" r="E84">
         <v>280</v>
-      </c>
-      <c t="s" s="3" r="D84">
-        <v>280</v>
-      </c>
-      <c t="s" s="3" r="E84">
-        <v>281</v>
       </c>
     </row>
     <row r="85">
       <c s="13" r="A85"/>
       <c t="s" s="11" r="B85">
+        <v>281</v>
+      </c>
+      <c t="s" s="11" r="C85">
         <v>282</v>
       </c>
-      <c t="s" s="11" r="C85">
+      <c t="s" s="3" r="D85">
+        <v>282</v>
+      </c>
+      <c t="s" s="3" r="E85">
         <v>283</v>
-      </c>
-      <c t="s" s="3" r="D85">
-        <v>283</v>
-      </c>
-      <c t="s" s="3" r="E85">
-        <v>284</v>
       </c>
     </row>
     <row r="86">
       <c s="13" r="A86"/>
       <c t="s" s="11" r="B86">
+        <v>284</v>
+      </c>
+      <c t="s" s="11" r="C86">
         <v>285</v>
       </c>
-      <c t="s" s="11" r="C86">
+      <c t="s" s="3" r="D86">
+        <v>285</v>
+      </c>
+      <c t="s" s="3" r="E86">
         <v>286</v>
-      </c>
-      <c t="s" s="3" r="D86">
-        <v>287</v>
-      </c>
-      <c t="s" s="3" r="E86">
-        <v>288</v>
       </c>
     </row>
     <row r="87">
       <c s="13" r="A87"/>
-      <c t="s" s="8" r="B87">
+      <c t="s" s="11" r="B87">
+        <v>287</v>
+      </c>
+      <c t="s" s="11" r="C87">
+        <v>288</v>
+      </c>
+      <c t="s" s="3" r="D87">
         <v>289</v>
       </c>
-      <c t="s" s="11" r="C87">
+      <c t="s" s="3" r="E87">
         <v>290</v>
-      </c>
-      <c t="s" s="3" r="D87">
-        <v>291</v>
-      </c>
-      <c t="s" s="3" r="E87">
-        <v>291</v>
       </c>
     </row>
     <row r="88">
       <c s="13" r="A88"/>
-      <c t="s" s="11" r="B88">
+      <c t="s" s="8" r="B88">
+        <v>291</v>
+      </c>
+      <c t="s" s="11" r="C88">
         <v>292</v>
       </c>
-      <c t="s" s="11" r="C88">
+      <c t="s" s="3" r="D88">
         <v>293</v>
       </c>
-      <c t="s" s="3" r="D88">
-        <v>294</v>
-      </c>
       <c t="s" s="3" r="E88">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="89">
       <c s="13" r="A89"/>
       <c t="s" s="11" r="B89">
+        <v>294</v>
+      </c>
+      <c t="s" s="11" r="C89">
+        <v>295</v>
+      </c>
+      <c t="s" s="3" r="D89">
         <v>296</v>
       </c>
-      <c t="s" s="11" r="C89">
+      <c t="s" s="3" r="E89">
         <v>297</v>
-      </c>
-      <c t="s" s="3" r="D89">
-        <v>298</v>
-      </c>
-      <c t="s" s="3" r="E89">
-        <v>299</v>
       </c>
     </row>
     <row r="90">
       <c s="13" r="A90"/>
       <c t="s" s="11" r="B90">
+        <v>298</v>
+      </c>
+      <c t="s" s="11" r="C90">
+        <v>299</v>
+      </c>
+      <c t="s" s="3" r="D90">
         <v>300</v>
       </c>
-      <c t="s" s="11" r="C90">
+      <c t="s" s="3" r="E90">
         <v>301</v>
-      </c>
-      <c t="s" s="3" r="D90">
-        <v>302</v>
-      </c>
-      <c t="s" s="3" r="E90">
-        <v>303</v>
       </c>
     </row>
     <row r="91">
       <c s="13" r="A91"/>
       <c t="s" s="11" r="B91">
+        <v>302</v>
+      </c>
+      <c t="s" s="11" r="C91">
+        <v>303</v>
+      </c>
+      <c t="s" s="3" r="D91">
         <v>304</v>
       </c>
-      <c t="s" s="11" r="C91">
+      <c t="s" s="3" r="E91">
         <v>305</v>
-      </c>
-      <c t="s" s="3" r="D91">
-        <v>306</v>
-      </c>
-      <c t="s" s="3" r="E91">
-        <v>307</v>
       </c>
     </row>
     <row r="92">
       <c s="13" r="A92"/>
       <c t="s" s="11" r="B92">
+        <v>306</v>
+      </c>
+      <c t="s" s="11" r="C92">
+        <v>307</v>
+      </c>
+      <c t="s" s="3" r="D92">
         <v>308</v>
       </c>
-      <c t="s" s="11" r="C92">
+      <c t="s" s="3" r="E92">
         <v>309</v>
-      </c>
-      <c t="s" s="3" r="D92">
-        <v>310</v>
-      </c>
-      <c t="s" s="3" r="E92">
-        <v>311</v>
       </c>
     </row>
     <row r="93">
       <c s="13" r="A93"/>
       <c t="s" s="11" r="B93">
+        <v>310</v>
+      </c>
+      <c t="s" s="11" r="C93">
+        <v>311</v>
+      </c>
+      <c t="s" s="3" r="D93">
         <v>312</v>
       </c>
-      <c t="s" s="11" r="C93">
+      <c t="s" s="3" r="E93">
         <v>313</v>
-      </c>
-      <c t="s" s="3" r="D93">
-        <v>314</v>
-      </c>
-      <c t="s" s="3" r="E93">
-        <v>315</v>
       </c>
     </row>
     <row r="94">
       <c s="13" r="A94"/>
       <c t="s" s="11" r="B94">
+        <v>314</v>
+      </c>
+      <c t="s" s="11" r="C94">
+        <v>315</v>
+      </c>
+      <c t="s" s="3" r="D94">
         <v>316</v>
       </c>
-      <c t="s" s="11" r="C94">
+      <c t="s" s="3" r="E94">
         <v>317</v>
-      </c>
-      <c t="s" s="3" r="D94">
-        <v>318</v>
-      </c>
-      <c t="s" s="3" r="E94">
-        <v>319</v>
       </c>
     </row>
     <row r="95">
       <c s="13" r="A95"/>
       <c t="s" s="11" r="B95">
+        <v>318</v>
+      </c>
+      <c t="s" s="11" r="C95">
+        <v>319</v>
+      </c>
+      <c t="s" s="3" r="D95">
         <v>320</v>
       </c>
-      <c t="s" s="11" r="C95">
+      <c t="s" s="3" r="E95">
         <v>321</v>
-      </c>
-      <c t="s" s="3" r="D95">
-        <v>322</v>
-      </c>
-      <c t="s" s="3" r="E95">
-        <v>323</v>
       </c>
     </row>
     <row r="96">
       <c s="13" r="A96"/>
       <c t="s" s="11" r="B96">
+        <v>322</v>
+      </c>
+      <c t="s" s="11" r="C96">
+        <v>323</v>
+      </c>
+      <c t="s" s="3" r="D96">
         <v>324</v>
       </c>
-      <c t="s" s="11" r="C96">
+      <c t="s" s="3" r="E96">
         <v>325</v>
-      </c>
-      <c t="s" s="3" r="D96">
-        <v>326</v>
-      </c>
-      <c t="s" s="3" r="E96">
-        <v>327</v>
       </c>
     </row>
     <row r="97">
       <c s="13" r="A97"/>
       <c t="s" s="11" r="B97">
+        <v>326</v>
+      </c>
+      <c t="s" s="11" r="C97">
+        <v>327</v>
+      </c>
+      <c t="s" s="3" r="D97">
         <v>328</v>
       </c>
-      <c t="s" s="11" r="C97">
+      <c t="s" s="3" r="E97">
         <v>329</v>
-      </c>
-      <c t="s" s="3" r="D97">
-        <v>330</v>
-      </c>
-      <c t="s" s="3" r="E97">
-        <v>331</v>
       </c>
     </row>
     <row r="98">
       <c s="13" r="A98"/>
       <c t="s" s="11" r="B98">
+        <v>330</v>
+      </c>
+      <c t="s" s="11" r="C98">
+        <v>331</v>
+      </c>
+      <c t="s" s="3" r="D98">
         <v>332</v>
       </c>
-      <c t="s" s="11" r="C98">
+      <c t="s" s="3" r="E98">
         <v>333</v>
-      </c>
-      <c t="s" s="3" r="D98">
-        <v>334</v>
-      </c>
-      <c t="s" s="3" r="E98">
-        <v>335</v>
       </c>
     </row>
     <row r="99">
       <c s="13" r="A99"/>
       <c t="s" s="11" r="B99">
+        <v>334</v>
+      </c>
+      <c t="s" s="11" r="C99">
+        <v>335</v>
+      </c>
+      <c t="s" s="3" r="D99">
         <v>336</v>
       </c>
-      <c t="s" s="11" r="C99">
+      <c t="s" s="3" r="E99">
         <v>337</v>
-      </c>
-      <c t="s" s="3" r="D99">
-        <v>338</v>
-      </c>
-      <c t="s" s="3" r="E99">
-        <v>339</v>
       </c>
     </row>
     <row r="100">
       <c s="13" r="A100"/>
       <c t="s" s="11" r="B100">
+        <v>338</v>
+      </c>
+      <c t="s" s="11" r="C100">
+        <v>339</v>
+      </c>
+      <c t="s" s="3" r="D100">
         <v>340</v>
       </c>
-      <c t="s" s="11" r="C100">
+      <c t="s" s="3" r="E100">
         <v>341</v>
-      </c>
-      <c t="s" s="3" r="D100">
-        <v>342</v>
-      </c>
-      <c t="s" s="3" r="E100">
-        <v>343</v>
       </c>
     </row>
     <row r="101">
       <c s="13" r="A101"/>
       <c t="s" s="11" r="B101">
+        <v>342</v>
+      </c>
+      <c t="s" s="11" r="C101">
+        <v>343</v>
+      </c>
+      <c t="s" s="3" r="D101">
         <v>344</v>
       </c>
-      <c t="s" s="11" r="C101">
+      <c t="s" s="3" r="E101">
         <v>345</v>
-      </c>
-      <c t="s" s="3" r="D101">
-        <v>346</v>
-      </c>
-      <c t="s" s="3" r="E101">
-        <v>347</v>
       </c>
     </row>
     <row r="102">
       <c s="13" r="A102"/>
       <c t="s" s="11" r="B102">
+        <v>346</v>
+      </c>
+      <c t="s" s="11" r="C102">
+        <v>347</v>
+      </c>
+      <c t="s" s="3" r="D102">
         <v>348</v>
       </c>
-      <c t="s" s="11" r="C102">
+      <c t="s" s="3" r="E102">
         <v>349</v>
-      </c>
-      <c t="s" s="3" r="D102">
-        <v>350</v>
-      </c>
-      <c t="s" s="3" r="E102">
-        <v>351</v>
       </c>
     </row>
     <row r="103">
       <c s="13" r="A103"/>
       <c t="s" s="11" r="B103">
+        <v>350</v>
+      </c>
+      <c t="s" s="11" r="C103">
+        <v>351</v>
+      </c>
+      <c t="s" s="3" r="D103">
         <v>352</v>
       </c>
-      <c t="s" s="8" r="C103">
+      <c t="s" s="3" r="E103">
         <v>353</v>
-      </c>
-      <c t="s" s="3" r="D103">
-        <v>354</v>
-      </c>
-      <c t="s" s="3" r="E103">
-        <v>355</v>
       </c>
     </row>
     <row r="104">
       <c s="13" r="A104"/>
-      <c t="s" s="8" r="B104">
+      <c t="s" s="11" r="B104">
+        <v>354</v>
+      </c>
+      <c t="s" s="8" r="C104">
+        <v>355</v>
+      </c>
+      <c t="s" s="3" r="D104">
         <v>356</v>
       </c>
-      <c t="s" s="8" r="C104">
+      <c t="s" s="3" r="E104">
         <v>357</v>
-      </c>
-      <c t="s" s="3" r="D104">
-        <v>358</v>
-      </c>
-      <c t="s" s="3" r="E104">
-        <v>359</v>
       </c>
     </row>
     <row r="105">
       <c s="13" r="A105"/>
-      <c t="s" s="11" r="B105">
+      <c t="s" s="8" r="B105">
+        <v>358</v>
+      </c>
+      <c t="s" s="8" r="C105">
+        <v>359</v>
+      </c>
+      <c t="s" s="3" r="D105">
         <v>360</v>
       </c>
-      <c t="s" s="8" r="C105">
-        <v>357</v>
-      </c>
-      <c t="s" s="3" r="D105">
-        <v>358</v>
-      </c>
       <c t="s" s="3" r="E105">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="106">
       <c s="13" r="A106"/>
       <c t="s" s="11" r="B106">
+        <v>362</v>
+      </c>
+      <c t="s" s="8" r="C106">
+        <v>359</v>
+      </c>
+      <c t="s" s="3" r="D106">
+        <v>360</v>
+      </c>
+      <c t="s" s="3" r="E106">
         <v>361</v>
-      </c>
-      <c t="s" s="1" r="C106">
-        <v>362</v>
-      </c>
-      <c t="s" s="3" r="D106">
-        <v>363</v>
-      </c>
-      <c t="s" s="3" r="E106">
-        <v>364</v>
       </c>
     </row>
     <row r="107">
       <c s="13" r="A107"/>
       <c t="s" s="11" r="B107">
+        <v>363</v>
+      </c>
+      <c t="s" s="1" r="C107">
+        <v>364</v>
+      </c>
+      <c t="s" s="3" r="D107">
         <v>365</v>
       </c>
-      <c t="s" s="1" r="C107">
+      <c t="s" s="3" r="E107">
         <v>366</v>
-      </c>
-      <c t="s" s="3" r="D107">
-        <v>367</v>
-      </c>
-      <c t="s" s="3" r="E107">
-        <v>368</v>
       </c>
     </row>
     <row r="108">
       <c s="13" r="A108"/>
       <c t="s" s="11" r="B108">
+        <v>367</v>
+      </c>
+      <c t="s" s="1" r="C108">
+        <v>368</v>
+      </c>
+      <c t="s" s="3" r="D108">
         <v>369</v>
       </c>
-      <c t="s" s="1" r="C108">
+      <c t="s" s="3" r="E108">
         <v>370</v>
-      </c>
-      <c t="s" s="3" r="D108">
-        <v>371</v>
-      </c>
-      <c t="s" s="1" r="E108">
-        <v>372</v>
       </c>
     </row>
     <row r="109">
       <c s="13" r="A109"/>
-      <c s="12" r="B109"/>
-      <c s="6" r="C109"/>
-      <c s="10" r="D109"/>
-      <c s="10" r="E109"/>
+      <c t="s" s="11" r="B109">
+        <v>371</v>
+      </c>
+      <c t="s" s="1" r="C109">
+        <v>372</v>
+      </c>
+      <c t="s" s="3" r="D109">
+        <v>373</v>
+      </c>
+      <c t="s" s="1" r="E109">
+        <v>374</v>
+      </c>
     </row>
     <row r="110">
-      <c t="s" s="13" r="A110">
-        <v>373</v>
-      </c>
-      <c t="s" s="11" r="B110">
-        <v>374</v>
-      </c>
-      <c t="s" s="8" r="C110">
+      <c s="13" r="A110"/>
+      <c s="12" r="B110"/>
+      <c s="6" r="C110"/>
+      <c s="10" r="D110"/>
+      <c s="10" r="E110"/>
+    </row>
+    <row r="111">
+      <c t="s" s="13" r="A111">
         <v>375</v>
       </c>
-      <c t="s" s="3" r="D110">
+      <c t="s" s="11" r="B111">
         <v>376</v>
       </c>
-      <c t="s" s="3" r="E110">
+      <c t="s" s="8" r="C111">
         <v>377</v>
       </c>
-    </row>
-    <row r="111">
-      <c s="13" r="A111"/>
-      <c t="s" s="11" r="B111">
+      <c t="s" s="3" r="D111">
         <v>378</v>
       </c>
-      <c t="s" s="8" r="C111">
+      <c t="s" s="3" r="E111">
         <v>379</v>
       </c>
-      <c t="s" s="3" r="D111">
+    </row>
+    <row r="112">
+      <c s="13" r="A112"/>
+      <c t="s" s="11" r="B112">
         <v>380</v>
       </c>
-      <c t="s" s="3" r="E111">
+      <c t="s" s="8" r="C112">
         <v>381</v>
       </c>
-    </row>
-    <row r="112">
-      <c s="20" r="A112"/>
-      <c s="5" r="B112"/>
-      <c s="25" r="C112"/>
-      <c s="15" r="D112"/>
-      <c s="15" r="E112"/>
+      <c t="s" s="3" r="D112">
+        <v>382</v>
+      </c>
+      <c t="s" s="3" r="E112">
+        <v>383</v>
+      </c>
     </row>
     <row r="113">
-      <c t="s" s="13" r="A113">
-        <v>382</v>
-      </c>
-      <c t="s" s="11" r="B113">
-        <v>383</v>
-      </c>
-      <c t="s" s="8" r="C113">
+      <c s="20" r="A113"/>
+      <c s="5" r="B113"/>
+      <c s="25" r="C113"/>
+      <c s="15" r="D113"/>
+      <c s="15" r="E113"/>
+    </row>
+    <row r="114">
+      <c t="s" s="13" r="A114">
         <v>384</v>
       </c>
-      <c t="s" s="3" r="D113">
+      <c t="s" s="11" r="B114">
         <v>385</v>
       </c>
-      <c t="s" s="3" r="E113">
+      <c t="s" s="8" r="C114">
         <v>386</v>
       </c>
-    </row>
-    <row r="114">
-      <c s="13" r="A114"/>
-      <c t="s" s="11" r="B114">
+      <c t="s" s="3" r="D114">
         <v>387</v>
       </c>
-      <c t="s" s="8" r="C114">
+      <c t="s" s="3" r="E114">
         <v>388</v>
-      </c>
-      <c t="s" s="3" r="D114">
-        <v>389</v>
-      </c>
-      <c t="s" s="3" r="E114">
-        <v>390</v>
       </c>
     </row>
     <row r="115">
       <c s="13" r="A115"/>
       <c t="s" s="11" r="B115">
+        <v>389</v>
+      </c>
+      <c t="s" s="8" r="C115">
+        <v>390</v>
+      </c>
+      <c t="s" s="3" r="D115">
         <v>391</v>
       </c>
-      <c t="s" s="8" r="C115">
+      <c t="s" s="3" r="E115">
         <v>392</v>
-      </c>
-      <c t="s" s="3" r="D115">
-        <v>393</v>
-      </c>
-      <c t="s" s="3" r="E115">
-        <v>394</v>
       </c>
     </row>
     <row r="116">
       <c s="13" r="A116"/>
       <c t="s" s="11" r="B116">
+        <v>393</v>
+      </c>
+      <c t="s" s="8" r="C116">
+        <v>394</v>
+      </c>
+      <c t="s" s="3" r="D116">
         <v>395</v>
       </c>
-      <c t="s" s="8" r="C116">
+      <c t="s" s="3" r="E116">
         <v>396</v>
-      </c>
-      <c t="s" s="3" r="D116">
-        <v>397</v>
-      </c>
-      <c t="s" s="3" r="E116">
-        <v>398</v>
       </c>
     </row>
     <row r="117">
       <c s="13" r="A117"/>
       <c t="s" s="11" r="B117">
+        <v>397</v>
+      </c>
+      <c t="s" s="8" r="C117">
+        <v>398</v>
+      </c>
+      <c t="s" s="3" r="D117">
         <v>399</v>
       </c>
-      <c t="s" s="8" r="C117">
+      <c t="s" s="3" r="E117">
         <v>400</v>
-      </c>
-      <c t="s" s="3" r="D117">
-        <v>401</v>
-      </c>
-      <c t="s" s="3" r="E117">
-        <v>402</v>
       </c>
     </row>
     <row r="118">
       <c s="13" r="A118"/>
-      <c s="5" r="B118"/>
-      <c s="25" r="C118"/>
-      <c s="15" r="D118"/>
-      <c s="15" r="E118"/>
+      <c t="s" s="11" r="B118">
+        <v>401</v>
+      </c>
+      <c t="s" s="8" r="C118">
+        <v>402</v>
+      </c>
+      <c t="s" s="3" r="D118">
+        <v>403</v>
+      </c>
+      <c t="s" s="3" r="E118">
+        <v>404</v>
+      </c>
     </row>
     <row r="119">
-      <c t="s" s="13" r="A119">
-        <v>403</v>
-      </c>
-      <c t="s" s="28" r="B119">
-        <v>404</v>
-      </c>
-      <c t="s" s="16" r="C119">
-        <v>403</v>
-      </c>
-      <c s="24" r="D119"/>
-      <c s="24" r="E119"/>
+      <c s="13" r="A119"/>
+      <c s="5" r="B119"/>
+      <c s="25" r="C119"/>
+      <c s="15" r="D119"/>
+      <c s="15" r="E119"/>
     </row>
     <row r="120">
-      <c s="13" r="A120"/>
-      <c s="12" r="B120"/>
-      <c s="6" r="C120"/>
-      <c s="10" r="D120"/>
-      <c s="10" r="E120"/>
+      <c t="s" s="13" r="A120">
+        <v>405</v>
+      </c>
+      <c t="s" s="28" r="B120">
+        <v>406</v>
+      </c>
+      <c t="s" s="16" r="C120">
+        <v>405</v>
+      </c>
+      <c s="24" r="D120"/>
+      <c s="24" r="E120"/>
     </row>
     <row r="121">
-      <c t="s" s="13" r="A121">
-        <v>405</v>
-      </c>
-      <c t="s" s="22" r="B121">
-        <v>406</v>
-      </c>
-      <c t="s" s="26" r="C121">
+      <c s="13" r="A121"/>
+      <c s="12" r="B121"/>
+      <c s="6" r="C121"/>
+      <c s="10" r="D121"/>
+      <c s="10" r="E121"/>
+    </row>
+    <row r="122">
+      <c t="s" s="13" r="A122">
         <v>407</v>
       </c>
-      <c s="30" r="D121"/>
-      <c s="30" r="E121"/>
-    </row>
-    <row r="122">
-      <c s="13" r="A122"/>
       <c t="s" s="22" r="B122">
         <v>408</v>
       </c>
@@ -3464,10 +3470,14 @@
     </row>
     <row r="123">
       <c s="13" r="A123"/>
-      <c s="12" r="B123"/>
-      <c s="6" r="C123"/>
-      <c s="10" r="D123"/>
-      <c s="10" r="E123"/>
+      <c t="s" s="22" r="B123">
+        <v>410</v>
+      </c>
+      <c t="s" s="26" r="C123">
+        <v>411</v>
+      </c>
+      <c s="30" r="D123"/>
+      <c s="30" r="E123"/>
     </row>
     <row r="124">
       <c s="13" r="A124"/>
@@ -3482,6 +3492,13 @@
       <c s="6" r="C125"/>
       <c s="10" r="D125"/>
       <c s="10" r="E125"/>
+    </row>
+    <row r="126">
+      <c s="13" r="A126"/>
+      <c s="12" r="B126"/>
+      <c s="6" r="C126"/>
+      <c s="10" r="D126"/>
+      <c s="10" r="E126"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
EWD-22149 - Create/Update/Delete Question - localization update
Former-commit-id: 5f7cf5c7862fba39cefa5a61094116ea7a3506c0
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="426">
   <si>
     <t>Page</t>
   </si>
@@ -288,6 +288,12 @@
     <t>Neues Lernziel hinzufügen</t>
   </si>
   <si>
+    <t>learningObjectiveListIsEmpty</t>
+  </si>
+  <si>
+    <t>Learning objective list is empty</t>
+  </si>
+  <si>
     <t>Objective</t>
   </si>
   <si>
@@ -417,6 +423,12 @@
     <t>Anzahl der verwandten Ziele</t>
   </si>
   <si>
+    <t>experienceListIsEmpty</t>
+  </si>
+  <si>
+    <t>Experience list is empty</t>
+  </si>
+  <si>
     <t>CreateObjective</t>
   </si>
   <si>
@@ -444,6 +456,18 @@
     <t>Thumbnail</t>
   </si>
   <si>
+    <t>typeObjectiveTitleHere</t>
+  </si>
+  <si>
+    <t>Type objective title here</t>
+  </si>
+  <si>
+    <t>ClickToAddObjective</t>
+  </si>
+  <si>
+    <t>Click to add objective</t>
+  </si>
+  <si>
     <t>CreateExperience</t>
   </si>
   <si>
@@ -469,6 +493,18 @@
   </si>
   <si>
     <t>Objectives in experience</t>
+  </si>
+  <si>
+    <t>typeExperienceTitleHere</t>
+  </si>
+  <si>
+    <t>Type experience title here</t>
+  </si>
+  <si>
+    <t>clickToAddExperience</t>
+  </si>
+  <si>
+    <t>Click to add experience</t>
   </si>
   <si>
     <t>Question</t>
@@ -725,6 +761,12 @@
   </si>
   <si>
     <t>Related question</t>
+  </si>
+  <si>
+    <t>createNewQuestion</t>
+  </si>
+  <si>
+    <t>Create new question</t>
   </si>
   <si>
     <t>customLocalizationPlugin</t>
@@ -2133,216 +2175,216 @@
     </row>
     <row r="26">
       <c s="5" r="A26"/>
-      <c s="5" r="B26"/>
-      <c s="5" r="C26"/>
-      <c s="15" r="D26"/>
-      <c s="7" r="E26"/>
+      <c t="s" s="14" r="B26">
+        <v>91</v>
+      </c>
+      <c t="s" s="14" r="C26">
+        <v>92</v>
+      </c>
+      <c s="17" r="D26"/>
+      <c s="17" r="E26"/>
     </row>
     <row r="27">
-      <c t="s" s="5" r="A27">
-        <v>91</v>
-      </c>
-      <c t="s" s="19" r="B27">
-        <v>92</v>
-      </c>
-      <c t="s" s="19" r="C27">
+      <c s="5" r="A27"/>
+      <c s="5" r="B27"/>
+      <c s="5" r="C27"/>
+      <c s="15" r="D27"/>
+      <c s="7" r="E27"/>
+    </row>
+    <row r="28">
+      <c t="s" s="5" r="A28">
         <v>93</v>
       </c>
-      <c s="9" r="D27"/>
-      <c s="9" r="E27"/>
-    </row>
-    <row r="28">
-      <c s="5" r="A28"/>
-      <c s="5" r="B28"/>
-      <c s="5" r="C28"/>
-      <c s="15" r="D28"/>
-      <c s="7" r="E28"/>
+      <c t="s" s="19" r="B28">
+        <v>94</v>
+      </c>
+      <c t="s" s="19" r="C28">
+        <v>95</v>
+      </c>
+      <c s="9" r="D28"/>
+      <c s="9" r="E28"/>
     </row>
     <row r="29">
-      <c t="s" s="27" r="A29">
-        <v>94</v>
-      </c>
-      <c t="s" s="11" r="B29">
-        <v>95</v>
-      </c>
-      <c t="s" s="11" r="C29">
-        <v>94</v>
-      </c>
-      <c t="s" s="3" r="D29">
+      <c s="5" r="A29"/>
+      <c s="5" r="B29"/>
+      <c s="5" r="C29"/>
+      <c s="15" r="D29"/>
+      <c s="7" r="E29"/>
+    </row>
+    <row r="30">
+      <c t="s" s="27" r="A30">
         <v>96</v>
       </c>
-      <c t="s" s="3" r="E29">
+      <c t="s" s="11" r="B30">
         <v>97</v>
       </c>
-    </row>
-    <row r="30">
-      <c s="27" r="A30"/>
-      <c t="s" s="11" r="B30">
+      <c t="s" s="11" r="C30">
+        <v>96</v>
+      </c>
+      <c t="s" s="3" r="D30">
         <v>98</v>
       </c>
-      <c t="s" s="11" r="C30">
+      <c t="s" s="3" r="E30">
         <v>99</v>
-      </c>
-      <c t="s" s="3" r="D30">
-        <v>100</v>
-      </c>
-      <c t="s" s="3" r="E30">
-        <v>101</v>
       </c>
     </row>
     <row r="31">
       <c s="27" r="A31"/>
       <c t="s" s="11" r="B31">
+        <v>100</v>
+      </c>
+      <c t="s" s="11" r="C31">
+        <v>101</v>
+      </c>
+      <c t="s" s="3" r="D31">
         <v>102</v>
       </c>
-      <c t="s" s="11" r="C31">
+      <c t="s" s="3" r="E31">
         <v>103</v>
-      </c>
-      <c t="s" s="3" r="D31">
-        <v>104</v>
-      </c>
-      <c t="s" s="3" r="E31">
-        <v>105</v>
       </c>
     </row>
     <row r="32">
       <c s="27" r="A32"/>
       <c t="s" s="11" r="B32">
+        <v>104</v>
+      </c>
+      <c t="s" s="11" r="C32">
+        <v>105</v>
+      </c>
+      <c t="s" s="3" r="D32">
         <v>106</v>
       </c>
-      <c t="s" s="11" r="C32">
+      <c t="s" s="3" r="E32">
         <v>107</v>
-      </c>
-      <c t="s" s="3" r="D32">
-        <v>108</v>
-      </c>
-      <c t="s" s="3" r="E32">
-        <v>109</v>
       </c>
     </row>
     <row r="33">
       <c s="27" r="A33"/>
       <c t="s" s="11" r="B33">
+        <v>108</v>
+      </c>
+      <c t="s" s="11" r="C33">
+        <v>109</v>
+      </c>
+      <c t="s" s="3" r="D33">
         <v>110</v>
       </c>
-      <c t="s" s="11" r="C33">
+      <c t="s" s="3" r="E33">
         <v>111</v>
-      </c>
-      <c t="s" s="3" r="D33">
-        <v>112</v>
-      </c>
-      <c t="s" s="3" r="E33">
-        <v>113</v>
       </c>
     </row>
     <row r="34">
       <c s="27" r="A34"/>
       <c t="s" s="11" r="B34">
+        <v>112</v>
+      </c>
+      <c t="s" s="11" r="C34">
+        <v>113</v>
+      </c>
+      <c t="s" s="3" r="D34">
         <v>114</v>
       </c>
-      <c t="s" s="11" r="C34">
+      <c t="s" s="3" r="E34">
         <v>115</v>
-      </c>
-      <c t="s" s="3" r="D34">
-        <v>116</v>
-      </c>
-      <c t="s" s="3" r="E34">
-        <v>117</v>
       </c>
     </row>
     <row r="35">
       <c s="27" r="A35"/>
       <c t="s" s="11" r="B35">
+        <v>116</v>
+      </c>
+      <c t="s" s="11" r="C35">
+        <v>117</v>
+      </c>
+      <c t="s" s="3" r="D35">
         <v>118</v>
       </c>
-      <c t="s" s="11" r="C35">
+      <c t="s" s="3" r="E35">
         <v>119</v>
-      </c>
-      <c t="s" s="3" r="D35">
-        <v>120</v>
-      </c>
-      <c t="s" s="3" r="E35">
-        <v>121</v>
       </c>
     </row>
     <row r="36">
       <c s="27" r="A36"/>
       <c t="s" s="11" r="B36">
+        <v>120</v>
+      </c>
+      <c t="s" s="11" r="C36">
+        <v>121</v>
+      </c>
+      <c t="s" s="3" r="D36">
         <v>122</v>
       </c>
-      <c t="s" s="11" r="C36">
+      <c t="s" s="3" r="E36">
         <v>123</v>
-      </c>
-      <c t="s" s="3" r="D36">
-        <v>124</v>
-      </c>
-      <c t="s" s="3" r="E36">
-        <v>125</v>
       </c>
     </row>
     <row r="37">
       <c s="27" r="A37"/>
       <c t="s" s="11" r="B37">
+        <v>124</v>
+      </c>
+      <c t="s" s="11" r="C37">
+        <v>125</v>
+      </c>
+      <c t="s" s="3" r="D37">
         <v>126</v>
       </c>
-      <c t="s" s="11" r="C37">
+      <c t="s" s="3" r="E37">
         <v>127</v>
-      </c>
-      <c t="s" s="3" r="D37">
-        <v>128</v>
-      </c>
-      <c t="s" s="3" r="E37">
-        <v>129</v>
       </c>
     </row>
     <row r="38">
       <c s="27" r="A38"/>
       <c t="s" s="11" r="B38">
+        <v>128</v>
+      </c>
+      <c t="s" s="11" r="C38">
+        <v>129</v>
+      </c>
+      <c t="s" s="3" r="D38">
         <v>130</v>
       </c>
-      <c t="s" s="11" r="C38">
+      <c t="s" s="3" r="E38">
         <v>131</v>
-      </c>
-      <c t="s" s="3" r="D38">
-        <v>132</v>
-      </c>
-      <c t="s" s="3" r="E38">
-        <v>133</v>
       </c>
     </row>
     <row r="39">
       <c s="27" r="A39"/>
-      <c s="27" r="B39"/>
-      <c s="27" r="C39"/>
-      <c s="7" r="D39"/>
-      <c s="7" r="E39"/>
+      <c t="s" s="11" r="B39">
+        <v>132</v>
+      </c>
+      <c t="s" s="11" r="C39">
+        <v>133</v>
+      </c>
+      <c t="s" s="3" r="D39">
+        <v>134</v>
+      </c>
+      <c t="s" s="3" r="E39">
+        <v>135</v>
+      </c>
     </row>
     <row r="40">
-      <c t="s" s="27" r="A40">
-        <v>134</v>
-      </c>
-      <c t="s" s="28" r="B40">
-        <v>135</v>
-      </c>
-      <c t="s" s="28" r="C40">
+      <c s="27" r="A40"/>
+      <c t="s" s="14" r="B40">
         <v>136</v>
       </c>
-      <c s="24" r="D40"/>
-      <c s="24" r="E40"/>
+      <c t="s" s="14" r="C40">
+        <v>137</v>
+      </c>
+      <c s="17" r="D40"/>
+      <c s="17" r="E40"/>
     </row>
     <row r="41">
       <c s="27" r="A41"/>
-      <c t="s" s="28" r="B41">
-        <v>137</v>
-      </c>
-      <c t="s" s="28" r="C41">
+      <c s="27" r="B41"/>
+      <c s="27" r="C41"/>
+      <c s="7" r="D41"/>
+      <c s="7" r="E41"/>
+    </row>
+    <row r="42">
+      <c t="s" s="27" r="A42">
         <v>138</v>
       </c>
-      <c s="24" r="D41"/>
-      <c s="24" r="E41"/>
-    </row>
-    <row r="42">
-      <c s="27" r="A42"/>
       <c t="s" s="28" r="B42">
         <v>139</v>
       </c>
@@ -2365,1140 +2407,1217 @@
     </row>
     <row r="44">
       <c s="27" r="A44"/>
-      <c s="28" r="B44"/>
-      <c s="28" r="C44"/>
+      <c t="s" s="28" r="B44">
+        <v>143</v>
+      </c>
+      <c t="s" s="28" r="C44">
+        <v>144</v>
+      </c>
       <c s="24" r="D44"/>
       <c s="24" r="E44"/>
     </row>
     <row r="45">
-      <c t="s" s="27" r="A45">
-        <v>143</v>
-      </c>
+      <c s="27" r="A45"/>
       <c t="s" s="28" r="B45">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c t="s" s="28" r="C45">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c s="24" r="D45"/>
       <c s="24" r="E45"/>
     </row>
     <row r="46">
       <c s="27" r="A46"/>
-      <c t="s" s="28" r="B46">
-        <v>146</v>
-      </c>
-      <c t="s" s="28" r="C46">
+      <c t="s" s="14" r="B46">
         <v>147</v>
       </c>
-      <c s="24" r="D46"/>
-      <c s="24" r="E46"/>
+      <c t="s" s="14" r="C46">
+        <v>148</v>
+      </c>
+      <c s="17" r="D46"/>
+      <c s="17" r="E46"/>
     </row>
     <row r="47">
       <c s="27" r="A47"/>
-      <c t="s" s="28" r="B47">
-        <v>148</v>
-      </c>
-      <c t="s" s="28" r="C47">
+      <c t="s" s="14" r="B47">
         <v>149</v>
       </c>
-      <c s="24" r="D47"/>
-      <c s="24" r="E47"/>
+      <c t="s" s="14" r="C47">
+        <v>150</v>
+      </c>
+      <c s="17" r="D47"/>
+      <c s="17" r="E47"/>
     </row>
     <row r="48">
-      <c s="27" r="A48"/>
-      <c t="s" s="28" r="B48">
-        <v>150</v>
-      </c>
-      <c t="s" s="28" r="C48">
+      <c s="5" r="A48"/>
+      <c s="5" r="B48"/>
+      <c s="5" r="C48"/>
+      <c s="15" r="D48"/>
+      <c s="15" r="E48"/>
+    </row>
+    <row r="49">
+      <c t="s" s="27" r="A49">
         <v>151</v>
       </c>
-      <c s="24" r="D48"/>
-      <c s="24" r="E48"/>
-    </row>
-    <row r="49">
-      <c s="27" r="A49"/>
-      <c s="27" r="B49"/>
-      <c s="27" r="C49"/>
-      <c s="7" r="D49"/>
-      <c s="7" r="E49"/>
+      <c t="s" s="28" r="B49">
+        <v>152</v>
+      </c>
+      <c t="s" s="28" r="C49">
+        <v>153</v>
+      </c>
+      <c s="24" r="D49"/>
+      <c s="24" r="E49"/>
     </row>
     <row r="50">
-      <c t="s" s="27" r="A50">
-        <v>152</v>
-      </c>
-      <c t="s" s="11" r="B50">
-        <v>153</v>
-      </c>
-      <c t="s" s="11" r="C50">
+      <c s="27" r="A50"/>
+      <c t="s" s="28" r="B50">
         <v>154</v>
       </c>
-      <c t="s" s="3" r="D50">
+      <c t="s" s="28" r="C50">
         <v>155</v>
       </c>
-      <c t="s" s="3" r="E50">
-        <v>17</v>
-      </c>
+      <c s="24" r="D50"/>
+      <c s="24" r="E50"/>
     </row>
     <row r="51">
       <c s="27" r="A51"/>
-      <c t="s" s="11" r="B51">
+      <c t="s" s="28" r="B51">
         <v>156</v>
       </c>
-      <c t="s" s="11" r="C51">
+      <c t="s" s="28" r="C51">
         <v>157</v>
       </c>
-      <c t="s" s="3" r="D51">
-        <v>158</v>
-      </c>
-      <c t="s" s="3" r="E51">
-        <v>159</v>
-      </c>
+      <c s="24" r="D51"/>
+      <c s="24" r="E51"/>
     </row>
     <row r="52">
       <c s="27" r="A52"/>
-      <c t="s" s="11" r="B52">
-        <v>160</v>
-      </c>
-      <c t="s" s="11" r="C52">
-        <v>161</v>
-      </c>
-      <c t="s" s="3" r="D52">
-        <v>162</v>
-      </c>
-      <c t="s" s="3" r="E52">
-        <v>163</v>
-      </c>
+      <c t="s" s="28" r="B52">
+        <v>158</v>
+      </c>
+      <c t="s" s="28" r="C52">
+        <v>159</v>
+      </c>
+      <c s="24" r="D52"/>
+      <c s="24" r="E52"/>
     </row>
     <row r="53">
       <c s="27" r="A53"/>
-      <c t="s" s="11" r="B53">
-        <v>164</v>
-      </c>
-      <c t="s" s="11" r="C53">
-        <v>165</v>
-      </c>
-      <c t="s" s="3" r="D53">
-        <v>166</v>
-      </c>
-      <c t="s" s="3" r="E53">
-        <v>167</v>
-      </c>
+      <c t="s" s="14" r="B53">
+        <v>160</v>
+      </c>
+      <c t="s" s="14" r="C53">
+        <v>161</v>
+      </c>
+      <c s="17" r="D53"/>
+      <c s="17" r="E53"/>
     </row>
     <row r="54">
       <c s="27" r="A54"/>
-      <c t="s" s="11" r="B54">
-        <v>168</v>
-      </c>
-      <c t="s" s="11" r="C54">
-        <v>169</v>
-      </c>
-      <c t="s" s="3" r="D54">
-        <v>170</v>
-      </c>
-      <c t="s" s="3" r="E54">
-        <v>171</v>
-      </c>
+      <c t="s" s="14" r="B54">
+        <v>162</v>
+      </c>
+      <c t="s" s="14" r="C54">
+        <v>163</v>
+      </c>
+      <c s="17" r="D54"/>
+      <c s="17" r="E54"/>
     </row>
     <row r="55">
       <c s="27" r="A55"/>
-      <c t="s" s="11" r="B55">
-        <v>172</v>
-      </c>
-      <c t="s" s="11" r="C55">
-        <v>173</v>
-      </c>
-      <c t="s" s="3" r="D55">
-        <v>174</v>
-      </c>
-      <c t="s" s="3" r="E55">
-        <v>175</v>
-      </c>
+      <c s="27" r="B55"/>
+      <c s="27" r="C55"/>
+      <c s="7" r="D55"/>
+      <c s="7" r="E55"/>
     </row>
     <row r="56">
-      <c s="27" r="A56"/>
+      <c t="s" s="27" r="A56">
+        <v>164</v>
+      </c>
       <c t="s" s="11" r="B56">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c t="s" s="11" r="C56">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c t="s" s="3" r="D56">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c t="s" s="3" r="E56">
-        <v>179</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57">
       <c s="27" r="A57"/>
       <c t="s" s="11" r="B57">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c t="s" s="11" r="C57">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c t="s" s="3" r="D57">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c t="s" s="3" r="E57">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="58">
       <c s="27" r="A58"/>
       <c t="s" s="11" r="B58">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c t="s" s="11" r="C58">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c t="s" s="3" r="D58">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c t="s" s="3" r="E58">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="59">
       <c s="27" r="A59"/>
-      <c s="27" r="B59"/>
-      <c s="27" r="C59"/>
-      <c s="7" r="D59"/>
-      <c s="7" r="E59"/>
+      <c t="s" s="11" r="B59">
+        <v>176</v>
+      </c>
+      <c t="s" s="11" r="C59">
+        <v>177</v>
+      </c>
+      <c t="s" s="3" r="D59">
+        <v>178</v>
+      </c>
+      <c t="s" s="3" r="E59">
+        <v>179</v>
+      </c>
     </row>
     <row r="60">
-      <c t="s" s="27" r="A60">
-        <v>188</v>
-      </c>
+      <c s="27" r="A60"/>
       <c t="s" s="11" r="B60">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c t="s" s="11" r="C60">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c t="s" s="3" r="D60">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c t="s" s="3" r="E60">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="61">
       <c s="27" r="A61"/>
       <c t="s" s="11" r="B61">
+        <v>184</v>
+      </c>
+      <c t="s" s="11" r="C61">
+        <v>185</v>
+      </c>
+      <c t="s" s="3" r="D61">
+        <v>186</v>
+      </c>
+      <c t="s" s="3" r="E61">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="62">
+      <c s="27" r="A62"/>
+      <c t="s" s="11" r="B62">
+        <v>188</v>
+      </c>
+      <c t="s" s="11" r="C62">
+        <v>189</v>
+      </c>
+      <c t="s" s="3" r="D62">
+        <v>190</v>
+      </c>
+      <c t="s" s="3" r="E62">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="63">
+      <c s="27" r="A63"/>
+      <c t="s" s="11" r="B63">
+        <v>192</v>
+      </c>
+      <c t="s" s="11" r="C63">
         <v>193</v>
       </c>
-      <c t="s" s="11" r="C61">
+      <c t="s" s="3" r="D63">
         <v>194</v>
       </c>
-      <c t="s" s="3" r="D61">
+      <c t="s" s="3" r="E63">
         <v>195</v>
       </c>
-      <c t="s" s="3" r="E61">
+    </row>
+    <row r="64">
+      <c s="27" r="A64"/>
+      <c t="s" s="11" r="B64">
         <v>196</v>
       </c>
-    </row>
-    <row r="62">
-      <c s="13" r="A62"/>
-      <c t="s" s="11" r="B62">
+      <c t="s" s="11" r="C64">
         <v>197</v>
       </c>
-      <c t="s" s="11" r="C62">
+      <c t="s" s="3" r="D64">
         <v>198</v>
       </c>
-      <c t="s" s="3" r="D62">
+      <c t="s" s="3" r="E64">
         <v>199</v>
       </c>
-      <c t="s" s="3" r="E62">
+    </row>
+    <row r="65">
+      <c s="27" r="A65"/>
+      <c s="27" r="B65"/>
+      <c s="27" r="C65"/>
+      <c s="7" r="D65"/>
+      <c s="7" r="E65"/>
+    </row>
+    <row r="66">
+      <c t="s" s="27" r="A66">
         <v>200</v>
       </c>
-    </row>
-    <row r="63">
-      <c s="13" r="A63"/>
-      <c t="s" s="11" r="B63">
+      <c t="s" s="11" r="B66">
         <v>201</v>
       </c>
-      <c t="s" s="11" r="C63">
+      <c t="s" s="11" r="C66">
         <v>202</v>
       </c>
-      <c t="s" s="3" r="D63">
+      <c t="s" s="3" r="D66">
         <v>203</v>
       </c>
-      <c t="s" s="3" r="E63">
+      <c t="s" s="3" r="E66">
         <v>204</v>
       </c>
     </row>
-    <row r="64">
-      <c s="13" r="A64"/>
-      <c t="s" s="11" r="B64">
+    <row r="67">
+      <c s="27" r="A67"/>
+      <c t="s" s="11" r="B67">
         <v>205</v>
       </c>
-      <c t="s" s="11" r="C64">
+      <c t="s" s="11" r="C67">
         <v>206</v>
       </c>
-      <c t="s" s="3" r="D64">
+      <c t="s" s="3" r="D67">
         <v>207</v>
       </c>
-      <c t="s" s="3" r="E64">
+      <c t="s" s="3" r="E67">
         <v>208</v>
-      </c>
-    </row>
-    <row r="65">
-      <c s="13" r="A65"/>
-      <c t="s" s="11" r="B65">
-        <v>209</v>
-      </c>
-      <c t="s" s="11" r="C65">
-        <v>210</v>
-      </c>
-      <c t="s" s="3" r="D65">
-        <v>211</v>
-      </c>
-      <c t="s" s="3" r="E65">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="66">
-      <c s="13" r="A66"/>
-      <c t="s" s="11" r="B66">
-        <v>213</v>
-      </c>
-      <c t="s" s="11" r="C66">
-        <v>214</v>
-      </c>
-      <c t="s" s="3" r="D66">
-        <v>215</v>
-      </c>
-      <c t="s" s="3" r="E66">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="67">
-      <c s="13" r="A67"/>
-      <c t="s" s="11" r="B67">
-        <v>217</v>
-      </c>
-      <c t="s" s="11" r="C67">
-        <v>218</v>
-      </c>
-      <c t="s" s="3" r="D67">
-        <v>219</v>
-      </c>
-      <c t="s" s="3" r="E67">
-        <v>220</v>
       </c>
     </row>
     <row r="68">
       <c s="13" r="A68"/>
       <c t="s" s="11" r="B68">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c t="s" s="11" r="C68">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c t="s" s="3" r="D68">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c t="s" s="3" r="E68">
-        <v>224</v>
+        <v>212</v>
       </c>
     </row>
     <row r="69">
       <c s="13" r="A69"/>
       <c t="s" s="11" r="B69">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c t="s" s="11" r="C69">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c t="s" s="3" r="D69">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c t="s" s="3" r="E69">
-        <v>228</v>
+        <v>216</v>
       </c>
     </row>
     <row r="70">
       <c s="13" r="A70"/>
       <c t="s" s="11" r="B70">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c t="s" s="11" r="C70">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c t="s" s="3" r="D70">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c t="s" s="3" r="E70">
-        <v>232</v>
+        <v>220</v>
       </c>
     </row>
     <row r="71">
       <c s="13" r="A71"/>
-      <c t="s" s="14" r="B71">
-        <v>233</v>
-      </c>
-      <c t="s" s="14" r="C71">
-        <v>234</v>
-      </c>
-      <c s="17" r="D71"/>
-      <c s="17" r="E71"/>
+      <c t="s" s="11" r="B71">
+        <v>221</v>
+      </c>
+      <c t="s" s="11" r="C71">
+        <v>222</v>
+      </c>
+      <c t="s" s="3" r="D71">
+        <v>223</v>
+      </c>
+      <c t="s" s="3" r="E71">
+        <v>224</v>
+      </c>
     </row>
     <row r="72">
       <c s="13" r="A72"/>
-      <c t="s" s="14" r="B72">
-        <v>235</v>
-      </c>
-      <c t="s" s="14" r="C72">
-        <v>236</v>
-      </c>
-      <c s="17" r="D72"/>
-      <c s="17" r="E72"/>
+      <c t="s" s="11" r="B72">
+        <v>225</v>
+      </c>
+      <c t="s" s="11" r="C72">
+        <v>226</v>
+      </c>
+      <c t="s" s="3" r="D72">
+        <v>227</v>
+      </c>
+      <c t="s" s="3" r="E72">
+        <v>228</v>
+      </c>
     </row>
     <row r="73">
       <c s="13" r="A73"/>
-      <c s="27" r="B73"/>
-      <c s="27" r="C73"/>
-      <c s="7" r="D73"/>
-      <c s="7" r="E73"/>
+      <c t="s" s="11" r="B73">
+        <v>229</v>
+      </c>
+      <c t="s" s="11" r="C73">
+        <v>230</v>
+      </c>
+      <c t="s" s="3" r="D73">
+        <v>231</v>
+      </c>
+      <c t="s" s="3" r="E73">
+        <v>232</v>
+      </c>
     </row>
     <row r="74">
-      <c t="s" s="13" r="A74">
-        <v>237</v>
-      </c>
+      <c s="13" r="A74"/>
       <c t="s" s="11" r="B74">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c t="s" s="11" r="C74">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c t="s" s="3" r="D74">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c t="s" s="3" r="E74">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="75">
       <c s="13" r="A75"/>
       <c t="s" s="11" r="B75">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c t="s" s="11" r="C75">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c t="s" s="3" r="D75">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c t="s" s="3" r="E75">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="76">
       <c s="13" r="A76"/>
       <c t="s" s="11" r="B76">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c t="s" s="11" r="C76">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c t="s" s="3" r="D76">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c t="s" s="3" r="E76">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="77">
       <c s="13" r="A77"/>
-      <c t="s" s="11" r="B77">
-        <v>250</v>
-      </c>
-      <c t="s" s="11" r="C77">
-        <v>251</v>
-      </c>
-      <c t="s" s="3" r="D77">
-        <v>252</v>
-      </c>
-      <c t="s" s="3" r="E77">
-        <v>253</v>
-      </c>
+      <c t="s" s="14" r="B77">
+        <v>245</v>
+      </c>
+      <c t="s" s="14" r="C77">
+        <v>246</v>
+      </c>
+      <c s="17" r="D77"/>
+      <c s="17" r="E77"/>
     </row>
     <row r="78">
       <c s="13" r="A78"/>
-      <c t="s" s="11" r="B78">
-        <v>254</v>
-      </c>
-      <c t="s" s="11" r="C78">
-        <v>255</v>
-      </c>
-      <c t="s" s="3" r="D78">
-        <v>256</v>
-      </c>
-      <c t="s" s="3" r="E78">
-        <v>257</v>
-      </c>
+      <c t="s" s="14" r="B78">
+        <v>247</v>
+      </c>
+      <c t="s" s="14" r="C78">
+        <v>248</v>
+      </c>
+      <c s="17" r="D78"/>
+      <c s="17" r="E78"/>
     </row>
     <row r="79">
       <c s="13" r="A79"/>
-      <c t="s" s="11" r="B79">
-        <v>258</v>
-      </c>
-      <c t="s" s="11" r="C79">
-        <v>259</v>
-      </c>
-      <c t="s" s="3" r="D79">
-        <v>260</v>
-      </c>
-      <c t="s" s="3" r="E79">
-        <v>259</v>
-      </c>
+      <c t="s" s="14" r="B79">
+        <v>249</v>
+      </c>
+      <c t="s" s="14" r="C79">
+        <v>250</v>
+      </c>
+      <c s="17" r="D79"/>
+      <c s="17" r="E79"/>
     </row>
     <row r="80">
       <c s="13" r="A80"/>
-      <c t="s" s="11" r="B80">
-        <v>261</v>
-      </c>
-      <c t="s" s="11" r="C80">
-        <v>262</v>
-      </c>
-      <c t="s" s="3" r="D80">
-        <v>263</v>
-      </c>
-      <c t="s" s="3" r="E80">
-        <v>264</v>
-      </c>
+      <c s="27" r="B80"/>
+      <c s="27" r="C80"/>
+      <c s="7" r="D80"/>
+      <c s="7" r="E80"/>
     </row>
     <row r="81">
-      <c s="13" r="A81"/>
+      <c t="s" s="13" r="A81">
+        <v>251</v>
+      </c>
       <c t="s" s="11" r="B81">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c t="s" s="11" r="C81">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c t="s" s="3" r="D81">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c t="s" s="3" r="E81">
-        <v>268</v>
+        <v>255</v>
       </c>
     </row>
     <row r="82">
       <c s="13" r="A82"/>
       <c t="s" s="11" r="B82">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c t="s" s="11" r="C82">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c t="s" s="3" r="D82">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c t="s" s="3" r="E82">
-        <v>272</v>
+        <v>259</v>
       </c>
     </row>
     <row r="83">
       <c s="13" r="A83"/>
       <c t="s" s="11" r="B83">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c t="s" s="11" r="C83">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c t="s" s="3" r="D83">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c t="s" s="3" r="E83">
-        <v>276</v>
+        <v>263</v>
       </c>
     </row>
     <row r="84">
       <c s="13" r="A84"/>
       <c t="s" s="11" r="B84">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c t="s" s="11" r="C84">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c t="s" s="3" r="D84">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c t="s" s="3" r="E84">
-        <v>280</v>
+        <v>267</v>
       </c>
     </row>
     <row r="85">
       <c s="13" r="A85"/>
       <c t="s" s="11" r="B85">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c t="s" s="11" r="C85">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c t="s" s="3" r="D85">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c t="s" s="3" r="E85">
-        <v>283</v>
+        <v>271</v>
       </c>
     </row>
     <row r="86">
       <c s="13" r="A86"/>
       <c t="s" s="11" r="B86">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c t="s" s="11" r="C86">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c t="s" s="3" r="D86">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c t="s" s="3" r="E86">
-        <v>286</v>
+        <v>273</v>
       </c>
     </row>
     <row r="87">
       <c s="13" r="A87"/>
       <c t="s" s="11" r="B87">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c t="s" s="11" r="C87">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c t="s" s="3" r="D87">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c t="s" s="3" r="E87">
-        <v>290</v>
+        <v>278</v>
       </c>
     </row>
     <row r="88">
       <c s="13" r="A88"/>
-      <c t="s" s="8" r="B88">
-        <v>291</v>
+      <c t="s" s="11" r="B88">
+        <v>279</v>
       </c>
       <c t="s" s="11" r="C88">
-        <v>292</v>
+        <v>280</v>
       </c>
       <c t="s" s="3" r="D88">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c t="s" s="3" r="E88">
-        <v>293</v>
+        <v>282</v>
       </c>
     </row>
     <row r="89">
       <c s="13" r="A89"/>
       <c t="s" s="11" r="B89">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c t="s" s="11" r="C89">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c t="s" s="3" r="D89">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c t="s" s="3" r="E89">
-        <v>297</v>
+        <v>286</v>
       </c>
     </row>
     <row r="90">
       <c s="13" r="A90"/>
       <c t="s" s="11" r="B90">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c t="s" s="11" r="C90">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c t="s" s="3" r="D90">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c t="s" s="3" r="E90">
-        <v>301</v>
+        <v>290</v>
       </c>
     </row>
     <row r="91">
       <c s="13" r="A91"/>
       <c t="s" s="11" r="B91">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c t="s" s="11" r="C91">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c t="s" s="3" r="D91">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c t="s" s="3" r="E91">
-        <v>305</v>
+        <v>294</v>
       </c>
     </row>
     <row r="92">
       <c s="13" r="A92"/>
       <c t="s" s="11" r="B92">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c t="s" s="11" r="C92">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c t="s" s="3" r="D92">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c t="s" s="3" r="E92">
-        <v>309</v>
+        <v>297</v>
       </c>
     </row>
     <row r="93">
       <c s="13" r="A93"/>
       <c t="s" s="11" r="B93">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c t="s" s="11" r="C93">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c t="s" s="3" r="D93">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c t="s" s="3" r="E93">
-        <v>313</v>
+        <v>300</v>
       </c>
     </row>
     <row r="94">
       <c s="13" r="A94"/>
       <c t="s" s="11" r="B94">
-        <v>314</v>
+        <v>301</v>
       </c>
       <c t="s" s="11" r="C94">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c t="s" s="3" r="D94">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c t="s" s="3" r="E94">
-        <v>317</v>
+        <v>304</v>
       </c>
     </row>
     <row r="95">
       <c s="13" r="A95"/>
-      <c t="s" s="11" r="B95">
-        <v>318</v>
+      <c t="s" s="8" r="B95">
+        <v>305</v>
       </c>
       <c t="s" s="11" r="C95">
-        <v>319</v>
+        <v>306</v>
       </c>
       <c t="s" s="3" r="D95">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c t="s" s="3" r="E95">
-        <v>321</v>
+        <v>307</v>
       </c>
     </row>
     <row r="96">
       <c s="13" r="A96"/>
       <c t="s" s="11" r="B96">
-        <v>322</v>
+        <v>308</v>
       </c>
       <c t="s" s="11" r="C96">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c t="s" s="3" r="D96">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c t="s" s="3" r="E96">
-        <v>325</v>
+        <v>311</v>
       </c>
     </row>
     <row r="97">
       <c s="13" r="A97"/>
       <c t="s" s="11" r="B97">
-        <v>326</v>
+        <v>312</v>
       </c>
       <c t="s" s="11" r="C97">
-        <v>327</v>
+        <v>313</v>
       </c>
       <c t="s" s="3" r="D97">
-        <v>328</v>
+        <v>314</v>
       </c>
       <c t="s" s="3" r="E97">
-        <v>329</v>
+        <v>315</v>
       </c>
     </row>
     <row r="98">
       <c s="13" r="A98"/>
       <c t="s" s="11" r="B98">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c t="s" s="11" r="C98">
-        <v>331</v>
+        <v>317</v>
       </c>
       <c t="s" s="3" r="D98">
-        <v>332</v>
+        <v>318</v>
       </c>
       <c t="s" s="3" r="E98">
-        <v>333</v>
+        <v>319</v>
       </c>
     </row>
     <row r="99">
       <c s="13" r="A99"/>
       <c t="s" s="11" r="B99">
-        <v>334</v>
+        <v>320</v>
       </c>
       <c t="s" s="11" r="C99">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c t="s" s="3" r="D99">
-        <v>336</v>
+        <v>322</v>
       </c>
       <c t="s" s="3" r="E99">
-        <v>337</v>
+        <v>323</v>
       </c>
     </row>
     <row r="100">
       <c s="13" r="A100"/>
       <c t="s" s="11" r="B100">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c t="s" s="11" r="C100">
-        <v>339</v>
+        <v>325</v>
       </c>
       <c t="s" s="3" r="D100">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c t="s" s="3" r="E100">
-        <v>341</v>
+        <v>327</v>
       </c>
     </row>
     <row r="101">
       <c s="13" r="A101"/>
       <c t="s" s="11" r="B101">
-        <v>342</v>
+        <v>328</v>
       </c>
       <c t="s" s="11" r="C101">
-        <v>343</v>
+        <v>329</v>
       </c>
       <c t="s" s="3" r="D101">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c t="s" s="3" r="E101">
-        <v>345</v>
+        <v>331</v>
       </c>
     </row>
     <row r="102">
       <c s="13" r="A102"/>
       <c t="s" s="11" r="B102">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c t="s" s="11" r="C102">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c t="s" s="3" r="D102">
-        <v>348</v>
+        <v>334</v>
       </c>
       <c t="s" s="3" r="E102">
-        <v>349</v>
+        <v>335</v>
       </c>
     </row>
     <row r="103">
       <c s="13" r="A103"/>
       <c t="s" s="11" r="B103">
-        <v>350</v>
+        <v>336</v>
       </c>
       <c t="s" s="11" r="C103">
-        <v>351</v>
+        <v>337</v>
       </c>
       <c t="s" s="3" r="D103">
-        <v>352</v>
+        <v>338</v>
       </c>
       <c t="s" s="3" r="E103">
-        <v>353</v>
+        <v>339</v>
       </c>
     </row>
     <row r="104">
       <c s="13" r="A104"/>
       <c t="s" s="11" r="B104">
-        <v>354</v>
-      </c>
-      <c t="s" s="8" r="C104">
-        <v>355</v>
+        <v>340</v>
+      </c>
+      <c t="s" s="11" r="C104">
+        <v>341</v>
       </c>
       <c t="s" s="3" r="D104">
-        <v>356</v>
+        <v>342</v>
       </c>
       <c t="s" s="3" r="E104">
-        <v>357</v>
+        <v>343</v>
       </c>
     </row>
     <row r="105">
       <c s="13" r="A105"/>
-      <c t="s" s="8" r="B105">
-        <v>358</v>
-      </c>
-      <c t="s" s="8" r="C105">
-        <v>359</v>
+      <c t="s" s="11" r="B105">
+        <v>344</v>
+      </c>
+      <c t="s" s="11" r="C105">
+        <v>345</v>
       </c>
       <c t="s" s="3" r="D105">
-        <v>360</v>
+        <v>346</v>
       </c>
       <c t="s" s="3" r="E105">
-        <v>361</v>
+        <v>347</v>
       </c>
     </row>
     <row r="106">
       <c s="13" r="A106"/>
       <c t="s" s="11" r="B106">
-        <v>362</v>
-      </c>
-      <c t="s" s="8" r="C106">
-        <v>359</v>
+        <v>348</v>
+      </c>
+      <c t="s" s="11" r="C106">
+        <v>349</v>
       </c>
       <c t="s" s="3" r="D106">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c t="s" s="3" r="E106">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="107">
       <c s="13" r="A107"/>
       <c t="s" s="11" r="B107">
-        <v>363</v>
-      </c>
-      <c t="s" s="1" r="C107">
-        <v>364</v>
+        <v>352</v>
+      </c>
+      <c t="s" s="11" r="C107">
+        <v>353</v>
       </c>
       <c t="s" s="3" r="D107">
-        <v>365</v>
+        <v>354</v>
       </c>
       <c t="s" s="3" r="E107">
-        <v>366</v>
+        <v>355</v>
       </c>
     </row>
     <row r="108">
       <c s="13" r="A108"/>
       <c t="s" s="11" r="B108">
-        <v>367</v>
-      </c>
-      <c t="s" s="1" r="C108">
-        <v>368</v>
+        <v>356</v>
+      </c>
+      <c t="s" s="11" r="C108">
+        <v>357</v>
       </c>
       <c t="s" s="3" r="D108">
-        <v>369</v>
+        <v>358</v>
       </c>
       <c t="s" s="3" r="E108">
-        <v>370</v>
+        <v>359</v>
       </c>
     </row>
     <row r="109">
       <c s="13" r="A109"/>
       <c t="s" s="11" r="B109">
-        <v>371</v>
-      </c>
-      <c t="s" s="1" r="C109">
-        <v>372</v>
+        <v>360</v>
+      </c>
+      <c t="s" s="11" r="C109">
+        <v>361</v>
       </c>
       <c t="s" s="3" r="D109">
-        <v>373</v>
-      </c>
-      <c t="s" s="1" r="E109">
-        <v>374</v>
+        <v>362</v>
+      </c>
+      <c t="s" s="3" r="E109">
+        <v>363</v>
       </c>
     </row>
     <row r="110">
       <c s="13" r="A110"/>
-      <c s="12" r="B110"/>
-      <c s="6" r="C110"/>
-      <c s="10" r="D110"/>
-      <c s="10" r="E110"/>
+      <c t="s" s="11" r="B110">
+        <v>364</v>
+      </c>
+      <c t="s" s="11" r="C110">
+        <v>365</v>
+      </c>
+      <c t="s" s="3" r="D110">
+        <v>366</v>
+      </c>
+      <c t="s" s="3" r="E110">
+        <v>367</v>
+      </c>
     </row>
     <row r="111">
-      <c t="s" s="13" r="A111">
-        <v>375</v>
-      </c>
+      <c s="13" r="A111"/>
       <c t="s" s="11" r="B111">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c t="s" s="8" r="C111">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c t="s" s="3" r="D111">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c t="s" s="3" r="E111">
-        <v>379</v>
+        <v>371</v>
       </c>
     </row>
     <row r="112">
       <c s="13" r="A112"/>
-      <c t="s" s="11" r="B112">
+      <c t="s" s="8" r="B112">
+        <v>372</v>
+      </c>
+      <c t="s" s="8" r="C112">
+        <v>373</v>
+      </c>
+      <c t="s" s="3" r="D112">
+        <v>374</v>
+      </c>
+      <c t="s" s="3" r="E112">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="113">
+      <c s="13" r="A113"/>
+      <c t="s" s="11" r="B113">
+        <v>376</v>
+      </c>
+      <c t="s" s="8" r="C113">
+        <v>373</v>
+      </c>
+      <c t="s" s="3" r="D113">
+        <v>374</v>
+      </c>
+      <c t="s" s="3" r="E113">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="114">
+      <c s="13" r="A114"/>
+      <c t="s" s="11" r="B114">
+        <v>377</v>
+      </c>
+      <c t="s" s="1" r="C114">
+        <v>378</v>
+      </c>
+      <c t="s" s="3" r="D114">
+        <v>379</v>
+      </c>
+      <c t="s" s="3" r="E114">
         <v>380</v>
-      </c>
-      <c t="s" s="8" r="C112">
-        <v>381</v>
-      </c>
-      <c t="s" s="3" r="D112">
-        <v>382</v>
-      </c>
-      <c t="s" s="3" r="E112">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="113">
-      <c s="20" r="A113"/>
-      <c s="5" r="B113"/>
-      <c s="25" r="C113"/>
-      <c s="15" r="D113"/>
-      <c s="15" r="E113"/>
-    </row>
-    <row r="114">
-      <c t="s" s="13" r="A114">
-        <v>384</v>
-      </c>
-      <c t="s" s="11" r="B114">
-        <v>385</v>
-      </c>
-      <c t="s" s="8" r="C114">
-        <v>386</v>
-      </c>
-      <c t="s" s="3" r="D114">
-        <v>387</v>
-      </c>
-      <c t="s" s="3" r="E114">
-        <v>388</v>
       </c>
     </row>
     <row r="115">
       <c s="13" r="A115"/>
       <c t="s" s="11" r="B115">
-        <v>389</v>
-      </c>
-      <c t="s" s="8" r="C115">
-        <v>390</v>
+        <v>381</v>
+      </c>
+      <c t="s" s="1" r="C115">
+        <v>382</v>
       </c>
       <c t="s" s="3" r="D115">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c t="s" s="3" r="E115">
-        <v>392</v>
+        <v>384</v>
       </c>
     </row>
     <row r="116">
       <c s="13" r="A116"/>
       <c t="s" s="11" r="B116">
-        <v>393</v>
-      </c>
-      <c t="s" s="8" r="C116">
-        <v>394</v>
+        <v>385</v>
+      </c>
+      <c t="s" s="1" r="C116">
+        <v>386</v>
       </c>
       <c t="s" s="3" r="D116">
-        <v>395</v>
-      </c>
-      <c t="s" s="3" r="E116">
-        <v>396</v>
+        <v>387</v>
+      </c>
+      <c t="s" s="1" r="E116">
+        <v>388</v>
       </c>
     </row>
     <row r="117">
       <c s="13" r="A117"/>
-      <c t="s" s="11" r="B117">
-        <v>397</v>
-      </c>
-      <c t="s" s="8" r="C117">
-        <v>398</v>
-      </c>
-      <c t="s" s="3" r="D117">
-        <v>399</v>
-      </c>
-      <c t="s" s="3" r="E117">
-        <v>400</v>
-      </c>
+      <c s="12" r="B117"/>
+      <c s="6" r="C117"/>
+      <c s="10" r="D117"/>
+      <c s="10" r="E117"/>
     </row>
     <row r="118">
-      <c s="13" r="A118"/>
+      <c t="s" s="13" r="A118">
+        <v>389</v>
+      </c>
       <c t="s" s="11" r="B118">
-        <v>401</v>
+        <v>390</v>
       </c>
       <c t="s" s="8" r="C118">
-        <v>402</v>
+        <v>391</v>
       </c>
       <c t="s" s="3" r="D118">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c t="s" s="3" r="E118">
-        <v>404</v>
+        <v>393</v>
       </c>
     </row>
     <row r="119">
       <c s="13" r="A119"/>
-      <c s="5" r="B119"/>
-      <c s="25" r="C119"/>
-      <c s="15" r="D119"/>
-      <c s="15" r="E119"/>
+      <c t="s" s="11" r="B119">
+        <v>394</v>
+      </c>
+      <c t="s" s="8" r="C119">
+        <v>395</v>
+      </c>
+      <c t="s" s="3" r="D119">
+        <v>396</v>
+      </c>
+      <c t="s" s="3" r="E119">
+        <v>397</v>
+      </c>
     </row>
     <row r="120">
-      <c t="s" s="13" r="A120">
+      <c s="20" r="A120"/>
+      <c s="5" r="B120"/>
+      <c s="25" r="C120"/>
+      <c s="15" r="D120"/>
+      <c s="15" r="E120"/>
+    </row>
+    <row r="121">
+      <c t="s" s="13" r="A121">
+        <v>398</v>
+      </c>
+      <c t="s" s="11" r="B121">
+        <v>399</v>
+      </c>
+      <c t="s" s="8" r="C121">
+        <v>400</v>
+      </c>
+      <c t="s" s="3" r="D121">
+        <v>401</v>
+      </c>
+      <c t="s" s="3" r="E121">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="122">
+      <c s="13" r="A122"/>
+      <c t="s" s="11" r="B122">
+        <v>403</v>
+      </c>
+      <c t="s" s="8" r="C122">
+        <v>404</v>
+      </c>
+      <c t="s" s="3" r="D122">
         <v>405</v>
       </c>
-      <c t="s" s="28" r="B120">
+      <c t="s" s="3" r="E122">
         <v>406</v>
       </c>
-      <c t="s" s="16" r="C120">
-        <v>405</v>
-      </c>
-      <c s="24" r="D120"/>
-      <c s="24" r="E120"/>
-    </row>
-    <row r="121">
-      <c s="13" r="A121"/>
-      <c s="12" r="B121"/>
-      <c s="6" r="C121"/>
-      <c s="10" r="D121"/>
-      <c s="10" r="E121"/>
-    </row>
-    <row r="122">
-      <c t="s" s="13" r="A122">
-        <v>407</v>
-      </c>
-      <c t="s" s="22" r="B122">
-        <v>408</v>
-      </c>
-      <c t="s" s="26" r="C122">
-        <v>409</v>
-      </c>
-      <c s="30" r="D122"/>
-      <c s="30" r="E122"/>
     </row>
     <row r="123">
       <c s="13" r="A123"/>
-      <c t="s" s="22" r="B123">
+      <c t="s" s="11" r="B123">
+        <v>407</v>
+      </c>
+      <c t="s" s="8" r="C123">
+        <v>408</v>
+      </c>
+      <c t="s" s="3" r="D123">
+        <v>409</v>
+      </c>
+      <c t="s" s="3" r="E123">
         <v>410</v>
       </c>
-      <c t="s" s="26" r="C123">
-        <v>411</v>
-      </c>
-      <c s="30" r="D123"/>
-      <c s="30" r="E123"/>
     </row>
     <row r="124">
       <c s="13" r="A124"/>
-      <c s="12" r="B124"/>
-      <c s="6" r="C124"/>
-      <c s="10" r="D124"/>
-      <c s="10" r="E124"/>
+      <c t="s" s="11" r="B124">
+        <v>411</v>
+      </c>
+      <c t="s" s="8" r="C124">
+        <v>412</v>
+      </c>
+      <c t="s" s="3" r="D124">
+        <v>413</v>
+      </c>
+      <c t="s" s="3" r="E124">
+        <v>414</v>
+      </c>
     </row>
     <row r="125">
       <c s="13" r="A125"/>
-      <c s="12" r="B125"/>
-      <c s="6" r="C125"/>
-      <c s="10" r="D125"/>
-      <c s="10" r="E125"/>
+      <c t="s" s="11" r="B125">
+        <v>415</v>
+      </c>
+      <c t="s" s="8" r="C125">
+        <v>416</v>
+      </c>
+      <c t="s" s="3" r="D125">
+        <v>417</v>
+      </c>
+      <c t="s" s="3" r="E125">
+        <v>418</v>
+      </c>
     </row>
     <row r="126">
       <c s="13" r="A126"/>
-      <c s="12" r="B126"/>
-      <c s="6" r="C126"/>
-      <c s="10" r="D126"/>
-      <c s="10" r="E126"/>
+      <c s="5" r="B126"/>
+      <c s="25" r="C126"/>
+      <c s="15" r="D126"/>
+      <c s="15" r="E126"/>
+    </row>
+    <row r="127">
+      <c t="s" s="13" r="A127">
+        <v>419</v>
+      </c>
+      <c t="s" s="28" r="B127">
+        <v>420</v>
+      </c>
+      <c t="s" s="16" r="C127">
+        <v>419</v>
+      </c>
+      <c s="24" r="D127"/>
+      <c s="24" r="E127"/>
+    </row>
+    <row r="128">
+      <c s="13" r="A128"/>
+      <c s="12" r="B128"/>
+      <c s="6" r="C128"/>
+      <c s="10" r="D128"/>
+      <c s="10" r="E128"/>
+    </row>
+    <row r="129">
+      <c t="s" s="13" r="A129">
+        <v>421</v>
+      </c>
+      <c t="s" s="22" r="B129">
+        <v>422</v>
+      </c>
+      <c t="s" s="26" r="C129">
+        <v>423</v>
+      </c>
+      <c s="30" r="D129"/>
+      <c s="30" r="E129"/>
+    </row>
+    <row r="130">
+      <c s="13" r="A130"/>
+      <c t="s" s="22" r="B130">
+        <v>424</v>
+      </c>
+      <c t="s" s="26" r="C130">
+        <v>425</v>
+      </c>
+      <c s="30" r="D130"/>
+      <c s="30" r="E130"/>
+    </row>
+    <row r="131">
+      <c s="13" r="A131"/>
+      <c s="12" r="B131"/>
+      <c s="6" r="C131"/>
+      <c s="10" r="D131"/>
+      <c s="10" r="E131"/>
+    </row>
+    <row r="132">
+      <c s="13" r="A132"/>
+      <c s="12" r="B132"/>
+      <c s="6" r="C132"/>
+      <c s="10" r="D132"/>
+      <c s="10" r="E132"/>
+    </row>
+    <row r="133">
+      <c s="13" r="A133"/>
+      <c s="12" r="B133"/>
+      <c s="6" r="C133"/>
+      <c s="10" r="D133"/>
+      <c s="10" r="E133"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
EWD-22238 - CUD Learning Objective: Create
Former-commit-id: 2110b7fbac61db93975c2637087b96e167e20802
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="444">
   <si>
     <t>Page</t>
   </si>
@@ -318,12 +318,18 @@
     <t>Liste der Lernziele ist leer</t>
   </si>
   <si>
-    <t>clickToAddNewObjective</t>
+    <t>clickToAddObjective</t>
   </si>
   <si>
     <t>Click to add objective</t>
   </si>
   <si>
+    <t>Klik om de doelstelling toe te voegen</t>
+  </si>
+  <si>
+    <t>Klicken, um Lernziel hinzuzufügen</t>
+  </si>
+  <si>
     <t>Objective</t>
   </si>
   <si>
@@ -474,7 +480,7 @@
     <t>Create New Objective</t>
   </si>
   <si>
-    <t>createObjectiveHint</t>
+    <t>createObjectiveTip</t>
   </si>
   <si>
     <t>Type objective title here</t>
@@ -484,15 +490,6 @@
   </si>
   <si>
     <t>Titel des Lernziels hier eingeben</t>
-  </si>
-  <si>
-    <t>ClickToAddObjective</t>
-  </si>
-  <si>
-    <t>Klik om de doelstelling toe te voegen</t>
-  </si>
-  <si>
-    <t>Klicken, um Lernziel hinzuzufügen</t>
   </si>
   <si>
     <t>CreateExperience</t>
@@ -2265,32 +2262,36 @@
       </c>
     </row>
     <row r="28">
-      <c s="5" r="A28"/>
-      <c t="s" s="19" r="B28">
+      <c s="27" r="A28"/>
+      <c t="s" s="11" r="B28">
         <v>101</v>
       </c>
-      <c t="s" s="19" r="C28">
+      <c t="s" s="11" r="C28">
         <v>102</v>
       </c>
-      <c s="9" r="D28"/>
-      <c s="9" r="E28"/>
+      <c t="s" s="3" r="D28">
+        <v>103</v>
+      </c>
+      <c t="s" s="3" r="E28">
+        <v>104</v>
+      </c>
     </row>
     <row r="29">
-      <c s="5" r="A29"/>
-      <c s="5" r="B29"/>
-      <c s="5" r="C29"/>
-      <c s="15" r="D29"/>
+      <c s="27" r="A29"/>
+      <c s="27" r="B29"/>
+      <c s="27" r="C29"/>
+      <c s="7" r="D29"/>
       <c s="7" r="E29"/>
     </row>
     <row r="30">
       <c t="s" s="5" r="A30">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c t="s" s="19" r="B30">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c t="s" s="19" r="C30">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c s="9" r="D30"/>
       <c s="9" r="E30"/>
@@ -2304,169 +2305,169 @@
     </row>
     <row r="32">
       <c t="s" s="27" r="A32">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c t="s" s="11" r="B32">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c t="s" s="11" r="C32">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c t="s" s="3" r="D32">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c t="s" s="3" r="E32">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33">
       <c s="27" r="A33"/>
       <c t="s" s="11" r="B33">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c t="s" s="11" r="C33">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c t="s" s="3" r="D33">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c t="s" s="3" r="E33">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34">
       <c s="27" r="A34"/>
       <c t="s" s="11" r="B34">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c t="s" s="11" r="C34">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c t="s" s="3" r="D34">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c t="s" s="3" r="E34">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35">
       <c s="27" r="A35"/>
       <c t="s" s="11" r="B35">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c t="s" s="11" r="C35">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c t="s" s="3" r="D35">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c t="s" s="3" r="E35">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36">
       <c s="27" r="A36"/>
       <c t="s" s="11" r="B36">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c t="s" s="11" r="C36">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c t="s" s="3" r="D36">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c t="s" s="3" r="E36">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37">
       <c s="27" r="A37"/>
       <c t="s" s="11" r="B37">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c t="s" s="11" r="C37">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c t="s" s="3" r="D37">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c t="s" s="3" r="E37">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38">
       <c s="27" r="A38"/>
       <c t="s" s="11" r="B38">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c t="s" s="11" r="C38">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c t="s" s="3" r="D38">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c t="s" s="3" r="E38">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="39">
       <c s="27" r="A39"/>
       <c t="s" s="11" r="B39">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c t="s" s="11" r="C39">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c t="s" s="3" r="D39">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c t="s" s="3" r="E39">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40">
       <c s="27" r="A40"/>
       <c t="s" s="11" r="B40">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c t="s" s="11" r="C40">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c t="s" s="3" r="D40">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c t="s" s="3" r="E40">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41">
       <c s="27" r="A41"/>
       <c t="s" s="11" r="B41">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c t="s" s="11" r="C41">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c t="s" s="3" r="D41">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c t="s" s="3" r="E41">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="42">
       <c s="27" r="A42"/>
       <c t="s" s="11" r="B42">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c t="s" s="11" r="C42">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c t="s" s="3" r="D42">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c t="s" s="3" r="E42">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="43">
@@ -2478,13 +2479,13 @@
     </row>
     <row r="44">
       <c t="s" s="27" r="A44">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c t="s" s="14" r="B44">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c t="s" s="14" r="C44">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c s="17" r="D44"/>
       <c s="17" r="E44"/>
@@ -2492,31 +2493,16 @@
     <row r="45">
       <c s="27" r="A45"/>
       <c t="s" s="11" r="B45">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c t="s" s="11" r="C45">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c t="s" s="3" r="D45">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c t="s" s="3" r="E45">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="46">
-      <c s="27" r="A46"/>
-      <c t="s" s="11" r="B46">
-        <v>157</v>
-      </c>
-      <c t="s" s="11" r="C46">
-        <v>102</v>
-      </c>
-      <c t="s" s="3" r="D46">
         <v>158</v>
-      </c>
-      <c t="s" s="3" r="E46">
-        <v>159</v>
       </c>
     </row>
     <row r="47">
@@ -2528,13 +2514,13 @@
     </row>
     <row r="48">
       <c t="s" s="27" r="A48">
+        <v>159</v>
+      </c>
+      <c t="s" s="28" r="B48">
         <v>160</v>
       </c>
-      <c t="s" s="28" r="B48">
+      <c t="s" s="28" r="C48">
         <v>161</v>
-      </c>
-      <c t="s" s="28" r="C48">
-        <v>162</v>
       </c>
       <c s="24" r="D48"/>
       <c s="24" r="E48"/>
@@ -2542,10 +2528,10 @@
     <row r="49">
       <c s="27" r="A49"/>
       <c t="s" s="28" r="B49">
+        <v>162</v>
+      </c>
+      <c t="s" s="28" r="C49">
         <v>163</v>
-      </c>
-      <c t="s" s="28" r="C49">
-        <v>164</v>
       </c>
       <c s="24" r="D49"/>
       <c s="24" r="E49"/>
@@ -2553,10 +2539,10 @@
     <row r="50">
       <c s="27" r="A50"/>
       <c t="s" s="28" r="B50">
+        <v>164</v>
+      </c>
+      <c t="s" s="28" r="C50">
         <v>165</v>
-      </c>
-      <c t="s" s="28" r="C50">
-        <v>166</v>
       </c>
       <c s="24" r="D50"/>
       <c s="24" r="E50"/>
@@ -2564,10 +2550,10 @@
     <row r="51">
       <c s="27" r="A51"/>
       <c t="s" s="28" r="B51">
+        <v>166</v>
+      </c>
+      <c t="s" s="28" r="C51">
         <v>167</v>
-      </c>
-      <c t="s" s="28" r="C51">
-        <v>168</v>
       </c>
       <c s="24" r="D51"/>
       <c s="24" r="E51"/>
@@ -2575,31 +2561,31 @@
     <row r="52">
       <c s="27" r="A52"/>
       <c t="s" s="11" r="B52">
+        <v>168</v>
+      </c>
+      <c t="s" s="11" r="C52">
         <v>169</v>
       </c>
-      <c t="s" s="11" r="C52">
+      <c t="s" s="3" r="D52">
         <v>170</v>
       </c>
-      <c t="s" s="3" r="D52">
+      <c t="s" s="3" r="E52">
         <v>171</v>
-      </c>
-      <c t="s" s="3" r="E52">
-        <v>172</v>
       </c>
     </row>
     <row r="53">
       <c s="27" r="A53"/>
       <c t="s" s="11" r="B53">
+        <v>172</v>
+      </c>
+      <c t="s" s="11" r="C53">
         <v>173</v>
       </c>
-      <c t="s" s="11" r="C53">
+      <c t="s" s="3" r="D53">
         <v>174</v>
       </c>
-      <c t="s" s="3" r="D53">
+      <c t="s" s="3" r="E53">
         <v>175</v>
-      </c>
-      <c t="s" s="3" r="E53">
-        <v>176</v>
       </c>
     </row>
     <row r="54">
@@ -2611,16 +2597,16 @@
     </row>
     <row r="55">
       <c t="s" s="27" r="A55">
+        <v>176</v>
+      </c>
+      <c t="s" s="11" r="B55">
         <v>177</v>
       </c>
-      <c t="s" s="11" r="B55">
+      <c t="s" s="11" r="C55">
         <v>178</v>
       </c>
-      <c t="s" s="11" r="C55">
+      <c t="s" s="3" r="D55">
         <v>179</v>
-      </c>
-      <c t="s" s="3" r="D55">
-        <v>180</v>
       </c>
       <c t="s" s="3" r="E55">
         <v>17</v>
@@ -2629,121 +2615,121 @@
     <row r="56">
       <c s="27" r="A56"/>
       <c t="s" s="11" r="B56">
+        <v>180</v>
+      </c>
+      <c t="s" s="11" r="C56">
         <v>181</v>
       </c>
-      <c t="s" s="11" r="C56">
+      <c t="s" s="3" r="D56">
         <v>182</v>
       </c>
-      <c t="s" s="3" r="D56">
+      <c t="s" s="3" r="E56">
         <v>183</v>
-      </c>
-      <c t="s" s="3" r="E56">
-        <v>184</v>
       </c>
     </row>
     <row r="57">
       <c s="27" r="A57"/>
       <c t="s" s="11" r="B57">
+        <v>184</v>
+      </c>
+      <c t="s" s="11" r="C57">
         <v>185</v>
       </c>
-      <c t="s" s="11" r="C57">
+      <c t="s" s="3" r="D57">
         <v>186</v>
       </c>
-      <c t="s" s="3" r="D57">
+      <c t="s" s="3" r="E57">
         <v>187</v>
-      </c>
-      <c t="s" s="3" r="E57">
-        <v>188</v>
       </c>
     </row>
     <row r="58">
       <c s="27" r="A58"/>
       <c t="s" s="11" r="B58">
+        <v>188</v>
+      </c>
+      <c t="s" s="11" r="C58">
         <v>189</v>
       </c>
-      <c t="s" s="11" r="C58">
+      <c t="s" s="3" r="D58">
         <v>190</v>
       </c>
-      <c t="s" s="3" r="D58">
+      <c t="s" s="3" r="E58">
         <v>191</v>
-      </c>
-      <c t="s" s="3" r="E58">
-        <v>192</v>
       </c>
     </row>
     <row r="59">
       <c s="27" r="A59"/>
       <c t="s" s="11" r="B59">
+        <v>192</v>
+      </c>
+      <c t="s" s="11" r="C59">
         <v>193</v>
       </c>
-      <c t="s" s="11" r="C59">
+      <c t="s" s="3" r="D59">
         <v>194</v>
       </c>
-      <c t="s" s="3" r="D59">
+      <c t="s" s="3" r="E59">
         <v>195</v>
-      </c>
-      <c t="s" s="3" r="E59">
-        <v>196</v>
       </c>
     </row>
     <row r="60">
       <c s="27" r="A60"/>
       <c t="s" s="11" r="B60">
+        <v>196</v>
+      </c>
+      <c t="s" s="11" r="C60">
         <v>197</v>
       </c>
-      <c t="s" s="11" r="C60">
+      <c t="s" s="3" r="D60">
         <v>198</v>
       </c>
-      <c t="s" s="3" r="D60">
+      <c t="s" s="3" r="E60">
         <v>199</v>
-      </c>
-      <c t="s" s="3" r="E60">
-        <v>200</v>
       </c>
     </row>
     <row r="61">
       <c s="27" r="A61"/>
       <c t="s" s="11" r="B61">
+        <v>200</v>
+      </c>
+      <c t="s" s="11" r="C61">
         <v>201</v>
       </c>
-      <c t="s" s="11" r="C61">
+      <c t="s" s="3" r="D61">
         <v>202</v>
       </c>
-      <c t="s" s="3" r="D61">
+      <c t="s" s="3" r="E61">
         <v>203</v>
-      </c>
-      <c t="s" s="3" r="E61">
-        <v>204</v>
       </c>
     </row>
     <row r="62">
       <c s="27" r="A62"/>
       <c t="s" s="11" r="B62">
+        <v>204</v>
+      </c>
+      <c t="s" s="11" r="C62">
         <v>205</v>
       </c>
-      <c t="s" s="11" r="C62">
+      <c t="s" s="3" r="D62">
         <v>206</v>
       </c>
-      <c t="s" s="3" r="D62">
+      <c t="s" s="3" r="E62">
         <v>207</v>
-      </c>
-      <c t="s" s="3" r="E62">
-        <v>208</v>
       </c>
     </row>
     <row r="63">
       <c s="27" r="A63"/>
       <c t="s" s="11" r="B63">
+        <v>208</v>
+      </c>
+      <c t="s" s="11" r="C63">
         <v>209</v>
       </c>
-      <c t="s" s="11" r="C63">
+      <c t="s" s="3" r="D63">
         <v>210</v>
       </c>
-      <c t="s" s="3" r="D63">
+      <c t="s" s="3" r="E63">
         <v>211</v>
-      </c>
-      <c t="s" s="3" r="E63">
-        <v>212</v>
       </c>
     </row>
     <row r="64">
@@ -2755,214 +2741,214 @@
     </row>
     <row r="65">
       <c t="s" s="27" r="A65">
+        <v>212</v>
+      </c>
+      <c t="s" s="11" r="B65">
         <v>213</v>
       </c>
-      <c t="s" s="11" r="B65">
+      <c t="s" s="11" r="C65">
         <v>214</v>
       </c>
-      <c t="s" s="11" r="C65">
+      <c t="s" s="3" r="D65">
         <v>215</v>
       </c>
-      <c t="s" s="3" r="D65">
+      <c t="s" s="3" r="E65">
         <v>216</v>
-      </c>
-      <c t="s" s="3" r="E65">
-        <v>217</v>
       </c>
     </row>
     <row r="66">
       <c s="27" r="A66"/>
       <c t="s" s="11" r="B66">
+        <v>217</v>
+      </c>
+      <c t="s" s="11" r="C66">
         <v>218</v>
       </c>
-      <c t="s" s="11" r="C66">
+      <c t="s" s="3" r="D66">
         <v>219</v>
       </c>
-      <c t="s" s="3" r="D66">
+      <c t="s" s="3" r="E66">
         <v>220</v>
-      </c>
-      <c t="s" s="3" r="E66">
-        <v>221</v>
       </c>
     </row>
     <row r="67">
       <c s="13" r="A67"/>
       <c t="s" s="11" r="B67">
+        <v>221</v>
+      </c>
+      <c t="s" s="11" r="C67">
         <v>222</v>
       </c>
-      <c t="s" s="11" r="C67">
+      <c t="s" s="3" r="D67">
         <v>223</v>
       </c>
-      <c t="s" s="3" r="D67">
+      <c t="s" s="3" r="E67">
         <v>224</v>
-      </c>
-      <c t="s" s="3" r="E67">
-        <v>225</v>
       </c>
     </row>
     <row r="68">
       <c s="13" r="A68"/>
       <c t="s" s="11" r="B68">
+        <v>225</v>
+      </c>
+      <c t="s" s="11" r="C68">
         <v>226</v>
       </c>
-      <c t="s" s="11" r="C68">
+      <c t="s" s="3" r="D68">
         <v>227</v>
       </c>
-      <c t="s" s="3" r="D68">
+      <c t="s" s="3" r="E68">
         <v>228</v>
-      </c>
-      <c t="s" s="3" r="E68">
-        <v>229</v>
       </c>
     </row>
     <row r="69">
       <c s="13" r="A69"/>
       <c t="s" s="11" r="B69">
+        <v>229</v>
+      </c>
+      <c t="s" s="11" r="C69">
         <v>230</v>
       </c>
-      <c t="s" s="11" r="C69">
+      <c t="s" s="3" r="D69">
         <v>231</v>
       </c>
-      <c t="s" s="3" r="D69">
+      <c t="s" s="3" r="E69">
         <v>232</v>
-      </c>
-      <c t="s" s="3" r="E69">
-        <v>233</v>
       </c>
     </row>
     <row r="70">
       <c s="13" r="A70"/>
       <c t="s" s="11" r="B70">
+        <v>233</v>
+      </c>
+      <c t="s" s="11" r="C70">
         <v>234</v>
       </c>
-      <c t="s" s="11" r="C70">
+      <c t="s" s="3" r="D70">
         <v>235</v>
       </c>
-      <c t="s" s="3" r="D70">
+      <c t="s" s="3" r="E70">
         <v>236</v>
-      </c>
-      <c t="s" s="3" r="E70">
-        <v>237</v>
       </c>
     </row>
     <row r="71">
       <c s="13" r="A71"/>
       <c t="s" s="11" r="B71">
+        <v>237</v>
+      </c>
+      <c t="s" s="11" r="C71">
         <v>238</v>
       </c>
-      <c t="s" s="11" r="C71">
+      <c t="s" s="3" r="D71">
         <v>239</v>
       </c>
-      <c t="s" s="3" r="D71">
+      <c t="s" s="3" r="E71">
         <v>240</v>
-      </c>
-      <c t="s" s="3" r="E71">
-        <v>241</v>
       </c>
     </row>
     <row r="72">
       <c s="13" r="A72"/>
       <c t="s" s="11" r="B72">
+        <v>241</v>
+      </c>
+      <c t="s" s="11" r="C72">
         <v>242</v>
       </c>
-      <c t="s" s="11" r="C72">
+      <c t="s" s="3" r="D72">
         <v>243</v>
       </c>
-      <c t="s" s="3" r="D72">
+      <c t="s" s="3" r="E72">
         <v>244</v>
-      </c>
-      <c t="s" s="3" r="E72">
-        <v>245</v>
       </c>
     </row>
     <row r="73">
       <c s="13" r="A73"/>
       <c t="s" s="11" r="B73">
+        <v>245</v>
+      </c>
+      <c t="s" s="11" r="C73">
         <v>246</v>
       </c>
-      <c t="s" s="11" r="C73">
+      <c t="s" s="3" r="D73">
         <v>247</v>
       </c>
-      <c t="s" s="3" r="D73">
+      <c t="s" s="3" r="E73">
         <v>248</v>
-      </c>
-      <c t="s" s="3" r="E73">
-        <v>249</v>
       </c>
     </row>
     <row r="74">
       <c s="13" r="A74"/>
       <c t="s" s="11" r="B74">
+        <v>249</v>
+      </c>
+      <c t="s" s="11" r="C74">
         <v>250</v>
       </c>
-      <c t="s" s="11" r="C74">
+      <c t="s" s="3" r="D74">
         <v>251</v>
       </c>
-      <c t="s" s="3" r="D74">
+      <c t="s" s="3" r="E74">
         <v>252</v>
-      </c>
-      <c t="s" s="3" r="E74">
-        <v>253</v>
       </c>
     </row>
     <row r="75">
       <c s="13" r="A75"/>
       <c t="s" s="11" r="B75">
+        <v>253</v>
+      </c>
+      <c t="s" s="11" r="C75">
         <v>254</v>
       </c>
-      <c t="s" s="11" r="C75">
+      <c t="s" s="3" r="D75">
         <v>255</v>
       </c>
-      <c t="s" s="3" r="D75">
+      <c t="s" s="3" r="E75">
         <v>256</v>
-      </c>
-      <c t="s" s="3" r="E75">
-        <v>257</v>
       </c>
     </row>
     <row r="76">
       <c s="13" r="A76"/>
       <c t="s" s="11" r="B76">
+        <v>257</v>
+      </c>
+      <c t="s" s="11" r="C76">
         <v>258</v>
       </c>
-      <c t="s" s="11" r="C76">
+      <c t="s" s="3" r="D76">
         <v>259</v>
       </c>
-      <c t="s" s="3" r="D76">
+      <c t="s" s="3" r="E76">
         <v>260</v>
-      </c>
-      <c t="s" s="3" r="E76">
-        <v>261</v>
       </c>
     </row>
     <row r="77">
       <c s="13" r="A77"/>
       <c t="s" s="11" r="B77">
+        <v>261</v>
+      </c>
+      <c t="s" s="11" r="C77">
         <v>262</v>
       </c>
-      <c t="s" s="11" r="C77">
+      <c t="s" s="3" r="D77">
         <v>263</v>
       </c>
-      <c t="s" s="3" r="D77">
+      <c t="s" s="3" r="E77">
         <v>264</v>
-      </c>
-      <c t="s" s="3" r="E77">
-        <v>265</v>
       </c>
     </row>
     <row r="78">
       <c s="13" r="A78"/>
       <c t="s" s="11" r="B78">
+        <v>265</v>
+      </c>
+      <c t="s" s="11" r="C78">
         <v>266</v>
       </c>
-      <c t="s" s="11" r="C78">
+      <c t="s" s="3" r="D78">
         <v>267</v>
       </c>
-      <c t="s" s="3" r="D78">
+      <c t="s" s="3" r="E78">
         <v>268</v>
-      </c>
-      <c t="s" s="3" r="E78">
-        <v>269</v>
       </c>
     </row>
     <row r="79">
@@ -2974,544 +2960,544 @@
     </row>
     <row r="80">
       <c t="s" s="13" r="A80">
+        <v>269</v>
+      </c>
+      <c t="s" s="11" r="B80">
         <v>270</v>
       </c>
-      <c t="s" s="11" r="B80">
+      <c t="s" s="11" r="C80">
         <v>271</v>
       </c>
-      <c t="s" s="11" r="C80">
+      <c t="s" s="3" r="D80">
         <v>272</v>
       </c>
-      <c t="s" s="3" r="D80">
+      <c t="s" s="3" r="E80">
         <v>273</v>
-      </c>
-      <c t="s" s="3" r="E80">
-        <v>274</v>
       </c>
     </row>
     <row r="81">
       <c s="13" r="A81"/>
       <c t="s" s="11" r="B81">
+        <v>274</v>
+      </c>
+      <c t="s" s="11" r="C81">
         <v>275</v>
       </c>
-      <c t="s" s="11" r="C81">
+      <c t="s" s="3" r="D81">
         <v>276</v>
       </c>
-      <c t="s" s="3" r="D81">
+      <c t="s" s="3" r="E81">
         <v>277</v>
-      </c>
-      <c t="s" s="3" r="E81">
-        <v>278</v>
       </c>
     </row>
     <row r="82">
       <c s="13" r="A82"/>
       <c t="s" s="11" r="B82">
+        <v>278</v>
+      </c>
+      <c t="s" s="11" r="C82">
         <v>279</v>
       </c>
-      <c t="s" s="11" r="C82">
+      <c t="s" s="3" r="D82">
         <v>280</v>
       </c>
-      <c t="s" s="3" r="D82">
+      <c t="s" s="3" r="E82">
         <v>281</v>
-      </c>
-      <c t="s" s="3" r="E82">
-        <v>282</v>
       </c>
     </row>
     <row r="83">
       <c s="13" r="A83"/>
       <c t="s" s="11" r="B83">
+        <v>282</v>
+      </c>
+      <c t="s" s="11" r="C83">
         <v>283</v>
       </c>
-      <c t="s" s="11" r="C83">
+      <c t="s" s="3" r="D83">
         <v>284</v>
       </c>
-      <c t="s" s="3" r="D83">
+      <c t="s" s="3" r="E83">
         <v>285</v>
-      </c>
-      <c t="s" s="3" r="E83">
-        <v>286</v>
       </c>
     </row>
     <row r="84">
       <c s="13" r="A84"/>
       <c t="s" s="11" r="B84">
+        <v>286</v>
+      </c>
+      <c t="s" s="11" r="C84">
         <v>287</v>
       </c>
-      <c t="s" s="11" r="C84">
+      <c t="s" s="3" r="D84">
         <v>288</v>
       </c>
-      <c t="s" s="3" r="D84">
+      <c t="s" s="3" r="E84">
         <v>289</v>
-      </c>
-      <c t="s" s="3" r="E84">
-        <v>290</v>
       </c>
     </row>
     <row r="85">
       <c s="13" r="A85"/>
       <c t="s" s="11" r="B85">
+        <v>290</v>
+      </c>
+      <c t="s" s="11" r="C85">
         <v>291</v>
       </c>
-      <c t="s" s="11" r="C85">
+      <c t="s" s="3" r="D85">
         <v>292</v>
       </c>
-      <c t="s" s="3" r="D85">
-        <v>293</v>
-      </c>
       <c t="s" s="3" r="E85">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="86">
       <c s="13" r="A86"/>
       <c t="s" s="11" r="B86">
+        <v>293</v>
+      </c>
+      <c t="s" s="11" r="C86">
         <v>294</v>
       </c>
-      <c t="s" s="11" r="C86">
+      <c t="s" s="3" r="D86">
         <v>295</v>
       </c>
-      <c t="s" s="3" r="D86">
+      <c t="s" s="3" r="E86">
         <v>296</v>
-      </c>
-      <c t="s" s="3" r="E86">
-        <v>297</v>
       </c>
     </row>
     <row r="87">
       <c s="13" r="A87"/>
       <c t="s" s="11" r="B87">
+        <v>297</v>
+      </c>
+      <c t="s" s="11" r="C87">
         <v>298</v>
       </c>
-      <c t="s" s="11" r="C87">
+      <c t="s" s="3" r="D87">
         <v>299</v>
       </c>
-      <c t="s" s="3" r="D87">
+      <c t="s" s="3" r="E87">
         <v>300</v>
-      </c>
-      <c t="s" s="3" r="E87">
-        <v>301</v>
       </c>
     </row>
     <row r="88">
       <c s="13" r="A88"/>
       <c t="s" s="11" r="B88">
+        <v>301</v>
+      </c>
+      <c t="s" s="11" r="C88">
         <v>302</v>
       </c>
-      <c t="s" s="11" r="C88">
+      <c t="s" s="3" r="D88">
         <v>303</v>
       </c>
-      <c t="s" s="3" r="D88">
+      <c t="s" s="3" r="E88">
         <v>304</v>
-      </c>
-      <c t="s" s="3" r="E88">
-        <v>305</v>
       </c>
     </row>
     <row r="89">
       <c s="13" r="A89"/>
       <c t="s" s="11" r="B89">
+        <v>305</v>
+      </c>
+      <c t="s" s="11" r="C89">
         <v>306</v>
       </c>
-      <c t="s" s="11" r="C89">
+      <c t="s" s="3" r="D89">
         <v>307</v>
       </c>
-      <c t="s" s="3" r="D89">
+      <c t="s" s="3" r="E89">
         <v>308</v>
-      </c>
-      <c t="s" s="3" r="E89">
-        <v>309</v>
       </c>
     </row>
     <row r="90">
       <c s="13" r="A90"/>
       <c t="s" s="11" r="B90">
+        <v>309</v>
+      </c>
+      <c t="s" s="11" r="C90">
         <v>310</v>
       </c>
-      <c t="s" s="11" r="C90">
+      <c t="s" s="3" r="D90">
         <v>311</v>
       </c>
-      <c t="s" s="3" r="D90">
+      <c t="s" s="3" r="E90">
         <v>312</v>
-      </c>
-      <c t="s" s="3" r="E90">
-        <v>313</v>
       </c>
     </row>
     <row r="91">
       <c s="13" r="A91"/>
       <c t="s" s="11" r="B91">
+        <v>313</v>
+      </c>
+      <c t="s" s="11" r="C91">
         <v>314</v>
       </c>
-      <c t="s" s="11" r="C91">
+      <c t="s" s="3" r="D91">
+        <v>314</v>
+      </c>
+      <c t="s" s="3" r="E91">
         <v>315</v>
-      </c>
-      <c t="s" s="3" r="D91">
-        <v>315</v>
-      </c>
-      <c t="s" s="3" r="E91">
-        <v>316</v>
       </c>
     </row>
     <row r="92">
       <c s="13" r="A92"/>
       <c t="s" s="11" r="B92">
+        <v>316</v>
+      </c>
+      <c t="s" s="11" r="C92">
         <v>317</v>
       </c>
-      <c t="s" s="11" r="C92">
+      <c t="s" s="3" r="D92">
+        <v>317</v>
+      </c>
+      <c t="s" s="3" r="E92">
         <v>318</v>
-      </c>
-      <c t="s" s="3" r="D92">
-        <v>318</v>
-      </c>
-      <c t="s" s="3" r="E92">
-        <v>319</v>
       </c>
     </row>
     <row r="93">
       <c s="13" r="A93"/>
       <c t="s" s="11" r="B93">
+        <v>319</v>
+      </c>
+      <c t="s" s="11" r="C93">
         <v>320</v>
       </c>
-      <c t="s" s="11" r="C93">
+      <c t="s" s="3" r="D93">
         <v>321</v>
       </c>
-      <c t="s" s="3" r="D93">
+      <c t="s" s="3" r="E93">
         <v>322</v>
-      </c>
-      <c t="s" s="3" r="E93">
-        <v>323</v>
       </c>
     </row>
     <row r="94">
       <c s="13" r="A94"/>
       <c t="s" s="8" r="B94">
+        <v>323</v>
+      </c>
+      <c t="s" s="11" r="C94">
         <v>324</v>
       </c>
-      <c t="s" s="11" r="C94">
+      <c t="s" s="3" r="D94">
         <v>325</v>
       </c>
-      <c t="s" s="3" r="D94">
-        <v>326</v>
-      </c>
       <c t="s" s="3" r="E94">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="95">
       <c s="13" r="A95"/>
       <c t="s" s="11" r="B95">
+        <v>326</v>
+      </c>
+      <c t="s" s="11" r="C95">
         <v>327</v>
       </c>
-      <c t="s" s="11" r="C95">
+      <c t="s" s="3" r="D95">
         <v>328</v>
       </c>
-      <c t="s" s="3" r="D95">
+      <c t="s" s="3" r="E95">
         <v>329</v>
-      </c>
-      <c t="s" s="3" r="E95">
-        <v>330</v>
       </c>
     </row>
     <row r="96">
       <c s="13" r="A96"/>
       <c t="s" s="11" r="B96">
+        <v>330</v>
+      </c>
+      <c t="s" s="11" r="C96">
         <v>331</v>
       </c>
-      <c t="s" s="11" r="C96">
+      <c t="s" s="3" r="D96">
         <v>332</v>
       </c>
-      <c t="s" s="3" r="D96">
+      <c t="s" s="3" r="E96">
         <v>333</v>
-      </c>
-      <c t="s" s="3" r="E96">
-        <v>334</v>
       </c>
     </row>
     <row r="97">
       <c s="13" r="A97"/>
       <c t="s" s="11" r="B97">
+        <v>334</v>
+      </c>
+      <c t="s" s="11" r="C97">
         <v>335</v>
       </c>
-      <c t="s" s="11" r="C97">
+      <c t="s" s="3" r="D97">
         <v>336</v>
       </c>
-      <c t="s" s="3" r="D97">
+      <c t="s" s="3" r="E97">
         <v>337</v>
-      </c>
-      <c t="s" s="3" r="E97">
-        <v>338</v>
       </c>
     </row>
     <row r="98">
       <c s="13" r="A98"/>
       <c t="s" s="11" r="B98">
+        <v>338</v>
+      </c>
+      <c t="s" s="11" r="C98">
         <v>339</v>
       </c>
-      <c t="s" s="11" r="C98">
+      <c t="s" s="3" r="D98">
         <v>340</v>
       </c>
-      <c t="s" s="3" r="D98">
+      <c t="s" s="3" r="E98">
         <v>341</v>
-      </c>
-      <c t="s" s="3" r="E98">
-        <v>342</v>
       </c>
     </row>
     <row r="99">
       <c s="13" r="A99"/>
       <c t="s" s="11" r="B99">
+        <v>342</v>
+      </c>
+      <c t="s" s="11" r="C99">
         <v>343</v>
       </c>
-      <c t="s" s="11" r="C99">
+      <c t="s" s="3" r="D99">
         <v>344</v>
       </c>
-      <c t="s" s="3" r="D99">
+      <c t="s" s="3" r="E99">
         <v>345</v>
-      </c>
-      <c t="s" s="3" r="E99">
-        <v>346</v>
       </c>
     </row>
     <row r="100">
       <c s="13" r="A100"/>
       <c t="s" s="11" r="B100">
+        <v>346</v>
+      </c>
+      <c t="s" s="11" r="C100">
         <v>347</v>
       </c>
-      <c t="s" s="11" r="C100">
+      <c t="s" s="3" r="D100">
         <v>348</v>
       </c>
-      <c t="s" s="3" r="D100">
+      <c t="s" s="3" r="E100">
         <v>349</v>
-      </c>
-      <c t="s" s="3" r="E100">
-        <v>350</v>
       </c>
     </row>
     <row r="101">
       <c s="13" r="A101"/>
       <c t="s" s="11" r="B101">
+        <v>350</v>
+      </c>
+      <c t="s" s="11" r="C101">
         <v>351</v>
       </c>
-      <c t="s" s="11" r="C101">
+      <c t="s" s="3" r="D101">
         <v>352</v>
       </c>
-      <c t="s" s="3" r="D101">
+      <c t="s" s="3" r="E101">
         <v>353</v>
-      </c>
-      <c t="s" s="3" r="E101">
-        <v>354</v>
       </c>
     </row>
     <row r="102">
       <c s="13" r="A102"/>
       <c t="s" s="11" r="B102">
+        <v>354</v>
+      </c>
+      <c t="s" s="11" r="C102">
         <v>355</v>
       </c>
-      <c t="s" s="11" r="C102">
+      <c t="s" s="3" r="D102">
         <v>356</v>
       </c>
-      <c t="s" s="3" r="D102">
+      <c t="s" s="3" r="E102">
         <v>357</v>
-      </c>
-      <c t="s" s="3" r="E102">
-        <v>358</v>
       </c>
     </row>
     <row r="103">
       <c s="13" r="A103"/>
       <c t="s" s="11" r="B103">
+        <v>358</v>
+      </c>
+      <c t="s" s="11" r="C103">
         <v>359</v>
       </c>
-      <c t="s" s="11" r="C103">
+      <c t="s" s="3" r="D103">
         <v>360</v>
       </c>
-      <c t="s" s="3" r="D103">
+      <c t="s" s="3" r="E103">
         <v>361</v>
-      </c>
-      <c t="s" s="3" r="E103">
-        <v>362</v>
       </c>
     </row>
     <row r="104">
       <c s="13" r="A104"/>
       <c t="s" s="11" r="B104">
+        <v>362</v>
+      </c>
+      <c t="s" s="11" r="C104">
         <v>363</v>
       </c>
-      <c t="s" s="11" r="C104">
+      <c t="s" s="3" r="D104">
         <v>364</v>
       </c>
-      <c t="s" s="3" r="D104">
+      <c t="s" s="3" r="E104">
         <v>365</v>
-      </c>
-      <c t="s" s="3" r="E104">
-        <v>366</v>
       </c>
     </row>
     <row r="105">
       <c s="13" r="A105"/>
       <c t="s" s="11" r="B105">
+        <v>366</v>
+      </c>
+      <c t="s" s="11" r="C105">
         <v>367</v>
       </c>
-      <c t="s" s="11" r="C105">
+      <c t="s" s="3" r="D105">
         <v>368</v>
       </c>
-      <c t="s" s="3" r="D105">
+      <c t="s" s="3" r="E105">
         <v>369</v>
-      </c>
-      <c t="s" s="3" r="E105">
-        <v>370</v>
       </c>
     </row>
     <row r="106">
       <c s="13" r="A106"/>
       <c t="s" s="11" r="B106">
+        <v>370</v>
+      </c>
+      <c t="s" s="11" r="C106">
         <v>371</v>
       </c>
-      <c t="s" s="11" r="C106">
+      <c t="s" s="3" r="D106">
         <v>372</v>
       </c>
-      <c t="s" s="3" r="D106">
+      <c t="s" s="3" r="E106">
         <v>373</v>
-      </c>
-      <c t="s" s="3" r="E106">
-        <v>374</v>
       </c>
     </row>
     <row r="107">
       <c s="13" r="A107"/>
       <c t="s" s="11" r="B107">
+        <v>374</v>
+      </c>
+      <c t="s" s="11" r="C107">
         <v>375</v>
       </c>
-      <c t="s" s="11" r="C107">
+      <c t="s" s="3" r="D107">
         <v>376</v>
       </c>
-      <c t="s" s="3" r="D107">
+      <c t="s" s="3" r="E107">
         <v>377</v>
-      </c>
-      <c t="s" s="3" r="E107">
-        <v>378</v>
       </c>
     </row>
     <row r="108">
       <c s="13" r="A108"/>
       <c t="s" s="11" r="B108">
+        <v>378</v>
+      </c>
+      <c t="s" s="11" r="C108">
         <v>379</v>
       </c>
-      <c t="s" s="11" r="C108">
+      <c t="s" s="3" r="D108">
         <v>380</v>
       </c>
-      <c t="s" s="3" r="D108">
+      <c t="s" s="3" r="E108">
         <v>381</v>
-      </c>
-      <c t="s" s="3" r="E108">
-        <v>382</v>
       </c>
     </row>
     <row r="109">
       <c s="13" r="A109"/>
       <c t="s" s="11" r="B109">
+        <v>382</v>
+      </c>
+      <c t="s" s="11" r="C109">
         <v>383</v>
       </c>
-      <c t="s" s="11" r="C109">
+      <c t="s" s="3" r="D109">
         <v>384</v>
       </c>
-      <c t="s" s="3" r="D109">
+      <c t="s" s="3" r="E109">
         <v>385</v>
-      </c>
-      <c t="s" s="3" r="E109">
-        <v>386</v>
       </c>
     </row>
     <row r="110">
       <c s="13" r="A110"/>
       <c t="s" s="11" r="B110">
+        <v>386</v>
+      </c>
+      <c t="s" s="8" r="C110">
         <v>387</v>
       </c>
-      <c t="s" s="8" r="C110">
+      <c t="s" s="3" r="D110">
         <v>388</v>
       </c>
-      <c t="s" s="3" r="D110">
+      <c t="s" s="3" r="E110">
         <v>389</v>
-      </c>
-      <c t="s" s="3" r="E110">
-        <v>390</v>
       </c>
     </row>
     <row r="111">
       <c s="13" r="A111"/>
       <c t="s" s="8" r="B111">
+        <v>390</v>
+      </c>
+      <c t="s" s="8" r="C111">
         <v>391</v>
       </c>
-      <c t="s" s="8" r="C111">
+      <c t="s" s="3" r="D111">
         <v>392</v>
       </c>
-      <c t="s" s="3" r="D111">
+      <c t="s" s="3" r="E111">
         <v>393</v>
-      </c>
-      <c t="s" s="3" r="E111">
-        <v>394</v>
       </c>
     </row>
     <row r="112">
       <c s="13" r="A112"/>
       <c t="s" s="11" r="B112">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c t="s" s="8" r="C112">
+        <v>391</v>
+      </c>
+      <c t="s" s="3" r="D112">
         <v>392</v>
       </c>
-      <c t="s" s="3" r="D112">
+      <c t="s" s="3" r="E112">
         <v>393</v>
-      </c>
-      <c t="s" s="3" r="E112">
-        <v>394</v>
       </c>
     </row>
     <row r="113">
       <c s="13" r="A113"/>
       <c t="s" s="11" r="B113">
+        <v>395</v>
+      </c>
+      <c t="s" s="1" r="C113">
         <v>396</v>
       </c>
-      <c t="s" s="1" r="C113">
+      <c t="s" s="3" r="D113">
         <v>397</v>
       </c>
-      <c t="s" s="3" r="D113">
+      <c t="s" s="3" r="E113">
         <v>398</v>
-      </c>
-      <c t="s" s="3" r="E113">
-        <v>399</v>
       </c>
     </row>
     <row r="114">
       <c s="13" r="A114"/>
       <c t="s" s="11" r="B114">
+        <v>399</v>
+      </c>
+      <c t="s" s="1" r="C114">
         <v>400</v>
       </c>
-      <c t="s" s="1" r="C114">
+      <c t="s" s="3" r="D114">
         <v>401</v>
       </c>
-      <c t="s" s="3" r="D114">
+      <c t="s" s="3" r="E114">
         <v>402</v>
-      </c>
-      <c t="s" s="3" r="E114">
-        <v>403</v>
       </c>
     </row>
     <row r="115">
       <c s="13" r="A115"/>
       <c t="s" s="11" r="B115">
+        <v>403</v>
+      </c>
+      <c t="s" s="1" r="C115">
         <v>404</v>
       </c>
-      <c t="s" s="1" r="C115">
+      <c t="s" s="3" r="D115">
         <v>405</v>
       </c>
-      <c t="s" s="3" r="D115">
+      <c t="s" s="1" r="E115">
         <v>406</v>
-      </c>
-      <c t="s" s="1" r="E115">
-        <v>407</v>
       </c>
     </row>
     <row r="116">
@@ -3523,34 +3509,34 @@
     </row>
     <row r="117">
       <c t="s" s="13" r="A117">
+        <v>407</v>
+      </c>
+      <c t="s" s="11" r="B117">
         <v>408</v>
       </c>
-      <c t="s" s="11" r="B117">
+      <c t="s" s="8" r="C117">
         <v>409</v>
       </c>
-      <c t="s" s="8" r="C117">
+      <c t="s" s="3" r="D117">
         <v>410</v>
       </c>
-      <c t="s" s="3" r="D117">
+      <c t="s" s="3" r="E117">
         <v>411</v>
-      </c>
-      <c t="s" s="3" r="E117">
-        <v>412</v>
       </c>
     </row>
     <row r="118">
       <c s="13" r="A118"/>
       <c t="s" s="11" r="B118">
+        <v>412</v>
+      </c>
+      <c t="s" s="8" r="C118">
         <v>413</v>
       </c>
-      <c t="s" s="8" r="C118">
+      <c t="s" s="3" r="D118">
         <v>414</v>
       </c>
-      <c t="s" s="3" r="D118">
+      <c t="s" s="3" r="E118">
         <v>415</v>
-      </c>
-      <c t="s" s="3" r="E118">
-        <v>416</v>
       </c>
     </row>
     <row r="119">
@@ -3562,79 +3548,79 @@
     </row>
     <row r="120">
       <c t="s" s="13" r="A120">
+        <v>416</v>
+      </c>
+      <c t="s" s="11" r="B120">
         <v>417</v>
       </c>
-      <c t="s" s="11" r="B120">
+      <c t="s" s="8" r="C120">
         <v>418</v>
       </c>
-      <c t="s" s="8" r="C120">
+      <c t="s" s="3" r="D120">
         <v>419</v>
       </c>
-      <c t="s" s="3" r="D120">
+      <c t="s" s="3" r="E120">
         <v>420</v>
-      </c>
-      <c t="s" s="3" r="E120">
-        <v>421</v>
       </c>
     </row>
     <row r="121">
       <c s="13" r="A121"/>
       <c t="s" s="11" r="B121">
+        <v>421</v>
+      </c>
+      <c t="s" s="8" r="C121">
         <v>422</v>
       </c>
-      <c t="s" s="8" r="C121">
+      <c t="s" s="3" r="D121">
         <v>423</v>
       </c>
-      <c t="s" s="3" r="D121">
+      <c t="s" s="3" r="E121">
         <v>424</v>
-      </c>
-      <c t="s" s="3" r="E121">
-        <v>425</v>
       </c>
     </row>
     <row r="122">
       <c s="13" r="A122"/>
       <c t="s" s="11" r="B122">
+        <v>425</v>
+      </c>
+      <c t="s" s="8" r="C122">
         <v>426</v>
       </c>
-      <c t="s" s="8" r="C122">
+      <c t="s" s="3" r="D122">
         <v>427</v>
       </c>
-      <c t="s" s="3" r="D122">
+      <c t="s" s="3" r="E122">
         <v>428</v>
-      </c>
-      <c t="s" s="3" r="E122">
-        <v>429</v>
       </c>
     </row>
     <row r="123">
       <c s="13" r="A123"/>
       <c t="s" s="11" r="B123">
+        <v>429</v>
+      </c>
+      <c t="s" s="8" r="C123">
         <v>430</v>
       </c>
-      <c t="s" s="8" r="C123">
+      <c t="s" s="3" r="D123">
         <v>431</v>
       </c>
-      <c t="s" s="3" r="D123">
+      <c t="s" s="3" r="E123">
         <v>432</v>
-      </c>
-      <c t="s" s="3" r="E123">
-        <v>433</v>
       </c>
     </row>
     <row r="124">
       <c s="13" r="A124"/>
       <c t="s" s="11" r="B124">
+        <v>433</v>
+      </c>
+      <c t="s" s="8" r="C124">
         <v>434</v>
       </c>
-      <c t="s" s="8" r="C124">
+      <c t="s" s="3" r="D124">
         <v>435</v>
       </c>
-      <c t="s" s="3" r="D124">
+      <c t="s" s="3" r="E124">
         <v>436</v>
-      </c>
-      <c t="s" s="3" r="E124">
-        <v>437</v>
       </c>
     </row>
     <row r="125">
@@ -3646,13 +3632,13 @@
     </row>
     <row r="126">
       <c t="s" s="13" r="A126">
+        <v>437</v>
+      </c>
+      <c t="s" s="28" r="B126">
         <v>438</v>
       </c>
-      <c t="s" s="28" r="B126">
-        <v>439</v>
-      </c>
       <c t="s" s="16" r="C126">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c s="24" r="D126"/>
       <c s="24" r="E126"/>
@@ -3666,13 +3652,13 @@
     </row>
     <row r="128">
       <c t="s" s="13" r="A128">
+        <v>439</v>
+      </c>
+      <c t="s" s="22" r="B128">
         <v>440</v>
       </c>
-      <c t="s" s="22" r="B128">
+      <c t="s" s="26" r="C128">
         <v>441</v>
-      </c>
-      <c t="s" s="26" r="C128">
-        <v>442</v>
       </c>
       <c s="30" r="D128"/>
       <c s="30" r="E128"/>
@@ -3680,10 +3666,10 @@
     <row r="129">
       <c s="13" r="A129"/>
       <c t="s" s="22" r="B129">
+        <v>442</v>
+      </c>
+      <c t="s" s="26" r="C129">
         <v>443</v>
-      </c>
-      <c t="s" s="26" r="C129">
-        <v>444</v>
       </c>
       <c s="30" r="D129"/>
       <c s="30" r="E129"/>

</xml_diff>

<commit_message>
EWD-22149 - Create/Update/Delete Question - Remove -> Delete tooltip
Former-commit-id: 0f59762dc14289f5fdf1cb3dc9f668721c3bbd9f
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="451">
   <si>
     <t>Page</t>
   </si>
@@ -259,6 +259,15 @@
   </si>
   <si>
     <t>Not built</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>Löschen</t>
   </si>
   <si>
     <t>Objectives</t>
@@ -2201,371 +2210,375 @@
       <c s="17" r="E22"/>
     </row>
     <row r="23">
-      <c s="5" r="A23"/>
-      <c s="5" r="B23"/>
-      <c s="5" r="C23"/>
-      <c s="15" r="D23"/>
-      <c s="15" r="E23"/>
+      <c s="27" r="A23"/>
+      <c t="s" s="11" r="B23">
+        <v>82</v>
+      </c>
+      <c t="s" s="11" r="C23">
+        <v>83</v>
+      </c>
+      <c t="s" s="3" r="D23">
+        <v>48</v>
+      </c>
+      <c t="s" s="3" r="E23">
+        <v>84</v>
+      </c>
     </row>
     <row r="24">
-      <c t="s" s="5" r="A24">
-        <v>82</v>
-      </c>
-      <c t="s" s="11" r="B24">
-        <v>83</v>
-      </c>
-      <c t="s" s="11" r="C24">
-        <v>84</v>
-      </c>
-      <c t="s" s="3" r="D24">
+      <c s="5" r="A24"/>
+      <c s="5" r="B24"/>
+      <c s="5" r="C24"/>
+      <c s="15" r="D24"/>
+      <c s="15" r="E24"/>
+    </row>
+    <row r="25">
+      <c t="s" s="5" r="A25">
         <v>85</v>
       </c>
-      <c t="s" s="3" r="E24">
+      <c t="s" s="11" r="B25">
         <v>86</v>
       </c>
-    </row>
-    <row r="25">
-      <c s="5" r="A25"/>
-      <c t="s" s="11" r="B25">
+      <c t="s" s="11" r="C25">
         <v>87</v>
       </c>
-      <c t="s" s="11" r="C25">
+      <c t="s" s="3" r="D25">
         <v>88</v>
       </c>
-      <c t="s" s="3" r="D25">
+      <c t="s" s="3" r="E25">
         <v>89</v>
-      </c>
-      <c t="s" s="3" r="E25">
-        <v>90</v>
       </c>
     </row>
     <row r="26">
       <c s="5" r="A26"/>
       <c t="s" s="11" r="B26">
+        <v>90</v>
+      </c>
+      <c t="s" s="11" r="C26">
         <v>91</v>
       </c>
-      <c t="s" s="11" r="C26">
+      <c t="s" s="3" r="D26">
         <v>92</v>
       </c>
-      <c t="s" s="3" r="D26">
+      <c t="s" s="3" r="E26">
         <v>93</v>
-      </c>
-      <c t="s" s="3" r="E26">
-        <v>94</v>
       </c>
     </row>
     <row r="27">
       <c s="5" r="A27"/>
       <c t="s" s="11" r="B27">
+        <v>94</v>
+      </c>
+      <c t="s" s="11" r="C27">
         <v>95</v>
       </c>
-      <c t="s" s="11" r="C27">
+      <c t="s" s="3" r="D27">
         <v>96</v>
       </c>
-      <c t="s" s="3" r="D27">
+      <c t="s" s="3" r="E27">
         <v>97</v>
-      </c>
-      <c t="s" s="3" r="E27">
-        <v>98</v>
       </c>
     </row>
     <row r="28">
       <c s="5" r="A28"/>
       <c t="s" s="11" r="B28">
+        <v>98</v>
+      </c>
+      <c t="s" s="11" r="C28">
         <v>99</v>
       </c>
-      <c t="s" s="11" r="C28">
+      <c t="s" s="3" r="D28">
         <v>100</v>
       </c>
-      <c t="s" s="3" r="D28">
+      <c t="s" s="3" r="E28">
         <v>101</v>
       </c>
-      <c t="s" s="3" r="E28">
+    </row>
+    <row r="29">
+      <c s="5" r="A29"/>
+      <c t="s" s="11" r="B29">
         <v>102</v>
       </c>
-    </row>
-    <row r="29">
-      <c s="27" r="A29"/>
-      <c t="s" s="11" r="B29">
+      <c t="s" s="11" r="C29">
         <v>103</v>
       </c>
-      <c t="s" s="11" r="C29">
+      <c t="s" s="3" r="D29">
         <v>104</v>
       </c>
-      <c t="s" s="3" r="D29">
+      <c t="s" s="3" r="E29">
         <v>105</v>
-      </c>
-      <c t="s" s="3" r="E29">
-        <v>106</v>
       </c>
     </row>
     <row r="30">
       <c s="27" r="A30"/>
-      <c t="s" s="14" r="B30">
+      <c t="s" s="11" r="B30">
+        <v>106</v>
+      </c>
+      <c t="s" s="11" r="C30">
         <v>107</v>
       </c>
-      <c t="s" s="14" r="C30">
+      <c t="s" s="3" r="D30">
         <v>108</v>
       </c>
-      <c s="17" r="D30"/>
-      <c s="17" r="E30"/>
+      <c t="s" s="3" r="E30">
+        <v>109</v>
+      </c>
     </row>
     <row r="31">
       <c s="27" r="A31"/>
-      <c s="27" r="B31"/>
-      <c s="27" r="C31"/>
-      <c s="7" r="D31"/>
-      <c s="7" r="E31"/>
+      <c t="s" s="14" r="B31">
+        <v>110</v>
+      </c>
+      <c t="s" s="14" r="C31">
+        <v>111</v>
+      </c>
+      <c s="17" r="D31"/>
+      <c s="17" r="E31"/>
     </row>
     <row r="32">
-      <c t="s" s="5" r="A32">
-        <v>109</v>
-      </c>
-      <c t="s" s="19" r="B32">
-        <v>110</v>
-      </c>
-      <c t="s" s="19" r="C32">
-        <v>111</v>
-      </c>
-      <c s="9" r="D32"/>
-      <c s="9" r="E32"/>
+      <c s="27" r="A32"/>
+      <c s="27" r="B32"/>
+      <c s="27" r="C32"/>
+      <c s="7" r="D32"/>
+      <c s="7" r="E32"/>
     </row>
     <row r="33">
-      <c s="5" r="A33"/>
-      <c s="5" r="B33"/>
-      <c s="5" r="C33"/>
-      <c s="15" r="D33"/>
-      <c s="7" r="E33"/>
+      <c t="s" s="5" r="A33">
+        <v>112</v>
+      </c>
+      <c t="s" s="19" r="B33">
+        <v>113</v>
+      </c>
+      <c t="s" s="19" r="C33">
+        <v>114</v>
+      </c>
+      <c s="9" r="D33"/>
+      <c s="9" r="E33"/>
     </row>
     <row r="34">
-      <c t="s" s="27" r="A34">
-        <v>112</v>
-      </c>
-      <c t="s" s="11" r="B34">
-        <v>113</v>
-      </c>
-      <c t="s" s="11" r="C34">
-        <v>112</v>
-      </c>
-      <c t="s" s="3" r="D34">
-        <v>114</v>
-      </c>
-      <c t="s" s="3" r="E34">
+      <c s="5" r="A34"/>
+      <c s="5" r="B34"/>
+      <c s="5" r="C34"/>
+      <c s="15" r="D34"/>
+      <c s="7" r="E34"/>
+    </row>
+    <row r="35">
+      <c t="s" s="27" r="A35">
         <v>115</v>
       </c>
-    </row>
-    <row r="35">
-      <c s="27" r="A35"/>
       <c t="s" s="11" r="B35">
         <v>116</v>
       </c>
       <c t="s" s="11" r="C35">
+        <v>115</v>
+      </c>
+      <c t="s" s="3" r="D35">
         <v>117</v>
       </c>
-      <c t="s" s="3" r="D35">
+      <c t="s" s="3" r="E35">
         <v>118</v>
-      </c>
-      <c t="s" s="3" r="E35">
-        <v>119</v>
       </c>
     </row>
     <row r="36">
       <c s="27" r="A36"/>
       <c t="s" s="11" r="B36">
+        <v>119</v>
+      </c>
+      <c t="s" s="11" r="C36">
         <v>120</v>
       </c>
-      <c t="s" s="11" r="C36">
+      <c t="s" s="3" r="D36">
         <v>121</v>
       </c>
-      <c t="s" s="3" r="D36">
+      <c t="s" s="3" r="E36">
         <v>122</v>
-      </c>
-      <c t="s" s="3" r="E36">
-        <v>123</v>
       </c>
     </row>
     <row r="37">
       <c s="27" r="A37"/>
       <c t="s" s="11" r="B37">
+        <v>123</v>
+      </c>
+      <c t="s" s="11" r="C37">
         <v>124</v>
       </c>
-      <c t="s" s="11" r="C37">
+      <c t="s" s="3" r="D37">
         <v>125</v>
       </c>
-      <c t="s" s="3" r="D37">
+      <c t="s" s="3" r="E37">
         <v>126</v>
-      </c>
-      <c t="s" s="3" r="E37">
-        <v>127</v>
       </c>
     </row>
     <row r="38">
       <c s="27" r="A38"/>
       <c t="s" s="11" r="B38">
+        <v>127</v>
+      </c>
+      <c t="s" s="11" r="C38">
         <v>128</v>
       </c>
-      <c t="s" s="11" r="C38">
+      <c t="s" s="3" r="D38">
         <v>129</v>
       </c>
-      <c t="s" s="3" r="D38">
+      <c t="s" s="3" r="E38">
         <v>130</v>
-      </c>
-      <c t="s" s="3" r="E38">
-        <v>131</v>
       </c>
     </row>
     <row r="39">
       <c s="27" r="A39"/>
       <c t="s" s="11" r="B39">
+        <v>131</v>
+      </c>
+      <c t="s" s="11" r="C39">
         <v>132</v>
       </c>
-      <c t="s" s="11" r="C39">
+      <c t="s" s="3" r="D39">
         <v>133</v>
       </c>
-      <c t="s" s="3" r="D39">
+      <c t="s" s="3" r="E39">
         <v>134</v>
-      </c>
-      <c t="s" s="3" r="E39">
-        <v>135</v>
       </c>
     </row>
     <row r="40">
       <c s="27" r="A40"/>
       <c t="s" s="11" r="B40">
+        <v>135</v>
+      </c>
+      <c t="s" s="11" r="C40">
         <v>136</v>
       </c>
-      <c t="s" s="11" r="C40">
+      <c t="s" s="3" r="D40">
         <v>137</v>
       </c>
-      <c t="s" s="3" r="D40">
+      <c t="s" s="3" r="E40">
         <v>138</v>
-      </c>
-      <c t="s" s="3" r="E40">
-        <v>139</v>
       </c>
     </row>
     <row r="41">
       <c s="27" r="A41"/>
       <c t="s" s="11" r="B41">
+        <v>139</v>
+      </c>
+      <c t="s" s="11" r="C41">
         <v>140</v>
       </c>
-      <c t="s" s="11" r="C41">
+      <c t="s" s="3" r="D41">
         <v>141</v>
       </c>
-      <c t="s" s="3" r="D41">
+      <c t="s" s="3" r="E41">
         <v>142</v>
-      </c>
-      <c t="s" s="3" r="E41">
-        <v>143</v>
       </c>
     </row>
     <row r="42">
       <c s="27" r="A42"/>
       <c t="s" s="11" r="B42">
+        <v>143</v>
+      </c>
+      <c t="s" s="11" r="C42">
         <v>144</v>
       </c>
-      <c t="s" s="11" r="C42">
+      <c t="s" s="3" r="D42">
         <v>145</v>
       </c>
-      <c t="s" s="3" r="D42">
+      <c t="s" s="3" r="E42">
         <v>146</v>
-      </c>
-      <c t="s" s="3" r="E42">
-        <v>147</v>
       </c>
     </row>
     <row r="43">
       <c s="27" r="A43"/>
       <c t="s" s="11" r="B43">
+        <v>147</v>
+      </c>
+      <c t="s" s="11" r="C43">
         <v>148</v>
       </c>
-      <c t="s" s="11" r="C43">
+      <c t="s" s="3" r="D43">
         <v>149</v>
       </c>
-      <c t="s" s="3" r="D43">
+      <c t="s" s="3" r="E43">
         <v>150</v>
-      </c>
-      <c t="s" s="3" r="E43">
-        <v>151</v>
       </c>
     </row>
     <row r="44">
       <c s="27" r="A44"/>
       <c t="s" s="11" r="B44">
+        <v>151</v>
+      </c>
+      <c t="s" s="11" r="C44">
         <v>152</v>
       </c>
-      <c t="s" s="11" r="C44">
+      <c t="s" s="3" r="D44">
         <v>153</v>
       </c>
-      <c t="s" s="3" r="D44">
+      <c t="s" s="3" r="E44">
         <v>154</v>
-      </c>
-      <c t="s" s="3" r="E44">
-        <v>155</v>
       </c>
     </row>
     <row r="45">
       <c s="27" r="A45"/>
-      <c s="27" r="B45"/>
-      <c s="27" r="C45"/>
-      <c s="7" r="D45"/>
-      <c s="7" r="E45"/>
+      <c t="s" s="11" r="B45">
+        <v>155</v>
+      </c>
+      <c t="s" s="11" r="C45">
+        <v>156</v>
+      </c>
+      <c t="s" s="3" r="D45">
+        <v>157</v>
+      </c>
+      <c t="s" s="3" r="E45">
+        <v>158</v>
+      </c>
     </row>
     <row r="46">
-      <c t="s" s="27" r="A46">
-        <v>156</v>
-      </c>
-      <c t="s" s="14" r="B46">
-        <v>157</v>
-      </c>
-      <c t="s" s="14" r="C46">
-        <v>158</v>
-      </c>
-      <c s="17" r="D46"/>
-      <c s="17" r="E46"/>
+      <c s="27" r="A46"/>
+      <c s="27" r="B46"/>
+      <c s="27" r="C46"/>
+      <c s="7" r="D46"/>
+      <c s="7" r="E46"/>
     </row>
     <row r="47">
-      <c s="27" r="A47"/>
-      <c t="s" s="11" r="B47">
+      <c t="s" s="27" r="A47">
         <v>159</v>
       </c>
-      <c t="s" s="11" r="C47">
+      <c t="s" s="14" r="B47">
         <v>160</v>
       </c>
-      <c t="s" s="3" r="D47">
+      <c t="s" s="14" r="C47">
         <v>161</v>
       </c>
-      <c t="s" s="3" r="E47">
+      <c s="17" r="D47"/>
+      <c s="17" r="E47"/>
+    </row>
+    <row r="48">
+      <c s="27" r="A48"/>
+      <c t="s" s="11" r="B48">
         <v>162</v>
       </c>
-    </row>
-    <row r="49">
-      <c s="5" r="A49"/>
-      <c s="5" r="B49"/>
-      <c s="5" r="C49"/>
-      <c s="15" r="D49"/>
-      <c s="15" r="E49"/>
+      <c t="s" s="11" r="C48">
+        <v>163</v>
+      </c>
+      <c t="s" s="3" r="D48">
+        <v>164</v>
+      </c>
+      <c t="s" s="3" r="E48">
+        <v>165</v>
+      </c>
     </row>
     <row r="50">
-      <c t="s" s="27" r="A50">
-        <v>163</v>
-      </c>
-      <c t="s" s="28" r="B50">
-        <v>164</v>
-      </c>
-      <c t="s" s="28" r="C50">
-        <v>165</v>
-      </c>
-      <c s="24" r="D50"/>
-      <c s="24" r="E50"/>
+      <c s="5" r="A50"/>
+      <c s="5" r="B50"/>
+      <c s="5" r="C50"/>
+      <c s="15" r="D50"/>
+      <c s="15" r="E50"/>
     </row>
     <row r="51">
-      <c s="27" r="A51"/>
+      <c t="s" s="27" r="A51">
+        <v>166</v>
+      </c>
       <c t="s" s="28" r="B51">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c t="s" s="28" r="C51">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c s="24" r="D51"/>
       <c s="24" r="E51"/>
@@ -2573,10 +2586,10 @@
     <row r="52">
       <c s="27" r="A52"/>
       <c t="s" s="28" r="B52">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c t="s" s="28" r="C52">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c s="24" r="D52"/>
       <c s="24" r="E52"/>
@@ -2584,70 +2597,66 @@
     <row r="53">
       <c s="27" r="A53"/>
       <c t="s" s="28" r="B53">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c t="s" s="28" r="C53">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c s="24" r="D53"/>
       <c s="24" r="E53"/>
     </row>
     <row r="54">
       <c s="27" r="A54"/>
-      <c t="s" s="11" r="B54">
-        <v>172</v>
-      </c>
-      <c t="s" s="11" r="C54">
+      <c t="s" s="28" r="B54">
         <v>173</v>
       </c>
-      <c t="s" s="3" r="D54">
+      <c t="s" s="28" r="C54">
         <v>174</v>
       </c>
-      <c t="s" s="3" r="E54">
-        <v>175</v>
-      </c>
+      <c s="24" r="D54"/>
+      <c s="24" r="E54"/>
     </row>
     <row r="55">
       <c s="27" r="A55"/>
       <c t="s" s="11" r="B55">
+        <v>175</v>
+      </c>
+      <c t="s" s="11" r="C55">
         <v>176</v>
       </c>
-      <c t="s" s="11" r="C55">
+      <c t="s" s="3" r="D55">
         <v>177</v>
       </c>
-      <c t="s" s="3" r="D55">
+      <c t="s" s="3" r="E55">
         <v>178</v>
-      </c>
-      <c t="s" s="3" r="E55">
-        <v>179</v>
       </c>
     </row>
     <row r="56">
       <c s="27" r="A56"/>
-      <c s="27" r="B56"/>
-      <c s="27" r="C56"/>
-      <c s="7" r="D56"/>
-      <c s="7" r="E56"/>
+      <c t="s" s="11" r="B56">
+        <v>179</v>
+      </c>
+      <c t="s" s="11" r="C56">
+        <v>180</v>
+      </c>
+      <c t="s" s="3" r="D56">
+        <v>181</v>
+      </c>
+      <c t="s" s="3" r="E56">
+        <v>182</v>
+      </c>
     </row>
     <row r="57">
-      <c t="s" s="27" r="A57">
-        <v>180</v>
-      </c>
-      <c t="s" s="11" r="B57">
-        <v>181</v>
-      </c>
-      <c t="s" s="11" r="C57">
-        <v>182</v>
-      </c>
-      <c t="s" s="3" r="D57">
+      <c s="27" r="A57"/>
+      <c s="27" r="B57"/>
+      <c s="27" r="C57"/>
+      <c s="7" r="D57"/>
+      <c s="7" r="E57"/>
+    </row>
+    <row r="58">
+      <c t="s" s="27" r="A58">
         <v>183</v>
       </c>
-      <c t="s" s="3" r="E57">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="58">
-      <c s="27" r="A58"/>
       <c t="s" s="11" r="B58">
         <v>184</v>
       </c>
@@ -2658,430 +2667,430 @@
         <v>186</v>
       </c>
       <c t="s" s="3" r="E58">
-        <v>187</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59">
       <c s="27" r="A59"/>
       <c t="s" s="11" r="B59">
+        <v>187</v>
+      </c>
+      <c t="s" s="11" r="C59">
         <v>188</v>
       </c>
-      <c t="s" s="11" r="C59">
+      <c t="s" s="3" r="D59">
         <v>189</v>
       </c>
-      <c t="s" s="3" r="D59">
+      <c t="s" s="3" r="E59">
         <v>190</v>
-      </c>
-      <c t="s" s="3" r="E59">
-        <v>191</v>
       </c>
     </row>
     <row r="60">
       <c s="27" r="A60"/>
       <c t="s" s="11" r="B60">
+        <v>191</v>
+      </c>
+      <c t="s" s="11" r="C60">
         <v>192</v>
       </c>
-      <c t="s" s="11" r="C60">
+      <c t="s" s="3" r="D60">
         <v>193</v>
       </c>
-      <c t="s" s="3" r="D60">
+      <c t="s" s="3" r="E60">
         <v>194</v>
-      </c>
-      <c t="s" s="3" r="E60">
-        <v>195</v>
       </c>
     </row>
     <row r="61">
       <c s="27" r="A61"/>
       <c t="s" s="11" r="B61">
+        <v>195</v>
+      </c>
+      <c t="s" s="11" r="C61">
         <v>196</v>
       </c>
-      <c t="s" s="11" r="C61">
+      <c t="s" s="3" r="D61">
         <v>197</v>
       </c>
-      <c t="s" s="3" r="D61">
+      <c t="s" s="3" r="E61">
         <v>198</v>
-      </c>
-      <c t="s" s="3" r="E61">
-        <v>199</v>
       </c>
     </row>
     <row r="62">
       <c s="27" r="A62"/>
       <c t="s" s="11" r="B62">
+        <v>199</v>
+      </c>
+      <c t="s" s="11" r="C62">
         <v>200</v>
       </c>
-      <c t="s" s="11" r="C62">
+      <c t="s" s="3" r="D62">
         <v>201</v>
       </c>
-      <c t="s" s="3" r="D62">
+      <c t="s" s="3" r="E62">
         <v>202</v>
-      </c>
-      <c t="s" s="3" r="E62">
-        <v>203</v>
       </c>
     </row>
     <row r="63">
       <c s="27" r="A63"/>
       <c t="s" s="11" r="B63">
+        <v>203</v>
+      </c>
+      <c t="s" s="11" r="C63">
         <v>204</v>
       </c>
-      <c t="s" s="11" r="C63">
+      <c t="s" s="3" r="D63">
         <v>205</v>
       </c>
-      <c t="s" s="3" r="D63">
+      <c t="s" s="3" r="E63">
         <v>206</v>
-      </c>
-      <c t="s" s="3" r="E63">
-        <v>207</v>
       </c>
     </row>
     <row r="64">
       <c s="27" r="A64"/>
       <c t="s" s="11" r="B64">
+        <v>207</v>
+      </c>
+      <c t="s" s="11" r="C64">
         <v>208</v>
       </c>
-      <c t="s" s="11" r="C64">
+      <c t="s" s="3" r="D64">
         <v>209</v>
       </c>
-      <c t="s" s="3" r="D64">
+      <c t="s" s="3" r="E64">
         <v>210</v>
-      </c>
-      <c t="s" s="3" r="E64">
-        <v>211</v>
       </c>
     </row>
     <row r="65">
       <c s="27" r="A65"/>
       <c t="s" s="11" r="B65">
+        <v>211</v>
+      </c>
+      <c t="s" s="11" r="C65">
         <v>212</v>
       </c>
-      <c t="s" s="11" r="C65">
+      <c t="s" s="3" r="D65">
         <v>213</v>
       </c>
-      <c t="s" s="3" r="D65">
+      <c t="s" s="3" r="E65">
         <v>214</v>
-      </c>
-      <c t="s" s="3" r="E65">
-        <v>215</v>
       </c>
     </row>
     <row r="66">
       <c s="27" r="A66"/>
-      <c s="27" r="B66"/>
-      <c s="27" r="C66"/>
-      <c s="7" r="D66"/>
-      <c s="7" r="E66"/>
+      <c t="s" s="11" r="B66">
+        <v>215</v>
+      </c>
+      <c t="s" s="11" r="C66">
+        <v>216</v>
+      </c>
+      <c t="s" s="3" r="D66">
+        <v>217</v>
+      </c>
+      <c t="s" s="3" r="E66">
+        <v>218</v>
+      </c>
     </row>
     <row r="67">
-      <c t="s" s="27" r="A67">
-        <v>216</v>
-      </c>
-      <c t="s" s="11" r="B67">
-        <v>217</v>
-      </c>
-      <c t="s" s="11" r="C67">
-        <v>218</v>
-      </c>
-      <c t="s" s="3" r="D67">
+      <c s="27" r="A67"/>
+      <c s="27" r="B67"/>
+      <c s="27" r="C67"/>
+      <c s="7" r="D67"/>
+      <c s="7" r="E67"/>
+    </row>
+    <row r="68">
+      <c t="s" s="27" r="A68">
         <v>219</v>
       </c>
-      <c t="s" s="3" r="E67">
+      <c t="s" s="11" r="B68">
         <v>220</v>
       </c>
-    </row>
-    <row r="68">
-      <c s="27" r="A68"/>
-      <c t="s" s="11" r="B68">
+      <c t="s" s="11" r="C68">
         <v>221</v>
       </c>
-      <c t="s" s="11" r="C68">
+      <c t="s" s="3" r="D68">
         <v>222</v>
       </c>
-      <c t="s" s="3" r="D68">
+      <c t="s" s="3" r="E68">
         <v>223</v>
       </c>
-      <c t="s" s="3" r="E68">
+    </row>
+    <row r="69">
+      <c s="27" r="A69"/>
+      <c t="s" s="11" r="B69">
         <v>224</v>
       </c>
-    </row>
-    <row r="69">
-      <c s="13" r="A69"/>
-      <c t="s" s="11" r="B69">
+      <c t="s" s="11" r="C69">
         <v>225</v>
       </c>
-      <c t="s" s="11" r="C69">
+      <c t="s" s="3" r="D69">
         <v>226</v>
       </c>
-      <c t="s" s="3" r="D69">
+      <c t="s" s="3" r="E69">
         <v>227</v>
-      </c>
-      <c t="s" s="3" r="E69">
-        <v>228</v>
       </c>
     </row>
     <row r="70">
       <c s="13" r="A70"/>
       <c t="s" s="11" r="B70">
+        <v>228</v>
+      </c>
+      <c t="s" s="11" r="C70">
         <v>229</v>
       </c>
-      <c t="s" s="11" r="C70">
+      <c t="s" s="3" r="D70">
         <v>230</v>
       </c>
-      <c t="s" s="3" r="D70">
+      <c t="s" s="3" r="E70">
         <v>231</v>
-      </c>
-      <c t="s" s="3" r="E70">
-        <v>232</v>
       </c>
     </row>
     <row r="71">
       <c s="13" r="A71"/>
       <c t="s" s="11" r="B71">
+        <v>232</v>
+      </c>
+      <c t="s" s="11" r="C71">
         <v>233</v>
       </c>
-      <c t="s" s="11" r="C71">
+      <c t="s" s="3" r="D71">
         <v>234</v>
       </c>
-      <c t="s" s="3" r="D71">
+      <c t="s" s="3" r="E71">
         <v>235</v>
-      </c>
-      <c t="s" s="3" r="E71">
-        <v>236</v>
       </c>
     </row>
     <row r="72">
       <c s="13" r="A72"/>
       <c t="s" s="11" r="B72">
+        <v>236</v>
+      </c>
+      <c t="s" s="11" r="C72">
         <v>237</v>
       </c>
-      <c t="s" s="11" r="C72">
+      <c t="s" s="3" r="D72">
         <v>238</v>
       </c>
-      <c t="s" s="3" r="D72">
+      <c t="s" s="3" r="E72">
         <v>239</v>
-      </c>
-      <c t="s" s="3" r="E72">
-        <v>240</v>
       </c>
     </row>
     <row r="73">
       <c s="13" r="A73"/>
       <c t="s" s="11" r="B73">
+        <v>240</v>
+      </c>
+      <c t="s" s="11" r="C73">
         <v>241</v>
       </c>
-      <c t="s" s="11" r="C73">
+      <c t="s" s="3" r="D73">
         <v>242</v>
       </c>
-      <c t="s" s="3" r="D73">
+      <c t="s" s="3" r="E73">
         <v>243</v>
-      </c>
-      <c t="s" s="3" r="E73">
-        <v>244</v>
       </c>
     </row>
     <row r="74">
       <c s="13" r="A74"/>
       <c t="s" s="11" r="B74">
+        <v>244</v>
+      </c>
+      <c t="s" s="11" r="C74">
         <v>245</v>
       </c>
-      <c t="s" s="11" r="C74">
+      <c t="s" s="3" r="D74">
         <v>246</v>
       </c>
-      <c t="s" s="3" r="D74">
+      <c t="s" s="3" r="E74">
         <v>247</v>
-      </c>
-      <c t="s" s="3" r="E74">
-        <v>248</v>
       </c>
     </row>
     <row r="75">
       <c s="13" r="A75"/>
       <c t="s" s="11" r="B75">
+        <v>248</v>
+      </c>
+      <c t="s" s="11" r="C75">
         <v>249</v>
       </c>
-      <c t="s" s="11" r="C75">
+      <c t="s" s="3" r="D75">
         <v>250</v>
       </c>
-      <c t="s" s="3" r="D75">
+      <c t="s" s="3" r="E75">
         <v>251</v>
-      </c>
-      <c t="s" s="3" r="E75">
-        <v>252</v>
       </c>
     </row>
     <row r="76">
       <c s="13" r="A76"/>
       <c t="s" s="11" r="B76">
+        <v>252</v>
+      </c>
+      <c t="s" s="11" r="C76">
         <v>253</v>
       </c>
-      <c t="s" s="11" r="C76">
+      <c t="s" s="3" r="D76">
         <v>254</v>
       </c>
-      <c t="s" s="3" r="D76">
+      <c t="s" s="3" r="E76">
         <v>255</v>
-      </c>
-      <c t="s" s="3" r="E76">
-        <v>256</v>
       </c>
     </row>
     <row r="77">
       <c s="13" r="A77"/>
       <c t="s" s="11" r="B77">
+        <v>256</v>
+      </c>
+      <c t="s" s="11" r="C77">
         <v>257</v>
       </c>
-      <c t="s" s="11" r="C77">
+      <c t="s" s="3" r="D77">
         <v>258</v>
       </c>
-      <c t="s" s="3" r="D77">
+      <c t="s" s="3" r="E77">
         <v>259</v>
-      </c>
-      <c t="s" s="3" r="E77">
-        <v>260</v>
       </c>
     </row>
     <row r="78">
       <c s="13" r="A78"/>
       <c t="s" s="11" r="B78">
+        <v>260</v>
+      </c>
+      <c t="s" s="11" r="C78">
         <v>261</v>
       </c>
-      <c t="s" s="11" r="C78">
+      <c t="s" s="3" r="D78">
         <v>262</v>
       </c>
-      <c t="s" s="3" r="D78">
+      <c t="s" s="3" r="E78">
         <v>263</v>
-      </c>
-      <c t="s" s="3" r="E78">
-        <v>264</v>
       </c>
     </row>
     <row r="79">
       <c s="13" r="A79"/>
       <c t="s" s="11" r="B79">
+        <v>264</v>
+      </c>
+      <c t="s" s="11" r="C79">
         <v>265</v>
       </c>
-      <c t="s" s="11" r="C79">
+      <c t="s" s="3" r="D79">
         <v>266</v>
       </c>
-      <c t="s" s="3" r="D79">
+      <c t="s" s="3" r="E79">
         <v>267</v>
-      </c>
-      <c t="s" s="3" r="E79">
-        <v>268</v>
       </c>
     </row>
     <row r="80">
       <c s="13" r="A80"/>
       <c t="s" s="11" r="B80">
+        <v>268</v>
+      </c>
+      <c t="s" s="11" r="C80">
         <v>269</v>
       </c>
-      <c t="s" s="11" r="C80">
+      <c t="s" s="3" r="D80">
         <v>270</v>
       </c>
-      <c t="s" s="3" r="D80">
+      <c t="s" s="3" r="E80">
         <v>271</v>
-      </c>
-      <c t="s" s="3" r="E80">
-        <v>272</v>
       </c>
     </row>
     <row r="81">
       <c s="13" r="A81"/>
-      <c s="27" r="B81"/>
-      <c s="27" r="C81"/>
-      <c s="7" r="D81"/>
-      <c s="7" r="E81"/>
+      <c t="s" s="11" r="B81">
+        <v>272</v>
+      </c>
+      <c t="s" s="11" r="C81">
+        <v>273</v>
+      </c>
+      <c t="s" s="3" r="D81">
+        <v>274</v>
+      </c>
+      <c t="s" s="3" r="E81">
+        <v>275</v>
+      </c>
     </row>
     <row r="82">
-      <c t="s" s="13" r="A82">
-        <v>273</v>
-      </c>
-      <c t="s" s="11" r="B82">
-        <v>274</v>
-      </c>
-      <c t="s" s="11" r="C82">
-        <v>275</v>
-      </c>
-      <c t="s" s="3" r="D82">
+      <c s="13" r="A82"/>
+      <c s="27" r="B82"/>
+      <c s="27" r="C82"/>
+      <c s="7" r="D82"/>
+      <c s="7" r="E82"/>
+    </row>
+    <row r="83">
+      <c t="s" s="13" r="A83">
         <v>276</v>
       </c>
-      <c t="s" s="3" r="E82">
+      <c t="s" s="11" r="B83">
         <v>277</v>
       </c>
-    </row>
-    <row r="83">
-      <c s="13" r="A83"/>
-      <c t="s" s="11" r="B83">
+      <c t="s" s="11" r="C83">
         <v>278</v>
       </c>
-      <c t="s" s="11" r="C83">
+      <c t="s" s="3" r="D83">
         <v>279</v>
       </c>
-      <c t="s" s="3" r="D83">
+      <c t="s" s="3" r="E83">
         <v>280</v>
-      </c>
-      <c t="s" s="3" r="E83">
-        <v>281</v>
       </c>
     </row>
     <row r="84">
       <c s="13" r="A84"/>
       <c t="s" s="11" r="B84">
+        <v>281</v>
+      </c>
+      <c t="s" s="11" r="C84">
         <v>282</v>
       </c>
-      <c t="s" s="11" r="C84">
+      <c t="s" s="3" r="D84">
         <v>283</v>
       </c>
-      <c t="s" s="3" r="D84">
+      <c t="s" s="3" r="E84">
         <v>284</v>
-      </c>
-      <c t="s" s="3" r="E84">
-        <v>285</v>
       </c>
     </row>
     <row r="85">
       <c s="13" r="A85"/>
       <c t="s" s="11" r="B85">
+        <v>285</v>
+      </c>
+      <c t="s" s="11" r="C85">
         <v>286</v>
       </c>
-      <c t="s" s="11" r="C85">
+      <c t="s" s="3" r="D85">
         <v>287</v>
       </c>
-      <c t="s" s="3" r="D85">
+      <c t="s" s="3" r="E85">
         <v>288</v>
-      </c>
-      <c t="s" s="3" r="E85">
-        <v>289</v>
       </c>
     </row>
     <row r="86">
       <c s="13" r="A86"/>
       <c t="s" s="11" r="B86">
+        <v>289</v>
+      </c>
+      <c t="s" s="11" r="C86">
         <v>290</v>
       </c>
-      <c t="s" s="11" r="C86">
+      <c t="s" s="3" r="D86">
         <v>291</v>
       </c>
-      <c t="s" s="3" r="D86">
+      <c t="s" s="3" r="E86">
         <v>292</v>
-      </c>
-      <c t="s" s="3" r="E86">
-        <v>293</v>
       </c>
     </row>
     <row r="87">
       <c s="13" r="A87"/>
       <c t="s" s="11" r="B87">
+        <v>293</v>
+      </c>
+      <c t="s" s="11" r="C87">
         <v>294</v>
       </c>
-      <c t="s" s="11" r="C87">
+      <c t="s" s="3" r="D87">
         <v>295</v>
       </c>
-      <c t="s" s="3" r="D87">
+      <c t="s" s="3" r="E87">
         <v>296</v>
-      </c>
-      <c t="s" s="3" r="E87">
-        <v>295</v>
       </c>
     </row>
     <row r="88">
@@ -3096,76 +3105,76 @@
         <v>299</v>
       </c>
       <c t="s" s="3" r="E88">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="89">
       <c s="13" r="A89"/>
       <c t="s" s="11" r="B89">
+        <v>300</v>
+      </c>
+      <c t="s" s="11" r="C89">
         <v>301</v>
       </c>
-      <c t="s" s="11" r="C89">
+      <c t="s" s="3" r="D89">
         <v>302</v>
       </c>
-      <c t="s" s="3" r="D89">
+      <c t="s" s="3" r="E89">
         <v>303</v>
-      </c>
-      <c t="s" s="3" r="E89">
-        <v>304</v>
       </c>
     </row>
     <row r="90">
       <c s="13" r="A90"/>
       <c t="s" s="11" r="B90">
+        <v>304</v>
+      </c>
+      <c t="s" s="11" r="C90">
         <v>305</v>
       </c>
-      <c t="s" s="11" r="C90">
+      <c t="s" s="3" r="D90">
         <v>306</v>
       </c>
-      <c t="s" s="3" r="D90">
+      <c t="s" s="3" r="E90">
         <v>307</v>
-      </c>
-      <c t="s" s="3" r="E90">
-        <v>308</v>
       </c>
     </row>
     <row r="91">
       <c s="13" r="A91"/>
       <c t="s" s="11" r="B91">
+        <v>308</v>
+      </c>
+      <c t="s" s="11" r="C91">
         <v>309</v>
       </c>
-      <c t="s" s="11" r="C91">
+      <c t="s" s="3" r="D91">
         <v>310</v>
       </c>
-      <c t="s" s="3" r="D91">
+      <c t="s" s="3" r="E91">
         <v>311</v>
-      </c>
-      <c t="s" s="3" r="E91">
-        <v>312</v>
       </c>
     </row>
     <row r="92">
       <c s="13" r="A92"/>
       <c t="s" s="11" r="B92">
+        <v>312</v>
+      </c>
+      <c t="s" s="11" r="C92">
         <v>313</v>
       </c>
-      <c t="s" s="11" r="C92">
+      <c t="s" s="3" r="D92">
         <v>314</v>
       </c>
-      <c t="s" s="3" r="D92">
+      <c t="s" s="3" r="E92">
         <v>315</v>
-      </c>
-      <c t="s" s="3" r="E92">
-        <v>316</v>
       </c>
     </row>
     <row r="93">
       <c s="13" r="A93"/>
       <c t="s" s="11" r="B93">
+        <v>316</v>
+      </c>
+      <c t="s" s="11" r="C93">
         <v>317</v>
-      </c>
-      <c t="s" s="11" r="C93">
-        <v>318</v>
       </c>
       <c t="s" s="3" r="D93">
         <v>318</v>
@@ -3198,22 +3207,22 @@
         <v>324</v>
       </c>
       <c t="s" s="3" r="D95">
+        <v>324</v>
+      </c>
+      <c t="s" s="3" r="E95">
         <v>325</v>
-      </c>
-      <c t="s" s="3" r="E95">
-        <v>326</v>
       </c>
     </row>
     <row r="96">
       <c s="13" r="A96"/>
-      <c t="s" s="8" r="B96">
+      <c t="s" s="11" r="B96">
+        <v>326</v>
+      </c>
+      <c t="s" s="11" r="C96">
         <v>327</v>
       </c>
-      <c t="s" s="11" r="C96">
+      <c t="s" s="3" r="D96">
         <v>328</v>
-      </c>
-      <c t="s" s="3" r="D96">
-        <v>329</v>
       </c>
       <c t="s" s="3" r="E96">
         <v>329</v>
@@ -3221,7 +3230,7 @@
     </row>
     <row r="97">
       <c s="13" r="A97"/>
-      <c t="s" s="11" r="B97">
+      <c t="s" s="8" r="B97">
         <v>330</v>
       </c>
       <c t="s" s="11" r="C97">
@@ -3231,489 +3240,497 @@
         <v>332</v>
       </c>
       <c t="s" s="3" r="E97">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="98">
       <c s="13" r="A98"/>
       <c t="s" s="11" r="B98">
+        <v>333</v>
+      </c>
+      <c t="s" s="11" r="C98">
         <v>334</v>
       </c>
-      <c t="s" s="11" r="C98">
+      <c t="s" s="3" r="D98">
         <v>335</v>
       </c>
-      <c t="s" s="3" r="D98">
+      <c t="s" s="3" r="E98">
         <v>336</v>
-      </c>
-      <c t="s" s="3" r="E98">
-        <v>337</v>
       </c>
     </row>
     <row r="99">
       <c s="13" r="A99"/>
       <c t="s" s="11" r="B99">
+        <v>337</v>
+      </c>
+      <c t="s" s="11" r="C99">
         <v>338</v>
       </c>
-      <c t="s" s="11" r="C99">
+      <c t="s" s="3" r="D99">
         <v>339</v>
       </c>
-      <c t="s" s="3" r="D99">
+      <c t="s" s="3" r="E99">
         <v>340</v>
-      </c>
-      <c t="s" s="3" r="E99">
-        <v>341</v>
       </c>
     </row>
     <row r="100">
       <c s="13" r="A100"/>
       <c t="s" s="11" r="B100">
+        <v>341</v>
+      </c>
+      <c t="s" s="11" r="C100">
         <v>342</v>
       </c>
-      <c t="s" s="11" r="C100">
+      <c t="s" s="3" r="D100">
         <v>343</v>
       </c>
-      <c t="s" s="3" r="D100">
+      <c t="s" s="3" r="E100">
         <v>344</v>
-      </c>
-      <c t="s" s="3" r="E100">
-        <v>345</v>
       </c>
     </row>
     <row r="101">
       <c s="13" r="A101"/>
       <c t="s" s="11" r="B101">
+        <v>345</v>
+      </c>
+      <c t="s" s="11" r="C101">
         <v>346</v>
       </c>
-      <c t="s" s="11" r="C101">
+      <c t="s" s="3" r="D101">
         <v>347</v>
       </c>
-      <c t="s" s="3" r="D101">
+      <c t="s" s="3" r="E101">
         <v>348</v>
-      </c>
-      <c t="s" s="3" r="E101">
-        <v>349</v>
       </c>
     </row>
     <row r="102">
       <c s="13" r="A102"/>
       <c t="s" s="11" r="B102">
+        <v>349</v>
+      </c>
+      <c t="s" s="11" r="C102">
         <v>350</v>
       </c>
-      <c t="s" s="11" r="C102">
+      <c t="s" s="3" r="D102">
         <v>351</v>
       </c>
-      <c t="s" s="3" r="D102">
+      <c t="s" s="3" r="E102">
         <v>352</v>
-      </c>
-      <c t="s" s="3" r="E102">
-        <v>353</v>
       </c>
     </row>
     <row r="103">
       <c s="13" r="A103"/>
       <c t="s" s="11" r="B103">
+        <v>353</v>
+      </c>
+      <c t="s" s="11" r="C103">
         <v>354</v>
       </c>
-      <c t="s" s="11" r="C103">
+      <c t="s" s="3" r="D103">
         <v>355</v>
       </c>
-      <c t="s" s="3" r="D103">
+      <c t="s" s="3" r="E103">
         <v>356</v>
-      </c>
-      <c t="s" s="3" r="E103">
-        <v>357</v>
       </c>
     </row>
     <row r="104">
       <c s="13" r="A104"/>
       <c t="s" s="11" r="B104">
+        <v>357</v>
+      </c>
+      <c t="s" s="11" r="C104">
         <v>358</v>
       </c>
-      <c t="s" s="11" r="C104">
+      <c t="s" s="3" r="D104">
         <v>359</v>
       </c>
-      <c t="s" s="3" r="D104">
+      <c t="s" s="3" r="E104">
         <v>360</v>
-      </c>
-      <c t="s" s="3" r="E104">
-        <v>361</v>
       </c>
     </row>
     <row r="105">
       <c s="13" r="A105"/>
       <c t="s" s="11" r="B105">
+        <v>361</v>
+      </c>
+      <c t="s" s="11" r="C105">
         <v>362</v>
       </c>
-      <c t="s" s="11" r="C105">
+      <c t="s" s="3" r="D105">
         <v>363</v>
       </c>
-      <c t="s" s="3" r="D105">
+      <c t="s" s="3" r="E105">
         <v>364</v>
-      </c>
-      <c t="s" s="3" r="E105">
-        <v>365</v>
       </c>
     </row>
     <row r="106">
       <c s="13" r="A106"/>
       <c t="s" s="11" r="B106">
+        <v>365</v>
+      </c>
+      <c t="s" s="11" r="C106">
         <v>366</v>
       </c>
-      <c t="s" s="11" r="C106">
+      <c t="s" s="3" r="D106">
         <v>367</v>
       </c>
-      <c t="s" s="3" r="D106">
+      <c t="s" s="3" r="E106">
         <v>368</v>
-      </c>
-      <c t="s" s="3" r="E106">
-        <v>369</v>
       </c>
     </row>
     <row r="107">
       <c s="13" r="A107"/>
       <c t="s" s="11" r="B107">
+        <v>369</v>
+      </c>
+      <c t="s" s="11" r="C107">
         <v>370</v>
       </c>
-      <c t="s" s="11" r="C107">
+      <c t="s" s="3" r="D107">
         <v>371</v>
       </c>
-      <c t="s" s="3" r="D107">
+      <c t="s" s="3" r="E107">
         <v>372</v>
-      </c>
-      <c t="s" s="3" r="E107">
-        <v>373</v>
       </c>
     </row>
     <row r="108">
       <c s="13" r="A108"/>
       <c t="s" s="11" r="B108">
+        <v>373</v>
+      </c>
+      <c t="s" s="11" r="C108">
         <v>374</v>
       </c>
-      <c t="s" s="11" r="C108">
+      <c t="s" s="3" r="D108">
         <v>375</v>
       </c>
-      <c t="s" s="3" r="D108">
+      <c t="s" s="3" r="E108">
         <v>376</v>
-      </c>
-      <c t="s" s="3" r="E108">
-        <v>377</v>
       </c>
     </row>
     <row r="109">
       <c s="13" r="A109"/>
       <c t="s" s="11" r="B109">
+        <v>377</v>
+      </c>
+      <c t="s" s="11" r="C109">
         <v>378</v>
       </c>
-      <c t="s" s="11" r="C109">
+      <c t="s" s="3" r="D109">
         <v>379</v>
       </c>
-      <c t="s" s="3" r="D109">
+      <c t="s" s="3" r="E109">
         <v>380</v>
-      </c>
-      <c t="s" s="3" r="E109">
-        <v>381</v>
       </c>
     </row>
     <row r="110">
       <c s="13" r="A110"/>
       <c t="s" s="11" r="B110">
+        <v>381</v>
+      </c>
+      <c t="s" s="11" r="C110">
         <v>382</v>
       </c>
-      <c t="s" s="11" r="C110">
+      <c t="s" s="3" r="D110">
         <v>383</v>
       </c>
-      <c t="s" s="3" r="D110">
+      <c t="s" s="3" r="E110">
         <v>384</v>
-      </c>
-      <c t="s" s="3" r="E110">
-        <v>385</v>
       </c>
     </row>
     <row r="111">
       <c s="13" r="A111"/>
       <c t="s" s="11" r="B111">
+        <v>385</v>
+      </c>
+      <c t="s" s="11" r="C111">
         <v>386</v>
       </c>
-      <c t="s" s="11" r="C111">
+      <c t="s" s="3" r="D111">
         <v>387</v>
       </c>
-      <c t="s" s="3" r="D111">
+      <c t="s" s="3" r="E111">
         <v>388</v>
-      </c>
-      <c t="s" s="3" r="E111">
-        <v>389</v>
       </c>
     </row>
     <row r="112">
       <c s="13" r="A112"/>
       <c t="s" s="11" r="B112">
+        <v>389</v>
+      </c>
+      <c t="s" s="11" r="C112">
         <v>390</v>
       </c>
-      <c t="s" s="8" r="C112">
+      <c t="s" s="3" r="D112">
         <v>391</v>
       </c>
-      <c t="s" s="3" r="D112">
+      <c t="s" s="3" r="E112">
         <v>392</v>
-      </c>
-      <c t="s" s="3" r="E112">
-        <v>393</v>
       </c>
     </row>
     <row r="113">
       <c s="13" r="A113"/>
-      <c t="s" s="8" r="B113">
+      <c t="s" s="11" r="B113">
+        <v>393</v>
+      </c>
+      <c t="s" s="8" r="C113">
         <v>394</v>
       </c>
-      <c t="s" s="8" r="C113">
+      <c t="s" s="3" r="D113">
         <v>395</v>
       </c>
-      <c t="s" s="3" r="D113">
+      <c t="s" s="3" r="E113">
         <v>396</v>
-      </c>
-      <c t="s" s="3" r="E113">
-        <v>397</v>
       </c>
     </row>
     <row r="114">
       <c s="13" r="A114"/>
-      <c t="s" s="11" r="B114">
+      <c t="s" s="8" r="B114">
+        <v>397</v>
+      </c>
+      <c t="s" s="8" r="C114">
         <v>398</v>
       </c>
-      <c t="s" s="8" r="C114">
-        <v>395</v>
-      </c>
       <c t="s" s="3" r="D114">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c t="s" s="3" r="E114">
-        <v>397</v>
+        <v>400</v>
       </c>
     </row>
     <row r="115">
       <c s="13" r="A115"/>
       <c t="s" s="11" r="B115">
+        <v>401</v>
+      </c>
+      <c t="s" s="8" r="C115">
+        <v>398</v>
+      </c>
+      <c t="s" s="3" r="D115">
         <v>399</v>
       </c>
-      <c t="s" s="1" r="C115">
+      <c t="s" s="3" r="E115">
         <v>400</v>
-      </c>
-      <c t="s" s="3" r="D115">
-        <v>401</v>
-      </c>
-      <c t="s" s="3" r="E115">
-        <v>402</v>
       </c>
     </row>
     <row r="116">
       <c s="13" r="A116"/>
       <c t="s" s="11" r="B116">
+        <v>402</v>
+      </c>
+      <c t="s" s="1" r="C116">
         <v>403</v>
       </c>
-      <c t="s" s="1" r="C116">
+      <c t="s" s="3" r="D116">
         <v>404</v>
       </c>
-      <c t="s" s="3" r="D116">
+      <c t="s" s="3" r="E116">
         <v>405</v>
-      </c>
-      <c t="s" s="3" r="E116">
-        <v>406</v>
       </c>
     </row>
     <row r="117">
       <c s="13" r="A117"/>
       <c t="s" s="11" r="B117">
+        <v>406</v>
+      </c>
+      <c t="s" s="1" r="C117">
         <v>407</v>
       </c>
-      <c t="s" s="1" r="C117">
+      <c t="s" s="3" r="D117">
         <v>408</v>
       </c>
-      <c t="s" s="3" r="D117">
+      <c t="s" s="3" r="E117">
         <v>409</v>
-      </c>
-      <c t="s" s="1" r="E117">
-        <v>410</v>
       </c>
     </row>
     <row r="118">
       <c s="13" r="A118"/>
-      <c s="12" r="B118"/>
-      <c s="6" r="C118"/>
-      <c s="10" r="D118"/>
-      <c s="10" r="E118"/>
+      <c t="s" s="11" r="B118">
+        <v>410</v>
+      </c>
+      <c t="s" s="1" r="C118">
+        <v>411</v>
+      </c>
+      <c t="s" s="3" r="D118">
+        <v>412</v>
+      </c>
+      <c t="s" s="1" r="E118">
+        <v>413</v>
+      </c>
     </row>
     <row r="119">
-      <c t="s" s="13" r="A119">
-        <v>411</v>
-      </c>
-      <c t="s" s="11" r="B119">
-        <v>412</v>
-      </c>
-      <c t="s" s="8" r="C119">
-        <v>413</v>
-      </c>
-      <c t="s" s="3" r="D119">
+      <c s="13" r="A119"/>
+      <c s="12" r="B119"/>
+      <c s="6" r="C119"/>
+      <c s="10" r="D119"/>
+      <c s="10" r="E119"/>
+    </row>
+    <row r="120">
+      <c t="s" s="13" r="A120">
         <v>414</v>
       </c>
-      <c t="s" s="3" r="E119">
+      <c t="s" s="11" r="B120">
         <v>415</v>
       </c>
-    </row>
-    <row r="120">
-      <c s="13" r="A120"/>
-      <c t="s" s="11" r="B120">
+      <c t="s" s="8" r="C120">
         <v>416</v>
       </c>
-      <c t="s" s="8" r="C120">
+      <c t="s" s="3" r="D120">
         <v>417</v>
       </c>
-      <c t="s" s="3" r="D120">
+      <c t="s" s="3" r="E120">
         <v>418</v>
       </c>
-      <c t="s" s="3" r="E120">
+    </row>
+    <row r="121">
+      <c s="13" r="A121"/>
+      <c t="s" s="11" r="B121">
         <v>419</v>
       </c>
-    </row>
-    <row r="121">
-      <c s="20" r="A121"/>
-      <c s="5" r="B121"/>
-      <c s="25" r="C121"/>
-      <c s="15" r="D121"/>
-      <c s="15" r="E121"/>
+      <c t="s" s="8" r="C121">
+        <v>420</v>
+      </c>
+      <c t="s" s="3" r="D121">
+        <v>421</v>
+      </c>
+      <c t="s" s="3" r="E121">
+        <v>422</v>
+      </c>
     </row>
     <row r="122">
-      <c t="s" s="13" r="A122">
-        <v>420</v>
-      </c>
-      <c t="s" s="11" r="B122">
-        <v>421</v>
-      </c>
-      <c t="s" s="8" r="C122">
-        <v>422</v>
-      </c>
-      <c t="s" s="3" r="D122">
+      <c s="20" r="A122"/>
+      <c s="5" r="B122"/>
+      <c s="25" r="C122"/>
+      <c s="15" r="D122"/>
+      <c s="15" r="E122"/>
+    </row>
+    <row r="123">
+      <c t="s" s="13" r="A123">
         <v>423</v>
       </c>
-      <c t="s" s="3" r="E122">
+      <c t="s" s="11" r="B123">
         <v>424</v>
       </c>
-    </row>
-    <row r="123">
-      <c s="13" r="A123"/>
-      <c t="s" s="11" r="B123">
+      <c t="s" s="8" r="C123">
         <v>425</v>
       </c>
-      <c t="s" s="8" r="C123">
+      <c t="s" s="3" r="D123">
         <v>426</v>
       </c>
-      <c t="s" s="3" r="D123">
+      <c t="s" s="3" r="E123">
         <v>427</v>
-      </c>
-      <c t="s" s="3" r="E123">
-        <v>428</v>
       </c>
     </row>
     <row r="124">
       <c s="13" r="A124"/>
       <c t="s" s="11" r="B124">
+        <v>428</v>
+      </c>
+      <c t="s" s="8" r="C124">
         <v>429</v>
       </c>
-      <c t="s" s="8" r="C124">
+      <c t="s" s="3" r="D124">
         <v>430</v>
       </c>
-      <c t="s" s="3" r="D124">
+      <c t="s" s="3" r="E124">
         <v>431</v>
-      </c>
-      <c t="s" s="3" r="E124">
-        <v>432</v>
       </c>
     </row>
     <row r="125">
       <c s="13" r="A125"/>
       <c t="s" s="11" r="B125">
+        <v>432</v>
+      </c>
+      <c t="s" s="8" r="C125">
         <v>433</v>
       </c>
-      <c t="s" s="8" r="C125">
+      <c t="s" s="3" r="D125">
         <v>434</v>
       </c>
-      <c t="s" s="3" r="D125">
+      <c t="s" s="3" r="E125">
         <v>435</v>
-      </c>
-      <c t="s" s="3" r="E125">
-        <v>436</v>
       </c>
     </row>
     <row r="126">
       <c s="13" r="A126"/>
       <c t="s" s="11" r="B126">
+        <v>436</v>
+      </c>
+      <c t="s" s="8" r="C126">
         <v>437</v>
       </c>
-      <c t="s" s="8" r="C126">
+      <c t="s" s="3" r="D126">
         <v>438</v>
       </c>
-      <c t="s" s="3" r="D126">
+      <c t="s" s="3" r="E126">
         <v>439</v>
-      </c>
-      <c t="s" s="3" r="E126">
-        <v>440</v>
       </c>
     </row>
     <row r="127">
       <c s="13" r="A127"/>
-      <c s="5" r="B127"/>
-      <c s="25" r="C127"/>
-      <c s="15" r="D127"/>
-      <c s="15" r="E127"/>
+      <c t="s" s="11" r="B127">
+        <v>440</v>
+      </c>
+      <c t="s" s="8" r="C127">
+        <v>441</v>
+      </c>
+      <c t="s" s="3" r="D127">
+        <v>442</v>
+      </c>
+      <c t="s" s="3" r="E127">
+        <v>443</v>
+      </c>
     </row>
     <row r="128">
-      <c t="s" s="13" r="A128">
-        <v>441</v>
-      </c>
-      <c t="s" s="28" r="B128">
-        <v>442</v>
-      </c>
-      <c t="s" s="16" r="C128">
-        <v>441</v>
-      </c>
-      <c s="24" r="D128"/>
-      <c s="24" r="E128"/>
+      <c s="13" r="A128"/>
+      <c s="5" r="B128"/>
+      <c s="25" r="C128"/>
+      <c s="15" r="D128"/>
+      <c s="15" r="E128"/>
     </row>
     <row r="129">
-      <c s="13" r="A129"/>
-      <c s="12" r="B129"/>
-      <c s="6" r="C129"/>
-      <c s="10" r="D129"/>
-      <c s="10" r="E129"/>
+      <c t="s" s="13" r="A129">
+        <v>444</v>
+      </c>
+      <c t="s" s="28" r="B129">
+        <v>445</v>
+      </c>
+      <c t="s" s="16" r="C129">
+        <v>444</v>
+      </c>
+      <c s="24" r="D129"/>
+      <c s="24" r="E129"/>
     </row>
     <row r="130">
-      <c t="s" s="13" r="A130">
-        <v>443</v>
-      </c>
-      <c t="s" s="22" r="B130">
-        <v>444</v>
-      </c>
-      <c t="s" s="26" r="C130">
-        <v>445</v>
-      </c>
-      <c s="30" r="D130"/>
-      <c s="30" r="E130"/>
+      <c s="13" r="A130"/>
+      <c s="12" r="B130"/>
+      <c s="6" r="C130"/>
+      <c s="10" r="D130"/>
+      <c s="10" r="E130"/>
     </row>
     <row r="131">
-      <c s="13" r="A131"/>
+      <c t="s" s="13" r="A131">
+        <v>446</v>
+      </c>
       <c t="s" s="22" r="B131">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c t="s" s="26" r="C131">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c s="30" r="D131"/>
       <c s="30" r="E131"/>
     </row>
     <row r="132">
       <c s="13" r="A132"/>
-      <c s="12" r="B132"/>
-      <c s="6" r="C132"/>
-      <c s="10" r="D132"/>
-      <c s="10" r="E132"/>
+      <c t="s" s="22" r="B132">
+        <v>449</v>
+      </c>
+      <c t="s" s="26" r="C132">
+        <v>450</v>
+      </c>
+      <c s="30" r="D132"/>
+      <c s="30" r="E132"/>
     </row>
     <row r="133">
       <c s="13" r="A133"/>
@@ -3728,6 +3745,13 @@
       <c s="6" r="C134"/>
       <c s="10" r="D134"/>
       <c s="10" r="E134"/>
+    </row>
+    <row r="135">
+      <c s="13" r="A135"/>
+      <c s="12" r="B135"/>
+      <c s="6" r="C135"/>
+      <c s="10" r="D135"/>
+      <c s="10" r="E135"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
EWD-22437 - CK editor localization Update resources
Former-commit-id: 7a8500d2ddffe8776cb5244ca3fc8d98b5be4633
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="463">
   <si>
     <t>Page</t>
   </si>
@@ -234,33 +234,33 @@
     <t>Aangemaakt op</t>
   </si>
   <si>
+    <t>Erstellt am</t>
+  </si>
+  <si>
+    <t>modifiedOn</t>
+  </si>
+  <si>
+    <t>Modified on</t>
+  </si>
+  <si>
+    <t>Gewijzigd op</t>
+  </si>
+  <si>
+    <t>Geändert am</t>
+  </si>
+  <si>
+    <t>builtOn</t>
+  </si>
+  <si>
+    <t>Built on</t>
+  </si>
+  <si>
+    <t>Samengesteld op</t>
+  </si>
+  <si>
     <t>Zusammengestellt am</t>
   </si>
   <si>
-    <t>modifiedOn</t>
-  </si>
-  <si>
-    <t>Modified on</t>
-  </si>
-  <si>
-    <t>Gewijzigd op</t>
-  </si>
-  <si>
-    <t>Geändert am</t>
-  </si>
-  <si>
-    <t>builtOn</t>
-  </si>
-  <si>
-    <t>Built on</t>
-  </si>
-  <si>
-    <t>Samengesteld op</t>
-  </si>
-  <si>
-    <t>Erstellt am</t>
-  </si>
-  <si>
     <t>notBuilt</t>
   </si>
   <si>
@@ -586,6 +586,12 @@
   </si>
   <si>
     <t>Klicken, um Umgebung hinzuzufügen</t>
+  </si>
+  <si>
+    <t>createNewExperience</t>
+  </si>
+  <si>
+    <t>Create New Experience</t>
   </si>
   <si>
     <t>Question</t>
@@ -1307,6 +1313,12 @@
   </si>
   <si>
     <t>Erfahrung aufbauen</t>
+  </si>
+  <si>
+    <t>noRelatedLearningObjectives</t>
+  </si>
+  <si>
+    <t>No related learning objectives</t>
   </si>
   <si>
     <t>Error pages</t>
@@ -1397,7 +1409,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -1418,6 +1430,15 @@
     </font>
     <font>
       <b/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
@@ -1543,7 +1564,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1561,6 +1582,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1649,7 +1682,7 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
@@ -1662,51 +1695,60 @@
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="2">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="3" applyFill="1">
+    <xf applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="4"/>
-    <xf applyAlignment="1" fillId="5" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="5" applyFill="1">
+    <xf applyAlignment="1" fillId="5" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="3" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="6">
-      <alignment vertical="bottom" horizontal="right"/>
+    <xf applyAlignment="1" fillId="6" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="4" applyFill="1">
+      <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="6" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+    <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="5"/>
+    <xf applyAlignment="1" fillId="7" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="6" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="7">
-      <alignment vertical="center" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" fillId="7" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="8" applyFill="1">
-      <alignment vertical="center" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="9">
-      <alignment vertical="center" horizontal="general" wrapText="1"/>
+      <alignment vertical="bottom" horizontal="right"/>
     </xf>
     <xf applyAlignment="1" fillId="8" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="9" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="10" applyFill="1">
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="8">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="10" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="11" applyFill="1">
+    <xf applyAlignment="1" fillId="9" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="9" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="11" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="10">
+      <alignment vertical="center" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="10" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+      <alignment vertical="center" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="11" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="11" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="12" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="12" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="13" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="13" applyFill="1">
+    <xf applyAlignment="1" fillId="13" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="14" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+    <xf applyAlignment="1" fillId="14" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="13" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="14"/>
-    <xf applyAlignment="1" fillId="15" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="15" applyFill="1">
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
+      <alignment vertical="center" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="15" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="14" applyFill="1">
+      <alignment vertical="center" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="16" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+      <alignment vertical="center" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="15"/>
+    <xf applyAlignment="1" fillId="17" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="16" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1733,17 +1775,17 @@
     <col min="5" customWidth="1" max="5" width="39.43"/>
   </cols>
   <sheetData>
-    <row s="5" customFormat="1" r="1">
-      <c t="s" s="10" r="A1">
+    <row s="7" customFormat="1" r="1">
+      <c t="s" s="12" r="A1">
         <v>0</v>
       </c>
-      <c t="s" s="10" r="B1">
+      <c t="s" s="12" r="B1">
         <v>1</v>
       </c>
-      <c t="s" s="10" r="C1">
+      <c t="s" s="12" r="C1">
         <v>2</v>
       </c>
-      <c t="s" s="10" r="D1">
+      <c t="s" s="12" r="D1">
         <v>3</v>
       </c>
       <c t="s" s="3" r="E1">
@@ -1754,331 +1796,331 @@
       <c t="s" s="2" r="A2">
         <v>5</v>
       </c>
-      <c t="s" s="6" r="B2">
+      <c t="s" s="8" r="B2">
         <v>6</v>
       </c>
-      <c t="s" s="6" r="C2">
+      <c t="s" s="8" r="C2">
         <v>7</v>
       </c>
-      <c t="s" s="6" r="D2">
+      <c t="s" s="8" r="D2">
         <v>8</v>
       </c>
-      <c t="s" s="6" r="E2">
+      <c t="s" s="8" r="E2">
         <v>9</v>
       </c>
     </row>
     <row r="3">
       <c s="2" r="A3"/>
-      <c t="s" s="6" r="B3">
+      <c t="s" s="8" r="B3">
         <v>10</v>
       </c>
-      <c t="s" s="6" r="C3">
+      <c t="s" s="8" r="C3">
         <v>11</v>
       </c>
-      <c t="s" s="6" r="D3">
+      <c t="s" s="8" r="D3">
         <v>12</v>
       </c>
-      <c t="s" s="6" r="E3">
+      <c t="s" s="8" r="E3">
         <v>13</v>
       </c>
     </row>
     <row r="4">
       <c s="2" r="A4"/>
-      <c t="s" s="6" r="B4">
+      <c t="s" s="8" r="B4">
         <v>14</v>
       </c>
-      <c t="s" s="6" r="C4">
+      <c t="s" s="8" r="C4">
         <v>15</v>
       </c>
-      <c t="s" s="6" r="D4">
+      <c t="s" s="8" r="D4">
         <v>16</v>
       </c>
-      <c t="s" s="6" r="E4">
+      <c t="s" s="8" r="E4">
         <v>17</v>
       </c>
     </row>
     <row r="5">
       <c s="2" r="A5"/>
-      <c t="s" s="6" r="B5">
+      <c t="s" s="8" r="B5">
         <v>18</v>
       </c>
-      <c t="s" s="6" r="C5">
+      <c t="s" s="8" r="C5">
         <v>19</v>
       </c>
-      <c t="s" s="6" r="D5">
+      <c t="s" s="8" r="D5">
         <v>20</v>
       </c>
-      <c t="s" s="6" r="E5">
+      <c t="s" s="8" r="E5">
         <v>21</v>
       </c>
     </row>
     <row r="6">
       <c s="2" r="A6"/>
-      <c t="s" s="6" r="B6">
+      <c t="s" s="8" r="B6">
         <v>22</v>
       </c>
-      <c t="s" s="6" r="C6">
+      <c t="s" s="8" r="C6">
         <v>23</v>
       </c>
-      <c t="s" s="6" r="D6">
+      <c t="s" s="8" r="D6">
         <v>23</v>
       </c>
-      <c t="s" s="6" r="E6">
+      <c t="s" s="8" r="E6">
         <v>23</v>
       </c>
     </row>
     <row r="7">
       <c s="2" r="A7"/>
-      <c t="s" s="6" r="B7">
+      <c t="s" s="8" r="B7">
         <v>24</v>
       </c>
-      <c t="s" s="6" r="C7">
+      <c t="s" s="8" r="C7">
         <v>25</v>
       </c>
-      <c t="s" s="6" r="D7">
+      <c t="s" s="8" r="D7">
         <v>25</v>
       </c>
-      <c t="s" s="6" r="E7">
+      <c t="s" s="8" r="E7">
         <v>25</v>
       </c>
     </row>
     <row r="8">
       <c s="2" r="A8"/>
-      <c t="s" s="6" r="B8">
+      <c t="s" s="8" r="B8">
         <v>26</v>
       </c>
-      <c t="s" s="6" r="C8">
+      <c t="s" s="8" r="C8">
         <v>27</v>
       </c>
-      <c t="s" s="6" r="D8">
+      <c t="s" s="8" r="D8">
         <v>28</v>
       </c>
-      <c t="s" s="6" r="E8">
+      <c t="s" s="8" r="E8">
         <v>29</v>
       </c>
     </row>
     <row r="9">
       <c s="2" r="A9"/>
-      <c t="s" s="6" r="B9">
+      <c t="s" s="8" r="B9">
         <v>30</v>
       </c>
-      <c t="s" s="6" r="C9">
+      <c t="s" s="8" r="C9">
         <v>31</v>
       </c>
-      <c t="s" s="6" r="D9">
+      <c t="s" s="8" r="D9">
         <v>32</v>
       </c>
-      <c t="s" s="6" r="E9">
+      <c t="s" s="8" r="E9">
         <v>33</v>
       </c>
     </row>
     <row r="10">
       <c s="2" r="A10"/>
-      <c t="s" s="6" r="B10">
+      <c t="s" s="8" r="B10">
         <v>34</v>
       </c>
-      <c t="s" s="6" r="C10">
+      <c t="s" s="8" r="C10">
         <v>35</v>
       </c>
-      <c t="s" s="6" r="D10">
+      <c t="s" s="8" r="D10">
         <v>36</v>
       </c>
-      <c t="s" s="6" r="E10">
+      <c t="s" s="8" r="E10">
         <v>37</v>
       </c>
     </row>
     <row r="11">
       <c s="2" r="A11"/>
-      <c t="s" s="6" r="B11">
+      <c t="s" s="8" r="B11">
         <v>38</v>
       </c>
-      <c t="s" s="6" r="C11">
+      <c t="s" s="8" r="C11">
         <v>39</v>
       </c>
-      <c t="s" s="6" r="D11">
+      <c t="s" s="8" r="D11">
         <v>40</v>
       </c>
-      <c t="s" s="6" r="E11">
+      <c t="s" s="8" r="E11">
         <v>41</v>
       </c>
     </row>
     <row r="12">
       <c s="2" r="A12"/>
-      <c t="s" s="6" r="B12">
+      <c t="s" s="8" r="B12">
         <v>42</v>
       </c>
-      <c t="s" s="6" r="C12">
+      <c t="s" s="8" r="C12">
         <v>43</v>
       </c>
-      <c t="s" s="6" r="D12">
+      <c t="s" s="8" r="D12">
         <v>44</v>
       </c>
-      <c t="s" s="6" r="E12">
+      <c t="s" s="8" r="E12">
         <v>45</v>
       </c>
     </row>
     <row r="13">
-      <c s="11" r="A13"/>
-      <c t="s" s="6" r="B13">
+      <c s="13" r="A13"/>
+      <c t="s" s="8" r="B13">
         <v>46</v>
       </c>
-      <c t="s" s="6" r="C13">
+      <c t="s" s="8" r="C13">
         <v>47</v>
       </c>
-      <c t="s" s="6" r="D13">
+      <c t="s" s="8" r="D13">
         <v>48</v>
       </c>
-      <c t="s" s="6" r="E13">
+      <c t="s" s="8" r="E13">
         <v>49</v>
       </c>
     </row>
     <row r="14">
-      <c s="11" r="A14"/>
-      <c t="s" s="6" r="B14">
+      <c s="13" r="A14"/>
+      <c t="s" s="8" r="B14">
         <v>50</v>
       </c>
-      <c t="s" s="6" r="C14">
+      <c t="s" s="8" r="C14">
         <v>51</v>
       </c>
-      <c t="s" s="6" r="D14">
+      <c t="s" s="8" r="D14">
         <v>52</v>
       </c>
-      <c t="s" s="6" r="E14">
+      <c t="s" s="8" r="E14">
         <v>53</v>
       </c>
     </row>
     <row r="15">
-      <c s="11" r="A15"/>
-      <c t="s" s="6" r="B15">
+      <c s="13" r="A15"/>
+      <c t="s" s="8" r="B15">
         <v>54</v>
       </c>
-      <c t="s" s="6" r="C15">
+      <c t="s" s="8" r="C15">
         <v>55</v>
       </c>
-      <c t="s" s="6" r="D15">
+      <c t="s" s="8" r="D15">
         <v>56</v>
       </c>
-      <c t="s" s="6" r="E15">
+      <c t="s" s="8" r="E15">
         <v>57</v>
       </c>
     </row>
     <row r="16">
-      <c s="11" r="A16"/>
-      <c t="s" s="6" r="B16">
+      <c s="13" r="A16"/>
+      <c t="s" s="8" r="B16">
         <v>58</v>
       </c>
-      <c t="s" s="6" r="C16">
+      <c t="s" s="8" r="C16">
         <v>59</v>
       </c>
-      <c t="s" s="6" r="D16">
+      <c t="s" s="8" r="D16">
         <v>60</v>
       </c>
-      <c t="s" s="6" r="E16">
+      <c t="s" s="8" r="E16">
         <v>61</v>
       </c>
     </row>
     <row r="17">
-      <c s="11" r="A17"/>
-      <c t="s" s="6" r="B17">
+      <c s="13" r="A17"/>
+      <c t="s" s="8" r="B17">
         <v>62</v>
       </c>
-      <c t="s" s="6" r="C17">
+      <c t="s" s="8" r="C17">
         <v>63</v>
       </c>
-      <c t="s" s="6" r="D17">
+      <c t="s" s="8" r="D17">
         <v>64</v>
       </c>
-      <c t="s" s="6" r="E17">
+      <c t="s" s="8" r="E17">
         <v>65</v>
       </c>
     </row>
     <row r="18">
-      <c s="11" r="A18"/>
-      <c t="s" s="6" r="B18">
+      <c s="13" r="A18"/>
+      <c t="s" s="8" r="B18">
         <v>66</v>
       </c>
-      <c t="s" s="6" r="C18">
+      <c t="s" s="8" r="C18">
         <v>67</v>
       </c>
-      <c t="s" s="6" r="D18">
+      <c t="s" s="8" r="D18">
         <v>68</v>
       </c>
-      <c t="s" s="6" r="E18">
+      <c t="s" s="8" r="E18">
         <v>69</v>
       </c>
     </row>
     <row r="19">
-      <c s="11" r="A19"/>
-      <c t="s" s="6" r="B19">
+      <c s="13" r="A19"/>
+      <c t="s" s="8" r="B19">
         <v>70</v>
       </c>
-      <c t="s" s="6" r="C19">
+      <c t="s" s="8" r="C19">
         <v>71</v>
       </c>
-      <c t="s" s="6" r="D19">
+      <c t="s" s="8" r="D19">
         <v>72</v>
       </c>
-      <c t="s" s="6" r="E19">
+      <c t="s" s="8" r="E19">
         <v>73</v>
       </c>
     </row>
     <row r="20">
-      <c s="11" r="A20"/>
-      <c t="s" s="6" r="B20">
+      <c s="13" r="A20"/>
+      <c t="s" s="8" r="B20">
         <v>74</v>
       </c>
-      <c t="s" s="6" r="C20">
+      <c t="s" s="8" r="C20">
         <v>75</v>
       </c>
-      <c t="s" s="6" r="D20">
+      <c t="s" s="8" r="D20">
         <v>76</v>
       </c>
-      <c t="s" s="6" r="E20">
+      <c t="s" s="8" r="E20">
         <v>77</v>
       </c>
     </row>
     <row r="21">
-      <c s="11" r="A21"/>
-      <c t="s" s="6" r="B21">
+      <c s="13" r="A21"/>
+      <c t="s" s="8" r="B21">
         <v>78</v>
       </c>
-      <c t="s" s="6" r="C21">
+      <c t="s" s="8" r="C21">
         <v>79</v>
       </c>
-      <c t="s" s="6" r="D21">
+      <c t="s" s="8" r="D21">
         <v>80</v>
       </c>
-      <c t="s" s="6" r="E21">
+      <c t="s" s="8" r="E21">
         <v>81</v>
       </c>
     </row>
     <row r="22">
-      <c s="11" r="A22"/>
-      <c t="s" s="6" r="B22">
+      <c s="13" r="A22"/>
+      <c t="s" s="8" r="B22">
         <v>82</v>
       </c>
-      <c t="s" s="6" r="C22">
+      <c t="s" s="8" r="C22">
         <v>83</v>
       </c>
-      <c t="s" s="6" r="D22">
+      <c t="s" s="8" r="D22">
         <v>84</v>
       </c>
-      <c t="s" s="6" r="E22">
+      <c t="s" s="8" r="E22">
         <v>85</v>
       </c>
     </row>
     <row r="23">
-      <c s="11" r="A23"/>
-      <c t="s" s="6" r="B23">
+      <c s="13" r="A23"/>
+      <c t="s" s="8" r="B23">
         <v>86</v>
       </c>
-      <c t="s" s="6" r="C23">
+      <c t="s" s="8" r="C23">
         <v>87</v>
       </c>
-      <c t="s" s="6" r="D23">
+      <c t="s" s="8" r="D23">
         <v>48</v>
       </c>
-      <c t="s" s="6" r="E23">
+      <c t="s" s="8" r="E23">
         <v>88</v>
       </c>
     </row>
@@ -2093,339 +2135,339 @@
       <c t="s" s="2" r="A25">
         <v>89</v>
       </c>
-      <c t="s" s="6" r="B25">
+      <c t="s" s="8" r="B25">
         <v>90</v>
       </c>
-      <c t="s" s="6" r="C25">
+      <c t="s" s="8" r="C25">
         <v>91</v>
       </c>
-      <c t="s" s="6" r="D25">
+      <c t="s" s="8" r="D25">
         <v>92</v>
       </c>
-      <c t="s" s="6" r="E25">
+      <c t="s" s="8" r="E25">
         <v>93</v>
       </c>
     </row>
     <row r="26">
       <c s="2" r="A26"/>
-      <c t="s" s="6" r="B26">
+      <c t="s" s="8" r="B26">
         <v>94</v>
       </c>
-      <c t="s" s="6" r="C26">
+      <c t="s" s="8" r="C26">
         <v>95</v>
       </c>
-      <c t="s" s="6" r="D26">
+      <c t="s" s="8" r="D26">
         <v>96</v>
       </c>
-      <c t="s" s="6" r="E26">
+      <c t="s" s="8" r="E26">
         <v>97</v>
       </c>
     </row>
     <row r="27">
       <c s="2" r="A27"/>
-      <c t="s" s="6" r="B27">
+      <c t="s" s="8" r="B27">
         <v>98</v>
       </c>
-      <c t="s" s="6" r="C27">
+      <c t="s" s="8" r="C27">
         <v>99</v>
       </c>
-      <c t="s" s="6" r="D27">
+      <c t="s" s="8" r="D27">
         <v>100</v>
       </c>
-      <c t="s" s="6" r="E27">
+      <c t="s" s="8" r="E27">
         <v>101</v>
       </c>
     </row>
     <row r="28">
       <c s="2" r="A28"/>
-      <c t="s" s="6" r="B28">
+      <c t="s" s="8" r="B28">
         <v>102</v>
       </c>
-      <c t="s" s="6" r="C28">
+      <c t="s" s="8" r="C28">
         <v>103</v>
       </c>
-      <c t="s" s="6" r="D28">
+      <c t="s" s="8" r="D28">
         <v>104</v>
       </c>
-      <c t="s" s="6" r="E28">
+      <c t="s" s="8" r="E28">
         <v>105</v>
       </c>
     </row>
     <row r="29">
       <c s="2" r="A29"/>
-      <c t="s" s="6" r="B29">
+      <c t="s" s="8" r="B29">
         <v>106</v>
       </c>
-      <c t="s" s="6" r="C29">
+      <c t="s" s="8" r="C29">
         <v>107</v>
       </c>
-      <c t="s" s="6" r="D29">
+      <c t="s" s="8" r="D29">
         <v>108</v>
       </c>
-      <c t="s" s="6" r="E29">
+      <c t="s" s="8" r="E29">
         <v>109</v>
       </c>
     </row>
     <row r="30">
-      <c s="11" r="A30"/>
-      <c t="s" s="6" r="B30">
+      <c s="13" r="A30"/>
+      <c t="s" s="8" r="B30">
         <v>110</v>
       </c>
-      <c t="s" s="6" r="C30">
+      <c t="s" s="8" r="C30">
         <v>111</v>
       </c>
-      <c t="s" s="6" r="D30">
+      <c t="s" s="8" r="D30">
         <v>112</v>
       </c>
-      <c t="s" s="6" r="E30">
+      <c t="s" s="8" r="E30">
         <v>113</v>
       </c>
     </row>
     <row r="31">
-      <c s="11" r="A31"/>
-      <c t="s" s="6" r="B31">
+      <c s="13" r="A31"/>
+      <c t="s" s="8" r="B31">
         <v>114</v>
       </c>
-      <c t="s" s="6" r="C31">
+      <c t="s" s="8" r="C31">
         <v>115</v>
       </c>
-      <c t="s" s="6" r="D31">
+      <c t="s" s="8" r="D31">
         <v>116</v>
       </c>
-      <c t="s" s="6" r="E31">
+      <c t="s" s="8" r="E31">
         <v>117</v>
       </c>
     </row>
     <row r="32">
-      <c s="11" r="A32"/>
-      <c s="11" r="B32"/>
-      <c s="11" r="C32"/>
-      <c s="11" r="D32"/>
-      <c s="11" r="E32"/>
+      <c s="13" r="A32"/>
+      <c s="13" r="B32"/>
+      <c s="13" r="C32"/>
+      <c s="13" r="D32"/>
+      <c s="13" r="E32"/>
     </row>
     <row r="33">
       <c t="s" s="2" r="A33">
         <v>118</v>
       </c>
-      <c t="s" s="16" r="B33">
+      <c t="s" s="18" r="B33">
         <v>119</v>
       </c>
-      <c t="s" s="16" r="C33">
+      <c t="s" s="18" r="C33">
         <v>120</v>
       </c>
-      <c s="16" r="D33"/>
-      <c s="16" r="E33"/>
+      <c s="18" r="D33"/>
+      <c s="18" r="E33"/>
     </row>
     <row r="34">
       <c s="2" r="A34"/>
       <c s="2" r="B34"/>
       <c s="2" r="C34"/>
       <c s="2" r="D34"/>
-      <c s="11" r="E34"/>
+      <c s="13" r="E34"/>
     </row>
     <row r="35">
-      <c t="s" s="11" r="A35">
+      <c t="s" s="13" r="A35">
         <v>121</v>
       </c>
-      <c t="s" s="6" r="B35">
+      <c t="s" s="8" r="B35">
         <v>122</v>
       </c>
-      <c t="s" s="6" r="C35">
+      <c t="s" s="8" r="C35">
         <v>121</v>
       </c>
-      <c t="s" s="6" r="D35">
+      <c t="s" s="8" r="D35">
         <v>123</v>
       </c>
-      <c t="s" s="6" r="E35">
+      <c t="s" s="8" r="E35">
         <v>124</v>
       </c>
     </row>
     <row r="36">
-      <c s="11" r="A36"/>
-      <c t="s" s="6" r="B36">
+      <c s="13" r="A36"/>
+      <c t="s" s="8" r="B36">
         <v>125</v>
       </c>
-      <c t="s" s="6" r="C36">
+      <c t="s" s="8" r="C36">
         <v>126</v>
       </c>
-      <c t="s" s="6" r="D36">
+      <c t="s" s="8" r="D36">
         <v>127</v>
       </c>
-      <c t="s" s="6" r="E36">
+      <c t="s" s="8" r="E36">
         <v>128</v>
       </c>
     </row>
     <row r="37">
-      <c s="11" r="A37"/>
-      <c t="s" s="6" r="B37">
+      <c s="13" r="A37"/>
+      <c t="s" s="8" r="B37">
         <v>129</v>
       </c>
-      <c t="s" s="6" r="C37">
+      <c t="s" s="8" r="C37">
         <v>130</v>
       </c>
-      <c t="s" s="6" r="D37">
+      <c t="s" s="8" r="D37">
         <v>131</v>
       </c>
-      <c t="s" s="6" r="E37">
+      <c t="s" s="8" r="E37">
         <v>132</v>
       </c>
     </row>
     <row r="38">
-      <c s="11" r="A38"/>
-      <c t="s" s="6" r="B38">
+      <c s="13" r="A38"/>
+      <c t="s" s="8" r="B38">
         <v>133</v>
       </c>
-      <c t="s" s="6" r="C38">
+      <c t="s" s="8" r="C38">
         <v>134</v>
       </c>
-      <c t="s" s="6" r="D38">
+      <c t="s" s="8" r="D38">
         <v>135</v>
       </c>
-      <c t="s" s="6" r="E38">
+      <c t="s" s="8" r="E38">
         <v>136</v>
       </c>
     </row>
     <row r="39">
-      <c s="11" r="A39"/>
-      <c t="s" s="6" r="B39">
+      <c s="13" r="A39"/>
+      <c t="s" s="8" r="B39">
         <v>137</v>
       </c>
-      <c t="s" s="6" r="C39">
+      <c t="s" s="8" r="C39">
         <v>138</v>
       </c>
-      <c t="s" s="6" r="D39">
+      <c t="s" s="8" r="D39">
         <v>139</v>
       </c>
-      <c t="s" s="6" r="E39">
+      <c t="s" s="8" r="E39">
         <v>140</v>
       </c>
     </row>
     <row r="40">
-      <c s="11" r="A40"/>
-      <c t="s" s="6" r="B40">
+      <c s="13" r="A40"/>
+      <c t="s" s="8" r="B40">
         <v>141</v>
       </c>
-      <c t="s" s="6" r="C40">
+      <c t="s" s="8" r="C40">
         <v>142</v>
       </c>
-      <c t="s" s="6" r="D40">
+      <c t="s" s="8" r="D40">
         <v>143</v>
       </c>
-      <c t="s" s="6" r="E40">
+      <c t="s" s="8" r="E40">
         <v>144</v>
       </c>
     </row>
     <row r="41">
-      <c s="11" r="A41"/>
-      <c t="s" s="6" r="B41">
+      <c s="13" r="A41"/>
+      <c t="s" s="8" r="B41">
         <v>145</v>
       </c>
-      <c t="s" s="6" r="C41">
+      <c t="s" s="8" r="C41">
         <v>146</v>
       </c>
-      <c t="s" s="6" r="D41">
+      <c t="s" s="8" r="D41">
         <v>147</v>
       </c>
-      <c t="s" s="6" r="E41">
+      <c t="s" s="8" r="E41">
         <v>148</v>
       </c>
     </row>
     <row r="42">
-      <c s="11" r="A42"/>
-      <c t="s" s="6" r="B42">
+      <c s="13" r="A42"/>
+      <c t="s" s="8" r="B42">
         <v>149</v>
       </c>
-      <c t="s" s="6" r="C42">
+      <c t="s" s="8" r="C42">
         <v>150</v>
       </c>
-      <c t="s" s="6" r="D42">
+      <c t="s" s="8" r="D42">
         <v>151</v>
       </c>
-      <c t="s" s="6" r="E42">
+      <c t="s" s="8" r="E42">
         <v>152</v>
       </c>
     </row>
     <row r="43">
-      <c s="11" r="A43"/>
-      <c t="s" s="6" r="B43">
+      <c s="13" r="A43"/>
+      <c t="s" s="8" r="B43">
         <v>153</v>
       </c>
-      <c t="s" s="6" r="C43">
+      <c t="s" s="8" r="C43">
         <v>154</v>
       </c>
-      <c t="s" s="6" r="D43">
+      <c t="s" s="8" r="D43">
         <v>155</v>
       </c>
-      <c t="s" s="6" r="E43">
+      <c t="s" s="8" r="E43">
         <v>156</v>
       </c>
     </row>
     <row r="44">
-      <c s="11" r="A44"/>
-      <c t="s" s="6" r="B44">
+      <c s="13" r="A44"/>
+      <c t="s" s="8" r="B44">
         <v>157</v>
       </c>
-      <c t="s" s="6" r="C44">
+      <c t="s" s="8" r="C44">
         <v>158</v>
       </c>
-      <c t="s" s="6" r="D44">
+      <c t="s" s="8" r="D44">
         <v>159</v>
       </c>
-      <c t="s" s="6" r="E44">
+      <c t="s" s="8" r="E44">
         <v>160</v>
       </c>
     </row>
     <row r="45">
-      <c s="11" r="A45"/>
-      <c t="s" s="6" r="B45">
+      <c s="13" r="A45"/>
+      <c t="s" s="8" r="B45">
         <v>161</v>
       </c>
-      <c t="s" s="6" r="C45">
+      <c t="s" s="8" r="C45">
         <v>162</v>
       </c>
-      <c t="s" s="6" r="D45">
+      <c t="s" s="8" r="D45">
         <v>163</v>
       </c>
-      <c t="s" s="6" r="E45">
+      <c t="s" s="8" r="E45">
         <v>164</v>
       </c>
     </row>
     <row r="46">
-      <c s="11" r="A46"/>
-      <c s="11" r="B46"/>
-      <c s="11" r="C46"/>
-      <c s="11" r="D46"/>
-      <c s="11" r="E46"/>
+      <c s="13" r="A46"/>
+      <c s="13" r="B46"/>
+      <c s="13" r="C46"/>
+      <c s="13" r="D46"/>
+      <c s="13" r="E46"/>
     </row>
     <row r="47">
-      <c t="s" s="11" r="A47">
+      <c t="s" s="13" r="A47">
         <v>165</v>
       </c>
-      <c t="s" s="6" r="B47">
+      <c t="s" s="8" r="B47">
         <v>166</v>
       </c>
-      <c t="s" s="6" r="C47">
+      <c t="s" s="8" r="C47">
         <v>167</v>
       </c>
-      <c t="s" s="6" r="D47">
+      <c t="s" s="8" r="D47">
         <v>168</v>
       </c>
-      <c t="s" s="6" r="E47">
+      <c t="s" s="8" r="E47">
         <v>169</v>
       </c>
     </row>
     <row r="48">
-      <c s="11" r="A48"/>
-      <c t="s" s="6" r="B48">
+      <c s="13" r="A48"/>
+      <c t="s" s="8" r="B48">
         <v>170</v>
       </c>
-      <c t="s" s="6" r="C48">
+      <c t="s" s="8" r="C48">
         <v>171</v>
       </c>
-      <c t="s" s="6" r="D48">
+      <c t="s" s="8" r="D48">
         <v>172</v>
       </c>
-      <c t="s" s="6" r="E48">
+      <c t="s" s="8" r="E48">
         <v>173</v>
       </c>
     </row>
@@ -2437,1187 +2479,1209 @@
       <c s="2" r="E50"/>
     </row>
     <row r="51">
-      <c t="s" s="11" r="A51">
+      <c t="s" s="13" r="A51">
         <v>174</v>
       </c>
-      <c t="s" s="14" r="B51">
+      <c t="s" s="16" r="B51">
         <v>175</v>
       </c>
-      <c t="s" s="14" r="C51">
+      <c t="s" s="16" r="C51">
         <v>176</v>
       </c>
-      <c s="14" r="D51"/>
-      <c s="14" r="E51"/>
+      <c s="16" r="D51"/>
+      <c s="16" r="E51"/>
     </row>
     <row r="52">
-      <c s="11" r="A52"/>
-      <c t="s" s="14" r="B52">
+      <c s="13" r="A52"/>
+      <c t="s" s="16" r="B52">
         <v>177</v>
       </c>
-      <c t="s" s="14" r="C52">
+      <c t="s" s="16" r="C52">
         <v>178</v>
       </c>
-      <c s="14" r="D52"/>
-      <c s="14" r="E52"/>
+      <c s="16" r="D52"/>
+      <c s="16" r="E52"/>
     </row>
     <row r="53">
-      <c s="11" r="A53"/>
-      <c t="s" s="14" r="B53">
+      <c s="13" r="A53"/>
+      <c t="s" s="16" r="B53">
         <v>179</v>
       </c>
-      <c t="s" s="14" r="C53">
+      <c t="s" s="16" r="C53">
         <v>180</v>
       </c>
-      <c s="14" r="D53"/>
-      <c s="14" r="E53"/>
+      <c s="16" r="D53"/>
+      <c s="16" r="E53"/>
     </row>
     <row r="54">
-      <c s="11" r="A54"/>
-      <c t="s" s="14" r="B54">
+      <c s="13" r="A54"/>
+      <c t="s" s="16" r="B54">
         <v>181</v>
       </c>
-      <c t="s" s="14" r="C54">
+      <c t="s" s="16" r="C54">
         <v>182</v>
       </c>
-      <c s="14" r="D54"/>
-      <c s="14" r="E54"/>
+      <c s="16" r="D54"/>
+      <c s="16" r="E54"/>
     </row>
     <row r="55">
-      <c s="11" r="A55"/>
-      <c t="s" s="6" r="B55">
+      <c s="13" r="A55"/>
+      <c t="s" s="8" r="B55">
         <v>183</v>
       </c>
-      <c t="s" s="6" r="C55">
+      <c t="s" s="8" r="C55">
         <v>184</v>
       </c>
-      <c t="s" s="6" r="D55">
+      <c t="s" s="8" r="D55">
         <v>185</v>
       </c>
-      <c t="s" s="6" r="E55">
+      <c t="s" s="8" r="E55">
         <v>186</v>
       </c>
     </row>
     <row r="56">
-      <c s="11" r="A56"/>
-      <c t="s" s="6" r="B56">
+      <c s="13" r="A56"/>
+      <c t="s" s="8" r="B56">
         <v>187</v>
       </c>
-      <c t="s" s="6" r="C56">
+      <c t="s" s="8" r="C56">
         <v>188</v>
       </c>
-      <c t="s" s="6" r="D56">
+      <c t="s" s="8" r="D56">
         <v>189</v>
       </c>
-      <c t="s" s="6" r="E56">
+      <c t="s" s="8" r="E56">
         <v>190</v>
       </c>
     </row>
     <row r="57">
-      <c s="11" r="A57"/>
-      <c s="11" r="B57"/>
-      <c s="11" r="C57"/>
-      <c s="11" r="D57"/>
-      <c s="11" r="E57"/>
+      <c s="13" r="A57"/>
+      <c t="s" s="5" r="B57">
+        <v>191</v>
+      </c>
+      <c t="s" s="5" r="C57">
+        <v>192</v>
+      </c>
+      <c s="5" r="D57"/>
+      <c s="5" r="E57"/>
     </row>
     <row r="58">
-      <c t="s" s="11" r="A58">
-        <v>191</v>
-      </c>
-      <c t="s" s="6" r="B58">
-        <v>192</v>
-      </c>
-      <c t="s" s="6" r="C58">
+      <c s="13" r="A58"/>
+      <c s="13" r="B58"/>
+      <c s="13" r="C58"/>
+      <c s="13" r="D58"/>
+      <c s="13" r="E58"/>
+    </row>
+    <row r="59">
+      <c t="s" s="13" r="A59">
         <v>193</v>
       </c>
-      <c t="s" s="6" r="D58">
+      <c t="s" s="8" r="B59">
         <v>194</v>
       </c>
-      <c t="s" s="6" r="E58">
+      <c t="s" s="8" r="C59">
+        <v>195</v>
+      </c>
+      <c t="s" s="8" r="D59">
+        <v>196</v>
+      </c>
+      <c t="s" s="8" r="E59">
         <v>17</v>
       </c>
     </row>
-    <row r="59">
-      <c s="11" r="A59"/>
-      <c t="s" s="6" r="B59">
-        <v>195</v>
-      </c>
-      <c t="s" s="6" r="C59">
-        <v>196</v>
-      </c>
-      <c t="s" s="6" r="D59">
+    <row r="60">
+      <c s="13" r="A60"/>
+      <c t="s" s="8" r="B60">
         <v>197</v>
       </c>
-      <c t="s" s="6" r="E59">
+      <c t="s" s="8" r="C60">
         <v>198</v>
       </c>
-    </row>
-    <row r="60">
-      <c s="11" r="A60"/>
-      <c t="s" s="6" r="B60">
+      <c t="s" s="8" r="D60">
         <v>199</v>
       </c>
-      <c t="s" s="6" r="C60">
+      <c t="s" s="8" r="E60">
         <v>200</v>
       </c>
-      <c t="s" s="6" r="D60">
+    </row>
+    <row r="61">
+      <c s="13" r="A61"/>
+      <c t="s" s="8" r="B61">
         <v>201</v>
       </c>
-      <c t="s" s="6" r="E60">
+      <c t="s" s="8" r="C61">
         <v>202</v>
       </c>
-    </row>
-    <row r="61">
-      <c s="11" r="A61"/>
-      <c t="s" s="6" r="B61">
+      <c t="s" s="8" r="D61">
         <v>203</v>
       </c>
-      <c t="s" s="6" r="C61">
+      <c t="s" s="8" r="E61">
         <v>204</v>
       </c>
-      <c t="s" s="6" r="D61">
+    </row>
+    <row r="62">
+      <c s="13" r="A62"/>
+      <c t="s" s="8" r="B62">
         <v>205</v>
       </c>
-      <c t="s" s="6" r="E61">
+      <c t="s" s="8" r="C62">
         <v>206</v>
       </c>
-    </row>
-    <row r="62">
-      <c s="11" r="A62"/>
-      <c t="s" s="6" r="B62">
+      <c t="s" s="8" r="D62">
         <v>207</v>
       </c>
-      <c t="s" s="6" r="C62">
+      <c t="s" s="8" r="E62">
         <v>208</v>
       </c>
-      <c t="s" s="6" r="D62">
+    </row>
+    <row r="63">
+      <c s="13" r="A63"/>
+      <c t="s" s="8" r="B63">
         <v>209</v>
       </c>
-      <c t="s" s="6" r="E62">
+      <c t="s" s="8" r="C63">
         <v>210</v>
       </c>
-    </row>
-    <row r="63">
-      <c s="11" r="A63"/>
-      <c t="s" s="6" r="B63">
+      <c t="s" s="8" r="D63">
         <v>211</v>
       </c>
-      <c t="s" s="6" r="C63">
+      <c t="s" s="8" r="E63">
         <v>212</v>
       </c>
-      <c t="s" s="6" r="D63">
+    </row>
+    <row r="64">
+      <c s="13" r="A64"/>
+      <c t="s" s="8" r="B64">
         <v>213</v>
       </c>
-      <c t="s" s="6" r="E63">
+      <c t="s" s="8" r="C64">
         <v>214</v>
       </c>
-    </row>
-    <row r="64">
-      <c s="11" r="A64"/>
-      <c t="s" s="6" r="B64">
+      <c t="s" s="8" r="D64">
         <v>215</v>
       </c>
-      <c t="s" s="6" r="C64">
+      <c t="s" s="8" r="E64">
         <v>216</v>
       </c>
-      <c t="s" s="6" r="D64">
+    </row>
+    <row r="65">
+      <c s="13" r="A65"/>
+      <c t="s" s="8" r="B65">
         <v>217</v>
       </c>
-      <c t="s" s="6" r="E64">
+      <c t="s" s="8" r="C65">
         <v>218</v>
       </c>
-    </row>
-    <row r="65">
-      <c s="11" r="A65"/>
-      <c t="s" s="6" r="B65">
+      <c t="s" s="8" r="D65">
         <v>219</v>
       </c>
-      <c t="s" s="6" r="C65">
+      <c t="s" s="8" r="E65">
         <v>220</v>
       </c>
-      <c t="s" s="6" r="D65">
+    </row>
+    <row r="66">
+      <c s="13" r="A66"/>
+      <c t="s" s="8" r="B66">
         <v>221</v>
       </c>
-      <c t="s" s="6" r="E65">
+      <c t="s" s="8" r="C66">
         <v>222</v>
       </c>
-    </row>
-    <row r="66">
-      <c s="11" r="A66"/>
-      <c t="s" s="6" r="B66">
+      <c t="s" s="8" r="D66">
         <v>223</v>
       </c>
-      <c t="s" s="6" r="C66">
+      <c t="s" s="8" r="E66">
         <v>224</v>
       </c>
-      <c t="s" s="6" r="D66">
+    </row>
+    <row r="67">
+      <c s="13" r="A67"/>
+      <c t="s" s="8" r="B67">
         <v>225</v>
       </c>
-      <c t="s" s="6" r="E66">
+      <c t="s" s="8" r="C67">
         <v>226</v>
       </c>
-    </row>
-    <row r="67">
-      <c s="11" r="A67"/>
-      <c s="11" r="B67"/>
-      <c s="11" r="C67"/>
-      <c s="11" r="D67"/>
-      <c s="11" r="E67"/>
+      <c t="s" s="8" r="D67">
+        <v>227</v>
+      </c>
+      <c t="s" s="8" r="E67">
+        <v>228</v>
+      </c>
     </row>
     <row r="68">
-      <c t="s" s="11" r="A68">
-        <v>227</v>
-      </c>
-      <c t="s" s="6" r="B68">
-        <v>228</v>
-      </c>
-      <c t="s" s="6" r="C68">
+      <c s="13" r="A68"/>
+      <c s="13" r="B68"/>
+      <c s="13" r="C68"/>
+      <c s="13" r="D68"/>
+      <c s="13" r="E68"/>
+    </row>
+    <row r="69">
+      <c t="s" s="13" r="A69">
         <v>229</v>
       </c>
-      <c t="s" s="6" r="D68">
+      <c t="s" s="8" r="B69">
         <v>230</v>
       </c>
-      <c t="s" s="6" r="E68">
+      <c t="s" s="8" r="C69">
         <v>231</v>
       </c>
-    </row>
-    <row r="69">
-      <c s="11" r="A69"/>
-      <c t="s" s="6" r="B69">
+      <c t="s" s="8" r="D69">
         <v>232</v>
       </c>
-      <c t="s" s="6" r="C69">
+      <c t="s" s="8" r="E69">
         <v>233</v>
       </c>
-      <c t="s" s="6" r="D69">
+    </row>
+    <row r="70">
+      <c s="13" r="A70"/>
+      <c t="s" s="8" r="B70">
         <v>234</v>
       </c>
-      <c t="s" s="6" r="E69">
+      <c t="s" s="8" r="C70">
         <v>235</v>
       </c>
-    </row>
-    <row r="70">
-      <c s="9" r="A70"/>
-      <c t="s" s="6" r="B70">
+      <c t="s" s="8" r="D70">
         <v>236</v>
       </c>
-      <c t="s" s="6" r="C70">
+      <c t="s" s="8" r="E70">
         <v>237</v>
       </c>
-      <c t="s" s="6" r="D70">
+    </row>
+    <row r="71">
+      <c s="11" r="A71"/>
+      <c t="s" s="8" r="B71">
         <v>238</v>
       </c>
-      <c t="s" s="6" r="E70">
+      <c t="s" s="8" r="C71">
         <v>239</v>
       </c>
-    </row>
-    <row r="71">
-      <c s="9" r="A71"/>
-      <c t="s" s="6" r="B71">
+      <c t="s" s="8" r="D71">
         <v>240</v>
       </c>
-      <c t="s" s="6" r="C71">
+      <c t="s" s="8" r="E71">
         <v>241</v>
       </c>
-      <c t="s" s="6" r="D71">
+    </row>
+    <row r="72">
+      <c s="11" r="A72"/>
+      <c t="s" s="8" r="B72">
         <v>242</v>
       </c>
-      <c t="s" s="6" r="E71">
+      <c t="s" s="8" r="C72">
         <v>243</v>
       </c>
-    </row>
-    <row r="72">
-      <c s="9" r="A72"/>
-      <c t="s" s="6" r="B72">
+      <c t="s" s="8" r="D72">
         <v>244</v>
       </c>
-      <c t="s" s="6" r="C72">
+      <c t="s" s="8" r="E72">
         <v>245</v>
       </c>
-      <c t="s" s="6" r="D72">
+    </row>
+    <row r="73">
+      <c s="11" r="A73"/>
+      <c t="s" s="8" r="B73">
         <v>246</v>
       </c>
-      <c t="s" s="6" r="E72">
+      <c t="s" s="8" r="C73">
         <v>247</v>
       </c>
-    </row>
-    <row r="73">
-      <c s="9" r="A73"/>
-      <c t="s" s="6" r="B73">
+      <c t="s" s="8" r="D73">
         <v>248</v>
       </c>
-      <c t="s" s="6" r="C73">
+      <c t="s" s="8" r="E73">
         <v>249</v>
       </c>
-      <c t="s" s="6" r="D73">
+    </row>
+    <row r="74">
+      <c s="11" r="A74"/>
+      <c t="s" s="8" r="B74">
         <v>250</v>
       </c>
-      <c t="s" s="6" r="E73">
+      <c t="s" s="8" r="C74">
         <v>251</v>
       </c>
-    </row>
-    <row r="74">
-      <c s="9" r="A74"/>
-      <c t="s" s="6" r="B74">
+      <c t="s" s="8" r="D74">
         <v>252</v>
       </c>
-      <c t="s" s="6" r="C74">
+      <c t="s" s="8" r="E74">
         <v>253</v>
       </c>
-      <c t="s" s="6" r="D74">
+    </row>
+    <row r="75">
+      <c s="11" r="A75"/>
+      <c t="s" s="8" r="B75">
         <v>254</v>
       </c>
-      <c t="s" s="6" r="E74">
+      <c t="s" s="8" r="C75">
         <v>255</v>
       </c>
-    </row>
-    <row r="75">
-      <c s="9" r="A75"/>
-      <c t="s" s="6" r="B75">
+      <c t="s" s="8" r="D75">
         <v>256</v>
       </c>
-      <c t="s" s="6" r="C75">
+      <c t="s" s="8" r="E75">
         <v>257</v>
       </c>
-      <c t="s" s="6" r="D75">
+    </row>
+    <row r="76">
+      <c s="11" r="A76"/>
+      <c t="s" s="8" r="B76">
         <v>258</v>
       </c>
-      <c t="s" s="6" r="E75">
+      <c t="s" s="8" r="C76">
         <v>259</v>
       </c>
-    </row>
-    <row r="76">
-      <c s="9" r="A76"/>
-      <c t="s" s="6" r="B76">
+      <c t="s" s="8" r="D76">
         <v>260</v>
       </c>
-      <c t="s" s="6" r="C76">
+      <c t="s" s="8" r="E76">
         <v>261</v>
       </c>
-      <c t="s" s="6" r="D76">
+    </row>
+    <row r="77">
+      <c s="11" r="A77"/>
+      <c t="s" s="8" r="B77">
         <v>262</v>
       </c>
-      <c t="s" s="6" r="E76">
+      <c t="s" s="8" r="C77">
         <v>263</v>
       </c>
-    </row>
-    <row r="77">
-      <c s="9" r="A77"/>
-      <c t="s" s="6" r="B77">
+      <c t="s" s="8" r="D77">
         <v>264</v>
       </c>
-      <c t="s" s="6" r="C77">
+      <c t="s" s="8" r="E77">
         <v>265</v>
       </c>
-      <c t="s" s="6" r="D77">
+    </row>
+    <row r="78">
+      <c s="11" r="A78"/>
+      <c t="s" s="8" r="B78">
         <v>266</v>
       </c>
-      <c t="s" s="6" r="E77">
+      <c t="s" s="8" r="C78">
         <v>267</v>
       </c>
-    </row>
-    <row r="78">
-      <c s="9" r="A78"/>
-      <c t="s" s="6" r="B78">
+      <c t="s" s="8" r="D78">
         <v>268</v>
       </c>
-      <c t="s" s="6" r="C78">
+      <c t="s" s="8" r="E78">
         <v>269</v>
       </c>
-      <c t="s" s="6" r="D78">
+    </row>
+    <row r="79">
+      <c s="11" r="A79"/>
+      <c t="s" s="8" r="B79">
         <v>270</v>
       </c>
-      <c t="s" s="6" r="E78">
+      <c t="s" s="8" r="C79">
         <v>271</v>
       </c>
-    </row>
-    <row r="79">
-      <c s="9" r="A79"/>
-      <c t="s" s="6" r="B79">
+      <c t="s" s="8" r="D79">
         <v>272</v>
       </c>
-      <c t="s" s="6" r="C79">
+      <c t="s" s="8" r="E79">
         <v>273</v>
       </c>
-      <c t="s" s="6" r="D79">
+    </row>
+    <row r="80">
+      <c s="11" r="A80"/>
+      <c t="s" s="8" r="B80">
         <v>274</v>
       </c>
-      <c t="s" s="6" r="E79">
+      <c t="s" s="8" r="C80">
         <v>275</v>
       </c>
-    </row>
-    <row r="80">
-      <c s="9" r="A80"/>
-      <c t="s" s="6" r="B80">
+      <c t="s" s="8" r="D80">
         <v>276</v>
       </c>
-      <c t="s" s="6" r="C80">
+      <c t="s" s="8" r="E80">
         <v>277</v>
       </c>
-      <c t="s" s="6" r="D80">
+    </row>
+    <row r="81">
+      <c s="11" r="A81"/>
+      <c t="s" s="8" r="B81">
         <v>278</v>
       </c>
-      <c t="s" s="6" r="E80">
+      <c t="s" s="8" r="C81">
         <v>279</v>
       </c>
-    </row>
-    <row r="81">
-      <c s="9" r="A81"/>
-      <c t="s" s="6" r="B81">
+      <c t="s" s="8" r="D81">
         <v>280</v>
       </c>
-      <c t="s" s="6" r="C81">
+      <c t="s" s="8" r="E81">
         <v>281</v>
       </c>
-      <c t="s" s="6" r="D81">
+    </row>
+    <row r="82">
+      <c s="11" r="A82"/>
+      <c t="s" s="8" r="B82">
         <v>282</v>
       </c>
-      <c t="s" s="6" r="E81">
+      <c t="s" s="8" r="C82">
         <v>283</v>
       </c>
-    </row>
-    <row r="82">
-      <c s="9" r="A82"/>
-      <c s="11" r="B82"/>
-      <c s="11" r="C82"/>
-      <c s="11" r="D82"/>
-      <c s="11" r="E82"/>
+      <c t="s" s="8" r="D82">
+        <v>284</v>
+      </c>
+      <c t="s" s="8" r="E82">
+        <v>285</v>
+      </c>
     </row>
     <row r="83">
-      <c t="s" s="9" r="A83">
-        <v>284</v>
-      </c>
-      <c t="s" s="6" r="B83">
-        <v>285</v>
-      </c>
-      <c t="s" s="6" r="C83">
+      <c s="11" r="A83"/>
+      <c s="13" r="B83"/>
+      <c s="13" r="C83"/>
+      <c s="13" r="D83"/>
+      <c s="13" r="E83"/>
+    </row>
+    <row r="84">
+      <c t="s" s="11" r="A84">
         <v>286</v>
       </c>
-      <c t="s" s="6" r="D83">
+      <c t="s" s="8" r="B84">
         <v>287</v>
       </c>
-      <c t="s" s="6" r="E83">
+      <c t="s" s="8" r="C84">
         <v>288</v>
       </c>
-    </row>
-    <row r="84">
-      <c s="9" r="A84"/>
-      <c t="s" s="6" r="B84">
+      <c t="s" s="8" r="D84">
         <v>289</v>
       </c>
-      <c t="s" s="6" r="C84">
+      <c t="s" s="8" r="E84">
         <v>290</v>
       </c>
-      <c t="s" s="6" r="D84">
+    </row>
+    <row r="85">
+      <c s="11" r="A85"/>
+      <c t="s" s="8" r="B85">
         <v>291</v>
       </c>
-      <c t="s" s="6" r="E84">
+      <c t="s" s="8" r="C85">
         <v>292</v>
       </c>
-    </row>
-    <row r="85">
-      <c s="9" r="A85"/>
-      <c t="s" s="6" r="B85">
+      <c t="s" s="8" r="D85">
         <v>293</v>
       </c>
-      <c t="s" s="6" r="C85">
+      <c t="s" s="8" r="E85">
         <v>294</v>
       </c>
-      <c t="s" s="6" r="D85">
+    </row>
+    <row r="86">
+      <c s="11" r="A86"/>
+      <c t="s" s="8" r="B86">
         <v>295</v>
       </c>
-      <c t="s" s="6" r="E85">
+      <c t="s" s="8" r="C86">
         <v>296</v>
       </c>
-    </row>
-    <row r="86">
-      <c s="9" r="A86"/>
-      <c t="s" s="6" r="B86">
+      <c t="s" s="8" r="D86">
         <v>297</v>
       </c>
-      <c t="s" s="6" r="C86">
+      <c t="s" s="8" r="E86">
         <v>298</v>
       </c>
-      <c t="s" s="6" r="D86">
+    </row>
+    <row r="87">
+      <c s="11" r="A87"/>
+      <c t="s" s="8" r="B87">
         <v>299</v>
       </c>
-      <c t="s" s="6" r="E86">
+      <c t="s" s="8" r="C87">
         <v>300</v>
       </c>
-    </row>
-    <row r="87">
-      <c s="9" r="A87"/>
-      <c t="s" s="6" r="B87">
+      <c t="s" s="8" r="D87">
         <v>301</v>
       </c>
-      <c t="s" s="6" r="C87">
+      <c t="s" s="8" r="E87">
         <v>302</v>
       </c>
-      <c t="s" s="6" r="D87">
+    </row>
+    <row r="88">
+      <c s="11" r="A88"/>
+      <c t="s" s="8" r="B88">
         <v>303</v>
       </c>
-      <c t="s" s="6" r="E87">
+      <c t="s" s="8" r="C88">
         <v>304</v>
       </c>
-    </row>
-    <row r="88">
-      <c s="9" r="A88"/>
-      <c t="s" s="6" r="B88">
+      <c t="s" s="8" r="D88">
         <v>305</v>
       </c>
-      <c t="s" s="6" r="C88">
+      <c t="s" s="8" r="E88">
         <v>306</v>
       </c>
-      <c t="s" s="6" r="D88">
+    </row>
+    <row r="89">
+      <c s="11" r="A89"/>
+      <c t="s" s="8" r="B89">
         <v>307</v>
       </c>
-      <c t="s" s="6" r="E88">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="89">
-      <c s="9" r="A89"/>
-      <c t="s" s="6" r="B89">
+      <c t="s" s="8" r="C89">
         <v>308</v>
       </c>
-      <c t="s" s="6" r="C89">
+      <c t="s" s="8" r="D89">
         <v>309</v>
       </c>
-      <c t="s" s="6" r="D89">
+      <c t="s" s="8" r="E89">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="90">
+      <c s="11" r="A90"/>
+      <c t="s" s="8" r="B90">
         <v>310</v>
       </c>
-      <c t="s" s="6" r="E89">
+      <c t="s" s="8" r="C90">
         <v>311</v>
       </c>
-    </row>
-    <row r="90">
-      <c s="9" r="A90"/>
-      <c t="s" s="6" r="B90">
+      <c t="s" s="8" r="D90">
         <v>312</v>
       </c>
-      <c t="s" s="6" r="C90">
+      <c t="s" s="8" r="E90">
         <v>313</v>
       </c>
-      <c t="s" s="6" r="D90">
+    </row>
+    <row r="91">
+      <c s="11" r="A91"/>
+      <c t="s" s="8" r="B91">
         <v>314</v>
       </c>
-      <c t="s" s="6" r="E90">
+      <c t="s" s="8" r="C91">
         <v>315</v>
       </c>
-    </row>
-    <row r="91">
-      <c s="9" r="A91"/>
-      <c t="s" s="6" r="B91">
+      <c t="s" s="8" r="D91">
         <v>316</v>
       </c>
-      <c t="s" s="6" r="C91">
+      <c t="s" s="8" r="E91">
         <v>317</v>
       </c>
-      <c t="s" s="6" r="D91">
+    </row>
+    <row r="92">
+      <c s="11" r="A92"/>
+      <c t="s" s="8" r="B92">
         <v>318</v>
       </c>
-      <c t="s" s="6" r="E91">
+      <c t="s" s="8" r="C92">
         <v>319</v>
       </c>
-    </row>
-    <row r="92">
-      <c s="9" r="A92"/>
-      <c t="s" s="6" r="B92">
+      <c t="s" s="8" r="D92">
         <v>320</v>
       </c>
-      <c t="s" s="6" r="C92">
+      <c t="s" s="8" r="E92">
         <v>321</v>
       </c>
-      <c t="s" s="6" r="D92">
+    </row>
+    <row r="93">
+      <c s="11" r="A93"/>
+      <c t="s" s="8" r="B93">
         <v>322</v>
       </c>
-      <c t="s" s="6" r="E92">
+      <c t="s" s="8" r="C93">
         <v>323</v>
       </c>
-    </row>
-    <row r="93">
-      <c s="9" r="A93"/>
-      <c t="s" s="6" r="B93">
+      <c t="s" s="8" r="D93">
         <v>324</v>
       </c>
-      <c t="s" s="6" r="C93">
+      <c t="s" s="8" r="E93">
         <v>325</v>
       </c>
-      <c t="s" s="6" r="D93">
+    </row>
+    <row r="94">
+      <c s="11" r="A94"/>
+      <c t="s" s="8" r="B94">
         <v>326</v>
       </c>
-      <c t="s" s="6" r="E93">
+      <c t="s" s="8" r="C94">
         <v>327</v>
       </c>
-    </row>
-    <row r="94">
-      <c s="9" r="A94"/>
-      <c t="s" s="6" r="B94">
+      <c t="s" s="8" r="D94">
         <v>328</v>
       </c>
-      <c t="s" s="6" r="C94">
+      <c t="s" s="8" r="E94">
         <v>329</v>
       </c>
-      <c t="s" s="6" r="D94">
-        <v>329</v>
-      </c>
-      <c t="s" s="6" r="E94">
+    </row>
+    <row r="95">
+      <c s="11" r="A95"/>
+      <c t="s" s="8" r="B95">
         <v>330</v>
       </c>
-    </row>
-    <row r="95">
-      <c s="9" r="A95"/>
-      <c t="s" s="6" r="B95">
+      <c t="s" s="8" r="C95">
         <v>331</v>
       </c>
-      <c t="s" s="6" r="C95">
+      <c t="s" s="8" r="D95">
+        <v>331</v>
+      </c>
+      <c t="s" s="8" r="E95">
         <v>332</v>
       </c>
-      <c t="s" s="6" r="D95">
-        <v>332</v>
-      </c>
-      <c t="s" s="6" r="E95">
+    </row>
+    <row r="96">
+      <c s="11" r="A96"/>
+      <c t="s" s="8" r="B96">
         <v>333</v>
       </c>
-    </row>
-    <row r="96">
-      <c s="9" r="A96"/>
-      <c t="s" s="6" r="B96">
+      <c t="s" s="8" r="C96">
         <v>334</v>
       </c>
-      <c t="s" s="6" r="C96">
+      <c t="s" s="8" r="D96">
+        <v>334</v>
+      </c>
+      <c t="s" s="8" r="E96">
         <v>335</v>
       </c>
-      <c t="s" s="6" r="D96">
+    </row>
+    <row r="97">
+      <c s="11" r="A97"/>
+      <c t="s" s="8" r="B97">
         <v>336</v>
       </c>
-      <c t="s" s="6" r="E96">
+      <c t="s" s="8" r="C97">
         <v>337</v>
       </c>
-    </row>
-    <row r="97">
-      <c s="9" r="A97"/>
-      <c t="s" s="15" r="B97">
+      <c t="s" s="8" r="D97">
         <v>338</v>
       </c>
-      <c t="s" s="6" r="C97">
+      <c t="s" s="8" r="E97">
         <v>339</v>
       </c>
-      <c t="s" s="6" r="D97">
+    </row>
+    <row r="98">
+      <c s="11" r="A98"/>
+      <c t="s" s="17" r="B98">
         <v>340</v>
       </c>
-      <c t="s" s="6" r="E97">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="98">
-      <c s="9" r="A98"/>
-      <c t="s" s="6" r="B98">
+      <c t="s" s="8" r="C98">
         <v>341</v>
       </c>
-      <c t="s" s="6" r="C98">
+      <c t="s" s="8" r="D98">
         <v>342</v>
       </c>
-      <c t="s" s="6" r="D98">
+      <c t="s" s="8" r="E98">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="99">
+      <c s="11" r="A99"/>
+      <c t="s" s="8" r="B99">
         <v>343</v>
       </c>
-      <c t="s" s="6" r="E98">
+      <c t="s" s="8" r="C99">
         <v>344</v>
       </c>
-    </row>
-    <row r="99">
-      <c s="9" r="A99"/>
-      <c t="s" s="6" r="B99">
+      <c t="s" s="8" r="D99">
         <v>345</v>
       </c>
-      <c t="s" s="6" r="C99">
+      <c t="s" s="8" r="E99">
         <v>346</v>
       </c>
-      <c t="s" s="6" r="D99">
+    </row>
+    <row r="100">
+      <c s="11" r="A100"/>
+      <c t="s" s="8" r="B100">
         <v>347</v>
       </c>
-      <c t="s" s="6" r="E99">
+      <c t="s" s="8" r="C100">
         <v>348</v>
       </c>
-    </row>
-    <row r="100">
-      <c s="9" r="A100"/>
-      <c t="s" s="6" r="B100">
+      <c t="s" s="8" r="D100">
         <v>349</v>
       </c>
-      <c t="s" s="6" r="C100">
+      <c t="s" s="8" r="E100">
         <v>350</v>
       </c>
-      <c t="s" s="6" r="D100">
+    </row>
+    <row r="101">
+      <c s="11" r="A101"/>
+      <c t="s" s="8" r="B101">
         <v>351</v>
       </c>
-      <c t="s" s="6" r="E100">
+      <c t="s" s="8" r="C101">
         <v>352</v>
       </c>
-    </row>
-    <row r="101">
-      <c s="9" r="A101"/>
-      <c t="s" s="6" r="B101">
+      <c t="s" s="8" r="D101">
         <v>353</v>
       </c>
-      <c t="s" s="6" r="C101">
+      <c t="s" s="8" r="E101">
         <v>354</v>
       </c>
-      <c t="s" s="6" r="D101">
+    </row>
+    <row r="102">
+      <c s="11" r="A102"/>
+      <c t="s" s="8" r="B102">
         <v>355</v>
       </c>
-      <c t="s" s="6" r="E101">
+      <c t="s" s="8" r="C102">
         <v>356</v>
       </c>
-    </row>
-    <row r="102">
-      <c s="9" r="A102"/>
-      <c t="s" s="6" r="B102">
+      <c t="s" s="8" r="D102">
         <v>357</v>
       </c>
-      <c t="s" s="6" r="C102">
+      <c t="s" s="8" r="E102">
         <v>358</v>
       </c>
-      <c t="s" s="6" r="D102">
+    </row>
+    <row r="103">
+      <c s="11" r="A103"/>
+      <c t="s" s="8" r="B103">
         <v>359</v>
       </c>
-      <c t="s" s="6" r="E102">
+      <c t="s" s="8" r="C103">
         <v>360</v>
       </c>
-    </row>
-    <row r="103">
-      <c s="9" r="A103"/>
-      <c t="s" s="6" r="B103">
+      <c t="s" s="8" r="D103">
         <v>361</v>
       </c>
-      <c t="s" s="6" r="C103">
+      <c t="s" s="8" r="E103">
         <v>362</v>
       </c>
-      <c t="s" s="6" r="D103">
+    </row>
+    <row r="104">
+      <c s="11" r="A104"/>
+      <c t="s" s="8" r="B104">
         <v>363</v>
       </c>
-      <c t="s" s="6" r="E103">
+      <c t="s" s="8" r="C104">
         <v>364</v>
       </c>
-    </row>
-    <row r="104">
-      <c s="9" r="A104"/>
-      <c t="s" s="6" r="B104">
+      <c t="s" s="8" r="D104">
         <v>365</v>
       </c>
-      <c t="s" s="6" r="C104">
+      <c t="s" s="8" r="E104">
         <v>366</v>
       </c>
-      <c t="s" s="6" r="D104">
+    </row>
+    <row r="105">
+      <c s="11" r="A105"/>
+      <c t="s" s="8" r="B105">
         <v>367</v>
       </c>
-      <c t="s" s="6" r="E104">
+      <c t="s" s="8" r="C105">
         <v>368</v>
       </c>
-    </row>
-    <row r="105">
-      <c s="9" r="A105"/>
-      <c t="s" s="6" r="B105">
+      <c t="s" s="8" r="D105">
         <v>369</v>
       </c>
-      <c t="s" s="6" r="C105">
+      <c t="s" s="8" r="E105">
         <v>370</v>
       </c>
-      <c t="s" s="6" r="D105">
+    </row>
+    <row r="106">
+      <c s="11" r="A106"/>
+      <c t="s" s="8" r="B106">
         <v>371</v>
       </c>
-      <c t="s" s="6" r="E105">
+      <c t="s" s="8" r="C106">
         <v>372</v>
       </c>
-    </row>
-    <row r="106">
-      <c s="9" r="A106"/>
-      <c t="s" s="6" r="B106">
+      <c t="s" s="8" r="D106">
         <v>373</v>
       </c>
-      <c t="s" s="6" r="C106">
+      <c t="s" s="8" r="E106">
         <v>374</v>
       </c>
-      <c t="s" s="6" r="D106">
+    </row>
+    <row r="107">
+      <c s="11" r="A107"/>
+      <c t="s" s="8" r="B107">
         <v>375</v>
       </c>
-      <c t="s" s="6" r="E106">
+      <c t="s" s="8" r="C107">
         <v>376</v>
       </c>
-    </row>
-    <row r="107">
-      <c s="9" r="A107"/>
-      <c t="s" s="6" r="B107">
+      <c t="s" s="8" r="D107">
         <v>377</v>
       </c>
-      <c t="s" s="6" r="C107">
+      <c t="s" s="8" r="E107">
         <v>378</v>
       </c>
-      <c t="s" s="6" r="D107">
+    </row>
+    <row r="108">
+      <c s="11" r="A108"/>
+      <c t="s" s="8" r="B108">
         <v>379</v>
       </c>
-      <c t="s" s="6" r="E107">
+      <c t="s" s="8" r="C108">
         <v>380</v>
       </c>
-    </row>
-    <row r="108">
-      <c s="9" r="A108"/>
-      <c t="s" s="6" r="B108">
+      <c t="s" s="8" r="D108">
         <v>381</v>
       </c>
-      <c t="s" s="6" r="C108">
+      <c t="s" s="8" r="E108">
         <v>382</v>
       </c>
-      <c t="s" s="6" r="D108">
+    </row>
+    <row r="109">
+      <c s="11" r="A109"/>
+      <c t="s" s="8" r="B109">
         <v>383</v>
       </c>
-      <c t="s" s="6" r="E108">
+      <c t="s" s="8" r="C109">
         <v>384</v>
       </c>
-    </row>
-    <row r="109">
-      <c s="9" r="A109"/>
-      <c t="s" s="6" r="B109">
+      <c t="s" s="8" r="D109">
         <v>385</v>
       </c>
-      <c t="s" s="6" r="C109">
+      <c t="s" s="8" r="E109">
         <v>386</v>
       </c>
-      <c t="s" s="6" r="D109">
+    </row>
+    <row r="110">
+      <c s="11" r="A110"/>
+      <c t="s" s="8" r="B110">
         <v>387</v>
       </c>
-      <c t="s" s="6" r="E109">
+      <c t="s" s="8" r="C110">
         <v>388</v>
       </c>
-    </row>
-    <row r="110">
-      <c s="9" r="A110"/>
-      <c t="s" s="6" r="B110">
+      <c t="s" s="8" r="D110">
         <v>389</v>
       </c>
-      <c t="s" s="6" r="C110">
+      <c t="s" s="8" r="E110">
         <v>390</v>
       </c>
-      <c t="s" s="6" r="D110">
+    </row>
+    <row r="111">
+      <c s="11" r="A111"/>
+      <c t="s" s="8" r="B111">
         <v>391</v>
       </c>
-      <c t="s" s="6" r="E110">
+      <c t="s" s="8" r="C111">
         <v>392</v>
       </c>
-    </row>
-    <row r="111">
-      <c s="9" r="A111"/>
-      <c t="s" s="6" r="B111">
+      <c t="s" s="8" r="D111">
         <v>393</v>
       </c>
-      <c t="s" s="6" r="C111">
+      <c t="s" s="8" r="E111">
         <v>394</v>
       </c>
-      <c t="s" s="6" r="D111">
+    </row>
+    <row r="112">
+      <c s="11" r="A112"/>
+      <c t="s" s="8" r="B112">
         <v>395</v>
       </c>
-      <c t="s" s="6" r="E111">
+      <c t="s" s="8" r="C112">
         <v>396</v>
       </c>
-    </row>
-    <row r="112">
-      <c s="9" r="A112"/>
-      <c t="s" s="6" r="B112">
+      <c t="s" s="8" r="D112">
         <v>397</v>
       </c>
-      <c t="s" s="6" r="C112">
+      <c t="s" s="8" r="E112">
         <v>398</v>
       </c>
-      <c t="s" s="6" r="D112">
+    </row>
+    <row r="113">
+      <c s="11" r="A113"/>
+      <c t="s" s="8" r="B113">
         <v>399</v>
       </c>
-      <c t="s" s="6" r="E112">
+      <c t="s" s="8" r="C113">
         <v>400</v>
       </c>
-    </row>
-    <row r="113">
-      <c s="9" r="A113"/>
-      <c t="s" s="6" r="B113">
+      <c t="s" s="8" r="D113">
         <v>401</v>
       </c>
-      <c t="s" s="15" r="C113">
+      <c t="s" s="8" r="E113">
         <v>402</v>
       </c>
-      <c t="s" s="6" r="D113">
+    </row>
+    <row r="114">
+      <c s="11" r="A114"/>
+      <c t="s" s="8" r="B114">
         <v>403</v>
       </c>
-      <c t="s" s="6" r="E113">
+      <c t="s" s="17" r="C114">
         <v>404</v>
       </c>
-    </row>
-    <row r="114">
-      <c s="9" r="A114"/>
-      <c t="s" s="15" r="B114">
+      <c t="s" s="8" r="D114">
         <v>405</v>
       </c>
-      <c t="s" s="15" r="C114">
+      <c t="s" s="8" r="E114">
         <v>406</v>
       </c>
-      <c t="s" s="6" r="D114">
+    </row>
+    <row r="115">
+      <c s="11" r="A115"/>
+      <c t="s" s="17" r="B115">
         <v>407</v>
       </c>
-      <c t="s" s="6" r="E114">
+      <c t="s" s="17" r="C115">
         <v>408</v>
       </c>
-    </row>
-    <row r="115">
-      <c s="9" r="A115"/>
-      <c t="s" s="6" r="B115">
+      <c t="s" s="8" r="D115">
         <v>409</v>
       </c>
-      <c t="s" s="15" r="C115">
-        <v>406</v>
-      </c>
-      <c t="s" s="6" r="D115">
-        <v>407</v>
-      </c>
-      <c t="s" s="6" r="E115">
+      <c t="s" s="8" r="E115">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="116">
+      <c s="11" r="A116"/>
+      <c t="s" s="8" r="B116">
+        <v>411</v>
+      </c>
+      <c t="s" s="17" r="C116">
         <v>408</v>
       </c>
-    </row>
-    <row r="116">
-      <c s="9" r="A116"/>
-      <c t="s" s="6" r="B116">
+      <c t="s" s="8" r="D116">
+        <v>409</v>
+      </c>
+      <c t="s" s="8" r="E116">
         <v>410</v>
       </c>
-      <c t="s" s="4" r="C116">
-        <v>411</v>
-      </c>
-      <c t="s" s="6" r="D116">
+    </row>
+    <row r="117">
+      <c s="11" r="A117"/>
+      <c t="s" s="8" r="B117">
         <v>412</v>
       </c>
-      <c t="s" s="6" r="E116">
+      <c t="s" s="6" r="C117">
         <v>413</v>
       </c>
-    </row>
-    <row r="117">
-      <c s="9" r="A117"/>
-      <c t="s" s="6" r="B117">
+      <c t="s" s="8" r="D117">
         <v>414</v>
       </c>
-      <c t="s" s="4" r="C117">
+      <c t="s" s="8" r="E117">
         <v>415</v>
       </c>
-      <c t="s" s="6" r="D117">
+    </row>
+    <row r="118">
+      <c s="11" r="A118"/>
+      <c t="s" s="8" r="B118">
         <v>416</v>
       </c>
-      <c t="s" s="6" r="E117">
+      <c t="s" s="6" r="C118">
         <v>417</v>
       </c>
-    </row>
-    <row r="118">
-      <c s="9" r="A118"/>
-      <c t="s" s="6" r="B118">
+      <c t="s" s="8" r="D118">
         <v>418</v>
       </c>
-      <c t="s" s="4" r="C118">
+      <c t="s" s="8" r="E118">
         <v>419</v>
       </c>
-      <c t="s" s="6" r="D118">
+    </row>
+    <row r="119">
+      <c s="11" r="A119"/>
+      <c t="s" s="8" r="B119">
         <v>420</v>
       </c>
-      <c t="s" s="4" r="E118">
+      <c t="s" s="6" r="C119">
         <v>421</v>
       </c>
-    </row>
-    <row r="119">
-      <c s="9" r="A119"/>
-      <c s="17" r="B119"/>
-      <c s="8" r="C119"/>
-      <c s="17" r="D119"/>
-      <c s="17" r="E119"/>
+      <c t="s" s="8" r="D119">
+        <v>422</v>
+      </c>
+      <c t="s" s="6" r="E119">
+        <v>423</v>
+      </c>
     </row>
     <row r="120">
-      <c t="s" s="9" r="A120">
-        <v>422</v>
-      </c>
-      <c t="s" s="6" r="B120">
-        <v>423</v>
-      </c>
-      <c t="s" s="15" r="C120">
+      <c s="11" r="A120"/>
+      <c s="20" r="B120"/>
+      <c s="10" r="C120"/>
+      <c s="20" r="D120"/>
+      <c s="20" r="E120"/>
+    </row>
+    <row r="121">
+      <c t="s" s="11" r="A121">
         <v>424</v>
       </c>
-      <c t="s" s="6" r="D120">
+      <c t="s" s="8" r="B121">
         <v>425</v>
       </c>
-      <c t="s" s="6" r="E120">
+      <c t="s" s="17" r="C121">
         <v>426</v>
       </c>
-    </row>
-    <row r="121">
-      <c s="9" r="A121"/>
-      <c t="s" s="6" r="B121">
+      <c t="s" s="8" r="D121">
         <v>427</v>
       </c>
-      <c t="s" s="15" r="C121">
+      <c t="s" s="8" r="E121">
         <v>428</v>
       </c>
-      <c t="s" s="6" r="D121">
+    </row>
+    <row r="122">
+      <c s="11" r="A122"/>
+      <c t="s" s="8" r="B122">
         <v>429</v>
       </c>
-      <c t="s" s="6" r="E121">
+      <c t="s" s="17" r="C122">
         <v>430</v>
       </c>
-    </row>
-    <row r="122">
-      <c s="13" r="A122"/>
-      <c s="2" r="B122"/>
-      <c s="12" r="C122"/>
-      <c s="2" r="D122"/>
-      <c s="2" r="E122"/>
+      <c t="s" s="8" r="D122">
+        <v>431</v>
+      </c>
+      <c t="s" s="8" r="E122">
+        <v>432</v>
+      </c>
     </row>
     <row r="123">
-      <c t="s" s="9" r="A123">
-        <v>431</v>
-      </c>
-      <c t="s" s="6" r="B123">
-        <v>432</v>
-      </c>
-      <c t="s" s="15" r="C123">
+      <c s="15" r="A123"/>
+      <c t="s" s="5" r="B123">
         <v>433</v>
       </c>
-      <c t="s" s="6" r="D123">
+      <c t="s" s="4" r="C123">
         <v>434</v>
       </c>
-      <c t="s" s="6" r="E123">
+      <c s="5" r="D123"/>
+      <c s="5" r="E123"/>
+    </row>
+    <row r="124">
+      <c s="11" r="A124"/>
+      <c s="13" r="B124"/>
+      <c s="19" r="C124"/>
+      <c s="13" r="D124"/>
+      <c s="13" r="E124"/>
+    </row>
+    <row r="125">
+      <c t="s" s="11" r="A125">
         <v>435</v>
       </c>
-    </row>
-    <row r="124">
-      <c s="9" r="A124"/>
-      <c t="s" s="6" r="B124">
+      <c t="s" s="8" r="B125">
         <v>436</v>
       </c>
-      <c t="s" s="15" r="C124">
+      <c t="s" s="17" r="C125">
         <v>437</v>
       </c>
-      <c t="s" s="6" r="D124">
+      <c t="s" s="8" r="D125">
         <v>438</v>
       </c>
-      <c t="s" s="6" r="E124">
+      <c t="s" s="8" r="E125">
         <v>439</v>
       </c>
     </row>
-    <row r="125">
-      <c s="9" r="A125"/>
-      <c t="s" s="6" r="B125">
+    <row r="126">
+      <c s="11" r="A126"/>
+      <c t="s" s="8" r="B126">
         <v>440</v>
       </c>
-      <c t="s" s="15" r="C125">
+      <c t="s" s="17" r="C126">
         <v>441</v>
       </c>
-      <c t="s" s="6" r="D125">
+      <c t="s" s="8" r="D126">
         <v>442</v>
       </c>
-      <c t="s" s="6" r="E125">
+      <c t="s" s="8" r="E126">
         <v>443</v>
       </c>
     </row>
-    <row r="126">
-      <c s="9" r="A126"/>
-      <c t="s" s="6" r="B126">
+    <row r="127">
+      <c s="11" r="A127"/>
+      <c t="s" s="8" r="B127">
         <v>444</v>
       </c>
-      <c t="s" s="15" r="C126">
+      <c t="s" s="17" r="C127">
         <v>445</v>
       </c>
-      <c t="s" s="6" r="D126">
+      <c t="s" s="8" r="D127">
         <v>446</v>
       </c>
-      <c t="s" s="6" r="E126">
+      <c t="s" s="8" r="E127">
         <v>447</v>
       </c>
     </row>
-    <row r="127">
-      <c s="9" r="A127"/>
-      <c t="s" s="6" r="B127">
+    <row r="128">
+      <c s="11" r="A128"/>
+      <c t="s" s="8" r="B128">
         <v>448</v>
       </c>
-      <c t="s" s="15" r="C127">
+      <c t="s" s="17" r="C128">
         <v>449</v>
       </c>
-      <c t="s" s="6" r="D127">
+      <c t="s" s="8" r="D128">
         <v>450</v>
       </c>
-      <c t="s" s="6" r="E127">
+      <c t="s" s="8" r="E128">
         <v>451</v>
       </c>
     </row>
-    <row r="128">
-      <c s="9" r="A128"/>
-      <c s="2" r="B128"/>
-      <c s="12" r="C128"/>
-      <c s="2" r="D128"/>
-      <c s="2" r="E128"/>
-    </row>
     <row r="129">
-      <c t="s" s="9" r="A129">
+      <c s="11" r="A129"/>
+      <c t="s" s="8" r="B129">
         <v>452</v>
       </c>
-      <c t="s" s="14" r="B129">
+      <c t="s" s="17" r="C129">
         <v>453</v>
       </c>
-      <c t="s" s="1" r="C129">
-        <v>452</v>
-      </c>
-      <c s="14" r="D129"/>
-      <c s="14" r="E129"/>
+      <c t="s" s="8" r="D129">
+        <v>454</v>
+      </c>
+      <c t="s" s="8" r="E129">
+        <v>455</v>
+      </c>
     </row>
     <row r="130">
-      <c s="9" r="A130"/>
-      <c s="17" r="B130"/>
-      <c s="8" r="C130"/>
-      <c s="17" r="D130"/>
-      <c s="17" r="E130"/>
+      <c s="11" r="A130"/>
+      <c s="2" r="B130"/>
+      <c s="14" r="C130"/>
+      <c s="2" r="D130"/>
+      <c s="2" r="E130"/>
     </row>
     <row r="131">
-      <c t="s" s="9" r="A131">
-        <v>454</v>
-      </c>
-      <c t="s" s="20" r="B131">
-        <v>455</v>
-      </c>
-      <c t="s" s="18" r="C131">
+      <c t="s" s="11" r="A131">
         <v>456</v>
       </c>
-      <c s="20" r="D131"/>
-      <c s="20" r="E131"/>
+      <c t="s" s="16" r="B131">
+        <v>457</v>
+      </c>
+      <c t="s" s="1" r="C131">
+        <v>456</v>
+      </c>
+      <c s="16" r="D131"/>
+      <c s="16" r="E131"/>
     </row>
     <row r="132">
-      <c s="9" r="A132"/>
-      <c t="s" s="20" r="B132">
-        <v>457</v>
-      </c>
-      <c t="s" s="18" r="C132">
-        <v>458</v>
-      </c>
+      <c s="11" r="A132"/>
+      <c s="20" r="B132"/>
+      <c s="10" r="C132"/>
       <c s="20" r="D132"/>
       <c s="20" r="E132"/>
     </row>
     <row r="133">
-      <c s="9" r="A133"/>
-      <c s="17" r="B133"/>
-      <c s="8" r="C133"/>
-      <c s="17" r="D133"/>
-      <c s="17" r="E133"/>
+      <c t="s" s="11" r="A133">
+        <v>458</v>
+      </c>
+      <c t="s" s="23" r="B133">
+        <v>459</v>
+      </c>
+      <c t="s" s="21" r="C133">
+        <v>460</v>
+      </c>
+      <c s="23" r="D133"/>
+      <c s="23" r="E133"/>
     </row>
     <row r="134">
-      <c s="9" r="A134"/>
-      <c s="17" r="B134"/>
-      <c s="8" r="C134"/>
-      <c s="17" r="D134"/>
-      <c s="17" r="E134"/>
+      <c s="11" r="A134"/>
+      <c t="s" s="23" r="B134">
+        <v>461</v>
+      </c>
+      <c t="s" s="21" r="C134">
+        <v>462</v>
+      </c>
+      <c s="23" r="D134"/>
+      <c s="23" r="E134"/>
     </row>
     <row r="135">
-      <c s="9" r="A135"/>
-      <c s="17" r="B135"/>
-      <c s="8" r="C135"/>
-      <c s="17" r="D135"/>
-      <c s="17" r="E135"/>
+      <c s="11" r="A135"/>
+      <c s="20" r="B135"/>
+      <c s="10" r="C135"/>
+      <c s="20" r="D135"/>
+      <c s="20" r="E135"/>
+    </row>
+    <row r="136">
+      <c s="11" r="A136"/>
+      <c s="20" r="B136"/>
+      <c s="10" r="C136"/>
+      <c s="20" r="D136"/>
+      <c s="20" r="E136"/>
+    </row>
+    <row r="137">
+      <c s="11" r="A137"/>
+      <c s="20" r="B137"/>
+      <c s="10" r="C137"/>
+      <c s="20" r="D137"/>
+      <c s="20" r="E137"/>
     </row>
   </sheetData>
 </worksheet>
@@ -3631,164 +3695,164 @@
   <sheetFormatPr customHeight="1" defaultColWidth="9.86" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c s="19" r="A1"/>
-      <c s="19" r="B1"/>
-      <c s="19" r="C1"/>
-      <c s="19" r="D1"/>
-      <c s="19" r="E1"/>
-      <c s="19" r="F1"/>
+      <c s="22" r="A1"/>
+      <c s="22" r="B1"/>
+      <c s="22" r="C1"/>
+      <c s="22" r="D1"/>
+      <c s="22" r="E1"/>
+      <c s="22" r="F1"/>
     </row>
     <row r="2">
-      <c s="19" r="A2"/>
-      <c s="19" r="B2"/>
-      <c s="19" r="C2"/>
-      <c s="19" r="D2"/>
-      <c s="19" r="E2"/>
-      <c s="19" r="F2"/>
+      <c s="22" r="A2"/>
+      <c s="22" r="B2"/>
+      <c s="22" r="C2"/>
+      <c s="22" r="D2"/>
+      <c s="22" r="E2"/>
+      <c s="22" r="F2"/>
     </row>
     <row r="3">
-      <c s="19" r="A3"/>
-      <c s="19" r="B3"/>
-      <c s="19" r="C3"/>
-      <c s="19" r="D3"/>
-      <c s="19" r="E3"/>
-      <c s="19" r="F3"/>
+      <c s="22" r="A3"/>
+      <c s="22" r="B3"/>
+      <c s="22" r="C3"/>
+      <c s="22" r="D3"/>
+      <c s="22" r="E3"/>
+      <c s="22" r="F3"/>
     </row>
     <row r="4">
-      <c s="19" r="A4"/>
-      <c s="19" r="B4"/>
-      <c s="19" r="C4"/>
-      <c s="19" r="D4"/>
-      <c s="19" r="E4"/>
-      <c s="19" r="F4"/>
+      <c s="22" r="A4"/>
+      <c s="22" r="B4"/>
+      <c s="22" r="C4"/>
+      <c s="22" r="D4"/>
+      <c s="22" r="E4"/>
+      <c s="22" r="F4"/>
     </row>
     <row r="5">
-      <c s="19" r="A5"/>
-      <c s="19" r="B5"/>
-      <c s="19" r="C5"/>
-      <c s="19" r="D5"/>
-      <c s="19" r="E5"/>
-      <c s="19" r="F5"/>
+      <c s="22" r="A5"/>
+      <c s="22" r="B5"/>
+      <c s="22" r="C5"/>
+      <c s="22" r="D5"/>
+      <c s="22" r="E5"/>
+      <c s="22" r="F5"/>
     </row>
     <row r="6">
-      <c s="19" r="A6"/>
-      <c s="19" r="B6"/>
-      <c s="19" r="C6"/>
-      <c s="19" r="D6"/>
-      <c s="19" r="E6"/>
-      <c s="19" r="F6"/>
+      <c s="22" r="A6"/>
+      <c s="22" r="B6"/>
+      <c s="22" r="C6"/>
+      <c s="22" r="D6"/>
+      <c s="22" r="E6"/>
+      <c s="22" r="F6"/>
     </row>
     <row r="7">
-      <c s="19" r="A7"/>
-      <c s="19" r="B7"/>
-      <c s="19" r="C7"/>
-      <c s="19" r="D7"/>
-      <c s="19" r="E7"/>
-      <c s="19" r="F7"/>
+      <c s="22" r="A7"/>
+      <c s="22" r="B7"/>
+      <c s="22" r="C7"/>
+      <c s="22" r="D7"/>
+      <c s="22" r="E7"/>
+      <c s="22" r="F7"/>
     </row>
     <row r="8">
-      <c s="19" r="A8"/>
-      <c s="19" r="B8"/>
-      <c s="19" r="C8"/>
-      <c s="19" r="D8"/>
-      <c s="19" r="E8"/>
-      <c s="19" r="F8"/>
+      <c s="22" r="A8"/>
+      <c s="22" r="B8"/>
+      <c s="22" r="C8"/>
+      <c s="22" r="D8"/>
+      <c s="22" r="E8"/>
+      <c s="22" r="F8"/>
     </row>
     <row r="9">
-      <c s="19" r="A9"/>
-      <c s="19" r="B9"/>
-      <c s="19" r="C9"/>
-      <c s="19" r="D9"/>
-      <c s="19" r="E9"/>
-      <c s="19" r="F9"/>
+      <c s="22" r="A9"/>
+      <c s="22" r="B9"/>
+      <c s="22" r="C9"/>
+      <c s="22" r="D9"/>
+      <c s="22" r="E9"/>
+      <c s="22" r="F9"/>
     </row>
     <row r="10">
-      <c s="19" r="A10"/>
-      <c s="19" r="B10"/>
-      <c s="19" r="C10"/>
-      <c s="19" r="D10"/>
-      <c s="19" r="E10"/>
-      <c s="19" r="F10"/>
+      <c s="22" r="A10"/>
+      <c s="22" r="B10"/>
+      <c s="22" r="C10"/>
+      <c s="22" r="D10"/>
+      <c s="22" r="E10"/>
+      <c s="22" r="F10"/>
     </row>
     <row r="11">
-      <c s="19" r="A11"/>
-      <c s="19" r="B11"/>
-      <c s="19" r="C11"/>
-      <c s="19" r="D11"/>
-      <c s="19" r="E11"/>
-      <c s="19" r="F11"/>
+      <c s="22" r="A11"/>
+      <c s="22" r="B11"/>
+      <c s="22" r="C11"/>
+      <c s="22" r="D11"/>
+      <c s="22" r="E11"/>
+      <c s="22" r="F11"/>
     </row>
     <row r="12">
-      <c s="19" r="A12"/>
-      <c s="19" r="B12"/>
-      <c s="19" r="C12"/>
-      <c s="19" r="D12"/>
-      <c s="19" r="E12"/>
-      <c s="19" r="F12"/>
+      <c s="22" r="A12"/>
+      <c s="22" r="B12"/>
+      <c s="22" r="C12"/>
+      <c s="22" r="D12"/>
+      <c s="22" r="E12"/>
+      <c s="22" r="F12"/>
     </row>
     <row r="13">
-      <c s="19" r="A13"/>
-      <c s="19" r="B13"/>
-      <c s="19" r="C13"/>
-      <c s="19" r="D13"/>
-      <c s="19" r="E13"/>
-      <c s="19" r="F13"/>
+      <c s="22" r="A13"/>
+      <c s="22" r="B13"/>
+      <c s="22" r="C13"/>
+      <c s="22" r="D13"/>
+      <c s="22" r="E13"/>
+      <c s="22" r="F13"/>
     </row>
     <row r="14">
-      <c s="19" r="A14"/>
-      <c s="19" r="B14"/>
-      <c s="19" r="C14"/>
-      <c s="19" r="D14"/>
-      <c s="19" r="E14"/>
-      <c s="19" r="F14"/>
+      <c s="22" r="A14"/>
+      <c s="22" r="B14"/>
+      <c s="22" r="C14"/>
+      <c s="22" r="D14"/>
+      <c s="22" r="E14"/>
+      <c s="22" r="F14"/>
     </row>
     <row r="15">
-      <c s="19" r="A15"/>
-      <c s="19" r="B15"/>
-      <c s="19" r="C15"/>
-      <c s="19" r="D15"/>
-      <c s="19" r="E15"/>
-      <c s="19" r="F15"/>
+      <c s="22" r="A15"/>
+      <c s="22" r="B15"/>
+      <c s="22" r="C15"/>
+      <c s="22" r="D15"/>
+      <c s="22" r="E15"/>
+      <c s="22" r="F15"/>
     </row>
     <row r="16">
-      <c s="19" r="A16"/>
-      <c s="19" r="B16"/>
-      <c s="19" r="C16"/>
-      <c s="19" r="D16"/>
-      <c s="19" r="E16"/>
-      <c s="19" r="F16"/>
+      <c s="22" r="A16"/>
+      <c s="22" r="B16"/>
+      <c s="22" r="C16"/>
+      <c s="22" r="D16"/>
+      <c s="22" r="E16"/>
+      <c s="22" r="F16"/>
     </row>
     <row r="17">
-      <c s="19" r="A17"/>
-      <c s="19" r="B17"/>
-      <c s="19" r="C17"/>
-      <c s="19" r="D17"/>
-      <c s="19" r="E17"/>
-      <c s="19" r="F17"/>
+      <c s="22" r="A17"/>
+      <c s="22" r="B17"/>
+      <c s="22" r="C17"/>
+      <c s="22" r="D17"/>
+      <c s="22" r="E17"/>
+      <c s="22" r="F17"/>
     </row>
     <row r="18">
-      <c s="19" r="A18"/>
-      <c s="19" r="B18"/>
-      <c s="19" r="C18"/>
-      <c s="19" r="D18"/>
-      <c s="19" r="E18"/>
-      <c s="19" r="F18"/>
+      <c s="22" r="A18"/>
+      <c s="22" r="B18"/>
+      <c s="22" r="C18"/>
+      <c s="22" r="D18"/>
+      <c s="22" r="E18"/>
+      <c s="22" r="F18"/>
     </row>
     <row r="19">
-      <c s="19" r="A19"/>
-      <c s="19" r="B19"/>
-      <c s="19" r="C19"/>
-      <c s="19" r="D19"/>
-      <c s="19" r="E19"/>
-      <c s="19" r="F19"/>
+      <c s="22" r="A19"/>
+      <c s="22" r="B19"/>
+      <c s="22" r="C19"/>
+      <c s="22" r="D19"/>
+      <c s="22" r="E19"/>
+      <c s="22" r="F19"/>
     </row>
     <row r="20">
-      <c s="19" r="A20"/>
-      <c s="19" r="B20"/>
-      <c s="19" r="C20"/>
-      <c s="19" r="D20"/>
-      <c s="19" r="E20"/>
-      <c s="19" r="F20"/>
+      <c s="22" r="A20"/>
+      <c s="22" r="B20"/>
+      <c s="22" r="C20"/>
+      <c s="22" r="D20"/>
+      <c s="22" r="E20"/>
+      <c s="22" r="F20"/>
     </row>
   </sheetData>
 </worksheet>
@@ -3802,164 +3866,164 @@
   <sheetFormatPr customHeight="1" defaultColWidth="9.86" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c s="19" r="A1"/>
-      <c s="19" r="B1"/>
-      <c s="19" r="C1"/>
-      <c s="19" r="D1"/>
-      <c s="19" r="E1"/>
-      <c s="19" r="F1"/>
+      <c s="22" r="A1"/>
+      <c s="22" r="B1"/>
+      <c s="22" r="C1"/>
+      <c s="22" r="D1"/>
+      <c s="22" r="E1"/>
+      <c s="22" r="F1"/>
     </row>
     <row r="2">
-      <c s="19" r="A2"/>
-      <c s="19" r="B2"/>
-      <c s="19" r="C2"/>
-      <c s="19" r="D2"/>
-      <c s="19" r="E2"/>
-      <c s="19" r="F2"/>
+      <c s="22" r="A2"/>
+      <c s="22" r="B2"/>
+      <c s="22" r="C2"/>
+      <c s="22" r="D2"/>
+      <c s="22" r="E2"/>
+      <c s="22" r="F2"/>
     </row>
     <row r="3">
-      <c s="19" r="A3"/>
-      <c s="19" r="B3"/>
-      <c s="19" r="C3"/>
-      <c s="19" r="D3"/>
-      <c s="19" r="E3"/>
-      <c s="19" r="F3"/>
+      <c s="22" r="A3"/>
+      <c s="22" r="B3"/>
+      <c s="22" r="C3"/>
+      <c s="22" r="D3"/>
+      <c s="22" r="E3"/>
+      <c s="22" r="F3"/>
     </row>
     <row r="4">
-      <c s="19" r="A4"/>
-      <c s="19" r="B4"/>
-      <c s="19" r="C4"/>
-      <c s="19" r="D4"/>
-      <c s="19" r="E4"/>
-      <c s="19" r="F4"/>
+      <c s="22" r="A4"/>
+      <c s="22" r="B4"/>
+      <c s="22" r="C4"/>
+      <c s="22" r="D4"/>
+      <c s="22" r="E4"/>
+      <c s="22" r="F4"/>
     </row>
     <row r="5">
-      <c s="19" r="A5"/>
-      <c s="19" r="B5"/>
-      <c s="19" r="C5"/>
-      <c s="19" r="D5"/>
-      <c s="19" r="E5"/>
-      <c s="19" r="F5"/>
+      <c s="22" r="A5"/>
+      <c s="22" r="B5"/>
+      <c s="22" r="C5"/>
+      <c s="22" r="D5"/>
+      <c s="22" r="E5"/>
+      <c s="22" r="F5"/>
     </row>
     <row r="6">
-      <c s="19" r="A6"/>
-      <c s="19" r="B6"/>
-      <c s="19" r="C6"/>
-      <c s="19" r="D6"/>
-      <c s="19" r="E6"/>
-      <c s="19" r="F6"/>
+      <c s="22" r="A6"/>
+      <c s="22" r="B6"/>
+      <c s="22" r="C6"/>
+      <c s="22" r="D6"/>
+      <c s="22" r="E6"/>
+      <c s="22" r="F6"/>
     </row>
     <row r="7">
-      <c s="19" r="A7"/>
-      <c s="19" r="B7"/>
-      <c s="19" r="C7"/>
-      <c s="19" r="D7"/>
-      <c s="19" r="E7"/>
-      <c s="19" r="F7"/>
+      <c s="22" r="A7"/>
+      <c s="22" r="B7"/>
+      <c s="22" r="C7"/>
+      <c s="22" r="D7"/>
+      <c s="22" r="E7"/>
+      <c s="22" r="F7"/>
     </row>
     <row r="8">
-      <c s="19" r="A8"/>
-      <c s="19" r="B8"/>
-      <c s="19" r="C8"/>
-      <c s="19" r="D8"/>
-      <c s="19" r="E8"/>
-      <c s="19" r="F8"/>
+      <c s="22" r="A8"/>
+      <c s="22" r="B8"/>
+      <c s="22" r="C8"/>
+      <c s="22" r="D8"/>
+      <c s="22" r="E8"/>
+      <c s="22" r="F8"/>
     </row>
     <row r="9">
-      <c s="19" r="A9"/>
-      <c s="19" r="B9"/>
-      <c s="19" r="C9"/>
-      <c s="19" r="D9"/>
-      <c s="19" r="E9"/>
-      <c s="19" r="F9"/>
+      <c s="22" r="A9"/>
+      <c s="22" r="B9"/>
+      <c s="22" r="C9"/>
+      <c s="22" r="D9"/>
+      <c s="22" r="E9"/>
+      <c s="22" r="F9"/>
     </row>
     <row r="10">
-      <c s="19" r="A10"/>
-      <c s="19" r="B10"/>
-      <c s="19" r="C10"/>
-      <c s="19" r="D10"/>
-      <c s="19" r="E10"/>
-      <c s="19" r="F10"/>
+      <c s="22" r="A10"/>
+      <c s="22" r="B10"/>
+      <c s="22" r="C10"/>
+      <c s="22" r="D10"/>
+      <c s="22" r="E10"/>
+      <c s="22" r="F10"/>
     </row>
     <row r="11">
-      <c s="19" r="A11"/>
-      <c s="19" r="B11"/>
-      <c s="19" r="C11"/>
-      <c s="19" r="D11"/>
-      <c s="19" r="E11"/>
-      <c s="19" r="F11"/>
+      <c s="22" r="A11"/>
+      <c s="22" r="B11"/>
+      <c s="22" r="C11"/>
+      <c s="22" r="D11"/>
+      <c s="22" r="E11"/>
+      <c s="22" r="F11"/>
     </row>
     <row r="12">
-      <c s="19" r="A12"/>
-      <c s="19" r="B12"/>
-      <c s="19" r="C12"/>
-      <c s="19" r="D12"/>
-      <c s="19" r="E12"/>
-      <c s="19" r="F12"/>
+      <c s="22" r="A12"/>
+      <c s="22" r="B12"/>
+      <c s="22" r="C12"/>
+      <c s="22" r="D12"/>
+      <c s="22" r="E12"/>
+      <c s="22" r="F12"/>
     </row>
     <row r="13">
-      <c s="19" r="A13"/>
-      <c s="19" r="B13"/>
-      <c s="19" r="C13"/>
-      <c s="19" r="D13"/>
-      <c s="19" r="E13"/>
-      <c s="19" r="F13"/>
+      <c s="22" r="A13"/>
+      <c s="22" r="B13"/>
+      <c s="22" r="C13"/>
+      <c s="22" r="D13"/>
+      <c s="22" r="E13"/>
+      <c s="22" r="F13"/>
     </row>
     <row r="14">
-      <c s="19" r="A14"/>
-      <c s="19" r="B14"/>
-      <c s="19" r="C14"/>
-      <c s="19" r="D14"/>
-      <c s="19" r="E14"/>
-      <c s="19" r="F14"/>
+      <c s="22" r="A14"/>
+      <c s="22" r="B14"/>
+      <c s="22" r="C14"/>
+      <c s="22" r="D14"/>
+      <c s="22" r="E14"/>
+      <c s="22" r="F14"/>
     </row>
     <row r="15">
-      <c s="19" r="A15"/>
-      <c s="19" r="B15"/>
-      <c s="19" r="C15"/>
-      <c s="19" r="D15"/>
-      <c s="19" r="E15"/>
-      <c s="19" r="F15"/>
+      <c s="22" r="A15"/>
+      <c s="22" r="B15"/>
+      <c s="22" r="C15"/>
+      <c s="22" r="D15"/>
+      <c s="22" r="E15"/>
+      <c s="22" r="F15"/>
     </row>
     <row r="16">
-      <c s="19" r="A16"/>
-      <c s="19" r="B16"/>
-      <c s="19" r="C16"/>
-      <c s="19" r="D16"/>
-      <c s="19" r="E16"/>
-      <c s="19" r="F16"/>
+      <c s="22" r="A16"/>
+      <c s="22" r="B16"/>
+      <c s="22" r="C16"/>
+      <c s="22" r="D16"/>
+      <c s="22" r="E16"/>
+      <c s="22" r="F16"/>
     </row>
     <row r="17">
-      <c s="19" r="A17"/>
-      <c s="19" r="B17"/>
-      <c s="19" r="C17"/>
-      <c s="19" r="D17"/>
-      <c s="19" r="E17"/>
-      <c s="19" r="F17"/>
+      <c s="22" r="A17"/>
+      <c s="22" r="B17"/>
+      <c s="22" r="C17"/>
+      <c s="22" r="D17"/>
+      <c s="22" r="E17"/>
+      <c s="22" r="F17"/>
     </row>
     <row r="18">
-      <c s="19" r="A18"/>
-      <c s="19" r="B18"/>
-      <c s="19" r="C18"/>
-      <c s="19" r="D18"/>
-      <c s="19" r="E18"/>
-      <c s="19" r="F18"/>
+      <c s="22" r="A18"/>
+      <c s="22" r="B18"/>
+      <c s="22" r="C18"/>
+      <c s="22" r="D18"/>
+      <c s="22" r="E18"/>
+      <c s="22" r="F18"/>
     </row>
     <row r="19">
-      <c s="19" r="A19"/>
-      <c s="19" r="B19"/>
-      <c s="19" r="C19"/>
-      <c s="19" r="D19"/>
-      <c s="19" r="E19"/>
-      <c s="19" r="F19"/>
+      <c s="22" r="A19"/>
+      <c s="22" r="B19"/>
+      <c s="22" r="C19"/>
+      <c s="22" r="D19"/>
+      <c s="22" r="E19"/>
+      <c s="22" r="F19"/>
     </row>
     <row r="20">
-      <c s="19" r="A20"/>
-      <c s="19" r="B20"/>
-      <c s="19" r="C20"/>
-      <c s="19" r="D20"/>
-      <c s="19" r="E20"/>
-      <c s="19" r="F20"/>
+      <c s="22" r="A20"/>
+      <c s="22" r="B20"/>
+      <c s="22" r="C20"/>
+      <c s="22" r="D20"/>
+      <c s="22" r="E20"/>
+      <c s="22" r="F20"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
EWD-22382 - CUD Experience: Delete
Former-commit-id: 9ec27b5374cf39cb9b6ce3a8833d7d0b6f1a616a
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="467">
   <si>
     <t>Page</t>
   </si>
@@ -498,16 +498,10 @@
     <t>Anzahl der verwandten Ziele</t>
   </si>
   <si>
-    <t>experienceListIsEmpty</t>
-  </si>
-  <si>
-    <t>Experience list is empty</t>
-  </si>
-  <si>
-    <t>Ervaringenlijst is leeg</t>
-  </si>
-  <si>
-    <t>Liste der Umgebungen ist leer</t>
+    <t>experiencesListIsEmpty</t>
+  </si>
+  <si>
+    <t>Experiences list is empty</t>
   </si>
   <si>
     <t>experienceCannotBeDeleted</t>
@@ -516,76 +510,76 @@
     <t>Experience cannot be deleted while it has related Learning Objective(s)</t>
   </si>
   <si>
+    <t>CreateObjective</t>
+  </si>
+  <si>
+    <t>createNewObjective</t>
+  </si>
+  <si>
+    <t>Create New Objective</t>
+  </si>
+  <si>
+    <t>Nieuwe doelstelling aanmaken</t>
+  </si>
+  <si>
+    <t>Neues Lernziel erstellen</t>
+  </si>
+  <si>
+    <t>createObjectiveTip</t>
+  </si>
+  <si>
+    <t>Type objective title here</t>
+  </si>
+  <si>
+    <t>Typ hier de titel van de doelstelling</t>
+  </si>
+  <si>
+    <t>Titel des Lernziels hier eingeben</t>
+  </si>
+  <si>
+    <t>CreateExperience</t>
+  </si>
+  <si>
+    <t>newExperience</t>
+  </si>
+  <si>
+    <t>New Experience</t>
+  </si>
+  <si>
+    <t>experienceTitle</t>
+  </si>
+  <si>
+    <t>Experience title</t>
+  </si>
+  <si>
+    <t>experienceTitlePlaceholder</t>
+  </si>
+  <si>
+    <t>Experience title...</t>
+  </si>
+  <si>
+    <t>objectivesInExperience</t>
+  </si>
+  <si>
+    <t>Objectives in experience</t>
+  </si>
+  <si>
+    <t>typeExperienceTitleHere</t>
+  </si>
+  <si>
+    <t>Type experience title here</t>
+  </si>
+  <si>
+    <t>Typ hier de titel van de ervaring</t>
+  </si>
+  <si>
+    <t>Titel der Umgebung hier eingeben</t>
+  </si>
+  <si>
     <t>clickToAddExperience</t>
   </si>
   <si>
     <t>Click to add experience</t>
-  </si>
-  <si>
-    <t>CreateObjective</t>
-  </si>
-  <si>
-    <t>createNewObjective</t>
-  </si>
-  <si>
-    <t>Create New Objective</t>
-  </si>
-  <si>
-    <t>Nieuwe doelstelling aanmaken</t>
-  </si>
-  <si>
-    <t>Neues Lernziel erstellen</t>
-  </si>
-  <si>
-    <t>createObjectiveTip</t>
-  </si>
-  <si>
-    <t>Type objective title here</t>
-  </si>
-  <si>
-    <t>Typ hier de titel van de doelstelling</t>
-  </si>
-  <si>
-    <t>Titel des Lernziels hier eingeben</t>
-  </si>
-  <si>
-    <t>CreateExperience</t>
-  </si>
-  <si>
-    <t>newExperience</t>
-  </si>
-  <si>
-    <t>New Experience</t>
-  </si>
-  <si>
-    <t>experienceTitle</t>
-  </si>
-  <si>
-    <t>Experience title</t>
-  </si>
-  <si>
-    <t>experienceTitlePlaceholder</t>
-  </si>
-  <si>
-    <t>Experience title...</t>
-  </si>
-  <si>
-    <t>objectivesInExperience</t>
-  </si>
-  <si>
-    <t>Objectives in experience</t>
-  </si>
-  <si>
-    <t>typeExperienceTitleHere</t>
-  </si>
-  <si>
-    <t>Type experience title here</t>
-  </si>
-  <si>
-    <t>Typ hier de titel van de ervaring</t>
-  </si>
-  <si>
-    <t>Titel der Umgebung hier eingeben</t>
   </si>
   <si>
     <t>Klik om ervaring toe te voegen</t>
@@ -2428,52 +2422,52 @@
     </row>
     <row r="45">
       <c s="12" r="A45"/>
-      <c t="s" s="7" r="B45">
+      <c t="s" s="4" r="B45">
         <v>161</v>
       </c>
-      <c t="s" s="7" r="C45">
+      <c t="s" s="4" r="C45">
         <v>162</v>
       </c>
-      <c t="s" s="7" r="D45">
-        <v>163</v>
-      </c>
-      <c t="s" s="7" r="E45">
-        <v>164</v>
-      </c>
+      <c s="4" r="D45"/>
+      <c s="4" r="E45"/>
     </row>
     <row r="46">
       <c s="12" r="A46"/>
       <c t="s" s="4" r="B46">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c t="s" s="4" r="C46">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c s="4" r="D46"/>
       <c s="4" r="E46"/>
     </row>
     <row r="47">
       <c s="12" r="A47"/>
-      <c t="s" s="4" r="B47">
+      <c s="12" r="B47"/>
+      <c s="12" r="C47"/>
+      <c s="12" r="D47"/>
+      <c s="12" r="E47"/>
+    </row>
+    <row r="48">
+      <c t="s" s="12" r="A48">
+        <v>165</v>
+      </c>
+      <c t="s" s="7" r="B48">
+        <v>166</v>
+      </c>
+      <c t="s" s="7" r="C48">
         <v>167</v>
       </c>
-      <c t="s" s="4" r="C47">
+      <c t="s" s="7" r="D48">
         <v>168</v>
       </c>
-      <c s="4" r="D47"/>
-      <c s="4" r="E47"/>
-    </row>
-    <row r="48">
-      <c s="12" r="A48"/>
-      <c s="12" r="B48"/>
-      <c s="12" r="C48"/>
-      <c s="12" r="D48"/>
-      <c s="12" r="E48"/>
+      <c t="s" s="7" r="E48">
+        <v>169</v>
+      </c>
     </row>
     <row r="49">
-      <c t="s" s="12" r="A49">
-        <v>169</v>
-      </c>
+      <c s="12" r="A49"/>
       <c t="s" s="7" r="B49">
         <v>170</v>
       </c>
@@ -2487,37 +2481,33 @@
         <v>173</v>
       </c>
     </row>
-    <row r="50">
-      <c s="12" r="A50"/>
-      <c t="s" s="7" r="B50">
+    <row r="51">
+      <c s="2" r="A51"/>
+      <c s="2" r="B51"/>
+      <c s="2" r="C51"/>
+      <c s="2" r="D51"/>
+      <c s="2" r="E51"/>
+    </row>
+    <row r="52">
+      <c t="s" s="12" r="A52">
         <v>174</v>
       </c>
-      <c t="s" s="7" r="C50">
+      <c t="s" s="15" r="B52">
         <v>175</v>
       </c>
-      <c t="s" s="7" r="D50">
+      <c t="s" s="15" r="C52">
         <v>176</v>
       </c>
-      <c t="s" s="7" r="E50">
+      <c s="15" r="D52"/>
+      <c s="15" r="E52"/>
+    </row>
+    <row r="53">
+      <c s="12" r="A53"/>
+      <c t="s" s="15" r="B53">
         <v>177</v>
       </c>
-    </row>
-    <row r="52">
-      <c s="2" r="A52"/>
-      <c s="2" r="B52"/>
-      <c s="2" r="C52"/>
-      <c s="2" r="D52"/>
-      <c s="2" r="E52"/>
-    </row>
-    <row r="53">
-      <c t="s" s="12" r="A53">
+      <c t="s" s="15" r="C53">
         <v>178</v>
-      </c>
-      <c t="s" s="15" r="B53">
-        <v>179</v>
-      </c>
-      <c t="s" s="15" r="C53">
-        <v>180</v>
       </c>
       <c s="15" r="D53"/>
       <c s="15" r="E53"/>
@@ -2525,10 +2515,10 @@
     <row r="54">
       <c s="12" r="A54"/>
       <c t="s" s="15" r="B54">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c t="s" s="15" r="C54">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c s="15" r="D54"/>
       <c s="15" r="E54"/>
@@ -2536,24 +2526,28 @@
     <row r="55">
       <c s="12" r="A55"/>
       <c t="s" s="15" r="B55">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c t="s" s="15" r="C55">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c s="15" r="D55"/>
       <c s="15" r="E55"/>
     </row>
     <row r="56">
       <c s="12" r="A56"/>
-      <c t="s" s="15" r="B56">
+      <c t="s" s="7" r="B56">
+        <v>183</v>
+      </c>
+      <c t="s" s="7" r="C56">
+        <v>184</v>
+      </c>
+      <c t="s" s="7" r="D56">
         <v>185</v>
       </c>
-      <c t="s" s="15" r="C56">
+      <c t="s" s="7" r="E56">
         <v>186</v>
       </c>
-      <c s="15" r="D56"/>
-      <c s="15" r="E56"/>
     </row>
     <row r="57">
       <c s="12" r="A57"/>
@@ -2572,476 +2566,476 @@
     </row>
     <row r="58">
       <c s="12" r="A58"/>
-      <c t="s" s="7" r="B58">
-        <v>167</v>
-      </c>
-      <c t="s" s="7" r="C58">
-        <v>168</v>
-      </c>
-      <c t="s" s="7" r="D58">
+      <c t="s" s="4" r="B58">
         <v>191</v>
       </c>
-      <c t="s" s="7" r="E58">
+      <c t="s" s="4" r="C58">
         <v>192</v>
+      </c>
+      <c t="s" s="4" r="D58">
+        <v>193</v>
+      </c>
+      <c t="s" s="4" r="E58">
+        <v>194</v>
       </c>
     </row>
     <row r="59">
       <c s="12" r="A59"/>
-      <c t="s" s="4" r="B59">
-        <v>193</v>
-      </c>
-      <c t="s" s="4" r="C59">
-        <v>194</v>
-      </c>
-      <c t="s" s="4" r="D59">
+      <c s="12" r="B59"/>
+      <c s="12" r="C59"/>
+      <c s="12" r="D59"/>
+      <c s="12" r="E59"/>
+    </row>
+    <row r="60">
+      <c t="s" s="12" r="A60">
         <v>195</v>
       </c>
-      <c t="s" s="4" r="E59">
+      <c t="s" s="7" r="B60">
         <v>196</v>
       </c>
-    </row>
-    <row r="60">
-      <c s="12" r="A60"/>
-      <c s="12" r="B60"/>
-      <c s="12" r="C60"/>
-      <c s="12" r="D60"/>
-      <c s="12" r="E60"/>
+      <c t="s" s="7" r="C60">
+        <v>197</v>
+      </c>
+      <c t="s" s="7" r="D60">
+        <v>198</v>
+      </c>
+      <c t="s" s="7" r="E60">
+        <v>17</v>
+      </c>
     </row>
     <row r="61">
-      <c t="s" s="12" r="A61">
-        <v>197</v>
-      </c>
+      <c s="12" r="A61"/>
       <c t="s" s="7" r="B61">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c t="s" s="7" r="C61">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c t="s" s="7" r="D61">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c t="s" s="7" r="E61">
-        <v>17</v>
+        <v>202</v>
       </c>
     </row>
     <row r="62">
       <c s="12" r="A62"/>
       <c t="s" s="7" r="B62">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c t="s" s="7" r="C62">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c t="s" s="7" r="D62">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c t="s" s="7" r="E62">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="63">
       <c s="12" r="A63"/>
       <c t="s" s="7" r="B63">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c t="s" s="7" r="C63">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c t="s" s="7" r="D63">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c t="s" s="7" r="E63">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="64">
       <c s="12" r="A64"/>
       <c t="s" s="7" r="B64">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c t="s" s="7" r="C64">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c t="s" s="7" r="D64">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c t="s" s="7" r="E64">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="65">
       <c s="12" r="A65"/>
       <c t="s" s="7" r="B65">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c t="s" s="7" r="C65">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c t="s" s="7" r="D65">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c t="s" s="7" r="E65">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="66">
       <c s="12" r="A66"/>
       <c t="s" s="7" r="B66">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c t="s" s="7" r="C66">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c t="s" s="7" r="D66">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c t="s" s="7" r="E66">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="67">
       <c s="12" r="A67"/>
       <c t="s" s="7" r="B67">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c t="s" s="7" r="C67">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c t="s" s="7" r="D67">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c t="s" s="7" r="E67">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="68">
       <c s="12" r="A68"/>
       <c t="s" s="7" r="B68">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c t="s" s="7" r="C68">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c t="s" s="7" r="D68">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c t="s" s="7" r="E68">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="69">
       <c s="12" r="A69"/>
-      <c t="s" s="7" r="B69">
-        <v>229</v>
-      </c>
-      <c t="s" s="7" r="C69">
-        <v>230</v>
-      </c>
-      <c t="s" s="7" r="D69">
+      <c s="12" r="B69"/>
+      <c s="12" r="C69"/>
+      <c s="12" r="D69"/>
+      <c s="12" r="E69"/>
+    </row>
+    <row r="70">
+      <c t="s" s="12" r="A70">
         <v>231</v>
       </c>
-      <c t="s" s="7" r="E69">
+      <c t="s" s="7" r="B70">
         <v>232</v>
       </c>
-    </row>
-    <row r="70">
-      <c s="12" r="A70"/>
-      <c s="12" r="B70"/>
-      <c s="12" r="C70"/>
-      <c s="12" r="D70"/>
-      <c s="12" r="E70"/>
+      <c t="s" s="7" r="C70">
+        <v>233</v>
+      </c>
+      <c t="s" s="7" r="D70">
+        <v>234</v>
+      </c>
+      <c t="s" s="7" r="E70">
+        <v>235</v>
+      </c>
     </row>
     <row r="71">
-      <c t="s" s="12" r="A71">
-        <v>233</v>
-      </c>
+      <c s="12" r="A71"/>
       <c t="s" s="7" r="B71">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c t="s" s="7" r="C71">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c t="s" s="7" r="D71">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c t="s" s="7" r="E71">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="72">
-      <c s="12" r="A72"/>
+      <c s="10" r="A72"/>
       <c t="s" s="7" r="B72">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c t="s" s="7" r="C72">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c t="s" s="7" r="D72">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c t="s" s="7" r="E72">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="73">
       <c s="10" r="A73"/>
       <c t="s" s="7" r="B73">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c t="s" s="7" r="C73">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c t="s" s="7" r="D73">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c t="s" s="7" r="E73">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="74">
       <c s="10" r="A74"/>
       <c t="s" s="7" r="B74">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c t="s" s="7" r="C74">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c t="s" s="7" r="D74">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c t="s" s="7" r="E74">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="75">
       <c s="10" r="A75"/>
       <c t="s" s="7" r="B75">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c t="s" s="7" r="C75">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c t="s" s="7" r="D75">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c t="s" s="7" r="E75">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="76">
       <c s="10" r="A76"/>
       <c t="s" s="7" r="B76">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c t="s" s="7" r="C76">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c t="s" s="7" r="D76">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c t="s" s="7" r="E76">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="77">
       <c s="10" r="A77"/>
       <c t="s" s="7" r="B77">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c t="s" s="7" r="C77">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c t="s" s="7" r="D77">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c t="s" s="7" r="E77">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="78">
       <c s="10" r="A78"/>
       <c t="s" s="7" r="B78">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c t="s" s="7" r="C78">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c t="s" s="7" r="D78">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c t="s" s="7" r="E78">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="79">
       <c s="10" r="A79"/>
       <c t="s" s="7" r="B79">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c t="s" s="7" r="C79">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c t="s" s="7" r="D79">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c t="s" s="7" r="E79">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="80">
       <c s="10" r="A80"/>
       <c t="s" s="7" r="B80">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c t="s" s="7" r="C80">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c t="s" s="7" r="D80">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c t="s" s="7" r="E80">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="81">
       <c s="10" r="A81"/>
       <c t="s" s="7" r="B81">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c t="s" s="7" r="C81">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c t="s" s="7" r="D81">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c t="s" s="7" r="E81">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="82">
       <c s="10" r="A82"/>
       <c t="s" s="7" r="B82">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c t="s" s="7" r="C82">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c t="s" s="7" r="D82">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c t="s" s="7" r="E82">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="83">
       <c s="10" r="A83"/>
       <c t="s" s="7" r="B83">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c t="s" s="7" r="C83">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c t="s" s="7" r="D83">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c t="s" s="7" r="E83">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="84">
       <c s="10" r="A84"/>
-      <c t="s" s="7" r="B84">
-        <v>286</v>
-      </c>
-      <c t="s" s="7" r="C84">
-        <v>287</v>
-      </c>
-      <c t="s" s="7" r="D84">
+      <c s="12" r="B84"/>
+      <c s="12" r="C84"/>
+      <c s="12" r="D84"/>
+      <c s="12" r="E84"/>
+    </row>
+    <row r="85">
+      <c t="s" s="10" r="A85">
         <v>288</v>
       </c>
-      <c t="s" s="7" r="E84">
+      <c t="s" s="7" r="B85">
         <v>289</v>
       </c>
-    </row>
-    <row r="85">
-      <c s="10" r="A85"/>
-      <c s="12" r="B85"/>
-      <c s="12" r="C85"/>
-      <c s="12" r="D85"/>
-      <c s="12" r="E85"/>
+      <c t="s" s="7" r="C85">
+        <v>290</v>
+      </c>
+      <c t="s" s="7" r="D85">
+        <v>291</v>
+      </c>
+      <c t="s" s="7" r="E85">
+        <v>292</v>
+      </c>
     </row>
     <row r="86">
-      <c t="s" s="10" r="A86">
-        <v>290</v>
-      </c>
+      <c s="10" r="A86"/>
       <c t="s" s="7" r="B86">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c t="s" s="7" r="C86">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c t="s" s="7" r="D86">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c t="s" s="7" r="E86">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="87">
       <c s="10" r="A87"/>
       <c t="s" s="7" r="B87">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c t="s" s="7" r="C87">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c t="s" s="7" r="D87">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c t="s" s="7" r="E87">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="88">
       <c s="10" r="A88"/>
       <c t="s" s="7" r="B88">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c t="s" s="7" r="C88">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c t="s" s="7" r="D88">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c t="s" s="7" r="E88">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="89">
       <c s="10" r="A89"/>
       <c t="s" s="7" r="B89">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c t="s" s="7" r="C89">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c t="s" s="7" r="D89">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c t="s" s="7" r="E89">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="90">
       <c s="10" r="A90"/>
       <c t="s" s="7" r="B90">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c t="s" s="7" r="C90">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c t="s" s="7" r="D90">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c t="s" s="7" r="E90">
         <v>310</v>
@@ -3050,637 +3044,633 @@
     <row r="91">
       <c s="10" r="A91"/>
       <c t="s" s="7" r="B91">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c t="s" s="7" r="C91">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c t="s" s="7" r="D91">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c t="s" s="7" r="E91">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="92">
       <c s="10" r="A92"/>
       <c t="s" s="7" r="B92">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c t="s" s="7" r="C92">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c t="s" s="7" r="D92">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c t="s" s="7" r="E92">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="93">
       <c s="10" r="A93"/>
       <c t="s" s="7" r="B93">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c t="s" s="7" r="C93">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c t="s" s="7" r="D93">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c t="s" s="7" r="E93">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="94">
       <c s="10" r="A94"/>
       <c t="s" s="7" r="B94">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c t="s" s="7" r="C94">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c t="s" s="7" r="D94">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c t="s" s="7" r="E94">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="95">
       <c s="10" r="A95"/>
       <c t="s" s="7" r="B95">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c t="s" s="7" r="C95">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c t="s" s="7" r="D95">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c t="s" s="7" r="E95">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="96">
       <c s="10" r="A96"/>
       <c t="s" s="7" r="B96">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c t="s" s="7" r="C96">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c t="s" s="7" r="D96">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c t="s" s="7" r="E96">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="97">
       <c s="10" r="A97"/>
       <c t="s" s="7" r="B97">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c t="s" s="7" r="C97">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c t="s" s="7" r="D97">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c t="s" s="7" r="E97">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="98">
       <c s="10" r="A98"/>
       <c t="s" s="7" r="B98">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c t="s" s="7" r="C98">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c t="s" s="7" r="D98">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c t="s" s="7" r="E98">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="99">
       <c s="10" r="A99"/>
-      <c t="s" s="7" r="B99">
-        <v>340</v>
+      <c t="s" s="16" r="B99">
+        <v>342</v>
       </c>
       <c t="s" s="7" r="C99">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c t="s" s="7" r="D99">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c t="s" s="7" r="E99">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="100">
       <c s="10" r="A100"/>
-      <c t="s" s="16" r="B100">
-        <v>344</v>
+      <c t="s" s="7" r="B100">
+        <v>345</v>
       </c>
       <c t="s" s="7" r="C100">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c t="s" s="7" r="D100">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c t="s" s="7" r="E100">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="101">
       <c s="10" r="A101"/>
       <c t="s" s="7" r="B101">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c t="s" s="7" r="C101">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c t="s" s="7" r="D101">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c t="s" s="7" r="E101">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="102">
       <c s="10" r="A102"/>
       <c t="s" s="7" r="B102">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c t="s" s="7" r="C102">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c t="s" s="7" r="D102">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c t="s" s="7" r="E102">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="103">
       <c s="10" r="A103"/>
       <c t="s" s="7" r="B103">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c t="s" s="7" r="C103">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c t="s" s="7" r="D103">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c t="s" s="7" r="E103">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="104">
       <c s="10" r="A104"/>
       <c t="s" s="7" r="B104">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c t="s" s="7" r="C104">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c t="s" s="7" r="D104">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c t="s" s="7" r="E104">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="105">
       <c s="10" r="A105"/>
       <c t="s" s="7" r="B105">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c t="s" s="7" r="C105">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c t="s" s="7" r="D105">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c t="s" s="7" r="E105">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="106">
       <c s="10" r="A106"/>
       <c t="s" s="7" r="B106">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c t="s" s="7" r="C106">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c t="s" s="7" r="D106">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c t="s" s="7" r="E106">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="107">
       <c s="10" r="A107"/>
       <c t="s" s="7" r="B107">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c t="s" s="7" r="C107">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c t="s" s="7" r="D107">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c t="s" s="7" r="E107">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="108">
       <c s="10" r="A108"/>
       <c t="s" s="7" r="B108">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c t="s" s="7" r="C108">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c t="s" s="7" r="D108">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c t="s" s="7" r="E108">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="109">
       <c s="10" r="A109"/>
       <c t="s" s="7" r="B109">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c t="s" s="7" r="C109">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c t="s" s="7" r="D109">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c t="s" s="7" r="E109">
-        <v>382</v>
+        <v>384</v>
       </c>
     </row>
     <row r="110">
       <c s="10" r="A110"/>
       <c t="s" s="7" r="B110">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c t="s" s="7" r="C110">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c t="s" s="7" r="D110">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c t="s" s="7" r="E110">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="111">
       <c s="10" r="A111"/>
       <c t="s" s="7" r="B111">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c t="s" s="7" r="C111">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c t="s" s="7" r="D111">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c t="s" s="7" r="E111">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="112">
       <c s="10" r="A112"/>
       <c t="s" s="7" r="B112">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c t="s" s="7" r="C112">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c t="s" s="7" r="D112">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c t="s" s="7" r="E112">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="113">
       <c s="10" r="A113"/>
       <c t="s" s="7" r="B113">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c t="s" s="7" r="C113">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c t="s" s="7" r="D113">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c t="s" s="7" r="E113">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="114">
       <c s="10" r="A114"/>
       <c t="s" s="7" r="B114">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c t="s" s="7" r="C114">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c t="s" s="7" r="D114">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c t="s" s="7" r="E114">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="115">
       <c s="10" r="A115"/>
       <c t="s" s="7" r="B115">
-        <v>403</v>
-      </c>
-      <c t="s" s="7" r="C115">
-        <v>404</v>
+        <v>405</v>
+      </c>
+      <c t="s" s="16" r="C115">
+        <v>406</v>
       </c>
       <c t="s" s="7" r="D115">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c t="s" s="7" r="E115">
-        <v>406</v>
+        <v>408</v>
       </c>
     </row>
     <row r="116">
       <c s="10" r="A116"/>
-      <c t="s" s="7" r="B116">
-        <v>407</v>
+      <c t="s" s="16" r="B116">
+        <v>409</v>
       </c>
       <c t="s" s="16" r="C116">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c t="s" s="7" r="D116">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c t="s" s="7" r="E116">
-        <v>410</v>
+        <v>412</v>
       </c>
     </row>
     <row r="117">
       <c s="10" r="A117"/>
-      <c t="s" s="16" r="B117">
+      <c t="s" s="7" r="B117">
+        <v>413</v>
+      </c>
+      <c t="s" s="16" r="C117">
+        <v>410</v>
+      </c>
+      <c t="s" s="7" r="D117">
         <v>411</v>
       </c>
-      <c t="s" s="16" r="C117">
+      <c t="s" s="7" r="E117">
         <v>412</v>
-      </c>
-      <c t="s" s="7" r="D117">
-        <v>413</v>
-      </c>
-      <c t="s" s="7" r="E117">
-        <v>414</v>
       </c>
     </row>
     <row r="118">
       <c s="10" r="A118"/>
       <c t="s" s="7" r="B118">
+        <v>414</v>
+      </c>
+      <c t="s" s="5" r="C118">
         <v>415</v>
       </c>
-      <c t="s" s="16" r="C118">
-        <v>412</v>
-      </c>
       <c t="s" s="7" r="D118">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c t="s" s="7" r="E118">
-        <v>414</v>
+        <v>417</v>
       </c>
     </row>
     <row r="119">
       <c s="10" r="A119"/>
       <c t="s" s="7" r="B119">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c t="s" s="5" r="C119">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c t="s" s="7" r="D119">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c t="s" s="7" r="E119">
-        <v>419</v>
+        <v>421</v>
       </c>
     </row>
     <row r="120">
       <c s="10" r="A120"/>
       <c t="s" s="7" r="B120">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c t="s" s="5" r="C120">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c t="s" s="7" r="D120">
-        <v>422</v>
-      </c>
-      <c t="s" s="7" r="E120">
-        <v>423</v>
+        <v>424</v>
+      </c>
+      <c t="s" s="5" r="E120">
+        <v>425</v>
       </c>
     </row>
     <row r="121">
       <c s="10" r="A121"/>
-      <c t="s" s="7" r="B121">
-        <v>424</v>
-      </c>
-      <c t="s" s="5" r="C121">
-        <v>425</v>
-      </c>
-      <c t="s" s="7" r="D121">
+      <c s="19" r="B121"/>
+      <c s="9" r="C121"/>
+      <c s="19" r="D121"/>
+      <c s="19" r="E121"/>
+    </row>
+    <row r="122">
+      <c t="s" s="10" r="A122">
         <v>426</v>
       </c>
-      <c t="s" s="5" r="E121">
+      <c t="s" s="7" r="B122">
         <v>427</v>
       </c>
-    </row>
-    <row r="122">
-      <c s="10" r="A122"/>
-      <c s="19" r="B122"/>
-      <c s="9" r="C122"/>
-      <c s="19" r="D122"/>
-      <c s="19" r="E122"/>
+      <c t="s" s="16" r="C122">
+        <v>428</v>
+      </c>
+      <c t="s" s="7" r="D122">
+        <v>429</v>
+      </c>
+      <c t="s" s="7" r="E122">
+        <v>430</v>
+      </c>
     </row>
     <row r="123">
-      <c t="s" s="10" r="A123">
-        <v>428</v>
-      </c>
+      <c s="10" r="A123"/>
       <c t="s" s="7" r="B123">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c t="s" s="16" r="C123">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c t="s" s="7" r="D123">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c t="s" s="7" r="E123">
-        <v>432</v>
+        <v>434</v>
       </c>
     </row>
     <row r="124">
-      <c s="10" r="A124"/>
+      <c s="14" r="A124"/>
       <c t="s" s="7" r="B124">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c t="s" s="16" r="C124">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c t="s" s="7" r="D124">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c t="s" s="7" r="E124">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
     <row r="125">
-      <c s="14" r="A125"/>
-      <c t="s" s="7" r="B125">
-        <v>437</v>
-      </c>
-      <c t="s" s="16" r="C125">
-        <v>438</v>
-      </c>
-      <c t="s" s="7" r="D125">
+      <c s="10" r="A125"/>
+      <c s="12" r="B125"/>
+      <c s="18" r="C125"/>
+      <c s="12" r="D125"/>
+      <c s="12" r="E125"/>
+    </row>
+    <row r="126">
+      <c t="s" s="10" r="A126">
         <v>439</v>
       </c>
-      <c t="s" s="7" r="E125">
+      <c t="s" s="7" r="B126">
         <v>440</v>
       </c>
-    </row>
-    <row r="126">
-      <c s="10" r="A126"/>
-      <c s="12" r="B126"/>
-      <c s="18" r="C126"/>
-      <c s="12" r="D126"/>
-      <c s="12" r="E126"/>
+      <c t="s" s="16" r="C126">
+        <v>441</v>
+      </c>
+      <c t="s" s="7" r="D126">
+        <v>442</v>
+      </c>
+      <c t="s" s="7" r="E126">
+        <v>443</v>
+      </c>
     </row>
     <row r="127">
-      <c t="s" s="10" r="A127">
-        <v>441</v>
-      </c>
+      <c s="10" r="A127"/>
       <c t="s" s="7" r="B127">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c t="s" s="16" r="C127">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c t="s" s="7" r="D127">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c t="s" s="7" r="E127">
-        <v>445</v>
+        <v>447</v>
       </c>
     </row>
     <row r="128">
       <c s="10" r="A128"/>
       <c t="s" s="7" r="B128">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c t="s" s="16" r="C128">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c t="s" s="7" r="D128">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c t="s" s="7" r="E128">
-        <v>449</v>
+        <v>451</v>
       </c>
     </row>
     <row r="129">
       <c s="10" r="A129"/>
       <c t="s" s="7" r="B129">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c t="s" s="16" r="C129">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c t="s" s="7" r="D129">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c t="s" s="7" r="E129">
-        <v>453</v>
+        <v>455</v>
       </c>
     </row>
     <row r="130">
       <c s="10" r="A130"/>
       <c t="s" s="7" r="B130">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c t="s" s="16" r="C130">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c t="s" s="7" r="D130">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c t="s" s="7" r="E130">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="131">
       <c s="10" r="A131"/>
-      <c t="s" s="7" r="B131">
-        <v>458</v>
-      </c>
-      <c t="s" s="16" r="C131">
-        <v>459</v>
-      </c>
-      <c t="s" s="7" r="D131">
+      <c s="2" r="B131"/>
+      <c s="13" r="C131"/>
+      <c s="2" r="D131"/>
+      <c s="2" r="E131"/>
+    </row>
+    <row r="132">
+      <c t="s" s="10" r="A132">
         <v>460</v>
       </c>
-      <c t="s" s="7" r="E131">
+      <c t="s" s="15" r="B132">
         <v>461</v>
       </c>
-    </row>
-    <row r="132">
-      <c s="10" r="A132"/>
-      <c s="2" r="B132"/>
-      <c s="13" r="C132"/>
-      <c s="2" r="D132"/>
-      <c s="2" r="E132"/>
+      <c t="s" s="1" r="C132">
+        <v>460</v>
+      </c>
+      <c s="15" r="D132"/>
+      <c s="15" r="E132"/>
     </row>
     <row r="133">
-      <c t="s" s="10" r="A133">
+      <c s="10" r="A133"/>
+      <c s="19" r="B133"/>
+      <c s="9" r="C133"/>
+      <c s="19" r="D133"/>
+      <c s="19" r="E133"/>
+    </row>
+    <row r="134">
+      <c t="s" s="10" r="A134">
         <v>462</v>
       </c>
-      <c t="s" s="15" r="B133">
+      <c t="s" s="22" r="B134">
         <v>463</v>
       </c>
-      <c t="s" s="1" r="C133">
-        <v>462</v>
-      </c>
-      <c s="15" r="D133"/>
-      <c s="15" r="E133"/>
-    </row>
-    <row r="134">
-      <c s="10" r="A134"/>
-      <c s="19" r="B134"/>
-      <c s="9" r="C134"/>
-      <c s="19" r="D134"/>
-      <c s="19" r="E134"/>
+      <c t="s" s="20" r="C134">
+        <v>464</v>
+      </c>
+      <c s="22" r="D134"/>
+      <c s="22" r="E134"/>
     </row>
     <row r="135">
-      <c t="s" s="10" r="A135">
-        <v>464</v>
-      </c>
+      <c s="10" r="A135"/>
       <c t="s" s="22" r="B135">
         <v>465</v>
       </c>
@@ -3692,14 +3682,10 @@
     </row>
     <row r="136">
       <c s="10" r="A136"/>
-      <c t="s" s="22" r="B136">
-        <v>467</v>
-      </c>
-      <c t="s" s="20" r="C136">
-        <v>468</v>
-      </c>
-      <c s="22" r="D136"/>
-      <c s="22" r="E136"/>
+      <c s="19" r="B136"/>
+      <c s="9" r="C136"/>
+      <c s="19" r="D136"/>
+      <c s="19" r="E136"/>
     </row>
     <row r="137">
       <c s="10" r="A137"/>
@@ -3714,13 +3700,6 @@
       <c s="9" r="C138"/>
       <c s="19" r="D138"/>
       <c s="19" r="E138"/>
-    </row>
-    <row r="139">
-      <c s="10" r="A139"/>
-      <c s="19" r="B139"/>
-      <c s="9" r="C139"/>
-      <c s="19" r="D139"/>
-      <c s="19" r="E139"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
EWD-22401 - Rename Experiences into Learning Experiences resources
Former-commit-id: 5f55b2a6c2b80d14484e554d093c8b4d2b8e6c66
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="517">
   <si>
     <t>Page</t>
   </si>
@@ -111,7 +111,7 @@
     <t>Select</t>
   </si>
   <si>
-    <t>Selecteer</t>
+    <t>Selecteren</t>
   </si>
   <si>
     <t>Auswählen</t>
@@ -231,7 +231,7 @@
     <t>Created on</t>
   </si>
   <si>
-    <t>Aangemaakt op</t>
+    <t>Gemaakt op</t>
   </si>
   <si>
     <t>Erstellt am</t>
@@ -363,6 +363,12 @@
     <t>Learning objective cannot be deleted, while it is included into learning experience(s) or contains questions.</t>
   </si>
   <si>
+    <t>Leerdoel kan niet worden verwijderd als het is opgenomen in een of meer leerervaringen of als het vragen bevat.</t>
+  </si>
+  <si>
+    <t>Ein Lernziel kann nicht gelöscht werden, wenn es in eine oder mehrere Lernerfahrungen eingeschlossen ist oder Fragen enthält. </t>
+  </si>
+  <si>
     <t>Objective</t>
   </si>
   <si>
@@ -381,12 +387,24 @@
     <t>Learning experiences</t>
   </si>
   <si>
+    <t>Leerervaringen</t>
+  </si>
+  <si>
+    <t>Lernerfahrungen</t>
+  </si>
+  <si>
     <t>experience</t>
   </si>
   <si>
     <t>Learning experience</t>
   </si>
   <si>
+    <t>Leerervaring</t>
+  </si>
+  <si>
+    <t>Lernerfahrung</t>
+  </si>
+  <si>
     <t>experienceBuildAction</t>
   </si>
   <si>
@@ -396,7 +414,7 @@
     <t>Samenstellen…</t>
   </si>
   <si>
-    <t>Erstellen</t>
+    <t>Zusammenstellen</t>
   </si>
   <si>
     <t>experienceDownloadAction</t>
@@ -420,7 +438,7 @@
     <t>samenstellen…</t>
   </si>
   <si>
-    <t>aufbau...</t>
+    <t>Wird zusammengestellt...</t>
   </si>
   <si>
     <t>experienceFailedStatus</t>
@@ -453,10 +471,10 @@
     <t>Rebuild</t>
   </si>
   <si>
-    <t>Opnieuw maken</t>
-  </si>
-  <si>
-    <t>Neu aufbauen</t>
+    <t>Opnieuw samenstellen</t>
+  </si>
+  <si>
+    <t>Neu zusammenstellen</t>
   </si>
   <si>
     <t>addNewExperience</t>
@@ -465,6 +483,12 @@
     <t>Add new learning experience</t>
   </si>
   <si>
+    <t>Nieuwe leerervaring toevoegen</t>
+  </si>
+  <si>
+    <t>Neue Lernerfahrung hinzufügen</t>
+  </si>
+  <si>
     <t>numberOfRelatedObjectives</t>
   </si>
   <si>
@@ -483,12 +507,24 @@
     <t>Learning experiences list is empty</t>
   </si>
   <si>
+    <t>Lijst met leerervaringen is leeg</t>
+  </si>
+  <si>
+    <t>Liste der Lernerfahrungen ist leer</t>
+  </si>
+  <si>
     <t>experienceCannotBeDeleted</t>
   </si>
   <si>
     <t>Learning experience cannot be deleted while it has included learning objective(s)</t>
   </si>
   <si>
+    <t>Leerervaring kan niet worden verwijderd als de ervaring een of meer leerdoelen bevat</t>
+  </si>
+  <si>
+    <t>Eine Lernerfahrung kann nicht gelöscht werden, wenn sie ein oder mehrere Lernziele enthält</t>
+  </si>
+  <si>
     <t>CreateObjective</t>
   </si>
   <si>
@@ -498,7 +534,7 @@
     <t>Create New Objective</t>
   </si>
   <si>
-    <t>Nieuwe doelstelling aanmaken</t>
+    <t>Nieuwe doelstelling maken</t>
   </si>
   <si>
     <t>Neues Lernziel erstellen</t>
@@ -549,24 +585,48 @@
     <t>Type learning experience title here</t>
   </si>
   <si>
+    <t>Typ hier de titel van de leerervaring</t>
+  </si>
+  <si>
+    <t>Titel der Lernerfahrung hier eingeben</t>
+  </si>
+  <si>
     <t>clickToAddExperience</t>
   </si>
   <si>
     <t>Click to add learning experience</t>
   </si>
   <si>
+    <t>Klik om leerervaring toe te voegen</t>
+  </si>
+  <si>
+    <t>Klicken, um neue Lernerfahrung hinzuzufügen</t>
+  </si>
+  <si>
     <t>createNewExperience</t>
   </si>
   <si>
     <t>Create new learning experience</t>
   </si>
   <si>
+    <t>Nieuwe leerervaring maken</t>
+  </si>
+  <si>
+    <t>Neue Lernerfahrung erstellen</t>
+  </si>
+  <si>
     <t>chooseTemplate</t>
   </si>
   <si>
     <t>Choose template</t>
   </si>
   <si>
+    <t>Sjabloon kiezen</t>
+  </si>
+  <si>
+    <t>Vorlage wählen</t>
+  </si>
+  <si>
     <t>Question</t>
   </si>
   <si>
@@ -577,6 +637,9 @@
   </si>
   <si>
     <t>Vorige</t>
+  </si>
+  <si>
+    <t>Vorheriges</t>
   </si>
   <si>
     <t>next</t>
@@ -841,7 +904,7 @@
     <t>Create new question</t>
   </si>
   <si>
-    <t>Nieuwe vraag aanmaken</t>
+    <t>Nieuwe vraag maken</t>
   </si>
   <si>
     <t>Neue Frage erstellen</t>
@@ -1282,6 +1345,12 @@
     <t>Build learning experience</t>
   </si>
   <si>
+    <t>Leerervaring samenstellen</t>
+  </si>
+  <si>
+    <t>Lernerfahrung zusammenstellen</t>
+  </si>
+  <si>
     <t>noRelatedLearningObjectives</t>
   </si>
   <si>
@@ -1300,58 +1369,118 @@
     <t>Click to add learning objective(s) into this learning experience</t>
   </si>
   <si>
+    <t>Klik om leerdoelen toe te voegen aan deze leerervaring</t>
+  </si>
+  <si>
+    <t>Klicken, um dieser Lernerfahrung ein oder mehrere Lernziele hinzuzufügen</t>
+  </si>
+  <si>
     <t>relateObjectivesHelpHint</t>
   </si>
   <si>
     <t>Move cursor over learning objective and select to include it into learning experience. Use Finish button when done</t>
   </si>
   <si>
+    <t>Verplaats de cursor over het leerdoel en selecteer het voor opname in de leeromgeving. Klik na afloop op de knop Afsluiten</t>
+  </si>
+  <si>
+    <t>Bewegen Sie den Mauszeiger über ein Lernziel und wählen Sie es aus, um es in die Lernerfahrung einzuschließen. Klicken Sie auf die Schaltfläche "Fertig stellen", wenn Sie fertig sind.</t>
+  </si>
+  <si>
     <t>clickToCreateNewObjective</t>
   </si>
   <si>
     <t>To create new learning objective click "+" button</t>
   </si>
   <si>
+    <t>Klik op "+" om een nieuw leerdoel te maken</t>
+  </si>
+  <si>
+    <t>Um ein neues Lernziel zu erstellen, klicken Sie auf die Schaltfläche "+".</t>
+  </si>
+  <si>
     <t>noObjectivesForRelating</t>
   </si>
   <si>
     <t>No learning objectives to include</t>
   </si>
   <si>
+    <t>Geen leerdoelen om op te nemen</t>
+  </si>
+  <si>
+    <t>Keine einzuschließenden Lernziele</t>
+  </si>
+  <si>
     <t>finish</t>
   </si>
   <si>
     <t>Finish</t>
   </si>
   <si>
+    <t>Afsluiten</t>
+  </si>
+  <si>
+    <t>Fertig stellen</t>
+  </si>
+  <si>
     <t>relate</t>
   </si>
   <si>
     <t>Include</t>
   </si>
   <si>
+    <t>Opnemen</t>
+  </si>
+  <si>
+    <t>Einschließen</t>
+  </si>
+  <si>
     <t>unrelate</t>
   </si>
   <si>
     <t>Exclude</t>
   </si>
   <si>
+    <t>Uitsluiten</t>
+  </si>
+  <si>
+    <t>Ausschließen</t>
+  </si>
+  <si>
     <t>relateObjectives</t>
   </si>
   <si>
     <t>Include learning objective(s)</t>
   </si>
   <si>
+    <t>Leerdoel(en) opnemen</t>
+  </si>
+  <si>
+    <t>Ein oder mehrere Lernziele einschließen</t>
+  </si>
+  <si>
     <t>unrelateObjectives</t>
   </si>
   <si>
     <t>Exclude selected learning objective(s)</t>
   </si>
   <si>
+    <t>Geselecteerde leerdoelen uitsluiten</t>
+  </si>
+  <si>
+    <t>Ausgewählte Lernziele ausschließen</t>
+  </si>
+  <si>
     <t>finishRelating</t>
   </si>
   <si>
     <t>Include selected learning objective(s)</t>
+  </si>
+  <si>
+    <t>Geselecteerde leerdoelen opnemen</t>
+  </si>
+  <si>
+    <t>Ausgewählte Lernziele einschließen</t>
   </si>
   <si>
     <t>Error pages</t>
@@ -1462,7 +1591,7 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <b val="0"/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
@@ -1471,7 +1600,7 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="0"/>
+      <b/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
@@ -1606,7 +1735,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1629,13 +1758,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FF00FF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1701,7 +1824,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1730,7 +1853,7 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
@@ -1740,66 +1863,63 @@
     <xf applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="1" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="2">
+    <xf applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="2" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="3">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="5" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="3" applyFill="1">
-      <alignment vertical="center" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" fillId="6" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="4" applyFill="1">
+    <xf applyAlignment="1" fillId="5" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="4" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
     <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="5"/>
-    <xf applyAlignment="1" fillId="7" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="6" applyFill="1">
+    <xf applyAlignment="1" fillId="6" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="6" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="7">
       <alignment vertical="bottom" horizontal="right"/>
     </xf>
-    <xf applyAlignment="1" fillId="8" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+    <xf applyAlignment="1" fillId="7" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="8">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="9" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="9" applyFill="1">
+    <xf applyAlignment="1" fillId="8" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="9" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="10">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="10" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+    <xf applyAlignment="1" fillId="9" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="11" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="11" applyFill="1">
+    <xf applyAlignment="1" fillId="10" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="11" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="12" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="12" applyFill="1">
+    <xf applyAlignment="1" fillId="11" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="12" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="13" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+    <xf applyAlignment="1" fillId="12" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="14" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="13" applyFill="1">
+    <xf applyAlignment="1" fillId="13" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="13" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="15" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="14" applyFill="1">
+    <xf applyAlignment="1" fillId="14" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="14" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="16" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="15" applyFill="1">
+    <xf applyAlignment="1" fillId="15" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="15" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="17" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+    <xf applyAlignment="1" fillId="16" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
     <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="16"/>
-    <xf applyAlignment="1" fillId="18" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="17" applyFill="1">
+    <xf applyAlignment="1" fillId="17" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="17" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1826,20 +1946,20 @@
     <col min="5" customWidth="1" max="5" width="39.43"/>
   </cols>
   <sheetData>
-    <row s="7" customFormat="1" r="1">
-      <c t="s" s="12" r="A1">
+    <row s="6" customFormat="1" r="1">
+      <c t="s" s="11" r="A1">
         <v>0</v>
       </c>
-      <c t="s" s="12" r="B1">
+      <c t="s" s="11" r="B1">
         <v>1</v>
       </c>
-      <c t="s" s="12" r="C1">
+      <c t="s" s="11" r="C1">
         <v>2</v>
       </c>
-      <c t="s" s="12" r="D1">
+      <c t="s" s="11" r="D1">
         <v>3</v>
       </c>
-      <c t="s" s="3" r="E1">
+      <c t="s" s="4" r="E1">
         <v>4</v>
       </c>
     </row>
@@ -1847,331 +1967,331 @@
       <c t="s" s="2" r="A2">
         <v>5</v>
       </c>
-      <c t="s" s="8" r="B2">
+      <c t="s" s="7" r="B2">
         <v>6</v>
       </c>
-      <c t="s" s="8" r="C2">
+      <c t="s" s="7" r="C2">
         <v>7</v>
       </c>
-      <c t="s" s="8" r="D2">
+      <c t="s" s="7" r="D2">
         <v>8</v>
       </c>
-      <c t="s" s="8" r="E2">
+      <c t="s" s="7" r="E2">
         <v>9</v>
       </c>
     </row>
     <row r="3">
       <c s="2" r="A3"/>
-      <c t="s" s="8" r="B3">
+      <c t="s" s="7" r="B3">
         <v>10</v>
       </c>
-      <c t="s" s="8" r="C3">
+      <c t="s" s="7" r="C3">
         <v>11</v>
       </c>
-      <c t="s" s="8" r="D3">
+      <c t="s" s="7" r="D3">
         <v>12</v>
       </c>
-      <c t="s" s="8" r="E3">
+      <c t="s" s="7" r="E3">
         <v>13</v>
       </c>
     </row>
     <row r="4">
       <c s="2" r="A4"/>
-      <c t="s" s="8" r="B4">
+      <c t="s" s="7" r="B4">
         <v>14</v>
       </c>
-      <c t="s" s="8" r="C4">
+      <c t="s" s="7" r="C4">
         <v>15</v>
       </c>
-      <c t="s" s="8" r="D4">
+      <c t="s" s="7" r="D4">
         <v>16</v>
       </c>
-      <c t="s" s="8" r="E4">
+      <c t="s" s="7" r="E4">
         <v>17</v>
       </c>
     </row>
     <row r="5">
       <c s="2" r="A5"/>
-      <c t="s" s="8" r="B5">
+      <c t="s" s="7" r="B5">
         <v>18</v>
       </c>
-      <c t="s" s="8" r="C5">
+      <c t="s" s="7" r="C5">
         <v>19</v>
       </c>
-      <c t="s" s="8" r="D5">
+      <c t="s" s="7" r="D5">
         <v>20</v>
       </c>
-      <c t="s" s="8" r="E5">
+      <c t="s" s="7" r="E5">
         <v>21</v>
       </c>
     </row>
     <row r="6">
       <c s="2" r="A6"/>
-      <c t="s" s="8" r="B6">
+      <c t="s" s="7" r="B6">
         <v>22</v>
       </c>
-      <c t="s" s="8" r="C6">
+      <c t="s" s="7" r="C6">
         <v>23</v>
       </c>
-      <c t="s" s="8" r="D6">
+      <c t="s" s="7" r="D6">
         <v>23</v>
       </c>
-      <c t="s" s="8" r="E6">
+      <c t="s" s="7" r="E6">
         <v>23</v>
       </c>
     </row>
     <row r="7">
       <c s="2" r="A7"/>
-      <c t="s" s="8" r="B7">
+      <c t="s" s="7" r="B7">
         <v>24</v>
       </c>
-      <c t="s" s="8" r="C7">
+      <c t="s" s="7" r="C7">
         <v>25</v>
       </c>
-      <c t="s" s="8" r="D7">
+      <c t="s" s="7" r="D7">
         <v>25</v>
       </c>
-      <c t="s" s="8" r="E7">
+      <c t="s" s="7" r="E7">
         <v>25</v>
       </c>
     </row>
     <row r="8">
       <c s="2" r="A8"/>
-      <c t="s" s="8" r="B8">
+      <c t="s" s="7" r="B8">
         <v>26</v>
       </c>
-      <c t="s" s="8" r="C8">
+      <c t="s" s="7" r="C8">
         <v>27</v>
       </c>
-      <c t="s" s="8" r="D8">
+      <c t="s" s="7" r="D8">
         <v>28</v>
       </c>
-      <c t="s" s="8" r="E8">
+      <c t="s" s="7" r="E8">
         <v>29</v>
       </c>
     </row>
     <row r="9">
       <c s="2" r="A9"/>
-      <c t="s" s="8" r="B9">
+      <c t="s" s="7" r="B9">
         <v>30</v>
       </c>
-      <c t="s" s="8" r="C9">
+      <c t="s" s="7" r="C9">
         <v>31</v>
       </c>
-      <c t="s" s="8" r="D9">
+      <c t="s" s="7" r="D9">
         <v>32</v>
       </c>
-      <c t="s" s="8" r="E9">
+      <c t="s" s="7" r="E9">
         <v>33</v>
       </c>
     </row>
     <row r="10">
       <c s="2" r="A10"/>
-      <c t="s" s="8" r="B10">
+      <c t="s" s="7" r="B10">
         <v>34</v>
       </c>
-      <c t="s" s="8" r="C10">
+      <c t="s" s="7" r="C10">
         <v>35</v>
       </c>
-      <c t="s" s="8" r="D10">
+      <c t="s" s="7" r="D10">
         <v>36</v>
       </c>
-      <c t="s" s="8" r="E10">
+      <c t="s" s="7" r="E10">
         <v>37</v>
       </c>
     </row>
     <row r="11">
       <c s="2" r="A11"/>
-      <c t="s" s="8" r="B11">
+      <c t="s" s="7" r="B11">
         <v>38</v>
       </c>
-      <c t="s" s="8" r="C11">
+      <c t="s" s="7" r="C11">
         <v>39</v>
       </c>
-      <c t="s" s="8" r="D11">
+      <c t="s" s="7" r="D11">
         <v>40</v>
       </c>
-      <c t="s" s="8" r="E11">
+      <c t="s" s="7" r="E11">
         <v>41</v>
       </c>
     </row>
     <row r="12">
       <c s="2" r="A12"/>
-      <c t="s" s="8" r="B12">
+      <c t="s" s="7" r="B12">
         <v>42</v>
       </c>
-      <c t="s" s="8" r="C12">
+      <c t="s" s="7" r="C12">
         <v>43</v>
       </c>
-      <c t="s" s="8" r="D12">
+      <c t="s" s="7" r="D12">
         <v>44</v>
       </c>
-      <c t="s" s="8" r="E12">
+      <c t="s" s="7" r="E12">
         <v>45</v>
       </c>
     </row>
     <row r="13">
-      <c s="13" r="A13"/>
-      <c t="s" s="8" r="B13">
+      <c s="12" r="A13"/>
+      <c t="s" s="7" r="B13">
         <v>46</v>
       </c>
-      <c t="s" s="8" r="C13">
+      <c t="s" s="7" r="C13">
         <v>47</v>
       </c>
-      <c t="s" s="8" r="D13">
+      <c t="s" s="7" r="D13">
         <v>48</v>
       </c>
-      <c t="s" s="8" r="E13">
+      <c t="s" s="7" r="E13">
         <v>49</v>
       </c>
     </row>
     <row r="14">
-      <c s="13" r="A14"/>
-      <c t="s" s="8" r="B14">
+      <c s="12" r="A14"/>
+      <c t="s" s="7" r="B14">
         <v>50</v>
       </c>
-      <c t="s" s="8" r="C14">
+      <c t="s" s="7" r="C14">
         <v>51</v>
       </c>
-      <c t="s" s="8" r="D14">
+      <c t="s" s="7" r="D14">
         <v>52</v>
       </c>
-      <c t="s" s="8" r="E14">
+      <c t="s" s="7" r="E14">
         <v>53</v>
       </c>
     </row>
     <row r="15">
-      <c s="13" r="A15"/>
-      <c t="s" s="8" r="B15">
+      <c s="12" r="A15"/>
+      <c t="s" s="7" r="B15">
         <v>54</v>
       </c>
-      <c t="s" s="8" r="C15">
+      <c t="s" s="7" r="C15">
         <v>55</v>
       </c>
-      <c t="s" s="8" r="D15">
+      <c t="s" s="7" r="D15">
         <v>56</v>
       </c>
-      <c t="s" s="8" r="E15">
+      <c t="s" s="7" r="E15">
         <v>57</v>
       </c>
     </row>
     <row r="16">
-      <c s="13" r="A16"/>
-      <c t="s" s="8" r="B16">
+      <c s="12" r="A16"/>
+      <c t="s" s="7" r="B16">
         <v>58</v>
       </c>
-      <c t="s" s="8" r="C16">
+      <c t="s" s="7" r="C16">
         <v>59</v>
       </c>
-      <c t="s" s="8" r="D16">
+      <c t="s" s="7" r="D16">
         <v>60</v>
       </c>
-      <c t="s" s="8" r="E16">
+      <c t="s" s="7" r="E16">
         <v>61</v>
       </c>
     </row>
     <row r="17">
-      <c s="13" r="A17"/>
-      <c t="s" s="8" r="B17">
+      <c s="12" r="A17"/>
+      <c t="s" s="7" r="B17">
         <v>62</v>
       </c>
-      <c t="s" s="8" r="C17">
+      <c t="s" s="7" r="C17">
         <v>63</v>
       </c>
-      <c t="s" s="8" r="D17">
+      <c t="s" s="7" r="D17">
         <v>64</v>
       </c>
-      <c t="s" s="8" r="E17">
+      <c t="s" s="7" r="E17">
         <v>65</v>
       </c>
     </row>
     <row r="18">
-      <c s="13" r="A18"/>
-      <c t="s" s="8" r="B18">
+      <c s="12" r="A18"/>
+      <c t="s" s="7" r="B18">
         <v>66</v>
       </c>
-      <c t="s" s="8" r="C18">
+      <c t="s" s="7" r="C18">
         <v>67</v>
       </c>
-      <c t="s" s="8" r="D18">
+      <c t="s" s="7" r="D18">
         <v>68</v>
       </c>
-      <c t="s" s="8" r="E18">
+      <c t="s" s="7" r="E18">
         <v>69</v>
       </c>
     </row>
     <row r="19">
-      <c s="13" r="A19"/>
-      <c t="s" s="8" r="B19">
+      <c s="12" r="A19"/>
+      <c t="s" s="7" r="B19">
         <v>70</v>
       </c>
-      <c t="s" s="8" r="C19">
+      <c t="s" s="7" r="C19">
         <v>71</v>
       </c>
-      <c t="s" s="8" r="D19">
+      <c t="s" s="7" r="D19">
         <v>72</v>
       </c>
-      <c t="s" s="8" r="E19">
+      <c t="s" s="7" r="E19">
         <v>73</v>
       </c>
     </row>
     <row r="20">
-      <c s="13" r="A20"/>
-      <c t="s" s="8" r="B20">
+      <c s="12" r="A20"/>
+      <c t="s" s="7" r="B20">
         <v>74</v>
       </c>
-      <c t="s" s="8" r="C20">
+      <c t="s" s="7" r="C20">
         <v>75</v>
       </c>
-      <c t="s" s="8" r="D20">
+      <c t="s" s="7" r="D20">
         <v>76</v>
       </c>
-      <c t="s" s="8" r="E20">
+      <c t="s" s="7" r="E20">
         <v>77</v>
       </c>
     </row>
     <row r="21">
-      <c s="13" r="A21"/>
-      <c t="s" s="8" r="B21">
+      <c s="12" r="A21"/>
+      <c t="s" s="7" r="B21">
         <v>78</v>
       </c>
-      <c t="s" s="8" r="C21">
+      <c t="s" s="7" r="C21">
         <v>79</v>
       </c>
-      <c t="s" s="8" r="D21">
+      <c t="s" s="7" r="D21">
         <v>80</v>
       </c>
-      <c t="s" s="8" r="E21">
+      <c t="s" s="7" r="E21">
         <v>81</v>
       </c>
     </row>
     <row r="22">
-      <c s="13" r="A22"/>
-      <c t="s" s="8" r="B22">
+      <c s="12" r="A22"/>
+      <c t="s" s="7" r="B22">
         <v>82</v>
       </c>
-      <c t="s" s="8" r="C22">
+      <c t="s" s="7" r="C22">
         <v>83</v>
       </c>
-      <c t="s" s="8" r="D22">
+      <c t="s" s="7" r="D22">
         <v>84</v>
       </c>
-      <c t="s" s="8" r="E22">
+      <c t="s" s="7" r="E22">
         <v>85</v>
       </c>
     </row>
     <row r="23">
-      <c s="13" r="A23"/>
-      <c t="s" s="8" r="B23">
+      <c s="12" r="A23"/>
+      <c t="s" s="7" r="B23">
         <v>86</v>
       </c>
-      <c t="s" s="8" r="C23">
+      <c t="s" s="7" r="C23">
         <v>87</v>
       </c>
-      <c t="s" s="8" r="D23">
+      <c t="s" s="7" r="D23">
         <v>48</v>
       </c>
-      <c t="s" s="8" r="E23">
+      <c t="s" s="7" r="E23">
         <v>88</v>
       </c>
     </row>
@@ -2186,331 +2306,355 @@
       <c t="s" s="2" r="A25">
         <v>89</v>
       </c>
-      <c t="s" s="8" r="B25">
+      <c t="s" s="7" r="B25">
         <v>90</v>
       </c>
-      <c t="s" s="8" r="C25">
+      <c t="s" s="7" r="C25">
         <v>91</v>
       </c>
-      <c t="s" s="8" r="D25">
+      <c t="s" s="7" r="D25">
         <v>92</v>
       </c>
-      <c t="s" s="8" r="E25">
+      <c t="s" s="7" r="E25">
         <v>93</v>
       </c>
     </row>
     <row r="26">
       <c s="2" r="A26"/>
-      <c t="s" s="8" r="B26">
+      <c t="s" s="7" r="B26">
         <v>94</v>
       </c>
-      <c t="s" s="8" r="C26">
+      <c t="s" s="7" r="C26">
         <v>95</v>
       </c>
-      <c t="s" s="8" r="D26">
+      <c t="s" s="7" r="D26">
         <v>96</v>
       </c>
-      <c t="s" s="8" r="E26">
+      <c t="s" s="7" r="E26">
         <v>97</v>
       </c>
     </row>
     <row r="27">
       <c s="2" r="A27"/>
-      <c t="s" s="8" r="B27">
+      <c t="s" s="7" r="B27">
         <v>98</v>
       </c>
-      <c t="s" s="8" r="C27">
+      <c t="s" s="7" r="C27">
         <v>99</v>
       </c>
-      <c t="s" s="8" r="D27">
+      <c t="s" s="7" r="D27">
         <v>100</v>
       </c>
-      <c t="s" s="8" r="E27">
+      <c t="s" s="7" r="E27">
         <v>101</v>
       </c>
     </row>
     <row r="28">
       <c s="2" r="A28"/>
-      <c t="s" s="8" r="B28">
+      <c t="s" s="7" r="B28">
         <v>102</v>
       </c>
-      <c t="s" s="8" r="C28">
+      <c t="s" s="7" r="C28">
         <v>103</v>
       </c>
-      <c t="s" s="8" r="D28">
+      <c t="s" s="7" r="D28">
         <v>104</v>
       </c>
-      <c t="s" s="8" r="E28">
+      <c t="s" s="7" r="E28">
         <v>105</v>
       </c>
     </row>
     <row r="29">
       <c s="2" r="A29"/>
-      <c t="s" s="8" r="B29">
+      <c t="s" s="7" r="B29">
         <v>106</v>
       </c>
-      <c t="s" s="8" r="C29">
+      <c t="s" s="7" r="C29">
         <v>107</v>
       </c>
-      <c t="s" s="8" r="D29">
+      <c t="s" s="7" r="D29">
         <v>108</v>
       </c>
-      <c t="s" s="8" r="E29">
+      <c t="s" s="7" r="E29">
         <v>109</v>
       </c>
     </row>
     <row r="30">
-      <c s="13" r="A30"/>
-      <c t="s" s="8" r="B30">
+      <c s="12" r="A30"/>
+      <c t="s" s="7" r="B30">
         <v>110</v>
       </c>
-      <c t="s" s="8" r="C30">
+      <c t="s" s="7" r="C30">
         <v>111</v>
       </c>
-      <c t="s" s="8" r="D30">
+      <c t="s" s="7" r="D30">
         <v>112</v>
       </c>
-      <c t="s" s="8" r="E30">
+      <c t="s" s="7" r="E30">
         <v>113</v>
       </c>
     </row>
     <row r="31">
-      <c s="13" r="A31"/>
-      <c t="s" s="5" r="B31">
+      <c s="12" r="A31"/>
+      <c t="s" s="7" r="B31">
         <v>114</v>
       </c>
-      <c t="s" s="5" r="C31">
+      <c t="s" s="7" r="C31">
         <v>115</v>
       </c>
-      <c s="5" r="D31"/>
-      <c s="5" r="E31"/>
+      <c t="s" s="7" r="D31">
+        <v>116</v>
+      </c>
+      <c t="s" s="7" r="E31">
+        <v>117</v>
+      </c>
     </row>
     <row r="32">
-      <c s="13" r="A32"/>
-      <c s="13" r="B32"/>
-      <c s="13" r="C32"/>
-      <c s="13" r="D32"/>
-      <c s="13" r="E32"/>
+      <c s="12" r="A32"/>
+      <c s="12" r="B32"/>
+      <c s="12" r="C32"/>
+      <c s="12" r="D32"/>
+      <c s="12" r="E32"/>
     </row>
     <row r="33">
       <c t="s" s="2" r="A33">
-        <v>116</v>
-      </c>
-      <c t="s" s="19" r="B33">
-        <v>117</v>
-      </c>
-      <c t="s" s="19" r="C33">
         <v>118</v>
       </c>
-      <c s="19" r="D33"/>
-      <c s="19" r="E33"/>
+      <c t="s" s="18" r="B33">
+        <v>119</v>
+      </c>
+      <c t="s" s="18" r="C33">
+        <v>120</v>
+      </c>
+      <c s="18" r="D33"/>
+      <c s="18" r="E33"/>
     </row>
     <row r="34">
       <c s="2" r="A34"/>
       <c s="2" r="B34"/>
       <c s="2" r="C34"/>
       <c s="2" r="D34"/>
-      <c s="13" r="E34"/>
+      <c s="12" r="E34"/>
     </row>
     <row r="35">
-      <c t="s" s="13" r="A35">
-        <v>119</v>
-      </c>
-      <c t="s" s="5" r="B35">
-        <v>120</v>
-      </c>
-      <c t="s" s="5" r="C35">
+      <c t="s" s="12" r="A35">
         <v>121</v>
       </c>
-      <c s="5" r="D35"/>
-      <c s="5" r="E35"/>
+      <c t="s" s="7" r="B35">
+        <v>122</v>
+      </c>
+      <c t="s" s="7" r="C35">
+        <v>123</v>
+      </c>
+      <c t="s" s="7" r="D35">
+        <v>124</v>
+      </c>
+      <c t="s" s="7" r="E35">
+        <v>125</v>
+      </c>
     </row>
     <row r="36">
-      <c s="13" r="A36"/>
-      <c t="s" s="5" r="B36">
-        <v>122</v>
-      </c>
-      <c t="s" s="5" r="C36">
-        <v>123</v>
-      </c>
-      <c s="5" r="D36"/>
-      <c s="5" r="E36"/>
+      <c s="12" r="A36"/>
+      <c t="s" s="7" r="B36">
+        <v>126</v>
+      </c>
+      <c t="s" s="7" r="C36">
+        <v>127</v>
+      </c>
+      <c t="s" s="7" r="D36">
+        <v>128</v>
+      </c>
+      <c t="s" s="7" r="E36">
+        <v>129</v>
+      </c>
     </row>
     <row r="37">
-      <c s="13" r="A37"/>
-      <c t="s" s="8" r="B37">
-        <v>124</v>
-      </c>
-      <c t="s" s="8" r="C37">
-        <v>125</v>
-      </c>
-      <c t="s" s="8" r="D37">
-        <v>126</v>
-      </c>
-      <c t="s" s="8" r="E37">
-        <v>127</v>
+      <c s="12" r="A37"/>
+      <c t="s" s="7" r="B37">
+        <v>130</v>
+      </c>
+      <c t="s" s="7" r="C37">
+        <v>131</v>
+      </c>
+      <c t="s" s="7" r="D37">
+        <v>132</v>
+      </c>
+      <c t="s" s="7" r="E37">
+        <v>133</v>
       </c>
     </row>
     <row r="38">
-      <c s="13" r="A38"/>
-      <c t="s" s="8" r="B38">
-        <v>128</v>
-      </c>
-      <c t="s" s="8" r="C38">
-        <v>129</v>
-      </c>
-      <c t="s" s="8" r="D38">
-        <v>130</v>
-      </c>
-      <c t="s" s="8" r="E38">
-        <v>131</v>
+      <c s="12" r="A38"/>
+      <c t="s" s="7" r="B38">
+        <v>134</v>
+      </c>
+      <c t="s" s="7" r="C38">
+        <v>135</v>
+      </c>
+      <c t="s" s="7" r="D38">
+        <v>136</v>
+      </c>
+      <c t="s" s="7" r="E38">
+        <v>137</v>
       </c>
     </row>
     <row r="39">
-      <c s="13" r="A39"/>
-      <c t="s" s="8" r="B39">
-        <v>132</v>
-      </c>
-      <c t="s" s="8" r="C39">
-        <v>133</v>
-      </c>
-      <c t="s" s="8" r="D39">
-        <v>134</v>
-      </c>
-      <c t="s" s="8" r="E39">
-        <v>135</v>
+      <c s="12" r="A39"/>
+      <c t="s" s="7" r="B39">
+        <v>138</v>
+      </c>
+      <c t="s" s="7" r="C39">
+        <v>139</v>
+      </c>
+      <c t="s" s="7" r="D39">
+        <v>140</v>
+      </c>
+      <c t="s" s="7" r="E39">
+        <v>141</v>
       </c>
     </row>
     <row r="40">
-      <c s="13" r="A40"/>
-      <c t="s" s="8" r="B40">
-        <v>136</v>
-      </c>
-      <c t="s" s="8" r="C40">
-        <v>137</v>
-      </c>
-      <c t="s" s="8" r="D40">
-        <v>138</v>
-      </c>
-      <c t="s" s="8" r="E40">
-        <v>139</v>
+      <c s="12" r="A40"/>
+      <c t="s" s="7" r="B40">
+        <v>142</v>
+      </c>
+      <c t="s" s="7" r="C40">
+        <v>143</v>
+      </c>
+      <c t="s" s="7" r="D40">
+        <v>144</v>
+      </c>
+      <c t="s" s="7" r="E40">
+        <v>145</v>
       </c>
     </row>
     <row r="41">
-      <c s="13" r="A41"/>
-      <c t="s" s="8" r="B41">
-        <v>140</v>
-      </c>
-      <c t="s" s="8" r="C41">
-        <v>141</v>
-      </c>
-      <c t="s" s="8" r="D41">
-        <v>142</v>
-      </c>
-      <c t="s" s="8" r="E41">
-        <v>143</v>
+      <c s="12" r="A41"/>
+      <c t="s" s="7" r="B41">
+        <v>146</v>
+      </c>
+      <c t="s" s="7" r="C41">
+        <v>147</v>
+      </c>
+      <c t="s" s="7" r="D41">
+        <v>148</v>
+      </c>
+      <c t="s" s="7" r="E41">
+        <v>149</v>
       </c>
     </row>
     <row r="42">
-      <c s="13" r="A42"/>
-      <c t="s" s="8" r="B42">
-        <v>144</v>
-      </c>
-      <c t="s" s="8" r="C42">
-        <v>145</v>
-      </c>
-      <c t="s" s="8" r="D42">
-        <v>146</v>
-      </c>
-      <c t="s" s="8" r="E42">
-        <v>147</v>
+      <c s="12" r="A42"/>
+      <c t="s" s="7" r="B42">
+        <v>150</v>
+      </c>
+      <c t="s" s="7" r="C42">
+        <v>151</v>
+      </c>
+      <c t="s" s="7" r="D42">
+        <v>152</v>
+      </c>
+      <c t="s" s="7" r="E42">
+        <v>153</v>
       </c>
     </row>
     <row r="43">
-      <c s="13" r="A43"/>
-      <c t="s" s="5" r="B43">
-        <v>148</v>
-      </c>
-      <c t="s" s="5" r="C43">
-        <v>149</v>
-      </c>
-      <c s="5" r="D43"/>
-      <c s="5" r="E43"/>
+      <c s="12" r="A43"/>
+      <c t="s" s="7" r="B43">
+        <v>154</v>
+      </c>
+      <c t="s" s="7" r="C43">
+        <v>155</v>
+      </c>
+      <c t="s" s="7" r="D43">
+        <v>156</v>
+      </c>
+      <c t="s" s="7" r="E43">
+        <v>157</v>
+      </c>
     </row>
     <row r="44">
-      <c s="13" r="A44"/>
-      <c t="s" s="8" r="B44">
-        <v>150</v>
-      </c>
-      <c t="s" s="8" r="C44">
-        <v>151</v>
-      </c>
-      <c t="s" s="8" r="D44">
-        <v>152</v>
-      </c>
-      <c t="s" s="8" r="E44">
-        <v>153</v>
+      <c s="12" r="A44"/>
+      <c t="s" s="7" r="B44">
+        <v>158</v>
+      </c>
+      <c t="s" s="7" r="C44">
+        <v>159</v>
+      </c>
+      <c t="s" s="7" r="D44">
+        <v>160</v>
+      </c>
+      <c t="s" s="7" r="E44">
+        <v>161</v>
       </c>
     </row>
     <row r="45">
-      <c s="13" r="A45"/>
-      <c t="s" s="5" r="B45">
-        <v>154</v>
-      </c>
-      <c t="s" s="5" r="C45">
-        <v>155</v>
-      </c>
-      <c s="5" r="D45"/>
-      <c s="5" r="E45"/>
+      <c s="12" r="A45"/>
+      <c t="s" s="7" r="B45">
+        <v>162</v>
+      </c>
+      <c t="s" s="7" r="C45">
+        <v>163</v>
+      </c>
+      <c t="s" s="7" r="D45">
+        <v>164</v>
+      </c>
+      <c t="s" s="7" r="E45">
+        <v>165</v>
+      </c>
     </row>
     <row r="46">
-      <c s="13" r="A46"/>
-      <c t="s" s="5" r="B46">
-        <v>156</v>
-      </c>
-      <c t="s" s="5" r="C46">
-        <v>157</v>
-      </c>
-      <c s="5" r="D46"/>
-      <c s="5" r="E46"/>
+      <c s="12" r="A46"/>
+      <c t="s" s="7" r="B46">
+        <v>166</v>
+      </c>
+      <c t="s" s="7" r="C46">
+        <v>167</v>
+      </c>
+      <c t="s" s="7" r="D46">
+        <v>168</v>
+      </c>
+      <c t="s" s="7" r="E46">
+        <v>169</v>
+      </c>
     </row>
     <row r="47">
-      <c s="13" r="A47"/>
-      <c s="13" r="B47"/>
-      <c s="13" r="C47"/>
-      <c s="13" r="D47"/>
-      <c s="13" r="E47"/>
+      <c s="12" r="A47"/>
+      <c s="12" r="B47"/>
+      <c s="12" r="C47"/>
+      <c s="12" r="D47"/>
+      <c s="12" r="E47"/>
     </row>
     <row r="48">
-      <c t="s" s="13" r="A48">
-        <v>158</v>
-      </c>
-      <c t="s" s="8" r="B48">
-        <v>159</v>
-      </c>
-      <c t="s" s="8" r="C48">
-        <v>160</v>
-      </c>
-      <c t="s" s="8" r="D48">
-        <v>161</v>
-      </c>
-      <c t="s" s="8" r="E48">
-        <v>162</v>
+      <c t="s" s="12" r="A48">
+        <v>170</v>
+      </c>
+      <c t="s" s="7" r="B48">
+        <v>171</v>
+      </c>
+      <c t="s" s="7" r="C48">
+        <v>172</v>
+      </c>
+      <c t="s" s="20" r="D48">
+        <v>173</v>
+      </c>
+      <c t="s" s="7" r="E48">
+        <v>174</v>
       </c>
     </row>
     <row r="49">
-      <c s="13" r="A49"/>
-      <c t="s" s="8" r="B49">
-        <v>163</v>
-      </c>
-      <c t="s" s="8" r="C49">
-        <v>164</v>
-      </c>
-      <c t="s" s="8" r="D49">
-        <v>165</v>
-      </c>
-      <c t="s" s="8" r="E49">
-        <v>166</v>
+      <c s="12" r="A49"/>
+      <c t="s" s="7" r="B49">
+        <v>175</v>
+      </c>
+      <c t="s" s="7" r="C49">
+        <v>176</v>
+      </c>
+      <c t="s" s="7" r="D49">
+        <v>177</v>
+      </c>
+      <c t="s" s="7" r="E49">
+        <v>178</v>
       </c>
     </row>
     <row r="51">
@@ -2521,1322 +2665,1382 @@
       <c s="2" r="E51"/>
     </row>
     <row r="52">
-      <c t="s" s="13" r="A52">
-        <v>167</v>
-      </c>
-      <c t="s" s="16" r="B52">
-        <v>168</v>
-      </c>
-      <c t="s" s="16" r="C52">
-        <v>169</v>
-      </c>
-      <c s="16" r="D52"/>
-      <c s="16" r="E52"/>
+      <c t="s" s="12" r="A52">
+        <v>179</v>
+      </c>
+      <c t="s" s="15" r="B52">
+        <v>180</v>
+      </c>
+      <c t="s" s="15" r="C52">
+        <v>181</v>
+      </c>
+      <c s="15" r="D52"/>
+      <c s="15" r="E52"/>
     </row>
     <row r="53">
-      <c s="13" r="A53"/>
-      <c t="s" s="16" r="B53">
-        <v>170</v>
-      </c>
-      <c t="s" s="16" r="C53">
-        <v>171</v>
-      </c>
-      <c s="16" r="D53"/>
-      <c s="16" r="E53"/>
+      <c s="12" r="A53"/>
+      <c t="s" s="15" r="B53">
+        <v>182</v>
+      </c>
+      <c t="s" s="15" r="C53">
+        <v>183</v>
+      </c>
+      <c s="15" r="D53"/>
+      <c s="15" r="E53"/>
     </row>
     <row r="54">
-      <c s="13" r="A54"/>
-      <c t="s" s="16" r="B54">
-        <v>172</v>
-      </c>
-      <c t="s" s="16" r="C54">
-        <v>173</v>
-      </c>
-      <c s="16" r="D54"/>
-      <c s="16" r="E54"/>
+      <c s="12" r="A54"/>
+      <c t="s" s="15" r="B54">
+        <v>184</v>
+      </c>
+      <c t="s" s="15" r="C54">
+        <v>185</v>
+      </c>
+      <c s="15" r="D54"/>
+      <c s="15" r="E54"/>
     </row>
     <row r="55">
-      <c s="13" r="A55"/>
-      <c t="s" s="16" r="B55">
-        <v>174</v>
-      </c>
-      <c t="s" s="16" r="C55">
-        <v>175</v>
-      </c>
-      <c s="16" r="D55"/>
-      <c s="16" r="E55"/>
+      <c s="12" r="A55"/>
+      <c t="s" s="15" r="B55">
+        <v>186</v>
+      </c>
+      <c t="s" s="15" r="C55">
+        <v>187</v>
+      </c>
+      <c s="15" r="D55"/>
+      <c s="15" r="E55"/>
     </row>
     <row r="56">
-      <c s="13" r="A56"/>
-      <c t="s" s="5" r="B56">
-        <v>176</v>
-      </c>
-      <c t="s" s="5" r="C56">
-        <v>177</v>
-      </c>
-      <c s="5" r="D56"/>
-      <c s="5" r="E56"/>
+      <c s="12" r="A56"/>
+      <c t="s" s="7" r="B56">
+        <v>188</v>
+      </c>
+      <c t="s" s="7" r="C56">
+        <v>189</v>
+      </c>
+      <c t="s" s="7" r="D56">
+        <v>190</v>
+      </c>
+      <c t="s" s="7" r="E56">
+        <v>191</v>
+      </c>
     </row>
     <row r="57">
-      <c s="13" r="A57"/>
-      <c t="s" s="5" r="B57">
-        <v>178</v>
-      </c>
-      <c t="s" s="5" r="C57">
-        <v>179</v>
-      </c>
-      <c s="5" r="D57"/>
-      <c s="5" r="E57"/>
+      <c s="12" r="A57"/>
+      <c t="s" s="7" r="B57">
+        <v>192</v>
+      </c>
+      <c t="s" s="7" r="C57">
+        <v>193</v>
+      </c>
+      <c t="s" s="7" r="D57">
+        <v>194</v>
+      </c>
+      <c t="s" s="7" r="E57">
+        <v>195</v>
+      </c>
     </row>
     <row r="58">
-      <c s="13" r="A58"/>
-      <c t="s" s="5" r="B58">
-        <v>180</v>
-      </c>
-      <c t="s" s="5" r="C58">
-        <v>181</v>
-      </c>
-      <c s="5" r="D58"/>
-      <c s="5" r="E58"/>
+      <c s="12" r="A58"/>
+      <c t="s" s="7" r="B58">
+        <v>196</v>
+      </c>
+      <c t="s" s="7" r="C58">
+        <v>197</v>
+      </c>
+      <c t="s" s="7" r="D58">
+        <v>198</v>
+      </c>
+      <c t="s" s="7" r="E58">
+        <v>199</v>
+      </c>
     </row>
     <row r="59">
-      <c s="13" r="A59"/>
-      <c t="s" s="5" r="B59">
-        <v>182</v>
-      </c>
-      <c t="s" s="5" r="C59">
-        <v>183</v>
-      </c>
-      <c s="5" r="D59"/>
-      <c s="5" r="E59"/>
+      <c s="12" r="A59"/>
+      <c t="s" s="7" r="B59">
+        <v>200</v>
+      </c>
+      <c t="s" s="7" r="C59">
+        <v>201</v>
+      </c>
+      <c t="s" s="7" r="D59">
+        <v>202</v>
+      </c>
+      <c t="s" s="7" r="E59">
+        <v>203</v>
+      </c>
     </row>
     <row r="60">
-      <c s="13" r="A60"/>
-      <c s="13" r="B60"/>
-      <c s="13" r="C60"/>
-      <c s="13" r="D60"/>
-      <c s="13" r="E60"/>
+      <c s="12" r="A60"/>
+      <c s="12" r="B60"/>
+      <c s="12" r="C60"/>
+      <c s="12" r="D60"/>
+      <c s="12" r="E60"/>
     </row>
     <row r="61">
-      <c t="s" s="13" r="A61">
-        <v>184</v>
-      </c>
-      <c t="s" s="8" r="B61">
-        <v>185</v>
-      </c>
-      <c t="s" s="8" r="C61">
-        <v>186</v>
-      </c>
-      <c t="s" s="8" r="D61">
-        <v>187</v>
-      </c>
-      <c t="s" s="8" r="E61">
-        <v>17</v>
+      <c t="s" s="12" r="A61">
+        <v>204</v>
+      </c>
+      <c t="s" s="7" r="B61">
+        <v>205</v>
+      </c>
+      <c t="s" s="7" r="C61">
+        <v>206</v>
+      </c>
+      <c t="s" s="7" r="D61">
+        <v>207</v>
+      </c>
+      <c t="s" s="7" r="E61">
+        <v>208</v>
       </c>
     </row>
     <row r="62">
-      <c s="13" r="A62"/>
-      <c t="s" s="8" r="B62">
-        <v>188</v>
-      </c>
-      <c t="s" s="8" r="C62">
-        <v>189</v>
-      </c>
-      <c t="s" s="8" r="D62">
-        <v>190</v>
-      </c>
-      <c t="s" s="8" r="E62">
-        <v>191</v>
+      <c s="12" r="A62"/>
+      <c t="s" s="7" r="B62">
+        <v>209</v>
+      </c>
+      <c t="s" s="7" r="C62">
+        <v>210</v>
+      </c>
+      <c t="s" s="7" r="D62">
+        <v>211</v>
+      </c>
+      <c t="s" s="7" r="E62">
+        <v>212</v>
       </c>
     </row>
     <row r="63">
-      <c s="13" r="A63"/>
-      <c t="s" s="8" r="B63">
-        <v>192</v>
-      </c>
-      <c t="s" s="8" r="C63">
-        <v>193</v>
-      </c>
-      <c t="s" s="8" r="D63">
-        <v>194</v>
-      </c>
-      <c t="s" s="8" r="E63">
-        <v>195</v>
+      <c s="12" r="A63"/>
+      <c t="s" s="7" r="B63">
+        <v>213</v>
+      </c>
+      <c t="s" s="7" r="C63">
+        <v>214</v>
+      </c>
+      <c t="s" s="7" r="D63">
+        <v>215</v>
+      </c>
+      <c t="s" s="7" r="E63">
+        <v>216</v>
       </c>
     </row>
     <row r="64">
-      <c s="13" r="A64"/>
-      <c t="s" s="8" r="B64">
-        <v>196</v>
-      </c>
-      <c t="s" s="8" r="C64">
-        <v>197</v>
-      </c>
-      <c t="s" s="8" r="D64">
-        <v>198</v>
-      </c>
-      <c t="s" s="8" r="E64">
-        <v>199</v>
+      <c s="12" r="A64"/>
+      <c t="s" s="7" r="B64">
+        <v>217</v>
+      </c>
+      <c t="s" s="7" r="C64">
+        <v>218</v>
+      </c>
+      <c t="s" s="7" r="D64">
+        <v>219</v>
+      </c>
+      <c t="s" s="7" r="E64">
+        <v>220</v>
       </c>
     </row>
     <row r="65">
-      <c s="13" r="A65"/>
-      <c t="s" s="8" r="B65">
-        <v>200</v>
-      </c>
-      <c t="s" s="8" r="C65">
-        <v>201</v>
-      </c>
-      <c t="s" s="8" r="D65">
-        <v>202</v>
-      </c>
-      <c t="s" s="8" r="E65">
-        <v>203</v>
+      <c s="12" r="A65"/>
+      <c t="s" s="7" r="B65">
+        <v>221</v>
+      </c>
+      <c t="s" s="7" r="C65">
+        <v>222</v>
+      </c>
+      <c t="s" s="7" r="D65">
+        <v>223</v>
+      </c>
+      <c t="s" s="7" r="E65">
+        <v>224</v>
       </c>
     </row>
     <row r="66">
-      <c s="13" r="A66"/>
-      <c t="s" s="8" r="B66">
-        <v>204</v>
-      </c>
-      <c t="s" s="8" r="C66">
-        <v>205</v>
-      </c>
-      <c t="s" s="8" r="D66">
-        <v>206</v>
-      </c>
-      <c t="s" s="8" r="E66">
-        <v>207</v>
+      <c s="12" r="A66"/>
+      <c t="s" s="7" r="B66">
+        <v>225</v>
+      </c>
+      <c t="s" s="7" r="C66">
+        <v>226</v>
+      </c>
+      <c t="s" s="7" r="D66">
+        <v>227</v>
+      </c>
+      <c t="s" s="7" r="E66">
+        <v>228</v>
       </c>
     </row>
     <row r="67">
-      <c s="13" r="A67"/>
-      <c t="s" s="8" r="B67">
-        <v>208</v>
-      </c>
-      <c t="s" s="8" r="C67">
-        <v>209</v>
-      </c>
-      <c t="s" s="8" r="D67">
-        <v>210</v>
-      </c>
-      <c t="s" s="8" r="E67">
-        <v>211</v>
+      <c s="12" r="A67"/>
+      <c t="s" s="7" r="B67">
+        <v>229</v>
+      </c>
+      <c t="s" s="7" r="C67">
+        <v>230</v>
+      </c>
+      <c t="s" s="7" r="D67">
+        <v>231</v>
+      </c>
+      <c t="s" s="7" r="E67">
+        <v>232</v>
       </c>
     </row>
     <row r="68">
-      <c s="13" r="A68"/>
-      <c t="s" s="8" r="B68">
-        <v>212</v>
-      </c>
-      <c t="s" s="8" r="C68">
-        <v>213</v>
-      </c>
-      <c t="s" s="8" r="D68">
-        <v>214</v>
-      </c>
-      <c t="s" s="8" r="E68">
-        <v>215</v>
+      <c s="12" r="A68"/>
+      <c t="s" s="7" r="B68">
+        <v>233</v>
+      </c>
+      <c t="s" s="7" r="C68">
+        <v>234</v>
+      </c>
+      <c t="s" s="7" r="D68">
+        <v>235</v>
+      </c>
+      <c t="s" s="7" r="E68">
+        <v>236</v>
       </c>
     </row>
     <row r="69">
-      <c s="13" r="A69"/>
-      <c t="s" s="8" r="B69">
-        <v>216</v>
-      </c>
-      <c t="s" s="8" r="C69">
-        <v>217</v>
-      </c>
-      <c t="s" s="8" r="D69">
-        <v>218</v>
-      </c>
-      <c t="s" s="8" r="E69">
-        <v>219</v>
+      <c s="12" r="A69"/>
+      <c t="s" s="7" r="B69">
+        <v>237</v>
+      </c>
+      <c t="s" s="7" r="C69">
+        <v>238</v>
+      </c>
+      <c t="s" s="7" r="D69">
+        <v>239</v>
+      </c>
+      <c t="s" s="7" r="E69">
+        <v>240</v>
       </c>
     </row>
     <row r="70">
-      <c s="13" r="A70"/>
-      <c s="13" r="B70"/>
-      <c s="13" r="C70"/>
-      <c s="13" r="D70"/>
-      <c s="13" r="E70"/>
+      <c s="12" r="A70"/>
+      <c s="12" r="B70"/>
+      <c s="12" r="C70"/>
+      <c s="12" r="D70"/>
+      <c s="12" r="E70"/>
     </row>
     <row r="71">
-      <c t="s" s="13" r="A71">
-        <v>220</v>
-      </c>
-      <c t="s" s="8" r="B71">
-        <v>221</v>
-      </c>
-      <c t="s" s="8" r="C71">
-        <v>222</v>
-      </c>
-      <c t="s" s="8" r="D71">
-        <v>223</v>
-      </c>
-      <c t="s" s="8" r="E71">
-        <v>224</v>
+      <c t="s" s="12" r="A71">
+        <v>241</v>
+      </c>
+      <c t="s" s="7" r="B71">
+        <v>242</v>
+      </c>
+      <c t="s" s="7" r="C71">
+        <v>243</v>
+      </c>
+      <c t="s" s="7" r="D71">
+        <v>244</v>
+      </c>
+      <c t="s" s="7" r="E71">
+        <v>245</v>
       </c>
     </row>
     <row r="72">
-      <c s="13" r="A72"/>
-      <c t="s" s="8" r="B72">
-        <v>225</v>
-      </c>
-      <c t="s" s="8" r="C72">
-        <v>226</v>
-      </c>
-      <c t="s" s="8" r="D72">
-        <v>227</v>
-      </c>
-      <c t="s" s="8" r="E72">
-        <v>228</v>
+      <c s="12" r="A72"/>
+      <c t="s" s="7" r="B72">
+        <v>246</v>
+      </c>
+      <c t="s" s="7" r="C72">
+        <v>247</v>
+      </c>
+      <c t="s" s="7" r="D72">
+        <v>248</v>
+      </c>
+      <c t="s" s="7" r="E72">
+        <v>249</v>
       </c>
     </row>
     <row r="73">
-      <c s="11" r="A73"/>
-      <c t="s" s="8" r="B73">
-        <v>229</v>
-      </c>
-      <c t="s" s="8" r="C73">
-        <v>230</v>
-      </c>
-      <c t="s" s="8" r="D73">
-        <v>231</v>
-      </c>
-      <c t="s" s="8" r="E73">
-        <v>232</v>
+      <c s="10" r="A73"/>
+      <c t="s" s="7" r="B73">
+        <v>250</v>
+      </c>
+      <c t="s" s="7" r="C73">
+        <v>251</v>
+      </c>
+      <c t="s" s="7" r="D73">
+        <v>252</v>
+      </c>
+      <c t="s" s="7" r="E73">
+        <v>253</v>
       </c>
     </row>
     <row r="74">
-      <c s="11" r="A74"/>
-      <c t="s" s="8" r="B74">
-        <v>233</v>
-      </c>
-      <c t="s" s="8" r="C74">
-        <v>234</v>
-      </c>
-      <c t="s" s="8" r="D74">
-        <v>235</v>
-      </c>
-      <c t="s" s="8" r="E74">
-        <v>236</v>
+      <c s="10" r="A74"/>
+      <c t="s" s="7" r="B74">
+        <v>254</v>
+      </c>
+      <c t="s" s="7" r="C74">
+        <v>255</v>
+      </c>
+      <c t="s" s="7" r="D74">
+        <v>256</v>
+      </c>
+      <c t="s" s="7" r="E74">
+        <v>257</v>
       </c>
     </row>
     <row r="75">
-      <c s="11" r="A75"/>
-      <c t="s" s="8" r="B75">
-        <v>237</v>
-      </c>
-      <c t="s" s="8" r="C75">
-        <v>238</v>
-      </c>
-      <c t="s" s="8" r="D75">
-        <v>239</v>
-      </c>
-      <c t="s" s="8" r="E75">
-        <v>240</v>
+      <c s="10" r="A75"/>
+      <c t="s" s="7" r="B75">
+        <v>258</v>
+      </c>
+      <c t="s" s="7" r="C75">
+        <v>259</v>
+      </c>
+      <c t="s" s="7" r="D75">
+        <v>260</v>
+      </c>
+      <c t="s" s="7" r="E75">
+        <v>261</v>
       </c>
     </row>
     <row r="76">
-      <c s="11" r="A76"/>
-      <c t="s" s="8" r="B76">
-        <v>241</v>
-      </c>
-      <c t="s" s="8" r="C76">
-        <v>242</v>
-      </c>
-      <c t="s" s="8" r="D76">
-        <v>243</v>
-      </c>
-      <c t="s" s="8" r="E76">
-        <v>244</v>
+      <c s="10" r="A76"/>
+      <c t="s" s="7" r="B76">
+        <v>262</v>
+      </c>
+      <c t="s" s="7" r="C76">
+        <v>263</v>
+      </c>
+      <c t="s" s="7" r="D76">
+        <v>264</v>
+      </c>
+      <c t="s" s="7" r="E76">
+        <v>265</v>
       </c>
     </row>
     <row r="77">
-      <c s="11" r="A77"/>
-      <c t="s" s="8" r="B77">
-        <v>245</v>
-      </c>
-      <c t="s" s="8" r="C77">
-        <v>246</v>
-      </c>
-      <c t="s" s="8" r="D77">
-        <v>247</v>
-      </c>
-      <c t="s" s="8" r="E77">
-        <v>248</v>
+      <c s="10" r="A77"/>
+      <c t="s" s="7" r="B77">
+        <v>266</v>
+      </c>
+      <c t="s" s="7" r="C77">
+        <v>267</v>
+      </c>
+      <c t="s" s="7" r="D77">
+        <v>268</v>
+      </c>
+      <c t="s" s="7" r="E77">
+        <v>269</v>
       </c>
     </row>
     <row r="78">
-      <c s="11" r="A78"/>
-      <c t="s" s="8" r="B78">
-        <v>249</v>
-      </c>
-      <c t="s" s="8" r="C78">
-        <v>250</v>
-      </c>
-      <c t="s" s="8" r="D78">
-        <v>251</v>
-      </c>
-      <c t="s" s="8" r="E78">
-        <v>252</v>
+      <c s="10" r="A78"/>
+      <c t="s" s="7" r="B78">
+        <v>270</v>
+      </c>
+      <c t="s" s="7" r="C78">
+        <v>271</v>
+      </c>
+      <c t="s" s="7" r="D78">
+        <v>272</v>
+      </c>
+      <c t="s" s="7" r="E78">
+        <v>273</v>
       </c>
     </row>
     <row r="79">
-      <c s="11" r="A79"/>
-      <c t="s" s="8" r="B79">
-        <v>253</v>
-      </c>
-      <c t="s" s="8" r="C79">
-        <v>254</v>
-      </c>
-      <c t="s" s="8" r="D79">
-        <v>255</v>
-      </c>
-      <c t="s" s="8" r="E79">
-        <v>256</v>
+      <c s="10" r="A79"/>
+      <c t="s" s="7" r="B79">
+        <v>274</v>
+      </c>
+      <c t="s" s="7" r="C79">
+        <v>275</v>
+      </c>
+      <c t="s" s="7" r="D79">
+        <v>276</v>
+      </c>
+      <c t="s" s="7" r="E79">
+        <v>277</v>
       </c>
     </row>
     <row r="80">
-      <c s="11" r="A80"/>
-      <c t="s" s="8" r="B80">
-        <v>257</v>
-      </c>
-      <c t="s" s="8" r="C80">
-        <v>258</v>
-      </c>
-      <c t="s" s="8" r="D80">
-        <v>259</v>
-      </c>
-      <c t="s" s="8" r="E80">
-        <v>260</v>
+      <c s="10" r="A80"/>
+      <c t="s" s="7" r="B80">
+        <v>278</v>
+      </c>
+      <c t="s" s="7" r="C80">
+        <v>279</v>
+      </c>
+      <c t="s" s="7" r="D80">
+        <v>280</v>
+      </c>
+      <c t="s" s="7" r="E80">
+        <v>281</v>
       </c>
     </row>
     <row r="81">
-      <c s="11" r="A81"/>
-      <c t="s" s="8" r="B81">
-        <v>261</v>
-      </c>
-      <c t="s" s="8" r="C81">
-        <v>262</v>
-      </c>
-      <c t="s" s="8" r="D81">
-        <v>263</v>
-      </c>
-      <c t="s" s="8" r="E81">
-        <v>264</v>
+      <c s="10" r="A81"/>
+      <c t="s" s="7" r="B81">
+        <v>282</v>
+      </c>
+      <c t="s" s="7" r="C81">
+        <v>283</v>
+      </c>
+      <c t="s" s="7" r="D81">
+        <v>284</v>
+      </c>
+      <c t="s" s="7" r="E81">
+        <v>285</v>
       </c>
     </row>
     <row r="82">
-      <c s="11" r="A82"/>
-      <c t="s" s="8" r="B82">
-        <v>265</v>
-      </c>
-      <c t="s" s="8" r="C82">
-        <v>266</v>
-      </c>
-      <c t="s" s="8" r="D82">
-        <v>267</v>
-      </c>
-      <c t="s" s="8" r="E82">
-        <v>268</v>
+      <c s="10" r="A82"/>
+      <c t="s" s="7" r="B82">
+        <v>286</v>
+      </c>
+      <c t="s" s="7" r="C82">
+        <v>287</v>
+      </c>
+      <c t="s" s="7" r="D82">
+        <v>288</v>
+      </c>
+      <c t="s" s="7" r="E82">
+        <v>289</v>
       </c>
     </row>
     <row r="83">
-      <c s="11" r="A83"/>
-      <c t="s" s="8" r="B83">
-        <v>269</v>
-      </c>
-      <c t="s" s="8" r="C83">
-        <v>270</v>
-      </c>
-      <c t="s" s="8" r="D83">
-        <v>271</v>
-      </c>
-      <c t="s" s="8" r="E83">
-        <v>272</v>
+      <c s="10" r="A83"/>
+      <c t="s" s="7" r="B83">
+        <v>290</v>
+      </c>
+      <c t="s" s="7" r="C83">
+        <v>291</v>
+      </c>
+      <c t="s" s="7" r="D83">
+        <v>292</v>
+      </c>
+      <c t="s" s="7" r="E83">
+        <v>293</v>
       </c>
     </row>
     <row r="84">
-      <c s="11" r="A84"/>
-      <c t="s" s="8" r="B84">
-        <v>273</v>
-      </c>
-      <c t="s" s="8" r="C84">
-        <v>274</v>
-      </c>
-      <c t="s" s="8" r="D84">
-        <v>275</v>
-      </c>
-      <c t="s" s="8" r="E84">
-        <v>276</v>
+      <c s="10" r="A84"/>
+      <c t="s" s="7" r="B84">
+        <v>294</v>
+      </c>
+      <c t="s" s="7" r="C84">
+        <v>295</v>
+      </c>
+      <c t="s" s="7" r="D84">
+        <v>296</v>
+      </c>
+      <c t="s" s="7" r="E84">
+        <v>297</v>
       </c>
     </row>
     <row r="85">
-      <c s="11" r="A85"/>
-      <c s="13" r="B85"/>
-      <c s="13" r="C85"/>
-      <c s="13" r="D85"/>
-      <c s="13" r="E85"/>
+      <c s="10" r="A85"/>
+      <c s="12" r="B85"/>
+      <c s="12" r="C85"/>
+      <c s="12" r="D85"/>
+      <c s="12" r="E85"/>
     </row>
     <row r="86">
-      <c t="s" s="11" r="A86">
-        <v>277</v>
-      </c>
-      <c t="s" s="8" r="B86">
-        <v>278</v>
-      </c>
-      <c t="s" s="8" r="C86">
-        <v>279</v>
-      </c>
-      <c t="s" s="8" r="D86">
-        <v>280</v>
-      </c>
-      <c t="s" s="8" r="E86">
-        <v>281</v>
+      <c t="s" s="10" r="A86">
+        <v>298</v>
+      </c>
+      <c t="s" s="7" r="B86">
+        <v>299</v>
+      </c>
+      <c t="s" s="7" r="C86">
+        <v>300</v>
+      </c>
+      <c t="s" s="7" r="D86">
+        <v>301</v>
+      </c>
+      <c t="s" s="7" r="E86">
+        <v>302</v>
       </c>
     </row>
     <row r="87">
-      <c s="11" r="A87"/>
-      <c t="s" s="8" r="B87">
-        <v>282</v>
-      </c>
-      <c t="s" s="8" r="C87">
-        <v>283</v>
-      </c>
-      <c t="s" s="8" r="D87">
-        <v>284</v>
-      </c>
-      <c t="s" s="8" r="E87">
-        <v>285</v>
+      <c s="10" r="A87"/>
+      <c t="s" s="7" r="B87">
+        <v>303</v>
+      </c>
+      <c t="s" s="7" r="C87">
+        <v>304</v>
+      </c>
+      <c t="s" s="7" r="D87">
+        <v>305</v>
+      </c>
+      <c t="s" s="7" r="E87">
+        <v>306</v>
       </c>
     </row>
     <row r="88">
-      <c s="11" r="A88"/>
-      <c t="s" s="8" r="B88">
-        <v>286</v>
-      </c>
-      <c t="s" s="8" r="C88">
-        <v>287</v>
-      </c>
-      <c t="s" s="8" r="D88">
-        <v>288</v>
-      </c>
-      <c t="s" s="8" r="E88">
-        <v>289</v>
+      <c s="10" r="A88"/>
+      <c t="s" s="7" r="B88">
+        <v>307</v>
+      </c>
+      <c t="s" s="7" r="C88">
+        <v>308</v>
+      </c>
+      <c t="s" s="7" r="D88">
+        <v>309</v>
+      </c>
+      <c t="s" s="7" r="E88">
+        <v>310</v>
       </c>
     </row>
     <row r="89">
-      <c s="11" r="A89"/>
-      <c t="s" s="8" r="B89">
-        <v>290</v>
-      </c>
-      <c t="s" s="8" r="C89">
-        <v>291</v>
-      </c>
-      <c t="s" s="8" r="D89">
-        <v>292</v>
-      </c>
-      <c t="s" s="8" r="E89">
-        <v>293</v>
+      <c s="10" r="A89"/>
+      <c t="s" s="7" r="B89">
+        <v>311</v>
+      </c>
+      <c t="s" s="7" r="C89">
+        <v>312</v>
+      </c>
+      <c t="s" s="7" r="D89">
+        <v>313</v>
+      </c>
+      <c t="s" s="7" r="E89">
+        <v>314</v>
       </c>
     </row>
     <row r="90">
-      <c s="11" r="A90"/>
-      <c t="s" s="8" r="B90">
-        <v>294</v>
-      </c>
-      <c t="s" s="8" r="C90">
-        <v>295</v>
-      </c>
-      <c t="s" s="8" r="D90">
-        <v>296</v>
-      </c>
-      <c t="s" s="8" r="E90">
-        <v>297</v>
+      <c s="10" r="A90"/>
+      <c t="s" s="7" r="B90">
+        <v>315</v>
+      </c>
+      <c t="s" s="7" r="C90">
+        <v>316</v>
+      </c>
+      <c t="s" s="7" r="D90">
+        <v>317</v>
+      </c>
+      <c t="s" s="7" r="E90">
+        <v>318</v>
       </c>
     </row>
     <row r="91">
-      <c s="11" r="A91"/>
-      <c t="s" s="8" r="B91">
-        <v>298</v>
-      </c>
-      <c t="s" s="8" r="C91">
-        <v>299</v>
-      </c>
-      <c t="s" s="8" r="D91">
-        <v>300</v>
-      </c>
-      <c t="s" s="8" r="E91">
-        <v>299</v>
+      <c s="10" r="A91"/>
+      <c t="s" s="7" r="B91">
+        <v>319</v>
+      </c>
+      <c t="s" s="7" r="C91">
+        <v>320</v>
+      </c>
+      <c t="s" s="7" r="D91">
+        <v>321</v>
+      </c>
+      <c t="s" s="7" r="E91">
+        <v>320</v>
       </c>
     </row>
     <row r="92">
-      <c s="11" r="A92"/>
-      <c t="s" s="8" r="B92">
-        <v>301</v>
-      </c>
-      <c t="s" s="8" r="C92">
-        <v>302</v>
-      </c>
-      <c t="s" s="8" r="D92">
-        <v>303</v>
-      </c>
-      <c t="s" s="8" r="E92">
-        <v>304</v>
+      <c s="10" r="A92"/>
+      <c t="s" s="7" r="B92">
+        <v>322</v>
+      </c>
+      <c t="s" s="7" r="C92">
+        <v>323</v>
+      </c>
+      <c t="s" s="7" r="D92">
+        <v>324</v>
+      </c>
+      <c t="s" s="7" r="E92">
+        <v>325</v>
       </c>
     </row>
     <row r="93">
-      <c s="11" r="A93"/>
-      <c t="s" s="8" r="B93">
-        <v>305</v>
-      </c>
-      <c t="s" s="8" r="C93">
-        <v>306</v>
-      </c>
-      <c t="s" s="8" r="D93">
-        <v>307</v>
-      </c>
-      <c t="s" s="8" r="E93">
-        <v>308</v>
+      <c s="10" r="A93"/>
+      <c t="s" s="7" r="B93">
+        <v>326</v>
+      </c>
+      <c t="s" s="7" r="C93">
+        <v>327</v>
+      </c>
+      <c t="s" s="7" r="D93">
+        <v>328</v>
+      </c>
+      <c t="s" s="7" r="E93">
+        <v>329</v>
       </c>
     </row>
     <row r="94">
-      <c s="11" r="A94"/>
-      <c t="s" s="8" r="B94">
-        <v>309</v>
-      </c>
-      <c t="s" s="8" r="C94">
-        <v>310</v>
-      </c>
-      <c t="s" s="8" r="D94">
-        <v>311</v>
-      </c>
-      <c t="s" s="8" r="E94">
-        <v>312</v>
+      <c s="10" r="A94"/>
+      <c t="s" s="7" r="B94">
+        <v>330</v>
+      </c>
+      <c t="s" s="7" r="C94">
+        <v>331</v>
+      </c>
+      <c t="s" s="7" r="D94">
+        <v>332</v>
+      </c>
+      <c t="s" s="7" r="E94">
+        <v>333</v>
       </c>
     </row>
     <row r="95">
-      <c s="11" r="A95"/>
-      <c t="s" s="8" r="B95">
-        <v>313</v>
-      </c>
-      <c t="s" s="8" r="C95">
-        <v>314</v>
-      </c>
-      <c t="s" s="8" r="D95">
-        <v>315</v>
-      </c>
-      <c t="s" s="8" r="E95">
-        <v>316</v>
+      <c s="10" r="A95"/>
+      <c t="s" s="7" r="B95">
+        <v>334</v>
+      </c>
+      <c t="s" s="7" r="C95">
+        <v>335</v>
+      </c>
+      <c t="s" s="7" r="D95">
+        <v>336</v>
+      </c>
+      <c t="s" s="7" r="E95">
+        <v>337</v>
       </c>
     </row>
     <row r="96">
-      <c s="11" r="A96"/>
-      <c t="s" s="8" r="B96">
-        <v>317</v>
-      </c>
-      <c t="s" s="8" r="C96">
-        <v>318</v>
-      </c>
-      <c t="s" s="8" r="D96">
-        <v>319</v>
-      </c>
-      <c t="s" s="8" r="E96">
-        <v>320</v>
+      <c s="10" r="A96"/>
+      <c t="s" s="7" r="B96">
+        <v>338</v>
+      </c>
+      <c t="s" s="7" r="C96">
+        <v>339</v>
+      </c>
+      <c t="s" s="7" r="D96">
+        <v>340</v>
+      </c>
+      <c t="s" s="7" r="E96">
+        <v>341</v>
       </c>
     </row>
     <row r="97">
-      <c s="11" r="A97"/>
-      <c t="s" s="8" r="B97">
-        <v>321</v>
-      </c>
-      <c t="s" s="8" r="C97">
-        <v>322</v>
-      </c>
-      <c t="s" s="8" r="D97">
-        <v>322</v>
-      </c>
-      <c t="s" s="8" r="E97">
-        <v>323</v>
+      <c s="10" r="A97"/>
+      <c t="s" s="7" r="B97">
+        <v>342</v>
+      </c>
+      <c t="s" s="7" r="C97">
+        <v>343</v>
+      </c>
+      <c t="s" s="7" r="D97">
+        <v>343</v>
+      </c>
+      <c t="s" s="7" r="E97">
+        <v>344</v>
       </c>
     </row>
     <row r="98">
-      <c s="11" r="A98"/>
-      <c t="s" s="8" r="B98">
-        <v>324</v>
-      </c>
-      <c t="s" s="8" r="C98">
-        <v>325</v>
-      </c>
-      <c t="s" s="8" r="D98">
-        <v>325</v>
-      </c>
-      <c t="s" s="8" r="E98">
-        <v>326</v>
+      <c s="10" r="A98"/>
+      <c t="s" s="7" r="B98">
+        <v>345</v>
+      </c>
+      <c t="s" s="7" r="C98">
+        <v>346</v>
+      </c>
+      <c t="s" s="7" r="D98">
+        <v>346</v>
+      </c>
+      <c t="s" s="7" r="E98">
+        <v>347</v>
       </c>
     </row>
     <row r="99">
-      <c s="11" r="A99"/>
-      <c t="s" s="8" r="B99">
-        <v>327</v>
-      </c>
-      <c t="s" s="8" r="C99">
-        <v>328</v>
-      </c>
-      <c t="s" s="8" r="D99">
-        <v>329</v>
-      </c>
-      <c t="s" s="8" r="E99">
-        <v>330</v>
+      <c s="10" r="A99"/>
+      <c t="s" s="7" r="B99">
+        <v>348</v>
+      </c>
+      <c t="s" s="7" r="C99">
+        <v>349</v>
+      </c>
+      <c t="s" s="7" r="D99">
+        <v>350</v>
+      </c>
+      <c t="s" s="7" r="E99">
+        <v>351</v>
       </c>
     </row>
     <row r="100">
-      <c s="11" r="A100"/>
-      <c t="s" s="17" r="B100">
-        <v>331</v>
-      </c>
-      <c t="s" s="8" r="C100">
-        <v>332</v>
-      </c>
-      <c t="s" s="8" r="D100">
-        <v>333</v>
-      </c>
-      <c t="s" s="8" r="E100">
-        <v>333</v>
+      <c s="10" r="A100"/>
+      <c t="s" s="16" r="B100">
+        <v>352</v>
+      </c>
+      <c t="s" s="7" r="C100">
+        <v>353</v>
+      </c>
+      <c t="s" s="7" r="D100">
+        <v>354</v>
+      </c>
+      <c t="s" s="7" r="E100">
+        <v>354</v>
       </c>
     </row>
     <row r="101">
-      <c s="11" r="A101"/>
-      <c t="s" s="8" r="B101">
-        <v>334</v>
-      </c>
-      <c t="s" s="8" r="C101">
-        <v>335</v>
-      </c>
-      <c t="s" s="8" r="D101">
-        <v>336</v>
-      </c>
-      <c t="s" s="8" r="E101">
-        <v>337</v>
+      <c s="10" r="A101"/>
+      <c t="s" s="7" r="B101">
+        <v>355</v>
+      </c>
+      <c t="s" s="7" r="C101">
+        <v>356</v>
+      </c>
+      <c t="s" s="7" r="D101">
+        <v>357</v>
+      </c>
+      <c t="s" s="7" r="E101">
+        <v>358</v>
       </c>
     </row>
     <row r="102">
-      <c s="11" r="A102"/>
-      <c t="s" s="8" r="B102">
-        <v>338</v>
-      </c>
-      <c t="s" s="8" r="C102">
-        <v>339</v>
-      </c>
-      <c t="s" s="8" r="D102">
-        <v>340</v>
-      </c>
-      <c t="s" s="8" r="E102">
-        <v>341</v>
+      <c s="10" r="A102"/>
+      <c t="s" s="7" r="B102">
+        <v>359</v>
+      </c>
+      <c t="s" s="7" r="C102">
+        <v>360</v>
+      </c>
+      <c t="s" s="7" r="D102">
+        <v>361</v>
+      </c>
+      <c t="s" s="7" r="E102">
+        <v>362</v>
       </c>
     </row>
     <row r="103">
-      <c s="11" r="A103"/>
-      <c t="s" s="8" r="B103">
-        <v>342</v>
-      </c>
-      <c t="s" s="8" r="C103">
-        <v>343</v>
-      </c>
-      <c t="s" s="8" r="D103">
-        <v>344</v>
-      </c>
-      <c t="s" s="8" r="E103">
-        <v>345</v>
+      <c s="10" r="A103"/>
+      <c t="s" s="7" r="B103">
+        <v>363</v>
+      </c>
+      <c t="s" s="7" r="C103">
+        <v>364</v>
+      </c>
+      <c t="s" s="7" r="D103">
+        <v>365</v>
+      </c>
+      <c t="s" s="7" r="E103">
+        <v>366</v>
       </c>
     </row>
     <row r="104">
-      <c s="11" r="A104"/>
-      <c t="s" s="8" r="B104">
-        <v>346</v>
-      </c>
-      <c t="s" s="8" r="C104">
-        <v>347</v>
-      </c>
-      <c t="s" s="8" r="D104">
-        <v>348</v>
-      </c>
-      <c t="s" s="8" r="E104">
-        <v>349</v>
+      <c s="10" r="A104"/>
+      <c t="s" s="7" r="B104">
+        <v>367</v>
+      </c>
+      <c t="s" s="7" r="C104">
+        <v>368</v>
+      </c>
+      <c t="s" s="7" r="D104">
+        <v>369</v>
+      </c>
+      <c t="s" s="7" r="E104">
+        <v>370</v>
       </c>
     </row>
     <row r="105">
-      <c s="11" r="A105"/>
-      <c t="s" s="8" r="B105">
-        <v>350</v>
-      </c>
-      <c t="s" s="8" r="C105">
-        <v>351</v>
-      </c>
-      <c t="s" s="8" r="D105">
-        <v>352</v>
-      </c>
-      <c t="s" s="8" r="E105">
-        <v>353</v>
+      <c s="10" r="A105"/>
+      <c t="s" s="7" r="B105">
+        <v>371</v>
+      </c>
+      <c t="s" s="7" r="C105">
+        <v>372</v>
+      </c>
+      <c t="s" s="7" r="D105">
+        <v>373</v>
+      </c>
+      <c t="s" s="7" r="E105">
+        <v>374</v>
       </c>
     </row>
     <row r="106">
-      <c s="11" r="A106"/>
-      <c t="s" s="8" r="B106">
-        <v>354</v>
-      </c>
-      <c t="s" s="8" r="C106">
-        <v>355</v>
-      </c>
-      <c t="s" s="8" r="D106">
-        <v>356</v>
-      </c>
-      <c t="s" s="8" r="E106">
-        <v>357</v>
+      <c s="10" r="A106"/>
+      <c t="s" s="7" r="B106">
+        <v>375</v>
+      </c>
+      <c t="s" s="7" r="C106">
+        <v>376</v>
+      </c>
+      <c t="s" s="7" r="D106">
+        <v>377</v>
+      </c>
+      <c t="s" s="7" r="E106">
+        <v>378</v>
       </c>
     </row>
     <row r="107">
-      <c s="11" r="A107"/>
-      <c t="s" s="8" r="B107">
-        <v>358</v>
-      </c>
-      <c t="s" s="8" r="C107">
-        <v>359</v>
-      </c>
-      <c t="s" s="8" r="D107">
-        <v>360</v>
-      </c>
-      <c t="s" s="8" r="E107">
-        <v>361</v>
+      <c s="10" r="A107"/>
+      <c t="s" s="7" r="B107">
+        <v>379</v>
+      </c>
+      <c t="s" s="7" r="C107">
+        <v>380</v>
+      </c>
+      <c t="s" s="7" r="D107">
+        <v>381</v>
+      </c>
+      <c t="s" s="7" r="E107">
+        <v>382</v>
       </c>
     </row>
     <row r="108">
-      <c s="11" r="A108"/>
-      <c t="s" s="8" r="B108">
-        <v>362</v>
-      </c>
-      <c t="s" s="8" r="C108">
-        <v>363</v>
-      </c>
-      <c t="s" s="8" r="D108">
-        <v>364</v>
-      </c>
-      <c t="s" s="8" r="E108">
-        <v>365</v>
+      <c s="10" r="A108"/>
+      <c t="s" s="7" r="B108">
+        <v>383</v>
+      </c>
+      <c t="s" s="7" r="C108">
+        <v>384</v>
+      </c>
+      <c t="s" s="7" r="D108">
+        <v>385</v>
+      </c>
+      <c t="s" s="7" r="E108">
+        <v>386</v>
       </c>
     </row>
     <row r="109">
-      <c s="11" r="A109"/>
-      <c t="s" s="8" r="B109">
-        <v>366</v>
-      </c>
-      <c t="s" s="8" r="C109">
-        <v>367</v>
-      </c>
-      <c t="s" s="8" r="D109">
-        <v>368</v>
-      </c>
-      <c t="s" s="8" r="E109">
-        <v>369</v>
+      <c s="10" r="A109"/>
+      <c t="s" s="7" r="B109">
+        <v>387</v>
+      </c>
+      <c t="s" s="7" r="C109">
+        <v>388</v>
+      </c>
+      <c t="s" s="7" r="D109">
+        <v>389</v>
+      </c>
+      <c t="s" s="7" r="E109">
+        <v>390</v>
       </c>
     </row>
     <row r="110">
-      <c s="11" r="A110"/>
-      <c t="s" s="8" r="B110">
-        <v>370</v>
-      </c>
-      <c t="s" s="8" r="C110">
-        <v>371</v>
-      </c>
-      <c t="s" s="8" r="D110">
-        <v>372</v>
-      </c>
-      <c t="s" s="8" r="E110">
-        <v>373</v>
+      <c s="10" r="A110"/>
+      <c t="s" s="7" r="B110">
+        <v>391</v>
+      </c>
+      <c t="s" s="7" r="C110">
+        <v>392</v>
+      </c>
+      <c t="s" s="7" r="D110">
+        <v>393</v>
+      </c>
+      <c t="s" s="7" r="E110">
+        <v>394</v>
       </c>
     </row>
     <row r="111">
-      <c s="11" r="A111"/>
-      <c t="s" s="8" r="B111">
-        <v>374</v>
-      </c>
-      <c t="s" s="8" r="C111">
-        <v>375</v>
-      </c>
-      <c t="s" s="8" r="D111">
-        <v>376</v>
-      </c>
-      <c t="s" s="8" r="E111">
-        <v>377</v>
+      <c s="10" r="A111"/>
+      <c t="s" s="7" r="B111">
+        <v>395</v>
+      </c>
+      <c t="s" s="7" r="C111">
+        <v>396</v>
+      </c>
+      <c t="s" s="7" r="D111">
+        <v>397</v>
+      </c>
+      <c t="s" s="7" r="E111">
+        <v>398</v>
       </c>
     </row>
     <row r="112">
-      <c s="11" r="A112"/>
-      <c t="s" s="8" r="B112">
-        <v>378</v>
-      </c>
-      <c t="s" s="8" r="C112">
-        <v>379</v>
-      </c>
-      <c t="s" s="8" r="D112">
-        <v>380</v>
-      </c>
-      <c t="s" s="8" r="E112">
-        <v>381</v>
+      <c s="10" r="A112"/>
+      <c t="s" s="7" r="B112">
+        <v>399</v>
+      </c>
+      <c t="s" s="7" r="C112">
+        <v>400</v>
+      </c>
+      <c t="s" s="7" r="D112">
+        <v>401</v>
+      </c>
+      <c t="s" s="7" r="E112">
+        <v>402</v>
       </c>
     </row>
     <row r="113">
-      <c s="11" r="A113"/>
-      <c t="s" s="8" r="B113">
-        <v>382</v>
-      </c>
-      <c t="s" s="8" r="C113">
-        <v>383</v>
-      </c>
-      <c t="s" s="8" r="D113">
-        <v>384</v>
-      </c>
-      <c t="s" s="8" r="E113">
-        <v>385</v>
+      <c s="10" r="A113"/>
+      <c t="s" s="7" r="B113">
+        <v>403</v>
+      </c>
+      <c t="s" s="7" r="C113">
+        <v>404</v>
+      </c>
+      <c t="s" s="7" r="D113">
+        <v>405</v>
+      </c>
+      <c t="s" s="7" r="E113">
+        <v>406</v>
       </c>
     </row>
     <row r="114">
-      <c s="11" r="A114"/>
-      <c t="s" s="8" r="B114">
-        <v>386</v>
-      </c>
-      <c t="s" s="8" r="C114">
-        <v>387</v>
-      </c>
-      <c t="s" s="8" r="D114">
-        <v>388</v>
-      </c>
-      <c t="s" s="8" r="E114">
-        <v>389</v>
+      <c s="10" r="A114"/>
+      <c t="s" s="7" r="B114">
+        <v>407</v>
+      </c>
+      <c t="s" s="7" r="C114">
+        <v>408</v>
+      </c>
+      <c t="s" s="7" r="D114">
+        <v>409</v>
+      </c>
+      <c t="s" s="7" r="E114">
+        <v>410</v>
       </c>
     </row>
     <row r="115">
-      <c s="11" r="A115"/>
-      <c t="s" s="8" r="B115">
-        <v>390</v>
-      </c>
-      <c t="s" s="8" r="C115">
-        <v>391</v>
-      </c>
-      <c t="s" s="8" r="D115">
-        <v>392</v>
-      </c>
-      <c t="s" s="8" r="E115">
-        <v>393</v>
+      <c s="10" r="A115"/>
+      <c t="s" s="7" r="B115">
+        <v>411</v>
+      </c>
+      <c t="s" s="7" r="C115">
+        <v>412</v>
+      </c>
+      <c t="s" s="7" r="D115">
+        <v>413</v>
+      </c>
+      <c t="s" s="7" r="E115">
+        <v>414</v>
       </c>
     </row>
     <row r="116">
-      <c s="11" r="A116"/>
-      <c t="s" s="8" r="B116">
-        <v>394</v>
-      </c>
-      <c t="s" s="17" r="C116">
-        <v>395</v>
-      </c>
-      <c t="s" s="8" r="D116">
-        <v>396</v>
-      </c>
-      <c t="s" s="8" r="E116">
-        <v>397</v>
+      <c s="10" r="A116"/>
+      <c t="s" s="7" r="B116">
+        <v>415</v>
+      </c>
+      <c t="s" s="16" r="C116">
+        <v>416</v>
+      </c>
+      <c t="s" s="7" r="D116">
+        <v>417</v>
+      </c>
+      <c t="s" s="7" r="E116">
+        <v>418</v>
       </c>
     </row>
     <row r="117">
-      <c s="11" r="A117"/>
-      <c t="s" s="17" r="B117">
-        <v>398</v>
-      </c>
-      <c t="s" s="17" r="C117">
-        <v>399</v>
-      </c>
-      <c t="s" s="8" r="D117">
-        <v>400</v>
-      </c>
-      <c t="s" s="8" r="E117">
-        <v>401</v>
+      <c s="10" r="A117"/>
+      <c t="s" s="16" r="B117">
+        <v>419</v>
+      </c>
+      <c t="s" s="16" r="C117">
+        <v>420</v>
+      </c>
+      <c t="s" s="7" r="D117">
+        <v>421</v>
+      </c>
+      <c t="s" s="7" r="E117">
+        <v>422</v>
       </c>
     </row>
     <row r="118">
-      <c s="11" r="A118"/>
-      <c t="s" s="8" r="B118">
-        <v>402</v>
-      </c>
-      <c t="s" s="17" r="C118">
-        <v>399</v>
-      </c>
-      <c t="s" s="8" r="D118">
-        <v>400</v>
-      </c>
-      <c t="s" s="8" r="E118">
-        <v>401</v>
+      <c s="10" r="A118"/>
+      <c t="s" s="7" r="B118">
+        <v>423</v>
+      </c>
+      <c t="s" s="16" r="C118">
+        <v>420</v>
+      </c>
+      <c t="s" s="7" r="D118">
+        <v>421</v>
+      </c>
+      <c t="s" s="7" r="E118">
+        <v>422</v>
       </c>
     </row>
     <row r="119">
-      <c s="11" r="A119"/>
-      <c t="s" s="8" r="B119">
-        <v>403</v>
-      </c>
-      <c t="s" s="6" r="C119">
-        <v>404</v>
-      </c>
-      <c t="s" s="8" r="D119">
-        <v>405</v>
-      </c>
-      <c t="s" s="8" r="E119">
-        <v>406</v>
+      <c s="10" r="A119"/>
+      <c t="s" s="7" r="B119">
+        <v>424</v>
+      </c>
+      <c t="s" s="5" r="C119">
+        <v>425</v>
+      </c>
+      <c t="s" s="7" r="D119">
+        <v>426</v>
+      </c>
+      <c t="s" s="7" r="E119">
+        <v>427</v>
       </c>
     </row>
     <row r="120">
-      <c s="11" r="A120"/>
-      <c t="s" s="8" r="B120">
-        <v>407</v>
-      </c>
-      <c t="s" s="6" r="C120">
-        <v>408</v>
-      </c>
-      <c t="s" s="8" r="D120">
-        <v>409</v>
-      </c>
-      <c t="s" s="8" r="E120">
-        <v>410</v>
+      <c s="10" r="A120"/>
+      <c t="s" s="7" r="B120">
+        <v>428</v>
+      </c>
+      <c t="s" s="5" r="C120">
+        <v>429</v>
+      </c>
+      <c t="s" s="7" r="D120">
+        <v>430</v>
+      </c>
+      <c t="s" s="7" r="E120">
+        <v>431</v>
       </c>
     </row>
     <row r="121">
-      <c s="11" r="A121"/>
-      <c t="s" s="8" r="B121">
-        <v>411</v>
-      </c>
-      <c t="s" s="6" r="C121">
-        <v>412</v>
-      </c>
-      <c t="s" s="8" r="D121">
-        <v>413</v>
-      </c>
-      <c t="s" s="6" r="E121">
-        <v>414</v>
+      <c s="10" r="A121"/>
+      <c t="s" s="7" r="B121">
+        <v>432</v>
+      </c>
+      <c t="s" s="5" r="C121">
+        <v>433</v>
+      </c>
+      <c t="s" s="7" r="D121">
+        <v>434</v>
+      </c>
+      <c t="s" s="5" r="E121">
+        <v>435</v>
       </c>
     </row>
     <row r="122">
-      <c s="11" r="A122"/>
-      <c s="20" r="B122"/>
-      <c s="10" r="C122"/>
-      <c s="20" r="D122"/>
-      <c s="20" r="E122"/>
+      <c s="10" r="A122"/>
+      <c s="19" r="B122"/>
+      <c s="9" r="C122"/>
+      <c s="19" r="D122"/>
+      <c s="19" r="E122"/>
     </row>
     <row r="123">
-      <c t="s" s="11" r="A123">
-        <v>415</v>
-      </c>
-      <c t="s" s="5" r="B123">
-        <v>416</v>
-      </c>
-      <c t="s" s="4" r="C123">
-        <v>417</v>
-      </c>
-      <c t="s" s="5" r="D123">
-        <v>418</v>
-      </c>
-      <c t="s" s="5" r="E123">
-        <v>419</v>
+      <c t="s" s="10" r="A123">
+        <v>436</v>
+      </c>
+      <c t="s" s="7" r="B123">
+        <v>437</v>
+      </c>
+      <c t="s" s="16" r="C123">
+        <v>438</v>
+      </c>
+      <c t="s" s="7" r="D123">
+        <v>439</v>
+      </c>
+      <c t="s" s="7" r="E123">
+        <v>440</v>
       </c>
     </row>
     <row r="124">
-      <c s="11" r="A124"/>
-      <c t="s" s="5" r="B124">
-        <v>420</v>
-      </c>
-      <c t="s" s="4" r="C124">
-        <v>421</v>
-      </c>
-      <c s="5" r="D124"/>
-      <c s="5" r="E124"/>
+      <c s="10" r="A124"/>
+      <c t="s" s="7" r="B124">
+        <v>441</v>
+      </c>
+      <c t="s" s="16" r="C124">
+        <v>442</v>
+      </c>
+      <c t="s" s="7" r="D124">
+        <v>443</v>
+      </c>
+      <c t="s" s="7" r="E124">
+        <v>444</v>
+      </c>
     </row>
     <row r="125">
-      <c s="15" r="A125"/>
-      <c t="s" s="5" r="B125">
-        <v>422</v>
-      </c>
-      <c t="s" s="4" r="C125">
-        <v>423</v>
-      </c>
-      <c t="s" s="5" r="D125">
-        <v>424</v>
-      </c>
-      <c t="s" s="5" r="E125">
-        <v>425</v>
+      <c s="14" r="A125"/>
+      <c t="s" s="7" r="B125">
+        <v>445</v>
+      </c>
+      <c t="s" s="16" r="C125">
+        <v>446</v>
+      </c>
+      <c t="s" s="7" r="D125">
+        <v>447</v>
+      </c>
+      <c t="s" s="7" r="E125">
+        <v>448</v>
       </c>
     </row>
     <row r="126">
-      <c s="11" r="A126"/>
-      <c t="s" s="21" r="B126">
-        <v>426</v>
-      </c>
-      <c t="s" s="4" r="C126">
-        <v>427</v>
-      </c>
-      <c s="21" r="D126"/>
-      <c s="21" r="E126"/>
+      <c s="10" r="A126"/>
+      <c t="s" s="3" r="B126">
+        <v>449</v>
+      </c>
+      <c t="s" s="16" r="C126">
+        <v>450</v>
+      </c>
+      <c t="s" s="3" r="D126">
+        <v>451</v>
+      </c>
+      <c t="s" s="3" r="E126">
+        <v>452</v>
+      </c>
     </row>
     <row r="127">
-      <c s="11" r="A127"/>
-      <c t="s" s="5" r="B127">
-        <v>428</v>
-      </c>
-      <c t="s" s="4" r="C127">
-        <v>429</v>
-      </c>
-      <c s="5" r="D127"/>
-      <c s="5" r="E127"/>
+      <c s="10" r="A127"/>
+      <c t="s" s="7" r="B127">
+        <v>453</v>
+      </c>
+      <c t="s" s="16" r="C127">
+        <v>454</v>
+      </c>
+      <c t="s" s="7" r="D127">
+        <v>455</v>
+      </c>
+      <c t="s" s="7" r="E127">
+        <v>456</v>
+      </c>
     </row>
     <row r="128">
-      <c s="11" r="A128"/>
-      <c t="s" s="5" r="B128">
-        <v>430</v>
-      </c>
-      <c t="s" s="4" r="C128">
-        <v>431</v>
-      </c>
-      <c s="5" r="D128"/>
-      <c s="5" r="E128"/>
+      <c s="10" r="A128"/>
+      <c t="s" s="7" r="B128">
+        <v>457</v>
+      </c>
+      <c t="s" s="16" r="C128">
+        <v>458</v>
+      </c>
+      <c t="s" s="7" r="D128">
+        <v>459</v>
+      </c>
+      <c t="s" s="7" r="E128">
+        <v>460</v>
+      </c>
     </row>
     <row r="129">
-      <c s="11" r="A129"/>
-      <c t="s" s="5" r="B129">
-        <v>432</v>
-      </c>
-      <c t="s" s="4" r="C129">
-        <v>433</v>
-      </c>
-      <c s="5" r="D129"/>
-      <c s="5" r="E129"/>
+      <c s="10" r="A129"/>
+      <c t="s" s="7" r="B129">
+        <v>461</v>
+      </c>
+      <c t="s" s="16" r="C129">
+        <v>462</v>
+      </c>
+      <c t="s" s="7" r="D129">
+        <v>463</v>
+      </c>
+      <c t="s" s="7" r="E129">
+        <v>464</v>
+      </c>
     </row>
     <row r="130">
-      <c s="11" r="A130"/>
-      <c t="s" s="5" r="B130">
-        <v>434</v>
-      </c>
-      <c t="s" s="4" r="C130">
-        <v>435</v>
-      </c>
-      <c s="5" r="D130"/>
-      <c s="5" r="E130"/>
+      <c s="10" r="A130"/>
+      <c t="s" s="7" r="B130">
+        <v>465</v>
+      </c>
+      <c t="s" s="16" r="C130">
+        <v>466</v>
+      </c>
+      <c t="s" s="7" r="D130">
+        <v>467</v>
+      </c>
+      <c t="s" s="7" r="E130">
+        <v>468</v>
+      </c>
     </row>
     <row r="131">
-      <c s="11" r="A131"/>
-      <c t="s" s="5" r="B131">
-        <v>436</v>
-      </c>
-      <c t="s" s="4" r="C131">
-        <v>437</v>
-      </c>
-      <c s="5" r="D131"/>
-      <c s="5" r="E131"/>
+      <c s="10" r="A131"/>
+      <c t="s" s="7" r="B131">
+        <v>469</v>
+      </c>
+      <c t="s" s="16" r="C131">
+        <v>470</v>
+      </c>
+      <c t="s" s="7" r="D131">
+        <v>471</v>
+      </c>
+      <c t="s" s="7" r="E131">
+        <v>472</v>
+      </c>
     </row>
     <row r="132">
-      <c s="11" r="A132"/>
-      <c t="s" s="5" r="B132">
-        <v>438</v>
-      </c>
-      <c t="s" s="4" r="C132">
-        <v>439</v>
-      </c>
-      <c s="5" r="D132"/>
-      <c s="5" r="E132"/>
+      <c s="10" r="A132"/>
+      <c t="s" s="7" r="B132">
+        <v>473</v>
+      </c>
+      <c t="s" s="16" r="C132">
+        <v>474</v>
+      </c>
+      <c t="s" s="7" r="D132">
+        <v>475</v>
+      </c>
+      <c t="s" s="7" r="E132">
+        <v>476</v>
+      </c>
     </row>
     <row r="133">
-      <c s="11" r="A133"/>
-      <c t="s" s="5" r="B133">
-        <v>440</v>
-      </c>
-      <c t="s" s="4" r="C133">
-        <v>441</v>
-      </c>
-      <c s="5" r="D133"/>
-      <c s="5" r="E133"/>
+      <c s="10" r="A133"/>
+      <c t="s" s="7" r="B133">
+        <v>477</v>
+      </c>
+      <c t="s" s="16" r="C133">
+        <v>478</v>
+      </c>
+      <c t="s" s="7" r="D133">
+        <v>479</v>
+      </c>
+      <c t="s" s="7" r="E133">
+        <v>480</v>
+      </c>
     </row>
     <row r="134">
-      <c s="11" r="A134"/>
-      <c t="s" s="5" r="B134">
-        <v>442</v>
-      </c>
-      <c t="s" s="4" r="C134">
-        <v>443</v>
-      </c>
-      <c s="5" r="D134"/>
-      <c s="5" r="E134"/>
+      <c s="10" r="A134"/>
+      <c t="s" s="7" r="B134">
+        <v>481</v>
+      </c>
+      <c t="s" s="16" r="C134">
+        <v>482</v>
+      </c>
+      <c t="s" s="7" r="D134">
+        <v>483</v>
+      </c>
+      <c t="s" s="7" r="E134">
+        <v>484</v>
+      </c>
     </row>
     <row r="135">
-      <c s="11" r="A135"/>
-      <c t="s" s="5" r="B135">
-        <v>444</v>
-      </c>
-      <c t="s" s="4" r="C135">
-        <v>445</v>
-      </c>
-      <c s="5" r="D135"/>
-      <c s="5" r="E135"/>
+      <c s="10" r="A135"/>
+      <c t="s" s="7" r="B135">
+        <v>485</v>
+      </c>
+      <c t="s" s="16" r="C135">
+        <v>486</v>
+      </c>
+      <c t="s" s="7" r="D135">
+        <v>487</v>
+      </c>
+      <c t="s" s="7" r="E135">
+        <v>488</v>
+      </c>
     </row>
     <row r="136">
-      <c s="11" r="A136"/>
-      <c s="13" r="B136"/>
-      <c s="18" r="C136"/>
-      <c s="13" r="D136"/>
-      <c s="13" r="E136"/>
+      <c s="10" r="A136"/>
+      <c s="12" r="B136"/>
+      <c s="17" r="C136"/>
+      <c s="12" r="D136"/>
+      <c s="12" r="E136"/>
     </row>
     <row r="137">
-      <c t="s" s="11" r="A137">
-        <v>446</v>
-      </c>
-      <c t="s" s="8" r="B137">
-        <v>447</v>
-      </c>
-      <c t="s" s="17" r="C137">
-        <v>448</v>
-      </c>
-      <c t="s" s="8" r="D137">
-        <v>449</v>
-      </c>
-      <c t="s" s="8" r="E137">
-        <v>450</v>
+      <c t="s" s="10" r="A137">
+        <v>489</v>
+      </c>
+      <c t="s" s="7" r="B137">
+        <v>490</v>
+      </c>
+      <c t="s" s="16" r="C137">
+        <v>491</v>
+      </c>
+      <c t="s" s="7" r="D137">
+        <v>492</v>
+      </c>
+      <c t="s" s="7" r="E137">
+        <v>493</v>
       </c>
     </row>
     <row r="138">
-      <c s="11" r="A138"/>
-      <c t="s" s="8" r="B138">
-        <v>451</v>
-      </c>
-      <c t="s" s="17" r="C138">
-        <v>452</v>
-      </c>
-      <c t="s" s="8" r="D138">
-        <v>453</v>
-      </c>
-      <c t="s" s="8" r="E138">
-        <v>454</v>
+      <c s="10" r="A138"/>
+      <c t="s" s="7" r="B138">
+        <v>494</v>
+      </c>
+      <c t="s" s="16" r="C138">
+        <v>495</v>
+      </c>
+      <c t="s" s="7" r="D138">
+        <v>496</v>
+      </c>
+      <c t="s" s="7" r="E138">
+        <v>497</v>
       </c>
     </row>
     <row r="139">
-      <c s="11" r="A139"/>
-      <c t="s" s="8" r="B139">
-        <v>455</v>
-      </c>
-      <c t="s" s="17" r="C139">
-        <v>456</v>
-      </c>
-      <c t="s" s="8" r="D139">
-        <v>457</v>
-      </c>
-      <c t="s" s="8" r="E139">
-        <v>458</v>
+      <c s="10" r="A139"/>
+      <c t="s" s="7" r="B139">
+        <v>498</v>
+      </c>
+      <c t="s" s="16" r="C139">
+        <v>499</v>
+      </c>
+      <c t="s" s="7" r="D139">
+        <v>500</v>
+      </c>
+      <c t="s" s="7" r="E139">
+        <v>501</v>
       </c>
     </row>
     <row r="140">
-      <c s="11" r="A140"/>
-      <c t="s" s="8" r="B140">
-        <v>459</v>
-      </c>
-      <c t="s" s="17" r="C140">
-        <v>460</v>
-      </c>
-      <c t="s" s="8" r="D140">
-        <v>461</v>
-      </c>
-      <c t="s" s="8" r="E140">
-        <v>462</v>
+      <c s="10" r="A140"/>
+      <c t="s" s="7" r="B140">
+        <v>502</v>
+      </c>
+      <c t="s" s="16" r="C140">
+        <v>503</v>
+      </c>
+      <c t="s" s="7" r="D140">
+        <v>504</v>
+      </c>
+      <c t="s" s="7" r="E140">
+        <v>505</v>
       </c>
     </row>
     <row r="141">
-      <c s="11" r="A141"/>
-      <c t="s" s="8" r="B141">
-        <v>463</v>
-      </c>
-      <c t="s" s="17" r="C141">
-        <v>464</v>
-      </c>
-      <c t="s" s="8" r="D141">
-        <v>465</v>
-      </c>
-      <c t="s" s="8" r="E141">
-        <v>466</v>
+      <c s="10" r="A141"/>
+      <c t="s" s="7" r="B141">
+        <v>506</v>
+      </c>
+      <c t="s" s="16" r="C141">
+        <v>507</v>
+      </c>
+      <c t="s" s="7" r="D141">
+        <v>508</v>
+      </c>
+      <c t="s" s="7" r="E141">
+        <v>509</v>
       </c>
     </row>
     <row r="142">
-      <c s="11" r="A142"/>
+      <c s="10" r="A142"/>
       <c s="2" r="B142"/>
-      <c s="14" r="C142"/>
+      <c s="13" r="C142"/>
       <c s="2" r="D142"/>
       <c s="2" r="E142"/>
     </row>
     <row r="143">
-      <c t="s" s="11" r="A143">
-        <v>467</v>
-      </c>
-      <c t="s" s="16" r="B143">
-        <v>468</v>
+      <c t="s" s="10" r="A143">
+        <v>510</v>
+      </c>
+      <c t="s" s="15" r="B143">
+        <v>511</v>
       </c>
       <c t="s" s="1" r="C143">
-        <v>467</v>
-      </c>
-      <c s="16" r="D143"/>
-      <c s="16" r="E143"/>
+        <v>510</v>
+      </c>
+      <c s="15" r="D143"/>
+      <c s="15" r="E143"/>
     </row>
     <row r="144">
-      <c s="11" r="A144"/>
-      <c s="20" r="B144"/>
-      <c s="10" r="C144"/>
-      <c s="20" r="D144"/>
-      <c s="20" r="E144"/>
+      <c s="10" r="A144"/>
+      <c s="19" r="B144"/>
+      <c s="9" r="C144"/>
+      <c s="19" r="D144"/>
+      <c s="19" r="E144"/>
     </row>
     <row r="145">
-      <c t="s" s="11" r="A145">
-        <v>469</v>
-      </c>
-      <c t="s" s="24" r="B145">
-        <v>470</v>
-      </c>
-      <c t="s" s="22" r="C145">
-        <v>471</v>
-      </c>
-      <c s="24" r="D145"/>
-      <c s="24" r="E145"/>
+      <c t="s" s="10" r="A145">
+        <v>512</v>
+      </c>
+      <c t="s" s="23" r="B145">
+        <v>513</v>
+      </c>
+      <c t="s" s="21" r="C145">
+        <v>514</v>
+      </c>
+      <c s="23" r="D145"/>
+      <c s="23" r="E145"/>
     </row>
     <row r="146">
-      <c s="11" r="A146"/>
-      <c t="s" s="24" r="B146">
-        <v>472</v>
-      </c>
-      <c t="s" s="22" r="C146">
-        <v>473</v>
-      </c>
-      <c s="24" r="D146"/>
-      <c s="24" r="E146"/>
+      <c s="10" r="A146"/>
+      <c t="s" s="23" r="B146">
+        <v>515</v>
+      </c>
+      <c t="s" s="21" r="C146">
+        <v>516</v>
+      </c>
+      <c s="23" r="D146"/>
+      <c s="23" r="E146"/>
     </row>
     <row r="147">
-      <c s="11" r="A147"/>
-      <c s="20" r="B147"/>
-      <c s="10" r="C147"/>
-      <c s="20" r="D147"/>
-      <c s="20" r="E147"/>
+      <c s="10" r="A147"/>
+      <c s="19" r="B147"/>
+      <c s="9" r="C147"/>
+      <c s="19" r="D147"/>
+      <c s="19" r="E147"/>
     </row>
     <row r="148">
-      <c s="11" r="A148"/>
-      <c s="20" r="B148"/>
-      <c s="10" r="C148"/>
-      <c s="20" r="D148"/>
-      <c s="20" r="E148"/>
+      <c s="10" r="A148"/>
+      <c s="19" r="B148"/>
+      <c s="9" r="C148"/>
+      <c s="19" r="D148"/>
+      <c s="19" r="E148"/>
     </row>
     <row r="149">
-      <c s="11" r="A149"/>
-      <c s="20" r="B149"/>
-      <c s="10" r="C149"/>
-      <c s="20" r="D149"/>
-      <c s="20" r="E149"/>
+      <c s="10" r="A149"/>
+      <c s="19" r="B149"/>
+      <c s="9" r="C149"/>
+      <c s="19" r="D149"/>
+      <c s="19" r="E149"/>
     </row>
   </sheetData>
 </worksheet>
@@ -3850,164 +4054,164 @@
   <sheetFormatPr customHeight="1" defaultColWidth="9.86" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c s="23" r="A1"/>
-      <c s="23" r="B1"/>
-      <c s="23" r="C1"/>
-      <c s="23" r="D1"/>
-      <c s="23" r="E1"/>
-      <c s="23" r="F1"/>
+      <c s="22" r="A1"/>
+      <c s="22" r="B1"/>
+      <c s="22" r="C1"/>
+      <c s="22" r="D1"/>
+      <c s="22" r="E1"/>
+      <c s="22" r="F1"/>
     </row>
     <row r="2">
-      <c s="23" r="A2"/>
-      <c s="23" r="B2"/>
-      <c s="23" r="C2"/>
-      <c s="23" r="D2"/>
-      <c s="23" r="E2"/>
-      <c s="23" r="F2"/>
+      <c s="22" r="A2"/>
+      <c s="22" r="B2"/>
+      <c s="22" r="C2"/>
+      <c s="22" r="D2"/>
+      <c s="22" r="E2"/>
+      <c s="22" r="F2"/>
     </row>
     <row r="3">
-      <c s="23" r="A3"/>
-      <c s="23" r="B3"/>
-      <c s="23" r="C3"/>
-      <c s="23" r="D3"/>
-      <c s="23" r="E3"/>
-      <c s="23" r="F3"/>
+      <c s="22" r="A3"/>
+      <c s="22" r="B3"/>
+      <c s="22" r="C3"/>
+      <c s="22" r="D3"/>
+      <c s="22" r="E3"/>
+      <c s="22" r="F3"/>
     </row>
     <row r="4">
-      <c s="23" r="A4"/>
-      <c s="23" r="B4"/>
-      <c s="23" r="C4"/>
-      <c s="23" r="D4"/>
-      <c s="23" r="E4"/>
-      <c s="23" r="F4"/>
+      <c s="22" r="A4"/>
+      <c s="22" r="B4"/>
+      <c s="22" r="C4"/>
+      <c s="22" r="D4"/>
+      <c s="22" r="E4"/>
+      <c s="22" r="F4"/>
     </row>
     <row r="5">
-      <c s="23" r="A5"/>
-      <c s="23" r="B5"/>
-      <c s="23" r="C5"/>
-      <c s="23" r="D5"/>
-      <c s="23" r="E5"/>
-      <c s="23" r="F5"/>
+      <c s="22" r="A5"/>
+      <c s="22" r="B5"/>
+      <c s="22" r="C5"/>
+      <c s="22" r="D5"/>
+      <c s="22" r="E5"/>
+      <c s="22" r="F5"/>
     </row>
     <row r="6">
-      <c s="23" r="A6"/>
-      <c s="23" r="B6"/>
-      <c s="23" r="C6"/>
-      <c s="23" r="D6"/>
-      <c s="23" r="E6"/>
-      <c s="23" r="F6"/>
+      <c s="22" r="A6"/>
+      <c s="22" r="B6"/>
+      <c s="22" r="C6"/>
+      <c s="22" r="D6"/>
+      <c s="22" r="E6"/>
+      <c s="22" r="F6"/>
     </row>
     <row r="7">
-      <c s="23" r="A7"/>
-      <c s="23" r="B7"/>
-      <c s="23" r="C7"/>
-      <c s="23" r="D7"/>
-      <c s="23" r="E7"/>
-      <c s="23" r="F7"/>
+      <c s="22" r="A7"/>
+      <c s="22" r="B7"/>
+      <c s="22" r="C7"/>
+      <c s="22" r="D7"/>
+      <c s="22" r="E7"/>
+      <c s="22" r="F7"/>
     </row>
     <row r="8">
-      <c s="23" r="A8"/>
-      <c s="23" r="B8"/>
-      <c s="23" r="C8"/>
-      <c s="23" r="D8"/>
-      <c s="23" r="E8"/>
-      <c s="23" r="F8"/>
+      <c s="22" r="A8"/>
+      <c s="22" r="B8"/>
+      <c s="22" r="C8"/>
+      <c s="22" r="D8"/>
+      <c s="22" r="E8"/>
+      <c s="22" r="F8"/>
     </row>
     <row r="9">
-      <c s="23" r="A9"/>
-      <c s="23" r="B9"/>
-      <c s="23" r="C9"/>
-      <c s="23" r="D9"/>
-      <c s="23" r="E9"/>
-      <c s="23" r="F9"/>
+      <c s="22" r="A9"/>
+      <c s="22" r="B9"/>
+      <c s="22" r="C9"/>
+      <c s="22" r="D9"/>
+      <c s="22" r="E9"/>
+      <c s="22" r="F9"/>
     </row>
     <row r="10">
-      <c s="23" r="A10"/>
-      <c s="23" r="B10"/>
-      <c s="23" r="C10"/>
-      <c s="23" r="D10"/>
-      <c s="23" r="E10"/>
-      <c s="23" r="F10"/>
+      <c s="22" r="A10"/>
+      <c s="22" r="B10"/>
+      <c s="22" r="C10"/>
+      <c s="22" r="D10"/>
+      <c s="22" r="E10"/>
+      <c s="22" r="F10"/>
     </row>
     <row r="11">
-      <c s="23" r="A11"/>
-      <c s="23" r="B11"/>
-      <c s="23" r="C11"/>
-      <c s="23" r="D11"/>
-      <c s="23" r="E11"/>
-      <c s="23" r="F11"/>
+      <c s="22" r="A11"/>
+      <c s="22" r="B11"/>
+      <c s="22" r="C11"/>
+      <c s="22" r="D11"/>
+      <c s="22" r="E11"/>
+      <c s="22" r="F11"/>
     </row>
     <row r="12">
-      <c s="23" r="A12"/>
-      <c s="23" r="B12"/>
-      <c s="23" r="C12"/>
-      <c s="23" r="D12"/>
-      <c s="23" r="E12"/>
-      <c s="23" r="F12"/>
+      <c s="22" r="A12"/>
+      <c s="22" r="B12"/>
+      <c s="22" r="C12"/>
+      <c s="22" r="D12"/>
+      <c s="22" r="E12"/>
+      <c s="22" r="F12"/>
     </row>
     <row r="13">
-      <c s="23" r="A13"/>
-      <c s="23" r="B13"/>
-      <c s="23" r="C13"/>
-      <c s="23" r="D13"/>
-      <c s="23" r="E13"/>
-      <c s="23" r="F13"/>
+      <c s="22" r="A13"/>
+      <c s="22" r="B13"/>
+      <c s="22" r="C13"/>
+      <c s="22" r="D13"/>
+      <c s="22" r="E13"/>
+      <c s="22" r="F13"/>
     </row>
     <row r="14">
-      <c s="23" r="A14"/>
-      <c s="23" r="B14"/>
-      <c s="23" r="C14"/>
-      <c s="23" r="D14"/>
-      <c s="23" r="E14"/>
-      <c s="23" r="F14"/>
+      <c s="22" r="A14"/>
+      <c s="22" r="B14"/>
+      <c s="22" r="C14"/>
+      <c s="22" r="D14"/>
+      <c s="22" r="E14"/>
+      <c s="22" r="F14"/>
     </row>
     <row r="15">
-      <c s="23" r="A15"/>
-      <c s="23" r="B15"/>
-      <c s="23" r="C15"/>
-      <c s="23" r="D15"/>
-      <c s="23" r="E15"/>
-      <c s="23" r="F15"/>
+      <c s="22" r="A15"/>
+      <c s="22" r="B15"/>
+      <c s="22" r="C15"/>
+      <c s="22" r="D15"/>
+      <c s="22" r="E15"/>
+      <c s="22" r="F15"/>
     </row>
     <row r="16">
-      <c s="23" r="A16"/>
-      <c s="23" r="B16"/>
-      <c s="23" r="C16"/>
-      <c s="23" r="D16"/>
-      <c s="23" r="E16"/>
-      <c s="23" r="F16"/>
+      <c s="22" r="A16"/>
+      <c s="22" r="B16"/>
+      <c s="22" r="C16"/>
+      <c s="22" r="D16"/>
+      <c s="22" r="E16"/>
+      <c s="22" r="F16"/>
     </row>
     <row r="17">
-      <c s="23" r="A17"/>
-      <c s="23" r="B17"/>
-      <c s="23" r="C17"/>
-      <c s="23" r="D17"/>
-      <c s="23" r="E17"/>
-      <c s="23" r="F17"/>
+      <c s="22" r="A17"/>
+      <c s="22" r="B17"/>
+      <c s="22" r="C17"/>
+      <c s="22" r="D17"/>
+      <c s="22" r="E17"/>
+      <c s="22" r="F17"/>
     </row>
     <row r="18">
-      <c s="23" r="A18"/>
-      <c s="23" r="B18"/>
-      <c s="23" r="C18"/>
-      <c s="23" r="D18"/>
-      <c s="23" r="E18"/>
-      <c s="23" r="F18"/>
+      <c s="22" r="A18"/>
+      <c s="22" r="B18"/>
+      <c s="22" r="C18"/>
+      <c s="22" r="D18"/>
+      <c s="22" r="E18"/>
+      <c s="22" r="F18"/>
     </row>
     <row r="19">
-      <c s="23" r="A19"/>
-      <c s="23" r="B19"/>
-      <c s="23" r="C19"/>
-      <c s="23" r="D19"/>
-      <c s="23" r="E19"/>
-      <c s="23" r="F19"/>
+      <c s="22" r="A19"/>
+      <c s="22" r="B19"/>
+      <c s="22" r="C19"/>
+      <c s="22" r="D19"/>
+      <c s="22" r="E19"/>
+      <c s="22" r="F19"/>
     </row>
     <row r="20">
-      <c s="23" r="A20"/>
-      <c s="23" r="B20"/>
-      <c s="23" r="C20"/>
-      <c s="23" r="D20"/>
-      <c s="23" r="E20"/>
-      <c s="23" r="F20"/>
+      <c s="22" r="A20"/>
+      <c s="22" r="B20"/>
+      <c s="22" r="C20"/>
+      <c s="22" r="D20"/>
+      <c s="22" r="E20"/>
+      <c s="22" r="F20"/>
     </row>
   </sheetData>
 </worksheet>
@@ -4021,164 +4225,164 @@
   <sheetFormatPr customHeight="1" defaultColWidth="9.86" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c s="23" r="A1"/>
-      <c s="23" r="B1"/>
-      <c s="23" r="C1"/>
-      <c s="23" r="D1"/>
-      <c s="23" r="E1"/>
-      <c s="23" r="F1"/>
+      <c s="22" r="A1"/>
+      <c s="22" r="B1"/>
+      <c s="22" r="C1"/>
+      <c s="22" r="D1"/>
+      <c s="22" r="E1"/>
+      <c s="22" r="F1"/>
     </row>
     <row r="2">
-      <c s="23" r="A2"/>
-      <c s="23" r="B2"/>
-      <c s="23" r="C2"/>
-      <c s="23" r="D2"/>
-      <c s="23" r="E2"/>
-      <c s="23" r="F2"/>
+      <c s="22" r="A2"/>
+      <c s="22" r="B2"/>
+      <c s="22" r="C2"/>
+      <c s="22" r="D2"/>
+      <c s="22" r="E2"/>
+      <c s="22" r="F2"/>
     </row>
     <row r="3">
-      <c s="23" r="A3"/>
-      <c s="23" r="B3"/>
-      <c s="23" r="C3"/>
-      <c s="23" r="D3"/>
-      <c s="23" r="E3"/>
-      <c s="23" r="F3"/>
+      <c s="22" r="A3"/>
+      <c s="22" r="B3"/>
+      <c s="22" r="C3"/>
+      <c s="22" r="D3"/>
+      <c s="22" r="E3"/>
+      <c s="22" r="F3"/>
     </row>
     <row r="4">
-      <c s="23" r="A4"/>
-      <c s="23" r="B4"/>
-      <c s="23" r="C4"/>
-      <c s="23" r="D4"/>
-      <c s="23" r="E4"/>
-      <c s="23" r="F4"/>
+      <c s="22" r="A4"/>
+      <c s="22" r="B4"/>
+      <c s="22" r="C4"/>
+      <c s="22" r="D4"/>
+      <c s="22" r="E4"/>
+      <c s="22" r="F4"/>
     </row>
     <row r="5">
-      <c s="23" r="A5"/>
-      <c s="23" r="B5"/>
-      <c s="23" r="C5"/>
-      <c s="23" r="D5"/>
-      <c s="23" r="E5"/>
-      <c s="23" r="F5"/>
+      <c s="22" r="A5"/>
+      <c s="22" r="B5"/>
+      <c s="22" r="C5"/>
+      <c s="22" r="D5"/>
+      <c s="22" r="E5"/>
+      <c s="22" r="F5"/>
     </row>
     <row r="6">
-      <c s="23" r="A6"/>
-      <c s="23" r="B6"/>
-      <c s="23" r="C6"/>
-      <c s="23" r="D6"/>
-      <c s="23" r="E6"/>
-      <c s="23" r="F6"/>
+      <c s="22" r="A6"/>
+      <c s="22" r="B6"/>
+      <c s="22" r="C6"/>
+      <c s="22" r="D6"/>
+      <c s="22" r="E6"/>
+      <c s="22" r="F6"/>
     </row>
     <row r="7">
-      <c s="23" r="A7"/>
-      <c s="23" r="B7"/>
-      <c s="23" r="C7"/>
-      <c s="23" r="D7"/>
-      <c s="23" r="E7"/>
-      <c s="23" r="F7"/>
+      <c s="22" r="A7"/>
+      <c s="22" r="B7"/>
+      <c s="22" r="C7"/>
+      <c s="22" r="D7"/>
+      <c s="22" r="E7"/>
+      <c s="22" r="F7"/>
     </row>
     <row r="8">
-      <c s="23" r="A8"/>
-      <c s="23" r="B8"/>
-      <c s="23" r="C8"/>
-      <c s="23" r="D8"/>
-      <c s="23" r="E8"/>
-      <c s="23" r="F8"/>
+      <c s="22" r="A8"/>
+      <c s="22" r="B8"/>
+      <c s="22" r="C8"/>
+      <c s="22" r="D8"/>
+      <c s="22" r="E8"/>
+      <c s="22" r="F8"/>
     </row>
     <row r="9">
-      <c s="23" r="A9"/>
-      <c s="23" r="B9"/>
-      <c s="23" r="C9"/>
-      <c s="23" r="D9"/>
-      <c s="23" r="E9"/>
-      <c s="23" r="F9"/>
+      <c s="22" r="A9"/>
+      <c s="22" r="B9"/>
+      <c s="22" r="C9"/>
+      <c s="22" r="D9"/>
+      <c s="22" r="E9"/>
+      <c s="22" r="F9"/>
     </row>
     <row r="10">
-      <c s="23" r="A10"/>
-      <c s="23" r="B10"/>
-      <c s="23" r="C10"/>
-      <c s="23" r="D10"/>
-      <c s="23" r="E10"/>
-      <c s="23" r="F10"/>
+      <c s="22" r="A10"/>
+      <c s="22" r="B10"/>
+      <c s="22" r="C10"/>
+      <c s="22" r="D10"/>
+      <c s="22" r="E10"/>
+      <c s="22" r="F10"/>
     </row>
     <row r="11">
-      <c s="23" r="A11"/>
-      <c s="23" r="B11"/>
-      <c s="23" r="C11"/>
-      <c s="23" r="D11"/>
-      <c s="23" r="E11"/>
-      <c s="23" r="F11"/>
+      <c s="22" r="A11"/>
+      <c s="22" r="B11"/>
+      <c s="22" r="C11"/>
+      <c s="22" r="D11"/>
+      <c s="22" r="E11"/>
+      <c s="22" r="F11"/>
     </row>
     <row r="12">
-      <c s="23" r="A12"/>
-      <c s="23" r="B12"/>
-      <c s="23" r="C12"/>
-      <c s="23" r="D12"/>
-      <c s="23" r="E12"/>
-      <c s="23" r="F12"/>
+      <c s="22" r="A12"/>
+      <c s="22" r="B12"/>
+      <c s="22" r="C12"/>
+      <c s="22" r="D12"/>
+      <c s="22" r="E12"/>
+      <c s="22" r="F12"/>
     </row>
     <row r="13">
-      <c s="23" r="A13"/>
-      <c s="23" r="B13"/>
-      <c s="23" r="C13"/>
-      <c s="23" r="D13"/>
-      <c s="23" r="E13"/>
-      <c s="23" r="F13"/>
+      <c s="22" r="A13"/>
+      <c s="22" r="B13"/>
+      <c s="22" r="C13"/>
+      <c s="22" r="D13"/>
+      <c s="22" r="E13"/>
+      <c s="22" r="F13"/>
     </row>
     <row r="14">
-      <c s="23" r="A14"/>
-      <c s="23" r="B14"/>
-      <c s="23" r="C14"/>
-      <c s="23" r="D14"/>
-      <c s="23" r="E14"/>
-      <c s="23" r="F14"/>
+      <c s="22" r="A14"/>
+      <c s="22" r="B14"/>
+      <c s="22" r="C14"/>
+      <c s="22" r="D14"/>
+      <c s="22" r="E14"/>
+      <c s="22" r="F14"/>
     </row>
     <row r="15">
-      <c s="23" r="A15"/>
-      <c s="23" r="B15"/>
-      <c s="23" r="C15"/>
-      <c s="23" r="D15"/>
-      <c s="23" r="E15"/>
-      <c s="23" r="F15"/>
+      <c s="22" r="A15"/>
+      <c s="22" r="B15"/>
+      <c s="22" r="C15"/>
+      <c s="22" r="D15"/>
+      <c s="22" r="E15"/>
+      <c s="22" r="F15"/>
     </row>
     <row r="16">
-      <c s="23" r="A16"/>
-      <c s="23" r="B16"/>
-      <c s="23" r="C16"/>
-      <c s="23" r="D16"/>
-      <c s="23" r="E16"/>
-      <c s="23" r="F16"/>
+      <c s="22" r="A16"/>
+      <c s="22" r="B16"/>
+      <c s="22" r="C16"/>
+      <c s="22" r="D16"/>
+      <c s="22" r="E16"/>
+      <c s="22" r="F16"/>
     </row>
     <row r="17">
-      <c s="23" r="A17"/>
-      <c s="23" r="B17"/>
-      <c s="23" r="C17"/>
-      <c s="23" r="D17"/>
-      <c s="23" r="E17"/>
-      <c s="23" r="F17"/>
+      <c s="22" r="A17"/>
+      <c s="22" r="B17"/>
+      <c s="22" r="C17"/>
+      <c s="22" r="D17"/>
+      <c s="22" r="E17"/>
+      <c s="22" r="F17"/>
     </row>
     <row r="18">
-      <c s="23" r="A18"/>
-      <c s="23" r="B18"/>
-      <c s="23" r="C18"/>
-      <c s="23" r="D18"/>
-      <c s="23" r="E18"/>
-      <c s="23" r="F18"/>
+      <c s="22" r="A18"/>
+      <c s="22" r="B18"/>
+      <c s="22" r="C18"/>
+      <c s="22" r="D18"/>
+      <c s="22" r="E18"/>
+      <c s="22" r="F18"/>
     </row>
     <row r="19">
-      <c s="23" r="A19"/>
-      <c s="23" r="B19"/>
-      <c s="23" r="C19"/>
-      <c s="23" r="D19"/>
-      <c s="23" r="E19"/>
-      <c s="23" r="F19"/>
+      <c s="22" r="A19"/>
+      <c s="22" r="B19"/>
+      <c s="22" r="C19"/>
+      <c s="22" r="D19"/>
+      <c s="22" r="E19"/>
+      <c s="22" r="F19"/>
     </row>
     <row r="20">
-      <c s="23" r="A20"/>
-      <c s="23" r="B20"/>
-      <c s="23" r="C20"/>
-      <c s="23" r="D20"/>
-      <c s="23" r="E20"/>
-      <c s="23" r="F20"/>
+      <c s="22" r="A20"/>
+      <c s="22" r="B20"/>
+      <c s="22" r="C20"/>
+      <c s="22" r="D20"/>
+      <c s="22" r="E20"/>
+      <c s="22" r="F20"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
EWD-22499 - Tooltip in IE
Former-commit-id: 3fc4c36c0a8c4380bef2b7e1514329349d742b3f
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="549">
   <si>
     <t>Page</t>
   </si>
@@ -732,18 +732,6 @@
     <t>Antwortoptionen</t>
   </si>
   <si>
-    <t>explanations</t>
-  </si>
-  <si>
-    <t>Explanations</t>
-  </si>
-  <si>
-    <t>Uitleg</t>
-  </si>
-  <si>
-    <t>Erläuterungen</t>
-  </si>
-  <si>
     <t>questionProperties</t>
   </si>
   <si>
@@ -754,18 +742,6 @@
   </si>
   <si>
     <t>Frageneigenschaften</t>
-  </si>
-  <si>
-    <t>clickToAddNewExplanation</t>
-  </si>
-  <si>
-    <t>Click here to add explanation</t>
-  </si>
-  <si>
-    <t>Klik hier als u uitleg wilt toevoegen</t>
-  </si>
-  <si>
-    <t>Hier klicken, um Erläuterung hinzuzufügen</t>
   </si>
   <si>
     <t>clickToAddNewAnswerOption</t>
@@ -3132,67 +3108,67 @@
     </row>
     <row r="77">
       <c s="6" r="A77"/>
-      <c t="s" s="3" r="B77">
+      <c t="s" s="18" r="B77">
         <v>251</v>
       </c>
-      <c t="s" s="3" r="C77">
+      <c t="s" s="18" r="C77">
         <v>252</v>
       </c>
-      <c t="s" s="3" r="D77">
-        <v>253</v>
-      </c>
-      <c t="s" s="3" r="E77">
-        <v>254</v>
-      </c>
+      <c s="18" r="D77"/>
+      <c s="18" r="E77"/>
     </row>
     <row r="78">
       <c s="6" r="A78"/>
-      <c t="s" s="3" r="B78">
-        <v>255</v>
-      </c>
-      <c t="s" s="3" r="C78">
-        <v>256</v>
-      </c>
-      <c t="s" s="3" r="D78">
-        <v>257</v>
-      </c>
-      <c t="s" s="3" r="E78">
-        <v>258</v>
-      </c>
+      <c t="s" s="18" r="B78">
+        <v>253</v>
+      </c>
+      <c t="s" s="18" r="C78">
+        <v>254</v>
+      </c>
+      <c s="18" r="D78"/>
+      <c s="18" r="E78"/>
     </row>
     <row r="79">
       <c s="6" r="A79"/>
-      <c t="s" s="18" r="B79">
+      <c s="6" r="B79"/>
+      <c s="6" r="C79"/>
+      <c s="6" r="D79"/>
+      <c s="6" r="E79"/>
+    </row>
+    <row r="80">
+      <c t="s" s="6" r="A80">
+        <v>255</v>
+      </c>
+      <c t="s" s="3" r="B80">
+        <v>256</v>
+      </c>
+      <c t="s" s="3" r="C80">
+        <v>257</v>
+      </c>
+      <c t="s" s="3" r="D80">
+        <v>258</v>
+      </c>
+      <c t="s" s="3" r="E80">
         <v>259</v>
       </c>
-      <c t="s" s="18" r="C79">
-        <v>260</v>
-      </c>
-      <c s="18" r="D79"/>
-      <c s="18" r="E79"/>
-    </row>
-    <row r="80">
-      <c s="6" r="A80"/>
-      <c t="s" s="18" r="B80">
-        <v>261</v>
-      </c>
-      <c t="s" s="18" r="C80">
-        <v>262</v>
-      </c>
-      <c s="18" r="D80"/>
-      <c s="18" r="E80"/>
     </row>
     <row r="81">
       <c s="6" r="A81"/>
-      <c s="6" r="B81"/>
-      <c s="6" r="C81"/>
-      <c s="6" r="D81"/>
-      <c s="6" r="E81"/>
+      <c t="s" s="3" r="B81">
+        <v>260</v>
+      </c>
+      <c t="s" s="3" r="C81">
+        <v>261</v>
+      </c>
+      <c t="s" s="3" r="D81">
+        <v>262</v>
+      </c>
+      <c t="s" s="3" r="E81">
+        <v>263</v>
+      </c>
     </row>
     <row r="82">
-      <c t="s" s="6" r="A82">
-        <v>263</v>
-      </c>
+      <c s="5" r="A82"/>
       <c t="s" s="3" r="B82">
         <v>264</v>
       </c>
@@ -3207,7 +3183,7 @@
       </c>
     </row>
     <row r="83">
-      <c s="6" r="A83"/>
+      <c s="5" r="A83"/>
       <c t="s" s="3" r="B83">
         <v>268</v>
       </c>
@@ -3373,45 +3349,45 @@
     </row>
     <row r="94">
       <c s="5" r="A94"/>
-      <c t="s" s="3" r="B94">
+      <c s="6" r="B94"/>
+      <c s="6" r="C94"/>
+      <c s="6" r="D94"/>
+      <c s="6" r="E94"/>
+    </row>
+    <row r="95">
+      <c t="s" s="5" r="A95">
         <v>312</v>
       </c>
-      <c t="s" s="3" r="C94">
+      <c t="s" s="3" r="B95">
         <v>313</v>
       </c>
-      <c t="s" s="3" r="D94">
+      <c t="s" s="3" r="C95">
         <v>314</v>
       </c>
-      <c t="s" s="3" r="E94">
+      <c t="s" s="3" r="D95">
         <v>315</v>
       </c>
-    </row>
-    <row r="95">
-      <c s="5" r="A95"/>
-      <c t="s" s="3" r="B95">
+      <c t="s" s="3" r="E95">
         <v>316</v>
-      </c>
-      <c t="s" s="3" r="C95">
-        <v>317</v>
-      </c>
-      <c t="s" s="3" r="D95">
-        <v>318</v>
-      </c>
-      <c t="s" s="3" r="E95">
-        <v>319</v>
       </c>
     </row>
     <row r="96">
       <c s="5" r="A96"/>
-      <c s="6" r="B96"/>
-      <c s="6" r="C96"/>
-      <c s="6" r="D96"/>
-      <c s="6" r="E96"/>
+      <c t="s" s="3" r="B96">
+        <v>317</v>
+      </c>
+      <c t="s" s="3" r="C96">
+        <v>318</v>
+      </c>
+      <c t="s" s="3" r="D96">
+        <v>319</v>
+      </c>
+      <c t="s" s="3" r="E96">
+        <v>320</v>
+      </c>
     </row>
     <row r="97">
-      <c t="s" s="5" r="A97">
-        <v>320</v>
-      </c>
+      <c s="5" r="A97"/>
       <c t="s" s="3" r="B97">
         <v>321</v>
       </c>
@@ -3467,37 +3443,37 @@
         <v>335</v>
       </c>
       <c t="s" s="3" r="E100">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="101">
       <c s="5" r="A101"/>
       <c t="s" s="3" r="B101">
+        <v>336</v>
+      </c>
+      <c t="s" s="3" r="C101">
         <v>337</v>
       </c>
-      <c t="s" s="3" r="C101">
+      <c t="s" s="3" r="D101">
         <v>338</v>
       </c>
-      <c t="s" s="3" r="D101">
+      <c t="s" s="3" r="E101">
         <v>339</v>
-      </c>
-      <c t="s" s="3" r="E101">
-        <v>340</v>
       </c>
     </row>
     <row r="102">
       <c s="5" r="A102"/>
       <c t="s" s="3" r="B102">
+        <v>340</v>
+      </c>
+      <c t="s" s="3" r="C102">
         <v>341</v>
       </c>
-      <c t="s" s="3" r="C102">
+      <c t="s" s="3" r="D102">
         <v>342</v>
       </c>
-      <c t="s" s="3" r="D102">
+      <c t="s" s="3" r="E102">
         <v>343</v>
-      </c>
-      <c t="s" s="3" r="E102">
-        <v>342</v>
       </c>
     </row>
     <row r="103">
@@ -3554,82 +3530,82 @@
         <v>357</v>
       </c>
       <c t="s" s="3" r="D106">
+        <v>357</v>
+      </c>
+      <c t="s" s="3" r="E106">
         <v>358</v>
-      </c>
-      <c t="s" s="3" r="E106">
-        <v>359</v>
       </c>
     </row>
     <row r="107">
       <c s="5" r="A107"/>
       <c t="s" s="3" r="B107">
+        <v>359</v>
+      </c>
+      <c t="s" s="3" r="C107">
         <v>360</v>
       </c>
-      <c t="s" s="3" r="C107">
+      <c t="s" s="3" r="D107">
+        <v>360</v>
+      </c>
+      <c t="s" s="3" r="E107">
         <v>361</v>
-      </c>
-      <c t="s" s="3" r="D107">
-        <v>362</v>
-      </c>
-      <c t="s" s="3" r="E107">
-        <v>363</v>
       </c>
     </row>
     <row r="108">
       <c s="5" r="A108"/>
       <c t="s" s="3" r="B108">
+        <v>362</v>
+      </c>
+      <c t="s" s="3" r="C108">
+        <v>363</v>
+      </c>
+      <c t="s" s="3" r="D108">
         <v>364</v>
       </c>
-      <c t="s" s="3" r="C108">
+      <c t="s" s="3" r="E108">
         <v>365</v>
-      </c>
-      <c t="s" s="3" r="D108">
-        <v>365</v>
-      </c>
-      <c t="s" s="3" r="E108">
-        <v>366</v>
       </c>
     </row>
     <row r="109">
       <c s="5" r="A109"/>
-      <c t="s" s="3" r="B109">
+      <c t="s" s="8" r="B109">
+        <v>366</v>
+      </c>
+      <c t="s" s="3" r="C109">
         <v>367</v>
-      </c>
-      <c t="s" s="3" r="C109">
-        <v>368</v>
       </c>
       <c t="s" s="3" r="D109">
         <v>368</v>
       </c>
       <c t="s" s="3" r="E109">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="110">
       <c s="5" r="A110"/>
       <c t="s" s="3" r="B110">
+        <v>369</v>
+      </c>
+      <c t="s" s="3" r="C110">
         <v>370</v>
       </c>
-      <c t="s" s="3" r="C110">
+      <c t="s" s="3" r="D110">
         <v>371</v>
       </c>
-      <c t="s" s="3" r="D110">
+      <c t="s" s="3" r="E110">
         <v>372</v>
-      </c>
-      <c t="s" s="3" r="E110">
-        <v>373</v>
       </c>
     </row>
     <row r="111">
       <c s="5" r="A111"/>
-      <c t="s" s="8" r="B111">
+      <c t="s" s="3" r="B111">
+        <v>373</v>
+      </c>
+      <c t="s" s="3" r="C111">
         <v>374</v>
       </c>
-      <c t="s" s="3" r="C111">
+      <c t="s" s="3" r="D111">
         <v>375</v>
-      </c>
-      <c t="s" s="3" r="D111">
-        <v>376</v>
       </c>
       <c t="s" s="3" r="E111">
         <v>376</v>
@@ -3835,7 +3811,7 @@
       <c t="s" s="3" r="B125">
         <v>429</v>
       </c>
-      <c t="s" s="3" r="C125">
+      <c t="s" s="8" r="C125">
         <v>430</v>
       </c>
       <c t="s" s="3" r="D125">
@@ -3847,10 +3823,10 @@
     </row>
     <row r="126">
       <c s="5" r="A126"/>
-      <c t="s" s="3" r="B126">
+      <c t="s" s="8" r="B126">
         <v>433</v>
       </c>
-      <c t="s" s="3" r="C126">
+      <c t="s" s="8" r="C126">
         <v>434</v>
       </c>
       <c t="s" s="3" r="D126">
@@ -3866,43 +3842,43 @@
         <v>437</v>
       </c>
       <c t="s" s="8" r="C127">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c t="s" s="3" r="D127">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c t="s" s="3" r="E127">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="128">
       <c s="5" r="A128"/>
-      <c t="s" s="8" r="B128">
+      <c t="s" s="3" r="B128">
+        <v>438</v>
+      </c>
+      <c t="s" s="1" r="C128">
+        <v>439</v>
+      </c>
+      <c t="s" s="3" r="D128">
+        <v>440</v>
+      </c>
+      <c t="s" s="3" r="E128">
         <v>441</v>
-      </c>
-      <c t="s" s="8" r="C128">
-        <v>442</v>
-      </c>
-      <c t="s" s="3" r="D128">
-        <v>443</v>
-      </c>
-      <c t="s" s="3" r="E128">
-        <v>444</v>
       </c>
     </row>
     <row r="129">
       <c s="5" r="A129"/>
       <c t="s" s="3" r="B129">
+        <v>442</v>
+      </c>
+      <c t="s" s="1" r="C129">
+        <v>443</v>
+      </c>
+      <c t="s" s="3" r="D129">
+        <v>444</v>
+      </c>
+      <c t="s" s="3" r="E129">
         <v>445</v>
-      </c>
-      <c t="s" s="8" r="C129">
-        <v>442</v>
-      </c>
-      <c t="s" s="3" r="D129">
-        <v>443</v>
-      </c>
-      <c t="s" s="3" r="E129">
-        <v>444</v>
       </c>
     </row>
     <row r="130">
@@ -3916,51 +3892,51 @@
       <c t="s" s="3" r="D130">
         <v>448</v>
       </c>
-      <c t="s" s="3" r="E130">
+      <c t="s" s="1" r="E130">
         <v>449</v>
       </c>
     </row>
     <row r="131">
       <c s="5" r="A131"/>
-      <c t="s" s="3" r="B131">
+      <c s="11" r="B131"/>
+      <c s="4" r="C131"/>
+      <c s="11" r="D131"/>
+      <c s="11" r="E131"/>
+    </row>
+    <row r="132">
+      <c t="s" s="5" r="A132">
         <v>450</v>
       </c>
-      <c t="s" s="1" r="C131">
+      <c t="s" s="3" r="B132">
         <v>451</v>
       </c>
-      <c t="s" s="3" r="D131">
+      <c t="s" s="8" r="C132">
         <v>452</v>
       </c>
-      <c t="s" s="3" r="E131">
+      <c t="s" s="3" r="D132">
         <v>453</v>
       </c>
-    </row>
-    <row r="132">
-      <c s="5" r="A132"/>
-      <c t="s" s="3" r="B132">
+      <c t="s" s="3" r="E132">
         <v>454</v>
-      </c>
-      <c t="s" s="1" r="C132">
-        <v>455</v>
-      </c>
-      <c t="s" s="3" r="D132">
-        <v>456</v>
-      </c>
-      <c t="s" s="1" r="E132">
-        <v>457</v>
       </c>
     </row>
     <row r="133">
       <c s="5" r="A133"/>
-      <c s="11" r="B133"/>
-      <c s="4" r="C133"/>
-      <c s="11" r="D133"/>
-      <c s="11" r="E133"/>
+      <c t="s" s="3" r="B133">
+        <v>455</v>
+      </c>
+      <c t="s" s="8" r="C133">
+        <v>456</v>
+      </c>
+      <c t="s" s="3" r="D133">
+        <v>457</v>
+      </c>
+      <c t="s" s="3" r="E133">
+        <v>458</v>
+      </c>
     </row>
     <row r="134">
-      <c t="s" s="5" r="A134">
-        <v>458</v>
-      </c>
+      <c s="7" r="A134"/>
       <c t="s" s="3" r="B134">
         <v>459</v>
       </c>
@@ -3976,21 +3952,21 @@
     </row>
     <row r="135">
       <c s="5" r="A135"/>
-      <c t="s" s="3" r="B135">
+      <c t="s" s="15" r="B135">
         <v>463</v>
       </c>
       <c t="s" s="8" r="C135">
         <v>464</v>
       </c>
-      <c t="s" s="3" r="D135">
+      <c t="s" s="15" r="D135">
         <v>465</v>
       </c>
-      <c t="s" s="3" r="E135">
+      <c t="s" s="15" r="E135">
         <v>466</v>
       </c>
     </row>
     <row r="136">
-      <c s="7" r="A136"/>
+      <c s="5" r="A136"/>
       <c t="s" s="3" r="B136">
         <v>467</v>
       </c>
@@ -4006,16 +3982,16 @@
     </row>
     <row r="137">
       <c s="5" r="A137"/>
-      <c t="s" s="15" r="B137">
+      <c t="s" s="3" r="B137">
         <v>471</v>
       </c>
       <c t="s" s="8" r="C137">
         <v>472</v>
       </c>
-      <c t="s" s="15" r="D137">
+      <c t="s" s="3" r="D137">
         <v>473</v>
       </c>
-      <c t="s" s="15" r="E137">
+      <c t="s" s="3" r="E137">
         <v>474</v>
       </c>
     </row>
@@ -4125,7 +4101,7 @@
       </c>
     </row>
     <row r="145">
-      <c s="5" r="A145"/>
+      <c s="12" r="A145"/>
       <c t="s" s="3" r="B145">
         <v>503</v>
       </c>
@@ -4141,41 +4117,33 @@
     </row>
     <row r="146">
       <c s="5" r="A146"/>
-      <c t="s" s="3" r="B146">
+      <c t="s" s="18" r="B146">
         <v>507</v>
       </c>
-      <c t="s" s="8" r="C146">
+      <c t="s" s="17" r="C146">
         <v>508</v>
       </c>
-      <c t="s" s="3" r="D146">
+      <c s="18" r="D146"/>
+      <c s="18" r="E146"/>
+    </row>
+    <row r="147">
+      <c s="5" r="A147"/>
+      <c t="s" s="18" r="B147">
         <v>509</v>
       </c>
-      <c t="s" s="3" r="E146">
+      <c t="s" s="17" r="C147">
         <v>510</v>
       </c>
-    </row>
-    <row r="147">
-      <c s="12" r="A147"/>
-      <c t="s" s="3" r="B147">
-        <v>511</v>
-      </c>
-      <c t="s" s="8" r="C147">
-        <v>512</v>
-      </c>
-      <c t="s" s="3" r="D147">
-        <v>513</v>
-      </c>
-      <c t="s" s="3" r="E147">
-        <v>514</v>
-      </c>
+      <c s="18" r="D147"/>
+      <c s="18" r="E147"/>
     </row>
     <row r="148">
       <c s="5" r="A148"/>
       <c t="s" s="18" r="B148">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c t="s" s="17" r="C148">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c s="18" r="D148"/>
       <c s="18" r="E148"/>
@@ -4183,10 +4151,10 @@
     <row r="149">
       <c s="5" r="A149"/>
       <c t="s" s="18" r="B149">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c t="s" s="17" r="C149">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c s="18" r="D149"/>
       <c s="18" r="E149"/>
@@ -4194,10 +4162,10 @@
     <row r="150">
       <c s="5" r="A150"/>
       <c t="s" s="18" r="B150">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c t="s" s="17" r="C150">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c s="18" r="D150"/>
       <c s="18" r="E150"/>
@@ -4205,10 +4173,10 @@
     <row r="151">
       <c s="5" r="A151"/>
       <c t="s" s="18" r="B151">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c t="s" s="17" r="C151">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c s="18" r="D151"/>
       <c s="18" r="E151"/>
@@ -4216,47 +4184,55 @@
     <row r="152">
       <c s="5" r="A152"/>
       <c t="s" s="18" r="B152">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c t="s" s="17" r="C152">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c s="18" r="D152"/>
       <c s="18" r="E152"/>
     </row>
     <row r="153">
       <c s="5" r="A153"/>
-      <c t="s" s="18" r="B153">
+      <c s="6" r="B153"/>
+      <c s="10" r="C153"/>
+      <c s="6" r="D153"/>
+      <c s="6" r="E153"/>
+    </row>
+    <row r="154">
+      <c t="s" s="5" r="A154">
+        <v>521</v>
+      </c>
+      <c t="s" s="3" r="B154">
+        <v>522</v>
+      </c>
+      <c t="s" s="8" r="C154">
+        <v>523</v>
+      </c>
+      <c t="s" s="3" r="D154">
+        <v>524</v>
+      </c>
+      <c t="s" s="3" r="E154">
         <v>525</v>
       </c>
-      <c t="s" s="17" r="C153">
-        <v>526</v>
-      </c>
-      <c s="18" r="D153"/>
-      <c s="18" r="E153"/>
-    </row>
-    <row r="154">
-      <c s="5" r="A154"/>
-      <c t="s" s="18" r="B154">
-        <v>527</v>
-      </c>
-      <c t="s" s="17" r="C154">
-        <v>528</v>
-      </c>
-      <c s="18" r="D154"/>
-      <c s="18" r="E154"/>
     </row>
     <row r="155">
       <c s="5" r="A155"/>
-      <c s="6" r="B155"/>
-      <c s="10" r="C155"/>
-      <c s="6" r="D155"/>
-      <c s="6" r="E155"/>
+      <c t="s" s="3" r="B155">
+        <v>526</v>
+      </c>
+      <c t="s" s="8" r="C155">
+        <v>527</v>
+      </c>
+      <c t="s" s="3" r="D155">
+        <v>528</v>
+      </c>
+      <c t="s" s="3" r="E155">
+        <v>529</v>
+      </c>
     </row>
     <row r="156">
-      <c t="s" s="5" r="A156">
-        <v>529</v>
-      </c>
+      <c s="5" r="A156"/>
       <c t="s" s="3" r="B156">
         <v>530</v>
       </c>
@@ -4302,84 +4278,68 @@
     </row>
     <row r="159">
       <c s="5" r="A159"/>
-      <c t="s" s="3" r="B159">
+      <c s="13" r="B159"/>
+      <c s="21" r="C159"/>
+      <c s="13" r="D159"/>
+      <c s="13" r="E159"/>
+    </row>
+    <row r="160">
+      <c t="s" s="5" r="A160">
         <v>542</v>
       </c>
-      <c t="s" s="8" r="C159">
+      <c t="s" s="22" r="B160">
         <v>543</v>
       </c>
-      <c t="s" s="3" r="D159">
-        <v>544</v>
-      </c>
-      <c t="s" s="3" r="E159">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="160">
-      <c s="5" r="A160"/>
-      <c t="s" s="3" r="B160">
-        <v>546</v>
-      </c>
-      <c t="s" s="8" r="C160">
-        <v>547</v>
-      </c>
-      <c t="s" s="3" r="D160">
-        <v>548</v>
-      </c>
-      <c t="s" s="3" r="E160">
-        <v>549</v>
-      </c>
+      <c t="s" s="14" r="C160">
+        <v>542</v>
+      </c>
+      <c s="22" r="D160"/>
+      <c s="22" r="E160"/>
     </row>
     <row r="161">
       <c s="5" r="A161"/>
-      <c s="13" r="B161"/>
-      <c s="21" r="C161"/>
-      <c s="13" r="D161"/>
-      <c s="13" r="E161"/>
+      <c s="11" r="B161"/>
+      <c s="4" r="C161"/>
+      <c s="11" r="D161"/>
+      <c s="11" r="E161"/>
     </row>
     <row r="162">
       <c t="s" s="5" r="A162">
-        <v>550</v>
-      </c>
-      <c t="s" s="22" r="B162">
-        <v>551</v>
-      </c>
-      <c t="s" s="14" r="C162">
-        <v>550</v>
-      </c>
-      <c s="22" r="D162"/>
-      <c s="22" r="E162"/>
+        <v>544</v>
+      </c>
+      <c t="s" s="25" r="B162">
+        <v>545</v>
+      </c>
+      <c t="s" s="23" r="C162">
+        <v>546</v>
+      </c>
+      <c s="25" r="D162"/>
+      <c s="25" r="E162"/>
     </row>
     <row r="163">
       <c s="5" r="A163"/>
-      <c s="11" r="B163"/>
-      <c s="4" r="C163"/>
-      <c s="11" r="D163"/>
-      <c s="11" r="E163"/>
+      <c t="s" s="25" r="B163">
+        <v>547</v>
+      </c>
+      <c t="s" s="23" r="C163">
+        <v>548</v>
+      </c>
+      <c s="25" r="D163"/>
+      <c s="25" r="E163"/>
     </row>
     <row r="164">
-      <c t="s" s="5" r="A164">
-        <v>552</v>
-      </c>
-      <c t="s" s="25" r="B164">
-        <v>553</v>
-      </c>
-      <c t="s" s="23" r="C164">
-        <v>554</v>
-      </c>
-      <c s="25" r="D164"/>
-      <c s="25" r="E164"/>
+      <c s="5" r="A164"/>
+      <c s="11" r="B164"/>
+      <c s="4" r="C164"/>
+      <c s="11" r="D164"/>
+      <c s="11" r="E164"/>
     </row>
     <row r="165">
       <c s="5" r="A165"/>
-      <c t="s" s="25" r="B165">
-        <v>555</v>
-      </c>
-      <c t="s" s="23" r="C165">
-        <v>556</v>
-      </c>
-      <c s="25" r="D165"/>
-      <c s="25" r="E165"/>
+      <c s="11" r="B165"/>
+      <c s="4" r="C165"/>
+      <c s="11" r="D165"/>
+      <c s="11" r="E165"/>
     </row>
     <row r="166">
       <c s="5" r="A166"/>
@@ -4387,20 +4347,6 @@
       <c s="4" r="C166"/>
       <c s="11" r="D166"/>
       <c s="11" r="E166"/>
-    </row>
-    <row r="167">
-      <c s="5" r="A167"/>
-      <c s="11" r="B167"/>
-      <c s="4" r="C167"/>
-      <c s="11" r="D167"/>
-      <c s="11" r="E167"/>
-    </row>
-    <row r="168">
-      <c s="5" r="A168"/>
-      <c s="11" r="B168"/>
-      <c s="4" r="C168"/>
-      <c s="11" r="D168"/>
-      <c s="11" r="E168"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
EWD-22511 - Explanation -> Learning object
Former-commit-id: e4dea27797a497de4135c29cad59fbe34844e591
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -828,10 +828,10 @@
     <t>Learning objects</t>
   </si>
   <si>
-    <t>Leerstof</t>
-  </si>
-  <si>
-    <t>Lerngegenstand</t>
+    <t>Leerobject</t>
+  </si>
+  <si>
+    <t>Lernobjekt</t>
   </si>
   <si>
     <t>clickToAddLearningObject</t>
@@ -840,10 +840,10 @@
     <t>Click here to add learning object</t>
   </si>
   <si>
-    <t>Klik hier om leerstof toe te voegen</t>
-  </si>
-  <si>
-    <t>Klicken Sie hier, um einen Lerngegenstand hinzuzufügen</t>
+    <t>Klik hier om een leerobject toe te voegen</t>
+  </si>
+  <si>
+    <t>Klicken Sie hier, um ein Lernobjekt hinzuzufügen</t>
   </si>
   <si>
     <t>Questions</t>
@@ -1772,7 +1772,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -1935,17 +1935,8 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
-  <fills count="19">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2040,12 +2031,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2069,7 +2054,7 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
@@ -2128,14 +2113,11 @@
     <xf applyAlignment="1" fillId="15" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="15" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="16" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="16" applyFill="1">
+    <xf applyAlignment="1" fillId="16" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="17" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
-      <alignment vertical="center" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="17"/>
-    <xf applyAlignment="1" fillId="18" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="18" applyFill="1">
+    <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="16"/>
+    <xf applyAlignment="1" fillId="17" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="17" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3243,7 +3225,7 @@
       <c t="s" s="7" r="C77">
         <v>270</v>
       </c>
-      <c t="s" s="20" r="D77">
+      <c t="s" s="7" r="D77">
         <v>271</v>
       </c>
       <c t="s" s="7" r="E77">
@@ -3258,7 +3240,7 @@
       <c t="s" s="7" r="C78">
         <v>274</v>
       </c>
-      <c t="s" s="20" r="D78">
+      <c t="s" s="7" r="D78">
         <v>275</v>
       </c>
       <c t="s" s="7" r="E78">
@@ -4472,25 +4454,25 @@
       <c t="s" s="10" r="A162">
         <v>579</v>
       </c>
-      <c t="s" s="23" r="B162">
+      <c t="s" s="22" r="B162">
         <v>580</v>
       </c>
-      <c t="s" s="21" r="C162">
+      <c t="s" s="20" r="C162">
         <v>581</v>
       </c>
-      <c s="23" r="D162"/>
-      <c s="23" r="E162"/>
+      <c s="22" r="D162"/>
+      <c s="22" r="E162"/>
     </row>
     <row r="163">
       <c s="10" r="A163"/>
-      <c t="s" s="23" r="B163">
+      <c t="s" s="22" r="B163">
         <v>582</v>
       </c>
-      <c t="s" s="21" r="C163">
+      <c t="s" s="20" r="C163">
         <v>583</v>
       </c>
-      <c s="23" r="D163"/>
-      <c s="23" r="E163"/>
+      <c s="22" r="D163"/>
+      <c s="22" r="E163"/>
     </row>
     <row r="164">
       <c s="10" r="A164"/>
@@ -4525,164 +4507,164 @@
   <sheetFormatPr customHeight="1" defaultColWidth="9.86" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c s="22" r="A1"/>
-      <c s="22" r="B1"/>
-      <c s="22" r="C1"/>
-      <c s="22" r="D1"/>
-      <c s="22" r="E1"/>
-      <c s="22" r="F1"/>
+      <c s="21" r="A1"/>
+      <c s="21" r="B1"/>
+      <c s="21" r="C1"/>
+      <c s="21" r="D1"/>
+      <c s="21" r="E1"/>
+      <c s="21" r="F1"/>
     </row>
     <row r="2">
-      <c s="22" r="A2"/>
-      <c s="22" r="B2"/>
-      <c s="22" r="C2"/>
-      <c s="22" r="D2"/>
-      <c s="22" r="E2"/>
-      <c s="22" r="F2"/>
+      <c s="21" r="A2"/>
+      <c s="21" r="B2"/>
+      <c s="21" r="C2"/>
+      <c s="21" r="D2"/>
+      <c s="21" r="E2"/>
+      <c s="21" r="F2"/>
     </row>
     <row r="3">
-      <c s="22" r="A3"/>
-      <c s="22" r="B3"/>
-      <c s="22" r="C3"/>
-      <c s="22" r="D3"/>
-      <c s="22" r="E3"/>
-      <c s="22" r="F3"/>
+      <c s="21" r="A3"/>
+      <c s="21" r="B3"/>
+      <c s="21" r="C3"/>
+      <c s="21" r="D3"/>
+      <c s="21" r="E3"/>
+      <c s="21" r="F3"/>
     </row>
     <row r="4">
-      <c s="22" r="A4"/>
-      <c s="22" r="B4"/>
-      <c s="22" r="C4"/>
-      <c s="22" r="D4"/>
-      <c s="22" r="E4"/>
-      <c s="22" r="F4"/>
+      <c s="21" r="A4"/>
+      <c s="21" r="B4"/>
+      <c s="21" r="C4"/>
+      <c s="21" r="D4"/>
+      <c s="21" r="E4"/>
+      <c s="21" r="F4"/>
     </row>
     <row r="5">
-      <c s="22" r="A5"/>
-      <c s="22" r="B5"/>
-      <c s="22" r="C5"/>
-      <c s="22" r="D5"/>
-      <c s="22" r="E5"/>
-      <c s="22" r="F5"/>
+      <c s="21" r="A5"/>
+      <c s="21" r="B5"/>
+      <c s="21" r="C5"/>
+      <c s="21" r="D5"/>
+      <c s="21" r="E5"/>
+      <c s="21" r="F5"/>
     </row>
     <row r="6">
-      <c s="22" r="A6"/>
-      <c s="22" r="B6"/>
-      <c s="22" r="C6"/>
-      <c s="22" r="D6"/>
-      <c s="22" r="E6"/>
-      <c s="22" r="F6"/>
+      <c s="21" r="A6"/>
+      <c s="21" r="B6"/>
+      <c s="21" r="C6"/>
+      <c s="21" r="D6"/>
+      <c s="21" r="E6"/>
+      <c s="21" r="F6"/>
     </row>
     <row r="7">
-      <c s="22" r="A7"/>
-      <c s="22" r="B7"/>
-      <c s="22" r="C7"/>
-      <c s="22" r="D7"/>
-      <c s="22" r="E7"/>
-      <c s="22" r="F7"/>
+      <c s="21" r="A7"/>
+      <c s="21" r="B7"/>
+      <c s="21" r="C7"/>
+      <c s="21" r="D7"/>
+      <c s="21" r="E7"/>
+      <c s="21" r="F7"/>
     </row>
     <row r="8">
-      <c s="22" r="A8"/>
-      <c s="22" r="B8"/>
-      <c s="22" r="C8"/>
-      <c s="22" r="D8"/>
-      <c s="22" r="E8"/>
-      <c s="22" r="F8"/>
+      <c s="21" r="A8"/>
+      <c s="21" r="B8"/>
+      <c s="21" r="C8"/>
+      <c s="21" r="D8"/>
+      <c s="21" r="E8"/>
+      <c s="21" r="F8"/>
     </row>
     <row r="9">
-      <c s="22" r="A9"/>
-      <c s="22" r="B9"/>
-      <c s="22" r="C9"/>
-      <c s="22" r="D9"/>
-      <c s="22" r="E9"/>
-      <c s="22" r="F9"/>
+      <c s="21" r="A9"/>
+      <c s="21" r="B9"/>
+      <c s="21" r="C9"/>
+      <c s="21" r="D9"/>
+      <c s="21" r="E9"/>
+      <c s="21" r="F9"/>
     </row>
     <row r="10">
-      <c s="22" r="A10"/>
-      <c s="22" r="B10"/>
-      <c s="22" r="C10"/>
-      <c s="22" r="D10"/>
-      <c s="22" r="E10"/>
-      <c s="22" r="F10"/>
+      <c s="21" r="A10"/>
+      <c s="21" r="B10"/>
+      <c s="21" r="C10"/>
+      <c s="21" r="D10"/>
+      <c s="21" r="E10"/>
+      <c s="21" r="F10"/>
     </row>
     <row r="11">
-      <c s="22" r="A11"/>
-      <c s="22" r="B11"/>
-      <c s="22" r="C11"/>
-      <c s="22" r="D11"/>
-      <c s="22" r="E11"/>
-      <c s="22" r="F11"/>
+      <c s="21" r="A11"/>
+      <c s="21" r="B11"/>
+      <c s="21" r="C11"/>
+      <c s="21" r="D11"/>
+      <c s="21" r="E11"/>
+      <c s="21" r="F11"/>
     </row>
     <row r="12">
-      <c s="22" r="A12"/>
-      <c s="22" r="B12"/>
-      <c s="22" r="C12"/>
-      <c s="22" r="D12"/>
-      <c s="22" r="E12"/>
-      <c s="22" r="F12"/>
+      <c s="21" r="A12"/>
+      <c s="21" r="B12"/>
+      <c s="21" r="C12"/>
+      <c s="21" r="D12"/>
+      <c s="21" r="E12"/>
+      <c s="21" r="F12"/>
     </row>
     <row r="13">
-      <c s="22" r="A13"/>
-      <c s="22" r="B13"/>
-      <c s="22" r="C13"/>
-      <c s="22" r="D13"/>
-      <c s="22" r="E13"/>
-      <c s="22" r="F13"/>
+      <c s="21" r="A13"/>
+      <c s="21" r="B13"/>
+      <c s="21" r="C13"/>
+      <c s="21" r="D13"/>
+      <c s="21" r="E13"/>
+      <c s="21" r="F13"/>
     </row>
     <row r="14">
-      <c s="22" r="A14"/>
-      <c s="22" r="B14"/>
-      <c s="22" r="C14"/>
-      <c s="22" r="D14"/>
-      <c s="22" r="E14"/>
-      <c s="22" r="F14"/>
+      <c s="21" r="A14"/>
+      <c s="21" r="B14"/>
+      <c s="21" r="C14"/>
+      <c s="21" r="D14"/>
+      <c s="21" r="E14"/>
+      <c s="21" r="F14"/>
     </row>
     <row r="15">
-      <c s="22" r="A15"/>
-      <c s="22" r="B15"/>
-      <c s="22" r="C15"/>
-      <c s="22" r="D15"/>
-      <c s="22" r="E15"/>
-      <c s="22" r="F15"/>
+      <c s="21" r="A15"/>
+      <c s="21" r="B15"/>
+      <c s="21" r="C15"/>
+      <c s="21" r="D15"/>
+      <c s="21" r="E15"/>
+      <c s="21" r="F15"/>
     </row>
     <row r="16">
-      <c s="22" r="A16"/>
-      <c s="22" r="B16"/>
-      <c s="22" r="C16"/>
-      <c s="22" r="D16"/>
-      <c s="22" r="E16"/>
-      <c s="22" r="F16"/>
+      <c s="21" r="A16"/>
+      <c s="21" r="B16"/>
+      <c s="21" r="C16"/>
+      <c s="21" r="D16"/>
+      <c s="21" r="E16"/>
+      <c s="21" r="F16"/>
     </row>
     <row r="17">
-      <c s="22" r="A17"/>
-      <c s="22" r="B17"/>
-      <c s="22" r="C17"/>
-      <c s="22" r="D17"/>
-      <c s="22" r="E17"/>
-      <c s="22" r="F17"/>
+      <c s="21" r="A17"/>
+      <c s="21" r="B17"/>
+      <c s="21" r="C17"/>
+      <c s="21" r="D17"/>
+      <c s="21" r="E17"/>
+      <c s="21" r="F17"/>
     </row>
     <row r="18">
-      <c s="22" r="A18"/>
-      <c s="22" r="B18"/>
-      <c s="22" r="C18"/>
-      <c s="22" r="D18"/>
-      <c s="22" r="E18"/>
-      <c s="22" r="F18"/>
+      <c s="21" r="A18"/>
+      <c s="21" r="B18"/>
+      <c s="21" r="C18"/>
+      <c s="21" r="D18"/>
+      <c s="21" r="E18"/>
+      <c s="21" r="F18"/>
     </row>
     <row r="19">
-      <c s="22" r="A19"/>
-      <c s="22" r="B19"/>
-      <c s="22" r="C19"/>
-      <c s="22" r="D19"/>
-      <c s="22" r="E19"/>
-      <c s="22" r="F19"/>
+      <c s="21" r="A19"/>
+      <c s="21" r="B19"/>
+      <c s="21" r="C19"/>
+      <c s="21" r="D19"/>
+      <c s="21" r="E19"/>
+      <c s="21" r="F19"/>
     </row>
     <row r="20">
-      <c s="22" r="A20"/>
-      <c s="22" r="B20"/>
-      <c s="22" r="C20"/>
-      <c s="22" r="D20"/>
-      <c s="22" r="E20"/>
-      <c s="22" r="F20"/>
+      <c s="21" r="A20"/>
+      <c s="21" r="B20"/>
+      <c s="21" r="C20"/>
+      <c s="21" r="D20"/>
+      <c s="21" r="E20"/>
+      <c s="21" r="F20"/>
     </row>
   </sheetData>
 </worksheet>
@@ -4696,164 +4678,164 @@
   <sheetFormatPr customHeight="1" defaultColWidth="9.86" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c s="22" r="A1"/>
-      <c s="22" r="B1"/>
-      <c s="22" r="C1"/>
-      <c s="22" r="D1"/>
-      <c s="22" r="E1"/>
-      <c s="22" r="F1"/>
+      <c s="21" r="A1"/>
+      <c s="21" r="B1"/>
+      <c s="21" r="C1"/>
+      <c s="21" r="D1"/>
+      <c s="21" r="E1"/>
+      <c s="21" r="F1"/>
     </row>
     <row r="2">
-      <c s="22" r="A2"/>
-      <c s="22" r="B2"/>
-      <c s="22" r="C2"/>
-      <c s="22" r="D2"/>
-      <c s="22" r="E2"/>
-      <c s="22" r="F2"/>
+      <c s="21" r="A2"/>
+      <c s="21" r="B2"/>
+      <c s="21" r="C2"/>
+      <c s="21" r="D2"/>
+      <c s="21" r="E2"/>
+      <c s="21" r="F2"/>
     </row>
     <row r="3">
-      <c s="22" r="A3"/>
-      <c s="22" r="B3"/>
-      <c s="22" r="C3"/>
-      <c s="22" r="D3"/>
-      <c s="22" r="E3"/>
-      <c s="22" r="F3"/>
+      <c s="21" r="A3"/>
+      <c s="21" r="B3"/>
+      <c s="21" r="C3"/>
+      <c s="21" r="D3"/>
+      <c s="21" r="E3"/>
+      <c s="21" r="F3"/>
     </row>
     <row r="4">
-      <c s="22" r="A4"/>
-      <c s="22" r="B4"/>
-      <c s="22" r="C4"/>
-      <c s="22" r="D4"/>
-      <c s="22" r="E4"/>
-      <c s="22" r="F4"/>
+      <c s="21" r="A4"/>
+      <c s="21" r="B4"/>
+      <c s="21" r="C4"/>
+      <c s="21" r="D4"/>
+      <c s="21" r="E4"/>
+      <c s="21" r="F4"/>
     </row>
     <row r="5">
-      <c s="22" r="A5"/>
-      <c s="22" r="B5"/>
-      <c s="22" r="C5"/>
-      <c s="22" r="D5"/>
-      <c s="22" r="E5"/>
-      <c s="22" r="F5"/>
+      <c s="21" r="A5"/>
+      <c s="21" r="B5"/>
+      <c s="21" r="C5"/>
+      <c s="21" r="D5"/>
+      <c s="21" r="E5"/>
+      <c s="21" r="F5"/>
     </row>
     <row r="6">
-      <c s="22" r="A6"/>
-      <c s="22" r="B6"/>
-      <c s="22" r="C6"/>
-      <c s="22" r="D6"/>
-      <c s="22" r="E6"/>
-      <c s="22" r="F6"/>
+      <c s="21" r="A6"/>
+      <c s="21" r="B6"/>
+      <c s="21" r="C6"/>
+      <c s="21" r="D6"/>
+      <c s="21" r="E6"/>
+      <c s="21" r="F6"/>
     </row>
     <row r="7">
-      <c s="22" r="A7"/>
-      <c s="22" r="B7"/>
-      <c s="22" r="C7"/>
-      <c s="22" r="D7"/>
-      <c s="22" r="E7"/>
-      <c s="22" r="F7"/>
+      <c s="21" r="A7"/>
+      <c s="21" r="B7"/>
+      <c s="21" r="C7"/>
+      <c s="21" r="D7"/>
+      <c s="21" r="E7"/>
+      <c s="21" r="F7"/>
     </row>
     <row r="8">
-      <c s="22" r="A8"/>
-      <c s="22" r="B8"/>
-      <c s="22" r="C8"/>
-      <c s="22" r="D8"/>
-      <c s="22" r="E8"/>
-      <c s="22" r="F8"/>
+      <c s="21" r="A8"/>
+      <c s="21" r="B8"/>
+      <c s="21" r="C8"/>
+      <c s="21" r="D8"/>
+      <c s="21" r="E8"/>
+      <c s="21" r="F8"/>
     </row>
     <row r="9">
-      <c s="22" r="A9"/>
-      <c s="22" r="B9"/>
-      <c s="22" r="C9"/>
-      <c s="22" r="D9"/>
-      <c s="22" r="E9"/>
-      <c s="22" r="F9"/>
+      <c s="21" r="A9"/>
+      <c s="21" r="B9"/>
+      <c s="21" r="C9"/>
+      <c s="21" r="D9"/>
+      <c s="21" r="E9"/>
+      <c s="21" r="F9"/>
     </row>
     <row r="10">
-      <c s="22" r="A10"/>
-      <c s="22" r="B10"/>
-      <c s="22" r="C10"/>
-      <c s="22" r="D10"/>
-      <c s="22" r="E10"/>
-      <c s="22" r="F10"/>
+      <c s="21" r="A10"/>
+      <c s="21" r="B10"/>
+      <c s="21" r="C10"/>
+      <c s="21" r="D10"/>
+      <c s="21" r="E10"/>
+      <c s="21" r="F10"/>
     </row>
     <row r="11">
-      <c s="22" r="A11"/>
-      <c s="22" r="B11"/>
-      <c s="22" r="C11"/>
-      <c s="22" r="D11"/>
-      <c s="22" r="E11"/>
-      <c s="22" r="F11"/>
+      <c s="21" r="A11"/>
+      <c s="21" r="B11"/>
+      <c s="21" r="C11"/>
+      <c s="21" r="D11"/>
+      <c s="21" r="E11"/>
+      <c s="21" r="F11"/>
     </row>
     <row r="12">
-      <c s="22" r="A12"/>
-      <c s="22" r="B12"/>
-      <c s="22" r="C12"/>
-      <c s="22" r="D12"/>
-      <c s="22" r="E12"/>
-      <c s="22" r="F12"/>
+      <c s="21" r="A12"/>
+      <c s="21" r="B12"/>
+      <c s="21" r="C12"/>
+      <c s="21" r="D12"/>
+      <c s="21" r="E12"/>
+      <c s="21" r="F12"/>
     </row>
     <row r="13">
-      <c s="22" r="A13"/>
-      <c s="22" r="B13"/>
-      <c s="22" r="C13"/>
-      <c s="22" r="D13"/>
-      <c s="22" r="E13"/>
-      <c s="22" r="F13"/>
+      <c s="21" r="A13"/>
+      <c s="21" r="B13"/>
+      <c s="21" r="C13"/>
+      <c s="21" r="D13"/>
+      <c s="21" r="E13"/>
+      <c s="21" r="F13"/>
     </row>
     <row r="14">
-      <c s="22" r="A14"/>
-      <c s="22" r="B14"/>
-      <c s="22" r="C14"/>
-      <c s="22" r="D14"/>
-      <c s="22" r="E14"/>
-      <c s="22" r="F14"/>
+      <c s="21" r="A14"/>
+      <c s="21" r="B14"/>
+      <c s="21" r="C14"/>
+      <c s="21" r="D14"/>
+      <c s="21" r="E14"/>
+      <c s="21" r="F14"/>
     </row>
     <row r="15">
-      <c s="22" r="A15"/>
-      <c s="22" r="B15"/>
-      <c s="22" r="C15"/>
-      <c s="22" r="D15"/>
-      <c s="22" r="E15"/>
-      <c s="22" r="F15"/>
+      <c s="21" r="A15"/>
+      <c s="21" r="B15"/>
+      <c s="21" r="C15"/>
+      <c s="21" r="D15"/>
+      <c s="21" r="E15"/>
+      <c s="21" r="F15"/>
     </row>
     <row r="16">
-      <c s="22" r="A16"/>
-      <c s="22" r="B16"/>
-      <c s="22" r="C16"/>
-      <c s="22" r="D16"/>
-      <c s="22" r="E16"/>
-      <c s="22" r="F16"/>
+      <c s="21" r="A16"/>
+      <c s="21" r="B16"/>
+      <c s="21" r="C16"/>
+      <c s="21" r="D16"/>
+      <c s="21" r="E16"/>
+      <c s="21" r="F16"/>
     </row>
     <row r="17">
-      <c s="22" r="A17"/>
-      <c s="22" r="B17"/>
-      <c s="22" r="C17"/>
-      <c s="22" r="D17"/>
-      <c s="22" r="E17"/>
-      <c s="22" r="F17"/>
+      <c s="21" r="A17"/>
+      <c s="21" r="B17"/>
+      <c s="21" r="C17"/>
+      <c s="21" r="D17"/>
+      <c s="21" r="E17"/>
+      <c s="21" r="F17"/>
     </row>
     <row r="18">
-      <c s="22" r="A18"/>
-      <c s="22" r="B18"/>
-      <c s="22" r="C18"/>
-      <c s="22" r="D18"/>
-      <c s="22" r="E18"/>
-      <c s="22" r="F18"/>
+      <c s="21" r="A18"/>
+      <c s="21" r="B18"/>
+      <c s="21" r="C18"/>
+      <c s="21" r="D18"/>
+      <c s="21" r="E18"/>
+      <c s="21" r="F18"/>
     </row>
     <row r="19">
-      <c s="22" r="A19"/>
-      <c s="22" r="B19"/>
-      <c s="22" r="C19"/>
-      <c s="22" r="D19"/>
-      <c s="22" r="E19"/>
-      <c s="22" r="F19"/>
+      <c s="21" r="A19"/>
+      <c s="21" r="B19"/>
+      <c s="21" r="C19"/>
+      <c s="21" r="D19"/>
+      <c s="21" r="E19"/>
+      <c s="21" r="F19"/>
     </row>
     <row r="20">
-      <c s="22" r="A20"/>
-      <c s="22" r="B20"/>
-      <c s="22" r="C20"/>
-      <c s="22" r="D20"/>
-      <c s="22" r="E20"/>
-      <c s="22" r="F20"/>
+      <c s="21" r="A20"/>
+      <c s="21" r="B20"/>
+      <c s="21" r="C20"/>
+      <c s="21" r="D20"/>
+      <c s="21" r="E20"/>
+      <c s="21" r="F20"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
EWD-22509 - Learning experience editor
Former-commit-id: b74d18c9524ff50d64b986191f3823d3151af18f
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="588">
   <si>
     <t>Page</t>
   </si>
@@ -1682,6 +1682,18 @@
   </si>
   <si>
     <t>Ausgewählte(s) Lernziel(e) trennen</t>
+  </si>
+  <si>
+    <t>learningExperienceEditor</t>
+  </si>
+  <si>
+    <t>Learning experience editor</t>
+  </si>
+  <si>
+    <t>Editor leerervaringen</t>
+  </si>
+  <si>
+    <t>Lernerfahrungs-Editor</t>
   </si>
   <si>
     <t>Error pages</t>
@@ -1772,7 +1784,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -1935,8 +1947,17 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1954,6 +1975,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2031,6 +2058,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2054,7 +2087,7 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
@@ -2081,43 +2114,49 @@
       <alignment vertical="bottom" horizontal="right"/>
     </xf>
     <xf applyAlignment="1" fillId="7" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="8" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="8">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="8" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="9" applyFill="1">
+    <xf applyAlignment="1" fillId="9" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="9" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="10">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="9" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+    <xf applyAlignment="1" fillId="10" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="10" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="11" applyFill="1">
+    <xf applyAlignment="1" fillId="11" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="11" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="11" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="12" applyFill="1">
+    <xf applyAlignment="1" fillId="12" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="12" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="12" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+    <xf applyAlignment="1" fillId="13" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="13" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="13" applyFill="1">
+    <xf applyAlignment="1" fillId="14" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="13" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="14" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="14" applyFill="1">
+    <xf applyAlignment="1" fillId="15" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="14" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="15" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="15" applyFill="1">
+    <xf applyAlignment="1" fillId="16" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="15" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="16" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+    <xf applyAlignment="1" fillId="17" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="16" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="16"/>
-    <xf applyAlignment="1" fillId="17" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="17" applyFill="1">
+    <xf applyAlignment="1" fillId="18" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+      <alignment vertical="center" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="17"/>
+    <xf applyAlignment="1" fillId="19" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="18" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2145,16 +2184,16 @@
   </cols>
   <sheetData>
     <row s="6" customFormat="1" r="1">
-      <c t="s" s="11" r="A1">
+      <c t="s" s="12" r="A1">
         <v>0</v>
       </c>
-      <c t="s" s="11" r="B1">
+      <c t="s" s="12" r="B1">
         <v>1</v>
       </c>
-      <c t="s" s="11" r="C1">
+      <c t="s" s="12" r="C1">
         <v>2</v>
       </c>
-      <c t="s" s="11" r="D1">
+      <c t="s" s="12" r="D1">
         <v>3</v>
       </c>
       <c t="s" s="4" r="E1">
@@ -2329,7 +2368,7 @@
       </c>
     </row>
     <row r="13">
-      <c s="12" r="A13"/>
+      <c s="13" r="A13"/>
       <c t="s" s="7" r="B13">
         <v>46</v>
       </c>
@@ -2344,7 +2383,7 @@
       </c>
     </row>
     <row r="14">
-      <c s="12" r="A14"/>
+      <c s="13" r="A14"/>
       <c t="s" s="7" r="B14">
         <v>50</v>
       </c>
@@ -2359,7 +2398,7 @@
       </c>
     </row>
     <row r="15">
-      <c s="12" r="A15"/>
+      <c s="13" r="A15"/>
       <c t="s" s="7" r="B15">
         <v>54</v>
       </c>
@@ -2374,7 +2413,7 @@
       </c>
     </row>
     <row r="16">
-      <c s="12" r="A16"/>
+      <c s="13" r="A16"/>
       <c t="s" s="7" r="B16">
         <v>58</v>
       </c>
@@ -2389,7 +2428,7 @@
       </c>
     </row>
     <row r="17">
-      <c s="12" r="A17"/>
+      <c s="13" r="A17"/>
       <c t="s" s="7" r="B17">
         <v>62</v>
       </c>
@@ -2404,7 +2443,7 @@
       </c>
     </row>
     <row r="18">
-      <c s="12" r="A18"/>
+      <c s="13" r="A18"/>
       <c t="s" s="7" r="B18">
         <v>66</v>
       </c>
@@ -2419,7 +2458,7 @@
       </c>
     </row>
     <row r="19">
-      <c s="12" r="A19"/>
+      <c s="13" r="A19"/>
       <c t="s" s="7" r="B19">
         <v>70</v>
       </c>
@@ -2434,7 +2473,7 @@
       </c>
     </row>
     <row r="20">
-      <c s="12" r="A20"/>
+      <c s="13" r="A20"/>
       <c t="s" s="7" r="B20">
         <v>74</v>
       </c>
@@ -2449,7 +2488,7 @@
       </c>
     </row>
     <row r="21">
-      <c s="12" r="A21"/>
+      <c s="13" r="A21"/>
       <c t="s" s="7" r="B21">
         <v>78</v>
       </c>
@@ -2464,7 +2503,7 @@
       </c>
     </row>
     <row r="22">
-      <c s="12" r="A22"/>
+      <c s="13" r="A22"/>
       <c t="s" s="7" r="B22">
         <v>82</v>
       </c>
@@ -2479,7 +2518,7 @@
       </c>
     </row>
     <row r="23">
-      <c s="12" r="A23"/>
+      <c s="13" r="A23"/>
       <c t="s" s="7" r="B23">
         <v>86</v>
       </c>
@@ -2494,7 +2533,7 @@
       </c>
     </row>
     <row r="24">
-      <c s="12" r="A24"/>
+      <c s="13" r="A24"/>
       <c t="s" s="7" r="B24">
         <v>89</v>
       </c>
@@ -2509,7 +2548,7 @@
       </c>
     </row>
     <row r="25">
-      <c s="12" r="A25"/>
+      <c s="13" r="A25"/>
       <c t="s" s="7" r="B25">
         <v>93</v>
       </c>
@@ -2524,7 +2563,7 @@
       </c>
     </row>
     <row r="26">
-      <c s="12" r="A26"/>
+      <c s="13" r="A26"/>
       <c t="s" s="7" r="B26">
         <v>97</v>
       </c>
@@ -2623,7 +2662,7 @@
       </c>
     </row>
     <row r="33">
-      <c s="12" r="A33"/>
+      <c s="13" r="A33"/>
       <c t="s" s="7" r="B33">
         <v>122</v>
       </c>
@@ -2638,7 +2677,7 @@
       </c>
     </row>
     <row r="34">
-      <c s="12" r="A34"/>
+      <c s="13" r="A34"/>
       <c t="s" s="7" r="B34">
         <v>126</v>
       </c>
@@ -2653,34 +2692,34 @@
       </c>
     </row>
     <row r="35">
-      <c s="12" r="A35"/>
-      <c s="12" r="B35"/>
-      <c s="12" r="C35"/>
-      <c s="12" r="D35"/>
-      <c s="12" r="E35"/>
+      <c s="13" r="A35"/>
+      <c s="13" r="B35"/>
+      <c s="13" r="C35"/>
+      <c s="13" r="D35"/>
+      <c s="13" r="E35"/>
     </row>
     <row r="36">
       <c t="s" s="2" r="A36">
         <v>130</v>
       </c>
-      <c t="s" s="17" r="B36">
+      <c t="s" s="18" r="B36">
         <v>131</v>
       </c>
-      <c t="s" s="17" r="C36">
+      <c t="s" s="18" r="C36">
         <v>132</v>
       </c>
-      <c s="17" r="D36"/>
-      <c s="17" r="E36"/>
+      <c s="18" r="D36"/>
+      <c s="18" r="E36"/>
     </row>
     <row r="37">
       <c s="2" r="A37"/>
       <c s="2" r="B37"/>
       <c s="2" r="C37"/>
       <c s="2" r="D37"/>
-      <c s="12" r="E37"/>
+      <c s="13" r="E37"/>
     </row>
     <row r="38">
-      <c t="s" s="12" r="A38">
+      <c t="s" s="13" r="A38">
         <v>133</v>
       </c>
       <c t="s" s="7" r="B38">
@@ -2697,7 +2736,7 @@
       </c>
     </row>
     <row r="39">
-      <c s="12" r="A39"/>
+      <c s="13" r="A39"/>
       <c t="s" s="7" r="B39">
         <v>138</v>
       </c>
@@ -2712,7 +2751,7 @@
       </c>
     </row>
     <row r="40">
-      <c s="12" r="A40"/>
+      <c s="13" r="A40"/>
       <c t="s" s="7" r="B40">
         <v>142</v>
       </c>
@@ -2727,7 +2766,7 @@
       </c>
     </row>
     <row r="41">
-      <c s="12" r="A41"/>
+      <c s="13" r="A41"/>
       <c t="s" s="7" r="B41">
         <v>146</v>
       </c>
@@ -2742,7 +2781,7 @@
       </c>
     </row>
     <row r="42">
-      <c s="12" r="A42"/>
+      <c s="13" r="A42"/>
       <c t="s" s="7" r="B42">
         <v>150</v>
       </c>
@@ -2757,7 +2796,7 @@
       </c>
     </row>
     <row r="43">
-      <c s="12" r="A43"/>
+      <c s="13" r="A43"/>
       <c t="s" s="7" r="B43">
         <v>154</v>
       </c>
@@ -2772,7 +2811,7 @@
       </c>
     </row>
     <row r="44">
-      <c s="12" r="A44"/>
+      <c s="13" r="A44"/>
       <c t="s" s="7" r="B44">
         <v>158</v>
       </c>
@@ -2787,7 +2826,7 @@
       </c>
     </row>
     <row r="45">
-      <c s="12" r="A45"/>
+      <c s="13" r="A45"/>
       <c t="s" s="7" r="B45">
         <v>162</v>
       </c>
@@ -2802,7 +2841,7 @@
       </c>
     </row>
     <row r="46">
-      <c s="12" r="A46"/>
+      <c s="13" r="A46"/>
       <c t="s" s="7" r="B46">
         <v>166</v>
       </c>
@@ -2817,7 +2856,7 @@
       </c>
     </row>
     <row r="47">
-      <c s="12" r="A47"/>
+      <c s="13" r="A47"/>
       <c t="s" s="7" r="B47">
         <v>170</v>
       </c>
@@ -2832,7 +2871,7 @@
       </c>
     </row>
     <row r="48">
-      <c s="12" r="A48"/>
+      <c s="13" r="A48"/>
       <c t="s" s="7" r="B48">
         <v>174</v>
       </c>
@@ -2847,7 +2886,7 @@
       </c>
     </row>
     <row r="49">
-      <c s="12" r="A49"/>
+      <c s="13" r="A49"/>
       <c t="s" s="7" r="B49">
         <v>178</v>
       </c>
@@ -2862,7 +2901,7 @@
       </c>
     </row>
     <row r="50">
-      <c s="12" r="A50"/>
+      <c s="13" r="A50"/>
       <c t="s" s="7" r="B50">
         <v>182</v>
       </c>
@@ -2877,7 +2916,7 @@
       </c>
     </row>
     <row r="51">
-      <c s="12" r="A51"/>
+      <c s="13" r="A51"/>
       <c t="s" s="7" r="B51">
         <v>186</v>
       </c>
@@ -2892,7 +2931,7 @@
       </c>
     </row>
     <row r="52">
-      <c s="12" r="A52"/>
+      <c s="13" r="A52"/>
       <c t="s" s="7" r="B52">
         <v>190</v>
       </c>
@@ -2907,7 +2946,7 @@
       </c>
     </row>
     <row r="53">
-      <c s="12" r="A53"/>
+      <c s="13" r="A53"/>
       <c t="s" s="7" r="B53">
         <v>194</v>
       </c>
@@ -2922,14 +2961,14 @@
       </c>
     </row>
     <row r="54">
-      <c s="12" r="A54"/>
-      <c s="12" r="B54"/>
-      <c s="12" r="C54"/>
-      <c s="12" r="D54"/>
-      <c s="12" r="E54"/>
+      <c s="13" r="A54"/>
+      <c s="13" r="B54"/>
+      <c s="13" r="C54"/>
+      <c s="13" r="D54"/>
+      <c s="13" r="E54"/>
     </row>
     <row r="55">
-      <c t="s" s="12" r="A55">
+      <c t="s" s="13" r="A55">
         <v>198</v>
       </c>
       <c t="s" s="7" r="B55">
@@ -2946,7 +2985,7 @@
       </c>
     </row>
     <row r="56">
-      <c s="12" r="A56"/>
+      <c s="13" r="A56"/>
       <c t="s" s="7" r="B56">
         <v>203</v>
       </c>
@@ -2968,53 +3007,53 @@
       <c s="2" r="E58"/>
     </row>
     <row r="59">
-      <c t="s" s="12" r="A59">
+      <c t="s" s="13" r="A59">
         <v>207</v>
       </c>
-      <c t="s" s="15" r="B59">
+      <c t="s" s="16" r="B59">
         <v>208</v>
       </c>
-      <c t="s" s="15" r="C59">
+      <c t="s" s="16" r="C59">
         <v>209</v>
       </c>
-      <c s="15" r="D59"/>
-      <c s="15" r="E59"/>
+      <c s="16" r="D59"/>
+      <c s="16" r="E59"/>
     </row>
     <row r="60">
-      <c s="12" r="A60"/>
-      <c t="s" s="15" r="B60">
+      <c s="13" r="A60"/>
+      <c t="s" s="16" r="B60">
         <v>210</v>
       </c>
-      <c t="s" s="15" r="C60">
+      <c t="s" s="16" r="C60">
         <v>211</v>
       </c>
-      <c s="15" r="D60"/>
-      <c s="15" r="E60"/>
+      <c s="16" r="D60"/>
+      <c s="16" r="E60"/>
     </row>
     <row r="61">
-      <c s="12" r="A61"/>
-      <c t="s" s="15" r="B61">
+      <c s="13" r="A61"/>
+      <c t="s" s="16" r="B61">
         <v>212</v>
       </c>
-      <c t="s" s="15" r="C61">
+      <c t="s" s="16" r="C61">
         <v>213</v>
       </c>
-      <c s="15" r="D61"/>
-      <c s="15" r="E61"/>
+      <c s="16" r="D61"/>
+      <c s="16" r="E61"/>
     </row>
     <row r="62">
-      <c s="12" r="A62"/>
-      <c t="s" s="15" r="B62">
+      <c s="13" r="A62"/>
+      <c t="s" s="16" r="B62">
         <v>214</v>
       </c>
-      <c t="s" s="15" r="C62">
+      <c t="s" s="16" r="C62">
         <v>215</v>
       </c>
-      <c s="15" r="D62"/>
-      <c s="15" r="E62"/>
+      <c s="16" r="D62"/>
+      <c s="16" r="E62"/>
     </row>
     <row r="63">
-      <c s="12" r="A63"/>
+      <c s="13" r="A63"/>
       <c t="s" s="7" r="B63">
         <v>216</v>
       </c>
@@ -3029,7 +3068,7 @@
       </c>
     </row>
     <row r="64">
-      <c s="12" r="A64"/>
+      <c s="13" r="A64"/>
       <c t="s" s="7" r="B64">
         <v>220</v>
       </c>
@@ -3044,7 +3083,7 @@
       </c>
     </row>
     <row r="65">
-      <c s="12" r="A65"/>
+      <c s="13" r="A65"/>
       <c t="s" s="7" r="B65">
         <v>224</v>
       </c>
@@ -3059,7 +3098,7 @@
       </c>
     </row>
     <row r="66">
-      <c s="12" r="A66"/>
+      <c s="13" r="A66"/>
       <c t="s" s="7" r="B66">
         <v>228</v>
       </c>
@@ -3074,7 +3113,7 @@
       </c>
     </row>
     <row r="67">
-      <c s="12" r="A67"/>
+      <c s="13" r="A67"/>
       <c t="s" s="7" r="B67">
         <v>232</v>
       </c>
@@ -3089,7 +3128,7 @@
       </c>
     </row>
     <row r="68">
-      <c s="12" r="A68"/>
+      <c s="13" r="A68"/>
       <c t="s" s="7" r="B68">
         <v>236</v>
       </c>
@@ -3104,14 +3143,14 @@
       </c>
     </row>
     <row r="69">
-      <c s="12" r="A69"/>
-      <c s="12" r="B69"/>
-      <c s="12" r="C69"/>
-      <c s="12" r="D69"/>
-      <c s="12" r="E69"/>
+      <c s="13" r="A69"/>
+      <c s="13" r="B69"/>
+      <c s="13" r="C69"/>
+      <c s="13" r="D69"/>
+      <c s="13" r="E69"/>
     </row>
     <row r="70">
-      <c t="s" s="12" r="A70">
+      <c t="s" s="13" r="A70">
         <v>240</v>
       </c>
       <c t="s" s="7" r="B70">
@@ -3128,7 +3167,7 @@
       </c>
     </row>
     <row r="71">
-      <c s="12" r="A71"/>
+      <c s="13" r="A71"/>
       <c t="s" s="7" r="B71">
         <v>245</v>
       </c>
@@ -3143,7 +3182,7 @@
       </c>
     </row>
     <row r="72">
-      <c s="12" r="A72"/>
+      <c s="13" r="A72"/>
       <c t="s" s="7" r="B72">
         <v>249</v>
       </c>
@@ -3158,7 +3197,7 @@
       </c>
     </row>
     <row r="73">
-      <c s="12" r="A73"/>
+      <c s="13" r="A73"/>
       <c t="s" s="7" r="B73">
         <v>253</v>
       </c>
@@ -3173,7 +3212,7 @@
       </c>
     </row>
     <row r="74">
-      <c s="12" r="A74"/>
+      <c s="13" r="A74"/>
       <c t="s" s="7" r="B74">
         <v>257</v>
       </c>
@@ -3188,7 +3227,7 @@
       </c>
     </row>
     <row r="75">
-      <c s="12" r="A75"/>
+      <c s="13" r="A75"/>
       <c t="s" s="7" r="B75">
         <v>261</v>
       </c>
@@ -3203,7 +3242,7 @@
       </c>
     </row>
     <row r="76">
-      <c s="12" r="A76"/>
+      <c s="13" r="A76"/>
       <c t="s" s="7" r="B76">
         <v>265</v>
       </c>
@@ -3218,7 +3257,7 @@
       </c>
     </row>
     <row r="77">
-      <c s="12" r="A77"/>
+      <c s="13" r="A77"/>
       <c t="s" s="7" r="B77">
         <v>269</v>
       </c>
@@ -3233,7 +3272,7 @@
       </c>
     </row>
     <row r="78">
-      <c s="12" r="A78"/>
+      <c s="13" r="A78"/>
       <c t="s" s="7" r="B78">
         <v>273</v>
       </c>
@@ -3248,14 +3287,14 @@
       </c>
     </row>
     <row r="79">
-      <c s="12" r="A79"/>
-      <c s="12" r="B79"/>
-      <c s="12" r="C79"/>
-      <c s="12" r="D79"/>
-      <c s="12" r="E79"/>
+      <c s="13" r="A79"/>
+      <c s="13" r="B79"/>
+      <c s="13" r="C79"/>
+      <c s="13" r="D79"/>
+      <c s="13" r="E79"/>
     </row>
     <row r="80">
-      <c t="s" s="12" r="A80">
+      <c t="s" s="13" r="A80">
         <v>277</v>
       </c>
       <c t="s" s="7" r="B80">
@@ -3272,7 +3311,7 @@
       </c>
     </row>
     <row r="81">
-      <c s="12" r="A81"/>
+      <c s="13" r="A81"/>
       <c t="s" s="7" r="B81">
         <v>282</v>
       </c>
@@ -3287,7 +3326,7 @@
       </c>
     </row>
     <row r="82">
-      <c s="10" r="A82"/>
+      <c s="11" r="A82"/>
       <c t="s" s="7" r="B82">
         <v>286</v>
       </c>
@@ -3302,7 +3341,7 @@
       </c>
     </row>
     <row r="83">
-      <c s="10" r="A83"/>
+      <c s="11" r="A83"/>
       <c t="s" s="7" r="B83">
         <v>290</v>
       </c>
@@ -3317,7 +3356,7 @@
       </c>
     </row>
     <row r="84">
-      <c s="10" r="A84"/>
+      <c s="11" r="A84"/>
       <c t="s" s="7" r="B84">
         <v>294</v>
       </c>
@@ -3332,7 +3371,7 @@
       </c>
     </row>
     <row r="85">
-      <c s="10" r="A85"/>
+      <c s="11" r="A85"/>
       <c t="s" s="7" r="B85">
         <v>298</v>
       </c>
@@ -3347,7 +3386,7 @@
       </c>
     </row>
     <row r="86">
-      <c s="10" r="A86"/>
+      <c s="11" r="A86"/>
       <c t="s" s="7" r="B86">
         <v>302</v>
       </c>
@@ -3362,7 +3401,7 @@
       </c>
     </row>
     <row r="87">
-      <c s="10" r="A87"/>
+      <c s="11" r="A87"/>
       <c t="s" s="7" r="B87">
         <v>306</v>
       </c>
@@ -3377,7 +3416,7 @@
       </c>
     </row>
     <row r="88">
-      <c s="10" r="A88"/>
+      <c s="11" r="A88"/>
       <c t="s" s="7" r="B88">
         <v>310</v>
       </c>
@@ -3392,7 +3431,7 @@
       </c>
     </row>
     <row r="89">
-      <c s="10" r="A89"/>
+      <c s="11" r="A89"/>
       <c t="s" s="7" r="B89">
         <v>314</v>
       </c>
@@ -3407,7 +3446,7 @@
       </c>
     </row>
     <row r="90">
-      <c s="10" r="A90"/>
+      <c s="11" r="A90"/>
       <c t="s" s="7" r="B90">
         <v>318</v>
       </c>
@@ -3422,7 +3461,7 @@
       </c>
     </row>
     <row r="91">
-      <c s="10" r="A91"/>
+      <c s="11" r="A91"/>
       <c t="s" s="7" r="B91">
         <v>322</v>
       </c>
@@ -3437,7 +3476,7 @@
       </c>
     </row>
     <row r="92">
-      <c s="10" r="A92"/>
+      <c s="11" r="A92"/>
       <c t="s" s="7" r="B92">
         <v>326</v>
       </c>
@@ -3452,7 +3491,7 @@
       </c>
     </row>
     <row r="93">
-      <c s="10" r="A93"/>
+      <c s="11" r="A93"/>
       <c t="s" s="7" r="B93">
         <v>330</v>
       </c>
@@ -3467,14 +3506,14 @@
       </c>
     </row>
     <row r="94">
-      <c s="10" r="A94"/>
-      <c s="12" r="B94"/>
-      <c s="12" r="C94"/>
-      <c s="12" r="D94"/>
-      <c s="12" r="E94"/>
+      <c s="11" r="A94"/>
+      <c s="13" r="B94"/>
+      <c s="13" r="C94"/>
+      <c s="13" r="D94"/>
+      <c s="13" r="E94"/>
     </row>
     <row r="95">
-      <c t="s" s="10" r="A95">
+      <c t="s" s="11" r="A95">
         <v>334</v>
       </c>
       <c t="s" s="7" r="B95">
@@ -3491,7 +3530,7 @@
       </c>
     </row>
     <row r="96">
-      <c s="10" r="A96"/>
+      <c s="11" r="A96"/>
       <c t="s" s="7" r="B96">
         <v>339</v>
       </c>
@@ -3506,7 +3545,7 @@
       </c>
     </row>
     <row r="97">
-      <c s="10" r="A97"/>
+      <c s="11" r="A97"/>
       <c t="s" s="7" r="B97">
         <v>343</v>
       </c>
@@ -3521,7 +3560,7 @@
       </c>
     </row>
     <row r="98">
-      <c s="10" r="A98"/>
+      <c s="11" r="A98"/>
       <c t="s" s="7" r="B98">
         <v>347</v>
       </c>
@@ -3536,7 +3575,7 @@
       </c>
     </row>
     <row r="99">
-      <c s="10" r="A99"/>
+      <c s="11" r="A99"/>
       <c t="s" s="7" r="B99">
         <v>351</v>
       </c>
@@ -3551,7 +3590,7 @@
       </c>
     </row>
     <row r="100">
-      <c s="10" r="A100"/>
+      <c s="11" r="A100"/>
       <c t="s" s="7" r="B100">
         <v>355</v>
       </c>
@@ -3566,7 +3605,7 @@
       </c>
     </row>
     <row r="101">
-      <c s="10" r="A101"/>
+      <c s="11" r="A101"/>
       <c t="s" s="7" r="B101">
         <v>358</v>
       </c>
@@ -3581,7 +3620,7 @@
       </c>
     </row>
     <row r="102">
-      <c s="10" r="A102"/>
+      <c s="11" r="A102"/>
       <c t="s" s="7" r="B102">
         <v>362</v>
       </c>
@@ -3596,7 +3635,7 @@
       </c>
     </row>
     <row r="103">
-      <c s="10" r="A103"/>
+      <c s="11" r="A103"/>
       <c t="s" s="7" r="B103">
         <v>366</v>
       </c>
@@ -3611,7 +3650,7 @@
       </c>
     </row>
     <row r="104">
-      <c s="10" r="A104"/>
+      <c s="11" r="A104"/>
       <c t="s" s="7" r="B104">
         <v>370</v>
       </c>
@@ -3626,7 +3665,7 @@
       </c>
     </row>
     <row r="105">
-      <c s="10" r="A105"/>
+      <c s="11" r="A105"/>
       <c t="s" s="7" r="B105">
         <v>374</v>
       </c>
@@ -3641,7 +3680,7 @@
       </c>
     </row>
     <row r="106">
-      <c s="10" r="A106"/>
+      <c s="11" r="A106"/>
       <c t="s" s="7" r="B106">
         <v>378</v>
       </c>
@@ -3656,7 +3695,7 @@
       </c>
     </row>
     <row r="107">
-      <c s="10" r="A107"/>
+      <c s="11" r="A107"/>
       <c t="s" s="7" r="B107">
         <v>381</v>
       </c>
@@ -3671,7 +3710,7 @@
       </c>
     </row>
     <row r="108">
-      <c s="10" r="A108"/>
+      <c s="11" r="A108"/>
       <c t="s" s="7" r="B108">
         <v>384</v>
       </c>
@@ -3686,8 +3725,8 @@
       </c>
     </row>
     <row r="109">
-      <c s="10" r="A109"/>
-      <c t="s" s="16" r="B109">
+      <c s="11" r="A109"/>
+      <c t="s" s="17" r="B109">
         <v>388</v>
       </c>
       <c t="s" s="7" r="C109">
@@ -3701,7 +3740,7 @@
       </c>
     </row>
     <row r="110">
-      <c s="10" r="A110"/>
+      <c s="11" r="A110"/>
       <c t="s" s="7" r="B110">
         <v>391</v>
       </c>
@@ -3716,7 +3755,7 @@
       </c>
     </row>
     <row r="111">
-      <c s="10" r="A111"/>
+      <c s="11" r="A111"/>
       <c t="s" s="7" r="B111">
         <v>395</v>
       </c>
@@ -3731,7 +3770,7 @@
       </c>
     </row>
     <row r="112">
-      <c s="10" r="A112"/>
+      <c s="11" r="A112"/>
       <c t="s" s="7" r="B112">
         <v>399</v>
       </c>
@@ -3746,7 +3785,7 @@
       </c>
     </row>
     <row r="113">
-      <c s="10" r="A113"/>
+      <c s="11" r="A113"/>
       <c t="s" s="7" r="B113">
         <v>403</v>
       </c>
@@ -3761,7 +3800,7 @@
       </c>
     </row>
     <row r="114">
-      <c s="10" r="A114"/>
+      <c s="11" r="A114"/>
       <c t="s" s="7" r="B114">
         <v>407</v>
       </c>
@@ -3776,7 +3815,7 @@
       </c>
     </row>
     <row r="115">
-      <c s="10" r="A115"/>
+      <c s="11" r="A115"/>
       <c t="s" s="7" r="B115">
         <v>411</v>
       </c>
@@ -3791,7 +3830,7 @@
       </c>
     </row>
     <row r="116">
-      <c s="10" r="A116"/>
+      <c s="11" r="A116"/>
       <c t="s" s="7" r="B116">
         <v>415</v>
       </c>
@@ -3806,7 +3845,7 @@
       </c>
     </row>
     <row r="117">
-      <c s="10" r="A117"/>
+      <c s="11" r="A117"/>
       <c t="s" s="7" r="B117">
         <v>419</v>
       </c>
@@ -3821,7 +3860,7 @@
       </c>
     </row>
     <row r="118">
-      <c s="10" r="A118"/>
+      <c s="11" r="A118"/>
       <c t="s" s="7" r="B118">
         <v>423</v>
       </c>
@@ -3836,7 +3875,7 @@
       </c>
     </row>
     <row r="119">
-      <c s="10" r="A119"/>
+      <c s="11" r="A119"/>
       <c t="s" s="7" r="B119">
         <v>427</v>
       </c>
@@ -3851,7 +3890,7 @@
       </c>
     </row>
     <row r="120">
-      <c s="10" r="A120"/>
+      <c s="11" r="A120"/>
       <c t="s" s="7" r="B120">
         <v>431</v>
       </c>
@@ -3866,7 +3905,7 @@
       </c>
     </row>
     <row r="121">
-      <c s="10" r="A121"/>
+      <c s="11" r="A121"/>
       <c t="s" s="7" r="B121">
         <v>435</v>
       </c>
@@ -3881,7 +3920,7 @@
       </c>
     </row>
     <row r="122">
-      <c s="10" r="A122"/>
+      <c s="11" r="A122"/>
       <c t="s" s="7" r="B122">
         <v>439</v>
       </c>
@@ -3896,7 +3935,7 @@
       </c>
     </row>
     <row r="123">
-      <c s="10" r="A123"/>
+      <c s="11" r="A123"/>
       <c t="s" s="7" r="B123">
         <v>443</v>
       </c>
@@ -3911,7 +3950,7 @@
       </c>
     </row>
     <row r="124">
-      <c s="10" r="A124"/>
+      <c s="11" r="A124"/>
       <c t="s" s="7" r="B124">
         <v>447</v>
       </c>
@@ -3926,11 +3965,11 @@
       </c>
     </row>
     <row r="125">
-      <c s="10" r="A125"/>
+      <c s="11" r="A125"/>
       <c t="s" s="7" r="B125">
         <v>451</v>
       </c>
-      <c t="s" s="16" r="C125">
+      <c t="s" s="17" r="C125">
         <v>452</v>
       </c>
       <c t="s" s="7" r="D125">
@@ -3941,11 +3980,11 @@
       </c>
     </row>
     <row r="126">
-      <c s="10" r="A126"/>
-      <c t="s" s="16" r="B126">
+      <c s="11" r="A126"/>
+      <c t="s" s="17" r="B126">
         <v>455</v>
       </c>
-      <c t="s" s="16" r="C126">
+      <c t="s" s="17" r="C126">
         <v>456</v>
       </c>
       <c t="s" s="7" r="D126">
@@ -3956,11 +3995,11 @@
       </c>
     </row>
     <row r="127">
-      <c s="10" r="A127"/>
+      <c s="11" r="A127"/>
       <c t="s" s="7" r="B127">
         <v>459</v>
       </c>
-      <c t="s" s="16" r="C127">
+      <c t="s" s="17" r="C127">
         <v>456</v>
       </c>
       <c t="s" s="7" r="D127">
@@ -3971,7 +4010,7 @@
       </c>
     </row>
     <row r="128">
-      <c s="10" r="A128"/>
+      <c s="11" r="A128"/>
       <c t="s" s="7" r="B128">
         <v>460</v>
       </c>
@@ -3986,7 +4025,7 @@
       </c>
     </row>
     <row r="129">
-      <c s="10" r="A129"/>
+      <c s="11" r="A129"/>
       <c t="s" s="7" r="B129">
         <v>464</v>
       </c>
@@ -4001,7 +4040,7 @@
       </c>
     </row>
     <row r="130">
-      <c s="10" r="A130"/>
+      <c s="11" r="A130"/>
       <c t="s" s="7" r="B130">
         <v>468</v>
       </c>
@@ -4016,20 +4055,20 @@
       </c>
     </row>
     <row r="131">
-      <c s="10" r="A131"/>
-      <c s="18" r="B131"/>
-      <c s="9" r="C131"/>
-      <c s="18" r="D131"/>
-      <c s="18" r="E131"/>
+      <c s="11" r="A131"/>
+      <c s="19" r="B131"/>
+      <c s="10" r="C131"/>
+      <c s="19" r="D131"/>
+      <c s="19" r="E131"/>
     </row>
     <row r="132">
-      <c t="s" s="10" r="A132">
+      <c t="s" s="11" r="A132">
         <v>472</v>
       </c>
       <c t="s" s="7" r="B132">
         <v>473</v>
       </c>
-      <c t="s" s="16" r="C132">
+      <c t="s" s="17" r="C132">
         <v>474</v>
       </c>
       <c t="s" s="7" r="D132">
@@ -4040,11 +4079,11 @@
       </c>
     </row>
     <row r="133">
-      <c s="10" r="A133"/>
+      <c s="11" r="A133"/>
       <c t="s" s="7" r="B133">
         <v>477</v>
       </c>
-      <c t="s" s="16" r="C133">
+      <c t="s" s="17" r="C133">
         <v>478</v>
       </c>
       <c t="s" s="7" r="D133">
@@ -4055,11 +4094,11 @@
       </c>
     </row>
     <row r="134">
-      <c s="14" r="A134"/>
+      <c s="15" r="A134"/>
       <c t="s" s="7" r="B134">
         <v>481</v>
       </c>
-      <c t="s" s="16" r="C134">
+      <c t="s" s="17" r="C134">
         <v>482</v>
       </c>
       <c t="s" s="7" r="D134">
@@ -4070,11 +4109,11 @@
       </c>
     </row>
     <row r="135">
-      <c s="10" r="A135"/>
+      <c s="11" r="A135"/>
       <c t="s" s="3" r="B135">
         <v>485</v>
       </c>
-      <c t="s" s="16" r="C135">
+      <c t="s" s="17" r="C135">
         <v>486</v>
       </c>
       <c t="s" s="3" r="D135">
@@ -4085,11 +4124,11 @@
       </c>
     </row>
     <row r="136">
-      <c s="10" r="A136"/>
+      <c s="11" r="A136"/>
       <c t="s" s="7" r="B136">
         <v>489</v>
       </c>
-      <c t="s" s="16" r="C136">
+      <c t="s" s="17" r="C136">
         <v>490</v>
       </c>
       <c t="s" s="7" r="D136">
@@ -4100,11 +4139,11 @@
       </c>
     </row>
     <row r="137">
-      <c s="10" r="A137"/>
+      <c s="11" r="A137"/>
       <c t="s" s="7" r="B137">
         <v>493</v>
       </c>
-      <c t="s" s="16" r="C137">
+      <c t="s" s="17" r="C137">
         <v>494</v>
       </c>
       <c t="s" s="7" r="D137">
@@ -4115,11 +4154,11 @@
       </c>
     </row>
     <row r="138">
-      <c s="10" r="A138"/>
+      <c s="11" r="A138"/>
       <c t="s" s="7" r="B138">
         <v>497</v>
       </c>
-      <c t="s" s="16" r="C138">
+      <c t="s" s="17" r="C138">
         <v>498</v>
       </c>
       <c t="s" s="7" r="D138">
@@ -4130,11 +4169,11 @@
       </c>
     </row>
     <row r="139">
-      <c s="10" r="A139"/>
+      <c s="11" r="A139"/>
       <c t="s" s="7" r="B139">
         <v>501</v>
       </c>
-      <c t="s" s="16" r="C139">
+      <c t="s" s="17" r="C139">
         <v>502</v>
       </c>
       <c t="s" s="7" r="D139">
@@ -4145,11 +4184,11 @@
       </c>
     </row>
     <row r="140">
-      <c s="10" r="A140"/>
+      <c s="11" r="A140"/>
       <c t="s" s="7" r="B140">
         <v>505</v>
       </c>
-      <c t="s" s="16" r="C140">
+      <c t="s" s="17" r="C140">
         <v>506</v>
       </c>
       <c t="s" s="7" r="D140">
@@ -4160,11 +4199,11 @@
       </c>
     </row>
     <row r="141">
-      <c s="10" r="A141"/>
+      <c s="11" r="A141"/>
       <c t="s" s="7" r="B141">
         <v>509</v>
       </c>
-      <c t="s" s="16" r="C141">
+      <c t="s" s="17" r="C141">
         <v>510</v>
       </c>
       <c t="s" s="7" r="D141">
@@ -4175,11 +4214,11 @@
       </c>
     </row>
     <row r="142">
-      <c s="10" r="A142"/>
+      <c s="11" r="A142"/>
       <c t="s" s="7" r="B142">
         <v>513</v>
       </c>
-      <c t="s" s="16" r="C142">
+      <c t="s" s="17" r="C142">
         <v>514</v>
       </c>
       <c t="s" s="7" r="D142">
@@ -4190,11 +4229,11 @@
       </c>
     </row>
     <row r="143">
-      <c s="10" r="A143"/>
+      <c s="11" r="A143"/>
       <c t="s" s="7" r="B143">
         <v>517</v>
       </c>
-      <c t="s" s="16" r="C143">
+      <c t="s" s="17" r="C143">
         <v>518</v>
       </c>
       <c t="s" s="7" r="D143">
@@ -4205,11 +4244,11 @@
       </c>
     </row>
     <row r="144">
-      <c s="10" r="A144"/>
+      <c s="11" r="A144"/>
       <c t="s" s="7" r="B144">
         <v>521</v>
       </c>
-      <c t="s" s="16" r="C144">
+      <c t="s" s="17" r="C144">
         <v>522</v>
       </c>
       <c t="s" s="7" r="D144">
@@ -4220,11 +4259,11 @@
       </c>
     </row>
     <row r="145">
-      <c s="19" r="A145"/>
+      <c s="20" r="A145"/>
       <c t="s" s="7" r="B145">
         <v>525</v>
       </c>
-      <c t="s" s="16" r="C145">
+      <c t="s" s="17" r="C145">
         <v>526</v>
       </c>
       <c t="s" s="7" r="D145">
@@ -4235,11 +4274,11 @@
       </c>
     </row>
     <row r="146">
-      <c s="10" r="A146"/>
+      <c s="11" r="A146"/>
       <c t="s" s="7" r="B146">
         <v>529</v>
       </c>
-      <c t="s" s="16" r="C146">
+      <c t="s" s="17" r="C146">
         <v>530</v>
       </c>
       <c t="s" s="7" r="D146">
@@ -4250,11 +4289,11 @@
       </c>
     </row>
     <row r="147">
-      <c s="10" r="A147"/>
+      <c s="11" r="A147"/>
       <c t="s" s="7" r="B147">
         <v>533</v>
       </c>
-      <c t="s" s="16" r="C147">
+      <c t="s" s="17" r="C147">
         <v>534</v>
       </c>
       <c t="s" s="7" r="D147">
@@ -4265,11 +4304,11 @@
       </c>
     </row>
     <row r="148">
-      <c s="10" r="A148"/>
+      <c s="11" r="A148"/>
       <c t="s" s="7" r="B148">
         <v>536</v>
       </c>
-      <c t="s" s="16" r="C148">
+      <c t="s" s="17" r="C148">
         <v>537</v>
       </c>
       <c t="s" s="7" r="D148">
@@ -4280,11 +4319,11 @@
       </c>
     </row>
     <row r="149">
-      <c s="10" r="A149"/>
+      <c s="11" r="A149"/>
       <c t="s" s="7" r="B149">
         <v>540</v>
       </c>
-      <c t="s" s="16" r="C149">
+      <c t="s" s="17" r="C149">
         <v>541</v>
       </c>
       <c t="s" s="7" r="D149">
@@ -4295,11 +4334,11 @@
       </c>
     </row>
     <row r="150">
-      <c s="10" r="A150"/>
+      <c s="11" r="A150"/>
       <c t="s" s="7" r="B150">
         <v>544</v>
       </c>
-      <c t="s" s="16" r="C150">
+      <c t="s" s="17" r="C150">
         <v>545</v>
       </c>
       <c t="s" s="7" r="D150">
@@ -4310,11 +4349,11 @@
       </c>
     </row>
     <row r="151">
-      <c s="10" r="A151"/>
+      <c s="11" r="A151"/>
       <c t="s" s="7" r="B151">
         <v>548</v>
       </c>
-      <c t="s" s="16" r="C151">
+      <c t="s" s="17" r="C151">
         <v>549</v>
       </c>
       <c t="s" s="7" r="D151">
@@ -4325,11 +4364,11 @@
       </c>
     </row>
     <row r="152">
-      <c s="10" r="A152"/>
+      <c s="11" r="A152"/>
       <c t="s" s="7" r="B152">
         <v>552</v>
       </c>
-      <c t="s" s="16" r="C152">
+      <c t="s" s="17" r="C152">
         <v>553</v>
       </c>
       <c t="s" s="7" r="D152">
@@ -4340,35 +4379,35 @@
       </c>
     </row>
     <row r="153">
-      <c s="10" r="A153"/>
-      <c s="2" r="B153"/>
-      <c s="13" r="C153"/>
-      <c s="2" r="D153"/>
-      <c s="2" r="E153"/>
+      <c s="11" r="A153"/>
+      <c t="s" s="9" r="B153">
+        <v>556</v>
+      </c>
+      <c t="s" s="7" r="C153">
+        <v>557</v>
+      </c>
+      <c t="s" s="21" r="D153">
+        <v>558</v>
+      </c>
+      <c t="s" s="21" r="E153">
+        <v>559</v>
+      </c>
     </row>
     <row r="154">
-      <c t="s" s="10" r="A154">
-        <v>556</v>
-      </c>
-      <c t="s" s="7" r="B154">
-        <v>557</v>
-      </c>
-      <c t="s" s="16" r="C154">
-        <v>558</v>
-      </c>
-      <c t="s" s="7" r="D154">
-        <v>559</v>
-      </c>
-      <c t="s" s="7" r="E154">
+      <c s="11" r="A154"/>
+      <c s="2" r="B154"/>
+      <c s="14" r="C154"/>
+      <c s="2" r="D154"/>
+      <c s="2" r="E154"/>
+    </row>
+    <row r="155">
+      <c t="s" s="11" r="A155">
         <v>560</v>
       </c>
-    </row>
-    <row r="155">
-      <c s="10" r="A155"/>
       <c t="s" s="7" r="B155">
         <v>561</v>
       </c>
-      <c t="s" s="16" r="C155">
+      <c t="s" s="17" r="C155">
         <v>562</v>
       </c>
       <c t="s" s="7" r="D155">
@@ -4379,11 +4418,11 @@
       </c>
     </row>
     <row r="156">
-      <c s="10" r="A156"/>
+      <c s="11" r="A156"/>
       <c t="s" s="7" r="B156">
         <v>565</v>
       </c>
-      <c t="s" s="16" r="C156">
+      <c t="s" s="17" r="C156">
         <v>566</v>
       </c>
       <c t="s" s="7" r="D156">
@@ -4394,11 +4433,11 @@
       </c>
     </row>
     <row r="157">
-      <c s="10" r="A157"/>
+      <c s="11" r="A157"/>
       <c t="s" s="7" r="B157">
         <v>569</v>
       </c>
-      <c t="s" s="16" r="C157">
+      <c t="s" s="17" r="C157">
         <v>570</v>
       </c>
       <c t="s" s="7" r="D157">
@@ -4409,11 +4448,11 @@
       </c>
     </row>
     <row r="158">
-      <c s="10" r="A158"/>
+      <c s="11" r="A158"/>
       <c t="s" s="7" r="B158">
         <v>573</v>
       </c>
-      <c t="s" s="16" r="C158">
+      <c t="s" s="17" r="C158">
         <v>574</v>
       </c>
       <c t="s" s="7" r="D158">
@@ -4424,76 +4463,91 @@
       </c>
     </row>
     <row r="159">
-      <c s="10" r="A159"/>
-      <c s="2" r="B159"/>
-      <c s="13" r="C159"/>
-      <c s="2" r="D159"/>
-      <c s="2" r="E159"/>
+      <c s="11" r="A159"/>
+      <c t="s" s="7" r="B159">
+        <v>577</v>
+      </c>
+      <c t="s" s="17" r="C159">
+        <v>578</v>
+      </c>
+      <c t="s" s="7" r="D159">
+        <v>579</v>
+      </c>
+      <c t="s" s="7" r="E159">
+        <v>580</v>
+      </c>
     </row>
     <row r="160">
-      <c t="s" s="10" r="A160">
-        <v>577</v>
-      </c>
-      <c t="s" s="15" r="B160">
-        <v>578</v>
-      </c>
-      <c t="s" s="1" r="C160">
-        <v>577</v>
-      </c>
-      <c s="15" r="D160"/>
-      <c s="15" r="E160"/>
+      <c s="11" r="A160"/>
+      <c s="2" r="B160"/>
+      <c s="14" r="C160"/>
+      <c s="2" r="D160"/>
+      <c s="2" r="E160"/>
     </row>
     <row r="161">
-      <c s="10" r="A161"/>
-      <c s="18" r="B161"/>
-      <c s="9" r="C161"/>
-      <c s="18" r="D161"/>
-      <c s="18" r="E161"/>
+      <c t="s" s="11" r="A161">
+        <v>581</v>
+      </c>
+      <c t="s" s="16" r="B161">
+        <v>582</v>
+      </c>
+      <c t="s" s="1" r="C161">
+        <v>581</v>
+      </c>
+      <c s="16" r="D161"/>
+      <c s="16" r="E161"/>
     </row>
     <row r="162">
-      <c t="s" s="10" r="A162">
-        <v>579</v>
-      </c>
-      <c t="s" s="22" r="B162">
-        <v>580</v>
-      </c>
-      <c t="s" s="20" r="C162">
-        <v>581</v>
-      </c>
-      <c s="22" r="D162"/>
-      <c s="22" r="E162"/>
+      <c s="11" r="A162"/>
+      <c s="19" r="B162"/>
+      <c s="10" r="C162"/>
+      <c s="19" r="D162"/>
+      <c s="19" r="E162"/>
     </row>
     <row r="163">
-      <c s="10" r="A163"/>
-      <c t="s" s="22" r="B163">
-        <v>582</v>
-      </c>
-      <c t="s" s="20" r="C163">
+      <c t="s" s="11" r="A163">
         <v>583</v>
       </c>
-      <c s="22" r="D163"/>
-      <c s="22" r="E163"/>
+      <c t="s" s="24" r="B163">
+        <v>584</v>
+      </c>
+      <c t="s" s="22" r="C163">
+        <v>585</v>
+      </c>
+      <c s="24" r="D163"/>
+      <c s="24" r="E163"/>
     </row>
     <row r="164">
-      <c s="10" r="A164"/>
-      <c s="18" r="B164"/>
-      <c s="9" r="C164"/>
-      <c s="18" r="D164"/>
-      <c s="18" r="E164"/>
+      <c s="11" r="A164"/>
+      <c t="s" s="24" r="B164">
+        <v>586</v>
+      </c>
+      <c t="s" s="22" r="C164">
+        <v>587</v>
+      </c>
+      <c s="24" r="D164"/>
+      <c s="24" r="E164"/>
     </row>
     <row r="165">
-      <c s="10" r="A165"/>
-      <c s="18" r="B165"/>
-      <c s="9" r="C165"/>
-      <c s="18" r="D165"/>
-      <c s="18" r="E165"/>
+      <c s="11" r="A165"/>
+      <c s="19" r="B165"/>
+      <c s="10" r="C165"/>
+      <c s="19" r="D165"/>
+      <c s="19" r="E165"/>
     </row>
     <row r="166">
-      <c s="10" r="A166"/>
-      <c s="18" r="B166"/>
-      <c s="9" r="C166"/>
-      <c s="18" r="D166"/>
-      <c s="18" r="E166"/>
+      <c s="11" r="A166"/>
+      <c s="19" r="B166"/>
+      <c s="10" r="C166"/>
+      <c s="19" r="D166"/>
+      <c s="19" r="E166"/>
+    </row>
+    <row r="167">
+      <c s="11" r="A167"/>
+      <c s="19" r="B167"/>
+      <c s="10" r="C167"/>
+      <c s="19" r="D167"/>
+      <c s="19" r="E167"/>
     </row>
   </sheetData>
 </worksheet>
@@ -4507,164 +4561,164 @@
   <sheetFormatPr customHeight="1" defaultColWidth="9.86" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c s="21" r="A1"/>
-      <c s="21" r="B1"/>
-      <c s="21" r="C1"/>
-      <c s="21" r="D1"/>
-      <c s="21" r="E1"/>
-      <c s="21" r="F1"/>
+      <c s="23" r="A1"/>
+      <c s="23" r="B1"/>
+      <c s="23" r="C1"/>
+      <c s="23" r="D1"/>
+      <c s="23" r="E1"/>
+      <c s="23" r="F1"/>
     </row>
     <row r="2">
-      <c s="21" r="A2"/>
-      <c s="21" r="B2"/>
-      <c s="21" r="C2"/>
-      <c s="21" r="D2"/>
-      <c s="21" r="E2"/>
-      <c s="21" r="F2"/>
+      <c s="23" r="A2"/>
+      <c s="23" r="B2"/>
+      <c s="23" r="C2"/>
+      <c s="23" r="D2"/>
+      <c s="23" r="E2"/>
+      <c s="23" r="F2"/>
     </row>
     <row r="3">
-      <c s="21" r="A3"/>
-      <c s="21" r="B3"/>
-      <c s="21" r="C3"/>
-      <c s="21" r="D3"/>
-      <c s="21" r="E3"/>
-      <c s="21" r="F3"/>
+      <c s="23" r="A3"/>
+      <c s="23" r="B3"/>
+      <c s="23" r="C3"/>
+      <c s="23" r="D3"/>
+      <c s="23" r="E3"/>
+      <c s="23" r="F3"/>
     </row>
     <row r="4">
-      <c s="21" r="A4"/>
-      <c s="21" r="B4"/>
-      <c s="21" r="C4"/>
-      <c s="21" r="D4"/>
-      <c s="21" r="E4"/>
-      <c s="21" r="F4"/>
+      <c s="23" r="A4"/>
+      <c s="23" r="B4"/>
+      <c s="23" r="C4"/>
+      <c s="23" r="D4"/>
+      <c s="23" r="E4"/>
+      <c s="23" r="F4"/>
     </row>
     <row r="5">
-      <c s="21" r="A5"/>
-      <c s="21" r="B5"/>
-      <c s="21" r="C5"/>
-      <c s="21" r="D5"/>
-      <c s="21" r="E5"/>
-      <c s="21" r="F5"/>
+      <c s="23" r="A5"/>
+      <c s="23" r="B5"/>
+      <c s="23" r="C5"/>
+      <c s="23" r="D5"/>
+      <c s="23" r="E5"/>
+      <c s="23" r="F5"/>
     </row>
     <row r="6">
-      <c s="21" r="A6"/>
-      <c s="21" r="B6"/>
-      <c s="21" r="C6"/>
-      <c s="21" r="D6"/>
-      <c s="21" r="E6"/>
-      <c s="21" r="F6"/>
+      <c s="23" r="A6"/>
+      <c s="23" r="B6"/>
+      <c s="23" r="C6"/>
+      <c s="23" r="D6"/>
+      <c s="23" r="E6"/>
+      <c s="23" r="F6"/>
     </row>
     <row r="7">
-      <c s="21" r="A7"/>
-      <c s="21" r="B7"/>
-      <c s="21" r="C7"/>
-      <c s="21" r="D7"/>
-      <c s="21" r="E7"/>
-      <c s="21" r="F7"/>
+      <c s="23" r="A7"/>
+      <c s="23" r="B7"/>
+      <c s="23" r="C7"/>
+      <c s="23" r="D7"/>
+      <c s="23" r="E7"/>
+      <c s="23" r="F7"/>
     </row>
     <row r="8">
-      <c s="21" r="A8"/>
-      <c s="21" r="B8"/>
-      <c s="21" r="C8"/>
-      <c s="21" r="D8"/>
-      <c s="21" r="E8"/>
-      <c s="21" r="F8"/>
+      <c s="23" r="A8"/>
+      <c s="23" r="B8"/>
+      <c s="23" r="C8"/>
+      <c s="23" r="D8"/>
+      <c s="23" r="E8"/>
+      <c s="23" r="F8"/>
     </row>
     <row r="9">
-      <c s="21" r="A9"/>
-      <c s="21" r="B9"/>
-      <c s="21" r="C9"/>
-      <c s="21" r="D9"/>
-      <c s="21" r="E9"/>
-      <c s="21" r="F9"/>
+      <c s="23" r="A9"/>
+      <c s="23" r="B9"/>
+      <c s="23" r="C9"/>
+      <c s="23" r="D9"/>
+      <c s="23" r="E9"/>
+      <c s="23" r="F9"/>
     </row>
     <row r="10">
-      <c s="21" r="A10"/>
-      <c s="21" r="B10"/>
-      <c s="21" r="C10"/>
-      <c s="21" r="D10"/>
-      <c s="21" r="E10"/>
-      <c s="21" r="F10"/>
+      <c s="23" r="A10"/>
+      <c s="23" r="B10"/>
+      <c s="23" r="C10"/>
+      <c s="23" r="D10"/>
+      <c s="23" r="E10"/>
+      <c s="23" r="F10"/>
     </row>
     <row r="11">
-      <c s="21" r="A11"/>
-      <c s="21" r="B11"/>
-      <c s="21" r="C11"/>
-      <c s="21" r="D11"/>
-      <c s="21" r="E11"/>
-      <c s="21" r="F11"/>
+      <c s="23" r="A11"/>
+      <c s="23" r="B11"/>
+      <c s="23" r="C11"/>
+      <c s="23" r="D11"/>
+      <c s="23" r="E11"/>
+      <c s="23" r="F11"/>
     </row>
     <row r="12">
-      <c s="21" r="A12"/>
-      <c s="21" r="B12"/>
-      <c s="21" r="C12"/>
-      <c s="21" r="D12"/>
-      <c s="21" r="E12"/>
-      <c s="21" r="F12"/>
+      <c s="23" r="A12"/>
+      <c s="23" r="B12"/>
+      <c s="23" r="C12"/>
+      <c s="23" r="D12"/>
+      <c s="23" r="E12"/>
+      <c s="23" r="F12"/>
     </row>
     <row r="13">
-      <c s="21" r="A13"/>
-      <c s="21" r="B13"/>
-      <c s="21" r="C13"/>
-      <c s="21" r="D13"/>
-      <c s="21" r="E13"/>
-      <c s="21" r="F13"/>
+      <c s="23" r="A13"/>
+      <c s="23" r="B13"/>
+      <c s="23" r="C13"/>
+      <c s="23" r="D13"/>
+      <c s="23" r="E13"/>
+      <c s="23" r="F13"/>
     </row>
     <row r="14">
-      <c s="21" r="A14"/>
-      <c s="21" r="B14"/>
-      <c s="21" r="C14"/>
-      <c s="21" r="D14"/>
-      <c s="21" r="E14"/>
-      <c s="21" r="F14"/>
+      <c s="23" r="A14"/>
+      <c s="23" r="B14"/>
+      <c s="23" r="C14"/>
+      <c s="23" r="D14"/>
+      <c s="23" r="E14"/>
+      <c s="23" r="F14"/>
     </row>
     <row r="15">
-      <c s="21" r="A15"/>
-      <c s="21" r="B15"/>
-      <c s="21" r="C15"/>
-      <c s="21" r="D15"/>
-      <c s="21" r="E15"/>
-      <c s="21" r="F15"/>
+      <c s="23" r="A15"/>
+      <c s="23" r="B15"/>
+      <c s="23" r="C15"/>
+      <c s="23" r="D15"/>
+      <c s="23" r="E15"/>
+      <c s="23" r="F15"/>
     </row>
     <row r="16">
-      <c s="21" r="A16"/>
-      <c s="21" r="B16"/>
-      <c s="21" r="C16"/>
-      <c s="21" r="D16"/>
-      <c s="21" r="E16"/>
-      <c s="21" r="F16"/>
+      <c s="23" r="A16"/>
+      <c s="23" r="B16"/>
+      <c s="23" r="C16"/>
+      <c s="23" r="D16"/>
+      <c s="23" r="E16"/>
+      <c s="23" r="F16"/>
     </row>
     <row r="17">
-      <c s="21" r="A17"/>
-      <c s="21" r="B17"/>
-      <c s="21" r="C17"/>
-      <c s="21" r="D17"/>
-      <c s="21" r="E17"/>
-      <c s="21" r="F17"/>
+      <c s="23" r="A17"/>
+      <c s="23" r="B17"/>
+      <c s="23" r="C17"/>
+      <c s="23" r="D17"/>
+      <c s="23" r="E17"/>
+      <c s="23" r="F17"/>
     </row>
     <row r="18">
-      <c s="21" r="A18"/>
-      <c s="21" r="B18"/>
-      <c s="21" r="C18"/>
-      <c s="21" r="D18"/>
-      <c s="21" r="E18"/>
-      <c s="21" r="F18"/>
+      <c s="23" r="A18"/>
+      <c s="23" r="B18"/>
+      <c s="23" r="C18"/>
+      <c s="23" r="D18"/>
+      <c s="23" r="E18"/>
+      <c s="23" r="F18"/>
     </row>
     <row r="19">
-      <c s="21" r="A19"/>
-      <c s="21" r="B19"/>
-      <c s="21" r="C19"/>
-      <c s="21" r="D19"/>
-      <c s="21" r="E19"/>
-      <c s="21" r="F19"/>
+      <c s="23" r="A19"/>
+      <c s="23" r="B19"/>
+      <c s="23" r="C19"/>
+      <c s="23" r="D19"/>
+      <c s="23" r="E19"/>
+      <c s="23" r="F19"/>
     </row>
     <row r="20">
-      <c s="21" r="A20"/>
-      <c s="21" r="B20"/>
-      <c s="21" r="C20"/>
-      <c s="21" r="D20"/>
-      <c s="21" r="E20"/>
-      <c s="21" r="F20"/>
+      <c s="23" r="A20"/>
+      <c s="23" r="B20"/>
+      <c s="23" r="C20"/>
+      <c s="23" r="D20"/>
+      <c s="23" r="E20"/>
+      <c s="23" r="F20"/>
     </row>
   </sheetData>
 </worksheet>
@@ -4678,164 +4732,164 @@
   <sheetFormatPr customHeight="1" defaultColWidth="9.86" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c s="21" r="A1"/>
-      <c s="21" r="B1"/>
-      <c s="21" r="C1"/>
-      <c s="21" r="D1"/>
-      <c s="21" r="E1"/>
-      <c s="21" r="F1"/>
+      <c s="23" r="A1"/>
+      <c s="23" r="B1"/>
+      <c s="23" r="C1"/>
+      <c s="23" r="D1"/>
+      <c s="23" r="E1"/>
+      <c s="23" r="F1"/>
     </row>
     <row r="2">
-      <c s="21" r="A2"/>
-      <c s="21" r="B2"/>
-      <c s="21" r="C2"/>
-      <c s="21" r="D2"/>
-      <c s="21" r="E2"/>
-      <c s="21" r="F2"/>
+      <c s="23" r="A2"/>
+      <c s="23" r="B2"/>
+      <c s="23" r="C2"/>
+      <c s="23" r="D2"/>
+      <c s="23" r="E2"/>
+      <c s="23" r="F2"/>
     </row>
     <row r="3">
-      <c s="21" r="A3"/>
-      <c s="21" r="B3"/>
-      <c s="21" r="C3"/>
-      <c s="21" r="D3"/>
-      <c s="21" r="E3"/>
-      <c s="21" r="F3"/>
+      <c s="23" r="A3"/>
+      <c s="23" r="B3"/>
+      <c s="23" r="C3"/>
+      <c s="23" r="D3"/>
+      <c s="23" r="E3"/>
+      <c s="23" r="F3"/>
     </row>
     <row r="4">
-      <c s="21" r="A4"/>
-      <c s="21" r="B4"/>
-      <c s="21" r="C4"/>
-      <c s="21" r="D4"/>
-      <c s="21" r="E4"/>
-      <c s="21" r="F4"/>
+      <c s="23" r="A4"/>
+      <c s="23" r="B4"/>
+      <c s="23" r="C4"/>
+      <c s="23" r="D4"/>
+      <c s="23" r="E4"/>
+      <c s="23" r="F4"/>
     </row>
     <row r="5">
-      <c s="21" r="A5"/>
-      <c s="21" r="B5"/>
-      <c s="21" r="C5"/>
-      <c s="21" r="D5"/>
-      <c s="21" r="E5"/>
-      <c s="21" r="F5"/>
+      <c s="23" r="A5"/>
+      <c s="23" r="B5"/>
+      <c s="23" r="C5"/>
+      <c s="23" r="D5"/>
+      <c s="23" r="E5"/>
+      <c s="23" r="F5"/>
     </row>
     <row r="6">
-      <c s="21" r="A6"/>
-      <c s="21" r="B6"/>
-      <c s="21" r="C6"/>
-      <c s="21" r="D6"/>
-      <c s="21" r="E6"/>
-      <c s="21" r="F6"/>
+      <c s="23" r="A6"/>
+      <c s="23" r="B6"/>
+      <c s="23" r="C6"/>
+      <c s="23" r="D6"/>
+      <c s="23" r="E6"/>
+      <c s="23" r="F6"/>
     </row>
     <row r="7">
-      <c s="21" r="A7"/>
-      <c s="21" r="B7"/>
-      <c s="21" r="C7"/>
-      <c s="21" r="D7"/>
-      <c s="21" r="E7"/>
-      <c s="21" r="F7"/>
+      <c s="23" r="A7"/>
+      <c s="23" r="B7"/>
+      <c s="23" r="C7"/>
+      <c s="23" r="D7"/>
+      <c s="23" r="E7"/>
+      <c s="23" r="F7"/>
     </row>
     <row r="8">
-      <c s="21" r="A8"/>
-      <c s="21" r="B8"/>
-      <c s="21" r="C8"/>
-      <c s="21" r="D8"/>
-      <c s="21" r="E8"/>
-      <c s="21" r="F8"/>
+      <c s="23" r="A8"/>
+      <c s="23" r="B8"/>
+      <c s="23" r="C8"/>
+      <c s="23" r="D8"/>
+      <c s="23" r="E8"/>
+      <c s="23" r="F8"/>
     </row>
     <row r="9">
-      <c s="21" r="A9"/>
-      <c s="21" r="B9"/>
-      <c s="21" r="C9"/>
-      <c s="21" r="D9"/>
-      <c s="21" r="E9"/>
-      <c s="21" r="F9"/>
+      <c s="23" r="A9"/>
+      <c s="23" r="B9"/>
+      <c s="23" r="C9"/>
+      <c s="23" r="D9"/>
+      <c s="23" r="E9"/>
+      <c s="23" r="F9"/>
     </row>
     <row r="10">
-      <c s="21" r="A10"/>
-      <c s="21" r="B10"/>
-      <c s="21" r="C10"/>
-      <c s="21" r="D10"/>
-      <c s="21" r="E10"/>
-      <c s="21" r="F10"/>
+      <c s="23" r="A10"/>
+      <c s="23" r="B10"/>
+      <c s="23" r="C10"/>
+      <c s="23" r="D10"/>
+      <c s="23" r="E10"/>
+      <c s="23" r="F10"/>
     </row>
     <row r="11">
-      <c s="21" r="A11"/>
-      <c s="21" r="B11"/>
-      <c s="21" r="C11"/>
-      <c s="21" r="D11"/>
-      <c s="21" r="E11"/>
-      <c s="21" r="F11"/>
+      <c s="23" r="A11"/>
+      <c s="23" r="B11"/>
+      <c s="23" r="C11"/>
+      <c s="23" r="D11"/>
+      <c s="23" r="E11"/>
+      <c s="23" r="F11"/>
     </row>
     <row r="12">
-      <c s="21" r="A12"/>
-      <c s="21" r="B12"/>
-      <c s="21" r="C12"/>
-      <c s="21" r="D12"/>
-      <c s="21" r="E12"/>
-      <c s="21" r="F12"/>
+      <c s="23" r="A12"/>
+      <c s="23" r="B12"/>
+      <c s="23" r="C12"/>
+      <c s="23" r="D12"/>
+      <c s="23" r="E12"/>
+      <c s="23" r="F12"/>
     </row>
     <row r="13">
-      <c s="21" r="A13"/>
-      <c s="21" r="B13"/>
-      <c s="21" r="C13"/>
-      <c s="21" r="D13"/>
-      <c s="21" r="E13"/>
-      <c s="21" r="F13"/>
+      <c s="23" r="A13"/>
+      <c s="23" r="B13"/>
+      <c s="23" r="C13"/>
+      <c s="23" r="D13"/>
+      <c s="23" r="E13"/>
+      <c s="23" r="F13"/>
     </row>
     <row r="14">
-      <c s="21" r="A14"/>
-      <c s="21" r="B14"/>
-      <c s="21" r="C14"/>
-      <c s="21" r="D14"/>
-      <c s="21" r="E14"/>
-      <c s="21" r="F14"/>
+      <c s="23" r="A14"/>
+      <c s="23" r="B14"/>
+      <c s="23" r="C14"/>
+      <c s="23" r="D14"/>
+      <c s="23" r="E14"/>
+      <c s="23" r="F14"/>
     </row>
     <row r="15">
-      <c s="21" r="A15"/>
-      <c s="21" r="B15"/>
-      <c s="21" r="C15"/>
-      <c s="21" r="D15"/>
-      <c s="21" r="E15"/>
-      <c s="21" r="F15"/>
+      <c s="23" r="A15"/>
+      <c s="23" r="B15"/>
+      <c s="23" r="C15"/>
+      <c s="23" r="D15"/>
+      <c s="23" r="E15"/>
+      <c s="23" r="F15"/>
     </row>
     <row r="16">
-      <c s="21" r="A16"/>
-      <c s="21" r="B16"/>
-      <c s="21" r="C16"/>
-      <c s="21" r="D16"/>
-      <c s="21" r="E16"/>
-      <c s="21" r="F16"/>
+      <c s="23" r="A16"/>
+      <c s="23" r="B16"/>
+      <c s="23" r="C16"/>
+      <c s="23" r="D16"/>
+      <c s="23" r="E16"/>
+      <c s="23" r="F16"/>
     </row>
     <row r="17">
-      <c s="21" r="A17"/>
-      <c s="21" r="B17"/>
-      <c s="21" r="C17"/>
-      <c s="21" r="D17"/>
-      <c s="21" r="E17"/>
-      <c s="21" r="F17"/>
+      <c s="23" r="A17"/>
+      <c s="23" r="B17"/>
+      <c s="23" r="C17"/>
+      <c s="23" r="D17"/>
+      <c s="23" r="E17"/>
+      <c s="23" r="F17"/>
     </row>
     <row r="18">
-      <c s="21" r="A18"/>
-      <c s="21" r="B18"/>
-      <c s="21" r="C18"/>
-      <c s="21" r="D18"/>
-      <c s="21" r="E18"/>
-      <c s="21" r="F18"/>
+      <c s="23" r="A18"/>
+      <c s="23" r="B18"/>
+      <c s="23" r="C18"/>
+      <c s="23" r="D18"/>
+      <c s="23" r="E18"/>
+      <c s="23" r="F18"/>
     </row>
     <row r="19">
-      <c s="21" r="A19"/>
-      <c s="21" r="B19"/>
-      <c s="21" r="C19"/>
-      <c s="21" r="D19"/>
-      <c s="21" r="E19"/>
-      <c s="21" r="F19"/>
+      <c s="23" r="A19"/>
+      <c s="23" r="B19"/>
+      <c s="23" r="C19"/>
+      <c s="23" r="D19"/>
+      <c s="23" r="E19"/>
+      <c s="23" r="F19"/>
     </row>
     <row r="20">
-      <c s="21" r="A20"/>
-      <c s="21" r="B20"/>
-      <c s="21" r="C20"/>
-      <c s="21" r="D20"/>
-      <c s="21" r="E20"/>
-      <c s="21" r="F20"/>
+      <c s="23" r="A20"/>
+      <c s="23" r="B20"/>
+      <c s="23" r="C20"/>
+      <c s="23" r="D20"/>
+      <c s="23" r="E20"/>
+      <c s="23" r="F20"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
EWD-22527 - Redesign application header 640x
Former-commit-id: e5bc915a356fc22de225c3991c7fb6bce553c547
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="738">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="741">
   <si>
     <t>Page</t>
   </si>
@@ -2127,6 +2127,15 @@
   </si>
   <si>
     <t>Abmelden</t>
+  </si>
+  <si>
+    <t>help</t>
+  </si>
+  <si>
+    <t>Help</t>
+  </si>
+  <si>
+    <t>Hilfe</t>
   </si>
   <si>
     <t>File uploader</t>
@@ -2235,7 +2244,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -2372,6 +2381,15 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <b/>
       <i val="0"/>
       <strike val="0"/>
@@ -2426,7 +2444,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2503,6 +2521,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2533,13 +2557,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FF666666"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF666666"/>
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2568,7 +2592,7 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
@@ -2618,35 +2642,38 @@
     <xf applyAlignment="1" fillId="13" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="13" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="14" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+    <xf applyAlignment="1" fillId="14" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="14" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="15" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="14" applyFill="1">
+    <xf applyAlignment="1" fillId="15" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="15">
+    <xf applyAlignment="1" fillId="16" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="15" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="16">
+      <alignment vertical="center" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="17">
       <alignment vertical="bottom" horizontal="right"/>
     </xf>
-    <xf applyAlignment="1" fillId="16" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+    <xf applyAlignment="1" fillId="17" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="17" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="17" applyFill="1">
+    <xf applyAlignment="1" fillId="18" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="18" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="18" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
-      <alignment vertical="center" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" fillId="19" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="18" applyFill="1">
+    <xf applyAlignment="1" fillId="19" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="19" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="20" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="19"/>
-    <xf applyAlignment="1" fillId="21" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="20" applyFill="1">
+    <xf applyAlignment="1" fillId="21" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+      <alignment vertical="center" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="20"/>
+    <xf applyAlignment="1" fillId="22" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="21" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2674,24 +2701,24 @@
   </cols>
   <sheetData>
     <row s="4" customFormat="1" r="1">
-      <c t="s" s="22" r="A1">
+      <c t="s" s="23" r="A1">
         <v>0</v>
       </c>
-      <c t="s" s="22" r="B1">
+      <c t="s" s="23" r="B1">
         <v>1</v>
       </c>
-      <c t="s" s="22" r="C1">
+      <c t="s" s="23" r="C1">
         <v>2</v>
       </c>
-      <c t="s" s="22" r="D1">
+      <c t="s" s="23" r="D1">
         <v>3</v>
       </c>
-      <c t="s" s="19" r="E1">
+      <c t="s" s="20" r="E1">
         <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c t="s" s="16" r="A2">
+      <c t="s" s="17" r="A2">
         <v>5</v>
       </c>
       <c t="s" s="5" r="B2">
@@ -2708,7 +2735,7 @@
       </c>
     </row>
     <row r="3">
-      <c s="16" r="A3"/>
+      <c s="17" r="A3"/>
       <c t="s" s="5" r="B3">
         <v>10</v>
       </c>
@@ -2723,7 +2750,7 @@
       </c>
     </row>
     <row r="4">
-      <c s="16" r="A4"/>
+      <c s="17" r="A4"/>
       <c t="s" s="5" r="B4">
         <v>14</v>
       </c>
@@ -2738,7 +2765,7 @@
       </c>
     </row>
     <row r="5">
-      <c s="16" r="A5"/>
+      <c s="17" r="A5"/>
       <c t="s" s="5" r="B5">
         <v>18</v>
       </c>
@@ -2753,7 +2780,7 @@
       </c>
     </row>
     <row r="6">
-      <c s="16" r="A6"/>
+      <c s="17" r="A6"/>
       <c t="s" s="5" r="B6">
         <v>22</v>
       </c>
@@ -2768,7 +2795,7 @@
       </c>
     </row>
     <row r="7">
-      <c s="16" r="A7"/>
+      <c s="17" r="A7"/>
       <c t="s" s="5" r="B7">
         <v>24</v>
       </c>
@@ -2783,7 +2810,7 @@
       </c>
     </row>
     <row r="8">
-      <c s="16" r="A8"/>
+      <c s="17" r="A8"/>
       <c t="s" s="5" r="B8">
         <v>26</v>
       </c>
@@ -2798,7 +2825,7 @@
       </c>
     </row>
     <row r="9">
-      <c s="16" r="A9"/>
+      <c s="17" r="A9"/>
       <c t="s" s="5" r="B9">
         <v>30</v>
       </c>
@@ -2813,7 +2840,7 @@
       </c>
     </row>
     <row r="10">
-      <c s="16" r="A10"/>
+      <c s="17" r="A10"/>
       <c t="s" s="5" r="B10">
         <v>34</v>
       </c>
@@ -2828,7 +2855,7 @@
       </c>
     </row>
     <row r="11">
-      <c s="16" r="A11"/>
+      <c s="17" r="A11"/>
       <c t="s" s="5" r="B11">
         <v>38</v>
       </c>
@@ -2843,7 +2870,7 @@
       </c>
     </row>
     <row r="12">
-      <c s="16" r="A12"/>
+      <c s="17" r="A12"/>
       <c t="s" s="5" r="B12">
         <v>42</v>
       </c>
@@ -3068,14 +3095,14 @@
       </c>
     </row>
     <row r="27">
-      <c s="16" r="A27"/>
-      <c s="16" r="B27"/>
-      <c s="16" r="C27"/>
-      <c s="16" r="D27"/>
-      <c s="16" r="E27"/>
+      <c s="17" r="A27"/>
+      <c s="17" r="B27"/>
+      <c s="17" r="C27"/>
+      <c s="17" r="D27"/>
+      <c s="17" r="E27"/>
     </row>
     <row r="28">
-      <c t="s" s="16" r="A28">
+      <c t="s" s="17" r="A28">
         <v>101</v>
       </c>
       <c t="s" s="5" r="B28">
@@ -3092,7 +3119,7 @@
       </c>
     </row>
     <row r="29">
-      <c s="16" r="A29"/>
+      <c s="17" r="A29"/>
       <c t="s" s="5" r="B29">
         <v>106</v>
       </c>
@@ -3107,7 +3134,7 @@
       </c>
     </row>
     <row r="30">
-      <c s="16" r="A30"/>
+      <c s="17" r="A30"/>
       <c t="s" s="5" r="B30">
         <v>110</v>
       </c>
@@ -3122,7 +3149,7 @@
       </c>
     </row>
     <row r="31">
-      <c s="16" r="A31"/>
+      <c s="17" r="A31"/>
       <c t="s" s="5" r="B31">
         <v>114</v>
       </c>
@@ -3137,7 +3164,7 @@
       </c>
     </row>
     <row r="32">
-      <c s="16" r="A32"/>
+      <c s="17" r="A32"/>
       <c t="s" s="5" r="B32">
         <v>118</v>
       </c>
@@ -3189,7 +3216,7 @@
       <c s="9" r="E35"/>
     </row>
     <row r="36">
-      <c t="s" s="16" r="A36">
+      <c t="s" s="17" r="A36">
         <v>130</v>
       </c>
       <c t="s" s="12" r="B36">
@@ -3202,10 +3229,10 @@
       <c s="12" r="E36"/>
     </row>
     <row r="37">
-      <c s="16" r="A37"/>
-      <c s="16" r="B37"/>
-      <c s="16" r="C37"/>
-      <c s="16" r="D37"/>
+      <c s="17" r="A37"/>
+      <c s="17" r="B37"/>
+      <c s="17" r="C37"/>
+      <c s="17" r="D37"/>
       <c s="9" r="E37"/>
     </row>
     <row r="38">
@@ -3490,11 +3517,11 @@
       </c>
     </row>
     <row r="58">
-      <c s="16" r="A58"/>
-      <c s="16" r="B58"/>
-      <c s="16" r="C58"/>
-      <c s="16" r="D58"/>
-      <c s="16" r="E58"/>
+      <c s="17" r="A58"/>
+      <c s="17" r="B58"/>
+      <c s="17" r="C58"/>
+      <c s="17" r="D58"/>
+      <c s="17" r="E58"/>
     </row>
     <row r="59">
       <c t="s" s="9" r="A59">
@@ -4600,16 +4627,16 @@
     </row>
     <row r="135">
       <c s="7" r="A135"/>
-      <c t="s" s="18" r="B135">
+      <c t="s" s="19" r="B135">
         <v>485</v>
       </c>
       <c t="s" s="11" r="C135">
         <v>486</v>
       </c>
-      <c t="s" s="18" r="D135">
+      <c t="s" s="19" r="D135">
         <v>487</v>
       </c>
-      <c t="s" s="18" r="E135">
+      <c t="s" s="19" r="E135">
         <v>488</v>
       </c>
     </row>
@@ -4870,7 +4897,7 @@
     </row>
     <row r="153">
       <c s="7" r="A153"/>
-      <c t="s" s="21" r="B153">
+      <c t="s" s="22" r="B153">
         <v>556</v>
       </c>
       <c t="s" s="5" r="C153">
@@ -4885,10 +4912,10 @@
     </row>
     <row r="154">
       <c s="7" r="A154"/>
-      <c s="16" r="B154"/>
-      <c s="23" r="C154"/>
-      <c s="16" r="D154"/>
-      <c s="16" r="E154"/>
+      <c s="17" r="B154"/>
+      <c s="25" r="C154"/>
+      <c s="17" r="D154"/>
+      <c s="17" r="E154"/>
     </row>
     <row r="155">
       <c t="s" s="7" r="A155">
@@ -4969,10 +4996,10 @@
     </row>
     <row r="160">
       <c s="7" r="A160"/>
-      <c s="16" r="B160"/>
-      <c s="23" r="C160"/>
-      <c s="16" r="D160"/>
-      <c s="16" r="E160"/>
+      <c s="17" r="B160"/>
+      <c s="25" r="C160"/>
+      <c s="17" r="D160"/>
+      <c s="17" r="E160"/>
     </row>
     <row r="161">
       <c t="s" s="7" r="A161">
@@ -4981,7 +5008,7 @@
       <c t="s" s="24" r="B161">
         <v>582</v>
       </c>
-      <c t="s" s="17" r="C161">
+      <c t="s" s="18" r="C161">
         <v>581</v>
       </c>
       <c s="24" r="D161"/>
@@ -4998,25 +5025,25 @@
       <c t="s" s="7" r="A163">
         <v>583</v>
       </c>
-      <c t="s" s="27" r="B163">
+      <c t="s" s="28" r="B163">
         <v>584</v>
       </c>
-      <c t="s" s="25" r="C163">
+      <c t="s" s="26" r="C163">
         <v>585</v>
       </c>
-      <c s="27" r="D163"/>
-      <c s="27" r="E163"/>
+      <c s="28" r="D163"/>
+      <c s="28" r="E163"/>
     </row>
     <row r="164">
       <c s="7" r="A164"/>
-      <c t="s" s="27" r="B164">
+      <c t="s" s="28" r="B164">
         <v>586</v>
       </c>
-      <c t="s" s="25" r="C164">
+      <c t="s" s="26" r="C164">
         <v>587</v>
       </c>
-      <c s="27" r="D164"/>
-      <c s="27" r="E164"/>
+      <c s="28" r="D164"/>
+      <c s="28" r="E164"/>
     </row>
     <row r="165">
       <c s="7" r="A165"/>
@@ -5029,10 +5056,10 @@
       <c t="s" s="7" r="A166">
         <v>588</v>
       </c>
-      <c t="s" s="21" r="B166">
+      <c t="s" s="22" r="B166">
         <v>589</v>
       </c>
-      <c t="s" s="21" r="C166">
+      <c t="s" s="22" r="C166">
         <v>590</v>
       </c>
       <c t="s" s="5" r="D166">
@@ -5044,10 +5071,10 @@
     </row>
     <row r="167">
       <c s="7" r="A167"/>
-      <c t="s" s="21" r="B167">
+      <c t="s" s="22" r="B167">
         <v>593</v>
       </c>
-      <c t="s" s="21" r="C167">
+      <c t="s" s="22" r="C167">
         <v>594</v>
       </c>
       <c t="s" s="5" r="D167">
@@ -5059,10 +5086,10 @@
     </row>
     <row r="168">
       <c s="7" r="A168"/>
-      <c t="s" s="21" r="B168">
+      <c t="s" s="22" r="B168">
         <v>596</v>
       </c>
-      <c t="s" s="21" r="C168">
+      <c t="s" s="22" r="C168">
         <v>597</v>
       </c>
       <c t="s" s="5" r="D168">
@@ -5074,10 +5101,10 @@
     </row>
     <row r="169">
       <c s="7" r="A169"/>
-      <c t="s" s="21" r="B169">
+      <c t="s" s="22" r="B169">
         <v>600</v>
       </c>
-      <c t="s" s="21" r="C169">
+      <c t="s" s="22" r="C169">
         <v>601</v>
       </c>
       <c t="s" s="5" r="D169">
@@ -5285,7 +5312,7 @@
     <row r="183">
       <c s="7" r="A183"/>
       <c s="14" r="B183"/>
-      <c s="23" r="C183"/>
+      <c s="25" r="C183"/>
       <c s="14" r="D183"/>
       <c s="14" r="E183"/>
     </row>
@@ -5293,7 +5320,7 @@
       <c t="s" s="7" r="A184">
         <v>656</v>
       </c>
-      <c t="s" s="21" r="B184">
+      <c t="s" s="22" r="B184">
         <v>657</v>
       </c>
       <c t="s" s="5" r="C184">
@@ -5505,142 +5532,150 @@
     </row>
     <row r="199">
       <c s="7" r="A199"/>
-      <c s="9" r="B199"/>
-      <c s="13" r="C199"/>
-      <c s="9" r="D199"/>
-      <c s="9" r="E199"/>
+      <c t="s" s="5" r="B199">
+        <v>704</v>
+      </c>
+      <c t="s" s="11" r="C199">
+        <v>705</v>
+      </c>
+      <c t="s" s="16" r="D199">
+        <v>705</v>
+      </c>
+      <c t="s" s="16" r="E199">
+        <v>706</v>
+      </c>
     </row>
     <row r="200">
-      <c t="s" s="7" r="A200">
-        <v>704</v>
-      </c>
-      <c t="s" s="5" r="B200">
-        <v>705</v>
-      </c>
-      <c t="s" s="11" r="C200">
-        <v>706</v>
-      </c>
-      <c t="s" s="5" r="D200">
+      <c s="7" r="A200"/>
+      <c s="9" r="B200"/>
+      <c s="13" r="C200"/>
+      <c s="9" r="D200"/>
+      <c s="9" r="E200"/>
+    </row>
+    <row r="201">
+      <c t="s" s="7" r="A201">
         <v>707</v>
       </c>
-      <c t="s" s="5" r="E200">
+      <c t="s" s="5" r="B201">
         <v>708</v>
       </c>
-    </row>
-    <row r="201">
-      <c s="7" r="A201"/>
-      <c t="s" s="5" r="B201">
+      <c t="s" s="11" r="C201">
         <v>709</v>
       </c>
-      <c t="s" s="11" r="C201">
+      <c t="s" s="5" r="D201">
         <v>710</v>
       </c>
-      <c t="s" s="5" r="D201">
+      <c t="s" s="5" r="E201">
         <v>711</v>
-      </c>
-      <c t="s" s="5" r="E201">
-        <v>712</v>
       </c>
     </row>
     <row r="202">
       <c s="7" r="A202"/>
       <c t="s" s="5" r="B202">
+        <v>712</v>
+      </c>
+      <c t="s" s="11" r="C202">
         <v>713</v>
       </c>
-      <c t="s" s="11" r="C202">
+      <c t="s" s="5" r="D202">
         <v>714</v>
       </c>
-      <c t="s" s="5" r="D202">
+      <c t="s" s="5" r="E202">
         <v>715</v>
-      </c>
-      <c t="s" s="5" r="E202">
-        <v>716</v>
       </c>
     </row>
     <row r="203">
       <c s="7" r="A203"/>
       <c t="s" s="5" r="B203">
+        <v>716</v>
+      </c>
+      <c t="s" s="11" r="C203">
         <v>717</v>
       </c>
-      <c t="s" s="11" r="C203">
+      <c t="s" s="5" r="D203">
         <v>718</v>
       </c>
-      <c t="s" s="5" r="D203">
+      <c t="s" s="5" r="E203">
         <v>719</v>
-      </c>
-      <c t="s" s="5" r="E203">
-        <v>720</v>
       </c>
     </row>
     <row r="204">
       <c s="7" r="A204"/>
-      <c s="14" r="B204"/>
-      <c s="23" r="C204"/>
-      <c s="14" r="D204"/>
-      <c s="14" r="E204"/>
+      <c t="s" s="5" r="B204">
+        <v>720</v>
+      </c>
+      <c t="s" s="11" r="C204">
+        <v>721</v>
+      </c>
+      <c t="s" s="5" r="D204">
+        <v>722</v>
+      </c>
+      <c t="s" s="5" r="E204">
+        <v>723</v>
+      </c>
     </row>
     <row r="205">
-      <c t="s" s="7" r="A205">
-        <v>721</v>
-      </c>
-      <c t="s" s="5" r="B205">
-        <v>722</v>
-      </c>
-      <c t="s" s="11" r="C205">
-        <v>723</v>
-      </c>
-      <c t="s" s="5" r="D205">
+      <c s="7" r="A205"/>
+      <c s="14" r="B205"/>
+      <c s="25" r="C205"/>
+      <c s="14" r="D205"/>
+      <c s="14" r="E205"/>
+    </row>
+    <row r="206">
+      <c t="s" s="7" r="A206">
         <v>724</v>
       </c>
-      <c t="s" s="5" r="E205">
+      <c t="s" s="5" r="B206">
         <v>725</v>
       </c>
-    </row>
-    <row r="206">
-      <c s="7" r="A206"/>
-      <c t="s" s="5" r="B206">
+      <c t="s" s="11" r="C206">
         <v>726</v>
       </c>
-      <c t="s" s="11" r="C206">
+      <c t="s" s="5" r="D206">
         <v>727</v>
       </c>
-      <c t="s" s="5" r="D206">
+      <c t="s" s="5" r="E206">
         <v>728</v>
-      </c>
-      <c t="s" s="5" r="E206">
-        <v>729</v>
       </c>
     </row>
     <row r="207">
       <c s="7" r="A207"/>
-      <c s="14" r="B207"/>
-      <c s="23" r="C207"/>
-      <c s="14" r="D207"/>
-      <c s="14" r="E207"/>
+      <c t="s" s="5" r="B207">
+        <v>729</v>
+      </c>
+      <c t="s" s="11" r="C207">
+        <v>730</v>
+      </c>
+      <c t="s" s="5" r="D207">
+        <v>731</v>
+      </c>
+      <c t="s" s="5" r="E207">
+        <v>732</v>
+      </c>
     </row>
     <row r="208">
-      <c t="s" s="7" r="A208">
-        <v>730</v>
-      </c>
-      <c t="s" s="5" r="B208">
-        <v>731</v>
-      </c>
-      <c t="s" s="11" r="C208">
-        <v>732</v>
-      </c>
-      <c t="s" s="5" r="D208">
+      <c s="7" r="A208"/>
+      <c s="14" r="B208"/>
+      <c s="25" r="C208"/>
+      <c s="14" r="D208"/>
+      <c s="14" r="E208"/>
+    </row>
+    <row r="209">
+      <c t="s" s="7" r="A209">
         <v>733</v>
       </c>
-      <c t="s" s="5" r="E208">
+      <c t="s" s="5" r="B209">
         <v>734</v>
       </c>
-    </row>
-    <row r="209">
-      <c s="7" r="A209"/>
-      <c s="14" r="B209"/>
-      <c s="6" r="C209"/>
-      <c s="14" r="D209"/>
-      <c s="14" r="E209"/>
+      <c t="s" s="11" r="C209">
+        <v>735</v>
+      </c>
+      <c t="s" s="5" r="D209">
+        <v>736</v>
+      </c>
+      <c t="s" s="5" r="E209">
+        <v>737</v>
+      </c>
     </row>
     <row r="210">
       <c s="7" r="A210"/>
@@ -5676,6 +5711,13 @@
       <c s="6" r="C214"/>
       <c s="14" r="D214"/>
       <c s="14" r="E214"/>
+    </row>
+    <row r="215">
+      <c s="7" r="A215"/>
+      <c s="14" r="B215"/>
+      <c s="6" r="C215"/>
+      <c s="14" r="D215"/>
+      <c s="14" r="E215"/>
     </row>
   </sheetData>
 </worksheet>
@@ -5693,17 +5735,17 @@
   <sheetData>
     <row customHeight="1" r="1" ht="112.5">
       <c t="s" s="2" r="A1">
-        <v>735</v>
+        <v>738</v>
       </c>
     </row>
     <row customHeight="1" r="2" ht="112.5">
       <c t="s" s="3" r="A2">
-        <v>736</v>
+        <v>739</v>
       </c>
     </row>
     <row customHeight="1" r="3" ht="112.5">
       <c t="s" s="8" r="A3">
-        <v>737</v>
+        <v>740</v>
       </c>
     </row>
   </sheetData>
@@ -5718,164 +5760,164 @@
   <sheetFormatPr customHeight="1" defaultColWidth="9.86" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c s="26" r="A1"/>
-      <c s="26" r="B1"/>
-      <c s="26" r="C1"/>
-      <c s="26" r="D1"/>
-      <c s="26" r="E1"/>
-      <c s="26" r="F1"/>
+      <c s="27" r="A1"/>
+      <c s="27" r="B1"/>
+      <c s="27" r="C1"/>
+      <c s="27" r="D1"/>
+      <c s="27" r="E1"/>
+      <c s="27" r="F1"/>
     </row>
     <row r="2">
-      <c s="26" r="A2"/>
-      <c s="26" r="B2"/>
-      <c s="26" r="C2"/>
-      <c s="26" r="D2"/>
-      <c s="26" r="E2"/>
-      <c s="26" r="F2"/>
+      <c s="27" r="A2"/>
+      <c s="27" r="B2"/>
+      <c s="27" r="C2"/>
+      <c s="27" r="D2"/>
+      <c s="27" r="E2"/>
+      <c s="27" r="F2"/>
     </row>
     <row r="3">
-      <c s="26" r="A3"/>
-      <c s="26" r="B3"/>
-      <c s="26" r="C3"/>
-      <c s="26" r="D3"/>
-      <c s="26" r="E3"/>
-      <c s="26" r="F3"/>
+      <c s="27" r="A3"/>
+      <c s="27" r="B3"/>
+      <c s="27" r="C3"/>
+      <c s="27" r="D3"/>
+      <c s="27" r="E3"/>
+      <c s="27" r="F3"/>
     </row>
     <row r="4">
-      <c s="26" r="A4"/>
-      <c s="26" r="B4"/>
-      <c s="26" r="C4"/>
-      <c s="26" r="D4"/>
-      <c s="26" r="E4"/>
-      <c s="26" r="F4"/>
+      <c s="27" r="A4"/>
+      <c s="27" r="B4"/>
+      <c s="27" r="C4"/>
+      <c s="27" r="D4"/>
+      <c s="27" r="E4"/>
+      <c s="27" r="F4"/>
     </row>
     <row r="5">
-      <c s="26" r="A5"/>
-      <c s="26" r="B5"/>
-      <c s="26" r="C5"/>
-      <c s="26" r="D5"/>
-      <c s="26" r="E5"/>
-      <c s="26" r="F5"/>
+      <c s="27" r="A5"/>
+      <c s="27" r="B5"/>
+      <c s="27" r="C5"/>
+      <c s="27" r="D5"/>
+      <c s="27" r="E5"/>
+      <c s="27" r="F5"/>
     </row>
     <row r="6">
-      <c s="26" r="A6"/>
-      <c s="26" r="B6"/>
-      <c s="26" r="C6"/>
-      <c s="26" r="D6"/>
-      <c s="26" r="E6"/>
-      <c s="26" r="F6"/>
+      <c s="27" r="A6"/>
+      <c s="27" r="B6"/>
+      <c s="27" r="C6"/>
+      <c s="27" r="D6"/>
+      <c s="27" r="E6"/>
+      <c s="27" r="F6"/>
     </row>
     <row r="7">
-      <c s="26" r="A7"/>
-      <c s="26" r="B7"/>
-      <c s="26" r="C7"/>
-      <c s="26" r="D7"/>
-      <c s="26" r="E7"/>
-      <c s="26" r="F7"/>
+      <c s="27" r="A7"/>
+      <c s="27" r="B7"/>
+      <c s="27" r="C7"/>
+      <c s="27" r="D7"/>
+      <c s="27" r="E7"/>
+      <c s="27" r="F7"/>
     </row>
     <row r="8">
-      <c s="26" r="A8"/>
-      <c s="26" r="B8"/>
-      <c s="26" r="C8"/>
-      <c s="26" r="D8"/>
-      <c s="26" r="E8"/>
-      <c s="26" r="F8"/>
+      <c s="27" r="A8"/>
+      <c s="27" r="B8"/>
+      <c s="27" r="C8"/>
+      <c s="27" r="D8"/>
+      <c s="27" r="E8"/>
+      <c s="27" r="F8"/>
     </row>
     <row r="9">
-      <c s="26" r="A9"/>
-      <c s="26" r="B9"/>
-      <c s="26" r="C9"/>
-      <c s="26" r="D9"/>
-      <c s="26" r="E9"/>
-      <c s="26" r="F9"/>
+      <c s="27" r="A9"/>
+      <c s="27" r="B9"/>
+      <c s="27" r="C9"/>
+      <c s="27" r="D9"/>
+      <c s="27" r="E9"/>
+      <c s="27" r="F9"/>
     </row>
     <row r="10">
-      <c s="26" r="A10"/>
-      <c s="26" r="B10"/>
-      <c s="26" r="C10"/>
-      <c s="26" r="D10"/>
-      <c s="26" r="E10"/>
-      <c s="26" r="F10"/>
+      <c s="27" r="A10"/>
+      <c s="27" r="B10"/>
+      <c s="27" r="C10"/>
+      <c s="27" r="D10"/>
+      <c s="27" r="E10"/>
+      <c s="27" r="F10"/>
     </row>
     <row r="11">
-      <c s="26" r="A11"/>
-      <c s="26" r="B11"/>
-      <c s="26" r="C11"/>
-      <c s="26" r="D11"/>
-      <c s="26" r="E11"/>
-      <c s="26" r="F11"/>
+      <c s="27" r="A11"/>
+      <c s="27" r="B11"/>
+      <c s="27" r="C11"/>
+      <c s="27" r="D11"/>
+      <c s="27" r="E11"/>
+      <c s="27" r="F11"/>
     </row>
     <row r="12">
-      <c s="26" r="A12"/>
-      <c s="26" r="B12"/>
-      <c s="26" r="C12"/>
-      <c s="26" r="D12"/>
-      <c s="26" r="E12"/>
-      <c s="26" r="F12"/>
+      <c s="27" r="A12"/>
+      <c s="27" r="B12"/>
+      <c s="27" r="C12"/>
+      <c s="27" r="D12"/>
+      <c s="27" r="E12"/>
+      <c s="27" r="F12"/>
     </row>
     <row r="13">
-      <c s="26" r="A13"/>
-      <c s="26" r="B13"/>
-      <c s="26" r="C13"/>
-      <c s="26" r="D13"/>
-      <c s="26" r="E13"/>
-      <c s="26" r="F13"/>
+      <c s="27" r="A13"/>
+      <c s="27" r="B13"/>
+      <c s="27" r="C13"/>
+      <c s="27" r="D13"/>
+      <c s="27" r="E13"/>
+      <c s="27" r="F13"/>
     </row>
     <row r="14">
-      <c s="26" r="A14"/>
-      <c s="26" r="B14"/>
-      <c s="26" r="C14"/>
-      <c s="26" r="D14"/>
-      <c s="26" r="E14"/>
-      <c s="26" r="F14"/>
+      <c s="27" r="A14"/>
+      <c s="27" r="B14"/>
+      <c s="27" r="C14"/>
+      <c s="27" r="D14"/>
+      <c s="27" r="E14"/>
+      <c s="27" r="F14"/>
     </row>
     <row r="15">
-      <c s="26" r="A15"/>
-      <c s="26" r="B15"/>
-      <c s="26" r="C15"/>
-      <c s="26" r="D15"/>
-      <c s="26" r="E15"/>
-      <c s="26" r="F15"/>
+      <c s="27" r="A15"/>
+      <c s="27" r="B15"/>
+      <c s="27" r="C15"/>
+      <c s="27" r="D15"/>
+      <c s="27" r="E15"/>
+      <c s="27" r="F15"/>
     </row>
     <row r="16">
-      <c s="26" r="A16"/>
-      <c s="26" r="B16"/>
-      <c s="26" r="C16"/>
-      <c s="26" r="D16"/>
-      <c s="26" r="E16"/>
-      <c s="26" r="F16"/>
+      <c s="27" r="A16"/>
+      <c s="27" r="B16"/>
+      <c s="27" r="C16"/>
+      <c s="27" r="D16"/>
+      <c s="27" r="E16"/>
+      <c s="27" r="F16"/>
     </row>
     <row r="17">
-      <c s="26" r="A17"/>
-      <c s="26" r="B17"/>
-      <c s="26" r="C17"/>
-      <c s="26" r="D17"/>
-      <c s="26" r="E17"/>
-      <c s="26" r="F17"/>
+      <c s="27" r="A17"/>
+      <c s="27" r="B17"/>
+      <c s="27" r="C17"/>
+      <c s="27" r="D17"/>
+      <c s="27" r="E17"/>
+      <c s="27" r="F17"/>
     </row>
     <row r="18">
-      <c s="26" r="A18"/>
-      <c s="26" r="B18"/>
-      <c s="26" r="C18"/>
-      <c s="26" r="D18"/>
-      <c s="26" r="E18"/>
-      <c s="26" r="F18"/>
+      <c s="27" r="A18"/>
+      <c s="27" r="B18"/>
+      <c s="27" r="C18"/>
+      <c s="27" r="D18"/>
+      <c s="27" r="E18"/>
+      <c s="27" r="F18"/>
     </row>
     <row r="19">
-      <c s="26" r="A19"/>
-      <c s="26" r="B19"/>
-      <c s="26" r="C19"/>
-      <c s="26" r="D19"/>
-      <c s="26" r="E19"/>
-      <c s="26" r="F19"/>
+      <c s="27" r="A19"/>
+      <c s="27" r="B19"/>
+      <c s="27" r="C19"/>
+      <c s="27" r="D19"/>
+      <c s="27" r="E19"/>
+      <c s="27" r="F19"/>
     </row>
     <row r="20">
-      <c s="26" r="A20"/>
-      <c s="26" r="B20"/>
-      <c s="26" r="C20"/>
-      <c s="26" r="D20"/>
-      <c s="26" r="E20"/>
-      <c s="26" r="F20"/>
+      <c s="27" r="A20"/>
+      <c s="27" r="B20"/>
+      <c s="27" r="C20"/>
+      <c s="27" r="D20"/>
+      <c s="27" r="E20"/>
+      <c s="27" r="F20"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
EWD-22567 - Help hint area and button
Former-commit-id: 1fb52bfbb3b49e5f9c6a3e3d6867f7becf84b85e
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="815">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="817">
   <si>
     <t>Page</t>
   </si>
@@ -2256,6 +2256,12 @@
   </si>
   <si>
     <t>Learning object was not found. Please refresh your data.</t>
+  </si>
+  <si>
+    <t>helpHintNotFoundError</t>
+  </si>
+  <si>
+    <t>Help hint was not found. Please refresh your data.</t>
   </si>
   <si>
     <t>View captions</t>
@@ -2603,7 +2609,7 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <b val="0"/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
@@ -2612,7 +2618,7 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="0"/>
+      <b/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
@@ -2666,7 +2672,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="23">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2767,6 +2773,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF999999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF00FF00"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2814,7 +2826,7 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
@@ -2870,32 +2882,35 @@
     <xf applyAlignment="1" fillId="15" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="14" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="15">
+    <xf applyAlignment="1" fillId="16" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="15" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="16" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="16" applyFill="1">
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="16">
+      <alignment vertical="center" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="17" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="17">
       <alignment vertical="bottom" horizontal="right"/>
     </xf>
-    <xf applyAlignment="1" fillId="17" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+    <xf applyAlignment="1" fillId="18" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="18" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="18" applyFill="1">
+    <xf applyAlignment="1" fillId="19" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="18" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="19" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+    <xf applyAlignment="1" fillId="20" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="20" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="19" applyFill="1">
+    <xf applyAlignment="1" fillId="21" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="19" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="21" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+    <xf applyAlignment="1" fillId="22" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
     <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="20"/>
-    <xf applyAlignment="1" fillId="22" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="21" applyFill="1">
+    <xf applyAlignment="1" fillId="23" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="21" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2923,19 +2938,19 @@
   </cols>
   <sheetData>
     <row s="4" customFormat="1" r="1">
-      <c t="s" s="23" r="A1">
+      <c t="s" s="24" r="A1">
         <v>0</v>
       </c>
-      <c t="s" s="23" r="B1">
+      <c t="s" s="24" r="B1">
         <v>1</v>
       </c>
-      <c t="s" s="23" r="C1">
+      <c t="s" s="24" r="C1">
         <v>2</v>
       </c>
-      <c t="s" s="23" r="D1">
+      <c t="s" s="24" r="D1">
         <v>3</v>
       </c>
-      <c t="s" s="19" r="E1">
+      <c t="s" s="20" r="E1">
         <v>4</v>
       </c>
     </row>
@@ -3749,47 +3764,47 @@
       <c t="s" s="9" r="A59">
         <v>207</v>
       </c>
-      <c t="s" s="25" r="B59">
+      <c t="s" s="26" r="B59">
         <v>208</v>
       </c>
-      <c t="s" s="25" r="C59">
+      <c t="s" s="26" r="C59">
         <v>209</v>
       </c>
-      <c s="25" r="D59"/>
-      <c s="25" r="E59"/>
+      <c s="26" r="D59"/>
+      <c s="26" r="E59"/>
     </row>
     <row r="60">
       <c s="9" r="A60"/>
-      <c t="s" s="25" r="B60">
+      <c t="s" s="26" r="B60">
         <v>210</v>
       </c>
-      <c t="s" s="25" r="C60">
+      <c t="s" s="26" r="C60">
         <v>211</v>
       </c>
-      <c s="25" r="D60"/>
-      <c s="25" r="E60"/>
+      <c s="26" r="D60"/>
+      <c s="26" r="E60"/>
     </row>
     <row r="61">
       <c s="9" r="A61"/>
-      <c t="s" s="25" r="B61">
+      <c t="s" s="26" r="B61">
         <v>212</v>
       </c>
-      <c t="s" s="25" r="C61">
+      <c t="s" s="26" r="C61">
         <v>213</v>
       </c>
-      <c s="25" r="D61"/>
-      <c s="25" r="E61"/>
+      <c s="26" r="D61"/>
+      <c s="26" r="E61"/>
     </row>
     <row r="62">
       <c s="9" r="A62"/>
-      <c t="s" s="25" r="B62">
+      <c t="s" s="26" r="B62">
         <v>214</v>
       </c>
-      <c t="s" s="25" r="C62">
+      <c t="s" s="26" r="C62">
         <v>215</v>
       </c>
-      <c s="25" r="D62"/>
-      <c s="25" r="E62"/>
+      <c s="26" r="D62"/>
+      <c s="26" r="E62"/>
     </row>
     <row r="63">
       <c s="9" r="A63"/>
@@ -4252,8 +4267,8 @@
       <c t="s" s="5" r="C94">
         <v>335</v>
       </c>
-      <c s="20" r="D94"/>
-      <c s="20" r="E94"/>
+      <c s="19" r="D94"/>
+      <c s="19" r="E94"/>
     </row>
     <row r="95">
       <c s="7" r="A95"/>
@@ -5131,7 +5146,7 @@
     <row r="154">
       <c s="7" r="A154"/>
       <c s="16" r="B154"/>
-      <c s="24" r="C154"/>
+      <c s="25" r="C154"/>
       <c s="16" r="D154"/>
       <c s="16" r="E154"/>
     </row>
@@ -5215,7 +5230,7 @@
     <row r="160">
       <c s="7" r="A160"/>
       <c s="16" r="B160"/>
-      <c s="24" r="C160"/>
+      <c s="25" r="C160"/>
       <c s="16" r="D160"/>
       <c s="16" r="E160"/>
     </row>
@@ -5223,14 +5238,14 @@
       <c t="s" s="7" r="A161">
         <v>579</v>
       </c>
-      <c t="s" s="25" r="B161">
+      <c t="s" s="26" r="B161">
         <v>580</v>
       </c>
       <c t="s" s="17" r="C161">
         <v>579</v>
       </c>
-      <c s="25" r="D161"/>
-      <c s="25" r="E161"/>
+      <c s="26" r="D161"/>
+      <c s="26" r="E161"/>
     </row>
     <row r="162">
       <c s="7" r="A162"/>
@@ -5243,25 +5258,25 @@
       <c t="s" s="7" r="A163">
         <v>581</v>
       </c>
-      <c t="s" s="28" r="B163">
+      <c t="s" s="29" r="B163">
         <v>582</v>
       </c>
-      <c t="s" s="26" r="C163">
+      <c t="s" s="27" r="C163">
         <v>583</v>
       </c>
-      <c s="28" r="D163"/>
-      <c s="28" r="E163"/>
+      <c s="29" r="D163"/>
+      <c s="29" r="E163"/>
     </row>
     <row r="164">
       <c s="7" r="A164"/>
-      <c t="s" s="28" r="B164">
+      <c t="s" s="29" r="B164">
         <v>584</v>
       </c>
-      <c t="s" s="26" r="C164">
+      <c t="s" s="27" r="C164">
         <v>585</v>
       </c>
-      <c s="28" r="D164"/>
-      <c s="28" r="E164"/>
+      <c s="29" r="D164"/>
+      <c s="29" r="E164"/>
     </row>
     <row r="165">
       <c s="7" r="A165"/>
@@ -5274,10 +5289,10 @@
       <c t="s" s="7" r="A166">
         <v>586</v>
       </c>
-      <c t="s" s="22" r="B166">
+      <c t="s" s="23" r="B166">
         <v>587</v>
       </c>
-      <c t="s" s="22" r="C166">
+      <c t="s" s="23" r="C166">
         <v>588</v>
       </c>
       <c t="s" s="5" r="D166">
@@ -5289,10 +5304,10 @@
     </row>
     <row r="167">
       <c s="7" r="A167"/>
-      <c t="s" s="22" r="B167">
+      <c t="s" s="23" r="B167">
         <v>591</v>
       </c>
-      <c t="s" s="22" r="C167">
+      <c t="s" s="23" r="C167">
         <v>592</v>
       </c>
       <c t="s" s="5" r="D167">
@@ -5304,10 +5319,10 @@
     </row>
     <row r="168">
       <c s="7" r="A168"/>
-      <c t="s" s="22" r="B168">
+      <c t="s" s="23" r="B168">
         <v>594</v>
       </c>
-      <c t="s" s="22" r="C168">
+      <c t="s" s="23" r="C168">
         <v>595</v>
       </c>
       <c t="s" s="5" r="D168">
@@ -5319,10 +5334,10 @@
     </row>
     <row r="169">
       <c s="7" r="A169"/>
-      <c t="s" s="22" r="B169">
+      <c t="s" s="23" r="B169">
         <v>598</v>
       </c>
-      <c t="s" s="22" r="C169">
+      <c t="s" s="23" r="C169">
         <v>599</v>
       </c>
       <c t="s" s="5" r="D169">
@@ -5530,7 +5545,7 @@
     <row r="183">
       <c s="7" r="A183"/>
       <c s="14" r="B183"/>
-      <c s="24" r="C183"/>
+      <c s="25" r="C183"/>
       <c s="14" r="D183"/>
       <c s="14" r="E183"/>
     </row>
@@ -5538,7 +5553,7 @@
       <c t="s" s="7" r="A184">
         <v>654</v>
       </c>
-      <c t="s" s="22" r="B184">
+      <c t="s" s="23" r="B184">
         <v>655</v>
       </c>
       <c t="s" s="5" r="C184">
@@ -5835,7 +5850,7 @@
     <row r="205">
       <c s="7" r="A205"/>
       <c s="14" r="B205"/>
-      <c s="24" r="C205"/>
+      <c s="25" r="C205"/>
       <c s="14" r="D205"/>
       <c s="14" r="E205"/>
     </row>
@@ -5874,7 +5889,7 @@
     <row r="208">
       <c s="7" r="A208"/>
       <c s="14" r="B208"/>
-      <c s="24" r="C208"/>
+      <c s="25" r="C208"/>
       <c s="14" r="D208"/>
       <c s="14" r="E208"/>
     </row>
@@ -5912,8 +5927,8 @@
       <c t="s" s="11" r="C211">
         <v>738</v>
       </c>
-      <c s="20" r="D211"/>
-      <c s="20" r="E211"/>
+      <c s="19" r="D211"/>
+      <c s="19" r="E211"/>
     </row>
     <row r="212">
       <c s="7" r="A212"/>
@@ -5923,8 +5938,8 @@
       <c t="s" s="11" r="C212">
         <v>740</v>
       </c>
-      <c s="20" r="D212"/>
-      <c s="20" r="E212"/>
+      <c s="19" r="D212"/>
+      <c s="19" r="E212"/>
     </row>
     <row r="213">
       <c s="7" r="A213"/>
@@ -5934,8 +5949,8 @@
       <c t="s" s="11" r="C213">
         <v>742</v>
       </c>
-      <c s="20" r="D213"/>
-      <c s="20" r="E213"/>
+      <c s="19" r="D213"/>
+      <c s="19" r="E213"/>
     </row>
     <row r="214">
       <c s="7" r="A214"/>
@@ -5945,8 +5960,8 @@
       <c t="s" s="11" r="C214">
         <v>744</v>
       </c>
-      <c s="20" r="D214"/>
-      <c s="20" r="E214"/>
+      <c s="19" r="D214"/>
+      <c s="19" r="E214"/>
     </row>
     <row r="215">
       <c s="7" r="A215"/>
@@ -5956,43 +5971,43 @@
       <c t="s" s="11" r="C215">
         <v>746</v>
       </c>
-      <c s="20" r="D215"/>
-      <c s="20" r="E215"/>
+      <c s="19" r="D215"/>
+      <c s="19" r="E215"/>
     </row>
     <row r="216">
-      <c s="15" r="A216"/>
-      <c s="14" r="B216"/>
-      <c s="6" r="C216"/>
-      <c s="14" r="D216"/>
-      <c s="14" r="E216"/>
+      <c s="7" r="A216"/>
+      <c t="s" s="5" r="B216">
+        <v>747</v>
+      </c>
+      <c t="s" s="11" r="C216">
+        <v>748</v>
+      </c>
+      <c s="19" r="D216"/>
+      <c s="19" r="E216"/>
     </row>
     <row r="217">
-      <c t="s" s="7" r="A217">
-        <v>747</v>
-      </c>
-      <c t="s" s="5" r="B217">
-        <v>748</v>
-      </c>
-      <c t="s" s="5" r="C217">
+      <c s="15" r="A217"/>
+      <c s="14" r="B217"/>
+      <c s="6" r="C217"/>
+      <c s="14" r="D217"/>
+      <c s="14" r="E217"/>
+    </row>
+    <row r="218">
+      <c t="s" s="7" r="A218">
         <v>749</v>
       </c>
-      <c t="s" s="5" r="D217">
+      <c t="s" s="5" r="B218">
         <v>750</v>
       </c>
-      <c t="s" s="5" r="E217">
+      <c t="s" s="5" r="C218">
         <v>751</v>
       </c>
-    </row>
-    <row r="218">
-      <c s="7" r="A218"/>
-      <c t="s" s="5" r="B218">
+      <c t="s" s="5" r="D218">
         <v>752</v>
       </c>
-      <c t="s" s="11" r="C218">
+      <c t="s" s="5" r="E218">
         <v>753</v>
       </c>
-      <c s="20" r="D218"/>
-      <c s="20" r="E218"/>
     </row>
     <row r="219">
       <c s="7" r="A219"/>
@@ -6002,8 +6017,8 @@
       <c t="s" s="11" r="C219">
         <v>755</v>
       </c>
-      <c s="20" r="D219"/>
-      <c s="20" r="E219"/>
+      <c s="19" r="D219"/>
+      <c s="19" r="E219"/>
     </row>
     <row r="220">
       <c s="7" r="A220"/>
@@ -6013,8 +6028,8 @@
       <c t="s" s="11" r="C220">
         <v>757</v>
       </c>
-      <c s="20" r="D220"/>
-      <c s="20" r="E220"/>
+      <c s="19" r="D220"/>
+      <c s="19" r="E220"/>
     </row>
     <row r="221">
       <c s="7" r="A221"/>
@@ -6022,52 +6037,52 @@
         <v>758</v>
       </c>
       <c t="s" s="11" r="C221">
-        <v>528</v>
-      </c>
-      <c s="20" r="D221"/>
-      <c s="20" r="E221"/>
+        <v>759</v>
+      </c>
+      <c s="19" r="D221"/>
+      <c s="19" r="E221"/>
     </row>
     <row r="222">
       <c s="7" r="A222"/>
       <c t="s" s="5" r="B222">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c t="s" s="11" r="C222">
-        <v>760</v>
-      </c>
-      <c s="20" r="D222"/>
-      <c s="20" r="E222"/>
+        <v>528</v>
+      </c>
+      <c s="19" r="D222"/>
+      <c s="19" r="E222"/>
     </row>
     <row r="223">
-      <c s="15" r="A223"/>
-      <c s="14" r="B223"/>
-      <c s="6" r="C223"/>
-      <c s="14" r="D223"/>
-      <c s="14" r="E223"/>
+      <c s="7" r="A223"/>
+      <c t="s" s="5" r="B223">
+        <v>761</v>
+      </c>
+      <c t="s" s="11" r="C223">
+        <v>762</v>
+      </c>
+      <c s="19" r="D223"/>
+      <c s="19" r="E223"/>
     </row>
     <row r="224">
-      <c t="s" s="7" r="A224">
-        <v>761</v>
-      </c>
-      <c t="s" s="5" r="B224">
-        <v>762</v>
-      </c>
-      <c t="s" s="11" r="C224">
+      <c s="15" r="A224"/>
+      <c s="14" r="B224"/>
+      <c s="6" r="C224"/>
+      <c s="14" r="D224"/>
+      <c s="14" r="E224"/>
+    </row>
+    <row r="225">
+      <c t="s" s="7" r="A225">
         <v>763</v>
       </c>
-      <c s="20" r="D224"/>
-      <c s="20" r="E224"/>
-    </row>
-    <row r="225">
-      <c s="7" r="A225"/>
       <c t="s" s="5" r="B225">
         <v>764</v>
       </c>
       <c t="s" s="11" r="C225">
         <v>765</v>
       </c>
-      <c s="20" r="D225"/>
-      <c s="20" r="E225"/>
+      <c s="19" r="D225"/>
+      <c s="19" r="E225"/>
     </row>
     <row r="226">
       <c s="7" r="A226"/>
@@ -6077,8 +6092,8 @@
       <c t="s" s="11" r="C226">
         <v>767</v>
       </c>
-      <c s="20" r="D226"/>
-      <c s="20" r="E226"/>
+      <c s="19" r="D226"/>
+      <c s="19" r="E226"/>
     </row>
     <row r="227">
       <c s="7" r="A227"/>
@@ -6088,8 +6103,8 @@
       <c t="s" s="11" r="C227">
         <v>769</v>
       </c>
-      <c s="20" r="D227"/>
-      <c s="20" r="E227"/>
+      <c s="19" r="D227"/>
+      <c s="19" r="E227"/>
     </row>
     <row r="228">
       <c s="7" r="A228"/>
@@ -6099,8 +6114,8 @@
       <c t="s" s="11" r="C228">
         <v>771</v>
       </c>
-      <c s="20" r="D228"/>
-      <c s="20" r="E228"/>
+      <c s="19" r="D228"/>
+      <c s="19" r="E228"/>
     </row>
     <row r="229">
       <c s="7" r="A229"/>
@@ -6110,8 +6125,8 @@
       <c t="s" s="11" r="C229">
         <v>773</v>
       </c>
-      <c s="20" r="D229"/>
-      <c s="20" r="E229"/>
+      <c s="19" r="D229"/>
+      <c s="19" r="E229"/>
     </row>
     <row r="230">
       <c s="7" r="A230"/>
@@ -6121,8 +6136,8 @@
       <c t="s" s="11" r="C230">
         <v>775</v>
       </c>
-      <c s="20" r="D230"/>
-      <c s="20" r="E230"/>
+      <c s="19" r="D230"/>
+      <c s="19" r="E230"/>
     </row>
     <row r="231">
       <c s="7" r="A231"/>
@@ -6132,8 +6147,8 @@
       <c t="s" s="11" r="C231">
         <v>777</v>
       </c>
-      <c s="20" r="D231"/>
-      <c s="20" r="E231"/>
+      <c s="19" r="D231"/>
+      <c s="19" r="E231"/>
     </row>
     <row r="232">
       <c s="7" r="A232"/>
@@ -6143,8 +6158,8 @@
       <c t="s" s="11" r="C232">
         <v>779</v>
       </c>
-      <c s="20" r="D232"/>
-      <c s="20" r="E232"/>
+      <c s="19" r="D232"/>
+      <c s="19" r="E232"/>
     </row>
     <row r="233">
       <c s="7" r="A233"/>
@@ -6154,8 +6169,8 @@
       <c t="s" s="11" r="C233">
         <v>781</v>
       </c>
-      <c s="20" r="D233"/>
-      <c s="20" r="E233"/>
+      <c s="19" r="D233"/>
+      <c s="19" r="E233"/>
     </row>
     <row r="234">
       <c s="7" r="A234"/>
@@ -6165,8 +6180,8 @@
       <c t="s" s="11" r="C234">
         <v>783</v>
       </c>
-      <c s="20" r="D234"/>
-      <c s="20" r="E234"/>
+      <c s="19" r="D234"/>
+      <c s="19" r="E234"/>
     </row>
     <row r="235">
       <c s="7" r="A235"/>
@@ -6176,8 +6191,8 @@
       <c t="s" s="11" r="C235">
         <v>785</v>
       </c>
-      <c s="20" r="D235"/>
-      <c s="20" r="E235"/>
+      <c s="19" r="D235"/>
+      <c s="19" r="E235"/>
     </row>
     <row r="236">
       <c s="7" r="A236"/>
@@ -6187,8 +6202,8 @@
       <c t="s" s="11" r="C236">
         <v>787</v>
       </c>
-      <c s="20" r="D236"/>
-      <c s="20" r="E236"/>
+      <c s="19" r="D236"/>
+      <c s="19" r="E236"/>
     </row>
     <row r="237">
       <c s="7" r="A237"/>
@@ -6198,8 +6213,8 @@
       <c t="s" s="11" r="C237">
         <v>789</v>
       </c>
-      <c s="20" r="D237"/>
-      <c s="20" r="E237"/>
+      <c s="19" r="D237"/>
+      <c s="19" r="E237"/>
     </row>
     <row r="238">
       <c s="7" r="A238"/>
@@ -6209,8 +6224,8 @@
       <c t="s" s="11" r="C238">
         <v>791</v>
       </c>
-      <c s="20" r="D238"/>
-      <c s="20" r="E238"/>
+      <c s="19" r="D238"/>
+      <c s="19" r="E238"/>
     </row>
     <row r="239">
       <c s="7" r="A239"/>
@@ -6220,8 +6235,8 @@
       <c t="s" s="11" r="C239">
         <v>793</v>
       </c>
-      <c s="20" r="D239"/>
-      <c s="20" r="E239"/>
+      <c s="19" r="D239"/>
+      <c s="19" r="E239"/>
     </row>
     <row r="240">
       <c s="7" r="A240"/>
@@ -6231,8 +6246,8 @@
       <c t="s" s="11" r="C240">
         <v>795</v>
       </c>
-      <c s="20" r="D240"/>
-      <c s="20" r="E240"/>
+      <c s="19" r="D240"/>
+      <c s="19" r="E240"/>
     </row>
     <row r="241">
       <c s="7" r="A241"/>
@@ -6242,8 +6257,8 @@
       <c t="s" s="11" r="C241">
         <v>797</v>
       </c>
-      <c s="20" r="D241"/>
-      <c s="20" r="E241"/>
+      <c s="19" r="D241"/>
+      <c s="19" r="E241"/>
     </row>
     <row r="242">
       <c s="7" r="A242"/>
@@ -6253,8 +6268,8 @@
       <c t="s" s="11" r="C242">
         <v>799</v>
       </c>
-      <c s="20" r="D242"/>
-      <c s="20" r="E242"/>
+      <c s="19" r="D242"/>
+      <c s="19" r="E242"/>
     </row>
     <row r="243">
       <c s="7" r="A243"/>
@@ -6264,112 +6279,116 @@
       <c t="s" s="11" r="C243">
         <v>801</v>
       </c>
-      <c s="20" r="D243"/>
-      <c s="20" r="E243"/>
+      <c s="19" r="D243"/>
+      <c s="19" r="E243"/>
     </row>
     <row r="244">
       <c s="7" r="A244"/>
-      <c s="14" r="B244"/>
-      <c s="6" r="C244"/>
-      <c s="14" r="D244"/>
-      <c s="14" r="E244"/>
+      <c t="s" s="5" r="B244">
+        <v>802</v>
+      </c>
+      <c t="s" s="11" r="C244">
+        <v>803</v>
+      </c>
+      <c s="19" r="D244"/>
+      <c s="19" r="E244"/>
     </row>
     <row r="245">
-      <c t="s" s="7" r="A245">
-        <v>802</v>
-      </c>
-      <c t="s" s="14" r="B245">
-        <v>803</v>
-      </c>
-      <c t="s" s="6" r="C245">
-        <v>804</v>
-      </c>
+      <c s="7" r="A245"/>
+      <c s="14" r="B245"/>
+      <c s="6" r="C245"/>
       <c s="14" r="D245"/>
       <c s="14" r="E245"/>
     </row>
     <row r="246">
-      <c s="7" r="A246"/>
-      <c t="s" s="14" r="B246">
+      <c t="s" s="15" r="A246">
+        <v>804</v>
+      </c>
+      <c t="s" s="12" r="B246">
         <v>805</v>
       </c>
-      <c t="s" s="6" r="C246">
-        <v>804</v>
-      </c>
-      <c s="14" r="D246"/>
-      <c s="14" r="E246"/>
+      <c t="s" s="21" r="C246">
+        <v>806</v>
+      </c>
+      <c s="12" r="D246"/>
+      <c s="12" r="E246"/>
     </row>
     <row r="247">
-      <c s="7" r="A247"/>
-      <c t="s" s="14" r="B247">
+      <c s="15" r="A247"/>
+      <c t="s" s="12" r="B247">
+        <v>807</v>
+      </c>
+      <c t="s" s="21" r="C247">
         <v>806</v>
       </c>
-      <c t="s" s="6" r="C247">
-        <v>804</v>
-      </c>
-      <c s="14" r="D247"/>
-      <c s="14" r="E247"/>
+      <c s="12" r="D247"/>
+      <c s="12" r="E247"/>
     </row>
     <row r="248">
-      <c s="7" r="A248"/>
-      <c t="s" s="14" r="B248">
-        <v>807</v>
-      </c>
-      <c t="s" s="6" r="C248">
-        <v>804</v>
-      </c>
-      <c s="14" r="D248"/>
-      <c s="14" r="E248"/>
+      <c s="15" r="A248"/>
+      <c t="s" s="12" r="B248">
+        <v>808</v>
+      </c>
+      <c t="s" s="21" r="C248">
+        <v>806</v>
+      </c>
+      <c s="12" r="D248"/>
+      <c s="12" r="E248"/>
     </row>
     <row r="249">
-      <c s="7" r="A249"/>
-      <c t="s" s="14" r="B249">
-        <v>808</v>
-      </c>
-      <c t="s" s="6" r="C249">
-        <v>804</v>
-      </c>
-      <c s="14" r="D249"/>
-      <c s="14" r="E249"/>
+      <c s="15" r="A249"/>
+      <c t="s" s="12" r="B249">
+        <v>809</v>
+      </c>
+      <c t="s" s="21" r="C249">
+        <v>806</v>
+      </c>
+      <c s="12" r="D249"/>
+      <c s="12" r="E249"/>
     </row>
     <row r="250">
-      <c s="7" r="A250"/>
-      <c t="s" s="14" r="B250">
-        <v>809</v>
-      </c>
-      <c t="s" s="6" r="C250">
-        <v>804</v>
-      </c>
-      <c s="14" r="D250"/>
-      <c s="14" r="E250"/>
+      <c s="15" r="A250"/>
+      <c t="s" s="12" r="B250">
+        <v>810</v>
+      </c>
+      <c t="s" s="21" r="C250">
+        <v>806</v>
+      </c>
+      <c s="12" r="D250"/>
+      <c s="12" r="E250"/>
     </row>
     <row r="251">
-      <c s="7" r="A251"/>
-      <c t="s" s="14" r="B251">
-        <v>810</v>
-      </c>
-      <c t="s" s="6" r="C251">
-        <v>804</v>
-      </c>
-      <c s="14" r="D251"/>
-      <c s="14" r="E251"/>
+      <c s="15" r="A251"/>
+      <c t="s" s="12" r="B251">
+        <v>811</v>
+      </c>
+      <c t="s" s="21" r="C251">
+        <v>806</v>
+      </c>
+      <c s="12" r="D251"/>
+      <c s="12" r="E251"/>
     </row>
     <row r="252">
-      <c s="7" r="A252"/>
-      <c t="s" s="14" r="B252">
-        <v>811</v>
-      </c>
-      <c t="s" s="6" r="C252">
-        <v>804</v>
-      </c>
-      <c s="14" r="D252"/>
-      <c s="14" r="E252"/>
+      <c s="15" r="A252"/>
+      <c t="s" s="12" r="B252">
+        <v>812</v>
+      </c>
+      <c t="s" s="21" r="C252">
+        <v>806</v>
+      </c>
+      <c s="12" r="D252"/>
+      <c s="12" r="E252"/>
     </row>
     <row r="253">
-      <c s="7" r="A253"/>
-      <c s="14" r="B253"/>
-      <c s="6" r="C253"/>
-      <c s="14" r="D253"/>
-      <c s="14" r="E253"/>
+      <c s="15" r="A253"/>
+      <c t="s" s="12" r="B253">
+        <v>813</v>
+      </c>
+      <c t="s" s="21" r="C253">
+        <v>806</v>
+      </c>
+      <c s="12" r="D253"/>
+      <c s="12" r="E253"/>
     </row>
     <row r="254">
       <c s="7" r="A254"/>
@@ -6440,6 +6459,13 @@
       <c s="6" r="C263"/>
       <c s="14" r="D263"/>
       <c s="14" r="E263"/>
+    </row>
+    <row r="264">
+      <c s="7" r="A264"/>
+      <c s="14" r="B264"/>
+      <c s="6" r="C264"/>
+      <c s="14" r="D264"/>
+      <c s="14" r="E264"/>
     </row>
   </sheetData>
 </worksheet>
@@ -6457,17 +6483,17 @@
   <sheetData>
     <row customHeight="1" r="1" ht="112.5">
       <c t="s" s="2" r="A1">
-        <v>812</v>
+        <v>814</v>
       </c>
     </row>
     <row customHeight="1" r="2" ht="112.5">
       <c t="s" s="3" r="A2">
-        <v>813</v>
+        <v>815</v>
       </c>
     </row>
     <row customHeight="1" r="3" ht="112.5">
       <c t="s" s="8" r="A3">
-        <v>814</v>
+        <v>816</v>
       </c>
     </row>
   </sheetData>
@@ -6482,164 +6508,164 @@
   <sheetFormatPr customHeight="1" defaultColWidth="9.86" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c s="27" r="A1"/>
-      <c s="27" r="B1"/>
-      <c s="27" r="C1"/>
-      <c s="27" r="D1"/>
-      <c s="27" r="E1"/>
-      <c s="27" r="F1"/>
+      <c s="28" r="A1"/>
+      <c s="28" r="B1"/>
+      <c s="28" r="C1"/>
+      <c s="28" r="D1"/>
+      <c s="28" r="E1"/>
+      <c s="28" r="F1"/>
     </row>
     <row r="2">
-      <c s="27" r="A2"/>
-      <c s="27" r="B2"/>
-      <c s="27" r="C2"/>
-      <c s="27" r="D2"/>
-      <c s="27" r="E2"/>
-      <c s="27" r="F2"/>
+      <c s="28" r="A2"/>
+      <c s="28" r="B2"/>
+      <c s="28" r="C2"/>
+      <c s="28" r="D2"/>
+      <c s="28" r="E2"/>
+      <c s="28" r="F2"/>
     </row>
     <row r="3">
-      <c s="27" r="A3"/>
-      <c s="27" r="B3"/>
-      <c s="27" r="C3"/>
-      <c s="27" r="D3"/>
-      <c s="27" r="E3"/>
-      <c s="27" r="F3"/>
+      <c s="28" r="A3"/>
+      <c s="28" r="B3"/>
+      <c s="28" r="C3"/>
+      <c s="28" r="D3"/>
+      <c s="28" r="E3"/>
+      <c s="28" r="F3"/>
     </row>
     <row r="4">
-      <c s="27" r="A4"/>
-      <c s="27" r="B4"/>
-      <c s="27" r="C4"/>
-      <c s="27" r="D4"/>
-      <c s="27" r="E4"/>
-      <c s="27" r="F4"/>
+      <c s="28" r="A4"/>
+      <c s="28" r="B4"/>
+      <c s="28" r="C4"/>
+      <c s="28" r="D4"/>
+      <c s="28" r="E4"/>
+      <c s="28" r="F4"/>
     </row>
     <row r="5">
-      <c s="27" r="A5"/>
-      <c s="27" r="B5"/>
-      <c s="27" r="C5"/>
-      <c s="27" r="D5"/>
-      <c s="27" r="E5"/>
-      <c s="27" r="F5"/>
+      <c s="28" r="A5"/>
+      <c s="28" r="B5"/>
+      <c s="28" r="C5"/>
+      <c s="28" r="D5"/>
+      <c s="28" r="E5"/>
+      <c s="28" r="F5"/>
     </row>
     <row r="6">
-      <c s="27" r="A6"/>
-      <c s="27" r="B6"/>
-      <c s="27" r="C6"/>
-      <c s="27" r="D6"/>
-      <c s="27" r="E6"/>
-      <c s="27" r="F6"/>
+      <c s="28" r="A6"/>
+      <c s="28" r="B6"/>
+      <c s="28" r="C6"/>
+      <c s="28" r="D6"/>
+      <c s="28" r="E6"/>
+      <c s="28" r="F6"/>
     </row>
     <row r="7">
-      <c s="27" r="A7"/>
-      <c s="27" r="B7"/>
-      <c s="27" r="C7"/>
-      <c s="27" r="D7"/>
-      <c s="27" r="E7"/>
-      <c s="27" r="F7"/>
+      <c s="28" r="A7"/>
+      <c s="28" r="B7"/>
+      <c s="28" r="C7"/>
+      <c s="28" r="D7"/>
+      <c s="28" r="E7"/>
+      <c s="28" r="F7"/>
     </row>
     <row r="8">
-      <c s="27" r="A8"/>
-      <c s="27" r="B8"/>
-      <c s="27" r="C8"/>
-      <c s="27" r="D8"/>
-      <c s="27" r="E8"/>
-      <c s="27" r="F8"/>
+      <c s="28" r="A8"/>
+      <c s="28" r="B8"/>
+      <c s="28" r="C8"/>
+      <c s="28" r="D8"/>
+      <c s="28" r="E8"/>
+      <c s="28" r="F8"/>
     </row>
     <row r="9">
-      <c s="27" r="A9"/>
-      <c s="27" r="B9"/>
-      <c s="27" r="C9"/>
-      <c s="27" r="D9"/>
-      <c s="27" r="E9"/>
-      <c s="27" r="F9"/>
+      <c s="28" r="A9"/>
+      <c s="28" r="B9"/>
+      <c s="28" r="C9"/>
+      <c s="28" r="D9"/>
+      <c s="28" r="E9"/>
+      <c s="28" r="F9"/>
     </row>
     <row r="10">
-      <c s="27" r="A10"/>
-      <c s="27" r="B10"/>
-      <c s="27" r="C10"/>
-      <c s="27" r="D10"/>
-      <c s="27" r="E10"/>
-      <c s="27" r="F10"/>
+      <c s="28" r="A10"/>
+      <c s="28" r="B10"/>
+      <c s="28" r="C10"/>
+      <c s="28" r="D10"/>
+      <c s="28" r="E10"/>
+      <c s="28" r="F10"/>
     </row>
     <row r="11">
-      <c s="27" r="A11"/>
-      <c s="27" r="B11"/>
-      <c s="27" r="C11"/>
-      <c s="27" r="D11"/>
-      <c s="27" r="E11"/>
-      <c s="27" r="F11"/>
+      <c s="28" r="A11"/>
+      <c s="28" r="B11"/>
+      <c s="28" r="C11"/>
+      <c s="28" r="D11"/>
+      <c s="28" r="E11"/>
+      <c s="28" r="F11"/>
     </row>
     <row r="12">
-      <c s="27" r="A12"/>
-      <c s="27" r="B12"/>
-      <c s="27" r="C12"/>
-      <c s="27" r="D12"/>
-      <c s="27" r="E12"/>
-      <c s="27" r="F12"/>
+      <c s="28" r="A12"/>
+      <c s="28" r="B12"/>
+      <c s="28" r="C12"/>
+      <c s="28" r="D12"/>
+      <c s="28" r="E12"/>
+      <c s="28" r="F12"/>
     </row>
     <row r="13">
-      <c s="27" r="A13"/>
-      <c s="27" r="B13"/>
-      <c s="27" r="C13"/>
-      <c s="27" r="D13"/>
-      <c s="27" r="E13"/>
-      <c s="27" r="F13"/>
+      <c s="28" r="A13"/>
+      <c s="28" r="B13"/>
+      <c s="28" r="C13"/>
+      <c s="28" r="D13"/>
+      <c s="28" r="E13"/>
+      <c s="28" r="F13"/>
     </row>
     <row r="14">
-      <c s="27" r="A14"/>
-      <c s="27" r="B14"/>
-      <c s="27" r="C14"/>
-      <c s="27" r="D14"/>
-      <c s="27" r="E14"/>
-      <c s="27" r="F14"/>
+      <c s="28" r="A14"/>
+      <c s="28" r="B14"/>
+      <c s="28" r="C14"/>
+      <c s="28" r="D14"/>
+      <c s="28" r="E14"/>
+      <c s="28" r="F14"/>
     </row>
     <row r="15">
-      <c s="27" r="A15"/>
-      <c s="27" r="B15"/>
-      <c s="27" r="C15"/>
-      <c s="27" r="D15"/>
-      <c s="27" r="E15"/>
-      <c s="27" r="F15"/>
+      <c s="28" r="A15"/>
+      <c s="28" r="B15"/>
+      <c s="28" r="C15"/>
+      <c s="28" r="D15"/>
+      <c s="28" r="E15"/>
+      <c s="28" r="F15"/>
     </row>
     <row r="16">
-      <c s="27" r="A16"/>
-      <c s="27" r="B16"/>
-      <c s="27" r="C16"/>
-      <c s="27" r="D16"/>
-      <c s="27" r="E16"/>
-      <c s="27" r="F16"/>
+      <c s="28" r="A16"/>
+      <c s="28" r="B16"/>
+      <c s="28" r="C16"/>
+      <c s="28" r="D16"/>
+      <c s="28" r="E16"/>
+      <c s="28" r="F16"/>
     </row>
     <row r="17">
-      <c s="27" r="A17"/>
-      <c s="27" r="B17"/>
-      <c s="27" r="C17"/>
-      <c s="27" r="D17"/>
-      <c s="27" r="E17"/>
-      <c s="27" r="F17"/>
+      <c s="28" r="A17"/>
+      <c s="28" r="B17"/>
+      <c s="28" r="C17"/>
+      <c s="28" r="D17"/>
+      <c s="28" r="E17"/>
+      <c s="28" r="F17"/>
     </row>
     <row r="18">
-      <c s="27" r="A18"/>
-      <c s="27" r="B18"/>
-      <c s="27" r="C18"/>
-      <c s="27" r="D18"/>
-      <c s="27" r="E18"/>
-      <c s="27" r="F18"/>
+      <c s="28" r="A18"/>
+      <c s="28" r="B18"/>
+      <c s="28" r="C18"/>
+      <c s="28" r="D18"/>
+      <c s="28" r="E18"/>
+      <c s="28" r="F18"/>
     </row>
     <row r="19">
-      <c s="27" r="A19"/>
-      <c s="27" r="B19"/>
-      <c s="27" r="C19"/>
-      <c s="27" r="D19"/>
-      <c s="27" r="E19"/>
-      <c s="27" r="F19"/>
+      <c s="28" r="A19"/>
+      <c s="28" r="B19"/>
+      <c s="28" r="C19"/>
+      <c s="28" r="D19"/>
+      <c s="28" r="E19"/>
+      <c s="28" r="F19"/>
     </row>
     <row r="20">
-      <c s="27" r="A20"/>
-      <c s="27" r="B20"/>
-      <c s="27" r="C20"/>
-      <c s="27" r="D20"/>
-      <c s="27" r="E20"/>
-      <c s="27" r="F20"/>
+      <c s="28" r="A20"/>
+      <c s="28" r="B20"/>
+      <c s="28" r="C20"/>
+      <c s="28" r="D20"/>
+      <c s="28" r="E20"/>
+      <c s="28" r="F20"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
EWD-22592 - Sign-Up in 2 steps buttons
Former-commit-id: 81a686768c813bef27d23b8136304629f44ff2eb
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="817">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="876">
   <si>
     <t>Page</t>
   </si>
@@ -1024,6 +1024,12 @@
     <t>Saved at</t>
   </si>
   <si>
+    <t>Opgeslagen om</t>
+  </si>
+  <si>
+    <t>Gespeichert am</t>
+  </si>
+  <si>
     <t>customLocalizationPlugin</t>
   </si>
   <si>
@@ -2234,36 +2240,72 @@
     <t>Learning experience was not found. Please refresh your data.</t>
   </si>
   <si>
+    <t>De leerervaring is niet gevonden. Vernieuw uw gegevens. </t>
+  </si>
+  <si>
+    <t>Die Lernerfahrung wurde nicht gefunden. Bitte aktualisieren Sie Ihre Daten.</t>
+  </si>
+  <si>
     <t>objectiveNotFoundError</t>
   </si>
   <si>
     <t>Learning objective was not found. Please refresh your data.</t>
   </si>
   <si>
+    <t>Het leerdoel is niet gevonden. Vernieuw uw gegevens.</t>
+  </si>
+  <si>
+    <t>Das Lernziel wurde nicht gefunden. Bitte aktualisieren Sie Ihre Daten.</t>
+  </si>
+  <si>
     <t>answerNotFoundError</t>
   </si>
   <si>
     <t>Answer option was not found. Please refresh your data.</t>
   </si>
   <si>
+    <t>De antwoordoptie is niet gevonden. Vernieuw uw gegevens.</t>
+  </si>
+  <si>
+    <t>Die Antwortoption wurde nicht gefunden. Bitte aktualisieren Sie Ihre Daten.</t>
+  </si>
+  <si>
     <t>questionNotFoundError</t>
   </si>
   <si>
     <t>Question was not found. Please refresh your data.</t>
   </si>
   <si>
+    <t>De vraag is niet gevonden. Vernieuw uw gegevens.</t>
+  </si>
+  <si>
+    <t>Die Frage wurde nicht gefunden. Bitte aktualisieren Sie Ihre Daten.</t>
+  </si>
+  <si>
     <t>learningObjectNotFoundError</t>
   </si>
   <si>
     <t>Learning object was not found. Please refresh your data.</t>
   </si>
   <si>
+    <t>Het leerobject is niet gevonden. Vernieuw uw gegevens.</t>
+  </si>
+  <si>
+    <t>Der Lerngegenstand wurde nicht gefunden. Bitte aktualisieren Sie Ihre Daten.</t>
+  </si>
+  <si>
     <t>helpHintNotFoundError</t>
   </si>
   <si>
     <t>Help hint was not found. Please refresh your data.</t>
   </si>
   <si>
+    <t>De helphint is niet gevonden. Vernieuw uw gegevens.</t>
+  </si>
+  <si>
+    <t>Der Hilfehinweis wurde nicht gefunden. Bitte aktualisieren Sie Ihre Daten.</t>
+  </si>
+  <si>
     <t>View captions</t>
   </si>
   <si>
@@ -2273,7 +2315,7 @@
     <t>Learning experience editor</t>
   </si>
   <si>
-    <t>Leerervaringen editor</t>
+    <t>Leerervaring-editor</t>
   </si>
   <si>
     <t>Lernerfahrungs-Editor</t>
@@ -2285,18 +2327,36 @@
     <t>Learning objective editor</t>
   </si>
   <si>
+    <t>Leerdoel-editor</t>
+  </si>
+  <si>
+    <t>Lernziel-Editor</t>
+  </si>
+  <si>
     <t>questionViewCaption</t>
   </si>
   <si>
     <t>Question editor</t>
   </si>
   <si>
+    <t>Vraag-editor</t>
+  </si>
+  <si>
+    <t>Frage-Editor</t>
+  </si>
+  <si>
     <t>createExperienceViewCaption</t>
   </si>
   <si>
     <t>Create learning experience</t>
   </si>
   <si>
+    <t>Leerervaring maken</t>
+  </si>
+  <si>
+    <t>Lernerfahrung erstellen</t>
+  </si>
+  <si>
     <t>createObjectiveViewCaption</t>
   </si>
   <si>
@@ -2306,6 +2366,12 @@
     <t>Create question</t>
   </si>
   <si>
+    <t>Vraag maken</t>
+  </si>
+  <si>
+    <t>Frage erstellen</t>
+  </si>
+  <si>
     <t>Sign-UP optional fields</t>
   </si>
   <si>
@@ -2315,72 +2381,141 @@
     <t>Full name</t>
   </si>
   <si>
+    <t>Volledige naam</t>
+  </si>
+  <si>
+    <t>Vollständiger Name</t>
+  </si>
+  <si>
     <t>PhoneNumberCaption</t>
   </si>
   <si>
     <t>Phone number</t>
   </si>
   <si>
+    <t>Telefoonnummer</t>
+  </si>
+  <si>
+    <t>Telefonnummer</t>
+  </si>
+  <si>
     <t>OrganizationNameCaption</t>
   </si>
   <si>
     <t>Organization name</t>
   </si>
   <si>
+    <t>Naam van organisatie</t>
+  </si>
+  <si>
+    <t>Name der Organisiation</t>
+  </si>
+  <si>
     <t>CountryCaption</t>
   </si>
   <si>
     <t>Country</t>
   </si>
   <si>
+    <t>Land</t>
+  </si>
+  <si>
     <t>howManyPeopleQuestion</t>
   </si>
   <si>
     <t>How many people at your company are authoring courses?</t>
   </si>
   <si>
+    <t>Hoeveel medewerkers in uw bedrijf schrijven cursusmateriaal?</t>
+  </si>
+  <si>
+    <t>Wie viele Personen in Ihrem Unternehmen erstellen Kurse?</t>
+  </si>
+  <si>
     <t>whenDoYouNeedToolQuestion</t>
   </si>
   <si>
     <t>How soon do you need an authoring tool?</t>
   </si>
   <si>
+    <t>Hoe snel hebt u een schrijftool nodig?</t>
+  </si>
+  <si>
+    <t>Wie bald benötigen Sie ein Autorentool?</t>
+  </si>
+  <si>
     <t>howAuthorTodayQuestion</t>
   </si>
   <si>
     <t>How do you author courses today?</t>
   </si>
   <si>
+    <t>Hoe schrijft u nu cursusmateriaal?</t>
+  </si>
+  <si>
+    <t>Wie erstellen Sie heute Kurse?</t>
+  </si>
+  <si>
     <t>chooseAnswer</t>
   </si>
   <si>
     <t>Choose answer</t>
   </si>
   <si>
+    <t>Kies een antwoord</t>
+  </si>
+  <si>
+    <t>Antwort auswählen</t>
+  </si>
+  <si>
     <t>now</t>
   </si>
   <si>
     <t>Now</t>
   </si>
   <si>
+    <t>Nu</t>
+  </si>
+  <si>
+    <t>Jetzt</t>
+  </si>
+  <si>
     <t>variant1Month</t>
   </si>
   <si>
     <t>1-3 Months</t>
   </si>
   <si>
+    <t>1-3 maanden</t>
+  </si>
+  <si>
+    <t>In 1 - 3 Monaten</t>
+  </si>
+  <si>
     <t>variantMore3Months</t>
   </si>
   <si>
     <t>&gt;3 Months</t>
   </si>
   <si>
+    <t>&gt;3 maanden</t>
+  </si>
+  <si>
+    <t>In mehr als 3 Monaten</t>
+  </si>
+  <si>
     <t>justLooking</t>
   </si>
   <si>
     <t>Just Looking</t>
   </si>
   <si>
+    <t>Ik oriënteer me alleen</t>
+  </si>
+  <si>
+    <t>Ich informiere mich nur.</t>
+  </si>
+  <si>
     <t>powerPoint</t>
   </si>
   <si>
@@ -2393,40 +2528,82 @@
     <t>Another authoring tool</t>
   </si>
   <si>
+    <t>Een andere schrijftool</t>
+  </si>
+  <si>
+    <t>Mit einem anderen Autorentool</t>
+  </si>
+  <si>
     <t>nothing</t>
   </si>
   <si>
     <t>Nothing</t>
   </si>
   <si>
+    <t>Geen</t>
+  </si>
+  <si>
+    <t>Keines</t>
+  </si>
+  <si>
     <t>other</t>
   </si>
   <si>
     <t>Other</t>
   </si>
   <si>
+    <t>Anders</t>
+  </si>
+  <si>
+    <t>Sonstiges</t>
+  </si>
+  <si>
     <t>skip</t>
   </si>
   <si>
     <t>Skip</t>
   </si>
   <si>
+    <t>Overslaan</t>
+  </si>
+  <si>
+    <t>Überspringen</t>
+  </si>
+  <si>
     <t>RequiredInformation</t>
   </si>
   <si>
     <t>Required information</t>
   </si>
   <si>
+    <t>Verplichte informatie</t>
+  </si>
+  <si>
+    <t>Erforderliche Information</t>
+  </si>
+  <si>
     <t>OptionalInformation</t>
   </si>
   <si>
     <t>Optional information</t>
   </si>
   <si>
+    <t>Optionele informatie</t>
+  </si>
+  <si>
+    <t>Optionale Information</t>
+  </si>
+  <si>
     <t>ChooseYourCountry</t>
   </si>
   <si>
     <t>Choose your country</t>
+  </si>
+  <si>
+    <t>Kies uw land</t>
+  </si>
+  <si>
+    <t>Wählen Sie Ihr Land aus.</t>
   </si>
   <si>
     <t>Help hints</t>
@@ -2749,6 +2926,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2762,12 +2945,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00FF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2791,13 +2968,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FF666666"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF666666"/>
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2876,10 +3053,10 @@
     <xf applyAlignment="1" fillId="13" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="13" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="14" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+    <xf applyAlignment="1" fillId="14" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="14" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="15" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="14" applyFill="1">
+    <xf applyAlignment="1" fillId="15" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="16" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="15" applyFill="1">
@@ -2900,10 +3077,10 @@
     <xf applyAlignment="1" fillId="19" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="18" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="20" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+    <xf applyAlignment="1" fillId="20" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="19" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="21" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="19" applyFill="1">
+    <xf applyAlignment="1" fillId="21" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="22" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
@@ -2955,7 +3132,7 @@
       </c>
     </row>
     <row r="2">
-      <c t="s" s="16" r="A2">
+      <c t="s" s="17" r="A2">
         <v>5</v>
       </c>
       <c t="s" s="5" r="B2">
@@ -2972,7 +3149,7 @@
       </c>
     </row>
     <row r="3">
-      <c s="16" r="A3"/>
+      <c s="17" r="A3"/>
       <c t="s" s="5" r="B3">
         <v>10</v>
       </c>
@@ -2987,7 +3164,7 @@
       </c>
     </row>
     <row r="4">
-      <c s="16" r="A4"/>
+      <c s="17" r="A4"/>
       <c t="s" s="5" r="B4">
         <v>14</v>
       </c>
@@ -3002,7 +3179,7 @@
       </c>
     </row>
     <row r="5">
-      <c s="16" r="A5"/>
+      <c s="17" r="A5"/>
       <c t="s" s="5" r="B5">
         <v>18</v>
       </c>
@@ -3017,7 +3194,7 @@
       </c>
     </row>
     <row r="6">
-      <c s="16" r="A6"/>
+      <c s="17" r="A6"/>
       <c t="s" s="5" r="B6">
         <v>22</v>
       </c>
@@ -3032,7 +3209,7 @@
       </c>
     </row>
     <row r="7">
-      <c s="16" r="A7"/>
+      <c s="17" r="A7"/>
       <c t="s" s="5" r="B7">
         <v>24</v>
       </c>
@@ -3047,7 +3224,7 @@
       </c>
     </row>
     <row r="8">
-      <c s="16" r="A8"/>
+      <c s="17" r="A8"/>
       <c t="s" s="5" r="B8">
         <v>26</v>
       </c>
@@ -3062,7 +3239,7 @@
       </c>
     </row>
     <row r="9">
-      <c s="16" r="A9"/>
+      <c s="17" r="A9"/>
       <c t="s" s="5" r="B9">
         <v>30</v>
       </c>
@@ -3077,7 +3254,7 @@
       </c>
     </row>
     <row r="10">
-      <c s="16" r="A10"/>
+      <c s="17" r="A10"/>
       <c t="s" s="5" r="B10">
         <v>34</v>
       </c>
@@ -3092,7 +3269,7 @@
       </c>
     </row>
     <row r="11">
-      <c s="16" r="A11"/>
+      <c s="17" r="A11"/>
       <c t="s" s="5" r="B11">
         <v>38</v>
       </c>
@@ -3107,7 +3284,7 @@
       </c>
     </row>
     <row r="12">
-      <c s="16" r="A12"/>
+      <c s="17" r="A12"/>
       <c t="s" s="5" r="B12">
         <v>42</v>
       </c>
@@ -3332,14 +3509,14 @@
       </c>
     </row>
     <row r="27">
-      <c s="16" r="A27"/>
-      <c s="16" r="B27"/>
-      <c s="16" r="C27"/>
-      <c s="16" r="D27"/>
-      <c s="16" r="E27"/>
+      <c s="17" r="A27"/>
+      <c s="17" r="B27"/>
+      <c s="17" r="C27"/>
+      <c s="17" r="D27"/>
+      <c s="17" r="E27"/>
     </row>
     <row r="28">
-      <c t="s" s="16" r="A28">
+      <c t="s" s="17" r="A28">
         <v>101</v>
       </c>
       <c t="s" s="5" r="B28">
@@ -3356,7 +3533,7 @@
       </c>
     </row>
     <row r="29">
-      <c s="16" r="A29"/>
+      <c s="17" r="A29"/>
       <c t="s" s="5" r="B29">
         <v>106</v>
       </c>
@@ -3371,7 +3548,7 @@
       </c>
     </row>
     <row r="30">
-      <c s="16" r="A30"/>
+      <c s="17" r="A30"/>
       <c t="s" s="5" r="B30">
         <v>110</v>
       </c>
@@ -3386,7 +3563,7 @@
       </c>
     </row>
     <row r="31">
-      <c s="16" r="A31"/>
+      <c s="17" r="A31"/>
       <c t="s" s="5" r="B31">
         <v>114</v>
       </c>
@@ -3401,7 +3578,7 @@
       </c>
     </row>
     <row r="32">
-      <c s="16" r="A32"/>
+      <c s="17" r="A32"/>
       <c t="s" s="5" r="B32">
         <v>118</v>
       </c>
@@ -3453,7 +3630,7 @@
       <c s="9" r="E35"/>
     </row>
     <row r="36">
-      <c t="s" s="16" r="A36">
+      <c t="s" s="17" r="A36">
         <v>130</v>
       </c>
       <c t="s" s="12" r="B36">
@@ -3466,10 +3643,10 @@
       <c s="12" r="E36"/>
     </row>
     <row r="37">
-      <c s="16" r="A37"/>
-      <c s="16" r="B37"/>
-      <c s="16" r="C37"/>
-      <c s="16" r="D37"/>
+      <c s="17" r="A37"/>
+      <c s="17" r="B37"/>
+      <c s="17" r="C37"/>
+      <c s="17" r="D37"/>
       <c s="9" r="E37"/>
     </row>
     <row r="38">
@@ -3754,57 +3931,57 @@
       </c>
     </row>
     <row r="58">
-      <c s="16" r="A58"/>
-      <c s="16" r="B58"/>
-      <c s="16" r="C58"/>
-      <c s="16" r="D58"/>
-      <c s="16" r="E58"/>
+      <c s="17" r="A58"/>
+      <c s="17" r="B58"/>
+      <c s="17" r="C58"/>
+      <c s="17" r="D58"/>
+      <c s="17" r="E58"/>
     </row>
     <row r="59">
       <c t="s" s="9" r="A59">
         <v>207</v>
       </c>
-      <c t="s" s="26" r="B59">
+      <c t="s" s="25" r="B59">
         <v>208</v>
       </c>
-      <c t="s" s="26" r="C59">
+      <c t="s" s="25" r="C59">
         <v>209</v>
       </c>
-      <c s="26" r="D59"/>
-      <c s="26" r="E59"/>
+      <c s="25" r="D59"/>
+      <c s="25" r="E59"/>
     </row>
     <row r="60">
       <c s="9" r="A60"/>
-      <c t="s" s="26" r="B60">
+      <c t="s" s="25" r="B60">
         <v>210</v>
       </c>
-      <c t="s" s="26" r="C60">
+      <c t="s" s="25" r="C60">
         <v>211</v>
       </c>
-      <c s="26" r="D60"/>
-      <c s="26" r="E60"/>
+      <c s="25" r="D60"/>
+      <c s="25" r="E60"/>
     </row>
     <row r="61">
       <c s="9" r="A61"/>
-      <c t="s" s="26" r="B61">
+      <c t="s" s="25" r="B61">
         <v>212</v>
       </c>
-      <c t="s" s="26" r="C61">
+      <c t="s" s="25" r="C61">
         <v>213</v>
       </c>
-      <c s="26" r="D61"/>
-      <c s="26" r="E61"/>
+      <c s="25" r="D61"/>
+      <c s="25" r="E61"/>
     </row>
     <row r="62">
       <c s="9" r="A62"/>
-      <c t="s" s="26" r="B62">
+      <c t="s" s="25" r="B62">
         <v>214</v>
       </c>
-      <c t="s" s="26" r="C62">
+      <c t="s" s="25" r="C62">
         <v>215</v>
       </c>
-      <c s="26" r="D62"/>
-      <c s="26" r="E62"/>
+      <c s="25" r="D62"/>
+      <c s="25" r="E62"/>
     </row>
     <row r="63">
       <c s="9" r="A63"/>
@@ -4267,8 +4444,12 @@
       <c t="s" s="5" r="C94">
         <v>335</v>
       </c>
-      <c s="19" r="D94"/>
-      <c s="19" r="E94"/>
+      <c t="s" s="5" r="D94">
+        <v>336</v>
+      </c>
+      <c t="s" s="5" r="E94">
+        <v>337</v>
+      </c>
     </row>
     <row r="95">
       <c s="7" r="A95"/>
@@ -4279,544 +4460,544 @@
     </row>
     <row r="96">
       <c t="s" s="7" r="A96">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c t="s" s="5" r="B96">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c t="s" s="5" r="C96">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c t="s" s="5" r="D96">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c t="s" s="5" r="E96">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="97">
       <c s="7" r="A97"/>
       <c t="s" s="5" r="B97">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c t="s" s="5" r="C97">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c t="s" s="5" r="D97">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c t="s" s="5" r="E97">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="98">
       <c s="7" r="A98"/>
       <c t="s" s="5" r="B98">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c t="s" s="5" r="C98">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c t="s" s="5" r="D98">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c t="s" s="5" r="E98">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="99">
       <c s="7" r="A99"/>
       <c t="s" s="5" r="B99">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c t="s" s="5" r="C99">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c t="s" s="5" r="D99">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c t="s" s="5" r="E99">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="100">
       <c s="7" r="A100"/>
       <c t="s" s="5" r="B100">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c t="s" s="5" r="C100">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c t="s" s="5" r="D100">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c t="s" s="5" r="E100">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="101">
       <c s="7" r="A101"/>
       <c t="s" s="5" r="B101">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c t="s" s="5" r="C101">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c t="s" s="5" r="D101">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c t="s" s="5" r="E101">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="102">
       <c s="7" r="A102"/>
       <c t="s" s="5" r="B102">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c t="s" s="5" r="C102">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c t="s" s="5" r="D102">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c t="s" s="5" r="E102">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="103">
       <c s="7" r="A103"/>
       <c t="s" s="5" r="B103">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c t="s" s="5" r="C103">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c t="s" s="5" r="D103">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c t="s" s="5" r="E103">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="104">
       <c s="7" r="A104"/>
       <c t="s" s="5" r="B104">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c t="s" s="5" r="C104">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c t="s" s="5" r="D104">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c t="s" s="5" r="E104">
-        <v>371</v>
+        <v>373</v>
       </c>
     </row>
     <row r="105">
       <c s="7" r="A105"/>
       <c t="s" s="5" r="B105">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c t="s" s="5" r="C105">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c t="s" s="5" r="D105">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c t="s" s="5" r="E105">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="106">
       <c s="7" r="A106"/>
       <c t="s" s="5" r="B106">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c t="s" s="5" r="C106">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c t="s" s="5" r="D106">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c t="s" s="5" r="E106">
-        <v>379</v>
+        <v>381</v>
       </c>
     </row>
     <row r="107">
       <c s="7" r="A107"/>
       <c t="s" s="5" r="B107">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c t="s" s="5" r="C107">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c t="s" s="5" r="D107">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c t="s" s="5" r="E107">
-        <v>382</v>
+        <v>384</v>
       </c>
     </row>
     <row r="108">
       <c s="7" r="A108"/>
       <c t="s" s="5" r="B108">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c t="s" s="5" r="C108">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c t="s" s="5" r="D108">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c t="s" s="5" r="E108">
-        <v>385</v>
+        <v>387</v>
       </c>
     </row>
     <row r="109">
       <c s="7" r="A109"/>
       <c t="s" s="5" r="B109">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c t="s" s="5" r="C109">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c t="s" s="5" r="D109">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c t="s" s="5" r="E109">
-        <v>389</v>
+        <v>391</v>
       </c>
     </row>
     <row r="110">
       <c s="7" r="A110"/>
       <c t="s" s="11" r="B110">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c t="s" s="5" r="C110">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c t="s" s="5" r="D110">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c t="s" s="5" r="E110">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="111">
       <c s="7" r="A111"/>
       <c t="s" s="5" r="B111">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c t="s" s="5" r="C111">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c t="s" s="5" r="D111">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c t="s" s="5" r="E111">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="112">
       <c s="7" r="A112"/>
       <c t="s" s="5" r="B112">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c t="s" s="5" r="C112">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c t="s" s="5" r="D112">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c t="s" s="5" r="E112">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="113">
       <c s="7" r="A113"/>
       <c t="s" s="5" r="B113">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c t="s" s="5" r="C113">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c t="s" s="5" r="D113">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c t="s" s="5" r="E113">
-        <v>404</v>
+        <v>406</v>
       </c>
     </row>
     <row r="114">
       <c s="7" r="A114"/>
       <c t="s" s="5" r="B114">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c t="s" s="5" r="C114">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c t="s" s="5" r="D114">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c t="s" s="5" r="E114">
-        <v>408</v>
+        <v>410</v>
       </c>
     </row>
     <row r="115">
       <c s="7" r="A115"/>
       <c t="s" s="5" r="B115">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c t="s" s="5" r="C115">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c t="s" s="5" r="D115">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c t="s" s="5" r="E115">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="116">
       <c s="7" r="A116"/>
       <c t="s" s="5" r="B116">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c t="s" s="5" r="C116">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c t="s" s="5" r="D116">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c t="s" s="5" r="E116">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
     <row r="117">
       <c s="7" r="A117"/>
       <c t="s" s="5" r="B117">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c t="s" s="5" r="C117">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c t="s" s="5" r="D117">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c t="s" s="5" r="E117">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="118">
       <c s="7" r="A118"/>
       <c t="s" s="5" r="B118">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c t="s" s="5" r="C118">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c t="s" s="5" r="D118">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c t="s" s="5" r="E118">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
     <row r="119">
       <c s="7" r="A119"/>
       <c t="s" s="5" r="B119">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c t="s" s="5" r="C119">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c t="s" s="5" r="D119">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c t="s" s="5" r="E119">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="120">
       <c s="7" r="A120"/>
       <c t="s" s="5" r="B120">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c t="s" s="5" r="C120">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c t="s" s="5" r="D120">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c t="s" s="5" r="E120">
-        <v>432</v>
+        <v>434</v>
       </c>
     </row>
     <row r="121">
       <c s="7" r="A121"/>
       <c t="s" s="5" r="B121">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c t="s" s="5" r="C121">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c t="s" s="5" r="D121">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c t="s" s="5" r="E121">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
     <row r="122">
       <c s="7" r="A122"/>
       <c t="s" s="5" r="B122">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c t="s" s="5" r="C122">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c t="s" s="5" r="D122">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c t="s" s="5" r="E122">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="123">
       <c s="7" r="A123"/>
       <c t="s" s="5" r="B123">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c t="s" s="5" r="C123">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c t="s" s="5" r="D123">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c t="s" s="5" r="E123">
-        <v>444</v>
+        <v>446</v>
       </c>
     </row>
     <row r="124">
       <c s="7" r="A124"/>
       <c t="s" s="5" r="B124">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c t="s" s="5" r="C124">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c t="s" s="5" r="D124">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c t="s" s="5" r="E124">
-        <v>448</v>
+        <v>450</v>
       </c>
     </row>
     <row r="125">
       <c s="7" r="A125"/>
       <c t="s" s="5" r="B125">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c t="s" s="5" r="C125">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c t="s" s="5" r="D125">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c t="s" s="5" r="E125">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="126">
       <c s="7" r="A126"/>
       <c t="s" s="5" r="B126">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c t="s" s="11" r="C126">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c t="s" s="5" r="D126">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c t="s" s="5" r="E126">
-        <v>456</v>
+        <v>458</v>
       </c>
     </row>
     <row r="127">
       <c s="7" r="A127"/>
       <c t="s" s="11" r="B127">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c t="s" s="11" r="C127">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c t="s" s="5" r="D127">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c t="s" s="5" r="E127">
-        <v>460</v>
+        <v>462</v>
       </c>
     </row>
     <row r="128">
       <c s="7" r="A128"/>
       <c t="s" s="5" r="B128">
+        <v>463</v>
+      </c>
+      <c t="s" s="11" r="C128">
+        <v>460</v>
+      </c>
+      <c t="s" s="5" r="D128">
         <v>461</v>
       </c>
-      <c t="s" s="11" r="C128">
-        <v>458</v>
-      </c>
-      <c t="s" s="5" r="D128">
-        <v>459</v>
-      </c>
       <c t="s" s="5" r="E128">
-        <v>460</v>
+        <v>462</v>
       </c>
     </row>
     <row r="129">
       <c s="7" r="A129"/>
       <c t="s" s="5" r="B129">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c t="s" s="1" r="C129">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c t="s" s="5" r="D129">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c t="s" s="5" r="E129">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="130">
       <c s="7" r="A130"/>
       <c t="s" s="5" r="B130">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c t="s" s="1" r="C130">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c t="s" s="5" r="D130">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c t="s" s="5" r="E130">
-        <v>469</v>
+        <v>471</v>
       </c>
     </row>
     <row r="131">
       <c s="7" r="A131"/>
       <c t="s" s="5" r="B131">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c t="s" s="1" r="C131">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c t="s" s="5" r="D131">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c t="s" s="1" r="E131">
-        <v>473</v>
+        <v>475</v>
       </c>
     </row>
     <row r="132">
@@ -4828,424 +5009,424 @@
     </row>
     <row r="133">
       <c t="s" s="7" r="A133">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c t="s" s="5" r="B133">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c t="s" s="11" r="C133">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c t="s" s="5" r="D133">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c t="s" s="5" r="E133">
-        <v>478</v>
+        <v>480</v>
       </c>
     </row>
     <row r="134">
       <c s="7" r="A134"/>
       <c t="s" s="5" r="B134">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c t="s" s="11" r="C134">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c t="s" s="5" r="D134">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c t="s" s="5" r="E134">
-        <v>482</v>
+        <v>484</v>
       </c>
     </row>
     <row r="135">
       <c s="10" r="A135"/>
       <c t="s" s="5" r="B135">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c t="s" s="11" r="C135">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c t="s" s="5" r="D135">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c t="s" s="5" r="E135">
-        <v>486</v>
+        <v>488</v>
       </c>
     </row>
     <row r="136">
       <c s="7" r="A136"/>
-      <c t="s" s="18" r="B136">
-        <v>487</v>
+      <c t="s" s="19" r="B136">
+        <v>489</v>
       </c>
       <c t="s" s="11" r="C136">
-        <v>488</v>
-      </c>
-      <c t="s" s="18" r="D136">
-        <v>489</v>
-      </c>
-      <c t="s" s="18" r="E136">
         <v>490</v>
+      </c>
+      <c t="s" s="19" r="D136">
+        <v>491</v>
+      </c>
+      <c t="s" s="19" r="E136">
+        <v>492</v>
       </c>
     </row>
     <row r="137">
       <c s="7" r="A137"/>
       <c t="s" s="5" r="B137">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c t="s" s="11" r="C137">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c t="s" s="5" r="D137">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c t="s" s="5" r="E137">
-        <v>494</v>
+        <v>496</v>
       </c>
     </row>
     <row r="138">
       <c s="7" r="A138"/>
       <c t="s" s="5" r="B138">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c t="s" s="11" r="C138">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c t="s" s="5" r="D138">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c t="s" s="5" r="E138">
-        <v>498</v>
+        <v>500</v>
       </c>
     </row>
     <row r="139">
       <c s="7" r="A139"/>
       <c t="s" s="5" r="B139">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c t="s" s="11" r="C139">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c t="s" s="5" r="D139">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c t="s" s="5" r="E139">
-        <v>502</v>
+        <v>504</v>
       </c>
     </row>
     <row r="140">
       <c s="7" r="A140"/>
       <c t="s" s="5" r="B140">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c t="s" s="11" r="C140">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c t="s" s="5" r="D140">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c t="s" s="5" r="E140">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="141">
       <c s="7" r="A141"/>
       <c t="s" s="5" r="B141">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c t="s" s="11" r="C141">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c t="s" s="5" r="D141">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c t="s" s="5" r="E141">
-        <v>510</v>
+        <v>512</v>
       </c>
     </row>
     <row r="142">
       <c s="7" r="A142"/>
       <c t="s" s="5" r="B142">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c t="s" s="11" r="C142">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c t="s" s="5" r="D142">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c t="s" s="5" r="E142">
-        <v>514</v>
+        <v>516</v>
       </c>
     </row>
     <row r="143">
       <c s="7" r="A143"/>
       <c t="s" s="5" r="B143">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c t="s" s="11" r="C143">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c t="s" s="5" r="D143">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c t="s" s="5" r="E143">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="144">
       <c s="7" r="A144"/>
       <c t="s" s="5" r="B144">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c t="s" s="11" r="C144">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c t="s" s="5" r="D144">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c t="s" s="5" r="E144">
-        <v>522</v>
+        <v>524</v>
       </c>
     </row>
     <row r="145">
       <c s="7" r="A145"/>
       <c t="s" s="5" r="B145">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c t="s" s="11" r="C145">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c t="s" s="5" r="D145">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c t="s" s="5" r="E145">
-        <v>526</v>
+        <v>528</v>
       </c>
     </row>
     <row r="146">
       <c s="15" r="A146"/>
       <c t="s" s="5" r="B146">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c t="s" s="11" r="C146">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c t="s" s="5" r="D146">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c t="s" s="5" r="E146">
-        <v>530</v>
+        <v>532</v>
       </c>
     </row>
     <row r="147">
       <c s="7" r="A147"/>
       <c t="s" s="5" r="B147">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c t="s" s="11" r="C147">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c t="s" s="5" r="D147">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c t="s" s="5" r="E147">
-        <v>534</v>
+        <v>536</v>
       </c>
     </row>
     <row r="148">
       <c s="7" r="A148"/>
       <c t="s" s="5" r="B148">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c t="s" s="11" r="C148">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c t="s" s="5" r="D148">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c t="s" s="5" r="E148">
-        <v>486</v>
+        <v>488</v>
       </c>
     </row>
     <row r="149">
       <c s="7" r="A149"/>
       <c t="s" s="5" r="B149">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c t="s" s="11" r="C149">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c t="s" s="5" r="D149">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c t="s" s="5" r="E149">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="150">
       <c s="7" r="A150"/>
       <c t="s" s="5" r="B150">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c t="s" s="11" r="C150">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c t="s" s="5" r="D150">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c t="s" s="5" r="E150">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
     <row r="151">
       <c s="7" r="A151"/>
       <c t="s" s="5" r="B151">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c t="s" s="11" r="C151">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c t="s" s="5" r="D151">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c t="s" s="5" r="E151">
-        <v>549</v>
+        <v>551</v>
       </c>
     </row>
     <row r="152">
       <c s="7" r="A152"/>
       <c t="s" s="5" r="B152">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c t="s" s="11" r="C152">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c t="s" s="5" r="D152">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c t="s" s="5" r="E152">
-        <v>553</v>
+        <v>555</v>
       </c>
     </row>
     <row r="153">
       <c s="7" r="A153"/>
       <c t="s" s="5" r="B153">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c t="s" s="11" r="C153">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c t="s" s="5" r="D153">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c t="s" s="5" r="E153">
-        <v>557</v>
+        <v>559</v>
       </c>
     </row>
     <row r="154">
       <c s="7" r="A154"/>
-      <c s="16" r="B154"/>
-      <c s="25" r="C154"/>
-      <c s="16" r="D154"/>
-      <c s="16" r="E154"/>
+      <c s="17" r="B154"/>
+      <c s="26" r="C154"/>
+      <c s="17" r="D154"/>
+      <c s="17" r="E154"/>
     </row>
     <row r="155">
       <c t="s" s="7" r="A155">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c t="s" s="5" r="B155">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c t="s" s="11" r="C155">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c t="s" s="5" r="D155">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c t="s" s="5" r="E155">
-        <v>562</v>
+        <v>564</v>
       </c>
     </row>
     <row r="156">
       <c s="7" r="A156"/>
       <c t="s" s="5" r="B156">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c t="s" s="11" r="C156">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c t="s" s="5" r="D156">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c t="s" s="5" r="E156">
-        <v>566</v>
+        <v>568</v>
       </c>
     </row>
     <row r="157">
       <c s="7" r="A157"/>
       <c t="s" s="5" r="B157">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c t="s" s="11" r="C157">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c t="s" s="5" r="D157">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c t="s" s="5" r="E157">
-        <v>570</v>
+        <v>572</v>
       </c>
     </row>
     <row r="158">
       <c s="7" r="A158"/>
       <c t="s" s="5" r="B158">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c t="s" s="11" r="C158">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c t="s" s="5" r="D158">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c t="s" s="5" r="E158">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
     <row r="159">
       <c s="7" r="A159"/>
       <c t="s" s="5" r="B159">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c t="s" s="11" r="C159">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c t="s" s="5" r="D159">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c t="s" s="5" r="E159">
-        <v>578</v>
+        <v>580</v>
       </c>
     </row>
     <row r="160">
       <c s="7" r="A160"/>
-      <c s="16" r="B160"/>
-      <c s="25" r="C160"/>
-      <c s="16" r="D160"/>
-      <c s="16" r="E160"/>
+      <c s="17" r="B160"/>
+      <c s="26" r="C160"/>
+      <c s="17" r="D160"/>
+      <c s="17" r="E160"/>
     </row>
     <row r="161">
       <c t="s" s="7" r="A161">
-        <v>579</v>
-      </c>
-      <c t="s" s="26" r="B161">
-        <v>580</v>
-      </c>
-      <c t="s" s="17" r="C161">
-        <v>579</v>
-      </c>
-      <c s="26" r="D161"/>
-      <c s="26" r="E161"/>
+        <v>581</v>
+      </c>
+      <c t="s" s="25" r="B161">
+        <v>582</v>
+      </c>
+      <c t="s" s="18" r="C161">
+        <v>581</v>
+      </c>
+      <c s="25" r="D161"/>
+      <c s="25" r="E161"/>
     </row>
     <row r="162">
       <c s="7" r="A162"/>
@@ -5256,13 +5437,13 @@
     </row>
     <row r="163">
       <c t="s" s="7" r="A163">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c t="s" s="29" r="B163">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c t="s" s="27" r="C163">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c s="29" r="D163"/>
       <c s="29" r="E163"/>
@@ -5270,10 +5451,10 @@
     <row r="164">
       <c s="7" r="A164"/>
       <c t="s" s="29" r="B164">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c t="s" s="27" r="C164">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c s="29" r="D164"/>
       <c s="29" r="E164"/>
@@ -5287,342 +5468,342 @@
     </row>
     <row r="166">
       <c t="s" s="7" r="A166">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c t="s" s="23" r="B166">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c t="s" s="23" r="C166">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c t="s" s="5" r="D166">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c t="s" s="5" r="E166">
-        <v>590</v>
+        <v>592</v>
       </c>
     </row>
     <row r="167">
       <c s="7" r="A167"/>
       <c t="s" s="23" r="B167">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c t="s" s="23" r="C167">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c t="s" s="5" r="D167">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c t="s" s="5" r="E167">
-        <v>593</v>
+        <v>595</v>
       </c>
     </row>
     <row r="168">
       <c s="7" r="A168"/>
       <c t="s" s="23" r="B168">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c t="s" s="23" r="C168">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c t="s" s="5" r="D168">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c t="s" s="5" r="E168">
-        <v>597</v>
+        <v>599</v>
       </c>
     </row>
     <row r="169">
       <c s="7" r="A169"/>
       <c t="s" s="23" r="B169">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c t="s" s="23" r="C169">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c t="s" s="5" r="D169">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c t="s" s="5" r="E169">
-        <v>601</v>
+        <v>603</v>
       </c>
     </row>
     <row r="170">
       <c s="7" r="A170"/>
       <c t="s" s="11" r="B170">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c t="s" s="11" r="C170">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c t="s" s="5" r="D170">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c t="s" s="5" r="E170">
-        <v>605</v>
+        <v>607</v>
       </c>
     </row>
     <row r="171">
       <c s="7" r="A171"/>
       <c t="s" s="11" r="B171">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c t="s" s="11" r="C171">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c t="s" s="5" r="D171">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c t="s" s="5" r="E171">
-        <v>609</v>
+        <v>611</v>
       </c>
     </row>
     <row r="172">
       <c s="7" r="A172"/>
       <c t="s" s="11" r="B172">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c t="s" s="11" r="C172">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c t="s" s="5" r="D172">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c t="s" s="5" r="E172">
-        <v>613</v>
+        <v>615</v>
       </c>
     </row>
     <row r="173">
       <c s="7" r="A173"/>
       <c t="s" s="11" r="B173">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c t="s" s="11" r="C173">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c t="s" s="5" r="D173">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c t="s" s="5" r="E173">
-        <v>617</v>
+        <v>619</v>
       </c>
     </row>
     <row r="174">
       <c s="7" r="A174"/>
       <c t="s" s="11" r="B174">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c t="s" s="11" r="C174">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c t="s" s="5" r="D174">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c t="s" s="5" r="E174">
-        <v>621</v>
+        <v>623</v>
       </c>
     </row>
     <row r="175">
       <c s="7" r="A175"/>
       <c t="s" s="11" r="B175">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c t="s" s="11" r="C175">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c t="s" s="5" r="D175">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c t="s" s="5" r="E175">
-        <v>625</v>
+        <v>627</v>
       </c>
     </row>
     <row r="176">
       <c s="7" r="A176"/>
       <c t="s" s="11" r="B176">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c t="s" s="11" r="C176">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c t="s" s="5" r="D176">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c t="s" s="5" r="E176">
-        <v>629</v>
+        <v>631</v>
       </c>
     </row>
     <row r="177">
       <c s="7" r="A177"/>
       <c t="s" s="5" r="B177">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c t="s" s="11" r="C177">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c t="s" s="5" r="D177">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c t="s" s="5" r="E177">
-        <v>633</v>
+        <v>635</v>
       </c>
     </row>
     <row r="178">
       <c s="7" r="A178"/>
       <c t="s" s="5" r="B178">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c t="s" s="11" r="C178">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c t="s" s="5" r="D178">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c t="s" s="5" r="E178">
-        <v>637</v>
+        <v>639</v>
       </c>
     </row>
     <row r="179">
       <c s="7" r="A179"/>
       <c t="s" s="5" r="B179">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c t="s" s="11" r="C179">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c t="s" s="5" r="D179">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c t="s" s="5" r="E179">
-        <v>641</v>
+        <v>643</v>
       </c>
     </row>
     <row r="180">
       <c s="7" r="A180"/>
       <c t="s" s="5" r="B180">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c t="s" s="11" r="C180">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c t="s" s="5" r="D180">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c t="s" s="5" r="E180">
-        <v>645</v>
+        <v>647</v>
       </c>
     </row>
     <row r="181">
       <c s="7" r="A181"/>
       <c t="s" s="5" r="B181">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c t="s" s="11" r="C181">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c t="s" s="5" r="D181">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c t="s" s="5" r="E181">
-        <v>649</v>
+        <v>651</v>
       </c>
     </row>
     <row r="182">
       <c s="7" r="A182"/>
       <c t="s" s="5" r="B182">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c t="s" s="11" r="C182">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c t="s" s="5" r="D182">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c t="s" s="5" r="E182">
-        <v>653</v>
+        <v>655</v>
       </c>
     </row>
     <row r="183">
       <c s="7" r="A183"/>
       <c s="14" r="B183"/>
-      <c s="25" r="C183"/>
+      <c s="26" r="C183"/>
       <c s="14" r="D183"/>
       <c s="14" r="E183"/>
     </row>
     <row r="184">
       <c t="s" s="7" r="A184">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c t="s" s="23" r="B184">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c t="s" s="5" r="C184">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c t="s" s="5" r="D184">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c t="s" s="5" r="E184">
-        <v>593</v>
+        <v>595</v>
       </c>
     </row>
     <row r="185">
       <c s="7" r="A185"/>
       <c t="s" s="5" r="B185">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c t="s" s="11" r="C185">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c t="s" s="5" r="D185">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c t="s" s="5" r="E185">
-        <v>597</v>
+        <v>599</v>
       </c>
     </row>
     <row r="186">
       <c t="s" s="5" r="B186">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c t="s" s="11" r="C186">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c t="s" s="5" r="D186">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c t="s" s="5" r="E186">
-        <v>660</v>
+        <v>662</v>
       </c>
     </row>
     <row r="187">
       <c s="7" r="A187"/>
       <c t="s" s="5" r="B187">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c t="s" s="11" r="C187">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c t="s" s="5" r="D187">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c t="s" s="5" r="E187">
-        <v>664</v>
+        <v>666</v>
       </c>
     </row>
     <row r="188">
       <c s="7" r="A188"/>
       <c t="s" s="5" r="B188">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c t="s" s="11" r="C188">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c t="s" s="5" r="D188">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c t="s" s="5" r="E188">
-        <v>668</v>
+        <v>670</v>
       </c>
     </row>
     <row r="189">
@@ -5634,109 +5815,109 @@
     </row>
     <row r="190">
       <c t="s" s="7" r="A190">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c t="s" s="5" r="B190">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c t="s" s="11" r="C190">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c t="s" s="5" r="D190">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c t="s" s="5" r="E190">
-        <v>672</v>
+        <v>674</v>
       </c>
     </row>
     <row r="191">
       <c s="7" r="A191"/>
       <c t="s" s="5" r="B191">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c t="s" s="11" r="C191">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c t="s" s="5" r="D191">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c t="s" s="5" r="E191">
-        <v>676</v>
+        <v>678</v>
       </c>
     </row>
     <row r="192">
       <c s="7" r="A192"/>
       <c t="s" s="5" r="B192">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c t="s" s="11" r="C192">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c t="s" s="5" r="D192">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c t="s" s="5" r="E192">
-        <v>680</v>
+        <v>682</v>
       </c>
     </row>
     <row r="193">
       <c s="7" r="A193"/>
       <c t="s" s="5" r="B193">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c t="s" s="11" r="C193">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c t="s" s="5" r="D193">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c t="s" s="5" r="E193">
-        <v>684</v>
+        <v>686</v>
       </c>
     </row>
     <row r="194">
       <c s="7" r="A194"/>
       <c t="s" s="5" r="B194">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c t="s" s="11" r="C194">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c t="s" s="5" r="D194">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c t="s" s="5" r="E194">
-        <v>688</v>
+        <v>690</v>
       </c>
     </row>
     <row r="195">
       <c s="7" r="A195"/>
       <c t="s" s="5" r="B195">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c t="s" s="11" r="C195">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c t="s" s="5" r="D195">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c t="s" s="5" r="E195">
-        <v>692</v>
+        <v>694</v>
       </c>
     </row>
     <row r="196">
       <c s="7" r="A196"/>
       <c t="s" s="5" r="B196">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c t="s" s="11" r="C196">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c t="s" s="5" r="D196">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c t="s" s="5" r="E196">
-        <v>696</v>
+        <v>698</v>
       </c>
     </row>
     <row r="197">
@@ -5748,34 +5929,34 @@
     </row>
     <row r="198">
       <c t="s" s="7" r="A198">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c t="s" s="5" r="B198">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c t="s" s="11" r="C198">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c t="s" s="5" r="D198">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c t="s" s="5" r="E198">
-        <v>701</v>
+        <v>703</v>
       </c>
     </row>
     <row r="199">
       <c s="7" r="A199"/>
       <c t="s" s="5" r="B199">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c t="s" s="11" r="C199">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c t="s" s="5" r="D199">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c t="s" s="5" r="E199">
-        <v>704</v>
+        <v>706</v>
       </c>
     </row>
     <row r="200">
@@ -5787,127 +5968,127 @@
     </row>
     <row r="201">
       <c t="s" s="7" r="A201">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c t="s" s="5" r="B201">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c t="s" s="11" r="C201">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c t="s" s="5" r="D201">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c t="s" s="5" r="E201">
-        <v>709</v>
+        <v>711</v>
       </c>
     </row>
     <row r="202">
       <c s="7" r="A202"/>
       <c t="s" s="5" r="B202">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c t="s" s="11" r="C202">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c t="s" s="5" r="D202">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c t="s" s="5" r="E202">
-        <v>713</v>
+        <v>715</v>
       </c>
     </row>
     <row r="203">
       <c s="7" r="A203"/>
       <c t="s" s="5" r="B203">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c t="s" s="11" r="C203">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c t="s" s="5" r="D203">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c t="s" s="5" r="E203">
-        <v>717</v>
+        <v>719</v>
       </c>
     </row>
     <row r="204">
       <c s="7" r="A204"/>
       <c t="s" s="5" r="B204">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c t="s" s="11" r="C204">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c t="s" s="5" r="D204">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c t="s" s="5" r="E204">
-        <v>721</v>
+        <v>723</v>
       </c>
     </row>
     <row r="205">
       <c s="7" r="A205"/>
       <c s="14" r="B205"/>
-      <c s="25" r="C205"/>
+      <c s="26" r="C205"/>
       <c s="14" r="D205"/>
       <c s="14" r="E205"/>
     </row>
     <row r="206">
       <c t="s" s="7" r="A206">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c t="s" s="5" r="B206">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c t="s" s="11" r="C206">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c t="s" s="5" r="D206">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c t="s" s="5" r="E206">
-        <v>726</v>
+        <v>728</v>
       </c>
     </row>
     <row r="207">
       <c s="7" r="A207"/>
       <c t="s" s="5" r="B207">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c t="s" s="11" r="C207">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c t="s" s="5" r="D207">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c t="s" s="5" r="E207">
-        <v>730</v>
+        <v>732</v>
       </c>
     </row>
     <row r="208">
       <c s="7" r="A208"/>
       <c s="14" r="B208"/>
-      <c s="25" r="C208"/>
+      <c s="26" r="C208"/>
       <c s="14" r="D208"/>
       <c s="14" r="E208"/>
     </row>
     <row r="209">
       <c t="s" s="7" r="A209">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c t="s" s="5" r="B209">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c t="s" s="11" r="C209">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c t="s" s="5" r="D209">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c t="s" s="5" r="E209">
-        <v>735</v>
+        <v>737</v>
       </c>
     </row>
     <row r="210">
@@ -5919,71 +6100,95 @@
     </row>
     <row r="211">
       <c t="s" s="7" r="A211">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c t="s" s="5" r="B211">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c t="s" s="11" r="C211">
-        <v>738</v>
-      </c>
-      <c s="19" r="D211"/>
-      <c s="19" r="E211"/>
+        <v>740</v>
+      </c>
+      <c t="s" s="5" r="D211">
+        <v>741</v>
+      </c>
+      <c t="s" s="5" r="E211">
+        <v>742</v>
+      </c>
     </row>
     <row r="212">
       <c s="7" r="A212"/>
       <c t="s" s="5" r="B212">
-        <v>739</v>
+        <v>743</v>
       </c>
       <c t="s" s="11" r="C212">
-        <v>740</v>
-      </c>
-      <c s="19" r="D212"/>
-      <c s="19" r="E212"/>
+        <v>744</v>
+      </c>
+      <c t="s" s="5" r="D212">
+        <v>745</v>
+      </c>
+      <c t="s" s="5" r="E212">
+        <v>746</v>
+      </c>
     </row>
     <row r="213">
       <c s="7" r="A213"/>
       <c t="s" s="5" r="B213">
-        <v>741</v>
+        <v>747</v>
       </c>
       <c t="s" s="11" r="C213">
-        <v>742</v>
-      </c>
-      <c s="19" r="D213"/>
-      <c s="19" r="E213"/>
+        <v>748</v>
+      </c>
+      <c t="s" s="5" r="D213">
+        <v>749</v>
+      </c>
+      <c t="s" s="5" r="E213">
+        <v>750</v>
+      </c>
     </row>
     <row r="214">
       <c s="7" r="A214"/>
       <c t="s" s="5" r="B214">
-        <v>743</v>
+        <v>751</v>
       </c>
       <c t="s" s="11" r="C214">
-        <v>744</v>
-      </c>
-      <c s="19" r="D214"/>
-      <c s="19" r="E214"/>
+        <v>752</v>
+      </c>
+      <c t="s" s="5" r="D214">
+        <v>753</v>
+      </c>
+      <c t="s" s="5" r="E214">
+        <v>754</v>
+      </c>
     </row>
     <row r="215">
       <c s="7" r="A215"/>
       <c t="s" s="5" r="B215">
-        <v>745</v>
+        <v>755</v>
       </c>
       <c t="s" s="11" r="C215">
-        <v>746</v>
-      </c>
-      <c s="19" r="D215"/>
-      <c s="19" r="E215"/>
+        <v>756</v>
+      </c>
+      <c t="s" s="5" r="D215">
+        <v>757</v>
+      </c>
+      <c t="s" s="5" r="E215">
+        <v>758</v>
+      </c>
     </row>
     <row r="216">
       <c s="7" r="A216"/>
       <c t="s" s="5" r="B216">
-        <v>747</v>
+        <v>759</v>
       </c>
       <c t="s" s="11" r="C216">
-        <v>748</v>
-      </c>
-      <c s="19" r="D216"/>
-      <c s="19" r="E216"/>
+        <v>760</v>
+      </c>
+      <c t="s" s="16" r="D216">
+        <v>761</v>
+      </c>
+      <c t="s" s="16" r="E216">
+        <v>762</v>
+      </c>
     </row>
     <row r="217">
       <c s="15" r="A217"/>
@@ -5994,75 +6199,95 @@
     </row>
     <row r="218">
       <c t="s" s="7" r="A218">
-        <v>749</v>
+        <v>763</v>
       </c>
       <c t="s" s="5" r="B218">
-        <v>750</v>
+        <v>764</v>
       </c>
       <c t="s" s="5" r="C218">
-        <v>751</v>
+        <v>765</v>
       </c>
       <c t="s" s="5" r="D218">
-        <v>752</v>
+        <v>766</v>
       </c>
       <c t="s" s="5" r="E218">
-        <v>753</v>
+        <v>767</v>
       </c>
     </row>
     <row r="219">
       <c s="7" r="A219"/>
       <c t="s" s="5" r="B219">
-        <v>754</v>
+        <v>768</v>
       </c>
       <c t="s" s="11" r="C219">
-        <v>755</v>
-      </c>
-      <c s="19" r="D219"/>
-      <c s="19" r="E219"/>
+        <v>769</v>
+      </c>
+      <c t="s" s="5" r="D219">
+        <v>770</v>
+      </c>
+      <c t="s" s="5" r="E219">
+        <v>771</v>
+      </c>
     </row>
     <row r="220">
       <c s="7" r="A220"/>
       <c t="s" s="5" r="B220">
-        <v>756</v>
+        <v>772</v>
       </c>
       <c t="s" s="11" r="C220">
-        <v>757</v>
-      </c>
-      <c s="19" r="D220"/>
-      <c s="19" r="E220"/>
+        <v>773</v>
+      </c>
+      <c t="s" s="5" r="D220">
+        <v>774</v>
+      </c>
+      <c t="s" s="5" r="E220">
+        <v>775</v>
+      </c>
     </row>
     <row r="221">
       <c s="7" r="A221"/>
       <c t="s" s="5" r="B221">
-        <v>758</v>
+        <v>776</v>
       </c>
       <c t="s" s="11" r="C221">
-        <v>759</v>
-      </c>
-      <c s="19" r="D221"/>
-      <c s="19" r="E221"/>
+        <v>777</v>
+      </c>
+      <c t="s" s="5" r="D221">
+        <v>778</v>
+      </c>
+      <c t="s" s="5" r="E221">
+        <v>779</v>
+      </c>
     </row>
     <row r="222">
       <c s="7" r="A222"/>
       <c t="s" s="5" r="B222">
-        <v>760</v>
+        <v>780</v>
       </c>
       <c t="s" s="11" r="C222">
-        <v>528</v>
-      </c>
-      <c s="19" r="D222"/>
-      <c s="19" r="E222"/>
+        <v>530</v>
+      </c>
+      <c t="s" s="5" r="D222">
+        <v>108</v>
+      </c>
+      <c t="s" s="5" r="E222">
+        <v>532</v>
+      </c>
     </row>
     <row r="223">
       <c s="7" r="A223"/>
       <c t="s" s="5" r="B223">
-        <v>761</v>
+        <v>781</v>
       </c>
       <c t="s" s="11" r="C223">
-        <v>762</v>
-      </c>
-      <c s="19" r="D223"/>
-      <c s="19" r="E223"/>
+        <v>782</v>
+      </c>
+      <c t="s" s="5" r="D223">
+        <v>783</v>
+      </c>
+      <c t="s" s="5" r="E223">
+        <v>784</v>
+      </c>
     </row>
     <row r="224">
       <c s="15" r="A224"/>
@@ -6073,225 +6298,305 @@
     </row>
     <row r="225">
       <c t="s" s="7" r="A225">
-        <v>763</v>
+        <v>785</v>
       </c>
       <c t="s" s="5" r="B225">
-        <v>764</v>
+        <v>786</v>
       </c>
       <c t="s" s="11" r="C225">
-        <v>765</v>
-      </c>
-      <c s="19" r="D225"/>
-      <c s="19" r="E225"/>
+        <v>787</v>
+      </c>
+      <c t="s" s="5" r="D225">
+        <v>788</v>
+      </c>
+      <c t="s" s="5" r="E225">
+        <v>789</v>
+      </c>
     </row>
     <row r="226">
       <c s="7" r="A226"/>
       <c t="s" s="5" r="B226">
-        <v>766</v>
+        <v>790</v>
       </c>
       <c t="s" s="11" r="C226">
-        <v>767</v>
-      </c>
-      <c s="19" r="D226"/>
-      <c s="19" r="E226"/>
+        <v>791</v>
+      </c>
+      <c t="s" s="5" r="D226">
+        <v>792</v>
+      </c>
+      <c t="s" s="5" r="E226">
+        <v>793</v>
+      </c>
     </row>
     <row r="227">
       <c s="7" r="A227"/>
       <c t="s" s="5" r="B227">
-        <v>768</v>
+        <v>794</v>
       </c>
       <c t="s" s="11" r="C227">
-        <v>769</v>
-      </c>
-      <c s="19" r="D227"/>
-      <c s="19" r="E227"/>
+        <v>795</v>
+      </c>
+      <c t="s" s="5" r="D227">
+        <v>796</v>
+      </c>
+      <c t="s" s="5" r="E227">
+        <v>797</v>
+      </c>
     </row>
     <row r="228">
       <c s="7" r="A228"/>
       <c t="s" s="5" r="B228">
-        <v>770</v>
+        <v>798</v>
       </c>
       <c t="s" s="11" r="C228">
-        <v>771</v>
-      </c>
-      <c s="19" r="D228"/>
-      <c s="19" r="E228"/>
+        <v>799</v>
+      </c>
+      <c t="s" s="5" r="D228">
+        <v>800</v>
+      </c>
+      <c t="s" s="5" r="E228">
+        <v>800</v>
+      </c>
     </row>
     <row r="229">
       <c s="7" r="A229"/>
       <c t="s" s="5" r="B229">
-        <v>772</v>
+        <v>801</v>
       </c>
       <c t="s" s="11" r="C229">
-        <v>773</v>
-      </c>
-      <c s="19" r="D229"/>
-      <c s="19" r="E229"/>
+        <v>802</v>
+      </c>
+      <c t="s" s="5" r="D229">
+        <v>803</v>
+      </c>
+      <c t="s" s="5" r="E229">
+        <v>804</v>
+      </c>
     </row>
     <row r="230">
       <c s="7" r="A230"/>
       <c t="s" s="5" r="B230">
-        <v>774</v>
+        <v>805</v>
       </c>
       <c t="s" s="11" r="C230">
-        <v>775</v>
-      </c>
-      <c s="19" r="D230"/>
-      <c s="19" r="E230"/>
+        <v>806</v>
+      </c>
+      <c t="s" s="5" r="D230">
+        <v>807</v>
+      </c>
+      <c t="s" s="5" r="E230">
+        <v>808</v>
+      </c>
     </row>
     <row r="231">
       <c s="7" r="A231"/>
       <c t="s" s="5" r="B231">
-        <v>776</v>
+        <v>809</v>
       </c>
       <c t="s" s="11" r="C231">
-        <v>777</v>
-      </c>
-      <c s="19" r="D231"/>
-      <c s="19" r="E231"/>
+        <v>810</v>
+      </c>
+      <c t="s" s="5" r="D231">
+        <v>811</v>
+      </c>
+      <c t="s" s="5" r="E231">
+        <v>812</v>
+      </c>
     </row>
     <row r="232">
       <c s="7" r="A232"/>
       <c t="s" s="5" r="B232">
-        <v>778</v>
+        <v>813</v>
       </c>
       <c t="s" s="11" r="C232">
-        <v>779</v>
-      </c>
-      <c s="19" r="D232"/>
-      <c s="19" r="E232"/>
+        <v>814</v>
+      </c>
+      <c t="s" s="5" r="D232">
+        <v>815</v>
+      </c>
+      <c t="s" s="5" r="E232">
+        <v>816</v>
+      </c>
     </row>
     <row r="233">
       <c s="7" r="A233"/>
       <c t="s" s="5" r="B233">
-        <v>780</v>
+        <v>817</v>
       </c>
       <c t="s" s="11" r="C233">
-        <v>781</v>
-      </c>
-      <c s="19" r="D233"/>
-      <c s="19" r="E233"/>
+        <v>818</v>
+      </c>
+      <c t="s" s="5" r="D233">
+        <v>819</v>
+      </c>
+      <c t="s" s="5" r="E233">
+        <v>820</v>
+      </c>
     </row>
     <row r="234">
       <c s="7" r="A234"/>
       <c t="s" s="5" r="B234">
-        <v>782</v>
+        <v>821</v>
       </c>
       <c t="s" s="11" r="C234">
-        <v>783</v>
-      </c>
-      <c s="19" r="D234"/>
-      <c s="19" r="E234"/>
+        <v>822</v>
+      </c>
+      <c t="s" s="5" r="D234">
+        <v>823</v>
+      </c>
+      <c t="s" s="5" r="E234">
+        <v>824</v>
+      </c>
     </row>
     <row r="235">
       <c s="7" r="A235"/>
       <c t="s" s="5" r="B235">
-        <v>784</v>
+        <v>825</v>
       </c>
       <c t="s" s="11" r="C235">
-        <v>785</v>
-      </c>
-      <c s="19" r="D235"/>
-      <c s="19" r="E235"/>
+        <v>826</v>
+      </c>
+      <c t="s" s="5" r="D235">
+        <v>827</v>
+      </c>
+      <c t="s" s="5" r="E235">
+        <v>828</v>
+      </c>
     </row>
     <row r="236">
       <c s="7" r="A236"/>
       <c t="s" s="5" r="B236">
-        <v>786</v>
+        <v>829</v>
       </c>
       <c t="s" s="11" r="C236">
-        <v>787</v>
-      </c>
-      <c s="19" r="D236"/>
-      <c s="19" r="E236"/>
+        <v>830</v>
+      </c>
+      <c t="s" s="5" r="D236">
+        <v>831</v>
+      </c>
+      <c t="s" s="5" r="E236">
+        <v>832</v>
+      </c>
     </row>
     <row r="237">
       <c s="7" r="A237"/>
       <c t="s" s="5" r="B237">
-        <v>788</v>
+        <v>833</v>
       </c>
       <c t="s" s="11" r="C237">
-        <v>789</v>
-      </c>
-      <c s="19" r="D237"/>
-      <c s="19" r="E237"/>
+        <v>834</v>
+      </c>
+      <c t="s" s="5" r="D237">
+        <v>834</v>
+      </c>
+      <c t="s" s="5" r="E237">
+        <v>834</v>
+      </c>
     </row>
     <row r="238">
       <c s="7" r="A238"/>
       <c t="s" s="5" r="B238">
-        <v>790</v>
+        <v>835</v>
       </c>
       <c t="s" s="11" r="C238">
-        <v>791</v>
-      </c>
-      <c s="19" r="D238"/>
-      <c s="19" r="E238"/>
+        <v>836</v>
+      </c>
+      <c t="s" s="5" r="D238">
+        <v>837</v>
+      </c>
+      <c t="s" s="5" r="E238">
+        <v>838</v>
+      </c>
     </row>
     <row r="239">
       <c s="7" r="A239"/>
       <c t="s" s="5" r="B239">
-        <v>792</v>
+        <v>839</v>
       </c>
       <c t="s" s="11" r="C239">
-        <v>793</v>
-      </c>
-      <c s="19" r="D239"/>
-      <c s="19" r="E239"/>
+        <v>840</v>
+      </c>
+      <c t="s" s="5" r="D239">
+        <v>841</v>
+      </c>
+      <c t="s" s="5" r="E239">
+        <v>842</v>
+      </c>
     </row>
     <row r="240">
       <c s="7" r="A240"/>
       <c t="s" s="5" r="B240">
-        <v>794</v>
+        <v>843</v>
       </c>
       <c t="s" s="11" r="C240">
-        <v>795</v>
-      </c>
-      <c s="19" r="D240"/>
-      <c s="19" r="E240"/>
+        <v>844</v>
+      </c>
+      <c t="s" s="5" r="D240">
+        <v>845</v>
+      </c>
+      <c t="s" s="5" r="E240">
+        <v>846</v>
+      </c>
     </row>
     <row r="241">
       <c s="7" r="A241"/>
       <c t="s" s="5" r="B241">
-        <v>796</v>
+        <v>847</v>
       </c>
       <c t="s" s="11" r="C241">
-        <v>797</v>
-      </c>
-      <c s="19" r="D241"/>
-      <c s="19" r="E241"/>
+        <v>848</v>
+      </c>
+      <c t="s" s="5" r="D241">
+        <v>849</v>
+      </c>
+      <c t="s" s="5" r="E241">
+        <v>850</v>
+      </c>
     </row>
     <row r="242">
       <c s="7" r="A242"/>
       <c t="s" s="5" r="B242">
-        <v>798</v>
+        <v>851</v>
       </c>
       <c t="s" s="11" r="C242">
-        <v>799</v>
-      </c>
-      <c s="19" r="D242"/>
-      <c s="19" r="E242"/>
+        <v>852</v>
+      </c>
+      <c t="s" s="5" r="D242">
+        <v>853</v>
+      </c>
+      <c t="s" s="5" r="E242">
+        <v>854</v>
+      </c>
     </row>
     <row r="243">
       <c s="7" r="A243"/>
       <c t="s" s="5" r="B243">
-        <v>800</v>
+        <v>855</v>
       </c>
       <c t="s" s="11" r="C243">
-        <v>801</v>
-      </c>
-      <c s="19" r="D243"/>
-      <c s="19" r="E243"/>
+        <v>856</v>
+      </c>
+      <c t="s" s="5" r="D243">
+        <v>857</v>
+      </c>
+      <c t="s" s="5" r="E243">
+        <v>858</v>
+      </c>
     </row>
     <row r="244">
       <c s="7" r="A244"/>
       <c t="s" s="5" r="B244">
-        <v>802</v>
+        <v>859</v>
       </c>
       <c t="s" s="11" r="C244">
-        <v>803</v>
-      </c>
-      <c s="19" r="D244"/>
-      <c s="19" r="E244"/>
+        <v>860</v>
+      </c>
+      <c t="s" s="5" r="D244">
+        <v>861</v>
+      </c>
+      <c t="s" s="5" r="E244">
+        <v>862</v>
+      </c>
     </row>
     <row r="245">
       <c s="7" r="A245"/>
@@ -6302,13 +6607,13 @@
     </row>
     <row r="246">
       <c t="s" s="15" r="A246">
-        <v>804</v>
+        <v>863</v>
       </c>
       <c t="s" s="12" r="B246">
-        <v>805</v>
+        <v>864</v>
       </c>
       <c t="s" s="21" r="C246">
-        <v>806</v>
+        <v>865</v>
       </c>
       <c s="12" r="D246"/>
       <c s="12" r="E246"/>
@@ -6316,10 +6621,10 @@
     <row r="247">
       <c s="15" r="A247"/>
       <c t="s" s="12" r="B247">
-        <v>807</v>
+        <v>866</v>
       </c>
       <c t="s" s="21" r="C247">
-        <v>806</v>
+        <v>865</v>
       </c>
       <c s="12" r="D247"/>
       <c s="12" r="E247"/>
@@ -6327,10 +6632,10 @@
     <row r="248">
       <c s="15" r="A248"/>
       <c t="s" s="12" r="B248">
-        <v>808</v>
+        <v>867</v>
       </c>
       <c t="s" s="21" r="C248">
-        <v>806</v>
+        <v>865</v>
       </c>
       <c s="12" r="D248"/>
       <c s="12" r="E248"/>
@@ -6338,10 +6643,10 @@
     <row r="249">
       <c s="15" r="A249"/>
       <c t="s" s="12" r="B249">
-        <v>809</v>
+        <v>868</v>
       </c>
       <c t="s" s="21" r="C249">
-        <v>806</v>
+        <v>865</v>
       </c>
       <c s="12" r="D249"/>
       <c s="12" r="E249"/>
@@ -6349,10 +6654,10 @@
     <row r="250">
       <c s="15" r="A250"/>
       <c t="s" s="12" r="B250">
-        <v>810</v>
+        <v>869</v>
       </c>
       <c t="s" s="21" r="C250">
-        <v>806</v>
+        <v>865</v>
       </c>
       <c s="12" r="D250"/>
       <c s="12" r="E250"/>
@@ -6360,10 +6665,10 @@
     <row r="251">
       <c s="15" r="A251"/>
       <c t="s" s="12" r="B251">
-        <v>811</v>
+        <v>870</v>
       </c>
       <c t="s" s="21" r="C251">
-        <v>806</v>
+        <v>865</v>
       </c>
       <c s="12" r="D251"/>
       <c s="12" r="E251"/>
@@ -6371,10 +6676,10 @@
     <row r="252">
       <c s="15" r="A252"/>
       <c t="s" s="12" r="B252">
-        <v>812</v>
+        <v>871</v>
       </c>
       <c t="s" s="21" r="C252">
-        <v>806</v>
+        <v>865</v>
       </c>
       <c s="12" r="D252"/>
       <c s="12" r="E252"/>
@@ -6382,10 +6687,10 @@
     <row r="253">
       <c s="15" r="A253"/>
       <c t="s" s="12" r="B253">
-        <v>813</v>
+        <v>872</v>
       </c>
       <c t="s" s="21" r="C253">
-        <v>806</v>
+        <v>865</v>
       </c>
       <c s="12" r="D253"/>
       <c s="12" r="E253"/>
@@ -6483,17 +6788,17 @@
   <sheetData>
     <row customHeight="1" r="1" ht="112.5">
       <c t="s" s="2" r="A1">
-        <v>814</v>
+        <v>873</v>
       </c>
     </row>
     <row customHeight="1" r="2" ht="112.5">
       <c t="s" s="3" r="A2">
-        <v>815</v>
+        <v>874</v>
       </c>
     </row>
     <row customHeight="1" r="3" ht="112.5">
       <c t="s" s="8" r="A3">
-        <v>816</v>
+        <v>875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EWD-22707 - 500 server error localization
Former-commit-id: 4120d576f147d57f0a00b77efe580b79a022fba6
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="965">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="984">
   <si>
     <t>Page</t>
   </si>
@@ -697,6 +697,12 @@
     <t>Erneute Veröffentlichung läuft...</t>
   </si>
   <si>
+    <t>copyLinkTitle</t>
+  </si>
+  <si>
+    <t>Copy link</t>
+  </si>
+  <si>
     <t>CreateObjective</t>
   </si>
   <si>
@@ -1722,10 +1728,10 @@
     <t>Something is not right</t>
   </si>
   <si>
-    <t>Er is iets niet goed.</t>
-  </si>
-  <si>
-    <t>Etwas ist nicht korrekt.</t>
+    <t>Er is iets niet goed</t>
+  </si>
+  <si>
+    <t>Etwas ist nicht korrekt</t>
   </si>
   <si>
     <t>serverErrorDescription</t>
@@ -1904,6 +1910,42 @@
   </si>
   <si>
     <t>Geben Sie eine gültige E-Mail-Adresse ein</t>
+  </si>
+  <si>
+    <t>EnterValidFullName</t>
+  </si>
+  <si>
+    <t>Enter a valid full name</t>
+  </si>
+  <si>
+    <t>Voer een geldig volledige naam in</t>
+  </si>
+  <si>
+    <t>Geben Sie eine gültige Vollständiger Name ein</t>
+  </si>
+  <si>
+    <t>EnterValidOrganization</t>
+  </si>
+  <si>
+    <t>Enter a valid organization name</t>
+  </si>
+  <si>
+    <t>Voer een geldig telefoonnummer in</t>
+  </si>
+  <si>
+    <t>Geben Sie eine gültige Telefonnummer ein</t>
+  </si>
+  <si>
+    <t>EnterValidPhoneNumber</t>
+  </si>
+  <si>
+    <t>Enter a valid phon number</t>
+  </si>
+  <si>
+    <t>Voer een geldig naam van organisatie in</t>
+  </si>
+  <si>
+    <t>Geben Sie eine gültige Name der Organisiation ein</t>
   </si>
   <si>
     <t>AccountAlreadyExists</t>
@@ -2933,6 +2975,21 @@
   </si>
   <si>
     <t>Ausblenden</t>
+  </si>
+  <si>
+    <t>sorryPage</t>
+  </si>
+  <si>
+    <t>publishIsInProgressTitle</t>
+  </si>
+  <si>
+    <t>This learning experience is being updated</t>
+  </si>
+  <si>
+    <t>publishIsInProgressText</t>
+  </si>
+  <si>
+    <t>Please, try again after few minutes</t>
   </si>
   <si>
     <t>Translated OK</t>
@@ -4328,617 +4385,613 @@
     </row>
     <row r="60">
       <c s="11" r="A60"/>
-      <c s="11" r="B60"/>
-      <c s="11" r="C60"/>
-      <c s="11" r="D60"/>
-      <c s="11" r="E60"/>
+      <c t="s" s="2" r="B60">
+        <v>227</v>
+      </c>
+      <c t="s" s="18" r="C60">
+        <v>228</v>
+      </c>
+      <c s="2" r="D60"/>
+      <c s="2" r="E60"/>
     </row>
     <row r="61">
-      <c t="s" s="11" r="A61">
-        <v>227</v>
-      </c>
-      <c t="s" s="7" r="B61">
-        <v>228</v>
-      </c>
-      <c t="s" s="7" r="C61">
+      <c s="11" r="A61"/>
+      <c s="11" r="B61"/>
+      <c s="11" r="C61"/>
+      <c s="11" r="D61"/>
+      <c s="11" r="E61"/>
+    </row>
+    <row r="62">
+      <c t="s" s="11" r="A62">
         <v>229</v>
       </c>
-      <c t="s" s="7" r="D61">
+      <c t="s" s="7" r="B62">
         <v>230</v>
       </c>
-      <c t="s" s="7" r="E61">
+      <c t="s" s="7" r="C62">
         <v>231</v>
       </c>
-    </row>
-    <row r="62">
-      <c s="11" r="A62"/>
-      <c t="s" s="7" r="B62">
+      <c t="s" s="7" r="D62">
         <v>232</v>
       </c>
-      <c t="s" s="7" r="C62">
+      <c t="s" s="7" r="E62">
         <v>233</v>
       </c>
-      <c t="s" s="7" r="D62">
+    </row>
+    <row r="63">
+      <c s="11" r="A63"/>
+      <c t="s" s="7" r="B63">
         <v>234</v>
       </c>
-      <c t="s" s="7" r="E62">
+      <c t="s" s="7" r="C63">
         <v>235</v>
       </c>
-    </row>
-    <row r="64">
-      <c s="19" r="A64"/>
-      <c s="19" r="B64"/>
-      <c s="19" r="C64"/>
-      <c s="19" r="D64"/>
-      <c s="19" r="E64"/>
+      <c t="s" s="7" r="D63">
+        <v>236</v>
+      </c>
+      <c t="s" s="7" r="E63">
+        <v>237</v>
+      </c>
     </row>
     <row r="65">
-      <c t="s" s="11" r="A65">
-        <v>236</v>
-      </c>
-      <c t="s" s="7" r="B65">
-        <v>237</v>
-      </c>
-      <c t="s" s="7" r="C65">
+      <c s="19" r="A65"/>
+      <c s="19" r="B65"/>
+      <c s="19" r="C65"/>
+      <c s="19" r="D65"/>
+      <c s="19" r="E65"/>
+    </row>
+    <row r="66">
+      <c t="s" s="11" r="A66">
         <v>238</v>
       </c>
-      <c t="s" s="7" r="D65">
+      <c t="s" s="7" r="B66">
         <v>239</v>
       </c>
-      <c t="s" s="7" r="E65">
+      <c t="s" s="7" r="C66">
         <v>240</v>
       </c>
-    </row>
-    <row r="66">
-      <c s="11" r="A66"/>
-      <c t="s" s="7" r="B66">
+      <c t="s" s="7" r="D66">
         <v>241</v>
       </c>
-      <c t="s" s="7" r="C66">
+      <c t="s" s="7" r="E66">
         <v>242</v>
-      </c>
-      <c t="s" s="7" r="D66">
-        <v>243</v>
-      </c>
-      <c t="s" s="7" r="E66">
-        <v>244</v>
       </c>
     </row>
     <row r="67">
       <c s="11" r="A67"/>
       <c t="s" s="7" r="B67">
+        <v>243</v>
+      </c>
+      <c t="s" s="7" r="C67">
+        <v>244</v>
+      </c>
+      <c t="s" s="7" r="D67">
         <v>245</v>
       </c>
-      <c t="s" s="7" r="C67">
+      <c t="s" s="7" r="E67">
         <v>246</v>
-      </c>
-      <c t="s" s="7" r="D67">
-        <v>247</v>
-      </c>
-      <c t="s" s="7" r="E67">
-        <v>248</v>
       </c>
     </row>
     <row r="68">
       <c s="11" r="A68"/>
       <c t="s" s="7" r="B68">
+        <v>247</v>
+      </c>
+      <c t="s" s="7" r="C68">
+        <v>248</v>
+      </c>
+      <c t="s" s="7" r="D68">
         <v>249</v>
       </c>
-      <c t="s" s="7" r="C68">
+      <c t="s" s="7" r="E68">
         <v>250</v>
-      </c>
-      <c t="s" s="7" r="D68">
-        <v>251</v>
-      </c>
-      <c t="s" s="7" r="E68">
-        <v>252</v>
       </c>
     </row>
     <row r="69">
       <c s="11" r="A69"/>
       <c t="s" s="7" r="B69">
+        <v>251</v>
+      </c>
+      <c t="s" s="7" r="C69">
+        <v>252</v>
+      </c>
+      <c t="s" s="7" r="D69">
         <v>253</v>
       </c>
-      <c t="s" s="7" r="C69">
+      <c t="s" s="7" r="E69">
         <v>254</v>
-      </c>
-      <c t="s" s="7" r="D69">
-        <v>255</v>
-      </c>
-      <c t="s" s="7" r="E69">
-        <v>256</v>
       </c>
     </row>
     <row r="70">
       <c s="11" r="A70"/>
       <c t="s" s="7" r="B70">
+        <v>255</v>
+      </c>
+      <c t="s" s="7" r="C70">
+        <v>256</v>
+      </c>
+      <c t="s" s="7" r="D70">
         <v>257</v>
       </c>
-      <c t="s" s="7" r="C70">
+      <c t="s" s="7" r="E70">
         <v>258</v>
-      </c>
-      <c t="s" s="7" r="D70">
-        <v>259</v>
-      </c>
-      <c t="s" s="7" r="E70">
-        <v>260</v>
       </c>
     </row>
     <row r="71">
       <c s="11" r="A71"/>
-      <c s="11" r="B71"/>
-      <c s="11" r="C71"/>
-      <c s="11" r="D71"/>
-      <c s="11" r="E71"/>
+      <c t="s" s="7" r="B71">
+        <v>259</v>
+      </c>
+      <c t="s" s="7" r="C71">
+        <v>260</v>
+      </c>
+      <c t="s" s="7" r="D71">
+        <v>261</v>
+      </c>
+      <c t="s" s="7" r="E71">
+        <v>262</v>
+      </c>
     </row>
     <row r="72">
-      <c t="s" s="11" r="A72">
-        <v>261</v>
-      </c>
-      <c t="s" s="7" r="B72">
-        <v>262</v>
-      </c>
-      <c t="s" s="7" r="C72">
+      <c s="11" r="A72"/>
+      <c s="11" r="B72"/>
+      <c s="11" r="C72"/>
+      <c s="11" r="D72"/>
+      <c s="11" r="E72"/>
+    </row>
+    <row r="73">
+      <c t="s" s="11" r="A73">
         <v>263</v>
       </c>
-      <c t="s" s="7" r="D72">
+      <c t="s" s="7" r="B73">
         <v>264</v>
       </c>
-      <c t="s" s="7" r="E72">
+      <c t="s" s="7" r="C73">
         <v>265</v>
       </c>
-    </row>
-    <row r="73">
-      <c s="11" r="A73"/>
-      <c t="s" s="7" r="B73">
+      <c t="s" s="7" r="D73">
         <v>266</v>
       </c>
-      <c t="s" s="7" r="C73">
+      <c t="s" s="7" r="E73">
         <v>267</v>
-      </c>
-      <c t="s" s="7" r="D73">
-        <v>268</v>
-      </c>
-      <c t="s" s="7" r="E73">
-        <v>269</v>
       </c>
     </row>
     <row r="74">
       <c s="11" r="A74"/>
       <c t="s" s="7" r="B74">
+        <v>268</v>
+      </c>
+      <c t="s" s="7" r="C74">
+        <v>269</v>
+      </c>
+      <c t="s" s="7" r="D74">
         <v>270</v>
       </c>
-      <c t="s" s="7" r="C74">
+      <c t="s" s="7" r="E74">
         <v>271</v>
-      </c>
-      <c t="s" s="7" r="D74">
-        <v>272</v>
-      </c>
-      <c t="s" s="7" r="E74">
-        <v>273</v>
       </c>
     </row>
     <row r="75">
       <c s="11" r="A75"/>
       <c t="s" s="7" r="B75">
+        <v>272</v>
+      </c>
+      <c t="s" s="7" r="C75">
+        <v>273</v>
+      </c>
+      <c t="s" s="7" r="D75">
         <v>274</v>
       </c>
-      <c t="s" s="7" r="C75">
+      <c t="s" s="7" r="E75">
         <v>275</v>
-      </c>
-      <c t="s" s="7" r="D75">
-        <v>276</v>
-      </c>
-      <c t="s" s="7" r="E75">
-        <v>277</v>
       </c>
     </row>
     <row r="76">
       <c s="11" r="A76"/>
       <c t="s" s="7" r="B76">
+        <v>276</v>
+      </c>
+      <c t="s" s="7" r="C76">
+        <v>277</v>
+      </c>
+      <c t="s" s="7" r="D76">
         <v>278</v>
       </c>
-      <c t="s" s="7" r="C76">
+      <c t="s" s="7" r="E76">
         <v>279</v>
-      </c>
-      <c t="s" s="7" r="D76">
-        <v>280</v>
-      </c>
-      <c t="s" s="7" r="E76">
-        <v>281</v>
       </c>
     </row>
     <row r="77">
       <c s="11" r="A77"/>
       <c t="s" s="7" r="B77">
+        <v>280</v>
+      </c>
+      <c t="s" s="7" r="C77">
+        <v>281</v>
+      </c>
+      <c t="s" s="7" r="D77">
         <v>282</v>
       </c>
-      <c t="s" s="7" r="C77">
+      <c t="s" s="7" r="E77">
         <v>283</v>
-      </c>
-      <c t="s" s="7" r="D77">
-        <v>284</v>
-      </c>
-      <c t="s" s="7" r="E77">
-        <v>285</v>
       </c>
     </row>
     <row r="78">
       <c s="11" r="A78"/>
       <c t="s" s="7" r="B78">
+        <v>284</v>
+      </c>
+      <c t="s" s="7" r="C78">
+        <v>285</v>
+      </c>
+      <c t="s" s="7" r="D78">
         <v>286</v>
       </c>
-      <c t="s" s="7" r="C78">
+      <c t="s" s="7" r="E78">
         <v>287</v>
-      </c>
-      <c t="s" s="7" r="D78">
-        <v>288</v>
-      </c>
-      <c t="s" s="7" r="E78">
-        <v>289</v>
       </c>
     </row>
     <row r="79">
       <c s="11" r="A79"/>
       <c t="s" s="7" r="B79">
+        <v>288</v>
+      </c>
+      <c t="s" s="7" r="C79">
+        <v>289</v>
+      </c>
+      <c t="s" s="7" r="D79">
         <v>290</v>
       </c>
-      <c t="s" s="7" r="C79">
+      <c t="s" s="7" r="E79">
         <v>291</v>
-      </c>
-      <c t="s" s="7" r="D79">
-        <v>292</v>
-      </c>
-      <c t="s" s="7" r="E79">
-        <v>293</v>
       </c>
     </row>
     <row r="80">
       <c s="11" r="A80"/>
       <c t="s" s="7" r="B80">
+        <v>292</v>
+      </c>
+      <c t="s" s="7" r="C80">
+        <v>293</v>
+      </c>
+      <c t="s" s="7" r="D80">
         <v>294</v>
       </c>
-      <c t="s" s="7" r="C80">
+      <c t="s" s="7" r="E80">
         <v>295</v>
-      </c>
-      <c t="s" s="7" r="D80">
-        <v>296</v>
-      </c>
-      <c t="s" s="7" r="E80">
-        <v>297</v>
       </c>
     </row>
     <row r="81">
       <c s="11" r="A81"/>
-      <c s="11" r="B81"/>
-      <c s="11" r="C81"/>
-      <c s="11" r="D81"/>
-      <c s="11" r="E81"/>
+      <c t="s" s="7" r="B81">
+        <v>296</v>
+      </c>
+      <c t="s" s="7" r="C81">
+        <v>297</v>
+      </c>
+      <c t="s" s="7" r="D81">
+        <v>298</v>
+      </c>
+      <c t="s" s="7" r="E81">
+        <v>299</v>
+      </c>
     </row>
     <row r="82">
-      <c t="s" s="11" r="A82">
-        <v>298</v>
-      </c>
-      <c t="s" s="7" r="B82">
-        <v>299</v>
-      </c>
-      <c t="s" s="7" r="C82">
+      <c s="11" r="A82"/>
+      <c s="11" r="B82"/>
+      <c s="11" r="C82"/>
+      <c s="11" r="D82"/>
+      <c s="11" r="E82"/>
+    </row>
+    <row r="83">
+      <c t="s" s="11" r="A83">
         <v>300</v>
       </c>
-      <c t="s" s="7" r="D82">
+      <c t="s" s="7" r="B83">
         <v>301</v>
       </c>
-      <c t="s" s="7" r="E82">
+      <c t="s" s="7" r="C83">
         <v>302</v>
       </c>
-    </row>
-    <row r="83">
-      <c s="11" r="A83"/>
-      <c t="s" s="7" r="B83">
+      <c t="s" s="7" r="D83">
         <v>303</v>
       </c>
-      <c t="s" s="7" r="C83">
+      <c t="s" s="7" r="E83">
         <v>304</v>
       </c>
-      <c t="s" s="7" r="D83">
+    </row>
+    <row r="84">
+      <c s="11" r="A84"/>
+      <c t="s" s="7" r="B84">
         <v>305</v>
       </c>
-      <c t="s" s="7" r="E83">
+      <c t="s" s="7" r="C84">
         <v>306</v>
       </c>
-    </row>
-    <row r="84">
-      <c s="9" r="A84"/>
-      <c t="s" s="7" r="B84">
+      <c t="s" s="7" r="D84">
         <v>307</v>
       </c>
-      <c t="s" s="7" r="C84">
+      <c t="s" s="7" r="E84">
         <v>308</v>
-      </c>
-      <c t="s" s="7" r="D84">
-        <v>309</v>
-      </c>
-      <c t="s" s="7" r="E84">
-        <v>310</v>
       </c>
     </row>
     <row r="85">
       <c s="9" r="A85"/>
       <c t="s" s="7" r="B85">
+        <v>309</v>
+      </c>
+      <c t="s" s="7" r="C85">
+        <v>310</v>
+      </c>
+      <c t="s" s="7" r="D85">
         <v>311</v>
       </c>
-      <c t="s" s="7" r="C85">
+      <c t="s" s="7" r="E85">
         <v>312</v>
-      </c>
-      <c t="s" s="7" r="D85">
-        <v>313</v>
-      </c>
-      <c t="s" s="7" r="E85">
-        <v>314</v>
       </c>
     </row>
     <row r="86">
       <c s="9" r="A86"/>
       <c t="s" s="7" r="B86">
+        <v>313</v>
+      </c>
+      <c t="s" s="7" r="C86">
+        <v>314</v>
+      </c>
+      <c t="s" s="7" r="D86">
         <v>315</v>
       </c>
-      <c t="s" s="7" r="C86">
+      <c t="s" s="7" r="E86">
         <v>316</v>
-      </c>
-      <c t="s" s="7" r="D86">
-        <v>317</v>
-      </c>
-      <c t="s" s="7" r="E86">
-        <v>318</v>
       </c>
     </row>
     <row r="87">
       <c s="9" r="A87"/>
       <c t="s" s="7" r="B87">
+        <v>317</v>
+      </c>
+      <c t="s" s="7" r="C87">
+        <v>318</v>
+      </c>
+      <c t="s" s="7" r="D87">
         <v>319</v>
       </c>
-      <c t="s" s="7" r="C87">
+      <c t="s" s="7" r="E87">
         <v>320</v>
-      </c>
-      <c t="s" s="7" r="D87">
-        <v>321</v>
-      </c>
-      <c t="s" s="7" r="E87">
-        <v>322</v>
       </c>
     </row>
     <row r="88">
       <c s="9" r="A88"/>
       <c t="s" s="7" r="B88">
+        <v>321</v>
+      </c>
+      <c t="s" s="7" r="C88">
+        <v>322</v>
+      </c>
+      <c t="s" s="7" r="D88">
         <v>323</v>
       </c>
-      <c t="s" s="7" r="C88">
+      <c t="s" s="7" r="E88">
         <v>324</v>
-      </c>
-      <c t="s" s="7" r="D88">
-        <v>325</v>
-      </c>
-      <c t="s" s="7" r="E88">
-        <v>326</v>
       </c>
     </row>
     <row r="89">
       <c s="9" r="A89"/>
       <c t="s" s="7" r="B89">
+        <v>325</v>
+      </c>
+      <c t="s" s="7" r="C89">
+        <v>326</v>
+      </c>
+      <c t="s" s="7" r="D89">
         <v>327</v>
       </c>
-      <c t="s" s="7" r="C89">
+      <c t="s" s="7" r="E89">
         <v>328</v>
-      </c>
-      <c t="s" s="7" r="D89">
-        <v>329</v>
-      </c>
-      <c t="s" s="7" r="E89">
-        <v>330</v>
       </c>
     </row>
     <row r="90">
       <c s="9" r="A90"/>
       <c t="s" s="7" r="B90">
+        <v>329</v>
+      </c>
+      <c t="s" s="7" r="C90">
+        <v>330</v>
+      </c>
+      <c t="s" s="7" r="D90">
         <v>331</v>
       </c>
-      <c t="s" s="7" r="C90">
+      <c t="s" s="7" r="E90">
         <v>332</v>
-      </c>
-      <c t="s" s="7" r="D90">
-        <v>333</v>
-      </c>
-      <c t="s" s="7" r="E90">
-        <v>334</v>
       </c>
     </row>
     <row r="91">
       <c s="9" r="A91"/>
       <c t="s" s="7" r="B91">
+        <v>333</v>
+      </c>
+      <c t="s" s="7" r="C91">
+        <v>334</v>
+      </c>
+      <c t="s" s="7" r="D91">
         <v>335</v>
       </c>
-      <c t="s" s="7" r="C91">
+      <c t="s" s="7" r="E91">
         <v>336</v>
-      </c>
-      <c t="s" s="7" r="D91">
-        <v>337</v>
-      </c>
-      <c t="s" s="7" r="E91">
-        <v>338</v>
       </c>
     </row>
     <row r="92">
       <c s="9" r="A92"/>
       <c t="s" s="7" r="B92">
+        <v>337</v>
+      </c>
+      <c t="s" s="7" r="C92">
+        <v>338</v>
+      </c>
+      <c t="s" s="7" r="D92">
         <v>339</v>
       </c>
-      <c t="s" s="7" r="C92">
+      <c t="s" s="7" r="E92">
         <v>340</v>
-      </c>
-      <c t="s" s="7" r="D92">
-        <v>341</v>
-      </c>
-      <c t="s" s="7" r="E92">
-        <v>342</v>
       </c>
     </row>
     <row r="93">
       <c s="9" r="A93"/>
       <c t="s" s="7" r="B93">
+        <v>341</v>
+      </c>
+      <c t="s" s="7" r="C93">
+        <v>342</v>
+      </c>
+      <c t="s" s="7" r="D93">
         <v>343</v>
       </c>
-      <c t="s" s="7" r="C93">
+      <c t="s" s="7" r="E93">
         <v>344</v>
-      </c>
-      <c t="s" s="7" r="D93">
-        <v>345</v>
-      </c>
-      <c t="s" s="7" r="E93">
-        <v>346</v>
       </c>
     </row>
     <row r="94">
       <c s="9" r="A94"/>
       <c t="s" s="7" r="B94">
+        <v>345</v>
+      </c>
+      <c t="s" s="7" r="C94">
+        <v>346</v>
+      </c>
+      <c t="s" s="7" r="D94">
         <v>347</v>
       </c>
-      <c t="s" s="7" r="C94">
+      <c t="s" s="7" r="E94">
         <v>348</v>
-      </c>
-      <c t="s" s="7" r="D94">
-        <v>349</v>
-      </c>
-      <c t="s" s="7" r="E94">
-        <v>350</v>
       </c>
     </row>
     <row r="95">
       <c s="9" r="A95"/>
       <c t="s" s="7" r="B95">
+        <v>349</v>
+      </c>
+      <c t="s" s="7" r="C95">
+        <v>350</v>
+      </c>
+      <c t="s" s="7" r="D95">
         <v>351</v>
       </c>
-      <c t="s" s="7" r="C95">
+      <c t="s" s="7" r="E95">
         <v>352</v>
-      </c>
-      <c t="s" s="7" r="D95">
-        <v>353</v>
-      </c>
-      <c t="s" s="7" r="E95">
-        <v>354</v>
       </c>
     </row>
     <row r="96">
       <c s="9" r="A96"/>
       <c t="s" s="7" r="B96">
+        <v>353</v>
+      </c>
+      <c t="s" s="7" r="C96">
+        <v>354</v>
+      </c>
+      <c t="s" s="7" r="D96">
         <v>355</v>
       </c>
-      <c t="s" s="7" r="C96">
+      <c t="s" s="7" r="E96">
         <v>356</v>
-      </c>
-      <c t="s" s="7" r="D96">
-        <v>357</v>
-      </c>
-      <c t="s" s="7" r="E96">
-        <v>358</v>
       </c>
     </row>
     <row r="97">
       <c s="9" r="A97"/>
-      <c s="11" r="B97"/>
-      <c s="11" r="C97"/>
-      <c s="11" r="D97"/>
-      <c s="11" r="E97"/>
+      <c t="s" s="7" r="B97">
+        <v>357</v>
+      </c>
+      <c t="s" s="7" r="C97">
+        <v>358</v>
+      </c>
+      <c t="s" s="7" r="D97">
+        <v>359</v>
+      </c>
+      <c t="s" s="7" r="E97">
+        <v>360</v>
+      </c>
     </row>
     <row r="98">
-      <c t="s" s="9" r="A98">
-        <v>359</v>
-      </c>
-      <c t="s" s="7" r="B98">
-        <v>360</v>
-      </c>
-      <c t="s" s="7" r="C98">
+      <c s="9" r="A98"/>
+      <c s="11" r="B98"/>
+      <c s="11" r="C98"/>
+      <c s="11" r="D98"/>
+      <c s="11" r="E98"/>
+    </row>
+    <row r="99">
+      <c t="s" s="9" r="A99">
         <v>361</v>
       </c>
-      <c t="s" s="7" r="D98">
+      <c t="s" s="7" r="B99">
         <v>362</v>
       </c>
-      <c t="s" s="7" r="E98">
+      <c t="s" s="7" r="C99">
         <v>363</v>
       </c>
-    </row>
-    <row r="99">
-      <c s="9" r="A99"/>
-      <c t="s" s="7" r="B99">
+      <c t="s" s="7" r="D99">
         <v>364</v>
       </c>
-      <c t="s" s="7" r="C99">
+      <c t="s" s="7" r="E99">
         <v>365</v>
-      </c>
-      <c t="s" s="7" r="D99">
-        <v>366</v>
-      </c>
-      <c t="s" s="7" r="E99">
-        <v>367</v>
       </c>
     </row>
     <row r="100">
       <c s="9" r="A100"/>
       <c t="s" s="7" r="B100">
+        <v>366</v>
+      </c>
+      <c t="s" s="7" r="C100">
+        <v>367</v>
+      </c>
+      <c t="s" s="7" r="D100">
         <v>368</v>
       </c>
-      <c t="s" s="7" r="C100">
+      <c t="s" s="7" r="E100">
         <v>369</v>
-      </c>
-      <c t="s" s="7" r="D100">
-        <v>370</v>
-      </c>
-      <c t="s" s="7" r="E100">
-        <v>371</v>
       </c>
     </row>
     <row r="101">
       <c s="9" r="A101"/>
       <c t="s" s="7" r="B101">
+        <v>370</v>
+      </c>
+      <c t="s" s="7" r="C101">
+        <v>371</v>
+      </c>
+      <c t="s" s="7" r="D101">
         <v>372</v>
       </c>
-      <c t="s" s="7" r="C101">
+      <c t="s" s="7" r="E101">
         <v>373</v>
-      </c>
-      <c t="s" s="7" r="D101">
-        <v>374</v>
-      </c>
-      <c t="s" s="7" r="E101">
-        <v>375</v>
       </c>
     </row>
     <row r="102">
       <c s="9" r="A102"/>
       <c t="s" s="7" r="B102">
+        <v>374</v>
+      </c>
+      <c t="s" s="7" r="C102">
+        <v>375</v>
+      </c>
+      <c t="s" s="7" r="D102">
         <v>376</v>
       </c>
-      <c t="s" s="7" r="C102">
+      <c t="s" s="7" r="E102">
         <v>377</v>
-      </c>
-      <c t="s" s="7" r="D102">
-        <v>378</v>
-      </c>
-      <c t="s" s="7" r="E102">
-        <v>379</v>
       </c>
     </row>
     <row r="103">
       <c s="9" r="A103"/>
       <c t="s" s="7" r="B103">
+        <v>378</v>
+      </c>
+      <c t="s" s="7" r="C103">
+        <v>379</v>
+      </c>
+      <c t="s" s="7" r="D103">
         <v>380</v>
       </c>
-      <c t="s" s="7" r="C103">
-        <v>202</v>
-      </c>
-      <c t="s" s="7" r="D103">
+      <c t="s" s="7" r="E103">
         <v>381</v>
-      </c>
-      <c t="s" s="7" r="E103">
-        <v>202</v>
       </c>
     </row>
     <row r="104">
@@ -4947,795 +5000,799 @@
         <v>382</v>
       </c>
       <c t="s" s="7" r="C104">
+        <v>202</v>
+      </c>
+      <c t="s" s="7" r="D104">
         <v>383</v>
       </c>
-      <c t="s" s="7" r="D104">
-        <v>384</v>
-      </c>
       <c t="s" s="7" r="E104">
-        <v>385</v>
+        <v>202</v>
       </c>
     </row>
     <row r="105">
       <c s="9" r="A105"/>
       <c t="s" s="7" r="B105">
+        <v>384</v>
+      </c>
+      <c t="s" s="7" r="C105">
+        <v>385</v>
+      </c>
+      <c t="s" s="7" r="D105">
         <v>386</v>
       </c>
-      <c t="s" s="7" r="C105">
+      <c t="s" s="7" r="E105">
         <v>387</v>
-      </c>
-      <c t="s" s="7" r="D105">
-        <v>388</v>
-      </c>
-      <c t="s" s="7" r="E105">
-        <v>389</v>
       </c>
     </row>
     <row r="106">
       <c s="9" r="A106"/>
       <c t="s" s="7" r="B106">
+        <v>388</v>
+      </c>
+      <c t="s" s="7" r="C106">
+        <v>389</v>
+      </c>
+      <c t="s" s="7" r="D106">
         <v>390</v>
       </c>
-      <c t="s" s="7" r="C106">
+      <c t="s" s="7" r="E106">
         <v>391</v>
-      </c>
-      <c t="s" s="7" r="D106">
-        <v>392</v>
-      </c>
-      <c t="s" s="7" r="E106">
-        <v>393</v>
       </c>
     </row>
     <row r="107">
       <c s="9" r="A107"/>
       <c t="s" s="7" r="B107">
+        <v>392</v>
+      </c>
+      <c t="s" s="7" r="C107">
+        <v>393</v>
+      </c>
+      <c t="s" s="7" r="D107">
         <v>394</v>
       </c>
-      <c t="s" s="7" r="C107">
+      <c t="s" s="7" r="E107">
         <v>395</v>
-      </c>
-      <c t="s" s="7" r="D107">
-        <v>396</v>
-      </c>
-      <c t="s" s="7" r="E107">
-        <v>397</v>
       </c>
     </row>
     <row r="108">
       <c s="9" r="A108"/>
       <c t="s" s="7" r="B108">
+        <v>396</v>
+      </c>
+      <c t="s" s="7" r="C108">
+        <v>397</v>
+      </c>
+      <c t="s" s="7" r="D108">
         <v>398</v>
       </c>
-      <c t="s" s="7" r="C108">
+      <c t="s" s="7" r="E108">
         <v>399</v>
-      </c>
-      <c t="s" s="7" r="D108">
-        <v>400</v>
-      </c>
-      <c t="s" s="7" r="E108">
-        <v>401</v>
       </c>
     </row>
     <row r="109">
       <c s="9" r="A109"/>
       <c t="s" s="7" r="B109">
+        <v>400</v>
+      </c>
+      <c t="s" s="7" r="C109">
+        <v>401</v>
+      </c>
+      <c t="s" s="7" r="D109">
         <v>402</v>
       </c>
-      <c t="s" s="7" r="C109">
+      <c t="s" s="7" r="E109">
         <v>403</v>
-      </c>
-      <c t="s" s="7" r="D109">
-        <v>403</v>
-      </c>
-      <c t="s" s="7" r="E109">
-        <v>404</v>
       </c>
     </row>
     <row r="110">
       <c s="9" r="A110"/>
       <c t="s" s="7" r="B110">
+        <v>404</v>
+      </c>
+      <c t="s" s="7" r="C110">
         <v>405</v>
       </c>
-      <c t="s" s="7" r="C110">
+      <c t="s" s="7" r="D110">
+        <v>405</v>
+      </c>
+      <c t="s" s="7" r="E110">
         <v>406</v>
-      </c>
-      <c t="s" s="7" r="D110">
-        <v>406</v>
-      </c>
-      <c t="s" s="7" r="E110">
-        <v>407</v>
       </c>
     </row>
     <row r="111">
       <c s="9" r="A111"/>
       <c t="s" s="7" r="B111">
+        <v>407</v>
+      </c>
+      <c t="s" s="7" r="C111">
         <v>408</v>
       </c>
-      <c t="s" s="7" r="C111">
+      <c t="s" s="7" r="D111">
+        <v>408</v>
+      </c>
+      <c t="s" s="7" r="E111">
         <v>409</v>
-      </c>
-      <c t="s" s="7" r="D111">
-        <v>410</v>
-      </c>
-      <c t="s" s="7" r="E111">
-        <v>411</v>
       </c>
     </row>
     <row r="112">
       <c s="9" r="A112"/>
-      <c t="s" s="13" r="B112">
+      <c t="s" s="7" r="B112">
+        <v>410</v>
+      </c>
+      <c t="s" s="7" r="C112">
+        <v>411</v>
+      </c>
+      <c t="s" s="7" r="D112">
         <v>412</v>
       </c>
-      <c t="s" s="7" r="C112">
+      <c t="s" s="7" r="E112">
         <v>413</v>
-      </c>
-      <c t="s" s="7" r="D112">
-        <v>414</v>
-      </c>
-      <c t="s" s="7" r="E112">
-        <v>414</v>
       </c>
     </row>
     <row r="113">
       <c s="9" r="A113"/>
-      <c t="s" s="7" r="B113">
+      <c t="s" s="13" r="B113">
+        <v>414</v>
+      </c>
+      <c t="s" s="7" r="C113">
         <v>415</v>
       </c>
-      <c t="s" s="7" r="C113">
+      <c t="s" s="7" r="D113">
         <v>416</v>
       </c>
-      <c t="s" s="7" r="D113">
-        <v>417</v>
-      </c>
       <c t="s" s="7" r="E113">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="114">
       <c s="9" r="A114"/>
       <c t="s" s="7" r="B114">
+        <v>417</v>
+      </c>
+      <c t="s" s="7" r="C114">
+        <v>418</v>
+      </c>
+      <c t="s" s="7" r="D114">
         <v>419</v>
       </c>
-      <c t="s" s="7" r="C114">
+      <c t="s" s="7" r="E114">
         <v>420</v>
-      </c>
-      <c t="s" s="7" r="D114">
-        <v>421</v>
-      </c>
-      <c t="s" s="7" r="E114">
-        <v>422</v>
       </c>
     </row>
     <row r="115">
       <c s="9" r="A115"/>
       <c t="s" s="7" r="B115">
+        <v>421</v>
+      </c>
+      <c t="s" s="7" r="C115">
+        <v>422</v>
+      </c>
+      <c t="s" s="7" r="D115">
         <v>423</v>
       </c>
-      <c t="s" s="7" r="C115">
+      <c t="s" s="7" r="E115">
         <v>424</v>
-      </c>
-      <c t="s" s="7" r="D115">
-        <v>425</v>
-      </c>
-      <c t="s" s="7" r="E115">
-        <v>426</v>
       </c>
     </row>
     <row r="116">
       <c s="9" r="A116"/>
       <c t="s" s="7" r="B116">
+        <v>425</v>
+      </c>
+      <c t="s" s="7" r="C116">
+        <v>426</v>
+      </c>
+      <c t="s" s="7" r="D116">
         <v>427</v>
       </c>
-      <c t="s" s="7" r="C116">
+      <c t="s" s="7" r="E116">
         <v>428</v>
-      </c>
-      <c t="s" s="7" r="D116">
-        <v>429</v>
-      </c>
-      <c t="s" s="7" r="E116">
-        <v>430</v>
       </c>
     </row>
     <row r="117">
       <c s="9" r="A117"/>
       <c t="s" s="7" r="B117">
+        <v>429</v>
+      </c>
+      <c t="s" s="7" r="C117">
+        <v>430</v>
+      </c>
+      <c t="s" s="7" r="D117">
         <v>431</v>
       </c>
-      <c t="s" s="7" r="C117">
+      <c t="s" s="7" r="E117">
         <v>432</v>
-      </c>
-      <c t="s" s="7" r="D117">
-        <v>433</v>
-      </c>
-      <c t="s" s="7" r="E117">
-        <v>434</v>
       </c>
     </row>
     <row r="118">
       <c s="9" r="A118"/>
       <c t="s" s="7" r="B118">
+        <v>433</v>
+      </c>
+      <c t="s" s="7" r="C118">
+        <v>434</v>
+      </c>
+      <c t="s" s="7" r="D118">
         <v>435</v>
       </c>
-      <c t="s" s="7" r="C118">
+      <c t="s" s="7" r="E118">
         <v>436</v>
-      </c>
-      <c t="s" s="7" r="D118">
-        <v>437</v>
-      </c>
-      <c t="s" s="7" r="E118">
-        <v>438</v>
       </c>
     </row>
     <row r="119">
       <c s="9" r="A119"/>
       <c t="s" s="7" r="B119">
+        <v>437</v>
+      </c>
+      <c t="s" s="7" r="C119">
+        <v>438</v>
+      </c>
+      <c t="s" s="7" r="D119">
         <v>439</v>
       </c>
-      <c t="s" s="7" r="C119">
+      <c t="s" s="7" r="E119">
         <v>440</v>
-      </c>
-      <c t="s" s="7" r="D119">
-        <v>441</v>
-      </c>
-      <c t="s" s="7" r="E119">
-        <v>442</v>
       </c>
     </row>
     <row r="120">
       <c s="9" r="A120"/>
       <c t="s" s="7" r="B120">
+        <v>441</v>
+      </c>
+      <c t="s" s="7" r="C120">
+        <v>442</v>
+      </c>
+      <c t="s" s="7" r="D120">
         <v>443</v>
       </c>
-      <c t="s" s="7" r="C120">
+      <c t="s" s="7" r="E120">
         <v>444</v>
-      </c>
-      <c t="s" s="7" r="D120">
-        <v>445</v>
-      </c>
-      <c t="s" s="7" r="E120">
-        <v>446</v>
       </c>
     </row>
     <row r="121">
       <c s="9" r="A121"/>
       <c t="s" s="7" r="B121">
+        <v>445</v>
+      </c>
+      <c t="s" s="7" r="C121">
+        <v>446</v>
+      </c>
+      <c t="s" s="7" r="D121">
         <v>447</v>
       </c>
-      <c t="s" s="7" r="C121">
+      <c t="s" s="7" r="E121">
         <v>448</v>
-      </c>
-      <c t="s" s="7" r="D121">
-        <v>449</v>
-      </c>
-      <c t="s" s="7" r="E121">
-        <v>450</v>
       </c>
     </row>
     <row r="122">
       <c s="9" r="A122"/>
       <c t="s" s="7" r="B122">
+        <v>449</v>
+      </c>
+      <c t="s" s="7" r="C122">
+        <v>450</v>
+      </c>
+      <c t="s" s="7" r="D122">
         <v>451</v>
       </c>
-      <c t="s" s="7" r="C122">
+      <c t="s" s="7" r="E122">
         <v>452</v>
-      </c>
-      <c t="s" s="7" r="D122">
-        <v>453</v>
-      </c>
-      <c t="s" s="7" r="E122">
-        <v>454</v>
       </c>
     </row>
     <row r="123">
       <c s="9" r="A123"/>
       <c t="s" s="7" r="B123">
+        <v>453</v>
+      </c>
+      <c t="s" s="7" r="C123">
+        <v>454</v>
+      </c>
+      <c t="s" s="7" r="D123">
         <v>455</v>
       </c>
-      <c t="s" s="7" r="C123">
+      <c t="s" s="7" r="E123">
         <v>456</v>
-      </c>
-      <c t="s" s="7" r="D123">
-        <v>457</v>
-      </c>
-      <c t="s" s="7" r="E123">
-        <v>458</v>
       </c>
     </row>
     <row r="124">
       <c s="9" r="A124"/>
       <c t="s" s="7" r="B124">
+        <v>457</v>
+      </c>
+      <c t="s" s="7" r="C124">
+        <v>458</v>
+      </c>
+      <c t="s" s="7" r="D124">
         <v>459</v>
       </c>
-      <c t="s" s="7" r="C124">
+      <c t="s" s="7" r="E124">
         <v>460</v>
-      </c>
-      <c t="s" s="7" r="D124">
-        <v>461</v>
-      </c>
-      <c t="s" s="7" r="E124">
-        <v>462</v>
       </c>
     </row>
     <row r="125">
       <c s="9" r="A125"/>
       <c t="s" s="7" r="B125">
+        <v>461</v>
+      </c>
+      <c t="s" s="7" r="C125">
+        <v>462</v>
+      </c>
+      <c t="s" s="7" r="D125">
         <v>463</v>
       </c>
-      <c t="s" s="7" r="C125">
+      <c t="s" s="7" r="E125">
         <v>464</v>
-      </c>
-      <c t="s" s="7" r="D125">
-        <v>465</v>
-      </c>
-      <c t="s" s="7" r="E125">
-        <v>466</v>
       </c>
     </row>
     <row r="126">
       <c s="9" r="A126"/>
       <c t="s" s="7" r="B126">
+        <v>465</v>
+      </c>
+      <c t="s" s="7" r="C126">
+        <v>466</v>
+      </c>
+      <c t="s" s="7" r="D126">
         <v>467</v>
       </c>
-      <c t="s" s="7" r="C126">
+      <c t="s" s="7" r="E126">
         <v>468</v>
-      </c>
-      <c t="s" s="7" r="D126">
-        <v>469</v>
-      </c>
-      <c t="s" s="7" r="E126">
-        <v>470</v>
       </c>
     </row>
     <row r="127">
       <c s="9" r="A127"/>
       <c t="s" s="7" r="B127">
+        <v>469</v>
+      </c>
+      <c t="s" s="7" r="C127">
+        <v>470</v>
+      </c>
+      <c t="s" s="7" r="D127">
         <v>471</v>
       </c>
-      <c t="s" s="7" r="C127">
+      <c t="s" s="7" r="E127">
         <v>472</v>
-      </c>
-      <c t="s" s="7" r="D127">
-        <v>473</v>
-      </c>
-      <c t="s" s="7" r="E127">
-        <v>474</v>
       </c>
     </row>
     <row r="128">
       <c s="9" r="A128"/>
       <c t="s" s="7" r="B128">
+        <v>473</v>
+      </c>
+      <c t="s" s="7" r="C128">
+        <v>474</v>
+      </c>
+      <c t="s" s="7" r="D128">
         <v>475</v>
       </c>
-      <c t="s" s="13" r="C128">
+      <c t="s" s="7" r="E128">
         <v>476</v>
-      </c>
-      <c t="s" s="7" r="D128">
-        <v>477</v>
-      </c>
-      <c t="s" s="7" r="E128">
-        <v>478</v>
       </c>
     </row>
     <row r="129">
       <c s="9" r="A129"/>
-      <c t="s" s="13" r="B129">
+      <c t="s" s="7" r="B129">
+        <v>477</v>
+      </c>
+      <c t="s" s="13" r="C129">
+        <v>478</v>
+      </c>
+      <c t="s" s="7" r="D129">
         <v>479</v>
       </c>
-      <c t="s" s="13" r="C129">
+      <c t="s" s="7" r="E129">
         <v>480</v>
-      </c>
-      <c t="s" s="7" r="D129">
-        <v>481</v>
-      </c>
-      <c t="s" s="7" r="E129">
-        <v>482</v>
       </c>
     </row>
     <row r="130">
       <c s="9" r="A130"/>
-      <c t="s" s="7" r="B130">
+      <c t="s" s="13" r="B130">
+        <v>481</v>
+      </c>
+      <c t="s" s="13" r="C130">
+        <v>482</v>
+      </c>
+      <c t="s" s="7" r="D130">
         <v>483</v>
       </c>
-      <c t="s" s="13" r="C130">
-        <v>480</v>
-      </c>
-      <c t="s" s="7" r="D130">
-        <v>481</v>
-      </c>
       <c t="s" s="7" r="E130">
-        <v>482</v>
+        <v>484</v>
       </c>
     </row>
     <row r="131">
       <c s="9" r="A131"/>
       <c t="s" s="7" r="B131">
+        <v>485</v>
+      </c>
+      <c t="s" s="13" r="C131">
+        <v>482</v>
+      </c>
+      <c t="s" s="7" r="D131">
+        <v>483</v>
+      </c>
+      <c t="s" s="7" r="E131">
         <v>484</v>
-      </c>
-      <c t="s" s="3" r="C131">
-        <v>485</v>
-      </c>
-      <c t="s" s="7" r="D131">
-        <v>486</v>
-      </c>
-      <c t="s" s="7" r="E131">
-        <v>487</v>
       </c>
     </row>
     <row r="132">
       <c s="9" r="A132"/>
       <c t="s" s="7" r="B132">
+        <v>486</v>
+      </c>
+      <c t="s" s="3" r="C132">
+        <v>487</v>
+      </c>
+      <c t="s" s="7" r="D132">
         <v>488</v>
       </c>
-      <c t="s" s="3" r="C132">
+      <c t="s" s="7" r="E132">
         <v>489</v>
-      </c>
-      <c t="s" s="7" r="D132">
-        <v>490</v>
-      </c>
-      <c t="s" s="7" r="E132">
-        <v>491</v>
       </c>
     </row>
     <row r="133">
       <c s="9" r="A133"/>
       <c t="s" s="7" r="B133">
+        <v>490</v>
+      </c>
+      <c t="s" s="3" r="C133">
+        <v>491</v>
+      </c>
+      <c t="s" s="7" r="D133">
         <v>492</v>
       </c>
-      <c t="s" s="3" r="C133">
+      <c t="s" s="7" r="E133">
         <v>493</v>
-      </c>
-      <c t="s" s="7" r="D133">
-        <v>494</v>
-      </c>
-      <c t="s" s="3" r="E133">
-        <v>495</v>
       </c>
     </row>
     <row r="134">
       <c s="9" r="A134"/>
-      <c s="16" r="B134"/>
-      <c s="8" r="C134"/>
-      <c s="16" r="D134"/>
-      <c s="16" r="E134"/>
+      <c t="s" s="7" r="B134">
+        <v>494</v>
+      </c>
+      <c t="s" s="3" r="C134">
+        <v>495</v>
+      </c>
+      <c t="s" s="7" r="D134">
+        <v>496</v>
+      </c>
+      <c t="s" s="3" r="E134">
+        <v>497</v>
+      </c>
     </row>
     <row r="135">
-      <c t="s" s="9" r="A135">
-        <v>496</v>
-      </c>
-      <c t="s" s="7" r="B135">
-        <v>497</v>
-      </c>
-      <c t="s" s="13" r="C135">
+      <c s="9" r="A135"/>
+      <c s="16" r="B135"/>
+      <c s="8" r="C135"/>
+      <c s="16" r="D135"/>
+      <c s="16" r="E135"/>
+    </row>
+    <row r="136">
+      <c t="s" s="9" r="A136">
         <v>498</v>
       </c>
-      <c t="s" s="7" r="D135">
+      <c t="s" s="7" r="B136">
         <v>499</v>
       </c>
-      <c t="s" s="7" r="E135">
+      <c t="s" s="13" r="C136">
         <v>500</v>
       </c>
-    </row>
-    <row r="136">
-      <c s="9" r="A136"/>
-      <c t="s" s="21" r="B136">
+      <c t="s" s="7" r="D136">
         <v>501</v>
       </c>
-      <c t="s" s="13" r="C136">
+      <c t="s" s="7" r="E136">
         <v>502</v>
-      </c>
-      <c t="s" s="21" r="D136">
-        <v>503</v>
-      </c>
-      <c t="s" s="21" r="E136">
-        <v>504</v>
       </c>
     </row>
     <row r="137">
       <c s="9" r="A137"/>
-      <c t="s" s="7" r="B137">
+      <c t="s" s="21" r="B137">
+        <v>503</v>
+      </c>
+      <c t="s" s="13" r="C137">
+        <v>504</v>
+      </c>
+      <c t="s" s="21" r="D137">
         <v>505</v>
       </c>
-      <c t="s" s="13" r="C137">
+      <c t="s" s="21" r="E137">
         <v>506</v>
-      </c>
-      <c t="s" s="7" r="D137">
-        <v>507</v>
-      </c>
-      <c t="s" s="7" r="E137">
-        <v>508</v>
       </c>
     </row>
     <row r="138">
       <c s="9" r="A138"/>
       <c t="s" s="7" r="B138">
+        <v>507</v>
+      </c>
+      <c t="s" s="13" r="C138">
+        <v>508</v>
+      </c>
+      <c t="s" s="7" r="D138">
         <v>509</v>
       </c>
-      <c t="s" s="13" r="C138">
+      <c t="s" s="7" r="E138">
         <v>510</v>
       </c>
-      <c t="s" s="7" r="D138">
+    </row>
+    <row r="139">
+      <c s="9" r="A139"/>
+      <c t="s" s="7" r="B139">
         <v>511</v>
       </c>
-      <c t="s" s="7" r="E138">
+      <c t="s" s="13" r="C139">
         <v>512</v>
       </c>
-    </row>
-    <row r="139">
-      <c s="17" r="A139"/>
-      <c t="s" s="7" r="B139">
+      <c t="s" s="7" r="D139">
         <v>513</v>
       </c>
-      <c t="s" s="13" r="C139">
+      <c t="s" s="7" r="E139">
         <v>514</v>
       </c>
-      <c t="s" s="7" r="D139">
+    </row>
+    <row r="140">
+      <c s="17" r="A140"/>
+      <c t="s" s="7" r="B140">
         <v>515</v>
       </c>
-      <c t="s" s="7" r="E139">
+      <c t="s" s="13" r="C140">
         <v>516</v>
       </c>
-    </row>
-    <row r="140">
-      <c s="9" r="A140"/>
-      <c t="s" s="7" r="B140">
+      <c t="s" s="7" r="D140">
         <v>517</v>
       </c>
-      <c t="s" s="13" r="C140">
+      <c t="s" s="7" r="E140">
         <v>518</v>
-      </c>
-      <c t="s" s="7" r="D140">
-        <v>519</v>
-      </c>
-      <c t="s" s="7" r="E140">
-        <v>520</v>
       </c>
     </row>
     <row r="141">
       <c s="9" r="A141"/>
       <c t="s" s="7" r="B141">
+        <v>519</v>
+      </c>
+      <c t="s" s="13" r="C141">
+        <v>520</v>
+      </c>
+      <c t="s" s="7" r="D141">
         <v>521</v>
       </c>
-      <c t="s" s="13" r="C141">
+      <c t="s" s="7" r="E141">
         <v>522</v>
-      </c>
-      <c t="s" s="7" r="D141">
-        <v>523</v>
-      </c>
-      <c t="s" s="7" r="E141">
-        <v>524</v>
       </c>
     </row>
     <row r="142">
       <c s="9" r="A142"/>
       <c t="s" s="7" r="B142">
+        <v>523</v>
+      </c>
+      <c t="s" s="13" r="C142">
+        <v>524</v>
+      </c>
+      <c t="s" s="7" r="D142">
         <v>525</v>
       </c>
-      <c t="s" s="13" r="C142">
+      <c t="s" s="7" r="E142">
         <v>526</v>
-      </c>
-      <c t="s" s="7" r="D142">
-        <v>527</v>
-      </c>
-      <c t="s" s="7" r="E142">
-        <v>528</v>
       </c>
     </row>
     <row r="143">
       <c s="9" r="A143"/>
       <c t="s" s="7" r="B143">
+        <v>527</v>
+      </c>
+      <c t="s" s="13" r="C143">
+        <v>528</v>
+      </c>
+      <c t="s" s="7" r="D143">
         <v>529</v>
       </c>
-      <c t="s" s="13" r="C143">
+      <c t="s" s="7" r="E143">
         <v>530</v>
-      </c>
-      <c t="s" s="7" r="D143">
-        <v>531</v>
-      </c>
-      <c t="s" s="7" r="E143">
-        <v>532</v>
       </c>
     </row>
     <row r="144">
       <c s="9" r="A144"/>
       <c t="s" s="7" r="B144">
+        <v>531</v>
+      </c>
+      <c t="s" s="13" r="C144">
+        <v>532</v>
+      </c>
+      <c t="s" s="7" r="D144">
         <v>533</v>
       </c>
-      <c t="s" s="13" r="C144">
+      <c t="s" s="7" r="E144">
         <v>534</v>
-      </c>
-      <c t="s" s="7" r="D144">
-        <v>535</v>
-      </c>
-      <c t="s" s="7" r="E144">
-        <v>536</v>
       </c>
     </row>
     <row r="145">
       <c s="9" r="A145"/>
       <c t="s" s="7" r="B145">
+        <v>535</v>
+      </c>
+      <c t="s" s="13" r="C145">
+        <v>536</v>
+      </c>
+      <c t="s" s="7" r="D145">
         <v>537</v>
       </c>
-      <c t="s" s="13" r="C145">
+      <c t="s" s="7" r="E145">
         <v>538</v>
-      </c>
-      <c t="s" s="7" r="D145">
-        <v>539</v>
-      </c>
-      <c t="s" s="7" r="E145">
-        <v>540</v>
       </c>
     </row>
     <row r="146">
       <c s="9" r="A146"/>
       <c t="s" s="7" r="B146">
+        <v>539</v>
+      </c>
+      <c t="s" s="13" r="C146">
+        <v>540</v>
+      </c>
+      <c t="s" s="7" r="D146">
         <v>541</v>
       </c>
-      <c t="s" s="13" r="C146">
+      <c t="s" s="7" r="E146">
         <v>542</v>
-      </c>
-      <c t="s" s="7" r="D146">
-        <v>543</v>
-      </c>
-      <c t="s" s="7" r="E146">
-        <v>544</v>
       </c>
     </row>
     <row r="147">
       <c s="9" r="A147"/>
-      <c s="19" r="B147"/>
-      <c s="27" r="C147"/>
-      <c s="19" r="D147"/>
-      <c s="19" r="E147"/>
+      <c t="s" s="7" r="B147">
+        <v>543</v>
+      </c>
+      <c t="s" s="13" r="C147">
+        <v>544</v>
+      </c>
+      <c t="s" s="7" r="D147">
+        <v>545</v>
+      </c>
+      <c t="s" s="7" r="E147">
+        <v>546</v>
+      </c>
     </row>
     <row r="148">
-      <c t="s" s="9" r="A148">
-        <v>545</v>
-      </c>
-      <c t="s" s="7" r="B148">
-        <v>546</v>
-      </c>
-      <c t="s" s="13" r="C148">
+      <c s="9" r="A148"/>
+      <c s="19" r="B148"/>
+      <c s="27" r="C148"/>
+      <c s="19" r="D148"/>
+      <c s="19" r="E148"/>
+    </row>
+    <row r="149">
+      <c t="s" s="9" r="A149">
         <v>547</v>
       </c>
-      <c t="s" s="7" r="D148">
+      <c t="s" s="7" r="B149">
         <v>548</v>
       </c>
-      <c t="s" s="7" r="E148">
+      <c t="s" s="13" r="C149">
         <v>549</v>
       </c>
-    </row>
-    <row r="149">
-      <c s="9" r="A149"/>
-      <c t="s" s="7" r="B149">
+      <c t="s" s="7" r="D149">
         <v>550</v>
       </c>
-      <c t="s" s="13" r="C149">
+      <c t="s" s="7" r="E149">
         <v>551</v>
-      </c>
-      <c t="s" s="7" r="D149">
-        <v>552</v>
-      </c>
-      <c t="s" s="7" r="E149">
-        <v>553</v>
       </c>
     </row>
     <row r="150">
       <c s="9" r="A150"/>
       <c t="s" s="7" r="B150">
+        <v>552</v>
+      </c>
+      <c t="s" s="13" r="C150">
+        <v>553</v>
+      </c>
+      <c t="s" s="7" r="D150">
         <v>554</v>
       </c>
-      <c t="s" s="13" r="C150">
+      <c t="s" s="7" r="E150">
         <v>555</v>
-      </c>
-      <c t="s" s="7" r="D150">
-        <v>556</v>
-      </c>
-      <c t="s" s="7" r="E150">
-        <v>557</v>
       </c>
     </row>
     <row r="151">
       <c s="9" r="A151"/>
       <c t="s" s="7" r="B151">
+        <v>556</v>
+      </c>
+      <c t="s" s="13" r="C151">
+        <v>557</v>
+      </c>
+      <c t="s" s="7" r="D151">
         <v>558</v>
       </c>
-      <c t="s" s="13" r="C151">
+      <c t="s" s="7" r="E151">
         <v>559</v>
-      </c>
-      <c t="s" s="7" r="D151">
-        <v>560</v>
-      </c>
-      <c t="s" s="7" r="E151">
-        <v>561</v>
       </c>
     </row>
     <row r="152">
       <c s="9" r="A152"/>
       <c t="s" s="7" r="B152">
+        <v>560</v>
+      </c>
+      <c t="s" s="13" r="C152">
+        <v>561</v>
+      </c>
+      <c t="s" s="7" r="D152">
         <v>562</v>
       </c>
-      <c t="s" s="13" r="C152">
+      <c t="s" s="7" r="E152">
         <v>563</v>
-      </c>
-      <c t="s" s="7" r="D152">
-        <v>564</v>
-      </c>
-      <c t="s" s="7" r="E152">
-        <v>565</v>
       </c>
     </row>
     <row r="153">
       <c s="9" r="A153"/>
       <c t="s" s="7" r="B153">
+        <v>564</v>
+      </c>
+      <c t="s" s="13" r="C153">
+        <v>565</v>
+      </c>
+      <c t="s" s="7" r="D153">
         <v>566</v>
       </c>
-      <c t="s" s="13" r="C153">
+      <c t="s" s="7" r="E153">
         <v>567</v>
-      </c>
-      <c t="s" s="7" r="D153">
-        <v>568</v>
-      </c>
-      <c t="s" s="7" r="E153">
-        <v>569</v>
       </c>
     </row>
     <row r="154">
       <c s="9" r="A154"/>
       <c t="s" s="7" r="B154">
+        <v>568</v>
+      </c>
+      <c t="s" s="13" r="C154">
+        <v>569</v>
+      </c>
+      <c t="s" s="7" r="D154">
         <v>570</v>
       </c>
-      <c t="s" s="13" r="C154">
+      <c t="s" s="7" r="E154">
         <v>571</v>
-      </c>
-      <c t="s" s="7" r="D154">
-        <v>572</v>
-      </c>
-      <c t="s" s="7" r="E154">
-        <v>573</v>
       </c>
     </row>
     <row r="155">
       <c s="9" r="A155"/>
-      <c s="19" r="B155"/>
-      <c s="27" r="C155"/>
-      <c s="19" r="D155"/>
-      <c s="19" r="E155"/>
+      <c t="s" s="7" r="B155">
+        <v>572</v>
+      </c>
+      <c t="s" s="13" r="C155">
+        <v>573</v>
+      </c>
+      <c t="s" s="7" r="D155">
+        <v>574</v>
+      </c>
+      <c t="s" s="7" r="E155">
+        <v>575</v>
+      </c>
     </row>
     <row r="156">
-      <c t="s" s="9" r="A156">
-        <v>574</v>
-      </c>
-      <c t="s" s="26" r="B156">
-        <v>575</v>
-      </c>
-      <c t="s" s="20" r="C156">
-        <v>574</v>
-      </c>
-      <c s="26" r="D156"/>
-      <c s="26" r="E156"/>
+      <c s="9" r="A156"/>
+      <c s="19" r="B156"/>
+      <c s="27" r="C156"/>
+      <c s="19" r="D156"/>
+      <c s="19" r="E156"/>
     </row>
     <row r="157">
-      <c s="9" r="A157"/>
-      <c s="16" r="B157"/>
-      <c s="8" r="C157"/>
-      <c s="16" r="D157"/>
-      <c s="16" r="E157"/>
+      <c t="s" s="9" r="A157">
+        <v>576</v>
+      </c>
+      <c t="s" s="26" r="B157">
+        <v>577</v>
+      </c>
+      <c t="s" s="20" r="C157">
+        <v>576</v>
+      </c>
+      <c s="26" r="D157"/>
+      <c s="26" r="E157"/>
     </row>
     <row r="158">
-      <c t="s" s="9" r="A158">
-        <v>576</v>
-      </c>
-      <c t="s" s="31" r="B158">
-        <v>577</v>
-      </c>
-      <c t="s" s="29" r="C158">
+      <c s="9" r="A158"/>
+      <c s="16" r="B158"/>
+      <c s="8" r="C158"/>
+      <c s="16" r="D158"/>
+      <c s="16" r="E158"/>
+    </row>
+    <row r="159">
+      <c t="s" s="9" r="A159">
         <v>578</v>
       </c>
-      <c s="31" r="D158"/>
-      <c s="31" r="E158"/>
-    </row>
-    <row r="159">
-      <c s="9" r="A159"/>
       <c t="s" s="31" r="B159">
         <v>579</v>
       </c>
@@ -5747,1070 +5804,1066 @@
     </row>
     <row r="160">
       <c s="9" r="A160"/>
-      <c s="8" r="B160"/>
-      <c s="8" r="C160"/>
-      <c s="16" r="D160"/>
-      <c s="16" r="E160"/>
+      <c t="s" s="31" r="B160">
+        <v>581</v>
+      </c>
+      <c t="s" s="29" r="C160">
+        <v>582</v>
+      </c>
+      <c s="31" r="D160"/>
+      <c s="31" r="E160"/>
     </row>
     <row r="161">
-      <c t="s" s="9" r="A161">
-        <v>581</v>
-      </c>
-      <c t="s" s="24" r="B161">
-        <v>582</v>
-      </c>
-      <c t="s" s="24" r="C161">
+      <c s="9" r="A161"/>
+      <c s="8" r="B161"/>
+      <c s="8" r="C161"/>
+      <c s="16" r="D161"/>
+      <c s="16" r="E161"/>
+    </row>
+    <row r="162">
+      <c t="s" s="9" r="A162">
         <v>583</v>
       </c>
-      <c t="s" s="7" r="D161">
+      <c t="s" s="24" r="B162">
         <v>584</v>
       </c>
-      <c t="s" s="7" r="E161">
+      <c t="s" s="24" r="C162">
         <v>585</v>
       </c>
-    </row>
-    <row r="162">
-      <c s="9" r="A162"/>
-      <c t="s" s="24" r="B162">
+      <c t="s" s="7" r="D162">
         <v>586</v>
       </c>
-      <c t="s" s="24" r="C162">
+      <c t="s" s="7" r="E162">
         <v>587</v>
-      </c>
-      <c t="s" s="7" r="D162">
-        <v>587</v>
-      </c>
-      <c t="s" s="7" r="E162">
-        <v>588</v>
       </c>
     </row>
     <row r="163">
       <c s="9" r="A163"/>
       <c t="s" s="24" r="B163">
+        <v>588</v>
+      </c>
+      <c t="s" s="24" r="C163">
         <v>589</v>
       </c>
-      <c t="s" s="24" r="C163">
+      <c t="s" s="7" r="D163">
+        <v>589</v>
+      </c>
+      <c t="s" s="7" r="E163">
         <v>590</v>
-      </c>
-      <c t="s" s="7" r="D163">
-        <v>591</v>
-      </c>
-      <c t="s" s="7" r="E163">
-        <v>592</v>
       </c>
     </row>
     <row r="164">
       <c s="9" r="A164"/>
       <c t="s" s="24" r="B164">
+        <v>591</v>
+      </c>
+      <c t="s" s="24" r="C164">
+        <v>592</v>
+      </c>
+      <c t="s" s="7" r="D164">
         <v>593</v>
       </c>
-      <c t="s" s="24" r="C164">
+      <c t="s" s="7" r="E164">
         <v>594</v>
-      </c>
-      <c t="s" s="7" r="D164">
-        <v>595</v>
-      </c>
-      <c t="s" s="7" r="E164">
-        <v>596</v>
       </c>
     </row>
     <row r="165">
       <c s="9" r="A165"/>
-      <c t="s" s="13" r="B165">
+      <c t="s" s="24" r="B165">
+        <v>595</v>
+      </c>
+      <c t="s" s="24" r="C165">
+        <v>596</v>
+      </c>
+      <c t="s" s="7" r="D165">
         <v>597</v>
       </c>
-      <c t="s" s="13" r="C165">
+      <c t="s" s="7" r="E165">
         <v>598</v>
-      </c>
-      <c t="s" s="7" r="D165">
-        <v>599</v>
-      </c>
-      <c t="s" s="7" r="E165">
-        <v>600</v>
       </c>
     </row>
     <row r="166">
       <c s="9" r="A166"/>
       <c t="s" s="13" r="B166">
+        <v>599</v>
+      </c>
+      <c t="s" s="13" r="C166">
+        <v>600</v>
+      </c>
+      <c t="s" s="7" r="D166">
         <v>601</v>
       </c>
-      <c t="s" s="13" r="C166">
+      <c t="s" s="7" r="E166">
         <v>602</v>
-      </c>
-      <c t="s" s="7" r="D166">
-        <v>603</v>
-      </c>
-      <c t="s" s="7" r="E166">
-        <v>604</v>
       </c>
     </row>
     <row r="167">
       <c s="9" r="A167"/>
       <c t="s" s="13" r="B167">
+        <v>603</v>
+      </c>
+      <c t="s" s="13" r="C167">
+        <v>604</v>
+      </c>
+      <c t="s" s="7" r="D167">
         <v>605</v>
       </c>
-      <c t="s" s="13" r="C167">
+      <c t="s" s="7" r="E167">
         <v>606</v>
-      </c>
-      <c t="s" s="7" r="D167">
-        <v>607</v>
-      </c>
-      <c t="s" s="7" r="E167">
-        <v>608</v>
       </c>
     </row>
     <row r="168">
       <c s="9" r="A168"/>
       <c t="s" s="13" r="B168">
+        <v>607</v>
+      </c>
+      <c t="s" s="13" r="C168">
+        <v>608</v>
+      </c>
+      <c t="s" s="7" r="D168">
         <v>609</v>
       </c>
-      <c t="s" s="13" r="C168">
+      <c t="s" s="7" r="E168">
         <v>610</v>
-      </c>
-      <c t="s" s="7" r="D168">
-        <v>611</v>
-      </c>
-      <c t="s" s="7" r="E168">
-        <v>612</v>
       </c>
     </row>
     <row r="169">
       <c s="9" r="A169"/>
       <c t="s" s="13" r="B169">
+        <v>611</v>
+      </c>
+      <c t="s" s="13" r="C169">
+        <v>612</v>
+      </c>
+      <c t="s" s="7" r="D169">
         <v>613</v>
       </c>
-      <c t="s" s="13" r="C169">
+      <c t="s" s="7" r="E169">
         <v>614</v>
-      </c>
-      <c t="s" s="7" r="D169">
-        <v>615</v>
-      </c>
-      <c t="s" s="7" r="E169">
-        <v>616</v>
       </c>
     </row>
     <row r="170">
       <c s="9" r="A170"/>
       <c t="s" s="13" r="B170">
+        <v>615</v>
+      </c>
+      <c t="s" s="13" r="C170">
+        <v>616</v>
+      </c>
+      <c t="s" s="7" r="D170">
         <v>617</v>
       </c>
-      <c t="s" s="13" r="C170">
+      <c t="s" s="7" r="E170">
         <v>618</v>
-      </c>
-      <c t="s" s="7" r="D170">
-        <v>619</v>
-      </c>
-      <c t="s" s="7" r="E170">
-        <v>620</v>
       </c>
     </row>
     <row r="171">
       <c s="9" r="A171"/>
       <c t="s" s="13" r="B171">
+        <v>619</v>
+      </c>
+      <c t="s" s="13" r="C171">
+        <v>620</v>
+      </c>
+      <c t="s" s="7" r="D171">
         <v>621</v>
       </c>
-      <c t="s" s="13" r="C171">
+      <c t="s" s="7" r="E171">
         <v>622</v>
-      </c>
-      <c t="s" s="7" r="D171">
-        <v>623</v>
-      </c>
-      <c t="s" s="7" r="E171">
-        <v>624</v>
       </c>
     </row>
     <row r="172">
       <c s="9" r="A172"/>
-      <c t="s" s="7" r="B172">
+      <c t="s" s="13" r="B172">
+        <v>623</v>
+      </c>
+      <c t="s" s="13" r="C172">
+        <v>624</v>
+      </c>
+      <c t="s" s="7" r="D172">
         <v>625</v>
       </c>
-      <c t="s" s="13" r="C172">
+      <c t="s" s="7" r="E172">
         <v>626</v>
-      </c>
-      <c t="s" s="7" r="D172">
-        <v>627</v>
-      </c>
-      <c t="s" s="7" r="E172">
-        <v>628</v>
       </c>
     </row>
     <row r="173">
       <c s="9" r="A173"/>
       <c t="s" s="7" r="B173">
+        <v>627</v>
+      </c>
+      <c t="s" s="13" r="C173">
+        <v>628</v>
+      </c>
+      <c t="s" s="7" r="D173">
         <v>629</v>
       </c>
-      <c t="s" s="13" r="C173">
+      <c t="s" s="7" r="E173">
         <v>630</v>
-      </c>
-      <c t="s" s="7" r="D173">
-        <v>631</v>
-      </c>
-      <c t="s" s="7" r="E173">
-        <v>632</v>
       </c>
     </row>
     <row r="174">
       <c s="9" r="A174"/>
-      <c t="s" s="7" r="B174">
+      <c t="s" s="18" r="B174">
+        <v>631</v>
+      </c>
+      <c t="s" s="32" r="C174">
+        <v>632</v>
+      </c>
+      <c t="s" s="18" r="D174">
         <v>633</v>
       </c>
-      <c t="s" s="13" r="C174">
+      <c t="s" s="18" r="E174">
         <v>634</v>
-      </c>
-      <c t="s" s="7" r="D174">
-        <v>635</v>
-      </c>
-      <c t="s" s="7" r="E174">
-        <v>636</v>
       </c>
     </row>
     <row r="175">
       <c s="9" r="A175"/>
-      <c t="s" s="7" r="B175">
+      <c t="s" s="18" r="B175">
+        <v>635</v>
+      </c>
+      <c t="s" s="32" r="C175">
+        <v>636</v>
+      </c>
+      <c t="s" s="18" r="D175">
         <v>637</v>
       </c>
-      <c t="s" s="13" r="C175">
+      <c t="s" s="18" r="E175">
         <v>638</v>
-      </c>
-      <c t="s" s="7" r="D175">
-        <v>639</v>
-      </c>
-      <c t="s" s="7" r="E175">
-        <v>640</v>
       </c>
     </row>
     <row r="176">
       <c s="9" r="A176"/>
-      <c t="s" s="7" r="B176">
+      <c t="s" s="18" r="B176">
+        <v>639</v>
+      </c>
+      <c t="s" s="32" r="C176">
+        <v>640</v>
+      </c>
+      <c t="s" s="18" r="D176">
         <v>641</v>
       </c>
-      <c t="s" s="13" r="C176">
+      <c t="s" s="18" r="E176">
         <v>642</v>
-      </c>
-      <c t="s" s="7" r="D176">
-        <v>643</v>
-      </c>
-      <c t="s" s="7" r="E176">
-        <v>644</v>
       </c>
     </row>
     <row r="177">
       <c s="9" r="A177"/>
       <c t="s" s="7" r="B177">
+        <v>643</v>
+      </c>
+      <c t="s" s="13" r="C177">
+        <v>644</v>
+      </c>
+      <c t="s" s="7" r="D177">
         <v>645</v>
       </c>
-      <c t="s" s="13" r="C177">
+      <c t="s" s="7" r="E177">
         <v>646</v>
-      </c>
-      <c t="s" s="7" r="D177">
-        <v>647</v>
-      </c>
-      <c t="s" s="7" r="E177">
-        <v>648</v>
       </c>
     </row>
     <row r="178">
       <c s="9" r="A178"/>
-      <c s="11" r="B178"/>
-      <c s="14" r="C178"/>
-      <c s="11" r="D178"/>
-      <c s="11" r="E178"/>
+      <c t="s" s="7" r="B178">
+        <v>647</v>
+      </c>
+      <c t="s" s="13" r="C178">
+        <v>648</v>
+      </c>
+      <c t="s" s="7" r="D178">
+        <v>649</v>
+      </c>
+      <c t="s" s="7" r="E178">
+        <v>650</v>
+      </c>
     </row>
     <row r="179">
       <c s="9" r="A179"/>
-      <c s="16" r="B179"/>
-      <c s="27" r="C179"/>
-      <c s="16" r="D179"/>
-      <c s="16" r="E179"/>
+      <c t="s" s="7" r="B179">
+        <v>651</v>
+      </c>
+      <c t="s" s="13" r="C179">
+        <v>652</v>
+      </c>
+      <c t="s" s="7" r="D179">
+        <v>653</v>
+      </c>
+      <c t="s" s="7" r="E179">
+        <v>654</v>
+      </c>
     </row>
     <row r="180">
-      <c t="s" s="9" r="A180">
-        <v>649</v>
-      </c>
-      <c t="s" s="24" r="B180">
-        <v>650</v>
-      </c>
-      <c t="s" s="7" r="C180">
-        <v>587</v>
+      <c s="9" r="A180"/>
+      <c t="s" s="7" r="B180">
+        <v>655</v>
+      </c>
+      <c t="s" s="13" r="C180">
+        <v>656</v>
       </c>
       <c t="s" s="7" r="D180">
-        <v>587</v>
+        <v>657</v>
       </c>
       <c t="s" s="7" r="E180">
-        <v>588</v>
+        <v>658</v>
       </c>
     </row>
     <row r="181">
       <c s="9" r="A181"/>
       <c t="s" s="7" r="B181">
-        <v>651</v>
+        <v>659</v>
       </c>
       <c t="s" s="13" r="C181">
-        <v>590</v>
+        <v>660</v>
       </c>
       <c t="s" s="7" r="D181">
-        <v>591</v>
+        <v>661</v>
       </c>
       <c t="s" s="7" r="E181">
-        <v>592</v>
+        <v>662</v>
       </c>
     </row>
     <row r="182">
-      <c t="s" s="7" r="B182">
-        <v>652</v>
-      </c>
-      <c t="s" s="13" r="C182">
-        <v>653</v>
-      </c>
-      <c t="s" s="7" r="D182">
-        <v>654</v>
-      </c>
-      <c t="s" s="7" r="E182">
-        <v>655</v>
-      </c>
+      <c s="9" r="A182"/>
+      <c s="11" r="B182"/>
+      <c s="14" r="C182"/>
+      <c s="11" r="D182"/>
+      <c s="11" r="E182"/>
     </row>
     <row r="183">
       <c s="9" r="A183"/>
-      <c t="s" s="7" r="B183">
-        <v>656</v>
-      </c>
-      <c t="s" s="13" r="C183">
-        <v>657</v>
-      </c>
-      <c t="s" s="7" r="D183">
-        <v>658</v>
-      </c>
-      <c t="s" s="7" r="E183">
-        <v>659</v>
-      </c>
+      <c s="16" r="B183"/>
+      <c s="27" r="C183"/>
+      <c s="16" r="D183"/>
+      <c s="16" r="E183"/>
     </row>
     <row r="184">
-      <c s="9" r="A184"/>
-      <c t="s" s="7" r="B184">
-        <v>660</v>
-      </c>
-      <c t="s" s="13" r="C184">
-        <v>661</v>
+      <c t="s" s="9" r="A184">
+        <v>663</v>
+      </c>
+      <c t="s" s="24" r="B184">
+        <v>664</v>
+      </c>
+      <c t="s" s="7" r="C184">
+        <v>589</v>
       </c>
       <c t="s" s="7" r="D184">
-        <v>662</v>
+        <v>589</v>
       </c>
       <c t="s" s="7" r="E184">
-        <v>663</v>
+        <v>590</v>
       </c>
     </row>
     <row r="185">
       <c s="9" r="A185"/>
-      <c s="11" r="B185"/>
-      <c s="14" r="C185"/>
-      <c s="16" r="D185"/>
-      <c s="16" r="E185"/>
+      <c t="s" s="7" r="B185">
+        <v>665</v>
+      </c>
+      <c t="s" s="13" r="C185">
+        <v>592</v>
+      </c>
+      <c t="s" s="7" r="D185">
+        <v>593</v>
+      </c>
+      <c t="s" s="7" r="E185">
+        <v>594</v>
+      </c>
     </row>
     <row r="186">
-      <c t="s" s="9" r="A186">
-        <v>664</v>
-      </c>
       <c t="s" s="7" r="B186">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c t="s" s="13" r="C186">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c t="s" s="7" r="D186">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c t="s" s="7" r="E186">
-        <v>667</v>
+        <v>669</v>
       </c>
     </row>
     <row r="187">
       <c s="9" r="A187"/>
       <c t="s" s="7" r="B187">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c t="s" s="13" r="C187">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c t="s" s="7" r="D187">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c t="s" s="7" r="E187">
-        <v>671</v>
+        <v>673</v>
       </c>
     </row>
     <row r="188">
       <c s="9" r="A188"/>
       <c t="s" s="7" r="B188">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c t="s" s="13" r="C188">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c t="s" s="7" r="D188">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c t="s" s="7" r="E188">
-        <v>675</v>
+        <v>677</v>
       </c>
     </row>
     <row r="189">
       <c s="9" r="A189"/>
-      <c t="s" s="7" r="B189">
-        <v>676</v>
-      </c>
-      <c t="s" s="13" r="C189">
-        <v>677</v>
-      </c>
-      <c t="s" s="7" r="D189">
+      <c s="11" r="B189"/>
+      <c s="14" r="C189"/>
+      <c s="16" r="D189"/>
+      <c s="16" r="E189"/>
+    </row>
+    <row r="190">
+      <c t="s" s="9" r="A190">
         <v>678</v>
       </c>
-      <c t="s" s="7" r="E189">
+      <c t="s" s="7" r="B190">
         <v>679</v>
       </c>
-    </row>
-    <row r="190">
-      <c s="9" r="A190"/>
-      <c t="s" s="7" r="B190">
+      <c t="s" s="13" r="C190">
+        <v>678</v>
+      </c>
+      <c t="s" s="7" r="D190">
         <v>680</v>
       </c>
-      <c t="s" s="13" r="C190">
+      <c t="s" s="7" r="E190">
         <v>681</v>
-      </c>
-      <c t="s" s="7" r="D190">
-        <v>682</v>
-      </c>
-      <c t="s" s="7" r="E190">
-        <v>683</v>
       </c>
     </row>
     <row r="191">
       <c s="9" r="A191"/>
       <c t="s" s="7" r="B191">
+        <v>682</v>
+      </c>
+      <c t="s" s="13" r="C191">
+        <v>683</v>
+      </c>
+      <c t="s" s="7" r="D191">
         <v>684</v>
       </c>
-      <c t="s" s="13" r="C191">
+      <c t="s" s="7" r="E191">
         <v>685</v>
-      </c>
-      <c t="s" s="7" r="D191">
-        <v>686</v>
-      </c>
-      <c t="s" s="7" r="E191">
-        <v>687</v>
       </c>
     </row>
     <row r="192">
       <c s="9" r="A192"/>
       <c t="s" s="7" r="B192">
+        <v>686</v>
+      </c>
+      <c t="s" s="13" r="C192">
+        <v>687</v>
+      </c>
+      <c t="s" s="7" r="D192">
         <v>688</v>
       </c>
-      <c t="s" s="13" r="C192">
+      <c t="s" s="7" r="E192">
         <v>689</v>
-      </c>
-      <c t="s" s="7" r="D192">
-        <v>690</v>
-      </c>
-      <c t="s" s="7" r="E192">
-        <v>691</v>
       </c>
     </row>
     <row r="193">
       <c s="9" r="A193"/>
-      <c s="11" r="B193"/>
-      <c s="14" r="C193"/>
-      <c s="11" r="D193"/>
-      <c s="11" r="E193"/>
+      <c t="s" s="7" r="B193">
+        <v>690</v>
+      </c>
+      <c t="s" s="13" r="C193">
+        <v>691</v>
+      </c>
+      <c t="s" s="7" r="D193">
+        <v>692</v>
+      </c>
+      <c t="s" s="7" r="E193">
+        <v>693</v>
+      </c>
     </row>
     <row r="194">
-      <c t="s" s="9" r="A194">
-        <v>692</v>
-      </c>
+      <c s="9" r="A194"/>
       <c t="s" s="7" r="B194">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c t="s" s="13" r="C194">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c t="s" s="7" r="D194">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c t="s" s="7" r="E194">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="195">
       <c s="9" r="A195"/>
       <c t="s" s="7" r="B195">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c t="s" s="13" r="C195">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c t="s" s="7" r="D195">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c t="s" s="7" r="E195">
-        <v>699</v>
+        <v>701</v>
       </c>
     </row>
     <row r="196">
       <c s="9" r="A196"/>
-      <c s="11" r="B196"/>
-      <c s="14" r="C196"/>
-      <c s="11" r="D196"/>
-      <c s="11" r="E196"/>
+      <c t="s" s="7" r="B196">
+        <v>702</v>
+      </c>
+      <c t="s" s="13" r="C196">
+        <v>703</v>
+      </c>
+      <c t="s" s="7" r="D196">
+        <v>704</v>
+      </c>
+      <c t="s" s="7" r="E196">
+        <v>705</v>
+      </c>
     </row>
     <row r="197">
-      <c t="s" s="9" r="A197">
-        <v>700</v>
-      </c>
-      <c t="s" s="7" r="B197">
-        <v>701</v>
-      </c>
-      <c t="s" s="13" r="C197">
-        <v>702</v>
-      </c>
-      <c t="s" s="7" r="D197">
-        <v>703</v>
-      </c>
-      <c t="s" s="7" r="E197">
-        <v>704</v>
-      </c>
+      <c s="9" r="A197"/>
+      <c s="11" r="B197"/>
+      <c s="14" r="C197"/>
+      <c s="11" r="D197"/>
+      <c s="11" r="E197"/>
     </row>
     <row r="198">
-      <c s="9" r="A198"/>
+      <c t="s" s="9" r="A198">
+        <v>706</v>
+      </c>
       <c t="s" s="7" r="B198">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c t="s" s="13" r="C198">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c t="s" s="7" r="D198">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c t="s" s="7" r="E198">
-        <v>708</v>
+        <v>710</v>
       </c>
     </row>
     <row r="199">
       <c s="9" r="A199"/>
       <c t="s" s="7" r="B199">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c t="s" s="13" r="C199">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c t="s" s="7" r="D199">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c t="s" s="7" r="E199">
-        <v>712</v>
+        <v>713</v>
       </c>
     </row>
     <row r="200">
       <c s="9" r="A200"/>
-      <c t="s" s="7" r="B200">
-        <v>713</v>
-      </c>
-      <c t="s" s="13" r="C200">
+      <c s="11" r="B200"/>
+      <c s="14" r="C200"/>
+      <c s="11" r="D200"/>
+      <c s="11" r="E200"/>
+    </row>
+    <row r="201">
+      <c t="s" s="9" r="A201">
         <v>714</v>
       </c>
-      <c t="s" s="7" r="D200">
+      <c t="s" s="7" r="B201">
         <v>715</v>
       </c>
-      <c t="s" s="7" r="E200">
+      <c t="s" s="13" r="C201">
         <v>716</v>
       </c>
-    </row>
-    <row r="201">
-      <c s="9" r="A201"/>
-      <c s="16" r="B201"/>
-      <c s="27" r="C201"/>
-      <c s="16" r="D201"/>
-      <c s="16" r="E201"/>
+      <c t="s" s="7" r="D201">
+        <v>717</v>
+      </c>
+      <c t="s" s="7" r="E201">
+        <v>718</v>
+      </c>
     </row>
     <row r="202">
-      <c t="s" s="9" r="A202">
-        <v>717</v>
-      </c>
+      <c s="9" r="A202"/>
       <c t="s" s="7" r="B202">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c t="s" s="13" r="C202">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c t="s" s="7" r="D202">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c t="s" s="7" r="E202">
-        <v>721</v>
+        <v>722</v>
       </c>
     </row>
     <row r="203">
       <c s="9" r="A203"/>
       <c t="s" s="7" r="B203">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c t="s" s="13" r="C203">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c t="s" s="7" r="D203">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c t="s" s="7" r="E203">
-        <v>725</v>
+        <v>726</v>
       </c>
     </row>
     <row r="204">
       <c s="9" r="A204"/>
-      <c s="16" r="B204"/>
-      <c s="27" r="C204"/>
-      <c s="16" r="D204"/>
-      <c s="16" r="E204"/>
+      <c t="s" s="7" r="B204">
+        <v>727</v>
+      </c>
+      <c t="s" s="13" r="C204">
+        <v>728</v>
+      </c>
+      <c t="s" s="7" r="D204">
+        <v>729</v>
+      </c>
+      <c t="s" s="7" r="E204">
+        <v>730</v>
+      </c>
     </row>
     <row r="205">
-      <c t="s" s="9" r="A205">
-        <v>726</v>
-      </c>
-      <c t="s" s="7" r="B205">
-        <v>727</v>
-      </c>
-      <c t="s" s="13" r="C205">
-        <v>728</v>
-      </c>
-      <c t="s" s="7" r="D205">
-        <v>729</v>
-      </c>
-      <c t="s" s="7" r="E205">
-        <v>730</v>
-      </c>
+      <c s="9" r="A205"/>
+      <c s="16" r="B205"/>
+      <c s="27" r="C205"/>
+      <c s="16" r="D205"/>
+      <c s="16" r="E205"/>
     </row>
     <row r="206">
-      <c s="9" r="A206"/>
-      <c s="16" r="B206"/>
-      <c s="8" r="C206"/>
-      <c s="16" r="D206"/>
-      <c s="16" r="E206"/>
+      <c t="s" s="9" r="A206">
+        <v>731</v>
+      </c>
+      <c t="s" s="7" r="B206">
+        <v>732</v>
+      </c>
+      <c t="s" s="13" r="C206">
+        <v>733</v>
+      </c>
+      <c t="s" s="7" r="D206">
+        <v>734</v>
+      </c>
+      <c t="s" s="7" r="E206">
+        <v>735</v>
+      </c>
     </row>
     <row r="207">
-      <c t="s" s="9" r="A207">
-        <v>731</v>
-      </c>
+      <c s="9" r="A207"/>
       <c t="s" s="7" r="B207">
-        <v>732</v>
+        <v>736</v>
       </c>
       <c t="s" s="13" r="C207">
-        <v>733</v>
+        <v>737</v>
       </c>
       <c t="s" s="7" r="D207">
-        <v>734</v>
+        <v>738</v>
       </c>
       <c t="s" s="7" r="E207">
-        <v>735</v>
+        <v>739</v>
       </c>
     </row>
     <row r="208">
       <c s="9" r="A208"/>
-      <c t="s" s="7" r="B208">
-        <v>736</v>
-      </c>
-      <c t="s" s="13" r="C208">
-        <v>737</v>
-      </c>
-      <c t="s" s="7" r="D208">
-        <v>738</v>
-      </c>
-      <c t="s" s="7" r="E208">
-        <v>739</v>
-      </c>
+      <c s="16" r="B208"/>
+      <c s="27" r="C208"/>
+      <c s="16" r="D208"/>
+      <c s="16" r="E208"/>
     </row>
     <row r="209">
-      <c s="9" r="A209"/>
+      <c t="s" s="9" r="A209">
+        <v>740</v>
+      </c>
       <c t="s" s="7" r="B209">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c t="s" s="13" r="C209">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c t="s" s="7" r="D209">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c t="s" s="7" r="E209">
-        <v>743</v>
+        <v>744</v>
       </c>
     </row>
     <row r="210">
       <c s="9" r="A210"/>
-      <c t="s" s="7" r="B210">
-        <v>744</v>
-      </c>
-      <c t="s" s="13" r="C210">
+      <c s="16" r="B210"/>
+      <c s="8" r="C210"/>
+      <c s="16" r="D210"/>
+      <c s="16" r="E210"/>
+    </row>
+    <row r="211">
+      <c t="s" s="9" r="A211">
         <v>745</v>
       </c>
-      <c t="s" s="7" r="D210">
+      <c t="s" s="7" r="B211">
         <v>746</v>
       </c>
-      <c t="s" s="7" r="E210">
+      <c t="s" s="13" r="C211">
         <v>747</v>
       </c>
-    </row>
-    <row r="211">
-      <c s="9" r="A211"/>
-      <c t="s" s="7" r="B211">
+      <c t="s" s="7" r="D211">
         <v>748</v>
       </c>
-      <c t="s" s="13" r="C211">
+      <c t="s" s="7" r="E211">
         <v>749</v>
-      </c>
-      <c t="s" s="7" r="D211">
-        <v>750</v>
-      </c>
-      <c t="s" s="7" r="E211">
-        <v>751</v>
       </c>
     </row>
     <row r="212">
       <c s="9" r="A212"/>
       <c t="s" s="7" r="B212">
+        <v>750</v>
+      </c>
+      <c t="s" s="13" r="C212">
+        <v>751</v>
+      </c>
+      <c t="s" s="7" r="D212">
         <v>752</v>
       </c>
-      <c t="s" s="13" r="C212">
+      <c t="s" s="7" r="E212">
         <v>753</v>
-      </c>
-      <c t="s" s="7" r="D212">
-        <v>754</v>
-      </c>
-      <c t="s" s="7" r="E212">
-        <v>755</v>
       </c>
     </row>
     <row r="213">
       <c s="9" r="A213"/>
       <c t="s" s="7" r="B213">
+        <v>754</v>
+      </c>
+      <c t="s" s="13" r="C213">
+        <v>755</v>
+      </c>
+      <c t="s" s="7" r="D213">
         <v>756</v>
       </c>
-      <c t="s" s="13" r="C213">
+      <c t="s" s="7" r="E213">
         <v>757</v>
-      </c>
-      <c t="s" s="7" r="D213">
-        <v>758</v>
-      </c>
-      <c t="s" s="7" r="E213">
-        <v>759</v>
       </c>
     </row>
     <row r="214">
       <c s="9" r="A214"/>
       <c t="s" s="7" r="B214">
+        <v>758</v>
+      </c>
+      <c t="s" s="13" r="C214">
+        <v>759</v>
+      </c>
+      <c t="s" s="7" r="D214">
         <v>760</v>
       </c>
-      <c t="s" s="13" r="C214">
+      <c t="s" s="7" r="E214">
         <v>761</v>
       </c>
-      <c t="s" s="7" r="D214">
+    </row>
+    <row r="215">
+      <c s="9" r="A215"/>
+      <c t="s" s="7" r="B215">
         <v>762</v>
       </c>
-      <c t="s" s="7" r="E214">
+      <c t="s" s="13" r="C215">
         <v>763</v>
       </c>
-    </row>
-    <row r="215">
-      <c s="17" r="A215"/>
-      <c s="16" r="B215"/>
-      <c s="8" r="C215"/>
-      <c s="16" r="D215"/>
-      <c s="16" r="E215"/>
+      <c t="s" s="7" r="D215">
+        <v>764</v>
+      </c>
+      <c t="s" s="7" r="E215">
+        <v>765</v>
+      </c>
     </row>
     <row r="216">
-      <c t="s" s="9" r="A216">
-        <v>764</v>
-      </c>
+      <c s="9" r="A216"/>
       <c t="s" s="7" r="B216">
-        <v>765</v>
-      </c>
-      <c t="s" s="7" r="C216">
         <v>766</v>
       </c>
+      <c t="s" s="13" r="C216">
+        <v>767</v>
+      </c>
       <c t="s" s="7" r="D216">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c t="s" s="7" r="E216">
-        <v>768</v>
+        <v>769</v>
       </c>
     </row>
     <row r="217">
       <c s="9" r="A217"/>
       <c t="s" s="7" r="B217">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c t="s" s="13" r="C217">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c t="s" s="7" r="D217">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c t="s" s="7" r="E217">
-        <v>772</v>
+        <v>773</v>
       </c>
     </row>
     <row r="218">
       <c s="9" r="A218"/>
       <c t="s" s="7" r="B218">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c t="s" s="13" r="C218">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c t="s" s="7" r="D218">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c t="s" s="7" r="E218">
-        <v>776</v>
+        <v>777</v>
       </c>
     </row>
     <row r="219">
-      <c s="9" r="A219"/>
-      <c t="s" s="7" r="B219">
-        <v>777</v>
-      </c>
-      <c t="s" s="13" r="C219">
+      <c s="17" r="A219"/>
+      <c s="16" r="B219"/>
+      <c s="8" r="C219"/>
+      <c s="16" r="D219"/>
+      <c s="16" r="E219"/>
+    </row>
+    <row r="220">
+      <c t="s" s="9" r="A220">
         <v>778</v>
       </c>
-      <c t="s" s="7" r="D219">
+      <c t="s" s="7" r="B220">
         <v>779</v>
       </c>
-      <c t="s" s="7" r="E219">
+      <c t="s" s="7" r="C220">
         <v>780</v>
       </c>
-    </row>
-    <row r="220">
-      <c s="9" r="A220"/>
-      <c t="s" s="7" r="B220">
+      <c t="s" s="7" r="D220">
         <v>781</v>
       </c>
-      <c t="s" s="13" r="C220">
-        <v>514</v>
-      </c>
-      <c t="s" s="7" r="D220">
-        <v>112</v>
-      </c>
       <c t="s" s="7" r="E220">
-        <v>516</v>
+        <v>782</v>
       </c>
     </row>
     <row r="221">
       <c s="9" r="A221"/>
       <c t="s" s="7" r="B221">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c t="s" s="13" r="C221">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c t="s" s="7" r="D221">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c t="s" s="7" r="E221">
-        <v>785</v>
+        <v>786</v>
       </c>
     </row>
     <row r="222">
-      <c s="17" r="A222"/>
-      <c s="16" r="B222"/>
-      <c s="8" r="C222"/>
-      <c s="16" r="D222"/>
-      <c s="16" r="E222"/>
+      <c s="9" r="A222"/>
+      <c t="s" s="7" r="B222">
+        <v>787</v>
+      </c>
+      <c t="s" s="13" r="C222">
+        <v>788</v>
+      </c>
+      <c t="s" s="7" r="D222">
+        <v>789</v>
+      </c>
+      <c t="s" s="7" r="E222">
+        <v>790</v>
+      </c>
     </row>
     <row r="223">
-      <c t="s" s="9" r="A223">
-        <v>786</v>
-      </c>
+      <c s="9" r="A223"/>
       <c t="s" s="7" r="B223">
-        <v>787</v>
+        <v>791</v>
       </c>
       <c t="s" s="13" r="C223">
-        <v>788</v>
+        <v>792</v>
       </c>
       <c t="s" s="7" r="D223">
-        <v>789</v>
+        <v>793</v>
       </c>
       <c t="s" s="7" r="E223">
-        <v>790</v>
+        <v>794</v>
       </c>
     </row>
     <row r="224">
       <c s="9" r="A224"/>
       <c t="s" s="7" r="B224">
-        <v>791</v>
+        <v>795</v>
       </c>
       <c t="s" s="13" r="C224">
-        <v>792</v>
+        <v>516</v>
       </c>
       <c t="s" s="7" r="D224">
-        <v>793</v>
+        <v>112</v>
       </c>
       <c t="s" s="7" r="E224">
-        <v>794</v>
+        <v>518</v>
       </c>
     </row>
     <row r="225">
       <c s="9" r="A225"/>
       <c t="s" s="7" r="B225">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c t="s" s="13" r="C225">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c t="s" s="7" r="D225">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c t="s" s="7" r="E225">
-        <v>798</v>
+        <v>799</v>
       </c>
     </row>
     <row r="226">
-      <c s="9" r="A226"/>
-      <c t="s" s="7" r="B226">
-        <v>799</v>
-      </c>
-      <c t="s" s="13" r="C226">
+      <c s="17" r="A226"/>
+      <c s="16" r="B226"/>
+      <c s="8" r="C226"/>
+      <c s="16" r="D226"/>
+      <c s="16" r="E226"/>
+    </row>
+    <row r="227">
+      <c t="s" s="9" r="A227">
         <v>800</v>
       </c>
-      <c t="s" s="7" r="D226">
+      <c t="s" s="7" r="B227">
         <v>801</v>
       </c>
-      <c t="s" s="7" r="E226">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="227">
-      <c s="9" r="A227"/>
-      <c t="s" s="7" r="B227">
+      <c t="s" s="13" r="C227">
         <v>802</v>
       </c>
-      <c t="s" s="13" r="C227">
+      <c t="s" s="7" r="D227">
         <v>803</v>
       </c>
-      <c t="s" s="7" r="D227">
+      <c t="s" s="7" r="E227">
         <v>804</v>
-      </c>
-      <c t="s" s="7" r="E227">
-        <v>805</v>
       </c>
     </row>
     <row r="228">
       <c s="9" r="A228"/>
       <c t="s" s="7" r="B228">
+        <v>805</v>
+      </c>
+      <c t="s" s="13" r="C228">
         <v>806</v>
       </c>
-      <c t="s" s="13" r="C228">
+      <c t="s" s="7" r="D228">
         <v>807</v>
       </c>
-      <c t="s" s="7" r="D228">
+      <c t="s" s="7" r="E228">
         <v>808</v>
-      </c>
-      <c t="s" s="7" r="E228">
-        <v>809</v>
       </c>
     </row>
     <row r="229">
       <c s="9" r="A229"/>
       <c t="s" s="7" r="B229">
+        <v>809</v>
+      </c>
+      <c t="s" s="13" r="C229">
         <v>810</v>
       </c>
-      <c t="s" s="13" r="C229">
+      <c t="s" s="7" r="D229">
         <v>811</v>
       </c>
-      <c t="s" s="7" r="D229">
+      <c t="s" s="7" r="E229">
         <v>812</v>
-      </c>
-      <c t="s" s="7" r="E229">
-        <v>813</v>
       </c>
     </row>
     <row r="230">
       <c s="9" r="A230"/>
       <c t="s" s="7" r="B230">
+        <v>813</v>
+      </c>
+      <c t="s" s="13" r="C230">
         <v>814</v>
       </c>
-      <c t="s" s="13" r="C230">
+      <c t="s" s="7" r="D230">
         <v>815</v>
       </c>
-      <c t="s" s="7" r="D230">
-        <v>816</v>
-      </c>
       <c t="s" s="7" r="E230">
-        <v>817</v>
+        <v>815</v>
       </c>
     </row>
     <row r="231">
       <c s="9" r="A231"/>
       <c t="s" s="7" r="B231">
+        <v>816</v>
+      </c>
+      <c t="s" s="13" r="C231">
+        <v>817</v>
+      </c>
+      <c t="s" s="7" r="D231">
         <v>818</v>
       </c>
-      <c t="s" s="13" r="C231">
+      <c t="s" s="7" r="E231">
         <v>819</v>
-      </c>
-      <c t="s" s="7" r="D231">
-        <v>820</v>
-      </c>
-      <c t="s" s="7" r="E231">
-        <v>821</v>
       </c>
     </row>
     <row r="232">
       <c s="9" r="A232"/>
       <c t="s" s="7" r="B232">
+        <v>820</v>
+      </c>
+      <c t="s" s="13" r="C232">
+        <v>821</v>
+      </c>
+      <c t="s" s="7" r="D232">
         <v>822</v>
       </c>
-      <c t="s" s="13" r="C232">
+      <c t="s" s="7" r="E232">
         <v>823</v>
-      </c>
-      <c t="s" s="7" r="D232">
-        <v>824</v>
-      </c>
-      <c t="s" s="7" r="E232">
-        <v>825</v>
       </c>
     </row>
     <row r="233">
       <c s="9" r="A233"/>
       <c t="s" s="7" r="B233">
+        <v>824</v>
+      </c>
+      <c t="s" s="13" r="C233">
+        <v>825</v>
+      </c>
+      <c t="s" s="7" r="D233">
         <v>826</v>
       </c>
-      <c t="s" s="13" r="C233">
+      <c t="s" s="7" r="E233">
         <v>827</v>
-      </c>
-      <c t="s" s="7" r="D233">
-        <v>828</v>
-      </c>
-      <c t="s" s="7" r="E233">
-        <v>829</v>
       </c>
     </row>
     <row r="234">
       <c s="9" r="A234"/>
       <c t="s" s="7" r="B234">
+        <v>828</v>
+      </c>
+      <c t="s" s="13" r="C234">
+        <v>829</v>
+      </c>
+      <c t="s" s="7" r="D234">
         <v>830</v>
       </c>
-      <c t="s" s="13" r="C234">
+      <c t="s" s="7" r="E234">
         <v>831</v>
-      </c>
-      <c t="s" s="7" r="D234">
-        <v>832</v>
-      </c>
-      <c t="s" s="7" r="E234">
-        <v>833</v>
       </c>
     </row>
     <row r="235">
       <c s="9" r="A235"/>
       <c t="s" s="7" r="B235">
+        <v>832</v>
+      </c>
+      <c t="s" s="13" r="C235">
+        <v>833</v>
+      </c>
+      <c t="s" s="7" r="D235">
         <v>834</v>
-      </c>
-      <c t="s" s="13" r="C235">
-        <v>835</v>
-      </c>
-      <c t="s" s="7" r="D235">
-        <v>835</v>
       </c>
       <c t="s" s="7" r="E235">
         <v>835</v>
@@ -6870,453 +6923,537 @@
         <v>849</v>
       </c>
       <c t="s" s="7" r="D239">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c t="s" s="7" r="E239">
-        <v>851</v>
+        <v>849</v>
       </c>
     </row>
     <row r="240">
       <c s="9" r="A240"/>
       <c t="s" s="7" r="B240">
+        <v>850</v>
+      </c>
+      <c t="s" s="13" r="C240">
+        <v>851</v>
+      </c>
+      <c t="s" s="7" r="D240">
         <v>852</v>
       </c>
-      <c t="s" s="13" r="C240">
+      <c t="s" s="7" r="E240">
         <v>853</v>
-      </c>
-      <c t="s" s="7" r="D240">
-        <v>854</v>
-      </c>
-      <c t="s" s="7" r="E240">
-        <v>855</v>
       </c>
     </row>
     <row r="241">
       <c s="9" r="A241"/>
       <c t="s" s="7" r="B241">
+        <v>854</v>
+      </c>
+      <c t="s" s="13" r="C241">
+        <v>855</v>
+      </c>
+      <c t="s" s="7" r="D241">
         <v>856</v>
       </c>
-      <c t="s" s="13" r="C241">
+      <c t="s" s="7" r="E241">
         <v>857</v>
-      </c>
-      <c t="s" s="7" r="D241">
-        <v>858</v>
-      </c>
-      <c t="s" s="7" r="E241">
-        <v>859</v>
       </c>
     </row>
     <row r="242">
       <c s="9" r="A242"/>
       <c t="s" s="7" r="B242">
+        <v>858</v>
+      </c>
+      <c t="s" s="13" r="C242">
+        <v>859</v>
+      </c>
+      <c t="s" s="7" r="D242">
         <v>860</v>
       </c>
-      <c t="s" s="13" r="C242">
+      <c t="s" s="7" r="E242">
         <v>861</v>
-      </c>
-      <c t="s" s="7" r="D242">
-        <v>862</v>
-      </c>
-      <c t="s" s="7" r="E242">
-        <v>863</v>
       </c>
     </row>
     <row r="243">
       <c s="9" r="A243"/>
-      <c s="16" r="B243"/>
-      <c s="8" r="C243"/>
-      <c s="16" r="D243"/>
-      <c s="16" r="E243"/>
+      <c t="s" s="7" r="B243">
+        <v>862</v>
+      </c>
+      <c t="s" s="13" r="C243">
+        <v>863</v>
+      </c>
+      <c t="s" s="7" r="D243">
+        <v>864</v>
+      </c>
+      <c t="s" s="7" r="E243">
+        <v>865</v>
+      </c>
     </row>
     <row r="244">
-      <c t="s" s="9" r="A244">
-        <v>864</v>
-      </c>
+      <c s="9" r="A244"/>
       <c t="s" s="7" r="B244">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c t="s" s="13" r="C244">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c t="s" s="7" r="D244">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c t="s" s="7" r="E244">
-        <v>868</v>
+        <v>869</v>
       </c>
     </row>
     <row r="245">
       <c s="9" r="A245"/>
       <c t="s" s="7" r="B245">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c t="s" s="13" r="C245">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c t="s" s="7" r="D245">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c t="s" s="7" r="E245">
-        <v>872</v>
+        <v>873</v>
       </c>
     </row>
     <row r="246">
       <c s="9" r="A246"/>
       <c t="s" s="7" r="B246">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c t="s" s="13" r="C246">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c t="s" s="7" r="D246">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c t="s" s="7" r="E246">
-        <v>876</v>
+        <v>877</v>
       </c>
     </row>
     <row r="247">
       <c s="9" r="A247"/>
-      <c t="s" s="7" r="B247">
-        <v>877</v>
-      </c>
-      <c t="s" s="13" r="C247">
+      <c s="16" r="B247"/>
+      <c s="8" r="C247"/>
+      <c s="16" r="D247"/>
+      <c s="16" r="E247"/>
+    </row>
+    <row r="248">
+      <c t="s" s="9" r="A248">
         <v>878</v>
       </c>
-      <c t="s" s="7" r="D247">
+      <c t="s" s="7" r="B248">
         <v>879</v>
       </c>
-      <c t="s" s="7" r="E247">
+      <c t="s" s="13" r="C248">
         <v>880</v>
       </c>
-    </row>
-    <row r="248">
-      <c s="9" r="A248"/>
-      <c t="s" s="7" r="B248">
+      <c t="s" s="7" r="D248">
         <v>881</v>
       </c>
-      <c t="s" s="13" r="C248">
-        <v>881</v>
-      </c>
-      <c t="s" s="18" r="D248">
+      <c t="s" s="7" r="E248">
         <v>882</v>
-      </c>
-      <c t="s" s="18" r="E248">
-        <v>883</v>
       </c>
     </row>
     <row r="249">
       <c s="9" r="A249"/>
       <c t="s" s="7" r="B249">
+        <v>883</v>
+      </c>
+      <c t="s" s="13" r="C249">
         <v>884</v>
       </c>
-      <c t="s" s="13" r="C249">
+      <c t="s" s="7" r="D249">
         <v>885</v>
       </c>
-      <c t="s" s="7" r="D249">
+      <c t="s" s="7" r="E249">
         <v>886</v>
-      </c>
-      <c t="s" s="7" r="E249">
-        <v>887</v>
       </c>
     </row>
     <row r="250">
       <c s="9" r="A250"/>
       <c t="s" s="7" r="B250">
+        <v>887</v>
+      </c>
+      <c t="s" s="13" r="C250">
         <v>888</v>
       </c>
-      <c t="s" s="13" r="C250">
+      <c t="s" s="7" r="D250">
         <v>889</v>
       </c>
-      <c t="s" s="7" r="D250">
+      <c t="s" s="7" r="E250">
         <v>890</v>
       </c>
-      <c t="s" s="7" r="E250">
+    </row>
+    <row r="251">
+      <c s="9" r="A251"/>
+      <c t="s" s="7" r="B251">
         <v>891</v>
       </c>
-    </row>
-    <row r="251">
-      <c t="s" s="16" r="A251">
+      <c t="s" s="13" r="C251">
         <v>892</v>
       </c>
-      <c s="24" r="B251"/>
-      <c t="s" s="13" r="C251">
+      <c t="s" s="7" r="D251">
         <v>893</v>
       </c>
-      <c t="s" s="18" r="D251">
+      <c t="s" s="7" r="E251">
         <v>894</v>
       </c>
-      <c t="s" s="18" r="E251">
+    </row>
+    <row r="252">
+      <c s="9" r="A252"/>
+      <c t="s" s="7" r="B252">
         <v>895</v>
       </c>
-    </row>
-    <row r="252">
-      <c s="17" r="A252"/>
-      <c s="16" r="B252"/>
-      <c s="8" r="C252"/>
-      <c s="16" r="D252"/>
-      <c s="16" r="E252"/>
+      <c t="s" s="13" r="C252">
+        <v>895</v>
+      </c>
+      <c t="s" s="18" r="D252">
+        <v>896</v>
+      </c>
+      <c t="s" s="18" r="E252">
+        <v>897</v>
+      </c>
     </row>
     <row r="253">
-      <c t="s" s="17" r="A253">
-        <v>896</v>
-      </c>
+      <c s="9" r="A253"/>
       <c t="s" s="7" r="B253">
-        <v>897</v>
-      </c>
-      <c t="s" s="7" r="C253">
         <v>898</v>
       </c>
+      <c t="s" s="13" r="C253">
+        <v>899</v>
+      </c>
       <c t="s" s="7" r="D253">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c t="s" s="7" r="E253">
-        <v>900</v>
+        <v>901</v>
       </c>
     </row>
     <row r="254">
+      <c s="9" r="A254"/>
       <c t="s" s="7" r="B254">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c t="s" s="13" r="C254">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c t="s" s="7" r="D254">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c t="s" s="7" r="E254">
-        <v>904</v>
+        <v>905</v>
       </c>
     </row>
     <row r="255">
-      <c t="s" s="7" r="B255">
-        <v>905</v>
-      </c>
-      <c t="s" s="7" r="C255">
+      <c t="s" s="16" r="A255">
         <v>906</v>
       </c>
-      <c t="s" s="7" r="D255">
+      <c s="24" r="B255"/>
+      <c t="s" s="13" r="C255">
         <v>907</v>
       </c>
-      <c t="s" s="7" r="E255">
+      <c t="s" s="18" r="D255">
         <v>908</v>
+      </c>
+      <c t="s" s="18" r="E255">
+        <v>909</v>
       </c>
     </row>
     <row r="256">
       <c s="17" r="A256"/>
-      <c t="s" s="7" r="B256">
-        <v>909</v>
-      </c>
-      <c t="s" s="13" r="C256">
+      <c s="16" r="B256"/>
+      <c s="8" r="C256"/>
+      <c s="16" r="D256"/>
+      <c s="16" r="E256"/>
+    </row>
+    <row r="257">
+      <c t="s" s="17" r="A257">
         <v>910</v>
       </c>
-      <c t="s" s="7" r="D256">
+      <c t="s" s="7" r="B257">
         <v>911</v>
       </c>
-      <c t="s" s="7" r="E256">
+      <c t="s" s="7" r="C257">
         <v>912</v>
       </c>
-    </row>
-    <row r="257">
-      <c s="17" r="A257"/>
-      <c t="s" s="7" r="B257">
+      <c t="s" s="7" r="D257">
         <v>913</v>
       </c>
-      <c t="s" s="7" r="C257">
+      <c t="s" s="7" r="E257">
         <v>914</v>
       </c>
-      <c t="s" s="7" r="D257">
+    </row>
+    <row r="258">
+      <c t="s" s="7" r="B258">
         <v>915</v>
       </c>
-      <c t="s" s="7" r="E257">
+      <c t="s" s="13" r="C258">
         <v>916</v>
       </c>
-    </row>
-    <row r="258">
-      <c s="17" r="A258"/>
-      <c t="s" s="7" r="B258">
+      <c t="s" s="7" r="D258">
         <v>917</v>
       </c>
-      <c t="s" s="13" r="C258">
+      <c t="s" s="7" r="E258">
         <v>918</v>
       </c>
-      <c t="s" s="7" r="D258">
+    </row>
+    <row r="259">
+      <c t="s" s="7" r="B259">
         <v>919</v>
       </c>
-      <c t="s" s="7" r="E258">
+      <c t="s" s="7" r="C259">
         <v>920</v>
       </c>
-    </row>
-    <row r="259">
-      <c s="17" r="A259"/>
-      <c t="s" s="7" r="B259">
+      <c t="s" s="7" r="D259">
         <v>921</v>
       </c>
-      <c t="s" s="7" r="C259">
+      <c t="s" s="7" r="E259">
         <v>922</v>
-      </c>
-      <c t="s" s="7" r="D259">
-        <v>923</v>
-      </c>
-      <c t="s" s="7" r="E259">
-        <v>924</v>
       </c>
     </row>
     <row r="260">
       <c s="17" r="A260"/>
       <c t="s" s="7" r="B260">
+        <v>923</v>
+      </c>
+      <c t="s" s="13" r="C260">
+        <v>924</v>
+      </c>
+      <c t="s" s="7" r="D260">
         <v>925</v>
       </c>
-      <c t="s" s="13" r="C260">
+      <c t="s" s="7" r="E260">
         <v>926</v>
-      </c>
-      <c t="s" s="7" r="D260">
-        <v>927</v>
-      </c>
-      <c t="s" s="7" r="E260">
-        <v>928</v>
       </c>
     </row>
     <row r="261">
       <c s="17" r="A261"/>
       <c t="s" s="7" r="B261">
+        <v>927</v>
+      </c>
+      <c t="s" s="7" r="C261">
+        <v>928</v>
+      </c>
+      <c t="s" s="7" r="D261">
         <v>929</v>
       </c>
-      <c t="s" s="7" r="C261">
+      <c t="s" s="7" r="E261">
         <v>930</v>
-      </c>
-      <c t="s" s="7" r="D261">
-        <v>931</v>
-      </c>
-      <c t="s" s="7" r="E261">
-        <v>932</v>
       </c>
     </row>
     <row r="262">
       <c s="17" r="A262"/>
       <c t="s" s="7" r="B262">
+        <v>931</v>
+      </c>
+      <c t="s" s="13" r="C262">
+        <v>932</v>
+      </c>
+      <c t="s" s="7" r="D262">
         <v>933</v>
       </c>
-      <c t="s" s="13" r="C262">
+      <c t="s" s="7" r="E262">
         <v>934</v>
-      </c>
-      <c t="s" s="7" r="D262">
-        <v>935</v>
-      </c>
-      <c t="s" s="7" r="E262">
-        <v>936</v>
       </c>
     </row>
     <row r="263">
       <c s="17" r="A263"/>
       <c t="s" s="7" r="B263">
+        <v>935</v>
+      </c>
+      <c t="s" s="7" r="C263">
+        <v>936</v>
+      </c>
+      <c t="s" s="7" r="D263">
         <v>937</v>
       </c>
-      <c t="s" s="7" r="C263">
+      <c t="s" s="7" r="E263">
         <v>938</v>
-      </c>
-      <c t="s" s="7" r="D263">
-        <v>939</v>
-      </c>
-      <c t="s" s="7" r="E263">
-        <v>940</v>
       </c>
     </row>
     <row r="264">
       <c s="17" r="A264"/>
       <c t="s" s="7" r="B264">
+        <v>939</v>
+      </c>
+      <c t="s" s="13" r="C264">
+        <v>940</v>
+      </c>
+      <c t="s" s="7" r="D264">
         <v>941</v>
       </c>
-      <c t="s" s="13" r="C264">
-        <v>934</v>
-      </c>
-      <c t="s" s="7" r="D264">
-        <v>935</v>
-      </c>
       <c t="s" s="7" r="E264">
-        <v>936</v>
+        <v>942</v>
       </c>
     </row>
     <row r="265">
       <c s="17" r="A265"/>
       <c t="s" s="7" r="B265">
-        <v>942</v>
-      </c>
-      <c t="s" s="13" r="C265">
         <v>943</v>
       </c>
+      <c t="s" s="7" r="C265">
+        <v>944</v>
+      </c>
       <c t="s" s="7" r="D265">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c t="s" s="7" r="E265">
-        <v>945</v>
+        <v>946</v>
       </c>
     </row>
     <row r="266">
       <c s="17" r="A266"/>
       <c t="s" s="7" r="B266">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c t="s" s="13" r="C266">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c t="s" s="7" r="D266">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c t="s" s="7" r="E266">
-        <v>949</v>
+        <v>950</v>
       </c>
     </row>
     <row r="267">
       <c s="17" r="A267"/>
       <c t="s" s="7" r="B267">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c t="s" s="7" r="C267">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c t="s" s="7" r="D267">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c t="s" s="7" r="E267">
-        <v>953</v>
+        <v>954</v>
       </c>
     </row>
     <row r="268">
       <c s="17" r="A268"/>
       <c t="s" s="7" r="B268">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c t="s" s="13" r="C268">
-        <v>955</v>
+        <v>948</v>
       </c>
       <c t="s" s="7" r="D268">
+        <v>949</v>
+      </c>
+      <c t="s" s="7" r="E268">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="269">
+      <c s="17" r="A269"/>
+      <c t="s" s="7" r="B269">
         <v>956</v>
       </c>
-      <c t="s" s="7" r="E268">
+      <c t="s" s="13" r="C269">
         <v>957</v>
       </c>
-    </row>
-    <row r="269">
-      <c s="9" r="A269"/>
-      <c t="s" s="7" r="B269">
+      <c t="s" s="7" r="D269">
         <v>958</v>
       </c>
-      <c t="s" s="13" r="C269">
+      <c t="s" s="7" r="E269">
         <v>959</v>
       </c>
-      <c t="s" s="7" r="D269">
+    </row>
+    <row r="270">
+      <c s="17" r="A270"/>
+      <c t="s" s="7" r="B270">
         <v>960</v>
       </c>
-      <c t="s" s="7" r="E269">
+      <c t="s" s="13" r="C270">
         <v>961</v>
       </c>
-    </row>
-    <row r="270">
-      <c s="9" r="A270"/>
-      <c s="8" r="C270"/>
-      <c s="16" r="D270"/>
-      <c s="16" r="E270"/>
+      <c t="s" s="7" r="D270">
+        <v>962</v>
+      </c>
+      <c t="s" s="7" r="E270">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="271">
+      <c s="17" r="A271"/>
+      <c t="s" s="7" r="B271">
+        <v>964</v>
+      </c>
+      <c t="s" s="7" r="C271">
+        <v>965</v>
+      </c>
+      <c t="s" s="7" r="D271">
+        <v>966</v>
+      </c>
+      <c t="s" s="7" r="E271">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="272">
+      <c s="17" r="A272"/>
+      <c t="s" s="7" r="B272">
+        <v>968</v>
+      </c>
+      <c t="s" s="13" r="C272">
+        <v>969</v>
+      </c>
+      <c t="s" s="7" r="D272">
+        <v>970</v>
+      </c>
+      <c t="s" s="7" r="E272">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="273">
+      <c s="9" r="A273"/>
+      <c t="s" s="7" r="B273">
+        <v>972</v>
+      </c>
+      <c t="s" s="13" r="C273">
+        <v>973</v>
+      </c>
+      <c t="s" s="7" r="D273">
+        <v>974</v>
+      </c>
+      <c t="s" s="7" r="E273">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="274">
+      <c t="s" s="9" r="A274">
+        <v>976</v>
+      </c>
+      <c t="s" s="2" r="B274">
+        <v>977</v>
+      </c>
+      <c t="s" s="32" r="C274">
+        <v>978</v>
+      </c>
+      <c s="18" r="D274"/>
+      <c s="18" r="E274"/>
+    </row>
+    <row r="275">
+      <c s="9" r="A275"/>
+      <c t="s" s="2" r="B275">
+        <v>979</v>
+      </c>
+      <c t="s" s="2" r="C275">
+        <v>980</v>
+      </c>
+      <c s="18" r="D275"/>
+      <c s="18" r="E275"/>
+    </row>
+    <row r="276">
+      <c s="9" r="A276"/>
+      <c s="8" r="C276"/>
+      <c s="16" r="D276"/>
+      <c s="16" r="E276"/>
     </row>
   </sheetData>
 </worksheet>
@@ -7334,17 +7471,17 @@
   <sheetData>
     <row customHeight="1" r="1" ht="112.5">
       <c t="s" s="4" r="A1">
-        <v>962</v>
+        <v>981</v>
       </c>
     </row>
     <row customHeight="1" r="2" ht="112.5">
       <c t="s" s="5" r="A2">
-        <v>963</v>
+        <v>982</v>
       </c>
     </row>
     <row customHeight="1" r="3" ht="112.5">
       <c t="s" s="10" r="A3">
-        <v>964</v>
+        <v>983</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EWD-22165 - Publish to easygenerator hosting : Add localization texts.
Former-commit-id: 358cde89955a546c98e3dbcd3b1a4b63b4c2b994
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="984">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="994">
   <si>
     <t>Page</t>
   </si>
@@ -703,6 +703,25 @@
     <t>Copy link</t>
   </si>
   <si>
+    <t>Koppeling kopiëren</t>
+  </si>
+  <si>
+    <t>Link kopieren</t>
+  </si>
+  <si>
+    <t>publishFailed</t>
+  </si>
+  <si>
+    <t>Failed. Try again.</t>
+  </si>
+  <si>
+    <t>Mislukt. Probeer het opnieuw.
+</t>
+  </si>
+  <si>
+    <t>Fehlgeschlagen. Versuchen Sie es erneut.</t>
+  </si>
+  <si>
     <t>CreateObjective</t>
   </si>
   <si>
@@ -1071,7 +1090,7 @@
     <t>Related question</t>
   </si>
   <si>
-    <t>Verwante vraag</t>
+    <t>Gerelateerde vraag</t>
   </si>
   <si>
     <t>Verwandte Frage</t>
@@ -2644,13 +2663,13 @@
     <t>ChooseYourCountry</t>
   </si>
   <si>
-    <t>Choose your country</t>
-  </si>
-  <si>
-    <t>Kies uw land</t>
-  </si>
-  <si>
-    <t>Wählen Sie Ihr Land aus</t>
+    <t>Choose your country...</t>
+  </si>
+  <si>
+    <t>Kies uw land...</t>
+  </si>
+  <si>
+    <t>Wählen Sie Ihr Land aus...</t>
   </si>
   <si>
     <t>Forgot password</t>
@@ -2986,10 +3005,22 @@
     <t>This learning experience is being updated</t>
   </si>
   <si>
+    <t>Deze leerervaring wordt bijgewerkt</t>
+  </si>
+  <si>
+    <t>Diese Lernerfahrung wird gerade aktualisiert.</t>
+  </si>
+  <si>
     <t>publishIsInProgressText</t>
   </si>
   <si>
     <t>Please, try again after few minutes</t>
+  </si>
+  <si>
+    <t>Wacht enkele minuten en probeer het opnieuw</t>
+  </si>
+  <si>
+    <t>Bitte versuchen Sie es in einigen Minuten erneut.</t>
   </si>
   <si>
     <t>Translated OK</t>
@@ -4385,3075 +4416,3104 @@
     </row>
     <row r="60">
       <c s="11" r="A60"/>
-      <c t="s" s="2" r="B60">
+      <c t="s" s="24" r="B60">
         <v>227</v>
       </c>
-      <c t="s" s="18" r="C60">
+      <c t="s" s="7" r="C60">
         <v>228</v>
       </c>
-      <c s="2" r="D60"/>
-      <c s="2" r="E60"/>
+      <c t="s" s="2" r="D60">
+        <v>229</v>
+      </c>
+      <c t="s" s="2" r="E60">
+        <v>230</v>
+      </c>
     </row>
     <row r="61">
       <c s="11" r="A61"/>
-      <c s="11" r="B61"/>
-      <c s="11" r="C61"/>
-      <c s="11" r="D61"/>
-      <c s="11" r="E61"/>
+      <c t="s" s="24" r="B61">
+        <v>231</v>
+      </c>
+      <c t="s" s="7" r="C61">
+        <v>232</v>
+      </c>
+      <c t="s" s="2" r="D61">
+        <v>233</v>
+      </c>
+      <c t="s" s="2" r="E61">
+        <v>234</v>
+      </c>
     </row>
     <row r="62">
-      <c t="s" s="11" r="A62">
-        <v>229</v>
-      </c>
-      <c t="s" s="7" r="B62">
-        <v>230</v>
-      </c>
-      <c t="s" s="7" r="C62">
-        <v>231</v>
-      </c>
-      <c t="s" s="7" r="D62">
-        <v>232</v>
-      </c>
-      <c t="s" s="7" r="E62">
-        <v>233</v>
-      </c>
+      <c s="11" r="A62"/>
+      <c s="11" r="B62"/>
+      <c s="11" r="C62"/>
+      <c s="11" r="D62"/>
+      <c s="11" r="E62"/>
     </row>
     <row r="63">
-      <c s="11" r="A63"/>
+      <c t="s" s="11" r="A63">
+        <v>235</v>
+      </c>
       <c t="s" s="7" r="B63">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c t="s" s="7" r="C63">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c t="s" s="7" r="D63">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c t="s" s="7" r="E63">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="65">
-      <c s="19" r="A65"/>
-      <c s="19" r="B65"/>
-      <c s="19" r="C65"/>
-      <c s="19" r="D65"/>
-      <c s="19" r="E65"/>
+        <v>239</v>
+      </c>
+    </row>
+    <row r="64">
+      <c s="11" r="A64"/>
+      <c t="s" s="7" r="B64">
+        <v>240</v>
+      </c>
+      <c t="s" s="7" r="C64">
+        <v>241</v>
+      </c>
+      <c t="s" s="7" r="D64">
+        <v>242</v>
+      </c>
+      <c t="s" s="7" r="E64">
+        <v>243</v>
+      </c>
     </row>
     <row r="66">
-      <c t="s" s="11" r="A66">
-        <v>238</v>
-      </c>
-      <c t="s" s="7" r="B66">
-        <v>239</v>
-      </c>
-      <c t="s" s="7" r="C66">
-        <v>240</v>
-      </c>
-      <c t="s" s="7" r="D66">
-        <v>241</v>
-      </c>
-      <c t="s" s="7" r="E66">
-        <v>242</v>
-      </c>
+      <c s="19" r="A66"/>
+      <c s="19" r="B66"/>
+      <c s="19" r="C66"/>
+      <c s="19" r="D66"/>
+      <c s="19" r="E66"/>
     </row>
     <row r="67">
-      <c s="11" r="A67"/>
+      <c t="s" s="11" r="A67">
+        <v>244</v>
+      </c>
       <c t="s" s="7" r="B67">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c t="s" s="7" r="C67">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c t="s" s="7" r="D67">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c t="s" s="7" r="E67">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="68">
       <c s="11" r="A68"/>
       <c t="s" s="7" r="B68">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c t="s" s="7" r="C68">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c t="s" s="7" r="D68">
-        <v>249</v>
-      </c>
-      <c t="s" s="7" r="E68">
-        <v>250</v>
+        <v>251</v>
+      </c>
+      <c t="s" s="18" r="E68">
+        <v>252</v>
       </c>
     </row>
     <row r="69">
       <c s="11" r="A69"/>
       <c t="s" s="7" r="B69">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c t="s" s="7" r="C69">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c t="s" s="7" r="D69">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c t="s" s="7" r="E69">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="70">
       <c s="11" r="A70"/>
       <c t="s" s="7" r="B70">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c t="s" s="7" r="C70">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c t="s" s="7" r="D70">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c t="s" s="7" r="E70">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="71">
       <c s="11" r="A71"/>
       <c t="s" s="7" r="B71">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c t="s" s="7" r="C71">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c t="s" s="7" r="D71">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c t="s" s="7" r="E71">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="72">
       <c s="11" r="A72"/>
-      <c s="11" r="B72"/>
-      <c s="11" r="C72"/>
-      <c s="11" r="D72"/>
-      <c s="11" r="E72"/>
+      <c t="s" s="7" r="B72">
+        <v>265</v>
+      </c>
+      <c t="s" s="7" r="C72">
+        <v>266</v>
+      </c>
+      <c t="s" s="7" r="D72">
+        <v>267</v>
+      </c>
+      <c t="s" s="7" r="E72">
+        <v>268</v>
+      </c>
     </row>
     <row r="73">
-      <c t="s" s="11" r="A73">
-        <v>263</v>
-      </c>
-      <c t="s" s="7" r="B73">
-        <v>264</v>
-      </c>
-      <c t="s" s="7" r="C73">
-        <v>265</v>
-      </c>
-      <c t="s" s="7" r="D73">
-        <v>266</v>
-      </c>
-      <c t="s" s="7" r="E73">
-        <v>267</v>
-      </c>
+      <c s="11" r="A73"/>
+      <c s="11" r="B73"/>
+      <c s="11" r="C73"/>
+      <c s="11" r="D73"/>
+      <c s="11" r="E73"/>
     </row>
     <row r="74">
-      <c s="11" r="A74"/>
+      <c t="s" s="11" r="A74">
+        <v>269</v>
+      </c>
       <c t="s" s="7" r="B74">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c t="s" s="7" r="C74">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c t="s" s="7" r="D74">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c t="s" s="7" r="E74">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="75">
       <c s="11" r="A75"/>
       <c t="s" s="7" r="B75">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c t="s" s="7" r="C75">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c t="s" s="7" r="D75">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c t="s" s="7" r="E75">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="76">
       <c s="11" r="A76"/>
       <c t="s" s="7" r="B76">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c t="s" s="7" r="C76">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c t="s" s="7" r="D76">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c t="s" s="7" r="E76">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="77">
       <c s="11" r="A77"/>
       <c t="s" s="7" r="B77">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c t="s" s="7" r="C77">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c t="s" s="7" r="D77">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c t="s" s="7" r="E77">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="78">
       <c s="11" r="A78"/>
       <c t="s" s="7" r="B78">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c t="s" s="7" r="C78">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c t="s" s="7" r="D78">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c t="s" s="7" r="E78">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="79">
       <c s="11" r="A79"/>
       <c t="s" s="7" r="B79">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c t="s" s="7" r="C79">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c t="s" s="7" r="D79">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c t="s" s="7" r="E79">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="80">
       <c s="11" r="A80"/>
       <c t="s" s="7" r="B80">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c t="s" s="7" r="C80">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c t="s" s="7" r="D80">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c t="s" s="7" r="E80">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="81">
       <c s="11" r="A81"/>
       <c t="s" s="7" r="B81">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c t="s" s="7" r="C81">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c t="s" s="7" r="D81">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c t="s" s="7" r="E81">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="82">
       <c s="11" r="A82"/>
-      <c s="11" r="B82"/>
-      <c s="11" r="C82"/>
-      <c s="11" r="D82"/>
-      <c s="11" r="E82"/>
+      <c t="s" s="7" r="B82">
+        <v>302</v>
+      </c>
+      <c t="s" s="7" r="C82">
+        <v>303</v>
+      </c>
+      <c t="s" s="7" r="D82">
+        <v>304</v>
+      </c>
+      <c t="s" s="7" r="E82">
+        <v>305</v>
+      </c>
     </row>
     <row r="83">
-      <c t="s" s="11" r="A83">
-        <v>300</v>
-      </c>
-      <c t="s" s="7" r="B83">
-        <v>301</v>
-      </c>
-      <c t="s" s="7" r="C83">
-        <v>302</v>
-      </c>
-      <c t="s" s="7" r="D83">
-        <v>303</v>
-      </c>
-      <c t="s" s="7" r="E83">
-        <v>304</v>
-      </c>
+      <c s="11" r="A83"/>
+      <c s="11" r="B83"/>
+      <c s="11" r="C83"/>
+      <c s="11" r="D83"/>
+      <c s="11" r="E83"/>
     </row>
     <row r="84">
-      <c s="11" r="A84"/>
+      <c t="s" s="11" r="A84">
+        <v>306</v>
+      </c>
       <c t="s" s="7" r="B84">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c t="s" s="7" r="C84">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c t="s" s="7" r="D84">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c t="s" s="7" r="E84">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="85">
-      <c s="9" r="A85"/>
+      <c s="11" r="A85"/>
       <c t="s" s="7" r="B85">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c t="s" s="7" r="C85">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c t="s" s="7" r="D85">
-        <v>311</v>
-      </c>
-      <c t="s" s="7" r="E85">
-        <v>312</v>
+        <v>313</v>
+      </c>
+      <c t="s" s="18" r="E85">
+        <v>314</v>
       </c>
     </row>
     <row r="86">
       <c s="9" r="A86"/>
       <c t="s" s="7" r="B86">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c t="s" s="7" r="C86">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c t="s" s="7" r="D86">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c t="s" s="7" r="E86">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="87">
       <c s="9" r="A87"/>
       <c t="s" s="7" r="B87">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c t="s" s="7" r="C87">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c t="s" s="7" r="D87">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c t="s" s="7" r="E87">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="88">
       <c s="9" r="A88"/>
       <c t="s" s="7" r="B88">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c t="s" s="7" r="C88">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c t="s" s="7" r="D88">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c t="s" s="7" r="E88">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="89">
       <c s="9" r="A89"/>
       <c t="s" s="7" r="B89">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c t="s" s="7" r="C89">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c t="s" s="7" r="D89">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c t="s" s="7" r="E89">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="90">
       <c s="9" r="A90"/>
       <c t="s" s="7" r="B90">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c t="s" s="7" r="C90">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c t="s" s="7" r="D90">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c t="s" s="7" r="E90">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="91">
       <c s="9" r="A91"/>
       <c t="s" s="7" r="B91">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c t="s" s="7" r="C91">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c t="s" s="7" r="D91">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c t="s" s="7" r="E91">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="92">
       <c s="9" r="A92"/>
       <c t="s" s="7" r="B92">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c t="s" s="7" r="C92">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c t="s" s="7" r="D92">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c t="s" s="7" r="E92">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="93">
       <c s="9" r="A93"/>
       <c t="s" s="7" r="B93">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c t="s" s="7" r="C93">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c t="s" s="7" r="D93">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c t="s" s="7" r="E93">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="94">
       <c s="9" r="A94"/>
       <c t="s" s="7" r="B94">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c t="s" s="7" r="C94">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c t="s" s="7" r="D94">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c t="s" s="7" r="E94">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="95">
       <c s="9" r="A95"/>
       <c t="s" s="7" r="B95">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c t="s" s="7" r="C95">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c t="s" s="7" r="D95">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c t="s" s="7" r="E95">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="96">
       <c s="9" r="A96"/>
       <c t="s" s="7" r="B96">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c t="s" s="7" r="C96">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c t="s" s="7" r="D96">
-        <v>355</v>
-      </c>
-      <c t="s" s="7" r="E96">
-        <v>356</v>
+        <v>357</v>
+      </c>
+      <c t="s" s="18" r="E96">
+        <v>358</v>
       </c>
     </row>
     <row r="97">
       <c s="9" r="A97"/>
       <c t="s" s="7" r="B97">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c t="s" s="7" r="C97">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c t="s" s="7" r="D97">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c t="s" s="7" r="E97">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="98">
       <c s="9" r="A98"/>
-      <c s="11" r="B98"/>
-      <c s="11" r="C98"/>
-      <c s="11" r="D98"/>
-      <c s="11" r="E98"/>
+      <c t="s" s="7" r="B98">
+        <v>363</v>
+      </c>
+      <c t="s" s="7" r="C98">
+        <v>364</v>
+      </c>
+      <c t="s" s="7" r="D98">
+        <v>365</v>
+      </c>
+      <c t="s" s="7" r="E98">
+        <v>366</v>
+      </c>
     </row>
     <row r="99">
-      <c t="s" s="9" r="A99">
-        <v>361</v>
-      </c>
-      <c t="s" s="7" r="B99">
-        <v>362</v>
-      </c>
-      <c t="s" s="7" r="C99">
-        <v>363</v>
-      </c>
-      <c t="s" s="7" r="D99">
-        <v>364</v>
-      </c>
-      <c t="s" s="7" r="E99">
-        <v>365</v>
-      </c>
+      <c s="9" r="A99"/>
+      <c s="11" r="B99"/>
+      <c s="11" r="C99"/>
+      <c s="11" r="D99"/>
+      <c s="11" r="E99"/>
     </row>
     <row r="100">
-      <c s="9" r="A100"/>
+      <c t="s" s="9" r="A100">
+        <v>367</v>
+      </c>
       <c t="s" s="7" r="B100">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c t="s" s="7" r="C100">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c t="s" s="7" r="D100">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c t="s" s="7" r="E100">
-        <v>369</v>
+        <v>371</v>
       </c>
     </row>
     <row r="101">
       <c s="9" r="A101"/>
       <c t="s" s="7" r="B101">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c t="s" s="7" r="C101">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c t="s" s="7" r="D101">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c t="s" s="7" r="E101">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
     <row r="102">
       <c s="9" r="A102"/>
       <c t="s" s="7" r="B102">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c t="s" s="7" r="C102">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c t="s" s="7" r="D102">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c t="s" s="7" r="E102">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
     <row r="103">
       <c s="9" r="A103"/>
       <c t="s" s="7" r="B103">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c t="s" s="7" r="C103">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c t="s" s="7" r="D103">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c t="s" s="7" r="E103">
-        <v>381</v>
+        <v>383</v>
       </c>
     </row>
     <row r="104">
       <c s="9" r="A104"/>
       <c t="s" s="7" r="B104">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c t="s" s="7" r="C104">
-        <v>202</v>
+        <v>385</v>
       </c>
       <c t="s" s="7" r="D104">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c t="s" s="7" r="E104">
-        <v>202</v>
+        <v>387</v>
       </c>
     </row>
     <row r="105">
       <c s="9" r="A105"/>
       <c t="s" s="7" r="B105">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c t="s" s="7" r="C105">
-        <v>385</v>
+        <v>202</v>
       </c>
       <c t="s" s="7" r="D105">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c t="s" s="7" r="E105">
-        <v>387</v>
+        <v>202</v>
       </c>
     </row>
     <row r="106">
       <c s="9" r="A106"/>
       <c t="s" s="7" r="B106">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c t="s" s="7" r="C106">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c t="s" s="7" r="D106">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c t="s" s="7" r="E106">
-        <v>391</v>
+        <v>393</v>
       </c>
     </row>
     <row r="107">
       <c s="9" r="A107"/>
       <c t="s" s="7" r="B107">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c t="s" s="7" r="C107">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c t="s" s="7" r="D107">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c t="s" s="7" r="E107">
-        <v>395</v>
+        <v>397</v>
       </c>
     </row>
     <row r="108">
       <c s="9" r="A108"/>
       <c t="s" s="7" r="B108">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c t="s" s="7" r="C108">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c t="s" s="7" r="D108">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c t="s" s="7" r="E108">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="109">
       <c s="9" r="A109"/>
       <c t="s" s="7" r="B109">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c t="s" s="7" r="C109">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c t="s" s="7" r="D109">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c t="s" s="7" r="E109">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
     <row r="110">
       <c s="9" r="A110"/>
       <c t="s" s="7" r="B110">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c t="s" s="7" r="C110">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c t="s" s="7" r="D110">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c t="s" s="7" r="E110">
-        <v>406</v>
+        <v>409</v>
       </c>
     </row>
     <row r="111">
       <c s="9" r="A111"/>
       <c t="s" s="7" r="B111">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c t="s" s="7" r="C111">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c t="s" s="7" r="D111">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c t="s" s="7" r="E111">
-        <v>409</v>
+        <v>412</v>
       </c>
     </row>
     <row r="112">
       <c s="9" r="A112"/>
       <c t="s" s="7" r="B112">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c t="s" s="7" r="C112">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c t="s" s="7" r="D112">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c t="s" s="7" r="E112">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
     <row r="113">
       <c s="9" r="A113"/>
-      <c t="s" s="13" r="B113">
-        <v>414</v>
+      <c t="s" s="7" r="B113">
+        <v>416</v>
       </c>
       <c t="s" s="7" r="C113">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c t="s" s="7" r="D113">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c t="s" s="7" r="E113">
-        <v>416</v>
+        <v>419</v>
       </c>
     </row>
     <row r="114">
       <c s="9" r="A114"/>
-      <c t="s" s="7" r="B114">
-        <v>417</v>
+      <c t="s" s="13" r="B114">
+        <v>420</v>
       </c>
       <c t="s" s="7" r="C114">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c t="s" s="7" r="D114">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c t="s" s="7" r="E114">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="115">
       <c s="9" r="A115"/>
       <c t="s" s="7" r="B115">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c t="s" s="7" r="C115">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c t="s" s="7" r="D115">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c t="s" s="7" r="E115">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
     <row r="116">
       <c s="9" r="A116"/>
       <c t="s" s="7" r="B116">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c t="s" s="7" r="C116">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c t="s" s="7" r="D116">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c t="s" s="7" r="E116">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="117">
       <c s="9" r="A117"/>
       <c t="s" s="7" r="B117">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c t="s" s="7" r="C117">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c t="s" s="7" r="D117">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c t="s" s="7" r="E117">
-        <v>432</v>
+        <v>434</v>
       </c>
     </row>
     <row r="118">
       <c s="9" r="A118"/>
       <c t="s" s="7" r="B118">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c t="s" s="7" r="C118">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c t="s" s="7" r="D118">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c t="s" s="7" r="E118">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
     <row r="119">
       <c s="9" r="A119"/>
       <c t="s" s="7" r="B119">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c t="s" s="7" r="C119">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c t="s" s="7" r="D119">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c t="s" s="7" r="E119">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="120">
       <c s="9" r="A120"/>
       <c t="s" s="7" r="B120">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c t="s" s="7" r="C120">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c t="s" s="7" r="D120">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c t="s" s="7" r="E120">
-        <v>444</v>
+        <v>446</v>
       </c>
     </row>
     <row r="121">
       <c s="9" r="A121"/>
       <c t="s" s="7" r="B121">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c t="s" s="7" r="C121">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c t="s" s="7" r="D121">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c t="s" s="7" r="E121">
-        <v>448</v>
+        <v>450</v>
       </c>
     </row>
     <row r="122">
       <c s="9" r="A122"/>
       <c t="s" s="7" r="B122">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c t="s" s="7" r="C122">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c t="s" s="7" r="D122">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c t="s" s="7" r="E122">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="123">
       <c s="9" r="A123"/>
       <c t="s" s="7" r="B123">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c t="s" s="7" r="C123">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c t="s" s="7" r="D123">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c t="s" s="7" r="E123">
-        <v>456</v>
+        <v>458</v>
       </c>
     </row>
     <row r="124">
       <c s="9" r="A124"/>
       <c t="s" s="7" r="B124">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c t="s" s="7" r="C124">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c t="s" s="7" r="D124">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c t="s" s="7" r="E124">
-        <v>460</v>
+        <v>462</v>
       </c>
     </row>
     <row r="125">
       <c s="9" r="A125"/>
       <c t="s" s="7" r="B125">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c t="s" s="7" r="C125">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c t="s" s="7" r="D125">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c t="s" s="7" r="E125">
-        <v>464</v>
+        <v>466</v>
       </c>
     </row>
     <row r="126">
       <c s="9" r="A126"/>
       <c t="s" s="7" r="B126">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c t="s" s="7" r="C126">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c t="s" s="7" r="D126">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c t="s" s="7" r="E126">
-        <v>468</v>
+        <v>470</v>
       </c>
     </row>
     <row r="127">
       <c s="9" r="A127"/>
       <c t="s" s="7" r="B127">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c t="s" s="7" r="C127">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c t="s" s="7" r="D127">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c t="s" s="7" r="E127">
-        <v>472</v>
+        <v>474</v>
       </c>
     </row>
     <row r="128">
       <c s="9" r="A128"/>
       <c t="s" s="7" r="B128">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c t="s" s="7" r="C128">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c t="s" s="7" r="D128">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c t="s" s="7" r="E128">
-        <v>476</v>
+        <v>478</v>
       </c>
     </row>
     <row r="129">
       <c s="9" r="A129"/>
       <c t="s" s="7" r="B129">
-        <v>477</v>
-      </c>
-      <c t="s" s="13" r="C129">
-        <v>478</v>
+        <v>479</v>
+      </c>
+      <c t="s" s="7" r="C129">
+        <v>480</v>
       </c>
       <c t="s" s="7" r="D129">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c t="s" s="7" r="E129">
-        <v>480</v>
+        <v>482</v>
       </c>
     </row>
     <row r="130">
       <c s="9" r="A130"/>
-      <c t="s" s="13" r="B130">
-        <v>481</v>
+      <c t="s" s="7" r="B130">
+        <v>483</v>
       </c>
       <c t="s" s="13" r="C130">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c t="s" s="7" r="D130">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c t="s" s="7" r="E130">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="131">
       <c s="9" r="A131"/>
-      <c t="s" s="7" r="B131">
-        <v>485</v>
+      <c t="s" s="13" r="B131">
+        <v>487</v>
       </c>
       <c t="s" s="13" r="C131">
-        <v>482</v>
+        <v>488</v>
       </c>
       <c t="s" s="7" r="D131">
-        <v>483</v>
+        <v>489</v>
       </c>
       <c t="s" s="7" r="E131">
-        <v>484</v>
+        <v>490</v>
       </c>
     </row>
     <row r="132">
       <c s="9" r="A132"/>
       <c t="s" s="7" r="B132">
-        <v>486</v>
-      </c>
-      <c t="s" s="3" r="C132">
-        <v>487</v>
+        <v>491</v>
+      </c>
+      <c t="s" s="13" r="C132">
+        <v>488</v>
       </c>
       <c t="s" s="7" r="D132">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c t="s" s="7" r="E132">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="133">
       <c s="9" r="A133"/>
       <c t="s" s="7" r="B133">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c t="s" s="3" r="C133">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c t="s" s="7" r="D133">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c t="s" s="7" r="E133">
-        <v>493</v>
+        <v>495</v>
       </c>
     </row>
     <row r="134">
       <c s="9" r="A134"/>
       <c t="s" s="7" r="B134">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c t="s" s="3" r="C134">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c t="s" s="7" r="D134">
-        <v>496</v>
-      </c>
-      <c t="s" s="3" r="E134">
-        <v>497</v>
+        <v>498</v>
+      </c>
+      <c t="s" s="7" r="E134">
+        <v>499</v>
       </c>
     </row>
     <row r="135">
       <c s="9" r="A135"/>
-      <c s="16" r="B135"/>
-      <c s="8" r="C135"/>
-      <c s="16" r="D135"/>
-      <c s="16" r="E135"/>
+      <c t="s" s="7" r="B135">
+        <v>500</v>
+      </c>
+      <c t="s" s="3" r="C135">
+        <v>501</v>
+      </c>
+      <c t="s" s="7" r="D135">
+        <v>502</v>
+      </c>
+      <c t="s" s="3" r="E135">
+        <v>503</v>
+      </c>
     </row>
     <row r="136">
-      <c t="s" s="9" r="A136">
-        <v>498</v>
-      </c>
-      <c t="s" s="7" r="B136">
-        <v>499</v>
-      </c>
-      <c t="s" s="13" r="C136">
-        <v>500</v>
-      </c>
-      <c t="s" s="7" r="D136">
-        <v>501</v>
-      </c>
-      <c t="s" s="7" r="E136">
-        <v>502</v>
-      </c>
+      <c s="9" r="A136"/>
+      <c s="16" r="B136"/>
+      <c s="8" r="C136"/>
+      <c s="16" r="D136"/>
+      <c s="16" r="E136"/>
     </row>
     <row r="137">
-      <c s="9" r="A137"/>
-      <c t="s" s="21" r="B137">
-        <v>503</v>
+      <c t="s" s="9" r="A137">
+        <v>504</v>
+      </c>
+      <c t="s" s="7" r="B137">
+        <v>505</v>
       </c>
       <c t="s" s="13" r="C137">
-        <v>504</v>
-      </c>
-      <c t="s" s="21" r="D137">
-        <v>505</v>
-      </c>
-      <c t="s" s="21" r="E137">
         <v>506</v>
+      </c>
+      <c t="s" s="7" r="D137">
+        <v>507</v>
+      </c>
+      <c t="s" s="7" r="E137">
+        <v>508</v>
       </c>
     </row>
     <row r="138">
       <c s="9" r="A138"/>
-      <c t="s" s="7" r="B138">
-        <v>507</v>
+      <c t="s" s="21" r="B138">
+        <v>509</v>
       </c>
       <c t="s" s="13" r="C138">
-        <v>508</v>
-      </c>
-      <c t="s" s="7" r="D138">
-        <v>509</v>
-      </c>
-      <c t="s" s="7" r="E138">
         <v>510</v>
+      </c>
+      <c t="s" s="21" r="D138">
+        <v>511</v>
+      </c>
+      <c t="s" s="21" r="E138">
+        <v>512</v>
       </c>
     </row>
     <row r="139">
       <c s="9" r="A139"/>
       <c t="s" s="7" r="B139">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c t="s" s="13" r="C139">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c t="s" s="7" r="D139">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c t="s" s="7" r="E139">
-        <v>514</v>
+        <v>516</v>
       </c>
     </row>
     <row r="140">
-      <c s="17" r="A140"/>
+      <c s="9" r="A140"/>
       <c t="s" s="7" r="B140">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c t="s" s="13" r="C140">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c t="s" s="7" r="D140">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c t="s" s="7" r="E140">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="141">
-      <c s="9" r="A141"/>
+      <c s="17" r="A141"/>
       <c t="s" s="7" r="B141">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c t="s" s="13" r="C141">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c t="s" s="7" r="D141">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c t="s" s="7" r="E141">
-        <v>522</v>
+        <v>524</v>
       </c>
     </row>
     <row r="142">
       <c s="9" r="A142"/>
       <c t="s" s="7" r="B142">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c t="s" s="13" r="C142">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c t="s" s="7" r="D142">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c t="s" s="7" r="E142">
-        <v>526</v>
+        <v>528</v>
       </c>
     </row>
     <row r="143">
       <c s="9" r="A143"/>
       <c t="s" s="7" r="B143">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c t="s" s="13" r="C143">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c t="s" s="7" r="D143">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c t="s" s="7" r="E143">
-        <v>530</v>
+        <v>532</v>
       </c>
     </row>
     <row r="144">
       <c s="9" r="A144"/>
       <c t="s" s="7" r="B144">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c t="s" s="13" r="C144">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c t="s" s="7" r="D144">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c t="s" s="7" r="E144">
-        <v>534</v>
+        <v>536</v>
       </c>
     </row>
     <row r="145">
       <c s="9" r="A145"/>
       <c t="s" s="7" r="B145">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c t="s" s="13" r="C145">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c t="s" s="7" r="D145">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c t="s" s="7" r="E145">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="146">
       <c s="9" r="A146"/>
       <c t="s" s="7" r="B146">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c t="s" s="13" r="C146">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c t="s" s="7" r="D146">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c t="s" s="7" r="E146">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="147">
       <c s="9" r="A147"/>
       <c t="s" s="7" r="B147">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c t="s" s="13" r="C147">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c t="s" s="7" r="D147">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c t="s" s="7" r="E147">
-        <v>546</v>
+        <v>548</v>
       </c>
     </row>
     <row r="148">
       <c s="9" r="A148"/>
-      <c s="19" r="B148"/>
-      <c s="27" r="C148"/>
-      <c s="19" r="D148"/>
-      <c s="19" r="E148"/>
+      <c t="s" s="7" r="B148">
+        <v>549</v>
+      </c>
+      <c t="s" s="13" r="C148">
+        <v>550</v>
+      </c>
+      <c t="s" s="7" r="D148">
+        <v>551</v>
+      </c>
+      <c t="s" s="7" r="E148">
+        <v>552</v>
+      </c>
     </row>
     <row r="149">
-      <c t="s" s="9" r="A149">
-        <v>547</v>
-      </c>
-      <c t="s" s="7" r="B149">
-        <v>548</v>
-      </c>
-      <c t="s" s="13" r="C149">
-        <v>549</v>
-      </c>
-      <c t="s" s="7" r="D149">
-        <v>550</v>
-      </c>
-      <c t="s" s="7" r="E149">
-        <v>551</v>
-      </c>
+      <c s="9" r="A149"/>
+      <c s="19" r="B149"/>
+      <c s="27" r="C149"/>
+      <c s="19" r="D149"/>
+      <c s="19" r="E149"/>
     </row>
     <row r="150">
-      <c s="9" r="A150"/>
+      <c t="s" s="9" r="A150">
+        <v>553</v>
+      </c>
       <c t="s" s="7" r="B150">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c t="s" s="13" r="C150">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c t="s" s="7" r="D150">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c t="s" s="7" r="E150">
-        <v>555</v>
+        <v>557</v>
       </c>
     </row>
     <row r="151">
       <c s="9" r="A151"/>
       <c t="s" s="7" r="B151">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c t="s" s="13" r="C151">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c t="s" s="7" r="D151">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c t="s" s="7" r="E151">
-        <v>559</v>
+        <v>561</v>
       </c>
     </row>
     <row r="152">
       <c s="9" r="A152"/>
       <c t="s" s="7" r="B152">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c t="s" s="13" r="C152">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c t="s" s="7" r="D152">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c t="s" s="7" r="E152">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="153">
       <c s="9" r="A153"/>
       <c t="s" s="7" r="B153">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c t="s" s="13" r="C153">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c t="s" s="7" r="D153">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c t="s" s="7" r="E153">
-        <v>567</v>
+        <v>569</v>
       </c>
     </row>
     <row r="154">
       <c s="9" r="A154"/>
       <c t="s" s="7" r="B154">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c t="s" s="13" r="C154">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c t="s" s="7" r="D154">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c t="s" s="7" r="E154">
-        <v>571</v>
+        <v>573</v>
       </c>
     </row>
     <row r="155">
       <c s="9" r="A155"/>
       <c t="s" s="7" r="B155">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c t="s" s="13" r="C155">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c t="s" s="7" r="D155">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c t="s" s="7" r="E155">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="156">
       <c s="9" r="A156"/>
-      <c s="19" r="B156"/>
-      <c s="27" r="C156"/>
-      <c s="19" r="D156"/>
-      <c s="19" r="E156"/>
+      <c t="s" s="7" r="B156">
+        <v>578</v>
+      </c>
+      <c t="s" s="13" r="C156">
+        <v>579</v>
+      </c>
+      <c t="s" s="7" r="D156">
+        <v>580</v>
+      </c>
+      <c t="s" s="7" r="E156">
+        <v>581</v>
+      </c>
     </row>
     <row r="157">
-      <c t="s" s="9" r="A157">
-        <v>576</v>
-      </c>
-      <c t="s" s="26" r="B157">
-        <v>577</v>
-      </c>
-      <c t="s" s="20" r="C157">
-        <v>576</v>
-      </c>
-      <c s="26" r="D157"/>
-      <c s="26" r="E157"/>
+      <c s="9" r="A157"/>
+      <c s="19" r="B157"/>
+      <c s="27" r="C157"/>
+      <c s="19" r="D157"/>
+      <c s="19" r="E157"/>
     </row>
     <row r="158">
-      <c s="9" r="A158"/>
-      <c s="16" r="B158"/>
-      <c s="8" r="C158"/>
-      <c s="16" r="D158"/>
-      <c s="16" r="E158"/>
+      <c t="s" s="9" r="A158">
+        <v>582</v>
+      </c>
+      <c t="s" s="26" r="B158">
+        <v>583</v>
+      </c>
+      <c t="s" s="20" r="C158">
+        <v>582</v>
+      </c>
+      <c s="26" r="D158"/>
+      <c s="26" r="E158"/>
     </row>
     <row r="159">
-      <c t="s" s="9" r="A159">
-        <v>578</v>
-      </c>
-      <c t="s" s="31" r="B159">
-        <v>579</v>
-      </c>
-      <c t="s" s="29" r="C159">
-        <v>580</v>
-      </c>
-      <c s="31" r="D159"/>
-      <c s="31" r="E159"/>
+      <c s="9" r="A159"/>
+      <c s="16" r="B159"/>
+      <c s="8" r="C159"/>
+      <c s="16" r="D159"/>
+      <c s="16" r="E159"/>
     </row>
     <row r="160">
-      <c s="9" r="A160"/>
+      <c t="s" s="9" r="A160">
+        <v>584</v>
+      </c>
       <c t="s" s="31" r="B160">
-        <v>581</v>
+        <v>585</v>
       </c>
       <c t="s" s="29" r="C160">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c s="31" r="D160"/>
       <c s="31" r="E160"/>
     </row>
     <row r="161">
       <c s="9" r="A161"/>
-      <c s="8" r="B161"/>
-      <c s="8" r="C161"/>
-      <c s="16" r="D161"/>
-      <c s="16" r="E161"/>
+      <c t="s" s="31" r="B161">
+        <v>587</v>
+      </c>
+      <c t="s" s="29" r="C161">
+        <v>588</v>
+      </c>
+      <c s="31" r="D161"/>
+      <c s="31" r="E161"/>
     </row>
     <row r="162">
-      <c t="s" s="9" r="A162">
-        <v>583</v>
-      </c>
-      <c t="s" s="24" r="B162">
-        <v>584</v>
-      </c>
-      <c t="s" s="24" r="C162">
-        <v>585</v>
-      </c>
-      <c t="s" s="7" r="D162">
-        <v>586</v>
-      </c>
-      <c t="s" s="7" r="E162">
-        <v>587</v>
-      </c>
+      <c s="9" r="A162"/>
+      <c s="8" r="B162"/>
+      <c s="8" r="C162"/>
+      <c s="16" r="D162"/>
+      <c s="16" r="E162"/>
     </row>
     <row r="163">
-      <c s="9" r="A163"/>
+      <c t="s" s="9" r="A163">
+        <v>589</v>
+      </c>
       <c t="s" s="24" r="B163">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c t="s" s="24" r="C163">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c t="s" s="7" r="D163">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c t="s" s="7" r="E163">
-        <v>590</v>
+        <v>593</v>
       </c>
     </row>
     <row r="164">
       <c s="9" r="A164"/>
       <c t="s" s="24" r="B164">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c t="s" s="24" r="C164">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c t="s" s="7" r="D164">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c t="s" s="7" r="E164">
-        <v>594</v>
+        <v>596</v>
       </c>
     </row>
     <row r="165">
       <c s="9" r="A165"/>
       <c t="s" s="24" r="B165">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c t="s" s="24" r="C165">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c t="s" s="7" r="D165">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c t="s" s="7" r="E165">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row r="166">
       <c s="9" r="A166"/>
-      <c t="s" s="13" r="B166">
-        <v>599</v>
-      </c>
-      <c t="s" s="13" r="C166">
-        <v>600</v>
+      <c t="s" s="24" r="B166">
+        <v>601</v>
+      </c>
+      <c t="s" s="24" r="C166">
+        <v>602</v>
       </c>
       <c t="s" s="7" r="D166">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c t="s" s="7" r="E166">
-        <v>602</v>
+        <v>604</v>
       </c>
     </row>
     <row r="167">
       <c s="9" r="A167"/>
       <c t="s" s="13" r="B167">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c t="s" s="13" r="C167">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c t="s" s="7" r="D167">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c t="s" s="7" r="E167">
-        <v>606</v>
+        <v>608</v>
       </c>
     </row>
     <row r="168">
       <c s="9" r="A168"/>
       <c t="s" s="13" r="B168">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c t="s" s="13" r="C168">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c t="s" s="7" r="D168">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c t="s" s="7" r="E168">
-        <v>610</v>
+        <v>612</v>
       </c>
     </row>
     <row r="169">
       <c s="9" r="A169"/>
       <c t="s" s="13" r="B169">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c t="s" s="13" r="C169">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c t="s" s="7" r="D169">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c t="s" s="7" r="E169">
-        <v>614</v>
+        <v>616</v>
       </c>
     </row>
     <row r="170">
       <c s="9" r="A170"/>
       <c t="s" s="13" r="B170">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c t="s" s="13" r="C170">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c t="s" s="7" r="D170">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c t="s" s="7" r="E170">
-        <v>618</v>
+        <v>620</v>
       </c>
     </row>
     <row r="171">
       <c s="9" r="A171"/>
       <c t="s" s="13" r="B171">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c t="s" s="13" r="C171">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c t="s" s="7" r="D171">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c t="s" s="7" r="E171">
-        <v>622</v>
+        <v>624</v>
       </c>
     </row>
     <row r="172">
       <c s="9" r="A172"/>
       <c t="s" s="13" r="B172">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c t="s" s="13" r="C172">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c t="s" s="7" r="D172">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c t="s" s="7" r="E172">
-        <v>626</v>
+        <v>628</v>
       </c>
     </row>
     <row r="173">
       <c s="9" r="A173"/>
-      <c t="s" s="7" r="B173">
-        <v>627</v>
+      <c t="s" s="13" r="B173">
+        <v>629</v>
       </c>
       <c t="s" s="13" r="C173">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c t="s" s="7" r="D173">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c t="s" s="7" r="E173">
-        <v>630</v>
+        <v>632</v>
       </c>
     </row>
     <row r="174">
       <c s="9" r="A174"/>
-      <c t="s" s="18" r="B174">
-        <v>631</v>
-      </c>
-      <c t="s" s="32" r="C174">
-        <v>632</v>
-      </c>
-      <c t="s" s="18" r="D174">
+      <c t="s" s="7" r="B174">
         <v>633</v>
       </c>
-      <c t="s" s="18" r="E174">
+      <c t="s" s="13" r="C174">
         <v>634</v>
+      </c>
+      <c t="s" s="7" r="D174">
+        <v>635</v>
+      </c>
+      <c t="s" s="7" r="E174">
+        <v>636</v>
       </c>
     </row>
     <row r="175">
       <c s="9" r="A175"/>
       <c t="s" s="18" r="B175">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c t="s" s="32" r="C175">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c t="s" s="18" r="D175">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c t="s" s="18" r="E175">
-        <v>638</v>
+        <v>640</v>
       </c>
     </row>
     <row r="176">
       <c s="9" r="A176"/>
       <c t="s" s="18" r="B176">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c t="s" s="32" r="C176">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c t="s" s="18" r="D176">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c t="s" s="18" r="E176">
-        <v>642</v>
+        <v>644</v>
       </c>
     </row>
     <row r="177">
       <c s="9" r="A177"/>
-      <c t="s" s="7" r="B177">
-        <v>643</v>
-      </c>
-      <c t="s" s="13" r="C177">
-        <v>644</v>
-      </c>
-      <c t="s" s="7" r="D177">
+      <c t="s" s="18" r="B177">
         <v>645</v>
       </c>
-      <c t="s" s="7" r="E177">
+      <c t="s" s="32" r="C177">
         <v>646</v>
+      </c>
+      <c t="s" s="18" r="D177">
+        <v>647</v>
+      </c>
+      <c t="s" s="18" r="E177">
+        <v>648</v>
       </c>
     </row>
     <row r="178">
       <c s="9" r="A178"/>
       <c t="s" s="7" r="B178">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c t="s" s="13" r="C178">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c t="s" s="7" r="D178">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c t="s" s="7" r="E178">
-        <v>650</v>
+        <v>652</v>
       </c>
     </row>
     <row r="179">
       <c s="9" r="A179"/>
       <c t="s" s="7" r="B179">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c t="s" s="13" r="C179">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c t="s" s="7" r="D179">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c t="s" s="7" r="E179">
-        <v>654</v>
+        <v>656</v>
       </c>
     </row>
     <row r="180">
       <c s="9" r="A180"/>
       <c t="s" s="7" r="B180">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c t="s" s="13" r="C180">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c t="s" s="7" r="D180">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c t="s" s="7" r="E180">
-        <v>658</v>
+        <v>660</v>
       </c>
     </row>
     <row r="181">
       <c s="9" r="A181"/>
       <c t="s" s="7" r="B181">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c t="s" s="13" r="C181">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c t="s" s="7" r="D181">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c t="s" s="7" r="E181">
-        <v>662</v>
+        <v>664</v>
       </c>
     </row>
     <row r="182">
       <c s="9" r="A182"/>
-      <c s="11" r="B182"/>
-      <c s="14" r="C182"/>
-      <c s="11" r="D182"/>
-      <c s="11" r="E182"/>
+      <c t="s" s="7" r="B182">
+        <v>665</v>
+      </c>
+      <c t="s" s="13" r="C182">
+        <v>666</v>
+      </c>
+      <c t="s" s="7" r="D182">
+        <v>667</v>
+      </c>
+      <c t="s" s="7" r="E182">
+        <v>668</v>
+      </c>
     </row>
     <row r="183">
       <c s="9" r="A183"/>
-      <c s="16" r="B183"/>
-      <c s="27" r="C183"/>
-      <c s="16" r="D183"/>
-      <c s="16" r="E183"/>
+      <c s="11" r="B183"/>
+      <c s="14" r="C183"/>
+      <c s="11" r="D183"/>
+      <c s="11" r="E183"/>
     </row>
     <row r="184">
-      <c t="s" s="9" r="A184">
-        <v>663</v>
-      </c>
-      <c t="s" s="24" r="B184">
-        <v>664</v>
-      </c>
-      <c t="s" s="7" r="C184">
-        <v>589</v>
-      </c>
-      <c t="s" s="7" r="D184">
-        <v>589</v>
-      </c>
-      <c t="s" s="7" r="E184">
-        <v>590</v>
-      </c>
+      <c s="9" r="A184"/>
+      <c s="16" r="B184"/>
+      <c s="27" r="C184"/>
+      <c s="16" r="D184"/>
+      <c s="16" r="E184"/>
     </row>
     <row r="185">
-      <c s="9" r="A185"/>
-      <c t="s" s="7" r="B185">
-        <v>665</v>
-      </c>
-      <c t="s" s="13" r="C185">
-        <v>592</v>
+      <c t="s" s="9" r="A185">
+        <v>669</v>
+      </c>
+      <c t="s" s="24" r="B185">
+        <v>670</v>
+      </c>
+      <c t="s" s="7" r="C185">
+        <v>595</v>
       </c>
       <c t="s" s="7" r="D185">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c t="s" s="7" r="E185">
-        <v>594</v>
+        <v>596</v>
       </c>
     </row>
     <row r="186">
+      <c s="9" r="A186"/>
       <c t="s" s="7" r="B186">
-        <v>666</v>
+        <v>671</v>
       </c>
       <c t="s" s="13" r="C186">
-        <v>667</v>
+        <v>598</v>
       </c>
       <c t="s" s="7" r="D186">
-        <v>668</v>
+        <v>599</v>
       </c>
       <c t="s" s="7" r="E186">
-        <v>669</v>
+        <v>600</v>
       </c>
     </row>
     <row r="187">
-      <c s="9" r="A187"/>
       <c t="s" s="7" r="B187">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c t="s" s="13" r="C187">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c t="s" s="7" r="D187">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c t="s" s="7" r="E187">
-        <v>673</v>
+        <v>675</v>
       </c>
     </row>
     <row r="188">
       <c s="9" r="A188"/>
       <c t="s" s="7" r="B188">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c t="s" s="13" r="C188">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c t="s" s="7" r="D188">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c t="s" s="7" r="E188">
-        <v>677</v>
+        <v>679</v>
       </c>
     </row>
     <row r="189">
       <c s="9" r="A189"/>
-      <c s="11" r="B189"/>
-      <c s="14" r="C189"/>
-      <c s="16" r="D189"/>
-      <c s="16" r="E189"/>
+      <c t="s" s="7" r="B189">
+        <v>680</v>
+      </c>
+      <c t="s" s="13" r="C189">
+        <v>681</v>
+      </c>
+      <c t="s" s="7" r="D189">
+        <v>682</v>
+      </c>
+      <c t="s" s="7" r="E189">
+        <v>683</v>
+      </c>
     </row>
     <row r="190">
-      <c t="s" s="9" r="A190">
-        <v>678</v>
-      </c>
-      <c t="s" s="7" r="B190">
-        <v>679</v>
-      </c>
-      <c t="s" s="13" r="C190">
-        <v>678</v>
-      </c>
-      <c t="s" s="7" r="D190">
-        <v>680</v>
-      </c>
-      <c t="s" s="7" r="E190">
-        <v>681</v>
-      </c>
+      <c s="9" r="A190"/>
+      <c s="11" r="B190"/>
+      <c s="14" r="C190"/>
+      <c s="16" r="D190"/>
+      <c s="16" r="E190"/>
     </row>
     <row r="191">
-      <c s="9" r="A191"/>
+      <c t="s" s="9" r="A191">
+        <v>684</v>
+      </c>
       <c t="s" s="7" r="B191">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c t="s" s="13" r="C191">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c t="s" s="7" r="D191">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c t="s" s="7" r="E191">
-        <v>685</v>
+        <v>687</v>
       </c>
     </row>
     <row r="192">
       <c s="9" r="A192"/>
       <c t="s" s="7" r="B192">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c t="s" s="13" r="C192">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c t="s" s="7" r="D192">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c t="s" s="7" r="E192">
-        <v>689</v>
+        <v>691</v>
       </c>
     </row>
     <row r="193">
       <c s="9" r="A193"/>
       <c t="s" s="7" r="B193">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c t="s" s="13" r="C193">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c t="s" s="7" r="D193">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c t="s" s="7" r="E193">
-        <v>693</v>
+        <v>695</v>
       </c>
     </row>
     <row r="194">
       <c s="9" r="A194"/>
       <c t="s" s="7" r="B194">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c t="s" s="13" r="C194">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c t="s" s="7" r="D194">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c t="s" s="7" r="E194">
-        <v>697</v>
+        <v>699</v>
       </c>
     </row>
     <row r="195">
       <c s="9" r="A195"/>
       <c t="s" s="7" r="B195">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c t="s" s="13" r="C195">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c t="s" s="7" r="D195">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c t="s" s="7" r="E195">
-        <v>701</v>
+        <v>703</v>
       </c>
     </row>
     <row r="196">
       <c s="9" r="A196"/>
       <c t="s" s="7" r="B196">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c t="s" s="13" r="C196">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c t="s" s="7" r="D196">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c t="s" s="7" r="E196">
-        <v>705</v>
+        <v>707</v>
       </c>
     </row>
     <row r="197">
       <c s="9" r="A197"/>
-      <c s="11" r="B197"/>
-      <c s="14" r="C197"/>
-      <c s="11" r="D197"/>
-      <c s="11" r="E197"/>
+      <c t="s" s="7" r="B197">
+        <v>708</v>
+      </c>
+      <c t="s" s="13" r="C197">
+        <v>709</v>
+      </c>
+      <c t="s" s="7" r="D197">
+        <v>710</v>
+      </c>
+      <c t="s" s="7" r="E197">
+        <v>711</v>
+      </c>
     </row>
     <row r="198">
-      <c t="s" s="9" r="A198">
-        <v>706</v>
-      </c>
-      <c t="s" s="7" r="B198">
-        <v>707</v>
-      </c>
-      <c t="s" s="13" r="C198">
-        <v>708</v>
-      </c>
-      <c t="s" s="7" r="D198">
-        <v>709</v>
-      </c>
-      <c t="s" s="7" r="E198">
-        <v>710</v>
-      </c>
+      <c s="9" r="A198"/>
+      <c s="11" r="B198"/>
+      <c s="14" r="C198"/>
+      <c s="11" r="D198"/>
+      <c s="11" r="E198"/>
     </row>
     <row r="199">
-      <c s="9" r="A199"/>
+      <c t="s" s="9" r="A199">
+        <v>712</v>
+      </c>
       <c t="s" s="7" r="B199">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c t="s" s="13" r="C199">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c t="s" s="7" r="D199">
-        <v>712</v>
+        <v>715</v>
       </c>
       <c t="s" s="7" r="E199">
-        <v>713</v>
+        <v>716</v>
       </c>
     </row>
     <row r="200">
       <c s="9" r="A200"/>
-      <c s="11" r="B200"/>
-      <c s="14" r="C200"/>
-      <c s="11" r="D200"/>
-      <c s="11" r="E200"/>
+      <c t="s" s="7" r="B200">
+        <v>717</v>
+      </c>
+      <c t="s" s="13" r="C200">
+        <v>718</v>
+      </c>
+      <c t="s" s="7" r="D200">
+        <v>718</v>
+      </c>
+      <c t="s" s="7" r="E200">
+        <v>719</v>
+      </c>
     </row>
     <row r="201">
-      <c t="s" s="9" r="A201">
-        <v>714</v>
-      </c>
-      <c t="s" s="7" r="B201">
-        <v>715</v>
-      </c>
-      <c t="s" s="13" r="C201">
-        <v>716</v>
-      </c>
-      <c t="s" s="7" r="D201">
-        <v>717</v>
-      </c>
-      <c t="s" s="7" r="E201">
-        <v>718</v>
-      </c>
+      <c s="9" r="A201"/>
+      <c s="11" r="B201"/>
+      <c s="14" r="C201"/>
+      <c s="11" r="D201"/>
+      <c s="11" r="E201"/>
     </row>
     <row r="202">
-      <c s="9" r="A202"/>
+      <c t="s" s="9" r="A202">
+        <v>720</v>
+      </c>
       <c t="s" s="7" r="B202">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c t="s" s="13" r="C202">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c t="s" s="7" r="D202">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c t="s" s="7" r="E202">
-        <v>722</v>
+        <v>724</v>
       </c>
     </row>
     <row r="203">
       <c s="9" r="A203"/>
       <c t="s" s="7" r="B203">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c t="s" s="13" r="C203">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c t="s" s="7" r="D203">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c t="s" s="7" r="E203">
-        <v>726</v>
+        <v>728</v>
       </c>
     </row>
     <row r="204">
       <c s="9" r="A204"/>
       <c t="s" s="7" r="B204">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c t="s" s="13" r="C204">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c t="s" s="7" r="D204">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c t="s" s="7" r="E204">
-        <v>730</v>
+        <v>732</v>
       </c>
     </row>
     <row r="205">
       <c s="9" r="A205"/>
-      <c s="16" r="B205"/>
-      <c s="27" r="C205"/>
-      <c s="16" r="D205"/>
-      <c s="16" r="E205"/>
+      <c t="s" s="7" r="B205">
+        <v>733</v>
+      </c>
+      <c t="s" s="13" r="C205">
+        <v>734</v>
+      </c>
+      <c t="s" s="7" r="D205">
+        <v>735</v>
+      </c>
+      <c t="s" s="7" r="E205">
+        <v>736</v>
+      </c>
     </row>
     <row r="206">
-      <c t="s" s="9" r="A206">
-        <v>731</v>
-      </c>
-      <c t="s" s="7" r="B206">
-        <v>732</v>
-      </c>
-      <c t="s" s="13" r="C206">
-        <v>733</v>
-      </c>
-      <c t="s" s="7" r="D206">
-        <v>734</v>
-      </c>
-      <c t="s" s="7" r="E206">
-        <v>735</v>
-      </c>
+      <c s="9" r="A206"/>
+      <c s="16" r="B206"/>
+      <c s="27" r="C206"/>
+      <c s="16" r="D206"/>
+      <c s="16" r="E206"/>
     </row>
     <row r="207">
-      <c s="9" r="A207"/>
+      <c t="s" s="9" r="A207">
+        <v>737</v>
+      </c>
       <c t="s" s="7" r="B207">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c t="s" s="13" r="C207">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c t="s" s="7" r="D207">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c t="s" s="7" r="E207">
-        <v>739</v>
+        <v>741</v>
       </c>
     </row>
     <row r="208">
       <c s="9" r="A208"/>
-      <c s="16" r="B208"/>
-      <c s="27" r="C208"/>
-      <c s="16" r="D208"/>
-      <c s="16" r="E208"/>
+      <c t="s" s="7" r="B208">
+        <v>742</v>
+      </c>
+      <c t="s" s="13" r="C208">
+        <v>743</v>
+      </c>
+      <c t="s" s="7" r="D208">
+        <v>744</v>
+      </c>
+      <c t="s" s="7" r="E208">
+        <v>745</v>
+      </c>
     </row>
     <row r="209">
-      <c t="s" s="9" r="A209">
-        <v>740</v>
-      </c>
-      <c t="s" s="7" r="B209">
-        <v>741</v>
-      </c>
-      <c t="s" s="13" r="C209">
-        <v>742</v>
-      </c>
-      <c t="s" s="7" r="D209">
-        <v>743</v>
-      </c>
-      <c t="s" s="7" r="E209">
-        <v>744</v>
-      </c>
+      <c s="9" r="A209"/>
+      <c s="16" r="B209"/>
+      <c s="27" r="C209"/>
+      <c s="16" r="D209"/>
+      <c s="16" r="E209"/>
     </row>
     <row r="210">
-      <c s="9" r="A210"/>
-      <c s="16" r="B210"/>
-      <c s="8" r="C210"/>
-      <c s="16" r="D210"/>
-      <c s="16" r="E210"/>
+      <c t="s" s="9" r="A210">
+        <v>746</v>
+      </c>
+      <c t="s" s="7" r="B210">
+        <v>747</v>
+      </c>
+      <c t="s" s="13" r="C210">
+        <v>748</v>
+      </c>
+      <c t="s" s="7" r="D210">
+        <v>749</v>
+      </c>
+      <c t="s" s="7" r="E210">
+        <v>750</v>
+      </c>
     </row>
     <row r="211">
-      <c t="s" s="9" r="A211">
-        <v>745</v>
-      </c>
-      <c t="s" s="7" r="B211">
-        <v>746</v>
-      </c>
-      <c t="s" s="13" r="C211">
-        <v>747</v>
-      </c>
-      <c t="s" s="7" r="D211">
-        <v>748</v>
-      </c>
-      <c t="s" s="7" r="E211">
-        <v>749</v>
-      </c>
+      <c s="9" r="A211"/>
+      <c s="16" r="B211"/>
+      <c s="8" r="C211"/>
+      <c s="16" r="D211"/>
+      <c s="16" r="E211"/>
     </row>
     <row r="212">
-      <c s="9" r="A212"/>
+      <c t="s" s="9" r="A212">
+        <v>751</v>
+      </c>
       <c t="s" s="7" r="B212">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c t="s" s="13" r="C212">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c t="s" s="7" r="D212">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c t="s" s="7" r="E212">
-        <v>753</v>
+        <v>755</v>
       </c>
     </row>
     <row r="213">
       <c s="9" r="A213"/>
       <c t="s" s="7" r="B213">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c t="s" s="13" r="C213">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c t="s" s="7" r="D213">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c t="s" s="7" r="E213">
-        <v>757</v>
+        <v>759</v>
       </c>
     </row>
     <row r="214">
       <c s="9" r="A214"/>
       <c t="s" s="7" r="B214">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c t="s" s="13" r="C214">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c t="s" s="7" r="D214">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c t="s" s="7" r="E214">
-        <v>761</v>
+        <v>763</v>
       </c>
     </row>
     <row r="215">
       <c s="9" r="A215"/>
       <c t="s" s="7" r="B215">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c t="s" s="13" r="C215">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c t="s" s="7" r="D215">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c t="s" s="7" r="E215">
-        <v>765</v>
+        <v>767</v>
       </c>
     </row>
     <row r="216">
       <c s="9" r="A216"/>
       <c t="s" s="7" r="B216">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c t="s" s="13" r="C216">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c t="s" s="7" r="D216">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c t="s" s="7" r="E216">
-        <v>769</v>
+        <v>771</v>
       </c>
     </row>
     <row r="217">
       <c s="9" r="A217"/>
       <c t="s" s="7" r="B217">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c t="s" s="13" r="C217">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c t="s" s="7" r="D217">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c t="s" s="7" r="E217">
-        <v>773</v>
+        <v>775</v>
       </c>
     </row>
     <row r="218">
       <c s="9" r="A218"/>
       <c t="s" s="7" r="B218">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c t="s" s="13" r="C218">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c t="s" s="7" r="D218">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c t="s" s="7" r="E218">
-        <v>777</v>
+        <v>779</v>
       </c>
     </row>
     <row r="219">
-      <c s="17" r="A219"/>
-      <c s="16" r="B219"/>
-      <c s="8" r="C219"/>
-      <c s="16" r="D219"/>
-      <c s="16" r="E219"/>
+      <c s="9" r="A219"/>
+      <c t="s" s="7" r="B219">
+        <v>780</v>
+      </c>
+      <c t="s" s="13" r="C219">
+        <v>781</v>
+      </c>
+      <c t="s" s="7" r="D219">
+        <v>782</v>
+      </c>
+      <c t="s" s="7" r="E219">
+        <v>783</v>
+      </c>
     </row>
     <row r="220">
-      <c t="s" s="9" r="A220">
-        <v>778</v>
-      </c>
-      <c t="s" s="7" r="B220">
-        <v>779</v>
-      </c>
-      <c t="s" s="7" r="C220">
-        <v>780</v>
-      </c>
-      <c t="s" s="7" r="D220">
-        <v>781</v>
-      </c>
-      <c t="s" s="7" r="E220">
-        <v>782</v>
-      </c>
+      <c s="17" r="A220"/>
+      <c s="16" r="B220"/>
+      <c s="8" r="C220"/>
+      <c s="16" r="D220"/>
+      <c s="16" r="E220"/>
     </row>
     <row r="221">
-      <c s="9" r="A221"/>
+      <c t="s" s="9" r="A221">
+        <v>784</v>
+      </c>
       <c t="s" s="7" r="B221">
-        <v>783</v>
-      </c>
-      <c t="s" s="13" r="C221">
-        <v>784</v>
+        <v>785</v>
+      </c>
+      <c t="s" s="7" r="C221">
+        <v>786</v>
       </c>
       <c t="s" s="7" r="D221">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c t="s" s="7" r="E221">
-        <v>786</v>
+        <v>788</v>
       </c>
     </row>
     <row r="222">
       <c s="9" r="A222"/>
       <c t="s" s="7" r="B222">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c t="s" s="13" r="C222">
-        <v>788</v>
+        <v>790</v>
       </c>
       <c t="s" s="7" r="D222">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c t="s" s="7" r="E222">
-        <v>790</v>
+        <v>792</v>
       </c>
     </row>
     <row r="223">
       <c s="9" r="A223"/>
       <c t="s" s="7" r="B223">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c t="s" s="13" r="C223">
-        <v>792</v>
+        <v>794</v>
       </c>
       <c t="s" s="7" r="D223">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c t="s" s="7" r="E223">
-        <v>794</v>
+        <v>796</v>
       </c>
     </row>
     <row r="224">
       <c s="9" r="A224"/>
       <c t="s" s="7" r="B224">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c t="s" s="13" r="C224">
-        <v>516</v>
+        <v>798</v>
       </c>
       <c t="s" s="7" r="D224">
-        <v>112</v>
+        <v>799</v>
       </c>
       <c t="s" s="7" r="E224">
-        <v>518</v>
+        <v>800</v>
       </c>
     </row>
     <row r="225">
       <c s="9" r="A225"/>
       <c t="s" s="7" r="B225">
-        <v>796</v>
+        <v>801</v>
       </c>
       <c t="s" s="13" r="C225">
-        <v>797</v>
+        <v>522</v>
       </c>
       <c t="s" s="7" r="D225">
-        <v>798</v>
+        <v>112</v>
       </c>
       <c t="s" s="7" r="E225">
-        <v>799</v>
+        <v>524</v>
       </c>
     </row>
     <row r="226">
-      <c s="17" r="A226"/>
-      <c s="16" r="B226"/>
-      <c s="8" r="C226"/>
-      <c s="16" r="D226"/>
-      <c s="16" r="E226"/>
+      <c s="9" r="A226"/>
+      <c t="s" s="7" r="B226">
+        <v>802</v>
+      </c>
+      <c t="s" s="13" r="C226">
+        <v>803</v>
+      </c>
+      <c t="s" s="7" r="D226">
+        <v>804</v>
+      </c>
+      <c t="s" s="7" r="E226">
+        <v>805</v>
+      </c>
     </row>
     <row r="227">
-      <c t="s" s="9" r="A227">
-        <v>800</v>
-      </c>
-      <c t="s" s="7" r="B227">
-        <v>801</v>
-      </c>
-      <c t="s" s="13" r="C227">
-        <v>802</v>
-      </c>
-      <c t="s" s="7" r="D227">
-        <v>803</v>
-      </c>
-      <c t="s" s="7" r="E227">
-        <v>804</v>
-      </c>
+      <c s="17" r="A227"/>
+      <c s="16" r="B227"/>
+      <c s="8" r="C227"/>
+      <c s="16" r="D227"/>
+      <c s="16" r="E227"/>
     </row>
     <row r="228">
-      <c s="9" r="A228"/>
+      <c t="s" s="9" r="A228">
+        <v>806</v>
+      </c>
       <c t="s" s="7" r="B228">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c t="s" s="13" r="C228">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c t="s" s="7" r="D228">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c t="s" s="7" r="E228">
-        <v>808</v>
+        <v>810</v>
       </c>
     </row>
     <row r="229">
       <c s="9" r="A229"/>
       <c t="s" s="7" r="B229">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c t="s" s="13" r="C229">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c t="s" s="7" r="D229">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c t="s" s="7" r="E229">
-        <v>812</v>
+        <v>814</v>
       </c>
     </row>
     <row r="230">
       <c s="9" r="A230"/>
       <c t="s" s="7" r="B230">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c t="s" s="13" r="C230">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c t="s" s="7" r="D230">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c t="s" s="7" r="E230">
-        <v>815</v>
+        <v>818</v>
       </c>
     </row>
     <row r="231">
       <c s="9" r="A231"/>
       <c t="s" s="7" r="B231">
-        <v>816</v>
+        <v>819</v>
       </c>
       <c t="s" s="13" r="C231">
-        <v>817</v>
+        <v>820</v>
       </c>
       <c t="s" s="7" r="D231">
-        <v>818</v>
+        <v>821</v>
       </c>
       <c t="s" s="7" r="E231">
-        <v>819</v>
+        <v>821</v>
       </c>
     </row>
     <row r="232">
       <c s="9" r="A232"/>
       <c t="s" s="7" r="B232">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c t="s" s="13" r="C232">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c t="s" s="7" r="D232">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c t="s" s="7" r="E232">
-        <v>823</v>
+        <v>825</v>
       </c>
     </row>
     <row r="233">
       <c s="9" r="A233"/>
       <c t="s" s="7" r="B233">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c t="s" s="13" r="C233">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c t="s" s="7" r="D233">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c t="s" s="7" r="E233">
-        <v>827</v>
+        <v>829</v>
       </c>
     </row>
     <row r="234">
       <c s="9" r="A234"/>
       <c t="s" s="7" r="B234">
-        <v>828</v>
+        <v>830</v>
       </c>
       <c t="s" s="13" r="C234">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c t="s" s="7" r="D234">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c t="s" s="7" r="E234">
-        <v>831</v>
+        <v>833</v>
       </c>
     </row>
     <row r="235">
       <c s="9" r="A235"/>
       <c t="s" s="7" r="B235">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c t="s" s="13" r="C235">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c t="s" s="7" r="D235">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c t="s" s="7" r="E235">
-        <v>835</v>
+        <v>837</v>
       </c>
     </row>
     <row r="236">
       <c s="9" r="A236"/>
       <c t="s" s="7" r="B236">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c t="s" s="13" r="C236">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c t="s" s="7" r="D236">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c t="s" s="7" r="E236">
-        <v>839</v>
+        <v>841</v>
       </c>
     </row>
     <row r="237">
       <c s="9" r="A237"/>
       <c t="s" s="7" r="B237">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c t="s" s="13" r="C237">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c t="s" s="7" r="D237">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c t="s" s="7" r="E237">
-        <v>843</v>
+        <v>845</v>
       </c>
     </row>
     <row r="238">
       <c s="9" r="A238"/>
       <c t="s" s="7" r="B238">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c t="s" s="13" r="C238">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c t="s" s="7" r="D238">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c t="s" s="7" r="E238">
-        <v>847</v>
+        <v>849</v>
       </c>
     </row>
     <row r="239">
       <c s="9" r="A239"/>
       <c t="s" s="7" r="B239">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c t="s" s="13" r="C239">
-        <v>849</v>
+        <v>851</v>
       </c>
       <c t="s" s="7" r="D239">
-        <v>849</v>
+        <v>852</v>
       </c>
       <c t="s" s="7" r="E239">
-        <v>849</v>
+        <v>853</v>
       </c>
     </row>
     <row r="240">
       <c s="9" r="A240"/>
       <c t="s" s="7" r="B240">
-        <v>850</v>
+        <v>854</v>
       </c>
       <c t="s" s="13" r="C240">
-        <v>851</v>
+        <v>855</v>
       </c>
       <c t="s" s="7" r="D240">
-        <v>852</v>
+        <v>855</v>
       </c>
       <c t="s" s="7" r="E240">
-        <v>853</v>
+        <v>855</v>
       </c>
     </row>
     <row r="241">
       <c s="9" r="A241"/>
       <c t="s" s="7" r="B241">
-        <v>854</v>
+        <v>856</v>
       </c>
       <c t="s" s="13" r="C241">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c t="s" s="7" r="D241">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c t="s" s="7" r="E241">
-        <v>857</v>
+        <v>859</v>
       </c>
     </row>
     <row r="242">
       <c s="9" r="A242"/>
       <c t="s" s="7" r="B242">
-        <v>858</v>
+        <v>860</v>
       </c>
       <c t="s" s="13" r="C242">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c t="s" s="7" r="D242">
-        <v>860</v>
+        <v>862</v>
       </c>
       <c t="s" s="7" r="E242">
-        <v>861</v>
+        <v>863</v>
       </c>
     </row>
     <row r="243">
       <c s="9" r="A243"/>
       <c t="s" s="7" r="B243">
-        <v>862</v>
+        <v>864</v>
       </c>
       <c t="s" s="13" r="C243">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c t="s" s="7" r="D243">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c t="s" s="7" r="E243">
-        <v>865</v>
+        <v>867</v>
       </c>
     </row>
     <row r="244">
       <c s="9" r="A244"/>
       <c t="s" s="7" r="B244">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c t="s" s="13" r="C244">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c t="s" s="7" r="D244">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c t="s" s="7" r="E244">
-        <v>869</v>
+        <v>871</v>
       </c>
     </row>
     <row r="245">
       <c s="9" r="A245"/>
       <c t="s" s="7" r="B245">
-        <v>870</v>
+        <v>872</v>
       </c>
       <c t="s" s="13" r="C245">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c t="s" s="7" r="D245">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c t="s" s="7" r="E245">
-        <v>873</v>
+        <v>875</v>
       </c>
     </row>
     <row r="246">
       <c s="9" r="A246"/>
       <c t="s" s="7" r="B246">
-        <v>874</v>
+        <v>876</v>
       </c>
       <c t="s" s="13" r="C246">
-        <v>875</v>
+        <v>877</v>
       </c>
       <c t="s" s="7" r="D246">
-        <v>876</v>
+        <v>878</v>
       </c>
       <c t="s" s="7" r="E246">
-        <v>877</v>
+        <v>879</v>
       </c>
     </row>
     <row r="247">
       <c s="9" r="A247"/>
-      <c s="16" r="B247"/>
-      <c s="8" r="C247"/>
-      <c s="16" r="D247"/>
-      <c s="16" r="E247"/>
+      <c t="s" s="7" r="B247">
+        <v>880</v>
+      </c>
+      <c t="s" s="13" r="C247">
+        <v>881</v>
+      </c>
+      <c t="s" s="7" r="D247">
+        <v>882</v>
+      </c>
+      <c t="s" s="7" r="E247">
+        <v>883</v>
+      </c>
     </row>
     <row r="248">
-      <c t="s" s="9" r="A248">
-        <v>878</v>
-      </c>
-      <c t="s" s="7" r="B248">
-        <v>879</v>
-      </c>
-      <c t="s" s="13" r="C248">
-        <v>880</v>
-      </c>
-      <c t="s" s="7" r="D248">
-        <v>881</v>
-      </c>
-      <c t="s" s="7" r="E248">
-        <v>882</v>
-      </c>
+      <c s="9" r="A248"/>
+      <c s="16" r="B248"/>
+      <c s="8" r="C248"/>
+      <c s="16" r="D248"/>
+      <c s="16" r="E248"/>
     </row>
     <row r="249">
-      <c s="9" r="A249"/>
+      <c t="s" s="9" r="A249">
+        <v>884</v>
+      </c>
       <c t="s" s="7" r="B249">
-        <v>883</v>
+        <v>885</v>
       </c>
       <c t="s" s="13" r="C249">
-        <v>884</v>
+        <v>886</v>
       </c>
       <c t="s" s="7" r="D249">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c t="s" s="7" r="E249">
-        <v>886</v>
+        <v>888</v>
       </c>
     </row>
     <row r="250">
       <c s="9" r="A250"/>
       <c t="s" s="7" r="B250">
-        <v>887</v>
+        <v>889</v>
       </c>
       <c t="s" s="13" r="C250">
-        <v>888</v>
+        <v>890</v>
       </c>
       <c t="s" s="7" r="D250">
-        <v>889</v>
+        <v>891</v>
       </c>
       <c t="s" s="7" r="E250">
-        <v>890</v>
+        <v>892</v>
       </c>
     </row>
     <row r="251">
       <c s="9" r="A251"/>
       <c t="s" s="7" r="B251">
-        <v>891</v>
+        <v>893</v>
       </c>
       <c t="s" s="13" r="C251">
-        <v>892</v>
+        <v>894</v>
       </c>
       <c t="s" s="7" r="D251">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c t="s" s="7" r="E251">
-        <v>894</v>
+        <v>896</v>
       </c>
     </row>
     <row r="252">
       <c s="9" r="A252"/>
       <c t="s" s="7" r="B252">
-        <v>895</v>
+        <v>897</v>
       </c>
       <c t="s" s="13" r="C252">
-        <v>895</v>
-      </c>
-      <c t="s" s="18" r="D252">
-        <v>896</v>
-      </c>
-      <c t="s" s="18" r="E252">
-        <v>897</v>
+        <v>898</v>
+      </c>
+      <c t="s" s="7" r="D252">
+        <v>899</v>
+      </c>
+      <c t="s" s="7" r="E252">
+        <v>900</v>
       </c>
     </row>
     <row r="253">
       <c s="9" r="A253"/>
       <c t="s" s="7" r="B253">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c t="s" s="13" r="C253">
-        <v>899</v>
-      </c>
-      <c t="s" s="7" r="D253">
-        <v>900</v>
-      </c>
-      <c t="s" s="7" r="E253">
         <v>901</v>
+      </c>
+      <c t="s" s="18" r="D253">
+        <v>902</v>
+      </c>
+      <c t="s" s="18" r="E253">
+        <v>903</v>
       </c>
     </row>
     <row r="254">
       <c s="9" r="A254"/>
       <c t="s" s="7" r="B254">
-        <v>902</v>
+        <v>904</v>
       </c>
       <c t="s" s="13" r="C254">
-        <v>903</v>
+        <v>905</v>
       </c>
       <c t="s" s="7" r="D254">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c t="s" s="7" r="E254">
-        <v>905</v>
+        <v>907</v>
       </c>
     </row>
     <row r="255">
-      <c t="s" s="16" r="A255">
-        <v>906</v>
-      </c>
-      <c s="24" r="B255"/>
+      <c s="9" r="A255"/>
+      <c t="s" s="7" r="B255">
+        <v>908</v>
+      </c>
       <c t="s" s="13" r="C255">
-        <v>907</v>
-      </c>
-      <c t="s" s="18" r="D255">
-        <v>908</v>
-      </c>
-      <c t="s" s="18" r="E255">
         <v>909</v>
       </c>
+      <c t="s" s="7" r="D255">
+        <v>910</v>
+      </c>
+      <c t="s" s="7" r="E255">
+        <v>911</v>
+      </c>
     </row>
     <row r="256">
-      <c s="17" r="A256"/>
-      <c s="16" r="B256"/>
-      <c s="8" r="C256"/>
-      <c s="16" r="D256"/>
-      <c s="16" r="E256"/>
+      <c t="s" s="16" r="A256">
+        <v>912</v>
+      </c>
+      <c s="24" r="B256"/>
+      <c t="s" s="13" r="C256">
+        <v>913</v>
+      </c>
+      <c t="s" s="18" r="D256">
+        <v>914</v>
+      </c>
+      <c t="s" s="18" r="E256">
+        <v>915</v>
+      </c>
     </row>
     <row r="257">
-      <c t="s" s="17" r="A257">
-        <v>910</v>
-      </c>
-      <c t="s" s="7" r="B257">
-        <v>911</v>
-      </c>
-      <c t="s" s="7" r="C257">
-        <v>912</v>
-      </c>
-      <c t="s" s="7" r="D257">
-        <v>913</v>
-      </c>
-      <c t="s" s="7" r="E257">
-        <v>914</v>
-      </c>
+      <c s="17" r="A257"/>
+      <c s="16" r="B257"/>
+      <c s="8" r="C257"/>
+      <c s="16" r="D257"/>
+      <c s="16" r="E257"/>
     </row>
     <row r="258">
+      <c t="s" s="17" r="A258">
+        <v>916</v>
+      </c>
       <c t="s" s="7" r="B258">
-        <v>915</v>
-      </c>
-      <c t="s" s="13" r="C258">
-        <v>916</v>
+        <v>917</v>
+      </c>
+      <c t="s" s="7" r="C258">
+        <v>918</v>
       </c>
       <c t="s" s="7" r="D258">
-        <v>917</v>
+        <v>919</v>
       </c>
       <c t="s" s="7" r="E258">
-        <v>918</v>
+        <v>920</v>
       </c>
     </row>
     <row r="259">
+      <c s="14" r="A259"/>
       <c t="s" s="7" r="B259">
-        <v>919</v>
-      </c>
-      <c t="s" s="7" r="C259">
-        <v>920</v>
+        <v>921</v>
+      </c>
+      <c t="s" s="13" r="C259">
+        <v>922</v>
       </c>
       <c t="s" s="7" r="D259">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c t="s" s="7" r="E259">
-        <v>922</v>
+        <v>924</v>
       </c>
     </row>
     <row r="260">
-      <c s="17" r="A260"/>
+      <c s="14" r="A260"/>
       <c t="s" s="7" r="B260">
-        <v>923</v>
-      </c>
-      <c t="s" s="13" r="C260">
-        <v>924</v>
+        <v>925</v>
+      </c>
+      <c t="s" s="7" r="C260">
+        <v>926</v>
       </c>
       <c t="s" s="7" r="D260">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c t="s" s="7" r="E260">
-        <v>926</v>
+        <v>928</v>
       </c>
     </row>
     <row r="261">
       <c s="17" r="A261"/>
       <c t="s" s="7" r="B261">
-        <v>927</v>
-      </c>
-      <c t="s" s="7" r="C261">
-        <v>928</v>
+        <v>929</v>
+      </c>
+      <c t="s" s="13" r="C261">
+        <v>930</v>
       </c>
       <c t="s" s="7" r="D261">
-        <v>929</v>
+        <v>931</v>
       </c>
       <c t="s" s="7" r="E261">
-        <v>930</v>
+        <v>932</v>
       </c>
     </row>
     <row r="262">
       <c s="17" r="A262"/>
       <c t="s" s="7" r="B262">
-        <v>931</v>
-      </c>
-      <c t="s" s="13" r="C262">
-        <v>932</v>
+        <v>933</v>
+      </c>
+      <c t="s" s="7" r="C262">
+        <v>934</v>
       </c>
       <c t="s" s="7" r="D262">
-        <v>933</v>
+        <v>935</v>
       </c>
       <c t="s" s="7" r="E262">
-        <v>934</v>
+        <v>936</v>
       </c>
     </row>
     <row r="263">
       <c s="17" r="A263"/>
       <c t="s" s="7" r="B263">
-        <v>935</v>
-      </c>
-      <c t="s" s="7" r="C263">
-        <v>936</v>
+        <v>937</v>
+      </c>
+      <c t="s" s="13" r="C263">
+        <v>938</v>
       </c>
       <c t="s" s="7" r="D263">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c t="s" s="7" r="E263">
-        <v>938</v>
+        <v>940</v>
       </c>
     </row>
     <row r="264">
       <c s="17" r="A264"/>
       <c t="s" s="7" r="B264">
-        <v>939</v>
-      </c>
-      <c t="s" s="13" r="C264">
-        <v>940</v>
+        <v>941</v>
+      </c>
+      <c t="s" s="7" r="C264">
+        <v>942</v>
       </c>
       <c t="s" s="7" r="D264">
-        <v>941</v>
+        <v>943</v>
       </c>
       <c t="s" s="7" r="E264">
-        <v>942</v>
+        <v>944</v>
       </c>
     </row>
     <row r="265">
       <c s="17" r="A265"/>
       <c t="s" s="7" r="B265">
-        <v>943</v>
-      </c>
-      <c t="s" s="7" r="C265">
-        <v>944</v>
+        <v>945</v>
+      </c>
+      <c t="s" s="13" r="C265">
+        <v>946</v>
       </c>
       <c t="s" s="7" r="D265">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c t="s" s="7" r="E265">
-        <v>946</v>
+        <v>948</v>
       </c>
     </row>
     <row r="266">
       <c s="17" r="A266"/>
       <c t="s" s="7" r="B266">
-        <v>947</v>
-      </c>
-      <c t="s" s="13" r="C266">
-        <v>948</v>
+        <v>949</v>
+      </c>
+      <c t="s" s="7" r="C266">
+        <v>950</v>
       </c>
       <c t="s" s="7" r="D266">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c t="s" s="7" r="E266">
-        <v>950</v>
+        <v>952</v>
       </c>
     </row>
     <row r="267">
       <c s="17" r="A267"/>
       <c t="s" s="7" r="B267">
-        <v>951</v>
-      </c>
-      <c t="s" s="7" r="C267">
-        <v>952</v>
+        <v>953</v>
+      </c>
+      <c t="s" s="13" r="C267">
+        <v>954</v>
       </c>
       <c t="s" s="7" r="D267">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c t="s" s="7" r="E267">
-        <v>954</v>
+        <v>956</v>
       </c>
     </row>
     <row r="268">
       <c s="17" r="A268"/>
       <c t="s" s="7" r="B268">
-        <v>955</v>
-      </c>
-      <c t="s" s="13" r="C268">
-        <v>948</v>
+        <v>957</v>
+      </c>
+      <c t="s" s="7" r="C268">
+        <v>958</v>
       </c>
       <c t="s" s="7" r="D268">
-        <v>949</v>
+        <v>959</v>
       </c>
       <c t="s" s="7" r="E268">
-        <v>950</v>
+        <v>960</v>
       </c>
     </row>
     <row r="269">
       <c s="17" r="A269"/>
       <c t="s" s="7" r="B269">
+        <v>961</v>
+      </c>
+      <c t="s" s="13" r="C269">
+        <v>954</v>
+      </c>
+      <c t="s" s="7" r="D269">
+        <v>955</v>
+      </c>
+      <c t="s" s="7" r="E269">
         <v>956</v>
-      </c>
-      <c t="s" s="13" r="C269">
-        <v>957</v>
-      </c>
-      <c t="s" s="7" r="D269">
-        <v>958</v>
-      </c>
-      <c t="s" s="7" r="E269">
-        <v>959</v>
       </c>
     </row>
     <row r="270">
       <c s="17" r="A270"/>
       <c t="s" s="7" r="B270">
-        <v>960</v>
+        <v>962</v>
       </c>
       <c t="s" s="13" r="C270">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c t="s" s="7" r="D270">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c t="s" s="7" r="E270">
-        <v>963</v>
+        <v>965</v>
       </c>
     </row>
     <row r="271">
       <c s="17" r="A271"/>
       <c t="s" s="7" r="B271">
-        <v>964</v>
-      </c>
-      <c t="s" s="7" r="C271">
-        <v>965</v>
+        <v>966</v>
+      </c>
+      <c t="s" s="13" r="C271">
+        <v>967</v>
       </c>
       <c t="s" s="7" r="D271">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c t="s" s="7" r="E271">
-        <v>967</v>
+        <v>969</v>
       </c>
     </row>
     <row r="272">
       <c s="17" r="A272"/>
       <c t="s" s="7" r="B272">
-        <v>968</v>
-      </c>
-      <c t="s" s="13" r="C272">
-        <v>969</v>
+        <v>970</v>
+      </c>
+      <c t="s" s="7" r="C272">
+        <v>971</v>
       </c>
       <c t="s" s="7" r="D272">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c t="s" s="7" r="E272">
-        <v>971</v>
+        <v>973</v>
       </c>
     </row>
     <row r="273">
-      <c s="9" r="A273"/>
+      <c s="17" r="A273"/>
       <c t="s" s="7" r="B273">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c t="s" s="13" r="C273">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c t="s" s="7" r="D273">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c t="s" s="7" r="E273">
-        <v>975</v>
+        <v>977</v>
       </c>
     </row>
     <row r="274">
-      <c t="s" s="9" r="A274">
-        <v>976</v>
-      </c>
-      <c t="s" s="2" r="B274">
-        <v>977</v>
-      </c>
-      <c t="s" s="32" r="C274">
+      <c s="9" r="A274"/>
+      <c t="s" s="7" r="B274">
         <v>978</v>
       </c>
-      <c s="18" r="D274"/>
-      <c s="18" r="E274"/>
+      <c t="s" s="13" r="C274">
+        <v>979</v>
+      </c>
+      <c t="s" s="7" r="D274">
+        <v>980</v>
+      </c>
+      <c t="s" s="7" r="E274">
+        <v>981</v>
+      </c>
     </row>
     <row r="275">
-      <c s="9" r="A275"/>
-      <c t="s" s="2" r="B275">
-        <v>979</v>
-      </c>
-      <c t="s" s="2" r="C275">
-        <v>980</v>
-      </c>
-      <c s="18" r="D275"/>
-      <c s="18" r="E275"/>
+      <c t="s" s="9" r="A275">
+        <v>982</v>
+      </c>
+      <c t="s" s="13" r="B275">
+        <v>983</v>
+      </c>
+      <c t="s" s="13" r="C275">
+        <v>984</v>
+      </c>
+      <c t="s" s="18" r="D275">
+        <v>985</v>
+      </c>
+      <c t="s" s="18" r="E275">
+        <v>986</v>
+      </c>
     </row>
     <row r="276">
       <c s="9" r="A276"/>
-      <c s="8" r="C276"/>
-      <c s="16" r="D276"/>
-      <c s="16" r="E276"/>
+      <c t="s" s="13" r="B276">
+        <v>987</v>
+      </c>
+      <c t="s" s="13" r="C276">
+        <v>988</v>
+      </c>
+      <c t="s" s="18" r="D276">
+        <v>989</v>
+      </c>
+      <c t="s" s="18" r="E276">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="277">
+      <c s="9" r="A277"/>
+      <c s="8" r="C277"/>
+      <c s="16" r="D277"/>
+      <c s="16" r="E277"/>
     </row>
   </sheetData>
 </worksheet>
@@ -7471,17 +7531,17 @@
   <sheetData>
     <row customHeight="1" r="1" ht="112.5">
       <c t="s" s="4" r="A1">
-        <v>981</v>
+        <v>991</v>
       </c>
     </row>
     <row customHeight="1" r="2" ht="112.5">
       <c t="s" s="5" r="A2">
-        <v>982</v>
+        <v>992</v>
       </c>
     </row>
     <row customHeight="1" r="3" ht="112.5">
       <c t="s" s="10" r="A3">
-        <v>983</v>
+        <v>993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
publish from list copy link
Former-commit-id: 8d9a9ca376d7f518b9c72055d91bb31cc0e58f9a
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="1008">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="1010">
   <si>
     <t>d</t>
   </si>
@@ -382,6 +382,12 @@
   </si>
   <si>
     <t>Send feedback</t>
+  </si>
+  <si>
+    <t>Feedback versturen</t>
+  </si>
+  <si>
+    <t>Feedback senden</t>
   </si>
   <si>
     <t>Objectives</t>
@@ -4095,14 +4101,18 @@
     </row>
     <row r="32">
       <c s="20" r="A32"/>
-      <c t="s" s="19" r="B32">
+      <c t="s" s="7" r="B32">
         <v>121</v>
       </c>
-      <c t="s" s="19" r="C32">
+      <c t="s" s="7" r="C32">
         <v>122</v>
       </c>
-      <c s="19" r="D32"/>
-      <c s="19" r="E32"/>
+      <c t="s" s="7" r="D32">
+        <v>123</v>
+      </c>
+      <c t="s" s="7" r="E32">
+        <v>124</v>
+      </c>
     </row>
     <row r="33">
       <c s="20" r="A33"/>
@@ -4113,109 +4123,109 @@
     </row>
     <row r="34">
       <c t="s" s="20" r="A34">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c t="s" s="7" r="B34">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c t="s" s="7" r="C34">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c t="s" s="7" r="D34">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c t="s" s="7" r="E34">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35">
       <c s="20" r="A35"/>
       <c t="s" s="7" r="B35">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c t="s" s="7" r="C35">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c t="s" s="7" r="D35">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c t="s" s="7" r="E35">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36">
       <c s="20" r="A36"/>
       <c t="s" s="7" r="B36">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c t="s" s="7" r="C36">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c t="s" s="7" r="D36">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c t="s" s="7" r="E36">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37">
       <c s="20" r="A37"/>
       <c t="s" s="7" r="B37">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c t="s" s="7" r="C37">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c t="s" s="7" r="D37">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c t="s" s="7" r="E37">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="38">
       <c s="20" r="A38"/>
       <c t="s" s="7" r="B38">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c t="s" s="7" r="C38">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c t="s" s="7" r="D38">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c t="s" s="7" r="E38">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39">
       <c s="12" r="A39"/>
       <c t="s" s="7" r="B39">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c t="s" s="7" r="C39">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c t="s" s="7" r="D39">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c t="s" s="7" r="E39">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40">
       <c s="12" r="A40"/>
       <c t="s" s="7" r="B40">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c t="s" s="7" r="C40">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c t="s" s="7" r="D40">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c t="s" s="7" r="E40">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41">
@@ -4227,379 +4237,379 @@
     </row>
     <row r="42">
       <c t="s" s="12" r="A42">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c t="s" s="7" r="B42">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c t="s" s="7" r="C42">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c t="s" s="7" r="D42">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c t="s" s="7" r="E42">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43">
       <c s="12" r="A43"/>
       <c t="s" s="7" r="B43">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c t="s" s="7" r="C43">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c t="s" s="7" r="D43">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c t="s" s="7" r="E43">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="44">
       <c s="12" r="A44"/>
       <c t="s" s="7" r="B44">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c t="s" s="7" r="C44">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c t="s" s="7" r="D44">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c t="s" s="7" r="E44">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="45">
       <c s="12" r="A45"/>
       <c t="s" s="7" r="B45">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c t="s" s="7" r="C45">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c t="s" s="7" r="D45">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c t="s" s="7" r="E45">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="46">
       <c s="12" r="A46"/>
       <c t="s" s="7" r="B46">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c t="s" s="7" r="C46">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c t="s" s="7" r="D46">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c t="s" s="7" r="E46">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="47">
       <c s="12" r="A47"/>
       <c t="s" s="7" r="B47">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c t="s" s="7" r="C47">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c t="s" s="7" r="D47">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c t="s" s="7" r="E47">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="48">
       <c s="12" r="A48"/>
       <c t="s" s="7" r="B48">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c t="s" s="7" r="C48">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c t="s" s="7" r="D48">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c t="s" s="7" r="E48">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="49">
       <c s="12" r="A49"/>
       <c t="s" s="7" r="B49">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c t="s" s="7" r="C49">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c t="s" s="7" r="D49">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c t="s" s="7" r="E49">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="50">
       <c s="12" r="A50"/>
       <c t="s" s="7" r="B50">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c t="s" s="7" r="C50">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c t="s" s="7" r="D50">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c t="s" s="7" r="E50">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="51">
       <c s="12" r="A51"/>
       <c t="s" s="7" r="B51">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c t="s" s="7" r="C51">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c t="s" s="7" r="D51">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c t="s" s="7" r="E51">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="52">
       <c s="12" r="A52"/>
       <c t="s" s="7" r="B52">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c t="s" s="7" r="C52">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c t="s" s="7" r="D52">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c t="s" s="7" r="E52">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="53">
       <c s="12" r="A53"/>
       <c t="s" s="7" r="B53">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c t="s" s="7" r="C53">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c t="s" s="7" r="D53">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c t="s" s="7" r="E53">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="54">
       <c s="12" r="A54"/>
       <c t="s" s="7" r="B54">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c t="s" s="7" r="C54">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c t="s" s="7" r="D54">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c t="s" s="7" r="E54">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="55">
       <c s="12" r="A55"/>
       <c t="s" s="7" r="B55">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c t="s" s="7" r="C55">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c t="s" s="7" r="D55">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c t="s" s="7" r="E55">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="56">
       <c s="12" r="A56"/>
       <c t="s" s="7" r="B56">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c t="s" s="7" r="C56">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c t="s" s="7" r="D56">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c t="s" s="7" r="E56">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="57">
       <c s="12" r="A57"/>
       <c t="s" s="7" r="B57">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c t="s" s="7" r="C57">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c t="s" s="7" r="D57">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c t="s" s="7" r="E57">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="58">
       <c s="12" r="A58"/>
       <c t="s" s="7" r="B58">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c t="s" s="7" r="C58">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c t="s" s="7" r="D58">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c t="s" s="7" r="E58">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="59">
       <c s="12" r="A59"/>
       <c t="s" s="7" r="B59">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c t="s" s="7" r="C59">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c t="s" s="7" r="D59">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c t="s" s="7" r="E59">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="60">
       <c s="12" r="A60"/>
       <c t="s" s="7" r="B60">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c t="s" s="7" r="C60">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c t="s" s="7" r="D60">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c t="s" s="7" r="E60">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="61">
       <c s="12" r="A61"/>
       <c t="s" s="7" r="B61">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c t="s" s="7" r="C61">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c t="s" s="7" r="D61">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c t="s" s="7" r="E61">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="62">
       <c s="12" r="A62"/>
       <c t="s" s="27" r="B62">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c t="s" s="7" r="C62">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c t="s" s="7" r="D62">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c t="s" s="7" r="E62">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="63">
       <c s="12" r="A63"/>
       <c t="s" s="27" r="B63">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c t="s" s="7" r="C63">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c t="s" s="7" r="D63">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c t="s" s="7" r="E63">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="64">
       <c s="12" r="A64"/>
       <c t="s" s="27" r="B64">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c t="s" s="7" r="C64">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c t="s" s="27" r="D64">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c t="s" s="27" r="E64">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="65">
       <c s="12" r="A65"/>
       <c t="s" s="6" r="B65">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c t="s" s="11" r="C65">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c t="s" s="6" r="D65">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c t="s" s="6" r="E65">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="66">
       <c s="12" r="A66"/>
       <c t="s" s="27" r="B66">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c t="s" s="7" r="C66">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c t="s" s="27" r="D66">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c t="s" s="27" r="E66">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="67">
@@ -4611,34 +4621,34 @@
     </row>
     <row r="68">
       <c t="s" s="12" r="A68">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c t="s" s="7" r="B68">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c t="s" s="7" r="C68">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c t="s" s="7" r="D68">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c t="s" s="7" r="E68">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="69">
       <c s="12" r="A69"/>
       <c t="s" s="7" r="B69">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c t="s" s="7" r="C69">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c t="s" s="7" r="D69">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c t="s" s="7" r="E69">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="71">
@@ -4650,94 +4660,94 @@
     </row>
     <row r="72">
       <c t="s" s="12" r="A72">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c t="s" s="7" r="B72">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c t="s" s="7" r="C72">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c t="s" s="7" r="D72">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c t="s" s="7" r="E72">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="73">
       <c s="12" r="A73"/>
       <c t="s" s="7" r="B73">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c t="s" s="7" r="C73">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c t="s" s="7" r="D73">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c t="s" s="7" r="E73">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="74">
       <c s="12" r="A74"/>
       <c t="s" s="7" r="B74">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c t="s" s="7" r="C74">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c t="s" s="7" r="D74">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c t="s" s="7" r="E74">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="75">
       <c s="12" r="A75"/>
       <c t="s" s="7" r="B75">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c t="s" s="7" r="C75">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c t="s" s="7" r="D75">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c t="s" s="7" r="E75">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="76">
       <c s="12" r="A76"/>
       <c t="s" s="7" r="B76">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c t="s" s="7" r="C76">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c t="s" s="7" r="D76">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c t="s" s="7" r="E76">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="77">
       <c s="12" r="A77"/>
       <c t="s" s="7" r="B77">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c t="s" s="7" r="C77">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c t="s" s="7" r="D77">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c t="s" s="7" r="E77">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="78">
@@ -4749,139 +4759,139 @@
     </row>
     <row r="79">
       <c t="s" s="12" r="A79">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c t="s" s="7" r="B79">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c t="s" s="7" r="C79">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c t="s" s="7" r="D79">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c t="s" s="7" r="E79">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="80">
       <c s="12" r="A80"/>
       <c t="s" s="7" r="B80">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c t="s" s="7" r="C80">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c t="s" s="7" r="D80">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c t="s" s="7" r="E80">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="81">
       <c s="12" r="A81"/>
       <c t="s" s="7" r="B81">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c t="s" s="7" r="C81">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c t="s" s="7" r="D81">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c t="s" s="7" r="E81">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="82">
       <c s="12" r="A82"/>
       <c t="s" s="7" r="B82">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c t="s" s="7" r="C82">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c t="s" s="7" r="D82">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c t="s" s="7" r="E82">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="83">
       <c s="12" r="A83"/>
       <c t="s" s="7" r="B83">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c t="s" s="7" r="C83">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c t="s" s="7" r="D83">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c t="s" s="7" r="E83">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="84">
       <c s="12" r="A84"/>
       <c t="s" s="7" r="B84">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c t="s" s="7" r="C84">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c t="s" s="7" r="D84">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c t="s" s="7" r="E84">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="85">
       <c s="12" r="A85"/>
       <c t="s" s="7" r="B85">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c t="s" s="7" r="C85">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c t="s" s="7" r="D85">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c t="s" s="7" r="E85">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="86">
       <c s="12" r="A86"/>
       <c t="s" s="7" r="B86">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c t="s" s="7" r="C86">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c t="s" s="7" r="D86">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c t="s" s="7" r="E86">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="87">
       <c s="12" r="A87"/>
       <c t="s" s="7" r="B87">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c t="s" s="7" r="C87">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c t="s" s="7" r="D87">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c t="s" s="7" r="E87">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="88">
@@ -4893,229 +4903,229 @@
     </row>
     <row r="89">
       <c t="s" s="12" r="A89">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c t="s" s="7" r="B89">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c t="s" s="7" r="C89">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c t="s" s="7" r="D89">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c t="s" s="7" r="E89">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="90">
       <c s="12" r="A90"/>
       <c t="s" s="7" r="B90">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c t="s" s="7" r="C90">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c t="s" s="7" r="D90">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c t="s" s="7" r="E90">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="91">
       <c s="9" r="A91"/>
       <c t="s" s="7" r="B91">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c t="s" s="7" r="C91">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c t="s" s="7" r="D91">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c t="s" s="7" r="E91">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="92">
       <c s="9" r="A92"/>
       <c t="s" s="7" r="B92">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c t="s" s="7" r="C92">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c t="s" s="7" r="D92">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c t="s" s="7" r="E92">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="93">
       <c s="9" r="A93"/>
       <c t="s" s="7" r="B93">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c t="s" s="7" r="C93">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c t="s" s="7" r="D93">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c t="s" s="7" r="E93">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="94">
       <c s="9" r="A94"/>
       <c t="s" s="7" r="B94">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c t="s" s="7" r="C94">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c t="s" s="7" r="D94">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c t="s" s="7" r="E94">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="95">
       <c s="9" r="A95"/>
       <c t="s" s="7" r="B95">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c t="s" s="7" r="C95">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c t="s" s="7" r="D95">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c t="s" s="7" r="E95">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="96">
       <c s="9" r="A96"/>
       <c t="s" s="7" r="B96">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c t="s" s="7" r="C96">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c t="s" s="7" r="D96">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c t="s" s="7" r="E96">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="97">
       <c s="9" r="A97"/>
       <c t="s" s="7" r="B97">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c t="s" s="7" r="C97">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c t="s" s="7" r="D97">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c t="s" s="7" r="E97">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="98">
       <c s="9" r="A98"/>
       <c t="s" s="7" r="B98">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c t="s" s="7" r="C98">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c t="s" s="7" r="D98">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c t="s" s="7" r="E98">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="99">
       <c s="9" r="A99"/>
       <c t="s" s="7" r="B99">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c t="s" s="7" r="C99">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c t="s" s="7" r="D99">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c t="s" s="7" r="E99">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="100">
       <c s="9" r="A100"/>
       <c t="s" s="7" r="B100">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c t="s" s="7" r="C100">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c t="s" s="7" r="D100">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c t="s" s="7" r="E100">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="101">
       <c s="9" r="A101"/>
       <c t="s" s="7" r="B101">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c t="s" s="7" r="C101">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c t="s" s="7" r="D101">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c t="s" s="7" r="E101">
-        <v>376</v>
+        <v>378</v>
       </c>
     </row>
     <row r="102">
       <c s="9" r="A102"/>
       <c t="s" s="7" r="B102">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c t="s" s="7" r="C102">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c t="s" s="7" r="D102">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c t="s" s="7" r="E102">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="103">
       <c s="9" r="A103"/>
       <c t="s" s="7" r="B103">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c t="s" s="7" r="C103">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c t="s" s="7" r="D103">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c t="s" s="7" r="E103">
-        <v>384</v>
+        <v>386</v>
       </c>
     </row>
     <row r="104">
@@ -5127,544 +5137,544 @@
     </row>
     <row r="105">
       <c t="s" s="9" r="A105">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c t="s" s="7" r="B105">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c t="s" s="7" r="C105">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c t="s" s="7" r="D105">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c t="s" s="7" r="E105">
-        <v>389</v>
+        <v>391</v>
       </c>
     </row>
     <row r="106">
       <c s="9" r="A106"/>
       <c t="s" s="7" r="B106">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c t="s" s="7" r="C106">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c t="s" s="7" r="D106">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c t="s" s="7" r="E106">
-        <v>393</v>
+        <v>395</v>
       </c>
     </row>
     <row r="107">
       <c s="9" r="A107"/>
       <c t="s" s="7" r="B107">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c t="s" s="7" r="C107">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c t="s" s="7" r="D107">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c t="s" s="7" r="E107">
-        <v>397</v>
+        <v>399</v>
       </c>
     </row>
     <row r="108">
       <c s="9" r="A108"/>
       <c t="s" s="7" r="B108">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c t="s" s="7" r="C108">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c t="s" s="7" r="D108">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c t="s" s="7" r="E108">
-        <v>401</v>
+        <v>403</v>
       </c>
     </row>
     <row r="109">
       <c s="9" r="A109"/>
       <c t="s" s="7" r="B109">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c t="s" s="7" r="C109">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c t="s" s="7" r="D109">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c t="s" s="7" r="E109">
-        <v>405</v>
+        <v>407</v>
       </c>
     </row>
     <row r="110">
       <c s="9" r="A110"/>
       <c t="s" s="7" r="B110">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c t="s" s="7" r="C110">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c t="s" s="7" r="D110">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c t="s" s="7" r="E110">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="111">
       <c s="9" r="A111"/>
       <c t="s" s="7" r="B111">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c t="s" s="7" r="C111">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c t="s" s="7" r="D111">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c t="s" s="7" r="E111">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="112">
       <c s="9" r="A112"/>
       <c t="s" s="7" r="B112">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c t="s" s="7" r="C112">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c t="s" s="7" r="D112">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c t="s" s="7" r="E112">
-        <v>415</v>
+        <v>417</v>
       </c>
     </row>
     <row r="113">
       <c s="9" r="A113"/>
       <c t="s" s="7" r="B113">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c t="s" s="7" r="C113">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c t="s" s="7" r="D113">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c t="s" s="7" r="E113">
-        <v>419</v>
+        <v>421</v>
       </c>
     </row>
     <row r="114">
       <c s="9" r="A114"/>
       <c t="s" s="7" r="B114">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c t="s" s="7" r="C114">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c t="s" s="7" r="D114">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c t="s" s="7" r="E114">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
     <row r="115">
       <c s="9" r="A115"/>
       <c t="s" s="7" r="B115">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c t="s" s="7" r="C115">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c t="s" s="7" r="D115">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c t="s" s="7" r="E115">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="116">
       <c s="9" r="A116"/>
       <c t="s" s="7" r="B116">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c t="s" s="7" r="C116">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c t="s" s="7" r="D116">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c t="s" s="7" r="E116">
-        <v>430</v>
+        <v>432</v>
       </c>
     </row>
     <row r="117">
       <c s="9" r="A117"/>
       <c t="s" s="7" r="B117">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c t="s" s="7" r="C117">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c t="s" s="7" r="D117">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c t="s" s="7" r="E117">
-        <v>433</v>
+        <v>435</v>
       </c>
     </row>
     <row r="118">
       <c s="9" r="A118"/>
       <c t="s" s="7" r="B118">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c t="s" s="7" r="C118">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c t="s" s="7" r="D118">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c t="s" s="7" r="E118">
-        <v>437</v>
+        <v>439</v>
       </c>
     </row>
     <row r="119">
       <c s="9" r="A119"/>
       <c t="s" s="14" r="B119">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c t="s" s="7" r="C119">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c t="s" s="7" r="D119">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c t="s" s="7" r="E119">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="120">
       <c s="9" r="A120"/>
       <c t="s" s="7" r="B120">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c t="s" s="7" r="C120">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c t="s" s="7" r="D120">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c t="s" s="7" r="E120">
-        <v>444</v>
+        <v>446</v>
       </c>
     </row>
     <row r="121">
       <c s="9" r="A121"/>
       <c t="s" s="7" r="B121">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c t="s" s="7" r="C121">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c t="s" s="7" r="D121">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c t="s" s="7" r="E121">
-        <v>448</v>
+        <v>450</v>
       </c>
     </row>
     <row r="122">
       <c s="9" r="A122"/>
       <c t="s" s="7" r="B122">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c t="s" s="7" r="C122">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c t="s" s="7" r="D122">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c t="s" s="7" r="E122">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="123">
       <c s="9" r="A123"/>
       <c t="s" s="7" r="B123">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c t="s" s="7" r="C123">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c t="s" s="7" r="D123">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c t="s" s="7" r="E123">
-        <v>456</v>
+        <v>458</v>
       </c>
     </row>
     <row r="124">
       <c s="9" r="A124"/>
       <c t="s" s="7" r="B124">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c t="s" s="7" r="C124">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c t="s" s="7" r="D124">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c t="s" s="7" r="E124">
-        <v>460</v>
+        <v>462</v>
       </c>
     </row>
     <row r="125">
       <c s="9" r="A125"/>
       <c t="s" s="7" r="B125">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c t="s" s="7" r="C125">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c t="s" s="7" r="D125">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c t="s" s="7" r="E125">
-        <v>464</v>
+        <v>466</v>
       </c>
     </row>
     <row r="126">
       <c s="9" r="A126"/>
       <c t="s" s="7" r="B126">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c t="s" s="7" r="C126">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c t="s" s="7" r="D126">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c t="s" s="7" r="E126">
-        <v>468</v>
+        <v>470</v>
       </c>
     </row>
     <row r="127">
       <c s="9" r="A127"/>
       <c t="s" s="7" r="B127">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c t="s" s="7" r="C127">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c t="s" s="7" r="D127">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c t="s" s="7" r="E127">
-        <v>472</v>
+        <v>474</v>
       </c>
     </row>
     <row r="128">
       <c s="9" r="A128"/>
       <c t="s" s="7" r="B128">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c t="s" s="7" r="C128">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c t="s" s="7" r="D128">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c t="s" s="7" r="E128">
-        <v>476</v>
+        <v>478</v>
       </c>
     </row>
     <row r="129">
       <c s="9" r="A129"/>
       <c t="s" s="7" r="B129">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c t="s" s="7" r="C129">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c t="s" s="7" r="D129">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c t="s" s="7" r="E129">
-        <v>480</v>
+        <v>482</v>
       </c>
     </row>
     <row r="130">
       <c s="9" r="A130"/>
       <c t="s" s="7" r="B130">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c t="s" s="7" r="C130">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c t="s" s="7" r="D130">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c t="s" s="7" r="E130">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="131">
       <c s="9" r="A131"/>
       <c t="s" s="7" r="B131">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c t="s" s="7" r="C131">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c t="s" s="7" r="D131">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c t="s" s="7" r="E131">
-        <v>488</v>
+        <v>490</v>
       </c>
     </row>
     <row r="132">
       <c s="9" r="A132"/>
       <c t="s" s="7" r="B132">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c t="s" s="7" r="C132">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c t="s" s="7" r="D132">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c t="s" s="7" r="E132">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="133">
       <c s="9" r="A133"/>
       <c t="s" s="7" r="B133">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c t="s" s="7" r="C133">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c t="s" s="7" r="D133">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c t="s" s="7" r="E133">
-        <v>496</v>
+        <v>498</v>
       </c>
     </row>
     <row r="134">
       <c s="9" r="A134"/>
       <c t="s" s="7" r="B134">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c t="s" s="7" r="C134">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c t="s" s="7" r="D134">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c t="s" s="7" r="E134">
-        <v>500</v>
+        <v>502</v>
       </c>
     </row>
     <row r="135">
       <c s="9" r="A135"/>
       <c t="s" s="7" r="B135">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c t="s" s="14" r="C135">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c t="s" s="7" r="D135">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c t="s" s="7" r="E135">
-        <v>504</v>
+        <v>506</v>
       </c>
     </row>
     <row r="136">
       <c s="9" r="A136"/>
       <c t="s" s="14" r="B136">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c t="s" s="14" r="C136">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c t="s" s="7" r="D136">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c t="s" s="7" r="E136">
-        <v>508</v>
+        <v>510</v>
       </c>
     </row>
     <row r="137">
       <c s="9" r="A137"/>
       <c t="s" s="7" r="B137">
+        <v>511</v>
+      </c>
+      <c t="s" s="14" r="C137">
+        <v>508</v>
+      </c>
+      <c t="s" s="7" r="D137">
         <v>509</v>
       </c>
-      <c t="s" s="14" r="C137">
-        <v>506</v>
-      </c>
-      <c t="s" s="7" r="D137">
-        <v>507</v>
-      </c>
       <c t="s" s="7" r="E137">
-        <v>508</v>
+        <v>510</v>
       </c>
     </row>
     <row r="138">
       <c s="9" r="A138"/>
       <c t="s" s="7" r="B138">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c t="s" s="2" r="C138">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c t="s" s="7" r="D138">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c t="s" s="7" r="E138">
-        <v>513</v>
+        <v>515</v>
       </c>
     </row>
     <row r="139">
       <c s="9" r="A139"/>
       <c t="s" s="7" r="B139">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c t="s" s="2" r="C139">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c t="s" s="7" r="D139">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c t="s" s="7" r="E139">
-        <v>517</v>
+        <v>519</v>
       </c>
     </row>
     <row r="140">
       <c s="9" r="A140"/>
       <c t="s" s="7" r="B140">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c t="s" s="2" r="C140">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c t="s" s="7" r="D140">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c t="s" s="2" r="E140">
-        <v>521</v>
+        <v>523</v>
       </c>
     </row>
     <row r="141">
@@ -5676,169 +5686,169 @@
     </row>
     <row r="142">
       <c t="s" s="9" r="A142">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c t="s" s="7" r="B142">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c t="s" s="14" r="C142">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c t="s" s="7" r="D142">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c t="s" s="7" r="E142">
-        <v>526</v>
+        <v>528</v>
       </c>
     </row>
     <row r="143">
       <c s="9" r="A143"/>
       <c t="s" s="22" r="B143">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c t="s" s="14" r="C143">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c t="s" s="22" r="D143">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c t="s" s="22" r="E143">
-        <v>530</v>
+        <v>532</v>
       </c>
     </row>
     <row r="144">
       <c s="9" r="A144"/>
       <c t="s" s="7" r="B144">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c t="s" s="14" r="C144">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c t="s" s="7" r="D144">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c t="s" s="7" r="E144">
-        <v>534</v>
+        <v>536</v>
       </c>
     </row>
     <row r="145">
       <c s="9" r="A145"/>
       <c t="s" s="7" r="B145">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c t="s" s="14" r="C145">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c t="s" s="7" r="D145">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c t="s" s="7" r="E145">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="146">
       <c s="18" r="A146"/>
       <c t="s" s="7" r="B146">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c t="s" s="14" r="C146">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c t="s" s="7" r="D146">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c t="s" s="7" r="E146">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="147">
       <c s="9" r="A147"/>
       <c t="s" s="7" r="B147">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c t="s" s="14" r="C147">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c t="s" s="7" r="D147">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c t="s" s="7" r="E147">
-        <v>546</v>
+        <v>548</v>
       </c>
     </row>
     <row r="148">
       <c s="9" r="A148"/>
       <c t="s" s="7" r="B148">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c t="s" s="14" r="C148">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c t="s" s="7" r="D148">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c t="s" s="7" r="E148">
-        <v>550</v>
+        <v>552</v>
       </c>
     </row>
     <row r="149">
       <c s="9" r="A149"/>
       <c t="s" s="7" r="B149">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c t="s" s="14" r="C149">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c t="s" s="7" r="D149">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c t="s" s="7" r="E149">
-        <v>554</v>
+        <v>556</v>
       </c>
     </row>
     <row r="150">
       <c s="9" r="A150"/>
       <c t="s" s="7" r="B150">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c t="s" s="14" r="C150">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c t="s" s="7" r="D150">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c t="s" s="7" r="E150">
-        <v>558</v>
+        <v>560</v>
       </c>
     </row>
     <row r="151">
       <c s="9" r="A151"/>
       <c t="s" s="7" r="B151">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c t="s" s="14" r="C151">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c t="s" s="7" r="D151">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c t="s" s="7" r="E151">
-        <v>562</v>
+        <v>564</v>
       </c>
     </row>
     <row r="152">
       <c s="9" r="A152"/>
       <c t="s" s="7" r="B152">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c t="s" s="14" r="C152">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c t="s" s="7" r="D152">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c t="s" s="7" r="E152">
-        <v>566</v>
+        <v>568</v>
       </c>
     </row>
     <row r="153">
@@ -5850,109 +5860,109 @@
     </row>
     <row r="154">
       <c t="s" s="9" r="A154">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c t="s" s="7" r="B154">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c t="s" s="14" r="C154">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c t="s" s="7" r="D154">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c t="s" s="7" r="E154">
-        <v>571</v>
+        <v>573</v>
       </c>
     </row>
     <row r="155">
       <c s="9" r="A155"/>
       <c t="s" s="7" r="B155">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c t="s" s="14" r="C155">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c t="s" s="7" r="D155">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c t="s" s="7" r="E155">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="156">
       <c s="9" r="A156"/>
       <c t="s" s="7" r="B156">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c t="s" s="14" r="C156">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c t="s" s="7" r="D156">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c t="s" s="7" r="E156">
-        <v>579</v>
+        <v>581</v>
       </c>
     </row>
     <row r="157">
       <c s="9" r="A157"/>
       <c t="s" s="7" r="B157">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c t="s" s="14" r="C157">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c t="s" s="7" r="D157">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c t="s" s="7" r="E157">
-        <v>583</v>
+        <v>585</v>
       </c>
     </row>
     <row r="158">
       <c s="9" r="A158"/>
       <c t="s" s="7" r="B158">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c t="s" s="14" r="C158">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c t="s" s="7" r="D158">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c t="s" s="7" r="E158">
-        <v>587</v>
+        <v>589</v>
       </c>
     </row>
     <row r="159">
       <c s="9" r="A159"/>
       <c t="s" s="7" r="B159">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c t="s" s="14" r="C159">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c t="s" s="7" r="D159">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c t="s" s="7" r="E159">
-        <v>591</v>
+        <v>593</v>
       </c>
     </row>
     <row r="160">
       <c s="9" r="A160"/>
       <c t="s" s="7" r="B160">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c t="s" s="14" r="C160">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c t="s" s="7" r="D160">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c t="s" s="7" r="E160">
-        <v>595</v>
+        <v>597</v>
       </c>
     </row>
     <row r="161">
@@ -5964,13 +5974,13 @@
     </row>
     <row r="162">
       <c t="s" s="9" r="A162">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c t="s" s="29" r="B162">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c t="s" s="21" r="C162">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c s="29" r="D162"/>
       <c s="29" r="E162"/>
@@ -5984,13 +5994,13 @@
     </row>
     <row r="164">
       <c t="s" s="9" r="A164">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c t="s" s="35" r="B164">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c t="s" s="33" r="C164">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c s="35" r="D164"/>
       <c s="35" r="E164"/>
@@ -5998,10 +6008,10 @@
     <row r="165">
       <c s="9" r="A165"/>
       <c t="s" s="35" r="B165">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c t="s" s="33" r="C165">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c s="35" r="D165"/>
       <c s="35" r="E165"/>
@@ -6015,1648 +6025,1641 @@
     </row>
     <row r="167">
       <c t="s" s="9" r="A167">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c t="s" s="27" r="B167">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c t="s" s="27" r="C167">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c t="s" s="7" r="D167">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c t="s" s="7" r="E167">
-        <v>607</v>
+        <v>609</v>
       </c>
     </row>
     <row r="168">
       <c s="9" r="A168"/>
       <c t="s" s="27" r="B168">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c t="s" s="27" r="C168">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c t="s" s="7" r="D168">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c t="s" s="7" r="E168">
-        <v>610</v>
+        <v>612</v>
       </c>
     </row>
     <row r="169">
       <c s="9" r="A169"/>
       <c t="s" s="27" r="B169">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c t="s" s="27" r="C169">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c t="s" s="7" r="D169">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c t="s" s="7" r="E169">
-        <v>614</v>
+        <v>616</v>
       </c>
     </row>
     <row r="170">
       <c s="9" r="A170"/>
       <c t="s" s="27" r="B170">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c t="s" s="27" r="C170">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c t="s" s="7" r="D170">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c t="s" s="7" r="E170">
-        <v>618</v>
+        <v>620</v>
       </c>
     </row>
     <row r="171">
       <c s="9" r="A171"/>
       <c t="s" s="14" r="B171">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c t="s" s="14" r="C171">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c t="s" s="7" r="D171">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c t="s" s="7" r="E171">
-        <v>622</v>
+        <v>624</v>
       </c>
     </row>
     <row r="172">
       <c s="9" r="A172"/>
       <c t="s" s="14" r="B172">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c t="s" s="14" r="C172">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c t="s" s="7" r="D172">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c t="s" s="7" r="E172">
-        <v>626</v>
+        <v>628</v>
       </c>
     </row>
     <row r="173">
       <c s="9" r="A173"/>
       <c t="s" s="14" r="B173">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c t="s" s="14" r="C173">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c t="s" s="7" r="D173">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c t="s" s="7" r="E173">
-        <v>630</v>
+        <v>632</v>
       </c>
     </row>
     <row r="174">
       <c s="9" r="A174"/>
       <c t="s" s="14" r="B174">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c t="s" s="14" r="C174">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c t="s" s="7" r="D174">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c t="s" s="7" r="E174">
-        <v>634</v>
+        <v>636</v>
       </c>
     </row>
     <row r="175">
       <c s="9" r="A175"/>
       <c t="s" s="14" r="B175">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c t="s" s="14" r="C175">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c t="s" s="7" r="D175">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c t="s" s="7" r="E175">
-        <v>638</v>
+        <v>640</v>
       </c>
     </row>
     <row r="176">
       <c s="9" r="A176"/>
       <c t="s" s="14" r="B176">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c t="s" s="14" r="C176">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c t="s" s="7" r="D176">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c t="s" s="7" r="E176">
-        <v>642</v>
+        <v>644</v>
       </c>
     </row>
     <row r="177">
       <c s="9" r="A177"/>
       <c t="s" s="14" r="B177">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c t="s" s="14" r="C177">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c t="s" s="7" r="D177">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c t="s" s="7" r="E177">
-        <v>646</v>
+        <v>648</v>
       </c>
     </row>
     <row r="178">
       <c s="9" r="A178"/>
       <c t="s" s="7" r="B178">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c t="s" s="14" r="C178">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c t="s" s="7" r="D178">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c t="s" s="7" r="E178">
-        <v>650</v>
+        <v>652</v>
       </c>
     </row>
     <row r="179">
       <c s="9" r="A179"/>
       <c t="s" s="7" r="B179">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c t="s" s="14" r="C179">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c t="s" s="7" r="D179">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c t="s" s="7" r="E179">
-        <v>654</v>
+        <v>656</v>
       </c>
     </row>
     <row r="180">
       <c s="9" r="A180"/>
       <c t="s" s="7" r="B180">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c t="s" s="14" r="C180">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c t="s" s="7" r="D180">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c t="s" s="7" r="E180">
-        <v>658</v>
+        <v>660</v>
       </c>
     </row>
     <row r="181">
       <c s="9" r="A181"/>
       <c t="s" s="7" r="B181">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c t="s" s="14" r="C181">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c t="s" s="7" r="D181">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c t="s" s="7" r="E181">
-        <v>662</v>
+        <v>664</v>
       </c>
     </row>
     <row r="182">
       <c s="9" r="A182"/>
       <c t="s" s="7" r="B182">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c t="s" s="14" r="C182">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c t="s" s="7" r="D182">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c t="s" s="7" r="E182">
-        <v>666</v>
+        <v>668</v>
       </c>
     </row>
     <row r="183">
       <c s="9" r="A183"/>
       <c t="s" s="7" r="B183">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c t="s" s="14" r="C183">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c t="s" s="7" r="D183">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c t="s" s="7" r="E183">
-        <v>670</v>
+        <v>672</v>
       </c>
     </row>
     <row r="184">
       <c s="9" r="A184"/>
       <c t="s" s="7" r="B184">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c t="s" s="14" r="C184">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c t="s" s="7" r="D184">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c t="s" s="7" r="E184">
-        <v>674</v>
+        <v>676</v>
       </c>
     </row>
     <row r="185">
       <c s="9" r="A185"/>
       <c t="s" s="7" r="B185">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c t="s" s="14" r="C185">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c t="s" s="7" r="D185">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c t="s" s="7" r="E185">
-        <v>678</v>
+        <v>680</v>
       </c>
     </row>
     <row r="186">
       <c s="9" r="A186"/>
       <c t="s" s="7" r="B186">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c t="s" s="14" r="C186">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c t="s" s="7" r="D186">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c t="s" s="7" r="E186">
-        <v>682</v>
+        <v>684</v>
       </c>
     </row>
     <row r="187">
       <c s="9" r="A187"/>
-      <c s="12" r="B187"/>
-      <c s="15" r="C187"/>
-      <c s="12" r="D187"/>
-      <c s="12" r="E187"/>
+      <c s="17" r="B187"/>
+      <c s="30" r="C187"/>
+      <c s="17" r="D187"/>
+      <c s="17" r="E187"/>
     </row>
     <row r="188">
-      <c s="9" r="A188"/>
-      <c s="17" r="B188"/>
-      <c s="30" r="C188"/>
-      <c s="17" r="D188"/>
-      <c s="17" r="E188"/>
+      <c t="s" s="9" r="A188">
+        <v>685</v>
+      </c>
+      <c t="s" s="27" r="B188">
+        <v>686</v>
+      </c>
+      <c t="s" s="7" r="C188">
+        <v>611</v>
+      </c>
+      <c t="s" s="7" r="D188">
+        <v>611</v>
+      </c>
+      <c t="s" s="7" r="E188">
+        <v>612</v>
+      </c>
     </row>
     <row r="189">
-      <c t="s" s="9" r="A189">
-        <v>683</v>
-      </c>
-      <c t="s" s="27" r="B189">
-        <v>684</v>
-      </c>
-      <c t="s" s="7" r="C189">
-        <v>609</v>
+      <c s="9" r="A189"/>
+      <c t="s" s="7" r="B189">
+        <v>687</v>
+      </c>
+      <c t="s" s="14" r="C189">
+        <v>614</v>
       </c>
       <c t="s" s="7" r="D189">
-        <v>609</v>
+        <v>615</v>
       </c>
       <c t="s" s="7" r="E189">
-        <v>610</v>
+        <v>616</v>
       </c>
     </row>
     <row r="190">
-      <c s="9" r="A190"/>
       <c t="s" s="7" r="B190">
-        <v>685</v>
+        <v>688</v>
       </c>
       <c t="s" s="14" r="C190">
-        <v>612</v>
+        <v>689</v>
       </c>
       <c t="s" s="7" r="D190">
-        <v>613</v>
+        <v>690</v>
       </c>
       <c t="s" s="7" r="E190">
-        <v>614</v>
+        <v>691</v>
       </c>
     </row>
     <row r="191">
+      <c s="9" r="A191"/>
       <c t="s" s="7" r="B191">
-        <v>686</v>
+        <v>692</v>
       </c>
       <c t="s" s="14" r="C191">
-        <v>687</v>
+        <v>693</v>
       </c>
       <c t="s" s="7" r="D191">
-        <v>688</v>
+        <v>694</v>
       </c>
       <c t="s" s="7" r="E191">
-        <v>689</v>
+        <v>695</v>
       </c>
     </row>
     <row r="192">
       <c s="9" r="A192"/>
       <c t="s" s="7" r="B192">
-        <v>690</v>
+        <v>696</v>
       </c>
       <c t="s" s="14" r="C192">
-        <v>691</v>
+        <v>697</v>
       </c>
       <c t="s" s="7" r="D192">
-        <v>692</v>
+        <v>698</v>
       </c>
       <c t="s" s="7" r="E192">
-        <v>693</v>
+        <v>699</v>
       </c>
     </row>
     <row r="193">
       <c s="9" r="A193"/>
-      <c t="s" s="7" r="B193">
-        <v>694</v>
-      </c>
-      <c t="s" s="14" r="C193">
-        <v>695</v>
-      </c>
-      <c t="s" s="7" r="D193">
-        <v>696</v>
-      </c>
-      <c t="s" s="7" r="E193">
-        <v>697</v>
-      </c>
+      <c s="12" r="B193"/>
+      <c s="15" r="C193"/>
+      <c s="17" r="D193"/>
+      <c s="17" r="E193"/>
     </row>
     <row r="194">
-      <c s="9" r="A194"/>
-      <c s="12" r="B194"/>
-      <c s="15" r="C194"/>
-      <c s="17" r="D194"/>
-      <c s="17" r="E194"/>
+      <c t="s" s="9" r="A194">
+        <v>700</v>
+      </c>
+      <c t="s" s="7" r="B194">
+        <v>701</v>
+      </c>
+      <c t="s" s="14" r="C194">
+        <v>700</v>
+      </c>
+      <c t="s" s="7" r="D194">
+        <v>702</v>
+      </c>
+      <c t="s" s="7" r="E194">
+        <v>703</v>
+      </c>
     </row>
     <row r="195">
-      <c t="s" s="9" r="A195">
-        <v>698</v>
-      </c>
+      <c s="9" r="A195"/>
       <c t="s" s="7" r="B195">
-        <v>699</v>
+        <v>704</v>
       </c>
       <c t="s" s="14" r="C195">
-        <v>698</v>
+        <v>705</v>
       </c>
       <c t="s" s="7" r="D195">
-        <v>700</v>
+        <v>706</v>
       </c>
       <c t="s" s="7" r="E195">
-        <v>701</v>
+        <v>707</v>
       </c>
     </row>
     <row r="196">
       <c s="9" r="A196"/>
       <c t="s" s="7" r="B196">
-        <v>702</v>
+        <v>708</v>
       </c>
       <c t="s" s="14" r="C196">
-        <v>703</v>
+        <v>709</v>
       </c>
       <c t="s" s="7" r="D196">
-        <v>704</v>
+        <v>710</v>
       </c>
       <c t="s" s="7" r="E196">
-        <v>705</v>
+        <v>711</v>
       </c>
     </row>
     <row r="197">
       <c s="9" r="A197"/>
       <c t="s" s="7" r="B197">
-        <v>706</v>
+        <v>712</v>
       </c>
       <c t="s" s="14" r="C197">
-        <v>707</v>
+        <v>713</v>
       </c>
       <c t="s" s="7" r="D197">
-        <v>708</v>
+        <v>714</v>
       </c>
       <c t="s" s="7" r="E197">
-        <v>709</v>
+        <v>715</v>
       </c>
     </row>
     <row r="198">
       <c s="9" r="A198"/>
       <c t="s" s="7" r="B198">
-        <v>710</v>
+        <v>716</v>
       </c>
       <c t="s" s="14" r="C198">
-        <v>711</v>
+        <v>717</v>
       </c>
       <c t="s" s="7" r="D198">
-        <v>712</v>
+        <v>718</v>
       </c>
       <c t="s" s="7" r="E198">
-        <v>713</v>
+        <v>719</v>
       </c>
     </row>
     <row r="199">
       <c s="9" r="A199"/>
       <c t="s" s="7" r="B199">
-        <v>714</v>
+        <v>720</v>
       </c>
       <c t="s" s="14" r="C199">
-        <v>715</v>
+        <v>721</v>
       </c>
       <c t="s" s="7" r="D199">
-        <v>716</v>
+        <v>722</v>
       </c>
       <c t="s" s="7" r="E199">
-        <v>717</v>
+        <v>723</v>
       </c>
     </row>
     <row r="200">
       <c s="9" r="A200"/>
       <c t="s" s="7" r="B200">
-        <v>718</v>
+        <v>724</v>
       </c>
       <c t="s" s="14" r="C200">
-        <v>719</v>
+        <v>725</v>
       </c>
       <c t="s" s="7" r="D200">
-        <v>720</v>
+        <v>726</v>
       </c>
       <c t="s" s="7" r="E200">
-        <v>721</v>
+        <v>727</v>
       </c>
     </row>
     <row r="201">
       <c s="9" r="A201"/>
-      <c t="s" s="7" r="B201">
-        <v>722</v>
-      </c>
-      <c t="s" s="14" r="C201">
-        <v>723</v>
-      </c>
-      <c t="s" s="7" r="D201">
-        <v>724</v>
-      </c>
-      <c t="s" s="7" r="E201">
-        <v>725</v>
-      </c>
+      <c s="12" r="B201"/>
+      <c s="15" r="C201"/>
+      <c s="12" r="D201"/>
+      <c s="12" r="E201"/>
     </row>
     <row r="202">
-      <c s="9" r="A202"/>
-      <c s="12" r="B202"/>
-      <c s="15" r="C202"/>
-      <c s="12" r="D202"/>
-      <c s="12" r="E202"/>
+      <c t="s" s="9" r="A202">
+        <v>728</v>
+      </c>
+      <c t="s" s="7" r="B202">
+        <v>729</v>
+      </c>
+      <c t="s" s="14" r="C202">
+        <v>730</v>
+      </c>
+      <c t="s" s="7" r="D202">
+        <v>731</v>
+      </c>
+      <c t="s" s="7" r="E202">
+        <v>732</v>
+      </c>
     </row>
     <row r="203">
-      <c t="s" s="9" r="A203">
-        <v>726</v>
-      </c>
+      <c s="9" r="A203"/>
       <c t="s" s="7" r="B203">
-        <v>727</v>
+        <v>733</v>
       </c>
       <c t="s" s="14" r="C203">
-        <v>728</v>
+        <v>734</v>
       </c>
       <c t="s" s="7" r="D203">
-        <v>729</v>
+        <v>734</v>
       </c>
       <c t="s" s="7" r="E203">
-        <v>730</v>
+        <v>735</v>
       </c>
     </row>
     <row r="204">
       <c s="9" r="A204"/>
-      <c t="s" s="7" r="B204">
-        <v>731</v>
-      </c>
-      <c t="s" s="14" r="C204">
-        <v>732</v>
-      </c>
-      <c t="s" s="7" r="D204">
-        <v>732</v>
-      </c>
-      <c t="s" s="7" r="E204">
-        <v>733</v>
-      </c>
+      <c s="12" r="B204"/>
+      <c s="15" r="C204"/>
+      <c s="12" r="D204"/>
+      <c s="12" r="E204"/>
     </row>
     <row r="205">
-      <c s="9" r="A205"/>
-      <c s="12" r="B205"/>
-      <c s="15" r="C205"/>
-      <c s="12" r="D205"/>
-      <c s="12" r="E205"/>
+      <c t="s" s="9" r="A205">
+        <v>736</v>
+      </c>
+      <c t="s" s="7" r="B205">
+        <v>737</v>
+      </c>
+      <c t="s" s="14" r="C205">
+        <v>738</v>
+      </c>
+      <c t="s" s="7" r="D205">
+        <v>739</v>
+      </c>
+      <c t="s" s="7" r="E205">
+        <v>740</v>
+      </c>
     </row>
     <row r="206">
-      <c t="s" s="9" r="A206">
-        <v>734</v>
-      </c>
+      <c s="9" r="A206"/>
       <c t="s" s="7" r="B206">
-        <v>735</v>
+        <v>741</v>
       </c>
       <c t="s" s="14" r="C206">
-        <v>736</v>
+        <v>742</v>
       </c>
       <c t="s" s="7" r="D206">
-        <v>737</v>
+        <v>743</v>
       </c>
       <c t="s" s="7" r="E206">
-        <v>738</v>
+        <v>744</v>
       </c>
     </row>
     <row r="207">
       <c s="9" r="A207"/>
       <c t="s" s="7" r="B207">
-        <v>739</v>
+        <v>745</v>
       </c>
       <c t="s" s="14" r="C207">
-        <v>740</v>
+        <v>746</v>
       </c>
       <c t="s" s="7" r="D207">
-        <v>741</v>
+        <v>747</v>
       </c>
       <c t="s" s="7" r="E207">
-        <v>742</v>
+        <v>748</v>
       </c>
     </row>
     <row r="208">
       <c s="9" r="A208"/>
       <c t="s" s="7" r="B208">
-        <v>743</v>
+        <v>749</v>
       </c>
       <c t="s" s="14" r="C208">
-        <v>744</v>
+        <v>750</v>
       </c>
       <c t="s" s="7" r="D208">
-        <v>745</v>
+        <v>751</v>
       </c>
       <c t="s" s="7" r="E208">
-        <v>746</v>
+        <v>752</v>
       </c>
     </row>
     <row r="209">
       <c s="9" r="A209"/>
-      <c t="s" s="7" r="B209">
-        <v>747</v>
-      </c>
-      <c t="s" s="14" r="C209">
-        <v>748</v>
-      </c>
-      <c t="s" s="7" r="D209">
-        <v>749</v>
-      </c>
-      <c t="s" s="7" r="E209">
-        <v>750</v>
-      </c>
+      <c s="17" r="B209"/>
+      <c s="30" r="C209"/>
+      <c s="17" r="D209"/>
+      <c s="17" r="E209"/>
     </row>
     <row r="210">
-      <c s="9" r="A210"/>
-      <c s="17" r="B210"/>
-      <c s="30" r="C210"/>
-      <c s="17" r="D210"/>
-      <c s="17" r="E210"/>
+      <c t="s" s="9" r="A210">
+        <v>753</v>
+      </c>
+      <c t="s" s="7" r="B210">
+        <v>754</v>
+      </c>
+      <c t="s" s="14" r="C210">
+        <v>755</v>
+      </c>
+      <c t="s" s="7" r="D210">
+        <v>756</v>
+      </c>
+      <c t="s" s="7" r="E210">
+        <v>757</v>
+      </c>
     </row>
     <row r="211">
-      <c t="s" s="9" r="A211">
-        <v>751</v>
-      </c>
+      <c s="9" r="A211"/>
       <c t="s" s="7" r="B211">
-        <v>752</v>
+        <v>758</v>
       </c>
       <c t="s" s="14" r="C211">
-        <v>753</v>
+        <v>759</v>
       </c>
       <c t="s" s="7" r="D211">
-        <v>754</v>
+        <v>760</v>
       </c>
       <c t="s" s="7" r="E211">
-        <v>755</v>
+        <v>761</v>
       </c>
     </row>
     <row r="212">
       <c s="9" r="A212"/>
-      <c t="s" s="7" r="B212">
-        <v>756</v>
-      </c>
-      <c t="s" s="14" r="C212">
-        <v>757</v>
-      </c>
-      <c t="s" s="7" r="D212">
-        <v>758</v>
-      </c>
-      <c t="s" s="7" r="E212">
-        <v>759</v>
-      </c>
+      <c s="17" r="B212"/>
+      <c s="30" r="C212"/>
+      <c s="17" r="D212"/>
+      <c s="17" r="E212"/>
     </row>
     <row r="213">
-      <c s="9" r="A213"/>
-      <c s="17" r="B213"/>
-      <c s="30" r="C213"/>
-      <c s="17" r="D213"/>
-      <c s="17" r="E213"/>
+      <c t="s" s="9" r="A213">
+        <v>762</v>
+      </c>
+      <c t="s" s="7" r="B213">
+        <v>763</v>
+      </c>
+      <c t="s" s="14" r="C213">
+        <v>764</v>
+      </c>
+      <c t="s" s="7" r="D213">
+        <v>765</v>
+      </c>
+      <c t="s" s="7" r="E213">
+        <v>766</v>
+      </c>
     </row>
     <row r="214">
-      <c t="s" s="9" r="A214">
-        <v>760</v>
-      </c>
-      <c t="s" s="7" r="B214">
-        <v>761</v>
-      </c>
-      <c t="s" s="14" r="C214">
-        <v>762</v>
-      </c>
-      <c t="s" s="7" r="D214">
-        <v>763</v>
-      </c>
-      <c t="s" s="7" r="E214">
-        <v>764</v>
-      </c>
+      <c s="9" r="A214"/>
+      <c s="17" r="B214"/>
+      <c s="8" r="C214"/>
+      <c s="17" r="D214"/>
+      <c s="17" r="E214"/>
     </row>
     <row r="215">
-      <c s="9" r="A215"/>
-      <c s="17" r="B215"/>
-      <c s="8" r="C215"/>
-      <c s="17" r="D215"/>
-      <c s="17" r="E215"/>
+      <c t="s" s="9" r="A215">
+        <v>767</v>
+      </c>
+      <c t="s" s="7" r="B215">
+        <v>768</v>
+      </c>
+      <c t="s" s="14" r="C215">
+        <v>769</v>
+      </c>
+      <c t="s" s="7" r="D215">
+        <v>770</v>
+      </c>
+      <c t="s" s="7" r="E215">
+        <v>771</v>
+      </c>
     </row>
     <row r="216">
-      <c t="s" s="9" r="A216">
-        <v>765</v>
-      </c>
+      <c s="9" r="A216"/>
       <c t="s" s="7" r="B216">
-        <v>766</v>
+        <v>772</v>
       </c>
       <c t="s" s="14" r="C216">
-        <v>767</v>
+        <v>773</v>
       </c>
       <c t="s" s="7" r="D216">
-        <v>768</v>
+        <v>774</v>
       </c>
       <c t="s" s="7" r="E216">
-        <v>769</v>
+        <v>775</v>
       </c>
     </row>
     <row r="217">
       <c s="9" r="A217"/>
       <c t="s" s="7" r="B217">
-        <v>770</v>
+        <v>776</v>
       </c>
       <c t="s" s="14" r="C217">
-        <v>771</v>
+        <v>777</v>
       </c>
       <c t="s" s="7" r="D217">
-        <v>772</v>
+        <v>778</v>
       </c>
       <c t="s" s="7" r="E217">
-        <v>773</v>
+        <v>779</v>
       </c>
     </row>
     <row r="218">
       <c s="9" r="A218"/>
       <c t="s" s="7" r="B218">
-        <v>774</v>
+        <v>780</v>
       </c>
       <c t="s" s="14" r="C218">
-        <v>775</v>
+        <v>781</v>
       </c>
       <c t="s" s="7" r="D218">
-        <v>776</v>
+        <v>782</v>
       </c>
       <c t="s" s="7" r="E218">
-        <v>777</v>
+        <v>783</v>
       </c>
     </row>
     <row r="219">
       <c s="9" r="A219"/>
       <c t="s" s="7" r="B219">
-        <v>778</v>
+        <v>784</v>
       </c>
       <c t="s" s="14" r="C219">
-        <v>779</v>
+        <v>785</v>
       </c>
       <c t="s" s="7" r="D219">
-        <v>780</v>
+        <v>786</v>
       </c>
       <c t="s" s="7" r="E219">
-        <v>781</v>
+        <v>787</v>
       </c>
     </row>
     <row r="220">
       <c s="9" r="A220"/>
       <c t="s" s="7" r="B220">
-        <v>782</v>
+        <v>788</v>
       </c>
       <c t="s" s="14" r="C220">
-        <v>783</v>
+        <v>789</v>
       </c>
       <c t="s" s="7" r="D220">
-        <v>784</v>
+        <v>790</v>
       </c>
       <c t="s" s="7" r="E220">
-        <v>785</v>
+        <v>791</v>
       </c>
     </row>
     <row r="221">
       <c s="9" r="A221"/>
       <c t="s" s="7" r="B221">
-        <v>786</v>
+        <v>792</v>
       </c>
       <c t="s" s="14" r="C221">
-        <v>787</v>
+        <v>793</v>
       </c>
       <c t="s" s="7" r="D221">
-        <v>788</v>
+        <v>794</v>
       </c>
       <c t="s" s="7" r="E221">
-        <v>789</v>
+        <v>795</v>
       </c>
     </row>
     <row r="222">
       <c s="9" r="A222"/>
       <c t="s" s="7" r="B222">
-        <v>790</v>
+        <v>796</v>
       </c>
       <c t="s" s="14" r="C222">
-        <v>791</v>
+        <v>797</v>
       </c>
       <c t="s" s="7" r="D222">
-        <v>792</v>
+        <v>798</v>
       </c>
       <c t="s" s="7" r="E222">
-        <v>793</v>
+        <v>799</v>
       </c>
     </row>
     <row r="223">
-      <c s="9" r="A223"/>
-      <c t="s" s="7" r="B223">
-        <v>794</v>
-      </c>
-      <c t="s" s="14" r="C223">
-        <v>795</v>
-      </c>
-      <c t="s" s="7" r="D223">
-        <v>796</v>
-      </c>
-      <c t="s" s="7" r="E223">
-        <v>797</v>
-      </c>
+      <c s="18" r="A223"/>
+      <c s="17" r="B223"/>
+      <c s="8" r="C223"/>
+      <c s="17" r="D223"/>
+      <c s="17" r="E223"/>
     </row>
     <row r="224">
-      <c s="18" r="A224"/>
-      <c s="17" r="B224"/>
-      <c s="8" r="C224"/>
-      <c s="17" r="D224"/>
-      <c s="17" r="E224"/>
+      <c t="s" s="9" r="A224">
+        <v>800</v>
+      </c>
+      <c t="s" s="7" r="B224">
+        <v>801</v>
+      </c>
+      <c t="s" s="7" r="C224">
+        <v>802</v>
+      </c>
+      <c t="s" s="7" r="D224">
+        <v>803</v>
+      </c>
+      <c t="s" s="7" r="E224">
+        <v>804</v>
+      </c>
     </row>
     <row r="225">
-      <c t="s" s="9" r="A225">
-        <v>798</v>
-      </c>
+      <c s="9" r="A225"/>
       <c t="s" s="7" r="B225">
-        <v>799</v>
-      </c>
-      <c t="s" s="7" r="C225">
-        <v>800</v>
+        <v>805</v>
+      </c>
+      <c t="s" s="14" r="C225">
+        <v>806</v>
       </c>
       <c t="s" s="7" r="D225">
-        <v>801</v>
+        <v>807</v>
       </c>
       <c t="s" s="7" r="E225">
-        <v>802</v>
+        <v>808</v>
       </c>
     </row>
     <row r="226">
       <c s="9" r="A226"/>
       <c t="s" s="7" r="B226">
-        <v>803</v>
+        <v>809</v>
       </c>
       <c t="s" s="14" r="C226">
-        <v>804</v>
+        <v>810</v>
       </c>
       <c t="s" s="7" r="D226">
-        <v>805</v>
+        <v>811</v>
       </c>
       <c t="s" s="7" r="E226">
-        <v>806</v>
+        <v>812</v>
       </c>
     </row>
     <row r="227">
       <c s="9" r="A227"/>
       <c t="s" s="7" r="B227">
-        <v>807</v>
+        <v>813</v>
       </c>
       <c t="s" s="14" r="C227">
-        <v>808</v>
+        <v>814</v>
       </c>
       <c t="s" s="7" r="D227">
-        <v>809</v>
+        <v>815</v>
       </c>
       <c t="s" s="7" r="E227">
-        <v>810</v>
+        <v>816</v>
       </c>
     </row>
     <row r="228">
       <c s="9" r="A228"/>
       <c t="s" s="7" r="B228">
-        <v>811</v>
+        <v>817</v>
       </c>
       <c t="s" s="14" r="C228">
-        <v>812</v>
+        <v>542</v>
       </c>
       <c t="s" s="7" r="D228">
-        <v>813</v>
+        <v>132</v>
       </c>
       <c t="s" s="7" r="E228">
-        <v>814</v>
+        <v>544</v>
       </c>
     </row>
     <row r="229">
       <c s="9" r="A229"/>
       <c t="s" s="7" r="B229">
-        <v>815</v>
+        <v>818</v>
       </c>
       <c t="s" s="14" r="C229">
-        <v>540</v>
+        <v>819</v>
       </c>
       <c t="s" s="7" r="D229">
-        <v>130</v>
+        <v>820</v>
       </c>
       <c t="s" s="7" r="E229">
-        <v>542</v>
+        <v>821</v>
       </c>
     </row>
     <row r="230">
-      <c s="9" r="A230"/>
-      <c t="s" s="7" r="B230">
-        <v>816</v>
-      </c>
-      <c t="s" s="14" r="C230">
-        <v>817</v>
-      </c>
-      <c t="s" s="7" r="D230">
-        <v>818</v>
-      </c>
-      <c t="s" s="7" r="E230">
-        <v>819</v>
-      </c>
+      <c s="18" r="A230"/>
+      <c s="17" r="B230"/>
+      <c s="8" r="C230"/>
+      <c s="17" r="D230"/>
+      <c s="17" r="E230"/>
     </row>
     <row r="231">
-      <c s="18" r="A231"/>
-      <c s="17" r="B231"/>
-      <c s="8" r="C231"/>
-      <c s="17" r="D231"/>
-      <c s="17" r="E231"/>
+      <c t="s" s="9" r="A231">
+        <v>822</v>
+      </c>
+      <c t="s" s="7" r="B231">
+        <v>823</v>
+      </c>
+      <c t="s" s="14" r="C231">
+        <v>824</v>
+      </c>
+      <c t="s" s="7" r="D231">
+        <v>825</v>
+      </c>
+      <c t="s" s="7" r="E231">
+        <v>826</v>
+      </c>
     </row>
     <row r="232">
-      <c t="s" s="9" r="A232">
-        <v>820</v>
-      </c>
+      <c s="9" r="A232"/>
       <c t="s" s="7" r="B232">
-        <v>821</v>
+        <v>827</v>
       </c>
       <c t="s" s="14" r="C232">
-        <v>822</v>
+        <v>828</v>
       </c>
       <c t="s" s="7" r="D232">
-        <v>823</v>
+        <v>829</v>
       </c>
       <c t="s" s="7" r="E232">
-        <v>824</v>
+        <v>830</v>
       </c>
     </row>
     <row r="233">
       <c s="9" r="A233"/>
       <c t="s" s="7" r="B233">
-        <v>825</v>
+        <v>831</v>
       </c>
       <c t="s" s="14" r="C233">
-        <v>826</v>
+        <v>832</v>
       </c>
       <c t="s" s="7" r="D233">
-        <v>827</v>
+        <v>833</v>
       </c>
       <c t="s" s="7" r="E233">
-        <v>828</v>
+        <v>834</v>
       </c>
     </row>
     <row r="234">
       <c s="9" r="A234"/>
       <c t="s" s="7" r="B234">
-        <v>829</v>
+        <v>835</v>
       </c>
       <c t="s" s="14" r="C234">
-        <v>830</v>
+        <v>836</v>
       </c>
       <c t="s" s="7" r="D234">
-        <v>831</v>
+        <v>837</v>
       </c>
       <c t="s" s="7" r="E234">
-        <v>832</v>
+        <v>837</v>
       </c>
     </row>
     <row r="235">
       <c s="9" r="A235"/>
       <c t="s" s="7" r="B235">
-        <v>833</v>
+        <v>838</v>
       </c>
       <c t="s" s="14" r="C235">
-        <v>834</v>
+        <v>839</v>
       </c>
       <c t="s" s="7" r="D235">
-        <v>835</v>
+        <v>840</v>
       </c>
       <c t="s" s="7" r="E235">
-        <v>835</v>
+        <v>841</v>
       </c>
     </row>
     <row r="236">
       <c s="9" r="A236"/>
       <c t="s" s="7" r="B236">
-        <v>836</v>
+        <v>842</v>
       </c>
       <c t="s" s="14" r="C236">
-        <v>837</v>
+        <v>843</v>
       </c>
       <c t="s" s="7" r="D236">
-        <v>838</v>
+        <v>844</v>
       </c>
       <c t="s" s="7" r="E236">
-        <v>839</v>
+        <v>845</v>
       </c>
     </row>
     <row r="237">
       <c s="9" r="A237"/>
       <c t="s" s="7" r="B237">
-        <v>840</v>
+        <v>846</v>
       </c>
       <c t="s" s="14" r="C237">
-        <v>841</v>
+        <v>847</v>
       </c>
       <c t="s" s="7" r="D237">
-        <v>842</v>
+        <v>848</v>
       </c>
       <c t="s" s="7" r="E237">
-        <v>843</v>
+        <v>849</v>
       </c>
     </row>
     <row r="238">
       <c s="9" r="A238"/>
       <c t="s" s="7" r="B238">
-        <v>844</v>
+        <v>850</v>
       </c>
       <c t="s" s="14" r="C238">
-        <v>845</v>
+        <v>851</v>
       </c>
       <c t="s" s="7" r="D238">
-        <v>846</v>
+        <v>852</v>
       </c>
       <c t="s" s="7" r="E238">
-        <v>847</v>
+        <v>853</v>
       </c>
     </row>
     <row r="239">
       <c s="9" r="A239"/>
       <c t="s" s="7" r="B239">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c t="s" s="14" r="C239">
-        <v>849</v>
+        <v>855</v>
       </c>
       <c t="s" s="7" r="D239">
-        <v>850</v>
+        <v>856</v>
       </c>
       <c t="s" s="7" r="E239">
-        <v>851</v>
+        <v>857</v>
       </c>
     </row>
     <row r="240">
       <c s="9" r="A240"/>
       <c t="s" s="7" r="B240">
-        <v>852</v>
+        <v>858</v>
       </c>
       <c t="s" s="14" r="C240">
-        <v>853</v>
+        <v>859</v>
       </c>
       <c t="s" s="7" r="D240">
-        <v>854</v>
+        <v>860</v>
       </c>
       <c t="s" s="7" r="E240">
-        <v>855</v>
+        <v>861</v>
       </c>
     </row>
     <row r="241">
       <c s="9" r="A241"/>
       <c t="s" s="7" r="B241">
-        <v>856</v>
+        <v>862</v>
       </c>
       <c t="s" s="14" r="C241">
-        <v>857</v>
+        <v>863</v>
       </c>
       <c t="s" s="7" r="D241">
-        <v>858</v>
+        <v>864</v>
       </c>
       <c t="s" s="7" r="E241">
-        <v>859</v>
+        <v>865</v>
       </c>
     </row>
     <row r="242">
       <c s="9" r="A242"/>
       <c t="s" s="7" r="B242">
-        <v>860</v>
+        <v>866</v>
       </c>
       <c t="s" s="14" r="C242">
-        <v>861</v>
+        <v>867</v>
       </c>
       <c t="s" s="7" r="D242">
-        <v>862</v>
+        <v>868</v>
       </c>
       <c t="s" s="7" r="E242">
-        <v>863</v>
+        <v>869</v>
       </c>
     </row>
     <row r="243">
       <c s="9" r="A243"/>
       <c t="s" s="7" r="B243">
-        <v>864</v>
+        <v>870</v>
       </c>
       <c t="s" s="14" r="C243">
-        <v>865</v>
+        <v>871</v>
       </c>
       <c t="s" s="7" r="D243">
-        <v>866</v>
+        <v>871</v>
       </c>
       <c t="s" s="7" r="E243">
-        <v>867</v>
+        <v>871</v>
       </c>
     </row>
     <row r="244">
       <c s="9" r="A244"/>
       <c t="s" s="7" r="B244">
-        <v>868</v>
+        <v>872</v>
       </c>
       <c t="s" s="14" r="C244">
-        <v>869</v>
+        <v>873</v>
       </c>
       <c t="s" s="7" r="D244">
-        <v>869</v>
+        <v>874</v>
       </c>
       <c t="s" s="7" r="E244">
-        <v>869</v>
+        <v>875</v>
       </c>
     </row>
     <row r="245">
       <c s="9" r="A245"/>
       <c t="s" s="7" r="B245">
-        <v>870</v>
+        <v>876</v>
       </c>
       <c t="s" s="14" r="C245">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c t="s" s="7" r="D245">
-        <v>872</v>
+        <v>878</v>
       </c>
       <c t="s" s="7" r="E245">
-        <v>873</v>
+        <v>879</v>
       </c>
     </row>
     <row r="246">
       <c s="9" r="A246"/>
       <c t="s" s="7" r="B246">
-        <v>874</v>
+        <v>880</v>
       </c>
       <c t="s" s="14" r="C246">
-        <v>875</v>
+        <v>881</v>
       </c>
       <c t="s" s="7" r="D246">
-        <v>876</v>
+        <v>882</v>
       </c>
       <c t="s" s="7" r="E246">
-        <v>877</v>
+        <v>883</v>
       </c>
     </row>
     <row r="247">
       <c s="9" r="A247"/>
       <c t="s" s="7" r="B247">
-        <v>878</v>
+        <v>884</v>
       </c>
       <c t="s" s="14" r="C247">
-        <v>879</v>
+        <v>885</v>
       </c>
       <c t="s" s="7" r="D247">
-        <v>880</v>
+        <v>886</v>
       </c>
       <c t="s" s="7" r="E247">
-        <v>881</v>
+        <v>887</v>
       </c>
     </row>
     <row r="248">
       <c s="9" r="A248"/>
       <c t="s" s="7" r="B248">
-        <v>882</v>
+        <v>888</v>
       </c>
       <c t="s" s="14" r="C248">
-        <v>883</v>
+        <v>889</v>
       </c>
       <c t="s" s="7" r="D248">
-        <v>884</v>
+        <v>890</v>
       </c>
       <c t="s" s="7" r="E248">
-        <v>885</v>
+        <v>891</v>
       </c>
     </row>
     <row r="249">
       <c s="9" r="A249"/>
       <c t="s" s="7" r="B249">
-        <v>886</v>
+        <v>892</v>
       </c>
       <c t="s" s="14" r="C249">
-        <v>887</v>
+        <v>893</v>
       </c>
       <c t="s" s="7" r="D249">
-        <v>888</v>
+        <v>894</v>
       </c>
       <c t="s" s="7" r="E249">
-        <v>889</v>
+        <v>895</v>
       </c>
     </row>
     <row r="250">
       <c s="9" r="A250"/>
       <c t="s" s="7" r="B250">
-        <v>890</v>
+        <v>896</v>
       </c>
       <c t="s" s="14" r="C250">
-        <v>891</v>
+        <v>897</v>
       </c>
       <c t="s" s="7" r="D250">
-        <v>892</v>
+        <v>898</v>
       </c>
       <c t="s" s="7" r="E250">
-        <v>893</v>
+        <v>899</v>
       </c>
     </row>
     <row r="251">
       <c s="9" r="A251"/>
-      <c t="s" s="7" r="B251">
-        <v>894</v>
-      </c>
-      <c t="s" s="14" r="C251">
-        <v>895</v>
-      </c>
-      <c t="s" s="7" r="D251">
-        <v>896</v>
-      </c>
-      <c t="s" s="7" r="E251">
-        <v>897</v>
-      </c>
+      <c s="17" r="B251"/>
+      <c s="8" r="C251"/>
+      <c s="17" r="D251"/>
+      <c s="17" r="E251"/>
     </row>
     <row r="252">
-      <c s="9" r="A252"/>
-      <c s="17" r="B252"/>
-      <c s="8" r="C252"/>
-      <c s="17" r="D252"/>
-      <c s="17" r="E252"/>
+      <c t="s" s="9" r="A252">
+        <v>900</v>
+      </c>
+      <c t="s" s="7" r="B252">
+        <v>901</v>
+      </c>
+      <c t="s" s="14" r="C252">
+        <v>902</v>
+      </c>
+      <c t="s" s="7" r="D252">
+        <v>903</v>
+      </c>
+      <c t="s" s="7" r="E252">
+        <v>904</v>
+      </c>
     </row>
     <row r="253">
-      <c t="s" s="9" r="A253">
-        <v>898</v>
-      </c>
+      <c s="9" r="A253"/>
       <c t="s" s="7" r="B253">
-        <v>899</v>
+        <v>905</v>
       </c>
       <c t="s" s="14" r="C253">
-        <v>900</v>
+        <v>906</v>
       </c>
       <c t="s" s="7" r="D253">
-        <v>901</v>
+        <v>907</v>
       </c>
       <c t="s" s="7" r="E253">
-        <v>902</v>
+        <v>908</v>
       </c>
     </row>
     <row r="254">
       <c s="9" r="A254"/>
       <c t="s" s="7" r="B254">
-        <v>903</v>
+        <v>909</v>
       </c>
       <c t="s" s="14" r="C254">
-        <v>904</v>
+        <v>910</v>
       </c>
       <c t="s" s="7" r="D254">
-        <v>905</v>
+        <v>911</v>
       </c>
       <c t="s" s="7" r="E254">
-        <v>906</v>
+        <v>912</v>
       </c>
     </row>
     <row r="255">
       <c s="9" r="A255"/>
       <c t="s" s="7" r="B255">
-        <v>907</v>
+        <v>913</v>
       </c>
       <c t="s" s="14" r="C255">
-        <v>908</v>
+        <v>914</v>
       </c>
       <c t="s" s="7" r="D255">
-        <v>909</v>
+        <v>915</v>
       </c>
       <c t="s" s="7" r="E255">
-        <v>910</v>
+        <v>916</v>
       </c>
     </row>
     <row r="256">
       <c s="9" r="A256"/>
       <c t="s" s="7" r="B256">
-        <v>911</v>
+        <v>917</v>
       </c>
       <c t="s" s="14" r="C256">
-        <v>912</v>
-      </c>
-      <c t="s" s="7" r="D256">
-        <v>913</v>
-      </c>
-      <c t="s" s="7" r="E256">
-        <v>914</v>
+        <v>917</v>
+      </c>
+      <c t="s" s="19" r="D256">
+        <v>918</v>
+      </c>
+      <c t="s" s="19" r="E256">
+        <v>919</v>
       </c>
     </row>
     <row r="257">
       <c s="9" r="A257"/>
       <c t="s" s="7" r="B257">
-        <v>915</v>
+        <v>920</v>
       </c>
       <c t="s" s="14" r="C257">
-        <v>915</v>
-      </c>
-      <c t="s" s="19" r="D257">
-        <v>916</v>
-      </c>
-      <c t="s" s="19" r="E257">
-        <v>917</v>
+        <v>921</v>
+      </c>
+      <c t="s" s="7" r="D257">
+        <v>922</v>
+      </c>
+      <c t="s" s="7" r="E257">
+        <v>923</v>
       </c>
     </row>
     <row r="258">
       <c s="9" r="A258"/>
       <c t="s" s="7" r="B258">
-        <v>918</v>
+        <v>924</v>
       </c>
       <c t="s" s="14" r="C258">
-        <v>919</v>
+        <v>925</v>
       </c>
       <c t="s" s="7" r="D258">
-        <v>920</v>
+        <v>926</v>
       </c>
       <c t="s" s="7" r="E258">
-        <v>921</v>
+        <v>927</v>
       </c>
     </row>
     <row r="259">
-      <c s="9" r="A259"/>
-      <c t="s" s="7" r="B259">
-        <v>922</v>
-      </c>
+      <c t="s" s="17" r="A259">
+        <v>928</v>
+      </c>
+      <c s="27" r="B259"/>
       <c t="s" s="14" r="C259">
-        <v>923</v>
-      </c>
-      <c t="s" s="7" r="D259">
-        <v>924</v>
-      </c>
-      <c t="s" s="7" r="E259">
-        <v>925</v>
+        <v>929</v>
+      </c>
+      <c t="s" s="19" r="D259">
+        <v>930</v>
+      </c>
+      <c t="s" s="19" r="E259">
+        <v>931</v>
       </c>
     </row>
     <row r="260">
-      <c t="s" s="17" r="A260">
-        <v>926</v>
-      </c>
-      <c s="27" r="B260"/>
-      <c t="s" s="14" r="C260">
-        <v>927</v>
-      </c>
-      <c t="s" s="19" r="D260">
-        <v>928</v>
-      </c>
-      <c t="s" s="19" r="E260">
-        <v>929</v>
-      </c>
+      <c s="18" r="A260"/>
+      <c s="17" r="B260"/>
+      <c s="8" r="C260"/>
+      <c s="17" r="D260"/>
+      <c s="17" r="E260"/>
     </row>
     <row r="261">
-      <c s="18" r="A261"/>
-      <c s="17" r="B261"/>
-      <c s="8" r="C261"/>
-      <c s="17" r="D261"/>
-      <c s="17" r="E261"/>
+      <c t="s" s="18" r="A261">
+        <v>932</v>
+      </c>
+      <c t="s" s="7" r="B261">
+        <v>933</v>
+      </c>
+      <c t="s" s="7" r="C261">
+        <v>934</v>
+      </c>
+      <c t="s" s="7" r="D261">
+        <v>935</v>
+      </c>
+      <c t="s" s="7" r="E261">
+        <v>936</v>
+      </c>
     </row>
     <row r="262">
-      <c t="s" s="18" r="A262">
-        <v>930</v>
-      </c>
+      <c s="15" r="A262"/>
       <c t="s" s="7" r="B262">
-        <v>931</v>
-      </c>
-      <c t="s" s="7" r="C262">
-        <v>932</v>
+        <v>937</v>
+      </c>
+      <c t="s" s="14" r="C262">
+        <v>938</v>
       </c>
       <c t="s" s="7" r="D262">
-        <v>933</v>
+        <v>939</v>
       </c>
       <c t="s" s="7" r="E262">
-        <v>934</v>
+        <v>940</v>
       </c>
     </row>
     <row r="263">
       <c s="15" r="A263"/>
       <c t="s" s="7" r="B263">
-        <v>935</v>
-      </c>
-      <c t="s" s="14" r="C263">
-        <v>936</v>
+        <v>941</v>
+      </c>
+      <c t="s" s="7" r="C263">
+        <v>942</v>
       </c>
       <c t="s" s="7" r="D263">
-        <v>937</v>
+        <v>943</v>
       </c>
       <c t="s" s="7" r="E263">
-        <v>938</v>
+        <v>944</v>
       </c>
     </row>
     <row r="264">
-      <c s="15" r="A264"/>
+      <c s="18" r="A264"/>
       <c t="s" s="7" r="B264">
-        <v>939</v>
-      </c>
-      <c t="s" s="7" r="C264">
-        <v>940</v>
+        <v>945</v>
+      </c>
+      <c t="s" s="14" r="C264">
+        <v>946</v>
       </c>
       <c t="s" s="7" r="D264">
-        <v>941</v>
+        <v>947</v>
       </c>
       <c t="s" s="7" r="E264">
-        <v>942</v>
+        <v>948</v>
       </c>
     </row>
     <row r="265">
       <c s="18" r="A265"/>
       <c t="s" s="7" r="B265">
-        <v>943</v>
-      </c>
-      <c t="s" s="14" r="C265">
-        <v>944</v>
+        <v>949</v>
+      </c>
+      <c t="s" s="7" r="C265">
+        <v>950</v>
       </c>
       <c t="s" s="7" r="D265">
-        <v>945</v>
+        <v>951</v>
       </c>
       <c t="s" s="7" r="E265">
-        <v>946</v>
+        <v>952</v>
       </c>
     </row>
     <row r="266">
       <c s="18" r="A266"/>
       <c t="s" s="7" r="B266">
-        <v>947</v>
-      </c>
-      <c t="s" s="7" r="C266">
-        <v>948</v>
+        <v>953</v>
+      </c>
+      <c t="s" s="14" r="C266">
+        <v>954</v>
       </c>
       <c t="s" s="7" r="D266">
-        <v>949</v>
+        <v>955</v>
       </c>
       <c t="s" s="7" r="E266">
-        <v>950</v>
+        <v>956</v>
       </c>
     </row>
     <row r="267">
       <c s="18" r="A267"/>
       <c t="s" s="7" r="B267">
-        <v>951</v>
-      </c>
-      <c t="s" s="14" r="C267">
-        <v>952</v>
+        <v>957</v>
+      </c>
+      <c t="s" s="7" r="C267">
+        <v>958</v>
       </c>
       <c t="s" s="7" r="D267">
-        <v>953</v>
+        <v>959</v>
       </c>
       <c t="s" s="7" r="E267">
-        <v>954</v>
+        <v>960</v>
       </c>
     </row>
     <row r="268">
       <c s="18" r="A268"/>
       <c t="s" s="7" r="B268">
-        <v>955</v>
-      </c>
-      <c t="s" s="7" r="C268">
-        <v>956</v>
+        <v>961</v>
+      </c>
+      <c t="s" s="14" r="C268">
+        <v>962</v>
       </c>
       <c t="s" s="7" r="D268">
-        <v>957</v>
+        <v>963</v>
       </c>
       <c t="s" s="7" r="E268">
-        <v>958</v>
+        <v>964</v>
       </c>
     </row>
     <row r="269">
       <c s="18" r="A269"/>
       <c t="s" s="7" r="B269">
-        <v>959</v>
-      </c>
-      <c t="s" s="14" r="C269">
-        <v>960</v>
+        <v>965</v>
+      </c>
+      <c t="s" s="7" r="C269">
+        <v>966</v>
       </c>
       <c t="s" s="7" r="D269">
-        <v>961</v>
+        <v>967</v>
       </c>
       <c t="s" s="7" r="E269">
-        <v>962</v>
+        <v>968</v>
       </c>
     </row>
     <row r="270">
       <c s="18" r="A270"/>
       <c t="s" s="7" r="B270">
-        <v>963</v>
-      </c>
-      <c t="s" s="7" r="C270">
-        <v>964</v>
+        <v>969</v>
+      </c>
+      <c t="s" s="14" r="C270">
+        <v>970</v>
       </c>
       <c t="s" s="7" r="D270">
-        <v>965</v>
+        <v>971</v>
       </c>
       <c t="s" s="7" r="E270">
-        <v>966</v>
+        <v>972</v>
       </c>
     </row>
     <row r="271">
       <c s="18" r="A271"/>
       <c t="s" s="7" r="B271">
-        <v>967</v>
-      </c>
-      <c t="s" s="14" r="C271">
-        <v>968</v>
+        <v>973</v>
+      </c>
+      <c t="s" s="7" r="C271">
+        <v>974</v>
       </c>
       <c t="s" s="7" r="D271">
-        <v>969</v>
+        <v>975</v>
       </c>
       <c t="s" s="7" r="E271">
-        <v>970</v>
+        <v>976</v>
       </c>
     </row>
     <row r="272">
       <c s="18" r="A272"/>
       <c t="s" s="7" r="B272">
+        <v>977</v>
+      </c>
+      <c t="s" s="14" r="C272">
+        <v>970</v>
+      </c>
+      <c t="s" s="7" r="D272">
         <v>971</v>
       </c>
-      <c t="s" s="7" r="C272">
+      <c t="s" s="7" r="E272">
         <v>972</v>
-      </c>
-      <c t="s" s="7" r="D272">
-        <v>973</v>
-      </c>
-      <c t="s" s="7" r="E272">
-        <v>974</v>
       </c>
     </row>
     <row r="273">
       <c s="18" r="A273"/>
       <c t="s" s="7" r="B273">
-        <v>975</v>
+        <v>978</v>
       </c>
       <c t="s" s="14" r="C273">
-        <v>968</v>
+        <v>979</v>
       </c>
       <c t="s" s="7" r="D273">
-        <v>969</v>
+        <v>980</v>
       </c>
       <c t="s" s="7" r="E273">
-        <v>970</v>
+        <v>981</v>
       </c>
     </row>
     <row r="274">
       <c s="18" r="A274"/>
       <c t="s" s="7" r="B274">
-        <v>976</v>
+        <v>982</v>
       </c>
       <c t="s" s="14" r="C274">
-        <v>977</v>
+        <v>983</v>
       </c>
       <c t="s" s="7" r="D274">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c t="s" s="7" r="E274">
-        <v>979</v>
+        <v>985</v>
       </c>
     </row>
     <row r="275">
       <c s="18" r="A275"/>
       <c t="s" s="7" r="B275">
-        <v>980</v>
-      </c>
-      <c t="s" s="14" r="C275">
-        <v>981</v>
+        <v>986</v>
+      </c>
+      <c t="s" s="7" r="C275">
+        <v>987</v>
       </c>
       <c t="s" s="7" r="D275">
-        <v>982</v>
+        <v>988</v>
       </c>
       <c t="s" s="7" r="E275">
-        <v>983</v>
+        <v>989</v>
       </c>
     </row>
     <row r="276">
       <c s="18" r="A276"/>
       <c t="s" s="7" r="B276">
-        <v>984</v>
-      </c>
-      <c t="s" s="7" r="C276">
-        <v>985</v>
+        <v>990</v>
+      </c>
+      <c t="s" s="14" r="C276">
+        <v>991</v>
       </c>
       <c t="s" s="7" r="D276">
-        <v>986</v>
+        <v>992</v>
       </c>
       <c t="s" s="7" r="E276">
-        <v>987</v>
+        <v>993</v>
       </c>
     </row>
     <row r="277">
-      <c s="18" r="A277"/>
+      <c s="9" r="A277"/>
       <c t="s" s="7" r="B277">
-        <v>988</v>
+        <v>994</v>
       </c>
       <c t="s" s="14" r="C277">
-        <v>989</v>
+        <v>995</v>
       </c>
       <c t="s" s="7" r="D277">
-        <v>990</v>
+        <v>996</v>
       </c>
       <c t="s" s="7" r="E277">
-        <v>991</v>
+        <v>997</v>
       </c>
     </row>
     <row r="278">
-      <c s="9" r="A278"/>
-      <c t="s" s="7" r="B278">
-        <v>992</v>
+      <c t="s" s="9" r="A278">
+        <v>998</v>
+      </c>
+      <c t="s" s="14" r="B278">
+        <v>999</v>
       </c>
       <c t="s" s="14" r="C278">
-        <v>993</v>
-      </c>
-      <c t="s" s="7" r="D278">
-        <v>994</v>
+        <v>1000</v>
+      </c>
+      <c t="s" s="19" r="D278">
+        <v>1001</v>
       </c>
       <c t="s" s="7" r="E278">
-        <v>995</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="279">
-      <c t="s" s="9" r="A279">
-        <v>996</v>
-      </c>
+      <c s="9" r="A279"/>
       <c t="s" s="14" r="B279">
-        <v>997</v>
+        <v>1003</v>
       </c>
       <c t="s" s="14" r="C279">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c t="s" s="19" r="D279">
-        <v>999</v>
+        <v>1005</v>
       </c>
       <c t="s" s="7" r="E279">
-        <v>1000</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="280">
       <c s="9" r="A280"/>
-      <c t="s" s="14" r="B280">
-        <v>1001</v>
-      </c>
-      <c t="s" s="14" r="C280">
-        <v>1002</v>
-      </c>
-      <c t="s" s="19" r="D280">
-        <v>1003</v>
-      </c>
-      <c t="s" s="7" r="E280">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="281">
-      <c s="9" r="A281"/>
-      <c s="8" r="C281"/>
-      <c s="17" r="D281"/>
-      <c s="17" r="E281"/>
+      <c s="8" r="C280"/>
+      <c s="17" r="D280"/>
+      <c s="17" r="E280"/>
     </row>
   </sheetData>
 </worksheet>
@@ -7674,17 +7677,17 @@
   <sheetData>
     <row customHeight="1" r="1" ht="112.5">
       <c t="s" s="3" r="A1">
-        <v>1005</v>
+        <v>1007</v>
       </c>
     </row>
     <row customHeight="1" r="2" ht="112.5">
       <c t="s" s="4" r="A2">
-        <v>1006</v>
+        <v>1008</v>
       </c>
     </row>
     <row customHeight="1" r="3" ht="112.5">
       <c t="s" s="10" r="A3">
-        <v>1007</v>
+        <v>1009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EWD-22796 - Connect/Disconnect LO localization; EWD-22802 - Objectives list filter localization
Former-commit-id: a58e8ebcb9016683ddb4dae47d57eb7f7955db03
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="1010">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="1039">
   <si>
     <t>d</t>
   </si>
@@ -807,6 +807,93 @@
   </si>
   <si>
     <t>Titel des Lernziels hier eingeben</t>
+  </si>
+  <si>
+    <t>filter</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>showAllConnectedLearningObjectives</t>
+  </si>
+  <si>
+    <t>show all connected learning objectives</t>
+  </si>
+  <si>
+    <t>Alle gekoppelde leerdoelen tonen</t>
+  </si>
+  <si>
+    <t>Alle verbundenen Lernziele anzeigen</t>
+  </si>
+  <si>
+    <t>show available learning objectives</t>
+  </si>
+  <si>
+    <t>Beschikbare leerdoelen tonen</t>
+  </si>
+  <si>
+    <t>Verfügbare Lernziele anzeigen</t>
+  </si>
+  <si>
+    <t>showOtherLearningObjectives</t>
+  </si>
+  <si>
+    <t>show other learning objectives</t>
+  </si>
+  <si>
+    <t>Andere leerdoelen tonen</t>
+  </si>
+  <si>
+    <t>Andere Lernziele anzeigen</t>
+  </si>
+  <si>
+    <t>createAndConnectLearningObjective</t>
+  </si>
+  <si>
+    <t>Create and connect learning objective</t>
+  </si>
+  <si>
+    <t>Leerdoel maken en koppelen</t>
+  </si>
+  <si>
+    <t>Lernziel erstellen und verbinden</t>
+  </si>
+  <si>
+    <t>connectSelected</t>
+  </si>
+  <si>
+    <t>Connect selected</t>
+  </si>
+  <si>
+    <t>Selectie koppelen</t>
+  </si>
+  <si>
+    <t>Auswahl verbinden</t>
+  </si>
+  <si>
+    <t>disconnectSelected</t>
+  </si>
+  <si>
+    <t>Disconnect selected</t>
+  </si>
+  <si>
+    <t>Selectie loskoppelen</t>
+  </si>
+  <si>
+    <t>Verbindung der Auswahl lösen</t>
+  </si>
+  <si>
+    <t>noLearningObjectivesToConnect</t>
+  </si>
+  <si>
+    <t>There are no learning objectives to connect</t>
+  </si>
+  <si>
+    <t>Er zijn geen leerdoelen om te koppelen</t>
+  </si>
+  <si>
+    <t>Es sind keine Lernziele zum Verbinden vorhanden</t>
   </si>
   <si>
     <t>CreateExperience</t>
@@ -3436,12 +3523,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00FF00"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -3485,6 +3566,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3572,38 +3659,38 @@
     <xf applyAlignment="1" fillId="20" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="18" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="21" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
-      <alignment vertical="center" horizontal="general" wrapText="1"/>
-    </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="19">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="20">
       <alignment vertical="bottom" horizontal="right"/>
     </xf>
-    <xf applyAlignment="1" fillId="22" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+    <xf applyAlignment="1" fillId="21" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="23" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="21" applyFill="1">
+    <xf applyAlignment="1" fillId="22" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="21" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="24" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="22" applyFill="1">
+    <xf applyAlignment="1" fillId="23" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="22" applyFill="1">
+      <alignment vertical="center" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="24" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="25" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="26" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
-      <alignment vertical="center" horizontal="general" wrapText="1"/>
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="27" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" fillId="28" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
     <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="23"/>
-    <xf applyAlignment="1" fillId="29" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="24" applyFill="1">
+    <xf applyAlignment="1" fillId="28" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="24" applyFill="1">
+      <alignment vertical="center" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="29" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3631,19 +3718,19 @@
   </cols>
   <sheetData>
     <row s="5" customFormat="1" r="1">
-      <c t="s" s="28" r="A1">
+      <c t="s" s="27" r="A1">
         <v>0</v>
       </c>
-      <c t="s" s="28" r="B1">
+      <c t="s" s="27" r="B1">
         <v>1</v>
       </c>
-      <c t="s" s="28" r="C1">
+      <c t="s" s="27" r="C1">
         <v>2</v>
       </c>
-      <c t="s" s="28" r="D1">
+      <c t="s" s="27" r="D1">
         <v>3</v>
       </c>
-      <c t="s" s="25" r="E1">
+      <c t="s" s="24" r="E1">
         <v>4</v>
       </c>
     </row>
@@ -4539,7 +4626,7 @@
     </row>
     <row r="62">
       <c s="12" r="A62"/>
-      <c t="s" s="27" r="B62">
+      <c t="s" s="26" r="B62">
         <v>235</v>
       </c>
       <c t="s" s="7" r="C62">
@@ -4554,7 +4641,7 @@
     </row>
     <row r="63">
       <c s="12" r="A63"/>
-      <c t="s" s="27" r="B63">
+      <c t="s" s="26" r="B63">
         <v>239</v>
       </c>
       <c t="s" s="7" r="C63">
@@ -4569,16 +4656,16 @@
     </row>
     <row r="64">
       <c s="12" r="A64"/>
-      <c t="s" s="27" r="B64">
+      <c t="s" s="26" r="B64">
         <v>243</v>
       </c>
       <c t="s" s="7" r="C64">
         <v>244</v>
       </c>
-      <c t="s" s="27" r="D64">
+      <c t="s" s="26" r="D64">
         <v>245</v>
       </c>
-      <c t="s" s="27" r="E64">
+      <c t="s" s="26" r="E64">
         <v>246</v>
       </c>
     </row>
@@ -4599,16 +4686,16 @@
     </row>
     <row r="66">
       <c s="12" r="A66"/>
-      <c t="s" s="27" r="B66">
+      <c t="s" s="26" r="B66">
         <v>251</v>
       </c>
       <c t="s" s="7" r="C66">
         <v>252</v>
       </c>
-      <c t="s" s="27" r="D66">
+      <c t="s" s="26" r="D66">
         <v>253</v>
       </c>
-      <c t="s" s="27" r="E66">
+      <c t="s" s="26" r="E66">
         <v>254</v>
       </c>
     </row>
@@ -4651,2274 +4738,2285 @@
         <v>263</v>
       </c>
     </row>
+    <row r="70">
+      <c t="s" s="14" r="B70">
+        <v>264</v>
+      </c>
+      <c t="s" s="14" r="C70">
+        <v>265</v>
+      </c>
+      <c t="s" s="14" r="D70">
+        <v>265</v>
+      </c>
+      <c t="s" s="14" r="E70">
+        <v>265</v>
+      </c>
+    </row>
     <row r="71">
-      <c s="20" r="A71"/>
-      <c s="20" r="B71"/>
-      <c s="20" r="C71"/>
-      <c s="20" r="D71"/>
-      <c s="20" r="E71"/>
+      <c t="s" s="14" r="B71">
+        <v>266</v>
+      </c>
+      <c t="s" s="14" r="C71">
+        <v>267</v>
+      </c>
+      <c t="s" s="35" r="D71">
+        <v>268</v>
+      </c>
+      <c t="s" s="35" r="E71">
+        <v>269</v>
+      </c>
     </row>
     <row r="72">
-      <c t="s" s="12" r="A72">
-        <v>264</v>
-      </c>
-      <c t="s" s="7" r="B72">
-        <v>265</v>
-      </c>
-      <c t="s" s="7" r="C72">
-        <v>266</v>
-      </c>
-      <c t="s" s="7" r="D72">
-        <v>267</v>
-      </c>
-      <c t="s" s="7" r="E72">
-        <v>268</v>
+      <c s="30" r="B72"/>
+      <c t="s" s="30" r="C72">
+        <v>270</v>
+      </c>
+      <c t="s" s="30" r="D72">
+        <v>271</v>
+      </c>
+      <c t="s" s="30" r="E72">
+        <v>272</v>
       </c>
     </row>
     <row r="73">
-      <c s="12" r="A73"/>
-      <c t="s" s="7" r="B73">
-        <v>269</v>
-      </c>
-      <c t="s" s="7" r="C73">
-        <v>270</v>
-      </c>
-      <c t="s" s="7" r="D73">
-        <v>271</v>
-      </c>
-      <c t="s" s="7" r="E73">
-        <v>272</v>
+      <c t="s" s="14" r="B73">
+        <v>273</v>
+      </c>
+      <c t="s" s="14" r="C73">
+        <v>274</v>
+      </c>
+      <c t="s" s="35" r="D73">
+        <v>275</v>
+      </c>
+      <c t="s" s="35" r="E73">
+        <v>276</v>
       </c>
     </row>
     <row r="74">
-      <c s="12" r="A74"/>
-      <c t="s" s="7" r="B74">
-        <v>273</v>
-      </c>
-      <c t="s" s="7" r="C74">
-        <v>274</v>
-      </c>
-      <c t="s" s="7" r="D74">
-        <v>275</v>
-      </c>
-      <c t="s" s="7" r="E74">
-        <v>276</v>
+      <c t="s" s="14" r="B74">
+        <v>277</v>
+      </c>
+      <c t="s" s="14" r="C74">
+        <v>278</v>
+      </c>
+      <c t="s" s="35" r="D74">
+        <v>279</v>
+      </c>
+      <c t="s" s="35" r="E74">
+        <v>280</v>
       </c>
     </row>
     <row r="75">
-      <c s="12" r="A75"/>
-      <c t="s" s="7" r="B75">
-        <v>277</v>
-      </c>
-      <c t="s" s="7" r="C75">
-        <v>278</v>
-      </c>
-      <c t="s" s="7" r="D75">
-        <v>279</v>
-      </c>
-      <c t="s" s="7" r="E75">
-        <v>280</v>
+      <c t="s" s="14" r="B75">
+        <v>281</v>
+      </c>
+      <c t="s" s="14" r="C75">
+        <v>282</v>
+      </c>
+      <c t="s" s="35" r="D75">
+        <v>283</v>
+      </c>
+      <c t="s" s="35" r="E75">
+        <v>284</v>
       </c>
     </row>
     <row r="76">
-      <c s="12" r="A76"/>
-      <c t="s" s="7" r="B76">
-        <v>281</v>
-      </c>
-      <c t="s" s="7" r="C76">
-        <v>282</v>
-      </c>
-      <c t="s" s="7" r="D76">
-        <v>283</v>
-      </c>
-      <c t="s" s="7" r="E76">
-        <v>284</v>
+      <c t="s" s="14" r="B76">
+        <v>285</v>
+      </c>
+      <c t="s" s="14" r="C76">
+        <v>286</v>
+      </c>
+      <c t="s" s="35" r="D76">
+        <v>287</v>
+      </c>
+      <c t="s" s="35" r="E76">
+        <v>288</v>
       </c>
     </row>
     <row r="77">
-      <c s="12" r="A77"/>
-      <c t="s" s="7" r="B77">
-        <v>285</v>
-      </c>
-      <c t="s" s="7" r="C77">
-        <v>286</v>
-      </c>
-      <c t="s" s="7" r="D77">
-        <v>287</v>
-      </c>
-      <c t="s" s="7" r="E77">
-        <v>288</v>
+      <c t="s" s="14" r="B77">
+        <v>289</v>
+      </c>
+      <c t="s" s="14" r="C77">
+        <v>290</v>
+      </c>
+      <c t="s" s="35" r="D77">
+        <v>291</v>
+      </c>
+      <c t="s" s="35" r="E77">
+        <v>292</v>
       </c>
     </row>
     <row r="78">
-      <c s="12" r="A78"/>
-      <c s="12" r="B78"/>
-      <c s="12" r="C78"/>
-      <c s="12" r="D78"/>
-      <c s="12" r="E78"/>
+      <c s="20" r="A78"/>
+      <c s="20" r="B78"/>
+      <c s="20" r="C78"/>
+      <c s="20" r="D78"/>
+      <c s="20" r="E78"/>
     </row>
     <row r="79">
       <c t="s" s="12" r="A79">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c t="s" s="7" r="B79">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c t="s" s="7" r="C79">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c t="s" s="7" r="D79">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c t="s" s="7" r="E79">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="80">
       <c s="12" r="A80"/>
       <c t="s" s="7" r="B80">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c t="s" s="7" r="C80">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c t="s" s="7" r="D80">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c t="s" s="7" r="E80">
-        <v>297</v>
+        <v>301</v>
       </c>
     </row>
     <row r="81">
       <c s="12" r="A81"/>
       <c t="s" s="7" r="B81">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c t="s" s="7" r="C81">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c t="s" s="7" r="D81">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c t="s" s="7" r="E81">
-        <v>301</v>
+        <v>305</v>
       </c>
     </row>
     <row r="82">
       <c s="12" r="A82"/>
       <c t="s" s="7" r="B82">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c t="s" s="7" r="C82">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c t="s" s="7" r="D82">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c t="s" s="7" r="E82">
-        <v>305</v>
+        <v>309</v>
       </c>
     </row>
     <row r="83">
       <c s="12" r="A83"/>
       <c t="s" s="7" r="B83">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c t="s" s="7" r="C83">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c t="s" s="7" r="D83">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c t="s" s="7" r="E83">
-        <v>309</v>
+        <v>313</v>
       </c>
     </row>
     <row r="84">
       <c s="12" r="A84"/>
       <c t="s" s="7" r="B84">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c t="s" s="7" r="C84">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c t="s" s="7" r="D84">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c t="s" s="7" r="E84">
-        <v>313</v>
+        <v>317</v>
       </c>
     </row>
     <row r="85">
       <c s="12" r="A85"/>
-      <c t="s" s="7" r="B85">
-        <v>314</v>
-      </c>
-      <c t="s" s="7" r="C85">
-        <v>315</v>
-      </c>
-      <c t="s" s="7" r="D85">
-        <v>316</v>
-      </c>
-      <c t="s" s="7" r="E85">
-        <v>317</v>
-      </c>
+      <c s="12" r="B85"/>
+      <c s="12" r="C85"/>
+      <c s="12" r="D85"/>
+      <c s="12" r="E85"/>
     </row>
     <row r="86">
-      <c s="12" r="A86"/>
+      <c t="s" s="12" r="A86">
+        <v>318</v>
+      </c>
       <c t="s" s="7" r="B86">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c t="s" s="7" r="C86">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c t="s" s="7" r="D86">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c t="s" s="7" r="E86">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="87">
       <c s="12" r="A87"/>
       <c t="s" s="7" r="B87">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c t="s" s="7" r="C87">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c t="s" s="7" r="D87">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c t="s" s="7" r="E87">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="88">
       <c s="12" r="A88"/>
-      <c s="12" r="B88"/>
-      <c s="12" r="C88"/>
-      <c s="12" r="D88"/>
-      <c s="12" r="E88"/>
+      <c t="s" s="7" r="B88">
+        <v>327</v>
+      </c>
+      <c t="s" s="7" r="C88">
+        <v>328</v>
+      </c>
+      <c t="s" s="7" r="D88">
+        <v>329</v>
+      </c>
+      <c t="s" s="7" r="E88">
+        <v>330</v>
+      </c>
     </row>
     <row r="89">
-      <c t="s" s="12" r="A89">
-        <v>326</v>
-      </c>
+      <c s="12" r="A89"/>
       <c t="s" s="7" r="B89">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c t="s" s="7" r="C89">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c t="s" s="7" r="D89">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c t="s" s="7" r="E89">
-        <v>330</v>
+        <v>334</v>
       </c>
     </row>
     <row r="90">
       <c s="12" r="A90"/>
       <c t="s" s="7" r="B90">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c t="s" s="7" r="C90">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c t="s" s="7" r="D90">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c t="s" s="7" r="E90">
-        <v>334</v>
+        <v>338</v>
       </c>
     </row>
     <row r="91">
-      <c s="9" r="A91"/>
+      <c s="12" r="A91"/>
       <c t="s" s="7" r="B91">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c t="s" s="7" r="C91">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c t="s" s="7" r="D91">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c t="s" s="7" r="E91">
-        <v>338</v>
+        <v>342</v>
       </c>
     </row>
     <row r="92">
-      <c s="9" r="A92"/>
+      <c s="12" r="A92"/>
       <c t="s" s="7" r="B92">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c t="s" s="7" r="C92">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c t="s" s="7" r="D92">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c t="s" s="7" r="E92">
-        <v>342</v>
+        <v>346</v>
       </c>
     </row>
     <row r="93">
-      <c s="9" r="A93"/>
+      <c s="12" r="A93"/>
       <c t="s" s="7" r="B93">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c t="s" s="7" r="C93">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c t="s" s="7" r="D93">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c t="s" s="7" r="E93">
-        <v>346</v>
+        <v>350</v>
       </c>
     </row>
     <row r="94">
-      <c s="9" r="A94"/>
+      <c s="12" r="A94"/>
       <c t="s" s="7" r="B94">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c t="s" s="7" r="C94">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c t="s" s="7" r="D94">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c t="s" s="7" r="E94">
-        <v>350</v>
+        <v>354</v>
       </c>
     </row>
     <row r="95">
-      <c s="9" r="A95"/>
-      <c t="s" s="7" r="B95">
-        <v>351</v>
-      </c>
-      <c t="s" s="7" r="C95">
-        <v>352</v>
-      </c>
-      <c t="s" s="7" r="D95">
-        <v>353</v>
-      </c>
-      <c t="s" s="7" r="E95">
-        <v>354</v>
-      </c>
+      <c s="12" r="A95"/>
+      <c s="12" r="B95"/>
+      <c s="12" r="C95"/>
+      <c s="12" r="D95"/>
+      <c s="12" r="E95"/>
     </row>
     <row r="96">
-      <c s="9" r="A96"/>
+      <c t="s" s="12" r="A96">
+        <v>355</v>
+      </c>
       <c t="s" s="7" r="B96">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c t="s" s="7" r="C96">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c t="s" s="7" r="D96">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c t="s" s="7" r="E96">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="97">
-      <c s="9" r="A97"/>
+      <c s="12" r="A97"/>
       <c t="s" s="7" r="B97">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c t="s" s="7" r="C97">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c t="s" s="7" r="D97">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c t="s" s="7" r="E97">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="98">
       <c s="9" r="A98"/>
       <c t="s" s="7" r="B98">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c t="s" s="7" r="C98">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c t="s" s="7" r="D98">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c t="s" s="7" r="E98">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="99">
       <c s="9" r="A99"/>
       <c t="s" s="7" r="B99">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c t="s" s="7" r="C99">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c t="s" s="7" r="D99">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c t="s" s="7" r="E99">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="100">
       <c s="9" r="A100"/>
       <c t="s" s="7" r="B100">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c t="s" s="7" r="C100">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c t="s" s="7" r="D100">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c t="s" s="7" r="E100">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="101">
       <c s="9" r="A101"/>
       <c t="s" s="7" r="B101">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c t="s" s="7" r="C101">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c t="s" s="7" r="D101">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c t="s" s="7" r="E101">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="102">
       <c s="9" r="A102"/>
       <c t="s" s="7" r="B102">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" s="7" r="C102">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c t="s" s="7" r="D102">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c t="s" s="7" r="E102">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="103">
       <c s="9" r="A103"/>
       <c t="s" s="7" r="B103">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c t="s" s="7" r="C103">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c t="s" s="7" r="D103">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c t="s" s="7" r="E103">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="104">
       <c s="9" r="A104"/>
-      <c s="12" r="B104"/>
-      <c s="12" r="C104"/>
-      <c s="12" r="D104"/>
-      <c s="12" r="E104"/>
+      <c t="s" s="7" r="B104">
+        <v>388</v>
+      </c>
+      <c t="s" s="7" r="C104">
+        <v>389</v>
+      </c>
+      <c t="s" s="7" r="D104">
+        <v>390</v>
+      </c>
+      <c t="s" s="7" r="E104">
+        <v>391</v>
+      </c>
     </row>
     <row r="105">
-      <c t="s" s="9" r="A105">
-        <v>387</v>
-      </c>
+      <c s="9" r="A105"/>
       <c t="s" s="7" r="B105">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c t="s" s="7" r="C105">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c t="s" s="7" r="D105">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c t="s" s="7" r="E105">
-        <v>391</v>
+        <v>395</v>
       </c>
     </row>
     <row r="106">
       <c s="9" r="A106"/>
       <c t="s" s="7" r="B106">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c t="s" s="7" r="C106">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c t="s" s="7" r="D106">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c t="s" s="7" r="E106">
-        <v>395</v>
+        <v>399</v>
       </c>
     </row>
     <row r="107">
       <c s="9" r="A107"/>
       <c t="s" s="7" r="B107">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c t="s" s="7" r="C107">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c t="s" s="7" r="D107">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c t="s" s="7" r="E107">
-        <v>399</v>
+        <v>403</v>
       </c>
     </row>
     <row r="108">
       <c s="9" r="A108"/>
       <c t="s" s="7" r="B108">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c t="s" s="7" r="C108">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c t="s" s="7" r="D108">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c t="s" s="7" r="E108">
-        <v>403</v>
+        <v>407</v>
       </c>
     </row>
     <row r="109">
       <c s="9" r="A109"/>
       <c t="s" s="7" r="B109">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c t="s" s="7" r="C109">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c t="s" s="7" r="D109">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c t="s" s="7" r="E109">
-        <v>407</v>
+        <v>411</v>
       </c>
     </row>
     <row r="110">
       <c s="9" r="A110"/>
       <c t="s" s="7" r="B110">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c t="s" s="7" r="C110">
-        <v>222</v>
+        <v>413</v>
       </c>
       <c t="s" s="7" r="D110">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c t="s" s="7" r="E110">
-        <v>222</v>
+        <v>415</v>
       </c>
     </row>
     <row r="111">
       <c s="9" r="A111"/>
-      <c t="s" s="7" r="B111">
-        <v>410</v>
-      </c>
-      <c t="s" s="7" r="C111">
-        <v>411</v>
-      </c>
-      <c t="s" s="7" r="D111">
-        <v>412</v>
-      </c>
-      <c t="s" s="7" r="E111">
-        <v>413</v>
-      </c>
+      <c s="12" r="B111"/>
+      <c s="12" r="C111"/>
+      <c s="12" r="D111"/>
+      <c s="12" r="E111"/>
     </row>
     <row r="112">
-      <c s="9" r="A112"/>
+      <c t="s" s="9" r="A112">
+        <v>416</v>
+      </c>
       <c t="s" s="7" r="B112">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c t="s" s="7" r="C112">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c t="s" s="7" r="D112">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c t="s" s="7" r="E112">
-        <v>417</v>
+        <v>420</v>
       </c>
     </row>
     <row r="113">
       <c s="9" r="A113"/>
       <c t="s" s="7" r="B113">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c t="s" s="7" r="C113">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c t="s" s="7" r="D113">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c t="s" s="7" r="E113">
-        <v>421</v>
+        <v>424</v>
       </c>
     </row>
     <row r="114">
       <c s="9" r="A114"/>
       <c t="s" s="7" r="B114">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c t="s" s="7" r="C114">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c t="s" s="7" r="D114">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c t="s" s="7" r="E114">
-        <v>425</v>
+        <v>428</v>
       </c>
     </row>
     <row r="115">
       <c s="9" r="A115"/>
       <c t="s" s="7" r="B115">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c t="s" s="7" r="C115">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c t="s" s="7" r="D115">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c t="s" s="7" r="E115">
-        <v>429</v>
+        <v>432</v>
       </c>
     </row>
     <row r="116">
       <c s="9" r="A116"/>
       <c t="s" s="7" r="B116">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c t="s" s="7" r="C116">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c t="s" s="7" r="D116">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c t="s" s="7" r="E116">
-        <v>432</v>
+        <v>436</v>
       </c>
     </row>
     <row r="117">
       <c s="9" r="A117"/>
       <c t="s" s="7" r="B117">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c t="s" s="7" r="C117">
-        <v>434</v>
+        <v>222</v>
       </c>
       <c t="s" s="7" r="D117">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c t="s" s="7" r="E117">
-        <v>435</v>
+        <v>222</v>
       </c>
     </row>
     <row r="118">
       <c s="9" r="A118"/>
       <c t="s" s="7" r="B118">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c t="s" s="7" r="C118">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c t="s" s="7" r="D118">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c t="s" s="7" r="E118">
-        <v>439</v>
+        <v>442</v>
       </c>
     </row>
     <row r="119">
       <c s="9" r="A119"/>
-      <c t="s" s="14" r="B119">
-        <v>440</v>
+      <c t="s" s="7" r="B119">
+        <v>443</v>
       </c>
       <c t="s" s="7" r="C119">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c t="s" s="7" r="D119">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c t="s" s="7" r="E119">
-        <v>442</v>
+        <v>446</v>
       </c>
     </row>
     <row r="120">
       <c s="9" r="A120"/>
       <c t="s" s="7" r="B120">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c t="s" s="7" r="C120">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c t="s" s="7" r="D120">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c t="s" s="7" r="E120">
-        <v>446</v>
+        <v>450</v>
       </c>
     </row>
     <row r="121">
       <c s="9" r="A121"/>
       <c t="s" s="7" r="B121">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c t="s" s="7" r="C121">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c t="s" s="7" r="D121">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c t="s" s="7" r="E121">
-        <v>450</v>
+        <v>454</v>
       </c>
     </row>
     <row r="122">
       <c s="9" r="A122"/>
       <c t="s" s="7" r="B122">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c t="s" s="7" r="C122">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c t="s" s="7" r="D122">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c t="s" s="7" r="E122">
-        <v>454</v>
+        <v>458</v>
       </c>
     </row>
     <row r="123">
       <c s="9" r="A123"/>
       <c t="s" s="7" r="B123">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c t="s" s="7" r="C123">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c t="s" s="7" r="D123">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c t="s" s="7" r="E123">
-        <v>458</v>
+        <v>461</v>
       </c>
     </row>
     <row r="124">
       <c s="9" r="A124"/>
       <c t="s" s="7" r="B124">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c t="s" s="7" r="C124">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c t="s" s="7" r="D124">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c t="s" s="7" r="E124">
-        <v>462</v>
+        <v>464</v>
       </c>
     </row>
     <row r="125">
       <c s="9" r="A125"/>
       <c t="s" s="7" r="B125">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c t="s" s="7" r="C125">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c t="s" s="7" r="D125">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c t="s" s="7" r="E125">
-        <v>466</v>
+        <v>468</v>
       </c>
     </row>
     <row r="126">
       <c s="9" r="A126"/>
-      <c t="s" s="7" r="B126">
-        <v>467</v>
+      <c t="s" s="14" r="B126">
+        <v>469</v>
       </c>
       <c t="s" s="7" r="C126">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c t="s" s="7" r="D126">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c t="s" s="7" r="E126">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="127">
       <c s="9" r="A127"/>
       <c t="s" s="7" r="B127">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c t="s" s="7" r="C127">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c t="s" s="7" r="D127">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c t="s" s="7" r="E127">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="128">
       <c s="9" r="A128"/>
       <c t="s" s="7" r="B128">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c t="s" s="7" r="C128">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c t="s" s="7" r="D128">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c t="s" s="7" r="E128">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="129">
       <c s="9" r="A129"/>
       <c t="s" s="7" r="B129">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c t="s" s="7" r="C129">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c t="s" s="7" r="D129">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c t="s" s="7" r="E129">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="130">
       <c s="9" r="A130"/>
       <c t="s" s="7" r="B130">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c t="s" s="7" r="C130">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c t="s" s="7" r="D130">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c t="s" s="7" r="E130">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="131">
       <c s="9" r="A131"/>
       <c t="s" s="7" r="B131">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c t="s" s="7" r="C131">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c t="s" s="7" r="D131">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c t="s" s="7" r="E131">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="132">
       <c s="9" r="A132"/>
       <c t="s" s="7" r="B132">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c t="s" s="7" r="C132">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c t="s" s="7" r="D132">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c t="s" s="7" r="E132">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="133">
       <c s="9" r="A133"/>
       <c t="s" s="7" r="B133">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c t="s" s="7" r="C133">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c t="s" s="7" r="D133">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c t="s" s="7" r="E133">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="134">
       <c s="9" r="A134"/>
       <c t="s" s="7" r="B134">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c t="s" s="7" r="C134">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c t="s" s="7" r="D134">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c t="s" s="7" r="E134">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="135">
       <c s="9" r="A135"/>
       <c t="s" s="7" r="B135">
-        <v>503</v>
-      </c>
-      <c t="s" s="14" r="C135">
         <v>504</v>
       </c>
+      <c t="s" s="7" r="C135">
+        <v>505</v>
+      </c>
       <c t="s" s="7" r="D135">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c t="s" s="7" r="E135">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="136">
       <c s="9" r="A136"/>
-      <c t="s" s="14" r="B136">
-        <v>507</v>
-      </c>
-      <c t="s" s="14" r="C136">
+      <c t="s" s="7" r="B136">
         <v>508</v>
       </c>
+      <c t="s" s="7" r="C136">
+        <v>509</v>
+      </c>
       <c t="s" s="7" r="D136">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c t="s" s="7" r="E136">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="137">
       <c s="9" r="A137"/>
       <c t="s" s="7" r="B137">
-        <v>511</v>
-      </c>
-      <c t="s" s="14" r="C137">
-        <v>508</v>
+        <v>512</v>
+      </c>
+      <c t="s" s="7" r="C137">
+        <v>513</v>
       </c>
       <c t="s" s="7" r="D137">
-        <v>509</v>
+        <v>514</v>
       </c>
       <c t="s" s="7" r="E137">
-        <v>510</v>
+        <v>515</v>
       </c>
     </row>
     <row r="138">
       <c s="9" r="A138"/>
       <c t="s" s="7" r="B138">
-        <v>512</v>
-      </c>
-      <c t="s" s="2" r="C138">
-        <v>513</v>
+        <v>516</v>
+      </c>
+      <c t="s" s="7" r="C138">
+        <v>517</v>
       </c>
       <c t="s" s="7" r="D138">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c t="s" s="7" r="E138">
-        <v>515</v>
+        <v>519</v>
       </c>
     </row>
     <row r="139">
       <c s="9" r="A139"/>
       <c t="s" s="7" r="B139">
-        <v>516</v>
-      </c>
-      <c t="s" s="2" r="C139">
-        <v>517</v>
+        <v>520</v>
+      </c>
+      <c t="s" s="7" r="C139">
+        <v>521</v>
       </c>
       <c t="s" s="7" r="D139">
-        <v>518</v>
+        <v>522</v>
       </c>
       <c t="s" s="7" r="E139">
-        <v>519</v>
+        <v>523</v>
       </c>
     </row>
     <row r="140">
       <c s="9" r="A140"/>
       <c t="s" s="7" r="B140">
-        <v>520</v>
-      </c>
-      <c t="s" s="2" r="C140">
-        <v>521</v>
+        <v>524</v>
+      </c>
+      <c t="s" s="7" r="C140">
+        <v>525</v>
       </c>
       <c t="s" s="7" r="D140">
-        <v>522</v>
-      </c>
-      <c t="s" s="2" r="E140">
-        <v>523</v>
+        <v>526</v>
+      </c>
+      <c t="s" s="7" r="E140">
+        <v>527</v>
       </c>
     </row>
     <row r="141">
       <c s="9" r="A141"/>
-      <c s="17" r="B141"/>
-      <c s="8" r="C141"/>
-      <c s="17" r="D141"/>
-      <c s="17" r="E141"/>
+      <c t="s" s="7" r="B141">
+        <v>528</v>
+      </c>
+      <c t="s" s="7" r="C141">
+        <v>529</v>
+      </c>
+      <c t="s" s="7" r="D141">
+        <v>530</v>
+      </c>
+      <c t="s" s="7" r="E141">
+        <v>531</v>
+      </c>
     </row>
     <row r="142">
-      <c t="s" s="9" r="A142">
-        <v>524</v>
-      </c>
+      <c s="9" r="A142"/>
       <c t="s" s="7" r="B142">
-        <v>525</v>
+        <v>532</v>
       </c>
       <c t="s" s="14" r="C142">
-        <v>526</v>
+        <v>533</v>
       </c>
       <c t="s" s="7" r="D142">
-        <v>527</v>
+        <v>534</v>
       </c>
       <c t="s" s="7" r="E142">
-        <v>528</v>
+        <v>535</v>
       </c>
     </row>
     <row r="143">
       <c s="9" r="A143"/>
-      <c t="s" s="22" r="B143">
-        <v>529</v>
+      <c t="s" s="14" r="B143">
+        <v>536</v>
       </c>
       <c t="s" s="14" r="C143">
-        <v>530</v>
-      </c>
-      <c t="s" s="22" r="D143">
-        <v>531</v>
-      </c>
-      <c t="s" s="22" r="E143">
-        <v>532</v>
+        <v>537</v>
+      </c>
+      <c t="s" s="7" r="D143">
+        <v>538</v>
+      </c>
+      <c t="s" s="7" r="E143">
+        <v>539</v>
       </c>
     </row>
     <row r="144">
       <c s="9" r="A144"/>
       <c t="s" s="7" r="B144">
-        <v>533</v>
+        <v>540</v>
       </c>
       <c t="s" s="14" r="C144">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c t="s" s="7" r="D144">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c t="s" s="7" r="E144">
-        <v>536</v>
+        <v>539</v>
       </c>
     </row>
     <row r="145">
       <c s="9" r="A145"/>
       <c t="s" s="7" r="B145">
-        <v>537</v>
-      </c>
-      <c t="s" s="14" r="C145">
-        <v>538</v>
+        <v>541</v>
+      </c>
+      <c t="s" s="2" r="C145">
+        <v>542</v>
       </c>
       <c t="s" s="7" r="D145">
-        <v>539</v>
+        <v>543</v>
       </c>
       <c t="s" s="7" r="E145">
-        <v>540</v>
+        <v>544</v>
       </c>
     </row>
     <row r="146">
-      <c s="18" r="A146"/>
+      <c s="9" r="A146"/>
       <c t="s" s="7" r="B146">
-        <v>541</v>
-      </c>
-      <c t="s" s="14" r="C146">
-        <v>542</v>
+        <v>545</v>
+      </c>
+      <c t="s" s="2" r="C146">
+        <v>546</v>
       </c>
       <c t="s" s="7" r="D146">
-        <v>543</v>
+        <v>547</v>
       </c>
       <c t="s" s="7" r="E146">
-        <v>544</v>
+        <v>548</v>
       </c>
     </row>
     <row r="147">
       <c s="9" r="A147"/>
       <c t="s" s="7" r="B147">
-        <v>545</v>
-      </c>
-      <c t="s" s="14" r="C147">
-        <v>546</v>
+        <v>549</v>
+      </c>
+      <c t="s" s="2" r="C147">
+        <v>550</v>
       </c>
       <c t="s" s="7" r="D147">
-        <v>547</v>
-      </c>
-      <c t="s" s="7" r="E147">
-        <v>548</v>
+        <v>551</v>
+      </c>
+      <c t="s" s="2" r="E147">
+        <v>552</v>
       </c>
     </row>
     <row r="148">
       <c s="9" r="A148"/>
-      <c t="s" s="7" r="B148">
-        <v>549</v>
-      </c>
-      <c t="s" s="14" r="C148">
-        <v>550</v>
-      </c>
-      <c t="s" s="7" r="D148">
-        <v>551</v>
-      </c>
-      <c t="s" s="7" r="E148">
-        <v>552</v>
-      </c>
+      <c s="17" r="B148"/>
+      <c s="8" r="C148"/>
+      <c s="17" r="D148"/>
+      <c s="17" r="E148"/>
     </row>
     <row r="149">
-      <c s="9" r="A149"/>
+      <c t="s" s="9" r="A149">
+        <v>553</v>
+      </c>
       <c t="s" s="7" r="B149">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c t="s" s="14" r="C149">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c t="s" s="7" r="D149">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c t="s" s="7" r="E149">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="150">
       <c s="9" r="A150"/>
-      <c t="s" s="7" r="B150">
-        <v>557</v>
+      <c t="s" s="22" r="B150">
+        <v>558</v>
       </c>
       <c t="s" s="14" r="C150">
-        <v>558</v>
-      </c>
-      <c t="s" s="7" r="D150">
         <v>559</v>
       </c>
-      <c t="s" s="7" r="E150">
+      <c t="s" s="22" r="D150">
         <v>560</v>
+      </c>
+      <c t="s" s="22" r="E150">
+        <v>561</v>
       </c>
     </row>
     <row r="151">
       <c s="9" r="A151"/>
       <c t="s" s="7" r="B151">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c t="s" s="14" r="C151">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c t="s" s="7" r="D151">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c t="s" s="7" r="E151">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="152">
       <c s="9" r="A152"/>
       <c t="s" s="7" r="B152">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c t="s" s="14" r="C152">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c t="s" s="7" r="D152">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c t="s" s="7" r="E152">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="153">
-      <c s="9" r="A153"/>
-      <c s="20" r="B153"/>
-      <c s="30" r="C153"/>
-      <c s="20" r="D153"/>
-      <c s="20" r="E153"/>
+      <c s="18" r="A153"/>
+      <c t="s" s="7" r="B153">
+        <v>570</v>
+      </c>
+      <c t="s" s="14" r="C153">
+        <v>571</v>
+      </c>
+      <c t="s" s="7" r="D153">
+        <v>572</v>
+      </c>
+      <c t="s" s="7" r="E153">
+        <v>573</v>
+      </c>
     </row>
     <row r="154">
-      <c t="s" s="9" r="A154">
-        <v>569</v>
-      </c>
+      <c s="9" r="A154"/>
       <c t="s" s="7" r="B154">
-        <v>570</v>
+        <v>574</v>
       </c>
       <c t="s" s="14" r="C154">
-        <v>571</v>
+        <v>575</v>
       </c>
       <c t="s" s="7" r="D154">
-        <v>572</v>
+        <v>576</v>
       </c>
       <c t="s" s="7" r="E154">
-        <v>573</v>
+        <v>577</v>
       </c>
     </row>
     <row r="155">
       <c s="9" r="A155"/>
       <c t="s" s="7" r="B155">
-        <v>574</v>
+        <v>578</v>
       </c>
       <c t="s" s="14" r="C155">
-        <v>575</v>
+        <v>579</v>
       </c>
       <c t="s" s="7" r="D155">
-        <v>576</v>
+        <v>580</v>
       </c>
       <c t="s" s="7" r="E155">
-        <v>577</v>
+        <v>581</v>
       </c>
     </row>
     <row r="156">
       <c s="9" r="A156"/>
       <c t="s" s="7" r="B156">
-        <v>578</v>
+        <v>582</v>
       </c>
       <c t="s" s="14" r="C156">
-        <v>579</v>
+        <v>583</v>
       </c>
       <c t="s" s="7" r="D156">
-        <v>580</v>
+        <v>584</v>
       </c>
       <c t="s" s="7" r="E156">
-        <v>581</v>
+        <v>585</v>
       </c>
     </row>
     <row r="157">
       <c s="9" r="A157"/>
       <c t="s" s="7" r="B157">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c t="s" s="14" r="C157">
-        <v>583</v>
+        <v>587</v>
       </c>
       <c t="s" s="7" r="D157">
-        <v>584</v>
+        <v>588</v>
       </c>
       <c t="s" s="7" r="E157">
-        <v>585</v>
+        <v>589</v>
       </c>
     </row>
     <row r="158">
       <c s="9" r="A158"/>
       <c t="s" s="7" r="B158">
-        <v>586</v>
+        <v>590</v>
       </c>
       <c t="s" s="14" r="C158">
-        <v>587</v>
+        <v>591</v>
       </c>
       <c t="s" s="7" r="D158">
-        <v>588</v>
+        <v>592</v>
       </c>
       <c t="s" s="7" r="E158">
-        <v>589</v>
+        <v>593</v>
       </c>
     </row>
     <row r="159">
       <c s="9" r="A159"/>
       <c t="s" s="7" r="B159">
-        <v>590</v>
+        <v>594</v>
       </c>
       <c t="s" s="14" r="C159">
-        <v>591</v>
+        <v>595</v>
       </c>
       <c t="s" s="7" r="D159">
-        <v>592</v>
+        <v>596</v>
       </c>
       <c t="s" s="7" r="E159">
-        <v>593</v>
+        <v>597</v>
       </c>
     </row>
     <row r="160">
       <c s="9" r="A160"/>
-      <c t="s" s="7" r="B160">
-        <v>594</v>
-      </c>
-      <c t="s" s="14" r="C160">
-        <v>595</v>
-      </c>
-      <c t="s" s="7" r="D160">
-        <v>596</v>
-      </c>
-      <c t="s" s="7" r="E160">
-        <v>597</v>
-      </c>
+      <c s="20" r="B160"/>
+      <c s="29" r="C160"/>
+      <c s="20" r="D160"/>
+      <c s="20" r="E160"/>
     </row>
     <row r="161">
-      <c s="9" r="A161"/>
-      <c s="20" r="B161"/>
-      <c s="30" r="C161"/>
-      <c s="20" r="D161"/>
-      <c s="20" r="E161"/>
+      <c t="s" s="9" r="A161">
+        <v>598</v>
+      </c>
+      <c t="s" s="7" r="B161">
+        <v>599</v>
+      </c>
+      <c t="s" s="14" r="C161">
+        <v>600</v>
+      </c>
+      <c t="s" s="7" r="D161">
+        <v>601</v>
+      </c>
+      <c t="s" s="7" r="E161">
+        <v>602</v>
+      </c>
     </row>
     <row r="162">
-      <c t="s" s="9" r="A162">
-        <v>598</v>
-      </c>
-      <c t="s" s="29" r="B162">
-        <v>599</v>
-      </c>
-      <c t="s" s="21" r="C162">
-        <v>598</v>
-      </c>
-      <c s="29" r="D162"/>
-      <c s="29" r="E162"/>
+      <c s="9" r="A162"/>
+      <c t="s" s="7" r="B162">
+        <v>603</v>
+      </c>
+      <c t="s" s="14" r="C162">
+        <v>604</v>
+      </c>
+      <c t="s" s="7" r="D162">
+        <v>605</v>
+      </c>
+      <c t="s" s="7" r="E162">
+        <v>606</v>
+      </c>
     </row>
     <row r="163">
       <c s="9" r="A163"/>
-      <c s="17" r="B163"/>
-      <c s="8" r="C163"/>
-      <c s="17" r="D163"/>
-      <c s="17" r="E163"/>
+      <c t="s" s="7" r="B163">
+        <v>607</v>
+      </c>
+      <c t="s" s="14" r="C163">
+        <v>608</v>
+      </c>
+      <c t="s" s="7" r="D163">
+        <v>609</v>
+      </c>
+      <c t="s" s="7" r="E163">
+        <v>610</v>
+      </c>
     </row>
     <row r="164">
-      <c t="s" s="9" r="A164">
-        <v>600</v>
-      </c>
-      <c t="s" s="35" r="B164">
-        <v>601</v>
-      </c>
-      <c t="s" s="33" r="C164">
-        <v>602</v>
-      </c>
-      <c s="35" r="D164"/>
-      <c s="35" r="E164"/>
+      <c s="9" r="A164"/>
+      <c t="s" s="7" r="B164">
+        <v>611</v>
+      </c>
+      <c t="s" s="14" r="C164">
+        <v>612</v>
+      </c>
+      <c t="s" s="7" r="D164">
+        <v>613</v>
+      </c>
+      <c t="s" s="7" r="E164">
+        <v>614</v>
+      </c>
     </row>
     <row r="165">
       <c s="9" r="A165"/>
-      <c t="s" s="35" r="B165">
-        <v>603</v>
-      </c>
-      <c t="s" s="33" r="C165">
-        <v>604</v>
-      </c>
-      <c s="35" r="D165"/>
-      <c s="35" r="E165"/>
+      <c t="s" s="7" r="B165">
+        <v>615</v>
+      </c>
+      <c t="s" s="14" r="C165">
+        <v>616</v>
+      </c>
+      <c t="s" s="7" r="D165">
+        <v>617</v>
+      </c>
+      <c t="s" s="7" r="E165">
+        <v>618</v>
+      </c>
     </row>
     <row r="166">
       <c s="9" r="A166"/>
-      <c s="8" r="B166"/>
-      <c s="8" r="C166"/>
-      <c s="17" r="D166"/>
-      <c s="17" r="E166"/>
+      <c t="s" s="7" r="B166">
+        <v>619</v>
+      </c>
+      <c t="s" s="14" r="C166">
+        <v>620</v>
+      </c>
+      <c t="s" s="7" r="D166">
+        <v>621</v>
+      </c>
+      <c t="s" s="7" r="E166">
+        <v>622</v>
+      </c>
     </row>
     <row r="167">
-      <c t="s" s="9" r="A167">
-        <v>605</v>
-      </c>
-      <c t="s" s="27" r="B167">
-        <v>606</v>
-      </c>
-      <c t="s" s="27" r="C167">
-        <v>607</v>
+      <c s="9" r="A167"/>
+      <c t="s" s="7" r="B167">
+        <v>623</v>
+      </c>
+      <c t="s" s="14" r="C167">
+        <v>624</v>
       </c>
       <c t="s" s="7" r="D167">
-        <v>608</v>
+        <v>625</v>
       </c>
       <c t="s" s="7" r="E167">
-        <v>609</v>
+        <v>626</v>
       </c>
     </row>
     <row r="168">
       <c s="9" r="A168"/>
-      <c t="s" s="27" r="B168">
-        <v>610</v>
-      </c>
-      <c t="s" s="27" r="C168">
-        <v>611</v>
-      </c>
-      <c t="s" s="7" r="D168">
-        <v>611</v>
-      </c>
-      <c t="s" s="7" r="E168">
-        <v>612</v>
-      </c>
+      <c s="20" r="B168"/>
+      <c s="29" r="C168"/>
+      <c s="20" r="D168"/>
+      <c s="20" r="E168"/>
     </row>
     <row r="169">
-      <c s="9" r="A169"/>
-      <c t="s" s="27" r="B169">
-        <v>613</v>
-      </c>
-      <c t="s" s="27" r="C169">
-        <v>614</v>
-      </c>
-      <c t="s" s="7" r="D169">
-        <v>615</v>
-      </c>
-      <c t="s" s="7" r="E169">
-        <v>616</v>
-      </c>
+      <c t="s" s="9" r="A169">
+        <v>627</v>
+      </c>
+      <c t="s" s="28" r="B169">
+        <v>628</v>
+      </c>
+      <c t="s" s="21" r="C169">
+        <v>627</v>
+      </c>
+      <c s="28" r="D169"/>
+      <c s="28" r="E169"/>
     </row>
     <row r="170">
       <c s="9" r="A170"/>
-      <c t="s" s="27" r="B170">
-        <v>617</v>
-      </c>
-      <c t="s" s="27" r="C170">
-        <v>618</v>
-      </c>
-      <c t="s" s="7" r="D170">
-        <v>619</v>
-      </c>
-      <c t="s" s="7" r="E170">
-        <v>620</v>
-      </c>
+      <c s="17" r="B170"/>
+      <c s="8" r="C170"/>
+      <c s="17" r="D170"/>
+      <c s="17" r="E170"/>
     </row>
     <row r="171">
-      <c s="9" r="A171"/>
-      <c t="s" s="14" r="B171">
-        <v>621</v>
-      </c>
-      <c t="s" s="14" r="C171">
-        <v>622</v>
-      </c>
-      <c t="s" s="7" r="D171">
-        <v>623</v>
-      </c>
-      <c t="s" s="7" r="E171">
-        <v>624</v>
-      </c>
+      <c t="s" s="9" r="A171">
+        <v>629</v>
+      </c>
+      <c t="s" s="34" r="B171">
+        <v>630</v>
+      </c>
+      <c t="s" s="32" r="C171">
+        <v>631</v>
+      </c>
+      <c s="34" r="D171"/>
+      <c s="34" r="E171"/>
     </row>
     <row r="172">
       <c s="9" r="A172"/>
-      <c t="s" s="14" r="B172">
-        <v>625</v>
-      </c>
-      <c t="s" s="14" r="C172">
-        <v>626</v>
-      </c>
-      <c t="s" s="7" r="D172">
-        <v>627</v>
-      </c>
-      <c t="s" s="7" r="E172">
-        <v>628</v>
-      </c>
+      <c t="s" s="34" r="B172">
+        <v>632</v>
+      </c>
+      <c t="s" s="32" r="C172">
+        <v>633</v>
+      </c>
+      <c s="34" r="D172"/>
+      <c s="34" r="E172"/>
     </row>
     <row r="173">
       <c s="9" r="A173"/>
-      <c t="s" s="14" r="B173">
-        <v>629</v>
-      </c>
-      <c t="s" s="14" r="C173">
-        <v>630</v>
-      </c>
-      <c t="s" s="7" r="D173">
-        <v>631</v>
-      </c>
-      <c t="s" s="7" r="E173">
-        <v>632</v>
-      </c>
+      <c s="8" r="B173"/>
+      <c s="8" r="C173"/>
+      <c s="17" r="D173"/>
+      <c s="17" r="E173"/>
     </row>
     <row r="174">
-      <c s="9" r="A174"/>
-      <c t="s" s="14" r="B174">
-        <v>633</v>
-      </c>
-      <c t="s" s="14" r="C174">
+      <c t="s" s="9" r="A174">
         <v>634</v>
       </c>
+      <c t="s" s="26" r="B174">
+        <v>635</v>
+      </c>
+      <c t="s" s="26" r="C174">
+        <v>636</v>
+      </c>
       <c t="s" s="7" r="D174">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c t="s" s="7" r="E174">
-        <v>636</v>
+        <v>638</v>
       </c>
     </row>
     <row r="175">
       <c s="9" r="A175"/>
-      <c t="s" s="14" r="B175">
-        <v>637</v>
-      </c>
-      <c t="s" s="14" r="C175">
-        <v>638</v>
+      <c t="s" s="26" r="B175">
+        <v>639</v>
+      </c>
+      <c t="s" s="26" r="C175">
+        <v>640</v>
       </c>
       <c t="s" s="7" r="D175">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c t="s" s="7" r="E175">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="176">
       <c s="9" r="A176"/>
-      <c t="s" s="14" r="B176">
-        <v>641</v>
-      </c>
-      <c t="s" s="14" r="C176">
+      <c t="s" s="26" r="B176">
         <v>642</v>
       </c>
+      <c t="s" s="26" r="C176">
+        <v>643</v>
+      </c>
       <c t="s" s="7" r="D176">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c t="s" s="7" r="E176">
-        <v>644</v>
+        <v>645</v>
       </c>
     </row>
     <row r="177">
       <c s="9" r="A177"/>
-      <c t="s" s="14" r="B177">
-        <v>645</v>
-      </c>
-      <c t="s" s="14" r="C177">
+      <c t="s" s="26" r="B177">
         <v>646</v>
       </c>
+      <c t="s" s="26" r="C177">
+        <v>647</v>
+      </c>
       <c t="s" s="7" r="D177">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c t="s" s="7" r="E177">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="178">
       <c s="9" r="A178"/>
-      <c t="s" s="7" r="B178">
-        <v>649</v>
+      <c t="s" s="14" r="B178">
+        <v>650</v>
       </c>
       <c t="s" s="14" r="C178">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c t="s" s="7" r="D178">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c t="s" s="7" r="E178">
-        <v>652</v>
+        <v>653</v>
       </c>
     </row>
     <row r="179">
       <c s="9" r="A179"/>
-      <c t="s" s="7" r="B179">
-        <v>653</v>
+      <c t="s" s="14" r="B179">
+        <v>654</v>
       </c>
       <c t="s" s="14" r="C179">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c t="s" s="7" r="D179">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c t="s" s="7" r="E179">
-        <v>656</v>
+        <v>657</v>
       </c>
     </row>
     <row r="180">
       <c s="9" r="A180"/>
-      <c t="s" s="7" r="B180">
-        <v>657</v>
+      <c t="s" s="14" r="B180">
+        <v>658</v>
       </c>
       <c t="s" s="14" r="C180">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c t="s" s="7" r="D180">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c t="s" s="7" r="E180">
-        <v>660</v>
+        <v>661</v>
       </c>
     </row>
     <row r="181">
       <c s="9" r="A181"/>
-      <c t="s" s="7" r="B181">
-        <v>661</v>
+      <c t="s" s="14" r="B181">
+        <v>662</v>
       </c>
       <c t="s" s="14" r="C181">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c t="s" s="7" r="D181">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c t="s" s="7" r="E181">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="182">
       <c s="9" r="A182"/>
-      <c t="s" s="7" r="B182">
-        <v>665</v>
+      <c t="s" s="14" r="B182">
+        <v>666</v>
       </c>
       <c t="s" s="14" r="C182">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c t="s" s="7" r="D182">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c t="s" s="7" r="E182">
-        <v>668</v>
+        <v>669</v>
       </c>
     </row>
     <row r="183">
       <c s="9" r="A183"/>
-      <c t="s" s="7" r="B183">
-        <v>669</v>
+      <c t="s" s="14" r="B183">
+        <v>670</v>
       </c>
       <c t="s" s="14" r="C183">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c t="s" s="7" r="D183">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c t="s" s="7" r="E183">
-        <v>672</v>
+        <v>673</v>
       </c>
     </row>
     <row r="184">
       <c s="9" r="A184"/>
-      <c t="s" s="7" r="B184">
-        <v>673</v>
+      <c t="s" s="14" r="B184">
+        <v>674</v>
       </c>
       <c t="s" s="14" r="C184">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c t="s" s="7" r="D184">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c t="s" s="7" r="E184">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="185">
       <c s="9" r="A185"/>
       <c t="s" s="7" r="B185">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c t="s" s="14" r="C185">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c t="s" s="7" r="D185">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c t="s" s="7" r="E185">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="186">
       <c s="9" r="A186"/>
       <c t="s" s="7" r="B186">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c t="s" s="14" r="C186">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c t="s" s="7" r="D186">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c t="s" s="7" r="E186">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="187">
       <c s="9" r="A187"/>
-      <c s="17" r="B187"/>
-      <c s="30" r="C187"/>
-      <c s="17" r="D187"/>
-      <c s="17" r="E187"/>
+      <c t="s" s="7" r="B187">
+        <v>686</v>
+      </c>
+      <c t="s" s="14" r="C187">
+        <v>687</v>
+      </c>
+      <c t="s" s="7" r="D187">
+        <v>688</v>
+      </c>
+      <c t="s" s="7" r="E187">
+        <v>689</v>
+      </c>
     </row>
     <row r="188">
-      <c t="s" s="9" r="A188">
-        <v>685</v>
-      </c>
-      <c t="s" s="27" r="B188">
-        <v>686</v>
-      </c>
-      <c t="s" s="7" r="C188">
-        <v>611</v>
+      <c s="9" r="A188"/>
+      <c t="s" s="7" r="B188">
+        <v>690</v>
+      </c>
+      <c t="s" s="14" r="C188">
+        <v>691</v>
       </c>
       <c t="s" s="7" r="D188">
-        <v>611</v>
+        <v>692</v>
       </c>
       <c t="s" s="7" r="E188">
-        <v>612</v>
+        <v>693</v>
       </c>
     </row>
     <row r="189">
       <c s="9" r="A189"/>
       <c t="s" s="7" r="B189">
-        <v>687</v>
+        <v>694</v>
       </c>
       <c t="s" s="14" r="C189">
-        <v>614</v>
+        <v>695</v>
       </c>
       <c t="s" s="7" r="D189">
-        <v>615</v>
+        <v>696</v>
       </c>
       <c t="s" s="7" r="E189">
-        <v>616</v>
+        <v>697</v>
       </c>
     </row>
     <row r="190">
+      <c s="9" r="A190"/>
       <c t="s" s="7" r="B190">
-        <v>688</v>
+        <v>698</v>
       </c>
       <c t="s" s="14" r="C190">
-        <v>689</v>
+        <v>699</v>
       </c>
       <c t="s" s="7" r="D190">
-        <v>690</v>
+        <v>700</v>
       </c>
       <c t="s" s="7" r="E190">
-        <v>691</v>
+        <v>701</v>
       </c>
     </row>
     <row r="191">
       <c s="9" r="A191"/>
       <c t="s" s="7" r="B191">
-        <v>692</v>
+        <v>702</v>
       </c>
       <c t="s" s="14" r="C191">
-        <v>693</v>
+        <v>703</v>
       </c>
       <c t="s" s="7" r="D191">
-        <v>694</v>
+        <v>704</v>
       </c>
       <c t="s" s="7" r="E191">
-        <v>695</v>
+        <v>705</v>
       </c>
     </row>
     <row r="192">
       <c s="9" r="A192"/>
       <c t="s" s="7" r="B192">
-        <v>696</v>
+        <v>706</v>
       </c>
       <c t="s" s="14" r="C192">
-        <v>697</v>
+        <v>707</v>
       </c>
       <c t="s" s="7" r="D192">
-        <v>698</v>
+        <v>708</v>
       </c>
       <c t="s" s="7" r="E192">
-        <v>699</v>
+        <v>709</v>
       </c>
     </row>
     <row r="193">
       <c s="9" r="A193"/>
-      <c s="12" r="B193"/>
-      <c s="15" r="C193"/>
-      <c s="17" r="D193"/>
-      <c s="17" r="E193"/>
+      <c t="s" s="7" r="B193">
+        <v>710</v>
+      </c>
+      <c t="s" s="14" r="C193">
+        <v>711</v>
+      </c>
+      <c t="s" s="7" r="D193">
+        <v>712</v>
+      </c>
+      <c t="s" s="7" r="E193">
+        <v>713</v>
+      </c>
     </row>
     <row r="194">
-      <c t="s" s="9" r="A194">
-        <v>700</v>
-      </c>
-      <c t="s" s="7" r="B194">
-        <v>701</v>
-      </c>
-      <c t="s" s="14" r="C194">
-        <v>700</v>
-      </c>
-      <c t="s" s="7" r="D194">
-        <v>702</v>
-      </c>
-      <c t="s" s="7" r="E194">
-        <v>703</v>
-      </c>
+      <c s="9" r="A194"/>
+      <c s="17" r="B194"/>
+      <c s="29" r="C194"/>
+      <c s="17" r="D194"/>
+      <c s="17" r="E194"/>
     </row>
     <row r="195">
-      <c s="9" r="A195"/>
-      <c t="s" s="7" r="B195">
-        <v>704</v>
-      </c>
-      <c t="s" s="14" r="C195">
-        <v>705</v>
+      <c t="s" s="9" r="A195">
+        <v>714</v>
+      </c>
+      <c t="s" s="26" r="B195">
+        <v>715</v>
+      </c>
+      <c t="s" s="7" r="C195">
+        <v>640</v>
       </c>
       <c t="s" s="7" r="D195">
-        <v>706</v>
+        <v>640</v>
       </c>
       <c t="s" s="7" r="E195">
-        <v>707</v>
+        <v>641</v>
       </c>
     </row>
     <row r="196">
       <c s="9" r="A196"/>
       <c t="s" s="7" r="B196">
-        <v>708</v>
+        <v>716</v>
       </c>
       <c t="s" s="14" r="C196">
-        <v>709</v>
+        <v>643</v>
       </c>
       <c t="s" s="7" r="D196">
-        <v>710</v>
+        <v>644</v>
       </c>
       <c t="s" s="7" r="E196">
-        <v>711</v>
+        <v>645</v>
       </c>
     </row>
     <row r="197">
-      <c s="9" r="A197"/>
       <c t="s" s="7" r="B197">
-        <v>712</v>
+        <v>717</v>
       </c>
       <c t="s" s="14" r="C197">
-        <v>713</v>
+        <v>718</v>
       </c>
       <c t="s" s="7" r="D197">
-        <v>714</v>
+        <v>719</v>
       </c>
       <c t="s" s="7" r="E197">
-        <v>715</v>
+        <v>720</v>
       </c>
     </row>
     <row r="198">
       <c s="9" r="A198"/>
       <c t="s" s="7" r="B198">
-        <v>716</v>
+        <v>721</v>
       </c>
       <c t="s" s="14" r="C198">
-        <v>717</v>
+        <v>722</v>
       </c>
       <c t="s" s="7" r="D198">
-        <v>718</v>
+        <v>723</v>
       </c>
       <c t="s" s="7" r="E198">
-        <v>719</v>
+        <v>724</v>
       </c>
     </row>
     <row r="199">
       <c s="9" r="A199"/>
       <c t="s" s="7" r="B199">
-        <v>720</v>
+        <v>725</v>
       </c>
       <c t="s" s="14" r="C199">
-        <v>721</v>
+        <v>726</v>
       </c>
       <c t="s" s="7" r="D199">
-        <v>722</v>
+        <v>727</v>
       </c>
       <c t="s" s="7" r="E199">
-        <v>723</v>
+        <v>728</v>
       </c>
     </row>
     <row r="200">
       <c s="9" r="A200"/>
-      <c t="s" s="7" r="B200">
-        <v>724</v>
-      </c>
-      <c t="s" s="14" r="C200">
-        <v>725</v>
-      </c>
-      <c t="s" s="7" r="D200">
-        <v>726</v>
-      </c>
-      <c t="s" s="7" r="E200">
-        <v>727</v>
-      </c>
+      <c s="12" r="B200"/>
+      <c s="15" r="C200"/>
+      <c s="17" r="D200"/>
+      <c s="17" r="E200"/>
     </row>
     <row r="201">
-      <c s="9" r="A201"/>
-      <c s="12" r="B201"/>
-      <c s="15" r="C201"/>
-      <c s="12" r="D201"/>
-      <c s="12" r="E201"/>
+      <c t="s" s="9" r="A201">
+        <v>729</v>
+      </c>
+      <c t="s" s="7" r="B201">
+        <v>730</v>
+      </c>
+      <c t="s" s="14" r="C201">
+        <v>729</v>
+      </c>
+      <c t="s" s="7" r="D201">
+        <v>731</v>
+      </c>
+      <c t="s" s="7" r="E201">
+        <v>732</v>
+      </c>
     </row>
     <row r="202">
-      <c t="s" s="9" r="A202">
-        <v>728</v>
-      </c>
+      <c s="9" r="A202"/>
       <c t="s" s="7" r="B202">
-        <v>729</v>
+        <v>733</v>
       </c>
       <c t="s" s="14" r="C202">
-        <v>730</v>
+        <v>734</v>
       </c>
       <c t="s" s="7" r="D202">
-        <v>731</v>
+        <v>735</v>
       </c>
       <c t="s" s="7" r="E202">
-        <v>732</v>
+        <v>736</v>
       </c>
     </row>
     <row r="203">
       <c s="9" r="A203"/>
       <c t="s" s="7" r="B203">
-        <v>733</v>
+        <v>737</v>
       </c>
       <c t="s" s="14" r="C203">
-        <v>734</v>
+        <v>738</v>
       </c>
       <c t="s" s="7" r="D203">
-        <v>734</v>
+        <v>739</v>
       </c>
       <c t="s" s="7" r="E203">
-        <v>735</v>
+        <v>740</v>
       </c>
     </row>
     <row r="204">
       <c s="9" r="A204"/>
-      <c s="12" r="B204"/>
-      <c s="15" r="C204"/>
-      <c s="12" r="D204"/>
-      <c s="12" r="E204"/>
+      <c t="s" s="7" r="B204">
+        <v>741</v>
+      </c>
+      <c t="s" s="14" r="C204">
+        <v>742</v>
+      </c>
+      <c t="s" s="7" r="D204">
+        <v>743</v>
+      </c>
+      <c t="s" s="7" r="E204">
+        <v>744</v>
+      </c>
     </row>
     <row r="205">
-      <c t="s" s="9" r="A205">
-        <v>736</v>
-      </c>
+      <c s="9" r="A205"/>
       <c t="s" s="7" r="B205">
-        <v>737</v>
+        <v>745</v>
       </c>
       <c t="s" s="14" r="C205">
-        <v>738</v>
+        <v>746</v>
       </c>
       <c t="s" s="7" r="D205">
-        <v>739</v>
+        <v>747</v>
       </c>
       <c t="s" s="7" r="E205">
-        <v>740</v>
+        <v>748</v>
       </c>
     </row>
     <row r="206">
       <c s="9" r="A206"/>
       <c t="s" s="7" r="B206">
-        <v>741</v>
+        <v>749</v>
       </c>
       <c t="s" s="14" r="C206">
-        <v>742</v>
+        <v>750</v>
       </c>
       <c t="s" s="7" r="D206">
-        <v>743</v>
+        <v>751</v>
       </c>
       <c t="s" s="7" r="E206">
-        <v>744</v>
+        <v>752</v>
       </c>
     </row>
     <row r="207">
       <c s="9" r="A207"/>
       <c t="s" s="7" r="B207">
-        <v>745</v>
+        <v>753</v>
       </c>
       <c t="s" s="14" r="C207">
-        <v>746</v>
+        <v>754</v>
       </c>
       <c t="s" s="7" r="D207">
-        <v>747</v>
+        <v>755</v>
       </c>
       <c t="s" s="7" r="E207">
-        <v>748</v>
+        <v>756</v>
       </c>
     </row>
     <row r="208">
       <c s="9" r="A208"/>
-      <c t="s" s="7" r="B208">
-        <v>749</v>
-      </c>
-      <c t="s" s="14" r="C208">
-        <v>750</v>
-      </c>
-      <c t="s" s="7" r="D208">
-        <v>751</v>
-      </c>
-      <c t="s" s="7" r="E208">
-        <v>752</v>
-      </c>
+      <c s="12" r="B208"/>
+      <c s="15" r="C208"/>
+      <c s="12" r="D208"/>
+      <c s="12" r="E208"/>
     </row>
     <row r="209">
-      <c s="9" r="A209"/>
-      <c s="17" r="B209"/>
-      <c s="30" r="C209"/>
-      <c s="17" r="D209"/>
-      <c s="17" r="E209"/>
+      <c t="s" s="9" r="A209">
+        <v>757</v>
+      </c>
+      <c t="s" s="7" r="B209">
+        <v>758</v>
+      </c>
+      <c t="s" s="14" r="C209">
+        <v>759</v>
+      </c>
+      <c t="s" s="7" r="D209">
+        <v>760</v>
+      </c>
+      <c t="s" s="7" r="E209">
+        <v>761</v>
+      </c>
     </row>
     <row r="210">
-      <c t="s" s="9" r="A210">
-        <v>753</v>
-      </c>
+      <c s="9" r="A210"/>
       <c t="s" s="7" r="B210">
-        <v>754</v>
+        <v>762</v>
       </c>
       <c t="s" s="14" r="C210">
-        <v>755</v>
+        <v>763</v>
       </c>
       <c t="s" s="7" r="D210">
-        <v>756</v>
+        <v>763</v>
       </c>
       <c t="s" s="7" r="E210">
-        <v>757</v>
+        <v>764</v>
       </c>
     </row>
     <row r="211">
       <c s="9" r="A211"/>
-      <c t="s" s="7" r="B211">
-        <v>758</v>
-      </c>
-      <c t="s" s="14" r="C211">
-        <v>759</v>
-      </c>
-      <c t="s" s="7" r="D211">
-        <v>760</v>
-      </c>
-      <c t="s" s="7" r="E211">
-        <v>761</v>
-      </c>
+      <c s="12" r="B211"/>
+      <c s="15" r="C211"/>
+      <c s="12" r="D211"/>
+      <c s="12" r="E211"/>
     </row>
     <row r="212">
-      <c s="9" r="A212"/>
-      <c s="17" r="B212"/>
-      <c s="30" r="C212"/>
-      <c s="17" r="D212"/>
-      <c s="17" r="E212"/>
+      <c t="s" s="9" r="A212">
+        <v>765</v>
+      </c>
+      <c t="s" s="7" r="B212">
+        <v>766</v>
+      </c>
+      <c t="s" s="14" r="C212">
+        <v>767</v>
+      </c>
+      <c t="s" s="7" r="D212">
+        <v>768</v>
+      </c>
+      <c t="s" s="7" r="E212">
+        <v>769</v>
+      </c>
     </row>
     <row r="213">
-      <c t="s" s="9" r="A213">
-        <v>762</v>
-      </c>
+      <c s="9" r="A213"/>
       <c t="s" s="7" r="B213">
-        <v>763</v>
+        <v>770</v>
       </c>
       <c t="s" s="14" r="C213">
-        <v>764</v>
+        <v>771</v>
       </c>
       <c t="s" s="7" r="D213">
-        <v>765</v>
+        <v>772</v>
       </c>
       <c t="s" s="7" r="E213">
-        <v>766</v>
+        <v>773</v>
       </c>
     </row>
     <row r="214">
       <c s="9" r="A214"/>
-      <c s="17" r="B214"/>
-      <c s="8" r="C214"/>
-      <c s="17" r="D214"/>
-      <c s="17" r="E214"/>
+      <c t="s" s="7" r="B214">
+        <v>774</v>
+      </c>
+      <c t="s" s="14" r="C214">
+        <v>775</v>
+      </c>
+      <c t="s" s="7" r="D214">
+        <v>776</v>
+      </c>
+      <c t="s" s="7" r="E214">
+        <v>777</v>
+      </c>
     </row>
     <row r="215">
-      <c t="s" s="9" r="A215">
-        <v>767</v>
-      </c>
+      <c s="9" r="A215"/>
       <c t="s" s="7" r="B215">
-        <v>768</v>
+        <v>778</v>
       </c>
       <c t="s" s="14" r="C215">
-        <v>769</v>
+        <v>779</v>
       </c>
       <c t="s" s="7" r="D215">
-        <v>770</v>
+        <v>780</v>
       </c>
       <c t="s" s="7" r="E215">
-        <v>771</v>
+        <v>781</v>
       </c>
     </row>
     <row r="216">
       <c s="9" r="A216"/>
-      <c t="s" s="7" r="B216">
-        <v>772</v>
-      </c>
-      <c t="s" s="14" r="C216">
-        <v>773</v>
-      </c>
-      <c t="s" s="7" r="D216">
-        <v>774</v>
-      </c>
-      <c t="s" s="7" r="E216">
-        <v>775</v>
-      </c>
+      <c s="17" r="B216"/>
+      <c s="29" r="C216"/>
+      <c s="17" r="D216"/>
+      <c s="17" r="E216"/>
     </row>
     <row r="217">
-      <c s="9" r="A217"/>
+      <c t="s" s="9" r="A217">
+        <v>782</v>
+      </c>
       <c t="s" s="7" r="B217">
-        <v>776</v>
+        <v>783</v>
       </c>
       <c t="s" s="14" r="C217">
-        <v>777</v>
+        <v>784</v>
       </c>
       <c t="s" s="7" r="D217">
-        <v>778</v>
+        <v>785</v>
       </c>
       <c t="s" s="7" r="E217">
-        <v>779</v>
+        <v>786</v>
       </c>
     </row>
     <row r="218">
       <c s="9" r="A218"/>
       <c t="s" s="7" r="B218">
-        <v>780</v>
+        <v>787</v>
       </c>
       <c t="s" s="14" r="C218">
-        <v>781</v>
+        <v>788</v>
       </c>
       <c t="s" s="7" r="D218">
-        <v>782</v>
+        <v>789</v>
       </c>
       <c t="s" s="7" r="E218">
-        <v>783</v>
+        <v>790</v>
       </c>
     </row>
     <row r="219">
       <c s="9" r="A219"/>
-      <c t="s" s="7" r="B219">
-        <v>784</v>
-      </c>
-      <c t="s" s="14" r="C219">
-        <v>785</v>
-      </c>
-      <c t="s" s="7" r="D219">
-        <v>786</v>
-      </c>
-      <c t="s" s="7" r="E219">
-        <v>787</v>
-      </c>
+      <c s="17" r="B219"/>
+      <c s="29" r="C219"/>
+      <c s="17" r="D219"/>
+      <c s="17" r="E219"/>
     </row>
     <row r="220">
-      <c s="9" r="A220"/>
+      <c t="s" s="9" r="A220">
+        <v>791</v>
+      </c>
       <c t="s" s="7" r="B220">
-        <v>788</v>
+        <v>792</v>
       </c>
       <c t="s" s="14" r="C220">
-        <v>789</v>
+        <v>793</v>
       </c>
       <c t="s" s="7" r="D220">
-        <v>790</v>
+        <v>794</v>
       </c>
       <c t="s" s="7" r="E220">
-        <v>791</v>
+        <v>795</v>
       </c>
     </row>
     <row r="221">
       <c s="9" r="A221"/>
-      <c t="s" s="7" r="B221">
-        <v>792</v>
-      </c>
-      <c t="s" s="14" r="C221">
-        <v>793</v>
-      </c>
-      <c t="s" s="7" r="D221">
-        <v>794</v>
-      </c>
-      <c t="s" s="7" r="E221">
-        <v>795</v>
-      </c>
+      <c s="17" r="B221"/>
+      <c s="8" r="C221"/>
+      <c s="17" r="D221"/>
+      <c s="17" r="E221"/>
     </row>
     <row r="222">
-      <c s="9" r="A222"/>
+      <c t="s" s="9" r="A222">
+        <v>796</v>
+      </c>
       <c t="s" s="7" r="B222">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c t="s" s="14" r="C222">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c t="s" s="7" r="D222">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c t="s" s="7" r="E222">
-        <v>799</v>
+        <v>800</v>
       </c>
     </row>
     <row r="223">
-      <c s="18" r="A223"/>
-      <c s="17" r="B223"/>
-      <c s="8" r="C223"/>
-      <c s="17" r="D223"/>
-      <c s="17" r="E223"/>
+      <c s="9" r="A223"/>
+      <c t="s" s="7" r="B223">
+        <v>801</v>
+      </c>
+      <c t="s" s="14" r="C223">
+        <v>802</v>
+      </c>
+      <c t="s" s="7" r="D223">
+        <v>803</v>
+      </c>
+      <c t="s" s="7" r="E223">
+        <v>804</v>
+      </c>
     </row>
     <row r="224">
-      <c t="s" s="9" r="A224">
-        <v>800</v>
-      </c>
+      <c s="9" r="A224"/>
       <c t="s" s="7" r="B224">
-        <v>801</v>
-      </c>
-      <c t="s" s="7" r="C224">
-        <v>802</v>
+        <v>805</v>
+      </c>
+      <c t="s" s="14" r="C224">
+        <v>806</v>
       </c>
       <c t="s" s="7" r="D224">
-        <v>803</v>
+        <v>807</v>
       </c>
       <c t="s" s="7" r="E224">
-        <v>804</v>
+        <v>808</v>
       </c>
     </row>
     <row r="225">
       <c s="9" r="A225"/>
       <c t="s" s="7" r="B225">
-        <v>805</v>
+        <v>809</v>
       </c>
       <c t="s" s="14" r="C225">
-        <v>806</v>
+        <v>810</v>
       </c>
       <c t="s" s="7" r="D225">
-        <v>807</v>
+        <v>811</v>
       </c>
       <c t="s" s="7" r="E225">
-        <v>808</v>
+        <v>812</v>
       </c>
     </row>
     <row r="226">
       <c s="9" r="A226"/>
       <c t="s" s="7" r="B226">
-        <v>809</v>
+        <v>813</v>
       </c>
       <c t="s" s="14" r="C226">
-        <v>810</v>
+        <v>814</v>
       </c>
       <c t="s" s="7" r="D226">
-        <v>811</v>
+        <v>815</v>
       </c>
       <c t="s" s="7" r="E226">
-        <v>812</v>
+        <v>816</v>
       </c>
     </row>
     <row r="227">
       <c s="9" r="A227"/>
       <c t="s" s="7" r="B227">
-        <v>813</v>
+        <v>817</v>
       </c>
       <c t="s" s="14" r="C227">
-        <v>814</v>
+        <v>818</v>
       </c>
       <c t="s" s="7" r="D227">
-        <v>815</v>
+        <v>819</v>
       </c>
       <c t="s" s="7" r="E227">
-        <v>816</v>
+        <v>820</v>
       </c>
     </row>
     <row r="228">
       <c s="9" r="A228"/>
       <c t="s" s="7" r="B228">
-        <v>817</v>
+        <v>821</v>
       </c>
       <c t="s" s="14" r="C228">
-        <v>542</v>
+        <v>822</v>
       </c>
       <c t="s" s="7" r="D228">
-        <v>132</v>
+        <v>823</v>
       </c>
       <c t="s" s="7" r="E228">
-        <v>544</v>
+        <v>824</v>
       </c>
     </row>
     <row r="229">
       <c s="9" r="A229"/>
       <c t="s" s="7" r="B229">
-        <v>818</v>
+        <v>825</v>
       </c>
       <c t="s" s="14" r="C229">
-        <v>819</v>
+        <v>826</v>
       </c>
       <c t="s" s="7" r="D229">
-        <v>820</v>
+        <v>827</v>
       </c>
       <c t="s" s="7" r="E229">
-        <v>821</v>
+        <v>828</v>
       </c>
     </row>
     <row r="230">
@@ -6930,736 +7028,835 @@
     </row>
     <row r="231">
       <c t="s" s="9" r="A231">
-        <v>822</v>
+        <v>829</v>
       </c>
       <c t="s" s="7" r="B231">
-        <v>823</v>
-      </c>
-      <c t="s" s="14" r="C231">
-        <v>824</v>
+        <v>830</v>
+      </c>
+      <c t="s" s="7" r="C231">
+        <v>831</v>
       </c>
       <c t="s" s="7" r="D231">
-        <v>825</v>
+        <v>832</v>
       </c>
       <c t="s" s="7" r="E231">
-        <v>826</v>
+        <v>833</v>
       </c>
     </row>
     <row r="232">
       <c s="9" r="A232"/>
       <c t="s" s="7" r="B232">
-        <v>827</v>
+        <v>834</v>
       </c>
       <c t="s" s="14" r="C232">
-        <v>828</v>
+        <v>835</v>
       </c>
       <c t="s" s="7" r="D232">
-        <v>829</v>
+        <v>836</v>
       </c>
       <c t="s" s="7" r="E232">
-        <v>830</v>
+        <v>837</v>
       </c>
     </row>
     <row r="233">
       <c s="9" r="A233"/>
       <c t="s" s="7" r="B233">
-        <v>831</v>
+        <v>838</v>
       </c>
       <c t="s" s="14" r="C233">
-        <v>832</v>
+        <v>839</v>
       </c>
       <c t="s" s="7" r="D233">
-        <v>833</v>
+        <v>840</v>
       </c>
       <c t="s" s="7" r="E233">
-        <v>834</v>
+        <v>841</v>
       </c>
     </row>
     <row r="234">
       <c s="9" r="A234"/>
       <c t="s" s="7" r="B234">
-        <v>835</v>
+        <v>842</v>
       </c>
       <c t="s" s="14" r="C234">
-        <v>836</v>
+        <v>843</v>
       </c>
       <c t="s" s="7" r="D234">
-        <v>837</v>
+        <v>844</v>
       </c>
       <c t="s" s="7" r="E234">
-        <v>837</v>
+        <v>845</v>
       </c>
     </row>
     <row r="235">
       <c s="9" r="A235"/>
       <c t="s" s="7" r="B235">
-        <v>838</v>
+        <v>846</v>
       </c>
       <c t="s" s="14" r="C235">
-        <v>839</v>
+        <v>571</v>
       </c>
       <c t="s" s="7" r="D235">
-        <v>840</v>
+        <v>132</v>
       </c>
       <c t="s" s="7" r="E235">
-        <v>841</v>
+        <v>573</v>
       </c>
     </row>
     <row r="236">
       <c s="9" r="A236"/>
       <c t="s" s="7" r="B236">
-        <v>842</v>
+        <v>847</v>
       </c>
       <c t="s" s="14" r="C236">
-        <v>843</v>
+        <v>848</v>
       </c>
       <c t="s" s="7" r="D236">
-        <v>844</v>
+        <v>849</v>
       </c>
       <c t="s" s="7" r="E236">
-        <v>845</v>
+        <v>850</v>
       </c>
     </row>
     <row r="237">
-      <c s="9" r="A237"/>
-      <c t="s" s="7" r="B237">
-        <v>846</v>
-      </c>
-      <c t="s" s="14" r="C237">
-        <v>847</v>
-      </c>
-      <c t="s" s="7" r="D237">
-        <v>848</v>
-      </c>
-      <c t="s" s="7" r="E237">
-        <v>849</v>
-      </c>
+      <c s="18" r="A237"/>
+      <c s="17" r="B237"/>
+      <c s="8" r="C237"/>
+      <c s="17" r="D237"/>
+      <c s="17" r="E237"/>
     </row>
     <row r="238">
-      <c s="9" r="A238"/>
+      <c t="s" s="9" r="A238">
+        <v>851</v>
+      </c>
       <c t="s" s="7" r="B238">
-        <v>850</v>
+        <v>852</v>
       </c>
       <c t="s" s="14" r="C238">
-        <v>851</v>
+        <v>853</v>
       </c>
       <c t="s" s="7" r="D238">
-        <v>852</v>
+        <v>854</v>
       </c>
       <c t="s" s="7" r="E238">
-        <v>853</v>
+        <v>855</v>
       </c>
     </row>
     <row r="239">
       <c s="9" r="A239"/>
       <c t="s" s="7" r="B239">
-        <v>854</v>
+        <v>856</v>
       </c>
       <c t="s" s="14" r="C239">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c t="s" s="7" r="D239">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c t="s" s="7" r="E239">
-        <v>857</v>
+        <v>859</v>
       </c>
     </row>
     <row r="240">
       <c s="9" r="A240"/>
       <c t="s" s="7" r="B240">
-        <v>858</v>
+        <v>860</v>
       </c>
       <c t="s" s="14" r="C240">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c t="s" s="7" r="D240">
-        <v>860</v>
+        <v>862</v>
       </c>
       <c t="s" s="7" r="E240">
-        <v>861</v>
+        <v>863</v>
       </c>
     </row>
     <row r="241">
       <c s="9" r="A241"/>
       <c t="s" s="7" r="B241">
-        <v>862</v>
+        <v>864</v>
       </c>
       <c t="s" s="14" r="C241">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c t="s" s="7" r="D241">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c t="s" s="7" r="E241">
-        <v>865</v>
+        <v>866</v>
       </c>
     </row>
     <row r="242">
       <c s="9" r="A242"/>
       <c t="s" s="7" r="B242">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c t="s" s="14" r="C242">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c t="s" s="7" r="D242">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c t="s" s="7" r="E242">
-        <v>869</v>
+        <v>870</v>
       </c>
     </row>
     <row r="243">
       <c s="9" r="A243"/>
       <c t="s" s="7" r="B243">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c t="s" s="14" r="C243">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c t="s" s="7" r="D243">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c t="s" s="7" r="E243">
-        <v>871</v>
+        <v>874</v>
       </c>
     </row>
     <row r="244">
       <c s="9" r="A244"/>
       <c t="s" s="7" r="B244">
-        <v>872</v>
+        <v>875</v>
       </c>
       <c t="s" s="14" r="C244">
-        <v>873</v>
+        <v>876</v>
       </c>
       <c t="s" s="7" r="D244">
-        <v>874</v>
+        <v>877</v>
       </c>
       <c t="s" s="7" r="E244">
-        <v>875</v>
+        <v>878</v>
       </c>
     </row>
     <row r="245">
       <c s="9" r="A245"/>
       <c t="s" s="7" r="B245">
-        <v>876</v>
+        <v>879</v>
       </c>
       <c t="s" s="14" r="C245">
-        <v>877</v>
+        <v>880</v>
       </c>
       <c t="s" s="7" r="D245">
-        <v>878</v>
+        <v>881</v>
       </c>
       <c t="s" s="7" r="E245">
-        <v>879</v>
+        <v>882</v>
       </c>
     </row>
     <row r="246">
       <c s="9" r="A246"/>
       <c t="s" s="7" r="B246">
-        <v>880</v>
+        <v>883</v>
       </c>
       <c t="s" s="14" r="C246">
-        <v>881</v>
+        <v>884</v>
       </c>
       <c t="s" s="7" r="D246">
-        <v>882</v>
+        <v>885</v>
       </c>
       <c t="s" s="7" r="E246">
-        <v>883</v>
+        <v>886</v>
       </c>
     </row>
     <row r="247">
       <c s="9" r="A247"/>
       <c t="s" s="7" r="B247">
-        <v>884</v>
+        <v>887</v>
       </c>
       <c t="s" s="14" r="C247">
-        <v>885</v>
+        <v>888</v>
       </c>
       <c t="s" s="7" r="D247">
-        <v>886</v>
+        <v>889</v>
       </c>
       <c t="s" s="7" r="E247">
-        <v>887</v>
+        <v>890</v>
       </c>
     </row>
     <row r="248">
       <c s="9" r="A248"/>
       <c t="s" s="7" r="B248">
-        <v>888</v>
+        <v>891</v>
       </c>
       <c t="s" s="14" r="C248">
-        <v>889</v>
+        <v>892</v>
       </c>
       <c t="s" s="7" r="D248">
-        <v>890</v>
+        <v>893</v>
       </c>
       <c t="s" s="7" r="E248">
-        <v>891</v>
+        <v>894</v>
       </c>
     </row>
     <row r="249">
       <c s="9" r="A249"/>
       <c t="s" s="7" r="B249">
-        <v>892</v>
+        <v>895</v>
       </c>
       <c t="s" s="14" r="C249">
-        <v>893</v>
+        <v>896</v>
       </c>
       <c t="s" s="7" r="D249">
-        <v>894</v>
+        <v>897</v>
       </c>
       <c t="s" s="7" r="E249">
-        <v>895</v>
+        <v>898</v>
       </c>
     </row>
     <row r="250">
       <c s="9" r="A250"/>
       <c t="s" s="7" r="B250">
-        <v>896</v>
+        <v>899</v>
       </c>
       <c t="s" s="14" r="C250">
-        <v>897</v>
+        <v>900</v>
       </c>
       <c t="s" s="7" r="D250">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c t="s" s="7" r="E250">
-        <v>899</v>
+        <v>900</v>
       </c>
     </row>
     <row r="251">
       <c s="9" r="A251"/>
-      <c s="17" r="B251"/>
-      <c s="8" r="C251"/>
-      <c s="17" r="D251"/>
-      <c s="17" r="E251"/>
+      <c t="s" s="7" r="B251">
+        <v>901</v>
+      </c>
+      <c t="s" s="14" r="C251">
+        <v>902</v>
+      </c>
+      <c t="s" s="7" r="D251">
+        <v>903</v>
+      </c>
+      <c t="s" s="7" r="E251">
+        <v>904</v>
+      </c>
     </row>
     <row r="252">
-      <c t="s" s="9" r="A252">
-        <v>900</v>
-      </c>
+      <c s="9" r="A252"/>
       <c t="s" s="7" r="B252">
-        <v>901</v>
+        <v>905</v>
       </c>
       <c t="s" s="14" r="C252">
-        <v>902</v>
+        <v>906</v>
       </c>
       <c t="s" s="7" r="D252">
-        <v>903</v>
+        <v>907</v>
       </c>
       <c t="s" s="7" r="E252">
-        <v>904</v>
+        <v>908</v>
       </c>
     </row>
     <row r="253">
       <c s="9" r="A253"/>
       <c t="s" s="7" r="B253">
-        <v>905</v>
+        <v>909</v>
       </c>
       <c t="s" s="14" r="C253">
-        <v>906</v>
+        <v>910</v>
       </c>
       <c t="s" s="7" r="D253">
-        <v>907</v>
+        <v>911</v>
       </c>
       <c t="s" s="7" r="E253">
-        <v>908</v>
+        <v>912</v>
       </c>
     </row>
     <row r="254">
       <c s="9" r="A254"/>
       <c t="s" s="7" r="B254">
-        <v>909</v>
+        <v>913</v>
       </c>
       <c t="s" s="14" r="C254">
-        <v>910</v>
+        <v>914</v>
       </c>
       <c t="s" s="7" r="D254">
-        <v>911</v>
+        <v>915</v>
       </c>
       <c t="s" s="7" r="E254">
-        <v>912</v>
+        <v>916</v>
       </c>
     </row>
     <row r="255">
       <c s="9" r="A255"/>
       <c t="s" s="7" r="B255">
-        <v>913</v>
+        <v>917</v>
       </c>
       <c t="s" s="14" r="C255">
-        <v>914</v>
+        <v>918</v>
       </c>
       <c t="s" s="7" r="D255">
-        <v>915</v>
+        <v>919</v>
       </c>
       <c t="s" s="7" r="E255">
-        <v>916</v>
+        <v>920</v>
       </c>
     </row>
     <row r="256">
       <c s="9" r="A256"/>
       <c t="s" s="7" r="B256">
-        <v>917</v>
+        <v>921</v>
       </c>
       <c t="s" s="14" r="C256">
-        <v>917</v>
-      </c>
-      <c t="s" s="19" r="D256">
-        <v>918</v>
-      </c>
-      <c t="s" s="19" r="E256">
-        <v>919</v>
+        <v>922</v>
+      </c>
+      <c t="s" s="7" r="D256">
+        <v>923</v>
+      </c>
+      <c t="s" s="7" r="E256">
+        <v>924</v>
       </c>
     </row>
     <row r="257">
       <c s="9" r="A257"/>
       <c t="s" s="7" r="B257">
-        <v>920</v>
+        <v>925</v>
       </c>
       <c t="s" s="14" r="C257">
-        <v>921</v>
+        <v>926</v>
       </c>
       <c t="s" s="7" r="D257">
-        <v>922</v>
+        <v>927</v>
       </c>
       <c t="s" s="7" r="E257">
-        <v>923</v>
+        <v>928</v>
       </c>
     </row>
     <row r="258">
       <c s="9" r="A258"/>
-      <c t="s" s="7" r="B258">
-        <v>924</v>
-      </c>
-      <c t="s" s="14" r="C258">
-        <v>925</v>
-      </c>
-      <c t="s" s="7" r="D258">
-        <v>926</v>
-      </c>
-      <c t="s" s="7" r="E258">
-        <v>927</v>
-      </c>
+      <c s="17" r="B258"/>
+      <c s="8" r="C258"/>
+      <c s="17" r="D258"/>
+      <c s="17" r="E258"/>
     </row>
     <row r="259">
-      <c t="s" s="17" r="A259">
-        <v>928</v>
-      </c>
-      <c s="27" r="B259"/>
+      <c t="s" s="9" r="A259">
+        <v>929</v>
+      </c>
+      <c t="s" s="7" r="B259">
+        <v>930</v>
+      </c>
       <c t="s" s="14" r="C259">
-        <v>929</v>
-      </c>
-      <c t="s" s="19" r="D259">
-        <v>930</v>
-      </c>
-      <c t="s" s="19" r="E259">
         <v>931</v>
       </c>
+      <c t="s" s="7" r="D259">
+        <v>932</v>
+      </c>
+      <c t="s" s="7" r="E259">
+        <v>933</v>
+      </c>
     </row>
     <row r="260">
-      <c s="18" r="A260"/>
-      <c s="17" r="B260"/>
-      <c s="8" r="C260"/>
-      <c s="17" r="D260"/>
-      <c s="17" r="E260"/>
+      <c s="9" r="A260"/>
+      <c t="s" s="7" r="B260">
+        <v>934</v>
+      </c>
+      <c t="s" s="14" r="C260">
+        <v>935</v>
+      </c>
+      <c t="s" s="7" r="D260">
+        <v>936</v>
+      </c>
+      <c t="s" s="7" r="E260">
+        <v>937</v>
+      </c>
     </row>
     <row r="261">
-      <c t="s" s="18" r="A261">
-        <v>932</v>
-      </c>
+      <c s="9" r="A261"/>
       <c t="s" s="7" r="B261">
-        <v>933</v>
-      </c>
-      <c t="s" s="7" r="C261">
-        <v>934</v>
+        <v>938</v>
+      </c>
+      <c t="s" s="14" r="C261">
+        <v>939</v>
       </c>
       <c t="s" s="7" r="D261">
-        <v>935</v>
+        <v>940</v>
       </c>
       <c t="s" s="7" r="E261">
-        <v>936</v>
+        <v>941</v>
       </c>
     </row>
     <row r="262">
-      <c s="15" r="A262"/>
+      <c s="9" r="A262"/>
       <c t="s" s="7" r="B262">
-        <v>937</v>
+        <v>942</v>
       </c>
       <c t="s" s="14" r="C262">
-        <v>938</v>
+        <v>943</v>
       </c>
       <c t="s" s="7" r="D262">
-        <v>939</v>
+        <v>944</v>
       </c>
       <c t="s" s="7" r="E262">
-        <v>940</v>
+        <v>945</v>
       </c>
     </row>
     <row r="263">
-      <c s="15" r="A263"/>
+      <c s="9" r="A263"/>
       <c t="s" s="7" r="B263">
-        <v>941</v>
-      </c>
-      <c t="s" s="7" r="C263">
-        <v>942</v>
-      </c>
-      <c t="s" s="7" r="D263">
-        <v>943</v>
-      </c>
-      <c t="s" s="7" r="E263">
-        <v>944</v>
+        <v>946</v>
+      </c>
+      <c t="s" s="14" r="C263">
+        <v>946</v>
+      </c>
+      <c t="s" s="19" r="D263">
+        <v>947</v>
+      </c>
+      <c t="s" s="19" r="E263">
+        <v>948</v>
       </c>
     </row>
     <row r="264">
-      <c s="18" r="A264"/>
+      <c s="9" r="A264"/>
       <c t="s" s="7" r="B264">
-        <v>945</v>
+        <v>949</v>
       </c>
       <c t="s" s="14" r="C264">
-        <v>946</v>
+        <v>950</v>
       </c>
       <c t="s" s="7" r="D264">
-        <v>947</v>
+        <v>951</v>
       </c>
       <c t="s" s="7" r="E264">
-        <v>948</v>
+        <v>952</v>
       </c>
     </row>
     <row r="265">
-      <c s="18" r="A265"/>
+      <c s="9" r="A265"/>
       <c t="s" s="7" r="B265">
-        <v>949</v>
-      </c>
-      <c t="s" s="7" r="C265">
-        <v>950</v>
+        <v>953</v>
+      </c>
+      <c t="s" s="14" r="C265">
+        <v>954</v>
       </c>
       <c t="s" s="7" r="D265">
-        <v>951</v>
+        <v>955</v>
       </c>
       <c t="s" s="7" r="E265">
-        <v>952</v>
+        <v>956</v>
       </c>
     </row>
     <row r="266">
-      <c s="18" r="A266"/>
-      <c t="s" s="7" r="B266">
-        <v>953</v>
-      </c>
+      <c t="s" s="17" r="A266">
+        <v>957</v>
+      </c>
+      <c s="26" r="B266"/>
       <c t="s" s="14" r="C266">
-        <v>954</v>
-      </c>
-      <c t="s" s="7" r="D266">
-        <v>955</v>
-      </c>
-      <c t="s" s="7" r="E266">
-        <v>956</v>
+        <v>958</v>
+      </c>
+      <c t="s" s="19" r="D266">
+        <v>959</v>
+      </c>
+      <c t="s" s="19" r="E266">
+        <v>960</v>
       </c>
     </row>
     <row r="267">
       <c s="18" r="A267"/>
-      <c t="s" s="7" r="B267">
-        <v>957</v>
-      </c>
-      <c t="s" s="7" r="C267">
-        <v>958</v>
-      </c>
-      <c t="s" s="7" r="D267">
-        <v>959</v>
-      </c>
-      <c t="s" s="7" r="E267">
-        <v>960</v>
-      </c>
+      <c s="17" r="B267"/>
+      <c s="8" r="C267"/>
+      <c s="17" r="D267"/>
+      <c s="17" r="E267"/>
     </row>
     <row r="268">
-      <c s="18" r="A268"/>
+      <c t="s" s="18" r="A268">
+        <v>961</v>
+      </c>
       <c t="s" s="7" r="B268">
-        <v>961</v>
-      </c>
-      <c t="s" s="14" r="C268">
         <v>962</v>
       </c>
+      <c t="s" s="7" r="C268">
+        <v>963</v>
+      </c>
       <c t="s" s="7" r="D268">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c t="s" s="7" r="E268">
-        <v>964</v>
+        <v>965</v>
       </c>
     </row>
     <row r="269">
-      <c s="18" r="A269"/>
+      <c s="15" r="A269"/>
       <c t="s" s="7" r="B269">
-        <v>965</v>
-      </c>
-      <c t="s" s="7" r="C269">
         <v>966</v>
       </c>
+      <c t="s" s="14" r="C269">
+        <v>967</v>
+      </c>
       <c t="s" s="7" r="D269">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c t="s" s="7" r="E269">
-        <v>968</v>
+        <v>969</v>
       </c>
     </row>
     <row r="270">
-      <c s="18" r="A270"/>
+      <c s="15" r="A270"/>
       <c t="s" s="7" r="B270">
-        <v>969</v>
-      </c>
-      <c t="s" s="14" r="C270">
         <v>970</v>
       </c>
+      <c t="s" s="7" r="C270">
+        <v>971</v>
+      </c>
       <c t="s" s="7" r="D270">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c t="s" s="7" r="E270">
-        <v>972</v>
+        <v>973</v>
       </c>
     </row>
     <row r="271">
       <c s="18" r="A271"/>
       <c t="s" s="7" r="B271">
-        <v>973</v>
-      </c>
-      <c t="s" s="7" r="C271">
         <v>974</v>
       </c>
+      <c t="s" s="14" r="C271">
+        <v>975</v>
+      </c>
       <c t="s" s="7" r="D271">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c t="s" s="7" r="E271">
-        <v>976</v>
+        <v>977</v>
       </c>
     </row>
     <row r="272">
       <c s="18" r="A272"/>
       <c t="s" s="7" r="B272">
-        <v>977</v>
-      </c>
-      <c t="s" s="14" r="C272">
-        <v>970</v>
+        <v>978</v>
+      </c>
+      <c t="s" s="7" r="C272">
+        <v>979</v>
       </c>
       <c t="s" s="7" r="D272">
-        <v>971</v>
+        <v>980</v>
       </c>
       <c t="s" s="7" r="E272">
-        <v>972</v>
+        <v>981</v>
       </c>
     </row>
     <row r="273">
       <c s="18" r="A273"/>
       <c t="s" s="7" r="B273">
-        <v>978</v>
+        <v>982</v>
       </c>
       <c t="s" s="14" r="C273">
-        <v>979</v>
+        <v>983</v>
       </c>
       <c t="s" s="7" r="D273">
-        <v>980</v>
+        <v>984</v>
       </c>
       <c t="s" s="7" r="E273">
-        <v>981</v>
+        <v>985</v>
       </c>
     </row>
     <row r="274">
       <c s="18" r="A274"/>
       <c t="s" s="7" r="B274">
-        <v>982</v>
-      </c>
-      <c t="s" s="14" r="C274">
-        <v>983</v>
+        <v>986</v>
+      </c>
+      <c t="s" s="7" r="C274">
+        <v>987</v>
       </c>
       <c t="s" s="7" r="D274">
-        <v>984</v>
+        <v>988</v>
       </c>
       <c t="s" s="7" r="E274">
-        <v>985</v>
+        <v>989</v>
       </c>
     </row>
     <row r="275">
       <c s="18" r="A275"/>
       <c t="s" s="7" r="B275">
-        <v>986</v>
-      </c>
-      <c t="s" s="7" r="C275">
-        <v>987</v>
+        <v>990</v>
+      </c>
+      <c t="s" s="14" r="C275">
+        <v>991</v>
       </c>
       <c t="s" s="7" r="D275">
-        <v>988</v>
+        <v>992</v>
       </c>
       <c t="s" s="7" r="E275">
-        <v>989</v>
+        <v>993</v>
       </c>
     </row>
     <row r="276">
       <c s="18" r="A276"/>
       <c t="s" s="7" r="B276">
-        <v>990</v>
-      </c>
-      <c t="s" s="14" r="C276">
-        <v>991</v>
+        <v>994</v>
+      </c>
+      <c t="s" s="7" r="C276">
+        <v>995</v>
       </c>
       <c t="s" s="7" r="D276">
-        <v>992</v>
+        <v>996</v>
       </c>
       <c t="s" s="7" r="E276">
-        <v>993</v>
+        <v>997</v>
       </c>
     </row>
     <row r="277">
-      <c s="9" r="A277"/>
+      <c s="18" r="A277"/>
       <c t="s" s="7" r="B277">
-        <v>994</v>
+        <v>998</v>
       </c>
       <c t="s" s="14" r="C277">
-        <v>995</v>
+        <v>999</v>
       </c>
       <c t="s" s="7" r="D277">
-        <v>996</v>
+        <v>1000</v>
       </c>
       <c t="s" s="7" r="E277">
-        <v>997</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="278">
-      <c t="s" s="9" r="A278">
-        <v>998</v>
-      </c>
-      <c t="s" s="14" r="B278">
+      <c s="18" r="A278"/>
+      <c t="s" s="7" r="B278">
+        <v>1002</v>
+      </c>
+      <c t="s" s="7" r="C278">
+        <v>1003</v>
+      </c>
+      <c t="s" s="7" r="D278">
+        <v>1004</v>
+      </c>
+      <c t="s" s="7" r="E278">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="279">
+      <c s="18" r="A279"/>
+      <c t="s" s="7" r="B279">
+        <v>1006</v>
+      </c>
+      <c t="s" s="14" r="C279">
         <v>999</v>
       </c>
-      <c t="s" s="14" r="C278">
+      <c t="s" s="7" r="D279">
         <v>1000</v>
       </c>
-      <c t="s" s="19" r="D278">
+      <c t="s" s="7" r="E279">
         <v>1001</v>
       </c>
-      <c t="s" s="7" r="E278">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="279">
-      <c s="9" r="A279"/>
-      <c t="s" s="14" r="B279">
-        <v>1003</v>
-      </c>
-      <c t="s" s="14" r="C279">
-        <v>1004</v>
-      </c>
-      <c t="s" s="19" r="D279">
-        <v>1005</v>
-      </c>
-      <c t="s" s="7" r="E279">
-        <v>1006</v>
-      </c>
     </row>
     <row r="280">
-      <c s="9" r="A280"/>
-      <c s="8" r="C280"/>
-      <c s="17" r="D280"/>
-      <c s="17" r="E280"/>
+      <c s="18" r="A280"/>
+      <c t="s" s="7" r="B280">
+        <v>1007</v>
+      </c>
+      <c t="s" s="14" r="C280">
+        <v>1008</v>
+      </c>
+      <c t="s" s="7" r="D280">
+        <v>1009</v>
+      </c>
+      <c t="s" s="7" r="E280">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="281">
+      <c s="18" r="A281"/>
+      <c t="s" s="7" r="B281">
+        <v>1011</v>
+      </c>
+      <c t="s" s="14" r="C281">
+        <v>1012</v>
+      </c>
+      <c t="s" s="7" r="D281">
+        <v>1013</v>
+      </c>
+      <c t="s" s="7" r="E281">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="282">
+      <c s="18" r="A282"/>
+      <c t="s" s="7" r="B282">
+        <v>1015</v>
+      </c>
+      <c t="s" s="7" r="C282">
+        <v>1016</v>
+      </c>
+      <c t="s" s="7" r="D282">
+        <v>1017</v>
+      </c>
+      <c t="s" s="7" r="E282">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="283">
+      <c s="18" r="A283"/>
+      <c t="s" s="7" r="B283">
+        <v>1019</v>
+      </c>
+      <c t="s" s="14" r="C283">
+        <v>1020</v>
+      </c>
+      <c t="s" s="7" r="D283">
+        <v>1021</v>
+      </c>
+      <c t="s" s="7" r="E283">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="284">
+      <c s="9" r="A284"/>
+      <c t="s" s="7" r="B284">
+        <v>1023</v>
+      </c>
+      <c t="s" s="14" r="C284">
+        <v>1024</v>
+      </c>
+      <c t="s" s="7" r="D284">
+        <v>1025</v>
+      </c>
+      <c t="s" s="7" r="E284">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="285">
+      <c t="s" s="9" r="A285">
+        <v>1027</v>
+      </c>
+      <c t="s" s="14" r="B285">
+        <v>1028</v>
+      </c>
+      <c t="s" s="14" r="C285">
+        <v>1029</v>
+      </c>
+      <c t="s" s="19" r="D285">
+        <v>1030</v>
+      </c>
+      <c t="s" s="7" r="E285">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="286">
+      <c s="9" r="A286"/>
+      <c t="s" s="14" r="B286">
+        <v>1032</v>
+      </c>
+      <c t="s" s="14" r="C286">
+        <v>1033</v>
+      </c>
+      <c t="s" s="19" r="D286">
+        <v>1034</v>
+      </c>
+      <c t="s" s="7" r="E286">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="287">
+      <c s="9" r="A287"/>
+      <c s="8" r="C287"/>
+      <c s="17" r="D287"/>
+      <c s="17" r="E287"/>
     </row>
   </sheetData>
 </worksheet>
@@ -7677,17 +7874,17 @@
   <sheetData>
     <row customHeight="1" r="1" ht="112.5">
       <c t="s" s="3" r="A1">
-        <v>1007</v>
+        <v>1036</v>
       </c>
     </row>
     <row customHeight="1" r="2" ht="112.5">
       <c t="s" s="4" r="A2">
-        <v>1008</v>
+        <v>1037</v>
       </c>
     </row>
     <row customHeight="1" r="3" ht="112.5">
       <c t="s" s="10" r="A3">
-        <v>1009</v>
+        <v>1038</v>
       </c>
     </row>
   </sheetData>
@@ -7702,164 +7899,164 @@
   <sheetFormatPr customHeight="1" defaultColWidth="9.86" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c s="34" r="A1"/>
-      <c s="34" r="B1"/>
-      <c s="34" r="C1"/>
-      <c s="34" r="D1"/>
-      <c s="34" r="E1"/>
-      <c s="34" r="F1"/>
+      <c s="33" r="A1"/>
+      <c s="33" r="B1"/>
+      <c s="33" r="C1"/>
+      <c s="33" r="D1"/>
+      <c s="33" r="E1"/>
+      <c s="33" r="F1"/>
     </row>
     <row r="2">
-      <c s="34" r="A2"/>
-      <c s="34" r="B2"/>
-      <c s="34" r="C2"/>
-      <c s="34" r="D2"/>
-      <c s="34" r="E2"/>
-      <c s="34" r="F2"/>
+      <c s="33" r="A2"/>
+      <c s="33" r="B2"/>
+      <c s="33" r="C2"/>
+      <c s="33" r="D2"/>
+      <c s="33" r="E2"/>
+      <c s="33" r="F2"/>
     </row>
     <row r="3">
-      <c s="34" r="A3"/>
-      <c s="34" r="B3"/>
-      <c s="34" r="C3"/>
-      <c s="34" r="D3"/>
-      <c s="34" r="E3"/>
-      <c s="34" r="F3"/>
+      <c s="33" r="A3"/>
+      <c s="33" r="B3"/>
+      <c s="33" r="C3"/>
+      <c s="33" r="D3"/>
+      <c s="33" r="E3"/>
+      <c s="33" r="F3"/>
     </row>
     <row r="4">
-      <c s="34" r="A4"/>
-      <c s="34" r="B4"/>
-      <c s="34" r="C4"/>
-      <c s="34" r="D4"/>
-      <c s="34" r="E4"/>
-      <c s="34" r="F4"/>
+      <c s="33" r="A4"/>
+      <c s="33" r="B4"/>
+      <c s="33" r="C4"/>
+      <c s="33" r="D4"/>
+      <c s="33" r="E4"/>
+      <c s="33" r="F4"/>
     </row>
     <row r="5">
-      <c s="34" r="A5"/>
-      <c s="34" r="B5"/>
-      <c s="34" r="C5"/>
-      <c s="34" r="D5"/>
-      <c s="34" r="E5"/>
-      <c s="34" r="F5"/>
+      <c s="33" r="A5"/>
+      <c s="33" r="B5"/>
+      <c s="33" r="C5"/>
+      <c s="33" r="D5"/>
+      <c s="33" r="E5"/>
+      <c s="33" r="F5"/>
     </row>
     <row r="6">
-      <c s="34" r="A6"/>
-      <c s="34" r="B6"/>
-      <c s="34" r="C6"/>
-      <c s="34" r="D6"/>
-      <c s="34" r="E6"/>
-      <c s="34" r="F6"/>
+      <c s="33" r="A6"/>
+      <c s="33" r="B6"/>
+      <c s="33" r="C6"/>
+      <c s="33" r="D6"/>
+      <c s="33" r="E6"/>
+      <c s="33" r="F6"/>
     </row>
     <row r="7">
-      <c s="34" r="A7"/>
-      <c s="34" r="B7"/>
-      <c s="34" r="C7"/>
-      <c s="34" r="D7"/>
-      <c s="34" r="E7"/>
-      <c s="34" r="F7"/>
+      <c s="33" r="A7"/>
+      <c s="33" r="B7"/>
+      <c s="33" r="C7"/>
+      <c s="33" r="D7"/>
+      <c s="33" r="E7"/>
+      <c s="33" r="F7"/>
     </row>
     <row r="8">
-      <c s="34" r="A8"/>
-      <c s="34" r="B8"/>
-      <c s="34" r="C8"/>
-      <c s="34" r="D8"/>
-      <c s="34" r="E8"/>
-      <c s="34" r="F8"/>
+      <c s="33" r="A8"/>
+      <c s="33" r="B8"/>
+      <c s="33" r="C8"/>
+      <c s="33" r="D8"/>
+      <c s="33" r="E8"/>
+      <c s="33" r="F8"/>
     </row>
     <row r="9">
-      <c s="34" r="A9"/>
-      <c s="34" r="B9"/>
-      <c s="34" r="C9"/>
-      <c s="34" r="D9"/>
-      <c s="34" r="E9"/>
-      <c s="34" r="F9"/>
+      <c s="33" r="A9"/>
+      <c s="33" r="B9"/>
+      <c s="33" r="C9"/>
+      <c s="33" r="D9"/>
+      <c s="33" r="E9"/>
+      <c s="33" r="F9"/>
     </row>
     <row r="10">
-      <c s="34" r="A10"/>
-      <c s="34" r="B10"/>
-      <c s="34" r="C10"/>
-      <c s="34" r="D10"/>
-      <c s="34" r="E10"/>
-      <c s="34" r="F10"/>
+      <c s="33" r="A10"/>
+      <c s="33" r="B10"/>
+      <c s="33" r="C10"/>
+      <c s="33" r="D10"/>
+      <c s="33" r="E10"/>
+      <c s="33" r="F10"/>
     </row>
     <row r="11">
-      <c s="34" r="A11"/>
-      <c s="34" r="B11"/>
-      <c s="34" r="C11"/>
-      <c s="34" r="D11"/>
-      <c s="34" r="E11"/>
-      <c s="34" r="F11"/>
+      <c s="33" r="A11"/>
+      <c s="33" r="B11"/>
+      <c s="33" r="C11"/>
+      <c s="33" r="D11"/>
+      <c s="33" r="E11"/>
+      <c s="33" r="F11"/>
     </row>
     <row r="12">
-      <c s="34" r="A12"/>
-      <c s="34" r="B12"/>
-      <c s="34" r="C12"/>
-      <c s="34" r="D12"/>
-      <c s="34" r="E12"/>
-      <c s="34" r="F12"/>
+      <c s="33" r="A12"/>
+      <c s="33" r="B12"/>
+      <c s="33" r="C12"/>
+      <c s="33" r="D12"/>
+      <c s="33" r="E12"/>
+      <c s="33" r="F12"/>
     </row>
     <row r="13">
-      <c s="34" r="A13"/>
-      <c s="34" r="B13"/>
-      <c s="34" r="C13"/>
-      <c s="34" r="D13"/>
-      <c s="34" r="E13"/>
-      <c s="34" r="F13"/>
+      <c s="33" r="A13"/>
+      <c s="33" r="B13"/>
+      <c s="33" r="C13"/>
+      <c s="33" r="D13"/>
+      <c s="33" r="E13"/>
+      <c s="33" r="F13"/>
     </row>
     <row r="14">
-      <c s="34" r="A14"/>
-      <c s="34" r="B14"/>
-      <c s="34" r="C14"/>
-      <c s="34" r="D14"/>
-      <c s="34" r="E14"/>
-      <c s="34" r="F14"/>
+      <c s="33" r="A14"/>
+      <c s="33" r="B14"/>
+      <c s="33" r="C14"/>
+      <c s="33" r="D14"/>
+      <c s="33" r="E14"/>
+      <c s="33" r="F14"/>
     </row>
     <row r="15">
-      <c s="34" r="A15"/>
-      <c s="34" r="B15"/>
-      <c s="34" r="C15"/>
-      <c s="34" r="D15"/>
-      <c s="34" r="E15"/>
-      <c s="34" r="F15"/>
+      <c s="33" r="A15"/>
+      <c s="33" r="B15"/>
+      <c s="33" r="C15"/>
+      <c s="33" r="D15"/>
+      <c s="33" r="E15"/>
+      <c s="33" r="F15"/>
     </row>
     <row r="16">
-      <c s="34" r="A16"/>
-      <c s="34" r="B16"/>
-      <c s="34" r="C16"/>
-      <c s="34" r="D16"/>
-      <c s="34" r="E16"/>
-      <c s="34" r="F16"/>
+      <c s="33" r="A16"/>
+      <c s="33" r="B16"/>
+      <c s="33" r="C16"/>
+      <c s="33" r="D16"/>
+      <c s="33" r="E16"/>
+      <c s="33" r="F16"/>
     </row>
     <row r="17">
-      <c s="34" r="A17"/>
-      <c s="34" r="B17"/>
-      <c s="34" r="C17"/>
-      <c s="34" r="D17"/>
-      <c s="34" r="E17"/>
-      <c s="34" r="F17"/>
+      <c s="33" r="A17"/>
+      <c s="33" r="B17"/>
+      <c s="33" r="C17"/>
+      <c s="33" r="D17"/>
+      <c s="33" r="E17"/>
+      <c s="33" r="F17"/>
     </row>
     <row r="18">
-      <c s="34" r="A18"/>
-      <c s="34" r="B18"/>
-      <c s="34" r="C18"/>
-      <c s="34" r="D18"/>
-      <c s="34" r="E18"/>
-      <c s="34" r="F18"/>
+      <c s="33" r="A18"/>
+      <c s="33" r="B18"/>
+      <c s="33" r="C18"/>
+      <c s="33" r="D18"/>
+      <c s="33" r="E18"/>
+      <c s="33" r="F18"/>
     </row>
     <row r="19">
-      <c s="34" r="A19"/>
-      <c s="34" r="B19"/>
-      <c s="34" r="C19"/>
-      <c s="34" r="D19"/>
-      <c s="34" r="E19"/>
-      <c s="34" r="F19"/>
+      <c s="33" r="A19"/>
+      <c s="33" r="B19"/>
+      <c s="33" r="C19"/>
+      <c s="33" r="D19"/>
+      <c s="33" r="E19"/>
+      <c s="33" r="F19"/>
     </row>
     <row r="20">
-      <c s="34" r="A20"/>
-      <c s="34" r="B20"/>
-      <c s="34" r="C20"/>
-      <c s="34" r="D20"/>
-      <c s="34" r="E20"/>
-      <c s="34" r="F20"/>
+      <c s="33" r="A20"/>
+      <c s="33" r="B20"/>
+      <c s="33" r="C20"/>
+      <c s="33" r="D20"/>
+      <c s="33" r="E20"/>
+      <c s="33" r="F20"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
Implement resources for explanations on delivery tab (EWD-22811)
Former-commit-id: 93f322a9e1fe8a19bbf352413fcd9b219ebf21d5
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="1107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="1111">
   <si>
     <t>nnot</t>
   </si>
@@ -885,12 +885,24 @@
     <t>Assemble learning experience</t>
   </si>
   <si>
+    <t>Leerervaring samenstellen</t>
+  </si>
+  <si>
+    <t>Lernerfahrung zusammenstellen</t>
+  </si>
+  <si>
     <t>updatePackageDescription</t>
   </si>
   <si>
     <t>Reassemble learning experience</t>
   </si>
   <si>
+    <t>Leerervaring opnieuw samenstellen</t>
+  </si>
+  <si>
+    <t>Lernerfahrung neu zusammenstellen</t>
+  </si>
+  <si>
     <t>publishOnlineDesciption</t>
   </si>
   <si>
@@ -931,6 +943,12 @@
   </si>
   <si>
     <t>Open link to view learning experience</t>
+  </si>
+  <si>
+    <t>Koppeling openen om leerervaring te bekijken</t>
+  </si>
+  <si>
+    <t>Link zur Lernerfahrung öffnen</t>
   </si>
   <si>
     <t>assemble</t>
@@ -1867,12 +1885,6 @@
   </si>
   <si>
     <t>Build learning experience</t>
-  </si>
-  <si>
-    <t>Leerervaring samenstellen</t>
-  </si>
-  <si>
-    <t>Lernerfahrung zusammenstellen</t>
   </si>
   <si>
     <t>clickToAddObjectivesIntoExperience</t>
@@ -3604,7 +3616,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="32">
+  <fills count="31">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3771,12 +3783,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -3806,7 +3812,7 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
@@ -3905,16 +3911,13 @@
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="28" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" fillId="29" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
     <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="23"/>
-    <xf applyAlignment="1" fillId="30" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="24" applyFill="1">
+    <xf applyAlignment="1" fillId="29" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="24" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="31" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+    <xf applyAlignment="1" fillId="30" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5044,90 +5047,101 @@
       </c>
     </row>
     <row r="75">
-      <c s="12" r="A75"/>
       <c t="s" s="7" r="B75">
         <v>287</v>
       </c>
       <c t="s" s="7" r="C75">
         <v>288</v>
       </c>
-      <c s="24" r="D75"/>
-      <c s="23" r="E75"/>
+      <c t="s" s="36" r="D75">
+        <v>289</v>
+      </c>
+      <c t="s" s="19" r="E75">
+        <v>290</v>
+      </c>
     </row>
     <row r="76">
       <c s="12" r="A76"/>
       <c t="s" s="7" r="B76">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c t="s" s="7" r="C76">
-        <v>290</v>
-      </c>
-      <c s="33" r="D76"/>
-      <c s="33" r="E76"/>
+        <v>292</v>
+      </c>
+      <c t="s" s="2" r="D76">
+        <v>293</v>
+      </c>
+      <c t="s" s="2" r="E76">
+        <v>294</v>
+      </c>
     </row>
     <row r="77">
       <c s="12" r="A77"/>
       <c t="s" s="27" r="B77">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c t="s" s="7" r="C77">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c t="s" s="2" r="D77">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c t="s" s="2" r="E77">
-        <v>294</v>
+        <v>298</v>
       </c>
     </row>
     <row r="78">
       <c s="12" r="A78"/>
       <c t="s" s="27" r="B78">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c t="s" s="7" r="C78">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c t="s" s="2" r="D78">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c t="s" s="2" r="E78">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row r="79">
       <c s="12" r="A79"/>
       <c t="s" s="7" r="B79">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c t="s" s="7" r="C79">
-        <v>300</v>
-      </c>
-      <c t="s" s="37" r="D79">
-        <v>301</v>
+        <v>304</v>
+      </c>
+      <c t="s" s="36" r="D79">
+        <v>305</v>
       </c>
       <c t="s" s="19" r="E79">
-        <v>302</v>
+        <v>306</v>
       </c>
     </row>
     <row r="80">
       <c s="12" r="A80"/>
       <c t="s" s="7" r="B80">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c t="s" s="7" r="C80">
-        <v>304</v>
-      </c>
-      <c s="24" r="D80"/>
-      <c s="23" r="E80"/>
+        <v>308</v>
+      </c>
+      <c t="s" s="24" r="D80">
+        <v>309</v>
+      </c>
+      <c t="s" s="23" r="E80">
+        <v>310</v>
+      </c>
     </row>
     <row r="81">
       <c s="12" r="A81"/>
       <c t="s" s="1" r="B81">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c t="s" s="1" r="C81">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c t="s" s="1" r="D81">
         <v>193</v>
@@ -5139,13 +5153,13 @@
     <row r="82">
       <c s="12" r="A82"/>
       <c t="s" s="1" r="B82">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c t="s" s="1" r="C82">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c t="s" s="1" r="D82">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c t="s" s="1" r="E82">
         <v>202</v>
@@ -5154,31 +5168,31 @@
     <row r="83">
       <c s="12" r="A83"/>
       <c t="s" s="1" r="B83">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c t="s" s="1" r="C83">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c t="s" s="1" r="D83">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c t="s" s="1" r="E83">
-        <v>313</v>
+        <v>319</v>
       </c>
     </row>
     <row r="84">
       <c s="12" r="A84"/>
       <c t="s" s="1" r="B84">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c t="s" s="1" r="C84">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c t="s" s="1" r="D84">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c t="s" s="1" r="E84">
-        <v>317</v>
+        <v>323</v>
       </c>
     </row>
     <row r="85">
@@ -5190,132 +5204,132 @@
     </row>
     <row r="86">
       <c t="s" s="12" r="A86">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c t="s" s="7" r="B86">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c t="s" s="7" r="C86">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c t="s" s="7" r="D86">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c t="s" s="7" r="E86">
-        <v>322</v>
+        <v>328</v>
       </c>
     </row>
     <row r="87">
       <c s="12" r="A87"/>
       <c t="s" s="7" r="B87">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c t="s" s="7" r="C87">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c t="s" s="7" r="D87">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c t="s" s="7" r="E87">
-        <v>326</v>
+        <v>332</v>
       </c>
     </row>
     <row r="88">
       <c t="s" s="14" r="B88">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c t="s" s="14" r="C88">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c t="s" s="14" r="D88">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c t="s" s="14" r="E88">
-        <v>328</v>
+        <v>334</v>
       </c>
     </row>
     <row r="89">
       <c t="s" s="14" r="B89">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c t="s" s="14" r="C89">
-        <v>330</v>
-      </c>
-      <c t="s" s="37" r="D89">
-        <v>331</v>
-      </c>
-      <c t="s" s="37" r="E89">
-        <v>332</v>
+        <v>336</v>
+      </c>
+      <c t="s" s="36" r="D89">
+        <v>337</v>
+      </c>
+      <c t="s" s="36" r="E89">
+        <v>338</v>
       </c>
     </row>
     <row r="90">
       <c t="s" s="14" r="B90">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c t="s" s="14" r="C90">
-        <v>334</v>
-      </c>
-      <c t="s" s="37" r="D90">
-        <v>335</v>
-      </c>
-      <c t="s" s="37" r="E90">
-        <v>336</v>
+        <v>340</v>
+      </c>
+      <c t="s" s="36" r="D90">
+        <v>341</v>
+      </c>
+      <c t="s" s="36" r="E90">
+        <v>342</v>
       </c>
     </row>
     <row r="91">
       <c t="s" s="14" r="B91">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c t="s" s="14" r="C91">
-        <v>338</v>
-      </c>
-      <c t="s" s="37" r="D91">
-        <v>339</v>
-      </c>
-      <c t="s" s="37" r="E91">
-        <v>340</v>
+        <v>344</v>
+      </c>
+      <c t="s" s="36" r="D91">
+        <v>345</v>
+      </c>
+      <c t="s" s="36" r="E91">
+        <v>346</v>
       </c>
     </row>
     <row r="92">
       <c t="s" s="14" r="B92">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c t="s" s="14" r="C92">
-        <v>342</v>
-      </c>
-      <c t="s" s="37" r="D92">
-        <v>343</v>
-      </c>
-      <c t="s" s="37" r="E92">
-        <v>344</v>
+        <v>348</v>
+      </c>
+      <c t="s" s="36" r="D92">
+        <v>349</v>
+      </c>
+      <c t="s" s="36" r="E92">
+        <v>350</v>
       </c>
     </row>
     <row r="93">
       <c t="s" s="14" r="B93">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c t="s" s="14" r="C93">
-        <v>346</v>
-      </c>
-      <c t="s" s="37" r="D93">
-        <v>347</v>
-      </c>
-      <c t="s" s="37" r="E93">
-        <v>348</v>
+        <v>352</v>
+      </c>
+      <c t="s" s="36" r="D93">
+        <v>353</v>
+      </c>
+      <c t="s" s="36" r="E93">
+        <v>354</v>
       </c>
     </row>
     <row r="94">
       <c t="s" s="14" r="B94">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c t="s" s="14" r="C94">
-        <v>350</v>
-      </c>
-      <c t="s" s="37" r="D94">
-        <v>351</v>
-      </c>
-      <c t="s" s="37" r="E94">
-        <v>352</v>
+        <v>356</v>
+      </c>
+      <c t="s" s="36" r="D94">
+        <v>357</v>
+      </c>
+      <c t="s" s="36" r="E94">
+        <v>358</v>
       </c>
     </row>
     <row r="95">
@@ -5327,94 +5341,94 @@
     </row>
     <row r="96">
       <c t="s" s="12" r="A96">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c t="s" s="7" r="B96">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c t="s" s="7" r="C96">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c t="s" s="7" r="D96">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c t="s" s="7" r="E96">
-        <v>357</v>
+        <v>363</v>
       </c>
     </row>
     <row r="97">
       <c s="12" r="A97"/>
       <c t="s" s="7" r="B97">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c t="s" s="7" r="C97">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c t="s" s="7" r="D97">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c t="s" s="7" r="E97">
-        <v>361</v>
+        <v>367</v>
       </c>
     </row>
     <row r="98">
       <c s="12" r="A98"/>
       <c t="s" s="7" r="B98">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c t="s" s="7" r="C98">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c t="s" s="7" r="D98">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c t="s" s="7" r="E98">
-        <v>365</v>
+        <v>371</v>
       </c>
     </row>
     <row r="99">
       <c s="12" r="A99"/>
       <c t="s" s="7" r="B99">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c t="s" s="7" r="C99">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c t="s" s="7" r="D99">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c t="s" s="7" r="E99">
-        <v>369</v>
+        <v>375</v>
       </c>
     </row>
     <row r="100">
       <c s="12" r="A100"/>
       <c t="s" s="7" r="B100">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c t="s" s="7" r="C100">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c t="s" s="7" r="D100">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c t="s" s="7" r="E100">
-        <v>373</v>
+        <v>379</v>
       </c>
     </row>
     <row r="101">
       <c s="12" r="A101"/>
       <c t="s" s="7" r="B101">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c t="s" s="7" r="C101">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c t="s" s="7" r="D101">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c t="s" s="7" r="E101">
-        <v>377</v>
+        <v>383</v>
       </c>
     </row>
     <row r="102">
@@ -5426,139 +5440,139 @@
     </row>
     <row r="103">
       <c t="s" s="12" r="A103">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c t="s" s="7" r="B103">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c t="s" s="7" r="C103">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c t="s" s="7" r="D103">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c t="s" s="7" r="E103">
-        <v>382</v>
+        <v>388</v>
       </c>
     </row>
     <row r="104">
       <c s="12" r="A104"/>
       <c t="s" s="7" r="B104">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c t="s" s="7" r="C104">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c t="s" s="7" r="D104">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c t="s" s="7" r="E104">
-        <v>386</v>
+        <v>392</v>
       </c>
     </row>
     <row r="105">
       <c s="12" r="A105"/>
       <c t="s" s="7" r="B105">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c t="s" s="7" r="C105">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c t="s" s="7" r="D105">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c t="s" s="7" r="E105">
-        <v>390</v>
+        <v>396</v>
       </c>
     </row>
     <row r="106">
       <c s="12" r="A106"/>
       <c t="s" s="7" r="B106">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c t="s" s="7" r="C106">
-        <v>392</v>
+        <v>398</v>
       </c>
       <c t="s" s="7" r="D106">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c t="s" s="7" r="E106">
-        <v>394</v>
+        <v>400</v>
       </c>
     </row>
     <row r="107">
       <c s="12" r="A107"/>
       <c t="s" s="7" r="B107">
-        <v>395</v>
+        <v>401</v>
       </c>
       <c t="s" s="7" r="C107">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c t="s" s="7" r="D107">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c t="s" s="7" r="E107">
-        <v>398</v>
+        <v>404</v>
       </c>
     </row>
     <row r="108">
       <c s="12" r="A108"/>
       <c t="s" s="7" r="B108">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c t="s" s="7" r="C108">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c t="s" s="7" r="D108">
-        <v>401</v>
+        <v>407</v>
       </c>
       <c t="s" s="7" r="E108">
-        <v>402</v>
+        <v>408</v>
       </c>
     </row>
     <row r="109">
       <c s="12" r="A109"/>
       <c t="s" s="7" r="B109">
-        <v>403</v>
+        <v>409</v>
       </c>
       <c t="s" s="7" r="C109">
-        <v>404</v>
+        <v>410</v>
       </c>
       <c t="s" s="7" r="D109">
-        <v>405</v>
+        <v>411</v>
       </c>
       <c t="s" s="7" r="E109">
-        <v>406</v>
+        <v>412</v>
       </c>
     </row>
     <row r="110">
       <c s="12" r="A110"/>
       <c t="s" s="7" r="B110">
-        <v>407</v>
+        <v>413</v>
       </c>
       <c t="s" s="7" r="C110">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c t="s" s="7" r="D110">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c t="s" s="7" r="E110">
-        <v>410</v>
+        <v>416</v>
       </c>
     </row>
     <row r="111">
       <c s="12" r="A111"/>
       <c t="s" s="7" r="B111">
-        <v>411</v>
+        <v>417</v>
       </c>
       <c t="s" s="7" r="C111">
-        <v>412</v>
+        <v>418</v>
       </c>
       <c t="s" s="7" r="D111">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c t="s" s="7" r="E111">
-        <v>414</v>
+        <v>420</v>
       </c>
     </row>
     <row r="112">
@@ -5570,229 +5584,229 @@
     </row>
     <row r="113">
       <c t="s" s="12" r="A113">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c t="s" s="7" r="B113">
-        <v>416</v>
+        <v>422</v>
       </c>
       <c t="s" s="7" r="C113">
-        <v>417</v>
+        <v>423</v>
       </c>
       <c t="s" s="7" r="D113">
-        <v>418</v>
+        <v>424</v>
       </c>
       <c t="s" s="7" r="E113">
-        <v>419</v>
+        <v>425</v>
       </c>
     </row>
     <row r="114">
       <c s="12" r="A114"/>
       <c t="s" s="7" r="B114">
-        <v>420</v>
+        <v>426</v>
       </c>
       <c t="s" s="7" r="C114">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c t="s" s="7" r="D114">
-        <v>422</v>
+        <v>428</v>
       </c>
       <c t="s" s="7" r="E114">
-        <v>423</v>
+        <v>429</v>
       </c>
     </row>
     <row r="115">
       <c s="11" r="A115"/>
       <c t="s" s="7" r="B115">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c t="s" s="7" r="C115">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c t="s" s="7" r="D115">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c t="s" s="7" r="E115">
-        <v>427</v>
+        <v>433</v>
       </c>
     </row>
     <row r="116">
       <c s="11" r="A116"/>
       <c t="s" s="7" r="B116">
-        <v>428</v>
+        <v>434</v>
       </c>
       <c t="s" s="7" r="C116">
-        <v>429</v>
+        <v>435</v>
       </c>
       <c t="s" s="7" r="D116">
-        <v>430</v>
+        <v>436</v>
       </c>
       <c t="s" s="7" r="E116">
-        <v>431</v>
+        <v>437</v>
       </c>
     </row>
     <row r="117">
       <c s="11" r="A117"/>
       <c t="s" s="7" r="B117">
-        <v>432</v>
+        <v>438</v>
       </c>
       <c t="s" s="7" r="C117">
-        <v>433</v>
+        <v>439</v>
       </c>
       <c t="s" s="7" r="D117">
-        <v>434</v>
+        <v>440</v>
       </c>
       <c t="s" s="7" r="E117">
-        <v>435</v>
+        <v>441</v>
       </c>
     </row>
     <row r="118">
       <c s="11" r="A118"/>
       <c t="s" s="7" r="B118">
-        <v>436</v>
+        <v>442</v>
       </c>
       <c t="s" s="7" r="C118">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c t="s" s="7" r="D118">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c t="s" s="7" r="E118">
-        <v>439</v>
+        <v>445</v>
       </c>
     </row>
     <row r="119">
       <c s="11" r="A119"/>
       <c t="s" s="7" r="B119">
-        <v>440</v>
+        <v>446</v>
       </c>
       <c t="s" s="7" r="C119">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c t="s" s="7" r="D119">
-        <v>442</v>
+        <v>448</v>
       </c>
       <c t="s" s="7" r="E119">
-        <v>443</v>
+        <v>449</v>
       </c>
     </row>
     <row r="120">
       <c s="11" r="A120"/>
       <c t="s" s="7" r="B120">
-        <v>444</v>
+        <v>450</v>
       </c>
       <c t="s" s="7" r="C120">
-        <v>445</v>
+        <v>451</v>
       </c>
       <c t="s" s="7" r="D120">
-        <v>446</v>
+        <v>452</v>
       </c>
       <c t="s" s="7" r="E120">
-        <v>447</v>
+        <v>453</v>
       </c>
     </row>
     <row r="121">
       <c s="11" r="A121"/>
       <c t="s" s="7" r="B121">
-        <v>448</v>
+        <v>454</v>
       </c>
       <c t="s" s="7" r="C121">
-        <v>449</v>
+        <v>455</v>
       </c>
       <c t="s" s="7" r="D121">
-        <v>450</v>
+        <v>456</v>
       </c>
       <c t="s" s="7" r="E121">
-        <v>451</v>
+        <v>457</v>
       </c>
     </row>
     <row r="122">
       <c s="11" r="A122"/>
       <c t="s" s="7" r="B122">
-        <v>452</v>
+        <v>458</v>
       </c>
       <c t="s" s="7" r="C122">
-        <v>453</v>
+        <v>459</v>
       </c>
       <c t="s" s="7" r="D122">
-        <v>454</v>
+        <v>460</v>
       </c>
       <c t="s" s="7" r="E122">
-        <v>455</v>
+        <v>461</v>
       </c>
     </row>
     <row r="123">
       <c s="11" r="A123"/>
       <c t="s" s="7" r="B123">
-        <v>456</v>
+        <v>462</v>
       </c>
       <c t="s" s="7" r="C123">
-        <v>457</v>
+        <v>463</v>
       </c>
       <c t="s" s="7" r="D123">
-        <v>458</v>
+        <v>464</v>
       </c>
       <c t="s" s="7" r="E123">
-        <v>459</v>
+        <v>465</v>
       </c>
     </row>
     <row r="124">
       <c s="11" r="A124"/>
       <c t="s" s="7" r="B124">
-        <v>460</v>
+        <v>466</v>
       </c>
       <c t="s" s="7" r="C124">
-        <v>461</v>
+        <v>467</v>
       </c>
       <c t="s" s="7" r="D124">
-        <v>462</v>
+        <v>468</v>
       </c>
       <c t="s" s="7" r="E124">
-        <v>463</v>
+        <v>469</v>
       </c>
     </row>
     <row r="125">
       <c s="11" r="A125"/>
       <c t="s" s="7" r="B125">
-        <v>464</v>
+        <v>470</v>
       </c>
       <c t="s" s="7" r="C125">
-        <v>465</v>
+        <v>471</v>
       </c>
       <c t="s" s="7" r="D125">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c t="s" s="7" r="E125">
-        <v>467</v>
+        <v>473</v>
       </c>
     </row>
     <row r="126">
       <c s="11" r="A126"/>
       <c t="s" s="7" r="B126">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c t="s" s="7" r="C126">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c t="s" s="7" r="D126">
-        <v>470</v>
+        <v>476</v>
       </c>
       <c t="s" s="7" r="E126">
-        <v>471</v>
+        <v>477</v>
       </c>
     </row>
     <row r="127">
       <c s="11" r="A127"/>
       <c t="s" s="7" r="B127">
-        <v>472</v>
+        <v>478</v>
       </c>
       <c t="s" s="7" r="C127">
-        <v>473</v>
+        <v>479</v>
       </c>
       <c t="s" s="7" r="D127">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c t="s" s="7" r="E127">
-        <v>475</v>
+        <v>481</v>
       </c>
     </row>
     <row r="128">
@@ -5804,91 +5818,91 @@
     </row>
     <row r="129">
       <c t="s" s="11" r="A129">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c t="s" s="7" r="B129">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c t="s" s="7" r="C129">
-        <v>478</v>
+        <v>484</v>
       </c>
       <c t="s" s="7" r="D129">
-        <v>479</v>
+        <v>485</v>
       </c>
       <c t="s" s="7" r="E129">
-        <v>480</v>
+        <v>486</v>
       </c>
     </row>
     <row r="130">
       <c s="11" r="A130"/>
       <c t="s" s="7" r="B130">
-        <v>481</v>
+        <v>487</v>
       </c>
       <c t="s" s="7" r="C130">
-        <v>482</v>
+        <v>488</v>
       </c>
       <c t="s" s="7" r="D130">
-        <v>483</v>
+        <v>489</v>
       </c>
       <c t="s" s="7" r="E130">
-        <v>484</v>
+        <v>490</v>
       </c>
     </row>
     <row r="131">
       <c s="11" r="A131"/>
       <c t="s" s="7" r="B131">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c t="s" s="7" r="C131">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c t="s" s="7" r="D131">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c t="s" s="7" r="E131">
-        <v>488</v>
+        <v>494</v>
       </c>
     </row>
     <row r="132">
       <c s="11" r="A132"/>
       <c t="s" s="7" r="B132">
-        <v>489</v>
+        <v>495</v>
       </c>
       <c t="s" s="7" r="C132">
-        <v>490</v>
+        <v>496</v>
       </c>
       <c t="s" s="7" r="D132">
-        <v>491</v>
+        <v>497</v>
       </c>
       <c t="s" s="7" r="E132">
-        <v>492</v>
+        <v>498</v>
       </c>
     </row>
     <row r="133">
       <c s="11" r="A133"/>
       <c t="s" s="7" r="B133">
-        <v>493</v>
+        <v>499</v>
       </c>
       <c t="s" s="7" r="C133">
-        <v>494</v>
+        <v>500</v>
       </c>
       <c t="s" s="7" r="D133">
-        <v>495</v>
+        <v>501</v>
       </c>
       <c t="s" s="7" r="E133">
-        <v>496</v>
+        <v>502</v>
       </c>
     </row>
     <row r="134">
       <c s="11" r="A134"/>
       <c t="s" s="7" r="B134">
-        <v>497</v>
+        <v>503</v>
       </c>
       <c t="s" s="7" r="C134">
         <v>250</v>
       </c>
       <c t="s" s="7" r="D134">
-        <v>498</v>
+        <v>504</v>
       </c>
       <c t="s" s="7" r="E134">
         <v>250</v>
@@ -5897,451 +5911,451 @@
     <row r="135">
       <c s="11" r="A135"/>
       <c t="s" s="7" r="B135">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c t="s" s="7" r="C135">
-        <v>500</v>
+        <v>506</v>
       </c>
       <c t="s" s="7" r="D135">
-        <v>501</v>
+        <v>507</v>
       </c>
       <c t="s" s="7" r="E135">
-        <v>502</v>
+        <v>508</v>
       </c>
     </row>
     <row r="136">
       <c s="11" r="A136"/>
       <c t="s" s="7" r="B136">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c t="s" s="7" r="C136">
-        <v>504</v>
+        <v>510</v>
       </c>
       <c t="s" s="7" r="D136">
-        <v>505</v>
+        <v>511</v>
       </c>
       <c t="s" s="7" r="E136">
-        <v>506</v>
+        <v>512</v>
       </c>
     </row>
     <row r="137">
       <c s="11" r="A137"/>
       <c t="s" s="7" r="B137">
-        <v>507</v>
+        <v>513</v>
       </c>
       <c t="s" s="7" r="C137">
-        <v>508</v>
+        <v>514</v>
       </c>
       <c t="s" s="7" r="D137">
-        <v>509</v>
+        <v>515</v>
       </c>
       <c t="s" s="7" r="E137">
-        <v>510</v>
+        <v>516</v>
       </c>
     </row>
     <row r="138">
       <c s="11" r="A138"/>
       <c t="s" s="7" r="B138">
-        <v>511</v>
+        <v>517</v>
       </c>
       <c t="s" s="7" r="C138">
-        <v>512</v>
+        <v>518</v>
       </c>
       <c t="s" s="7" r="D138">
-        <v>513</v>
+        <v>519</v>
       </c>
       <c t="s" s="7" r="E138">
-        <v>514</v>
+        <v>520</v>
       </c>
     </row>
     <row r="139">
       <c s="11" r="A139"/>
       <c t="s" s="7" r="B139">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c t="s" s="7" r="C139">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c t="s" s="7" r="D139">
-        <v>517</v>
+        <v>523</v>
       </c>
       <c t="s" s="7" r="E139">
-        <v>518</v>
+        <v>524</v>
       </c>
     </row>
     <row r="140">
       <c s="11" r="A140"/>
       <c t="s" s="7" r="B140">
-        <v>519</v>
+        <v>525</v>
       </c>
       <c t="s" s="7" r="C140">
-        <v>520</v>
+        <v>526</v>
       </c>
       <c t="s" s="7" r="D140">
-        <v>520</v>
+        <v>526</v>
       </c>
       <c t="s" s="7" r="E140">
-        <v>521</v>
+        <v>527</v>
       </c>
     </row>
     <row r="141">
       <c s="11" r="A141"/>
       <c t="s" s="7" r="B141">
-        <v>522</v>
+        <v>528</v>
       </c>
       <c t="s" s="7" r="C141">
-        <v>523</v>
+        <v>529</v>
       </c>
       <c t="s" s="7" r="D141">
-        <v>523</v>
+        <v>529</v>
       </c>
       <c t="s" s="7" r="E141">
-        <v>524</v>
+        <v>530</v>
       </c>
     </row>
     <row r="142">
       <c s="11" r="A142"/>
       <c t="s" s="7" r="B142">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c t="s" s="7" r="C142">
-        <v>526</v>
+        <v>532</v>
       </c>
       <c t="s" s="7" r="D142">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c t="s" s="7" r="E142">
-        <v>528</v>
+        <v>534</v>
       </c>
     </row>
     <row r="143">
       <c s="11" r="A143"/>
       <c t="s" s="14" r="B143">
-        <v>529</v>
+        <v>535</v>
       </c>
       <c t="s" s="7" r="C143">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c t="s" s="7" r="D143">
-        <v>531</v>
+        <v>537</v>
       </c>
       <c t="s" s="7" r="E143">
-        <v>531</v>
+        <v>537</v>
       </c>
     </row>
     <row r="144">
       <c s="11" r="A144"/>
       <c t="s" s="7" r="B144">
-        <v>532</v>
+        <v>538</v>
       </c>
       <c t="s" s="7" r="C144">
-        <v>533</v>
+        <v>539</v>
       </c>
       <c t="s" s="7" r="D144">
-        <v>534</v>
+        <v>540</v>
       </c>
       <c t="s" s="7" r="E144">
-        <v>535</v>
+        <v>541</v>
       </c>
     </row>
     <row r="145">
       <c s="11" r="A145"/>
       <c t="s" s="7" r="B145">
-        <v>536</v>
+        <v>542</v>
       </c>
       <c t="s" s="7" r="C145">
-        <v>537</v>
+        <v>543</v>
       </c>
       <c t="s" s="7" r="D145">
-        <v>538</v>
+        <v>544</v>
       </c>
       <c t="s" s="7" r="E145">
-        <v>539</v>
+        <v>545</v>
       </c>
     </row>
     <row r="146">
       <c s="11" r="A146"/>
       <c t="s" s="7" r="B146">
-        <v>540</v>
+        <v>546</v>
       </c>
       <c t="s" s="7" r="C146">
-        <v>541</v>
+        <v>547</v>
       </c>
       <c t="s" s="7" r="D146">
-        <v>542</v>
+        <v>548</v>
       </c>
       <c t="s" s="7" r="E146">
-        <v>543</v>
+        <v>549</v>
       </c>
     </row>
     <row r="147">
       <c s="11" r="A147"/>
       <c t="s" s="7" r="B147">
-        <v>544</v>
+        <v>550</v>
       </c>
       <c t="s" s="7" r="C147">
-        <v>545</v>
+        <v>551</v>
       </c>
       <c t="s" s="7" r="D147">
-        <v>546</v>
+        <v>552</v>
       </c>
       <c t="s" s="7" r="E147">
-        <v>547</v>
+        <v>553</v>
       </c>
     </row>
     <row r="148">
       <c s="11" r="A148"/>
       <c t="s" s="7" r="B148">
-        <v>548</v>
+        <v>554</v>
       </c>
       <c t="s" s="7" r="C148">
-        <v>549</v>
+        <v>555</v>
       </c>
       <c t="s" s="7" r="D148">
-        <v>550</v>
+        <v>556</v>
       </c>
       <c t="s" s="7" r="E148">
-        <v>551</v>
+        <v>557</v>
       </c>
     </row>
     <row r="149">
       <c s="11" r="A149"/>
       <c t="s" s="7" r="B149">
-        <v>552</v>
+        <v>558</v>
       </c>
       <c t="s" s="7" r="C149">
-        <v>553</v>
+        <v>559</v>
       </c>
       <c t="s" s="7" r="D149">
-        <v>554</v>
+        <v>560</v>
       </c>
       <c t="s" s="7" r="E149">
-        <v>555</v>
+        <v>561</v>
       </c>
     </row>
     <row r="150">
       <c s="11" r="A150"/>
       <c t="s" s="7" r="B150">
-        <v>556</v>
+        <v>562</v>
       </c>
       <c t="s" s="7" r="C150">
-        <v>557</v>
+        <v>563</v>
       </c>
       <c t="s" s="7" r="D150">
-        <v>558</v>
+        <v>564</v>
       </c>
       <c t="s" s="7" r="E150">
-        <v>559</v>
+        <v>565</v>
       </c>
     </row>
     <row r="151">
       <c s="11" r="A151"/>
       <c t="s" s="7" r="B151">
-        <v>560</v>
+        <v>566</v>
       </c>
       <c t="s" s="7" r="C151">
-        <v>561</v>
+        <v>567</v>
       </c>
       <c t="s" s="7" r="D151">
-        <v>562</v>
+        <v>568</v>
       </c>
       <c t="s" s="7" r="E151">
-        <v>563</v>
+        <v>569</v>
       </c>
     </row>
     <row r="152">
       <c s="11" r="A152"/>
       <c t="s" s="7" r="B152">
-        <v>564</v>
+        <v>570</v>
       </c>
       <c t="s" s="7" r="C152">
-        <v>565</v>
+        <v>571</v>
       </c>
       <c t="s" s="7" r="D152">
-        <v>566</v>
+        <v>572</v>
       </c>
       <c t="s" s="7" r="E152">
-        <v>567</v>
+        <v>573</v>
       </c>
     </row>
     <row r="153">
       <c s="11" r="A153"/>
       <c t="s" s="7" r="B153">
-        <v>568</v>
+        <v>574</v>
       </c>
       <c t="s" s="7" r="C153">
-        <v>569</v>
+        <v>575</v>
       </c>
       <c t="s" s="7" r="D153">
-        <v>570</v>
+        <v>576</v>
       </c>
       <c t="s" s="7" r="E153">
-        <v>571</v>
+        <v>577</v>
       </c>
     </row>
     <row r="154">
       <c s="11" r="A154"/>
       <c t="s" s="7" r="B154">
-        <v>572</v>
+        <v>578</v>
       </c>
       <c t="s" s="7" r="C154">
-        <v>573</v>
+        <v>579</v>
       </c>
       <c t="s" s="7" r="D154">
-        <v>574</v>
+        <v>580</v>
       </c>
       <c t="s" s="7" r="E154">
-        <v>575</v>
+        <v>581</v>
       </c>
     </row>
     <row r="155">
       <c s="11" r="A155"/>
       <c t="s" s="7" r="B155">
-        <v>576</v>
+        <v>582</v>
       </c>
       <c t="s" s="7" r="C155">
-        <v>577</v>
+        <v>583</v>
       </c>
       <c t="s" s="7" r="D155">
-        <v>578</v>
+        <v>584</v>
       </c>
       <c t="s" s="7" r="E155">
-        <v>579</v>
+        <v>585</v>
       </c>
     </row>
     <row r="156">
       <c s="11" r="A156"/>
       <c t="s" s="7" r="B156">
-        <v>580</v>
+        <v>586</v>
       </c>
       <c t="s" s="7" r="C156">
-        <v>581</v>
+        <v>587</v>
       </c>
       <c t="s" s="7" r="D156">
-        <v>582</v>
+        <v>588</v>
       </c>
       <c t="s" s="7" r="E156">
-        <v>583</v>
+        <v>589</v>
       </c>
     </row>
     <row r="157">
       <c s="11" r="A157"/>
       <c t="s" s="7" r="B157">
-        <v>584</v>
+        <v>590</v>
       </c>
       <c t="s" s="7" r="C157">
-        <v>585</v>
+        <v>591</v>
       </c>
       <c t="s" s="7" r="D157">
-        <v>586</v>
+        <v>592</v>
       </c>
       <c t="s" s="7" r="E157">
-        <v>587</v>
+        <v>593</v>
       </c>
     </row>
     <row r="158">
       <c s="11" r="A158"/>
       <c t="s" s="7" r="B158">
-        <v>588</v>
+        <v>594</v>
       </c>
       <c t="s" s="7" r="C158">
-        <v>589</v>
+        <v>595</v>
       </c>
       <c t="s" s="7" r="D158">
-        <v>590</v>
+        <v>596</v>
       </c>
       <c t="s" s="7" r="E158">
-        <v>591</v>
+        <v>597</v>
       </c>
     </row>
     <row r="159">
       <c s="11" r="A159"/>
       <c t="s" s="7" r="B159">
-        <v>592</v>
+        <v>598</v>
       </c>
       <c t="s" s="14" r="C159">
-        <v>593</v>
+        <v>599</v>
       </c>
       <c t="s" s="7" r="D159">
-        <v>594</v>
+        <v>600</v>
       </c>
       <c t="s" s="7" r="E159">
-        <v>595</v>
+        <v>601</v>
       </c>
     </row>
     <row r="160">
       <c s="11" r="A160"/>
       <c t="s" s="14" r="B160">
-        <v>596</v>
+        <v>602</v>
       </c>
       <c t="s" s="14" r="C160">
-        <v>597</v>
+        <v>603</v>
       </c>
       <c t="s" s="7" r="D160">
-        <v>598</v>
+        <v>604</v>
       </c>
       <c t="s" s="7" r="E160">
-        <v>599</v>
+        <v>605</v>
       </c>
     </row>
     <row r="161">
       <c s="11" r="A161"/>
       <c t="s" s="7" r="B161">
-        <v>600</v>
+        <v>606</v>
       </c>
       <c t="s" s="14" r="C161">
-        <v>597</v>
+        <v>603</v>
       </c>
       <c t="s" s="7" r="D161">
-        <v>598</v>
+        <v>604</v>
       </c>
       <c t="s" s="7" r="E161">
-        <v>599</v>
+        <v>605</v>
       </c>
     </row>
     <row r="162">
       <c s="11" r="A162"/>
       <c t="s" s="7" r="B162">
-        <v>601</v>
+        <v>607</v>
       </c>
       <c t="s" s="3" r="C162">
-        <v>602</v>
+        <v>608</v>
       </c>
       <c t="s" s="7" r="D162">
-        <v>603</v>
+        <v>609</v>
       </c>
       <c t="s" s="7" r="E162">
-        <v>604</v>
+        <v>610</v>
       </c>
     </row>
     <row r="163">
       <c s="11" r="A163"/>
       <c t="s" s="7" r="B163">
-        <v>605</v>
+        <v>611</v>
       </c>
       <c t="s" s="3" r="C163">
-        <v>606</v>
+        <v>612</v>
       </c>
       <c t="s" s="7" r="D163">
-        <v>607</v>
+        <v>613</v>
       </c>
       <c t="s" s="7" r="E163">
-        <v>608</v>
+        <v>614</v>
       </c>
     </row>
     <row r="164">
       <c s="11" r="A164"/>
       <c t="s" s="7" r="B164">
-        <v>609</v>
+        <v>615</v>
       </c>
       <c t="s" s="3" r="C164">
-        <v>610</v>
+        <v>616</v>
       </c>
       <c t="s" s="7" r="D164">
-        <v>611</v>
+        <v>617</v>
       </c>
       <c t="s" s="3" r="E164">
-        <v>612</v>
+        <v>618</v>
       </c>
     </row>
     <row r="165">
@@ -6353,199 +6367,199 @@
     </row>
     <row r="166">
       <c t="s" s="11" r="A166">
-        <v>613</v>
+        <v>619</v>
       </c>
       <c t="s" s="7" r="B166">
-        <v>614</v>
+        <v>620</v>
       </c>
       <c t="s" s="14" r="C166">
-        <v>615</v>
+        <v>621</v>
       </c>
       <c t="s" s="7" r="D166">
-        <v>616</v>
+        <v>289</v>
       </c>
       <c t="s" s="7" r="E166">
-        <v>617</v>
+        <v>290</v>
       </c>
     </row>
     <row r="167">
       <c s="11" r="A167"/>
       <c t="s" s="22" r="B167">
-        <v>618</v>
+        <v>622</v>
       </c>
       <c t="s" s="14" r="C167">
-        <v>619</v>
+        <v>623</v>
       </c>
       <c t="s" s="22" r="D167">
-        <v>620</v>
+        <v>624</v>
       </c>
       <c t="s" s="22" r="E167">
-        <v>621</v>
+        <v>625</v>
       </c>
     </row>
     <row r="168">
       <c s="11" r="A168"/>
       <c t="s" s="7" r="B168">
-        <v>622</v>
+        <v>626</v>
       </c>
       <c t="s" s="14" r="C168">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c t="s" s="7" r="D168">
-        <v>624</v>
+        <v>628</v>
       </c>
       <c t="s" s="7" r="E168">
-        <v>625</v>
+        <v>629</v>
       </c>
     </row>
     <row r="169">
       <c s="11" r="A169"/>
       <c t="s" s="7" r="B169">
-        <v>626</v>
+        <v>630</v>
       </c>
       <c t="s" s="14" r="C169">
-        <v>627</v>
+        <v>631</v>
       </c>
       <c t="s" s="7" r="D169">
-        <v>628</v>
+        <v>632</v>
       </c>
       <c t="s" s="7" r="E169">
-        <v>629</v>
+        <v>633</v>
       </c>
     </row>
     <row r="170">
       <c s="18" r="A170"/>
       <c t="s" s="7" r="B170">
-        <v>630</v>
+        <v>634</v>
       </c>
       <c t="s" s="14" r="C170">
-        <v>631</v>
+        <v>635</v>
       </c>
       <c t="s" s="7" r="D170">
-        <v>632</v>
+        <v>636</v>
       </c>
       <c t="s" s="7" r="E170">
-        <v>633</v>
+        <v>637</v>
       </c>
     </row>
     <row r="171">
       <c s="11" r="A171"/>
       <c t="s" s="7" r="B171">
-        <v>634</v>
+        <v>638</v>
       </c>
       <c t="s" s="14" r="C171">
-        <v>635</v>
+        <v>639</v>
       </c>
       <c t="s" s="7" r="D171">
-        <v>636</v>
+        <v>640</v>
       </c>
       <c t="s" s="7" r="E171">
-        <v>637</v>
+        <v>641</v>
       </c>
     </row>
     <row r="172">
       <c s="11" r="A172"/>
       <c t="s" s="7" r="B172">
-        <v>638</v>
+        <v>642</v>
       </c>
       <c t="s" s="14" r="C172">
-        <v>639</v>
+        <v>643</v>
       </c>
       <c t="s" s="7" r="D172">
-        <v>640</v>
+        <v>644</v>
       </c>
       <c t="s" s="7" r="E172">
-        <v>641</v>
+        <v>645</v>
       </c>
     </row>
     <row r="173">
       <c s="11" r="A173"/>
       <c t="s" s="7" r="B173">
-        <v>642</v>
+        <v>646</v>
       </c>
       <c t="s" s="14" r="C173">
-        <v>643</v>
+        <v>647</v>
       </c>
       <c t="s" s="7" r="D173">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c t="s" s="7" r="E173">
-        <v>645</v>
+        <v>649</v>
       </c>
     </row>
     <row r="174">
       <c s="11" r="A174"/>
       <c t="s" s="7" r="B174">
-        <v>646</v>
+        <v>650</v>
       </c>
       <c t="s" s="14" r="C174">
-        <v>647</v>
+        <v>651</v>
       </c>
       <c t="s" s="7" r="D174">
-        <v>648</v>
+        <v>652</v>
       </c>
       <c t="s" s="7" r="E174">
-        <v>649</v>
+        <v>653</v>
       </c>
     </row>
     <row r="175">
       <c s="11" r="A175"/>
       <c t="s" s="7" r="B175">
-        <v>650</v>
+        <v>654</v>
       </c>
       <c t="s" s="14" r="C175">
-        <v>651</v>
+        <v>655</v>
       </c>
       <c t="s" s="7" r="D175">
-        <v>652</v>
+        <v>656</v>
       </c>
       <c t="s" s="7" r="E175">
-        <v>653</v>
+        <v>657</v>
       </c>
     </row>
     <row r="176">
       <c s="11" r="A176"/>
       <c t="s" s="7" r="B176">
-        <v>654</v>
+        <v>658</v>
       </c>
       <c t="s" s="14" r="C176">
-        <v>655</v>
+        <v>659</v>
       </c>
       <c t="s" s="7" r="D176">
-        <v>656</v>
+        <v>660</v>
       </c>
       <c t="s" s="7" r="E176">
-        <v>657</v>
+        <v>661</v>
       </c>
     </row>
     <row r="177">
       <c s="11" r="A177"/>
       <c t="s" s="7" r="B177">
-        <v>658</v>
+        <v>662</v>
       </c>
       <c t="s" s="14" r="C177">
-        <v>659</v>
+        <v>663</v>
       </c>
       <c t="s" s="7" r="D177">
-        <v>660</v>
+        <v>664</v>
       </c>
       <c t="s" s="7" r="E177">
-        <v>661</v>
+        <v>665</v>
       </c>
     </row>
     <row r="178">
       <c s="11" r="A178"/>
       <c t="s" s="7" r="B178">
-        <v>662</v>
+        <v>666</v>
       </c>
       <c t="s" s="14" r="C178">
-        <v>663</v>
+        <v>667</v>
       </c>
       <c t="s" s="7" r="D178">
-        <v>664</v>
+        <v>668</v>
       </c>
       <c t="s" s="7" r="E178">
-        <v>665</v>
+        <v>669</v>
       </c>
     </row>
     <row r="179">
@@ -6557,109 +6571,109 @@
     </row>
     <row r="180">
       <c t="s" s="11" r="A180">
-        <v>666</v>
+        <v>670</v>
       </c>
       <c t="s" s="7" r="B180">
-        <v>667</v>
+        <v>671</v>
       </c>
       <c t="s" s="14" r="C180">
-        <v>668</v>
+        <v>672</v>
       </c>
       <c t="s" s="7" r="D180">
-        <v>669</v>
+        <v>673</v>
       </c>
       <c t="s" s="7" r="E180">
-        <v>670</v>
+        <v>674</v>
       </c>
     </row>
     <row r="181">
       <c s="11" r="A181"/>
       <c t="s" s="7" r="B181">
-        <v>671</v>
+        <v>675</v>
       </c>
       <c t="s" s="14" r="C181">
-        <v>672</v>
+        <v>676</v>
       </c>
       <c t="s" s="7" r="D181">
-        <v>673</v>
+        <v>677</v>
       </c>
       <c t="s" s="7" r="E181">
-        <v>674</v>
+        <v>678</v>
       </c>
     </row>
     <row r="182">
       <c s="11" r="A182"/>
       <c t="s" s="7" r="B182">
-        <v>675</v>
+        <v>679</v>
       </c>
       <c t="s" s="14" r="C182">
-        <v>676</v>
+        <v>680</v>
       </c>
       <c t="s" s="7" r="D182">
-        <v>677</v>
+        <v>681</v>
       </c>
       <c t="s" s="7" r="E182">
-        <v>678</v>
+        <v>682</v>
       </c>
     </row>
     <row r="183">
       <c s="11" r="A183"/>
       <c t="s" s="7" r="B183">
-        <v>679</v>
+        <v>683</v>
       </c>
       <c t="s" s="14" r="C183">
-        <v>680</v>
+        <v>684</v>
       </c>
       <c t="s" s="7" r="D183">
-        <v>681</v>
+        <v>685</v>
       </c>
       <c t="s" s="7" r="E183">
-        <v>682</v>
+        <v>686</v>
       </c>
     </row>
     <row r="184">
       <c s="11" r="A184"/>
       <c t="s" s="7" r="B184">
-        <v>683</v>
+        <v>687</v>
       </c>
       <c t="s" s="14" r="C184">
-        <v>684</v>
+        <v>688</v>
       </c>
       <c t="s" s="7" r="D184">
-        <v>685</v>
+        <v>689</v>
       </c>
       <c t="s" s="7" r="E184">
-        <v>686</v>
+        <v>690</v>
       </c>
     </row>
     <row r="185">
       <c s="11" r="A185"/>
       <c t="s" s="7" r="B185">
-        <v>687</v>
+        <v>691</v>
       </c>
       <c t="s" s="14" r="C185">
-        <v>688</v>
+        <v>692</v>
       </c>
       <c t="s" s="7" r="D185">
-        <v>689</v>
+        <v>693</v>
       </c>
       <c t="s" s="7" r="E185">
-        <v>690</v>
+        <v>694</v>
       </c>
     </row>
     <row r="186">
       <c s="11" r="A186"/>
       <c t="s" s="7" r="B186">
-        <v>691</v>
+        <v>695</v>
       </c>
       <c t="s" s="14" r="C186">
-        <v>692</v>
+        <v>696</v>
       </c>
       <c t="s" s="7" r="D186">
-        <v>693</v>
+        <v>697</v>
       </c>
       <c t="s" s="7" r="E186">
-        <v>694</v>
+        <v>698</v>
       </c>
     </row>
     <row r="187">
@@ -6671,13 +6685,13 @@
     </row>
     <row r="188">
       <c t="s" s="11" r="A188">
-        <v>695</v>
+        <v>699</v>
       </c>
       <c t="s" s="29" r="B188">
-        <v>696</v>
+        <v>700</v>
       </c>
       <c t="s" s="21" r="C188">
-        <v>695</v>
+        <v>699</v>
       </c>
       <c s="29" r="D188"/>
       <c s="29" r="E188"/>
@@ -6691,27 +6705,27 @@
     </row>
     <row r="190">
       <c t="s" s="11" r="A190">
-        <v>697</v>
-      </c>
-      <c t="s" s="36" r="B190">
-        <v>698</v>
-      </c>
-      <c t="s" s="34" r="C190">
-        <v>699</v>
-      </c>
-      <c s="36" r="D190"/>
-      <c s="36" r="E190"/>
+        <v>701</v>
+      </c>
+      <c t="s" s="35" r="B190">
+        <v>702</v>
+      </c>
+      <c t="s" s="33" r="C190">
+        <v>703</v>
+      </c>
+      <c s="35" r="D190"/>
+      <c s="35" r="E190"/>
     </row>
     <row r="191">
       <c s="11" r="A191"/>
-      <c t="s" s="36" r="B191">
-        <v>700</v>
-      </c>
-      <c t="s" s="34" r="C191">
-        <v>701</v>
-      </c>
-      <c s="36" r="D191"/>
-      <c s="36" r="E191"/>
+      <c t="s" s="35" r="B191">
+        <v>704</v>
+      </c>
+      <c t="s" s="33" r="C191">
+        <v>705</v>
+      </c>
+      <c s="35" r="D191"/>
+      <c s="35" r="E191"/>
     </row>
     <row r="192">
       <c s="11" r="A192"/>
@@ -6722,304 +6736,304 @@
     </row>
     <row r="193">
       <c t="s" s="11" r="A193">
-        <v>702</v>
+        <v>706</v>
       </c>
       <c t="s" s="27" r="B193">
-        <v>703</v>
+        <v>707</v>
       </c>
       <c t="s" s="27" r="C193">
-        <v>704</v>
+        <v>708</v>
       </c>
       <c t="s" s="7" r="D193">
-        <v>705</v>
+        <v>709</v>
       </c>
       <c t="s" s="7" r="E193">
-        <v>706</v>
+        <v>710</v>
       </c>
     </row>
     <row r="194">
       <c s="11" r="A194"/>
       <c t="s" s="27" r="B194">
-        <v>707</v>
+        <v>711</v>
       </c>
       <c t="s" s="27" r="C194">
-        <v>708</v>
+        <v>712</v>
       </c>
       <c t="s" s="7" r="D194">
-        <v>708</v>
+        <v>712</v>
       </c>
       <c t="s" s="7" r="E194">
-        <v>709</v>
+        <v>713</v>
       </c>
     </row>
     <row r="195">
       <c s="11" r="A195"/>
       <c t="s" s="27" r="B195">
-        <v>710</v>
+        <v>714</v>
       </c>
       <c t="s" s="27" r="C195">
-        <v>711</v>
+        <v>715</v>
       </c>
       <c t="s" s="7" r="D195">
-        <v>712</v>
+        <v>716</v>
       </c>
       <c t="s" s="7" r="E195">
-        <v>713</v>
+        <v>717</v>
       </c>
     </row>
     <row r="196">
       <c s="11" r="A196"/>
       <c t="s" s="27" r="B196">
-        <v>714</v>
+        <v>718</v>
       </c>
       <c t="s" s="27" r="C196">
-        <v>715</v>
+        <v>719</v>
       </c>
       <c t="s" s="7" r="D196">
-        <v>716</v>
+        <v>720</v>
       </c>
       <c t="s" s="7" r="E196">
-        <v>717</v>
+        <v>721</v>
       </c>
     </row>
     <row r="197">
       <c s="11" r="A197"/>
       <c t="s" s="14" r="B197">
-        <v>718</v>
+        <v>722</v>
       </c>
       <c t="s" s="14" r="C197">
-        <v>719</v>
+        <v>723</v>
       </c>
       <c t="s" s="7" r="D197">
-        <v>720</v>
+        <v>724</v>
       </c>
       <c t="s" s="7" r="E197">
-        <v>721</v>
+        <v>725</v>
       </c>
     </row>
     <row r="198">
       <c s="11" r="A198"/>
       <c t="s" s="14" r="B198">
-        <v>722</v>
+        <v>726</v>
       </c>
       <c t="s" s="14" r="C198">
-        <v>723</v>
+        <v>727</v>
       </c>
       <c t="s" s="7" r="D198">
-        <v>724</v>
+        <v>728</v>
       </c>
       <c t="s" s="7" r="E198">
-        <v>725</v>
+        <v>729</v>
       </c>
     </row>
     <row r="199">
       <c s="11" r="A199"/>
       <c t="s" s="14" r="B199">
-        <v>726</v>
+        <v>730</v>
       </c>
       <c t="s" s="14" r="C199">
-        <v>727</v>
+        <v>731</v>
       </c>
       <c t="s" s="7" r="D199">
-        <v>728</v>
+        <v>732</v>
       </c>
       <c t="s" s="7" r="E199">
-        <v>729</v>
+        <v>733</v>
       </c>
     </row>
     <row r="200">
       <c s="11" r="A200"/>
       <c t="s" s="14" r="B200">
-        <v>730</v>
+        <v>734</v>
       </c>
       <c t="s" s="14" r="C200">
-        <v>731</v>
+        <v>735</v>
       </c>
       <c t="s" s="7" r="D200">
-        <v>732</v>
+        <v>736</v>
       </c>
       <c t="s" s="7" r="E200">
-        <v>733</v>
+        <v>737</v>
       </c>
     </row>
     <row r="201">
       <c s="11" r="A201"/>
       <c t="s" s="14" r="B201">
-        <v>734</v>
+        <v>738</v>
       </c>
       <c t="s" s="14" r="C201">
-        <v>735</v>
+        <v>739</v>
       </c>
       <c t="s" s="7" r="D201">
-        <v>736</v>
+        <v>740</v>
       </c>
       <c t="s" s="7" r="E201">
-        <v>737</v>
+        <v>741</v>
       </c>
     </row>
     <row r="202">
       <c s="11" r="A202"/>
       <c t="s" s="14" r="B202">
-        <v>738</v>
+        <v>742</v>
       </c>
       <c t="s" s="14" r="C202">
-        <v>739</v>
+        <v>743</v>
       </c>
       <c t="s" s="7" r="D202">
-        <v>740</v>
+        <v>744</v>
       </c>
       <c t="s" s="7" r="E202">
-        <v>741</v>
+        <v>745</v>
       </c>
     </row>
     <row r="203">
       <c s="11" r="A203"/>
       <c t="s" s="14" r="B203">
-        <v>742</v>
+        <v>746</v>
       </c>
       <c t="s" s="14" r="C203">
-        <v>743</v>
+        <v>747</v>
       </c>
       <c t="s" s="7" r="D203">
-        <v>744</v>
+        <v>748</v>
       </c>
       <c t="s" s="7" r="E203">
-        <v>745</v>
+        <v>749</v>
       </c>
     </row>
     <row r="204">
       <c s="11" r="A204"/>
       <c t="s" s="7" r="B204">
-        <v>746</v>
+        <v>750</v>
       </c>
       <c t="s" s="14" r="C204">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c t="s" s="7" r="D204">
-        <v>748</v>
+        <v>752</v>
       </c>
       <c t="s" s="7" r="E204">
-        <v>749</v>
+        <v>753</v>
       </c>
     </row>
     <row r="205">
       <c s="11" r="A205"/>
       <c t="s" s="7" r="B205">
-        <v>750</v>
+        <v>754</v>
       </c>
       <c t="s" s="14" r="C205">
-        <v>751</v>
+        <v>755</v>
       </c>
       <c t="s" s="19" r="D205">
-        <v>752</v>
+        <v>756</v>
       </c>
       <c t="s" s="19" r="E205">
-        <v>753</v>
+        <v>757</v>
       </c>
     </row>
     <row r="206">
       <c s="11" r="A206"/>
       <c t="s" s="7" r="B206">
-        <v>754</v>
+        <v>758</v>
       </c>
       <c t="s" s="14" r="C206">
-        <v>755</v>
+        <v>759</v>
       </c>
       <c t="s" s="19" r="D206">
-        <v>756</v>
+        <v>760</v>
       </c>
       <c t="s" s="19" r="E206">
-        <v>757</v>
+        <v>761</v>
       </c>
     </row>
     <row r="207">
       <c s="11" r="A207"/>
       <c t="s" s="7" r="B207">
-        <v>758</v>
+        <v>762</v>
       </c>
       <c t="s" s="14" r="C207">
-        <v>759</v>
+        <v>763</v>
       </c>
       <c t="s" s="19" r="D207">
-        <v>760</v>
+        <v>764</v>
       </c>
       <c t="s" s="19" r="E207">
-        <v>761</v>
+        <v>765</v>
       </c>
     </row>
     <row r="208">
       <c s="11" r="A208"/>
       <c t="s" s="7" r="B208">
-        <v>762</v>
+        <v>766</v>
       </c>
       <c t="s" s="14" r="C208">
-        <v>763</v>
+        <v>767</v>
       </c>
       <c t="s" s="7" r="D208">
-        <v>764</v>
+        <v>768</v>
       </c>
       <c t="s" s="7" r="E208">
-        <v>765</v>
+        <v>769</v>
       </c>
     </row>
     <row r="209">
       <c s="11" r="A209"/>
       <c t="s" s="7" r="B209">
-        <v>766</v>
+        <v>770</v>
       </c>
       <c t="s" s="14" r="C209">
-        <v>767</v>
+        <v>771</v>
       </c>
       <c t="s" s="7" r="D209">
-        <v>768</v>
+        <v>772</v>
       </c>
       <c t="s" s="7" r="E209">
-        <v>769</v>
+        <v>773</v>
       </c>
     </row>
     <row r="210">
       <c s="11" r="A210"/>
       <c t="s" s="7" r="B210">
-        <v>770</v>
+        <v>774</v>
       </c>
       <c t="s" s="14" r="C210">
-        <v>771</v>
+        <v>775</v>
       </c>
       <c t="s" s="7" r="D210">
-        <v>772</v>
+        <v>776</v>
       </c>
       <c t="s" s="7" r="E210">
-        <v>773</v>
+        <v>777</v>
       </c>
     </row>
     <row r="211">
       <c s="11" r="A211"/>
       <c t="s" s="7" r="B211">
-        <v>774</v>
+        <v>778</v>
       </c>
       <c t="s" s="14" r="C211">
-        <v>775</v>
+        <v>779</v>
       </c>
       <c t="s" s="7" r="D211">
-        <v>776</v>
+        <v>780</v>
       </c>
       <c t="s" s="7" r="E211">
-        <v>777</v>
+        <v>781</v>
       </c>
     </row>
     <row r="212">
       <c s="11" r="A212"/>
       <c t="s" s="7" r="B212">
-        <v>778</v>
+        <v>782</v>
       </c>
       <c t="s" s="14" r="C212">
-        <v>779</v>
+        <v>783</v>
       </c>
       <c t="s" s="7" r="D212">
-        <v>780</v>
+        <v>784</v>
       </c>
       <c t="s" s="7" r="E212">
-        <v>781</v>
+        <v>785</v>
       </c>
     </row>
     <row r="213">
@@ -7031,78 +7045,78 @@
     </row>
     <row r="214">
       <c t="s" s="11" r="A214">
-        <v>782</v>
+        <v>786</v>
       </c>
       <c t="s" s="27" r="B214">
-        <v>783</v>
+        <v>787</v>
       </c>
       <c t="s" s="7" r="C214">
-        <v>708</v>
+        <v>712</v>
       </c>
       <c t="s" s="7" r="D214">
-        <v>708</v>
+        <v>712</v>
       </c>
       <c t="s" s="7" r="E214">
-        <v>709</v>
+        <v>713</v>
       </c>
     </row>
     <row r="215">
       <c s="11" r="A215"/>
       <c t="s" s="7" r="B215">
-        <v>784</v>
+        <v>788</v>
       </c>
       <c t="s" s="14" r="C215">
-        <v>711</v>
+        <v>715</v>
       </c>
       <c t="s" s="7" r="D215">
-        <v>712</v>
+        <v>716</v>
       </c>
       <c t="s" s="7" r="E215">
-        <v>713</v>
+        <v>717</v>
       </c>
     </row>
     <row r="216">
       <c t="s" s="7" r="B216">
-        <v>785</v>
+        <v>789</v>
       </c>
       <c t="s" s="14" r="C216">
-        <v>786</v>
+        <v>790</v>
       </c>
       <c t="s" s="7" r="D216">
-        <v>787</v>
+        <v>791</v>
       </c>
       <c t="s" s="7" r="E216">
-        <v>788</v>
+        <v>792</v>
       </c>
     </row>
     <row r="217">
       <c s="11" r="A217"/>
       <c t="s" s="7" r="B217">
-        <v>789</v>
+        <v>793</v>
       </c>
       <c t="s" s="14" r="C217">
-        <v>790</v>
+        <v>794</v>
       </c>
       <c t="s" s="7" r="D217">
-        <v>791</v>
+        <v>795</v>
       </c>
       <c t="s" s="7" r="E217">
-        <v>792</v>
+        <v>796</v>
       </c>
     </row>
     <row r="218">
       <c s="11" r="A218"/>
       <c t="s" s="7" r="B218">
-        <v>793</v>
+        <v>797</v>
       </c>
       <c t="s" s="14" r="C218">
-        <v>794</v>
+        <v>798</v>
       </c>
       <c t="s" s="7" r="D218">
-        <v>795</v>
+        <v>799</v>
       </c>
       <c t="s" s="7" r="E218">
-        <v>796</v>
+        <v>800</v>
       </c>
     </row>
     <row r="219">
@@ -7114,109 +7128,109 @@
     </row>
     <row r="220">
       <c t="s" s="11" r="A220">
-        <v>797</v>
+        <v>801</v>
       </c>
       <c t="s" s="7" r="B220">
-        <v>798</v>
+        <v>802</v>
       </c>
       <c t="s" s="14" r="C220">
-        <v>797</v>
+        <v>801</v>
       </c>
       <c t="s" s="7" r="D220">
-        <v>799</v>
+        <v>803</v>
       </c>
       <c t="s" s="7" r="E220">
-        <v>800</v>
+        <v>804</v>
       </c>
     </row>
     <row r="221">
       <c s="11" r="A221"/>
       <c t="s" s="7" r="B221">
-        <v>801</v>
+        <v>805</v>
       </c>
       <c t="s" s="14" r="C221">
-        <v>802</v>
+        <v>806</v>
       </c>
       <c t="s" s="7" r="D221">
-        <v>803</v>
+        <v>807</v>
       </c>
       <c t="s" s="7" r="E221">
-        <v>804</v>
+        <v>808</v>
       </c>
     </row>
     <row r="222">
       <c s="11" r="A222"/>
       <c t="s" s="7" r="B222">
-        <v>805</v>
+        <v>809</v>
       </c>
       <c t="s" s="14" r="C222">
-        <v>806</v>
+        <v>810</v>
       </c>
       <c t="s" s="7" r="D222">
-        <v>807</v>
+        <v>811</v>
       </c>
       <c t="s" s="7" r="E222">
-        <v>808</v>
+        <v>812</v>
       </c>
     </row>
     <row r="223">
       <c s="11" r="A223"/>
       <c t="s" s="7" r="B223">
-        <v>809</v>
+        <v>813</v>
       </c>
       <c t="s" s="14" r="C223">
-        <v>810</v>
+        <v>814</v>
       </c>
       <c t="s" s="7" r="D223">
-        <v>811</v>
+        <v>815</v>
       </c>
       <c t="s" s="7" r="E223">
-        <v>812</v>
+        <v>816</v>
       </c>
     </row>
     <row r="224">
       <c s="11" r="A224"/>
       <c t="s" s="7" r="B224">
-        <v>813</v>
+        <v>817</v>
       </c>
       <c t="s" s="14" r="C224">
-        <v>814</v>
+        <v>818</v>
       </c>
       <c t="s" s="7" r="D224">
-        <v>815</v>
+        <v>819</v>
       </c>
       <c t="s" s="7" r="E224">
-        <v>816</v>
+        <v>820</v>
       </c>
     </row>
     <row r="225">
       <c s="11" r="A225"/>
       <c t="s" s="7" r="B225">
-        <v>817</v>
+        <v>821</v>
       </c>
       <c t="s" s="14" r="C225">
-        <v>818</v>
+        <v>822</v>
       </c>
       <c t="s" s="7" r="D225">
-        <v>819</v>
+        <v>823</v>
       </c>
       <c t="s" s="7" r="E225">
-        <v>820</v>
+        <v>824</v>
       </c>
     </row>
     <row r="226">
       <c s="11" r="A226"/>
       <c t="s" s="7" r="B226">
-        <v>821</v>
+        <v>825</v>
       </c>
       <c t="s" s="14" r="C226">
-        <v>822</v>
+        <v>826</v>
       </c>
       <c t="s" s="7" r="D226">
-        <v>823</v>
+        <v>827</v>
       </c>
       <c t="s" s="7" r="E226">
-        <v>824</v>
+        <v>828</v>
       </c>
     </row>
     <row r="227">
@@ -7228,34 +7242,34 @@
     </row>
     <row r="228">
       <c t="s" s="11" r="A228">
-        <v>825</v>
+        <v>829</v>
       </c>
       <c t="s" s="7" r="B228">
-        <v>826</v>
+        <v>830</v>
       </c>
       <c t="s" s="14" r="C228">
-        <v>827</v>
+        <v>831</v>
       </c>
       <c t="s" s="7" r="D228">
-        <v>828</v>
+        <v>832</v>
       </c>
       <c t="s" s="7" r="E228">
-        <v>829</v>
+        <v>833</v>
       </c>
     </row>
     <row r="229">
       <c s="11" r="A229"/>
       <c t="s" s="7" r="B229">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c t="s" s="14" r="C229">
-        <v>831</v>
+        <v>835</v>
       </c>
       <c t="s" s="7" r="D229">
-        <v>831</v>
+        <v>835</v>
       </c>
       <c t="s" s="7" r="E229">
-        <v>832</v>
+        <v>836</v>
       </c>
     </row>
     <row r="230">
@@ -7267,64 +7281,64 @@
     </row>
     <row r="231">
       <c t="s" s="11" r="A231">
-        <v>833</v>
+        <v>837</v>
       </c>
       <c t="s" s="7" r="B231">
-        <v>834</v>
+        <v>838</v>
       </c>
       <c t="s" s="14" r="C231">
-        <v>835</v>
+        <v>839</v>
       </c>
       <c t="s" s="7" r="D231">
-        <v>836</v>
+        <v>840</v>
       </c>
       <c t="s" s="7" r="E231">
-        <v>837</v>
+        <v>841</v>
       </c>
     </row>
     <row r="232">
       <c s="11" r="A232"/>
       <c t="s" s="7" r="B232">
-        <v>838</v>
+        <v>842</v>
       </c>
       <c t="s" s="14" r="C232">
-        <v>839</v>
+        <v>843</v>
       </c>
       <c t="s" s="7" r="D232">
-        <v>840</v>
+        <v>844</v>
       </c>
       <c t="s" s="7" r="E232">
-        <v>841</v>
+        <v>845</v>
       </c>
     </row>
     <row r="233">
       <c s="11" r="A233"/>
       <c t="s" s="7" r="B233">
-        <v>842</v>
+        <v>846</v>
       </c>
       <c t="s" s="14" r="C233">
-        <v>843</v>
+        <v>847</v>
       </c>
       <c t="s" s="7" r="D233">
-        <v>844</v>
+        <v>848</v>
       </c>
       <c t="s" s="7" r="E233">
-        <v>845</v>
+        <v>849</v>
       </c>
     </row>
     <row r="234">
       <c s="11" r="A234"/>
       <c t="s" s="7" r="B234">
-        <v>846</v>
+        <v>850</v>
       </c>
       <c t="s" s="14" r="C234">
-        <v>847</v>
+        <v>851</v>
       </c>
       <c t="s" s="7" r="D234">
-        <v>848</v>
+        <v>852</v>
       </c>
       <c t="s" s="7" r="E234">
-        <v>849</v>
+        <v>853</v>
       </c>
     </row>
     <row r="235">
@@ -7336,34 +7350,34 @@
     </row>
     <row r="236">
       <c t="s" s="11" r="A236">
-        <v>850</v>
+        <v>854</v>
       </c>
       <c t="s" s="7" r="B236">
-        <v>851</v>
+        <v>855</v>
       </c>
       <c t="s" s="14" r="C236">
-        <v>852</v>
+        <v>856</v>
       </c>
       <c t="s" s="7" r="D236">
-        <v>853</v>
+        <v>857</v>
       </c>
       <c t="s" s="7" r="E236">
-        <v>854</v>
+        <v>858</v>
       </c>
     </row>
     <row r="237">
       <c s="11" r="A237"/>
       <c t="s" s="7" r="B237">
-        <v>855</v>
+        <v>859</v>
       </c>
       <c t="s" s="14" r="C237">
-        <v>856</v>
+        <v>860</v>
       </c>
       <c t="s" s="7" r="D237">
-        <v>857</v>
+        <v>861</v>
       </c>
       <c t="s" s="7" r="E237">
-        <v>858</v>
+        <v>862</v>
       </c>
     </row>
     <row r="238">
@@ -7375,19 +7389,19 @@
     </row>
     <row r="239">
       <c t="s" s="11" r="A239">
-        <v>859</v>
+        <v>863</v>
       </c>
       <c t="s" s="7" r="B239">
-        <v>860</v>
+        <v>864</v>
       </c>
       <c t="s" s="14" r="C239">
-        <v>861</v>
+        <v>865</v>
       </c>
       <c t="s" s="7" r="D239">
-        <v>862</v>
+        <v>866</v>
       </c>
       <c t="s" s="7" r="E239">
-        <v>863</v>
+        <v>867</v>
       </c>
     </row>
     <row r="240">
@@ -7399,124 +7413,124 @@
     </row>
     <row r="241">
       <c t="s" s="11" r="A241">
-        <v>864</v>
+        <v>868</v>
       </c>
       <c t="s" s="7" r="B241">
-        <v>865</v>
+        <v>869</v>
       </c>
       <c t="s" s="14" r="C241">
-        <v>866</v>
+        <v>870</v>
       </c>
       <c t="s" s="7" r="D241">
-        <v>867</v>
+        <v>871</v>
       </c>
       <c t="s" s="7" r="E241">
-        <v>868</v>
+        <v>872</v>
       </c>
     </row>
     <row r="242">
       <c s="11" r="A242"/>
       <c t="s" s="7" r="B242">
-        <v>869</v>
+        <v>873</v>
       </c>
       <c t="s" s="14" r="C242">
-        <v>870</v>
+        <v>874</v>
       </c>
       <c t="s" s="7" r="D242">
-        <v>871</v>
+        <v>875</v>
       </c>
       <c t="s" s="7" r="E242">
-        <v>872</v>
+        <v>876</v>
       </c>
     </row>
     <row r="243">
       <c s="11" r="A243"/>
       <c t="s" s="7" r="B243">
-        <v>873</v>
+        <v>877</v>
       </c>
       <c t="s" s="14" r="C243">
-        <v>874</v>
+        <v>878</v>
       </c>
       <c t="s" s="7" r="D243">
-        <v>875</v>
+        <v>879</v>
       </c>
       <c t="s" s="7" r="E243">
-        <v>876</v>
+        <v>880</v>
       </c>
     </row>
     <row r="244">
       <c s="11" r="A244"/>
       <c t="s" s="7" r="B244">
-        <v>877</v>
+        <v>881</v>
       </c>
       <c t="s" s="14" r="C244">
-        <v>878</v>
+        <v>882</v>
       </c>
       <c t="s" s="7" r="D244">
-        <v>879</v>
+        <v>883</v>
       </c>
       <c t="s" s="7" r="E244">
-        <v>880</v>
+        <v>884</v>
       </c>
     </row>
     <row r="245">
       <c s="11" r="A245"/>
       <c t="s" s="7" r="B245">
-        <v>881</v>
+        <v>885</v>
       </c>
       <c t="s" s="14" r="C245">
-        <v>882</v>
+        <v>886</v>
       </c>
       <c t="s" s="7" r="D245">
-        <v>883</v>
+        <v>887</v>
       </c>
       <c t="s" s="7" r="E245">
-        <v>884</v>
+        <v>888</v>
       </c>
     </row>
     <row r="246">
       <c s="11" r="A246"/>
       <c t="s" s="7" r="B246">
-        <v>885</v>
+        <v>889</v>
       </c>
       <c t="s" s="14" r="C246">
-        <v>886</v>
+        <v>890</v>
       </c>
       <c t="s" s="7" r="D246">
-        <v>887</v>
+        <v>891</v>
       </c>
       <c t="s" s="7" r="E246">
-        <v>888</v>
+        <v>892</v>
       </c>
     </row>
     <row r="247">
       <c s="11" r="A247"/>
       <c t="s" s="7" r="B247">
-        <v>889</v>
+        <v>893</v>
       </c>
       <c t="s" s="14" r="C247">
-        <v>890</v>
+        <v>894</v>
       </c>
       <c t="s" s="7" r="D247">
-        <v>891</v>
+        <v>895</v>
       </c>
       <c t="s" s="7" r="E247">
-        <v>892</v>
+        <v>896</v>
       </c>
     </row>
     <row r="248">
       <c s="11" r="A248"/>
       <c t="s" s="7" r="B248">
-        <v>893</v>
+        <v>897</v>
       </c>
       <c t="s" s="14" r="C248">
-        <v>894</v>
+        <v>898</v>
       </c>
       <c t="s" s="7" r="D248">
-        <v>895</v>
+        <v>899</v>
       </c>
       <c t="s" s="7" r="E248">
-        <v>896</v>
+        <v>900</v>
       </c>
     </row>
     <row r="249">
@@ -7528,94 +7542,94 @@
     </row>
     <row r="250">
       <c t="s" s="11" r="A250">
-        <v>897</v>
+        <v>901</v>
       </c>
       <c t="s" s="7" r="B250">
-        <v>898</v>
+        <v>902</v>
       </c>
       <c t="s" s="7" r="C250">
-        <v>899</v>
+        <v>903</v>
       </c>
       <c t="s" s="7" r="D250">
-        <v>900</v>
+        <v>904</v>
       </c>
       <c t="s" s="7" r="E250">
-        <v>901</v>
+        <v>905</v>
       </c>
     </row>
     <row r="251">
       <c s="11" r="A251"/>
       <c t="s" s="7" r="B251">
-        <v>902</v>
+        <v>906</v>
       </c>
       <c t="s" s="14" r="C251">
-        <v>903</v>
+        <v>907</v>
       </c>
       <c t="s" s="7" r="D251">
-        <v>904</v>
+        <v>908</v>
       </c>
       <c t="s" s="7" r="E251">
-        <v>905</v>
+        <v>909</v>
       </c>
     </row>
     <row r="252">
       <c s="11" r="A252"/>
       <c t="s" s="7" r="B252">
-        <v>906</v>
+        <v>910</v>
       </c>
       <c t="s" s="14" r="C252">
-        <v>907</v>
+        <v>911</v>
       </c>
       <c t="s" s="7" r="D252">
-        <v>908</v>
+        <v>912</v>
       </c>
       <c t="s" s="7" r="E252">
-        <v>909</v>
+        <v>913</v>
       </c>
     </row>
     <row r="253">
       <c s="11" r="A253"/>
       <c t="s" s="7" r="B253">
-        <v>910</v>
+        <v>914</v>
       </c>
       <c t="s" s="14" r="C253">
-        <v>911</v>
+        <v>915</v>
       </c>
       <c t="s" s="7" r="D253">
-        <v>912</v>
+        <v>916</v>
       </c>
       <c t="s" s="7" r="E253">
-        <v>913</v>
+        <v>917</v>
       </c>
     </row>
     <row r="254">
       <c s="11" r="A254"/>
       <c t="s" s="7" r="B254">
-        <v>914</v>
+        <v>918</v>
       </c>
       <c t="s" s="14" r="C254">
-        <v>631</v>
+        <v>635</v>
       </c>
       <c t="s" s="7" r="D254">
         <v>160</v>
       </c>
       <c t="s" s="7" r="E254">
-        <v>633</v>
+        <v>637</v>
       </c>
     </row>
     <row r="255">
       <c s="11" r="A255"/>
       <c t="s" s="7" r="B255">
-        <v>915</v>
+        <v>919</v>
       </c>
       <c t="s" s="14" r="C255">
-        <v>916</v>
+        <v>920</v>
       </c>
       <c t="s" s="7" r="D255">
-        <v>917</v>
+        <v>921</v>
       </c>
       <c t="s" s="7" r="E255">
-        <v>918</v>
+        <v>922</v>
       </c>
     </row>
     <row r="256">
@@ -7627,304 +7641,304 @@
     </row>
     <row r="257">
       <c t="s" s="11" r="A257">
-        <v>919</v>
+        <v>923</v>
       </c>
       <c t="s" s="7" r="B257">
-        <v>920</v>
+        <v>924</v>
       </c>
       <c t="s" s="14" r="C257">
-        <v>921</v>
+        <v>925</v>
       </c>
       <c t="s" s="7" r="D257">
-        <v>922</v>
+        <v>926</v>
       </c>
       <c t="s" s="7" r="E257">
-        <v>923</v>
+        <v>927</v>
       </c>
     </row>
     <row r="258">
       <c s="11" r="A258"/>
       <c t="s" s="7" r="B258">
-        <v>924</v>
+        <v>928</v>
       </c>
       <c t="s" s="14" r="C258">
-        <v>925</v>
+        <v>929</v>
       </c>
       <c t="s" s="7" r="D258">
-        <v>926</v>
+        <v>930</v>
       </c>
       <c t="s" s="7" r="E258">
-        <v>927</v>
+        <v>931</v>
       </c>
     </row>
     <row r="259">
       <c s="11" r="A259"/>
       <c t="s" s="7" r="B259">
-        <v>928</v>
+        <v>932</v>
       </c>
       <c t="s" s="14" r="C259">
-        <v>929</v>
+        <v>933</v>
       </c>
       <c t="s" s="7" r="D259">
-        <v>930</v>
+        <v>934</v>
       </c>
       <c t="s" s="7" r="E259">
-        <v>931</v>
+        <v>935</v>
       </c>
     </row>
     <row r="260">
       <c s="11" r="A260"/>
       <c t="s" s="7" r="B260">
-        <v>932</v>
+        <v>936</v>
       </c>
       <c t="s" s="14" r="C260">
-        <v>933</v>
+        <v>937</v>
       </c>
       <c t="s" s="7" r="D260">
-        <v>934</v>
+        <v>938</v>
       </c>
       <c t="s" s="7" r="E260">
-        <v>934</v>
+        <v>938</v>
       </c>
     </row>
     <row r="261">
       <c s="11" r="A261"/>
       <c t="s" s="7" r="B261">
-        <v>935</v>
+        <v>939</v>
       </c>
       <c t="s" s="14" r="C261">
-        <v>936</v>
+        <v>940</v>
       </c>
       <c t="s" s="7" r="D261">
-        <v>937</v>
+        <v>941</v>
       </c>
       <c t="s" s="7" r="E261">
-        <v>938</v>
+        <v>942</v>
       </c>
     </row>
     <row r="262">
       <c s="11" r="A262"/>
       <c t="s" s="7" r="B262">
-        <v>939</v>
+        <v>943</v>
       </c>
       <c t="s" s="14" r="C262">
-        <v>940</v>
+        <v>944</v>
       </c>
       <c t="s" s="7" r="D262">
-        <v>941</v>
+        <v>945</v>
       </c>
       <c t="s" s="7" r="E262">
-        <v>942</v>
+        <v>946</v>
       </c>
     </row>
     <row r="263">
       <c s="11" r="A263"/>
       <c t="s" s="7" r="B263">
-        <v>943</v>
+        <v>947</v>
       </c>
       <c t="s" s="14" r="C263">
-        <v>944</v>
+        <v>948</v>
       </c>
       <c t="s" s="7" r="D263">
-        <v>945</v>
+        <v>949</v>
       </c>
       <c t="s" s="7" r="E263">
-        <v>946</v>
+        <v>950</v>
       </c>
     </row>
     <row r="264">
       <c s="11" r="A264"/>
       <c t="s" s="7" r="B264">
-        <v>947</v>
+        <v>951</v>
       </c>
       <c t="s" s="14" r="C264">
-        <v>948</v>
+        <v>952</v>
       </c>
       <c t="s" s="7" r="D264">
-        <v>949</v>
+        <v>953</v>
       </c>
       <c t="s" s="7" r="E264">
-        <v>950</v>
+        <v>954</v>
       </c>
     </row>
     <row r="265">
       <c s="11" r="A265"/>
       <c t="s" s="7" r="B265">
-        <v>951</v>
+        <v>955</v>
       </c>
       <c t="s" s="14" r="C265">
-        <v>952</v>
+        <v>956</v>
       </c>
       <c t="s" s="7" r="D265">
-        <v>953</v>
+        <v>957</v>
       </c>
       <c t="s" s="7" r="E265">
-        <v>954</v>
+        <v>958</v>
       </c>
     </row>
     <row r="266">
       <c s="11" r="A266"/>
       <c t="s" s="7" r="B266">
-        <v>955</v>
+        <v>959</v>
       </c>
       <c t="s" s="14" r="C266">
-        <v>956</v>
+        <v>960</v>
       </c>
       <c t="s" s="7" r="D266">
-        <v>957</v>
+        <v>961</v>
       </c>
       <c t="s" s="7" r="E266">
-        <v>958</v>
+        <v>962</v>
       </c>
     </row>
     <row r="267">
       <c s="11" r="A267"/>
       <c t="s" s="7" r="B267">
-        <v>959</v>
+        <v>963</v>
       </c>
       <c t="s" s="14" r="C267">
-        <v>960</v>
+        <v>964</v>
       </c>
       <c t="s" s="7" r="D267">
-        <v>961</v>
+        <v>965</v>
       </c>
       <c t="s" s="7" r="E267">
-        <v>962</v>
+        <v>966</v>
       </c>
     </row>
     <row r="268">
       <c s="11" r="A268"/>
       <c t="s" s="7" r="B268">
-        <v>963</v>
+        <v>967</v>
       </c>
       <c t="s" s="14" r="C268">
-        <v>964</v>
+        <v>968</v>
       </c>
       <c t="s" s="7" r="D268">
-        <v>965</v>
+        <v>969</v>
       </c>
       <c t="s" s="7" r="E268">
-        <v>966</v>
+        <v>970</v>
       </c>
     </row>
     <row r="269">
       <c s="11" r="A269"/>
       <c t="s" s="7" r="B269">
-        <v>967</v>
+        <v>971</v>
       </c>
       <c t="s" s="14" r="C269">
-        <v>968</v>
+        <v>972</v>
       </c>
       <c t="s" s="7" r="D269">
-        <v>968</v>
+        <v>972</v>
       </c>
       <c t="s" s="7" r="E269">
-        <v>968</v>
+        <v>972</v>
       </c>
     </row>
     <row r="270">
       <c s="11" r="A270"/>
       <c t="s" s="7" r="B270">
-        <v>969</v>
+        <v>973</v>
       </c>
       <c t="s" s="14" r="C270">
-        <v>970</v>
+        <v>974</v>
       </c>
       <c t="s" s="7" r="D270">
-        <v>971</v>
+        <v>975</v>
       </c>
       <c t="s" s="7" r="E270">
-        <v>972</v>
+        <v>976</v>
       </c>
     </row>
     <row r="271">
       <c s="11" r="A271"/>
       <c t="s" s="7" r="B271">
-        <v>973</v>
+        <v>977</v>
       </c>
       <c t="s" s="14" r="C271">
-        <v>974</v>
+        <v>978</v>
       </c>
       <c t="s" s="7" r="D271">
-        <v>975</v>
+        <v>979</v>
       </c>
       <c t="s" s="7" r="E271">
-        <v>976</v>
+        <v>980</v>
       </c>
     </row>
     <row r="272">
       <c s="11" r="A272"/>
       <c t="s" s="7" r="B272">
-        <v>977</v>
+        <v>981</v>
       </c>
       <c t="s" s="14" r="C272">
-        <v>978</v>
+        <v>982</v>
       </c>
       <c t="s" s="7" r="D272">
-        <v>979</v>
+        <v>983</v>
       </c>
       <c t="s" s="7" r="E272">
-        <v>980</v>
+        <v>984</v>
       </c>
     </row>
     <row r="273">
       <c s="11" r="A273"/>
       <c t="s" s="7" r="B273">
-        <v>981</v>
+        <v>985</v>
       </c>
       <c t="s" s="14" r="C273">
-        <v>982</v>
+        <v>986</v>
       </c>
       <c t="s" s="7" r="D273">
-        <v>983</v>
+        <v>987</v>
       </c>
       <c t="s" s="7" r="E273">
-        <v>984</v>
+        <v>988</v>
       </c>
     </row>
     <row r="274">
       <c s="11" r="A274"/>
       <c t="s" s="7" r="B274">
-        <v>985</v>
+        <v>989</v>
       </c>
       <c t="s" s="14" r="C274">
-        <v>986</v>
+        <v>990</v>
       </c>
       <c t="s" s="7" r="D274">
-        <v>987</v>
+        <v>991</v>
       </c>
       <c t="s" s="7" r="E274">
-        <v>988</v>
+        <v>992</v>
       </c>
     </row>
     <row r="275">
       <c s="11" r="A275"/>
       <c t="s" s="7" r="B275">
-        <v>989</v>
+        <v>993</v>
       </c>
       <c t="s" s="14" r="C275">
-        <v>990</v>
+        <v>994</v>
       </c>
       <c t="s" s="7" r="D275">
-        <v>991</v>
+        <v>995</v>
       </c>
       <c t="s" s="7" r="E275">
-        <v>992</v>
+        <v>996</v>
       </c>
     </row>
     <row r="276">
       <c s="11" r="A276"/>
       <c t="s" s="7" r="B276">
-        <v>993</v>
+        <v>997</v>
       </c>
       <c t="s" s="14" r="C276">
-        <v>994</v>
+        <v>998</v>
       </c>
       <c t="s" s="7" r="D276">
-        <v>995</v>
+        <v>999</v>
       </c>
       <c t="s" s="7" r="E276">
-        <v>996</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="277">
@@ -7936,124 +7950,124 @@
     </row>
     <row r="278">
       <c t="s" s="11" r="A278">
-        <v>997</v>
+        <v>1001</v>
       </c>
       <c t="s" s="7" r="B278">
-        <v>998</v>
+        <v>1002</v>
       </c>
       <c t="s" s="14" r="C278">
-        <v>999</v>
+        <v>1003</v>
       </c>
       <c t="s" s="7" r="D278">
-        <v>1000</v>
+        <v>1004</v>
       </c>
       <c t="s" s="7" r="E278">
-        <v>1001</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="279">
       <c s="11" r="A279"/>
       <c t="s" s="7" r="B279">
-        <v>1002</v>
+        <v>1006</v>
       </c>
       <c t="s" s="14" r="C279">
-        <v>1003</v>
+        <v>1007</v>
       </c>
       <c t="s" s="7" r="D279">
-        <v>1004</v>
+        <v>1008</v>
       </c>
       <c t="s" s="7" r="E279">
-        <v>1005</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="280">
       <c s="11" r="A280"/>
       <c t="s" s="7" r="B280">
-        <v>1006</v>
+        <v>1010</v>
       </c>
       <c t="s" s="14" r="C280">
-        <v>1007</v>
+        <v>1011</v>
       </c>
       <c t="s" s="7" r="D280">
-        <v>1008</v>
+        <v>1012</v>
       </c>
       <c t="s" s="7" r="E280">
-        <v>1009</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="281">
       <c s="11" r="A281"/>
       <c t="s" s="7" r="B281">
-        <v>1010</v>
+        <v>1014</v>
       </c>
       <c t="s" s="14" r="C281">
-        <v>1011</v>
+        <v>1015</v>
       </c>
       <c t="s" s="7" r="D281">
-        <v>1012</v>
+        <v>1016</v>
       </c>
       <c t="s" s="7" r="E281">
-        <v>1013</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="282">
       <c s="11" r="A282"/>
       <c t="s" s="7" r="B282">
-        <v>1014</v>
+        <v>1018</v>
       </c>
       <c t="s" s="14" r="C282">
-        <v>1014</v>
+        <v>1018</v>
       </c>
       <c t="s" s="19" r="D282">
-        <v>1015</v>
+        <v>1019</v>
       </c>
       <c t="s" s="19" r="E282">
-        <v>1016</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="283">
       <c s="11" r="A283"/>
       <c t="s" s="7" r="B283">
-        <v>1017</v>
+        <v>1021</v>
       </c>
       <c t="s" s="14" r="C283">
-        <v>1018</v>
+        <v>1022</v>
       </c>
       <c t="s" s="7" r="D283">
-        <v>1019</v>
+        <v>1023</v>
       </c>
       <c t="s" s="7" r="E283">
-        <v>1020</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="284">
       <c s="11" r="A284"/>
       <c t="s" s="7" r="B284">
-        <v>1021</v>
+        <v>1025</v>
       </c>
       <c t="s" s="14" r="C284">
-        <v>1022</v>
+        <v>1026</v>
       </c>
       <c t="s" s="7" r="D284">
-        <v>1023</v>
+        <v>1027</v>
       </c>
       <c t="s" s="7" r="E284">
-        <v>1024</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="285">
       <c t="s" s="17" r="A285">
-        <v>1025</v>
+        <v>1029</v>
       </c>
       <c s="27" r="B285"/>
       <c t="s" s="14" r="C285">
-        <v>1026</v>
+        <v>1030</v>
       </c>
       <c t="s" s="19" r="D285">
-        <v>1027</v>
+        <v>1031</v>
       </c>
       <c t="s" s="19" r="E285">
-        <v>1028</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="286">
@@ -8065,291 +8079,291 @@
     </row>
     <row r="287">
       <c t="s" s="18" r="A287">
-        <v>1029</v>
+        <v>1033</v>
       </c>
       <c t="s" s="7" r="B287">
-        <v>1030</v>
+        <v>1034</v>
       </c>
       <c t="s" s="7" r="C287">
-        <v>1031</v>
+        <v>1035</v>
       </c>
       <c t="s" s="7" r="D287">
-        <v>1032</v>
+        <v>1036</v>
       </c>
       <c t="s" s="7" r="E287">
-        <v>1033</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="288">
       <c s="15" r="A288"/>
       <c t="s" s="7" r="B288">
-        <v>1034</v>
+        <v>1038</v>
       </c>
       <c t="s" s="14" r="C288">
-        <v>1035</v>
+        <v>1039</v>
       </c>
       <c t="s" s="7" r="D288">
-        <v>1036</v>
+        <v>1040</v>
       </c>
       <c t="s" s="7" r="E288">
-        <v>1037</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="289">
       <c s="15" r="A289"/>
       <c t="s" s="7" r="B289">
-        <v>1038</v>
+        <v>1042</v>
       </c>
       <c t="s" s="7" r="C289">
-        <v>1039</v>
+        <v>1043</v>
       </c>
       <c t="s" s="7" r="D289">
-        <v>1040</v>
+        <v>1044</v>
       </c>
       <c t="s" s="7" r="E289">
-        <v>1041</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="290">
       <c s="18" r="A290"/>
       <c t="s" s="7" r="B290">
-        <v>1042</v>
+        <v>1046</v>
       </c>
       <c t="s" s="14" r="C290">
-        <v>1043</v>
+        <v>1047</v>
       </c>
       <c t="s" s="7" r="D290">
-        <v>1044</v>
+        <v>1048</v>
       </c>
       <c t="s" s="7" r="E290">
-        <v>1045</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="291">
       <c s="18" r="A291"/>
       <c t="s" s="7" r="B291">
-        <v>1046</v>
+        <v>1050</v>
       </c>
       <c t="s" s="7" r="C291">
-        <v>1047</v>
+        <v>1051</v>
       </c>
       <c t="s" s="7" r="D291">
-        <v>1048</v>
+        <v>1052</v>
       </c>
       <c t="s" s="7" r="E291">
-        <v>1049</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="292">
       <c s="18" r="A292"/>
       <c t="s" s="7" r="B292">
-        <v>1050</v>
+        <v>1054</v>
       </c>
       <c t="s" s="14" r="C292">
-        <v>1051</v>
+        <v>1055</v>
       </c>
       <c t="s" s="7" r="D292">
-        <v>1052</v>
+        <v>1056</v>
       </c>
       <c t="s" s="7" r="E292">
-        <v>1053</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="293">
       <c s="18" r="A293"/>
       <c t="s" s="7" r="B293">
-        <v>1054</v>
+        <v>1058</v>
       </c>
       <c t="s" s="7" r="C293">
-        <v>1055</v>
+        <v>1059</v>
       </c>
       <c t="s" s="7" r="D293">
-        <v>1056</v>
+        <v>1060</v>
       </c>
       <c t="s" s="7" r="E293">
-        <v>1057</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="294">
       <c s="18" r="A294"/>
       <c t="s" s="7" r="B294">
-        <v>1058</v>
+        <v>1062</v>
       </c>
       <c t="s" s="14" r="C294">
-        <v>1059</v>
+        <v>1063</v>
       </c>
       <c t="s" s="7" r="D294">
-        <v>1060</v>
+        <v>1064</v>
       </c>
       <c t="s" s="7" r="E294">
-        <v>1061</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="295">
       <c s="18" r="A295"/>
       <c t="s" s="7" r="B295">
-        <v>1062</v>
+        <v>1066</v>
       </c>
       <c t="s" s="7" r="C295">
-        <v>1063</v>
+        <v>1067</v>
       </c>
       <c t="s" s="7" r="D295">
-        <v>1064</v>
+        <v>1068</v>
       </c>
       <c t="s" s="7" r="E295">
-        <v>1065</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="296">
       <c s="18" r="A296"/>
       <c t="s" s="7" r="B296">
-        <v>1066</v>
+        <v>1070</v>
       </c>
       <c t="s" s="14" r="C296">
-        <v>1067</v>
+        <v>1071</v>
       </c>
       <c t="s" s="7" r="D296">
-        <v>1068</v>
+        <v>1072</v>
       </c>
       <c t="s" s="7" r="E296">
-        <v>1069</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="297">
       <c s="18" r="A297"/>
       <c t="s" s="7" r="B297">
-        <v>1070</v>
+        <v>1074</v>
       </c>
       <c t="s" s="7" r="C297">
-        <v>1071</v>
+        <v>1075</v>
       </c>
       <c t="s" s="7" r="D297">
-        <v>1072</v>
+        <v>1076</v>
       </c>
       <c t="s" s="7" r="E297">
-        <v>1073</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="298">
       <c s="18" r="A298"/>
       <c t="s" s="7" r="B298">
-        <v>1074</v>
+        <v>1078</v>
       </c>
       <c t="s" s="14" r="C298">
-        <v>1067</v>
+        <v>1071</v>
       </c>
       <c t="s" s="7" r="D298">
-        <v>1068</v>
+        <v>1072</v>
       </c>
       <c t="s" s="7" r="E298">
-        <v>1069</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="299">
       <c s="18" r="A299"/>
       <c t="s" s="7" r="B299">
-        <v>1075</v>
+        <v>1079</v>
       </c>
       <c t="s" s="14" r="C299">
-        <v>1076</v>
+        <v>1080</v>
       </c>
       <c t="s" s="7" r="D299">
-        <v>1077</v>
+        <v>1081</v>
       </c>
       <c t="s" s="7" r="E299">
-        <v>1078</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="300">
       <c s="18" r="A300"/>
       <c t="s" s="7" r="B300">
-        <v>1079</v>
+        <v>1083</v>
       </c>
       <c t="s" s="14" r="C300">
-        <v>1080</v>
+        <v>1084</v>
       </c>
       <c t="s" s="7" r="D300">
-        <v>1081</v>
+        <v>1085</v>
       </c>
       <c t="s" s="7" r="E300">
-        <v>1082</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="301">
       <c s="18" r="A301"/>
       <c t="s" s="7" r="B301">
-        <v>1083</v>
+        <v>1087</v>
       </c>
       <c t="s" s="7" r="C301">
-        <v>1084</v>
+        <v>1088</v>
       </c>
       <c t="s" s="7" r="D301">
-        <v>1085</v>
+        <v>1089</v>
       </c>
       <c t="s" s="7" r="E301">
-        <v>1086</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="302">
       <c s="18" r="A302"/>
       <c t="s" s="7" r="B302">
-        <v>1087</v>
+        <v>1091</v>
       </c>
       <c t="s" s="14" r="C302">
-        <v>1088</v>
+        <v>1092</v>
       </c>
       <c t="s" s="7" r="D302">
-        <v>1089</v>
+        <v>1093</v>
       </c>
       <c t="s" s="7" r="E302">
-        <v>1090</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="303">
       <c s="11" r="A303"/>
       <c t="s" s="7" r="B303">
-        <v>1091</v>
+        <v>1095</v>
       </c>
       <c t="s" s="14" r="C303">
-        <v>1092</v>
+        <v>1096</v>
       </c>
       <c t="s" s="7" r="D303">
-        <v>1093</v>
+        <v>1097</v>
       </c>
       <c t="s" s="7" r="E303">
-        <v>1094</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="304">
       <c t="s" s="11" r="A304">
-        <v>1095</v>
+        <v>1099</v>
       </c>
       <c t="s" s="14" r="B304">
-        <v>1096</v>
+        <v>1100</v>
       </c>
       <c t="s" s="14" r="C304">
-        <v>1097</v>
+        <v>1101</v>
       </c>
       <c t="s" s="19" r="D304">
-        <v>1098</v>
+        <v>1102</v>
       </c>
       <c t="s" s="7" r="E304">
-        <v>1099</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="305">
       <c s="11" r="A305"/>
       <c t="s" s="14" r="B305">
-        <v>1100</v>
+        <v>1104</v>
       </c>
       <c t="s" s="14" r="C305">
-        <v>1101</v>
+        <v>1105</v>
       </c>
       <c t="s" s="19" r="D305">
-        <v>1102</v>
+        <v>1106</v>
       </c>
       <c t="s" s="7" r="E305">
-        <v>1103</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="306">
@@ -8374,17 +8388,17 @@
   <sheetData>
     <row customHeight="1" r="1" ht="112.5">
       <c t="s" s="4" r="A1">
-        <v>1104</v>
+        <v>1108</v>
       </c>
     </row>
     <row customHeight="1" r="2" ht="112.5">
       <c t="s" s="5" r="A2">
-        <v>1105</v>
+        <v>1109</v>
       </c>
     </row>
     <row customHeight="1" r="3" ht="112.5">
       <c t="s" s="10" r="A3">
-        <v>1106</v>
+        <v>1110</v>
       </c>
     </row>
   </sheetData>
@@ -8399,164 +8413,164 @@
   <sheetFormatPr customHeight="1" defaultColWidth="9.86" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c s="35" r="A1"/>
-      <c s="35" r="B1"/>
-      <c s="35" r="C1"/>
-      <c s="35" r="D1"/>
-      <c s="35" r="E1"/>
-      <c s="35" r="F1"/>
+      <c s="34" r="A1"/>
+      <c s="34" r="B1"/>
+      <c s="34" r="C1"/>
+      <c s="34" r="D1"/>
+      <c s="34" r="E1"/>
+      <c s="34" r="F1"/>
     </row>
     <row r="2">
-      <c s="35" r="A2"/>
-      <c s="35" r="B2"/>
-      <c s="35" r="C2"/>
-      <c s="35" r="D2"/>
-      <c s="35" r="E2"/>
-      <c s="35" r="F2"/>
+      <c s="34" r="A2"/>
+      <c s="34" r="B2"/>
+      <c s="34" r="C2"/>
+      <c s="34" r="D2"/>
+      <c s="34" r="E2"/>
+      <c s="34" r="F2"/>
     </row>
     <row r="3">
-      <c s="35" r="A3"/>
-      <c s="35" r="B3"/>
-      <c s="35" r="C3"/>
-      <c s="35" r="D3"/>
-      <c s="35" r="E3"/>
-      <c s="35" r="F3"/>
+      <c s="34" r="A3"/>
+      <c s="34" r="B3"/>
+      <c s="34" r="C3"/>
+      <c s="34" r="D3"/>
+      <c s="34" r="E3"/>
+      <c s="34" r="F3"/>
     </row>
     <row r="4">
-      <c s="35" r="A4"/>
-      <c s="35" r="B4"/>
-      <c s="35" r="C4"/>
-      <c s="35" r="D4"/>
-      <c s="35" r="E4"/>
-      <c s="35" r="F4"/>
+      <c s="34" r="A4"/>
+      <c s="34" r="B4"/>
+      <c s="34" r="C4"/>
+      <c s="34" r="D4"/>
+      <c s="34" r="E4"/>
+      <c s="34" r="F4"/>
     </row>
     <row r="5">
-      <c s="35" r="A5"/>
-      <c s="35" r="B5"/>
-      <c s="35" r="C5"/>
-      <c s="35" r="D5"/>
-      <c s="35" r="E5"/>
-      <c s="35" r="F5"/>
+      <c s="34" r="A5"/>
+      <c s="34" r="B5"/>
+      <c s="34" r="C5"/>
+      <c s="34" r="D5"/>
+      <c s="34" r="E5"/>
+      <c s="34" r="F5"/>
     </row>
     <row r="6">
-      <c s="35" r="A6"/>
-      <c s="35" r="B6"/>
-      <c s="35" r="C6"/>
-      <c s="35" r="D6"/>
-      <c s="35" r="E6"/>
-      <c s="35" r="F6"/>
+      <c s="34" r="A6"/>
+      <c s="34" r="B6"/>
+      <c s="34" r="C6"/>
+      <c s="34" r="D6"/>
+      <c s="34" r="E6"/>
+      <c s="34" r="F6"/>
     </row>
     <row r="7">
-      <c s="35" r="A7"/>
-      <c s="35" r="B7"/>
-      <c s="35" r="C7"/>
-      <c s="35" r="D7"/>
-      <c s="35" r="E7"/>
-      <c s="35" r="F7"/>
+      <c s="34" r="A7"/>
+      <c s="34" r="B7"/>
+      <c s="34" r="C7"/>
+      <c s="34" r="D7"/>
+      <c s="34" r="E7"/>
+      <c s="34" r="F7"/>
     </row>
     <row r="8">
-      <c s="35" r="A8"/>
-      <c s="35" r="B8"/>
-      <c s="35" r="C8"/>
-      <c s="35" r="D8"/>
-      <c s="35" r="E8"/>
-      <c s="35" r="F8"/>
+      <c s="34" r="A8"/>
+      <c s="34" r="B8"/>
+      <c s="34" r="C8"/>
+      <c s="34" r="D8"/>
+      <c s="34" r="E8"/>
+      <c s="34" r="F8"/>
     </row>
     <row r="9">
-      <c s="35" r="A9"/>
-      <c s="35" r="B9"/>
-      <c s="35" r="C9"/>
-      <c s="35" r="D9"/>
-      <c s="35" r="E9"/>
-      <c s="35" r="F9"/>
+      <c s="34" r="A9"/>
+      <c s="34" r="B9"/>
+      <c s="34" r="C9"/>
+      <c s="34" r="D9"/>
+      <c s="34" r="E9"/>
+      <c s="34" r="F9"/>
     </row>
     <row r="10">
-      <c s="35" r="A10"/>
-      <c s="35" r="B10"/>
-      <c s="35" r="C10"/>
-      <c s="35" r="D10"/>
-      <c s="35" r="E10"/>
-      <c s="35" r="F10"/>
+      <c s="34" r="A10"/>
+      <c s="34" r="B10"/>
+      <c s="34" r="C10"/>
+      <c s="34" r="D10"/>
+      <c s="34" r="E10"/>
+      <c s="34" r="F10"/>
     </row>
     <row r="11">
-      <c s="35" r="A11"/>
-      <c s="35" r="B11"/>
-      <c s="35" r="C11"/>
-      <c s="35" r="D11"/>
-      <c s="35" r="E11"/>
-      <c s="35" r="F11"/>
+      <c s="34" r="A11"/>
+      <c s="34" r="B11"/>
+      <c s="34" r="C11"/>
+      <c s="34" r="D11"/>
+      <c s="34" r="E11"/>
+      <c s="34" r="F11"/>
     </row>
     <row r="12">
-      <c s="35" r="A12"/>
-      <c s="35" r="B12"/>
-      <c s="35" r="C12"/>
-      <c s="35" r="D12"/>
-      <c s="35" r="E12"/>
-      <c s="35" r="F12"/>
+      <c s="34" r="A12"/>
+      <c s="34" r="B12"/>
+      <c s="34" r="C12"/>
+      <c s="34" r="D12"/>
+      <c s="34" r="E12"/>
+      <c s="34" r="F12"/>
     </row>
     <row r="13">
-      <c s="35" r="A13"/>
-      <c s="35" r="B13"/>
-      <c s="35" r="C13"/>
-      <c s="35" r="D13"/>
-      <c s="35" r="E13"/>
-      <c s="35" r="F13"/>
+      <c s="34" r="A13"/>
+      <c s="34" r="B13"/>
+      <c s="34" r="C13"/>
+      <c s="34" r="D13"/>
+      <c s="34" r="E13"/>
+      <c s="34" r="F13"/>
     </row>
     <row r="14">
-      <c s="35" r="A14"/>
-      <c s="35" r="B14"/>
-      <c s="35" r="C14"/>
-      <c s="35" r="D14"/>
-      <c s="35" r="E14"/>
-      <c s="35" r="F14"/>
+      <c s="34" r="A14"/>
+      <c s="34" r="B14"/>
+      <c s="34" r="C14"/>
+      <c s="34" r="D14"/>
+      <c s="34" r="E14"/>
+      <c s="34" r="F14"/>
     </row>
     <row r="15">
-      <c s="35" r="A15"/>
-      <c s="35" r="B15"/>
-      <c s="35" r="C15"/>
-      <c s="35" r="D15"/>
-      <c s="35" r="E15"/>
-      <c s="35" r="F15"/>
+      <c s="34" r="A15"/>
+      <c s="34" r="B15"/>
+      <c s="34" r="C15"/>
+      <c s="34" r="D15"/>
+      <c s="34" r="E15"/>
+      <c s="34" r="F15"/>
     </row>
     <row r="16">
-      <c s="35" r="A16"/>
-      <c s="35" r="B16"/>
-      <c s="35" r="C16"/>
-      <c s="35" r="D16"/>
-      <c s="35" r="E16"/>
-      <c s="35" r="F16"/>
+      <c s="34" r="A16"/>
+      <c s="34" r="B16"/>
+      <c s="34" r="C16"/>
+      <c s="34" r="D16"/>
+      <c s="34" r="E16"/>
+      <c s="34" r="F16"/>
     </row>
     <row r="17">
-      <c s="35" r="A17"/>
-      <c s="35" r="B17"/>
-      <c s="35" r="C17"/>
-      <c s="35" r="D17"/>
-      <c s="35" r="E17"/>
-      <c s="35" r="F17"/>
+      <c s="34" r="A17"/>
+      <c s="34" r="B17"/>
+      <c s="34" r="C17"/>
+      <c s="34" r="D17"/>
+      <c s="34" r="E17"/>
+      <c s="34" r="F17"/>
     </row>
     <row r="18">
-      <c s="35" r="A18"/>
-      <c s="35" r="B18"/>
-      <c s="35" r="C18"/>
-      <c s="35" r="D18"/>
-      <c s="35" r="E18"/>
-      <c s="35" r="F18"/>
+      <c s="34" r="A18"/>
+      <c s="34" r="B18"/>
+      <c s="34" r="C18"/>
+      <c s="34" r="D18"/>
+      <c s="34" r="E18"/>
+      <c s="34" r="F18"/>
     </row>
     <row r="19">
-      <c s="35" r="A19"/>
-      <c s="35" r="B19"/>
-      <c s="35" r="C19"/>
-      <c s="35" r="D19"/>
-      <c s="35" r="E19"/>
-      <c s="35" r="F19"/>
+      <c s="34" r="A19"/>
+      <c s="34" r="B19"/>
+      <c s="34" r="C19"/>
+      <c s="34" r="D19"/>
+      <c s="34" r="E19"/>
+      <c s="34" r="F19"/>
     </row>
     <row r="20">
-      <c s="35" r="A20"/>
-      <c s="35" r="B20"/>
-      <c s="35" r="C20"/>
-      <c s="35" r="D20"/>
-      <c s="35" r="E20"/>
-      <c s="35" r="F20"/>
+      <c s="34" r="A20"/>
+      <c s="34" r="B20"/>
+      <c s="34" r="C20"/>
+      <c s="34" r="D20"/>
+      <c s="34" r="E20"/>
+      <c s="34" r="F20"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
EWD-22745 - Question content in editor
Former-commit-id: 711a7088029048f2f05e143c563c05290a718708
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="1132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="1144">
   <si>
     <t>nnot</t>
   </si>
@@ -1329,6 +1329,30 @@
   </si>
   <si>
     <t>Als falsch markieren</t>
+  </si>
+  <si>
+    <t>questionContent</t>
+  </si>
+  <si>
+    <t>Question content</t>
+  </si>
+  <si>
+    <t>Inhoud vraag</t>
+  </si>
+  <si>
+    <t>Frageninhalt</t>
+  </si>
+  <si>
+    <t>defineQuestionContent</t>
+  </si>
+  <si>
+    <t>Define question content</t>
+  </si>
+  <si>
+    <t>Inhoud vraag definiëren</t>
+  </si>
+  <si>
+    <t>Frageninhalt definieren</t>
   </si>
   <si>
     <t>Questions</t>
@@ -3433,10 +3457,22 @@
     <t>Embed Media</t>
   </si>
   <si>
+    <t>Media invoegen</t>
+  </si>
+  <si>
+    <t>Medien einbetten</t>
+  </si>
+  <si>
     <t>pasteEmbedCodeHere</t>
   </si>
   <si>
     <t>Paste Embed Code Here</t>
+  </si>
+  <si>
+    <t>Code hier invoegen</t>
+  </si>
+  <si>
+    <t>Code hier einbetten</t>
   </si>
   <si>
     <t>Translated OK</t>
@@ -3452,7 +3488,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="26">
+  <fonts count="24">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -3616,15 +3652,6 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <b/>
       <i val="0"/>
       <strike val="0"/>
@@ -3678,17 +3705,8 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="29">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3789,12 +3807,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF00FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -3808,18 +3820,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00FF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3861,19 +3861,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF00FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3902,7 +3890,7 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="35">
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
@@ -3961,62 +3949,47 @@
     <xf applyAlignment="1" fillId="16" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="15" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="17" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+    <xf applyAlignment="1" fillId="17" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="16" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="18" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="16" applyFill="1">
+    <xf applyAlignment="1" fillId="18" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="19" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+    <xf applyAlignment="1" fillId="19" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="17" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="20" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="17" applyFill="1">
-      <alignment vertical="center" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" fillId="21" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="18" applyFill="1">
-      <alignment vertical="center" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" fillId="22" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="18">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="19">
+      <alignment vertical="bottom" horizontal="right"/>
+    </xf>
+    <xf applyAlignment="1" fillId="20" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="21" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="20" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="20">
-      <alignment vertical="bottom" horizontal="right"/>
+    <xf applyAlignment="1" fillId="22" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="21" applyFill="1">
+      <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="23" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+      <alignment vertical="center" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="24" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="24" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="21" applyFill="1">
-      <alignment vertical="center" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" fillId="25" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="22" applyFill="1">
+    <xf applyAlignment="1" fillId="25" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="26" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="27" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="22"/>
+    <xf applyAlignment="1" fillId="27" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="23" applyFill="1">
+      <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="28" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
-      <alignment vertical="center" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" fillId="29" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" fillId="30" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
-      <alignment vertical="center" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="23"/>
-    <xf applyAlignment="1" fillId="31" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="24" applyFill="1">
-      <alignment vertical="center" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" fillId="32" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="25" applyFill="1">
-      <alignment vertical="center" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" fillId="33" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4044,24 +4017,24 @@
   </cols>
   <sheetData>
     <row s="6" customFormat="1" r="1">
-      <c t="s" s="29" r="A1">
+      <c t="s" s="26" r="A1">
         <v>0</v>
       </c>
-      <c t="s" s="29" r="B1">
+      <c t="s" s="26" r="B1">
         <v>1</v>
       </c>
-      <c t="s" s="29" r="C1">
+      <c t="s" s="26" r="C1">
         <v>2</v>
       </c>
-      <c t="s" s="29" r="D1">
+      <c t="s" s="26" r="D1">
         <v>3</v>
       </c>
-      <c t="s" s="26" r="E1">
+      <c t="s" s="23" r="E1">
         <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c t="s" s="21" r="A2">
+      <c t="s" s="20" r="A2">
         <v>5</v>
       </c>
       <c t="s" s="7" r="B2">
@@ -4078,7 +4051,7 @@
       </c>
     </row>
     <row r="3">
-      <c s="21" r="A3"/>
+      <c s="20" r="A3"/>
       <c t="s" s="7" r="B3">
         <v>10</v>
       </c>
@@ -4093,7 +4066,7 @@
       </c>
     </row>
     <row r="4">
-      <c s="21" r="A4"/>
+      <c s="20" r="A4"/>
       <c t="s" s="7" r="B4">
         <v>14</v>
       </c>
@@ -4108,7 +4081,7 @@
       </c>
     </row>
     <row r="5">
-      <c s="21" r="A5"/>
+      <c s="20" r="A5"/>
       <c t="s" s="7" r="B5">
         <v>18</v>
       </c>
@@ -4123,7 +4096,7 @@
       </c>
     </row>
     <row r="6">
-      <c s="21" r="A6"/>
+      <c s="20" r="A6"/>
       <c t="s" s="7" r="B6">
         <v>22</v>
       </c>
@@ -4138,7 +4111,7 @@
       </c>
     </row>
     <row r="7">
-      <c s="21" r="A7"/>
+      <c s="20" r="A7"/>
       <c t="s" s="7" r="B7">
         <v>24</v>
       </c>
@@ -4153,7 +4126,7 @@
       </c>
     </row>
     <row r="8">
-      <c s="21" r="A8"/>
+      <c s="20" r="A8"/>
       <c t="s" s="7" r="B8">
         <v>26</v>
       </c>
@@ -4168,7 +4141,7 @@
       </c>
     </row>
     <row r="9">
-      <c s="21" r="A9"/>
+      <c s="20" r="A9"/>
       <c t="s" s="7" r="B9">
         <v>30</v>
       </c>
@@ -4183,7 +4156,7 @@
       </c>
     </row>
     <row r="10">
-      <c s="21" r="A10"/>
+      <c s="20" r="A10"/>
       <c t="s" s="7" r="B10">
         <v>34</v>
       </c>
@@ -4198,7 +4171,7 @@
       </c>
     </row>
     <row r="11">
-      <c s="21" r="A11"/>
+      <c s="20" r="A11"/>
       <c t="s" s="7" r="B11">
         <v>38</v>
       </c>
@@ -4213,7 +4186,7 @@
       </c>
     </row>
     <row r="12">
-      <c s="21" r="A12"/>
+      <c s="20" r="A12"/>
       <c t="s" s="7" r="B12">
         <v>42</v>
       </c>
@@ -4513,7 +4486,7 @@
       </c>
     </row>
     <row r="32">
-      <c s="21" r="A32"/>
+      <c s="20" r="A32"/>
       <c t="s" s="7" r="B32">
         <v>121</v>
       </c>
@@ -4528,7 +4501,7 @@
       </c>
     </row>
     <row r="33">
-      <c s="21" r="A33"/>
+      <c s="20" r="A33"/>
       <c t="s" s="7" r="B33">
         <v>125</v>
       </c>
@@ -4543,7 +4516,7 @@
       </c>
     </row>
     <row r="34">
-      <c s="21" r="A34"/>
+      <c s="20" r="A34"/>
       <c t="s" s="7" r="B34">
         <v>129</v>
       </c>
@@ -4558,7 +4531,7 @@
       </c>
     </row>
     <row r="35">
-      <c s="21" r="A35"/>
+      <c s="20" r="A35"/>
       <c t="s" s="7" r="B35">
         <v>133</v>
       </c>
@@ -4573,7 +4546,7 @@
       </c>
     </row>
     <row r="36">
-      <c s="21" r="A36"/>
+      <c s="20" r="A36"/>
       <c t="s" s="7" r="B36">
         <v>137</v>
       </c>
@@ -4588,7 +4561,7 @@
       </c>
     </row>
     <row r="37">
-      <c s="21" r="A37"/>
+      <c s="20" r="A37"/>
       <c t="s" s="7" r="B37">
         <v>141</v>
       </c>
@@ -4603,7 +4576,7 @@
       </c>
     </row>
     <row r="38">
-      <c s="21" r="A38"/>
+      <c s="20" r="A38"/>
       <c t="s" s="7" r="B38">
         <v>145</v>
       </c>
@@ -4618,7 +4591,7 @@
       </c>
     </row>
     <row r="39">
-      <c s="21" r="A39"/>
+      <c s="20" r="A39"/>
       <c t="s" s="7" r="B39">
         <v>149</v>
       </c>
@@ -4633,14 +4606,14 @@
       </c>
     </row>
     <row r="40">
-      <c s="21" r="A40"/>
-      <c s="21" r="B40"/>
-      <c s="21" r="C40"/>
-      <c s="21" r="D40"/>
-      <c s="21" r="E40"/>
+      <c s="20" r="A40"/>
+      <c s="20" r="B40"/>
+      <c s="20" r="C40"/>
+      <c s="20" r="D40"/>
+      <c s="20" r="E40"/>
     </row>
     <row r="41">
-      <c t="s" s="21" r="A41">
+      <c t="s" s="20" r="A41">
         <v>153</v>
       </c>
       <c t="s" s="7" r="B41">
@@ -4657,7 +4630,7 @@
       </c>
     </row>
     <row r="42">
-      <c s="21" r="A42"/>
+      <c s="20" r="A42"/>
       <c t="s" s="7" r="B42">
         <v>158</v>
       </c>
@@ -4672,7 +4645,7 @@
       </c>
     </row>
     <row r="43">
-      <c s="21" r="A43"/>
+      <c s="20" r="A43"/>
       <c t="s" s="7" r="B43">
         <v>162</v>
       </c>
@@ -4687,7 +4660,7 @@
       </c>
     </row>
     <row r="44">
-      <c s="21" r="A44"/>
+      <c s="20" r="A44"/>
       <c t="s" s="7" r="B44">
         <v>166</v>
       </c>
@@ -4702,7 +4675,7 @@
       </c>
     </row>
     <row r="45">
-      <c s="21" r="A45"/>
+      <c s="20" r="A45"/>
       <c t="s" s="7" r="B45">
         <v>170</v>
       </c>
@@ -5057,7 +5030,7 @@
     </row>
     <row r="69">
       <c s="12" r="A69"/>
-      <c t="s" s="28" r="B69">
+      <c t="s" s="25" r="B69">
         <v>263</v>
       </c>
       <c t="s" s="7" r="C69">
@@ -5072,7 +5045,7 @@
     </row>
     <row r="70">
       <c s="12" r="A70"/>
-      <c t="s" s="28" r="B70">
+      <c t="s" s="25" r="B70">
         <v>267</v>
       </c>
       <c t="s" s="7" r="C70">
@@ -5087,52 +5060,52 @@
     </row>
     <row r="71">
       <c s="12" r="A71"/>
-      <c t="s" s="28" r="B71">
+      <c t="s" s="25" r="B71">
         <v>271</v>
       </c>
       <c t="s" s="7" r="C71">
         <v>272</v>
       </c>
-      <c t="s" s="28" r="D71">
+      <c t="s" s="25" r="D71">
         <v>273</v>
       </c>
-      <c t="s" s="28" r="E71">
+      <c t="s" s="25" r="E71">
         <v>274</v>
       </c>
     </row>
     <row r="72">
       <c s="1" r="A72"/>
-      <c t="s" s="32" r="B72">
+      <c t="s" s="29" r="B72">
         <v>275</v>
       </c>
       <c t="s" s="1" r="C72">
         <v>276</v>
       </c>
-      <c t="s" s="32" r="D72">
+      <c t="s" s="29" r="D72">
         <v>277</v>
       </c>
-      <c t="s" s="32" r="E72">
+      <c t="s" s="29" r="E72">
         <v>278</v>
       </c>
     </row>
     <row r="73">
       <c s="12" r="A73"/>
-      <c t="s" s="28" r="B73">
+      <c t="s" s="25" r="B73">
         <v>279</v>
       </c>
       <c t="s" s="7" r="C73">
         <v>280</v>
       </c>
-      <c t="s" s="28" r="D73">
+      <c t="s" s="25" r="D73">
         <v>281</v>
       </c>
-      <c t="s" s="28" r="E73">
+      <c t="s" s="25" r="E73">
         <v>282</v>
       </c>
     </row>
     <row r="74">
       <c s="12" r="A74"/>
-      <c t="s" s="28" r="B74">
+      <c t="s" s="25" r="B74">
         <v>283</v>
       </c>
       <c t="s" s="7" r="C74">
@@ -5152,7 +5125,7 @@
       <c t="s" s="7" r="C75">
         <v>288</v>
       </c>
-      <c t="s" s="39" r="D75">
+      <c t="s" s="34" r="D75">
         <v>289</v>
       </c>
       <c t="s" s="19" r="E75">
@@ -5176,7 +5149,7 @@
     </row>
     <row r="77">
       <c s="12" r="A77"/>
-      <c t="s" s="28" r="B77">
+      <c t="s" s="25" r="B77">
         <v>295</v>
       </c>
       <c t="s" s="7" r="C77">
@@ -5191,7 +5164,7 @@
     </row>
     <row r="78">
       <c s="12" r="A78"/>
-      <c t="s" s="28" r="B78">
+      <c t="s" s="25" r="B78">
         <v>299</v>
       </c>
       <c t="s" s="7" r="C78">
@@ -5212,7 +5185,7 @@
       <c t="s" s="7" r="C79">
         <v>304</v>
       </c>
-      <c t="s" s="39" r="D79">
+      <c t="s" s="34" r="D79">
         <v>305</v>
       </c>
       <c t="s" s="19" r="E79">
@@ -5227,7 +5200,7 @@
       <c t="s" s="7" r="C80">
         <v>308</v>
       </c>
-      <c t="s" s="39" r="D80">
+      <c t="s" s="34" r="D80">
         <v>309</v>
       </c>
       <c t="s" s="19" r="E80">
@@ -5354,10 +5327,10 @@
       <c t="s" s="14" r="C89">
         <v>336</v>
       </c>
-      <c t="s" s="39" r="D89">
+      <c t="s" s="34" r="D89">
         <v>337</v>
       </c>
-      <c t="s" s="39" r="E89">
+      <c t="s" s="34" r="E89">
         <v>338</v>
       </c>
     </row>
@@ -5368,10 +5341,10 @@
       <c t="s" s="14" r="C90">
         <v>340</v>
       </c>
-      <c t="s" s="39" r="D90">
+      <c t="s" s="34" r="D90">
         <v>341</v>
       </c>
-      <c t="s" s="39" r="E90">
+      <c t="s" s="34" r="E90">
         <v>342</v>
       </c>
     </row>
@@ -5382,10 +5355,10 @@
       <c t="s" s="14" r="C91">
         <v>344</v>
       </c>
-      <c t="s" s="39" r="D91">
+      <c t="s" s="34" r="D91">
         <v>345</v>
       </c>
-      <c t="s" s="39" r="E91">
+      <c t="s" s="34" r="E91">
         <v>346</v>
       </c>
     </row>
@@ -5396,10 +5369,10 @@
       <c t="s" s="14" r="C92">
         <v>348</v>
       </c>
-      <c t="s" s="39" r="D92">
+      <c t="s" s="34" r="D92">
         <v>349</v>
       </c>
-      <c t="s" s="39" r="E92">
+      <c t="s" s="34" r="E92">
         <v>350</v>
       </c>
     </row>
@@ -5410,10 +5383,10 @@
       <c t="s" s="14" r="C93">
         <v>352</v>
       </c>
-      <c t="s" s="39" r="D93">
+      <c t="s" s="34" r="D93">
         <v>353</v>
       </c>
-      <c t="s" s="39" r="E93">
+      <c t="s" s="34" r="E93">
         <v>354</v>
       </c>
     </row>
@@ -5424,19 +5397,19 @@
       <c t="s" s="14" r="C94">
         <v>356</v>
       </c>
-      <c t="s" s="39" r="D94">
+      <c t="s" s="34" r="D94">
         <v>357</v>
       </c>
-      <c t="s" s="39" r="E94">
+      <c t="s" s="34" r="E94">
         <v>358</v>
       </c>
     </row>
     <row r="95">
-      <c s="21" r="A95"/>
-      <c s="21" r="B95"/>
-      <c s="21" r="C95"/>
-      <c s="21" r="D95"/>
-      <c s="21" r="E95"/>
+      <c s="20" r="A95"/>
+      <c s="20" r="B95"/>
+      <c s="20" r="C95"/>
+      <c s="20" r="D95"/>
+      <c s="20" r="E95"/>
     </row>
     <row r="96">
       <c t="s" s="12" r="A96">
@@ -5670,7 +5643,7 @@
       <c t="s" s="7" r="D111">
         <v>419</v>
       </c>
-      <c t="s" s="37" r="E111">
+      <c t="s" s="7" r="E111">
         <v>420</v>
       </c>
     </row>
@@ -5736,45 +5709,45 @@
     </row>
     <row r="116">
       <c s="12" r="A116"/>
-      <c s="12" r="B116"/>
-      <c s="12" r="C116"/>
-      <c s="12" r="D116"/>
-      <c s="12" r="E116"/>
+      <c t="s" s="7" r="B116">
+        <v>437</v>
+      </c>
+      <c t="s" s="7" r="C116">
+        <v>438</v>
+      </c>
+      <c t="s" s="19" r="D116">
+        <v>439</v>
+      </c>
+      <c t="s" s="19" r="E116">
+        <v>440</v>
+      </c>
     </row>
     <row r="117">
-      <c t="s" s="12" r="A117">
-        <v>437</v>
-      </c>
+      <c s="12" r="A117"/>
       <c t="s" s="7" r="B117">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c t="s" s="7" r="C117">
-        <v>439</v>
-      </c>
-      <c t="s" s="7" r="D117">
-        <v>440</v>
-      </c>
-      <c t="s" s="7" r="E117">
-        <v>441</v>
+        <v>442</v>
+      </c>
+      <c t="s" s="19" r="D117">
+        <v>443</v>
+      </c>
+      <c t="s" s="19" r="E117">
+        <v>444</v>
       </c>
     </row>
     <row r="118">
       <c s="12" r="A118"/>
-      <c t="s" s="7" r="B118">
-        <v>442</v>
-      </c>
-      <c t="s" s="7" r="C118">
-        <v>443</v>
-      </c>
-      <c t="s" s="7" r="D118">
-        <v>444</v>
-      </c>
-      <c t="s" s="7" r="E118">
+      <c s="12" r="B118"/>
+      <c s="12" r="C118"/>
+      <c s="12" r="D118"/>
+      <c s="12" r="E118"/>
+    </row>
+    <row r="119">
+      <c t="s" s="12" r="A119">
         <v>445</v>
       </c>
-    </row>
-    <row r="119">
-      <c s="11" r="A119"/>
       <c t="s" s="7" r="B119">
         <v>446</v>
       </c>
@@ -5789,7 +5762,7 @@
       </c>
     </row>
     <row r="120">
-      <c s="11" r="A120"/>
+      <c s="12" r="A120"/>
       <c t="s" s="7" r="B120">
         <v>450</v>
       </c>
@@ -5970,45 +5943,45 @@
     </row>
     <row r="132">
       <c s="11" r="A132"/>
-      <c s="12" r="B132"/>
-      <c s="12" r="C132"/>
-      <c s="12" r="D132"/>
-      <c s="12" r="E132"/>
+      <c t="s" s="7" r="B132">
+        <v>498</v>
+      </c>
+      <c t="s" s="7" r="C132">
+        <v>499</v>
+      </c>
+      <c t="s" s="7" r="D132">
+        <v>500</v>
+      </c>
+      <c t="s" s="7" r="E132">
+        <v>501</v>
+      </c>
     </row>
     <row r="133">
-      <c t="s" s="11" r="A133">
-        <v>498</v>
-      </c>
+      <c s="11" r="A133"/>
       <c t="s" s="7" r="B133">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c t="s" s="7" r="C133">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c t="s" s="7" r="D133">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c t="s" s="7" r="E133">
-        <v>502</v>
+        <v>505</v>
       </c>
     </row>
     <row r="134">
       <c s="11" r="A134"/>
-      <c t="s" s="7" r="B134">
-        <v>503</v>
-      </c>
-      <c t="s" s="7" r="C134">
-        <v>504</v>
-      </c>
-      <c t="s" s="7" r="D134">
-        <v>505</v>
-      </c>
-      <c t="s" s="7" r="E134">
+      <c s="12" r="B134"/>
+      <c s="12" r="C134"/>
+      <c s="12" r="D134"/>
+      <c s="12" r="E134"/>
+    </row>
+    <row r="135">
+      <c t="s" s="11" r="A135">
         <v>506</v>
       </c>
-    </row>
-    <row r="135">
-      <c s="11" r="A135"/>
       <c t="s" s="7" r="B135">
         <v>507</v>
       </c>
@@ -6058,43 +6031,43 @@
         <v>519</v>
       </c>
       <c t="s" s="7" r="C138">
-        <v>250</v>
+        <v>520</v>
       </c>
       <c t="s" s="7" r="D138">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c t="s" s="7" r="E138">
-        <v>250</v>
+        <v>522</v>
       </c>
     </row>
     <row r="139">
       <c s="11" r="A139"/>
       <c t="s" s="7" r="B139">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c t="s" s="7" r="C139">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c t="s" s="7" r="D139">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c t="s" s="7" r="E139">
-        <v>524</v>
+        <v>526</v>
       </c>
     </row>
     <row r="140">
       <c s="11" r="A140"/>
       <c t="s" s="7" r="B140">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c t="s" s="7" r="C140">
-        <v>526</v>
+        <v>250</v>
       </c>
       <c t="s" s="7" r="D140">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c t="s" s="7" r="E140">
-        <v>528</v>
+        <v>250</v>
       </c>
     </row>
     <row r="141">
@@ -6151,82 +6124,82 @@
         <v>542</v>
       </c>
       <c t="s" s="7" r="D144">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c t="s" s="7" r="E144">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="145">
       <c s="11" r="A145"/>
       <c t="s" s="7" r="B145">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c t="s" s="7" r="C145">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c t="s" s="7" r="D145">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c t="s" s="7" r="E145">
-        <v>546</v>
+        <v>548</v>
       </c>
     </row>
     <row r="146">
       <c s="11" r="A146"/>
       <c t="s" s="7" r="B146">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c t="s" s="7" r="C146">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c t="s" s="7" r="D146">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c t="s" s="7" r="E146">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="147">
       <c s="11" r="A147"/>
-      <c t="s" s="14" r="B147">
-        <v>551</v>
+      <c t="s" s="7" r="B147">
+        <v>552</v>
       </c>
       <c t="s" s="7" r="C147">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c t="s" s="7" r="D147">
         <v>553</v>
       </c>
       <c t="s" s="7" r="E147">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="148">
       <c s="11" r="A148"/>
       <c t="s" s="7" r="B148">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c t="s" s="7" r="C148">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c t="s" s="7" r="D148">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c t="s" s="7" r="E148">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="149">
       <c s="11" r="A149"/>
-      <c t="s" s="7" r="B149">
-        <v>558</v>
+      <c t="s" s="14" r="B149">
+        <v>559</v>
       </c>
       <c t="s" s="7" r="C149">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c t="s" s="7" r="D149">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c t="s" s="7" r="E149">
         <v>561</v>
@@ -6432,7 +6405,7 @@
       <c t="s" s="7" r="B163">
         <v>614</v>
       </c>
-      <c t="s" s="14" r="C163">
+      <c t="s" s="7" r="C163">
         <v>615</v>
       </c>
       <c t="s" s="7" r="D163">
@@ -6444,10 +6417,10 @@
     </row>
     <row r="164">
       <c s="11" r="A164"/>
-      <c t="s" s="14" r="B164">
+      <c t="s" s="7" r="B164">
         <v>618</v>
       </c>
-      <c t="s" s="14" r="C164">
+      <c t="s" s="7" r="C164">
         <v>619</v>
       </c>
       <c t="s" s="7" r="D164">
@@ -6463,43 +6436,43 @@
         <v>622</v>
       </c>
       <c t="s" s="14" r="C165">
-        <v>619</v>
+        <v>623</v>
       </c>
       <c t="s" s="7" r="D165">
-        <v>620</v>
+        <v>624</v>
       </c>
       <c t="s" s="7" r="E165">
-        <v>621</v>
+        <v>625</v>
       </c>
     </row>
     <row r="166">
       <c s="11" r="A166"/>
-      <c t="s" s="7" r="B166">
-        <v>623</v>
-      </c>
-      <c t="s" s="3" r="C166">
-        <v>624</v>
+      <c t="s" s="14" r="B166">
+        <v>626</v>
+      </c>
+      <c t="s" s="14" r="C166">
+        <v>627</v>
       </c>
       <c t="s" s="7" r="D166">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c t="s" s="7" r="E166">
-        <v>626</v>
+        <v>629</v>
       </c>
     </row>
     <row r="167">
       <c s="11" r="A167"/>
       <c t="s" s="7" r="B167">
+        <v>630</v>
+      </c>
+      <c t="s" s="14" r="C167">
         <v>627</v>
       </c>
-      <c t="s" s="3" r="C167">
+      <c t="s" s="7" r="D167">
         <v>628</v>
       </c>
-      <c t="s" s="7" r="D167">
+      <c t="s" s="7" r="E167">
         <v>629</v>
-      </c>
-      <c t="s" s="7" r="E167">
-        <v>630</v>
       </c>
     </row>
     <row r="168">
@@ -6513,81 +6486,81 @@
       <c t="s" s="7" r="D168">
         <v>633</v>
       </c>
-      <c t="s" s="3" r="E168">
+      <c t="s" s="7" r="E168">
         <v>634</v>
       </c>
     </row>
     <row r="169">
       <c s="11" r="A169"/>
-      <c s="17" r="B169"/>
-      <c s="9" r="C169"/>
-      <c s="17" r="D169"/>
-      <c s="17" r="E169"/>
+      <c t="s" s="7" r="B169">
+        <v>635</v>
+      </c>
+      <c t="s" s="3" r="C169">
+        <v>636</v>
+      </c>
+      <c t="s" s="7" r="D169">
+        <v>637</v>
+      </c>
+      <c t="s" s="7" r="E169">
+        <v>638</v>
+      </c>
     </row>
     <row r="170">
-      <c t="s" s="11" r="A170">
-        <v>635</v>
-      </c>
+      <c s="11" r="A170"/>
       <c t="s" s="7" r="B170">
-        <v>636</v>
-      </c>
-      <c t="s" s="14" r="C170">
-        <v>637</v>
+        <v>639</v>
+      </c>
+      <c t="s" s="3" r="C170">
+        <v>640</v>
       </c>
       <c t="s" s="7" r="D170">
-        <v>289</v>
-      </c>
-      <c t="s" s="7" r="E170">
-        <v>290</v>
+        <v>641</v>
+      </c>
+      <c t="s" s="3" r="E170">
+        <v>642</v>
       </c>
     </row>
     <row r="171">
       <c s="11" r="A171"/>
-      <c t="s" s="23" r="B171">
-        <v>638</v>
-      </c>
-      <c t="s" s="14" r="C171">
-        <v>639</v>
-      </c>
-      <c t="s" s="23" r="D171">
-        <v>640</v>
-      </c>
-      <c t="s" s="23" r="E171">
-        <v>641</v>
-      </c>
+      <c s="17" r="B171"/>
+      <c s="9" r="C171"/>
+      <c s="17" r="D171"/>
+      <c s="17" r="E171"/>
     </row>
     <row r="172">
-      <c s="11" r="A172"/>
+      <c t="s" s="11" r="A172">
+        <v>643</v>
+      </c>
       <c t="s" s="7" r="B172">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c t="s" s="14" r="C172">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c t="s" s="7" r="D172">
-        <v>644</v>
+        <v>289</v>
       </c>
       <c t="s" s="7" r="E172">
-        <v>645</v>
+        <v>290</v>
       </c>
     </row>
     <row r="173">
       <c s="11" r="A173"/>
-      <c t="s" s="7" r="B173">
+      <c t="s" s="22" r="B173">
         <v>646</v>
       </c>
       <c t="s" s="14" r="C173">
         <v>647</v>
       </c>
-      <c t="s" s="7" r="D173">
+      <c t="s" s="22" r="D173">
         <v>648</v>
       </c>
-      <c t="s" s="7" r="E173">
+      <c t="s" s="22" r="E173">
         <v>649</v>
       </c>
     </row>
     <row r="174">
-      <c s="18" r="A174"/>
+      <c s="11" r="A174"/>
       <c t="s" s="7" r="B174">
         <v>650</v>
       </c>
@@ -6617,7 +6590,7 @@
       </c>
     </row>
     <row r="176">
-      <c s="11" r="A176"/>
+      <c s="18" r="A176"/>
       <c t="s" s="7" r="B176">
         <v>658</v>
       </c>
@@ -6711,64 +6684,64 @@
       <c t="s" s="7" r="B182">
         <v>682</v>
       </c>
-      <c t="s" s="20" r="C182">
+      <c t="s" s="14" r="C182">
         <v>683</v>
       </c>
-      <c t="s" s="37" r="D182">
+      <c t="s" s="7" r="D182">
         <v>684</v>
       </c>
-      <c t="s" s="37" r="E182">
+      <c t="s" s="7" r="E182">
         <v>685</v>
       </c>
     </row>
     <row r="183">
       <c s="11" r="A183"/>
-      <c s="12" r="B183"/>
-      <c s="15" r="C183"/>
-      <c s="12" r="D183"/>
-      <c s="12" r="E183"/>
+      <c t="s" s="7" r="B183">
+        <v>686</v>
+      </c>
+      <c t="s" s="14" r="C183">
+        <v>687</v>
+      </c>
+      <c t="s" s="7" r="D183">
+        <v>688</v>
+      </c>
+      <c t="s" s="7" r="E183">
+        <v>689</v>
+      </c>
     </row>
     <row r="184">
       <c s="11" r="A184"/>
-      <c s="21" r="B184"/>
-      <c s="31" r="C184"/>
-      <c s="21" r="D184"/>
-      <c s="21" r="E184"/>
+      <c t="s" s="7" r="B184">
+        <v>690</v>
+      </c>
+      <c t="s" s="14" r="C184">
+        <v>691</v>
+      </c>
+      <c t="s" s="7" r="D184">
+        <v>692</v>
+      </c>
+      <c t="s" s="7" r="E184">
+        <v>693</v>
+      </c>
     </row>
     <row r="185">
-      <c t="s" s="11" r="A185">
-        <v>686</v>
-      </c>
-      <c t="s" s="7" r="B185">
-        <v>687</v>
-      </c>
-      <c t="s" s="14" r="C185">
-        <v>688</v>
-      </c>
-      <c t="s" s="7" r="D185">
-        <v>689</v>
-      </c>
-      <c t="s" s="7" r="E185">
-        <v>690</v>
-      </c>
+      <c s="11" r="A185"/>
+      <c s="12" r="B185"/>
+      <c s="15" r="C185"/>
+      <c s="12" r="D185"/>
+      <c s="12" r="E185"/>
     </row>
     <row r="186">
       <c s="11" r="A186"/>
-      <c t="s" s="7" r="B186">
-        <v>691</v>
-      </c>
-      <c t="s" s="14" r="C186">
-        <v>692</v>
-      </c>
-      <c t="s" s="7" r="D186">
-        <v>693</v>
-      </c>
-      <c t="s" s="7" r="E186">
+      <c s="20" r="B186"/>
+      <c s="28" r="C186"/>
+      <c s="20" r="D186"/>
+      <c s="20" r="E186"/>
+    </row>
+    <row r="187">
+      <c t="s" s="11" r="A187">
         <v>694</v>
       </c>
-    </row>
-    <row r="187">
-      <c s="11" r="A187"/>
       <c t="s" s="7" r="B187">
         <v>695</v>
       </c>
@@ -6844,116 +6817,116 @@
     </row>
     <row r="192">
       <c s="11" r="A192"/>
-      <c s="21" r="B192"/>
-      <c s="31" r="C192"/>
-      <c s="21" r="D192"/>
-      <c s="21" r="E192"/>
+      <c t="s" s="7" r="B192">
+        <v>715</v>
+      </c>
+      <c t="s" s="14" r="C192">
+        <v>716</v>
+      </c>
+      <c t="s" s="7" r="D192">
+        <v>717</v>
+      </c>
+      <c t="s" s="7" r="E192">
+        <v>718</v>
+      </c>
     </row>
     <row r="193">
-      <c t="s" s="11" r="A193">
-        <v>715</v>
-      </c>
-      <c t="s" s="30" r="B193">
-        <v>716</v>
-      </c>
-      <c t="s" s="22" r="C193">
-        <v>715</v>
-      </c>
-      <c s="30" r="D193"/>
-      <c s="30" r="E193"/>
+      <c s="11" r="A193"/>
+      <c t="s" s="7" r="B193">
+        <v>719</v>
+      </c>
+      <c t="s" s="14" r="C193">
+        <v>720</v>
+      </c>
+      <c t="s" s="7" r="D193">
+        <v>721</v>
+      </c>
+      <c t="s" s="7" r="E193">
+        <v>722</v>
+      </c>
     </row>
     <row r="194">
       <c s="11" r="A194"/>
-      <c s="17" r="B194"/>
-      <c s="9" r="C194"/>
-      <c s="17" r="D194"/>
-      <c s="17" r="E194"/>
+      <c s="20" r="B194"/>
+      <c s="28" r="C194"/>
+      <c s="20" r="D194"/>
+      <c s="20" r="E194"/>
     </row>
     <row r="195">
       <c t="s" s="11" r="A195">
-        <v>717</v>
-      </c>
-      <c t="s" s="38" r="B195">
-        <v>718</v>
-      </c>
-      <c t="s" s="35" r="C195">
-        <v>719</v>
-      </c>
-      <c s="38" r="D195"/>
-      <c s="38" r="E195"/>
+        <v>723</v>
+      </c>
+      <c t="s" s="27" r="B195">
+        <v>724</v>
+      </c>
+      <c t="s" s="21" r="C195">
+        <v>723</v>
+      </c>
+      <c s="27" r="D195"/>
+      <c s="27" r="E195"/>
     </row>
     <row r="196">
       <c s="11" r="A196"/>
-      <c t="s" s="38" r="B196">
-        <v>720</v>
-      </c>
-      <c t="s" s="35" r="C196">
-        <v>721</v>
-      </c>
-      <c s="38" r="D196"/>
-      <c s="38" r="E196"/>
+      <c s="17" r="B196"/>
+      <c s="9" r="C196"/>
+      <c s="17" r="D196"/>
+      <c s="17" r="E196"/>
     </row>
     <row r="197">
-      <c s="11" r="A197"/>
-      <c s="9" r="B197"/>
-      <c s="9" r="C197"/>
-      <c s="17" r="D197"/>
-      <c s="17" r="E197"/>
+      <c t="s" s="11" r="A197">
+        <v>725</v>
+      </c>
+      <c t="s" s="33" r="B197">
+        <v>726</v>
+      </c>
+      <c t="s" s="31" r="C197">
+        <v>727</v>
+      </c>
+      <c s="33" r="D197"/>
+      <c s="33" r="E197"/>
     </row>
     <row r="198">
-      <c t="s" s="11" r="A198">
-        <v>722</v>
-      </c>
-      <c t="s" s="28" r="B198">
-        <v>723</v>
-      </c>
-      <c t="s" s="28" r="C198">
-        <v>724</v>
-      </c>
-      <c t="s" s="7" r="D198">
-        <v>725</v>
-      </c>
-      <c t="s" s="7" r="E198">
-        <v>726</v>
-      </c>
+      <c s="11" r="A198"/>
+      <c t="s" s="33" r="B198">
+        <v>728</v>
+      </c>
+      <c t="s" s="31" r="C198">
+        <v>729</v>
+      </c>
+      <c s="33" r="D198"/>
+      <c s="33" r="E198"/>
     </row>
     <row r="199">
       <c s="11" r="A199"/>
-      <c t="s" s="28" r="B199">
-        <v>727</v>
-      </c>
-      <c t="s" s="28" r="C199">
-        <v>728</v>
-      </c>
-      <c t="s" s="7" r="D199">
-        <v>728</v>
-      </c>
-      <c t="s" s="7" r="E199">
-        <v>729</v>
-      </c>
+      <c s="9" r="B199"/>
+      <c s="9" r="C199"/>
+      <c s="17" r="D199"/>
+      <c s="17" r="E199"/>
     </row>
     <row r="200">
-      <c s="11" r="A200"/>
-      <c t="s" s="28" r="B200">
+      <c t="s" s="11" r="A200">
         <v>730</v>
       </c>
-      <c t="s" s="28" r="C200">
+      <c t="s" s="25" r="B200">
         <v>731</v>
       </c>
+      <c t="s" s="25" r="C200">
+        <v>732</v>
+      </c>
       <c t="s" s="7" r="D200">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c t="s" s="7" r="E200">
-        <v>733</v>
+        <v>734</v>
       </c>
     </row>
     <row r="201">
       <c s="11" r="A201"/>
-      <c t="s" s="28" r="B201">
-        <v>734</v>
-      </c>
-      <c t="s" s="28" r="C201">
+      <c t="s" s="25" r="B201">
         <v>735</v>
+      </c>
+      <c t="s" s="25" r="C201">
+        <v>736</v>
       </c>
       <c t="s" s="7" r="D201">
         <v>736</v>
@@ -6964,10 +6937,10 @@
     </row>
     <row r="202">
       <c s="11" r="A202"/>
-      <c t="s" s="14" r="B202">
+      <c t="s" s="25" r="B202">
         <v>738</v>
       </c>
-      <c t="s" s="14" r="C202">
+      <c t="s" s="25" r="C202">
         <v>739</v>
       </c>
       <c t="s" s="7" r="D202">
@@ -6979,10 +6952,10 @@
     </row>
     <row r="203">
       <c s="11" r="A203"/>
-      <c t="s" s="14" r="B203">
+      <c t="s" s="25" r="B203">
         <v>742</v>
       </c>
-      <c t="s" s="14" r="C203">
+      <c t="s" s="25" r="C203">
         <v>743</v>
       </c>
       <c t="s" s="7" r="D203">
@@ -7069,7 +7042,7 @@
     </row>
     <row r="209">
       <c s="11" r="A209"/>
-      <c t="s" s="7" r="B209">
+      <c t="s" s="14" r="B209">
         <v>766</v>
       </c>
       <c t="s" s="14" r="C209">
@@ -7084,16 +7057,16 @@
     </row>
     <row r="210">
       <c s="11" r="A210"/>
-      <c t="s" s="7" r="B210">
+      <c t="s" s="14" r="B210">
         <v>770</v>
       </c>
       <c t="s" s="14" r="C210">
         <v>771</v>
       </c>
-      <c t="s" s="19" r="D210">
+      <c t="s" s="7" r="D210">
         <v>772</v>
       </c>
-      <c t="s" s="19" r="E210">
+      <c t="s" s="7" r="E210">
         <v>773</v>
       </c>
     </row>
@@ -7105,10 +7078,10 @@
       <c t="s" s="14" r="C211">
         <v>775</v>
       </c>
-      <c t="s" s="19" r="D211">
+      <c t="s" s="7" r="D211">
         <v>776</v>
       </c>
-      <c t="s" s="19" r="E211">
+      <c t="s" s="7" r="E211">
         <v>777</v>
       </c>
     </row>
@@ -7135,10 +7108,10 @@
       <c t="s" s="14" r="C213">
         <v>783</v>
       </c>
-      <c t="s" s="7" r="D213">
+      <c t="s" s="19" r="D213">
         <v>784</v>
       </c>
-      <c t="s" s="7" r="E213">
+      <c t="s" s="19" r="E213">
         <v>785</v>
       </c>
     </row>
@@ -7150,10 +7123,10 @@
       <c t="s" s="14" r="C214">
         <v>787</v>
       </c>
-      <c t="s" s="7" r="D214">
+      <c t="s" s="19" r="D214">
         <v>788</v>
       </c>
-      <c t="s" s="7" r="E214">
+      <c t="s" s="19" r="E214">
         <v>789</v>
       </c>
     </row>
@@ -7204,74 +7177,74 @@
     </row>
     <row r="218">
       <c s="11" r="A218"/>
-      <c s="17" r="B218"/>
-      <c s="31" r="C218"/>
-      <c s="17" r="D218"/>
-      <c s="17" r="E218"/>
+      <c t="s" s="7" r="B218">
+        <v>802</v>
+      </c>
+      <c t="s" s="14" r="C218">
+        <v>803</v>
+      </c>
+      <c t="s" s="7" r="D218">
+        <v>804</v>
+      </c>
+      <c t="s" s="7" r="E218">
+        <v>805</v>
+      </c>
     </row>
     <row r="219">
-      <c t="s" s="11" r="A219">
-        <v>802</v>
-      </c>
-      <c t="s" s="28" r="B219">
-        <v>803</v>
-      </c>
-      <c t="s" s="7" r="C219">
-        <v>728</v>
+      <c s="11" r="A219"/>
+      <c t="s" s="7" r="B219">
+        <v>806</v>
+      </c>
+      <c t="s" s="14" r="C219">
+        <v>807</v>
       </c>
       <c t="s" s="7" r="D219">
-        <v>728</v>
+        <v>808</v>
       </c>
       <c t="s" s="7" r="E219">
-        <v>729</v>
+        <v>809</v>
       </c>
     </row>
     <row r="220">
       <c s="11" r="A220"/>
-      <c t="s" s="7" r="B220">
-        <v>804</v>
-      </c>
-      <c t="s" s="14" r="C220">
-        <v>731</v>
-      </c>
-      <c t="s" s="7" r="D220">
-        <v>732</v>
-      </c>
-      <c t="s" s="7" r="E220">
-        <v>733</v>
-      </c>
+      <c s="17" r="B220"/>
+      <c s="28" r="C220"/>
+      <c s="17" r="D220"/>
+      <c s="17" r="E220"/>
     </row>
     <row r="221">
-      <c t="s" s="7" r="B221">
-        <v>805</v>
-      </c>
-      <c t="s" s="14" r="C221">
-        <v>806</v>
+      <c t="s" s="11" r="A221">
+        <v>810</v>
+      </c>
+      <c t="s" s="25" r="B221">
+        <v>811</v>
+      </c>
+      <c t="s" s="7" r="C221">
+        <v>736</v>
       </c>
       <c t="s" s="7" r="D221">
-        <v>807</v>
+        <v>736</v>
       </c>
       <c t="s" s="7" r="E221">
-        <v>808</v>
+        <v>737</v>
       </c>
     </row>
     <row r="222">
       <c s="11" r="A222"/>
       <c t="s" s="7" r="B222">
-        <v>809</v>
+        <v>812</v>
       </c>
       <c t="s" s="14" r="C222">
-        <v>810</v>
+        <v>739</v>
       </c>
       <c t="s" s="7" r="D222">
-        <v>811</v>
+        <v>740</v>
       </c>
       <c t="s" s="7" r="E222">
-        <v>812</v>
+        <v>741</v>
       </c>
     </row>
     <row r="223">
-      <c s="11" r="A223"/>
       <c t="s" s="7" r="B223">
         <v>813</v>
       </c>
@@ -7287,50 +7260,50 @@
     </row>
     <row r="224">
       <c s="11" r="A224"/>
-      <c s="12" r="B224"/>
-      <c s="15" r="C224"/>
-      <c s="17" r="D224"/>
-      <c s="17" r="E224"/>
+      <c t="s" s="7" r="B224">
+        <v>817</v>
+      </c>
+      <c t="s" s="14" r="C224">
+        <v>818</v>
+      </c>
+      <c t="s" s="7" r="D224">
+        <v>819</v>
+      </c>
+      <c t="s" s="7" r="E224">
+        <v>820</v>
+      </c>
     </row>
     <row r="225">
-      <c t="s" s="11" r="A225">
-        <v>817</v>
-      </c>
+      <c s="11" r="A225"/>
       <c t="s" s="7" r="B225">
-        <v>818</v>
+        <v>821</v>
       </c>
       <c t="s" s="14" r="C225">
-        <v>817</v>
+        <v>822</v>
       </c>
       <c t="s" s="7" r="D225">
-        <v>819</v>
+        <v>823</v>
       </c>
       <c t="s" s="7" r="E225">
-        <v>820</v>
+        <v>824</v>
       </c>
     </row>
     <row r="226">
       <c s="11" r="A226"/>
-      <c t="s" s="7" r="B226">
-        <v>821</v>
-      </c>
-      <c t="s" s="14" r="C226">
-        <v>822</v>
-      </c>
-      <c t="s" s="7" r="D226">
-        <v>823</v>
-      </c>
-      <c t="s" s="7" r="E226">
-        <v>824</v>
-      </c>
+      <c s="12" r="B226"/>
+      <c s="15" r="C226"/>
+      <c s="17" r="D226"/>
+      <c s="17" r="E226"/>
     </row>
     <row r="227">
-      <c s="11" r="A227"/>
+      <c t="s" s="11" r="A227">
+        <v>825</v>
+      </c>
       <c t="s" s="7" r="B227">
+        <v>826</v>
+      </c>
+      <c t="s" s="14" r="C227">
         <v>825</v>
-      </c>
-      <c t="s" s="14" r="C227">
-        <v>826</v>
       </c>
       <c t="s" s="7" r="D227">
         <v>827</v>
@@ -7401,84 +7374,84 @@
     </row>
     <row r="232">
       <c s="11" r="A232"/>
-      <c s="12" r="B232"/>
-      <c s="15" r="C232"/>
-      <c s="12" r="D232"/>
-      <c s="12" r="E232"/>
+      <c t="s" s="7" r="B232">
+        <v>845</v>
+      </c>
+      <c t="s" s="14" r="C232">
+        <v>846</v>
+      </c>
+      <c t="s" s="7" r="D232">
+        <v>847</v>
+      </c>
+      <c t="s" s="7" r="E232">
+        <v>848</v>
+      </c>
     </row>
     <row r="233">
-      <c t="s" s="11" r="A233">
-        <v>845</v>
-      </c>
+      <c s="11" r="A233"/>
       <c t="s" s="7" r="B233">
-        <v>846</v>
+        <v>849</v>
       </c>
       <c t="s" s="14" r="C233">
-        <v>847</v>
+        <v>850</v>
       </c>
       <c t="s" s="7" r="D233">
-        <v>848</v>
+        <v>851</v>
       </c>
       <c t="s" s="7" r="E233">
-        <v>849</v>
+        <v>852</v>
       </c>
     </row>
     <row r="234">
       <c s="11" r="A234"/>
-      <c t="s" s="7" r="B234">
-        <v>850</v>
-      </c>
-      <c t="s" s="14" r="C234">
-        <v>851</v>
-      </c>
-      <c t="s" s="7" r="D234">
-        <v>851</v>
-      </c>
-      <c t="s" s="7" r="E234">
-        <v>852</v>
-      </c>
+      <c s="12" r="B234"/>
+      <c s="15" r="C234"/>
+      <c s="12" r="D234"/>
+      <c s="12" r="E234"/>
     </row>
     <row r="235">
-      <c s="11" r="A235"/>
-      <c s="12" r="B235"/>
-      <c s="15" r="C235"/>
-      <c s="12" r="D235"/>
-      <c s="12" r="E235"/>
+      <c t="s" s="11" r="A235">
+        <v>853</v>
+      </c>
+      <c t="s" s="7" r="B235">
+        <v>854</v>
+      </c>
+      <c t="s" s="14" r="C235">
+        <v>855</v>
+      </c>
+      <c t="s" s="7" r="D235">
+        <v>856</v>
+      </c>
+      <c t="s" s="7" r="E235">
+        <v>857</v>
+      </c>
     </row>
     <row r="236">
-      <c t="s" s="11" r="A236">
-        <v>853</v>
-      </c>
+      <c s="11" r="A236"/>
       <c t="s" s="7" r="B236">
-        <v>854</v>
+        <v>858</v>
       </c>
       <c t="s" s="14" r="C236">
-        <v>855</v>
+        <v>859</v>
       </c>
       <c t="s" s="7" r="D236">
-        <v>856</v>
+        <v>859</v>
       </c>
       <c t="s" s="7" r="E236">
-        <v>857</v>
+        <v>860</v>
       </c>
     </row>
     <row r="237">
       <c s="11" r="A237"/>
-      <c t="s" s="7" r="B237">
-        <v>858</v>
-      </c>
-      <c t="s" s="14" r="C237">
-        <v>859</v>
-      </c>
-      <c t="s" s="7" r="D237">
-        <v>860</v>
-      </c>
-      <c t="s" s="7" r="E237">
+      <c s="12" r="B237"/>
+      <c s="15" r="C237"/>
+      <c s="12" r="D237"/>
+      <c s="12" r="E237"/>
+    </row>
+    <row r="238">
+      <c t="s" s="11" r="A238">
         <v>861</v>
       </c>
-    </row>
-    <row r="238">
-      <c s="11" r="A238"/>
       <c t="s" s="7" r="B238">
         <v>862</v>
       </c>
@@ -7509,108 +7482,108 @@
     </row>
     <row r="240">
       <c s="11" r="A240"/>
-      <c s="17" r="B240"/>
-      <c s="31" r="C240"/>
-      <c s="17" r="D240"/>
-      <c s="17" r="E240"/>
+      <c t="s" s="7" r="B240">
+        <v>870</v>
+      </c>
+      <c t="s" s="14" r="C240">
+        <v>871</v>
+      </c>
+      <c t="s" s="7" r="D240">
+        <v>872</v>
+      </c>
+      <c t="s" s="7" r="E240">
+        <v>873</v>
+      </c>
     </row>
     <row r="241">
-      <c t="s" s="11" r="A241">
-        <v>870</v>
-      </c>
+      <c s="11" r="A241"/>
       <c t="s" s="7" r="B241">
-        <v>871</v>
+        <v>874</v>
       </c>
       <c t="s" s="14" r="C241">
-        <v>872</v>
+        <v>875</v>
       </c>
       <c t="s" s="7" r="D241">
-        <v>873</v>
+        <v>876</v>
       </c>
       <c t="s" s="7" r="E241">
-        <v>874</v>
+        <v>877</v>
       </c>
     </row>
     <row r="242">
       <c s="11" r="A242"/>
-      <c t="s" s="7" r="B242">
-        <v>875</v>
-      </c>
-      <c t="s" s="14" r="C242">
-        <v>876</v>
-      </c>
-      <c t="s" s="7" r="D242">
-        <v>877</v>
-      </c>
-      <c t="s" s="7" r="E242">
+      <c s="17" r="B242"/>
+      <c s="28" r="C242"/>
+      <c s="17" r="D242"/>
+      <c s="17" r="E242"/>
+    </row>
+    <row r="243">
+      <c t="s" s="11" r="A243">
         <v>878</v>
       </c>
-    </row>
-    <row r="243">
-      <c s="11" r="A243"/>
-      <c s="17" r="B243"/>
-      <c s="31" r="C243"/>
-      <c s="17" r="D243"/>
-      <c s="17" r="E243"/>
+      <c t="s" s="7" r="B243">
+        <v>879</v>
+      </c>
+      <c t="s" s="14" r="C243">
+        <v>880</v>
+      </c>
+      <c t="s" s="7" r="D243">
+        <v>881</v>
+      </c>
+      <c t="s" s="7" r="E243">
+        <v>882</v>
+      </c>
     </row>
     <row r="244">
-      <c t="s" s="11" r="A244">
-        <v>879</v>
-      </c>
+      <c s="11" r="A244"/>
       <c t="s" s="7" r="B244">
-        <v>880</v>
+        <v>883</v>
       </c>
       <c t="s" s="14" r="C244">
-        <v>881</v>
+        <v>884</v>
       </c>
       <c t="s" s="7" r="D244">
-        <v>882</v>
+        <v>885</v>
       </c>
       <c t="s" s="7" r="E244">
-        <v>883</v>
+        <v>886</v>
       </c>
     </row>
     <row r="245">
       <c s="11" r="A245"/>
       <c s="17" r="B245"/>
-      <c s="9" r="C245"/>
+      <c s="28" r="C245"/>
       <c s="17" r="D245"/>
       <c s="17" r="E245"/>
     </row>
     <row r="246">
       <c t="s" s="11" r="A246">
-        <v>884</v>
+        <v>887</v>
       </c>
       <c t="s" s="7" r="B246">
-        <v>885</v>
+        <v>888</v>
       </c>
       <c t="s" s="14" r="C246">
-        <v>886</v>
+        <v>889</v>
       </c>
       <c t="s" s="7" r="D246">
-        <v>887</v>
+        <v>890</v>
       </c>
       <c t="s" s="7" r="E246">
-        <v>888</v>
+        <v>891</v>
       </c>
     </row>
     <row r="247">
       <c s="11" r="A247"/>
-      <c t="s" s="7" r="B247">
-        <v>889</v>
-      </c>
-      <c t="s" s="14" r="C247">
-        <v>890</v>
-      </c>
-      <c t="s" s="7" r="D247">
-        <v>891</v>
-      </c>
-      <c t="s" s="7" r="E247">
+      <c s="17" r="B247"/>
+      <c s="9" r="C247"/>
+      <c s="17" r="D247"/>
+      <c s="17" r="E247"/>
+    </row>
+    <row r="248">
+      <c t="s" s="11" r="A248">
         <v>892</v>
       </c>
-    </row>
-    <row r="248">
-      <c s="11" r="A248"/>
       <c t="s" s="7" r="B248">
         <v>893</v>
       </c>
@@ -7700,50 +7673,50 @@
       </c>
     </row>
     <row r="254">
-      <c s="18" r="A254"/>
-      <c s="17" r="B254"/>
-      <c s="9" r="C254"/>
-      <c s="17" r="D254"/>
-      <c s="17" r="E254"/>
+      <c s="11" r="A254"/>
+      <c t="s" s="7" r="B254">
+        <v>917</v>
+      </c>
+      <c t="s" s="14" r="C254">
+        <v>918</v>
+      </c>
+      <c t="s" s="7" r="D254">
+        <v>919</v>
+      </c>
+      <c t="s" s="7" r="E254">
+        <v>920</v>
+      </c>
     </row>
     <row r="255">
-      <c t="s" s="11" r="A255">
-        <v>917</v>
-      </c>
+      <c s="11" r="A255"/>
       <c t="s" s="7" r="B255">
-        <v>918</v>
-      </c>
-      <c t="s" s="7" r="C255">
-        <v>919</v>
+        <v>921</v>
+      </c>
+      <c t="s" s="14" r="C255">
+        <v>922</v>
       </c>
       <c t="s" s="7" r="D255">
-        <v>920</v>
+        <v>923</v>
       </c>
       <c t="s" s="7" r="E255">
-        <v>921</v>
+        <v>924</v>
       </c>
     </row>
     <row r="256">
-      <c s="11" r="A256"/>
-      <c t="s" s="7" r="B256">
-        <v>922</v>
-      </c>
-      <c t="s" s="14" r="C256">
-        <v>923</v>
-      </c>
-      <c t="s" s="7" r="D256">
-        <v>924</v>
-      </c>
-      <c t="s" s="7" r="E256">
+      <c s="18" r="A256"/>
+      <c s="17" r="B256"/>
+      <c s="9" r="C256"/>
+      <c s="17" r="D256"/>
+      <c s="17" r="E256"/>
+    </row>
+    <row r="257">
+      <c t="s" s="11" r="A257">
         <v>925</v>
       </c>
-    </row>
-    <row r="257">
-      <c s="11" r="A257"/>
       <c t="s" s="7" r="B257">
         <v>926</v>
       </c>
-      <c t="s" s="14" r="C257">
+      <c t="s" s="7" r="C257">
         <v>927</v>
       </c>
       <c t="s" s="7" r="D257">
@@ -7774,71 +7747,71 @@
         <v>934</v>
       </c>
       <c t="s" s="14" r="C259">
-        <v>651</v>
+        <v>935</v>
       </c>
       <c t="s" s="7" r="D259">
-        <v>160</v>
+        <v>936</v>
       </c>
       <c t="s" s="7" r="E259">
-        <v>653</v>
+        <v>937</v>
       </c>
     </row>
     <row r="260">
       <c s="11" r="A260"/>
       <c t="s" s="7" r="B260">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c t="s" s="14" r="C260">
-        <v>936</v>
+        <v>939</v>
       </c>
       <c t="s" s="7" r="D260">
-        <v>937</v>
+        <v>940</v>
       </c>
       <c t="s" s="7" r="E260">
-        <v>938</v>
+        <v>941</v>
       </c>
     </row>
     <row r="261">
-      <c s="18" r="A261"/>
-      <c s="17" r="B261"/>
-      <c s="9" r="C261"/>
-      <c s="17" r="D261"/>
-      <c s="17" r="E261"/>
+      <c s="11" r="A261"/>
+      <c t="s" s="7" r="B261">
+        <v>942</v>
+      </c>
+      <c t="s" s="14" r="C261">
+        <v>659</v>
+      </c>
+      <c t="s" s="7" r="D261">
+        <v>160</v>
+      </c>
+      <c t="s" s="7" r="E261">
+        <v>661</v>
+      </c>
     </row>
     <row r="262">
-      <c t="s" s="11" r="A262">
-        <v>939</v>
-      </c>
+      <c s="11" r="A262"/>
       <c t="s" s="7" r="B262">
-        <v>940</v>
+        <v>943</v>
       </c>
       <c t="s" s="14" r="C262">
-        <v>941</v>
+        <v>944</v>
       </c>
       <c t="s" s="7" r="D262">
-        <v>942</v>
+        <v>945</v>
       </c>
       <c t="s" s="7" r="E262">
-        <v>943</v>
+        <v>946</v>
       </c>
     </row>
     <row r="263">
-      <c s="11" r="A263"/>
-      <c t="s" s="7" r="B263">
-        <v>944</v>
-      </c>
-      <c t="s" s="14" r="C263">
-        <v>945</v>
-      </c>
-      <c t="s" s="7" r="D263">
-        <v>946</v>
-      </c>
-      <c t="s" s="7" r="E263">
+      <c s="18" r="A263"/>
+      <c s="17" r="B263"/>
+      <c s="9" r="C263"/>
+      <c s="17" r="D263"/>
+      <c s="17" r="E263"/>
+    </row>
+    <row r="264">
+      <c t="s" s="11" r="A264">
         <v>947</v>
       </c>
-    </row>
-    <row r="264">
-      <c s="11" r="A264"/>
       <c t="s" s="7" r="B264">
         <v>948</v>
       </c>
@@ -7864,34 +7837,34 @@
         <v>954</v>
       </c>
       <c t="s" s="7" r="E265">
-        <v>954</v>
+        <v>955</v>
       </c>
     </row>
     <row r="266">
       <c s="11" r="A266"/>
       <c t="s" s="7" r="B266">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c t="s" s="14" r="C266">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c t="s" s="7" r="D266">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c t="s" s="7" r="E266">
-        <v>958</v>
+        <v>959</v>
       </c>
     </row>
     <row r="267">
       <c s="11" r="A267"/>
       <c t="s" s="7" r="B267">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c t="s" s="14" r="C267">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c t="s" s="7" r="D267">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c t="s" s="7" r="E267">
         <v>962</v>
@@ -7996,37 +7969,37 @@
         <v>988</v>
       </c>
       <c t="s" s="7" r="D274">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c t="s" s="7" r="E274">
-        <v>988</v>
+        <v>990</v>
       </c>
     </row>
     <row r="275">
       <c s="11" r="A275"/>
       <c t="s" s="7" r="B275">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c t="s" s="14" r="C275">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c t="s" s="7" r="D275">
-        <v>991</v>
+        <v>993</v>
       </c>
       <c t="s" s="7" r="E275">
-        <v>992</v>
+        <v>994</v>
       </c>
     </row>
     <row r="276">
       <c s="11" r="A276"/>
       <c t="s" s="7" r="B276">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c t="s" s="14" r="C276">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c t="s" s="7" r="D276">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c t="s" s="7" r="E276">
         <v>996</v>
@@ -8109,45 +8082,45 @@
     </row>
     <row r="282">
       <c s="11" r="A282"/>
-      <c s="17" r="B282"/>
-      <c s="9" r="C282"/>
-      <c s="17" r="D282"/>
-      <c s="17" r="E282"/>
+      <c t="s" s="7" r="B282">
+        <v>1017</v>
+      </c>
+      <c t="s" s="14" r="C282">
+        <v>1018</v>
+      </c>
+      <c t="s" s="7" r="D282">
+        <v>1019</v>
+      </c>
+      <c t="s" s="7" r="E282">
+        <v>1020</v>
+      </c>
     </row>
     <row r="283">
-      <c t="s" s="11" r="A283">
-        <v>1017</v>
-      </c>
+      <c s="11" r="A283"/>
       <c t="s" s="7" r="B283">
-        <v>1018</v>
+        <v>1021</v>
       </c>
       <c t="s" s="14" r="C283">
-        <v>1019</v>
+        <v>1022</v>
       </c>
       <c t="s" s="7" r="D283">
-        <v>1020</v>
+        <v>1023</v>
       </c>
       <c t="s" s="7" r="E283">
-        <v>1021</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="284">
       <c s="11" r="A284"/>
-      <c t="s" s="7" r="B284">
-        <v>1022</v>
-      </c>
-      <c t="s" s="14" r="C284">
-        <v>1023</v>
-      </c>
-      <c t="s" s="7" r="D284">
-        <v>1024</v>
-      </c>
-      <c t="s" s="7" r="E284">
+      <c s="17" r="B284"/>
+      <c s="9" r="C284"/>
+      <c s="17" r="D284"/>
+      <c s="17" r="E284"/>
+    </row>
+    <row r="285">
+      <c t="s" s="11" r="A285">
         <v>1025</v>
       </c>
-    </row>
-    <row r="285">
-      <c s="11" r="A285"/>
       <c t="s" s="7" r="B285">
         <v>1026</v>
       </c>
@@ -8182,101 +8155,101 @@
         <v>1034</v>
       </c>
       <c t="s" s="14" r="C287">
-        <v>1034</v>
-      </c>
-      <c t="s" s="19" r="D287">
         <v>1035</v>
       </c>
-      <c t="s" s="19" r="E287">
+      <c t="s" s="7" r="D287">
         <v>1036</v>
+      </c>
+      <c t="s" s="7" r="E287">
+        <v>1037</v>
       </c>
     </row>
     <row r="288">
       <c s="11" r="A288"/>
       <c t="s" s="7" r="B288">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c t="s" s="14" r="C288">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c t="s" s="7" r="D288">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c t="s" s="7" r="E288">
-        <v>1040</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="289">
       <c s="11" r="A289"/>
       <c t="s" s="7" r="B289">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c t="s" s="14" r="C289">
         <v>1042</v>
       </c>
-      <c t="s" s="7" r="D289">
+      <c t="s" s="19" r="D289">
         <v>1043</v>
       </c>
-      <c t="s" s="7" r="E289">
+      <c t="s" s="19" r="E289">
         <v>1044</v>
       </c>
     </row>
     <row r="290">
-      <c t="s" s="17" r="A290">
+      <c s="11" r="A290"/>
+      <c t="s" s="7" r="B290">
         <v>1045</v>
       </c>
-      <c s="28" r="B290"/>
       <c t="s" s="14" r="C290">
         <v>1046</v>
       </c>
-      <c t="s" s="19" r="D290">
+      <c t="s" s="7" r="D290">
         <v>1047</v>
       </c>
-      <c t="s" s="19" r="E290">
+      <c t="s" s="7" r="E290">
         <v>1048</v>
       </c>
     </row>
     <row r="291">
-      <c s="18" r="A291"/>
-      <c s="17" r="B291"/>
-      <c s="9" r="C291"/>
-      <c s="17" r="D291"/>
-      <c s="17" r="E291"/>
+      <c s="11" r="A291"/>
+      <c t="s" s="7" r="B291">
+        <v>1049</v>
+      </c>
+      <c t="s" s="14" r="C291">
+        <v>1050</v>
+      </c>
+      <c t="s" s="7" r="D291">
+        <v>1051</v>
+      </c>
+      <c t="s" s="7" r="E291">
+        <v>1052</v>
+      </c>
     </row>
     <row r="292">
-      <c t="s" s="18" r="A292">
-        <v>1049</v>
-      </c>
-      <c t="s" s="7" r="B292">
-        <v>1050</v>
-      </c>
-      <c t="s" s="7" r="C292">
-        <v>1051</v>
-      </c>
-      <c t="s" s="7" r="D292">
-        <v>1052</v>
-      </c>
-      <c t="s" s="7" r="E292">
+      <c t="s" s="17" r="A292">
         <v>1053</v>
       </c>
+      <c s="25" r="B292"/>
+      <c t="s" s="14" r="C292">
+        <v>1054</v>
+      </c>
+      <c t="s" s="19" r="D292">
+        <v>1055</v>
+      </c>
+      <c t="s" s="19" r="E292">
+        <v>1056</v>
+      </c>
     </row>
     <row r="293">
-      <c s="15" r="A293"/>
-      <c t="s" s="7" r="B293">
-        <v>1054</v>
-      </c>
-      <c t="s" s="14" r="C293">
-        <v>1055</v>
-      </c>
-      <c t="s" s="7" r="D293">
-        <v>1056</v>
-      </c>
-      <c t="s" s="7" r="E293">
+      <c s="18" r="A293"/>
+      <c s="17" r="B293"/>
+      <c s="9" r="C293"/>
+      <c s="17" r="D293"/>
+      <c s="17" r="E293"/>
+    </row>
+    <row r="294">
+      <c t="s" s="18" r="A294">
         <v>1057</v>
       </c>
-    </row>
-    <row r="294">
-      <c s="15" r="A294"/>
       <c t="s" s="7" r="B294">
         <v>1058</v>
       </c>
@@ -8291,7 +8264,7 @@
       </c>
     </row>
     <row r="295">
-      <c s="18" r="A295"/>
+      <c s="15" r="A295"/>
       <c t="s" s="7" r="B295">
         <v>1062</v>
       </c>
@@ -8306,7 +8279,7 @@
       </c>
     </row>
     <row r="296">
-      <c s="18" r="A296"/>
+      <c s="15" r="A296"/>
       <c t="s" s="7" r="B296">
         <v>1066</v>
       </c>
@@ -8416,43 +8389,43 @@
         <v>1094</v>
       </c>
       <c t="s" s="14" r="C303">
-        <v>1087</v>
+        <v>1095</v>
       </c>
       <c t="s" s="7" r="D303">
-        <v>1088</v>
+        <v>1096</v>
       </c>
       <c t="s" s="7" r="E303">
-        <v>1089</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="304">
       <c s="18" r="A304"/>
       <c t="s" s="7" r="B304">
-        <v>1095</v>
-      </c>
-      <c t="s" s="14" r="C304">
-        <v>1096</v>
+        <v>1098</v>
+      </c>
+      <c t="s" s="7" r="C304">
+        <v>1099</v>
       </c>
       <c t="s" s="7" r="D304">
-        <v>1097</v>
+        <v>1100</v>
       </c>
       <c t="s" s="7" r="E304">
-        <v>1098</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="305">
       <c s="18" r="A305"/>
       <c t="s" s="7" r="B305">
-        <v>1099</v>
+        <v>1102</v>
       </c>
       <c t="s" s="14" r="C305">
-        <v>1100</v>
+        <v>1095</v>
       </c>
       <c t="s" s="7" r="D305">
-        <v>1101</v>
+        <v>1096</v>
       </c>
       <c t="s" s="7" r="E305">
-        <v>1102</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="306">
@@ -8460,7 +8433,7 @@
       <c t="s" s="7" r="B306">
         <v>1103</v>
       </c>
-      <c t="s" s="7" r="C306">
+      <c t="s" s="14" r="C306">
         <v>1104</v>
       </c>
       <c t="s" s="7" r="D306">
@@ -8486,11 +8459,11 @@
       </c>
     </row>
     <row r="308">
-      <c s="11" r="A308"/>
+      <c s="18" r="A308"/>
       <c t="s" s="7" r="B308">
         <v>1111</v>
       </c>
-      <c t="s" s="14" r="C308">
+      <c t="s" s="7" r="C308">
         <v>1112</v>
       </c>
       <c t="s" s="7" r="D308">
@@ -8501,72 +8474,110 @@
       </c>
     </row>
     <row r="309">
-      <c t="s" s="11" r="A309">
+      <c s="18" r="A309"/>
+      <c t="s" s="7" r="B309">
         <v>1115</v>
       </c>
-      <c t="s" s="14" r="B309">
+      <c t="s" s="14" r="C309">
         <v>1116</v>
       </c>
-      <c t="s" s="14" r="C309">
+      <c t="s" s="7" r="D309">
         <v>1117</v>
       </c>
-      <c t="s" s="19" r="D309">
+      <c t="s" s="7" r="E309">
         <v>1118</v>
-      </c>
-      <c t="s" s="7" r="E309">
-        <v>1119</v>
       </c>
     </row>
     <row r="310">
       <c s="11" r="A310"/>
-      <c t="s" s="14" r="B310">
+      <c t="s" s="7" r="B310">
+        <v>1119</v>
+      </c>
+      <c t="s" s="14" r="C310">
         <v>1120</v>
       </c>
-      <c t="s" s="14" r="C310">
+      <c t="s" s="7" r="D310">
         <v>1121</v>
       </c>
-      <c t="s" s="19" r="D310">
+      <c t="s" s="7" r="E310">
         <v>1122</v>
       </c>
-      <c t="s" s="7" r="E310">
+    </row>
+    <row r="311">
+      <c t="s" s="11" r="A311">
         <v>1123</v>
       </c>
-    </row>
-    <row r="311">
-      <c s="11" r="A311"/>
-      <c s="9" r="C311"/>
-      <c s="17" r="D311"/>
-      <c s="17" r="E311"/>
+      <c t="s" s="14" r="B311">
+        <v>1124</v>
+      </c>
+      <c t="s" s="14" r="C311">
+        <v>1125</v>
+      </c>
+      <c t="s" s="19" r="D311">
+        <v>1126</v>
+      </c>
+      <c t="s" s="7" r="E311">
+        <v>1127</v>
+      </c>
     </row>
     <row r="312">
-      <c t="s" s="11" r="A312">
-        <v>1124</v>
-      </c>
-      <c t="s" s="34" r="B312">
-        <v>1125</v>
-      </c>
-      <c t="s" s="25" r="C312">
-        <v>1126</v>
-      </c>
-      <c s="24" r="D312"/>
-      <c s="24" r="E312"/>
+      <c s="11" r="A312"/>
+      <c t="s" s="14" r="B312">
+        <v>1128</v>
+      </c>
+      <c t="s" s="14" r="C312">
+        <v>1129</v>
+      </c>
+      <c t="s" s="19" r="D312">
+        <v>1130</v>
+      </c>
+      <c t="s" s="7" r="E312">
+        <v>1131</v>
+      </c>
     </row>
     <row r="313">
       <c s="11" r="A313"/>
-      <c t="s" s="34" r="B313">
-        <v>1127</v>
-      </c>
-      <c t="s" s="25" r="C313">
-        <v>1128</v>
-      </c>
-      <c s="24" r="D313"/>
-      <c s="24" r="E313"/>
+      <c s="9" r="C313"/>
+      <c s="17" r="D313"/>
+      <c s="17" r="E313"/>
     </row>
     <row r="314">
-      <c s="11" r="A314"/>
-      <c s="9" r="C314"/>
-      <c s="17" r="D314"/>
-      <c s="17" r="E314"/>
+      <c t="s" s="11" r="A314">
+        <v>1132</v>
+      </c>
+      <c t="s" s="25" r="B314">
+        <v>1133</v>
+      </c>
+      <c t="s" s="14" r="C314">
+        <v>1134</v>
+      </c>
+      <c t="s" s="7" r="D314">
+        <v>1135</v>
+      </c>
+      <c t="s" s="7" r="E314">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="315">
+      <c s="11" r="A315"/>
+      <c t="s" s="25" r="B315">
+        <v>1137</v>
+      </c>
+      <c t="s" s="14" r="C315">
+        <v>1138</v>
+      </c>
+      <c t="s" s="7" r="D315">
+        <v>1139</v>
+      </c>
+      <c t="s" s="7" r="E315">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="316">
+      <c s="11" r="A316"/>
+      <c s="9" r="C316"/>
+      <c s="17" r="D316"/>
+      <c s="17" r="E316"/>
     </row>
   </sheetData>
 </worksheet>
@@ -8584,17 +8595,17 @@
   <sheetData>
     <row customHeight="1" r="1" ht="112.5">
       <c t="s" s="4" r="A1">
-        <v>1129</v>
+        <v>1141</v>
       </c>
     </row>
     <row customHeight="1" r="2" ht="112.5">
       <c t="s" s="5" r="A2">
-        <v>1130</v>
+        <v>1142</v>
       </c>
     </row>
     <row customHeight="1" r="3" ht="112.5">
       <c t="s" s="10" r="A3">
-        <v>1131</v>
+        <v>1143</v>
       </c>
     </row>
   </sheetData>
@@ -8609,164 +8620,164 @@
   <sheetFormatPr customHeight="1" defaultColWidth="9.86" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c s="36" r="A1"/>
-      <c s="36" r="B1"/>
-      <c s="36" r="C1"/>
-      <c s="36" r="D1"/>
-      <c s="36" r="E1"/>
-      <c s="36" r="F1"/>
+      <c s="32" r="A1"/>
+      <c s="32" r="B1"/>
+      <c s="32" r="C1"/>
+      <c s="32" r="D1"/>
+      <c s="32" r="E1"/>
+      <c s="32" r="F1"/>
     </row>
     <row r="2">
-      <c s="36" r="A2"/>
-      <c s="36" r="B2"/>
-      <c s="36" r="C2"/>
-      <c s="36" r="D2"/>
-      <c s="36" r="E2"/>
-      <c s="36" r="F2"/>
+      <c s="32" r="A2"/>
+      <c s="32" r="B2"/>
+      <c s="32" r="C2"/>
+      <c s="32" r="D2"/>
+      <c s="32" r="E2"/>
+      <c s="32" r="F2"/>
     </row>
     <row r="3">
-      <c s="36" r="A3"/>
-      <c s="36" r="B3"/>
-      <c s="36" r="C3"/>
-      <c s="36" r="D3"/>
-      <c s="36" r="E3"/>
-      <c s="36" r="F3"/>
+      <c s="32" r="A3"/>
+      <c s="32" r="B3"/>
+      <c s="32" r="C3"/>
+      <c s="32" r="D3"/>
+      <c s="32" r="E3"/>
+      <c s="32" r="F3"/>
     </row>
     <row r="4">
-      <c s="36" r="A4"/>
-      <c s="36" r="B4"/>
-      <c s="36" r="C4"/>
-      <c s="36" r="D4"/>
-      <c s="36" r="E4"/>
-      <c s="36" r="F4"/>
+      <c s="32" r="A4"/>
+      <c s="32" r="B4"/>
+      <c s="32" r="C4"/>
+      <c s="32" r="D4"/>
+      <c s="32" r="E4"/>
+      <c s="32" r="F4"/>
     </row>
     <row r="5">
-      <c s="36" r="A5"/>
-      <c s="36" r="B5"/>
-      <c s="36" r="C5"/>
-      <c s="36" r="D5"/>
-      <c s="36" r="E5"/>
-      <c s="36" r="F5"/>
+      <c s="32" r="A5"/>
+      <c s="32" r="B5"/>
+      <c s="32" r="C5"/>
+      <c s="32" r="D5"/>
+      <c s="32" r="E5"/>
+      <c s="32" r="F5"/>
     </row>
     <row r="6">
-      <c s="36" r="A6"/>
-      <c s="36" r="B6"/>
-      <c s="36" r="C6"/>
-      <c s="36" r="D6"/>
-      <c s="36" r="E6"/>
-      <c s="36" r="F6"/>
+      <c s="32" r="A6"/>
+      <c s="32" r="B6"/>
+      <c s="32" r="C6"/>
+      <c s="32" r="D6"/>
+      <c s="32" r="E6"/>
+      <c s="32" r="F6"/>
     </row>
     <row r="7">
-      <c s="36" r="A7"/>
-      <c s="36" r="B7"/>
-      <c s="36" r="C7"/>
-      <c s="36" r="D7"/>
-      <c s="36" r="E7"/>
-      <c s="36" r="F7"/>
+      <c s="32" r="A7"/>
+      <c s="32" r="B7"/>
+      <c s="32" r="C7"/>
+      <c s="32" r="D7"/>
+      <c s="32" r="E7"/>
+      <c s="32" r="F7"/>
     </row>
     <row r="8">
-      <c s="36" r="A8"/>
-      <c s="36" r="B8"/>
-      <c s="36" r="C8"/>
-      <c s="36" r="D8"/>
-      <c s="36" r="E8"/>
-      <c s="36" r="F8"/>
+      <c s="32" r="A8"/>
+      <c s="32" r="B8"/>
+      <c s="32" r="C8"/>
+      <c s="32" r="D8"/>
+      <c s="32" r="E8"/>
+      <c s="32" r="F8"/>
     </row>
     <row r="9">
-      <c s="36" r="A9"/>
-      <c s="36" r="B9"/>
-      <c s="36" r="C9"/>
-      <c s="36" r="D9"/>
-      <c s="36" r="E9"/>
-      <c s="36" r="F9"/>
+      <c s="32" r="A9"/>
+      <c s="32" r="B9"/>
+      <c s="32" r="C9"/>
+      <c s="32" r="D9"/>
+      <c s="32" r="E9"/>
+      <c s="32" r="F9"/>
     </row>
     <row r="10">
-      <c s="36" r="A10"/>
-      <c s="36" r="B10"/>
-      <c s="36" r="C10"/>
-      <c s="36" r="D10"/>
-      <c s="36" r="E10"/>
-      <c s="36" r="F10"/>
+      <c s="32" r="A10"/>
+      <c s="32" r="B10"/>
+      <c s="32" r="C10"/>
+      <c s="32" r="D10"/>
+      <c s="32" r="E10"/>
+      <c s="32" r="F10"/>
     </row>
     <row r="11">
-      <c s="36" r="A11"/>
-      <c s="36" r="B11"/>
-      <c s="36" r="C11"/>
-      <c s="36" r="D11"/>
-      <c s="36" r="E11"/>
-      <c s="36" r="F11"/>
+      <c s="32" r="A11"/>
+      <c s="32" r="B11"/>
+      <c s="32" r="C11"/>
+      <c s="32" r="D11"/>
+      <c s="32" r="E11"/>
+      <c s="32" r="F11"/>
     </row>
     <row r="12">
-      <c s="36" r="A12"/>
-      <c s="36" r="B12"/>
-      <c s="36" r="C12"/>
-      <c s="36" r="D12"/>
-      <c s="36" r="E12"/>
-      <c s="36" r="F12"/>
+      <c s="32" r="A12"/>
+      <c s="32" r="B12"/>
+      <c s="32" r="C12"/>
+      <c s="32" r="D12"/>
+      <c s="32" r="E12"/>
+      <c s="32" r="F12"/>
     </row>
     <row r="13">
-      <c s="36" r="A13"/>
-      <c s="36" r="B13"/>
-      <c s="36" r="C13"/>
-      <c s="36" r="D13"/>
-      <c s="36" r="E13"/>
-      <c s="36" r="F13"/>
+      <c s="32" r="A13"/>
+      <c s="32" r="B13"/>
+      <c s="32" r="C13"/>
+      <c s="32" r="D13"/>
+      <c s="32" r="E13"/>
+      <c s="32" r="F13"/>
     </row>
     <row r="14">
-      <c s="36" r="A14"/>
-      <c s="36" r="B14"/>
-      <c s="36" r="C14"/>
-      <c s="36" r="D14"/>
-      <c s="36" r="E14"/>
-      <c s="36" r="F14"/>
+      <c s="32" r="A14"/>
+      <c s="32" r="B14"/>
+      <c s="32" r="C14"/>
+      <c s="32" r="D14"/>
+      <c s="32" r="E14"/>
+      <c s="32" r="F14"/>
     </row>
     <row r="15">
-      <c s="36" r="A15"/>
-      <c s="36" r="B15"/>
-      <c s="36" r="C15"/>
-      <c s="36" r="D15"/>
-      <c s="36" r="E15"/>
-      <c s="36" r="F15"/>
+      <c s="32" r="A15"/>
+      <c s="32" r="B15"/>
+      <c s="32" r="C15"/>
+      <c s="32" r="D15"/>
+      <c s="32" r="E15"/>
+      <c s="32" r="F15"/>
     </row>
     <row r="16">
-      <c s="36" r="A16"/>
-      <c s="36" r="B16"/>
-      <c s="36" r="C16"/>
-      <c s="36" r="D16"/>
-      <c s="36" r="E16"/>
-      <c s="36" r="F16"/>
+      <c s="32" r="A16"/>
+      <c s="32" r="B16"/>
+      <c s="32" r="C16"/>
+      <c s="32" r="D16"/>
+      <c s="32" r="E16"/>
+      <c s="32" r="F16"/>
     </row>
     <row r="17">
-      <c s="36" r="A17"/>
-      <c s="36" r="B17"/>
-      <c s="36" r="C17"/>
-      <c s="36" r="D17"/>
-      <c s="36" r="E17"/>
-      <c s="36" r="F17"/>
+      <c s="32" r="A17"/>
+      <c s="32" r="B17"/>
+      <c s="32" r="C17"/>
+      <c s="32" r="D17"/>
+      <c s="32" r="E17"/>
+      <c s="32" r="F17"/>
     </row>
     <row r="18">
-      <c s="36" r="A18"/>
-      <c s="36" r="B18"/>
-      <c s="36" r="C18"/>
-      <c s="36" r="D18"/>
-      <c s="36" r="E18"/>
-      <c s="36" r="F18"/>
+      <c s="32" r="A18"/>
+      <c s="32" r="B18"/>
+      <c s="32" r="C18"/>
+      <c s="32" r="D18"/>
+      <c s="32" r="E18"/>
+      <c s="32" r="F18"/>
     </row>
     <row r="19">
-      <c s="36" r="A19"/>
-      <c s="36" r="B19"/>
-      <c s="36" r="C19"/>
-      <c s="36" r="D19"/>
-      <c s="36" r="E19"/>
-      <c s="36" r="F19"/>
+      <c s="32" r="A19"/>
+      <c s="32" r="B19"/>
+      <c s="32" r="C19"/>
+      <c s="32" r="D19"/>
+      <c s="32" r="E19"/>
+      <c s="32" r="F19"/>
     </row>
     <row r="20">
-      <c s="36" r="A20"/>
-      <c s="36" r="B20"/>
-      <c s="36" r="C20"/>
-      <c s="36" r="D20"/>
-      <c s="36" r="E20"/>
-      <c s="36" r="F20"/>
+      <c s="32" r="A20"/>
+      <c s="32" r="B20"/>
+      <c s="32" r="C20"/>
+      <c s="32" r="D20"/>
+      <c s="32" r="E20"/>
+      <c s="32" r="F20"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
EWD-22844 - Create question in one step
Former-commit-id: 8a024c4a258bc63313234c4cd9ecf250dba3ba3a
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="1150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="1152">
   <si>
     <t>nnot</t>
   </si>
@@ -1555,6 +1555,12 @@
   </si>
   <si>
     <t>Gespeichert am</t>
+  </si>
+  <si>
+    <t>newQuestionTitle</t>
+  </si>
+  <si>
+    <t>What question do you want to ask?</t>
   </si>
   <si>
     <t>customLocalizationPlugin</t>
@@ -6060,101 +6066,97 @@
     </row>
     <row r="137">
       <c s="11" r="A137"/>
-      <c s="12" r="B137"/>
-      <c s="12" r="C137"/>
-      <c s="12" r="D137"/>
-      <c s="12" r="E137"/>
+      <c t="s" s="19" r="B137">
+        <v>512</v>
+      </c>
+      <c t="s" s="19" r="C137">
+        <v>513</v>
+      </c>
+      <c s="19" r="D137"/>
+      <c s="19" r="E137"/>
     </row>
     <row r="138">
-      <c t="s" s="11" r="A138">
-        <v>512</v>
-      </c>
-      <c t="s" s="7" r="B138">
-        <v>513</v>
-      </c>
-      <c t="s" s="7" r="C138">
+      <c s="11" r="A138"/>
+      <c s="12" r="B138"/>
+      <c s="12" r="C138"/>
+      <c s="12" r="D138"/>
+      <c s="12" r="E138"/>
+    </row>
+    <row r="139">
+      <c t="s" s="11" r="A139">
         <v>514</v>
       </c>
-      <c t="s" s="7" r="D138">
+      <c t="s" s="7" r="B139">
         <v>515</v>
       </c>
-      <c t="s" s="7" r="E138">
+      <c t="s" s="7" r="C139">
         <v>516</v>
       </c>
-    </row>
-    <row r="139">
-      <c s="11" r="A139"/>
-      <c t="s" s="7" r="B139">
+      <c t="s" s="7" r="D139">
         <v>517</v>
       </c>
-      <c t="s" s="7" r="C139">
+      <c t="s" s="7" r="E139">
         <v>518</v>
-      </c>
-      <c t="s" s="7" r="D139">
-        <v>519</v>
-      </c>
-      <c t="s" s="7" r="E139">
-        <v>520</v>
       </c>
     </row>
     <row r="140">
       <c s="11" r="A140"/>
       <c t="s" s="7" r="B140">
+        <v>519</v>
+      </c>
+      <c t="s" s="7" r="C140">
+        <v>520</v>
+      </c>
+      <c t="s" s="7" r="D140">
         <v>521</v>
       </c>
-      <c t="s" s="7" r="C140">
+      <c t="s" s="7" r="E140">
         <v>522</v>
-      </c>
-      <c t="s" s="7" r="D140">
-        <v>523</v>
-      </c>
-      <c t="s" s="7" r="E140">
-        <v>524</v>
       </c>
     </row>
     <row r="141">
       <c s="11" r="A141"/>
       <c t="s" s="7" r="B141">
+        <v>523</v>
+      </c>
+      <c t="s" s="7" r="C141">
+        <v>524</v>
+      </c>
+      <c t="s" s="7" r="D141">
         <v>525</v>
       </c>
-      <c t="s" s="7" r="C141">
+      <c t="s" s="7" r="E141">
         <v>526</v>
-      </c>
-      <c t="s" s="7" r="D141">
-        <v>527</v>
-      </c>
-      <c t="s" s="7" r="E141">
-        <v>528</v>
       </c>
     </row>
     <row r="142">
       <c s="11" r="A142"/>
       <c t="s" s="7" r="B142">
+        <v>527</v>
+      </c>
+      <c t="s" s="7" r="C142">
+        <v>528</v>
+      </c>
+      <c t="s" s="7" r="D142">
         <v>529</v>
       </c>
-      <c t="s" s="7" r="C142">
+      <c t="s" s="7" r="E142">
         <v>530</v>
-      </c>
-      <c t="s" s="7" r="D142">
-        <v>531</v>
-      </c>
-      <c t="s" s="7" r="E142">
-        <v>532</v>
       </c>
     </row>
     <row r="143">
       <c s="11" r="A143"/>
       <c t="s" s="7" r="B143">
+        <v>531</v>
+      </c>
+      <c t="s" s="7" r="C143">
+        <v>532</v>
+      </c>
+      <c t="s" s="7" r="D143">
         <v>533</v>
       </c>
-      <c t="s" s="7" r="C143">
-        <v>250</v>
-      </c>
-      <c t="s" s="7" r="D143">
+      <c t="s" s="7" r="E143">
         <v>534</v>
-      </c>
-      <c t="s" s="7" r="E143">
-        <v>250</v>
       </c>
     </row>
     <row r="144">
@@ -6163,810 +6165,814 @@
         <v>535</v>
       </c>
       <c t="s" s="7" r="C144">
+        <v>250</v>
+      </c>
+      <c t="s" s="7" r="D144">
         <v>536</v>
       </c>
-      <c t="s" s="7" r="D144">
-        <v>537</v>
-      </c>
       <c t="s" s="7" r="E144">
-        <v>538</v>
+        <v>250</v>
       </c>
     </row>
     <row r="145">
       <c s="11" r="A145"/>
       <c t="s" s="7" r="B145">
+        <v>537</v>
+      </c>
+      <c t="s" s="7" r="C145">
+        <v>538</v>
+      </c>
+      <c t="s" s="7" r="D145">
         <v>539</v>
       </c>
-      <c t="s" s="7" r="C145">
+      <c t="s" s="7" r="E145">
         <v>540</v>
-      </c>
-      <c t="s" s="7" r="D145">
-        <v>541</v>
-      </c>
-      <c t="s" s="7" r="E145">
-        <v>542</v>
       </c>
     </row>
     <row r="146">
       <c s="11" r="A146"/>
       <c t="s" s="7" r="B146">
+        <v>541</v>
+      </c>
+      <c t="s" s="7" r="C146">
+        <v>542</v>
+      </c>
+      <c t="s" s="7" r="D146">
         <v>543</v>
       </c>
-      <c t="s" s="7" r="C146">
+      <c t="s" s="7" r="E146">
         <v>544</v>
-      </c>
-      <c t="s" s="7" r="D146">
-        <v>545</v>
-      </c>
-      <c t="s" s="7" r="E146">
-        <v>546</v>
       </c>
     </row>
     <row r="147">
       <c s="11" r="A147"/>
       <c t="s" s="7" r="B147">
+        <v>545</v>
+      </c>
+      <c t="s" s="7" r="C147">
+        <v>546</v>
+      </c>
+      <c t="s" s="7" r="D147">
         <v>547</v>
       </c>
-      <c t="s" s="7" r="C147">
+      <c t="s" s="7" r="E147">
         <v>548</v>
-      </c>
-      <c t="s" s="7" r="D147">
-        <v>549</v>
-      </c>
-      <c t="s" s="7" r="E147">
-        <v>550</v>
       </c>
     </row>
     <row r="148">
       <c s="11" r="A148"/>
       <c t="s" s="7" r="B148">
+        <v>549</v>
+      </c>
+      <c t="s" s="7" r="C148">
+        <v>550</v>
+      </c>
+      <c t="s" s="7" r="D148">
         <v>551</v>
       </c>
-      <c t="s" s="7" r="C148">
+      <c t="s" s="7" r="E148">
         <v>552</v>
-      </c>
-      <c t="s" s="7" r="D148">
-        <v>553</v>
-      </c>
-      <c t="s" s="7" r="E148">
-        <v>554</v>
       </c>
     </row>
     <row r="149">
       <c s="11" r="A149"/>
       <c t="s" s="7" r="B149">
+        <v>553</v>
+      </c>
+      <c t="s" s="7" r="C149">
+        <v>554</v>
+      </c>
+      <c t="s" s="7" r="D149">
         <v>555</v>
       </c>
-      <c t="s" s="7" r="C149">
+      <c t="s" s="7" r="E149">
         <v>556</v>
-      </c>
-      <c t="s" s="7" r="D149">
-        <v>556</v>
-      </c>
-      <c t="s" s="7" r="E149">
-        <v>557</v>
       </c>
     </row>
     <row r="150">
       <c s="11" r="A150"/>
       <c t="s" s="7" r="B150">
+        <v>557</v>
+      </c>
+      <c t="s" s="7" r="C150">
         <v>558</v>
       </c>
-      <c t="s" s="7" r="C150">
+      <c t="s" s="7" r="D150">
+        <v>558</v>
+      </c>
+      <c t="s" s="7" r="E150">
         <v>559</v>
-      </c>
-      <c t="s" s="7" r="D150">
-        <v>559</v>
-      </c>
-      <c t="s" s="7" r="E150">
-        <v>560</v>
       </c>
     </row>
     <row r="151">
       <c s="11" r="A151"/>
       <c t="s" s="7" r="B151">
+        <v>560</v>
+      </c>
+      <c t="s" s="7" r="C151">
         <v>561</v>
       </c>
-      <c t="s" s="7" r="C151">
+      <c t="s" s="7" r="D151">
+        <v>561</v>
+      </c>
+      <c t="s" s="7" r="E151">
         <v>562</v>
-      </c>
-      <c t="s" s="7" r="D151">
-        <v>563</v>
-      </c>
-      <c t="s" s="7" r="E151">
-        <v>564</v>
       </c>
     </row>
     <row r="152">
       <c s="11" r="A152"/>
-      <c t="s" s="14" r="B152">
+      <c t="s" s="7" r="B152">
+        <v>563</v>
+      </c>
+      <c t="s" s="7" r="C152">
+        <v>564</v>
+      </c>
+      <c t="s" s="7" r="D152">
         <v>565</v>
       </c>
-      <c t="s" s="7" r="C152">
+      <c t="s" s="7" r="E152">
         <v>566</v>
-      </c>
-      <c t="s" s="7" r="D152">
-        <v>567</v>
-      </c>
-      <c t="s" s="7" r="E152">
-        <v>567</v>
       </c>
     </row>
     <row r="153">
       <c s="11" r="A153"/>
-      <c t="s" s="7" r="B153">
+      <c t="s" s="14" r="B153">
+        <v>567</v>
+      </c>
+      <c t="s" s="7" r="C153">
         <v>568</v>
       </c>
-      <c t="s" s="7" r="C153">
+      <c t="s" s="7" r="D153">
         <v>569</v>
       </c>
-      <c t="s" s="7" r="D153">
-        <v>570</v>
-      </c>
       <c t="s" s="7" r="E153">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="154">
       <c s="11" r="A154"/>
       <c t="s" s="7" r="B154">
+        <v>570</v>
+      </c>
+      <c t="s" s="7" r="C154">
+        <v>571</v>
+      </c>
+      <c t="s" s="7" r="D154">
         <v>572</v>
       </c>
-      <c t="s" s="7" r="C154">
+      <c t="s" s="7" r="E154">
         <v>573</v>
-      </c>
-      <c t="s" s="7" r="D154">
-        <v>574</v>
-      </c>
-      <c t="s" s="7" r="E154">
-        <v>575</v>
       </c>
     </row>
     <row r="155">
       <c s="11" r="A155"/>
       <c t="s" s="7" r="B155">
+        <v>574</v>
+      </c>
+      <c t="s" s="7" r="C155">
+        <v>575</v>
+      </c>
+      <c t="s" s="7" r="D155">
         <v>576</v>
       </c>
-      <c t="s" s="7" r="C155">
+      <c t="s" s="7" r="E155">
         <v>577</v>
-      </c>
-      <c t="s" s="7" r="D155">
-        <v>578</v>
-      </c>
-      <c t="s" s="7" r="E155">
-        <v>579</v>
       </c>
     </row>
     <row r="156">
       <c s="11" r="A156"/>
       <c t="s" s="7" r="B156">
+        <v>578</v>
+      </c>
+      <c t="s" s="7" r="C156">
+        <v>579</v>
+      </c>
+      <c t="s" s="7" r="D156">
         <v>580</v>
       </c>
-      <c t="s" s="7" r="C156">
+      <c t="s" s="7" r="E156">
         <v>581</v>
-      </c>
-      <c t="s" s="7" r="D156">
-        <v>582</v>
-      </c>
-      <c t="s" s="7" r="E156">
-        <v>583</v>
       </c>
     </row>
     <row r="157">
       <c s="11" r="A157"/>
       <c t="s" s="7" r="B157">
+        <v>582</v>
+      </c>
+      <c t="s" s="7" r="C157">
+        <v>583</v>
+      </c>
+      <c t="s" s="7" r="D157">
         <v>584</v>
       </c>
-      <c t="s" s="7" r="C157">
+      <c t="s" s="7" r="E157">
         <v>585</v>
-      </c>
-      <c t="s" s="7" r="D157">
-        <v>586</v>
-      </c>
-      <c t="s" s="7" r="E157">
-        <v>587</v>
       </c>
     </row>
     <row r="158">
       <c s="11" r="A158"/>
       <c t="s" s="7" r="B158">
+        <v>586</v>
+      </c>
+      <c t="s" s="7" r="C158">
+        <v>587</v>
+      </c>
+      <c t="s" s="7" r="D158">
         <v>588</v>
       </c>
-      <c t="s" s="7" r="C158">
+      <c t="s" s="7" r="E158">
         <v>589</v>
-      </c>
-      <c t="s" s="7" r="D158">
-        <v>590</v>
-      </c>
-      <c t="s" s="7" r="E158">
-        <v>591</v>
       </c>
     </row>
     <row r="159">
       <c s="11" r="A159"/>
       <c t="s" s="7" r="B159">
+        <v>590</v>
+      </c>
+      <c t="s" s="7" r="C159">
+        <v>591</v>
+      </c>
+      <c t="s" s="7" r="D159">
         <v>592</v>
       </c>
-      <c t="s" s="7" r="C159">
+      <c t="s" s="7" r="E159">
         <v>593</v>
-      </c>
-      <c t="s" s="7" r="D159">
-        <v>594</v>
-      </c>
-      <c t="s" s="7" r="E159">
-        <v>595</v>
       </c>
     </row>
     <row r="160">
       <c s="11" r="A160"/>
       <c t="s" s="7" r="B160">
+        <v>594</v>
+      </c>
+      <c t="s" s="7" r="C160">
+        <v>595</v>
+      </c>
+      <c t="s" s="7" r="D160">
         <v>596</v>
       </c>
-      <c t="s" s="7" r="C160">
+      <c t="s" s="7" r="E160">
         <v>597</v>
-      </c>
-      <c t="s" s="7" r="D160">
-        <v>598</v>
-      </c>
-      <c t="s" s="7" r="E160">
-        <v>599</v>
       </c>
     </row>
     <row r="161">
       <c s="11" r="A161"/>
       <c t="s" s="7" r="B161">
+        <v>598</v>
+      </c>
+      <c t="s" s="7" r="C161">
+        <v>599</v>
+      </c>
+      <c t="s" s="7" r="D161">
         <v>600</v>
       </c>
-      <c t="s" s="7" r="C161">
+      <c t="s" s="7" r="E161">
         <v>601</v>
-      </c>
-      <c t="s" s="7" r="D161">
-        <v>602</v>
-      </c>
-      <c t="s" s="7" r="E161">
-        <v>603</v>
       </c>
     </row>
     <row r="162">
       <c s="11" r="A162"/>
       <c t="s" s="7" r="B162">
+        <v>602</v>
+      </c>
+      <c t="s" s="7" r="C162">
+        <v>603</v>
+      </c>
+      <c t="s" s="7" r="D162">
         <v>604</v>
       </c>
-      <c t="s" s="7" r="C162">
+      <c t="s" s="7" r="E162">
         <v>605</v>
-      </c>
-      <c t="s" s="7" r="D162">
-        <v>606</v>
-      </c>
-      <c t="s" s="7" r="E162">
-        <v>607</v>
       </c>
     </row>
     <row r="163">
       <c s="11" r="A163"/>
       <c t="s" s="7" r="B163">
+        <v>606</v>
+      </c>
+      <c t="s" s="7" r="C163">
+        <v>607</v>
+      </c>
+      <c t="s" s="7" r="D163">
         <v>608</v>
       </c>
-      <c t="s" s="7" r="C163">
+      <c t="s" s="7" r="E163">
         <v>609</v>
-      </c>
-      <c t="s" s="7" r="D163">
-        <v>610</v>
-      </c>
-      <c t="s" s="7" r="E163">
-        <v>611</v>
       </c>
     </row>
     <row r="164">
       <c s="11" r="A164"/>
       <c t="s" s="7" r="B164">
+        <v>610</v>
+      </c>
+      <c t="s" s="7" r="C164">
+        <v>611</v>
+      </c>
+      <c t="s" s="7" r="D164">
         <v>612</v>
       </c>
-      <c t="s" s="7" r="C164">
+      <c t="s" s="7" r="E164">
         <v>613</v>
-      </c>
-      <c t="s" s="7" r="D164">
-        <v>614</v>
-      </c>
-      <c t="s" s="7" r="E164">
-        <v>615</v>
       </c>
     </row>
     <row r="165">
       <c s="11" r="A165"/>
       <c t="s" s="7" r="B165">
+        <v>614</v>
+      </c>
+      <c t="s" s="7" r="C165">
+        <v>615</v>
+      </c>
+      <c t="s" s="7" r="D165">
         <v>616</v>
       </c>
-      <c t="s" s="7" r="C165">
+      <c t="s" s="7" r="E165">
         <v>617</v>
-      </c>
-      <c t="s" s="7" r="D165">
-        <v>618</v>
-      </c>
-      <c t="s" s="7" r="E165">
-        <v>619</v>
       </c>
     </row>
     <row r="166">
       <c s="11" r="A166"/>
       <c t="s" s="7" r="B166">
+        <v>618</v>
+      </c>
+      <c t="s" s="7" r="C166">
+        <v>619</v>
+      </c>
+      <c t="s" s="7" r="D166">
         <v>620</v>
       </c>
-      <c t="s" s="7" r="C166">
+      <c t="s" s="7" r="E166">
         <v>621</v>
-      </c>
-      <c t="s" s="7" r="D166">
-        <v>622</v>
-      </c>
-      <c t="s" s="7" r="E166">
-        <v>623</v>
       </c>
     </row>
     <row r="167">
       <c s="11" r="A167"/>
       <c t="s" s="7" r="B167">
+        <v>622</v>
+      </c>
+      <c t="s" s="7" r="C167">
+        <v>623</v>
+      </c>
+      <c t="s" s="7" r="D167">
         <v>624</v>
       </c>
-      <c t="s" s="7" r="C167">
+      <c t="s" s="7" r="E167">
         <v>625</v>
-      </c>
-      <c t="s" s="7" r="D167">
-        <v>626</v>
-      </c>
-      <c t="s" s="7" r="E167">
-        <v>627</v>
       </c>
     </row>
     <row r="168">
       <c s="11" r="A168"/>
       <c t="s" s="7" r="B168">
+        <v>626</v>
+      </c>
+      <c t="s" s="7" r="C168">
+        <v>627</v>
+      </c>
+      <c t="s" s="7" r="D168">
         <v>628</v>
       </c>
-      <c t="s" s="14" r="C168">
+      <c t="s" s="7" r="E168">
         <v>629</v>
-      </c>
-      <c t="s" s="7" r="D168">
-        <v>630</v>
-      </c>
-      <c t="s" s="7" r="E168">
-        <v>631</v>
       </c>
     </row>
     <row r="169">
       <c s="11" r="A169"/>
-      <c t="s" s="14" r="B169">
+      <c t="s" s="7" r="B169">
+        <v>630</v>
+      </c>
+      <c t="s" s="14" r="C169">
+        <v>631</v>
+      </c>
+      <c t="s" s="7" r="D169">
         <v>632</v>
       </c>
-      <c t="s" s="14" r="C169">
+      <c t="s" s="7" r="E169">
         <v>633</v>
-      </c>
-      <c t="s" s="7" r="D169">
-        <v>634</v>
-      </c>
-      <c t="s" s="7" r="E169">
-        <v>635</v>
       </c>
     </row>
     <row r="170">
       <c s="11" r="A170"/>
-      <c t="s" s="7" r="B170">
+      <c t="s" s="14" r="B170">
+        <v>634</v>
+      </c>
+      <c t="s" s="14" r="C170">
+        <v>635</v>
+      </c>
+      <c t="s" s="7" r="D170">
         <v>636</v>
       </c>
-      <c t="s" s="14" r="C170">
-        <v>633</v>
-      </c>
-      <c t="s" s="7" r="D170">
-        <v>634</v>
-      </c>
       <c t="s" s="7" r="E170">
-        <v>635</v>
+        <v>637</v>
       </c>
     </row>
     <row r="171">
       <c s="11" r="A171"/>
       <c t="s" s="7" r="B171">
+        <v>638</v>
+      </c>
+      <c t="s" s="14" r="C171">
+        <v>635</v>
+      </c>
+      <c t="s" s="7" r="D171">
+        <v>636</v>
+      </c>
+      <c t="s" s="7" r="E171">
         <v>637</v>
-      </c>
-      <c t="s" s="3" r="C171">
-        <v>638</v>
-      </c>
-      <c t="s" s="7" r="D171">
-        <v>639</v>
-      </c>
-      <c t="s" s="7" r="E171">
-        <v>640</v>
       </c>
     </row>
     <row r="172">
       <c s="11" r="A172"/>
       <c t="s" s="7" r="B172">
+        <v>639</v>
+      </c>
+      <c t="s" s="3" r="C172">
+        <v>640</v>
+      </c>
+      <c t="s" s="7" r="D172">
         <v>641</v>
       </c>
-      <c t="s" s="3" r="C172">
+      <c t="s" s="7" r="E172">
         <v>642</v>
-      </c>
-      <c t="s" s="7" r="D172">
-        <v>643</v>
-      </c>
-      <c t="s" s="7" r="E172">
-        <v>644</v>
       </c>
     </row>
     <row r="173">
       <c s="11" r="A173"/>
       <c t="s" s="7" r="B173">
+        <v>643</v>
+      </c>
+      <c t="s" s="3" r="C173">
+        <v>644</v>
+      </c>
+      <c t="s" s="7" r="D173">
         <v>645</v>
       </c>
-      <c t="s" s="3" r="C173">
+      <c t="s" s="7" r="E173">
         <v>646</v>
-      </c>
-      <c t="s" s="7" r="D173">
-        <v>647</v>
-      </c>
-      <c t="s" s="3" r="E173">
-        <v>648</v>
       </c>
     </row>
     <row r="174">
       <c s="11" r="A174"/>
-      <c s="17" r="B174"/>
-      <c s="9" r="C174"/>
-      <c s="17" r="D174"/>
-      <c s="17" r="E174"/>
+      <c t="s" s="7" r="B174">
+        <v>647</v>
+      </c>
+      <c t="s" s="3" r="C174">
+        <v>648</v>
+      </c>
+      <c t="s" s="7" r="D174">
+        <v>649</v>
+      </c>
+      <c t="s" s="3" r="E174">
+        <v>650</v>
+      </c>
     </row>
     <row r="175">
-      <c t="s" s="11" r="A175">
-        <v>649</v>
-      </c>
-      <c t="s" s="7" r="B175">
-        <v>650</v>
-      </c>
-      <c t="s" s="14" r="C175">
+      <c s="11" r="A175"/>
+      <c s="17" r="B175"/>
+      <c s="9" r="C175"/>
+      <c s="17" r="D175"/>
+      <c s="17" r="E175"/>
+    </row>
+    <row r="176">
+      <c t="s" s="11" r="A176">
         <v>651</v>
       </c>
-      <c t="s" s="7" r="D175">
-        <v>289</v>
-      </c>
-      <c t="s" s="7" r="E175">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="176">
-      <c s="11" r="A176"/>
-      <c t="s" s="22" r="B176">
+      <c t="s" s="7" r="B176">
         <v>652</v>
       </c>
       <c t="s" s="14" r="C176">
         <v>653</v>
       </c>
-      <c t="s" s="22" r="D176">
-        <v>654</v>
-      </c>
-      <c t="s" s="22" r="E176">
-        <v>655</v>
+      <c t="s" s="7" r="D176">
+        <v>289</v>
+      </c>
+      <c t="s" s="7" r="E176">
+        <v>290</v>
       </c>
     </row>
     <row r="177">
       <c s="11" r="A177"/>
-      <c t="s" s="7" r="B177">
+      <c t="s" s="22" r="B177">
+        <v>654</v>
+      </c>
+      <c t="s" s="14" r="C177">
+        <v>655</v>
+      </c>
+      <c t="s" s="22" r="D177">
         <v>656</v>
       </c>
-      <c t="s" s="14" r="C177">
+      <c t="s" s="22" r="E177">
         <v>657</v>
-      </c>
-      <c t="s" s="7" r="D177">
-        <v>658</v>
-      </c>
-      <c t="s" s="7" r="E177">
-        <v>659</v>
       </c>
     </row>
     <row r="178">
       <c s="11" r="A178"/>
       <c t="s" s="7" r="B178">
+        <v>658</v>
+      </c>
+      <c t="s" s="14" r="C178">
+        <v>659</v>
+      </c>
+      <c t="s" s="7" r="D178">
         <v>660</v>
       </c>
-      <c t="s" s="14" r="C178">
+      <c t="s" s="7" r="E178">
         <v>661</v>
       </c>
-      <c t="s" s="7" r="D178">
+    </row>
+    <row r="179">
+      <c s="11" r="A179"/>
+      <c t="s" s="7" r="B179">
         <v>662</v>
       </c>
-      <c t="s" s="7" r="E178">
+      <c t="s" s="14" r="C179">
         <v>663</v>
       </c>
-    </row>
-    <row r="179">
-      <c s="18" r="A179"/>
-      <c t="s" s="7" r="B179">
+      <c t="s" s="7" r="D179">
         <v>664</v>
       </c>
-      <c t="s" s="14" r="C179">
+      <c t="s" s="7" r="E179">
         <v>665</v>
       </c>
-      <c t="s" s="7" r="D179">
+    </row>
+    <row r="180">
+      <c s="18" r="A180"/>
+      <c t="s" s="7" r="B180">
         <v>666</v>
       </c>
-      <c t="s" s="7" r="E179">
+      <c t="s" s="14" r="C180">
         <v>667</v>
       </c>
-    </row>
-    <row r="180">
-      <c s="11" r="A180"/>
-      <c t="s" s="7" r="B180">
+      <c t="s" s="7" r="D180">
         <v>668</v>
       </c>
-      <c t="s" s="14" r="C180">
+      <c t="s" s="7" r="E180">
         <v>669</v>
-      </c>
-      <c t="s" s="7" r="D180">
-        <v>670</v>
-      </c>
-      <c t="s" s="7" r="E180">
-        <v>671</v>
       </c>
     </row>
     <row r="181">
       <c s="11" r="A181"/>
       <c t="s" s="7" r="B181">
+        <v>670</v>
+      </c>
+      <c t="s" s="14" r="C181">
+        <v>671</v>
+      </c>
+      <c t="s" s="7" r="D181">
         <v>672</v>
       </c>
-      <c t="s" s="14" r="C181">
+      <c t="s" s="7" r="E181">
         <v>673</v>
-      </c>
-      <c t="s" s="7" r="D181">
-        <v>674</v>
-      </c>
-      <c t="s" s="7" r="E181">
-        <v>675</v>
       </c>
     </row>
     <row r="182">
       <c s="11" r="A182"/>
       <c t="s" s="7" r="B182">
+        <v>674</v>
+      </c>
+      <c t="s" s="14" r="C182">
+        <v>675</v>
+      </c>
+      <c t="s" s="7" r="D182">
         <v>676</v>
       </c>
-      <c t="s" s="14" r="C182">
+      <c t="s" s="7" r="E182">
         <v>677</v>
-      </c>
-      <c t="s" s="7" r="D182">
-        <v>678</v>
-      </c>
-      <c t="s" s="7" r="E182">
-        <v>679</v>
       </c>
     </row>
     <row r="183">
       <c s="11" r="A183"/>
       <c t="s" s="7" r="B183">
+        <v>678</v>
+      </c>
+      <c t="s" s="14" r="C183">
+        <v>679</v>
+      </c>
+      <c t="s" s="7" r="D183">
         <v>680</v>
       </c>
-      <c t="s" s="14" r="C183">
+      <c t="s" s="7" r="E183">
         <v>681</v>
-      </c>
-      <c t="s" s="7" r="D183">
-        <v>682</v>
-      </c>
-      <c t="s" s="7" r="E183">
-        <v>683</v>
       </c>
     </row>
     <row r="184">
       <c s="11" r="A184"/>
       <c t="s" s="7" r="B184">
+        <v>682</v>
+      </c>
+      <c t="s" s="14" r="C184">
+        <v>683</v>
+      </c>
+      <c t="s" s="7" r="D184">
         <v>684</v>
       </c>
-      <c t="s" s="14" r="C184">
+      <c t="s" s="7" r="E184">
         <v>685</v>
-      </c>
-      <c t="s" s="7" r="D184">
-        <v>686</v>
-      </c>
-      <c t="s" s="7" r="E184">
-        <v>687</v>
       </c>
     </row>
     <row r="185">
       <c s="11" r="A185"/>
       <c t="s" s="7" r="B185">
+        <v>686</v>
+      </c>
+      <c t="s" s="14" r="C185">
+        <v>687</v>
+      </c>
+      <c t="s" s="7" r="D185">
         <v>688</v>
       </c>
-      <c t="s" s="14" r="C185">
+      <c t="s" s="7" r="E185">
         <v>689</v>
-      </c>
-      <c t="s" s="7" r="D185">
-        <v>690</v>
-      </c>
-      <c t="s" s="7" r="E185">
-        <v>691</v>
       </c>
     </row>
     <row r="186">
       <c s="11" r="A186"/>
       <c t="s" s="7" r="B186">
+        <v>690</v>
+      </c>
+      <c t="s" s="14" r="C186">
+        <v>691</v>
+      </c>
+      <c t="s" s="7" r="D186">
         <v>692</v>
       </c>
-      <c t="s" s="14" r="C186">
+      <c t="s" s="7" r="E186">
         <v>693</v>
-      </c>
-      <c t="s" s="7" r="D186">
-        <v>694</v>
-      </c>
-      <c t="s" s="7" r="E186">
-        <v>695</v>
       </c>
     </row>
     <row r="187">
       <c s="11" r="A187"/>
       <c t="s" s="7" r="B187">
+        <v>694</v>
+      </c>
+      <c t="s" s="14" r="C187">
+        <v>695</v>
+      </c>
+      <c t="s" s="7" r="D187">
         <v>696</v>
       </c>
-      <c t="s" s="14" r="C187">
+      <c t="s" s="7" r="E187">
         <v>697</v>
-      </c>
-      <c t="s" s="7" r="D187">
-        <v>698</v>
-      </c>
-      <c t="s" s="7" r="E187">
-        <v>699</v>
       </c>
     </row>
     <row r="188">
       <c s="11" r="A188"/>
-      <c s="20" r="B188"/>
-      <c s="31" r="C188"/>
-      <c s="20" r="D188"/>
-      <c s="20" r="E188"/>
+      <c t="s" s="7" r="B188">
+        <v>698</v>
+      </c>
+      <c t="s" s="14" r="C188">
+        <v>699</v>
+      </c>
+      <c t="s" s="7" r="D188">
+        <v>700</v>
+      </c>
+      <c t="s" s="7" r="E188">
+        <v>701</v>
+      </c>
     </row>
     <row r="189">
-      <c t="s" s="11" r="A189">
-        <v>700</v>
-      </c>
-      <c t="s" s="7" r="B189">
-        <v>701</v>
-      </c>
-      <c t="s" s="14" r="C189">
+      <c s="11" r="A189"/>
+      <c s="20" r="B189"/>
+      <c s="31" r="C189"/>
+      <c s="20" r="D189"/>
+      <c s="20" r="E189"/>
+    </row>
+    <row r="190">
+      <c t="s" s="11" r="A190">
         <v>702</v>
       </c>
-      <c t="s" s="7" r="D189">
+      <c t="s" s="7" r="B190">
         <v>703</v>
       </c>
-      <c t="s" s="7" r="E189">
+      <c t="s" s="14" r="C190">
         <v>704</v>
       </c>
-    </row>
-    <row r="190">
-      <c s="11" r="A190"/>
-      <c t="s" s="7" r="B190">
+      <c t="s" s="7" r="D190">
         <v>705</v>
       </c>
-      <c t="s" s="14" r="C190">
+      <c t="s" s="7" r="E190">
         <v>706</v>
-      </c>
-      <c t="s" s="7" r="D190">
-        <v>707</v>
-      </c>
-      <c t="s" s="7" r="E190">
-        <v>708</v>
       </c>
     </row>
     <row r="191">
       <c s="11" r="A191"/>
       <c t="s" s="7" r="B191">
+        <v>707</v>
+      </c>
+      <c t="s" s="14" r="C191">
+        <v>708</v>
+      </c>
+      <c t="s" s="7" r="D191">
         <v>709</v>
       </c>
-      <c t="s" s="14" r="C191">
+      <c t="s" s="7" r="E191">
         <v>710</v>
-      </c>
-      <c t="s" s="7" r="D191">
-        <v>711</v>
-      </c>
-      <c t="s" s="7" r="E191">
-        <v>712</v>
       </c>
     </row>
     <row r="192">
       <c s="11" r="A192"/>
       <c t="s" s="7" r="B192">
+        <v>711</v>
+      </c>
+      <c t="s" s="14" r="C192">
+        <v>712</v>
+      </c>
+      <c t="s" s="7" r="D192">
         <v>713</v>
       </c>
-      <c t="s" s="14" r="C192">
+      <c t="s" s="7" r="E192">
         <v>714</v>
-      </c>
-      <c t="s" s="7" r="D192">
-        <v>715</v>
-      </c>
-      <c t="s" s="7" r="E192">
-        <v>716</v>
       </c>
     </row>
     <row r="193">
       <c s="11" r="A193"/>
       <c t="s" s="7" r="B193">
+        <v>715</v>
+      </c>
+      <c t="s" s="14" r="C193">
+        <v>716</v>
+      </c>
+      <c t="s" s="7" r="D193">
         <v>717</v>
       </c>
-      <c t="s" s="14" r="C193">
+      <c t="s" s="7" r="E193">
         <v>718</v>
-      </c>
-      <c t="s" s="7" r="D193">
-        <v>719</v>
-      </c>
-      <c t="s" s="7" r="E193">
-        <v>720</v>
       </c>
     </row>
     <row r="194">
       <c s="11" r="A194"/>
       <c t="s" s="7" r="B194">
+        <v>719</v>
+      </c>
+      <c t="s" s="14" r="C194">
+        <v>720</v>
+      </c>
+      <c t="s" s="7" r="D194">
         <v>721</v>
       </c>
-      <c t="s" s="14" r="C194">
+      <c t="s" s="7" r="E194">
         <v>722</v>
-      </c>
-      <c t="s" s="7" r="D194">
-        <v>723</v>
-      </c>
-      <c t="s" s="7" r="E194">
-        <v>724</v>
       </c>
     </row>
     <row r="195">
       <c s="11" r="A195"/>
       <c t="s" s="7" r="B195">
+        <v>723</v>
+      </c>
+      <c t="s" s="14" r="C195">
+        <v>724</v>
+      </c>
+      <c t="s" s="7" r="D195">
         <v>725</v>
       </c>
-      <c t="s" s="14" r="C195">
+      <c t="s" s="7" r="E195">
         <v>726</v>
-      </c>
-      <c t="s" s="7" r="D195">
-        <v>727</v>
-      </c>
-      <c t="s" s="7" r="E195">
-        <v>728</v>
       </c>
     </row>
     <row r="196">
       <c s="11" r="A196"/>
-      <c s="20" r="B196"/>
-      <c s="31" r="C196"/>
-      <c s="20" r="D196"/>
-      <c s="20" r="E196"/>
+      <c t="s" s="7" r="B196">
+        <v>727</v>
+      </c>
+      <c t="s" s="14" r="C196">
+        <v>728</v>
+      </c>
+      <c t="s" s="7" r="D196">
+        <v>729</v>
+      </c>
+      <c t="s" s="7" r="E196">
+        <v>730</v>
+      </c>
     </row>
     <row r="197">
-      <c t="s" s="11" r="A197">
-        <v>729</v>
-      </c>
-      <c t="s" s="30" r="B197">
-        <v>730</v>
-      </c>
-      <c t="s" s="21" r="C197">
-        <v>729</v>
-      </c>
-      <c s="30" r="D197"/>
-      <c s="30" r="E197"/>
+      <c s="11" r="A197"/>
+      <c s="20" r="B197"/>
+      <c s="31" r="C197"/>
+      <c s="20" r="D197"/>
+      <c s="20" r="E197"/>
     </row>
     <row r="198">
-      <c s="11" r="A198"/>
-      <c s="17" r="B198"/>
-      <c s="9" r="C198"/>
-      <c s="17" r="D198"/>
-      <c s="17" r="E198"/>
+      <c t="s" s="11" r="A198">
+        <v>731</v>
+      </c>
+      <c t="s" s="30" r="B198">
+        <v>732</v>
+      </c>
+      <c t="s" s="21" r="C198">
+        <v>731</v>
+      </c>
+      <c s="30" r="D198"/>
+      <c s="30" r="E198"/>
     </row>
     <row r="199">
-      <c t="s" s="11" r="A199">
-        <v>731</v>
-      </c>
-      <c t="s" s="36" r="B199">
-        <v>732</v>
-      </c>
-      <c t="s" s="34" r="C199">
+      <c s="11" r="A199"/>
+      <c s="17" r="B199"/>
+      <c s="9" r="C199"/>
+      <c s="17" r="D199"/>
+      <c s="17" r="E199"/>
+    </row>
+    <row r="200">
+      <c t="s" s="11" r="A200">
         <v>733</v>
       </c>
-      <c s="36" r="D199"/>
-      <c s="36" r="E199"/>
-    </row>
-    <row r="200">
-      <c s="11" r="A200"/>
       <c t="s" s="36" r="B200">
         <v>734</v>
       </c>
@@ -6978,1115 +6984,1111 @@
     </row>
     <row r="201">
       <c s="11" r="A201"/>
-      <c s="9" r="B201"/>
-      <c s="9" r="C201"/>
-      <c s="17" r="D201"/>
-      <c s="17" r="E201"/>
+      <c t="s" s="36" r="B201">
+        <v>736</v>
+      </c>
+      <c t="s" s="34" r="C201">
+        <v>737</v>
+      </c>
+      <c s="36" r="D201"/>
+      <c s="36" r="E201"/>
     </row>
     <row r="202">
-      <c t="s" s="11" r="A202">
-        <v>736</v>
-      </c>
-      <c t="s" s="28" r="B202">
-        <v>737</v>
-      </c>
-      <c t="s" s="28" r="C202">
+      <c s="11" r="A202"/>
+      <c s="9" r="B202"/>
+      <c s="9" r="C202"/>
+      <c s="17" r="D202"/>
+      <c s="17" r="E202"/>
+    </row>
+    <row r="203">
+      <c t="s" s="11" r="A203">
         <v>738</v>
       </c>
-      <c t="s" s="7" r="D202">
+      <c t="s" s="28" r="B203">
         <v>739</v>
       </c>
-      <c t="s" s="7" r="E202">
+      <c t="s" s="28" r="C203">
         <v>740</v>
       </c>
-    </row>
-    <row r="203">
-      <c s="11" r="A203"/>
-      <c t="s" s="28" r="B203">
+      <c t="s" s="7" r="D203">
         <v>741</v>
       </c>
-      <c t="s" s="28" r="C203">
+      <c t="s" s="7" r="E203">
         <v>742</v>
-      </c>
-      <c t="s" s="7" r="D203">
-        <v>742</v>
-      </c>
-      <c t="s" s="7" r="E203">
-        <v>743</v>
       </c>
     </row>
     <row r="204">
       <c s="11" r="A204"/>
       <c t="s" s="28" r="B204">
+        <v>743</v>
+      </c>
+      <c t="s" s="28" r="C204">
         <v>744</v>
       </c>
-      <c t="s" s="28" r="C204">
+      <c t="s" s="7" r="D204">
+        <v>744</v>
+      </c>
+      <c t="s" s="7" r="E204">
         <v>745</v>
-      </c>
-      <c t="s" s="7" r="D204">
-        <v>746</v>
-      </c>
-      <c t="s" s="7" r="E204">
-        <v>747</v>
       </c>
     </row>
     <row r="205">
       <c s="11" r="A205"/>
       <c t="s" s="28" r="B205">
+        <v>746</v>
+      </c>
+      <c t="s" s="28" r="C205">
+        <v>747</v>
+      </c>
+      <c t="s" s="7" r="D205">
         <v>748</v>
       </c>
-      <c t="s" s="28" r="C205">
+      <c t="s" s="7" r="E205">
         <v>749</v>
-      </c>
-      <c t="s" s="7" r="D205">
-        <v>750</v>
-      </c>
-      <c t="s" s="7" r="E205">
-        <v>751</v>
       </c>
     </row>
     <row r="206">
       <c s="11" r="A206"/>
-      <c t="s" s="14" r="B206">
+      <c t="s" s="28" r="B206">
+        <v>750</v>
+      </c>
+      <c t="s" s="28" r="C206">
+        <v>751</v>
+      </c>
+      <c t="s" s="7" r="D206">
         <v>752</v>
       </c>
-      <c t="s" s="14" r="C206">
+      <c t="s" s="7" r="E206">
         <v>753</v>
-      </c>
-      <c t="s" s="7" r="D206">
-        <v>754</v>
-      </c>
-      <c t="s" s="7" r="E206">
-        <v>755</v>
       </c>
     </row>
     <row r="207">
       <c s="11" r="A207"/>
       <c t="s" s="14" r="B207">
+        <v>754</v>
+      </c>
+      <c t="s" s="14" r="C207">
+        <v>755</v>
+      </c>
+      <c t="s" s="7" r="D207">
         <v>756</v>
       </c>
-      <c t="s" s="14" r="C207">
+      <c t="s" s="7" r="E207">
         <v>757</v>
-      </c>
-      <c t="s" s="7" r="D207">
-        <v>758</v>
-      </c>
-      <c t="s" s="7" r="E207">
-        <v>759</v>
       </c>
     </row>
     <row r="208">
       <c s="11" r="A208"/>
       <c t="s" s="14" r="B208">
+        <v>758</v>
+      </c>
+      <c t="s" s="14" r="C208">
+        <v>759</v>
+      </c>
+      <c t="s" s="7" r="D208">
         <v>760</v>
       </c>
-      <c t="s" s="14" r="C208">
+      <c t="s" s="7" r="E208">
         <v>761</v>
-      </c>
-      <c t="s" s="7" r="D208">
-        <v>762</v>
-      </c>
-      <c t="s" s="7" r="E208">
-        <v>763</v>
       </c>
     </row>
     <row r="209">
       <c s="11" r="A209"/>
       <c t="s" s="14" r="B209">
+        <v>762</v>
+      </c>
+      <c t="s" s="14" r="C209">
+        <v>763</v>
+      </c>
+      <c t="s" s="7" r="D209">
         <v>764</v>
       </c>
-      <c t="s" s="14" r="C209">
+      <c t="s" s="7" r="E209">
         <v>765</v>
-      </c>
-      <c t="s" s="7" r="D209">
-        <v>766</v>
-      </c>
-      <c t="s" s="7" r="E209">
-        <v>767</v>
       </c>
     </row>
     <row r="210">
       <c s="11" r="A210"/>
       <c t="s" s="14" r="B210">
+        <v>766</v>
+      </c>
+      <c t="s" s="14" r="C210">
+        <v>767</v>
+      </c>
+      <c t="s" s="7" r="D210">
         <v>768</v>
       </c>
-      <c t="s" s="14" r="C210">
+      <c t="s" s="7" r="E210">
         <v>769</v>
-      </c>
-      <c t="s" s="7" r="D210">
-        <v>770</v>
-      </c>
-      <c t="s" s="7" r="E210">
-        <v>771</v>
       </c>
     </row>
     <row r="211">
       <c s="11" r="A211"/>
-      <c s="11" r="B211"/>
-      <c s="11" r="C211"/>
-      <c s="11" r="D211"/>
-      <c s="11" r="E211"/>
+      <c t="s" s="14" r="B211">
+        <v>770</v>
+      </c>
+      <c t="s" s="14" r="C211">
+        <v>771</v>
+      </c>
+      <c t="s" s="7" r="D211">
+        <v>772</v>
+      </c>
+      <c t="s" s="7" r="E211">
+        <v>773</v>
+      </c>
     </row>
     <row r="212">
       <c s="11" r="A212"/>
-      <c t="s" s="14" r="B212">
-        <v>772</v>
-      </c>
-      <c t="s" s="14" r="C212">
-        <v>773</v>
-      </c>
-      <c t="s" s="7" r="D212">
-        <v>774</v>
-      </c>
-      <c t="s" s="7" r="E212">
-        <v>775</v>
-      </c>
+      <c s="11" r="B212"/>
+      <c s="11" r="C212"/>
+      <c s="11" r="D212"/>
+      <c s="11" r="E212"/>
     </row>
     <row r="213">
       <c s="11" r="A213"/>
-      <c t="s" s="7" r="B213">
+      <c t="s" s="14" r="B213">
+        <v>774</v>
+      </c>
+      <c t="s" s="14" r="C213">
+        <v>775</v>
+      </c>
+      <c t="s" s="7" r="D213">
         <v>776</v>
       </c>
-      <c t="s" s="14" r="C213">
+      <c t="s" s="7" r="E213">
         <v>777</v>
-      </c>
-      <c t="s" s="7" r="D213">
-        <v>778</v>
-      </c>
-      <c t="s" s="7" r="E213">
-        <v>779</v>
       </c>
     </row>
     <row r="214">
       <c s="11" r="A214"/>
       <c t="s" s="7" r="B214">
+        <v>778</v>
+      </c>
+      <c t="s" s="14" r="C214">
+        <v>779</v>
+      </c>
+      <c t="s" s="7" r="D214">
         <v>780</v>
       </c>
-      <c t="s" s="14" r="C214">
+      <c t="s" s="7" r="E214">
         <v>781</v>
-      </c>
-      <c t="s" s="7" r="D214">
-        <v>782</v>
-      </c>
-      <c t="s" s="7" r="E214">
-        <v>783</v>
       </c>
     </row>
     <row r="215">
       <c s="11" r="A215"/>
       <c t="s" s="7" r="B215">
+        <v>782</v>
+      </c>
+      <c t="s" s="14" r="C215">
+        <v>783</v>
+      </c>
+      <c t="s" s="7" r="D215">
         <v>784</v>
       </c>
-      <c t="s" s="14" r="C215">
+      <c t="s" s="7" r="E215">
         <v>785</v>
-      </c>
-      <c t="s" s="7" r="D215">
-        <v>786</v>
-      </c>
-      <c t="s" s="7" r="E215">
-        <v>787</v>
       </c>
     </row>
     <row r="216">
       <c s="11" r="A216"/>
       <c t="s" s="7" r="B216">
+        <v>786</v>
+      </c>
+      <c t="s" s="14" r="C216">
+        <v>787</v>
+      </c>
+      <c t="s" s="7" r="D216">
         <v>788</v>
       </c>
-      <c t="s" s="14" r="C216">
+      <c t="s" s="7" r="E216">
         <v>789</v>
-      </c>
-      <c t="s" s="7" r="D216">
-        <v>790</v>
-      </c>
-      <c t="s" s="7" r="E216">
-        <v>791</v>
       </c>
     </row>
     <row r="217">
       <c s="11" r="A217"/>
       <c t="s" s="7" r="B217">
+        <v>790</v>
+      </c>
+      <c t="s" s="14" r="C217">
+        <v>791</v>
+      </c>
+      <c t="s" s="7" r="D217">
         <v>792</v>
       </c>
-      <c t="s" s="14" r="C217">
+      <c t="s" s="7" r="E217">
         <v>793</v>
-      </c>
-      <c t="s" s="26" r="D217">
-        <v>794</v>
-      </c>
-      <c t="s" s="26" r="E217">
-        <v>795</v>
       </c>
     </row>
     <row r="218">
       <c s="11" r="A218"/>
       <c t="s" s="7" r="B218">
+        <v>794</v>
+      </c>
+      <c t="s" s="14" r="C218">
+        <v>795</v>
+      </c>
+      <c t="s" s="26" r="D218">
         <v>796</v>
       </c>
-      <c t="s" s="14" r="C218">
+      <c t="s" s="26" r="E218">
         <v>797</v>
-      </c>
-      <c t="s" s="7" r="D218">
-        <v>798</v>
-      </c>
-      <c t="s" s="7" r="E218">
-        <v>799</v>
       </c>
     </row>
     <row r="219">
       <c s="11" r="A219"/>
       <c t="s" s="7" r="B219">
+        <v>798</v>
+      </c>
+      <c t="s" s="14" r="C219">
+        <v>799</v>
+      </c>
+      <c t="s" s="7" r="D219">
         <v>800</v>
       </c>
-      <c t="s" s="14" r="C219">
+      <c t="s" s="7" r="E219">
         <v>801</v>
-      </c>
-      <c t="s" s="7" r="D219">
-        <v>802</v>
-      </c>
-      <c t="s" s="7" r="E219">
-        <v>803</v>
       </c>
     </row>
     <row r="220">
       <c s="11" r="A220"/>
       <c t="s" s="7" r="B220">
+        <v>802</v>
+      </c>
+      <c t="s" s="14" r="C220">
+        <v>803</v>
+      </c>
+      <c t="s" s="7" r="D220">
         <v>804</v>
       </c>
-      <c t="s" s="14" r="C220">
+      <c t="s" s="7" r="E220">
         <v>805</v>
-      </c>
-      <c t="s" s="7" r="D220">
-        <v>806</v>
-      </c>
-      <c t="s" s="7" r="E220">
-        <v>807</v>
       </c>
     </row>
     <row r="221">
       <c s="11" r="A221"/>
       <c t="s" s="7" r="B221">
+        <v>806</v>
+      </c>
+      <c t="s" s="14" r="C221">
+        <v>807</v>
+      </c>
+      <c t="s" s="7" r="D221">
         <v>808</v>
       </c>
-      <c t="s" s="14" r="C221">
+      <c t="s" s="7" r="E221">
         <v>809</v>
-      </c>
-      <c t="s" s="7" r="D221">
-        <v>810</v>
-      </c>
-      <c t="s" s="7" r="E221">
-        <v>811</v>
       </c>
     </row>
     <row r="222">
       <c s="11" r="A222"/>
       <c t="s" s="7" r="B222">
+        <v>810</v>
+      </c>
+      <c t="s" s="14" r="C222">
+        <v>811</v>
+      </c>
+      <c t="s" s="7" r="D222">
         <v>812</v>
       </c>
-      <c t="s" s="14" r="C222">
+      <c t="s" s="7" r="E222">
         <v>813</v>
-      </c>
-      <c t="s" s="7" r="D222">
-        <v>814</v>
-      </c>
-      <c t="s" s="7" r="E222">
-        <v>815</v>
       </c>
     </row>
     <row r="223">
       <c s="11" r="A223"/>
-      <c s="17" r="B223"/>
-      <c s="31" r="C223"/>
-      <c s="17" r="D223"/>
-      <c s="17" r="E223"/>
+      <c t="s" s="7" r="B223">
+        <v>814</v>
+      </c>
+      <c t="s" s="14" r="C223">
+        <v>815</v>
+      </c>
+      <c t="s" s="7" r="D223">
+        <v>816</v>
+      </c>
+      <c t="s" s="7" r="E223">
+        <v>817</v>
+      </c>
     </row>
     <row r="224">
-      <c t="s" s="11" r="A224">
-        <v>816</v>
-      </c>
-      <c t="s" s="28" r="B224">
-        <v>817</v>
-      </c>
-      <c t="s" s="7" r="C224">
-        <v>742</v>
-      </c>
-      <c t="s" s="7" r="D224">
-        <v>742</v>
-      </c>
-      <c t="s" s="7" r="E224">
-        <v>743</v>
-      </c>
+      <c s="11" r="A224"/>
+      <c s="17" r="B224"/>
+      <c s="31" r="C224"/>
+      <c s="17" r="D224"/>
+      <c s="17" r="E224"/>
     </row>
     <row r="225">
-      <c s="11" r="A225"/>
-      <c t="s" s="7" r="B225">
+      <c t="s" s="11" r="A225">
         <v>818</v>
       </c>
-      <c t="s" s="14" r="C225">
+      <c t="s" s="28" r="B225">
+        <v>819</v>
+      </c>
+      <c t="s" s="7" r="C225">
+        <v>744</v>
+      </c>
+      <c t="s" s="7" r="D225">
+        <v>744</v>
+      </c>
+      <c t="s" s="7" r="E225">
         <v>745</v>
       </c>
-      <c t="s" s="7" r="D225">
-        <v>746</v>
-      </c>
-      <c t="s" s="7" r="E225">
+    </row>
+    <row r="226">
+      <c s="11" r="A226"/>
+      <c t="s" s="7" r="B226">
+        <v>820</v>
+      </c>
+      <c t="s" s="14" r="C226">
         <v>747</v>
       </c>
-    </row>
-    <row r="226">
-      <c t="s" s="7" r="B226">
-        <v>819</v>
-      </c>
-      <c t="s" s="14" r="C226">
-        <v>820</v>
-      </c>
       <c t="s" s="7" r="D226">
+        <v>748</v>
+      </c>
+      <c t="s" s="7" r="E226">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="227">
+      <c t="s" s="7" r="B227">
         <v>821</v>
       </c>
-      <c t="s" s="7" r="E226">
+      <c t="s" s="14" r="C227">
         <v>822</v>
       </c>
-    </row>
-    <row r="227">
-      <c s="11" r="A227"/>
-      <c t="s" s="7" r="B227">
+      <c t="s" s="7" r="D227">
         <v>823</v>
       </c>
-      <c t="s" s="14" r="C227">
+      <c t="s" s="7" r="E227">
         <v>824</v>
-      </c>
-      <c t="s" s="7" r="D227">
-        <v>825</v>
-      </c>
-      <c t="s" s="7" r="E227">
-        <v>826</v>
       </c>
     </row>
     <row r="228">
       <c s="11" r="A228"/>
       <c t="s" s="7" r="B228">
+        <v>825</v>
+      </c>
+      <c t="s" s="14" r="C228">
+        <v>826</v>
+      </c>
+      <c t="s" s="7" r="D228">
         <v>827</v>
       </c>
-      <c t="s" s="14" r="C228">
+      <c t="s" s="7" r="E228">
         <v>828</v>
-      </c>
-      <c t="s" s="7" r="D228">
-        <v>829</v>
-      </c>
-      <c t="s" s="7" r="E228">
-        <v>830</v>
       </c>
     </row>
     <row r="229">
       <c s="11" r="A229"/>
-      <c s="12" r="B229"/>
-      <c s="15" r="C229"/>
-      <c s="17" r="D229"/>
-      <c s="17" r="E229"/>
+      <c t="s" s="7" r="B229">
+        <v>829</v>
+      </c>
+      <c t="s" s="14" r="C229">
+        <v>830</v>
+      </c>
+      <c t="s" s="7" r="D229">
+        <v>831</v>
+      </c>
+      <c t="s" s="7" r="E229">
+        <v>832</v>
+      </c>
     </row>
     <row r="230">
-      <c t="s" s="11" r="A230">
-        <v>831</v>
-      </c>
-      <c t="s" s="7" r="B230">
-        <v>832</v>
-      </c>
-      <c t="s" s="14" r="C230">
-        <v>831</v>
-      </c>
-      <c t="s" s="7" r="D230">
+      <c s="11" r="A230"/>
+      <c s="12" r="B230"/>
+      <c s="15" r="C230"/>
+      <c s="17" r="D230"/>
+      <c s="17" r="E230"/>
+    </row>
+    <row r="231">
+      <c t="s" s="11" r="A231">
         <v>833</v>
       </c>
-      <c t="s" s="7" r="E230">
+      <c t="s" s="7" r="B231">
         <v>834</v>
       </c>
-    </row>
-    <row r="231">
-      <c s="11" r="A231"/>
-      <c t="s" s="7" r="B231">
+      <c t="s" s="14" r="C231">
+        <v>833</v>
+      </c>
+      <c t="s" s="7" r="D231">
         <v>835</v>
       </c>
-      <c t="s" s="14" r="C231">
+      <c t="s" s="7" r="E231">
         <v>836</v>
-      </c>
-      <c t="s" s="7" r="D231">
-        <v>837</v>
-      </c>
-      <c t="s" s="7" r="E231">
-        <v>838</v>
       </c>
     </row>
     <row r="232">
       <c s="11" r="A232"/>
       <c t="s" s="7" r="B232">
+        <v>837</v>
+      </c>
+      <c t="s" s="14" r="C232">
+        <v>838</v>
+      </c>
+      <c t="s" s="7" r="D232">
         <v>839</v>
       </c>
-      <c t="s" s="14" r="C232">
+      <c t="s" s="7" r="E232">
         <v>840</v>
-      </c>
-      <c t="s" s="7" r="D232">
-        <v>841</v>
-      </c>
-      <c t="s" s="7" r="E232">
-        <v>842</v>
       </c>
     </row>
     <row r="233">
       <c s="11" r="A233"/>
       <c t="s" s="7" r="B233">
+        <v>841</v>
+      </c>
+      <c t="s" s="14" r="C233">
+        <v>842</v>
+      </c>
+      <c t="s" s="7" r="D233">
         <v>843</v>
       </c>
-      <c t="s" s="14" r="C233">
+      <c t="s" s="7" r="E233">
         <v>844</v>
-      </c>
-      <c t="s" s="7" r="D233">
-        <v>845</v>
-      </c>
-      <c t="s" s="7" r="E233">
-        <v>846</v>
       </c>
     </row>
     <row r="234">
       <c s="11" r="A234"/>
       <c t="s" s="7" r="B234">
+        <v>845</v>
+      </c>
+      <c t="s" s="14" r="C234">
+        <v>846</v>
+      </c>
+      <c t="s" s="7" r="D234">
         <v>847</v>
       </c>
-      <c t="s" s="14" r="C234">
+      <c t="s" s="7" r="E234">
         <v>848</v>
-      </c>
-      <c t="s" s="7" r="D234">
-        <v>849</v>
-      </c>
-      <c t="s" s="7" r="E234">
-        <v>850</v>
       </c>
     </row>
     <row r="235">
       <c s="11" r="A235"/>
       <c t="s" s="7" r="B235">
+        <v>849</v>
+      </c>
+      <c t="s" s="14" r="C235">
+        <v>850</v>
+      </c>
+      <c t="s" s="7" r="D235">
         <v>851</v>
       </c>
-      <c t="s" s="14" r="C235">
+      <c t="s" s="7" r="E235">
         <v>852</v>
-      </c>
-      <c t="s" s="7" r="D235">
-        <v>853</v>
-      </c>
-      <c t="s" s="7" r="E235">
-        <v>854</v>
       </c>
     </row>
     <row r="236">
       <c s="11" r="A236"/>
       <c t="s" s="7" r="B236">
+        <v>853</v>
+      </c>
+      <c t="s" s="14" r="C236">
+        <v>854</v>
+      </c>
+      <c t="s" s="7" r="D236">
         <v>855</v>
       </c>
-      <c t="s" s="14" r="C236">
+      <c t="s" s="7" r="E236">
         <v>856</v>
-      </c>
-      <c t="s" s="7" r="D236">
-        <v>857</v>
-      </c>
-      <c t="s" s="7" r="E236">
-        <v>858</v>
       </c>
     </row>
     <row r="237">
       <c s="11" r="A237"/>
-      <c s="12" r="B237"/>
-      <c s="15" r="C237"/>
-      <c s="12" r="D237"/>
-      <c s="12" r="E237"/>
+      <c t="s" s="7" r="B237">
+        <v>857</v>
+      </c>
+      <c t="s" s="14" r="C237">
+        <v>858</v>
+      </c>
+      <c t="s" s="7" r="D237">
+        <v>859</v>
+      </c>
+      <c t="s" s="7" r="E237">
+        <v>860</v>
+      </c>
     </row>
     <row r="238">
-      <c t="s" s="11" r="A238">
-        <v>859</v>
-      </c>
-      <c t="s" s="7" r="B238">
-        <v>860</v>
-      </c>
-      <c t="s" s="14" r="C238">
+      <c s="11" r="A238"/>
+      <c s="12" r="B238"/>
+      <c s="15" r="C238"/>
+      <c s="12" r="D238"/>
+      <c s="12" r="E238"/>
+    </row>
+    <row r="239">
+      <c t="s" s="11" r="A239">
         <v>861</v>
       </c>
-      <c t="s" s="7" r="D238">
+      <c t="s" s="7" r="B239">
         <v>862</v>
       </c>
-      <c t="s" s="7" r="E238">
+      <c t="s" s="14" r="C239">
         <v>863</v>
       </c>
-    </row>
-    <row r="239">
-      <c s="11" r="A239"/>
-      <c t="s" s="7" r="B239">
+      <c t="s" s="7" r="D239">
         <v>864</v>
       </c>
-      <c t="s" s="14" r="C239">
+      <c t="s" s="7" r="E239">
         <v>865</v>
-      </c>
-      <c t="s" s="7" r="D239">
-        <v>865</v>
-      </c>
-      <c t="s" s="7" r="E239">
-        <v>866</v>
       </c>
     </row>
     <row r="240">
       <c s="11" r="A240"/>
-      <c s="12" r="B240"/>
-      <c s="15" r="C240"/>
-      <c s="12" r="D240"/>
-      <c s="12" r="E240"/>
+      <c t="s" s="7" r="B240">
+        <v>866</v>
+      </c>
+      <c t="s" s="14" r="C240">
+        <v>867</v>
+      </c>
+      <c t="s" s="7" r="D240">
+        <v>867</v>
+      </c>
+      <c t="s" s="7" r="E240">
+        <v>868</v>
+      </c>
     </row>
     <row r="241">
-      <c t="s" s="11" r="A241">
-        <v>867</v>
-      </c>
-      <c t="s" s="7" r="B241">
-        <v>868</v>
-      </c>
-      <c t="s" s="14" r="C241">
+      <c s="11" r="A241"/>
+      <c s="12" r="B241"/>
+      <c s="15" r="C241"/>
+      <c s="12" r="D241"/>
+      <c s="12" r="E241"/>
+    </row>
+    <row r="242">
+      <c t="s" s="11" r="A242">
         <v>869</v>
       </c>
-      <c t="s" s="7" r="D241">
+      <c t="s" s="7" r="B242">
         <v>870</v>
       </c>
-      <c t="s" s="7" r="E241">
+      <c t="s" s="14" r="C242">
         <v>871</v>
       </c>
-    </row>
-    <row r="242">
-      <c s="11" r="A242"/>
-      <c t="s" s="7" r="B242">
+      <c t="s" s="7" r="D242">
         <v>872</v>
       </c>
-      <c t="s" s="14" r="C242">
+      <c t="s" s="7" r="E242">
         <v>873</v>
-      </c>
-      <c t="s" s="7" r="D242">
-        <v>874</v>
-      </c>
-      <c t="s" s="7" r="E242">
-        <v>875</v>
       </c>
     </row>
     <row r="243">
       <c s="11" r="A243"/>
       <c t="s" s="7" r="B243">
+        <v>874</v>
+      </c>
+      <c t="s" s="14" r="C243">
+        <v>875</v>
+      </c>
+      <c t="s" s="7" r="D243">
         <v>876</v>
       </c>
-      <c t="s" s="14" r="C243">
+      <c t="s" s="7" r="E243">
         <v>877</v>
-      </c>
-      <c t="s" s="7" r="D243">
-        <v>878</v>
-      </c>
-      <c t="s" s="7" r="E243">
-        <v>879</v>
       </c>
     </row>
     <row r="244">
       <c s="11" r="A244"/>
       <c t="s" s="7" r="B244">
+        <v>878</v>
+      </c>
+      <c t="s" s="14" r="C244">
+        <v>879</v>
+      </c>
+      <c t="s" s="7" r="D244">
         <v>880</v>
       </c>
-      <c t="s" s="14" r="C244">
+      <c t="s" s="7" r="E244">
         <v>881</v>
-      </c>
-      <c t="s" s="7" r="D244">
-        <v>882</v>
-      </c>
-      <c t="s" s="7" r="E244">
-        <v>883</v>
       </c>
     </row>
     <row r="245">
       <c s="11" r="A245"/>
-      <c s="17" r="B245"/>
-      <c s="31" r="C245"/>
-      <c s="17" r="D245"/>
-      <c s="17" r="E245"/>
+      <c t="s" s="7" r="B245">
+        <v>882</v>
+      </c>
+      <c t="s" s="14" r="C245">
+        <v>883</v>
+      </c>
+      <c t="s" s="7" r="D245">
+        <v>884</v>
+      </c>
+      <c t="s" s="7" r="E245">
+        <v>885</v>
+      </c>
     </row>
     <row r="246">
-      <c t="s" s="11" r="A246">
-        <v>884</v>
-      </c>
-      <c t="s" s="7" r="B246">
-        <v>885</v>
-      </c>
-      <c t="s" s="14" r="C246">
+      <c s="11" r="A246"/>
+      <c s="17" r="B246"/>
+      <c s="31" r="C246"/>
+      <c s="17" r="D246"/>
+      <c s="17" r="E246"/>
+    </row>
+    <row r="247">
+      <c t="s" s="11" r="A247">
         <v>886</v>
       </c>
-      <c t="s" s="7" r="D246">
+      <c t="s" s="7" r="B247">
         <v>887</v>
       </c>
-      <c t="s" s="7" r="E246">
+      <c t="s" s="14" r="C247">
         <v>888</v>
       </c>
-    </row>
-    <row r="247">
-      <c s="11" r="A247"/>
-      <c t="s" s="7" r="B247">
+      <c t="s" s="7" r="D247">
         <v>889</v>
       </c>
-      <c t="s" s="14" r="C247">
+      <c t="s" s="7" r="E247">
         <v>890</v>
-      </c>
-      <c t="s" s="7" r="D247">
-        <v>891</v>
-      </c>
-      <c t="s" s="7" r="E247">
-        <v>892</v>
       </c>
     </row>
     <row r="248">
       <c s="11" r="A248"/>
-      <c s="17" r="B248"/>
-      <c s="31" r="C248"/>
-      <c s="17" r="D248"/>
-      <c s="17" r="E248"/>
+      <c t="s" s="7" r="B248">
+        <v>891</v>
+      </c>
+      <c t="s" s="14" r="C248">
+        <v>892</v>
+      </c>
+      <c t="s" s="7" r="D248">
+        <v>893</v>
+      </c>
+      <c t="s" s="7" r="E248">
+        <v>894</v>
+      </c>
     </row>
     <row r="249">
-      <c t="s" s="11" r="A249">
-        <v>893</v>
-      </c>
-      <c t="s" s="7" r="B249">
-        <v>894</v>
-      </c>
-      <c t="s" s="14" r="C249">
+      <c s="11" r="A249"/>
+      <c s="17" r="B249"/>
+      <c s="31" r="C249"/>
+      <c s="17" r="D249"/>
+      <c s="17" r="E249"/>
+    </row>
+    <row r="250">
+      <c t="s" s="11" r="A250">
         <v>895</v>
       </c>
-      <c t="s" s="7" r="D249">
+      <c t="s" s="7" r="B250">
         <v>896</v>
       </c>
-      <c t="s" s="7" r="E249">
+      <c t="s" s="14" r="C250">
         <v>897</v>
       </c>
-    </row>
-    <row r="250">
-      <c s="11" r="A250"/>
-      <c s="17" r="B250"/>
-      <c s="9" r="C250"/>
-      <c s="17" r="D250"/>
-      <c s="17" r="E250"/>
+      <c t="s" s="7" r="D250">
+        <v>898</v>
+      </c>
+      <c t="s" s="7" r="E250">
+        <v>899</v>
+      </c>
     </row>
     <row r="251">
-      <c t="s" s="11" r="A251">
-        <v>898</v>
-      </c>
-      <c t="s" s="7" r="B251">
-        <v>899</v>
-      </c>
-      <c t="s" s="14" r="C251">
+      <c s="11" r="A251"/>
+      <c s="17" r="B251"/>
+      <c s="9" r="C251"/>
+      <c s="17" r="D251"/>
+      <c s="17" r="E251"/>
+    </row>
+    <row r="252">
+      <c t="s" s="11" r="A252">
         <v>900</v>
       </c>
-      <c t="s" s="7" r="D251">
+      <c t="s" s="7" r="B252">
         <v>901</v>
       </c>
-      <c t="s" s="7" r="E251">
+      <c t="s" s="14" r="C252">
         <v>902</v>
       </c>
-    </row>
-    <row r="252">
-      <c s="11" r="A252"/>
-      <c t="s" s="7" r="B252">
+      <c t="s" s="7" r="D252">
         <v>903</v>
       </c>
-      <c t="s" s="14" r="C252">
+      <c t="s" s="7" r="E252">
         <v>904</v>
-      </c>
-      <c t="s" s="7" r="D252">
-        <v>905</v>
-      </c>
-      <c t="s" s="7" r="E252">
-        <v>906</v>
       </c>
     </row>
     <row r="253">
       <c s="11" r="A253"/>
       <c t="s" s="7" r="B253">
+        <v>905</v>
+      </c>
+      <c t="s" s="14" r="C253">
+        <v>906</v>
+      </c>
+      <c t="s" s="7" r="D253">
         <v>907</v>
       </c>
-      <c t="s" s="14" r="C253">
+      <c t="s" s="7" r="E253">
         <v>908</v>
-      </c>
-      <c t="s" s="7" r="D253">
-        <v>909</v>
-      </c>
-      <c t="s" s="7" r="E253">
-        <v>910</v>
       </c>
     </row>
     <row r="254">
       <c s="11" r="A254"/>
       <c t="s" s="7" r="B254">
+        <v>909</v>
+      </c>
+      <c t="s" s="14" r="C254">
+        <v>910</v>
+      </c>
+      <c t="s" s="7" r="D254">
         <v>911</v>
       </c>
-      <c t="s" s="14" r="C254">
+      <c t="s" s="7" r="E254">
         <v>912</v>
-      </c>
-      <c t="s" s="7" r="D254">
-        <v>913</v>
-      </c>
-      <c t="s" s="7" r="E254">
-        <v>914</v>
       </c>
     </row>
     <row r="255">
       <c s="11" r="A255"/>
       <c t="s" s="7" r="B255">
+        <v>913</v>
+      </c>
+      <c t="s" s="14" r="C255">
+        <v>914</v>
+      </c>
+      <c t="s" s="7" r="D255">
         <v>915</v>
       </c>
-      <c t="s" s="14" r="C255">
+      <c t="s" s="7" r="E255">
         <v>916</v>
-      </c>
-      <c t="s" s="7" r="D255">
-        <v>917</v>
-      </c>
-      <c t="s" s="7" r="E255">
-        <v>918</v>
       </c>
     </row>
     <row r="256">
       <c s="11" r="A256"/>
       <c t="s" s="7" r="B256">
+        <v>917</v>
+      </c>
+      <c t="s" s="14" r="C256">
+        <v>918</v>
+      </c>
+      <c t="s" s="7" r="D256">
         <v>919</v>
       </c>
-      <c t="s" s="14" r="C256">
+      <c t="s" s="7" r="E256">
         <v>920</v>
-      </c>
-      <c t="s" s="7" r="D256">
-        <v>921</v>
-      </c>
-      <c t="s" s="7" r="E256">
-        <v>922</v>
       </c>
     </row>
     <row r="257">
       <c s="11" r="A257"/>
       <c t="s" s="7" r="B257">
+        <v>921</v>
+      </c>
+      <c t="s" s="14" r="C257">
+        <v>922</v>
+      </c>
+      <c t="s" s="7" r="D257">
         <v>923</v>
       </c>
-      <c t="s" s="14" r="C257">
+      <c t="s" s="7" r="E257">
         <v>924</v>
-      </c>
-      <c t="s" s="7" r="D257">
-        <v>925</v>
-      </c>
-      <c t="s" s="7" r="E257">
-        <v>926</v>
       </c>
     </row>
     <row r="258">
       <c s="11" r="A258"/>
       <c t="s" s="7" r="B258">
+        <v>925</v>
+      </c>
+      <c t="s" s="14" r="C258">
+        <v>926</v>
+      </c>
+      <c t="s" s="7" r="D258">
         <v>927</v>
       </c>
-      <c t="s" s="14" r="C258">
+      <c t="s" s="7" r="E258">
         <v>928</v>
       </c>
-      <c t="s" s="7" r="D258">
+    </row>
+    <row r="259">
+      <c s="11" r="A259"/>
+      <c t="s" s="7" r="B259">
         <v>929</v>
       </c>
-      <c t="s" s="7" r="E258">
+      <c t="s" s="14" r="C259">
         <v>930</v>
       </c>
-    </row>
-    <row r="259">
-      <c s="18" r="A259"/>
-      <c s="17" r="B259"/>
-      <c s="9" r="C259"/>
-      <c s="17" r="D259"/>
-      <c s="17" r="E259"/>
+      <c t="s" s="7" r="D259">
+        <v>931</v>
+      </c>
+      <c t="s" s="7" r="E259">
+        <v>932</v>
+      </c>
     </row>
     <row r="260">
-      <c t="s" s="11" r="A260">
-        <v>931</v>
-      </c>
-      <c t="s" s="7" r="B260">
-        <v>932</v>
-      </c>
-      <c t="s" s="7" r="C260">
+      <c s="18" r="A260"/>
+      <c s="17" r="B260"/>
+      <c s="9" r="C260"/>
+      <c s="17" r="D260"/>
+      <c s="17" r="E260"/>
+    </row>
+    <row r="261">
+      <c t="s" s="11" r="A261">
         <v>933</v>
       </c>
-      <c t="s" s="7" r="D260">
+      <c t="s" s="7" r="B261">
         <v>934</v>
       </c>
-      <c t="s" s="7" r="E260">
+      <c t="s" s="7" r="C261">
         <v>935</v>
       </c>
-    </row>
-    <row r="261">
-      <c s="11" r="A261"/>
-      <c t="s" s="7" r="B261">
+      <c t="s" s="7" r="D261">
         <v>936</v>
       </c>
-      <c t="s" s="14" r="C261">
+      <c t="s" s="7" r="E261">
         <v>937</v>
-      </c>
-      <c t="s" s="7" r="D261">
-        <v>938</v>
-      </c>
-      <c t="s" s="7" r="E261">
-        <v>939</v>
       </c>
     </row>
     <row r="262">
       <c s="11" r="A262"/>
       <c t="s" s="7" r="B262">
+        <v>938</v>
+      </c>
+      <c t="s" s="14" r="C262">
+        <v>939</v>
+      </c>
+      <c t="s" s="7" r="D262">
         <v>940</v>
       </c>
-      <c t="s" s="14" r="C262">
+      <c t="s" s="7" r="E262">
         <v>941</v>
-      </c>
-      <c t="s" s="7" r="D262">
-        <v>942</v>
-      </c>
-      <c t="s" s="7" r="E262">
-        <v>943</v>
       </c>
     </row>
     <row r="263">
       <c s="11" r="A263"/>
       <c t="s" s="7" r="B263">
+        <v>942</v>
+      </c>
+      <c t="s" s="14" r="C263">
+        <v>943</v>
+      </c>
+      <c t="s" s="7" r="D263">
         <v>944</v>
       </c>
-      <c t="s" s="14" r="C263">
+      <c t="s" s="7" r="E263">
         <v>945</v>
-      </c>
-      <c t="s" s="7" r="D263">
-        <v>946</v>
-      </c>
-      <c t="s" s="7" r="E263">
-        <v>947</v>
       </c>
     </row>
     <row r="264">
       <c s="11" r="A264"/>
       <c t="s" s="7" r="B264">
+        <v>946</v>
+      </c>
+      <c t="s" s="14" r="C264">
+        <v>947</v>
+      </c>
+      <c t="s" s="7" r="D264">
         <v>948</v>
       </c>
-      <c t="s" s="14" r="C264">
-        <v>665</v>
-      </c>
-      <c t="s" s="7" r="D264">
-        <v>160</v>
-      </c>
       <c t="s" s="7" r="E264">
-        <v>667</v>
+        <v>949</v>
       </c>
     </row>
     <row r="265">
       <c s="11" r="A265"/>
       <c t="s" s="7" r="B265">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c t="s" s="14" r="C265">
-        <v>950</v>
+        <v>667</v>
       </c>
       <c t="s" s="7" r="D265">
+        <v>160</v>
+      </c>
+      <c t="s" s="7" r="E265">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="266">
+      <c s="11" r="A266"/>
+      <c t="s" s="7" r="B266">
         <v>951</v>
       </c>
-      <c t="s" s="7" r="E265">
+      <c t="s" s="14" r="C266">
         <v>952</v>
       </c>
-    </row>
-    <row r="266">
-      <c s="18" r="A266"/>
-      <c s="17" r="B266"/>
-      <c s="9" r="C266"/>
-      <c s="17" r="D266"/>
-      <c s="17" r="E266"/>
+      <c t="s" s="7" r="D266">
+        <v>953</v>
+      </c>
+      <c t="s" s="7" r="E266">
+        <v>954</v>
+      </c>
     </row>
     <row r="267">
-      <c t="s" s="11" r="A267">
-        <v>953</v>
-      </c>
-      <c t="s" s="7" r="B267">
-        <v>954</v>
-      </c>
-      <c t="s" s="14" r="C267">
+      <c s="18" r="A267"/>
+      <c s="17" r="B267"/>
+      <c s="9" r="C267"/>
+      <c s="17" r="D267"/>
+      <c s="17" r="E267"/>
+    </row>
+    <row r="268">
+      <c t="s" s="11" r="A268">
         <v>955</v>
       </c>
-      <c t="s" s="7" r="D267">
+      <c t="s" s="7" r="B268">
         <v>956</v>
       </c>
-      <c t="s" s="7" r="E267">
+      <c t="s" s="14" r="C268">
         <v>957</v>
       </c>
-    </row>
-    <row r="268">
-      <c s="11" r="A268"/>
-      <c t="s" s="7" r="B268">
+      <c t="s" s="7" r="D268">
         <v>958</v>
       </c>
-      <c t="s" s="14" r="C268">
+      <c t="s" s="7" r="E268">
         <v>959</v>
-      </c>
-      <c t="s" s="7" r="D268">
-        <v>960</v>
-      </c>
-      <c t="s" s="7" r="E268">
-        <v>961</v>
       </c>
     </row>
     <row r="269">
       <c s="11" r="A269"/>
       <c t="s" s="7" r="B269">
+        <v>960</v>
+      </c>
+      <c t="s" s="14" r="C269">
+        <v>961</v>
+      </c>
+      <c t="s" s="7" r="D269">
         <v>962</v>
       </c>
-      <c t="s" s="14" r="C269">
+      <c t="s" s="7" r="E269">
         <v>963</v>
-      </c>
-      <c t="s" s="7" r="D269">
-        <v>964</v>
-      </c>
-      <c t="s" s="7" r="E269">
-        <v>965</v>
       </c>
     </row>
     <row r="270">
       <c s="11" r="A270"/>
       <c t="s" s="7" r="B270">
+        <v>964</v>
+      </c>
+      <c t="s" s="14" r="C270">
+        <v>965</v>
+      </c>
+      <c t="s" s="7" r="D270">
         <v>966</v>
       </c>
-      <c t="s" s="14" r="C270">
+      <c t="s" s="7" r="E270">
         <v>967</v>
-      </c>
-      <c t="s" s="7" r="D270">
-        <v>968</v>
-      </c>
-      <c t="s" s="7" r="E270">
-        <v>968</v>
       </c>
     </row>
     <row r="271">
       <c s="11" r="A271"/>
       <c t="s" s="7" r="B271">
+        <v>968</v>
+      </c>
+      <c t="s" s="14" r="C271">
         <v>969</v>
       </c>
-      <c t="s" s="14" r="C271">
+      <c t="s" s="7" r="D271">
         <v>970</v>
       </c>
-      <c t="s" s="7" r="D271">
-        <v>971</v>
-      </c>
       <c t="s" s="7" r="E271">
-        <v>972</v>
+        <v>970</v>
       </c>
     </row>
     <row r="272">
       <c s="11" r="A272"/>
       <c t="s" s="7" r="B272">
+        <v>971</v>
+      </c>
+      <c t="s" s="14" r="C272">
+        <v>972</v>
+      </c>
+      <c t="s" s="7" r="D272">
         <v>973</v>
       </c>
-      <c t="s" s="14" r="C272">
+      <c t="s" s="7" r="E272">
         <v>974</v>
-      </c>
-      <c t="s" s="7" r="D272">
-        <v>975</v>
-      </c>
-      <c t="s" s="7" r="E272">
-        <v>976</v>
       </c>
     </row>
     <row r="273">
       <c s="11" r="A273"/>
       <c t="s" s="7" r="B273">
+        <v>975</v>
+      </c>
+      <c t="s" s="14" r="C273">
+        <v>976</v>
+      </c>
+      <c t="s" s="7" r="D273">
         <v>977</v>
       </c>
-      <c t="s" s="14" r="C273">
+      <c t="s" s="7" r="E273">
         <v>978</v>
-      </c>
-      <c t="s" s="7" r="D273">
-        <v>979</v>
-      </c>
-      <c t="s" s="7" r="E273">
-        <v>980</v>
       </c>
     </row>
     <row r="274">
       <c s="11" r="A274"/>
       <c t="s" s="7" r="B274">
+        <v>979</v>
+      </c>
+      <c t="s" s="14" r="C274">
+        <v>980</v>
+      </c>
+      <c t="s" s="7" r="D274">
         <v>981</v>
       </c>
-      <c t="s" s="14" r="C274">
+      <c t="s" s="7" r="E274">
         <v>982</v>
-      </c>
-      <c t="s" s="7" r="D274">
-        <v>983</v>
-      </c>
-      <c t="s" s="7" r="E274">
-        <v>984</v>
       </c>
     </row>
     <row r="275">
       <c s="11" r="A275"/>
       <c t="s" s="7" r="B275">
+        <v>983</v>
+      </c>
+      <c t="s" s="14" r="C275">
+        <v>984</v>
+      </c>
+      <c t="s" s="7" r="D275">
         <v>985</v>
       </c>
-      <c t="s" s="14" r="C275">
+      <c t="s" s="7" r="E275">
         <v>986</v>
-      </c>
-      <c t="s" s="7" r="D275">
-        <v>987</v>
-      </c>
-      <c t="s" s="7" r="E275">
-        <v>988</v>
       </c>
     </row>
     <row r="276">
       <c s="11" r="A276"/>
       <c t="s" s="7" r="B276">
+        <v>987</v>
+      </c>
+      <c t="s" s="14" r="C276">
+        <v>988</v>
+      </c>
+      <c t="s" s="7" r="D276">
         <v>989</v>
       </c>
-      <c t="s" s="14" r="C276">
+      <c t="s" s="7" r="E276">
         <v>990</v>
-      </c>
-      <c t="s" s="7" r="D276">
-        <v>991</v>
-      </c>
-      <c t="s" s="7" r="E276">
-        <v>992</v>
       </c>
     </row>
     <row r="277">
       <c s="11" r="A277"/>
       <c t="s" s="7" r="B277">
+        <v>991</v>
+      </c>
+      <c t="s" s="14" r="C277">
+        <v>992</v>
+      </c>
+      <c t="s" s="7" r="D277">
         <v>993</v>
       </c>
-      <c t="s" s="14" r="C277">
+      <c t="s" s="7" r="E277">
         <v>994</v>
-      </c>
-      <c t="s" s="7" r="D277">
-        <v>995</v>
-      </c>
-      <c t="s" s="7" r="E277">
-        <v>996</v>
       </c>
     </row>
     <row r="278">
       <c s="11" r="A278"/>
       <c t="s" s="7" r="B278">
+        <v>995</v>
+      </c>
+      <c t="s" s="14" r="C278">
+        <v>996</v>
+      </c>
+      <c t="s" s="7" r="D278">
         <v>997</v>
       </c>
-      <c t="s" s="14" r="C278">
+      <c t="s" s="7" r="E278">
         <v>998</v>
-      </c>
-      <c t="s" s="7" r="D278">
-        <v>999</v>
-      </c>
-      <c t="s" s="7" r="E278">
-        <v>1000</v>
       </c>
     </row>
     <row r="279">
       <c s="11" r="A279"/>
       <c t="s" s="7" r="B279">
+        <v>999</v>
+      </c>
+      <c t="s" s="14" r="C279">
+        <v>1000</v>
+      </c>
+      <c t="s" s="7" r="D279">
         <v>1001</v>
-      </c>
-      <c t="s" s="14" r="C279">
-        <v>1002</v>
-      </c>
-      <c t="s" s="7" r="D279">
-        <v>1002</v>
       </c>
       <c t="s" s="7" r="E279">
         <v>1002</v>
@@ -8101,570 +8103,585 @@
         <v>1004</v>
       </c>
       <c t="s" s="7" r="D280">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c t="s" s="7" r="E280">
-        <v>1006</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="281">
       <c s="11" r="A281"/>
       <c t="s" s="7" r="B281">
+        <v>1005</v>
+      </c>
+      <c t="s" s="14" r="C281">
+        <v>1006</v>
+      </c>
+      <c t="s" s="7" r="D281">
         <v>1007</v>
       </c>
-      <c t="s" s="14" r="C281">
+      <c t="s" s="7" r="E281">
         <v>1008</v>
-      </c>
-      <c t="s" s="7" r="D281">
-        <v>1009</v>
-      </c>
-      <c t="s" s="7" r="E281">
-        <v>1010</v>
       </c>
     </row>
     <row r="282">
       <c s="11" r="A282"/>
       <c t="s" s="7" r="B282">
+        <v>1009</v>
+      </c>
+      <c t="s" s="14" r="C282">
+        <v>1010</v>
+      </c>
+      <c t="s" s="7" r="D282">
         <v>1011</v>
       </c>
-      <c t="s" s="14" r="C282">
+      <c t="s" s="7" r="E282">
         <v>1012</v>
-      </c>
-      <c t="s" s="7" r="D282">
-        <v>1013</v>
-      </c>
-      <c t="s" s="7" r="E282">
-        <v>1014</v>
       </c>
     </row>
     <row r="283">
       <c s="11" r="A283"/>
       <c t="s" s="7" r="B283">
+        <v>1013</v>
+      </c>
+      <c t="s" s="14" r="C283">
+        <v>1014</v>
+      </c>
+      <c t="s" s="7" r="D283">
         <v>1015</v>
       </c>
-      <c t="s" s="14" r="C283">
+      <c t="s" s="7" r="E283">
         <v>1016</v>
-      </c>
-      <c t="s" s="7" r="D283">
-        <v>1017</v>
-      </c>
-      <c t="s" s="7" r="E283">
-        <v>1018</v>
       </c>
     </row>
     <row r="284">
       <c s="11" r="A284"/>
       <c t="s" s="7" r="B284">
+        <v>1017</v>
+      </c>
+      <c t="s" s="14" r="C284">
+        <v>1018</v>
+      </c>
+      <c t="s" s="7" r="D284">
         <v>1019</v>
       </c>
-      <c t="s" s="14" r="C284">
+      <c t="s" s="7" r="E284">
         <v>1020</v>
-      </c>
-      <c t="s" s="7" r="D284">
-        <v>1021</v>
-      </c>
-      <c t="s" s="7" r="E284">
-        <v>1022</v>
       </c>
     </row>
     <row r="285">
       <c s="11" r="A285"/>
       <c t="s" s="7" r="B285">
+        <v>1021</v>
+      </c>
+      <c t="s" s="14" r="C285">
+        <v>1022</v>
+      </c>
+      <c t="s" s="7" r="D285">
         <v>1023</v>
       </c>
-      <c t="s" s="14" r="C285">
+      <c t="s" s="7" r="E285">
         <v>1024</v>
-      </c>
-      <c t="s" s="7" r="D285">
-        <v>1025</v>
-      </c>
-      <c t="s" s="7" r="E285">
-        <v>1026</v>
       </c>
     </row>
     <row r="286">
       <c s="11" r="A286"/>
       <c t="s" s="7" r="B286">
+        <v>1025</v>
+      </c>
+      <c t="s" s="14" r="C286">
+        <v>1026</v>
+      </c>
+      <c t="s" s="7" r="D286">
         <v>1027</v>
       </c>
-      <c t="s" s="14" r="C286">
+      <c t="s" s="7" r="E286">
         <v>1028</v>
-      </c>
-      <c t="s" s="7" r="D286">
-        <v>1029</v>
-      </c>
-      <c t="s" s="7" r="E286">
-        <v>1030</v>
       </c>
     </row>
     <row r="287">
       <c s="11" r="A287"/>
-      <c s="17" r="B287"/>
-      <c s="9" r="C287"/>
-      <c s="17" r="D287"/>
-      <c s="17" r="E287"/>
+      <c t="s" s="7" r="B287">
+        <v>1029</v>
+      </c>
+      <c t="s" s="14" r="C287">
+        <v>1030</v>
+      </c>
+      <c t="s" s="7" r="D287">
+        <v>1031</v>
+      </c>
+      <c t="s" s="7" r="E287">
+        <v>1032</v>
+      </c>
     </row>
     <row r="288">
-      <c t="s" s="11" r="A288">
-        <v>1031</v>
-      </c>
-      <c t="s" s="7" r="B288">
-        <v>1032</v>
-      </c>
-      <c t="s" s="14" r="C288">
+      <c s="11" r="A288"/>
+      <c s="17" r="B288"/>
+      <c s="9" r="C288"/>
+      <c s="17" r="D288"/>
+      <c s="17" r="E288"/>
+    </row>
+    <row r="289">
+      <c t="s" s="11" r="A289">
         <v>1033</v>
       </c>
-      <c t="s" s="7" r="D288">
+      <c t="s" s="7" r="B289">
         <v>1034</v>
       </c>
-      <c t="s" s="7" r="E288">
+      <c t="s" s="14" r="C289">
         <v>1035</v>
       </c>
-    </row>
-    <row r="289">
-      <c s="11" r="A289"/>
-      <c t="s" s="7" r="B289">
+      <c t="s" s="7" r="D289">
         <v>1036</v>
       </c>
-      <c t="s" s="14" r="C289">
+      <c t="s" s="7" r="E289">
         <v>1037</v>
-      </c>
-      <c t="s" s="7" r="D289">
-        <v>1038</v>
-      </c>
-      <c t="s" s="7" r="E289">
-        <v>1039</v>
       </c>
     </row>
     <row r="290">
       <c s="11" r="A290"/>
       <c t="s" s="7" r="B290">
+        <v>1038</v>
+      </c>
+      <c t="s" s="14" r="C290">
+        <v>1039</v>
+      </c>
+      <c t="s" s="7" r="D290">
         <v>1040</v>
       </c>
-      <c t="s" s="14" r="C290">
+      <c t="s" s="7" r="E290">
         <v>1041</v>
-      </c>
-      <c t="s" s="7" r="D290">
-        <v>1042</v>
-      </c>
-      <c t="s" s="7" r="E290">
-        <v>1043</v>
       </c>
     </row>
     <row r="291">
       <c s="11" r="A291"/>
       <c t="s" s="7" r="B291">
+        <v>1042</v>
+      </c>
+      <c t="s" s="14" r="C291">
+        <v>1043</v>
+      </c>
+      <c t="s" s="7" r="D291">
         <v>1044</v>
       </c>
-      <c t="s" s="14" r="C291">
+      <c t="s" s="7" r="E291">
         <v>1045</v>
-      </c>
-      <c t="s" s="7" r="D291">
-        <v>1046</v>
-      </c>
-      <c t="s" s="7" r="E291">
-        <v>1047</v>
       </c>
     </row>
     <row r="292">
       <c s="11" r="A292"/>
       <c t="s" s="7" r="B292">
+        <v>1046</v>
+      </c>
+      <c t="s" s="14" r="C292">
+        <v>1047</v>
+      </c>
+      <c t="s" s="7" r="D292">
         <v>1048</v>
       </c>
-      <c t="s" s="14" r="C292">
-        <v>1048</v>
-      </c>
-      <c t="s" s="19" r="D292">
+      <c t="s" s="7" r="E292">
         <v>1049</v>
-      </c>
-      <c t="s" s="19" r="E292">
-        <v>1050</v>
       </c>
     </row>
     <row r="293">
       <c s="11" r="A293"/>
       <c t="s" s="7" r="B293">
+        <v>1050</v>
+      </c>
+      <c t="s" s="14" r="C293">
+        <v>1050</v>
+      </c>
+      <c t="s" s="19" r="D293">
         <v>1051</v>
       </c>
-      <c t="s" s="14" r="C293">
+      <c t="s" s="19" r="E293">
         <v>1052</v>
-      </c>
-      <c t="s" s="7" r="D293">
-        <v>1053</v>
-      </c>
-      <c t="s" s="7" r="E293">
-        <v>1054</v>
       </c>
     </row>
     <row r="294">
       <c s="11" r="A294"/>
       <c t="s" s="7" r="B294">
+        <v>1053</v>
+      </c>
+      <c t="s" s="14" r="C294">
+        <v>1054</v>
+      </c>
+      <c t="s" s="7" r="D294">
         <v>1055</v>
       </c>
-      <c t="s" s="14" r="C294">
+      <c t="s" s="7" r="E294">
         <v>1056</v>
       </c>
-      <c t="s" s="7" r="D294">
+    </row>
+    <row r="295">
+      <c s="11" r="A295"/>
+      <c t="s" s="7" r="B295">
         <v>1057</v>
       </c>
-      <c t="s" s="7" r="E294">
+      <c t="s" s="14" r="C295">
         <v>1058</v>
       </c>
-    </row>
-    <row r="295">
-      <c t="s" s="17" r="A295">
+      <c t="s" s="7" r="D295">
         <v>1059</v>
       </c>
-      <c s="28" r="B295"/>
-      <c t="s" s="14" r="C295">
+      <c t="s" s="7" r="E295">
         <v>1060</v>
       </c>
-      <c t="s" s="19" r="D295">
+    </row>
+    <row r="296">
+      <c t="s" s="17" r="A296">
         <v>1061</v>
       </c>
-      <c t="s" s="19" r="E295">
+      <c s="28" r="B296"/>
+      <c t="s" s="14" r="C296">
         <v>1062</v>
       </c>
-    </row>
-    <row r="296">
-      <c s="18" r="A296"/>
-      <c s="17" r="B296"/>
-      <c s="9" r="C296"/>
-      <c s="17" r="D296"/>
-      <c s="17" r="E296"/>
+      <c t="s" s="19" r="D296">
+        <v>1063</v>
+      </c>
+      <c t="s" s="19" r="E296">
+        <v>1064</v>
+      </c>
     </row>
     <row r="297">
-      <c t="s" s="18" r="A297">
-        <v>1063</v>
-      </c>
-      <c t="s" s="7" r="B297">
-        <v>1064</v>
-      </c>
-      <c t="s" s="7" r="C297">
+      <c s="18" r="A297"/>
+      <c s="17" r="B297"/>
+      <c s="9" r="C297"/>
+      <c s="17" r="D297"/>
+      <c s="17" r="E297"/>
+    </row>
+    <row r="298">
+      <c t="s" s="18" r="A298">
         <v>1065</v>
       </c>
-      <c t="s" s="7" r="D297">
+      <c t="s" s="7" r="B298">
         <v>1066</v>
       </c>
-      <c t="s" s="7" r="E297">
+      <c t="s" s="7" r="C298">
         <v>1067</v>
       </c>
-    </row>
-    <row r="298">
-      <c s="15" r="A298"/>
-      <c t="s" s="7" r="B298">
+      <c t="s" s="7" r="D298">
         <v>1068</v>
       </c>
-      <c t="s" s="14" r="C298">
+      <c t="s" s="7" r="E298">
         <v>1069</v>
-      </c>
-      <c t="s" s="7" r="D298">
-        <v>1070</v>
-      </c>
-      <c t="s" s="7" r="E298">
-        <v>1071</v>
       </c>
     </row>
     <row r="299">
       <c s="15" r="A299"/>
       <c t="s" s="7" r="B299">
+        <v>1070</v>
+      </c>
+      <c t="s" s="14" r="C299">
+        <v>1071</v>
+      </c>
+      <c t="s" s="7" r="D299">
         <v>1072</v>
       </c>
-      <c t="s" s="7" r="C299">
+      <c t="s" s="7" r="E299">
         <v>1073</v>
       </c>
-      <c t="s" s="7" r="D299">
+    </row>
+    <row r="300">
+      <c s="15" r="A300"/>
+      <c t="s" s="7" r="B300">
         <v>1074</v>
       </c>
-      <c t="s" s="7" r="E299">
+      <c t="s" s="7" r="C300">
         <v>1075</v>
       </c>
-    </row>
-    <row r="300">
-      <c s="18" r="A300"/>
-      <c t="s" s="7" r="B300">
+      <c t="s" s="7" r="D300">
         <v>1076</v>
       </c>
-      <c t="s" s="14" r="C300">
+      <c t="s" s="7" r="E300">
         <v>1077</v>
-      </c>
-      <c t="s" s="7" r="D300">
-        <v>1078</v>
-      </c>
-      <c t="s" s="7" r="E300">
-        <v>1079</v>
       </c>
     </row>
     <row r="301">
       <c s="18" r="A301"/>
       <c t="s" s="7" r="B301">
+        <v>1078</v>
+      </c>
+      <c t="s" s="14" r="C301">
+        <v>1079</v>
+      </c>
+      <c t="s" s="7" r="D301">
         <v>1080</v>
       </c>
-      <c t="s" s="7" r="C301">
+      <c t="s" s="7" r="E301">
         <v>1081</v>
-      </c>
-      <c t="s" s="7" r="D301">
-        <v>1082</v>
-      </c>
-      <c t="s" s="7" r="E301">
-        <v>1083</v>
       </c>
     </row>
     <row r="302">
       <c s="18" r="A302"/>
       <c t="s" s="7" r="B302">
+        <v>1082</v>
+      </c>
+      <c t="s" s="7" r="C302">
+        <v>1083</v>
+      </c>
+      <c t="s" s="7" r="D302">
         <v>1084</v>
       </c>
-      <c t="s" s="14" r="C302">
+      <c t="s" s="7" r="E302">
         <v>1085</v>
-      </c>
-      <c t="s" s="7" r="D302">
-        <v>1086</v>
-      </c>
-      <c t="s" s="7" r="E302">
-        <v>1087</v>
       </c>
     </row>
     <row r="303">
       <c s="18" r="A303"/>
       <c t="s" s="7" r="B303">
+        <v>1086</v>
+      </c>
+      <c t="s" s="14" r="C303">
+        <v>1087</v>
+      </c>
+      <c t="s" s="7" r="D303">
         <v>1088</v>
       </c>
-      <c t="s" s="7" r="C303">
+      <c t="s" s="7" r="E303">
         <v>1089</v>
-      </c>
-      <c t="s" s="7" r="D303">
-        <v>1090</v>
-      </c>
-      <c t="s" s="7" r="E303">
-        <v>1091</v>
       </c>
     </row>
     <row r="304">
       <c s="18" r="A304"/>
       <c t="s" s="7" r="B304">
+        <v>1090</v>
+      </c>
+      <c t="s" s="7" r="C304">
+        <v>1091</v>
+      </c>
+      <c t="s" s="7" r="D304">
         <v>1092</v>
       </c>
-      <c t="s" s="14" r="C304">
+      <c t="s" s="7" r="E304">
         <v>1093</v>
-      </c>
-      <c t="s" s="7" r="D304">
-        <v>1094</v>
-      </c>
-      <c t="s" s="7" r="E304">
-        <v>1095</v>
       </c>
     </row>
     <row r="305">
       <c s="18" r="A305"/>
       <c t="s" s="7" r="B305">
+        <v>1094</v>
+      </c>
+      <c t="s" s="14" r="C305">
+        <v>1095</v>
+      </c>
+      <c t="s" s="7" r="D305">
         <v>1096</v>
       </c>
-      <c t="s" s="7" r="C305">
+      <c t="s" s="7" r="E305">
         <v>1097</v>
-      </c>
-      <c t="s" s="7" r="D305">
-        <v>1098</v>
-      </c>
-      <c t="s" s="7" r="E305">
-        <v>1099</v>
       </c>
     </row>
     <row r="306">
       <c s="18" r="A306"/>
       <c t="s" s="7" r="B306">
+        <v>1098</v>
+      </c>
+      <c t="s" s="7" r="C306">
+        <v>1099</v>
+      </c>
+      <c t="s" s="7" r="D306">
         <v>1100</v>
       </c>
-      <c t="s" s="14" r="C306">
+      <c t="s" s="7" r="E306">
         <v>1101</v>
-      </c>
-      <c t="s" s="7" r="D306">
-        <v>1102</v>
-      </c>
-      <c t="s" s="7" r="E306">
-        <v>1103</v>
       </c>
     </row>
     <row r="307">
       <c s="18" r="A307"/>
       <c t="s" s="7" r="B307">
+        <v>1102</v>
+      </c>
+      <c t="s" s="14" r="C307">
+        <v>1103</v>
+      </c>
+      <c t="s" s="7" r="D307">
         <v>1104</v>
       </c>
-      <c t="s" s="7" r="C307">
+      <c t="s" s="7" r="E307">
         <v>1105</v>
-      </c>
-      <c t="s" s="7" r="D307">
-        <v>1106</v>
-      </c>
-      <c t="s" s="7" r="E307">
-        <v>1107</v>
       </c>
     </row>
     <row r="308">
       <c s="18" r="A308"/>
       <c t="s" s="7" r="B308">
+        <v>1106</v>
+      </c>
+      <c t="s" s="7" r="C308">
+        <v>1107</v>
+      </c>
+      <c t="s" s="7" r="D308">
         <v>1108</v>
       </c>
-      <c t="s" s="14" r="C308">
-        <v>1101</v>
-      </c>
-      <c t="s" s="7" r="D308">
-        <v>1102</v>
-      </c>
       <c t="s" s="7" r="E308">
-        <v>1103</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="309">
       <c s="18" r="A309"/>
       <c t="s" s="7" r="B309">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c t="s" s="14" r="C309">
-        <v>1110</v>
+        <v>1103</v>
       </c>
       <c t="s" s="7" r="D309">
-        <v>1111</v>
+        <v>1104</v>
       </c>
       <c t="s" s="7" r="E309">
-        <v>1112</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="310">
       <c s="18" r="A310"/>
       <c t="s" s="7" r="B310">
+        <v>1111</v>
+      </c>
+      <c t="s" s="14" r="C310">
+        <v>1112</v>
+      </c>
+      <c t="s" s="7" r="D310">
         <v>1113</v>
       </c>
-      <c t="s" s="14" r="C310">
+      <c t="s" s="7" r="E310">
         <v>1114</v>
-      </c>
-      <c t="s" s="7" r="D310">
-        <v>1115</v>
-      </c>
-      <c t="s" s="7" r="E310">
-        <v>1116</v>
       </c>
     </row>
     <row r="311">
       <c s="18" r="A311"/>
       <c t="s" s="7" r="B311">
+        <v>1115</v>
+      </c>
+      <c t="s" s="14" r="C311">
+        <v>1116</v>
+      </c>
+      <c t="s" s="7" r="D311">
         <v>1117</v>
       </c>
-      <c t="s" s="7" r="C311">
+      <c t="s" s="7" r="E311">
         <v>1118</v>
-      </c>
-      <c t="s" s="7" r="D311">
-        <v>1119</v>
-      </c>
-      <c t="s" s="7" r="E311">
-        <v>1120</v>
       </c>
     </row>
     <row r="312">
       <c s="18" r="A312"/>
       <c t="s" s="7" r="B312">
+        <v>1119</v>
+      </c>
+      <c t="s" s="7" r="C312">
+        <v>1120</v>
+      </c>
+      <c t="s" s="7" r="D312">
         <v>1121</v>
       </c>
-      <c t="s" s="14" r="C312">
+      <c t="s" s="7" r="E312">
         <v>1122</v>
       </c>
-      <c t="s" s="7" r="D312">
+    </row>
+    <row r="313">
+      <c s="18" r="A313"/>
+      <c t="s" s="7" r="B313">
         <v>1123</v>
       </c>
-      <c t="s" s="7" r="E312">
+      <c t="s" s="14" r="C313">
         <v>1124</v>
       </c>
-    </row>
-    <row r="313">
-      <c s="11" r="A313"/>
-      <c t="s" s="7" r="B313">
+      <c t="s" s="7" r="D313">
         <v>1125</v>
       </c>
-      <c t="s" s="14" r="C313">
+      <c t="s" s="7" r="E313">
         <v>1126</v>
       </c>
-      <c t="s" s="7" r="D313">
+    </row>
+    <row r="314">
+      <c s="11" r="A314"/>
+      <c t="s" s="7" r="B314">
         <v>1127</v>
       </c>
-      <c t="s" s="7" r="E313">
+      <c t="s" s="14" r="C314">
         <v>1128</v>
       </c>
-    </row>
-    <row r="314">
-      <c t="s" s="11" r="A314">
+      <c t="s" s="7" r="D314">
         <v>1129</v>
       </c>
-      <c t="s" s="14" r="B314">
+      <c t="s" s="7" r="E314">
         <v>1130</v>
       </c>
-      <c t="s" s="14" r="C314">
+    </row>
+    <row r="315">
+      <c t="s" s="11" r="A315">
         <v>1131</v>
       </c>
-      <c t="s" s="19" r="D314">
+      <c t="s" s="14" r="B315">
         <v>1132</v>
       </c>
-      <c t="s" s="7" r="E314">
+      <c t="s" s="14" r="C315">
         <v>1133</v>
       </c>
-    </row>
-    <row r="315">
-      <c s="11" r="A315"/>
-      <c t="s" s="14" r="B315">
+      <c t="s" s="19" r="D315">
         <v>1134</v>
       </c>
-      <c t="s" s="14" r="C315">
+      <c t="s" s="7" r="E315">
         <v>1135</v>
-      </c>
-      <c t="s" s="19" r="D315">
-        <v>1136</v>
-      </c>
-      <c t="s" s="7" r="E315">
-        <v>1137</v>
       </c>
     </row>
     <row r="316">
       <c s="11" r="A316"/>
-      <c s="9" r="C316"/>
-      <c s="17" r="D316"/>
-      <c s="17" r="E316"/>
+      <c t="s" s="14" r="B316">
+        <v>1136</v>
+      </c>
+      <c t="s" s="14" r="C316">
+        <v>1137</v>
+      </c>
+      <c t="s" s="19" r="D316">
+        <v>1138</v>
+      </c>
+      <c t="s" s="7" r="E316">
+        <v>1139</v>
+      </c>
     </row>
     <row r="317">
-      <c t="s" s="11" r="A317">
-        <v>1138</v>
-      </c>
-      <c t="s" s="28" r="B317">
-        <v>1139</v>
-      </c>
-      <c t="s" s="14" r="C317">
+      <c s="11" r="A317"/>
+      <c s="9" r="C317"/>
+      <c s="17" r="D317"/>
+      <c s="17" r="E317"/>
+    </row>
+    <row r="318">
+      <c t="s" s="11" r="A318">
         <v>1140</v>
       </c>
-      <c t="s" s="7" r="D317">
+      <c t="s" s="28" r="B318">
         <v>1141</v>
       </c>
-      <c t="s" s="7" r="E317">
+      <c t="s" s="14" r="C318">
         <v>1142</v>
       </c>
-    </row>
-    <row r="318">
-      <c s="11" r="A318"/>
-      <c t="s" s="28" r="B318">
+      <c t="s" s="7" r="D318">
         <v>1143</v>
       </c>
-      <c t="s" s="14" r="C318">
+      <c t="s" s="7" r="E318">
         <v>1144</v>
-      </c>
-      <c t="s" s="7" r="D318">
-        <v>1145</v>
-      </c>
-      <c t="s" s="7" r="E318">
-        <v>1146</v>
       </c>
     </row>
     <row r="319">
       <c s="11" r="A319"/>
-      <c s="9" r="C319"/>
-      <c s="17" r="D319"/>
-      <c s="17" r="E319"/>
+      <c t="s" s="28" r="B319">
+        <v>1145</v>
+      </c>
+      <c t="s" s="14" r="C319">
+        <v>1146</v>
+      </c>
+      <c t="s" s="7" r="D319">
+        <v>1147</v>
+      </c>
+      <c t="s" s="7" r="E319">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="320">
+      <c s="11" r="A320"/>
+      <c s="9" r="C320"/>
+      <c s="17" r="D320"/>
+      <c s="17" r="E320"/>
     </row>
   </sheetData>
 </worksheet>
@@ -8682,17 +8699,17 @@
   <sheetData>
     <row customHeight="1" r="1" ht="112.5">
       <c t="s" s="4" r="A1">
-        <v>1147</v>
+        <v>1149</v>
       </c>
     </row>
     <row customHeight="1" r="2" ht="112.5">
       <c t="s" s="5" r="A2">
-        <v>1148</v>
+        <v>1150</v>
       </c>
     </row>
     <row customHeight="1" r="3" ht="112.5">
       <c t="s" s="10" r="A3">
-        <v>1149</v>
+        <v>1151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EWD-22953 - Three dots in the end
Former-commit-id: b087f03b959e431d71e14fd3fbf0fcc74ce52449
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -1099,13 +1099,13 @@
     <t>typeExperienceTitleHere</t>
   </si>
   <si>
-    <t>Type learning experience title here</t>
-  </si>
-  <si>
-    <t>Typ hier de titel van de leerervaring</t>
-  </si>
-  <si>
-    <t>Titel der Lernerfahrung hier eingeben</t>
+    <t>Type learning experience title here...</t>
+  </si>
+  <si>
+    <t>Typ hier de titel van de leerervaring...</t>
+  </si>
+  <si>
+    <t>Titel der Lernerfahrung hier eingeben...</t>
   </si>
   <si>
     <t>clickToAddExperience</t>
@@ -3546,7 +3546,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -3799,8 +3799,17 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3997,6 +4006,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -4020,7 +4035,7 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
@@ -4133,11 +4148,14 @@
     <xf applyAlignment="1" fillId="32" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="26"/>
-    <xf applyAlignment="1" fillId="33" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+    <xf applyAlignment="1" fillId="33" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="26" applyFill="1">
+      <alignment vertical="center" horizontal="right" wrapText="1"/>
+    </xf>
+    <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="27"/>
+    <xf applyAlignment="1" fillId="34" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="34" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="27" applyFill="1">
+    <xf applyAlignment="1" fillId="35" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="28" applyFill="1">
       <alignment vertical="center" horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5256,7 +5274,7 @@
       <c t="s" s="7" r="C74">
         <v>283</v>
       </c>
-      <c t="s" s="39" r="D74">
+      <c t="s" s="40" r="D74">
         <v>284</v>
       </c>
       <c t="s" s="20" r="E74">
@@ -5316,7 +5334,7 @@
       <c t="s" s="7" r="C78">
         <v>299</v>
       </c>
-      <c t="s" s="39" r="D78">
+      <c t="s" s="40" r="D78">
         <v>300</v>
       </c>
       <c t="s" s="20" r="E78">
@@ -5331,7 +5349,7 @@
       <c t="s" s="7" r="C79">
         <v>303</v>
       </c>
-      <c t="s" s="39" r="D79">
+      <c t="s" s="40" r="D79">
         <v>304</v>
       </c>
       <c t="s" s="20" r="E79">
@@ -5458,10 +5476,10 @@
       <c t="s" s="15" r="C88">
         <v>331</v>
       </c>
-      <c t="s" s="39" r="D88">
+      <c t="s" s="40" r="D88">
         <v>332</v>
       </c>
-      <c t="s" s="39" r="E88">
+      <c t="s" s="40" r="E88">
         <v>333</v>
       </c>
     </row>
@@ -5472,10 +5490,10 @@
       <c t="s" s="15" r="C89">
         <v>335</v>
       </c>
-      <c t="s" s="39" r="D89">
+      <c t="s" s="40" r="D89">
         <v>336</v>
       </c>
-      <c t="s" s="39" r="E89">
+      <c t="s" s="40" r="E89">
         <v>337</v>
       </c>
     </row>
@@ -5486,10 +5504,10 @@
       <c t="s" s="15" r="C90">
         <v>339</v>
       </c>
-      <c t="s" s="39" r="D90">
+      <c t="s" s="40" r="D90">
         <v>340</v>
       </c>
-      <c t="s" s="39" r="E90">
+      <c t="s" s="40" r="E90">
         <v>341</v>
       </c>
     </row>
@@ -5500,10 +5518,10 @@
       <c t="s" s="15" r="C91">
         <v>343</v>
       </c>
-      <c t="s" s="39" r="D91">
+      <c t="s" s="40" r="D91">
         <v>344</v>
       </c>
-      <c t="s" s="39" r="E91">
+      <c t="s" s="40" r="E91">
         <v>345</v>
       </c>
     </row>
@@ -5514,10 +5532,10 @@
       <c t="s" s="15" r="C92">
         <v>347</v>
       </c>
-      <c t="s" s="39" r="D92">
+      <c t="s" s="40" r="D92">
         <v>348</v>
       </c>
-      <c t="s" s="39" r="E92">
+      <c t="s" s="40" r="E92">
         <v>349</v>
       </c>
     </row>
@@ -5528,10 +5546,10 @@
       <c t="s" s="15" r="C93">
         <v>351</v>
       </c>
-      <c t="s" s="39" r="D93">
+      <c t="s" s="40" r="D93">
         <v>352</v>
       </c>
-      <c t="s" s="39" r="E93">
+      <c t="s" s="40" r="E93">
         <v>353</v>
       </c>
     </row>
@@ -5865,7 +5883,7 @@
     </row>
     <row r="117">
       <c s="13" r="A117"/>
-      <c t="s" s="7" r="B117">
+      <c t="s" s="38" r="B117">
         <v>438</v>
       </c>
       <c t="s" s="7" r="C117">
@@ -7103,25 +7121,25 @@
       <c t="s" s="12" r="A203">
         <v>744</v>
       </c>
-      <c t="s" s="40" r="B203">
+      <c t="s" s="41" r="B203">
         <v>745</v>
       </c>
       <c t="s" s="37" r="C203">
         <v>746</v>
       </c>
-      <c s="40" r="D203"/>
-      <c s="40" r="E203"/>
+      <c s="41" r="D203"/>
+      <c s="41" r="E203"/>
     </row>
     <row r="204">
       <c s="12" r="A204"/>
-      <c t="s" s="40" r="B204">
+      <c t="s" s="41" r="B204">
         <v>747</v>
       </c>
       <c t="s" s="37" r="C204">
         <v>748</v>
       </c>
-      <c s="40" r="D204"/>
-      <c s="40" r="E204"/>
+      <c s="41" r="D204"/>
+      <c s="41" r="E204"/>
     </row>
     <row r="205">
       <c s="12" r="A205"/>
@@ -8854,164 +8872,164 @@
   <sheetFormatPr customHeight="1" defaultColWidth="9.86" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c s="38" r="A1"/>
-      <c s="38" r="B1"/>
-      <c s="38" r="C1"/>
-      <c s="38" r="D1"/>
-      <c s="38" r="E1"/>
-      <c s="38" r="F1"/>
+      <c s="39" r="A1"/>
+      <c s="39" r="B1"/>
+      <c s="39" r="C1"/>
+      <c s="39" r="D1"/>
+      <c s="39" r="E1"/>
+      <c s="39" r="F1"/>
     </row>
     <row r="2">
-      <c s="38" r="A2"/>
-      <c s="38" r="B2"/>
-      <c s="38" r="C2"/>
-      <c s="38" r="D2"/>
-      <c s="38" r="E2"/>
-      <c s="38" r="F2"/>
+      <c s="39" r="A2"/>
+      <c s="39" r="B2"/>
+      <c s="39" r="C2"/>
+      <c s="39" r="D2"/>
+      <c s="39" r="E2"/>
+      <c s="39" r="F2"/>
     </row>
     <row r="3">
-      <c s="38" r="A3"/>
-      <c s="38" r="B3"/>
-      <c s="38" r="C3"/>
-      <c s="38" r="D3"/>
-      <c s="38" r="E3"/>
-      <c s="38" r="F3"/>
+      <c s="39" r="A3"/>
+      <c s="39" r="B3"/>
+      <c s="39" r="C3"/>
+      <c s="39" r="D3"/>
+      <c s="39" r="E3"/>
+      <c s="39" r="F3"/>
     </row>
     <row r="4">
-      <c s="38" r="A4"/>
-      <c s="38" r="B4"/>
-      <c s="38" r="C4"/>
-      <c s="38" r="D4"/>
-      <c s="38" r="E4"/>
-      <c s="38" r="F4"/>
+      <c s="39" r="A4"/>
+      <c s="39" r="B4"/>
+      <c s="39" r="C4"/>
+      <c s="39" r="D4"/>
+      <c s="39" r="E4"/>
+      <c s="39" r="F4"/>
     </row>
     <row r="5">
-      <c s="38" r="A5"/>
-      <c s="38" r="B5"/>
-      <c s="38" r="C5"/>
-      <c s="38" r="D5"/>
-      <c s="38" r="E5"/>
-      <c s="38" r="F5"/>
+      <c s="39" r="A5"/>
+      <c s="39" r="B5"/>
+      <c s="39" r="C5"/>
+      <c s="39" r="D5"/>
+      <c s="39" r="E5"/>
+      <c s="39" r="F5"/>
     </row>
     <row r="6">
-      <c s="38" r="A6"/>
-      <c s="38" r="B6"/>
-      <c s="38" r="C6"/>
-      <c s="38" r="D6"/>
-      <c s="38" r="E6"/>
-      <c s="38" r="F6"/>
+      <c s="39" r="A6"/>
+      <c s="39" r="B6"/>
+      <c s="39" r="C6"/>
+      <c s="39" r="D6"/>
+      <c s="39" r="E6"/>
+      <c s="39" r="F6"/>
     </row>
     <row r="7">
-      <c s="38" r="A7"/>
-      <c s="38" r="B7"/>
-      <c s="38" r="C7"/>
-      <c s="38" r="D7"/>
-      <c s="38" r="E7"/>
-      <c s="38" r="F7"/>
+      <c s="39" r="A7"/>
+      <c s="39" r="B7"/>
+      <c s="39" r="C7"/>
+      <c s="39" r="D7"/>
+      <c s="39" r="E7"/>
+      <c s="39" r="F7"/>
     </row>
     <row r="8">
-      <c s="38" r="A8"/>
-      <c s="38" r="B8"/>
-      <c s="38" r="C8"/>
-      <c s="38" r="D8"/>
-      <c s="38" r="E8"/>
-      <c s="38" r="F8"/>
+      <c s="39" r="A8"/>
+      <c s="39" r="B8"/>
+      <c s="39" r="C8"/>
+      <c s="39" r="D8"/>
+      <c s="39" r="E8"/>
+      <c s="39" r="F8"/>
     </row>
     <row r="9">
-      <c s="38" r="A9"/>
-      <c s="38" r="B9"/>
-      <c s="38" r="C9"/>
-      <c s="38" r="D9"/>
-      <c s="38" r="E9"/>
-      <c s="38" r="F9"/>
+      <c s="39" r="A9"/>
+      <c s="39" r="B9"/>
+      <c s="39" r="C9"/>
+      <c s="39" r="D9"/>
+      <c s="39" r="E9"/>
+      <c s="39" r="F9"/>
     </row>
     <row r="10">
-      <c s="38" r="A10"/>
-      <c s="38" r="B10"/>
-      <c s="38" r="C10"/>
-      <c s="38" r="D10"/>
-      <c s="38" r="E10"/>
-      <c s="38" r="F10"/>
+      <c s="39" r="A10"/>
+      <c s="39" r="B10"/>
+      <c s="39" r="C10"/>
+      <c s="39" r="D10"/>
+      <c s="39" r="E10"/>
+      <c s="39" r="F10"/>
     </row>
     <row r="11">
-      <c s="38" r="A11"/>
-      <c s="38" r="B11"/>
-      <c s="38" r="C11"/>
-      <c s="38" r="D11"/>
-      <c s="38" r="E11"/>
-      <c s="38" r="F11"/>
+      <c s="39" r="A11"/>
+      <c s="39" r="B11"/>
+      <c s="39" r="C11"/>
+      <c s="39" r="D11"/>
+      <c s="39" r="E11"/>
+      <c s="39" r="F11"/>
     </row>
     <row r="12">
-      <c s="38" r="A12"/>
-      <c s="38" r="B12"/>
-      <c s="38" r="C12"/>
-      <c s="38" r="D12"/>
-      <c s="38" r="E12"/>
-      <c s="38" r="F12"/>
+      <c s="39" r="A12"/>
+      <c s="39" r="B12"/>
+      <c s="39" r="C12"/>
+      <c s="39" r="D12"/>
+      <c s="39" r="E12"/>
+      <c s="39" r="F12"/>
     </row>
     <row r="13">
-      <c s="38" r="A13"/>
-      <c s="38" r="B13"/>
-      <c s="38" r="C13"/>
-      <c s="38" r="D13"/>
-      <c s="38" r="E13"/>
-      <c s="38" r="F13"/>
+      <c s="39" r="A13"/>
+      <c s="39" r="B13"/>
+      <c s="39" r="C13"/>
+      <c s="39" r="D13"/>
+      <c s="39" r="E13"/>
+      <c s="39" r="F13"/>
     </row>
     <row r="14">
-      <c s="38" r="A14"/>
-      <c s="38" r="B14"/>
-      <c s="38" r="C14"/>
-      <c s="38" r="D14"/>
-      <c s="38" r="E14"/>
-      <c s="38" r="F14"/>
+      <c s="39" r="A14"/>
+      <c s="39" r="B14"/>
+      <c s="39" r="C14"/>
+      <c s="39" r="D14"/>
+      <c s="39" r="E14"/>
+      <c s="39" r="F14"/>
     </row>
     <row r="15">
-      <c s="38" r="A15"/>
-      <c s="38" r="B15"/>
-      <c s="38" r="C15"/>
-      <c s="38" r="D15"/>
-      <c s="38" r="E15"/>
-      <c s="38" r="F15"/>
+      <c s="39" r="A15"/>
+      <c s="39" r="B15"/>
+      <c s="39" r="C15"/>
+      <c s="39" r="D15"/>
+      <c s="39" r="E15"/>
+      <c s="39" r="F15"/>
     </row>
     <row r="16">
-      <c s="38" r="A16"/>
-      <c s="38" r="B16"/>
-      <c s="38" r="C16"/>
-      <c s="38" r="D16"/>
-      <c s="38" r="E16"/>
-      <c s="38" r="F16"/>
+      <c s="39" r="A16"/>
+      <c s="39" r="B16"/>
+      <c s="39" r="C16"/>
+      <c s="39" r="D16"/>
+      <c s="39" r="E16"/>
+      <c s="39" r="F16"/>
     </row>
     <row r="17">
-      <c s="38" r="A17"/>
-      <c s="38" r="B17"/>
-      <c s="38" r="C17"/>
-      <c s="38" r="D17"/>
-      <c s="38" r="E17"/>
-      <c s="38" r="F17"/>
+      <c s="39" r="A17"/>
+      <c s="39" r="B17"/>
+      <c s="39" r="C17"/>
+      <c s="39" r="D17"/>
+      <c s="39" r="E17"/>
+      <c s="39" r="F17"/>
     </row>
     <row r="18">
-      <c s="38" r="A18"/>
-      <c s="38" r="B18"/>
-      <c s="38" r="C18"/>
-      <c s="38" r="D18"/>
-      <c s="38" r="E18"/>
-      <c s="38" r="F18"/>
+      <c s="39" r="A18"/>
+      <c s="39" r="B18"/>
+      <c s="39" r="C18"/>
+      <c s="39" r="D18"/>
+      <c s="39" r="E18"/>
+      <c s="39" r="F18"/>
     </row>
     <row r="19">
-      <c s="38" r="A19"/>
-      <c s="38" r="B19"/>
-      <c s="38" r="C19"/>
-      <c s="38" r="D19"/>
-      <c s="38" r="E19"/>
-      <c s="38" r="F19"/>
+      <c s="39" r="A19"/>
+      <c s="39" r="B19"/>
+      <c s="39" r="C19"/>
+      <c s="39" r="D19"/>
+      <c s="39" r="E19"/>
+      <c s="39" r="F19"/>
     </row>
     <row r="20">
-      <c s="38" r="A20"/>
-      <c s="38" r="B20"/>
-      <c s="38" r="C20"/>
-      <c s="38" r="D20"/>
-      <c s="38" r="E20"/>
-      <c s="38" r="F20"/>
+      <c s="39" r="A20"/>
+      <c s="39" r="B20"/>
+      <c s="39" r="C20"/>
+      <c s="39" r="D20"/>
+      <c s="39" r="E20"/>
+      <c s="39" r="F20"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
EWD-22919 - Meaningful "saved" notification
Former-commit-id: 5480b06275025485212de3d445d51ce21320dd4b
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="1274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="1273">
   <si>
     <t>Key</t>
   </si>
@@ -2417,9 +2417,6 @@
   </si>
   <si>
     <t>introApplicationContentDesc</t>
-  </si>
-  <si>
-    <t>How to provide learner with a learning experience?</t>
   </si>
   <si>
     <t>Hoe biedt u cursisten een leerervaring?</t>
@@ -7670,104 +7667,102 @@
       <c t="s" s="23" r="B213">
         <v>798</v>
       </c>
-      <c t="s" s="30" r="C213">
+      <c s="31" r="C213"/>
+      <c t="s" s="43" r="D213">
         <v>799</v>
       </c>
-      <c t="s" s="43" r="D213">
+      <c t="s" s="43" r="E213">
         <v>800</v>
-      </c>
-      <c t="s" s="43" r="E213">
-        <v>801</v>
       </c>
     </row>
     <row r="214">
       <c s="12" r="A214"/>
       <c t="s" s="23" r="B214">
+        <v>801</v>
+      </c>
+      <c t="s" s="31" r="C214">
         <v>802</v>
       </c>
-      <c t="s" s="31" r="C214">
+      <c t="s" s="43" r="D214">
         <v>803</v>
       </c>
-      <c t="s" s="43" r="D214">
+      <c t="s" s="43" r="E214">
         <v>804</v>
-      </c>
-      <c t="s" s="43" r="E214">
-        <v>805</v>
       </c>
     </row>
     <row r="215">
       <c s="12" r="A215"/>
       <c t="s" s="23" r="B215">
+        <v>805</v>
+      </c>
+      <c t="s" s="30" r="C215">
         <v>806</v>
       </c>
-      <c t="s" s="30" r="C215">
+      <c t="s" s="43" r="D215">
         <v>807</v>
       </c>
-      <c t="s" s="43" r="D215">
+      <c t="s" s="43" r="E215">
         <v>808</v>
-      </c>
-      <c t="s" s="43" r="E215">
-        <v>809</v>
       </c>
     </row>
     <row r="216">
       <c s="12" r="A216"/>
       <c t="s" s="23" r="B216">
+        <v>809</v>
+      </c>
+      <c t="s" s="31" r="C216">
         <v>810</v>
       </c>
-      <c t="s" s="31" r="C216">
+      <c t="s" s="43" r="D216">
         <v>811</v>
       </c>
-      <c t="s" s="43" r="D216">
+      <c t="s" s="43" r="E216">
         <v>812</v>
-      </c>
-      <c t="s" s="43" r="E216">
-        <v>813</v>
       </c>
     </row>
     <row r="217">
       <c s="12" r="A217"/>
       <c t="s" s="23" r="B217">
+        <v>813</v>
+      </c>
+      <c t="s" s="30" r="C217">
         <v>814</v>
       </c>
-      <c t="s" s="30" r="C217">
+      <c t="s" s="43" r="D217">
         <v>815</v>
       </c>
-      <c t="s" s="43" r="D217">
+      <c t="s" s="43" r="E217">
         <v>816</v>
-      </c>
-      <c t="s" s="43" r="E217">
-        <v>817</v>
       </c>
     </row>
     <row r="218">
       <c s="12" r="A218"/>
       <c t="s" s="23" r="B218">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c t="s" s="31" r="C218">
         <v>324</v>
       </c>
       <c t="s" s="43" r="D218">
+        <v>818</v>
+      </c>
+      <c t="s" s="43" r="E218">
         <v>819</v>
-      </c>
-      <c t="s" s="43" r="E218">
-        <v>820</v>
       </c>
     </row>
     <row r="219">
       <c s="12" r="A219"/>
       <c t="s" s="23" r="B219">
+        <v>820</v>
+      </c>
+      <c t="s" s="30" r="C219">
         <v>821</v>
       </c>
-      <c t="s" s="30" r="C219">
+      <c t="s" s="43" r="D219">
         <v>822</v>
       </c>
-      <c t="s" s="43" r="D219">
+      <c t="s" s="43" r="E219">
         <v>823</v>
-      </c>
-      <c t="s" s="43" r="E219">
-        <v>824</v>
       </c>
     </row>
     <row r="220">
@@ -7779,109 +7774,109 @@
     </row>
     <row r="221">
       <c t="s" s="12" r="A221">
+        <v>824</v>
+      </c>
+      <c t="s" s="7" r="B221">
         <v>825</v>
       </c>
-      <c t="s" s="7" r="B221">
+      <c t="s" s="15" r="C221">
         <v>826</v>
       </c>
-      <c t="s" s="15" r="C221">
+      <c t="s" s="7" r="D221">
         <v>827</v>
       </c>
-      <c t="s" s="7" r="D221">
+      <c t="s" s="7" r="E221">
         <v>828</v>
-      </c>
-      <c t="s" s="7" r="E221">
-        <v>829</v>
       </c>
     </row>
     <row r="222">
       <c s="12" r="A222"/>
       <c t="s" s="7" r="B222">
+        <v>829</v>
+      </c>
+      <c t="s" s="15" r="C222">
         <v>830</v>
       </c>
-      <c t="s" s="15" r="C222">
+      <c t="s" s="7" r="D222">
         <v>831</v>
       </c>
-      <c t="s" s="7" r="D222">
+      <c t="s" s="7" r="E222">
         <v>832</v>
-      </c>
-      <c t="s" s="7" r="E222">
-        <v>833</v>
       </c>
     </row>
     <row r="223">
       <c s="12" r="A223"/>
       <c t="s" s="7" r="B223">
+        <v>833</v>
+      </c>
+      <c t="s" s="15" r="C223">
         <v>834</v>
       </c>
-      <c t="s" s="15" r="C223">
+      <c t="s" s="7" r="D223">
         <v>835</v>
       </c>
-      <c t="s" s="7" r="D223">
+      <c t="s" s="7" r="E223">
         <v>836</v>
-      </c>
-      <c t="s" s="7" r="E223">
-        <v>837</v>
       </c>
     </row>
     <row r="224">
       <c s="12" r="A224"/>
       <c t="s" s="7" r="B224">
+        <v>837</v>
+      </c>
+      <c t="s" s="15" r="C224">
         <v>838</v>
       </c>
-      <c t="s" s="15" r="C224">
+      <c t="s" s="7" r="D224">
         <v>839</v>
       </c>
-      <c t="s" s="7" r="D224">
+      <c t="s" s="7" r="E224">
         <v>840</v>
-      </c>
-      <c t="s" s="7" r="E224">
-        <v>841</v>
       </c>
     </row>
     <row r="225">
       <c s="12" r="A225"/>
       <c t="s" s="7" r="B225">
+        <v>841</v>
+      </c>
+      <c t="s" s="15" r="C225">
         <v>842</v>
       </c>
-      <c t="s" s="15" r="C225">
+      <c t="s" s="7" r="D225">
         <v>843</v>
       </c>
-      <c t="s" s="7" r="D225">
+      <c t="s" s="7" r="E225">
         <v>844</v>
-      </c>
-      <c t="s" s="7" r="E225">
-        <v>845</v>
       </c>
     </row>
     <row r="226">
       <c s="12" r="A226"/>
       <c t="s" s="7" r="B226">
+        <v>845</v>
+      </c>
+      <c t="s" s="15" r="C226">
         <v>846</v>
       </c>
-      <c t="s" s="15" r="C226">
+      <c t="s" s="7" r="D226">
         <v>847</v>
       </c>
-      <c t="s" s="7" r="D226">
+      <c t="s" s="7" r="E226">
         <v>848</v>
-      </c>
-      <c t="s" s="7" r="E226">
-        <v>849</v>
       </c>
     </row>
     <row r="227">
       <c s="12" r="A227"/>
       <c t="s" s="7" r="B227">
+        <v>849</v>
+      </c>
+      <c t="s" s="15" r="C227">
         <v>850</v>
       </c>
-      <c t="s" s="15" r="C227">
+      <c t="s" s="7" r="D227">
         <v>851</v>
       </c>
-      <c t="s" s="7" r="D227">
+      <c t="s" s="7" r="E227">
         <v>852</v>
-      </c>
-      <c t="s" s="7" r="E227">
-        <v>853</v>
       </c>
     </row>
     <row r="228">
@@ -7893,13 +7888,13 @@
     </row>
     <row r="229">
       <c t="s" s="12" r="A229">
+        <v>853</v>
+      </c>
+      <c t="s" s="36" r="B229">
         <v>854</v>
       </c>
-      <c t="s" s="36" r="B229">
-        <v>855</v>
-      </c>
       <c t="s" s="25" r="C229">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c s="36" r="D229"/>
       <c s="36" r="E229"/>
@@ -7913,13 +7908,13 @@
     </row>
     <row r="231">
       <c t="s" s="12" r="A231">
+        <v>855</v>
+      </c>
+      <c t="s" s="44" r="B231">
         <v>856</v>
       </c>
-      <c t="s" s="44" r="B231">
+      <c t="s" s="41" r="C231">
         <v>857</v>
-      </c>
-      <c t="s" s="41" r="C231">
-        <v>858</v>
       </c>
       <c s="44" r="D231"/>
       <c s="44" r="E231"/>
@@ -7927,10 +7922,10 @@
     <row r="232">
       <c s="12" r="A232"/>
       <c t="s" s="44" r="B232">
+        <v>858</v>
+      </c>
+      <c t="s" s="41" r="C232">
         <v>859</v>
-      </c>
-      <c t="s" s="41" r="C232">
-        <v>860</v>
       </c>
       <c s="44" r="D232"/>
       <c s="44" r="E232"/>
@@ -7944,139 +7939,139 @@
     </row>
     <row r="234">
       <c t="s" s="12" r="A234">
+        <v>860</v>
+      </c>
+      <c t="s" s="33" r="B234">
         <v>861</v>
       </c>
-      <c t="s" s="33" r="B234">
+      <c t="s" s="33" r="C234">
         <v>862</v>
       </c>
-      <c t="s" s="33" r="C234">
+      <c t="s" s="7" r="D234">
         <v>863</v>
       </c>
-      <c t="s" s="7" r="D234">
+      <c t="s" s="7" r="E234">
         <v>864</v>
-      </c>
-      <c t="s" s="7" r="E234">
-        <v>865</v>
       </c>
     </row>
     <row r="235">
       <c s="12" r="A235"/>
       <c t="s" s="33" r="B235">
+        <v>865</v>
+      </c>
+      <c t="s" s="33" r="C235">
         <v>866</v>
       </c>
-      <c t="s" s="33" r="C235">
+      <c t="s" s="7" r="D235">
+        <v>866</v>
+      </c>
+      <c t="s" s="7" r="E235">
         <v>867</v>
-      </c>
-      <c t="s" s="7" r="D235">
-        <v>867</v>
-      </c>
-      <c t="s" s="7" r="E235">
-        <v>868</v>
       </c>
     </row>
     <row r="236">
       <c s="12" r="A236"/>
       <c t="s" s="33" r="B236">
+        <v>868</v>
+      </c>
+      <c t="s" s="33" r="C236">
         <v>869</v>
       </c>
-      <c t="s" s="33" r="C236">
+      <c t="s" s="7" r="D236">
         <v>870</v>
       </c>
-      <c t="s" s="7" r="D236">
+      <c t="s" s="7" r="E236">
         <v>871</v>
-      </c>
-      <c t="s" s="7" r="E236">
-        <v>872</v>
       </c>
     </row>
     <row r="237">
       <c s="12" r="A237"/>
       <c t="s" s="33" r="B237">
+        <v>872</v>
+      </c>
+      <c t="s" s="33" r="C237">
         <v>873</v>
       </c>
-      <c t="s" s="33" r="C237">
+      <c t="s" s="7" r="D237">
         <v>874</v>
       </c>
-      <c t="s" s="7" r="D237">
+      <c t="s" s="7" r="E237">
         <v>875</v>
-      </c>
-      <c t="s" s="7" r="E237">
-        <v>876</v>
       </c>
     </row>
     <row r="238">
       <c s="12" r="A238"/>
       <c t="s" s="15" r="B238">
+        <v>876</v>
+      </c>
+      <c t="s" s="15" r="C238">
         <v>877</v>
       </c>
-      <c t="s" s="15" r="C238">
+      <c t="s" s="7" r="D238">
         <v>878</v>
       </c>
-      <c t="s" s="7" r="D238">
+      <c t="s" s="7" r="E238">
         <v>879</v>
-      </c>
-      <c t="s" s="7" r="E238">
-        <v>880</v>
       </c>
     </row>
     <row r="239">
       <c s="12" r="A239"/>
       <c t="s" s="15" r="B239">
+        <v>880</v>
+      </c>
+      <c t="s" s="15" r="C239">
         <v>881</v>
       </c>
-      <c t="s" s="15" r="C239">
+      <c t="s" s="7" r="D239">
         <v>882</v>
       </c>
-      <c t="s" s="7" r="D239">
+      <c t="s" s="7" r="E239">
         <v>883</v>
-      </c>
-      <c t="s" s="7" r="E239">
-        <v>884</v>
       </c>
     </row>
     <row r="240">
       <c s="12" r="A240"/>
       <c t="s" s="15" r="B240">
+        <v>884</v>
+      </c>
+      <c t="s" s="15" r="C240">
         <v>885</v>
       </c>
-      <c t="s" s="15" r="C240">
+      <c t="s" s="7" r="D240">
         <v>886</v>
       </c>
-      <c t="s" s="7" r="D240">
+      <c t="s" s="7" r="E240">
         <v>887</v>
-      </c>
-      <c t="s" s="7" r="E240">
-        <v>888</v>
       </c>
     </row>
     <row r="241">
       <c s="12" r="A241"/>
       <c t="s" s="15" r="B241">
+        <v>888</v>
+      </c>
+      <c t="s" s="15" r="C241">
         <v>889</v>
       </c>
-      <c t="s" s="15" r="C241">
+      <c t="s" s="7" r="D241">
         <v>890</v>
       </c>
-      <c t="s" s="7" r="D241">
+      <c t="s" s="7" r="E241">
         <v>891</v>
-      </c>
-      <c t="s" s="7" r="E241">
-        <v>892</v>
       </c>
     </row>
     <row r="242">
       <c s="12" r="A242"/>
       <c t="s" s="15" r="B242">
+        <v>892</v>
+      </c>
+      <c t="s" s="15" r="C242">
         <v>893</v>
       </c>
-      <c t="s" s="15" r="C242">
+      <c t="s" s="7" r="D242">
         <v>894</v>
       </c>
-      <c t="s" s="7" r="D242">
+      <c t="s" s="7" r="E242">
         <v>895</v>
-      </c>
-      <c t="s" s="7" r="E242">
-        <v>896</v>
       </c>
     </row>
     <row r="243">
@@ -8089,166 +8084,166 @@
     <row r="244">
       <c s="12" r="A244"/>
       <c t="s" s="15" r="B244">
+        <v>896</v>
+      </c>
+      <c t="s" s="15" r="C244">
         <v>897</v>
       </c>
-      <c t="s" s="15" r="C244">
+      <c t="s" s="7" r="D244">
         <v>898</v>
       </c>
-      <c t="s" s="7" r="D244">
+      <c t="s" s="7" r="E244">
         <v>899</v>
-      </c>
-      <c t="s" s="7" r="E244">
-        <v>900</v>
       </c>
     </row>
     <row r="245">
       <c s="12" r="A245"/>
       <c t="s" s="7" r="B245">
+        <v>900</v>
+      </c>
+      <c t="s" s="15" r="C245">
         <v>901</v>
       </c>
-      <c t="s" s="15" r="C245">
+      <c t="s" s="7" r="D245">
         <v>902</v>
       </c>
-      <c t="s" s="7" r="D245">
+      <c t="s" s="7" r="E245">
         <v>903</v>
-      </c>
-      <c t="s" s="7" r="E245">
-        <v>904</v>
       </c>
     </row>
     <row r="246">
       <c s="12" r="A246"/>
       <c t="s" s="7" r="B246">
+        <v>904</v>
+      </c>
+      <c t="s" s="15" r="C246">
         <v>905</v>
       </c>
-      <c t="s" s="15" r="C246">
+      <c t="s" s="7" r="D246">
         <v>906</v>
       </c>
-      <c t="s" s="7" r="D246">
+      <c t="s" s="7" r="E246">
         <v>907</v>
-      </c>
-      <c t="s" s="7" r="E246">
-        <v>908</v>
       </c>
     </row>
     <row r="247">
       <c s="12" r="A247"/>
       <c t="s" s="7" r="B247">
+        <v>908</v>
+      </c>
+      <c t="s" s="15" r="C247">
         <v>909</v>
       </c>
-      <c t="s" s="15" r="C247">
+      <c t="s" s="7" r="D247">
         <v>910</v>
       </c>
-      <c t="s" s="7" r="D247">
+      <c t="s" s="7" r="E247">
         <v>911</v>
-      </c>
-      <c t="s" s="7" r="E247">
-        <v>912</v>
       </c>
     </row>
     <row r="248">
       <c s="12" r="A248"/>
       <c t="s" s="7" r="B248">
+        <v>912</v>
+      </c>
+      <c t="s" s="15" r="C248">
         <v>913</v>
       </c>
-      <c t="s" s="15" r="C248">
+      <c t="s" s="7" r="D248">
         <v>914</v>
       </c>
-      <c t="s" s="7" r="D248">
+      <c t="s" s="7" r="E248">
         <v>915</v>
-      </c>
-      <c t="s" s="7" r="E248">
-        <v>916</v>
       </c>
     </row>
     <row r="249">
       <c s="12" r="A249"/>
       <c t="s" s="7" r="B249">
+        <v>916</v>
+      </c>
+      <c t="s" s="15" r="C249">
         <v>917</v>
       </c>
-      <c t="s" s="15" r="C249">
+      <c t="s" s="30" r="D249">
         <v>918</v>
       </c>
-      <c t="s" s="30" r="D249">
+      <c t="s" s="30" r="E249">
         <v>919</v>
-      </c>
-      <c t="s" s="30" r="E249">
-        <v>920</v>
       </c>
     </row>
     <row r="250">
       <c s="12" r="A250"/>
       <c t="s" s="7" r="B250">
+        <v>920</v>
+      </c>
+      <c t="s" s="15" r="C250">
         <v>921</v>
       </c>
-      <c t="s" s="15" r="C250">
+      <c t="s" s="7" r="D250">
         <v>922</v>
       </c>
-      <c t="s" s="7" r="D250">
+      <c t="s" s="7" r="E250">
         <v>923</v>
-      </c>
-      <c t="s" s="7" r="E250">
-        <v>924</v>
       </c>
     </row>
     <row r="251">
       <c s="12" r="A251"/>
       <c t="s" s="7" r="B251">
+        <v>924</v>
+      </c>
+      <c t="s" s="15" r="C251">
         <v>925</v>
       </c>
-      <c t="s" s="15" r="C251">
+      <c t="s" s="7" r="D251">
         <v>926</v>
       </c>
-      <c t="s" s="7" r="D251">
+      <c t="s" s="7" r="E251">
         <v>927</v>
-      </c>
-      <c t="s" s="7" r="E251">
-        <v>928</v>
       </c>
     </row>
     <row r="252">
       <c s="12" r="A252"/>
       <c t="s" s="7" r="B252">
+        <v>928</v>
+      </c>
+      <c t="s" s="15" r="C252">
         <v>929</v>
       </c>
-      <c t="s" s="15" r="C252">
+      <c t="s" s="7" r="D252">
         <v>930</v>
       </c>
-      <c t="s" s="7" r="D252">
+      <c t="s" s="7" r="E252">
         <v>931</v>
-      </c>
-      <c t="s" s="7" r="E252">
-        <v>932</v>
       </c>
     </row>
     <row r="253">
       <c s="12" r="A253"/>
       <c t="s" s="7" r="B253">
+        <v>932</v>
+      </c>
+      <c t="s" s="15" r="C253">
         <v>933</v>
       </c>
-      <c t="s" s="15" r="C253">
+      <c t="s" s="7" r="D253">
         <v>934</v>
       </c>
-      <c t="s" s="7" r="D253">
+      <c t="s" s="7" r="E253">
         <v>935</v>
-      </c>
-      <c t="s" s="7" r="E253">
-        <v>936</v>
       </c>
     </row>
     <row r="254">
       <c s="12" r="A254"/>
       <c t="s" s="7" r="B254">
+        <v>936</v>
+      </c>
+      <c t="s" s="15" r="C254">
         <v>937</v>
       </c>
-      <c t="s" s="15" r="C254">
+      <c t="s" s="7" r="D254">
         <v>938</v>
       </c>
-      <c t="s" s="7" r="D254">
+      <c t="s" s="7" r="E254">
         <v>939</v>
-      </c>
-      <c t="s" s="7" r="E254">
-        <v>940</v>
       </c>
     </row>
     <row r="255">
@@ -8260,78 +8255,78 @@
     </row>
     <row r="256">
       <c t="s" s="12" r="A256">
+        <v>940</v>
+      </c>
+      <c t="s" s="33" r="B256">
         <v>941</v>
       </c>
-      <c t="s" s="33" r="B256">
-        <v>942</v>
-      </c>
       <c t="s" s="7" r="C256">
+        <v>866</v>
+      </c>
+      <c t="s" s="7" r="D256">
+        <v>866</v>
+      </c>
+      <c t="s" s="7" r="E256">
         <v>867</v>
-      </c>
-      <c t="s" s="7" r="D256">
-        <v>867</v>
-      </c>
-      <c t="s" s="7" r="E256">
-        <v>868</v>
       </c>
     </row>
     <row r="257">
       <c s="12" r="A257"/>
       <c t="s" s="7" r="B257">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c t="s" s="15" r="C257">
+        <v>869</v>
+      </c>
+      <c t="s" s="7" r="D257">
         <v>870</v>
       </c>
-      <c t="s" s="7" r="D257">
+      <c t="s" s="7" r="E257">
         <v>871</v>
-      </c>
-      <c t="s" s="7" r="E257">
-        <v>872</v>
       </c>
     </row>
     <row r="258">
       <c t="s" s="7" r="B258">
+        <v>943</v>
+      </c>
+      <c t="s" s="15" r="C258">
         <v>944</v>
       </c>
-      <c t="s" s="15" r="C258">
+      <c t="s" s="7" r="D258">
         <v>945</v>
       </c>
-      <c t="s" s="7" r="D258">
+      <c t="s" s="7" r="E258">
         <v>946</v>
-      </c>
-      <c t="s" s="7" r="E258">
-        <v>947</v>
       </c>
     </row>
     <row r="259">
       <c s="12" r="A259"/>
       <c t="s" s="7" r="B259">
+        <v>947</v>
+      </c>
+      <c t="s" s="15" r="C259">
         <v>948</v>
       </c>
-      <c t="s" s="15" r="C259">
+      <c t="s" s="7" r="D259">
         <v>949</v>
       </c>
-      <c t="s" s="7" r="D259">
+      <c t="s" s="7" r="E259">
         <v>950</v>
-      </c>
-      <c t="s" s="7" r="E259">
-        <v>951</v>
       </c>
     </row>
     <row r="260">
       <c s="12" r="A260"/>
       <c t="s" s="7" r="B260">
+        <v>951</v>
+      </c>
+      <c t="s" s="15" r="C260">
         <v>952</v>
       </c>
-      <c t="s" s="15" r="C260">
+      <c t="s" s="7" r="D260">
         <v>953</v>
       </c>
-      <c t="s" s="7" r="D260">
+      <c t="s" s="7" r="E260">
         <v>954</v>
-      </c>
-      <c t="s" s="7" r="E260">
-        <v>955</v>
       </c>
     </row>
     <row r="261">
@@ -8343,109 +8338,109 @@
     </row>
     <row r="262">
       <c t="s" s="12" r="A262">
+        <v>955</v>
+      </c>
+      <c t="s" s="7" r="B262">
         <v>956</v>
       </c>
-      <c t="s" s="7" r="B262">
+      <c t="s" s="15" r="C262">
+        <v>955</v>
+      </c>
+      <c t="s" s="7" r="D262">
         <v>957</v>
       </c>
-      <c t="s" s="15" r="C262">
-        <v>956</v>
-      </c>
-      <c t="s" s="7" r="D262">
+      <c t="s" s="7" r="E262">
         <v>958</v>
-      </c>
-      <c t="s" s="7" r="E262">
-        <v>959</v>
       </c>
     </row>
     <row r="263">
       <c s="12" r="A263"/>
       <c t="s" s="7" r="B263">
+        <v>959</v>
+      </c>
+      <c t="s" s="15" r="C263">
         <v>960</v>
       </c>
-      <c t="s" s="15" r="C263">
+      <c t="s" s="7" r="D263">
         <v>961</v>
       </c>
-      <c t="s" s="7" r="D263">
+      <c t="s" s="7" r="E263">
         <v>962</v>
-      </c>
-      <c t="s" s="7" r="E263">
-        <v>963</v>
       </c>
     </row>
     <row r="264">
       <c s="12" r="A264"/>
       <c t="s" s="7" r="B264">
+        <v>963</v>
+      </c>
+      <c t="s" s="15" r="C264">
         <v>964</v>
       </c>
-      <c t="s" s="15" r="C264">
+      <c t="s" s="7" r="D264">
         <v>965</v>
       </c>
-      <c t="s" s="7" r="D264">
+      <c t="s" s="7" r="E264">
         <v>966</v>
-      </c>
-      <c t="s" s="7" r="E264">
-        <v>967</v>
       </c>
     </row>
     <row r="265">
       <c s="12" r="A265"/>
       <c t="s" s="7" r="B265">
+        <v>967</v>
+      </c>
+      <c t="s" s="15" r="C265">
         <v>968</v>
       </c>
-      <c t="s" s="15" r="C265">
+      <c t="s" s="7" r="D265">
         <v>969</v>
       </c>
-      <c t="s" s="7" r="D265">
+      <c t="s" s="7" r="E265">
         <v>970</v>
-      </c>
-      <c t="s" s="7" r="E265">
-        <v>971</v>
       </c>
     </row>
     <row r="266">
       <c s="12" r="A266"/>
       <c t="s" s="7" r="B266">
+        <v>971</v>
+      </c>
+      <c t="s" s="15" r="C266">
         <v>972</v>
       </c>
-      <c t="s" s="15" r="C266">
+      <c t="s" s="7" r="D266">
         <v>973</v>
       </c>
-      <c t="s" s="7" r="D266">
+      <c t="s" s="7" r="E266">
         <v>974</v>
-      </c>
-      <c t="s" s="7" r="E266">
-        <v>975</v>
       </c>
     </row>
     <row r="267">
       <c s="12" r="A267"/>
       <c t="s" s="7" r="B267">
+        <v>975</v>
+      </c>
+      <c t="s" s="15" r="C267">
         <v>976</v>
       </c>
-      <c t="s" s="15" r="C267">
+      <c t="s" s="7" r="D267">
         <v>977</v>
       </c>
-      <c t="s" s="7" r="D267">
+      <c t="s" s="7" r="E267">
         <v>978</v>
-      </c>
-      <c t="s" s="7" r="E267">
-        <v>979</v>
       </c>
     </row>
     <row r="268">
       <c s="12" r="A268"/>
       <c t="s" s="7" r="B268">
+        <v>979</v>
+      </c>
+      <c t="s" s="15" r="C268">
         <v>980</v>
       </c>
-      <c t="s" s="15" r="C268">
+      <c t="s" s="7" r="D268">
         <v>981</v>
       </c>
-      <c t="s" s="7" r="D268">
+      <c t="s" s="7" r="E268">
         <v>982</v>
-      </c>
-      <c t="s" s="7" r="E268">
-        <v>983</v>
       </c>
     </row>
     <row r="269">
@@ -8457,34 +8452,34 @@
     </row>
     <row r="270">
       <c t="s" s="12" r="A270">
+        <v>983</v>
+      </c>
+      <c t="s" s="7" r="B270">
         <v>984</v>
       </c>
-      <c t="s" s="7" r="B270">
+      <c t="s" s="15" r="C270">
         <v>985</v>
       </c>
-      <c t="s" s="15" r="C270">
+      <c t="s" s="7" r="D270">
         <v>986</v>
       </c>
-      <c t="s" s="7" r="D270">
+      <c t="s" s="7" r="E270">
         <v>987</v>
-      </c>
-      <c t="s" s="7" r="E270">
-        <v>988</v>
       </c>
     </row>
     <row r="271">
       <c s="12" r="A271"/>
       <c t="s" s="7" r="B271">
+        <v>988</v>
+      </c>
+      <c t="s" s="15" r="C271">
         <v>989</v>
       </c>
-      <c t="s" s="15" r="C271">
+      <c t="s" s="7" r="D271">
+        <v>989</v>
+      </c>
+      <c t="s" s="7" r="E271">
         <v>990</v>
-      </c>
-      <c t="s" s="7" r="D271">
-        <v>990</v>
-      </c>
-      <c t="s" s="7" r="E271">
-        <v>991</v>
       </c>
     </row>
     <row r="272">
@@ -8496,64 +8491,64 @@
     </row>
     <row r="273">
       <c t="s" s="12" r="A273">
+        <v>991</v>
+      </c>
+      <c t="s" s="7" r="B273">
         <v>992</v>
       </c>
-      <c t="s" s="7" r="B273">
+      <c t="s" s="15" r="C273">
         <v>993</v>
       </c>
-      <c t="s" s="15" r="C273">
+      <c t="s" s="7" r="D273">
         <v>994</v>
       </c>
-      <c t="s" s="7" r="D273">
+      <c t="s" s="7" r="E273">
         <v>995</v>
-      </c>
-      <c t="s" s="7" r="E273">
-        <v>996</v>
       </c>
     </row>
     <row r="274">
       <c s="12" r="A274"/>
       <c t="s" s="7" r="B274">
+        <v>996</v>
+      </c>
+      <c t="s" s="15" r="C274">
         <v>997</v>
       </c>
-      <c t="s" s="15" r="C274">
+      <c t="s" s="7" r="D274">
         <v>998</v>
       </c>
-      <c t="s" s="7" r="D274">
+      <c t="s" s="7" r="E274">
         <v>999</v>
-      </c>
-      <c t="s" s="7" r="E274">
-        <v>1000</v>
       </c>
     </row>
     <row r="275">
       <c s="12" r="A275"/>
       <c t="s" s="7" r="B275">
+        <v>1000</v>
+      </c>
+      <c t="s" s="15" r="C275">
         <v>1001</v>
       </c>
-      <c t="s" s="15" r="C275">
+      <c t="s" s="7" r="D275">
         <v>1002</v>
       </c>
-      <c t="s" s="7" r="D275">
+      <c t="s" s="7" r="E275">
         <v>1003</v>
-      </c>
-      <c t="s" s="7" r="E275">
-        <v>1004</v>
       </c>
     </row>
     <row r="276">
       <c s="12" r="A276"/>
       <c t="s" s="7" r="B276">
+        <v>1004</v>
+      </c>
+      <c t="s" s="15" r="C276">
         <v>1005</v>
       </c>
-      <c t="s" s="15" r="C276">
+      <c t="s" s="7" r="D276">
         <v>1006</v>
       </c>
-      <c t="s" s="7" r="D276">
+      <c t="s" s="7" r="E276">
         <v>1007</v>
-      </c>
-      <c t="s" s="7" r="E276">
-        <v>1008</v>
       </c>
     </row>
     <row r="277">
@@ -8565,34 +8560,34 @@
     </row>
     <row r="278">
       <c t="s" s="12" r="A278">
+        <v>1008</v>
+      </c>
+      <c t="s" s="7" r="B278">
         <v>1009</v>
       </c>
-      <c t="s" s="7" r="B278">
+      <c t="s" s="15" r="C278">
         <v>1010</v>
       </c>
-      <c t="s" s="15" r="C278">
+      <c t="s" s="7" r="D278">
         <v>1011</v>
       </c>
-      <c t="s" s="7" r="D278">
+      <c t="s" s="7" r="E278">
         <v>1012</v>
-      </c>
-      <c t="s" s="7" r="E278">
-        <v>1013</v>
       </c>
     </row>
     <row r="279">
       <c s="12" r="A279"/>
       <c t="s" s="7" r="B279">
+        <v>1013</v>
+      </c>
+      <c t="s" s="15" r="C279">
         <v>1014</v>
       </c>
-      <c t="s" s="15" r="C279">
+      <c t="s" s="7" r="D279">
         <v>1015</v>
       </c>
-      <c t="s" s="7" r="D279">
+      <c t="s" s="7" r="E279">
         <v>1016</v>
-      </c>
-      <c t="s" s="7" r="E279">
-        <v>1017</v>
       </c>
     </row>
     <row r="280">
@@ -8604,19 +8599,19 @@
     </row>
     <row r="281">
       <c t="s" s="12" r="A281">
+        <v>1017</v>
+      </c>
+      <c t="s" s="7" r="B281">
         <v>1018</v>
       </c>
-      <c t="s" s="7" r="B281">
+      <c t="s" s="15" r="C281">
         <v>1019</v>
       </c>
-      <c t="s" s="15" r="C281">
+      <c t="s" s="7" r="D281">
         <v>1020</v>
       </c>
-      <c t="s" s="7" r="D281">
+      <c t="s" s="7" r="E281">
         <v>1021</v>
-      </c>
-      <c t="s" s="7" r="E281">
-        <v>1022</v>
       </c>
     </row>
     <row r="282">
@@ -8628,124 +8623,124 @@
     </row>
     <row r="283">
       <c t="s" s="12" r="A283">
+        <v>1022</v>
+      </c>
+      <c t="s" s="7" r="B283">
         <v>1023</v>
       </c>
-      <c t="s" s="7" r="B283">
+      <c t="s" s="15" r="C283">
         <v>1024</v>
       </c>
-      <c t="s" s="15" r="C283">
+      <c t="s" s="7" r="D283">
         <v>1025</v>
       </c>
-      <c t="s" s="7" r="D283">
+      <c t="s" s="7" r="E283">
         <v>1026</v>
-      </c>
-      <c t="s" s="7" r="E283">
-        <v>1027</v>
       </c>
     </row>
     <row r="284">
       <c s="12" r="A284"/>
       <c t="s" s="7" r="B284">
+        <v>1027</v>
+      </c>
+      <c t="s" s="15" r="C284">
         <v>1028</v>
       </c>
-      <c t="s" s="15" r="C284">
+      <c t="s" s="7" r="D284">
         <v>1029</v>
       </c>
-      <c t="s" s="7" r="D284">
+      <c t="s" s="7" r="E284">
         <v>1030</v>
-      </c>
-      <c t="s" s="7" r="E284">
-        <v>1031</v>
       </c>
     </row>
     <row r="285">
       <c s="12" r="A285"/>
       <c t="s" s="7" r="B285">
+        <v>1031</v>
+      </c>
+      <c t="s" s="15" r="C285">
         <v>1032</v>
       </c>
-      <c t="s" s="15" r="C285">
+      <c t="s" s="7" r="D285">
         <v>1033</v>
       </c>
-      <c t="s" s="7" r="D285">
+      <c t="s" s="7" r="E285">
         <v>1034</v>
-      </c>
-      <c t="s" s="7" r="E285">
-        <v>1035</v>
       </c>
     </row>
     <row r="286">
       <c s="12" r="A286"/>
       <c t="s" s="7" r="B286">
+        <v>1035</v>
+      </c>
+      <c t="s" s="15" r="C286">
         <v>1036</v>
       </c>
-      <c t="s" s="15" r="C286">
+      <c t="s" s="7" r="D286">
         <v>1037</v>
       </c>
-      <c t="s" s="7" r="D286">
+      <c t="s" s="7" r="E286">
         <v>1038</v>
-      </c>
-      <c t="s" s="7" r="E286">
-        <v>1039</v>
       </c>
     </row>
     <row r="287">
       <c s="12" r="A287"/>
       <c t="s" s="7" r="B287">
+        <v>1039</v>
+      </c>
+      <c t="s" s="15" r="C287">
         <v>1040</v>
       </c>
-      <c t="s" s="15" r="C287">
+      <c t="s" s="7" r="D287">
         <v>1041</v>
       </c>
-      <c t="s" s="7" r="D287">
+      <c t="s" s="7" r="E287">
         <v>1042</v>
-      </c>
-      <c t="s" s="7" r="E287">
-        <v>1043</v>
       </c>
     </row>
     <row r="288">
       <c s="12" r="A288"/>
       <c t="s" s="7" r="B288">
+        <v>1043</v>
+      </c>
+      <c t="s" s="15" r="C288">
         <v>1044</v>
       </c>
-      <c t="s" s="15" r="C288">
+      <c t="s" s="7" r="D288">
         <v>1045</v>
       </c>
-      <c t="s" s="7" r="D288">
+      <c t="s" s="7" r="E288">
         <v>1046</v>
-      </c>
-      <c t="s" s="7" r="E288">
-        <v>1047</v>
       </c>
     </row>
     <row r="289">
       <c s="12" r="A289"/>
       <c t="s" s="7" r="B289">
+        <v>1047</v>
+      </c>
+      <c t="s" s="15" r="C289">
         <v>1048</v>
       </c>
-      <c t="s" s="15" r="C289">
+      <c t="s" s="7" r="D289">
         <v>1049</v>
       </c>
-      <c t="s" s="7" r="D289">
+      <c t="s" s="7" r="E289">
         <v>1050</v>
-      </c>
-      <c t="s" s="7" r="E289">
-        <v>1051</v>
       </c>
     </row>
     <row r="290">
       <c s="12" r="A290"/>
       <c t="s" s="7" r="B290">
+        <v>1051</v>
+      </c>
+      <c t="s" s="15" r="C290">
         <v>1052</v>
       </c>
-      <c t="s" s="15" r="C290">
+      <c t="s" s="7" r="D290">
         <v>1053</v>
       </c>
-      <c t="s" s="7" r="D290">
+      <c t="s" s="7" r="E290">
         <v>1054</v>
-      </c>
-      <c t="s" s="7" r="E290">
-        <v>1055</v>
       </c>
     </row>
     <row r="291">
@@ -8757,70 +8752,70 @@
     </row>
     <row r="292">
       <c t="s" s="12" r="A292">
+        <v>1055</v>
+      </c>
+      <c t="s" s="7" r="B292">
         <v>1056</v>
       </c>
-      <c t="s" s="7" r="B292">
+      <c t="s" s="7" r="C292">
         <v>1057</v>
       </c>
-      <c t="s" s="7" r="C292">
+      <c t="s" s="7" r="D292">
         <v>1058</v>
       </c>
-      <c t="s" s="7" r="D292">
+      <c t="s" s="7" r="E292">
         <v>1059</v>
-      </c>
-      <c t="s" s="7" r="E292">
-        <v>1060</v>
       </c>
     </row>
     <row r="293">
       <c s="12" r="A293"/>
       <c t="s" s="7" r="B293">
+        <v>1060</v>
+      </c>
+      <c t="s" s="15" r="C293">
         <v>1061</v>
       </c>
-      <c t="s" s="15" r="C293">
+      <c t="s" s="7" r="D293">
         <v>1062</v>
       </c>
-      <c t="s" s="7" r="D293">
+      <c t="s" s="7" r="E293">
         <v>1063</v>
-      </c>
-      <c t="s" s="7" r="E293">
-        <v>1064</v>
       </c>
     </row>
     <row r="294">
       <c s="12" r="A294"/>
       <c t="s" s="7" r="B294">
+        <v>1064</v>
+      </c>
+      <c t="s" s="15" r="C294">
         <v>1065</v>
       </c>
-      <c t="s" s="15" r="C294">
+      <c t="s" s="7" r="D294">
         <v>1066</v>
       </c>
-      <c t="s" s="7" r="D294">
+      <c t="s" s="7" r="E294">
         <v>1067</v>
-      </c>
-      <c t="s" s="7" r="E294">
-        <v>1068</v>
       </c>
     </row>
     <row r="295">
       <c s="12" r="A295"/>
       <c t="s" s="7" r="B295">
+        <v>1068</v>
+      </c>
+      <c t="s" s="15" r="C295">
+        <v>802</v>
+      </c>
+      <c t="s" s="7" r="D295">
         <v>1069</v>
       </c>
-      <c t="s" s="15" r="C295">
-        <v>803</v>
-      </c>
-      <c t="s" s="7" r="D295">
+      <c t="s" s="7" r="E295">
         <v>1070</v>
-      </c>
-      <c t="s" s="7" r="E295">
-        <v>1071</v>
       </c>
     </row>
     <row r="296">
       <c s="12" r="A296"/>
       <c t="s" s="7" r="B296">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c t="s" s="15" r="C296">
         <v>696</v>
@@ -8835,16 +8830,16 @@
     <row r="297">
       <c s="12" r="A297"/>
       <c t="s" s="7" r="B297">
+        <v>1072</v>
+      </c>
+      <c t="s" s="15" r="C297">
         <v>1073</v>
       </c>
-      <c t="s" s="15" r="C297">
+      <c t="s" s="7" r="D297">
         <v>1074</v>
       </c>
-      <c t="s" s="7" r="D297">
+      <c t="s" s="7" r="E297">
         <v>1075</v>
-      </c>
-      <c t="s" s="7" r="E297">
-        <v>1076</v>
       </c>
     </row>
     <row r="298">
@@ -8856,304 +8851,304 @@
     </row>
     <row r="299">
       <c t="s" s="12" r="A299">
+        <v>1076</v>
+      </c>
+      <c t="s" s="7" r="B299">
         <v>1077</v>
       </c>
-      <c t="s" s="7" r="B299">
+      <c t="s" s="15" r="C299">
         <v>1078</v>
       </c>
-      <c t="s" s="15" r="C299">
+      <c t="s" s="7" r="D299">
         <v>1079</v>
       </c>
-      <c t="s" s="7" r="D299">
+      <c t="s" s="7" r="E299">
         <v>1080</v>
-      </c>
-      <c t="s" s="7" r="E299">
-        <v>1081</v>
       </c>
     </row>
     <row r="300">
       <c s="12" r="A300"/>
       <c t="s" s="7" r="B300">
+        <v>1081</v>
+      </c>
+      <c t="s" s="15" r="C300">
         <v>1082</v>
       </c>
-      <c t="s" s="15" r="C300">
+      <c t="s" s="7" r="D300">
         <v>1083</v>
       </c>
-      <c t="s" s="7" r="D300">
+      <c t="s" s="7" r="E300">
         <v>1084</v>
-      </c>
-      <c t="s" s="7" r="E300">
-        <v>1085</v>
       </c>
     </row>
     <row r="301">
       <c s="12" r="A301"/>
       <c t="s" s="7" r="B301">
+        <v>1085</v>
+      </c>
+      <c t="s" s="15" r="C301">
         <v>1086</v>
       </c>
-      <c t="s" s="15" r="C301">
+      <c t="s" s="7" r="D301">
         <v>1087</v>
       </c>
-      <c t="s" s="7" r="D301">
+      <c t="s" s="7" r="E301">
         <v>1088</v>
-      </c>
-      <c t="s" s="7" r="E301">
-        <v>1089</v>
       </c>
     </row>
     <row r="302">
       <c s="12" r="A302"/>
       <c t="s" s="7" r="B302">
+        <v>1089</v>
+      </c>
+      <c t="s" s="15" r="C302">
         <v>1090</v>
       </c>
-      <c t="s" s="15" r="C302">
+      <c t="s" s="7" r="D302">
         <v>1091</v>
       </c>
-      <c t="s" s="7" r="D302">
-        <v>1092</v>
-      </c>
       <c t="s" s="7" r="E302">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="303">
       <c s="12" r="A303"/>
       <c t="s" s="7" r="B303">
+        <v>1092</v>
+      </c>
+      <c t="s" s="15" r="C303">
         <v>1093</v>
       </c>
-      <c t="s" s="15" r="C303">
+      <c t="s" s="7" r="D303">
         <v>1094</v>
       </c>
-      <c t="s" s="7" r="D303">
+      <c t="s" s="7" r="E303">
         <v>1095</v>
-      </c>
-      <c t="s" s="7" r="E303">
-        <v>1096</v>
       </c>
     </row>
     <row r="304">
       <c s="12" r="A304"/>
       <c t="s" s="7" r="B304">
+        <v>1096</v>
+      </c>
+      <c t="s" s="15" r="C304">
         <v>1097</v>
       </c>
-      <c t="s" s="15" r="C304">
+      <c t="s" s="7" r="D304">
         <v>1098</v>
       </c>
-      <c t="s" s="7" r="D304">
+      <c t="s" s="7" r="E304">
         <v>1099</v>
-      </c>
-      <c t="s" s="7" r="E304">
-        <v>1100</v>
       </c>
     </row>
     <row r="305">
       <c s="12" r="A305"/>
       <c t="s" s="7" r="B305">
+        <v>1100</v>
+      </c>
+      <c t="s" s="15" r="C305">
         <v>1101</v>
       </c>
-      <c t="s" s="15" r="C305">
+      <c t="s" s="7" r="D305">
         <v>1102</v>
       </c>
-      <c t="s" s="7" r="D305">
+      <c t="s" s="7" r="E305">
         <v>1103</v>
-      </c>
-      <c t="s" s="7" r="E305">
-        <v>1104</v>
       </c>
     </row>
     <row r="306">
       <c s="12" r="A306"/>
       <c t="s" s="7" r="B306">
+        <v>1104</v>
+      </c>
+      <c t="s" s="15" r="C306">
         <v>1105</v>
       </c>
-      <c t="s" s="15" r="C306">
+      <c t="s" s="7" r="D306">
         <v>1106</v>
       </c>
-      <c t="s" s="7" r="D306">
+      <c t="s" s="7" r="E306">
         <v>1107</v>
-      </c>
-      <c t="s" s="7" r="E306">
-        <v>1108</v>
       </c>
     </row>
     <row r="307">
       <c s="12" r="A307"/>
       <c t="s" s="7" r="B307">
+        <v>1108</v>
+      </c>
+      <c t="s" s="15" r="C307">
         <v>1109</v>
       </c>
-      <c t="s" s="15" r="C307">
+      <c t="s" s="7" r="D307">
         <v>1110</v>
       </c>
-      <c t="s" s="7" r="D307">
+      <c t="s" s="7" r="E307">
         <v>1111</v>
-      </c>
-      <c t="s" s="7" r="E307">
-        <v>1112</v>
       </c>
     </row>
     <row r="308">
       <c s="12" r="A308"/>
       <c t="s" s="7" r="B308">
+        <v>1112</v>
+      </c>
+      <c t="s" s="15" r="C308">
         <v>1113</v>
       </c>
-      <c t="s" s="15" r="C308">
+      <c t="s" s="7" r="D308">
         <v>1114</v>
       </c>
-      <c t="s" s="7" r="D308">
+      <c t="s" s="7" r="E308">
         <v>1115</v>
-      </c>
-      <c t="s" s="7" r="E308">
-        <v>1116</v>
       </c>
     </row>
     <row r="309">
       <c s="12" r="A309"/>
       <c t="s" s="7" r="B309">
+        <v>1116</v>
+      </c>
+      <c t="s" s="15" r="C309">
         <v>1117</v>
       </c>
-      <c t="s" s="15" r="C309">
+      <c t="s" s="7" r="D309">
         <v>1118</v>
       </c>
-      <c t="s" s="7" r="D309">
+      <c t="s" s="7" r="E309">
         <v>1119</v>
-      </c>
-      <c t="s" s="7" r="E309">
-        <v>1120</v>
       </c>
     </row>
     <row r="310">
       <c s="12" r="A310"/>
       <c t="s" s="7" r="B310">
+        <v>1120</v>
+      </c>
+      <c t="s" s="15" r="C310">
         <v>1121</v>
       </c>
-      <c t="s" s="15" r="C310">
+      <c t="s" s="7" r="D310">
         <v>1122</v>
       </c>
-      <c t="s" s="7" r="D310">
+      <c t="s" s="7" r="E310">
         <v>1123</v>
-      </c>
-      <c t="s" s="7" r="E310">
-        <v>1124</v>
       </c>
     </row>
     <row r="311">
       <c s="12" r="A311"/>
       <c t="s" s="7" r="B311">
+        <v>1124</v>
+      </c>
+      <c t="s" s="15" r="C311">
         <v>1125</v>
       </c>
-      <c t="s" s="15" r="C311">
-        <v>1126</v>
-      </c>
       <c t="s" s="7" r="D311">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c t="s" s="7" r="E311">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="312">
       <c s="12" r="A312"/>
       <c t="s" s="7" r="B312">
+        <v>1126</v>
+      </c>
+      <c t="s" s="15" r="C312">
         <v>1127</v>
       </c>
-      <c t="s" s="15" r="C312">
+      <c t="s" s="7" r="D312">
         <v>1128</v>
       </c>
-      <c t="s" s="7" r="D312">
+      <c t="s" s="7" r="E312">
         <v>1129</v>
-      </c>
-      <c t="s" s="7" r="E312">
-        <v>1130</v>
       </c>
     </row>
     <row r="313">
       <c s="12" r="A313"/>
       <c t="s" s="7" r="B313">
+        <v>1130</v>
+      </c>
+      <c t="s" s="15" r="C313">
         <v>1131</v>
       </c>
-      <c t="s" s="15" r="C313">
+      <c t="s" s="7" r="D313">
         <v>1132</v>
       </c>
-      <c t="s" s="7" r="D313">
+      <c t="s" s="7" r="E313">
         <v>1133</v>
-      </c>
-      <c t="s" s="7" r="E313">
-        <v>1134</v>
       </c>
     </row>
     <row r="314">
       <c s="12" r="A314"/>
       <c t="s" s="7" r="B314">
+        <v>1134</v>
+      </c>
+      <c t="s" s="15" r="C314">
         <v>1135</v>
       </c>
-      <c t="s" s="15" r="C314">
+      <c t="s" s="7" r="D314">
         <v>1136</v>
       </c>
-      <c t="s" s="7" r="D314">
+      <c t="s" s="7" r="E314">
         <v>1137</v>
-      </c>
-      <c t="s" s="7" r="E314">
-        <v>1138</v>
       </c>
     </row>
     <row r="315">
       <c s="12" r="A315"/>
       <c t="s" s="7" r="B315">
+        <v>1138</v>
+      </c>
+      <c t="s" s="15" r="C315">
         <v>1139</v>
       </c>
-      <c t="s" s="15" r="C315">
+      <c t="s" s="7" r="D315">
         <v>1140</v>
       </c>
-      <c t="s" s="7" r="D315">
+      <c t="s" s="7" r="E315">
         <v>1141</v>
-      </c>
-      <c t="s" s="7" r="E315">
-        <v>1142</v>
       </c>
     </row>
     <row r="316">
       <c s="12" r="A316"/>
       <c t="s" s="7" r="B316">
+        <v>1142</v>
+      </c>
+      <c t="s" s="15" r="C316">
         <v>1143</v>
       </c>
-      <c t="s" s="15" r="C316">
+      <c t="s" s="7" r="D316">
         <v>1144</v>
       </c>
-      <c t="s" s="7" r="D316">
+      <c t="s" s="7" r="E316">
         <v>1145</v>
-      </c>
-      <c t="s" s="7" r="E316">
-        <v>1146</v>
       </c>
     </row>
     <row r="317">
       <c s="12" r="A317"/>
       <c t="s" s="7" r="B317">
+        <v>1146</v>
+      </c>
+      <c t="s" s="15" r="C317">
         <v>1147</v>
       </c>
-      <c t="s" s="15" r="C317">
+      <c t="s" s="7" r="D317">
         <v>1148</v>
       </c>
-      <c t="s" s="7" r="D317">
+      <c t="s" s="7" r="E317">
         <v>1149</v>
-      </c>
-      <c t="s" s="7" r="E317">
-        <v>1150</v>
       </c>
     </row>
     <row r="318">
       <c s="12" r="A318"/>
       <c t="s" s="7" r="B318">
+        <v>1150</v>
+      </c>
+      <c t="s" s="15" r="C318">
         <v>1151</v>
       </c>
-      <c t="s" s="15" r="C318">
+      <c t="s" s="7" r="D318">
         <v>1152</v>
       </c>
-      <c t="s" s="7" r="D318">
+      <c t="s" s="7" r="E318">
         <v>1153</v>
-      </c>
-      <c t="s" s="7" r="E318">
-        <v>1154</v>
       </c>
     </row>
     <row r="319">
@@ -9165,124 +9160,124 @@
     </row>
     <row r="320">
       <c t="s" s="12" r="A320">
+        <v>1154</v>
+      </c>
+      <c t="s" s="7" r="B320">
         <v>1155</v>
       </c>
-      <c t="s" s="7" r="B320">
+      <c t="s" s="15" r="C320">
         <v>1156</v>
       </c>
-      <c t="s" s="15" r="C320">
+      <c t="s" s="7" r="D320">
         <v>1157</v>
       </c>
-      <c t="s" s="7" r="D320">
+      <c t="s" s="7" r="E320">
         <v>1158</v>
-      </c>
-      <c t="s" s="7" r="E320">
-        <v>1159</v>
       </c>
     </row>
     <row r="321">
       <c s="12" r="A321"/>
       <c t="s" s="7" r="B321">
+        <v>1159</v>
+      </c>
+      <c t="s" s="15" r="C321">
         <v>1160</v>
       </c>
-      <c t="s" s="15" r="C321">
+      <c t="s" s="7" r="D321">
         <v>1161</v>
       </c>
-      <c t="s" s="7" r="D321">
+      <c t="s" s="7" r="E321">
         <v>1162</v>
-      </c>
-      <c t="s" s="7" r="E321">
-        <v>1163</v>
       </c>
     </row>
     <row r="322">
       <c s="12" r="A322"/>
       <c t="s" s="7" r="B322">
+        <v>1163</v>
+      </c>
+      <c t="s" s="15" r="C322">
         <v>1164</v>
       </c>
-      <c t="s" s="15" r="C322">
+      <c t="s" s="7" r="D322">
         <v>1165</v>
       </c>
-      <c t="s" s="7" r="D322">
+      <c t="s" s="7" r="E322">
         <v>1166</v>
-      </c>
-      <c t="s" s="7" r="E322">
-        <v>1167</v>
       </c>
     </row>
     <row r="323">
       <c s="12" r="A323"/>
       <c t="s" s="7" r="B323">
+        <v>1167</v>
+      </c>
+      <c t="s" s="15" r="C323">
         <v>1168</v>
       </c>
-      <c t="s" s="15" r="C323">
+      <c t="s" s="7" r="D323">
         <v>1169</v>
       </c>
-      <c t="s" s="7" r="D323">
+      <c t="s" s="7" r="E323">
         <v>1170</v>
-      </c>
-      <c t="s" s="7" r="E323">
-        <v>1171</v>
       </c>
     </row>
     <row r="324">
       <c s="12" r="A324"/>
       <c t="s" s="7" r="B324">
+        <v>1171</v>
+      </c>
+      <c t="s" s="15" r="C324">
+        <v>1171</v>
+      </c>
+      <c t="s" s="21" r="D324">
         <v>1172</v>
       </c>
-      <c t="s" s="15" r="C324">
-        <v>1172</v>
-      </c>
-      <c t="s" s="21" r="D324">
+      <c t="s" s="21" r="E324">
         <v>1173</v>
-      </c>
-      <c t="s" s="21" r="E324">
-        <v>1174</v>
       </c>
     </row>
     <row r="325">
       <c s="12" r="A325"/>
       <c t="s" s="7" r="B325">
+        <v>1174</v>
+      </c>
+      <c t="s" s="15" r="C325">
         <v>1175</v>
       </c>
-      <c t="s" s="15" r="C325">
+      <c t="s" s="7" r="D325">
         <v>1176</v>
       </c>
-      <c t="s" s="7" r="D325">
+      <c t="s" s="7" r="E325">
         <v>1177</v>
-      </c>
-      <c t="s" s="7" r="E325">
-        <v>1178</v>
       </c>
     </row>
     <row r="326">
       <c s="12" r="A326"/>
       <c t="s" s="7" r="B326">
+        <v>1178</v>
+      </c>
+      <c t="s" s="15" r="C326">
         <v>1179</v>
       </c>
-      <c t="s" s="15" r="C326">
+      <c t="s" s="7" r="D326">
         <v>1180</v>
       </c>
-      <c t="s" s="7" r="D326">
+      <c t="s" s="7" r="E326">
         <v>1181</v>
-      </c>
-      <c t="s" s="7" r="E326">
-        <v>1182</v>
       </c>
     </row>
     <row r="327">
       <c t="s" s="18" r="A327">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c s="33" r="B327"/>
       <c t="s" s="15" r="C327">
+        <v>1183</v>
+      </c>
+      <c t="s" s="21" r="D327">
         <v>1184</v>
       </c>
-      <c t="s" s="21" r="D327">
+      <c t="s" s="21" r="E327">
         <v>1185</v>
-      </c>
-      <c t="s" s="21" r="E327">
-        <v>1186</v>
       </c>
     </row>
     <row r="328">
@@ -9294,291 +9289,291 @@
     </row>
     <row r="329">
       <c t="s" s="20" r="A329">
+        <v>1186</v>
+      </c>
+      <c t="s" s="7" r="B329">
         <v>1187</v>
       </c>
-      <c t="s" s="7" r="B329">
+      <c t="s" s="7" r="C329">
         <v>1188</v>
       </c>
-      <c t="s" s="7" r="C329">
+      <c t="s" s="7" r="D329">
         <v>1189</v>
       </c>
-      <c t="s" s="7" r="D329">
+      <c t="s" s="7" r="E329">
         <v>1190</v>
-      </c>
-      <c t="s" s="7" r="E329">
-        <v>1191</v>
       </c>
     </row>
     <row r="330">
       <c s="16" r="A330"/>
       <c t="s" s="7" r="B330">
+        <v>1191</v>
+      </c>
+      <c t="s" s="15" r="C330">
         <v>1192</v>
       </c>
-      <c t="s" s="15" r="C330">
+      <c t="s" s="7" r="D330">
         <v>1193</v>
       </c>
-      <c t="s" s="7" r="D330">
+      <c t="s" s="7" r="E330">
         <v>1194</v>
-      </c>
-      <c t="s" s="7" r="E330">
-        <v>1195</v>
       </c>
     </row>
     <row r="331">
       <c s="16" r="A331"/>
       <c t="s" s="7" r="B331">
+        <v>1195</v>
+      </c>
+      <c t="s" s="7" r="C331">
         <v>1196</v>
       </c>
-      <c t="s" s="7" r="C331">
+      <c t="s" s="7" r="D331">
         <v>1197</v>
       </c>
-      <c t="s" s="7" r="D331">
+      <c t="s" s="7" r="E331">
         <v>1198</v>
-      </c>
-      <c t="s" s="7" r="E331">
-        <v>1199</v>
       </c>
     </row>
     <row r="332">
       <c s="20" r="A332"/>
       <c t="s" s="7" r="B332">
+        <v>1199</v>
+      </c>
+      <c t="s" s="15" r="C332">
         <v>1200</v>
       </c>
-      <c t="s" s="15" r="C332">
+      <c t="s" s="7" r="D332">
         <v>1201</v>
       </c>
-      <c t="s" s="7" r="D332">
+      <c t="s" s="7" r="E332">
         <v>1202</v>
-      </c>
-      <c t="s" s="7" r="E332">
-        <v>1203</v>
       </c>
     </row>
     <row r="333">
       <c s="20" r="A333"/>
       <c t="s" s="7" r="B333">
+        <v>1203</v>
+      </c>
+      <c t="s" s="7" r="C333">
         <v>1204</v>
       </c>
-      <c t="s" s="7" r="C333">
+      <c t="s" s="7" r="D333">
         <v>1205</v>
       </c>
-      <c t="s" s="7" r="D333">
+      <c t="s" s="7" r="E333">
         <v>1206</v>
-      </c>
-      <c t="s" s="7" r="E333">
-        <v>1207</v>
       </c>
     </row>
     <row r="334">
       <c s="20" r="A334"/>
       <c t="s" s="7" r="B334">
+        <v>1207</v>
+      </c>
+      <c t="s" s="15" r="C334">
         <v>1208</v>
       </c>
-      <c t="s" s="15" r="C334">
+      <c t="s" s="7" r="D334">
         <v>1209</v>
       </c>
-      <c t="s" s="7" r="D334">
+      <c t="s" s="7" r="E334">
         <v>1210</v>
-      </c>
-      <c t="s" s="7" r="E334">
-        <v>1211</v>
       </c>
     </row>
     <row r="335">
       <c s="20" r="A335"/>
       <c t="s" s="7" r="B335">
+        <v>1211</v>
+      </c>
+      <c t="s" s="7" r="C335">
         <v>1212</v>
       </c>
-      <c t="s" s="7" r="C335">
+      <c t="s" s="7" r="D335">
         <v>1213</v>
       </c>
-      <c t="s" s="7" r="D335">
+      <c t="s" s="7" r="E335">
         <v>1214</v>
-      </c>
-      <c t="s" s="7" r="E335">
-        <v>1215</v>
       </c>
     </row>
     <row r="336">
       <c s="20" r="A336"/>
       <c t="s" s="7" r="B336">
+        <v>1215</v>
+      </c>
+      <c t="s" s="15" r="C336">
         <v>1216</v>
       </c>
-      <c t="s" s="15" r="C336">
+      <c t="s" s="7" r="D336">
         <v>1217</v>
       </c>
-      <c t="s" s="7" r="D336">
+      <c t="s" s="7" r="E336">
         <v>1218</v>
-      </c>
-      <c t="s" s="7" r="E336">
-        <v>1219</v>
       </c>
     </row>
     <row r="337">
       <c s="20" r="A337"/>
       <c t="s" s="7" r="B337">
+        <v>1219</v>
+      </c>
+      <c t="s" s="7" r="C337">
         <v>1220</v>
       </c>
-      <c t="s" s="7" r="C337">
+      <c t="s" s="7" r="D337">
         <v>1221</v>
       </c>
-      <c t="s" s="7" r="D337">
+      <c t="s" s="7" r="E337">
         <v>1222</v>
-      </c>
-      <c t="s" s="7" r="E337">
-        <v>1223</v>
       </c>
     </row>
     <row r="338">
       <c s="20" r="A338"/>
       <c t="s" s="7" r="B338">
+        <v>1223</v>
+      </c>
+      <c t="s" s="15" r="C338">
         <v>1224</v>
       </c>
-      <c t="s" s="15" r="C338">
+      <c t="s" s="7" r="D338">
         <v>1225</v>
       </c>
-      <c t="s" s="7" r="D338">
+      <c t="s" s="7" r="E338">
         <v>1226</v>
-      </c>
-      <c t="s" s="7" r="E338">
-        <v>1227</v>
       </c>
     </row>
     <row r="339">
       <c s="20" r="A339"/>
       <c t="s" s="7" r="B339">
+        <v>1227</v>
+      </c>
+      <c t="s" s="7" r="C339">
         <v>1228</v>
       </c>
-      <c t="s" s="7" r="C339">
+      <c t="s" s="7" r="D339">
         <v>1229</v>
       </c>
-      <c t="s" s="7" r="D339">
+      <c t="s" s="7" r="E339">
         <v>1230</v>
-      </c>
-      <c t="s" s="7" r="E339">
-        <v>1231</v>
       </c>
     </row>
     <row r="340">
       <c s="20" r="A340"/>
       <c t="s" s="7" r="B340">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c t="s" s="15" r="C340">
+        <v>1224</v>
+      </c>
+      <c t="s" s="7" r="D340">
         <v>1225</v>
       </c>
-      <c t="s" s="7" r="D340">
+      <c t="s" s="7" r="E340">
         <v>1226</v>
-      </c>
-      <c t="s" s="7" r="E340">
-        <v>1227</v>
       </c>
     </row>
     <row r="341">
       <c s="20" r="A341"/>
       <c t="s" s="7" r="B341">
+        <v>1232</v>
+      </c>
+      <c t="s" s="15" r="C341">
         <v>1233</v>
       </c>
-      <c t="s" s="15" r="C341">
+      <c t="s" s="7" r="D341">
         <v>1234</v>
       </c>
-      <c t="s" s="7" r="D341">
+      <c t="s" s="7" r="E341">
         <v>1235</v>
-      </c>
-      <c t="s" s="7" r="E341">
-        <v>1236</v>
       </c>
     </row>
     <row r="342">
       <c s="20" r="A342"/>
       <c t="s" s="7" r="B342">
+        <v>1236</v>
+      </c>
+      <c t="s" s="15" r="C342">
         <v>1237</v>
       </c>
-      <c t="s" s="15" r="C342">
+      <c t="s" s="7" r="D342">
         <v>1238</v>
       </c>
-      <c t="s" s="7" r="D342">
+      <c t="s" s="7" r="E342">
         <v>1239</v>
-      </c>
-      <c t="s" s="7" r="E342">
-        <v>1240</v>
       </c>
     </row>
     <row r="343">
       <c s="8" r="A343"/>
       <c t="s" s="1" r="B343">
+        <v>1240</v>
+      </c>
+      <c t="s" s="1" r="C343">
         <v>1241</v>
       </c>
-      <c t="s" s="1" r="C343">
+      <c t="s" s="1" r="D343">
         <v>1242</v>
       </c>
-      <c t="s" s="1" r="D343">
+      <c t="s" s="1" r="E343">
         <v>1243</v>
-      </c>
-      <c t="s" s="1" r="E343">
-        <v>1244</v>
       </c>
     </row>
     <row r="344">
       <c s="8" r="A344"/>
       <c t="s" s="1" r="B344">
+        <v>1244</v>
+      </c>
+      <c t="s" s="39" r="C344">
         <v>1245</v>
       </c>
-      <c t="s" s="39" r="C344">
+      <c t="s" s="1" r="D344">
         <v>1246</v>
       </c>
-      <c t="s" s="1" r="D344">
+      <c t="s" s="1" r="E344">
         <v>1247</v>
-      </c>
-      <c t="s" s="1" r="E344">
-        <v>1248</v>
       </c>
     </row>
     <row r="345">
       <c s="12" r="A345"/>
       <c t="s" s="7" r="B345">
+        <v>1248</v>
+      </c>
+      <c t="s" s="15" r="C345">
         <v>1249</v>
       </c>
-      <c t="s" s="15" r="C345">
+      <c t="s" s="7" r="D345">
         <v>1250</v>
       </c>
-      <c t="s" s="7" r="D345">
+      <c t="s" s="7" r="E345">
         <v>1251</v>
-      </c>
-      <c t="s" s="7" r="E345">
-        <v>1252</v>
       </c>
     </row>
     <row r="346">
       <c t="s" s="12" r="A346">
+        <v>1252</v>
+      </c>
+      <c t="s" s="15" r="B346">
         <v>1253</v>
       </c>
-      <c t="s" s="15" r="B346">
+      <c t="s" s="15" r="C346">
         <v>1254</v>
       </c>
-      <c t="s" s="15" r="C346">
+      <c t="s" s="21" r="D346">
         <v>1255</v>
       </c>
-      <c t="s" s="21" r="D346">
+      <c t="s" s="7" r="E346">
         <v>1256</v>
-      </c>
-      <c t="s" s="7" r="E346">
-        <v>1257</v>
       </c>
     </row>
     <row r="347">
       <c s="12" r="A347"/>
       <c t="s" s="15" r="B347">
+        <v>1257</v>
+      </c>
+      <c t="s" s="15" r="C347">
         <v>1258</v>
       </c>
-      <c t="s" s="15" r="C347">
+      <c t="s" s="21" r="D347">
         <v>1259</v>
       </c>
-      <c t="s" s="21" r="D347">
+      <c t="s" s="7" r="E347">
         <v>1260</v>
-      </c>
-      <c t="s" s="7" r="E347">
-        <v>1261</v>
       </c>
     </row>
     <row r="348">
@@ -9589,34 +9584,34 @@
     </row>
     <row r="349">
       <c t="s" s="12" r="A349">
+        <v>1261</v>
+      </c>
+      <c t="s" s="33" r="B349">
         <v>1262</v>
       </c>
-      <c t="s" s="33" r="B349">
+      <c t="s" s="15" r="C349">
         <v>1263</v>
       </c>
-      <c t="s" s="15" r="C349">
+      <c t="s" s="7" r="D349">
         <v>1264</v>
       </c>
-      <c t="s" s="7" r="D349">
+      <c t="s" s="7" r="E349">
         <v>1265</v>
-      </c>
-      <c t="s" s="7" r="E349">
-        <v>1266</v>
       </c>
     </row>
     <row r="350">
       <c s="12" r="A350"/>
       <c t="s" s="33" r="B350">
+        <v>1266</v>
+      </c>
+      <c t="s" s="15" r="C350">
         <v>1267</v>
       </c>
-      <c t="s" s="15" r="C350">
+      <c t="s" s="7" r="D350">
         <v>1268</v>
       </c>
-      <c t="s" s="7" r="D350">
+      <c t="s" s="7" r="E350">
         <v>1269</v>
-      </c>
-      <c t="s" s="7" r="E350">
-        <v>1270</v>
       </c>
     </row>
     <row r="351">
@@ -9641,17 +9636,17 @@
   <sheetData>
     <row customHeight="1" r="1" ht="112.5">
       <c t="s" s="3" r="A1">
-        <v>1271</v>
+        <v>1270</v>
       </c>
     </row>
     <row customHeight="1" r="2" ht="112.5">
       <c t="s" s="5" r="A2">
-        <v>1272</v>
+        <v>1271</v>
       </c>
     </row>
     <row customHeight="1" r="3" ht="112.5">
       <c t="s" s="11" r="A3">
-        <v>1273</v>
+        <v>1272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EWD-22840 - Introduction page
Former-commit-id: 382620cf6701e45b056bd1d91eef7b63d426d85a
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="1273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1324" uniqueCount="1278">
   <si>
     <t>Key</t>
   </si>
@@ -2217,6 +2217,18 @@
     <t>Introduction page</t>
   </si>
   <si>
+    <t>introWelcomePageTitle</t>
+  </si>
+  <si>
+    <t>Welcome page</t>
+  </si>
+  <si>
+    <t>Welkompagina</t>
+  </si>
+  <si>
+    <t>Willkommensseite</t>
+  </si>
+  <si>
     <t>introWelcome</t>
   </si>
   <si>
@@ -2417,6 +2429,9 @@
   </si>
   <si>
     <t>introApplicationContentDesc</t>
+  </si>
+  <si>
+    <t>How to provide learner with a learning experience?</t>
   </si>
   <si>
     <t>Hoe biedt u cursisten een leerervaring?</t>
@@ -7423,7 +7438,6 @@
       </c>
     </row>
     <row r="197">
-      <c s="12" r="A197"/>
       <c t="s" s="23" r="B197">
         <v>736</v>
       </c>
@@ -7464,19 +7478,19 @@
         <v>746</v>
       </c>
       <c t="s" s="43" r="E199">
-        <v>746</v>
+        <v>747</v>
       </c>
     </row>
     <row r="200">
       <c s="12" r="A200"/>
       <c t="s" s="23" r="B200">
-        <v>747</v>
-      </c>
-      <c t="s" s="30" r="C200">
         <v>748</v>
       </c>
+      <c t="s" s="31" r="C200">
+        <v>749</v>
+      </c>
       <c t="s" s="43" r="D200">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c t="s" s="43" r="E200">
         <v>750</v>
@@ -7487,7 +7501,7 @@
       <c t="s" s="23" r="B201">
         <v>751</v>
       </c>
-      <c t="s" s="31" r="C201">
+      <c t="s" s="30" r="C201">
         <v>752</v>
       </c>
       <c t="s" s="43" r="D201">
@@ -7563,22 +7577,22 @@
         <v>771</v>
       </c>
       <c t="s" s="31" r="C206">
-        <v>367</v>
+        <v>772</v>
       </c>
       <c t="s" s="43" r="D206">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c t="s" s="43" r="E206">
-        <v>773</v>
+        <v>774</v>
       </c>
     </row>
     <row r="207">
       <c s="12" r="A207"/>
       <c t="s" s="23" r="B207">
-        <v>774</v>
-      </c>
-      <c t="s" s="30" r="C207">
         <v>775</v>
+      </c>
+      <c t="s" s="31" r="C207">
+        <v>367</v>
       </c>
       <c t="s" s="43" r="D207">
         <v>776</v>
@@ -7592,7 +7606,7 @@
       <c t="s" s="23" r="B208">
         <v>778</v>
       </c>
-      <c t="s" s="31" r="C208">
+      <c t="s" s="30" r="C208">
         <v>779</v>
       </c>
       <c t="s" s="43" r="D208">
@@ -7637,7 +7651,7 @@
       <c t="s" s="23" r="B211">
         <v>790</v>
       </c>
-      <c t="s" s="30" r="C211">
+      <c t="s" s="31" r="C211">
         <v>791</v>
       </c>
       <c t="s" s="43" r="D211">
@@ -7652,7 +7666,7 @@
       <c t="s" s="23" r="B212">
         <v>794</v>
       </c>
-      <c t="s" s="31" r="C212">
+      <c t="s" s="30" r="C212">
         <v>795</v>
       </c>
       <c t="s" s="43" r="D212">
@@ -7667,1894 +7681,1894 @@
       <c t="s" s="23" r="B213">
         <v>798</v>
       </c>
-      <c s="31" r="C213"/>
+      <c t="s" s="31" r="C213">
+        <v>799</v>
+      </c>
       <c t="s" s="43" r="D213">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c t="s" s="43" r="E213">
-        <v>800</v>
+        <v>801</v>
       </c>
     </row>
     <row r="214">
       <c s="12" r="A214"/>
       <c t="s" s="23" r="B214">
-        <v>801</v>
-      </c>
-      <c t="s" s="31" r="C214">
         <v>802</v>
       </c>
+      <c t="s" s="30" r="C214">
+        <v>803</v>
+      </c>
       <c t="s" s="43" r="D214">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c t="s" s="43" r="E214">
-        <v>804</v>
+        <v>805</v>
       </c>
     </row>
     <row r="215">
       <c s="12" r="A215"/>
       <c t="s" s="23" r="B215">
-        <v>805</v>
-      </c>
-      <c t="s" s="30" r="C215">
         <v>806</v>
       </c>
+      <c t="s" s="31" r="C215">
+        <v>807</v>
+      </c>
       <c t="s" s="43" r="D215">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c t="s" s="43" r="E215">
-        <v>808</v>
+        <v>809</v>
       </c>
     </row>
     <row r="216">
       <c s="12" r="A216"/>
       <c t="s" s="23" r="B216">
-        <v>809</v>
-      </c>
-      <c t="s" s="31" r="C216">
         <v>810</v>
       </c>
+      <c t="s" s="30" r="C216">
+        <v>811</v>
+      </c>
       <c t="s" s="43" r="D216">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c t="s" s="43" r="E216">
-        <v>812</v>
+        <v>813</v>
       </c>
     </row>
     <row r="217">
       <c s="12" r="A217"/>
       <c t="s" s="23" r="B217">
-        <v>813</v>
-      </c>
-      <c t="s" s="30" r="C217">
         <v>814</v>
       </c>
+      <c t="s" s="31" r="C217">
+        <v>815</v>
+      </c>
       <c t="s" s="43" r="D217">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c t="s" s="43" r="E217">
-        <v>816</v>
+        <v>817</v>
       </c>
     </row>
     <row r="218">
       <c s="12" r="A218"/>
       <c t="s" s="23" r="B218">
-        <v>817</v>
-      </c>
-      <c t="s" s="31" r="C218">
-        <v>324</v>
+        <v>818</v>
+      </c>
+      <c t="s" s="30" r="C218">
+        <v>819</v>
       </c>
       <c t="s" s="43" r="D218">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c t="s" s="43" r="E218">
-        <v>819</v>
+        <v>821</v>
       </c>
     </row>
     <row r="219">
       <c s="12" r="A219"/>
       <c t="s" s="23" r="B219">
-        <v>820</v>
-      </c>
-      <c t="s" s="30" r="C219">
-        <v>821</v>
+        <v>822</v>
+      </c>
+      <c t="s" s="31" r="C219">
+        <v>324</v>
       </c>
       <c t="s" s="43" r="D219">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c t="s" s="43" r="E219">
-        <v>823</v>
+        <v>824</v>
       </c>
     </row>
     <row r="220">
       <c s="12" r="A220"/>
-      <c s="13" r="B220"/>
-      <c s="16" r="C220"/>
-      <c s="13" r="D220"/>
-      <c s="13" r="E220"/>
+      <c t="s" s="23" r="B220">
+        <v>825</v>
+      </c>
+      <c t="s" s="30" r="C220">
+        <v>826</v>
+      </c>
+      <c t="s" s="43" r="D220">
+        <v>827</v>
+      </c>
+      <c t="s" s="43" r="E220">
+        <v>828</v>
+      </c>
     </row>
     <row r="221">
-      <c t="s" s="12" r="A221">
-        <v>824</v>
-      </c>
-      <c t="s" s="7" r="B221">
-        <v>825</v>
-      </c>
-      <c t="s" s="15" r="C221">
-        <v>826</v>
-      </c>
-      <c t="s" s="7" r="D221">
-        <v>827</v>
-      </c>
-      <c t="s" s="7" r="E221">
-        <v>828</v>
-      </c>
+      <c s="12" r="A221"/>
+      <c s="13" r="B221"/>
+      <c s="16" r="C221"/>
+      <c s="13" r="D221"/>
+      <c s="13" r="E221"/>
     </row>
     <row r="222">
-      <c s="12" r="A222"/>
+      <c t="s" s="12" r="A222">
+        <v>829</v>
+      </c>
       <c t="s" s="7" r="B222">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c t="s" s="15" r="C222">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c t="s" s="7" r="D222">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c t="s" s="7" r="E222">
-        <v>832</v>
+        <v>833</v>
       </c>
     </row>
     <row r="223">
       <c s="12" r="A223"/>
       <c t="s" s="7" r="B223">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c t="s" s="15" r="C223">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c t="s" s="7" r="D223">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c t="s" s="7" r="E223">
-        <v>836</v>
+        <v>837</v>
       </c>
     </row>
     <row r="224">
       <c s="12" r="A224"/>
       <c t="s" s="7" r="B224">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c t="s" s="15" r="C224">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c t="s" s="7" r="D224">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c t="s" s="7" r="E224">
-        <v>840</v>
+        <v>841</v>
       </c>
     </row>
     <row r="225">
       <c s="12" r="A225"/>
       <c t="s" s="7" r="B225">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c t="s" s="15" r="C225">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c t="s" s="7" r="D225">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c t="s" s="7" r="E225">
-        <v>844</v>
+        <v>845</v>
       </c>
     </row>
     <row r="226">
       <c s="12" r="A226"/>
       <c t="s" s="7" r="B226">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c t="s" s="15" r="C226">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c t="s" s="7" r="D226">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c t="s" s="7" r="E226">
-        <v>848</v>
+        <v>849</v>
       </c>
     </row>
     <row r="227">
       <c s="12" r="A227"/>
       <c t="s" s="7" r="B227">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c t="s" s="15" r="C227">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c t="s" s="7" r="D227">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c t="s" s="7" r="E227">
-        <v>852</v>
+        <v>853</v>
       </c>
     </row>
     <row r="228">
       <c s="12" r="A228"/>
-      <c s="24" r="B228"/>
-      <c s="37" r="C228"/>
-      <c s="24" r="D228"/>
-      <c s="24" r="E228"/>
+      <c t="s" s="7" r="B228">
+        <v>854</v>
+      </c>
+      <c t="s" s="15" r="C228">
+        <v>855</v>
+      </c>
+      <c t="s" s="7" r="D228">
+        <v>856</v>
+      </c>
+      <c t="s" s="7" r="E228">
+        <v>857</v>
+      </c>
     </row>
     <row r="229">
-      <c t="s" s="12" r="A229">
-        <v>853</v>
-      </c>
-      <c t="s" s="36" r="B229">
-        <v>854</v>
-      </c>
-      <c t="s" s="25" r="C229">
-        <v>853</v>
-      </c>
-      <c s="36" r="D229"/>
-      <c s="36" r="E229"/>
+      <c s="12" r="A229"/>
+      <c s="24" r="B229"/>
+      <c s="37" r="C229"/>
+      <c s="24" r="D229"/>
+      <c s="24" r="E229"/>
     </row>
     <row r="230">
-      <c s="12" r="A230"/>
-      <c s="18" r="B230"/>
-      <c s="9" r="C230"/>
-      <c s="18" r="D230"/>
-      <c s="18" r="E230"/>
+      <c t="s" s="12" r="A230">
+        <v>858</v>
+      </c>
+      <c t="s" s="36" r="B230">
+        <v>859</v>
+      </c>
+      <c t="s" s="25" r="C230">
+        <v>858</v>
+      </c>
+      <c s="36" r="D230"/>
+      <c s="36" r="E230"/>
     </row>
     <row r="231">
-      <c t="s" s="12" r="A231">
-        <v>855</v>
-      </c>
-      <c t="s" s="44" r="B231">
-        <v>856</v>
-      </c>
-      <c t="s" s="41" r="C231">
-        <v>857</v>
-      </c>
-      <c s="44" r="D231"/>
-      <c s="44" r="E231"/>
+      <c s="12" r="A231"/>
+      <c s="18" r="B231"/>
+      <c s="9" r="C231"/>
+      <c s="18" r="D231"/>
+      <c s="18" r="E231"/>
     </row>
     <row r="232">
-      <c s="12" r="A232"/>
+      <c t="s" s="12" r="A232">
+        <v>860</v>
+      </c>
       <c t="s" s="44" r="B232">
-        <v>858</v>
+        <v>861</v>
       </c>
       <c t="s" s="41" r="C232">
-        <v>859</v>
+        <v>862</v>
       </c>
       <c s="44" r="D232"/>
       <c s="44" r="E232"/>
     </row>
     <row r="233">
       <c s="12" r="A233"/>
-      <c s="9" r="B233"/>
-      <c s="9" r="C233"/>
-      <c s="18" r="D233"/>
-      <c s="18" r="E233"/>
+      <c t="s" s="44" r="B233">
+        <v>863</v>
+      </c>
+      <c t="s" s="41" r="C233">
+        <v>864</v>
+      </c>
+      <c s="44" r="D233"/>
+      <c s="44" r="E233"/>
     </row>
     <row r="234">
-      <c t="s" s="12" r="A234">
-        <v>860</v>
-      </c>
-      <c t="s" s="33" r="B234">
-        <v>861</v>
-      </c>
-      <c t="s" s="33" r="C234">
-        <v>862</v>
-      </c>
-      <c t="s" s="7" r="D234">
-        <v>863</v>
-      </c>
-      <c t="s" s="7" r="E234">
-        <v>864</v>
-      </c>
+      <c s="12" r="A234"/>
+      <c s="9" r="B234"/>
+      <c s="9" r="C234"/>
+      <c s="18" r="D234"/>
+      <c s="18" r="E234"/>
     </row>
     <row r="235">
-      <c s="12" r="A235"/>
+      <c t="s" s="12" r="A235">
+        <v>865</v>
+      </c>
       <c t="s" s="33" r="B235">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c t="s" s="33" r="C235">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c t="s" s="7" r="D235">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c t="s" s="7" r="E235">
-        <v>867</v>
+        <v>869</v>
       </c>
     </row>
     <row r="236">
       <c s="12" r="A236"/>
       <c t="s" s="33" r="B236">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c t="s" s="33" r="C236">
-        <v>869</v>
+        <v>871</v>
       </c>
       <c t="s" s="7" r="D236">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c t="s" s="7" r="E236">
-        <v>871</v>
+        <v>872</v>
       </c>
     </row>
     <row r="237">
       <c s="12" r="A237"/>
       <c t="s" s="33" r="B237">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c t="s" s="33" r="C237">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c t="s" s="7" r="D237">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c t="s" s="7" r="E237">
-        <v>875</v>
+        <v>876</v>
       </c>
     </row>
     <row r="238">
       <c s="12" r="A238"/>
-      <c t="s" s="15" r="B238">
-        <v>876</v>
-      </c>
-      <c t="s" s="15" r="C238">
+      <c t="s" s="33" r="B238">
         <v>877</v>
       </c>
+      <c t="s" s="33" r="C238">
+        <v>878</v>
+      </c>
       <c t="s" s="7" r="D238">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c t="s" s="7" r="E238">
-        <v>879</v>
+        <v>880</v>
       </c>
     </row>
     <row r="239">
       <c s="12" r="A239"/>
       <c t="s" s="15" r="B239">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c t="s" s="15" r="C239">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c t="s" s="7" r="D239">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c t="s" s="7" r="E239">
-        <v>883</v>
+        <v>884</v>
       </c>
     </row>
     <row r="240">
       <c s="12" r="A240"/>
       <c t="s" s="15" r="B240">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c t="s" s="15" r="C240">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c t="s" s="7" r="D240">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c t="s" s="7" r="E240">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="241">
       <c s="12" r="A241"/>
       <c t="s" s="15" r="B241">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c t="s" s="15" r="C241">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c t="s" s="7" r="D241">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c t="s" s="7" r="E241">
-        <v>891</v>
+        <v>892</v>
       </c>
     </row>
     <row r="242">
       <c s="12" r="A242"/>
       <c t="s" s="15" r="B242">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c t="s" s="15" r="C242">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c t="s" s="7" r="D242">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c t="s" s="7" r="E242">
-        <v>895</v>
+        <v>896</v>
       </c>
     </row>
     <row r="243">
       <c s="12" r="A243"/>
-      <c s="12" r="B243"/>
-      <c s="12" r="C243"/>
-      <c s="12" r="D243"/>
-      <c s="12" r="E243"/>
+      <c t="s" s="15" r="B243">
+        <v>897</v>
+      </c>
+      <c t="s" s="15" r="C243">
+        <v>898</v>
+      </c>
+      <c t="s" s="7" r="D243">
+        <v>899</v>
+      </c>
+      <c t="s" s="7" r="E243">
+        <v>900</v>
+      </c>
     </row>
     <row r="244">
       <c s="12" r="A244"/>
-      <c t="s" s="15" r="B244">
-        <v>896</v>
-      </c>
-      <c t="s" s="15" r="C244">
-        <v>897</v>
-      </c>
-      <c t="s" s="7" r="D244">
-        <v>898</v>
-      </c>
-      <c t="s" s="7" r="E244">
-        <v>899</v>
-      </c>
+      <c s="12" r="B244"/>
+      <c s="12" r="C244"/>
+      <c s="12" r="D244"/>
+      <c s="12" r="E244"/>
     </row>
     <row r="245">
       <c s="12" r="A245"/>
-      <c t="s" s="7" r="B245">
-        <v>900</v>
+      <c t="s" s="15" r="B245">
+        <v>901</v>
       </c>
       <c t="s" s="15" r="C245">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c t="s" s="7" r="D245">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c t="s" s="7" r="E245">
-        <v>903</v>
+        <v>904</v>
       </c>
     </row>
     <row r="246">
       <c s="12" r="A246"/>
       <c t="s" s="7" r="B246">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c t="s" s="15" r="C246">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c t="s" s="7" r="D246">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c t="s" s="7" r="E246">
-        <v>907</v>
+        <v>908</v>
       </c>
     </row>
     <row r="247">
       <c s="12" r="A247"/>
       <c t="s" s="7" r="B247">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c t="s" s="15" r="C247">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c t="s" s="7" r="D247">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c t="s" s="7" r="E247">
-        <v>911</v>
+        <v>912</v>
       </c>
     </row>
     <row r="248">
       <c s="12" r="A248"/>
       <c t="s" s="7" r="B248">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c t="s" s="15" r="C248">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c t="s" s="7" r="D248">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c t="s" s="7" r="E248">
-        <v>915</v>
+        <v>916</v>
       </c>
     </row>
     <row r="249">
       <c s="12" r="A249"/>
       <c t="s" s="7" r="B249">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c t="s" s="15" r="C249">
-        <v>917</v>
-      </c>
-      <c t="s" s="30" r="D249">
         <v>918</v>
       </c>
-      <c t="s" s="30" r="E249">
+      <c t="s" s="7" r="D249">
         <v>919</v>
+      </c>
+      <c t="s" s="7" r="E249">
+        <v>920</v>
       </c>
     </row>
     <row r="250">
       <c s="12" r="A250"/>
       <c t="s" s="7" r="B250">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c t="s" s="15" r="C250">
-        <v>921</v>
-      </c>
-      <c t="s" s="7" r="D250">
         <v>922</v>
       </c>
-      <c t="s" s="7" r="E250">
+      <c t="s" s="30" r="D250">
         <v>923</v>
+      </c>
+      <c t="s" s="30" r="E250">
+        <v>924</v>
       </c>
     </row>
     <row r="251">
       <c s="12" r="A251"/>
       <c t="s" s="7" r="B251">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c t="s" s="15" r="C251">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c t="s" s="7" r="D251">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c t="s" s="7" r="E251">
-        <v>927</v>
+        <v>928</v>
       </c>
     </row>
     <row r="252">
       <c s="12" r="A252"/>
       <c t="s" s="7" r="B252">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c t="s" s="15" r="C252">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c t="s" s="7" r="D252">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c t="s" s="7" r="E252">
-        <v>931</v>
+        <v>932</v>
       </c>
     </row>
     <row r="253">
       <c s="12" r="A253"/>
       <c t="s" s="7" r="B253">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c t="s" s="15" r="C253">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c t="s" s="7" r="D253">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c t="s" s="7" r="E253">
-        <v>935</v>
+        <v>936</v>
       </c>
     </row>
     <row r="254">
       <c s="12" r="A254"/>
       <c t="s" s="7" r="B254">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c t="s" s="15" r="C254">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c t="s" s="7" r="D254">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c t="s" s="7" r="E254">
-        <v>939</v>
+        <v>940</v>
       </c>
     </row>
     <row r="255">
       <c s="12" r="A255"/>
-      <c s="18" r="B255"/>
-      <c s="37" r="C255"/>
-      <c s="18" r="D255"/>
-      <c s="18" r="E255"/>
+      <c t="s" s="7" r="B255">
+        <v>941</v>
+      </c>
+      <c t="s" s="15" r="C255">
+        <v>942</v>
+      </c>
+      <c t="s" s="7" r="D255">
+        <v>943</v>
+      </c>
+      <c t="s" s="7" r="E255">
+        <v>944</v>
+      </c>
     </row>
     <row r="256">
-      <c t="s" s="12" r="A256">
-        <v>940</v>
-      </c>
-      <c t="s" s="33" r="B256">
-        <v>941</v>
-      </c>
-      <c t="s" s="7" r="C256">
-        <v>866</v>
-      </c>
-      <c t="s" s="7" r="D256">
-        <v>866</v>
-      </c>
-      <c t="s" s="7" r="E256">
-        <v>867</v>
-      </c>
+      <c s="12" r="A256"/>
+      <c s="18" r="B256"/>
+      <c s="37" r="C256"/>
+      <c s="18" r="D256"/>
+      <c s="18" r="E256"/>
     </row>
     <row r="257">
-      <c s="12" r="A257"/>
-      <c t="s" s="7" r="B257">
-        <v>942</v>
-      </c>
-      <c t="s" s="15" r="C257">
-        <v>869</v>
+      <c t="s" s="12" r="A257">
+        <v>945</v>
+      </c>
+      <c t="s" s="33" r="B257">
+        <v>946</v>
+      </c>
+      <c t="s" s="7" r="C257">
+        <v>871</v>
       </c>
       <c t="s" s="7" r="D257">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c t="s" s="7" r="E257">
-        <v>871</v>
+        <v>872</v>
       </c>
     </row>
     <row r="258">
+      <c s="12" r="A258"/>
       <c t="s" s="7" r="B258">
-        <v>943</v>
+        <v>947</v>
       </c>
       <c t="s" s="15" r="C258">
-        <v>944</v>
+        <v>874</v>
       </c>
       <c t="s" s="7" r="D258">
-        <v>945</v>
+        <v>875</v>
       </c>
       <c t="s" s="7" r="E258">
-        <v>946</v>
+        <v>876</v>
       </c>
     </row>
     <row r="259">
-      <c s="12" r="A259"/>
       <c t="s" s="7" r="B259">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c t="s" s="15" r="C259">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c t="s" s="7" r="D259">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c t="s" s="7" r="E259">
-        <v>950</v>
+        <v>951</v>
       </c>
     </row>
     <row r="260">
       <c s="12" r="A260"/>
       <c t="s" s="7" r="B260">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c t="s" s="15" r="C260">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c t="s" s="7" r="D260">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c t="s" s="7" r="E260">
-        <v>954</v>
+        <v>955</v>
       </c>
     </row>
     <row r="261">
       <c s="12" r="A261"/>
-      <c s="13" r="B261"/>
-      <c s="16" r="C261"/>
-      <c s="18" r="D261"/>
-      <c s="18" r="E261"/>
+      <c t="s" s="7" r="B261">
+        <v>956</v>
+      </c>
+      <c t="s" s="15" r="C261">
+        <v>957</v>
+      </c>
+      <c t="s" s="7" r="D261">
+        <v>958</v>
+      </c>
+      <c t="s" s="7" r="E261">
+        <v>959</v>
+      </c>
     </row>
     <row r="262">
-      <c t="s" s="12" r="A262">
-        <v>955</v>
-      </c>
-      <c t="s" s="7" r="B262">
-        <v>956</v>
-      </c>
-      <c t="s" s="15" r="C262">
-        <v>955</v>
-      </c>
-      <c t="s" s="7" r="D262">
-        <v>957</v>
-      </c>
-      <c t="s" s="7" r="E262">
-        <v>958</v>
-      </c>
+      <c s="12" r="A262"/>
+      <c s="13" r="B262"/>
+      <c s="16" r="C262"/>
+      <c s="18" r="D262"/>
+      <c s="18" r="E262"/>
     </row>
     <row r="263">
-      <c s="12" r="A263"/>
+      <c t="s" s="12" r="A263">
+        <v>960</v>
+      </c>
       <c t="s" s="7" r="B263">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c t="s" s="15" r="C263">
         <v>960</v>
       </c>
       <c t="s" s="7" r="D263">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c t="s" s="7" r="E263">
-        <v>962</v>
+        <v>963</v>
       </c>
     </row>
     <row r="264">
       <c s="12" r="A264"/>
       <c t="s" s="7" r="B264">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c t="s" s="15" r="C264">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c t="s" s="7" r="D264">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c t="s" s="7" r="E264">
-        <v>966</v>
+        <v>967</v>
       </c>
     </row>
     <row r="265">
       <c s="12" r="A265"/>
       <c t="s" s="7" r="B265">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c t="s" s="15" r="C265">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c t="s" s="7" r="D265">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c t="s" s="7" r="E265">
-        <v>970</v>
+        <v>971</v>
       </c>
     </row>
     <row r="266">
       <c s="12" r="A266"/>
       <c t="s" s="7" r="B266">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c t="s" s="15" r="C266">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c t="s" s="7" r="D266">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c t="s" s="7" r="E266">
-        <v>974</v>
+        <v>975</v>
       </c>
     </row>
     <row r="267">
       <c s="12" r="A267"/>
       <c t="s" s="7" r="B267">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c t="s" s="15" r="C267">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c t="s" s="7" r="D267">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c t="s" s="7" r="E267">
-        <v>978</v>
+        <v>979</v>
       </c>
     </row>
     <row r="268">
       <c s="12" r="A268"/>
       <c t="s" s="7" r="B268">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c t="s" s="15" r="C268">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c t="s" s="7" r="D268">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c t="s" s="7" r="E268">
-        <v>982</v>
+        <v>983</v>
       </c>
     </row>
     <row r="269">
       <c s="12" r="A269"/>
-      <c s="13" r="B269"/>
-      <c s="16" r="C269"/>
-      <c s="13" r="D269"/>
-      <c s="13" r="E269"/>
+      <c t="s" s="7" r="B269">
+        <v>984</v>
+      </c>
+      <c t="s" s="15" r="C269">
+        <v>985</v>
+      </c>
+      <c t="s" s="7" r="D269">
+        <v>986</v>
+      </c>
+      <c t="s" s="7" r="E269">
+        <v>987</v>
+      </c>
     </row>
     <row r="270">
-      <c t="s" s="12" r="A270">
-        <v>983</v>
-      </c>
-      <c t="s" s="7" r="B270">
-        <v>984</v>
-      </c>
-      <c t="s" s="15" r="C270">
-        <v>985</v>
-      </c>
-      <c t="s" s="7" r="D270">
-        <v>986</v>
-      </c>
-      <c t="s" s="7" r="E270">
-        <v>987</v>
-      </c>
+      <c s="12" r="A270"/>
+      <c s="13" r="B270"/>
+      <c s="16" r="C270"/>
+      <c s="13" r="D270"/>
+      <c s="13" r="E270"/>
     </row>
     <row r="271">
-      <c s="12" r="A271"/>
+      <c t="s" s="12" r="A271">
+        <v>988</v>
+      </c>
       <c t="s" s="7" r="B271">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c t="s" s="15" r="C271">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c t="s" s="7" r="D271">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c t="s" s="7" r="E271">
-        <v>990</v>
+        <v>992</v>
       </c>
     </row>
     <row r="272">
       <c s="12" r="A272"/>
-      <c s="13" r="B272"/>
-      <c s="16" r="C272"/>
-      <c s="13" r="D272"/>
-      <c s="13" r="E272"/>
+      <c t="s" s="7" r="B272">
+        <v>993</v>
+      </c>
+      <c t="s" s="15" r="C272">
+        <v>994</v>
+      </c>
+      <c t="s" s="7" r="D272">
+        <v>994</v>
+      </c>
+      <c t="s" s="7" r="E272">
+        <v>995</v>
+      </c>
     </row>
     <row r="273">
-      <c t="s" s="12" r="A273">
-        <v>991</v>
-      </c>
-      <c t="s" s="7" r="B273">
-        <v>992</v>
-      </c>
-      <c t="s" s="15" r="C273">
-        <v>993</v>
-      </c>
-      <c t="s" s="7" r="D273">
-        <v>994</v>
-      </c>
-      <c t="s" s="7" r="E273">
-        <v>995</v>
-      </c>
+      <c s="12" r="A273"/>
+      <c s="13" r="B273"/>
+      <c s="16" r="C273"/>
+      <c s="13" r="D273"/>
+      <c s="13" r="E273"/>
     </row>
     <row r="274">
-      <c s="12" r="A274"/>
+      <c t="s" s="12" r="A274">
+        <v>996</v>
+      </c>
       <c t="s" s="7" r="B274">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c t="s" s="15" r="C274">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c t="s" s="7" r="D274">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c t="s" s="7" r="E274">
-        <v>999</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="275">
       <c s="12" r="A275"/>
       <c t="s" s="7" r="B275">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c t="s" s="15" r="C275">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c t="s" s="7" r="D275">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c t="s" s="7" r="E275">
-        <v>1003</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="276">
       <c s="12" r="A276"/>
       <c t="s" s="7" r="B276">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c t="s" s="15" r="C276">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c t="s" s="7" r="D276">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c t="s" s="7" r="E276">
-        <v>1007</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="277">
       <c s="12" r="A277"/>
-      <c s="18" r="B277"/>
-      <c s="37" r="C277"/>
-      <c s="18" r="D277"/>
-      <c s="18" r="E277"/>
+      <c t="s" s="7" r="B277">
+        <v>1009</v>
+      </c>
+      <c t="s" s="15" r="C277">
+        <v>1010</v>
+      </c>
+      <c t="s" s="7" r="D277">
+        <v>1011</v>
+      </c>
+      <c t="s" s="7" r="E277">
+        <v>1012</v>
+      </c>
     </row>
     <row r="278">
-      <c t="s" s="12" r="A278">
-        <v>1008</v>
-      </c>
-      <c t="s" s="7" r="B278">
-        <v>1009</v>
-      </c>
-      <c t="s" s="15" r="C278">
-        <v>1010</v>
-      </c>
-      <c t="s" s="7" r="D278">
-        <v>1011</v>
-      </c>
-      <c t="s" s="7" r="E278">
-        <v>1012</v>
-      </c>
+      <c s="12" r="A278"/>
+      <c s="18" r="B278"/>
+      <c s="37" r="C278"/>
+      <c s="18" r="D278"/>
+      <c s="18" r="E278"/>
     </row>
     <row r="279">
-      <c s="12" r="A279"/>
+      <c t="s" s="12" r="A279">
+        <v>1013</v>
+      </c>
       <c t="s" s="7" r="B279">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c t="s" s="15" r="C279">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c t="s" s="7" r="D279">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c t="s" s="7" r="E279">
-        <v>1016</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="280">
       <c s="12" r="A280"/>
-      <c s="18" r="B280"/>
-      <c s="37" r="C280"/>
-      <c s="18" r="D280"/>
-      <c s="18" r="E280"/>
+      <c t="s" s="7" r="B280">
+        <v>1018</v>
+      </c>
+      <c t="s" s="15" r="C280">
+        <v>1019</v>
+      </c>
+      <c t="s" s="7" r="D280">
+        <v>1020</v>
+      </c>
+      <c t="s" s="7" r="E280">
+        <v>1021</v>
+      </c>
     </row>
     <row r="281">
-      <c t="s" s="12" r="A281">
-        <v>1017</v>
-      </c>
-      <c t="s" s="7" r="B281">
-        <v>1018</v>
-      </c>
-      <c t="s" s="15" r="C281">
-        <v>1019</v>
-      </c>
-      <c t="s" s="7" r="D281">
-        <v>1020</v>
-      </c>
-      <c t="s" s="7" r="E281">
-        <v>1021</v>
-      </c>
+      <c s="12" r="A281"/>
+      <c s="18" r="B281"/>
+      <c s="37" r="C281"/>
+      <c s="18" r="D281"/>
+      <c s="18" r="E281"/>
     </row>
     <row r="282">
-      <c s="12" r="A282"/>
-      <c s="18" r="B282"/>
-      <c s="9" r="C282"/>
-      <c s="18" r="D282"/>
-      <c s="18" r="E282"/>
+      <c t="s" s="12" r="A282">
+        <v>1022</v>
+      </c>
+      <c t="s" s="7" r="B282">
+        <v>1023</v>
+      </c>
+      <c t="s" s="15" r="C282">
+        <v>1024</v>
+      </c>
+      <c t="s" s="7" r="D282">
+        <v>1025</v>
+      </c>
+      <c t="s" s="7" r="E282">
+        <v>1026</v>
+      </c>
     </row>
     <row r="283">
-      <c t="s" s="12" r="A283">
-        <v>1022</v>
-      </c>
-      <c t="s" s="7" r="B283">
-        <v>1023</v>
-      </c>
-      <c t="s" s="15" r="C283">
-        <v>1024</v>
-      </c>
-      <c t="s" s="7" r="D283">
-        <v>1025</v>
-      </c>
-      <c t="s" s="7" r="E283">
-        <v>1026</v>
-      </c>
+      <c s="12" r="A283"/>
+      <c s="18" r="B283"/>
+      <c s="9" r="C283"/>
+      <c s="18" r="D283"/>
+      <c s="18" r="E283"/>
     </row>
     <row r="284">
-      <c s="12" r="A284"/>
+      <c t="s" s="12" r="A284">
+        <v>1027</v>
+      </c>
       <c t="s" s="7" r="B284">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c t="s" s="15" r="C284">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c t="s" s="7" r="D284">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c t="s" s="7" r="E284">
-        <v>1030</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="285">
       <c s="12" r="A285"/>
       <c t="s" s="7" r="B285">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c t="s" s="15" r="C285">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c t="s" s="7" r="D285">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c t="s" s="7" r="E285">
-        <v>1034</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="286">
       <c s="12" r="A286"/>
       <c t="s" s="7" r="B286">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c t="s" s="15" r="C286">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c t="s" s="7" r="D286">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c t="s" s="7" r="E286">
-        <v>1038</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="287">
       <c s="12" r="A287"/>
       <c t="s" s="7" r="B287">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c t="s" s="15" r="C287">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c t="s" s="7" r="D287">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c t="s" s="7" r="E287">
-        <v>1042</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="288">
       <c s="12" r="A288"/>
       <c t="s" s="7" r="B288">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c t="s" s="15" r="C288">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c t="s" s="7" r="D288">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c t="s" s="7" r="E288">
-        <v>1046</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="289">
       <c s="12" r="A289"/>
       <c t="s" s="7" r="B289">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c t="s" s="15" r="C289">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c t="s" s="7" r="D289">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c t="s" s="7" r="E289">
-        <v>1050</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="290">
       <c s="12" r="A290"/>
       <c t="s" s="7" r="B290">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c t="s" s="15" r="C290">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c t="s" s="7" r="D290">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c t="s" s="7" r="E290">
-        <v>1054</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="291">
-      <c s="20" r="A291"/>
-      <c s="18" r="B291"/>
-      <c s="9" r="C291"/>
-      <c s="18" r="D291"/>
-      <c s="18" r="E291"/>
+      <c s="12" r="A291"/>
+      <c t="s" s="7" r="B291">
+        <v>1056</v>
+      </c>
+      <c t="s" s="15" r="C291">
+        <v>1057</v>
+      </c>
+      <c t="s" s="7" r="D291">
+        <v>1058</v>
+      </c>
+      <c t="s" s="7" r="E291">
+        <v>1059</v>
+      </c>
     </row>
     <row r="292">
-      <c t="s" s="12" r="A292">
-        <v>1055</v>
-      </c>
-      <c t="s" s="7" r="B292">
-        <v>1056</v>
-      </c>
-      <c t="s" s="7" r="C292">
-        <v>1057</v>
-      </c>
-      <c t="s" s="7" r="D292">
-        <v>1058</v>
-      </c>
-      <c t="s" s="7" r="E292">
-        <v>1059</v>
-      </c>
+      <c s="20" r="A292"/>
+      <c s="18" r="B292"/>
+      <c s="9" r="C292"/>
+      <c s="18" r="D292"/>
+      <c s="18" r="E292"/>
     </row>
     <row r="293">
-      <c s="12" r="A293"/>
+      <c t="s" s="12" r="A293">
+        <v>1060</v>
+      </c>
       <c t="s" s="7" r="B293">
-        <v>1060</v>
-      </c>
-      <c t="s" s="15" r="C293">
         <v>1061</v>
       </c>
+      <c t="s" s="7" r="C293">
+        <v>1062</v>
+      </c>
       <c t="s" s="7" r="D293">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c t="s" s="7" r="E293">
-        <v>1063</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="294">
       <c s="12" r="A294"/>
       <c t="s" s="7" r="B294">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c t="s" s="15" r="C294">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c t="s" s="7" r="D294">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c t="s" s="7" r="E294">
-        <v>1067</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="295">
       <c s="12" r="A295"/>
       <c t="s" s="7" r="B295">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c t="s" s="15" r="C295">
-        <v>802</v>
+        <v>1070</v>
       </c>
       <c t="s" s="7" r="D295">
-        <v>1069</v>
+        <v>1071</v>
       </c>
       <c t="s" s="7" r="E295">
-        <v>1070</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="296">
       <c s="12" r="A296"/>
       <c t="s" s="7" r="B296">
-        <v>1071</v>
+        <v>1073</v>
       </c>
       <c t="s" s="15" r="C296">
-        <v>696</v>
+        <v>807</v>
       </c>
       <c t="s" s="7" r="D296">
-        <v>159</v>
+        <v>1074</v>
       </c>
       <c t="s" s="7" r="E296">
-        <v>698</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="297">
       <c s="12" r="A297"/>
       <c t="s" s="7" r="B297">
-        <v>1072</v>
+        <v>1076</v>
       </c>
       <c t="s" s="15" r="C297">
-        <v>1073</v>
+        <v>696</v>
       </c>
       <c t="s" s="7" r="D297">
-        <v>1074</v>
+        <v>159</v>
       </c>
       <c t="s" s="7" r="E297">
-        <v>1075</v>
+        <v>698</v>
       </c>
     </row>
     <row r="298">
-      <c s="20" r="A298"/>
-      <c s="18" r="B298"/>
-      <c s="9" r="C298"/>
-      <c s="18" r="D298"/>
-      <c s="18" r="E298"/>
+      <c s="12" r="A298"/>
+      <c t="s" s="7" r="B298">
+        <v>1077</v>
+      </c>
+      <c t="s" s="15" r="C298">
+        <v>1078</v>
+      </c>
+      <c t="s" s="7" r="D298">
+        <v>1079</v>
+      </c>
+      <c t="s" s="7" r="E298">
+        <v>1080</v>
+      </c>
     </row>
     <row r="299">
-      <c t="s" s="12" r="A299">
-        <v>1076</v>
-      </c>
-      <c t="s" s="7" r="B299">
-        <v>1077</v>
-      </c>
-      <c t="s" s="15" r="C299">
-        <v>1078</v>
-      </c>
-      <c t="s" s="7" r="D299">
-        <v>1079</v>
-      </c>
-      <c t="s" s="7" r="E299">
-        <v>1080</v>
-      </c>
+      <c s="20" r="A299"/>
+      <c s="18" r="B299"/>
+      <c s="9" r="C299"/>
+      <c s="18" r="D299"/>
+      <c s="18" r="E299"/>
     </row>
     <row r="300">
-      <c s="12" r="A300"/>
+      <c t="s" s="12" r="A300">
+        <v>1081</v>
+      </c>
       <c t="s" s="7" r="B300">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c t="s" s="15" r="C300">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c t="s" s="7" r="D300">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c t="s" s="7" r="E300">
-        <v>1084</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="301">
       <c s="12" r="A301"/>
       <c t="s" s="7" r="B301">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c t="s" s="15" r="C301">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c t="s" s="7" r="D301">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c t="s" s="7" r="E301">
-        <v>1088</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="302">
       <c s="12" r="A302"/>
       <c t="s" s="7" r="B302">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c t="s" s="15" r="C302">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c t="s" s="7" r="D302">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c t="s" s="7" r="E302">
-        <v>1091</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="303">
       <c s="12" r="A303"/>
       <c t="s" s="7" r="B303">
-        <v>1092</v>
+        <v>1094</v>
       </c>
       <c t="s" s="15" r="C303">
-        <v>1093</v>
+        <v>1095</v>
       </c>
       <c t="s" s="7" r="D303">
-        <v>1094</v>
+        <v>1096</v>
       </c>
       <c t="s" s="7" r="E303">
-        <v>1095</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="304">
       <c s="12" r="A304"/>
       <c t="s" s="7" r="B304">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c t="s" s="15" r="C304">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c t="s" s="7" r="D304">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c t="s" s="7" r="E304">
-        <v>1099</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="305">
       <c s="12" r="A305"/>
       <c t="s" s="7" r="B305">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c t="s" s="15" r="C305">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c t="s" s="7" r="D305">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c t="s" s="7" r="E305">
-        <v>1103</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="306">
       <c s="12" r="A306"/>
       <c t="s" s="7" r="B306">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c t="s" s="15" r="C306">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c t="s" s="7" r="D306">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c t="s" s="7" r="E306">
-        <v>1107</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="307">
       <c s="12" r="A307"/>
       <c t="s" s="7" r="B307">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c t="s" s="15" r="C307">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c t="s" s="7" r="D307">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c t="s" s="7" r="E307">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="308">
       <c s="12" r="A308"/>
       <c t="s" s="7" r="B308">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c t="s" s="15" r="C308">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c t="s" s="7" r="D308">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c t="s" s="7" r="E308">
-        <v>1115</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="309">
       <c s="12" r="A309"/>
       <c t="s" s="7" r="B309">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c t="s" s="15" r="C309">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c t="s" s="7" r="D309">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c t="s" s="7" r="E309">
-        <v>1119</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="310">
       <c s="12" r="A310"/>
       <c t="s" s="7" r="B310">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c t="s" s="15" r="C310">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c t="s" s="7" r="D310">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c t="s" s="7" r="E310">
-        <v>1123</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="311">
       <c s="12" r="A311"/>
       <c t="s" s="7" r="B311">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c t="s" s="15" r="C311">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c t="s" s="7" r="D311">
-        <v>1125</v>
+        <v>1127</v>
       </c>
       <c t="s" s="7" r="E311">
-        <v>1125</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="312">
       <c s="12" r="A312"/>
       <c t="s" s="7" r="B312">
-        <v>1126</v>
+        <v>1129</v>
       </c>
       <c t="s" s="15" r="C312">
-        <v>1127</v>
+        <v>1130</v>
       </c>
       <c t="s" s="7" r="D312">
-        <v>1128</v>
+        <v>1130</v>
       </c>
       <c t="s" s="7" r="E312">
-        <v>1129</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="313">
       <c s="12" r="A313"/>
       <c t="s" s="7" r="B313">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c t="s" s="15" r="C313">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c t="s" s="7" r="D313">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c t="s" s="7" r="E313">
-        <v>1133</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="314">
       <c s="12" r="A314"/>
       <c t="s" s="7" r="B314">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c t="s" s="15" r="C314">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c t="s" s="7" r="D314">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c t="s" s="7" r="E314">
-        <v>1137</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="315">
       <c s="12" r="A315"/>
       <c t="s" s="7" r="B315">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c t="s" s="15" r="C315">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c t="s" s="7" r="D315">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c t="s" s="7" r="E315">
-        <v>1141</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="316">
       <c s="12" r="A316"/>
       <c t="s" s="7" r="B316">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c t="s" s="15" r="C316">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c t="s" s="7" r="D316">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c t="s" s="7" r="E316">
-        <v>1145</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="317">
       <c s="12" r="A317"/>
       <c t="s" s="7" r="B317">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c t="s" s="15" r="C317">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c t="s" s="7" r="D317">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c t="s" s="7" r="E317">
-        <v>1149</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="318">
       <c s="12" r="A318"/>
       <c t="s" s="7" r="B318">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c t="s" s="15" r="C318">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c t="s" s="7" r="D318">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c t="s" s="7" r="E318">
-        <v>1153</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="319">
       <c s="12" r="A319"/>
-      <c s="18" r="B319"/>
-      <c s="9" r="C319"/>
-      <c s="18" r="D319"/>
-      <c s="18" r="E319"/>
+      <c t="s" s="7" r="B319">
+        <v>1155</v>
+      </c>
+      <c t="s" s="15" r="C319">
+        <v>1156</v>
+      </c>
+      <c t="s" s="7" r="D319">
+        <v>1157</v>
+      </c>
+      <c t="s" s="7" r="E319">
+        <v>1158</v>
+      </c>
     </row>
     <row r="320">
-      <c t="s" s="12" r="A320">
-        <v>1154</v>
-      </c>
-      <c t="s" s="7" r="B320">
-        <v>1155</v>
-      </c>
-      <c t="s" s="15" r="C320">
-        <v>1156</v>
-      </c>
-      <c t="s" s="7" r="D320">
-        <v>1157</v>
-      </c>
-      <c t="s" s="7" r="E320">
-        <v>1158</v>
-      </c>
+      <c s="12" r="A320"/>
+      <c s="18" r="B320"/>
+      <c s="9" r="C320"/>
+      <c s="18" r="D320"/>
+      <c s="18" r="E320"/>
     </row>
     <row r="321">
-      <c s="12" r="A321"/>
+      <c t="s" s="12" r="A321">
+        <v>1159</v>
+      </c>
       <c t="s" s="7" r="B321">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c t="s" s="15" r="C321">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c t="s" s="7" r="D321">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c t="s" s="7" r="E321">
-        <v>1162</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="322">
       <c s="12" r="A322"/>
       <c t="s" s="7" r="B322">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c t="s" s="15" r="C322">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c t="s" s="7" r="D322">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c t="s" s="7" r="E322">
-        <v>1166</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="323">
       <c s="12" r="A323"/>
       <c t="s" s="7" r="B323">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c t="s" s="15" r="C323">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c t="s" s="7" r="D323">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c t="s" s="7" r="E323">
-        <v>1170</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="324">
       <c s="12" r="A324"/>
       <c t="s" s="7" r="B324">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c t="s" s="15" r="C324">
-        <v>1171</v>
-      </c>
-      <c t="s" s="21" r="D324">
-        <v>1172</v>
-      </c>
-      <c t="s" s="21" r="E324">
         <v>1173</v>
+      </c>
+      <c t="s" s="7" r="D324">
+        <v>1174</v>
+      </c>
+      <c t="s" s="7" r="E324">
+        <v>1175</v>
       </c>
     </row>
     <row r="325">
       <c s="12" r="A325"/>
       <c t="s" s="7" r="B325">
-        <v>1174</v>
+        <v>1176</v>
       </c>
       <c t="s" s="15" r="C325">
-        <v>1175</v>
-      </c>
-      <c t="s" s="7" r="D325">
         <v>1176</v>
       </c>
-      <c t="s" s="7" r="E325">
+      <c t="s" s="21" r="D325">
         <v>1177</v>
+      </c>
+      <c t="s" s="21" r="E325">
+        <v>1178</v>
       </c>
     </row>
     <row r="326">
       <c s="12" r="A326"/>
       <c t="s" s="7" r="B326">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c t="s" s="15" r="C326">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c t="s" s="7" r="D326">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c t="s" s="7" r="E326">
-        <v>1181</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="327">
-      <c t="s" s="18" r="A327">
-        <v>1182</v>
-      </c>
-      <c s="33" r="B327"/>
+      <c s="12" r="A327"/>
+      <c t="s" s="7" r="B327">
+        <v>1183</v>
+      </c>
       <c t="s" s="15" r="C327">
-        <v>1183</v>
-      </c>
-      <c t="s" s="21" r="D327">
         <v>1184</v>
       </c>
-      <c t="s" s="21" r="E327">
+      <c t="s" s="7" r="D327">
         <v>1185</v>
       </c>
+      <c t="s" s="7" r="E327">
+        <v>1186</v>
+      </c>
     </row>
     <row r="328">
-      <c s="20" r="A328"/>
-      <c s="18" r="B328"/>
-      <c s="9" r="C328"/>
-      <c s="18" r="D328"/>
-      <c s="18" r="E328"/>
+      <c t="s" s="18" r="A328">
+        <v>1187</v>
+      </c>
+      <c s="33" r="B328"/>
+      <c t="s" s="15" r="C328">
+        <v>1188</v>
+      </c>
+      <c t="s" s="21" r="D328">
+        <v>1189</v>
+      </c>
+      <c t="s" s="21" r="E328">
+        <v>1190</v>
+      </c>
     </row>
     <row r="329">
-      <c t="s" s="20" r="A329">
-        <v>1186</v>
-      </c>
-      <c t="s" s="7" r="B329">
-        <v>1187</v>
-      </c>
-      <c t="s" s="7" r="C329">
-        <v>1188</v>
-      </c>
-      <c t="s" s="7" r="D329">
-        <v>1189</v>
-      </c>
-      <c t="s" s="7" r="E329">
-        <v>1190</v>
-      </c>
+      <c s="20" r="A329"/>
+      <c s="18" r="B329"/>
+      <c s="9" r="C329"/>
+      <c s="18" r="D329"/>
+      <c s="18" r="E329"/>
     </row>
     <row r="330">
-      <c s="16" r="A330"/>
+      <c t="s" s="20" r="A330">
+        <v>1191</v>
+      </c>
       <c t="s" s="7" r="B330">
-        <v>1191</v>
-      </c>
-      <c t="s" s="15" r="C330">
         <v>1192</v>
       </c>
+      <c t="s" s="7" r="C330">
+        <v>1193</v>
+      </c>
       <c t="s" s="7" r="D330">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c t="s" s="7" r="E330">
-        <v>1194</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="331">
       <c s="16" r="A331"/>
       <c t="s" s="7" r="B331">
-        <v>1195</v>
-      </c>
-      <c t="s" s="7" r="C331">
         <v>1196</v>
       </c>
+      <c t="s" s="15" r="C331">
+        <v>1197</v>
+      </c>
       <c t="s" s="7" r="D331">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c t="s" s="7" r="E331">
-        <v>1198</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="332">
-      <c s="20" r="A332"/>
+      <c s="16" r="A332"/>
       <c t="s" s="7" r="B332">
-        <v>1199</v>
-      </c>
-      <c t="s" s="15" r="C332">
         <v>1200</v>
       </c>
+      <c t="s" s="7" r="C332">
+        <v>1201</v>
+      </c>
       <c t="s" s="7" r="D332">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c t="s" s="7" r="E332">
-        <v>1202</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="333">
       <c s="20" r="A333"/>
       <c t="s" s="7" r="B333">
-        <v>1203</v>
-      </c>
-      <c t="s" s="7" r="C333">
         <v>1204</v>
       </c>
+      <c t="s" s="15" r="C333">
+        <v>1205</v>
+      </c>
       <c t="s" s="7" r="D333">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c t="s" s="7" r="E333">
-        <v>1206</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="334">
       <c s="20" r="A334"/>
       <c t="s" s="7" r="B334">
-        <v>1207</v>
-      </c>
-      <c t="s" s="15" r="C334">
         <v>1208</v>
       </c>
+      <c t="s" s="7" r="C334">
+        <v>1209</v>
+      </c>
       <c t="s" s="7" r="D334">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c t="s" s="7" r="E334">
-        <v>1210</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="335">
       <c s="20" r="A335"/>
       <c t="s" s="7" r="B335">
-        <v>1211</v>
-      </c>
-      <c t="s" s="7" r="C335">
         <v>1212</v>
       </c>
+      <c t="s" s="15" r="C335">
+        <v>1213</v>
+      </c>
       <c t="s" s="7" r="D335">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c t="s" s="7" r="E335">
-        <v>1214</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="336">
       <c s="20" r="A336"/>
       <c t="s" s="7" r="B336">
-        <v>1215</v>
-      </c>
-      <c t="s" s="15" r="C336">
         <v>1216</v>
       </c>
+      <c t="s" s="7" r="C336">
+        <v>1217</v>
+      </c>
       <c t="s" s="7" r="D336">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c t="s" s="7" r="E336">
-        <v>1218</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="337">
       <c s="20" r="A337"/>
       <c t="s" s="7" r="B337">
-        <v>1219</v>
-      </c>
-      <c t="s" s="7" r="C337">
         <v>1220</v>
       </c>
+      <c t="s" s="15" r="C337">
+        <v>1221</v>
+      </c>
       <c t="s" s="7" r="D337">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c t="s" s="7" r="E337">
-        <v>1222</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="338">
       <c s="20" r="A338"/>
       <c t="s" s="7" r="B338">
-        <v>1223</v>
-      </c>
-      <c t="s" s="15" r="C338">
         <v>1224</v>
       </c>
+      <c t="s" s="7" r="C338">
+        <v>1225</v>
+      </c>
       <c t="s" s="7" r="D338">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c t="s" s="7" r="E338">
-        <v>1226</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="339">
       <c s="20" r="A339"/>
       <c t="s" s="7" r="B339">
-        <v>1227</v>
-      </c>
-      <c t="s" s="7" r="C339">
         <v>1228</v>
       </c>
+      <c t="s" s="15" r="C339">
+        <v>1229</v>
+      </c>
       <c t="s" s="7" r="D339">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c t="s" s="7" r="E339">
-        <v>1230</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="340">
       <c s="20" r="A340"/>
       <c t="s" s="7" r="B340">
-        <v>1231</v>
-      </c>
-      <c t="s" s="15" r="C340">
-        <v>1224</v>
+        <v>1232</v>
+      </c>
+      <c t="s" s="7" r="C340">
+        <v>1233</v>
       </c>
       <c t="s" s="7" r="D340">
-        <v>1225</v>
+        <v>1234</v>
       </c>
       <c t="s" s="7" r="E340">
-        <v>1226</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="341">
       <c s="20" r="A341"/>
       <c t="s" s="7" r="B341">
-        <v>1232</v>
+        <v>1236</v>
       </c>
       <c t="s" s="15" r="C341">
-        <v>1233</v>
+        <v>1229</v>
       </c>
       <c t="s" s="7" r="D341">
-        <v>1234</v>
+        <v>1230</v>
       </c>
       <c t="s" s="7" r="E341">
-        <v>1235</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="342">
       <c s="20" r="A342"/>
       <c t="s" s="7" r="B342">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c t="s" s="15" r="C342">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c t="s" s="7" r="D342">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c t="s" s="7" r="E342">
-        <v>1239</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="343">
-      <c s="8" r="A343"/>
-      <c t="s" s="1" r="B343">
-        <v>1240</v>
-      </c>
-      <c t="s" s="1" r="C343">
+      <c s="20" r="A343"/>
+      <c t="s" s="7" r="B343">
         <v>1241</v>
       </c>
-      <c t="s" s="1" r="D343">
+      <c t="s" s="15" r="C343">
         <v>1242</v>
       </c>
-      <c t="s" s="1" r="E343">
+      <c t="s" s="7" r="D343">
         <v>1243</v>
+      </c>
+      <c t="s" s="7" r="E343">
+        <v>1244</v>
       </c>
     </row>
     <row r="344">
       <c s="8" r="A344"/>
       <c t="s" s="1" r="B344">
-        <v>1244</v>
-      </c>
-      <c t="s" s="39" r="C344">
         <v>1245</v>
       </c>
+      <c t="s" s="1" r="C344">
+        <v>1246</v>
+      </c>
       <c t="s" s="1" r="D344">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c t="s" s="1" r="E344">
-        <v>1247</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="345">
-      <c s="12" r="A345"/>
-      <c t="s" s="7" r="B345">
-        <v>1248</v>
-      </c>
-      <c t="s" s="15" r="C345">
+      <c s="8" r="A345"/>
+      <c t="s" s="1" r="B345">
         <v>1249</v>
       </c>
-      <c t="s" s="7" r="D345">
+      <c t="s" s="39" r="C345">
         <v>1250</v>
       </c>
-      <c t="s" s="7" r="E345">
+      <c t="s" s="1" r="D345">
         <v>1251</v>
       </c>
+      <c t="s" s="1" r="E345">
+        <v>1252</v>
+      </c>
     </row>
     <row r="346">
-      <c t="s" s="12" r="A346">
-        <v>1252</v>
-      </c>
-      <c t="s" s="15" r="B346">
+      <c s="12" r="A346"/>
+      <c t="s" s="7" r="B346">
         <v>1253</v>
       </c>
       <c t="s" s="15" r="C346">
         <v>1254</v>
       </c>
-      <c t="s" s="21" r="D346">
+      <c t="s" s="7" r="D346">
         <v>1255</v>
       </c>
       <c t="s" s="7" r="E346">
@@ -9562,63 +9576,80 @@
       </c>
     </row>
     <row r="347">
-      <c s="12" r="A347"/>
+      <c t="s" s="12" r="A347">
+        <v>1257</v>
+      </c>
       <c t="s" s="15" r="B347">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c t="s" s="15" r="C347">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c t="s" s="21" r="D347">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c t="s" s="7" r="E347">
-        <v>1260</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="348">
       <c s="12" r="A348"/>
-      <c s="9" r="C348"/>
-      <c s="18" r="D348"/>
-      <c s="18" r="E348"/>
+      <c t="s" s="15" r="B348">
+        <v>1262</v>
+      </c>
+      <c t="s" s="15" r="C348">
+        <v>1263</v>
+      </c>
+      <c t="s" s="21" r="D348">
+        <v>1264</v>
+      </c>
+      <c t="s" s="7" r="E348">
+        <v>1265</v>
+      </c>
     </row>
     <row r="349">
-      <c t="s" s="12" r="A349">
-        <v>1261</v>
-      </c>
-      <c t="s" s="33" r="B349">
-        <v>1262</v>
-      </c>
-      <c t="s" s="15" r="C349">
-        <v>1263</v>
-      </c>
-      <c t="s" s="7" r="D349">
-        <v>1264</v>
-      </c>
-      <c t="s" s="7" r="E349">
-        <v>1265</v>
-      </c>
+      <c s="12" r="A349"/>
+      <c s="9" r="C349"/>
+      <c s="18" r="D349"/>
+      <c s="18" r="E349"/>
     </row>
     <row r="350">
-      <c s="12" r="A350"/>
+      <c t="s" s="12" r="A350">
+        <v>1266</v>
+      </c>
       <c t="s" s="33" r="B350">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c t="s" s="15" r="C350">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c t="s" s="7" r="D350">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c t="s" s="7" r="E350">
-        <v>1269</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="351">
       <c s="12" r="A351"/>
-      <c s="9" r="C351"/>
-      <c s="18" r="D351"/>
-      <c s="18" r="E351"/>
+      <c t="s" s="33" r="B351">
+        <v>1271</v>
+      </c>
+      <c t="s" s="15" r="C351">
+        <v>1272</v>
+      </c>
+      <c t="s" s="7" r="D351">
+        <v>1273</v>
+      </c>
+      <c t="s" s="7" r="E351">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="352">
+      <c s="12" r="A352"/>
+      <c s="9" r="C352"/>
+      <c s="18" r="D352"/>
+      <c s="18" r="E352"/>
     </row>
   </sheetData>
 </worksheet>
@@ -9636,17 +9667,17 @@
   <sheetData>
     <row customHeight="1" r="1" ht="112.5">
       <c t="s" s="3" r="A1">
-        <v>1270</v>
+        <v>1275</v>
       </c>
     </row>
     <row customHeight="1" r="2" ht="112.5">
       <c t="s" s="5" r="A2">
-        <v>1271</v>
+        <v>1276</v>
       </c>
     </row>
     <row customHeight="1" r="3" ht="112.5">
       <c t="s" s="11" r="A3">
-        <v>1272</v>
+        <v>1277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EWD-22956 - Rename "Learning experiences"
Former-commit-id: eb8496d23a8ab211c430accd55c7af1e54b458bb
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -2295,7 +2295,7 @@
     <t>Fertig stellen</t>
   </si>
   <si>
-    <t>createObjectiveFromExperience</t>
+    <t>createObjectiveFromCourse</t>
   </si>
   <si>
     <t>Create learning objective</t>
@@ -2665,7 +2665,7 @@
     <t>Erstellen Sie eine Lernerfahrung</t>
   </si>
   <si>
-    <t>introCreateLE</t>
+    <t>introCreateCourse</t>
   </si>
   <si>
     <t>Create course</t>
@@ -2689,7 +2689,7 @@
     <t>Benennen Sie die Lernerfahrung und bestimmen Sie, wie Sie die Lernerfahrung präsentieren möchten, als Kurs oder als Quiz.</t>
   </si>
   <si>
-    <t>introCreateLEDesc</t>
+    <t>introCreateCourseDesc</t>
   </si>
   <si>
     <t>Name the course and choose how you want to present it, as a freestyle course or as a quiz.</t>
@@ -2713,7 +2713,7 @@
     <t>Verbinden Sie Lernziele mit Lernerfahrungen</t>
   </si>
   <si>
-    <t>introConnectLOtoLE</t>
+    <t>introConnectLOtoCourse</t>
   </si>
   <si>
     <t>Connect learning objectives to the course</t>
@@ -2737,7 +2737,7 @@
     <t>Stellen Sie Ihre Lernerfahrung (Kurs oder Quiz) zusammen, indem Sie ihr Lernziele hinzufügen.</t>
   </si>
   <si>
-    <t>introConnectLOtoLEDesc</t>
+    <t>introConnectLOtoCourseDesc</t>
   </si>
   <si>
     <t>Assemble your course (freestyle course or quiz) by adding learning objectives to it. </t>
@@ -2758,7 +2758,7 @@
     <t>Veröffentlichen Sie die Lernerfahrung</t>
   </si>
   <si>
-    <t>introPublishLE</t>
+    <t>introPublishCourse</t>
   </si>
   <si>
     <t>Publiceer de cursus</t>
@@ -2767,7 +2767,7 @@
     <t>Veröffentlichen Sie den Kurs</t>
   </si>
   <si>
-    <t>introPublishLEDesc</t>
+    <t>introPublishCourseDesc</t>
   </si>
   <si>
     <t>To easygenerator web-server or to your own web server.</t>
@@ -8643,17 +8643,17 @@
       </c>
     </row>
     <row r="243">
-      <c s="39" r="A243"/>
-      <c t="s" s="1" r="B243">
+      <c s="49" r="A243"/>
+      <c t="s" s="55" r="B243">
         <v>901</v>
       </c>
-      <c t="s" s="51" r="C243">
+      <c t="s" s="14" r="C243">
         <v>902</v>
       </c>
-      <c t="s" s="9" r="D243">
+      <c t="s" s="47" r="D243">
         <v>903</v>
       </c>
-      <c t="s" s="9" r="E243">
+      <c t="s" s="47" r="E243">
         <v>904</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Localization resources updated - removed extra dots
Former-commit-id: 7c81f32e32613da3d8a982a1e39d9db8e001766a
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -906,10 +906,10 @@
     <t>Download the course as SCORM 1.2 package in order to publish it to LMS</t>
   </si>
   <si>
-    <t>Hier kunt u de cursus als "SCORM 1.2"-pakket downloaden, zodat u het vervolgens in LMS unt publiceren.</t>
-  </si>
-  <si>
-    <t>Hier können Sie den Kurs als "SCORM 1.2"-Paket herunterladen, damit Sie ihn anschließend in "LMS" veröffentlichen können.</t>
+    <t>Hier kunt u de cursus als "SCORM 1.2"-pakket downloaden, zodat u het vervolgens in LMS unt publiceren</t>
+  </si>
+  <si>
+    <t>Hier können Sie den Kurs als "SCORM 1.2"-Paket herunterladen, damit Sie ihn anschließend in "LMS" veröffentlichen können</t>
   </si>
   <si>
     <t>assembling</t>

</xml_diff>

<commit_message>
EWD-23118 - Incorrect view of course in review mode
Former-commit-id: 0f7bcc6ae56dc7a0b2cf740f7a6a3ecba1e9e111
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="1296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="1295">
   <si>
     <t>Key</t>
   </si>
@@ -3843,9 +3843,6 @@
   </si>
   <si>
     <t>reviewPublishingCourse</t>
-  </si>
-  <si>
-    <t>Publishing...</t>
   </si>
   <si>
     <t>Feedback</t>
@@ -9840,135 +9837,135 @@
         <v>1263</v>
       </c>
       <c t="s" r="C357">
-        <v>1264</v>
+        <v>217</v>
       </c>
       <c t="s" r="D357">
-        <v>1264</v>
+        <v>217</v>
       </c>
       <c t="s" r="E357">
-        <v>1264</v>
+        <v>217</v>
       </c>
     </row>
     <row r="359">
       <c t="s" r="A359">
+        <v>1264</v>
+      </c>
+      <c t="s" r="B359">
         <v>1265</v>
       </c>
-      <c t="s" r="B359">
-        <v>1266</v>
-      </c>
       <c t="s" r="C359">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c t="s" r="D359">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c t="s" r="E359">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="360">
       <c s="15" r="A360"/>
       <c t="s" s="4" r="B360">
+        <v>1266</v>
+      </c>
+      <c t="s" s="4" r="C360">
         <v>1267</v>
       </c>
-      <c t="s" s="4" r="C360">
+      <c t="s" s="4" r="D360">
         <v>1268</v>
       </c>
-      <c t="s" s="4" r="D360">
+      <c t="s" s="4" r="E360">
         <v>1269</v>
-      </c>
-      <c t="s" s="4" r="E360">
-        <v>1270</v>
       </c>
     </row>
     <row r="361">
       <c s="15" r="A361"/>
       <c t="s" s="4" r="B361">
+        <v>1270</v>
+      </c>
+      <c t="s" s="4" r="C361">
         <v>1271</v>
       </c>
-      <c t="s" s="4" r="C361">
+      <c t="s" s="39" r="D361">
         <v>1272</v>
       </c>
-      <c t="s" s="39" r="D361">
+      <c t="s" s="39" r="E361">
         <v>1273</v>
-      </c>
-      <c t="s" s="39" r="E361">
-        <v>1274</v>
       </c>
     </row>
     <row r="362">
       <c s="15" r="A362"/>
       <c t="s" s="4" r="B362">
+        <v>1274</v>
+      </c>
+      <c t="s" s="4" r="C362">
         <v>1275</v>
       </c>
-      <c t="s" s="4" r="C362">
+      <c t="s" s="39" r="D362">
         <v>1276</v>
       </c>
-      <c t="s" s="39" r="D362">
+      <c t="s" s="39" r="E362">
         <v>1277</v>
-      </c>
-      <c t="s" s="39" r="E362">
-        <v>1278</v>
       </c>
     </row>
     <row r="363">
       <c s="15" r="A363"/>
       <c t="s" s="4" r="B363">
+        <v>1278</v>
+      </c>
+      <c t="s" s="4" r="C363">
         <v>1279</v>
       </c>
-      <c t="s" s="4" r="C363">
+      <c t="s" s="39" r="D363">
         <v>1280</v>
       </c>
-      <c t="s" s="39" r="D363">
+      <c t="s" s="39" r="E363">
         <v>1281</v>
-      </c>
-      <c t="s" s="39" r="E363">
-        <v>1282</v>
       </c>
     </row>
     <row r="364">
       <c s="15" r="A364"/>
       <c t="s" s="4" r="B364">
+        <v>1282</v>
+      </c>
+      <c t="s" s="4" r="C364">
         <v>1283</v>
       </c>
-      <c t="s" s="4" r="C364">
+      <c t="s" s="39" r="D364">
         <v>1284</v>
       </c>
-      <c t="s" s="39" r="D364">
+      <c t="s" s="39" r="E364">
         <v>1285</v>
-      </c>
-      <c t="s" s="39" r="E364">
-        <v>1286</v>
       </c>
     </row>
     <row r="365">
       <c s="15" r="A365"/>
       <c t="s" s="4" r="B365">
+        <v>1286</v>
+      </c>
+      <c t="s" s="4" r="C365">
         <v>1287</v>
       </c>
-      <c t="s" s="4" r="C365">
+      <c t="s" s="39" r="D365">
         <v>1288</v>
       </c>
-      <c t="s" s="39" r="D365">
+      <c t="s" s="39" r="E365">
         <v>1289</v>
-      </c>
-      <c t="s" s="39" r="E365">
-        <v>1290</v>
       </c>
     </row>
     <row r="366">
       <c s="15" r="A366"/>
       <c t="s" r="B366">
+        <v>1290</v>
+      </c>
+      <c t="s" r="C366">
         <v>1291</v>
       </c>
-      <c t="s" r="C366">
-        <v>1292</v>
-      </c>
       <c t="s" r="D366">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c t="s" r="E366">
-        <v>1292</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="376">
@@ -9991,17 +9988,17 @@
   <sheetData>
     <row customHeight="1" r="1" ht="112.5">
       <c t="s" s="3" r="A1">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row customHeight="1" r="2" ht="112.5">
       <c t="s" s="32" r="A2">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row customHeight="1" r="3" ht="112.5">
       <c t="s" s="6" r="A3">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EWD-23127 - Incorrect message after sending feedback
Former-commit-id: bb685cc5503aac519c4ab1cda8dc7ebb8b5037bb
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="1295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="1293">
   <si>
     <t>Key</t>
   </si>
@@ -3914,14 +3914,7 @@
     <t>successFeedback</t>
   </si>
   <si>
-    <t>Your feedback has been sent successfully</t>
-  </si>
-  <si>
-    <t>Uw feedback is verzonden
-</t>
-  </si>
-  <si>
-    <t>Ihr Feedback wurde gesendet</t>
+    <t>Feedback was sent</t>
   </si>
   <si>
     <t>feedbackTabTitle</t>
@@ -9947,25 +9940,25 @@
         <v>1287</v>
       </c>
       <c t="s" s="39" r="D365">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c t="s" s="39" r="E365">
-        <v>1289</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="366">
       <c s="15" r="A366"/>
       <c t="s" r="B366">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c t="s" r="C366">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c t="s" r="D366">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c t="s" r="E366">
-        <v>1291</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="376">
@@ -9988,17 +9981,17 @@
   <sheetData>
     <row customHeight="1" r="1" ht="112.5">
       <c t="s" s="3" r="A1">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row customHeight="1" r="2" ht="112.5">
       <c t="s" s="32" r="A2">
-        <v>1293</v>
+        <v>1291</v>
       </c>
     </row>
     <row customHeight="1" r="3" ht="112.5">
       <c t="s" s="6" r="A3">
-        <v>1294</v>
+        <v>1292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EWD-23048 - External review: Read comments in the app
Former-commit-id: 6ab97c4fd6948c91114874e47f9e8158a5e927e2
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="1293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="1295">
   <si>
     <t>Key</t>
   </si>
@@ -3818,7 +3818,7 @@
     <t>reviewTabTitle</t>
   </si>
   <si>
-    <t>Share course for review</t>
+    <t>Comments</t>
   </si>
   <si>
     <t>reviewTabHelp</t>
@@ -3843,6 +3843,12 @@
   </si>
   <si>
     <t>reviewPublishingCourse</t>
+  </si>
+  <si>
+    <t>reviewNoComments</t>
+  </si>
+  <si>
+    <t>No comments yet</t>
   </si>
   <si>
     <t>Feedback</t>
@@ -9748,12 +9754,6 @@
       <c t="s" r="C351">
         <v>1252</v>
       </c>
-      <c t="s" r="D351">
-        <v>1252</v>
-      </c>
-      <c t="s" r="E351">
-        <v>1252</v>
-      </c>
     </row>
     <row r="352">
       <c t="s" r="B352">
@@ -9762,12 +9762,6 @@
       <c t="s" r="C352">
         <v>1255</v>
       </c>
-      <c t="s" r="D352">
-        <v>1255</v>
-      </c>
-      <c t="s" r="E352">
-        <v>1255</v>
-      </c>
     </row>
     <row r="353">
       <c t="s" r="B353">
@@ -9776,12 +9770,6 @@
       <c t="s" r="C353">
         <v>1257</v>
       </c>
-      <c t="s" r="D353">
-        <v>1257</v>
-      </c>
-      <c t="s" r="E353">
-        <v>1257</v>
-      </c>
     </row>
     <row r="354">
       <c t="s" r="B354">
@@ -9790,12 +9778,6 @@
       <c t="s" r="C354">
         <v>1259</v>
       </c>
-      <c t="s" r="D354">
-        <v>1259</v>
-      </c>
-      <c t="s" r="E354">
-        <v>1259</v>
-      </c>
     </row>
     <row r="355">
       <c t="s" r="B355">
@@ -9804,12 +9786,6 @@
       <c t="s" r="C355">
         <v>705</v>
       </c>
-      <c t="s" r="D355">
-        <v>705</v>
-      </c>
-      <c t="s" r="E355">
-        <v>705</v>
-      </c>
     </row>
     <row r="356">
       <c t="s" r="B356">
@@ -9818,12 +9794,6 @@
       <c t="s" r="C356">
         <v>1262</v>
       </c>
-      <c t="s" r="D356">
-        <v>1262</v>
-      </c>
-      <c t="s" r="E356">
-        <v>1262</v>
-      </c>
     </row>
     <row r="357">
       <c t="s" r="B357">
@@ -9832,115 +9802,102 @@
       <c t="s" r="C357">
         <v>217</v>
       </c>
-      <c t="s" r="D357">
-        <v>217</v>
-      </c>
-      <c t="s" r="E357">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="359">
-      <c t="s" r="A359">
+    </row>
+    <row r="358">
+      <c t="s" r="B358">
         <v>1264</v>
       </c>
-      <c t="s" r="B359">
+      <c t="s" r="C358">
         <v>1265</v>
       </c>
-      <c t="s" r="C359">
-        <v>1264</v>
-      </c>
-      <c t="s" r="D359">
-        <v>1264</v>
-      </c>
-      <c t="s" r="E359">
-        <v>1264</v>
-      </c>
     </row>
     <row r="360">
-      <c s="15" r="A360"/>
-      <c t="s" s="4" r="B360">
+      <c t="s" r="A360">
         <v>1266</v>
       </c>
-      <c t="s" s="4" r="C360">
+      <c t="s" r="B360">
         <v>1267</v>
       </c>
-      <c t="s" s="4" r="D360">
-        <v>1268</v>
-      </c>
-      <c t="s" s="4" r="E360">
-        <v>1269</v>
+      <c t="s" r="C360">
+        <v>1266</v>
+      </c>
+      <c t="s" r="D360">
+        <v>1266</v>
+      </c>
+      <c t="s" r="E360">
+        <v>1266</v>
       </c>
     </row>
     <row r="361">
       <c s="15" r="A361"/>
       <c t="s" s="4" r="B361">
+        <v>1268</v>
+      </c>
+      <c t="s" s="4" r="C361">
+        <v>1269</v>
+      </c>
+      <c t="s" s="4" r="D361">
         <v>1270</v>
       </c>
-      <c t="s" s="4" r="C361">
+      <c t="s" s="4" r="E361">
         <v>1271</v>
-      </c>
-      <c t="s" s="39" r="D361">
-        <v>1272</v>
-      </c>
-      <c t="s" s="39" r="E361">
-        <v>1273</v>
       </c>
     </row>
     <row r="362">
       <c s="15" r="A362"/>
       <c t="s" s="4" r="B362">
+        <v>1272</v>
+      </c>
+      <c t="s" s="4" r="C362">
+        <v>1273</v>
+      </c>
+      <c t="s" s="39" r="D362">
         <v>1274</v>
       </c>
-      <c t="s" s="4" r="C362">
+      <c t="s" s="39" r="E362">
         <v>1275</v>
-      </c>
-      <c t="s" s="39" r="D362">
-        <v>1276</v>
-      </c>
-      <c t="s" s="39" r="E362">
-        <v>1277</v>
       </c>
     </row>
     <row r="363">
       <c s="15" r="A363"/>
       <c t="s" s="4" r="B363">
+        <v>1276</v>
+      </c>
+      <c t="s" s="4" r="C363">
+        <v>1277</v>
+      </c>
+      <c t="s" s="39" r="D363">
         <v>1278</v>
       </c>
-      <c t="s" s="4" r="C363">
+      <c t="s" s="39" r="E363">
         <v>1279</v>
-      </c>
-      <c t="s" s="39" r="D363">
-        <v>1280</v>
-      </c>
-      <c t="s" s="39" r="E363">
-        <v>1281</v>
       </c>
     </row>
     <row r="364">
       <c s="15" r="A364"/>
       <c t="s" s="4" r="B364">
+        <v>1280</v>
+      </c>
+      <c t="s" s="4" r="C364">
+        <v>1281</v>
+      </c>
+      <c t="s" s="39" r="D364">
         <v>1282</v>
       </c>
-      <c t="s" s="4" r="C364">
+      <c t="s" s="39" r="E364">
         <v>1283</v>
-      </c>
-      <c t="s" s="39" r="D364">
-        <v>1284</v>
-      </c>
-      <c t="s" s="39" r="E364">
-        <v>1285</v>
       </c>
     </row>
     <row r="365">
       <c s="15" r="A365"/>
       <c t="s" s="4" r="B365">
+        <v>1284</v>
+      </c>
+      <c t="s" s="4" r="C365">
+        <v>1285</v>
+      </c>
+      <c t="s" s="39" r="D365">
         <v>1286</v>
-      </c>
-      <c t="s" s="4" r="C365">
-        <v>1287</v>
-      </c>
-      <c t="s" s="39" r="D365">
-        <v>1287</v>
       </c>
       <c t="s" s="39" r="E365">
         <v>1287</v>
@@ -9948,22 +9905,37 @@
     </row>
     <row r="366">
       <c s="15" r="A366"/>
-      <c t="s" r="B366">
+      <c t="s" s="4" r="B366">
         <v>1288</v>
       </c>
-      <c t="s" r="C366">
+      <c t="s" s="4" r="C366">
         <v>1289</v>
       </c>
-      <c t="s" r="D366">
+      <c t="s" s="39" r="D366">
         <v>1289</v>
       </c>
-      <c t="s" r="E366">
+      <c t="s" s="39" r="E366">
         <v>1289</v>
       </c>
     </row>
-    <row r="376">
-      <c s="48" r="D376"/>
-      <c s="48" r="E376"/>
+    <row r="367">
+      <c s="15" r="A367"/>
+      <c t="s" r="B367">
+        <v>1290</v>
+      </c>
+      <c t="s" r="C367">
+        <v>1291</v>
+      </c>
+      <c t="s" r="D367">
+        <v>1291</v>
+      </c>
+      <c t="s" r="E367">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="377">
+      <c s="48" r="D377"/>
+      <c s="48" r="E377"/>
     </row>
   </sheetData>
 </worksheet>
@@ -9981,17 +9953,17 @@
   <sheetData>
     <row customHeight="1" r="1" ht="112.5">
       <c t="s" s="3" r="A1">
-        <v>1290</v>
+        <v>1292</v>
       </c>
     </row>
     <row customHeight="1" r="2" ht="112.5">
       <c t="s" s="32" r="A2">
-        <v>1291</v>
+        <v>1293</v>
       </c>
     </row>
     <row customHeight="1" r="3" ht="112.5">
       <c t="s" s="6" r="A3">
-        <v>1292</v>
+        <v>1294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EWD-23058 - External review: As a paid feature
Former-commit-id: ac501258ea7759319f183fec8a7fd3c2632d223b
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="1295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1360" uniqueCount="1299">
   <si>
     <t>Key</t>
   </si>
@@ -3849,6 +3849,18 @@
   </si>
   <si>
     <t>No comments yet</t>
+  </si>
+  <si>
+    <t>reviewNotPaidMessage</t>
+  </si>
+  <si>
+    <t>Starter plan users only. Please &lt;u style="color: #2cb7ff;"&gt;upgrade&lt;/u&gt; to use this functionality.</t>
+  </si>
+  <si>
+    <t>upgradeToStarterPlanToUseCommentsErrorMessage</t>
+  </si>
+  <si>
+    <t>Please upgrade your account to "Starter plan" to be able to see comments.</t>
   </si>
   <si>
     <t>Feedback</t>
@@ -9811,131 +9823,159 @@
         <v>1265</v>
       </c>
     </row>
+    <row r="359">
+      <c t="s" r="B359">
+        <v>1266</v>
+      </c>
+      <c t="s" r="C359">
+        <v>1267</v>
+      </c>
+      <c t="s" r="D359">
+        <v>1267</v>
+      </c>
+      <c t="s" r="E359">
+        <v>1267</v>
+      </c>
+    </row>
     <row r="360">
-      <c t="s" r="A360">
-        <v>1266</v>
-      </c>
       <c t="s" r="B360">
-        <v>1267</v>
-      </c>
-      <c t="s" r="C360">
-        <v>1266</v>
+        <v>1268</v>
+      </c>
+      <c t="s" s="4" r="C360">
+        <v>1269</v>
       </c>
       <c t="s" r="D360">
-        <v>1266</v>
+        <v>1269</v>
       </c>
       <c t="s" r="E360">
-        <v>1266</v>
-      </c>
-    </row>
-    <row r="361">
-      <c s="15" r="A361"/>
-      <c t="s" s="4" r="B361">
-        <v>1268</v>
-      </c>
-      <c t="s" s="4" r="C361">
         <v>1269</v>
       </c>
-      <c t="s" s="4" r="D361">
+    </row>
+    <row r="362">
+      <c t="s" r="A362">
         <v>1270</v>
       </c>
-      <c t="s" s="4" r="E361">
+      <c t="s" r="B362">
         <v>1271</v>
       </c>
-    </row>
-    <row r="362">
-      <c s="15" r="A362"/>
-      <c t="s" s="4" r="B362">
-        <v>1272</v>
-      </c>
-      <c t="s" s="4" r="C362">
-        <v>1273</v>
-      </c>
-      <c t="s" s="39" r="D362">
-        <v>1274</v>
-      </c>
-      <c t="s" s="39" r="E362">
-        <v>1275</v>
+      <c t="s" r="C362">
+        <v>1270</v>
+      </c>
+      <c t="s" r="D362">
+        <v>1270</v>
+      </c>
+      <c t="s" r="E362">
+        <v>1270</v>
       </c>
     </row>
     <row r="363">
       <c s="15" r="A363"/>
       <c t="s" s="4" r="B363">
-        <v>1276</v>
+        <v>1272</v>
       </c>
       <c t="s" s="4" r="C363">
-        <v>1277</v>
-      </c>
-      <c t="s" s="39" r="D363">
-        <v>1278</v>
-      </c>
-      <c t="s" s="39" r="E363">
-        <v>1279</v>
+        <v>1273</v>
+      </c>
+      <c t="s" s="4" r="D363">
+        <v>1274</v>
+      </c>
+      <c t="s" s="4" r="E363">
+        <v>1275</v>
       </c>
     </row>
     <row r="364">
       <c s="15" r="A364"/>
       <c t="s" s="4" r="B364">
-        <v>1280</v>
+        <v>1276</v>
       </c>
       <c t="s" s="4" r="C364">
-        <v>1281</v>
+        <v>1277</v>
       </c>
       <c t="s" s="39" r="D364">
-        <v>1282</v>
+        <v>1278</v>
       </c>
       <c t="s" s="39" r="E364">
-        <v>1283</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="365">
       <c s="15" r="A365"/>
       <c t="s" s="4" r="B365">
-        <v>1284</v>
+        <v>1280</v>
       </c>
       <c t="s" s="4" r="C365">
-        <v>1285</v>
+        <v>1281</v>
       </c>
       <c t="s" s="39" r="D365">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c t="s" s="39" r="E365">
-        <v>1287</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="366">
       <c s="15" r="A366"/>
       <c t="s" s="4" r="B366">
-        <v>1288</v>
+        <v>1284</v>
       </c>
       <c t="s" s="4" r="C366">
-        <v>1289</v>
+        <v>1285</v>
       </c>
       <c t="s" s="39" r="D366">
-        <v>1289</v>
+        <v>1286</v>
       </c>
       <c t="s" s="39" r="E366">
-        <v>1289</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="367">
       <c s="15" r="A367"/>
-      <c t="s" r="B367">
+      <c t="s" s="4" r="B367">
+        <v>1288</v>
+      </c>
+      <c t="s" s="4" r="C367">
+        <v>1289</v>
+      </c>
+      <c t="s" s="39" r="D367">
         <v>1290</v>
       </c>
-      <c t="s" r="C367">
+      <c t="s" s="39" r="E367">
         <v>1291</v>
       </c>
-      <c t="s" r="D367">
-        <v>1291</v>
-      </c>
-      <c t="s" r="E367">
-        <v>1291</v>
-      </c>
-    </row>
-    <row r="377">
-      <c s="48" r="D377"/>
-      <c s="48" r="E377"/>
+    </row>
+    <row r="368">
+      <c s="15" r="A368"/>
+      <c t="s" s="4" r="B368">
+        <v>1292</v>
+      </c>
+      <c t="s" s="4" r="C368">
+        <v>1293</v>
+      </c>
+      <c t="s" s="39" r="D368">
+        <v>1293</v>
+      </c>
+      <c t="s" s="39" r="E368">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="369">
+      <c s="15" r="A369"/>
+      <c t="s" r="B369">
+        <v>1294</v>
+      </c>
+      <c t="s" r="C369">
+        <v>1295</v>
+      </c>
+      <c t="s" r="D369">
+        <v>1295</v>
+      </c>
+      <c t="s" r="E369">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="379">
+      <c s="48" r="D379"/>
+      <c s="48" r="E379"/>
     </row>
   </sheetData>
 </worksheet>
@@ -9953,17 +9993,17 @@
   <sheetData>
     <row customHeight="1" r="1" ht="112.5">
       <c t="s" s="3" r="A1">
-        <v>1292</v>
+        <v>1296</v>
       </c>
     </row>
     <row customHeight="1" r="2" ht="112.5">
       <c t="s" s="32" r="A2">
-        <v>1293</v>
+        <v>1297</v>
       </c>
     </row>
     <row customHeight="1" r="3" ht="112.5">
       <c t="s" s="6" r="A3">
-        <v>1294</v>
+        <v>1298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EWD-23181 - Incorrect title for template demo
Former-commit-id: a3f5eff48add9f4505ef1b3fcf947ae74c1eb476
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -1188,10 +1188,10 @@
     <t>Erstellen und fortfahren</t>
   </si>
   <si>
-    <t>previewDemo</t>
-  </si>
-  <si>
-    <t>Preview demo</t>
+    <t>previewTemplate</t>
+  </si>
+  <si>
+    <t>Preview template</t>
   </si>
   <si>
     <t>Question</t>

</xml_diff>

<commit_message>
EWD-23208 - Different text for "get link" and "upload course" states
Former-commit-id: f8e2d47307ddc057c3f8687d4957d52108c1b072
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="1308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="1312">
   <si>
     <t>Key</t>
   </si>
@@ -3847,10 +3847,16 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>reviewTabHelp</t>
-  </si>
-  <si>
-    <t>Press the button and then share the link with your external reviewers:</t>
+    <t>getReviewTabHelp</t>
+  </si>
+  <si>
+    <t>Press the get link button and then share the link with your external reviewers:</t>
+  </si>
+  <si>
+    <t>updateReviewTabHelp</t>
+  </si>
+  <si>
+    <t>Press the upload button and then share the link with your external reviewers:</t>
   </si>
   <si>
     <t>reviewGetLink</t>
@@ -3887,6 +3893,12 @@
   </si>
   <si>
     <t>Please upgrade your account to "Starter plan" to be able to see comments.</t>
+  </si>
+  <si>
+    <t>loadingCourseError</t>
+  </si>
+  <si>
+    <t>Smth went wrong!</t>
   </si>
   <si>
     <t>Feedback</t>
@@ -9890,17 +9902,17 @@
         <v>1269</v>
       </c>
       <c t="s" s="45" r="C361">
-        <v>708</v>
+        <v>1270</v>
       </c>
       <c s="45" r="D361"/>
       <c s="45" r="E361"/>
     </row>
     <row r="362">
       <c t="s" s="45" r="B362">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c t="s" s="45" r="C362">
-        <v>1271</v>
+        <v>708</v>
       </c>
       <c s="45" r="D362"/>
       <c s="45" r="E362"/>
@@ -9910,17 +9922,17 @@
         <v>1272</v>
       </c>
       <c t="s" s="45" r="C363">
-        <v>217</v>
+        <v>1273</v>
       </c>
       <c s="45" r="D363"/>
       <c s="45" r="E363"/>
     </row>
     <row r="364">
       <c t="s" s="45" r="B364">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c t="s" s="45" r="C364">
-        <v>1274</v>
+        <v>217</v>
       </c>
       <c s="45" r="D364"/>
       <c s="45" r="E364"/>
@@ -9939,141 +9951,159 @@
       <c t="s" s="45" r="B366">
         <v>1277</v>
       </c>
-      <c t="s" s="4" r="C366">
+      <c t="s" s="45" r="C366">
         <v>1278</v>
       </c>
-      <c t="s" s="45" r="D366">
-        <v>1278</v>
-      </c>
-      <c t="s" s="45" r="E366">
-        <v>1278</v>
+      <c s="45" r="D366"/>
+      <c s="45" r="E366"/>
+    </row>
+    <row r="367">
+      <c t="s" s="45" r="B367">
+        <v>1279</v>
+      </c>
+      <c t="s" s="4" r="C367">
+        <v>1280</v>
+      </c>
+      <c t="s" s="45" r="D367">
+        <v>1280</v>
+      </c>
+      <c t="s" s="45" r="E367">
+        <v>1280</v>
       </c>
     </row>
     <row r="368">
-      <c t="s" r="A368">
-        <v>1279</v>
-      </c>
-      <c t="s" s="45" r="B368">
-        <v>1280</v>
-      </c>
-      <c t="s" s="45" r="C368">
-        <v>1279</v>
-      </c>
-      <c t="s" s="45" r="D368">
-        <v>1279</v>
-      </c>
-      <c t="s" s="45" r="E368">
-        <v>1279</v>
-      </c>
-    </row>
-    <row r="369">
-      <c s="15" r="A369"/>
-      <c t="s" s="4" r="B369">
+      <c t="s" r="B368">
         <v>1281</v>
       </c>
-      <c t="s" s="4" r="C369">
+      <c t="s" r="C368">
         <v>1282</v>
       </c>
-      <c t="s" s="4" r="D369">
+    </row>
+    <row r="370">
+      <c t="s" r="A370">
         <v>1283</v>
       </c>
-      <c t="s" s="4" r="E369">
+      <c t="s" s="45" r="B370">
         <v>1284</v>
       </c>
-    </row>
-    <row r="370">
-      <c s="15" r="A370"/>
-      <c t="s" s="4" r="B370">
-        <v>1285</v>
-      </c>
-      <c t="s" s="4" r="C370">
-        <v>1286</v>
-      </c>
-      <c t="s" s="39" r="D370">
-        <v>1287</v>
-      </c>
-      <c t="s" s="39" r="E370">
-        <v>1288</v>
+      <c t="s" s="45" r="C370">
+        <v>1283</v>
+      </c>
+      <c t="s" s="45" r="D370">
+        <v>1283</v>
+      </c>
+      <c t="s" s="45" r="E370">
+        <v>1283</v>
       </c>
     </row>
     <row r="371">
       <c s="15" r="A371"/>
       <c t="s" s="4" r="B371">
-        <v>1289</v>
+        <v>1285</v>
       </c>
       <c t="s" s="4" r="C371">
-        <v>1290</v>
-      </c>
-      <c t="s" s="39" r="D371">
-        <v>1291</v>
-      </c>
-      <c t="s" s="39" r="E371">
-        <v>1292</v>
+        <v>1286</v>
+      </c>
+      <c t="s" s="4" r="D371">
+        <v>1287</v>
+      </c>
+      <c t="s" s="4" r="E371">
+        <v>1288</v>
       </c>
     </row>
     <row r="372">
       <c s="15" r="A372"/>
       <c t="s" s="4" r="B372">
-        <v>1293</v>
+        <v>1289</v>
       </c>
       <c t="s" s="4" r="C372">
-        <v>1294</v>
+        <v>1290</v>
       </c>
       <c t="s" s="39" r="D372">
-        <v>1295</v>
+        <v>1291</v>
       </c>
       <c t="s" s="39" r="E372">
-        <v>1296</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="373">
       <c s="15" r="A373"/>
       <c t="s" s="4" r="B373">
-        <v>1297</v>
+        <v>1293</v>
       </c>
       <c t="s" s="4" r="C373">
-        <v>1298</v>
+        <v>1294</v>
       </c>
       <c t="s" s="39" r="D373">
-        <v>1299</v>
+        <v>1295</v>
       </c>
       <c t="s" s="39" r="E373">
-        <v>1300</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="374">
       <c s="15" r="A374"/>
       <c t="s" s="4" r="B374">
-        <v>1301</v>
+        <v>1297</v>
       </c>
       <c t="s" s="4" r="C374">
-        <v>1302</v>
+        <v>1298</v>
       </c>
       <c t="s" s="39" r="D374">
-        <v>1302</v>
+        <v>1299</v>
       </c>
       <c t="s" s="39" r="E374">
-        <v>1302</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="375">
       <c s="15" r="A375"/>
-      <c t="s" r="B375">
+      <c t="s" s="4" r="B375">
+        <v>1301</v>
+      </c>
+      <c t="s" s="4" r="C375">
+        <v>1302</v>
+      </c>
+      <c t="s" s="39" r="D375">
         <v>1303</v>
       </c>
-      <c t="s" r="C375">
+      <c t="s" s="39" r="E375">
         <v>1304</v>
       </c>
-      <c t="s" r="D375">
-        <v>1304</v>
-      </c>
-      <c t="s" r="E375">
-        <v>1304</v>
-      </c>
-    </row>
-    <row r="385">
-      <c s="48" r="D385"/>
-      <c s="48" r="E385"/>
+    </row>
+    <row r="376">
+      <c s="15" r="A376"/>
+      <c t="s" s="4" r="B376">
+        <v>1305</v>
+      </c>
+      <c t="s" s="4" r="C376">
+        <v>1306</v>
+      </c>
+      <c t="s" s="39" r="D376">
+        <v>1306</v>
+      </c>
+      <c t="s" s="39" r="E376">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="377">
+      <c s="15" r="A377"/>
+      <c t="s" r="B377">
+        <v>1307</v>
+      </c>
+      <c t="s" r="C377">
+        <v>1308</v>
+      </c>
+      <c t="s" r="D377">
+        <v>1308</v>
+      </c>
+      <c t="s" r="E377">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="387">
+      <c s="48" r="D387"/>
+      <c s="48" r="E387"/>
     </row>
   </sheetData>
 </worksheet>
@@ -10091,17 +10121,17 @@
   <sheetData>
     <row customHeight="1" r="1" ht="112.5">
       <c t="s" s="3" r="A1">
-        <v>1305</v>
+        <v>1309</v>
       </c>
     </row>
     <row customHeight="1" r="2" ht="112.5">
       <c t="s" s="32" r="A2">
-        <v>1306</v>
+        <v>1310</v>
       </c>
     </row>
     <row customHeight="1" r="3" ht="112.5">
       <c t="s" s="6" r="A3">
-        <v>1307</v>
+        <v>1311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EWD-22846 - Navigation sidebar (resources)
Former-commit-id: 16715c21ee5cb140f9ef0131b56d5ee79a296404
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="1312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="1318">
   <si>
     <t>Key</t>
   </si>
@@ -2264,7 +2264,7 @@
     <t>introElearningPrincipleOne</t>
   </si>
   <si>
-    <t>All learning processes starts with the definition of &lt;strong&gt;learning objectives&lt;/strong&gt;. </t>
+    <t>All learning processes start with the definition of &lt;strong&gt;learning objectives&lt;/strong&gt;. </t>
   </si>
   <si>
     <t>Alle leerprocessen beginnen met de definitie van de &lt;strong&gt;leerdoelen&lt;/strong&gt;.</t>
@@ -3766,7 +3766,7 @@
     <t>deliverHelpHint</t>
   </si>
   <si>
-    <t>&lt;p&gt;To publish this course on your own webserver - download course as HTML/JavaScript package;&lt;/p&gt;&lt;p&gt;To publish the course to an LMS - download the course as SCORM 1.2 package;&lt;/p&gt;&lt;p&gt;Or publish the course on easygenerator webserver - just get a link and share it with your learners.&lt;/p&gt;</t>
+    <t>&lt;p&gt;To publish this course on &lt;strong&gt;your own webserver&lt;/strong&gt; - download course as HTML/JavaScript package;&lt;/p&gt;&lt;p&gt;To publish the course to an &lt;strong&gt;LMS&lt;/strong&gt; - download the course as SCORM 1.2 package;&lt;/p&gt;&lt;p&gt;Or publish the course on &lt;strong&gt;easygenerator webserver&lt;/strong&gt; - just get a link and share it with your learners.&lt;/p&gt;</t>
   </si>
   <si>
     <t>helpCloseButton</t>
@@ -3977,6 +3977,24 @@
   </si>
   <si>
     <t>Give feedback</t>
+  </si>
+  <si>
+    <t>Navigation tree</t>
+  </si>
+  <si>
+    <t>hideNavigationTree</t>
+  </si>
+  <si>
+    <t>Hide navigation</t>
+  </si>
+  <si>
+    <t>createCourseTreeNodeTitle</t>
+  </si>
+  <si>
+    <t>createObjectiveTreeNodeTitle</t>
+  </si>
+  <si>
+    <t>createQuestionTreeNodeTitle</t>
   </si>
   <si>
     <t>Translated OK</t>
@@ -10101,6 +10119,65 @@
         <v>1308</v>
       </c>
     </row>
+    <row r="379">
+      <c t="s" r="A379">
+        <v>1309</v>
+      </c>
+      <c t="s" r="B379">
+        <v>1310</v>
+      </c>
+      <c t="s" r="C379">
+        <v>1311</v>
+      </c>
+      <c t="s" r="D379">
+        <v>1311</v>
+      </c>
+      <c t="s" r="E379">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="380">
+      <c t="s" r="B380">
+        <v>1312</v>
+      </c>
+      <c t="s" r="C380">
+        <v>159</v>
+      </c>
+      <c t="s" r="D380">
+        <v>159</v>
+      </c>
+      <c t="s" r="E380">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="381">
+      <c t="s" r="B381">
+        <v>1313</v>
+      </c>
+      <c t="s" r="C381">
+        <v>130</v>
+      </c>
+      <c t="s" r="D381">
+        <v>130</v>
+      </c>
+      <c t="s" r="E381">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="382">
+      <c t="s" r="B382">
+        <v>1314</v>
+      </c>
+      <c t="s" r="C382">
+        <v>394</v>
+      </c>
+      <c t="s" r="D382">
+        <v>394</v>
+      </c>
+      <c t="s" r="E382">
+        <v>394</v>
+      </c>
+    </row>
     <row r="387">
       <c s="48" r="D387"/>
       <c s="48" r="E387"/>
@@ -10121,17 +10198,17 @@
   <sheetData>
     <row customHeight="1" r="1" ht="112.5">
       <c t="s" s="3" r="A1">
-        <v>1309</v>
+        <v>1315</v>
       </c>
     </row>
     <row customHeight="1" r="2" ht="112.5">
       <c t="s" s="32" r="A2">
-        <v>1310</v>
+        <v>1316</v>
       </c>
     </row>
     <row customHeight="1" r="3" ht="112.5">
       <c t="s" s="6" r="A3">
-        <v>1311</v>
+        <v>1317</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EWD-23252 - Add tooltip to tree icon
Former-commit-id: 7dc0ac03fafbee4d5ed032d1a3bfecfb72b18639
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="1317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1393" uniqueCount="1319">
   <si>
     <t>Key</t>
   </si>
@@ -3992,6 +3992,12 @@
   </si>
   <si>
     <t>createQuestionTreeNodeTitle</t>
+  </si>
+  <si>
+    <t>openNavigationBar</t>
+  </si>
+  <si>
+    <t>Open navigation bar</t>
   </si>
   <si>
     <t>Translated OK</t>
@@ -10175,6 +10181,20 @@
         <v>393</v>
       </c>
     </row>
+    <row r="383">
+      <c t="s" r="B383">
+        <v>1314</v>
+      </c>
+      <c t="s" r="C383">
+        <v>1315</v>
+      </c>
+      <c t="s" r="D383">
+        <v>1315</v>
+      </c>
+      <c t="s" r="E383">
+        <v>1315</v>
+      </c>
+    </row>
     <row r="387">
       <c s="48" r="D387"/>
       <c s="48" r="E387"/>
@@ -10195,17 +10215,17 @@
   <sheetData>
     <row customHeight="1" r="1" ht="112.5">
       <c t="s" s="3" r="A1">
-        <v>1314</v>
+        <v>1316</v>
       </c>
     </row>
     <row customHeight="1" r="2" ht="112.5">
       <c t="s" s="32" r="A2">
-        <v>1315</v>
+        <v>1317</v>
       </c>
     </row>
     <row customHeight="1" r="3" ht="112.5">
       <c t="s" s="6" r="A3">
-        <v>1316</v>
+        <v>1318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EWD-23294 - Remove userproperties view and clean all multilanguage occurrences.
Former-commit-id: fb4e689d0c97cacf50bbb160b1a63c1ea42d864d
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1393" uniqueCount="1319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="1317">
   <si>
     <t>Key</t>
   </si>
@@ -2542,12 +2542,6 @@
   </si>
   <si>
     <t>Leider ist ein Fehler aufgetreten. Prüfen Sie die URL auf eventuelle Fehler; verwenden Sie die Navigationselemente oben, oder klicken Sie unten auf den Link "Start".</t>
-  </si>
-  <si>
-    <t>User properties</t>
-  </si>
-  <si>
-    <t>userProperties</t>
   </si>
   <si>
     <t>Not supported browsers</t>
@@ -8095,2048 +8089,2056 @@
       <c t="s" s="36" r="A229">
         <v>841</v>
       </c>
-      <c t="s" s="24" r="B229">
+      <c t="s" s="29" r="B229">
         <v>842</v>
       </c>
-      <c t="s" s="16" r="C229">
-        <v>841</v>
-      </c>
-      <c s="24" r="D229"/>
-      <c s="24" r="E229"/>
+      <c t="s" s="26" r="C229">
+        <v>843</v>
+      </c>
+      <c s="29" r="D229"/>
+      <c s="29" r="E229"/>
     </row>
     <row r="230">
       <c s="36" r="A230"/>
-      <c s="11" r="B230"/>
-      <c s="35" r="C230"/>
-      <c s="11" r="D230"/>
-      <c s="11" r="E230"/>
+      <c t="s" s="29" r="B230">
+        <v>844</v>
+      </c>
+      <c t="s" s="26" r="C230">
+        <v>845</v>
+      </c>
+      <c s="29" r="D230"/>
+      <c s="29" r="E230"/>
     </row>
     <row r="231">
-      <c t="s" s="36" r="A231">
-        <v>843</v>
-      </c>
-      <c t="s" s="29" r="B231">
-        <v>844</v>
-      </c>
-      <c t="s" s="26" r="C231">
-        <v>845</v>
-      </c>
-      <c s="29" r="D231"/>
-      <c s="29" r="E231"/>
+      <c s="36" r="A231"/>
+      <c s="35" r="B231"/>
+      <c s="35" r="C231"/>
+      <c s="11" r="D231"/>
+      <c s="11" r="E231"/>
     </row>
     <row r="232">
-      <c s="36" r="A232"/>
-      <c t="s" s="29" r="B232">
+      <c t="s" s="36" r="A232">
         <v>846</v>
       </c>
-      <c t="s" s="26" r="C232">
+      <c t="s" s="45" r="B232">
         <v>847</v>
       </c>
-      <c s="29" r="D232"/>
-      <c s="29" r="E232"/>
+      <c t="s" s="45" r="C232">
+        <v>848</v>
+      </c>
+      <c t="s" s="4" r="D232">
+        <v>849</v>
+      </c>
+      <c t="s" s="4" r="E232">
+        <v>850</v>
+      </c>
     </row>
     <row r="233">
       <c s="36" r="A233"/>
-      <c s="35" r="B233"/>
-      <c s="35" r="C233"/>
-      <c s="11" r="D233"/>
-      <c s="11" r="E233"/>
+      <c t="s" s="45" r="B233">
+        <v>851</v>
+      </c>
+      <c t="s" s="45" r="C233">
+        <v>852</v>
+      </c>
+      <c t="s" s="4" r="D233">
+        <v>852</v>
+      </c>
+      <c t="s" s="4" r="E233">
+        <v>853</v>
+      </c>
     </row>
     <row r="234">
-      <c t="s" s="36" r="A234">
-        <v>848</v>
-      </c>
+      <c s="36" r="A234"/>
       <c t="s" s="45" r="B234">
-        <v>849</v>
+        <v>854</v>
       </c>
       <c t="s" s="45" r="C234">
-        <v>850</v>
+        <v>855</v>
       </c>
       <c t="s" s="4" r="D234">
-        <v>851</v>
+        <v>856</v>
       </c>
       <c t="s" s="4" r="E234">
-        <v>852</v>
+        <v>857</v>
       </c>
     </row>
     <row r="235">
       <c s="36" r="A235"/>
       <c t="s" s="45" r="B235">
-        <v>853</v>
+        <v>858</v>
       </c>
       <c t="s" s="45" r="C235">
-        <v>854</v>
+        <v>859</v>
       </c>
       <c t="s" s="4" r="D235">
-        <v>854</v>
+        <v>860</v>
       </c>
       <c t="s" s="4" r="E235">
-        <v>855</v>
+        <v>318</v>
       </c>
     </row>
     <row r="236">
       <c s="36" r="A236"/>
-      <c t="s" s="45" r="B236">
-        <v>856</v>
-      </c>
-      <c t="s" s="45" r="C236">
-        <v>857</v>
+      <c t="s" s="8" r="B236">
+        <v>861</v>
+      </c>
+      <c t="s" s="8" r="C236">
+        <v>862</v>
       </c>
       <c t="s" s="4" r="D236">
-        <v>858</v>
+        <v>863</v>
       </c>
       <c t="s" s="4" r="E236">
-        <v>859</v>
+        <v>864</v>
       </c>
     </row>
     <row r="237">
       <c s="36" r="A237"/>
-      <c t="s" s="45" r="B237">
-        <v>860</v>
-      </c>
-      <c t="s" s="45" r="C237">
-        <v>861</v>
+      <c t="s" s="8" r="B237">
+        <v>865</v>
+      </c>
+      <c t="s" s="8" r="C237">
+        <v>866</v>
       </c>
       <c t="s" s="4" r="D237">
-        <v>862</v>
+        <v>867</v>
       </c>
       <c t="s" s="4" r="E237">
-        <v>318</v>
+        <v>868</v>
       </c>
     </row>
     <row r="238">
       <c s="36" r="A238"/>
       <c t="s" s="8" r="B238">
-        <v>863</v>
+        <v>869</v>
       </c>
       <c t="s" s="8" r="C238">
-        <v>864</v>
+        <v>870</v>
       </c>
       <c t="s" s="4" r="D238">
-        <v>865</v>
+        <v>871</v>
       </c>
       <c t="s" s="4" r="E238">
-        <v>866</v>
+        <v>872</v>
       </c>
     </row>
     <row r="239">
       <c s="36" r="A239"/>
       <c t="s" s="8" r="B239">
-        <v>867</v>
+        <v>873</v>
       </c>
       <c t="s" s="8" r="C239">
-        <v>868</v>
+        <v>874</v>
       </c>
       <c t="s" s="4" r="D239">
-        <v>869</v>
+        <v>875</v>
       </c>
       <c t="s" s="4" r="E239">
-        <v>870</v>
+        <v>876</v>
       </c>
     </row>
     <row r="240">
       <c s="36" r="A240"/>
       <c t="s" s="8" r="B240">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c t="s" s="8" r="C240">
-        <v>872</v>
+        <v>878</v>
       </c>
       <c t="s" s="4" r="D240">
-        <v>873</v>
+        <v>879</v>
       </c>
       <c t="s" s="4" r="E240">
-        <v>874</v>
+        <v>880</v>
       </c>
     </row>
     <row r="241">
       <c s="36" r="A241"/>
       <c t="s" s="8" r="B241">
-        <v>875</v>
+        <v>881</v>
       </c>
       <c t="s" s="8" r="C241">
-        <v>876</v>
-      </c>
-      <c t="s" s="4" r="D241">
-        <v>877</v>
-      </c>
-      <c t="s" s="4" r="E241">
-        <v>878</v>
+        <v>882</v>
+      </c>
+      <c t="s" s="17" r="D241">
+        <v>883</v>
+      </c>
+      <c t="s" s="17" r="E241">
+        <v>884</v>
       </c>
     </row>
     <row r="242">
       <c s="36" r="A242"/>
       <c t="s" s="8" r="B242">
-        <v>879</v>
+        <v>885</v>
       </c>
       <c t="s" s="8" r="C242">
-        <v>880</v>
-      </c>
-      <c t="s" s="4" r="D242">
-        <v>881</v>
-      </c>
-      <c t="s" s="4" r="E242">
-        <v>882</v>
+        <v>886</v>
+      </c>
+      <c t="s" s="17" r="D242">
+        <v>887</v>
+      </c>
+      <c t="s" s="17" r="E242">
+        <v>888</v>
       </c>
     </row>
     <row r="243">
       <c s="36" r="A243"/>
-      <c t="s" s="8" r="B243">
-        <v>883</v>
-      </c>
-      <c t="s" s="8" r="C243">
-        <v>884</v>
-      </c>
-      <c t="s" s="17" r="D243">
-        <v>885</v>
-      </c>
-      <c t="s" s="17" r="E243">
-        <v>886</v>
-      </c>
+      <c s="36" r="B243"/>
+      <c s="36" r="C243"/>
+      <c s="36" r="D243"/>
+      <c s="36" r="E243"/>
     </row>
     <row r="244">
       <c s="36" r="A244"/>
       <c t="s" s="8" r="B244">
-        <v>887</v>
+        <v>889</v>
       </c>
       <c t="s" s="8" r="C244">
-        <v>888</v>
-      </c>
-      <c t="s" s="17" r="D244">
-        <v>889</v>
-      </c>
-      <c t="s" s="17" r="E244">
         <v>890</v>
+      </c>
+      <c t="s" s="4" r="D244">
+        <v>891</v>
+      </c>
+      <c t="s" s="4" r="E244">
+        <v>892</v>
       </c>
     </row>
     <row r="245">
       <c s="36" r="A245"/>
-      <c s="36" r="B245"/>
-      <c s="36" r="C245"/>
-      <c s="36" r="D245"/>
-      <c s="36" r="E245"/>
+      <c t="s" s="4" r="B245">
+        <v>893</v>
+      </c>
+      <c t="s" s="8" r="C245">
+        <v>894</v>
+      </c>
+      <c t="s" s="4" r="D245">
+        <v>895</v>
+      </c>
+      <c t="s" s="4" r="E245">
+        <v>896</v>
+      </c>
     </row>
     <row r="246">
       <c s="36" r="A246"/>
-      <c t="s" s="8" r="B246">
-        <v>891</v>
+      <c t="s" s="4" r="B246">
+        <v>897</v>
       </c>
       <c t="s" s="8" r="C246">
-        <v>892</v>
+        <v>898</v>
       </c>
       <c t="s" s="4" r="D246">
-        <v>893</v>
+        <v>899</v>
       </c>
       <c t="s" s="4" r="E246">
-        <v>894</v>
+        <v>900</v>
       </c>
     </row>
     <row r="247">
       <c s="36" r="A247"/>
       <c t="s" s="4" r="B247">
-        <v>895</v>
+        <v>901</v>
       </c>
       <c t="s" s="8" r="C247">
-        <v>896</v>
+        <v>902</v>
       </c>
       <c t="s" s="4" r="D247">
-        <v>897</v>
+        <v>903</v>
       </c>
       <c t="s" s="4" r="E247">
-        <v>898</v>
+        <v>904</v>
       </c>
     </row>
     <row r="248">
       <c s="36" r="A248"/>
       <c t="s" s="4" r="B248">
-        <v>899</v>
+        <v>905</v>
       </c>
       <c t="s" s="8" r="C248">
-        <v>900</v>
+        <v>906</v>
       </c>
       <c t="s" s="4" r="D248">
-        <v>901</v>
+        <v>907</v>
       </c>
       <c t="s" s="4" r="E248">
-        <v>902</v>
+        <v>908</v>
       </c>
     </row>
     <row r="249">
       <c s="36" r="A249"/>
       <c t="s" s="4" r="B249">
-        <v>903</v>
+        <v>909</v>
       </c>
       <c t="s" s="8" r="C249">
-        <v>904</v>
-      </c>
-      <c t="s" s="4" r="D249">
-        <v>905</v>
-      </c>
-      <c t="s" s="4" r="E249">
-        <v>906</v>
+        <v>910</v>
+      </c>
+      <c t="s" s="44" r="D249">
+        <v>911</v>
+      </c>
+      <c t="s" s="44" r="E249">
+        <v>912</v>
       </c>
     </row>
     <row r="250">
       <c s="36" r="A250"/>
       <c t="s" s="4" r="B250">
-        <v>907</v>
+        <v>913</v>
       </c>
       <c t="s" s="8" r="C250">
-        <v>908</v>
+        <v>914</v>
       </c>
       <c t="s" s="4" r="D250">
-        <v>909</v>
+        <v>915</v>
       </c>
       <c t="s" s="4" r="E250">
-        <v>910</v>
+        <v>916</v>
       </c>
     </row>
     <row r="251">
       <c s="36" r="A251"/>
       <c t="s" s="4" r="B251">
-        <v>911</v>
+        <v>917</v>
       </c>
       <c t="s" s="8" r="C251">
-        <v>912</v>
-      </c>
-      <c t="s" s="44" r="D251">
-        <v>913</v>
-      </c>
-      <c t="s" s="44" r="E251">
-        <v>914</v>
+        <v>918</v>
+      </c>
+      <c t="s" s="4" r="D251">
+        <v>919</v>
+      </c>
+      <c t="s" s="4" r="E251">
+        <v>920</v>
       </c>
     </row>
     <row r="252">
       <c s="36" r="A252"/>
       <c t="s" s="4" r="B252">
-        <v>915</v>
+        <v>921</v>
       </c>
       <c t="s" s="8" r="C252">
-        <v>916</v>
+        <v>922</v>
       </c>
       <c t="s" s="4" r="D252">
-        <v>917</v>
+        <v>923</v>
       </c>
       <c t="s" s="4" r="E252">
-        <v>918</v>
+        <v>924</v>
       </c>
     </row>
     <row r="253">
       <c s="36" r="A253"/>
       <c t="s" s="4" r="B253">
-        <v>919</v>
+        <v>925</v>
       </c>
       <c t="s" s="8" r="C253">
-        <v>920</v>
+        <v>926</v>
       </c>
       <c t="s" s="4" r="D253">
-        <v>921</v>
+        <v>927</v>
       </c>
       <c t="s" s="4" r="E253">
-        <v>922</v>
+        <v>928</v>
       </c>
     </row>
     <row r="254">
       <c s="36" r="A254"/>
       <c t="s" s="4" r="B254">
-        <v>923</v>
+        <v>929</v>
       </c>
       <c t="s" s="8" r="C254">
-        <v>924</v>
+        <v>930</v>
       </c>
       <c t="s" s="4" r="D254">
-        <v>925</v>
+        <v>931</v>
       </c>
       <c t="s" s="4" r="E254">
-        <v>926</v>
+        <v>932</v>
       </c>
     </row>
     <row r="255">
       <c s="36" r="A255"/>
-      <c t="s" s="4" r="B255">
-        <v>927</v>
-      </c>
-      <c t="s" s="8" r="C255">
-        <v>928</v>
-      </c>
-      <c t="s" s="4" r="D255">
-        <v>929</v>
-      </c>
-      <c t="s" s="4" r="E255">
-        <v>930</v>
-      </c>
+      <c s="11" r="B255"/>
+      <c s="49" r="C255"/>
+      <c s="11" r="D255"/>
+      <c s="11" r="E255"/>
     </row>
     <row r="256">
-      <c s="36" r="A256"/>
-      <c t="s" s="4" r="B256">
-        <v>931</v>
-      </c>
-      <c t="s" s="8" r="C256">
-        <v>932</v>
+      <c t="s" s="36" r="A256">
+        <v>933</v>
+      </c>
+      <c t="s" s="45" r="B256">
+        <v>934</v>
+      </c>
+      <c t="s" s="4" r="C256">
+        <v>852</v>
       </c>
       <c t="s" s="4" r="D256">
-        <v>933</v>
+        <v>852</v>
       </c>
       <c t="s" s="4" r="E256">
-        <v>934</v>
+        <v>853</v>
       </c>
     </row>
     <row r="257">
       <c s="36" r="A257"/>
-      <c s="11" r="B257"/>
-      <c s="49" r="C257"/>
-      <c s="11" r="D257"/>
-      <c s="11" r="E257"/>
+      <c t="s" s="4" r="B257">
+        <v>935</v>
+      </c>
+      <c t="s" s="8" r="C257">
+        <v>855</v>
+      </c>
+      <c t="s" s="4" r="D257">
+        <v>856</v>
+      </c>
+      <c t="s" s="4" r="E257">
+        <v>857</v>
+      </c>
     </row>
     <row r="258">
-      <c t="s" s="36" r="A258">
-        <v>935</v>
-      </c>
-      <c t="s" s="45" r="B258">
+      <c t="s" s="4" r="B258">
         <v>936</v>
       </c>
-      <c t="s" s="4" r="C258">
-        <v>854</v>
+      <c t="s" s="8" r="C258">
+        <v>937</v>
       </c>
       <c t="s" s="4" r="D258">
-        <v>854</v>
+        <v>938</v>
       </c>
       <c t="s" s="4" r="E258">
-        <v>855</v>
+        <v>939</v>
       </c>
     </row>
     <row r="259">
       <c s="36" r="A259"/>
       <c t="s" s="4" r="B259">
-        <v>937</v>
+        <v>940</v>
       </c>
       <c t="s" s="8" r="C259">
-        <v>857</v>
+        <v>941</v>
       </c>
       <c t="s" s="4" r="D259">
-        <v>858</v>
+        <v>942</v>
       </c>
       <c t="s" s="4" r="E259">
-        <v>859</v>
+        <v>943</v>
       </c>
     </row>
     <row r="260">
+      <c s="36" r="A260"/>
       <c t="s" s="4" r="B260">
-        <v>938</v>
+        <v>944</v>
       </c>
       <c t="s" s="8" r="C260">
-        <v>939</v>
+        <v>945</v>
       </c>
       <c t="s" s="4" r="D260">
-        <v>940</v>
+        <v>946</v>
       </c>
       <c t="s" s="4" r="E260">
-        <v>941</v>
+        <v>947</v>
       </c>
     </row>
     <row r="261">
       <c s="36" r="A261"/>
-      <c t="s" s="4" r="B261">
-        <v>942</v>
-      </c>
-      <c t="s" s="8" r="C261">
-        <v>943</v>
-      </c>
-      <c t="s" s="4" r="D261">
-        <v>944</v>
-      </c>
-      <c t="s" s="4" r="E261">
-        <v>945</v>
-      </c>
+      <c s="7" r="B261"/>
+      <c s="9" r="C261"/>
+      <c s="11" r="D261"/>
+      <c s="11" r="E261"/>
     </row>
     <row r="262">
-      <c s="36" r="A262"/>
+      <c t="s" s="36" r="A262">
+        <v>948</v>
+      </c>
       <c t="s" s="4" r="B262">
-        <v>946</v>
+        <v>949</v>
       </c>
       <c t="s" s="8" r="C262">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c t="s" s="4" r="D262">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c t="s" s="4" r="E262">
-        <v>949</v>
+        <v>951</v>
       </c>
     </row>
     <row r="263">
       <c s="36" r="A263"/>
-      <c s="7" r="B263"/>
-      <c s="9" r="C263"/>
-      <c s="11" r="D263"/>
-      <c s="11" r="E263"/>
+      <c t="s" s="4" r="B263">
+        <v>952</v>
+      </c>
+      <c t="s" s="8" r="C263">
+        <v>953</v>
+      </c>
+      <c t="s" s="4" r="D263">
+        <v>954</v>
+      </c>
+      <c t="s" s="4" r="E263">
+        <v>955</v>
+      </c>
     </row>
     <row r="264">
-      <c t="s" s="36" r="A264">
-        <v>950</v>
-      </c>
+      <c s="36" r="A264"/>
       <c t="s" s="4" r="B264">
-        <v>951</v>
+        <v>956</v>
       </c>
       <c t="s" s="8" r="C264">
-        <v>950</v>
+        <v>957</v>
       </c>
       <c t="s" s="4" r="D264">
-        <v>952</v>
+        <v>958</v>
       </c>
       <c t="s" s="4" r="E264">
-        <v>953</v>
+        <v>959</v>
       </c>
     </row>
     <row r="265">
       <c s="36" r="A265"/>
       <c t="s" s="4" r="B265">
-        <v>954</v>
+        <v>960</v>
       </c>
       <c t="s" s="8" r="C265">
-        <v>955</v>
+        <v>961</v>
       </c>
       <c t="s" s="4" r="D265">
-        <v>956</v>
+        <v>962</v>
       </c>
       <c t="s" s="4" r="E265">
-        <v>957</v>
+        <v>963</v>
       </c>
     </row>
     <row r="266">
       <c s="36" r="A266"/>
       <c t="s" s="4" r="B266">
-        <v>958</v>
+        <v>964</v>
       </c>
       <c t="s" s="8" r="C266">
-        <v>959</v>
+        <v>965</v>
       </c>
       <c t="s" s="4" r="D266">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c t="s" s="4" r="E266">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="267">
       <c s="36" r="A267"/>
       <c t="s" s="4" r="B267">
-        <v>962</v>
+        <v>968</v>
       </c>
       <c t="s" s="8" r="C267">
-        <v>963</v>
+        <v>969</v>
       </c>
       <c t="s" s="4" r="D267">
-        <v>964</v>
+        <v>970</v>
       </c>
       <c t="s" s="4" r="E267">
-        <v>965</v>
+        <v>971</v>
       </c>
     </row>
     <row r="268">
       <c s="36" r="A268"/>
       <c t="s" s="4" r="B268">
-        <v>966</v>
+        <v>972</v>
       </c>
       <c t="s" s="8" r="C268">
-        <v>967</v>
+        <v>973</v>
       </c>
       <c t="s" s="4" r="D268">
-        <v>968</v>
+        <v>974</v>
       </c>
       <c t="s" s="4" r="E268">
-        <v>969</v>
+        <v>975</v>
       </c>
     </row>
     <row r="269">
       <c s="36" r="A269"/>
-      <c t="s" s="4" r="B269">
-        <v>970</v>
-      </c>
-      <c t="s" s="8" r="C269">
-        <v>971</v>
-      </c>
-      <c t="s" s="4" r="D269">
-        <v>972</v>
-      </c>
-      <c t="s" s="4" r="E269">
-        <v>973</v>
-      </c>
+      <c s="7" r="B269"/>
+      <c s="9" r="C269"/>
+      <c s="7" r="D269"/>
+      <c s="7" r="E269"/>
     </row>
     <row r="270">
-      <c s="36" r="A270"/>
+      <c t="s" s="36" r="A270">
+        <v>976</v>
+      </c>
       <c t="s" s="4" r="B270">
-        <v>974</v>
+        <v>977</v>
       </c>
       <c t="s" s="8" r="C270">
-        <v>975</v>
+        <v>978</v>
       </c>
       <c t="s" s="4" r="D270">
-        <v>976</v>
+        <v>979</v>
       </c>
       <c t="s" s="4" r="E270">
-        <v>977</v>
+        <v>980</v>
       </c>
     </row>
     <row r="271">
       <c s="36" r="A271"/>
-      <c s="7" r="B271"/>
-      <c s="9" r="C271"/>
-      <c s="7" r="D271"/>
-      <c s="7" r="E271"/>
+      <c t="s" s="4" r="B271">
+        <v>981</v>
+      </c>
+      <c t="s" s="8" r="C271">
+        <v>982</v>
+      </c>
+      <c t="s" s="4" r="D271">
+        <v>982</v>
+      </c>
+      <c t="s" s="4" r="E271">
+        <v>983</v>
+      </c>
     </row>
     <row r="272">
-      <c t="s" s="36" r="A272">
-        <v>978</v>
-      </c>
-      <c t="s" s="4" r="B272">
-        <v>979</v>
-      </c>
-      <c t="s" s="8" r="C272">
-        <v>980</v>
-      </c>
-      <c t="s" s="4" r="D272">
-        <v>981</v>
-      </c>
-      <c t="s" s="4" r="E272">
-        <v>982</v>
-      </c>
+      <c s="36" r="A272"/>
+      <c s="7" r="B272"/>
+      <c s="9" r="C272"/>
+      <c s="7" r="D272"/>
+      <c s="7" r="E272"/>
     </row>
     <row r="273">
-      <c s="36" r="A273"/>
+      <c t="s" s="36" r="A273">
+        <v>984</v>
+      </c>
       <c t="s" s="4" r="B273">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c t="s" s="8" r="C273">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c t="s" s="4" r="D273">
-        <v>984</v>
+        <v>987</v>
       </c>
       <c t="s" s="4" r="E273">
-        <v>985</v>
+        <v>988</v>
       </c>
     </row>
     <row r="274">
       <c s="36" r="A274"/>
-      <c s="7" r="B274"/>
-      <c s="9" r="C274"/>
-      <c s="7" r="D274"/>
-      <c s="7" r="E274"/>
+      <c t="s" s="4" r="B274">
+        <v>989</v>
+      </c>
+      <c t="s" s="8" r="C274">
+        <v>990</v>
+      </c>
+      <c t="s" s="4" r="D274">
+        <v>991</v>
+      </c>
+      <c t="s" s="4" r="E274">
+        <v>992</v>
+      </c>
     </row>
     <row r="275">
-      <c t="s" s="36" r="A275">
-        <v>986</v>
-      </c>
+      <c s="36" r="A275"/>
       <c t="s" s="4" r="B275">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c t="s" s="8" r="C275">
-        <v>988</v>
+        <v>994</v>
       </c>
       <c t="s" s="4" r="D275">
-        <v>989</v>
+        <v>995</v>
       </c>
       <c t="s" s="4" r="E275">
-        <v>990</v>
+        <v>996</v>
       </c>
     </row>
     <row r="276">
       <c s="36" r="A276"/>
       <c t="s" s="4" r="B276">
-        <v>991</v>
+        <v>997</v>
       </c>
       <c t="s" s="8" r="C276">
-        <v>992</v>
+        <v>998</v>
       </c>
       <c t="s" s="4" r="D276">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c t="s" s="4" r="E276">
-        <v>994</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="277">
       <c s="36" r="A277"/>
-      <c t="s" s="4" r="B277">
-        <v>995</v>
-      </c>
-      <c t="s" s="8" r="C277">
-        <v>996</v>
-      </c>
-      <c t="s" s="4" r="D277">
-        <v>997</v>
-      </c>
-      <c t="s" s="4" r="E277">
-        <v>998</v>
-      </c>
+      <c s="11" r="B277"/>
+      <c s="49" r="C277"/>
+      <c s="11" r="D277"/>
+      <c s="11" r="E277"/>
     </row>
     <row r="278">
-      <c s="36" r="A278"/>
+      <c t="s" s="36" r="A278">
+        <v>1001</v>
+      </c>
       <c t="s" s="4" r="B278">
-        <v>999</v>
+        <v>1002</v>
       </c>
       <c t="s" s="8" r="C278">
-        <v>1000</v>
+        <v>1003</v>
       </c>
       <c t="s" s="4" r="D278">
-        <v>1001</v>
+        <v>1004</v>
       </c>
       <c t="s" s="4" r="E278">
-        <v>1002</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="279">
       <c s="36" r="A279"/>
-      <c s="11" r="B279"/>
-      <c s="49" r="C279"/>
-      <c s="11" r="D279"/>
-      <c s="11" r="E279"/>
+      <c t="s" s="4" r="B279">
+        <v>1006</v>
+      </c>
+      <c t="s" s="8" r="C279">
+        <v>1007</v>
+      </c>
+      <c t="s" s="4" r="D279">
+        <v>1008</v>
+      </c>
+      <c t="s" s="4" r="E279">
+        <v>1009</v>
+      </c>
     </row>
     <row r="280">
-      <c t="s" s="36" r="A280">
-        <v>1003</v>
-      </c>
-      <c t="s" s="4" r="B280">
-        <v>1004</v>
-      </c>
-      <c t="s" s="8" r="C280">
-        <v>1005</v>
-      </c>
-      <c t="s" s="4" r="D280">
-        <v>1006</v>
-      </c>
-      <c t="s" s="4" r="E280">
-        <v>1007</v>
-      </c>
+      <c s="36" r="A280"/>
+      <c s="11" r="B280"/>
+      <c s="49" r="C280"/>
+      <c s="11" r="D280"/>
+      <c s="11" r="E280"/>
     </row>
     <row r="281">
-      <c s="36" r="A281"/>
+      <c t="s" s="36" r="A281">
+        <v>1010</v>
+      </c>
       <c t="s" s="4" r="B281">
-        <v>1008</v>
+        <v>1011</v>
       </c>
       <c t="s" s="8" r="C281">
-        <v>1009</v>
+        <v>1012</v>
       </c>
       <c t="s" s="4" r="D281">
-        <v>1010</v>
+        <v>1013</v>
       </c>
       <c t="s" s="4" r="E281">
-        <v>1011</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="282">
       <c s="36" r="A282"/>
       <c s="11" r="B282"/>
-      <c s="49" r="C282"/>
+      <c s="35" r="C282"/>
       <c s="11" r="D282"/>
       <c s="11" r="E282"/>
     </row>
     <row r="283">
       <c t="s" s="36" r="A283">
-        <v>1012</v>
+        <v>1015</v>
       </c>
       <c t="s" s="4" r="B283">
-        <v>1013</v>
-      </c>
-      <c t="s" s="8" r="C283">
-        <v>1014</v>
-      </c>
-      <c t="s" s="4" r="D283">
-        <v>1015</v>
-      </c>
-      <c t="s" s="4" r="E283">
         <v>1016</v>
+      </c>
+      <c t="s" s="28" r="C283">
+        <v>1017</v>
+      </c>
+      <c t="s" s="39" r="D283">
+        <v>1018</v>
+      </c>
+      <c t="s" s="39" r="E283">
+        <v>1019</v>
       </c>
     </row>
     <row r="284">
       <c s="36" r="A284"/>
-      <c s="11" r="B284"/>
-      <c s="35" r="C284"/>
-      <c s="11" r="D284"/>
-      <c s="11" r="E284"/>
+      <c t="s" s="4" r="B284">
+        <v>1020</v>
+      </c>
+      <c t="s" s="8" r="C284">
+        <v>1021</v>
+      </c>
+      <c t="s" s="4" r="D284">
+        <v>1022</v>
+      </c>
+      <c t="s" s="4" r="E284">
+        <v>1023</v>
+      </c>
     </row>
     <row r="285">
-      <c t="s" s="36" r="A285">
-        <v>1017</v>
-      </c>
+      <c s="36" r="A285"/>
       <c t="s" s="4" r="B285">
-        <v>1018</v>
-      </c>
-      <c t="s" s="28" r="C285">
-        <v>1019</v>
-      </c>
-      <c t="s" s="39" r="D285">
-        <v>1020</v>
-      </c>
-      <c t="s" s="39" r="E285">
-        <v>1021</v>
+        <v>1024</v>
+      </c>
+      <c t="s" s="8" r="C285">
+        <v>1025</v>
+      </c>
+      <c t="s" s="4" r="D285">
+        <v>1026</v>
+      </c>
+      <c t="s" s="4" r="E285">
+        <v>1027</v>
       </c>
     </row>
     <row r="286">
       <c s="36" r="A286"/>
       <c t="s" s="4" r="B286">
-        <v>1022</v>
+        <v>1028</v>
       </c>
       <c t="s" s="8" r="C286">
-        <v>1023</v>
+        <v>1029</v>
       </c>
       <c t="s" s="4" r="D286">
-        <v>1024</v>
+        <v>1030</v>
       </c>
       <c t="s" s="4" r="E286">
-        <v>1025</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="287">
       <c s="36" r="A287"/>
       <c t="s" s="4" r="B287">
-        <v>1026</v>
+        <v>1032</v>
       </c>
       <c t="s" s="8" r="C287">
-        <v>1027</v>
+        <v>1033</v>
       </c>
       <c t="s" s="4" r="D287">
-        <v>1028</v>
+        <v>1034</v>
       </c>
       <c t="s" s="4" r="E287">
-        <v>1029</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="288">
       <c s="36" r="A288"/>
       <c t="s" s="4" r="B288">
-        <v>1030</v>
+        <v>1036</v>
       </c>
       <c t="s" s="8" r="C288">
-        <v>1031</v>
+        <v>1037</v>
       </c>
       <c t="s" s="4" r="D288">
-        <v>1032</v>
+        <v>1038</v>
       </c>
       <c t="s" s="4" r="E288">
-        <v>1033</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="289">
       <c s="36" r="A289"/>
       <c t="s" s="4" r="B289">
-        <v>1034</v>
+        <v>1040</v>
       </c>
       <c t="s" s="8" r="C289">
-        <v>1035</v>
+        <v>1041</v>
       </c>
       <c t="s" s="4" r="D289">
-        <v>1036</v>
+        <v>1042</v>
       </c>
       <c t="s" s="4" r="E289">
-        <v>1037</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="290">
       <c s="36" r="A290"/>
       <c t="s" s="4" r="B290">
-        <v>1038</v>
+        <v>1044</v>
       </c>
       <c t="s" s="8" r="C290">
-        <v>1039</v>
+        <v>1045</v>
       </c>
       <c t="s" s="4" r="D290">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c t="s" s="4" r="E290">
-        <v>1041</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="291">
-      <c s="36" r="A291"/>
-      <c t="s" s="4" r="B291">
-        <v>1042</v>
-      </c>
-      <c t="s" s="8" r="C291">
-        <v>1043</v>
-      </c>
-      <c t="s" s="4" r="D291">
-        <v>1044</v>
-      </c>
-      <c t="s" s="4" r="E291">
-        <v>1045</v>
-      </c>
+      <c s="12" r="A291"/>
+      <c s="11" r="B291"/>
+      <c s="35" r="C291"/>
+      <c s="11" r="D291"/>
+      <c s="11" r="E291"/>
     </row>
     <row r="292">
-      <c s="36" r="A292"/>
+      <c t="s" s="36" r="A292">
+        <v>1048</v>
+      </c>
       <c t="s" s="4" r="B292">
-        <v>1046</v>
+        <v>1049</v>
       </c>
       <c t="s" s="8" r="C292">
-        <v>1047</v>
+        <v>1050</v>
       </c>
       <c t="s" s="4" r="D292">
-        <v>1048</v>
+        <v>1051</v>
       </c>
       <c t="s" s="4" r="E292">
-        <v>1049</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="293">
-      <c s="12" r="A293"/>
-      <c s="11" r="B293"/>
-      <c s="35" r="C293"/>
-      <c s="11" r="D293"/>
-      <c s="11" r="E293"/>
+      <c s="36" r="A293"/>
+      <c t="s" s="4" r="B293">
+        <v>1053</v>
+      </c>
+      <c t="s" s="8" r="C293">
+        <v>1054</v>
+      </c>
+      <c t="s" s="4" r="D293">
+        <v>1055</v>
+      </c>
+      <c t="s" s="4" r="E293">
+        <v>1056</v>
+      </c>
     </row>
     <row r="294">
-      <c t="s" s="36" r="A294">
-        <v>1050</v>
-      </c>
+      <c s="36" r="A294"/>
       <c t="s" s="4" r="B294">
-        <v>1051</v>
+        <v>1057</v>
       </c>
       <c t="s" s="8" r="C294">
-        <v>1052</v>
+        <v>1058</v>
       </c>
       <c t="s" s="4" r="D294">
-        <v>1053</v>
+        <v>1059</v>
       </c>
       <c t="s" s="4" r="E294">
-        <v>1054</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="295">
       <c s="36" r="A295"/>
       <c t="s" s="4" r="B295">
-        <v>1055</v>
+        <v>1061</v>
       </c>
       <c t="s" s="8" r="C295">
-        <v>1056</v>
+        <v>790</v>
       </c>
       <c t="s" s="4" r="D295">
-        <v>1057</v>
+        <v>1062</v>
       </c>
       <c t="s" s="4" r="E295">
-        <v>1058</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="296">
       <c s="36" r="A296"/>
       <c t="s" s="4" r="B296">
-        <v>1059</v>
+        <v>1064</v>
       </c>
       <c t="s" s="8" r="C296">
-        <v>1060</v>
+        <v>679</v>
       </c>
       <c t="s" s="4" r="D296">
-        <v>1061</v>
+        <v>131</v>
       </c>
       <c t="s" s="4" r="E296">
-        <v>1062</v>
+        <v>681</v>
       </c>
     </row>
     <row r="297">
       <c s="36" r="A297"/>
       <c t="s" s="4" r="B297">
-        <v>1063</v>
+        <v>1065</v>
       </c>
       <c t="s" s="8" r="C297">
-        <v>790</v>
+        <v>1066</v>
       </c>
       <c t="s" s="4" r="D297">
-        <v>1064</v>
+        <v>1067</v>
       </c>
       <c t="s" s="4" r="E297">
-        <v>1065</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="298">
-      <c s="36" r="A298"/>
-      <c t="s" s="4" r="B298">
-        <v>1066</v>
-      </c>
-      <c t="s" s="8" r="C298">
-        <v>679</v>
-      </c>
-      <c t="s" s="4" r="D298">
-        <v>131</v>
-      </c>
-      <c t="s" s="4" r="E298">
-        <v>681</v>
-      </c>
+      <c s="12" r="A298"/>
+      <c s="11" r="B298"/>
+      <c s="35" r="C298"/>
+      <c s="11" r="D298"/>
+      <c s="11" r="E298"/>
     </row>
     <row r="299">
-      <c s="36" r="A299"/>
+      <c t="s" s="36" r="A299">
+        <v>1069</v>
+      </c>
       <c t="s" s="4" r="B299">
-        <v>1067</v>
+        <v>1070</v>
       </c>
       <c t="s" s="8" r="C299">
-        <v>1068</v>
+        <v>1071</v>
       </c>
       <c t="s" s="4" r="D299">
-        <v>1069</v>
+        <v>1072</v>
       </c>
       <c t="s" s="4" r="E299">
-        <v>1070</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="300">
-      <c s="12" r="A300"/>
-      <c s="11" r="B300"/>
-      <c s="35" r="C300"/>
-      <c s="11" r="D300"/>
-      <c s="11" r="E300"/>
+      <c s="36" r="A300"/>
+      <c t="s" s="4" r="B300">
+        <v>1074</v>
+      </c>
+      <c t="s" s="8" r="C300">
+        <v>1075</v>
+      </c>
+      <c t="s" s="4" r="D300">
+        <v>1076</v>
+      </c>
+      <c t="s" s="4" r="E300">
+        <v>1077</v>
+      </c>
     </row>
     <row r="301">
-      <c t="s" s="36" r="A301">
-        <v>1071</v>
-      </c>
+      <c s="36" r="A301"/>
       <c t="s" s="4" r="B301">
-        <v>1072</v>
+        <v>1078</v>
       </c>
       <c t="s" s="8" r="C301">
-        <v>1073</v>
+        <v>1079</v>
       </c>
       <c t="s" s="4" r="D301">
-        <v>1074</v>
+        <v>1080</v>
       </c>
       <c t="s" s="4" r="E301">
-        <v>1075</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="302">
       <c s="36" r="A302"/>
       <c t="s" s="4" r="B302">
-        <v>1076</v>
+        <v>1082</v>
       </c>
       <c t="s" s="8" r="C302">
-        <v>1077</v>
+        <v>1083</v>
       </c>
       <c t="s" s="4" r="D302">
-        <v>1078</v>
+        <v>1084</v>
       </c>
       <c t="s" s="4" r="E302">
-        <v>1079</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="303">
       <c s="36" r="A303"/>
       <c t="s" s="4" r="B303">
-        <v>1080</v>
+        <v>1085</v>
       </c>
       <c t="s" s="8" r="C303">
-        <v>1081</v>
+        <v>1086</v>
       </c>
       <c t="s" s="4" r="D303">
-        <v>1082</v>
+        <v>1087</v>
       </c>
       <c t="s" s="4" r="E303">
-        <v>1083</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="304">
       <c s="36" r="A304"/>
       <c t="s" s="4" r="B304">
-        <v>1084</v>
+        <v>1089</v>
       </c>
       <c t="s" s="8" r="C304">
-        <v>1085</v>
+        <v>1090</v>
       </c>
       <c t="s" s="4" r="D304">
-        <v>1086</v>
+        <v>1091</v>
       </c>
       <c t="s" s="4" r="E304">
-        <v>1086</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="305">
       <c s="36" r="A305"/>
       <c t="s" s="4" r="B305">
-        <v>1087</v>
+        <v>1093</v>
       </c>
       <c t="s" s="8" r="C305">
-        <v>1088</v>
+        <v>1094</v>
       </c>
       <c t="s" s="4" r="D305">
-        <v>1089</v>
+        <v>1095</v>
       </c>
       <c t="s" s="4" r="E305">
-        <v>1090</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="306">
       <c s="36" r="A306"/>
       <c t="s" s="4" r="B306">
-        <v>1091</v>
+        <v>1097</v>
       </c>
       <c t="s" s="8" r="C306">
-        <v>1092</v>
+        <v>1098</v>
       </c>
       <c t="s" s="4" r="D306">
-        <v>1093</v>
+        <v>1099</v>
       </c>
       <c t="s" s="4" r="E306">
-        <v>1094</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="307">
       <c s="36" r="A307"/>
       <c t="s" s="4" r="B307">
-        <v>1095</v>
+        <v>1101</v>
       </c>
       <c t="s" s="8" r="C307">
-        <v>1096</v>
+        <v>1102</v>
       </c>
       <c t="s" s="4" r="D307">
-        <v>1097</v>
+        <v>1103</v>
       </c>
       <c t="s" s="4" r="E307">
-        <v>1098</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="308">
       <c s="36" r="A308"/>
       <c t="s" s="4" r="B308">
-        <v>1099</v>
+        <v>1105</v>
       </c>
       <c t="s" s="8" r="C308">
-        <v>1100</v>
+        <v>1106</v>
       </c>
       <c t="s" s="4" r="D308">
-        <v>1101</v>
+        <v>1107</v>
       </c>
       <c t="s" s="4" r="E308">
-        <v>1102</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="309">
       <c s="36" r="A309"/>
       <c t="s" s="4" r="B309">
-        <v>1103</v>
+        <v>1109</v>
       </c>
       <c t="s" s="8" r="C309">
-        <v>1104</v>
+        <v>1110</v>
       </c>
       <c t="s" s="4" r="D309">
-        <v>1105</v>
+        <v>1111</v>
       </c>
       <c t="s" s="4" r="E309">
-        <v>1106</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="310">
       <c s="36" r="A310"/>
       <c t="s" s="4" r="B310">
-        <v>1107</v>
+        <v>1113</v>
       </c>
       <c t="s" s="8" r="C310">
-        <v>1108</v>
+        <v>1114</v>
       </c>
       <c t="s" s="4" r="D310">
-        <v>1109</v>
+        <v>1115</v>
       </c>
       <c t="s" s="4" r="E310">
-        <v>1110</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="311">
       <c s="36" r="A311"/>
       <c t="s" s="4" r="B311">
-        <v>1111</v>
+        <v>1117</v>
       </c>
       <c t="s" s="8" r="C311">
-        <v>1112</v>
+        <v>1118</v>
       </c>
       <c t="s" s="4" r="D311">
-        <v>1113</v>
+        <v>1118</v>
       </c>
       <c t="s" s="4" r="E311">
-        <v>1114</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="312">
       <c s="36" r="A312"/>
       <c t="s" s="4" r="B312">
-        <v>1115</v>
+        <v>1119</v>
       </c>
       <c t="s" s="8" r="C312">
-        <v>1116</v>
+        <v>1120</v>
       </c>
       <c t="s" s="4" r="D312">
-        <v>1117</v>
+        <v>1121</v>
       </c>
       <c t="s" s="4" r="E312">
-        <v>1118</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="313">
       <c s="36" r="A313"/>
       <c t="s" s="4" r="B313">
-        <v>1119</v>
+        <v>1123</v>
       </c>
       <c t="s" s="8" r="C313">
-        <v>1120</v>
+        <v>1124</v>
       </c>
       <c t="s" s="4" r="D313">
-        <v>1120</v>
+        <v>1125</v>
       </c>
       <c t="s" s="4" r="E313">
-        <v>1120</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="314">
       <c s="36" r="A314"/>
       <c t="s" s="4" r="B314">
-        <v>1121</v>
+        <v>1127</v>
       </c>
       <c t="s" s="8" r="C314">
-        <v>1122</v>
+        <v>1128</v>
       </c>
       <c t="s" s="4" r="D314">
-        <v>1123</v>
+        <v>1129</v>
       </c>
       <c t="s" s="4" r="E314">
-        <v>1124</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="315">
       <c s="36" r="A315"/>
       <c t="s" s="4" r="B315">
-        <v>1125</v>
+        <v>1131</v>
       </c>
       <c t="s" s="8" r="C315">
-        <v>1126</v>
+        <v>1132</v>
       </c>
       <c t="s" s="4" r="D315">
-        <v>1127</v>
+        <v>1133</v>
       </c>
       <c t="s" s="4" r="E315">
-        <v>1128</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="316">
       <c s="36" r="A316"/>
       <c t="s" s="4" r="B316">
-        <v>1129</v>
+        <v>1135</v>
       </c>
       <c t="s" s="8" r="C316">
-        <v>1130</v>
+        <v>1136</v>
       </c>
       <c t="s" s="4" r="D316">
-        <v>1131</v>
+        <v>1137</v>
       </c>
       <c t="s" s="4" r="E316">
-        <v>1132</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="317">
       <c s="36" r="A317"/>
       <c t="s" s="4" r="B317">
-        <v>1133</v>
+        <v>1139</v>
       </c>
       <c t="s" s="8" r="C317">
-        <v>1134</v>
+        <v>1140</v>
       </c>
       <c t="s" s="4" r="D317">
-        <v>1135</v>
+        <v>1141</v>
       </c>
       <c t="s" s="4" r="E317">
-        <v>1136</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="318">
       <c s="36" r="A318"/>
       <c t="s" s="4" r="B318">
-        <v>1137</v>
+        <v>1143</v>
       </c>
       <c t="s" s="8" r="C318">
-        <v>1138</v>
+        <v>1144</v>
       </c>
       <c t="s" s="4" r="D318">
-        <v>1139</v>
+        <v>1145</v>
       </c>
       <c t="s" s="4" r="E318">
-        <v>1140</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="319">
       <c s="36" r="A319"/>
-      <c t="s" s="4" r="B319">
-        <v>1141</v>
-      </c>
-      <c t="s" s="8" r="C319">
-        <v>1142</v>
-      </c>
-      <c t="s" s="4" r="D319">
-        <v>1143</v>
-      </c>
-      <c t="s" s="4" r="E319">
-        <v>1144</v>
-      </c>
+      <c s="11" r="B319"/>
+      <c s="35" r="C319"/>
+      <c s="11" r="D319"/>
+      <c s="11" r="E319"/>
     </row>
     <row r="320">
-      <c s="36" r="A320"/>
+      <c t="s" s="36" r="A320">
+        <v>1147</v>
+      </c>
       <c t="s" s="4" r="B320">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c t="s" s="8" r="C320">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c t="s" s="4" r="D320">
-        <v>1147</v>
+        <v>1150</v>
       </c>
       <c t="s" s="4" r="E320">
-        <v>1148</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="321">
       <c s="36" r="A321"/>
-      <c s="11" r="B321"/>
-      <c s="35" r="C321"/>
-      <c s="11" r="D321"/>
-      <c s="11" r="E321"/>
+      <c t="s" s="4" r="B321">
+        <v>1152</v>
+      </c>
+      <c t="s" s="8" r="C321">
+        <v>1153</v>
+      </c>
+      <c t="s" s="4" r="D321">
+        <v>1154</v>
+      </c>
+      <c t="s" s="4" r="E321">
+        <v>1155</v>
+      </c>
     </row>
     <row r="322">
-      <c t="s" s="36" r="A322">
-        <v>1149</v>
-      </c>
+      <c s="36" r="A322"/>
       <c t="s" s="4" r="B322">
-        <v>1150</v>
+        <v>1156</v>
       </c>
       <c t="s" s="8" r="C322">
-        <v>1151</v>
+        <v>1157</v>
       </c>
       <c t="s" s="4" r="D322">
-        <v>1152</v>
+        <v>1158</v>
       </c>
       <c t="s" s="4" r="E322">
-        <v>1153</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="323">
       <c s="36" r="A323"/>
       <c t="s" s="4" r="B323">
-        <v>1154</v>
+        <v>1160</v>
       </c>
       <c t="s" s="8" r="C323">
-        <v>1155</v>
+        <v>1161</v>
       </c>
       <c t="s" s="4" r="D323">
-        <v>1156</v>
+        <v>1162</v>
       </c>
       <c t="s" s="4" r="E323">
-        <v>1157</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="324">
       <c s="36" r="A324"/>
       <c t="s" s="4" r="B324">
-        <v>1158</v>
+        <v>1164</v>
       </c>
       <c t="s" s="8" r="C324">
-        <v>1159</v>
-      </c>
-      <c t="s" s="4" r="D324">
-        <v>1160</v>
-      </c>
-      <c t="s" s="4" r="E324">
-        <v>1161</v>
+        <v>1164</v>
+      </c>
+      <c t="s" s="39" r="D324">
+        <v>1165</v>
+      </c>
+      <c t="s" s="39" r="E324">
+        <v>1166</v>
       </c>
     </row>
     <row r="325">
       <c s="36" r="A325"/>
       <c t="s" s="4" r="B325">
-        <v>1162</v>
+        <v>1167</v>
       </c>
       <c t="s" s="8" r="C325">
-        <v>1163</v>
+        <v>1168</v>
       </c>
       <c t="s" s="4" r="D325">
-        <v>1164</v>
+        <v>1169</v>
       </c>
       <c t="s" s="4" r="E325">
-        <v>1165</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="326">
       <c s="36" r="A326"/>
       <c t="s" s="4" r="B326">
-        <v>1166</v>
+        <v>1171</v>
       </c>
       <c t="s" s="8" r="C326">
-        <v>1166</v>
-      </c>
-      <c t="s" s="39" r="D326">
-        <v>1167</v>
-      </c>
-      <c t="s" s="39" r="E326">
-        <v>1168</v>
+        <v>1172</v>
+      </c>
+      <c t="s" s="4" r="D326">
+        <v>1173</v>
+      </c>
+      <c t="s" s="4" r="E326">
+        <v>1174</v>
       </c>
     </row>
     <row r="327">
-      <c s="36" r="A327"/>
-      <c t="s" s="4" r="B327">
-        <v>1169</v>
-      </c>
+      <c t="s" s="11" r="A327">
+        <v>1175</v>
+      </c>
+      <c s="45" r="B327"/>
       <c t="s" s="8" r="C327">
-        <v>1170</v>
-      </c>
-      <c t="s" s="4" r="D327">
-        <v>1171</v>
-      </c>
-      <c t="s" s="4" r="E327">
-        <v>1172</v>
+        <v>1176</v>
+      </c>
+      <c t="s" s="39" r="D327">
+        <v>1177</v>
+      </c>
+      <c t="s" s="39" r="E327">
+        <v>1178</v>
       </c>
     </row>
     <row r="328">
-      <c s="36" r="A328"/>
-      <c t="s" s="4" r="B328">
-        <v>1173</v>
-      </c>
-      <c t="s" s="8" r="C328">
-        <v>1174</v>
-      </c>
-      <c t="s" s="4" r="D328">
-        <v>1175</v>
-      </c>
-      <c t="s" s="4" r="E328">
-        <v>1176</v>
-      </c>
+      <c s="12" r="A328"/>
+      <c s="11" r="B328"/>
+      <c s="35" r="C328"/>
+      <c s="11" r="D328"/>
+      <c s="11" r="E328"/>
     </row>
     <row r="329">
-      <c t="s" s="11" r="A329">
-        <v>1177</v>
-      </c>
-      <c s="45" r="B329"/>
-      <c t="s" s="8" r="C329">
-        <v>1178</v>
+      <c t="s" s="12" r="A329">
+        <v>1179</v>
+      </c>
+      <c t="s" s="4" r="B329">
+        <v>1180</v>
+      </c>
+      <c t="s" s="44" r="C329">
+        <v>1181</v>
       </c>
       <c t="s" s="39" r="D329">
-        <v>1179</v>
+        <v>1182</v>
       </c>
       <c t="s" s="39" r="E329">
-        <v>1180</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="330">
-      <c s="12" r="A330"/>
-      <c s="11" r="B330"/>
-      <c s="35" r="C330"/>
-      <c s="11" r="D330"/>
-      <c s="11" r="E330"/>
+      <c s="9" r="A330"/>
+      <c t="s" s="4" r="B330">
+        <v>1184</v>
+      </c>
+      <c t="s" s="8" r="C330">
+        <v>1185</v>
+      </c>
+      <c t="s" s="4" r="D330">
+        <v>1186</v>
+      </c>
+      <c t="s" s="4" r="E330">
+        <v>1187</v>
+      </c>
     </row>
     <row r="331">
-      <c t="s" s="12" r="A331">
-        <v>1181</v>
-      </c>
+      <c s="49" r="A331"/>
       <c t="s" s="4" r="B331">
-        <v>1182</v>
-      </c>
-      <c t="s" s="44" r="C331">
-        <v>1183</v>
-      </c>
-      <c t="s" s="39" r="D331">
-        <v>1184</v>
-      </c>
-      <c t="s" s="39" r="E331">
-        <v>1185</v>
+        <v>1188</v>
+      </c>
+      <c t="s" s="4" r="C331">
+        <v>1189</v>
+      </c>
+      <c t="s" s="4" r="D331">
+        <v>1190</v>
+      </c>
+      <c t="s" s="4" r="E331">
+        <v>1191</v>
       </c>
     </row>
     <row r="332">
-      <c s="9" r="A332"/>
+      <c s="37" r="A332"/>
       <c t="s" s="4" r="B332">
-        <v>1186</v>
+        <v>1192</v>
       </c>
       <c t="s" s="8" r="C332">
-        <v>1187</v>
-      </c>
-      <c t="s" s="4" r="D332">
-        <v>1188</v>
-      </c>
-      <c t="s" s="4" r="E332">
-        <v>1189</v>
+        <v>1193</v>
+      </c>
+      <c t="s" s="39" r="D332">
+        <v>1194</v>
+      </c>
+      <c t="s" s="39" r="E332">
+        <v>1195</v>
       </c>
     </row>
     <row r="333">
-      <c s="49" r="A333"/>
+      <c s="12" r="A333"/>
       <c t="s" s="4" r="B333">
-        <v>1190</v>
-      </c>
-      <c t="s" s="4" r="C333">
-        <v>1191</v>
-      </c>
-      <c t="s" s="4" r="D333">
-        <v>1192</v>
+        <v>1196</v>
+      </c>
+      <c t="s" s="44" r="C333">
+        <v>1197</v>
+      </c>
+      <c t="s" s="44" r="D333">
+        <v>1198</v>
       </c>
       <c t="s" s="4" r="E333">
-        <v>1193</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="334">
-      <c s="37" r="A334"/>
+      <c s="12" r="A334"/>
       <c t="s" s="4" r="B334">
-        <v>1194</v>
+        <v>1200</v>
       </c>
       <c t="s" s="8" r="C334">
-        <v>1195</v>
-      </c>
-      <c t="s" s="39" r="D334">
-        <v>1196</v>
-      </c>
-      <c t="s" s="39" r="E334">
-        <v>1197</v>
+        <v>1201</v>
+      </c>
+      <c t="s" s="8" r="D334">
+        <v>1202</v>
+      </c>
+      <c t="s" s="4" r="E334">
+        <v>1203</v>
       </c>
     </row>
     <row r="335">
       <c s="12" r="A335"/>
       <c t="s" s="4" r="B335">
-        <v>1198</v>
-      </c>
-      <c t="s" s="44" r="C335">
-        <v>1199</v>
-      </c>
-      <c t="s" s="44" r="D335">
-        <v>1200</v>
+        <v>1204</v>
+      </c>
+      <c t="s" s="4" r="C335">
+        <v>1205</v>
+      </c>
+      <c t="s" s="4" r="D335">
+        <v>1206</v>
       </c>
       <c t="s" s="4" r="E335">
-        <v>1201</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="336">
       <c s="12" r="A336"/>
       <c t="s" s="4" r="B336">
-        <v>1202</v>
+        <v>1208</v>
       </c>
       <c t="s" s="8" r="C336">
-        <v>1203</v>
-      </c>
-      <c t="s" s="8" r="D336">
-        <v>1204</v>
+        <v>1209</v>
+      </c>
+      <c t="s" s="4" r="D336">
+        <v>1210</v>
       </c>
       <c t="s" s="4" r="E336">
-        <v>1205</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="337">
       <c s="12" r="A337"/>
       <c t="s" s="4" r="B337">
-        <v>1206</v>
+        <v>1212</v>
       </c>
       <c t="s" s="4" r="C337">
-        <v>1207</v>
+        <v>1213</v>
       </c>
       <c t="s" s="4" r="D337">
-        <v>1208</v>
+        <v>1214</v>
       </c>
       <c t="s" s="4" r="E337">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="338">
+      <c s="37" r="A338"/>
+      <c t="s" s="4" r="B338">
+        <v>1216</v>
+      </c>
+      <c t="s" s="8" r="C338">
         <v>1209</v>
       </c>
-    </row>
-    <row r="338">
-      <c s="12" r="A338"/>
-      <c t="s" s="4" r="B338">
+      <c t="s" s="4" r="D338">
         <v>1210</v>
       </c>
-      <c t="s" s="8" r="C338">
+      <c t="s" s="4" r="E338">
         <v>1211</v>
-      </c>
-      <c t="s" s="4" r="D338">
-        <v>1212</v>
-      </c>
-      <c t="s" s="4" r="E338">
-        <v>1213</v>
       </c>
     </row>
     <row r="339">
       <c s="12" r="A339"/>
       <c t="s" s="4" r="B339">
-        <v>1214</v>
+        <v>1217</v>
       </c>
       <c t="s" s="4" r="C339">
-        <v>1215</v>
+        <v>1218</v>
       </c>
       <c t="s" s="4" r="D339">
-        <v>1216</v>
+        <v>1219</v>
       </c>
       <c t="s" s="4" r="E339">
-        <v>1217</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="340">
-      <c s="37" r="A340"/>
+      <c s="12" r="A340"/>
       <c t="s" s="4" r="B340">
-        <v>1218</v>
+        <v>1221</v>
       </c>
       <c t="s" s="8" r="C340">
+        <v>1209</v>
+      </c>
+      <c t="s" s="4" r="D340">
+        <v>1210</v>
+      </c>
+      <c t="s" s="4" r="E340">
         <v>1211</v>
-      </c>
-      <c t="s" s="4" r="D340">
-        <v>1212</v>
-      </c>
-      <c t="s" s="4" r="E340">
-        <v>1213</v>
       </c>
     </row>
     <row r="341">
       <c s="12" r="A341"/>
       <c t="s" s="4" r="B341">
-        <v>1219</v>
-      </c>
-      <c t="s" s="4" r="C341">
-        <v>1220</v>
+        <v>1222</v>
+      </c>
+      <c t="s" s="8" r="C341">
+        <v>1223</v>
       </c>
       <c t="s" s="4" r="D341">
-        <v>1221</v>
+        <v>1224</v>
       </c>
       <c t="s" s="4" r="E341">
-        <v>1222</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="342">
       <c s="12" r="A342"/>
       <c t="s" s="4" r="B342">
-        <v>1223</v>
+        <v>1226</v>
       </c>
       <c t="s" s="8" r="C342">
-        <v>1211</v>
+        <v>1227</v>
       </c>
       <c t="s" s="4" r="D342">
-        <v>1212</v>
+        <v>1228</v>
       </c>
       <c t="s" s="4" r="E342">
-        <v>1213</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="343">
-      <c s="12" r="A343"/>
+      <c s="36" r="A343"/>
       <c t="s" s="4" r="B343">
-        <v>1224</v>
-      </c>
-      <c t="s" s="8" r="C343">
-        <v>1225</v>
-      </c>
-      <c t="s" s="4" r="D343">
-        <v>1226</v>
-      </c>
-      <c t="s" s="4" r="E343">
-        <v>1227</v>
-      </c>
+        <v>1230</v>
+      </c>
+      <c t="s" s="44" r="C343">
+        <v>1197</v>
+      </c>
+      <c s="15" r="D343"/>
+      <c s="15" r="E343"/>
     </row>
     <row r="344">
-      <c s="12" r="A344"/>
+      <c s="36" r="A344"/>
       <c t="s" s="4" r="B344">
-        <v>1228</v>
+        <v>1231</v>
       </c>
       <c t="s" s="8" r="C344">
-        <v>1229</v>
-      </c>
-      <c t="s" s="4" r="D344">
-        <v>1230</v>
-      </c>
-      <c t="s" s="4" r="E344">
-        <v>1231</v>
-      </c>
+        <v>1201</v>
+      </c>
+      <c s="15" r="D344"/>
+      <c s="15" r="E344"/>
     </row>
     <row r="345">
       <c s="36" r="A345"/>
       <c t="s" s="4" r="B345">
         <v>1232</v>
       </c>
-      <c t="s" s="44" r="C345">
-        <v>1199</v>
-      </c>
-      <c s="15" r="D345"/>
-      <c s="15" r="E345"/>
+      <c t="s" s="8" r="C345">
+        <v>1233</v>
+      </c>
+      <c s="7" r="D345"/>
+      <c s="7" r="E345"/>
     </row>
     <row r="346">
       <c s="36" r="A346"/>
       <c t="s" s="4" r="B346">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c t="s" s="8" r="C346">
-        <v>1203</v>
-      </c>
-      <c s="15" r="D346"/>
-      <c s="15" r="E346"/>
+        <v>1235</v>
+      </c>
+      <c s="7" r="D346"/>
+      <c s="7" r="E346"/>
     </row>
     <row r="347">
       <c s="36" r="A347"/>
       <c t="s" s="4" r="B347">
-        <v>1234</v>
+        <v>1236</v>
       </c>
       <c t="s" s="8" r="C347">
-        <v>1235</v>
-      </c>
-      <c s="7" r="D347"/>
-      <c s="7" r="E347"/>
+        <v>1237</v>
+      </c>
+      <c t="s" s="4" r="D347">
+        <v>1238</v>
+      </c>
+      <c t="s" s="4" r="E347">
+        <v>1239</v>
+      </c>
     </row>
     <row r="348">
-      <c s="36" r="A348"/>
-      <c t="s" s="4" r="B348">
-        <v>1236</v>
-      </c>
-      <c t="s" s="8" r="C348">
-        <v>1237</v>
-      </c>
+      <c s="9" r="B348"/>
+      <c s="9" r="C348"/>
       <c s="7" r="D348"/>
       <c s="7" r="E348"/>
     </row>
     <row r="349">
-      <c s="36" r="A349"/>
-      <c t="s" s="4" r="B349">
-        <v>1238</v>
+      <c t="s" s="36" r="A349">
+        <v>1240</v>
+      </c>
+      <c t="s" s="8" r="B349">
+        <v>1241</v>
       </c>
       <c t="s" s="8" r="C349">
-        <v>1239</v>
-      </c>
-      <c t="s" s="4" r="D349">
-        <v>1240</v>
-      </c>
-      <c t="s" s="4" r="E349">
-        <v>1241</v>
+        <v>1242</v>
+      </c>
+      <c t="s" s="39" r="D349">
+        <v>1243</v>
+      </c>
+      <c t="s" s="39" r="E349">
+        <v>1244</v>
       </c>
     </row>
     <row r="350">
-      <c s="9" r="B350"/>
-      <c s="9" r="C350"/>
-      <c s="7" r="D350"/>
-      <c s="7" r="E350"/>
+      <c s="36" r="A350"/>
+      <c t="s" s="8" r="B350">
+        <v>1245</v>
+      </c>
+      <c t="s" s="8" r="C350">
+        <v>1246</v>
+      </c>
+      <c t="s" s="39" r="D350">
+        <v>1247</v>
+      </c>
+      <c t="s" s="4" r="E350">
+        <v>1248</v>
+      </c>
     </row>
     <row r="351">
-      <c t="s" s="36" r="A351">
-        <v>1242</v>
-      </c>
-      <c t="s" s="8" r="B351">
-        <v>1243</v>
-      </c>
-      <c t="s" s="8" r="C351">
-        <v>1244</v>
-      </c>
-      <c t="s" s="39" r="D351">
-        <v>1245</v>
-      </c>
-      <c t="s" s="39" r="E351">
-        <v>1246</v>
-      </c>
+      <c s="36" r="A351"/>
+      <c s="35" r="C351"/>
+      <c s="11" r="D351"/>
+      <c s="11" r="E351"/>
     </row>
     <row r="352">
-      <c s="36" r="A352"/>
-      <c t="s" s="8" r="B352">
-        <v>1247</v>
+      <c t="s" s="36" r="A352">
+        <v>1249</v>
+      </c>
+      <c t="s" s="45" r="B352">
+        <v>1250</v>
       </c>
       <c t="s" s="8" r="C352">
-        <v>1248</v>
-      </c>
-      <c t="s" s="39" r="D352">
-        <v>1249</v>
+        <v>1251</v>
+      </c>
+      <c t="s" s="4" r="D352">
+        <v>1252</v>
       </c>
       <c t="s" s="4" r="E352">
-        <v>1250</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="353">
       <c s="36" r="A353"/>
-      <c s="35" r="C353"/>
-      <c s="11" r="D353"/>
-      <c s="11" r="E353"/>
+      <c t="s" s="45" r="B353">
+        <v>1254</v>
+      </c>
+      <c t="s" s="8" r="C353">
+        <v>1255</v>
+      </c>
+      <c t="s" s="4" r="D353">
+        <v>1256</v>
+      </c>
+      <c t="s" s="4" r="E353">
+        <v>1257</v>
+      </c>
     </row>
     <row r="354">
-      <c t="s" s="36" r="A354">
-        <v>1251</v>
-      </c>
-      <c t="s" s="45" r="B354">
-        <v>1252</v>
-      </c>
-      <c t="s" s="8" r="C354">
-        <v>1253</v>
-      </c>
-      <c t="s" s="4" r="D354">
-        <v>1254</v>
-      </c>
-      <c t="s" s="4" r="E354">
-        <v>1255</v>
-      </c>
+      <c s="36" r="A354"/>
+      <c s="35" r="C354"/>
+      <c s="11" r="D354"/>
+      <c s="11" r="E354"/>
     </row>
     <row r="355">
-      <c s="36" r="A355"/>
+      <c t="s" r="A355">
+        <v>1258</v>
+      </c>
       <c t="s" s="45" r="B355">
-        <v>1256</v>
-      </c>
-      <c t="s" s="8" r="C355">
-        <v>1257</v>
-      </c>
-      <c t="s" s="4" r="D355">
+        <v>1259</v>
+      </c>
+      <c t="s" s="45" r="C355">
         <v>1258</v>
       </c>
-      <c t="s" s="4" r="E355">
-        <v>1259</v>
-      </c>
+      <c s="45" r="D355"/>
+      <c s="45" r="E355"/>
     </row>
     <row r="356">
-      <c s="36" r="A356"/>
-      <c s="35" r="C356"/>
-      <c s="11" r="D356"/>
-      <c s="11" r="E356"/>
+      <c t="s" s="45" r="B356">
+        <v>1260</v>
+      </c>
+      <c t="s" s="45" r="C356">
+        <v>1261</v>
+      </c>
+      <c s="45" r="D356"/>
+      <c s="45" r="E356"/>
     </row>
     <row r="357">
-      <c t="s" r="A357">
-        <v>1260</v>
-      </c>
       <c t="s" s="45" r="B357">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c t="s" s="45" r="C357">
-        <v>1260</v>
+        <v>1263</v>
       </c>
       <c s="45" r="D357"/>
       <c s="45" r="E357"/>
     </row>
     <row r="358">
       <c t="s" s="45" r="B358">
-        <v>1262</v>
+        <v>1264</v>
       </c>
       <c t="s" s="45" r="C358">
-        <v>1263</v>
+        <v>1265</v>
       </c>
       <c s="45" r="D358"/>
       <c s="45" r="E358"/>
     </row>
     <row r="359">
       <c t="s" s="45" r="B359">
-        <v>1264</v>
+        <v>1266</v>
       </c>
       <c t="s" s="45" r="C359">
-        <v>1265</v>
+        <v>1267</v>
       </c>
       <c s="45" r="D359"/>
       <c s="45" r="E359"/>
     </row>
     <row r="360">
       <c t="s" s="45" r="B360">
-        <v>1266</v>
+        <v>1268</v>
       </c>
       <c t="s" s="45" r="C360">
-        <v>1267</v>
+        <v>707</v>
       </c>
       <c s="45" r="D360"/>
       <c s="45" r="E360"/>
     </row>
     <row r="361">
       <c t="s" s="45" r="B361">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c t="s" s="45" r="C361">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c s="45" r="D361"/>
       <c s="45" r="E361"/>
     </row>
     <row r="362">
       <c t="s" s="45" r="B362">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c t="s" s="45" r="C362">
-        <v>707</v>
+        <v>216</v>
       </c>
       <c s="45" r="D362"/>
       <c s="45" r="E362"/>
     </row>
     <row r="363">
       <c t="s" s="45" r="B363">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c t="s" s="45" r="C363">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c s="45" r="D363"/>
       <c s="45" r="E363"/>
     </row>
     <row r="364">
       <c t="s" s="45" r="B364">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c t="s" s="45" r="C364">
-        <v>216</v>
+        <v>1275</v>
       </c>
       <c s="45" r="D364"/>
       <c s="45" r="E364"/>
     </row>
     <row r="365">
       <c t="s" s="45" r="B365">
-        <v>1274</v>
-      </c>
-      <c t="s" s="45" r="C365">
-        <v>1275</v>
-      </c>
-      <c s="45" r="D365"/>
-      <c s="45" r="E365"/>
+        <v>1276</v>
+      </c>
+      <c t="s" s="4" r="C365">
+        <v>1277</v>
+      </c>
+      <c t="s" s="45" r="D365">
+        <v>1277</v>
+      </c>
+      <c t="s" s="45" r="E365">
+        <v>1277</v>
+      </c>
     </row>
     <row r="366">
-      <c t="s" s="45" r="B366">
-        <v>1276</v>
-      </c>
-      <c t="s" s="45" r="C366">
-        <v>1277</v>
-      </c>
-      <c s="45" r="D366"/>
-      <c s="45" r="E366"/>
-    </row>
-    <row r="367">
-      <c t="s" s="45" r="B367">
+      <c t="s" r="B366">
         <v>1278</v>
       </c>
-      <c t="s" s="4" r="C367">
+      <c t="s" r="C366">
         <v>1279</v>
       </c>
-      <c t="s" s="45" r="D367">
-        <v>1279</v>
-      </c>
-      <c t="s" s="45" r="E367">
-        <v>1279</v>
-      </c>
     </row>
     <row r="368">
-      <c t="s" r="B368">
+      <c t="s" r="A368">
         <v>1280</v>
       </c>
-      <c t="s" r="C368">
+      <c t="s" s="45" r="B368">
         <v>1281</v>
       </c>
+      <c t="s" s="45" r="C368">
+        <v>1280</v>
+      </c>
+      <c t="s" s="45" r="D368">
+        <v>1280</v>
+      </c>
+      <c t="s" s="45" r="E368">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="369">
+      <c s="15" r="A369"/>
+      <c t="s" s="4" r="B369">
+        <v>1282</v>
+      </c>
+      <c t="s" s="4" r="C369">
+        <v>1283</v>
+      </c>
+      <c t="s" s="4" r="D369">
+        <v>1284</v>
+      </c>
+      <c t="s" s="4" r="E369">
+        <v>1285</v>
+      </c>
     </row>
     <row r="370">
-      <c t="s" r="A370">
-        <v>1282</v>
-      </c>
-      <c t="s" s="45" r="B370">
-        <v>1283</v>
-      </c>
-      <c t="s" s="45" r="C370">
-        <v>1282</v>
-      </c>
-      <c t="s" s="45" r="D370">
-        <v>1282</v>
-      </c>
-      <c t="s" s="45" r="E370">
-        <v>1282</v>
+      <c s="15" r="A370"/>
+      <c t="s" s="4" r="B370">
+        <v>1286</v>
+      </c>
+      <c t="s" s="4" r="C370">
+        <v>1287</v>
+      </c>
+      <c t="s" s="39" r="D370">
+        <v>1288</v>
+      </c>
+      <c t="s" s="39" r="E370">
+        <v>1289</v>
       </c>
     </row>
     <row r="371">
       <c s="15" r="A371"/>
       <c t="s" s="4" r="B371">
-        <v>1284</v>
+        <v>1290</v>
       </c>
       <c t="s" s="4" r="C371">
-        <v>1285</v>
-      </c>
-      <c t="s" s="4" r="D371">
-        <v>1286</v>
-      </c>
-      <c t="s" s="4" r="E371">
-        <v>1287</v>
+        <v>1291</v>
+      </c>
+      <c t="s" s="39" r="D371">
+        <v>1292</v>
+      </c>
+      <c t="s" s="39" r="E371">
+        <v>1293</v>
       </c>
     </row>
     <row r="372">
       <c s="15" r="A372"/>
       <c t="s" s="4" r="B372">
-        <v>1288</v>
+        <v>1294</v>
       </c>
       <c t="s" s="4" r="C372">
-        <v>1289</v>
+        <v>1295</v>
       </c>
       <c t="s" s="39" r="D372">
-        <v>1290</v>
+        <v>1296</v>
       </c>
       <c t="s" s="39" r="E372">
-        <v>1291</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="373">
       <c s="15" r="A373"/>
       <c t="s" s="4" r="B373">
-        <v>1292</v>
+        <v>1298</v>
       </c>
       <c t="s" s="4" r="C373">
-        <v>1293</v>
+        <v>1299</v>
       </c>
       <c t="s" s="39" r="D373">
-        <v>1294</v>
+        <v>1300</v>
       </c>
       <c t="s" s="39" r="E373">
-        <v>1295</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="374">
       <c s="15" r="A374"/>
       <c t="s" s="4" r="B374">
-        <v>1296</v>
+        <v>1302</v>
       </c>
       <c t="s" s="4" r="C374">
-        <v>1297</v>
+        <v>1303</v>
       </c>
       <c t="s" s="39" r="D374">
-        <v>1298</v>
+        <v>1303</v>
       </c>
       <c t="s" s="39" r="E374">
-        <v>1299</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="375">
       <c s="15" r="A375"/>
-      <c t="s" s="4" r="B375">
-        <v>1300</v>
-      </c>
-      <c t="s" s="4" r="C375">
-        <v>1301</v>
-      </c>
-      <c t="s" s="39" r="D375">
-        <v>1302</v>
-      </c>
-      <c t="s" s="39" r="E375">
-        <v>1303</v>
-      </c>
-    </row>
-    <row r="376">
-      <c s="15" r="A376"/>
-      <c t="s" s="4" r="B376">
+      <c t="s" r="B375">
         <v>1304</v>
       </c>
-      <c t="s" s="4" r="C376">
+      <c t="s" r="C375">
         <v>1305</v>
       </c>
-      <c t="s" s="39" r="D376">
+      <c t="s" r="D375">
         <v>1305</v>
       </c>
-      <c t="s" s="39" r="E376">
+      <c t="s" r="E375">
         <v>1305</v>
       </c>
     </row>
     <row r="377">
-      <c s="15" r="A377"/>
+      <c t="s" r="A377">
+        <v>1306</v>
+      </c>
       <c t="s" r="B377">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c t="s" r="C377">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c t="s" r="D377">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c t="s" r="E377">
-        <v>1307</v>
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="378">
+      <c t="s" r="B378">
+        <v>1309</v>
+      </c>
+      <c t="s" r="C378">
+        <v>158</v>
+      </c>
+      <c t="s" r="D378">
+        <v>158</v>
+      </c>
+      <c t="s" r="E378">
+        <v>158</v>
       </c>
     </row>
     <row r="379">
-      <c t="s" r="A379">
-        <v>1308</v>
-      </c>
       <c t="s" r="B379">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c t="s" r="C379">
-        <v>1310</v>
+        <v>130</v>
       </c>
       <c t="s" r="D379">
-        <v>1310</v>
+        <v>130</v>
       </c>
       <c t="s" r="E379">
-        <v>1310</v>
+        <v>130</v>
       </c>
     </row>
     <row r="380">
@@ -10144,13 +10146,13 @@
         <v>1311</v>
       </c>
       <c t="s" r="C380">
-        <v>158</v>
+        <v>393</v>
       </c>
       <c t="s" r="D380">
-        <v>158</v>
+        <v>393</v>
       </c>
       <c t="s" r="E380">
-        <v>158</v>
+        <v>393</v>
       </c>
     </row>
     <row r="381">
@@ -10158,46 +10160,18 @@
         <v>1312</v>
       </c>
       <c t="s" r="C381">
-        <v>130</v>
+        <v>1313</v>
       </c>
       <c t="s" r="D381">
-        <v>130</v>
+        <v>1313</v>
       </c>
       <c t="s" r="E381">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="382">
-      <c t="s" r="B382">
         <v>1313</v>
       </c>
-      <c t="s" r="C382">
-        <v>393</v>
-      </c>
-      <c t="s" r="D382">
-        <v>393</v>
-      </c>
-      <c t="s" r="E382">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="383">
-      <c t="s" r="B383">
-        <v>1314</v>
-      </c>
-      <c t="s" r="C383">
-        <v>1315</v>
-      </c>
-      <c t="s" r="D383">
-        <v>1315</v>
-      </c>
-      <c t="s" r="E383">
-        <v>1315</v>
-      </c>
-    </row>
-    <row r="387">
-      <c s="48" r="D387"/>
-      <c s="48" r="E387"/>
+    </row>
+    <row r="385">
+      <c s="48" r="D385"/>
+      <c s="48" r="E385"/>
     </row>
   </sheetData>
 </worksheet>
@@ -10215,17 +10189,17 @@
   <sheetData>
     <row customHeight="1" r="1" ht="112.5">
       <c t="s" s="3" r="A1">
-        <v>1316</v>
+        <v>1314</v>
       </c>
     </row>
     <row customHeight="1" r="2" ht="112.5">
       <c t="s" s="32" r="A2">
-        <v>1317</v>
+        <v>1315</v>
       </c>
     </row>
     <row customHeight="1" r="3" ht="112.5">
       <c t="s" s="6" r="A3">
-        <v>1318</v>
+        <v>1316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EWD-23377 - Remove "Welcome" page
Former-commit-id: a94e266720bde2698bfc8f832587e121a33f9900
</commit_message>
<xml_diff>
--- a/sources/easygenerator.Web/App/localization/resources.xlsx
+++ b/sources/easygenerator.Web/App/localization/resources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="1315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="1218">
   <si>
     <t>Key</t>
   </si>
@@ -2153,301 +2153,6 @@
     <t>Einstellungen der Kursvorlage:</t>
   </si>
   <si>
-    <t>Introduction page</t>
-  </si>
-  <si>
-    <t>introWelcomePageTitle</t>
-  </si>
-  <si>
-    <t>Welcome page</t>
-  </si>
-  <si>
-    <t>Welkompagina</t>
-  </si>
-  <si>
-    <t>Willkommensseite</t>
-  </si>
-  <si>
-    <t>introWelcome</t>
-  </si>
-  <si>
-    <t>Welcome to easygenerator web-edition!</t>
-  </si>
-  <si>
-    <t>Welkom bij de webversie van easygenerator!</t>
-  </si>
-  <si>
-    <t>Willkommen zur Webversion von easygenerator!</t>
-  </si>
-  <si>
-    <t>introBeforeStartOne</t>
-  </si>
-  <si>
-    <t>Before you start please take a moment to read about our concept. </t>
-  </si>
-  <si>
-    <t>Neem voordat u begint even de tijd om ons concept door te lezen.</t>
-  </si>
-  <si>
-    <t>Nehmen Sie sich vor dem Beginn etwas Zeit, um unser Konzept zu lesen.</t>
-  </si>
-  <si>
-    <t>introBeforeStartTwo</t>
-  </si>
-  <si>
-    <t>When you understand the big picture you can work a lot more effective with easygenerator.</t>
-  </si>
-  <si>
-    <t>Als u de achterliggende gedachte begrijpt, kunt u easygenerator een stuk effectiever gebruiken.</t>
-  </si>
-  <si>
-    <t>Wenn Sie das Gesamtbild verstanden haben, können Sie viel effektiver mit easygenerator arbeiten.</t>
-  </si>
-  <si>
-    <t>introStartButton</t>
-  </si>
-  <si>
-    <t>Start easygenerator</t>
-  </si>
-  <si>
-    <t>Easygenerator starten</t>
-  </si>
-  <si>
-    <t>introDoNotShowAgain</t>
-  </si>
-  <si>
-    <t>Do not show this starting page again</t>
-  </si>
-  <si>
-    <t>Laat deze startpagina niet meer zien</t>
-  </si>
-  <si>
-    <t>Diese Startseite nicht mehr anzeigen</t>
-  </si>
-  <si>
-    <t>introDidacticalConcept</t>
-  </si>
-  <si>
-    <t>Didactical concept</t>
-  </si>
-  <si>
-    <t>Didactisch concept</t>
-  </si>
-  <si>
-    <t>Didaktisches Konzept</t>
-  </si>
-  <si>
-    <t>introDidacticalConceptDesc</t>
-  </si>
-  <si>
-    <t>We provide better e-learning based on:</t>
-  </si>
-  <si>
-    <t>Wij leveren betere e-learning omdat:</t>
-  </si>
-  <si>
-    <t>Wir bieten besseres e-Learning, weil:</t>
-  </si>
-  <si>
-    <t>introElearningPrincipleOne</t>
-  </si>
-  <si>
-    <t>All learning processes start with the definition of &lt;strong&gt;learning objectives&lt;/strong&gt;. </t>
-  </si>
-  <si>
-    <t>Alle leerprocessen beginnen met de definitie van de &lt;strong&gt;leerdoelen&lt;/strong&gt;.</t>
-  </si>
-  <si>
-    <t>Alle Lernprozesse mit der Definition von &lt;strong&gt;Lernzielen&lt;/strong&gt; beginnen.</t>
-  </si>
-  <si>
-    <t>introElearningPrincipleTwo</t>
-  </si>
-  <si>
-    <t>Progress is measured by &lt;strong&gt;answering questions&lt;/strong&gt; not by reading pages.</t>
-  </si>
-  <si>
-    <t>De vooruitgang wordt gemeten aan de hand van het &lt;strong&gt;beantwoorden van vragen&lt;/strong&gt; in plaats van door het lezen van pagina's.</t>
-  </si>
-  <si>
-    <t>Der Fortschritt durch &lt;strong&gt;die Beantwortung von Fragen&lt;/strong&gt; (und nicht durch das Lesen von Seiten) gemessen wird.</t>
-  </si>
-  <si>
-    <t>introStartProcessWith</t>
-  </si>
-  <si>
-    <t>Start your authoring process with:</t>
-  </si>
-  <si>
-    <t>Begin uw authoringproces met:</t>
-  </si>
-  <si>
-    <t>Starten Sie den Authoringprozess mit:</t>
-  </si>
-  <si>
-    <t>introDefineLO</t>
-  </si>
-  <si>
-    <t>Definiëren van leerdoelen</t>
-  </si>
-  <si>
-    <t>Definieren von Lernzielen,
-</t>
-  </si>
-  <si>
-    <t>introDefineLODesc</t>
-  </si>
-  <si>
-    <t>That describes specific skills or knowledge that learner need to acquire.</t>
-  </si>
-  <si>
-    <t>die specifieke vaardigheden of kennis beschrijven die de cursist zich eigen moet maken.</t>
-  </si>
-  <si>
-    <t>die spezifischen Fähigkeiten oder Kenntnisse beschreiben, die der Kursteilnehmer sich aneignen muss.</t>
-  </si>
-  <si>
-    <t>introCreateQuestions</t>
-  </si>
-  <si>
-    <t>Create questions</t>
-  </si>
-  <si>
-    <t>Vragen maken</t>
-  </si>
-  <si>
-    <t>Erstellen von Fragen,</t>
-  </si>
-  <si>
-    <t>introCreateQuestionsDesc</t>
-  </si>
-  <si>
-    <t>That will assess if the learner has mastered the learning objectives.</t>
-  </si>
-  <si>
-    <t>die beoordelen of de cursist de leerdoelen heeft bereikt.</t>
-  </si>
-  <si>
-    <t>die  prüfen, ob der Lernende die Lernziele erreicht hat.</t>
-  </si>
-  <si>
-    <t>introAddLContent</t>
-  </si>
-  <si>
-    <t>Add learning content</t>
-  </si>
-  <si>
-    <t>Leerinhoud toevoegen</t>
-  </si>
-  <si>
-    <t>Hinzufügen von Lerninhalten</t>
-  </si>
-  <si>
-    <t>introAddLContentDesc</t>
-  </si>
-  <si>
-    <t>The information that will help the learner to answer the questions.</t>
-  </si>
-  <si>
-    <t>De informatie die de cursist helpt om de vragen te beantwoorden.</t>
-  </si>
-  <si>
-    <t>Die Informationen, die dem Kursteilnehmer helfen, die Fragen zu beantworten.</t>
-  </si>
-  <si>
-    <t>introApplicationContent</t>
-  </si>
-  <si>
-    <t>Application concept</t>
-  </si>
-  <si>
-    <t>Toepassingsconcept</t>
-  </si>
-  <si>
-    <t>Anwendungskonzept</t>
-  </si>
-  <si>
-    <t>introApplicationContentDesc</t>
-  </si>
-  <si>
-    <t>How to provide a learner with a course?</t>
-  </si>
-  <si>
-    <t>Hoe biedt u een cursist toegang tot een cursus?</t>
-  </si>
-  <si>
-    <t>Wie wird einem Lernenden ein Kurs zur Verfügung gestellt?</t>
-  </si>
-  <si>
-    <t>introCreateCourse</t>
-  </si>
-  <si>
-    <t>Create course</t>
-  </si>
-  <si>
-    <t>Een cursus maken</t>
-  </si>
-  <si>
-    <t>Kurs erstellen</t>
-  </si>
-  <si>
-    <t>introCreateCourseDesc</t>
-  </si>
-  <si>
-    <t>Name the course and choose how you want to present it, as a simple course or as a quiz.</t>
-  </si>
-  <si>
-    <t>Geef de cursus een naam en geef aan of u deze als 'vrije stijl' of 'toets' wilt aanbieden.</t>
-  </si>
-  <si>
-    <t>Benenennen Sie den Kurs, und wählen Sie, wie er präsentiert werden soll, als Freestyle-Kurs oder als Quiz.</t>
-  </si>
-  <si>
-    <t>introConnectLOtoCourse</t>
-  </si>
-  <si>
-    <t>Connect learning objectives to the course</t>
-  </si>
-  <si>
-    <t>Verbind leerdoelen aan de cursus</t>
-  </si>
-  <si>
-    <t>Verbinden Sie Lernziele mit dem Kurs</t>
-  </si>
-  <si>
-    <t>introConnectLOtoCourseDesc</t>
-  </si>
-  <si>
-    <t>Assemble your course (simple course or quiz) by adding learning objectives to it. </t>
-  </si>
-  <si>
-    <t>Stel uw cursus (vrije stijl of toets) samen door er leerdoelen aan toe te voegen. </t>
-  </si>
-  <si>
-    <t>Stellen Sie Ihren Kurs (Freestyle-Kurs oder Quiz) zusammen, indem Sie ihm Lernziele zuordnen.</t>
-  </si>
-  <si>
-    <t>introPublishCourse</t>
-  </si>
-  <si>
-    <t>Publiceer de cursus</t>
-  </si>
-  <si>
-    <t>Veröffentlichen Sie den Kurs</t>
-  </si>
-  <si>
-    <t>introPublishCourseDesc</t>
-  </si>
-  <si>
-    <t>Publish to easygenerator web-server or to your own web server.</t>
-  </si>
-  <si>
-    <t>Publiceer de cursus naar de webserver van easygenerator of naar uw eigen webserver.</t>
-  </si>
-  <si>
-    <t>Veröffentlichen Sie ihn auf dem easygenerator-Webserver oder auf Ihrem eigenen Webserver.</t>
-  </si>
-  <si>
     <t>Error pages</t>
   </si>
   <si>
@@ -3198,6 +2903,9 @@
   </si>
   <si>
     <t>createCourseViewCaption</t>
+  </si>
+  <si>
+    <t>Create course</t>
   </si>
   <si>
     <t>Maak een cursus</t>
@@ -7633,1476 +7341,1477 @@
       <c t="s" s="36" r="A195">
         <v>711</v>
       </c>
-      <c t="s" s="1" r="B195">
+      <c t="s" s="6" r="B195">
         <v>712</v>
       </c>
-      <c t="s" s="45" r="C195">
+      <c t="s" s="11" r="C195">
         <v>713</v>
       </c>
-      <c t="s" s="33" r="D195">
+      <c t="s" s="2" r="D195">
         <v>714</v>
       </c>
-      <c t="s" s="33" r="E195">
+      <c t="s" s="2" r="E195">
         <v>715</v>
       </c>
     </row>
     <row r="196">
-      <c t="s" s="1" r="B196">
+      <c s="36" r="A196"/>
+      <c t="s" s="6" r="B196">
         <v>716</v>
       </c>
-      <c t="s" s="45" r="C196">
+      <c t="s" s="11" r="C196">
         <v>717</v>
       </c>
-      <c t="s" s="33" r="D196">
+      <c t="s" s="2" r="D196">
         <v>718</v>
       </c>
-      <c t="s" s="33" r="E196">
+      <c t="s" s="2" r="E196">
         <v>719</v>
       </c>
     </row>
     <row r="197">
       <c s="36" r="A197"/>
-      <c t="s" s="1" r="B197">
+      <c t="s" s="6" r="B197">
         <v>720</v>
       </c>
-      <c t="s" s="45" r="C197">
+      <c t="s" s="11" r="C197">
         <v>721</v>
       </c>
-      <c t="s" s="33" r="D197">
+      <c t="s" s="2" r="D197">
         <v>722</v>
       </c>
-      <c t="s" s="33" r="E197">
+      <c t="s" s="2" r="E197">
         <v>723</v>
       </c>
     </row>
     <row r="198">
       <c s="36" r="A198"/>
-      <c t="s" s="1" r="B198">
+      <c t="s" s="6" r="B198">
         <v>724</v>
       </c>
-      <c t="s" s="45" r="C198">
+      <c t="s" s="11" r="C198">
         <v>725</v>
       </c>
-      <c t="s" s="33" r="D198">
+      <c t="s" s="2" r="D198">
         <v>726</v>
       </c>
-      <c t="s" s="33" r="E198">
+      <c t="s" s="2" r="E198">
         <v>727</v>
       </c>
     </row>
     <row r="199">
       <c s="36" r="A199"/>
-      <c t="s" s="1" r="B199">
+      <c t="s" s="6" r="B199">
         <v>728</v>
       </c>
       <c t="s" s="11" r="C199">
         <v>729</v>
       </c>
-      <c t="s" s="33" r="D199">
+      <c t="s" s="2" r="D199">
         <v>730</v>
       </c>
-      <c t="s" s="33" r="E199">
-        <v>730</v>
+      <c t="s" s="2" r="E199">
+        <v>731</v>
       </c>
     </row>
     <row r="200">
       <c s="36" r="A200"/>
-      <c t="s" s="1" r="B200">
-        <v>731</v>
-      </c>
-      <c t="s" s="45" r="C200">
+      <c t="s" s="6" r="B200">
         <v>732</v>
       </c>
-      <c t="s" s="33" r="D200">
+      <c t="s" s="11" r="C200">
         <v>733</v>
       </c>
-      <c t="s" s="33" r="E200">
+      <c t="s" s="2" r="D200">
         <v>734</v>
+      </c>
+      <c t="s" s="2" r="E200">
+        <v>735</v>
       </c>
     </row>
     <row r="201">
       <c s="36" r="A201"/>
-      <c t="s" s="1" r="B201">
-        <v>735</v>
-      </c>
-      <c t="s" s="45" r="C201">
+      <c t="s" s="6" r="B201">
         <v>736</v>
       </c>
-      <c t="s" s="33" r="D201">
+      <c t="s" s="11" r="C201">
         <v>737</v>
       </c>
-      <c t="s" s="33" r="E201">
+      <c t="s" s="2" r="D201">
         <v>738</v>
+      </c>
+      <c t="s" s="2" r="E201">
+        <v>739</v>
       </c>
     </row>
     <row r="202">
       <c s="36" r="A202"/>
-      <c t="s" s="1" r="B202">
-        <v>739</v>
-      </c>
-      <c t="s" s="45" r="C202">
+      <c s="18" r="B202"/>
+      <c s="50" r="C202"/>
+      <c s="2" r="D202"/>
+      <c s="2" r="E202"/>
+    </row>
+    <row r="203">
+      <c t="s" s="36" r="A203">
         <v>740</v>
       </c>
-      <c t="s" s="33" r="D202">
+      <c t="s" s="29" r="B203">
         <v>741</v>
       </c>
-      <c t="s" s="33" r="E202">
+      <c t="s" s="26" r="C203">
         <v>742</v>
       </c>
-    </row>
-    <row r="203">
-      <c s="36" r="A203"/>
-      <c t="s" s="1" r="B203">
-        <v>743</v>
-      </c>
-      <c t="s" s="45" r="C203">
-        <v>744</v>
-      </c>
-      <c t="s" s="33" r="D203">
-        <v>745</v>
-      </c>
-      <c t="s" s="33" r="E203">
-        <v>746</v>
-      </c>
+      <c s="2" r="D203"/>
+      <c s="2" r="E203"/>
     </row>
     <row r="204">
       <c s="36" r="A204"/>
-      <c t="s" s="1" r="B204">
-        <v>747</v>
-      </c>
-      <c t="s" s="45" r="C204">
-        <v>748</v>
-      </c>
-      <c t="s" s="33" r="D204">
-        <v>749</v>
-      </c>
-      <c t="s" s="33" r="E204">
-        <v>750</v>
-      </c>
+      <c t="s" s="29" r="B204">
+        <v>743</v>
+      </c>
+      <c t="s" s="26" r="C204">
+        <v>744</v>
+      </c>
+      <c s="2" r="D204"/>
+      <c s="2" r="E204"/>
     </row>
     <row r="205">
       <c s="36" r="A205"/>
-      <c t="s" s="1" r="B205">
-        <v>751</v>
-      </c>
-      <c t="s" s="45" r="C205">
-        <v>752</v>
-      </c>
-      <c t="s" s="33" r="D205">
-        <v>753</v>
-      </c>
-      <c t="s" s="33" r="E205">
-        <v>754</v>
-      </c>
+      <c s="35" r="B205"/>
+      <c s="35" r="C205"/>
+      <c s="2" r="D205"/>
+      <c s="2" r="E205"/>
     </row>
     <row r="206">
-      <c s="36" r="A206"/>
-      <c t="s" s="1" r="B206">
-        <v>755</v>
-      </c>
-      <c t="s" s="45" r="C206">
-        <v>363</v>
-      </c>
-      <c t="s" s="33" r="D206">
-        <v>756</v>
-      </c>
-      <c t="s" s="33" r="E206">
-        <v>757</v>
+      <c t="s" s="36" r="A206">
+        <v>745</v>
+      </c>
+      <c t="s" s="47" r="B206">
+        <v>746</v>
+      </c>
+      <c t="s" s="47" r="C206">
+        <v>747</v>
+      </c>
+      <c t="s" s="2" r="D206">
+        <v>748</v>
+      </c>
+      <c t="s" s="2" r="E206">
+        <v>749</v>
       </c>
     </row>
     <row r="207">
       <c s="36" r="A207"/>
-      <c t="s" s="1" r="B207">
-        <v>758</v>
-      </c>
-      <c t="s" s="45" r="C207">
-        <v>759</v>
-      </c>
-      <c t="s" s="33" r="D207">
-        <v>760</v>
-      </c>
-      <c t="s" s="33" r="E207">
-        <v>761</v>
+      <c t="s" s="47" r="B207">
+        <v>750</v>
+      </c>
+      <c t="s" s="47" r="C207">
+        <v>751</v>
+      </c>
+      <c t="s" s="2" r="D207">
+        <v>751</v>
+      </c>
+      <c t="s" s="2" r="E207">
+        <v>752</v>
       </c>
     </row>
     <row r="208">
       <c s="36" r="A208"/>
-      <c t="s" s="1" r="B208">
-        <v>762</v>
-      </c>
-      <c t="s" s="45" r="C208">
-        <v>763</v>
-      </c>
-      <c t="s" s="33" r="D208">
-        <v>764</v>
-      </c>
-      <c t="s" s="33" r="E208">
-        <v>765</v>
+      <c t="s" s="47" r="B208">
+        <v>753</v>
+      </c>
+      <c t="s" s="47" r="C208">
+        <v>754</v>
+      </c>
+      <c t="s" s="2" r="D208">
+        <v>755</v>
+      </c>
+      <c t="s" s="2" r="E208">
+        <v>756</v>
       </c>
     </row>
     <row r="209">
       <c s="36" r="A209"/>
-      <c t="s" s="1" r="B209">
-        <v>766</v>
-      </c>
-      <c t="s" s="45" r="C209">
-        <v>767</v>
-      </c>
-      <c t="s" s="33" r="D209">
-        <v>768</v>
-      </c>
-      <c t="s" s="33" r="E209">
-        <v>769</v>
+      <c t="s" s="47" r="B209">
+        <v>757</v>
+      </c>
+      <c t="s" s="47" r="C209">
+        <v>758</v>
+      </c>
+      <c t="s" s="2" r="D209">
+        <v>759</v>
+      </c>
+      <c t="s" s="2" r="E209">
+        <v>318</v>
       </c>
     </row>
     <row r="210">
       <c s="36" r="A210"/>
-      <c t="s" s="1" r="B210">
-        <v>770</v>
-      </c>
-      <c t="s" s="45" r="C210">
-        <v>771</v>
-      </c>
-      <c t="s" s="33" r="D210">
-        <v>772</v>
-      </c>
-      <c t="s" s="33" r="E210">
-        <v>773</v>
+      <c t="s" s="11" r="B210">
+        <v>760</v>
+      </c>
+      <c t="s" s="11" r="C210">
+        <v>761</v>
+      </c>
+      <c t="s" s="2" r="D210">
+        <v>762</v>
+      </c>
+      <c t="s" s="2" r="E210">
+        <v>763</v>
       </c>
     </row>
     <row r="211">
       <c s="36" r="A211"/>
-      <c t="s" s="1" r="B211">
-        <v>774</v>
-      </c>
-      <c t="s" s="45" r="C211">
-        <v>775</v>
-      </c>
-      <c t="s" s="33" r="D211">
-        <v>776</v>
-      </c>
-      <c t="s" s="33" r="E211">
-        <v>777</v>
+      <c t="s" s="11" r="B211">
+        <v>764</v>
+      </c>
+      <c t="s" s="11" r="C211">
+        <v>765</v>
+      </c>
+      <c t="s" s="2" r="D211">
+        <v>766</v>
+      </c>
+      <c t="s" s="2" r="E211">
+        <v>767</v>
       </c>
     </row>
     <row r="212">
       <c s="36" r="A212"/>
-      <c t="s" s="1" r="B212">
-        <v>778</v>
-      </c>
-      <c t="s" s="45" r="C212">
-        <v>779</v>
-      </c>
-      <c t="s" s="33" r="D212">
-        <v>780</v>
-      </c>
-      <c t="s" s="33" r="E212">
-        <v>781</v>
+      <c t="s" s="11" r="B212">
+        <v>768</v>
+      </c>
+      <c t="s" s="11" r="C212">
+        <v>769</v>
+      </c>
+      <c t="s" s="2" r="D212">
+        <v>770</v>
+      </c>
+      <c t="s" s="2" r="E212">
+        <v>771</v>
       </c>
     </row>
     <row r="213">
       <c s="36" r="A213"/>
-      <c t="s" s="1" r="B213">
-        <v>782</v>
-      </c>
-      <c t="s" s="45" r="C213">
-        <v>783</v>
-      </c>
-      <c t="s" s="33" r="D213">
-        <v>784</v>
-      </c>
-      <c t="s" s="33" r="E213">
-        <v>785</v>
+      <c t="s" s="11" r="B213">
+        <v>772</v>
+      </c>
+      <c t="s" s="11" r="C213">
+        <v>773</v>
+      </c>
+      <c t="s" s="2" r="D213">
+        <v>774</v>
+      </c>
+      <c t="s" s="2" r="E213">
+        <v>775</v>
       </c>
     </row>
     <row r="214">
       <c s="36" r="A214"/>
-      <c t="s" s="1" r="B214">
-        <v>786</v>
-      </c>
-      <c t="s" s="45" r="C214">
-        <v>787</v>
-      </c>
-      <c t="s" s="33" r="D214">
-        <v>788</v>
-      </c>
-      <c t="s" s="33" r="E214">
-        <v>789</v>
+      <c t="s" s="11" r="B214">
+        <v>776</v>
+      </c>
+      <c t="s" s="11" r="C214">
+        <v>777</v>
+      </c>
+      <c t="s" s="2" r="D214">
+        <v>778</v>
+      </c>
+      <c t="s" s="2" r="E214">
+        <v>779</v>
       </c>
     </row>
     <row r="215">
       <c s="36" r="A215"/>
-      <c t="s" s="1" r="B215">
-        <v>790</v>
-      </c>
-      <c t="s" s="45" r="C215">
-        <v>791</v>
-      </c>
-      <c t="s" s="33" r="D215">
-        <v>792</v>
-      </c>
-      <c t="s" s="33" r="E215">
-        <v>793</v>
+      <c t="s" s="11" r="B215">
+        <v>780</v>
+      </c>
+      <c t="s" s="11" r="C215">
+        <v>781</v>
+      </c>
+      <c t="s" s="46" r="D215">
+        <v>782</v>
+      </c>
+      <c t="s" s="46" r="E215">
+        <v>783</v>
       </c>
     </row>
     <row r="216">
       <c s="36" r="A216"/>
-      <c t="s" s="1" r="B216">
-        <v>794</v>
-      </c>
-      <c t="s" s="45" r="C216">
-        <v>795</v>
-      </c>
-      <c t="s" s="33" r="D216">
-        <v>796</v>
-      </c>
-      <c t="s" s="33" r="E216">
-        <v>797</v>
+      <c t="s" s="11" r="B216">
+        <v>784</v>
+      </c>
+      <c t="s" s="11" r="C216">
+        <v>785</v>
+      </c>
+      <c t="s" s="46" r="D216">
+        <v>786</v>
+      </c>
+      <c t="s" s="46" r="E216">
+        <v>787</v>
       </c>
     </row>
     <row r="217">
       <c s="36" r="A217"/>
-      <c t="s" s="1" r="B217">
-        <v>798</v>
-      </c>
-      <c t="s" s="45" r="C217">
-        <v>799</v>
-      </c>
-      <c t="s" s="33" r="D217">
-        <v>800</v>
-      </c>
-      <c t="s" s="33" r="E217">
-        <v>801</v>
-      </c>
+      <c s="36" r="B217"/>
+      <c s="36" r="C217"/>
+      <c s="46" r="D217"/>
+      <c s="46" r="E217"/>
     </row>
     <row r="218">
       <c s="36" r="A218"/>
-      <c t="s" s="1" r="B218">
-        <v>802</v>
-      </c>
-      <c t="s" s="45" r="C218">
-        <v>252</v>
-      </c>
-      <c t="s" s="33" r="D218">
-        <v>803</v>
-      </c>
-      <c t="s" s="33" r="E218">
-        <v>804</v>
+      <c t="s" s="11" r="B218">
+        <v>788</v>
+      </c>
+      <c t="s" s="11" r="C218">
+        <v>789</v>
+      </c>
+      <c t="s" s="2" r="D218">
+        <v>790</v>
+      </c>
+      <c t="s" s="2" r="E218">
+        <v>791</v>
       </c>
     </row>
     <row r="219">
       <c s="36" r="A219"/>
-      <c t="s" s="1" r="B219">
-        <v>805</v>
-      </c>
-      <c t="s" s="45" r="C219">
-        <v>806</v>
-      </c>
-      <c t="s" s="23" r="D219">
-        <v>807</v>
-      </c>
-      <c t="s" s="23" r="E219">
-        <v>808</v>
+      <c t="s" s="6" r="B219">
+        <v>792</v>
+      </c>
+      <c t="s" s="11" r="C219">
+        <v>793</v>
+      </c>
+      <c t="s" s="2" r="D219">
+        <v>794</v>
+      </c>
+      <c t="s" s="2" r="E219">
+        <v>795</v>
       </c>
     </row>
     <row r="220">
       <c s="36" r="A220"/>
-      <c s="10" r="B220"/>
-      <c s="12" r="C220"/>
-      <c s="2" r="D220"/>
-      <c s="2" r="E220"/>
+      <c t="s" s="6" r="B220">
+        <v>796</v>
+      </c>
+      <c t="s" s="11" r="C220">
+        <v>797</v>
+      </c>
+      <c t="s" s="2" r="D220">
+        <v>798</v>
+      </c>
+      <c t="s" s="2" r="E220">
+        <v>799</v>
+      </c>
     </row>
     <row r="221">
-      <c t="s" s="36" r="A221">
-        <v>809</v>
-      </c>
+      <c s="36" r="A221"/>
       <c t="s" s="6" r="B221">
-        <v>810</v>
+        <v>800</v>
       </c>
       <c t="s" s="11" r="C221">
-        <v>811</v>
+        <v>801</v>
       </c>
       <c t="s" s="2" r="D221">
-        <v>812</v>
+        <v>802</v>
       </c>
       <c t="s" s="2" r="E221">
-        <v>813</v>
+        <v>803</v>
       </c>
     </row>
     <row r="222">
       <c s="36" r="A222"/>
       <c t="s" s="6" r="B222">
-        <v>814</v>
+        <v>804</v>
       </c>
       <c t="s" s="11" r="C222">
-        <v>815</v>
+        <v>805</v>
       </c>
       <c t="s" s="2" r="D222">
-        <v>816</v>
+        <v>806</v>
       </c>
       <c t="s" s="2" r="E222">
-        <v>817</v>
+        <v>807</v>
       </c>
     </row>
     <row r="223">
       <c s="36" r="A223"/>
       <c t="s" s="6" r="B223">
-        <v>818</v>
+        <v>808</v>
       </c>
       <c t="s" s="11" r="C223">
-        <v>819</v>
-      </c>
-      <c t="s" s="2" r="D223">
-        <v>820</v>
-      </c>
-      <c t="s" s="2" r="E223">
-        <v>821</v>
+        <v>809</v>
+      </c>
+      <c t="s" s="23" r="D223">
+        <v>810</v>
+      </c>
+      <c t="s" s="23" r="E223">
+        <v>811</v>
       </c>
     </row>
     <row r="224">
       <c s="36" r="A224"/>
       <c t="s" s="6" r="B224">
-        <v>822</v>
+        <v>812</v>
       </c>
       <c t="s" s="11" r="C224">
-        <v>823</v>
+        <v>813</v>
       </c>
       <c t="s" s="2" r="D224">
-        <v>824</v>
+        <v>814</v>
       </c>
       <c t="s" s="2" r="E224">
-        <v>825</v>
+        <v>815</v>
       </c>
     </row>
     <row r="225">
       <c s="36" r="A225"/>
       <c t="s" s="6" r="B225">
-        <v>826</v>
+        <v>816</v>
       </c>
       <c t="s" s="11" r="C225">
-        <v>827</v>
+        <v>817</v>
       </c>
       <c t="s" s="2" r="D225">
-        <v>828</v>
+        <v>818</v>
       </c>
       <c t="s" s="2" r="E225">
-        <v>829</v>
+        <v>819</v>
       </c>
     </row>
     <row r="226">
       <c s="36" r="A226"/>
       <c t="s" s="6" r="B226">
-        <v>830</v>
+        <v>820</v>
       </c>
       <c t="s" s="11" r="C226">
-        <v>831</v>
+        <v>821</v>
       </c>
       <c t="s" s="2" r="D226">
-        <v>832</v>
+        <v>822</v>
       </c>
       <c t="s" s="2" r="E226">
-        <v>833</v>
+        <v>823</v>
       </c>
     </row>
     <row r="227">
       <c s="36" r="A227"/>
       <c t="s" s="6" r="B227">
-        <v>834</v>
+        <v>824</v>
       </c>
       <c t="s" s="11" r="C227">
-        <v>835</v>
+        <v>825</v>
       </c>
       <c t="s" s="2" r="D227">
-        <v>836</v>
+        <v>826</v>
       </c>
       <c t="s" s="2" r="E227">
-        <v>837</v>
+        <v>827</v>
       </c>
     </row>
     <row r="228">
       <c s="36" r="A228"/>
-      <c s="18" r="B228"/>
-      <c s="50" r="C228"/>
-      <c s="2" r="D228"/>
-      <c s="2" r="E228"/>
+      <c t="s" s="6" r="B228">
+        <v>828</v>
+      </c>
+      <c t="s" s="11" r="C228">
+        <v>829</v>
+      </c>
+      <c t="s" s="2" r="D228">
+        <v>830</v>
+      </c>
+      <c t="s" s="2" r="E228">
+        <v>831</v>
+      </c>
     </row>
     <row r="229">
-      <c t="s" s="36" r="A229">
-        <v>838</v>
-      </c>
-      <c t="s" s="29" r="B229">
-        <v>839</v>
-      </c>
-      <c t="s" s="26" r="C229">
-        <v>840</v>
-      </c>
+      <c s="36" r="A229"/>
+      <c s="14" r="B229"/>
+      <c s="50" r="C229"/>
       <c s="2" r="D229"/>
       <c s="2" r="E229"/>
     </row>
     <row r="230">
-      <c s="36" r="A230"/>
-      <c t="s" s="29" r="B230">
-        <v>841</v>
-      </c>
-      <c t="s" s="26" r="C230">
-        <v>842</v>
-      </c>
-      <c s="2" r="D230"/>
-      <c s="2" r="E230"/>
+      <c t="s" s="36" r="A230">
+        <v>832</v>
+      </c>
+      <c t="s" s="47" r="B230">
+        <v>833</v>
+      </c>
+      <c t="s" s="6" r="C230">
+        <v>751</v>
+      </c>
+      <c t="s" s="2" r="D230">
+        <v>751</v>
+      </c>
+      <c t="s" s="2" r="E230">
+        <v>752</v>
+      </c>
     </row>
     <row r="231">
       <c s="36" r="A231"/>
-      <c s="35" r="B231"/>
-      <c s="35" r="C231"/>
-      <c s="2" r="D231"/>
-      <c s="2" r="E231"/>
+      <c t="s" s="6" r="B231">
+        <v>834</v>
+      </c>
+      <c t="s" s="11" r="C231">
+        <v>754</v>
+      </c>
+      <c t="s" s="2" r="D231">
+        <v>755</v>
+      </c>
+      <c t="s" s="2" r="E231">
+        <v>756</v>
+      </c>
     </row>
     <row r="232">
-      <c t="s" s="36" r="A232">
-        <v>843</v>
-      </c>
-      <c t="s" s="47" r="B232">
-        <v>844</v>
-      </c>
-      <c t="s" s="47" r="C232">
-        <v>845</v>
+      <c t="s" s="6" r="B232">
+        <v>835</v>
+      </c>
+      <c t="s" s="11" r="C232">
+        <v>836</v>
       </c>
       <c t="s" s="2" r="D232">
-        <v>846</v>
+        <v>837</v>
       </c>
       <c t="s" s="2" r="E232">
-        <v>847</v>
+        <v>838</v>
       </c>
     </row>
     <row r="233">
       <c s="36" r="A233"/>
-      <c t="s" s="47" r="B233">
-        <v>848</v>
-      </c>
-      <c t="s" s="47" r="C233">
-        <v>849</v>
+      <c t="s" s="6" r="B233">
+        <v>839</v>
+      </c>
+      <c t="s" s="11" r="C233">
+        <v>840</v>
       </c>
       <c t="s" s="2" r="D233">
-        <v>849</v>
+        <v>841</v>
       </c>
       <c t="s" s="2" r="E233">
-        <v>850</v>
+        <v>842</v>
       </c>
     </row>
     <row r="234">
       <c s="36" r="A234"/>
-      <c t="s" s="47" r="B234">
-        <v>851</v>
-      </c>
-      <c t="s" s="47" r="C234">
-        <v>852</v>
+      <c t="s" s="6" r="B234">
+        <v>843</v>
+      </c>
+      <c t="s" s="11" r="C234">
+        <v>844</v>
       </c>
       <c t="s" s="2" r="D234">
-        <v>853</v>
+        <v>845</v>
       </c>
       <c t="s" s="2" r="E234">
-        <v>854</v>
+        <v>846</v>
       </c>
     </row>
     <row r="235">
       <c s="36" r="A235"/>
-      <c t="s" s="47" r="B235">
-        <v>855</v>
-      </c>
-      <c t="s" s="47" r="C235">
-        <v>856</v>
-      </c>
-      <c t="s" s="2" r="D235">
-        <v>857</v>
-      </c>
-      <c t="s" s="2" r="E235">
-        <v>318</v>
-      </c>
+      <c s="10" r="B235"/>
+      <c s="12" r="C235"/>
+      <c s="2" r="D235"/>
+      <c s="2" r="E235"/>
     </row>
     <row r="236">
-      <c s="36" r="A236"/>
-      <c t="s" s="11" r="B236">
-        <v>858</v>
+      <c t="s" s="36" r="A236">
+        <v>847</v>
+      </c>
+      <c t="s" s="6" r="B236">
+        <v>848</v>
       </c>
       <c t="s" s="11" r="C236">
-        <v>859</v>
+        <v>847</v>
       </c>
       <c t="s" s="2" r="D236">
-        <v>860</v>
+        <v>849</v>
       </c>
       <c t="s" s="2" r="E236">
-        <v>861</v>
+        <v>850</v>
       </c>
     </row>
     <row r="237">
       <c s="36" r="A237"/>
-      <c t="s" s="11" r="B237">
-        <v>862</v>
+      <c t="s" s="6" r="B237">
+        <v>851</v>
       </c>
       <c t="s" s="11" r="C237">
-        <v>863</v>
+        <v>852</v>
       </c>
       <c t="s" s="2" r="D237">
-        <v>864</v>
+        <v>853</v>
       </c>
       <c t="s" s="2" r="E237">
-        <v>865</v>
+        <v>854</v>
       </c>
     </row>
     <row r="238">
       <c s="36" r="A238"/>
-      <c t="s" s="11" r="B238">
-        <v>866</v>
+      <c t="s" s="6" r="B238">
+        <v>855</v>
       </c>
       <c t="s" s="11" r="C238">
-        <v>867</v>
+        <v>856</v>
       </c>
       <c t="s" s="2" r="D238">
-        <v>868</v>
+        <v>857</v>
       </c>
       <c t="s" s="2" r="E238">
-        <v>869</v>
+        <v>858</v>
       </c>
     </row>
     <row r="239">
       <c s="36" r="A239"/>
-      <c t="s" s="11" r="B239">
-        <v>870</v>
+      <c t="s" s="6" r="B239">
+        <v>859</v>
       </c>
       <c t="s" s="11" r="C239">
-        <v>871</v>
+        <v>860</v>
       </c>
       <c t="s" s="2" r="D239">
-        <v>872</v>
+        <v>861</v>
       </c>
       <c t="s" s="2" r="E239">
-        <v>873</v>
+        <v>862</v>
       </c>
     </row>
     <row r="240">
       <c s="36" r="A240"/>
-      <c t="s" s="11" r="B240">
-        <v>874</v>
+      <c t="s" s="6" r="B240">
+        <v>863</v>
       </c>
       <c t="s" s="11" r="C240">
-        <v>875</v>
+        <v>864</v>
       </c>
       <c t="s" s="2" r="D240">
-        <v>876</v>
+        <v>865</v>
       </c>
       <c t="s" s="2" r="E240">
-        <v>877</v>
+        <v>866</v>
       </c>
     </row>
     <row r="241">
       <c s="36" r="A241"/>
-      <c t="s" s="11" r="B241">
-        <v>878</v>
+      <c t="s" s="6" r="B241">
+        <v>867</v>
       </c>
       <c t="s" s="11" r="C241">
-        <v>879</v>
-      </c>
-      <c t="s" s="46" r="D241">
-        <v>880</v>
-      </c>
-      <c t="s" s="46" r="E241">
-        <v>881</v>
+        <v>868</v>
+      </c>
+      <c t="s" s="2" r="D241">
+        <v>869</v>
+      </c>
+      <c t="s" s="2" r="E241">
+        <v>870</v>
       </c>
     </row>
     <row r="242">
       <c s="36" r="A242"/>
-      <c t="s" s="11" r="B242">
-        <v>882</v>
+      <c t="s" s="6" r="B242">
+        <v>871</v>
       </c>
       <c t="s" s="11" r="C242">
-        <v>883</v>
-      </c>
-      <c t="s" s="46" r="D242">
-        <v>884</v>
-      </c>
-      <c t="s" s="46" r="E242">
-        <v>885</v>
+        <v>872</v>
+      </c>
+      <c t="s" s="2" r="D242">
+        <v>873</v>
+      </c>
+      <c t="s" s="2" r="E242">
+        <v>874</v>
       </c>
     </row>
     <row r="243">
       <c s="36" r="A243"/>
-      <c s="36" r="B243"/>
-      <c s="36" r="C243"/>
-      <c s="46" r="D243"/>
-      <c s="46" r="E243"/>
+      <c s="10" r="B243"/>
+      <c s="12" r="C243"/>
+      <c s="2" r="D243"/>
+      <c s="2" r="E243"/>
     </row>
     <row r="244">
-      <c s="36" r="A244"/>
-      <c t="s" s="11" r="B244">
-        <v>886</v>
+      <c t="s" s="36" r="A244">
+        <v>875</v>
+      </c>
+      <c t="s" s="6" r="B244">
+        <v>876</v>
       </c>
       <c t="s" s="11" r="C244">
-        <v>887</v>
+        <v>877</v>
       </c>
       <c t="s" s="2" r="D244">
-        <v>888</v>
+        <v>878</v>
       </c>
       <c t="s" s="2" r="E244">
-        <v>889</v>
+        <v>879</v>
       </c>
     </row>
     <row r="245">
       <c s="36" r="A245"/>
       <c t="s" s="6" r="B245">
-        <v>890</v>
+        <v>880</v>
       </c>
       <c t="s" s="11" r="C245">
-        <v>891</v>
+        <v>881</v>
       </c>
       <c t="s" s="2" r="D245">
-        <v>892</v>
+        <v>881</v>
       </c>
       <c t="s" s="2" r="E245">
-        <v>893</v>
+        <v>882</v>
       </c>
     </row>
     <row r="246">
       <c s="36" r="A246"/>
-      <c t="s" s="6" r="B246">
-        <v>894</v>
-      </c>
-      <c t="s" s="11" r="C246">
-        <v>895</v>
-      </c>
-      <c t="s" s="2" r="D246">
-        <v>896</v>
-      </c>
-      <c t="s" s="2" r="E246">
-        <v>897</v>
-      </c>
+      <c s="10" r="B246"/>
+      <c s="12" r="C246"/>
+      <c s="2" r="D246"/>
+      <c s="2" r="E246"/>
     </row>
     <row r="247">
-      <c s="36" r="A247"/>
+      <c t="s" s="36" r="A247">
+        <v>883</v>
+      </c>
       <c t="s" s="6" r="B247">
-        <v>898</v>
+        <v>884</v>
       </c>
       <c t="s" s="11" r="C247">
-        <v>899</v>
+        <v>885</v>
       </c>
       <c t="s" s="2" r="D247">
-        <v>900</v>
+        <v>886</v>
       </c>
       <c t="s" s="2" r="E247">
-        <v>901</v>
+        <v>887</v>
       </c>
     </row>
     <row r="248">
       <c s="36" r="A248"/>
       <c t="s" s="6" r="B248">
-        <v>902</v>
+        <v>888</v>
       </c>
       <c t="s" s="11" r="C248">
-        <v>903</v>
+        <v>889</v>
       </c>
       <c t="s" s="2" r="D248">
-        <v>904</v>
+        <v>890</v>
       </c>
       <c t="s" s="2" r="E248">
-        <v>905</v>
+        <v>891</v>
       </c>
     </row>
     <row r="249">
       <c s="36" r="A249"/>
       <c t="s" s="6" r="B249">
-        <v>906</v>
+        <v>892</v>
       </c>
       <c t="s" s="11" r="C249">
-        <v>907</v>
-      </c>
-      <c t="s" s="23" r="D249">
-        <v>908</v>
-      </c>
-      <c t="s" s="23" r="E249">
-        <v>909</v>
+        <v>893</v>
+      </c>
+      <c t="s" s="2" r="D249">
+        <v>894</v>
+      </c>
+      <